<commit_message>
trained models are stored + diagnoser is maybe ready
</commit_message>
<xml_diff>
--- a/experimental results/e2000_Acrobot.xlsx
+++ b/experimental results/e2000_Acrobot.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="305">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="303">
   <si>
     <t>01_i_domain_name</t>
   </si>
@@ -70,766 +70,760 @@
     <t>[1,1,2]</t>
   </si>
   <si>
-    <t>[15, 40, 41, 42, 53, 55, 66, 69, 70]</t>
-  </si>
-  <si>
-    <t>[0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 1, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 1, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2]</t>
-  </si>
-  <si>
-    <t>['[-0.03763371 -0.01533471  0.06554052 -0.01816017]', '[-0.00754409 -0.05458322  0.2277812  -0.36241836]', '[ 0.04879627 -0.15231473  0.32089719 -0.5887683 ]', '[ 0.11397169 -0.27767857  0.31375488 -0.63332862]', '[ 0.16759438 -0.39312519  0.2086893  -0.49480525]', '[ 0.1930193  -0.46685036  0.03906408 -0.22816919]', '[ 0.15689524 -0.41528579 -0.3922057   0.73207416]', '[ 0.04309269 -0.18588535 -0.71796191  1.51055937]', '[-0.1147829   0.15904975 -0.81547211  1.84906375]', '[-0.26363568  0.51494657 -0.63159042  1.62703318]', '[-0.35418658  0.78351571 -0.2539271   1.01663306]', '[-0.36122763  0.91144819  0.18313112  0.25239067]', '[-0.26190848  0.82452699  0.79137833 -1.10754289]', '[-0.05546354  0.48017359  1.23429726 -2.2781243 ]', '[ 0.20909957 -0.04617758  1.33805656 -2.84269804]', '[ 0.4338505  -0.55785781  0.84805213 -2.15416029]', '[ 0.54411235 -0.9088711   0.23229783 -1.31062519]', '[ 0.52393536 -1.07260775 -0.42702541 -0.31831069]', '[ 0.35974646 -0.97931431 -1.18360253  1.23792287]', '[ 0.06653892 -0.58888907 -1.69685647  2.6040146 ]', '[-0.29014723  0.0146915  -1.77739719  3.25525804]', '[-0.6026696   0.63119819 -1.26446668  2.75245598]', '[-0.7733342   1.07759912 -0.41456703  1.67016058]', '[-0.76478963  1.29221739  0.493699    0.46747102]', '[-0.56475857  1.20855233  1.47115693 -1.30498865]', '[-0.19437129  0.77344772  2.17666703 -3.00375101]', '[ 0.27380456  0.05373306  2.39044378 -3.97413489]', '[ 0.70570428 -0.70219442  1.81628335 -3.36979743]', '[ 0.97215691 -1.2508318   0.81545936 -2.08895769]', '[ 1.02638887 -1.5374708  -0.27354814 -0.77647533]', '[ 0.85039812 -1.50810663 -1.45795886  1.08609947]', '[ 0.45864643 -1.09377036 -2.41291479  3.06763652]', '[-0.08941807 -0.29880789 -2.96219916  4.69970881]', '[-0.65833398  0.64277316 -2.56022809  4.36604385]', '[-1.06954389  1.36962149 -1.50603098  2.86960002]', '[-1.25303457  1.80046653 -0.32099756  1.46308562]', '[-1.19798253  1.95789308  0.86191516  0.10156751]', '[-0.90231962  1.78652505  2.05694835 -1.85114411]', '[-0.39450095  1.20016267  2.97077234 -4.0417293 ]', '[ 0.25925319  0.19049266  3.4321998  -5.78146579]', '[ 0.87738275 -0.87971178  2.58084621 -4.56532946]', '[ 1.26414748 -1.60052753  1.27236747 -2.6874927 ]', '[ 1.38544858 -1.97592742 -0.05695913 -1.09262457]', '[ 1.24455424 -2.03694563 -1.33538713  0.50529499]', '[ 0.85574795 -1.73572757 -2.50980703  2.55986947]', '[ 0.26100408 -0.99098482 -3.3848437   4.90166432]', '[-0.4585068   0.1601927  -3.60679906  6.14517394]', '[-1.08640485  1.25002122 -2.55194055  4.53011332]', '[-1.4675753   1.98259192 -1.25508593  2.87255425]', '[-1.58839726  2.42034546  0.04325397  1.52491282]', '[-1.45309087  2.59081773  1.2989955   0.16184205]', '[-1.06476292  2.43477902  2.54241849 -1.7550503 ]', '[-0.46402616  1.87217068  3.37995243 -3.91899898]', '[ 0.24766292  0.88078079  3.66979677 -5.9232865 ]', '[ 0.96182243 -0.39937804  3.24952712 -6.34225658]', '[ 1.46040321 -1.46525616  1.69057645 -4.28698311]', '[ 1.64782616 -2.17125737  0.18902551 -2.81746832]', '[ 1.54128786 -2.59479645 -1.23343141 -1.40185548]', '[ 1.15380151 -2.68396673 -2.59816505  0.52450651]', '[ 0.53013284 -2.38143123 -3.52791518  2.50565257]', '[-0.20080539 -1.68522966 -3.66060889  4.4232215 ]', '[-0.90372842 -0.64350859 -3.31345545  5.82817931]', '[-1.48165266  0.51637696 -2.32681643  5.43731254]', '[-1.79510533  1.46454785 -0.76793597  4.03696213]', '[-1.78049131  2.13587956  0.92075914  2.65143933]', '[-1.42704294  2.48369846  2.57039868  0.77328163]', '[-0.77859651  2.4287353   3.810517   -1.34414705]', '[ 0.04174318  1.92828639  4.21804957 -3.61943615]', '[ 0.85103668  1.01827234  3.79761596 -5.32707703]', '[ 1.52269656 -0.06834511  2.82743793 -5.22570896]', '[ 1.95153449 -0.98819014  1.43725805 -3.94393765]', '[ 2.10439819 -1.68864872  0.06899327 -3.06607377]', '[ 1.9682971  -2.19981076 -1.44959828 -1.96979882]', '[ 1.51198205 -2.39705738 -3.08375512  0.09529889]', '[ 0.75938863 -2.12363224 -4.33037208  2.72719178]', '[-0.15974441 -1.28531868 -4.73761044  5.63644387]', '[-1.09457479  0.04600497 -4.43204498  7.11966874]', '[-1.84678911  1.31345131 -3.02322424  5.3827863 ]', '[-2.31957853  2.25370649 -1.75884488  4.17401861]', '[-2.57304816  3.01895479 -0.85152342  3.51699117]', '[-2.69212594 -2.62126772 -0.40896088  2.90406145]', '[-2.75202379 -2.10950219 -0.20343055  2.19595886]', '[-2.77145559 -1.75020593  0.02319961  1.38013099]']</t>
-  </si>
-  <si>
-    <t>[0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50, 51, 52, 53, 54, 55, 56, 57, 58, 59, 60, 61, 62, 63, 64, 65, 66, 67, 68, 69, 70, 71, 72, 73, 74, 75, 76, 77, 78, 79, 80, 81, 82]</t>
-  </si>
-  <si>
-    <t>[array([-0.03763371, -0.01533471,  0.06554052, -0.01816017], dtype=float32), array([-0.00754409, -0.05458322,  0.2277812 , -0.36241836]), array([ 0.04879627, -0.15231473,  0.32089719, -0.5887683 ]), array([ 0.11397169, -0.27767857,  0.31375488, -0.63332862]), array([ 0.16759438, -0.39312519,  0.2086893 , -0.49480525]), array([ 0.1930193 , -0.46685036,  0.03906408, -0.22816919]), array([ 0.15689524, -0.41528579, -0.3922057 ,  0.73207416]), array([ 0.04309269, -0.18588535, -0.71796191,  1.51055937]), array([-0.1147829 ,  0.15904975, -0.81547211,  1.84906375]), array([-0.26363568,  0.51494657, -0.63159042,  1.62703318]), array([-0.35418658,  0.78351571, -0.2539271 ,  1.01663306]), array([-0.36122763,  0.91144819,  0.18313112,  0.25239067]), array([-0.26190848,  0.82452699,  0.79137833, -1.10754289]), array([-0.05546354,  0.48017359,  1.23429726, -2.2781243 ]), array([ 0.20909957, -0.04617758,  1.33805656, -2.84269804]), array([ 0.4338505 , -0.55785781,  0.84805213, -2.15416029]), array([ 0.54411235, -0.9088711 ,  0.23229783, -1.31062519]), array([ 0.52393536, -1.07260775, -0.42702541, -0.31831069]), array([ 0.35974646, -0.97931431, -1.18360253,  1.23792287]), array([ 0.06653892, -0.58888907, -1.69685647,  2.6040146 ]), array([-0.29014723,  0.0146915 , -1.77739719,  3.25525804]), array([-0.6026696 ,  0.63119819, -1.26446668,  2.75245598]), array([-0.7733342 ,  1.07759912, -0.41456703,  1.67016058]), array([-0.76478963,  1.29221739,  0.493699  ,  0.46747102]), array([-0.56475857,  1.20855233,  1.47115693, -1.30498865]), array([-0.19437129,  0.77344772,  2.17666703, -3.00375101]), array([ 0.27380456,  0.05373306,  2.39044378, -3.97413489]), array([ 0.70570428, -0.70219442,  1.81628335, -3.36979743]), array([ 0.97215691, -1.2508318 ,  0.81545936, -2.08895769]), array([ 1.02638887, -1.5374708 , -0.27354814, -0.77647533]), array([ 0.85039812, -1.50810663, -1.45795886,  1.08609947]), array([ 0.45864643, -1.09377036, -2.41291479,  3.06763652]), array([-0.08941807, -0.29880789, -2.96219916,  4.69970881]), array([-0.65833398,  0.64277316, -2.56022809,  4.36604385]), array([-1.06954389,  1.36962149, -1.50603098,  2.86960002]), array([-1.25303457,  1.80046653, -0.32099756,  1.46308562]), array([-1.19798253,  1.95789308,  0.86191516,  0.10156751]), array([-0.90231962,  1.78652505,  2.05694835, -1.85114411]), array([-0.39450095,  1.20016267,  2.97077234, -4.0417293 ]), array([ 0.25925319,  0.19049266,  3.4321998 , -5.78146579]), array([ 0.87738275, -0.87971178,  2.58084621, -4.56532946]), array([ 1.26414748, -1.60052753,  1.27236747, -2.6874927 ]), array([ 1.38544858, -1.97592742, -0.05695913, -1.09262457]), array([ 1.24455424, -2.03694563, -1.33538713,  0.50529499]), array([ 0.85574795, -1.73572757, -2.50980703,  2.55986947]), array([ 0.26100408, -0.99098482, -3.3848437 ,  4.90166432]), array([-0.4585068 ,  0.1601927 , -3.60679906,  6.14517394]), array([-1.08640485,  1.25002122, -2.55194055,  4.53011332]), array([-1.4675753 ,  1.98259192, -1.25508593,  2.87255425]), array([-1.58839726,  2.42034546,  0.04325397,  1.52491282]), array([-1.45309087,  2.59081773,  1.2989955 ,  0.16184205]), array([-1.06476292,  2.43477902,  2.54241849, -1.7550503 ]), array([-0.46402616,  1.87217068,  3.37995243, -3.91899898]), array([ 0.24766292,  0.88078079,  3.66979677, -5.9232865 ]), array([ 0.96182243, -0.39937804,  3.24952712, -6.34225658]), array([ 1.46040321, -1.46525616,  1.69057645, -4.28698311]), array([ 1.64782616, -2.17125737,  0.18902551, -2.81746832]), array([ 1.54128786, -2.59479645, -1.23343141, -1.40185548]), array([ 1.15380151, -2.68396673, -2.59816505,  0.52450651]), array([ 0.53013284, -2.38143123, -3.52791518,  2.50565257]), array([-0.20080539, -1.68522966, -3.66060889,  4.4232215 ]), array([-0.90372842, -0.64350859, -3.31345545,  5.82817931]), array([-1.48165266,  0.51637696, -2.32681643,  5.43731254]), array([-1.79510533,  1.46454785, -0.76793597,  4.03696213]), array([-1.78049131,  2.13587956,  0.92075914,  2.65143933]), array([-1.42704294,  2.48369846,  2.57039868,  0.77328163]), array([-0.77859651,  2.4287353 ,  3.810517  , -1.34414705]), array([ 0.04174318,  1.92828639,  4.21804957, -3.61943615]), array([ 0.85103668,  1.01827234,  3.79761596, -5.32707703]), array([ 1.52269656, -0.06834511,  2.82743793, -5.22570896]), array([ 1.95153449, -0.98819014,  1.43725805, -3.94393765]), array([ 2.10439819, -1.68864872,  0.06899327, -3.06607377]), array([ 1.9682971 , -2.19981076, -1.44959828, -1.96979882]), array([ 1.51198205, -2.39705738, -3.08375512,  0.09529889]), array([ 0.75938863, -2.12363224, -4.33037208,  2.72719178]), array([-0.15974441, -1.28531868, -4.73761044,  5.63644387]), array([-1.09457479,  0.04600497, -4.43204498,  7.11966874]), array([-1.84678911,  1.31345131, -3.02322424,  5.3827863 ]), array([-2.31957853,  2.25370649, -1.75884488,  4.17401861]), array([-2.57304816,  3.01895479, -0.85152342,  3.51699117]), array([-2.69212594, -2.62126772, -0.40896088,  2.90406145]), array([-2.75202379, -2.10950219, -0.20343055,  2.19595886]), array([-2.77145559, -1.75020593,  0.02319961,  1.38013099])]</t>
-  </si>
-  <si>
-    <t>['[1,1,1]', '[1,1,2]', '[0,2,1]', '[1,2,0]', '[1,0,2]', '[2,1,0]', '[2,2,2]', '[2,0,1]', '[0,0,0]', '[0,1,1]']</t>
-  </si>
-  <si>
-    <t>[1, 3, 5, 17, 25, 28, 29, 36, 50, 52, 55, 56, 70, 71, 90]</t>
-  </si>
-  <si>
-    <t>[0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 1, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2]</t>
-  </si>
-  <si>
-    <t>['[-0.03763371 -0.01533471  0.06554052 -0.01816017]', '[-0.0208055  -0.02030166  0.09914155 -0.02801351]', '[ 0.013578   -0.05917353  0.23628798 -0.34824344]', '[ 0.05569493 -0.11750576  0.17467028 -0.21881458]', '[ 0.09321032 -0.17559542  0.19101534 -0.34617425]', '[ 0.11494541 -0.21477236  0.02111502 -0.03635698]', '[ 0.08803171 -0.15527598 -0.28298244  0.61721212]', '[ 0.00771379  0.02051943 -0.49814643  1.09748723]', '[-0.09992322  0.2613885  -0.54781767  1.25079563]', '[-0.19899582  0.49621087 -0.41673597  1.04534563]', '[-0.2580581   0.66242577 -0.16029595  0.58814693]', '[-0.26017189  0.72426166  0.13930997  0.02389421]', '[-0.18064923  0.61001101  0.64091503 -1.14763298]', '[-0.01369954  0.28056091  0.99109498 -2.07970048]', '[ 0.19459177 -0.18092928  1.02977955 -2.41098167]', '[ 0.37243687 -0.63206098  0.69861701 -2.00005475]', '[ 0.46011212 -0.95316036  0.16174322 -1.17326704]', '[ 0.42537627 -1.06524089 -0.49664074  0.05178195]', '[ 0.25924884 -0.90689492 -1.13554472  1.51266653]', '[-0.01379993 -0.47540523 -1.54414875  2.72653459]', '[-0.3292649   0.13059648 -1.52098835  3.15699007]', '[-0.58467466  0.71332982 -0.96429096  2.53978023]', '[-0.69777494  1.11628807 -0.14936694  1.45645161]', '[-0.64433925  1.29003413  0.66881172  0.2760153 ]', '[-0.42231877  1.17306991  1.50990699 -1.43665973]', '[-0.07111479  0.75438868  1.94117555 -2.68416081]', '[ 0.33560416  0.11506689  2.03003906 -3.52819267]', '[ 0.69501986 -0.56511932  1.46746056 -3.08665122]', '[ 0.88484758 -1.04433681  0.40582077 -1.6728194 ]', '[ 0.85542822 -1.23060088 -0.68977317 -0.18289421]', '[ 0.60841282 -1.08579727 -1.74321229  1.63796675]', '[ 0.17832049 -0.58015369 -2.48775454  3.3472159 ]', '[-0.34375825  0.18072445 -2.59235808  3.98171196]', '[-0.80094618  0.89723241 -1.88397553  3.01969304]', '[-1.07621992  1.36710168 -0.84333561  1.68029916]', '[-1.13342628  1.57404756  0.27330188  0.39205272]', '[-0.96138203  1.4949075   1.42725158 -1.20563517]', '[-0.56540277  1.05321555  2.49310348 -3.23510873]', '[ 0.0113307   0.21668057  3.15814153 -4.92308468]', '[ 0.62238874 -0.7540897   2.77772679 -4.41696087]', '[ 1.07994183 -1.47825656  1.75394785 -2.81118852]', '[ 1.3155028  -1.89414321  0.59014308 -1.38352358]', '[ 1.31415662 -2.03876785 -0.60072395 -0.06057471]', '[ 1.06553321 -1.86592768 -1.86135998  1.82843448]', '[ 0.58306205 -1.28468987 -2.92653754  4.04232752]', '[-0.0847069  -0.2500291  -3.62797837  6.06844474]', '[-0.77254409  0.92469989 -3.04195448  5.2214648 ]', '[-1.26346642  1.77978029 -1.84454069  3.37719485]', '[-1.50715244  2.30491798 -0.58893267  1.92168017]', '[-1.4996076   2.55585612  0.658817    0.58515642]', '[-1.24179447  2.51280732  1.89719688 -1.03892162]', '[-0.75115069  2.10667206  2.94433604 -3.0686173 ]', '[-0.10232982  1.28889494  3.47932462 -5.1244788 ]', '[ 0.62238743  0.06803783  3.60579568 -6.69912743]', '[ 1.23849155 -1.1549658   2.39888115 -5.21942904]', '[ 1.55850322 -1.9974746   0.81330062 -3.2998074 ]', '[ 1.57044612 -2.49545596 -0.67315969 -1.689312  ]', '[ 1.2986808  -2.66814272 -2.01579712 -0.01993775]', '[ 0.77618569 -2.47751205 -3.13130432  1.93926147]', '[ 0.09234814 -1.88910959 -3.58371692  3.9415999 ]', '[-0.61872587 -0.91421549 -3.47042516  5.71068298]', '[-1.25889434  0.28924493 -2.77290606  5.92294658]', '[-1.66806933  1.33138402 -1.2555823   4.43284872]', '[-1.75262899  2.07397804  0.41554441  3.00084845]', '[-1.50681376  2.5209658   2.01039429  1.42845401]', '[-0.95694488  2.59279724  3.40787004 -0.72214057]', '[-0.19225508  2.23462428  4.07616574 -2.83353375]', '[ 0.60463631  1.48427487  3.77488619 -4.56516921]', '[ 1.29350512  0.47005764  3.06774191 -5.36755914]', '[ 1.80209119 -0.56059541  1.94693929 -4.75905338]', '[ 2.0437454  -1.38238628  0.45220323 -3.4845811 ]', '[ 1.97431739 -1.9539648  -1.16770936 -2.17853514]', '[ 1.56743599 -2.19561235 -2.87876971 -0.12629193]', '[ 0.84521836 -1.95779586 -4.24202173  2.6145786 ]', '[-0.07485538 -1.12191763 -4.84132411  5.71998814]', '[-1.03854339  0.21431364 -4.57029885  6.9790663 ]', '[-1.81714158  1.42422078 -3.17722849  5.02486828]', '[-2.3301561   2.2910843  -2.01209242  3.80860829]', '[-2.64537499  2.9885467  -1.2110065   3.21949944]', '[-2.84417791 -2.69675176 -0.84890382  2.76526985]', '[-3.00618859 -2.18918544 -0.81006941  2.31250086]', '[ 3.10437013 -1.76915516 -0.94043909  1.90481599]', '[ 2.89022499 -1.41553677 -1.23543911  1.67834162]', '[ 2.59262333 -1.07101999 -1.79753279  1.8611174 ]', '[ 2.14388001 -0.62283996 -2.76832495  2.76322308]', '[ 1.45724194  0.07984364 -4.11959981  4.22839031]', '[ 0.52410904  0.94915399 -5.05787374  3.98867039]', '[-0.48248325  1.49296868 -4.75168545  1.17199164]', '[-1.26836817  1.37985302 -2.91345312 -2.23872055]', '[-1.61508074  0.65930246 -0.61613458 -4.75076672]', '[-1.57368646 -0.4423301   0.80340423 -5.95566189]', '[-1.35925283 -1.65810243  1.25556969 -6.1511537 ]', '[-1.06639394 -2.94008932  1.77879106 -6.84478005]', '[-0.57436901  1.78582576  3.34265856 -9.14334295]', '[  0.30809831  -0.46266441   4.77707735 -12.0710905 ]', '[ 1.02961658 -2.49830425  2.38468285 -8.41655723]', '[ 1.38261929  2.24454689  1.48083514 -7.35257474]', '[ 1.70357908  0.72221633  1.74291001 -8.04722953]', '[ 1.97085641 -0.86179138  0.48704549 -7.23042004]', '[ 1.76567136 -2.0340609  -2.6230204  -4.3708335 ]', '[ 0.95918744 -2.55301129 -5.18679452 -0.85836464]', '[-0.19571955 -2.42116394 -6.04826071  2.01773684]', '[-1.34091358 -1.81653864 -5.216629    3.81408913]', '[-2.26983894 -0.97516263 -4.14719494  4.44988441]']</t>
-  </si>
-  <si>
-    <t>[0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50, 51, 52, 53, 54, 55, 56, 57, 58, 59, 60, 61, 62, 63, 64, 65, 66, 67, 68, 69, 70, 71, 72, 73, 74, 75, 76, 77, 78, 79, 80, 81, 82, 83, 84, 85, 86, 87, 88, 89, 90, 91, 92, 93, 94, 95, 96, 97, 98, 99, 100, 101, 102, 103]</t>
-  </si>
-  <si>
-    <t>[array([-0.03763371, -0.01533471,  0.06554052, -0.01816017], dtype=float32), array([-0.0208055 , -0.02030166,  0.09914155, -0.02801351]), array([ 0.013578  , -0.05917353,  0.23628798, -0.34824344]), array([ 0.05569493, -0.11750576,  0.17467028, -0.21881458]), array([ 0.09321032, -0.17559542,  0.19101534, -0.34617425]), array([ 0.11494541, -0.21477236,  0.02111502, -0.03635698]), array([ 0.08803171, -0.15527598, -0.28298244,  0.61721212]), array([ 0.00771379,  0.02051943, -0.49814643,  1.09748723]), array([-0.09992322,  0.2613885 , -0.54781767,  1.25079563]), array([-0.19899582,  0.49621087, -0.41673597,  1.04534563]), array([-0.2580581 ,  0.66242577, -0.16029595,  0.58814693]), array([-0.26017189,  0.72426166,  0.13930997,  0.02389421]), array([-0.18064923,  0.61001101,  0.64091503, -1.14763298]), array([-0.01369954,  0.28056091,  0.99109498, -2.07970048]), array([ 0.19459177, -0.18092928,  1.02977955, -2.41098167]), array([ 0.37243687, -0.63206098,  0.69861701, -2.00005475]), array([ 0.46011212, -0.95316036,  0.16174322, -1.17326704]), array([ 0.42537627, -1.06524089, -0.49664074,  0.05178195]), array([ 0.25924884, -0.90689492, -1.13554472,  1.51266653]), array([-0.01379993, -0.47540523, -1.54414875,  2.72653459]), array([-0.3292649 ,  0.13059648, -1.52098835,  3.15699007]), array([-0.58467466,  0.71332982, -0.96429096,  2.53978023]), array([-0.69777494,  1.11628807, -0.14936694,  1.45645161]), array([-0.64433925,  1.29003413,  0.66881172,  0.2760153 ]), array([-0.42231877,  1.17306991,  1.50990699, -1.43665973]), array([-0.07111479,  0.75438868,  1.94117555, -2.68416081]), array([ 0.33560416,  0.11506689,  2.03003906, -3.52819267]), array([ 0.69501986, -0.56511932,  1.46746056, -3.08665122]), array([ 0.88484758, -1.04433681,  0.40582077, -1.6728194 ]), array([ 0.85542822, -1.23060088, -0.68977317, -0.18289421]), array([ 0.60841282, -1.08579727, -1.74321229,  1.63796675]), array([ 0.17832049, -0.58015369, -2.48775454,  3.3472159 ]), array([-0.34375825,  0.18072445, -2.59235808,  3.98171196]), array([-0.80094618,  0.89723241, -1.88397553,  3.01969304]), array([-1.07621992,  1.36710168, -0.84333561,  1.68029916]), array([-1.13342628,  1.57404756,  0.27330188,  0.39205272]), array([-0.96138203,  1.4949075 ,  1.42725158, -1.20563517]), array([-0.56540277,  1.05321555,  2.49310348, -3.23510873]), array([ 0.0113307 ,  0.21668057,  3.15814153, -4.92308468]), array([ 0.62238874, -0.7540897 ,  2.77772679, -4.41696087]), array([ 1.07994183, -1.47825656,  1.75394785, -2.81118852]), array([ 1.3155028 , -1.89414321,  0.59014308, -1.38352358]), array([ 1.31415662, -2.03876785, -0.60072395, -0.06057471]), array([ 1.06553321, -1.86592768, -1.86135998,  1.82843448]), array([ 0.58306205, -1.28468987, -2.92653754,  4.04232752]), array([-0.0847069 , -0.2500291 , -3.62797837,  6.06844474]), array([-0.77254409,  0.92469989, -3.04195448,  5.2214648 ]), array([-1.26346642,  1.77978029, -1.84454069,  3.37719485]), array([-1.50715244,  2.30491798, -0.58893267,  1.92168017]), array([-1.4996076 ,  2.55585612,  0.658817  ,  0.58515642]), array([-1.24179447,  2.51280732,  1.89719688, -1.03892162]), array([-0.75115069,  2.10667206,  2.94433604, -3.0686173 ]), array([-0.10232982,  1.28889494,  3.47932462, -5.1244788 ]), array([ 0.62238743,  0.06803783,  3.60579568, -6.69912743]), array([ 1.23849155, -1.1549658 ,  2.39888115, -5.21942904]), array([ 1.55850322, -1.9974746 ,  0.81330062, -3.2998074 ]), array([ 1.57044612, -2.49545596, -0.67315969, -1.689312  ]), array([ 1.2986808 , -2.66814272, -2.01579712, -0.01993775]), array([ 0.77618569, -2.47751205, -3.13130432,  1.93926147]), array([ 0.09234814, -1.88910959, -3.58371692,  3.9415999 ]), array([-0.61872587, -0.91421549, -3.47042516,  5.71068298]), array([-1.25889434,  0.28924493, -2.77290606,  5.92294658]), array([-1.66806933,  1.33138402, -1.2555823 ,  4.43284872]), array([-1.75262899,  2.07397804,  0.41554441,  3.00084845]), array([-1.50681376,  2.5209658 ,  2.01039429,  1.42845401]), array([-0.95694488,  2.59279724,  3.40787004, -0.72214057]), array([-0.19225508,  2.23462428,  4.07616574, -2.83353375]), array([ 0.60463631,  1.48427487,  3.77488619, -4.56516921]), array([ 1.29350512,  0.47005764,  3.06774191, -5.36755914]), array([ 1.80209119, -0.56059541,  1.94693929, -4.75905338]), array([ 2.0437454 , -1.38238628,  0.45220323, -3.4845811 ]), array([ 1.97431739, -1.9539648 , -1.16770936, -2.17853514]), array([ 1.56743599, -2.19561235, -2.87876971, -0.12629193]), array([ 0.84521836, -1.95779586, -4.24202173,  2.6145786 ]), array([-0.07485538, -1.12191763, -4.84132411,  5.71998814]), array([-1.03854339,  0.21431364, -4.57029885,  6.9790663 ]), array([-1.81714158,  1.42422078, -3.17722849,  5.02486828]), array([-2.3301561 ,  2.2910843 , -2.01209242,  3.80860829]), array([-2.64537499,  2.9885467 , -1.2110065 ,  3.21949944]), array([-2.84417791, -2.69675176, -0.84890382,  2.76526985]), array([-3.00618859, -2.18918544, -0.81006941,  2.31250086]), array([ 3.10437013, -1.76915516, -0.94043909,  1.90481599]), array([ 2.89022499, -1.41553677, -1.23543911,  1.67834162]), array([ 2.59262333, -1.07101999, -1.79753279,  1.8611174 ]), array([ 2.14388001, -0.62283996, -2.76832495,  2.76322308]), array([ 1.45724194,  0.07984364, -4.11959981,  4.22839031]), array([ 0.52410904,  0.94915399, -5.05787374,  3.98867039]), array([-0.48248325,  1.49296868, -4.75168545,  1.17199164]), array([-1.26836817,  1.37985302, -2.91345312, -2.23872055]), array([-1.61508074,  0.65930246, -0.61613458, -4.75076672]), array([-1.57368646, -0.4423301 ,  0.80340423, -5.95566189]), array([-1.35925283, -1.65810243,  1.25556969, -6.1511537 ]), array([-1.06639394, -2.94008932,  1.77879106, -6.84478005]), array([-0.57436901,  1.78582576,  3.34265856, -9.14334295]), array([  0.30809831,  -0.46266441,   4.77707735, -12.0710905 ]), array([ 1.02961658, -2.49830425,  2.38468285, -8.41655723]), array([ 1.38261929,  2.24454689,  1.48083514, -7.35257474]), array([ 1.70357908,  0.72221633,  1.74291001, -8.04722953]), array([ 1.97085641, -0.86179138,  0.48704549, -7.23042004]), array([ 1.76567136, -2.0340609 , -2.6230204 , -4.3708335 ]), array([ 0.95918744, -2.55301129, -5.18679452, -0.85836464]), array([-0.19571955, -2.42116394, -6.04826071,  2.01773684]), array([-1.34091358, -1.81653864, -5.216629  ,  3.81408913]), array([-2.26983894, -0.97516263, -4.14719494,  4.44988441])]</t>
-  </si>
-  <si>
-    <t>['[0,0,0]', '[1,1,1]', '[2,0,1]', '[0,2,1]', '[1,0,2]', '[2,2,2]', '[1,1,2]', '[1,2,0]', '[2,1,0]', '[0,1,1]']</t>
-  </si>
-  <si>
-    <t>[2, 13, 15, 16, 26, 29, 30, 38, 39, 40, 42, 50, 51, 54, 65, 67, 69, 70, 71, 80, 81, 84, 85]</t>
-  </si>
-  <si>
-    <t>[0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 1, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 1, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 1, 0, 0, 0, 0, 0, 0, 0, 0, 1, 1, 1, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2]</t>
-  </si>
-  <si>
-    <t>['[-0.03763371 -0.01533471  0.06554052 -0.01816017]', '[-0.00754409 -0.05458322  0.2277812  -0.36241836]', '[ 0.03557041 -0.11811661  0.19275289 -0.25552579]', '[ 0.07892797 -0.1849336   0.22986116 -0.39424827]', '[ 0.12271824 -0.267417    0.19671429 -0.40996627]', '[ 0.15338212 -0.34091394  0.10180504 -0.30861109]', '[ 0.16107551 -0.38557729 -0.0273968  -0.13010444]', '[ 0.11689442 -0.32478194 -0.40419263  0.72290359]', '[ 0.00699758 -0.10946448 -0.66682387  1.37864006]', '[-0.13518691  0.19851722 -0.71460523  1.62157325]', '[-0.26216055  0.50605306 -0.52049404  1.38437545]', '[-0.33248769  0.73016948 -0.16679196  0.82126441]', '[-0.32601137  0.82598862  0.22935372  0.12936813]', '[-0.23310864  0.75237898  0.68098455 -0.84867834]', '[-0.05199092  0.4669668   1.09481076 -1.9534796 ]', '[ 0.17177326  0.03966882  1.08297445 -2.20563548]', '[ 0.35604853 -0.36621616  0.70891984 -1.75321128]', '[ 0.45270788 -0.66444852  0.23325569 -1.17687632]', '[ 0.4445464  -0.82360354 -0.31342495 -0.39921041]', '[ 0.30954221 -0.76187415 -1.0094624   1.00035337]', '[ 0.05595999 -0.43759942 -1.47573908  2.17481945]', '[-0.25360483  0.06316573 -1.53948539  2.68467845]', '[-0.52539341  0.57112116 -1.10888983  2.26738845]', '[-0.67705457  0.93606471 -0.3804693   1.3384434 ]', '[-0.67304307  1.09772826  0.41729355  0.26857392]', '[-0.49553157  0.98500559  1.32807675 -1.39027622]', '[-0.17004724  0.58165138  1.86742313 -2.57337335]', '[ 0.23160718 -0.02572826  2.04685411 -3.31076392]', '[ 0.60240398 -0.65297327  1.568263   -2.79140887]', '[ 0.82248658 -1.07361519  0.60517813 -1.38992621]', '[ 0.84025911 -1.20743645 -0.42515924  0.05322303]', '[ 0.64735119 -1.02204979 -1.48009051  1.80706959]', '[ 0.26309435 -0.48863013 -2.30098295  3.45598492]', '[-0.23082223  0.2857871  -2.49686718  4.00553376]', '[-0.67884917  1.0010593  -1.89057012  2.99253081]', '[-0.96567402  1.46252668 -0.9489651   1.62299375]', '[-1.05195817  1.65531974  0.09162765  0.31232484]', '[-0.9138075   1.53738981  1.27509378 -1.50955901]', '[-0.56057132  1.06626713  2.2219813  -3.21263214]', '[-0.04814964  0.27117236  2.79661727 -4.55414132]', '[ 0.49165791 -0.61781215  2.44337951 -4.01042004]', '[ 0.89795444 -1.28784675  1.56423359 -2.6337518 ]', '[ 1.09700996 -1.64909104  0.41613217 -1.00493376]', '[ 1.06353494 -1.69505132 -0.74409615  0.54889826]', '[ 0.79718856 -1.39700237 -1.8960272   2.46639721]', '[ 0.31763711 -0.69551535 -2.84822387  4.51929882]', '[-0.29540514  0.32593323 -3.09010244  5.28132737]', '[-0.84138707  1.25356408 -2.26936097  3.828653  ]', '[-1.18685648  1.85640639 -1.16591782  2.24214184]', '[-1.30314298  2.16490622  0.00699825  0.86028355]', '[-1.17901679  2.17921702  1.21844396 -0.73086459]', '[-0.82708377  1.86187882  2.25947341 -2.47841034]', '[-0.28672542  1.146977    3.09949128 -4.70095926]', '[ 0.38427971  0.01597864  3.44165403 -6.2384889 ]', '[ 0.97985671 -1.09641616  2.36933346 -4.59934022]', '[ 1.32513565 -1.84502254  1.07255557 -2.93946594]', '[ 1.40825385 -2.28950136 -0.23645068 -1.52120098]', '[ 1.22933591 -2.43098018 -1.52785603  0.12073893]', '[ 0.80695634 -2.2122894  -2.63255035  2.09187231]', '[ 0.20980735 -1.58336507 -3.25927539  4.21779605]', '[-0.4711149  -0.53306286 -3.46898415  6.12251142]', '[-1.10476081  0.68997325 -2.66353943  5.6494184 ]', '[-1.48884843  1.64497887 -1.15020417  3.9217163 ]', '[-1.56452636  2.27926454  0.38272279  2.43942766]', '[-1.34463095  2.61711625  1.78380245  0.92262504]', '[-0.86307794  2.62498259  2.96218674 -0.83811695]', '[-0.1965416   2.26962954  3.56223723 -2.68283291]', '[ 0.4952368   1.59758385  3.24435793 -3.93955144]', '[ 1.08388237  0.71888727  2.60286174 -4.70386025]', '[ 1.50128026 -0.1766842   1.50181667 -4.07716378]', '[ 1.66198199 -0.87073788  0.0679292  -2.81724414]', '[ 1.51685823 -1.28520154 -1.53805584 -1.24995426]', '[ 1.04010155 -1.30215696 -3.18243568  1.18847199]', '[ 0.27854307 -0.7796659  -4.31298482  3.9922082 ]', '[-0.61501349  0.18167305 -4.39136286  5.09001453]', '[-1.39297551  1.05124991 -3.29227865  3.42916171]', '[-1.92801688  1.57820859 -2.07923664  1.97305114]', '[-2.23622675  1.88957903 -1.03036261  1.2318007 ]', '[-2.34785835  2.09273442 -0.09477685  0.82071748]', '[-2.26565423  2.19226117  0.93024602  0.13695917]', '[-1.96658518  2.12112596  2.08706002 -0.94412254]', '[-1.42257474  1.76477828  3.35764437 -2.77358848]', '[-0.62062808  0.92007883  4.63443003 -5.78254431]', '[ 0.37973262 -0.4449266   5.06712084 -7.06527338]', '[ 1.28349934 -1.58197478  3.89474652 -4.19821241]', '[ 1.93800669 -2.19256355  2.66258737 -2.09673869]', '[ 2.36659525 -2.50278792  1.6644645  -1.11988117]', '[ 2.62131847 -2.67380743  0.92489652 -0.65045076]', '[ 2.74342423 -2.75909027  0.320519   -0.22883456]', '[ 2.75448876 -2.77046746 -0.20707014  0.11285619]', '[ 2.65723331 -2.71026158 -0.78424932  0.51010337]', '[ 2.42294339 -2.53253372 -1.59813361  1.32166245]', '[ 1.9997098  -2.14953934 -2.68045203  2.62891539]', '[ 1.33433935 -1.41317451 -4.01352231  4.95793719]', '[ 0.38372467 -0.09705747 -5.36444202  7.87457265]', '[-0.67285286  1.34644041 -4.93960617  5.86666758]', '[-1.56537514  2.22912695 -3.94825256  3.13716903]', '[-2.24588245  2.68138626 -2.883646    1.56513058]', '[-2.74358869  2.91366401 -2.17547116  0.88122774]', '[ 3.13353088  3.07550793 -1.97382122  0.83426715]', '[ 2.71570835 -2.99965033 -2.29488383  1.34157439]', '[ 2.18053306 -2.62916961 -3.13771747  2.49697153]', '[ 1.43746715 -1.9310796  -4.32409067  4.72501156]', '[ 0.43970763 -0.62732747 -5.65461045  8.38641137]', '[-0.70464203  1.07789067 -5.40345368  7.56955661]', '[-1.6714284   2.26453498 -4.28865508  4.53859207]', '[-2.42972838  3.00407911 -3.34565323  3.08469265]', '[-3.04596742 -2.71614054 -2.93560918  2.69057028]', '[ 2.63042613 -2.14593971 -3.2572678   3.18432724]', '[ 1.88695847 -1.35470735 -4.30111778  5.0147983 ]', '[ 0.86607329 -0.03831953 -5.85377283  7.88275853]', '[-0.33719614  1.40000356 -5.90585695  5.68229485]', '[-1.44304788  2.16876411 -5.01363961  2.13277705]', '[-2.30810625  2.34191173 -3.63727848 -0.15358126]', '[-2.92264319  2.19884207 -2.60385542 -1.06656161]', '[ 2.89050277  1.98534337 -2.21440842 -0.92167265]', '[ 2.42870866  1.87284022 -2.51559029 -0.13490451]']</t>
+    <t>[13, 15, 26, 28, 52, 54, 56]</t>
+  </si>
+  <si>
+    <t>[0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 1, 0, 0, 0, 0, 0, 0, 1, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 1, 2, 2, 2, 2, 2]</t>
+  </si>
+  <si>
+    <t>['[-0.03763371 -0.01533471  0.06554052 -0.01816017]', '[-0.00754409 -0.05458322  0.2277812  -0.36241836]', '[ 0.04879627 -0.15231473  0.32089719 -0.5887683 ]', '[ 0.11397169 -0.27767857  0.31375488 -0.63332862]', '[ 0.16759438 -0.39312519  0.2086893  -0.49480525]', '[ 0.1930193  -0.46685036  0.03906408 -0.22816919]', '[ 0.15689524 -0.41528579 -0.3922057   0.73207416]', '[ 0.04309269 -0.18588535 -0.71796191  1.51055937]', '[-0.1147829   0.15904975 -0.81547211  1.84906375]', '[-0.26363568  0.51494657 -0.63159042  1.62703318]', '[-0.35418658  0.78351571 -0.2539271   1.01663306]', '[-0.36122763  0.91144819  0.18313112  0.25239067]', '[-0.26190848  0.82452699  0.79137833 -1.10754289]', '[-0.06765079  0.51219552  1.11217066 -1.95689148]', '[ 0.17532613  0.04396445  1.25425673 -2.6049767 ]', '[ 0.39111247 -0.43697999  0.84272736 -2.08435815]', '[ 0.50708835 -0.78788177  0.29006272 -1.36933649]', '[ 0.5023162  -0.97179071 -0.33507169 -0.45577232]', '[ 0.35726604 -0.91052543 -1.08650431  1.05526664]', '[ 0.08313265 -0.56118898 -1.60465094  2.37781439]', '[-0.2570542  -0.003705   -1.71044997  3.03532744]', '[-0.56183546  0.57696629 -1.25645645  2.61924196]', '[-0.73654599  1.00450379 -0.46032451  1.6093302 ]', '[-0.74104817  1.21214762  0.41202209  0.45719682]', '[-0.55857354  1.13008255  1.38101385 -1.27750459]', '[-0.20543927  0.70532997  2.0953316  -2.92337579]', '[ 0.23425699  0.0428761   2.1900859  -3.49059668]', '[ 0.63366982 -0.62606623  1.70205626 -3.00746296]', '[ 0.87617216 -1.0865808   0.693427   -1.57145367]', '[ 0.91643358 -1.28134035 -0.29282505 -0.37063728]', '[ 0.74347579 -1.17724836 -1.41341051  1.42348542]', '[ 0.36476431 -0.70864555 -2.32302881  3.23262182]', '[-0.15139388  0.06550877 -2.70473425  4.24857821]', '[-0.65252905  0.8581215  -2.18529757  3.45013189]', '[-0.99685495  1.40794929 -1.22227074  2.03983956]', '[-1.13358259  1.68091281 -0.13620451  0.70367259]', '[-1.03504466  1.64216817  1.10945388 -1.10505014]', '[-0.69775491  1.22577426  2.23678003 -3.09803486]', '[-0.15637512  0.39916882  3.09261666 -5.04417129]', '[ 0.46961132 -0.64579489  2.96629018 -4.96994785]', '[ 0.97331958 -1.4790458   2.01262598 -3.31268053]', '[ 1.26422838 -1.98567034  0.8812327  -1.79724277]', '[ 1.32251789 -2.20891452 -0.29885338 -0.44330195]', '[ 1.13441413 -2.11704864 -1.56152828  1.38633171]', '[ 0.71077786 -1.63739843 -2.63605264  3.46771804]', '[ 0.09575459 -0.7083837  -3.45842657  5.78309327]', '[-0.60822358  0.53872453 -3.33191319  6.12016147]', '[-1.15904869  1.57724396 -2.11796251  4.21513246]', '[-1.45177729  2.25520615 -0.80887999  2.63055049]', '[-1.48439305  2.64249484  0.47343597  1.24945533]', '[-1.26170732  2.73300723  1.73273773 -0.35253981]', '[-0.80009794  2.47767424  2.81721499 -2.21537065]', '[-0.18025119  1.86120216  3.27826189 -3.95500361]', '[ 0.48717009  0.87838718  3.34438879 -5.79884206]', '[ 1.10172431 -0.31566946  2.62102097 -5.71431839]', '[ 1.48517407 -1.31379588  1.14564975 -4.18799076]', '[ 1.54380355 -1.97419613 -0.55158335 -2.4323769 ]', '[ 1.27367368 -2.27873223 -2.1077508  -0.57552976]', '[ 0.72131452 -2.16902858 -3.31424022  1.6975452 ]', '[ 7.15878507e-04 -1.59831456e+00 -3.76412714e+00  3.98069805e+00]', '[-0.74443068 -0.61147868 -3.6037346   5.69070122]', '[-1.38706959  0.52780324 -2.67525523  5.33135933]', '[-1.77819437  1.4518951  -1.21136835  3.92266612]', '[-1.86811013  2.11341909  0.31708533  2.69694341]', '[-1.65302827  2.5175405   1.81760423  1.29289324]', '[-1.14096153  2.57019683  3.24760916 -0.80744454]', '[-0.39205737  2.18231848  4.09994435 -3.08980419]', '[ 0.43592952  1.34035452  4.07212059 -5.26266737]', '[ 1.20919184  0.14629635  3.55626092 -6.33029847]', '[ 1.79671067 -1.02112386  2.22766367 -5.14717593]', '[ 2.09176915 -1.92228169  0.72243252 -3.93175198]', '[ 2.08751865 -2.60333266 -0.74397421 -2.86034641]', '[ 1.80168706 -3.03203307 -2.08429758 -1.39672496]', '[ 1.2534659  -3.13773426 -3.383047    0.32503986]', '[ 0.46767158 -2.91688424 -4.36456788  1.83100518]', '[-0.42072942 -2.42826498 -4.31806849  2.98169281]', '[-1.19269482 -1.76711981 -3.31513743  3.49170062]', '[-1.73896068 -1.08654366 -2.16023901  3.20453522]']</t>
+  </si>
+  <si>
+    <t>[0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50, 51, 52, 53, 54, 55, 56, 57, 58, 59, 60, 61, 62, 63, 64, 65, 66, 67, 68, 69, 70, 71, 72, 73, 74, 75, 76, 77]</t>
+  </si>
+  <si>
+    <t>[array([-0.03763371, -0.01533471,  0.06554052, -0.01816017], dtype=float32), array([-0.00754409, -0.05458322,  0.2277812 , -0.36241836]), array([ 0.04879627, -0.15231473,  0.32089719, -0.5887683 ]), array([ 0.11397169, -0.27767857,  0.31375488, -0.63332862]), array([ 0.16759438, -0.39312519,  0.2086893 , -0.49480525]), array([ 0.1930193 , -0.46685036,  0.03906408, -0.22816919]), array([ 0.15689524, -0.41528579, -0.3922057 ,  0.73207416]), array([ 0.04309269, -0.18588535, -0.71796191,  1.51055937]), array([-0.1147829 ,  0.15904975, -0.81547211,  1.84906375]), array([-0.26363568,  0.51494657, -0.63159042,  1.62703318]), array([-0.35418658,  0.78351571, -0.2539271 ,  1.01663306]), array([-0.36122763,  0.91144819,  0.18313112,  0.25239067]), array([-0.26190848,  0.82452699,  0.79137833, -1.10754289]), array([-0.06765079,  0.51219552,  1.11217066, -1.95689148]), array([ 0.17532613,  0.04396445,  1.25425673, -2.6049767 ]), array([ 0.39111247, -0.43697999,  0.84272736, -2.08435815]), array([ 0.50708835, -0.78788177,  0.29006272, -1.36933649]), array([ 0.5023162 , -0.97179071, -0.33507169, -0.45577232]), array([ 0.35726604, -0.91052543, -1.08650431,  1.05526664]), array([ 0.08313265, -0.56118898, -1.60465094,  2.37781439]), array([-0.2570542 , -0.003705  , -1.71044997,  3.03532744]), array([-0.56183546,  0.57696629, -1.25645645,  2.61924196]), array([-0.73654599,  1.00450379, -0.46032451,  1.6093302 ]), array([-0.74104817,  1.21214762,  0.41202209,  0.45719682]), array([-0.55857354,  1.13008255,  1.38101385, -1.27750459]), array([-0.20543927,  0.70532997,  2.0953316 , -2.92337579]), array([ 0.23425699,  0.0428761 ,  2.1900859 , -3.49059668]), array([ 0.63366982, -0.62606623,  1.70205626, -3.00746296]), array([ 0.87617216, -1.0865808 ,  0.693427  , -1.57145367]), array([ 0.91643358, -1.28134035, -0.29282505, -0.37063728]), array([ 0.74347579, -1.17724836, -1.41341051,  1.42348542]), array([ 0.36476431, -0.70864555, -2.32302881,  3.23262182]), array([-0.15139388,  0.06550877, -2.70473425,  4.24857821]), array([-0.65252905,  0.8581215 , -2.18529757,  3.45013189]), array([-0.99685495,  1.40794929, -1.22227074,  2.03983956]), array([-1.13358259,  1.68091281, -0.13620451,  0.70367259]), array([-1.03504466,  1.64216817,  1.10945388, -1.10505014]), array([-0.69775491,  1.22577426,  2.23678003, -3.09803486]), array([-0.15637512,  0.39916882,  3.09261666, -5.04417129]), array([ 0.46961132, -0.64579489,  2.96629018, -4.96994785]), array([ 0.97331958, -1.4790458 ,  2.01262598, -3.31268053]), array([ 1.26422838, -1.98567034,  0.8812327 , -1.79724277]), array([ 1.32251789, -2.20891452, -0.29885338, -0.44330195]), array([ 1.13441413, -2.11704864, -1.56152828,  1.38633171]), array([ 0.71077786, -1.63739843, -2.63605264,  3.46771804]), array([ 0.09575459, -0.7083837 , -3.45842657,  5.78309327]), array([-0.60822358,  0.53872453, -3.33191319,  6.12016147]), array([-1.15904869,  1.57724396, -2.11796251,  4.21513246]), array([-1.45177729,  2.25520615, -0.80887999,  2.63055049]), array([-1.48439305,  2.64249484,  0.47343597,  1.24945533]), array([-1.26170732,  2.73300723,  1.73273773, -0.35253981]), array([-0.80009794,  2.47767424,  2.81721499, -2.21537065]), array([-0.18025119,  1.86120216,  3.27826189, -3.95500361]), array([ 0.48717009,  0.87838718,  3.34438879, -5.79884206]), array([ 1.10172431, -0.31566946,  2.62102097, -5.71431839]), array([ 1.48517407, -1.31379588,  1.14564975, -4.18799076]), array([ 1.54380355, -1.97419613, -0.55158335, -2.4323769 ]), array([ 1.27367368, -2.27873223, -2.1077508 , -0.57552976]), array([ 0.72131452, -2.16902858, -3.31424022,  1.6975452 ]), array([ 7.15878507e-04, -1.59831456e+00, -3.76412714e+00,  3.98069805e+00]), array([-0.74443068, -0.61147868, -3.6037346 ,  5.69070122]), array([-1.38706959,  0.52780324, -2.67525523,  5.33135933]), array([-1.77819437,  1.4518951 , -1.21136835,  3.92266612]), array([-1.86811013,  2.11341909,  0.31708533,  2.69694341]), array([-1.65302827,  2.5175405 ,  1.81760423,  1.29289324]), array([-1.14096153,  2.57019683,  3.24760916, -0.80744454]), array([-0.39205737,  2.18231848,  4.09994435, -3.08980419]), array([ 0.43592952,  1.34035452,  4.07212059, -5.26266737]), array([ 1.20919184,  0.14629635,  3.55626092, -6.33029847]), array([ 1.79671067, -1.02112386,  2.22766367, -5.14717593]), array([ 2.09176915, -1.92228169,  0.72243252, -3.93175198]), array([ 2.08751865, -2.60333266, -0.74397421, -2.86034641]), array([ 1.80168706, -3.03203307, -2.08429758, -1.39672496]), array([ 1.2534659 , -3.13773426, -3.383047  ,  0.32503986]), array([ 0.46767158, -2.91688424, -4.36456788,  1.83100518]), array([-0.42072942, -2.42826498, -4.31806849,  2.98169281]), array([-1.19269482, -1.76711981, -3.31513743,  3.49170062]), array([-1.73896068, -1.08654366, -2.16023901,  3.20453522])]</t>
+  </si>
+  <si>
+    <t>['[1,0,2]', '[2,0,1]', '[2,1,0]', '[1,1,1]', '[1,1,2]', '[2,2,2]', '[1,2,0]', '[0,0,0]', '[0,2,1]', '[0,1,1]']</t>
+  </si>
+  <si>
+    <t>[1, 2, 3, 4, 11, 12, 14, 15, 23, 26, 27, 36, 50, 53, 62, 64, 66, 79, 80, 81, 84, 94, 98, 103, 106]</t>
+  </si>
+  <si>
+    <t>[0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 1, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 1, 0, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 2, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 1, 1, 1]</t>
+  </si>
+  <si>
+    <t>['[-0.03763371 -0.01533471  0.06554052 -0.01816017]', '[-0.0208055  -0.02030166  0.09914155 -0.02801351]', '[ 0.00031733 -0.02489487  0.10765546 -0.0138725 ]', '[ 0.02044082 -0.02428802  0.08954248  0.02288616]', '[ 0.03470698 -0.01491644  0.05056501  0.07132823]', '[ 0.02674144  0.03818636 -0.12667052  0.44879208]', '[-0.01270905  0.15667936 -0.25571586  0.70881747]', '[-0.06940829  0.30836147 -0.29491305  0.77301892]', '[-0.12394901  0.4517198  -0.23590169  0.62988145]', '[-0.15876359  0.5498143  -0.10369689  0.33260441]', '[-0.16331677  0.57991751  0.05921824 -0.03571874]', '[-0.12364641  0.50409537  0.32874453 -0.70766221]', '[-0.03775164  0.30783049  0.50916352 -1.21389118]', '[ 0.08230598  0.00646819  0.65728545 -1.72868582]', '[ 0.19568549 -0.31507497  0.44233374 -1.41248958]', '[ 0.24874947 -0.53479727  0.07445597 -0.74782605]', '[ 0.23595115 -0.63810948 -0.20073382 -0.27426624]', '[ 0.14742637 -0.58013997 -0.66567061  0.83618659]', '[-0.01939148 -0.31783734 -0.96592123  1.72834895]', '[-0.21983454  0.076846   -0.98395001  2.11374101]', '[-0.38978057  0.48207252 -0.6674177   1.84275323]', '[-0.47222115  0.78451792 -0.13764198  1.13696494]', '[-0.44241747  0.92659954  0.42850603  0.27466328]', '[-0.2969758   0.86563019  0.99635034 -0.86631968]', '[-0.04757255  0.56249264  1.45034925 -2.10777273]', '[ 0.2584103   0.06159147  1.53384919 -2.76269678]', '[ 0.51864472 -0.44284576  1.00062574 -2.15327876]', '[ 0.64004688 -0.76638388  0.19132099 -1.04153368]', '[ 0.60432129 -0.88229543 -0.54242326 -0.10764761]', '[ 0.4079933  -0.74864162 -1.38634301  1.42701983]', '[ 0.06968139 -0.32969906 -1.92750117  2.66529605]', '[-0.32527116  0.25215479 -1.91696905  2.95736156]', '[-0.65701707  0.77985912 -1.32994403  2.20576702]', '[-0.83902777  1.11184625 -0.46613469  1.09408394]', '[-0.83932004  1.21461842  0.46112044 -0.07093376]', '[-0.63951702  1.0251702   1.51197729 -1.82999924]', '[-0.2616722   0.51843218  2.20167563 -3.15919849]', '[ 0.21395941 -0.2034311   2.42405615 -3.80450374]', '[ 0.65274314 -0.89454293  1.86677089 -2.93908627]', '[ 0.93712889 -1.35189602  0.94564656 -1.62494592]', '[ 1.0240896  -1.54762693 -0.08196095 -0.33790695]', '[ 0.88829899 -1.43541913 -1.26118846  1.47666847]', '[ 0.52866204 -0.9459777  -2.30232215  3.43111534]', '[-0.00802694 -0.08780122 -2.93986125  4.9139598 ]', '[-0.57194947  0.85930628 -2.54107361  4.23475273]', '[-0.98801807  1.5499509  -1.57951911  2.6643483 ]', '[-1.19490095  1.93742494 -0.47686634  1.23775612]', '[-1.17706993  2.05025012  0.64991972 -0.11140783]', '[-0.92680053  1.84217945  1.82477888 -2.00109468]', '[-0.46155983  1.23160737  2.79047679 -4.14682128]', '[ 0.15567802  0.226621    3.25079973 -5.64458026]', '[ 0.76425679 -0.86592842  2.64913772 -4.8876352 ]', '[ 1.17793317 -1.67076303  1.46049398 -3.18225116]', '[ 1.33749466 -2.13637621  0.13839901 -1.51118459]', '[ 1.23680774 -2.27910904 -1.12837625  0.09311214]', '[ 0.8912676  -2.06920112 -2.28074366  2.03863213]', '[ 0.34865743 -1.44738321 -3.08722212  4.21753696]', '[-0.32123065 -0.38673495 -3.50907455  6.18710227]', '[-0.96771353  0.82563469 -2.74604185  5.47624599]', '[-1.3783685   1.73816156 -1.34147599  3.69062889]', '[-1.50467912  2.32652827  0.06993412  2.22248   ]', '[-1.3566487   2.62784761  1.3881135   0.78057076]', '[-0.95623511  2.61500368  2.56381554 -0.91209257]', '[-0.35880734  2.24405095  3.29428305 -2.7895904 ]', '[ 0.3033413   1.53169032  3.22862931 -4.27286   ]', '[ 0.91643551  0.54961063  2.8442498  -5.38030175]', '[ 1.38482927 -0.47326027  1.7223726  -4.58814772]', '[ 1.58541622 -1.26571917  0.23807437 -3.29195166]', '[ 1.4692997  -1.77627758 -1.40616565 -1.75484799]', '[ 1.01918761 -1.89206239 -3.01880385  0.66660649]', '[ 0.30741648 -1.48844217 -3.96740664  3.38058882]', '[-0.51641135 -0.56763838 -4.14639398  5.59720953]', '[-1.28038503  0.56379949 -3.32083148  5.26457089]', '[-1.81004141  1.46066593 -1.97295524  3.75153232]', '[-2.07553053  2.10208941 -0.69324963  2.72392477]', '[-2.09020735  2.55633163  0.54009027  1.7981905 ]', '[-1.85496917  2.78461889  1.81264305  0.43406188]', '[-1.35821362  2.68842028  3.14069955 -1.45582017]', '[-0.62100992  2.17530848  4.12465459 -3.75406874]', '[ 0.2344219   1.18616378  4.34489918 -6.11676899]', '[ 1.0771235  -0.17089466  3.87928332 -6.88282127]', '[ 1.70225195 -1.35544975  2.31483137 -4.8713996 ]', '[ 2.01907563 -2.19086441  0.87168037 -3.57129266]', '[ 2.0598091  -2.79771187 -0.4335836  -2.49173889]', '[ 1.85103295  3.12489697 -1.64022525 -1.09073733]', '[ 1.39624277  3.07402095 -2.91297447  0.57867459]', '[ 0.69458257 -2.93335038 -4.02397793  2.15951161]', '[-0.15200381 -2.35149146 -4.25027032  3.63665763]', '[-0.93853546 -1.50288906 -3.53337639  4.74688676]', '[-1.55773107 -0.50520701 -2.64915078  5.0811824 ]', '[-1.98479867  0.46771409 -1.57901445  4.54443169]', '[-2.17278505  1.296916   -0.25620106  3.73183877]', '[-2.0659278   1.94341225  1.37367756  2.64500377]', '[-1.60842918  2.28662274  3.17924566  0.66092218]', '[-0.82010017  2.16175321  4.58061929 -2.00323338]', '[ 0.15773596  1.44686435  5.02515263 -5.11153915]', '[ 1.14133471  0.19142435  4.67688751 -6.97739019]', '[ 1.95453407 -1.09283412  3.37691237 -5.59242821]', '[ 2.50118011 -2.05963166  2.17318561 -4.27282099]', '[ 2.86011064 -2.87553671  1.5020366  -3.9589731 ]', '[-3.13987448  2.62487563  1.44442183 -3.90100808]', '[-2.80730144  1.83124432  1.95954335 -4.10926551]', '[-2.32737828  0.93426885  2.92344133 -5.02859319]', '[-1.62032859 -0.20019217  4.14970334 -6.21016244]', '[-0.68310746 -1.42960161  5.14442443 -5.64450128]', '[ 0.4054655  -2.34470213  5.56435198 -3.37151709]', '[ 1.44233084 -2.76017655  4.62930153 -0.86634941]', '[ 2.23746553 -2.75073925  3.33567779  0.83744682]', '[ 2.78671876 -2.45874671  2.20617258  1.93711197]', '[ 3.14061373 -2.03020734  1.40130092  2.22017936]', '[-2.9045135  -1.61307365  1.0658723   1.86169083]']</t>
+  </si>
+  <si>
+    <t>[0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50, 51, 52, 53, 54, 55, 56, 57, 58, 59, 60, 61, 62, 63, 64, 65, 66, 67, 68, 69, 70, 71, 72, 73, 74, 75, 76, 77, 78, 79, 80, 81, 82, 83, 84, 85, 86, 87, 88, 89, 90, 91, 92, 93, 94, 95, 96, 97, 98, 99, 100, 101, 102, 103, 104, 105, 106, 107, 108, 109, 110]</t>
+  </si>
+  <si>
+    <t>[array([-0.03763371, -0.01533471,  0.06554052, -0.01816017], dtype=float32), array([-0.0208055 , -0.02030166,  0.09914155, -0.02801351]), array([ 0.00031733, -0.02489487,  0.10765546, -0.0138725 ]), array([ 0.02044082, -0.02428802,  0.08954248,  0.02288616]), array([ 0.03470698, -0.01491644,  0.05056501,  0.07132823]), array([ 0.02674144,  0.03818636, -0.12667052,  0.44879208]), array([-0.01270905,  0.15667936, -0.25571586,  0.70881747]), array([-0.06940829,  0.30836147, -0.29491305,  0.77301892]), array([-0.12394901,  0.4517198 , -0.23590169,  0.62988145]), array([-0.15876359,  0.5498143 , -0.10369689,  0.33260441]), array([-0.16331677,  0.57991751,  0.05921824, -0.03571874]), array([-0.12364641,  0.50409537,  0.32874453, -0.70766221]), array([-0.03775164,  0.30783049,  0.50916352, -1.21389118]), array([ 0.08230598,  0.00646819,  0.65728545, -1.72868582]), array([ 0.19568549, -0.31507497,  0.44233374, -1.41248958]), array([ 0.24874947, -0.53479727,  0.07445597, -0.74782605]), array([ 0.23595115, -0.63810948, -0.20073382, -0.27426624]), array([ 0.14742637, -0.58013997, -0.66567061,  0.83618659]), array([-0.01939148, -0.31783734, -0.96592123,  1.72834895]), array([-0.21983454,  0.076846  , -0.98395001,  2.11374101]), array([-0.38978057,  0.48207252, -0.6674177 ,  1.84275323]), array([-0.47222115,  0.78451792, -0.13764198,  1.13696494]), array([-0.44241747,  0.92659954,  0.42850603,  0.27466328]), array([-0.2969758 ,  0.86563019,  0.99635034, -0.86631968]), array([-0.04757255,  0.56249264,  1.45034925, -2.10777273]), array([ 0.2584103 ,  0.06159147,  1.53384919, -2.76269678]), array([ 0.51864472, -0.44284576,  1.00062574, -2.15327876]), array([ 0.64004688, -0.76638388,  0.19132099, -1.04153368]), array([ 0.60432129, -0.88229543, -0.54242326, -0.10764761]), array([ 0.4079933 , -0.74864162, -1.38634301,  1.42701983]), array([ 0.06968139, -0.32969906, -1.92750117,  2.66529605]), array([-0.32527116,  0.25215479, -1.91696905,  2.95736156]), array([-0.65701707,  0.77985912, -1.32994403,  2.20576702]), array([-0.83902777,  1.11184625, -0.46613469,  1.09408394]), array([-0.83932004,  1.21461842,  0.46112044, -0.07093376]), array([-0.63951702,  1.0251702 ,  1.51197729, -1.82999924]), array([-0.2616722 ,  0.51843218,  2.20167563, -3.15919849]), array([ 0.21395941, -0.2034311 ,  2.42405615, -3.80450374]), array([ 0.65274314, -0.89454293,  1.86677089, -2.93908627]), array([ 0.93712889, -1.35189602,  0.94564656, -1.62494592]), array([ 1.0240896 , -1.54762693, -0.08196095, -0.33790695]), array([ 0.88829899, -1.43541913, -1.26118846,  1.47666847]), array([ 0.52866204, -0.9459777 , -2.30232215,  3.43111534]), array([-0.00802694, -0.08780122, -2.93986125,  4.9139598 ]), array([-0.57194947,  0.85930628, -2.54107361,  4.23475273]), array([-0.98801807,  1.5499509 , -1.57951911,  2.6643483 ]), array([-1.19490095,  1.93742494, -0.47686634,  1.23775612]), array([-1.17706993,  2.05025012,  0.64991972, -0.11140783]), array([-0.92680053,  1.84217945,  1.82477888, -2.00109468]), array([-0.46155983,  1.23160737,  2.79047679, -4.14682128]), array([ 0.15567802,  0.226621  ,  3.25079973, -5.64458026]), array([ 0.76425679, -0.86592842,  2.64913772, -4.8876352 ]), array([ 1.17793317, -1.67076303,  1.46049398, -3.18225116]), array([ 1.33749466, -2.13637621,  0.13839901, -1.51118459]), array([ 1.23680774, -2.27910904, -1.12837625,  0.09311214]), array([ 0.8912676 , -2.06920112, -2.28074366,  2.03863213]), array([ 0.34865743, -1.44738321, -3.08722212,  4.21753696]), array([-0.32123065, -0.38673495, -3.50907455,  6.18710227]), array([-0.96771353,  0.82563469, -2.74604185,  5.47624599]), array([-1.3783685 ,  1.73816156, -1.34147599,  3.69062889]), array([-1.50467912,  2.32652827,  0.06993412,  2.22248   ]), array([-1.3566487 ,  2.62784761,  1.3881135 ,  0.78057076]), array([-0.95623511,  2.61500368,  2.56381554, -0.91209257]), array([-0.35880734,  2.24405095,  3.29428305, -2.7895904 ]), array([ 0.3033413 ,  1.53169032,  3.22862931, -4.27286   ]), array([ 0.91643551,  0.54961063,  2.8442498 , -5.38030175]), array([ 1.38482927, -0.47326027,  1.7223726 , -4.58814772]), array([ 1.58541622, -1.26571917,  0.23807437, -3.29195166]), array([ 1.4692997 , -1.77627758, -1.40616565, -1.75484799]), array([ 1.01918761, -1.89206239, -3.01880385,  0.66660649]), array([ 0.30741648, -1.48844217, -3.96740664,  3.38058882]), array([-0.51641135, -0.56763838, -4.14639398,  5.59720953]), array([-1.28038503,  0.56379949, -3.32083148,  5.26457089]), array([-1.81004141,  1.46066593, -1.97295524,  3.75153232]), array([-2.07553053,  2.10208941, -0.69324963,  2.72392477]), array([-2.09020735,  2.55633163,  0.54009027,  1.7981905 ]), array([-1.85496917,  2.78461889,  1.81264305,  0.43406188]), array([-1.35821362,  2.68842028,  3.14069955, -1.45582017]), array([-0.62100992,  2.17530848,  4.12465459, -3.75406874]), array([ 0.2344219 ,  1.18616378,  4.34489918, -6.11676899]), array([ 1.0771235 , -0.17089466,  3.87928332, -6.88282127]), array([ 1.70225195, -1.35544975,  2.31483137, -4.8713996 ]), array([ 2.01907563, -2.19086441,  0.87168037, -3.57129266]), array([ 2.0598091 , -2.79771187, -0.4335836 , -2.49173889]), array([ 1.85103295,  3.12489697, -1.64022525, -1.09073733]), array([ 1.39624277,  3.07402095, -2.91297447,  0.57867459]), array([ 0.69458257, -2.93335038, -4.02397793,  2.15951161]), array([-0.15200381, -2.35149146, -4.25027032,  3.63665763]), array([-0.93853546, -1.50288906, -3.53337639,  4.74688676]), array([-1.55773107, -0.50520701, -2.64915078,  5.0811824 ]), array([-1.98479867,  0.46771409, -1.57901445,  4.54443169]), array([-2.17278505,  1.296916  , -0.25620106,  3.73183877]), array([-2.0659278 ,  1.94341225,  1.37367756,  2.64500377]), array([-1.60842918,  2.28662274,  3.17924566,  0.66092218]), array([-0.82010017,  2.16175321,  4.58061929, -2.00323338]), array([ 0.15773596,  1.44686435,  5.02515263, -5.11153915]), array([ 1.14133471,  0.19142435,  4.67688751, -6.97739019]), array([ 1.95453407, -1.09283412,  3.37691237, -5.59242821]), array([ 2.50118011, -2.05963166,  2.17318561, -4.27282099]), array([ 2.86011064, -2.87553671,  1.5020366 , -3.9589731 ]), array([-3.13987448,  2.62487563,  1.44442183, -3.90100808]), array([-2.80730144,  1.83124432,  1.95954335, -4.10926551]), array([-2.32737828,  0.93426885,  2.92344133, -5.02859319]), array([-1.62032859, -0.20019217,  4.14970334, -6.21016244]), array([-0.68310746, -1.42960161,  5.14442443, -5.64450128]), array([ 0.4054655 , -2.34470213,  5.56435198, -3.37151709]), array([ 1.44233084, -2.76017655,  4.62930153, -0.86634941]), array([ 2.23746553, -2.75073925,  3.33567779,  0.83744682]), array([ 2.78671876, -2.45874671,  2.20617258,  1.93711197]), array([ 3.14061373, -2.03020734,  1.40130092,  2.22017936]), array([-2.9045135 , -1.61307365,  1.0658723 ,  1.86169083])]</t>
+  </si>
+  <si>
+    <t>['[1,1,1]', '[2,0,1]', '[2,2,2]', '[1,2,0]', '[0,0,0]', '[0,1,1]', '[2,1,0]', '[1,1,2]', '[1,0,2]', '[0,2,1]']</t>
+  </si>
+  <si>
+    <t>[2, 3, 5, 12, 14, 24, 25, 26, 27, 35, 36, 38, 39, 49, 50, 51, 53, 62, 63, 64, 65, 66, 67, 76, 78, 79, 80, 81, 82, 92, 94, 96, 97, 98, 108, 110, 112]</t>
+  </si>
+  <si>
+    <t>[0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 1, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 1, 0, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 2, 1, 0, 0, 0, 0, 0]</t>
+  </si>
+  <si>
+    <t>['[-0.03763371 -0.01533471  0.06554052 -0.01816017]', '[-0.00754409 -0.05458322  0.2277812  -0.36241836]', '[ 0.03557041 -0.11811661  0.19275289 -0.25552579]', '[ 0.06573284 -0.15080759  0.10193248 -0.0615216 ]', '[ 0.08768179 -0.17469111  0.11234335 -0.16976787]', '[ 0.09523697 -0.18090679 -0.03829061  0.10940563]', '[ 0.06000234 -0.09864639 -0.30437559  0.69380029]', '[-0.01985892  0.08334246 -0.47178968  1.08116023]', '[-0.11783554  0.31199017 -0.48029711  1.14954875]', '[-0.2011667   0.52140908 -0.33128832  0.90041953]', '[-0.24358784  0.65811933 -0.08318448  0.44430741]', '[-0.20880857  0.63078758  0.42352537 -0.71035739]', '[-0.09314223  0.41594815  0.7076211  -1.39485795]', '[ 0.07354807  0.06406103  0.91533808 -2.03908225]', '[ 0.2382292  -0.32249597  0.68381277 -1.73011006]', '[ 0.34424559 -0.62958613  0.34839893 -1.28163752]', '[ 0.37060424 -0.81874967 -0.09003773 -0.58801564]', '[ 0.2872667  -0.80044296 -0.72515145  0.76054055]', '[ 0.09127798 -0.52441293 -1.19760749  1.95108522]', '[-0.17102871 -0.05392178 -1.35867069  2.62991763]', '[-0.42056048  0.46611885 -1.06531444  2.43192294]', '[-0.57447818  0.8763863  -0.44096475  1.60994664]', '[-0.59077767  1.09710052  0.27731396  0.58327431]', '[-0.4483304   1.05151762  1.1188781  -1.03137478]', '[-0.16944767  0.72223621  1.62038731 -2.21028745]', '[ 0.17366561  0.20522451  1.72987403 -2.81759096]', '[ 0.48507221 -0.3338102   1.30181907 -2.41677506]', '[ 0.66914611 -0.71644344  0.50348291 -1.35130265]', '[ 0.69131617 -0.89372297 -0.28556865 -0.40460722]', '[ 0.53624646 -0.81490702 -1.23911063  1.18669895]', '[ 0.21188491 -0.42932862 -1.94426869  2.59732263]', '[-0.2061059   0.16662735 -2.12586859  3.15922083]', '[-0.59226684  0.74757025 -1.64802326  2.50123377]', '[-0.84150033  1.13577715 -0.81039816  1.35467033]', '[-0.90894083  1.28737414  0.14196766  0.16045865]', '[-0.77668283  1.17120556  1.16457113 -1.32925982]', '[-0.45420191  0.7545392   2.01612432 -2.810167  ]', '[ 0.01356905  0.05240271  2.54993702 -4.00739701]', '[ 0.49310931 -0.6946844   2.12210386 -3.22797994]', '[ 0.83035707 -1.19065473  1.20799695 -1.7032191 ]', '[ 0.97632381 -1.40492972  0.23729252 -0.44541736]', '[ 0.90478274 -1.31746132 -0.94670879  1.32907818]', '[ 0.60320588 -0.86500741 -2.04286765  3.20448987]', '[ 0.11001254 -0.05928193 -2.77342574  4.6375156 ]', '[-0.43630901  0.84365671 -2.53692711  4.08216094]', '[-0.86617165  1.51148434 -1.71266098  2.5699308 ]', '[-1.10899795  1.87969702 -0.69553679  1.13746788]', '[-1.13993096  1.97303015  0.38727097 -0.20027539]', '[-0.94237501  1.75025384  1.57070241 -2.0564411 ]', '[-0.53038974  1.15838316  2.51503695 -3.88886721]', '[ 0.0403593   0.21294437  3.06816647 -5.32978129]', '[ 0.61577694 -0.79822677  2.51457314 -4.42454868]', '[ 1.0201036  -1.52676191  1.48990634 -2.85002563]', '[ 1.1965864  -1.92755344  0.27138165 -1.19088314]', '[ 1.13001001 -2.00793153 -0.92462291  0.39323947]', '[ 0.82873694 -1.73913305 -2.05392366  2.33076386]', '[ 0.32467815 -1.05808    -2.94432797  4.50173163]', '[-0.31862045  0.02187809 -3.31955935  5.93437476]', '[-0.9095641   1.10797149 -2.44118731  4.63376   ]', '[-1.27405013  1.8607713  -1.19064939  2.94726397]', '[-1.38435103  2.30564325  0.08497619  1.52236178]', '[-1.24393192  2.46981375  1.30080293  0.1086519 ]', '[-0.87075058  2.32270927  2.37672191 -1.59580644]', '[-0.32470312  1.82587922  2.99465989 -3.3779169 ]', '[ 0.29379366  0.97943964  3.12250333 -5.00869081]', '[ 0.88503169 -0.08999003  2.6367512  -5.32437367]', '[ 1.28513368 -1.0140427   1.28403676 -3.78192078]', '[ 1.38876255 -1.60081063 -0.24974827 -2.0952666 ]', '[ 1.19705001 -1.86916264 -1.64496046 -0.546054  ]', '[ 0.7359021  -1.75493678 -2.88463248  1.72639047]', '[ 0.08343498 -1.17141492 -3.54243042  4.07979896]', '[-0.6400156  -0.17789642 -3.54867899  5.52710074]', '[-1.2600804   0.85523173 -2.5199393   4.51594304]', '[-1.62833115  1.60730981 -1.15465375  3.05566754]', '[-1.72127839  2.09532514  0.22606337  1.83289894]', '[-1.53883581  2.33080104  1.58910163  0.47672722]', '[-1.08851597  2.24339534  2.86508666 -1.40817694]', '[-0.41872698  1.72430901  3.73253823 -3.82797361]', '[ 0.35755226  0.73901825  3.93829683 -5.87981231]', '[ 1.09109881 -0.46133706  3.19582242 -5.61875533]', '[ 1.58409234 -1.39661833  1.7114133  -3.74469575]', '[ 1.778773   -1.99222819  0.24309372 -2.26156241]', '[ 1.68363964 -2.30280631 -1.18712171 -0.81312776]', '[ 1.30295438 -2.2756356  -2.58948857  1.15112099]', '[ 0.67028424 -1.81233321 -3.65728386  3.5599002 ]', '[-0.12644992 -0.82998573 -4.23636251  6.20876028]', '[-0.95926168  0.51179006 -3.83719864  6.55863325]', '[-1.58721669  1.62268962 -2.41424968  4.5576843 ]', '[-1.932386    2.38648798 -1.05917296  3.17453932]', '[-2.02058182  2.90867354  0.15090242  2.05069504]', '[-1.87328097 -3.10230432  1.31904436  0.65165199]', '[-1.48275202 -3.14001169  2.59621743 -1.03935142]', '[-0.8468085   2.78059635  3.6952508  -2.60594595]', '[-0.05134342  2.06886207  4.10558645 -4.54124101]', '[ 0.74111027  0.99221292  3.76365013 -6.12185633]', '[ 1.43302055 -0.29776412  3.00146834 -6.35491089]', '[ 1.87187997 -1.39436041  1.34699542 -4.59672731]', '[ 1.97088704 -2.16395068 -0.35130777 -3.12414463]', '[ 1.73825714 -2.63431914 -1.94618747 -1.53310228]', '[ 1.1999356  -2.73990551 -3.38931607  0.50684429]', '[ 0.41655324 -2.42569071 -4.30046428  2.63866166]', '[-0.44589137 -1.69436457 -4.17179076  4.60482272]', '[-1.21937295 -0.63491182 -3.52249601  5.7895705 ]', '[-1.8258291   0.50296738 -2.45733368  5.33776914]', '[-2.18153944  1.46375926 -1.08131654  4.30124924]', '[-2.2510632   2.23588936  0.39930638  3.40834646]', '[-2.02505958  2.80864991  1.83147498  2.26321021]', '[-1.52502221  3.10498143  3.14658974  0.68996146]', '[-0.77697467  3.09569269  4.27019696 -0.71337851]', '[ 0.13827461  2.83771485  4.70163649 -1.75591469]', '[ 1.01841709  2.4592827   3.94751176 -1.89687366]', '[ 1.69050538  2.11104569  2.75379904 -1.46831276]', '[ 2.12180441  1.92858308  1.60098402 -0.29958079]']</t>
+  </si>
+  <si>
+    <t>[0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50, 51, 52, 53, 54, 55, 56, 57, 58, 59, 60, 61, 62, 63, 64, 65, 66, 67, 68, 69, 70, 71, 72, 73, 74, 75, 76, 77, 78, 79, 80, 81, 82, 83, 84, 85, 86, 87, 88, 89, 90, 91, 92, 93, 94, 95, 96, 97, 98, 99, 100, 101, 102, 103, 104, 105, 106, 107, 108, 109, 110, 111, 112]</t>
+  </si>
+  <si>
+    <t>[array([-0.03763371, -0.01533471,  0.06554052, -0.01816017], dtype=float32), array([-0.00754409, -0.05458322,  0.2277812 , -0.36241836]), array([ 0.03557041, -0.11811661,  0.19275289, -0.25552579]), array([ 0.06573284, -0.15080759,  0.10193248, -0.0615216 ]), array([ 0.08768179, -0.17469111,  0.11234335, -0.16976787]), array([ 0.09523697, -0.18090679, -0.03829061,  0.10940563]), array([ 0.06000234, -0.09864639, -0.30437559,  0.69380029]), array([-0.01985892,  0.08334246, -0.47178968,  1.08116023]), array([-0.11783554,  0.31199017, -0.48029711,  1.14954875]), array([-0.2011667 ,  0.52140908, -0.33128832,  0.90041953]), array([-0.24358784,  0.65811933, -0.08318448,  0.44430741]), array([-0.20880857,  0.63078758,  0.42352537, -0.71035739]), array([-0.09314223,  0.41594815,  0.7076211 , -1.39485795]), array([ 0.07354807,  0.06406103,  0.91533808, -2.03908225]), array([ 0.2382292 , -0.32249597,  0.68381277, -1.73011006]), array([ 0.34424559, -0.62958613,  0.34839893, -1.28163752]), array([ 0.37060424, -0.81874967, -0.09003773, -0.58801564]), array([ 0.2872667 , -0.80044296, -0.72515145,  0.76054055]), array([ 0.09127798, -0.52441293, -1.19760749,  1.95108522]), array([-0.17102871, -0.05392178, -1.35867069,  2.62991763]), array([-0.42056048,  0.46611885, -1.06531444,  2.43192294]), array([-0.57447818,  0.8763863 , -0.44096475,  1.60994664]), array([-0.59077767,  1.09710052,  0.27731396,  0.58327431]), array([-0.4483304 ,  1.05151762,  1.1188781 , -1.03137478]), array([-0.16944767,  0.72223621,  1.62038731, -2.21028745]), array([ 0.17366561,  0.20522451,  1.72987403, -2.81759096]), array([ 0.48507221, -0.3338102 ,  1.30181907, -2.41677506]), array([ 0.66914611, -0.71644344,  0.50348291, -1.35130265]), array([ 0.69131617, -0.89372297, -0.28556865, -0.40460722]), array([ 0.53624646, -0.81490702, -1.23911063,  1.18669895]), array([ 0.21188491, -0.42932862, -1.94426869,  2.59732263]), array([-0.2061059 ,  0.16662735, -2.12586859,  3.15922083]), array([-0.59226684,  0.74757025, -1.64802326,  2.50123377]), array([-0.84150033,  1.13577715, -0.81039816,  1.35467033]), array([-0.90894083,  1.28737414,  0.14196766,  0.16045865]), array([-0.77668283,  1.17120556,  1.16457113, -1.32925982]), array([-0.45420191,  0.7545392 ,  2.01612432, -2.810167  ]), array([ 0.01356905,  0.05240271,  2.54993702, -4.00739701]), array([ 0.49310931, -0.6946844 ,  2.12210386, -3.22797994]), array([ 0.83035707, -1.19065473,  1.20799695, -1.7032191 ]), array([ 0.97632381, -1.40492972,  0.23729252, -0.44541736]), array([ 0.90478274, -1.31746132, -0.94670879,  1.32907818]), array([ 0.60320588, -0.86500741, -2.04286765,  3.20448987]), array([ 0.11001254, -0.05928193, -2.77342574,  4.6375156 ]), array([-0.43630901,  0.84365671, -2.53692711,  4.08216094]), array([-0.86617165,  1.51148434, -1.71266098,  2.5699308 ]), array([-1.10899795,  1.87969702, -0.69553679,  1.13746788]), array([-1.13993096,  1.97303015,  0.38727097, -0.20027539]), array([-0.94237501,  1.75025384,  1.57070241, -2.0564411 ]), array([-0.53038974,  1.15838316,  2.51503695, -3.88886721]), array([ 0.0403593 ,  0.21294437,  3.06816647, -5.32978129]), array([ 0.61577694, -0.79822677,  2.51457314, -4.42454868]), array([ 1.0201036 , -1.52676191,  1.48990634, -2.85002563]), array([ 1.1965864 , -1.92755344,  0.27138165, -1.19088314]), array([ 1.13001001, -2.00793153, -0.92462291,  0.39323947]), array([ 0.82873694, -1.73913305, -2.05392366,  2.33076386]), array([ 0.32467815, -1.05808   , -2.94432797,  4.50173163]), array([-0.31862045,  0.02187809, -3.31955935,  5.93437476]), array([-0.9095641 ,  1.10797149, -2.44118731,  4.63376   ]), array([-1.27405013,  1.8607713 , -1.19064939,  2.94726397]), array([-1.38435103,  2.30564325,  0.08497619,  1.52236178]), array([-1.24393192,  2.46981375,  1.30080293,  0.1086519 ]), array([-0.87075058,  2.32270927,  2.37672191, -1.59580644]), array([-0.32470312,  1.82587922,  2.99465989, -3.3779169 ]), array([ 0.29379366,  0.97943964,  3.12250333, -5.00869081]), array([ 0.88503169, -0.08999003,  2.6367512 , -5.32437367]), array([ 1.28513368, -1.0140427 ,  1.28403676, -3.78192078]), array([ 1.38876255, -1.60081063, -0.24974827, -2.0952666 ]), array([ 1.19705001, -1.86916264, -1.64496046, -0.546054  ]), array([ 0.7359021 , -1.75493678, -2.88463248,  1.72639047]), array([ 0.08343498, -1.17141492, -3.54243042,  4.07979896]), array([-0.6400156 , -0.17789642, -3.54867899,  5.52710074]), array([-1.2600804 ,  0.85523173, -2.5199393 ,  4.51594304]), array([-1.62833115,  1.60730981, -1.15465375,  3.05566754]), array([-1.72127839,  2.09532514,  0.22606337,  1.83289894]), array([-1.53883581,  2.33080104,  1.58910163,  0.47672722]), array([-1.08851597,  2.24339534,  2.86508666, -1.40817694]), array([-0.41872698,  1.72430901,  3.73253823, -3.82797361]), array([ 0.35755226,  0.73901825,  3.93829683, -5.87981231]), array([ 1.09109881, -0.46133706,  3.19582242, -5.61875533]), array([ 1.58409234, -1.39661833,  1.7114133 , -3.74469575]), array([ 1.778773  , -1.99222819,  0.24309372, -2.26156241]), array([ 1.68363964, -2.30280631, -1.18712171, -0.81312776]), array([ 1.30295438, -2.2756356 , -2.58948857,  1.15112099]), array([ 0.67028424, -1.81233321, -3.65728386,  3.5599002 ]), array([-0.12644992, -0.82998573, -4.23636251,  6.20876028]), array([-0.95926168,  0.51179006, -3.83719864,  6.55863325]), array([-1.58721669,  1.62268962, -2.41424968,  4.5576843 ]), array([-1.932386  ,  2.38648798, -1.05917296,  3.17453932]), array([-2.02058182,  2.90867354,  0.15090242,  2.05069504]), array([-1.87328097, -3.10230432,  1.31904436,  0.65165199]), array([-1.48275202, -3.14001169,  2.59621743, -1.03935142]), array([-0.8468085 ,  2.78059635,  3.6952508 , -2.60594595]), array([-0.05134342,  2.06886207,  4.10558645, -4.54124101]), array([ 0.74111027,  0.99221292,  3.76365013, -6.12185633]), array([ 1.43302055, -0.29776412,  3.00146834, -6.35491089]), array([ 1.87187997, -1.39436041,  1.34699542, -4.59672731]), array([ 1.97088704, -2.16395068, -0.35130777, -3.12414463]), array([ 1.73825714, -2.63431914, -1.94618747, -1.53310228]), array([ 1.1999356 , -2.73990551, -3.38931607,  0.50684429]), array([ 0.41655324, -2.42569071, -4.30046428,  2.63866166]), array([-0.44589137, -1.69436457, -4.17179076,  4.60482272]), array([-1.21937295, -0.63491182, -3.52249601,  5.7895705 ]), array([-1.8258291 ,  0.50296738, -2.45733368,  5.33776914]), array([-2.18153944,  1.46375926, -1.08131654,  4.30124924]), array([-2.2510632 ,  2.23588936,  0.39930638,  3.40834646]), array([-2.02505958,  2.80864991,  1.83147498,  2.26321021]), array([-1.52502221,  3.10498143,  3.14658974,  0.68996146]), array([-0.77697467,  3.09569269,  4.27019696, -0.71337851]), array([ 0.13827461,  2.83771485,  4.70163649, -1.75591469]), array([ 1.01841709,  2.4592827 ,  3.94751176, -1.89687366]), array([ 1.69050538,  2.11104569,  2.75379904, -1.46831276]), array([ 2.12180441,  1.92858308,  1.60098402, -0.29958079])]</t>
+  </si>
+  <si>
+    <t>['[1,1,1]', '[0,1,1]', '[1,1,2]', '[2,2,2]', '[2,1,0]', '[2,0,1]', '[0,2,1]', '[0,0,0]', '[1,0,2]', '[1,2,0]']</t>
+  </si>
+  <si>
+    <t>[2, 3, 4, 10, 11, 12, 13, 14, 15, 22, 23, 24, 25, 26, 27, 34, 35, 36, 38, 47, 48, 50, 51, 52, 59, 60, 61, 62, 63, 64, 65, 73, 75, 76, 78, 89, 90, 91, 93, 94, 104, 105, 106, 107, 108, 110, 111, 135]</t>
+  </si>
+  <si>
+    <t>[0, 0, 0, 0, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 1, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 2, 1, 0, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 0]</t>
+  </si>
+  <si>
+    <t>['[-0.03763371 -0.01533471  0.06554052 -0.01816017]', '[-0.00754409 -0.05458322  0.2277812  -0.36241836]', '[ 0.03557041 -0.11811661  0.19275289 -0.25552579]', '[ 0.06573284 -0.15080759  0.10193248 -0.0615216 ]', '[ 0.074488   -0.14056792 -0.01570518  0.16324094]', '[ 0.0468304  -0.05365918 -0.2524561   0.68648779]', '[-0.02061264  0.12130227 -0.40215537  1.0211927 ]', '[-0.10448049  0.33483216 -0.41240073  1.06374113]', '[-0.1761943   0.52730539 -0.2859239   0.82140039]', '[-0.21298189  0.65079539 -0.07346104  0.39337098]', '[-0.19212995  0.64846565  0.27715937 -0.41293313]', '[-0.10660509  0.49187639  0.55985047 -1.12292914]', '[ 0.021488    0.21786825  0.6886195  -1.55484306]', '[ 0.15337484 -0.09922105  0.59187778 -1.53720831]', '[ 0.24389477 -0.36692594  0.28745974 -1.08262716]', '[ 0.26166575 -0.51579602 -0.1148525  -0.38458434]', '[ 0.18712274 -0.48534019 -0.61447033  0.67533186]', '[ 0.0263001  -0.25870795 -0.95744582  1.53540312]', '[-0.17690425  0.09632708 -1.02091804  1.91674039]', '[-0.35930334  0.46532182 -0.75478628  1.68257882]', '[-0.46347947  0.74089284 -0.26396362  1.02856258]', '[-0.46045743  0.86608449  0.29276867  0.21259315]', '[-0.33969482  0.79574358  0.89140368 -0.90051559]', '[-0.11745464  0.51893566  1.28619756 -1.80956275]', '[ 0.15161533  0.10811253  1.33792133 -2.18227936]', '[ 0.3890225  -0.30146311  0.97503665 -1.80181373]', '[ 0.52247757 -0.57873892  0.33138254 -0.92203162]', '[ 0.5162382  -0.65983765 -0.39212674  0.11824509]', '[ 0.359005   -0.50179582 -1.15108729  1.43427005]', '[ 0.07432934 -0.11021843 -1.62981679  2.37610475]', '[-0.25880622  0.38817032 -1.61372955  2.44919109]', '[-0.53902979  0.81410806 -1.13072396  1.72365492]', '[-0.69504227  1.0586634  -0.40631815  0.70191642]', '[-0.69705453  1.09173223  0.38550195 -0.37250046]', '[-0.53449182  0.88159238  1.21736737 -1.71788694]', '[-0.225276    0.4185011   1.81517748 -2.82835195]', '[ 0.15617165 -0.18769167  1.89444208 -3.03499951]', '[ 0.50328055 -0.74953284  1.49485166 -2.44189481]', '[ 0.72027925 -1.10316121  0.64685153 -1.07294738]', '[ 0.76640933 -1.20491402 -0.19022598  0.05800505]', '[ 0.62581122 -1.02320911 -1.20008201  1.76203708]', '[ 0.297529   -0.50379416 -2.03179207  3.37149285]', '[-0.14968338  0.25979197 -2.30869996  4.00203107]', '[-0.57040364  0.9862097  -1.80393443  3.09655406]', '[-0.8488688   1.47255203 -0.95056243  1.75821211]', '[-0.94367525  1.69252725  0.00883504  0.44820133]', '[-0.83021553  1.60369089  1.11089355 -1.34704976]', '[-0.5175632   1.1713159   1.9829065  -2.98500716]', '[-0.05644156  0.42192773  2.5439735  -4.37427354]', '[ 0.45566642 -0.49645925  2.41249689 -4.46653555]', '[ 0.84473966 -1.23398847  1.42326837 -2.84164091]', '[ 1.01666185 -1.63712243  0.29006598 -1.21081391]', '[ 0.96204588 -1.72251049 -0.82299982  0.35978466]', '[ 0.68863623 -1.46303655 -1.8785869   2.25908589]', '[ 0.22629964 -0.81059518 -2.69395792  4.24011849]', '[-0.34983748  0.16682356 -2.8989069   5.17709059]', '[-0.85698834  1.09842754 -2.05948647  3.93444622]', '[-1.15487151  1.72777135 -0.9025585   2.38729695]', '[-1.21561017  2.06416867  0.29232854  0.98665177]', '[-1.03633693  2.09861118  1.47205484 -0.6568045 ]', '[-0.64430551  1.79286145  2.39075062 -2.42214684]', '[-0.1064528   1.12527839  2.92331703 -4.22908107]', '[ 0.49156896  0.15133701  2.92002237 -5.21474844]', '[ 0.98879069 -0.79945435  1.92384158 -4.03534313]', '[ 1.23877673 -1.43466091  0.56291475 -2.33222618]', '[ 1.21460452 -1.73916644 -0.79279827 -0.7077382 ]', '[ 0.92389084 -1.6840992  -2.07137268  1.29480401]', '[ 0.40914155 -1.20557369 -3.01147098  3.50943607]', '[-0.24956859 -0.30145514 -3.45259741  5.3001205 ]', '[-0.89306797  0.73608745 -2.80557727  4.68841374]', '[-1.33381524  1.5102845  -1.57393621  3.06918927]', '[-1.51938966  1.98488192 -0.27896726  1.71004412]', '[-1.44587632  2.19617617  1.00705406  0.38370084]', '[-1.116793    2.10286739  2.24871978 -1.36259679]', '[-0.56147896  1.60770174  3.2373467  -3.64437807]', '[ 0.14108863  0.664058    3.69970383 -5.66689125]', '[ 0.84817639 -0.49724438  3.15594876 -5.44014435]', '[ 1.35628676 -1.42067522  1.87860916 -3.76016371]', '[ 1.58864148 -2.00262732  0.45107782 -2.11905213]', '[ 1.54605889 -2.29742117 -0.8711535  -0.81320304]', '[ 1.2329095  -2.27284905 -2.22897016  1.10397485]', '[ 0.67541866 -1.83357068 -3.27471187  3.35068035]', '[-0.04713175 -0.91266652 -3.88665113  5.83279255]', '[-0.82596557  0.38049305 -3.66183671  6.50904971]', '[-1.42670775  1.49832164 -2.28410042  4.59878565]', '[-1.74084155  2.25932023 -0.86884781  3.09451962]', '[-1.78023625  2.7506066   0.45682259  1.82001584]', '[-1.55833539  2.96191047  1.75164881  0.27737831]', '[-1.07874207  2.83737579  3.008917   -1.53193498]', '[-0.39281996  2.36449784  3.72304629 -3.20805453]', '[ 0.35175262  1.55800357  3.6152784  -4.80863922]', '[ 1.02696664  0.48749408  3.06726857 -5.67445647]', '[ 1.54298355 -0.61197323  1.97220956 -5.05067741]', '[ 1.7747606  -1.46058617  0.32153948 -3.44778439]', '[ 1.66665909 -1.99037717 -1.40250187 -1.80389682]', '[ 1.21641867 -2.1305882  -3.04132544  0.48391817]', '[ 0.48893851 -1.76731922 -4.10477044  3.19790892]', '[-0.37181699 -0.85457446 -4.39526603  5.80088624]', '[-1.20959245  0.39428619 -3.78201621  6.12696613]', '[-1.82780466  1.45112385 -2.3847574   4.44558824]', '[-2.17379096  2.22101431 -1.10141203  3.34783139]', '[-2.27861957  2.8064348   0.02197117  2.50655669]', '[-2.1763075  -3.06933825  0.98477951  1.53572655]', '[-1.87679236 -2.89445261  2.0341864   0.19155957]', '[-1.35080945 -2.99560066  3.23971303 -1.1940878 ]', '[-0.59276069  2.91760777  4.24130439 -2.49224473]', '[ 0.27587963  2.2952719   4.24736741 -3.69998766]', '[ 1.04280511  1.471626    3.34672907 -4.40283459]', '[ 1.6052549   0.59687897  2.26604769 -4.19702626]', '[ 1.95675297 -0.19842432  1.23723608 -3.70985019]', '[ 2.08044843 -0.84825628 -0.0239457  -2.7831202 ]', '[ 1.93182598 -1.29569359 -1.50967318 -1.59803897]', '[ 1.45336436 -1.40535283 -3.27449123  0.67216351]', '[ 0.64039707 -0.95953369 -4.76476096  3.86851474]', '[-0.39094215  0.075914   -5.28985515  5.87985599]', '[-1.35873207  1.08550699 -4.23475707  3.87646947]', '[-2.07863115  1.65038595 -3.00032734  1.96741822]', '[-2.5825073   1.95171429 -2.11068461  1.21690264]', '[-2.95238137  2.19049637 -1.66179141  1.27564229]', '[ 3.00880689  2.49292204 -1.62696392  1.80963801]', '[ 2.65243718  2.93346654 -2.01394505  2.64314012]', '[ 2.1708691  -2.70993744 -2.88100445  3.85017187]', '[ 1.47343008 -1.74521968 -4.15875614  6.06236792]', '[ 0.47455921 -0.16130732 -5.7360397   9.51851401]', '[-0.64986027  1.57640429 -5.2098518   7.0204451 ]', '[-1.60396217  2.68547051 -4.29462232  4.34685166]', '[-2.35734678 -2.87282783 -3.27534952  3.07751418]', '[-2.95000917 -2.31689935 -2.76832662  2.58939002]', '[ 2.771713   -1.79102005 -2.96754231  2.81713572]', '[ 2.09844697 -1.11435193 -3.89137469  4.18943795]', '[ 1.17131834 -0.03297716 -5.37772511  6.48445594]', '[ 0.02270109  1.20023683 -5.8606277   5.09237068]', '[-1.09016462  1.85178336 -5.04150296  1.36430659]', '[-1.91554338  1.79298111 -3.10839819 -1.74835555]', '[-2.33007256  1.2435394  -1.10546372 -3.53531883]', '[-2.39075396  0.41401698  0.38713412 -4.66035595]']</t>
+  </si>
+  <si>
+    <t>[0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50, 51, 52, 53, 54, 55, 56, 57, 58, 59, 60, 61, 62, 63, 64, 65, 66, 67, 68, 69, 70, 71, 72, 73, 74, 75, 76, 77, 78, 79, 80, 81, 82, 83, 84, 85, 86, 87, 88, 89, 90, 91, 92, 93, 94, 95, 96, 97, 98, 99, 100, 101, 102, 103, 104, 105, 106, 107, 108, 109, 110, 111, 112, 113, 114, 115, 116, 117, 118, 119, 120, 121, 122, 123, 124, 125, 126, 127, 128, 129, 130, 131, 132, 133, 134, 135]</t>
+  </si>
+  <si>
+    <t>[array([-0.03763371, -0.01533471,  0.06554052, -0.01816017], dtype=float32), array([-0.00754409, -0.05458322,  0.2277812 , -0.36241836]), array([ 0.03557041, -0.11811661,  0.19275289, -0.25552579]), array([ 0.06573284, -0.15080759,  0.10193248, -0.0615216 ]), array([ 0.074488  , -0.14056792, -0.01570518,  0.16324094]), array([ 0.0468304 , -0.05365918, -0.2524561 ,  0.68648779]), array([-0.02061264,  0.12130227, -0.40215537,  1.0211927 ]), array([-0.10448049,  0.33483216, -0.41240073,  1.06374113]), array([-0.1761943 ,  0.52730539, -0.2859239 ,  0.82140039]), array([-0.21298189,  0.65079539, -0.07346104,  0.39337098]), array([-0.19212995,  0.64846565,  0.27715937, -0.41293313]), array([-0.10660509,  0.49187639,  0.55985047, -1.12292914]), array([ 0.021488  ,  0.21786825,  0.6886195 , -1.55484306]), array([ 0.15337484, -0.09922105,  0.59187778, -1.53720831]), array([ 0.24389477, -0.36692594,  0.28745974, -1.08262716]), array([ 0.26166575, -0.51579602, -0.1148525 , -0.38458434]), array([ 0.18712274, -0.48534019, -0.61447033,  0.67533186]), array([ 0.0263001 , -0.25870795, -0.95744582,  1.53540312]), array([-0.17690425,  0.09632708, -1.02091804,  1.91674039]), array([-0.35930334,  0.46532182, -0.75478628,  1.68257882]), array([-0.46347947,  0.74089284, -0.26396362,  1.02856258]), array([-0.46045743,  0.86608449,  0.29276867,  0.21259315]), array([-0.33969482,  0.79574358,  0.89140368, -0.90051559]), array([-0.11745464,  0.51893566,  1.28619756, -1.80956275]), array([ 0.15161533,  0.10811253,  1.33792133, -2.18227936]), array([ 0.3890225 , -0.30146311,  0.97503665, -1.80181373]), array([ 0.52247757, -0.57873892,  0.33138254, -0.92203162]), array([ 0.5162382 , -0.65983765, -0.39212674,  0.11824509]), array([ 0.359005  , -0.50179582, -1.15108729,  1.43427005]), array([ 0.07432934, -0.11021843, -1.62981679,  2.37610475]), array([-0.25880622,  0.38817032, -1.61372955,  2.44919109]), array([-0.53902979,  0.81410806, -1.13072396,  1.72365492]), array([-0.69504227,  1.0586634 , -0.40631815,  0.70191642]), array([-0.69705453,  1.09173223,  0.38550195, -0.37250046]), array([-0.53449182,  0.88159238,  1.21736737, -1.71788694]), array([-0.225276  ,  0.4185011 ,  1.81517748, -2.82835195]), array([ 0.15617165, -0.18769167,  1.89444208, -3.03499951]), array([ 0.50328055, -0.74953284,  1.49485166, -2.44189481]), array([ 0.72027925, -1.10316121,  0.64685153, -1.07294738]), array([ 0.76640933, -1.20491402, -0.19022598,  0.05800505]), array([ 0.62581122, -1.02320911, -1.20008201,  1.76203708]), array([ 0.297529  , -0.50379416, -2.03179207,  3.37149285]), array([-0.14968338,  0.25979197, -2.30869996,  4.00203107]), array([-0.57040364,  0.9862097 , -1.80393443,  3.09655406]), array([-0.8488688 ,  1.47255203, -0.95056243,  1.75821211]), array([-0.94367525,  1.69252725,  0.00883504,  0.44820133]), array([-0.83021553,  1.60369089,  1.11089355, -1.34704976]), array([-0.5175632 ,  1.1713159 ,  1.9829065 , -2.98500716]), array([-0.05644156,  0.42192773,  2.5439735 , -4.37427354]), array([ 0.45566642, -0.49645925,  2.41249689, -4.46653555]), array([ 0.84473966, -1.23398847,  1.42326837, -2.84164091]), array([ 1.01666185, -1.63712243,  0.29006598, -1.21081391]), array([ 0.96204588, -1.72251049, -0.82299982,  0.35978466]), array([ 0.68863623, -1.46303655, -1.8785869 ,  2.25908589]), array([ 0.22629964, -0.81059518, -2.69395792,  4.24011849]), array([-0.34983748,  0.16682356, -2.8989069 ,  5.17709059]), array([-0.85698834,  1.09842754, -2.05948647,  3.93444622]), array([-1.15487151,  1.72777135, -0.9025585 ,  2.38729695]), array([-1.21561017,  2.06416867,  0.29232854,  0.98665177]), array([-1.03633693,  2.09861118,  1.47205484, -0.6568045 ]), array([-0.64430551,  1.79286145,  2.39075062, -2.42214684]), array([-0.1064528 ,  1.12527839,  2.92331703, -4.22908107]), array([ 0.49156896,  0.15133701,  2.92002237, -5.21474844]), array([ 0.98879069, -0.79945435,  1.92384158, -4.03534313]), array([ 1.23877673, -1.43466091,  0.56291475, -2.33222618]), array([ 1.21460452, -1.73916644, -0.79279827, -0.7077382 ]), array([ 0.92389084, -1.6840992 , -2.07137268,  1.29480401]), array([ 0.40914155, -1.20557369, -3.01147098,  3.50943607]), array([-0.24956859, -0.30145514, -3.45259741,  5.3001205 ]), array([-0.89306797,  0.73608745, -2.80557727,  4.68841374]), array([-1.33381524,  1.5102845 , -1.57393621,  3.06918927]), array([-1.51938966,  1.98488192, -0.27896726,  1.71004412]), array([-1.44587632,  2.19617617,  1.00705406,  0.38370084]), array([-1.116793  ,  2.10286739,  2.24871978, -1.36259679]), array([-0.56147896,  1.60770174,  3.2373467 , -3.64437807]), array([ 0.14108863,  0.664058  ,  3.69970383, -5.66689125]), array([ 0.84817639, -0.49724438,  3.15594876, -5.44014435]), array([ 1.35628676, -1.42067522,  1.87860916, -3.76016371]), array([ 1.58864148, -2.00262732,  0.45107782, -2.11905213]), array([ 1.54605889, -2.29742117, -0.8711535 , -0.81320304]), array([ 1.2329095 , -2.27284905, -2.22897016,  1.10397485]), array([ 0.67541866, -1.83357068, -3.27471187,  3.35068035]), array([-0.04713175, -0.91266652, -3.88665113,  5.83279255]), array([-0.82596557,  0.38049305, -3.66183671,  6.50904971]), array([-1.42670775,  1.49832164, -2.28410042,  4.59878565]), array([-1.74084155,  2.25932023, -0.86884781,  3.09451962]), array([-1.78023625,  2.7506066 ,  0.45682259,  1.82001584]), array([-1.55833539,  2.96191047,  1.75164881,  0.27737831]), array([-1.07874207,  2.83737579,  3.008917  , -1.53193498]), array([-0.39281996,  2.36449784,  3.72304629, -3.20805453]), array([ 0.35175262,  1.55800357,  3.6152784 , -4.80863922]), array([ 1.02696664,  0.48749408,  3.06726857, -5.67445647]), array([ 1.54298355, -0.61197323,  1.97220956, -5.05067741]), array([ 1.7747606 , -1.46058617,  0.32153948, -3.44778439]), array([ 1.66665909, -1.99037717, -1.40250187, -1.80389682]), array([ 1.21641867, -2.1305882 , -3.04132544,  0.48391817]), array([ 0.48893851, -1.76731922, -4.10477044,  3.19790892]), array([-0.37181699, -0.85457446, -4.39526603,  5.80088624]), array([-1.20959245,  0.39428619, -3.78201621,  6.12696613]), array([-1.82780466,  1.45112385, -2.3847574 ,  4.44558824]), array([-2.17379096,  2.22101431, -1.10141203,  3.34783139]), array([-2.27861957,  2.8064348 ,  0.02197117,  2.50655669]), array([-2.1763075 , -3.06933825,  0.98477951,  1.53572655]), array([-1.87679236, -2.89445261,  2.0341864 ,  0.19155957]), array([-1.35080945, -2.99560066,  3.23971303, -1.1940878 ]), array([-0.59276069,  2.91760777,  4.24130439, -2.49224473]), array([ 0.27587963,  2.2952719 ,  4.24736741, -3.69998766]), array([ 1.04280511,  1.471626  ,  3.34672907, -4.40283459]), array([ 1.6052549 ,  0.59687897,  2.26604769, -4.19702626]), array([ 1.95675297, -0.19842432,  1.23723608, -3.70985019]), array([ 2.08044843, -0.84825628, -0.0239457 , -2.7831202 ]), array([ 1.93182598, -1.29569359, -1.50967318, -1.59803897]), array([ 1.45336436, -1.40535283, -3.27449123,  0.67216351]), array([ 0.64039707, -0.95953369, -4.76476096,  3.86851474]), array([-0.39094215,  0.075914  , -5.28985515,  5.87985599]), array([-1.35873207,  1.08550699, -4.23475707,  3.87646947]), array([-2.07863115,  1.65038595, -3.00032734,  1.96741822]), array([-2.5825073 ,  1.95171429, -2.11068461,  1.21690264]), array([-2.95238137,  2.19049637, -1.66179141,  1.27564229]), array([ 3.00880689,  2.49292204, -1.62696392,  1.80963801]), array([ 2.65243718,  2.93346654, -2.01394505,  2.64314012]), array([ 2.1708691 , -2.70993744, -2.88100445,  3.85017187]), array([ 1.47343008, -1.74521968, -4.15875614,  6.06236792]), array([ 0.47455921, -0.16130732, -5.7360397 ,  9.51851401]), array([-0.64986027,  1.57640429, -5.2098518 ,  7.0204451 ]), array([-1.60396217,  2.68547051, -4.29462232,  4.34685166]), array([-2.35734678, -2.87282783, -3.27534952,  3.07751418]), array([-2.95000917, -2.31689935, -2.76832662,  2.58939002]), array([ 2.771713  , -1.79102005, -2.96754231,  2.81713572]), array([ 2.09844697, -1.11435193, -3.89137469,  4.18943795]), array([ 1.17131834, -0.03297716, -5.37772511,  6.48445594]), array([ 0.02270109,  1.20023683, -5.8606277 ,  5.09237068]), array([-1.09016462,  1.85178336, -5.04150296,  1.36430659]), array([-1.91554338,  1.79298111, -3.10839819, -1.74835555]), array([-2.33007256,  1.2435394 , -1.10546372, -3.53531883]), array([-2.39075396,  0.41401698,  0.38713412, -4.66035595])]</t>
+  </si>
+  <si>
+    <t>['[1,1,1]', '[1,2,0]', '[0,2,1]', '[2,2,2]', '[0,1,1]', '[1,0,2]', '[2,1,0]', '[0,0,0]', '[2,0,1]', '[1,1,2]']</t>
+  </si>
+  <si>
+    <t>[1, 2, 3, 4, 11, 12, 13, 14, 15, 16, 23, 24, 25, 26, 27, 34, 35, 36, 37, 38, 39, 46, 47, 48, 49, 50, 51, 59, 60, 61, 62, 63, 64, 72, 73, 74, 75, 76, 77, 86, 87, 88, 89, 90, 91, 92, 101, 102, 103, 104, 105, 106, 107, 116, 117, 118, 119, 120, 121, 122, 130, 131, 132, 133, 134, 135, 136, 137, 149, 166, 167, 168, 169, 170, 171, 172, 173, 174, 175, 176, 177, 178, 179]</t>
+  </si>
+  <si>
+    <t>[0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 1, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 1, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 1, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 0, 1, 2, 2, 2, 2, 2, 2, 2, 2, 2, 1, 0, 1, 1, 2, 2, 2, 1, 2, 2, 2, 2, 2, 2, 2, 1, 2, 2, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 1, 1, 2]</t>
+  </si>
+  <si>
+    <t>['[-0.03763371 -0.01533471  0.06554052 -0.01816017]', '[-0.0208055  -0.02030166  0.09914155 -0.02801351]', '[ 0.00031733 -0.02489487  0.10765546 -0.0138725 ]', '[ 0.02044082 -0.02428802  0.08954248  0.02288616]', '[ 0.03470698 -0.01491644  0.05056501  0.07132823]', '[ 0.02674144  0.03818636 -0.12667052  0.44879208]', '[-0.01270905  0.15667936 -0.25571586  0.70881747]', '[-0.06940829  0.30836147 -0.29491305  0.77301892]', '[-0.12394901  0.4517198  -0.23590169  0.62988145]', '[-0.15876359  0.5498143  -0.10369689  0.33260441]', '[-0.16331677  0.57991751  0.05921824 -0.03571874]', '[-0.12364641  0.50409537  0.32874453 -0.70766221]', '[-0.03775164  0.30783049  0.50916352 -1.21389118]', '[ 0.06909397  0.04061776  0.52882372 -1.39480458]', '[ 0.16087913 -0.22270668  0.3614133  -1.17772404]', '[ 0.20472536 -0.40990137  0.06420388 -0.6597987 ]', '[ 0.18455416 -0.47825444 -0.26212436 -0.01817226]', '[ 0.09156532 -0.38679677 -0.64742279  0.90761115]', '[-0.06271277 -0.13292697 -0.85786545  1.56672789]', '[-0.23333411  0.20632363 -0.80133675  1.73587805]', '[-0.36498881  0.52600302 -0.4801429   1.39142644]', '[-0.41539568  0.74217732 -0.01227622  0.7395642 ]', '[-0.36944782  0.81527715  0.46213933 -0.01083091]', '[-0.22642744  0.71066606  0.93936783 -1.01021577]', '[-0.00892589  0.42883145  1.18897233 -1.74077443]', '[ 0.22660096  0.0517002   1.1068182  -1.92405165]', '[ 0.41005532 -0.29693012  0.6808143  -1.47495926]', '[ 0.48521772 -0.51258559  0.05370639 -0.64539491]', '[ 0.417663   -0.51547329 -0.71588293  0.61057794]', '[ 0.20989945 -0.2789723  -1.31808193  1.6972301 ]', '[-0.08492151  0.12510753 -1.555619    2.21640575]', '[-0.37963177  0.55019577 -1.32030983  1.91504598]', '[-0.58989289  0.85617843 -0.74359286  1.09612783]', '[-0.66706415  0.97859659 -0.01685984  0.11844472]', '[-0.58535204  0.87309513  0.82205171 -1.16698164]', '[-0.34814683  0.51985272  1.50786441 -2.31349921]', '[-0.00845867 -0.01084392  1.80187214 -2.83660639]', '[ 0.33251678 -0.53972913  1.5220548  -2.29877877]', '[ 0.57395443 -0.88909757  0.8506743  -1.14546192]', '[ 0.66227792 -0.9897414   0.02017728  0.14415152]', '[ 0.56997838 -0.80175587 -0.93344798  1.72881771]', '[ 0.29908242 -0.30913141 -1.72312117  3.11534711]', '[-0.08315313  0.37699688 -1.98491703  3.51987652]', '[-0.44967675  1.01119311 -1.6016925   2.68937509]', '[-0.70314623  1.42828109 -0.90116783  1.46392917]', '[-0.80177252  1.59623253 -0.07487256  0.2180398 ]', '[-0.72394184  1.49081901  0.8443507  -1.27627909]', '[-0.47088945  1.08272659  1.65970504 -2.80278718]', '[-0.07741763  0.38520798  2.19752525 -4.04435356]', '[ 0.35720396 -0.43419659  2.00983042 -3.86699684]', '[ 0.68247785 -1.07790494  1.18689067 -2.48691537]', '[ 0.8218953  -1.42254632  0.19968977 -0.96426762]', '[ 0.75459258 -1.43976003 -0.85807324  0.79326183]', '[ 0.48761236 -1.10140602 -1.78195125  2.59637368]', '[ 0.05897502 -0.41058711 -2.42976401  4.19816012]', '[-0.4314646   0.47314784 -2.31833387  4.31615657]', '[-0.81672247  1.21668414 -1.46858326  3.02633097]', '[-1.00690155  1.67989017 -0.42147508  1.61848727]', '[-0.98493444  1.86772757  0.63078134  0.26001653]', '[-0.75610554  1.75789692  1.62055782 -1.36967148]', '[-0.35595715  1.31549434  2.3275385  -3.05204563]', '[ 0.15035756  0.55372516  2.65209298 -4.43210369]', '[ 0.65139012 -0.34680402  2.2070832  -4.25226899]', '[ 0.985684   -1.05481891  1.0818817  -2.7503158 ]', '[ 1.07698896 -1.44506632 -0.16850092 -1.15785884]', '[ 0.91472109 -1.49041281 -1.42578234  0.72126271]', '[ 0.52287851 -1.1461743  -2.44221275  2.73697075]', '[-0.0361505  -0.40732268 -3.04996577  4.50173997]', '[-0.63332802  0.52271794 -2.74921409  4.43041987]', '[-1.08521394  1.26868163 -1.71335421  2.97168385]', '[-1.30937357  1.72013613 -0.51800962  1.57270265]', '[-1.29116306  1.90318794  0.69559698  0.25067901]', '[-1.02953854  1.78773441  1.89146013 -1.44270084]', '[-0.55192063  1.30869456  2.83147306 -3.37840682]', '[ 0.07603713  0.44640653  3.34164683 -5.06850996]', '[ 0.71210682 -0.56024523  2.83323751 -4.58992558]', '[ 1.16215327 -1.30108095  1.62634935 -2.79800121]', '[ 1.35782358 -1.69718345  0.32701124 -1.20027476]', '[ 1.29357522 -1.78600472 -0.96168782  0.32617383]', '[ 0.97175376 -1.52812432 -2.22977299  2.30896536]', '[ 0.41597596 -0.83828934 -3.27848897  4.59869571]', '[-0.29589598  0.23917885 -3.63462951  5.7170532 ]', '[-0.94771759  1.24507869 -2.7652793   4.12809826]', '[-1.3858772   1.8946614  -1.59986594  2.43902533]', '[-1.58385127  2.24551268 -0.37549195  1.10482016]', '[-1.53593163  2.34055771  0.85171873 -0.16574769]', '[-1.24009148  2.1465686   2.08624736 -1.82154505]', '[-0.71580124  1.58642695  3.11066757 -3.85121969]', '[-0.01649641  0.58958886  3.7980246  -6.00223423]', '[ 0.72271584 -0.63022441  3.35288458 -5.6346347 ]', '[ 1.26589318 -1.54531652  2.04677077 -3.52825443]', '[ 1.54074324 -2.07682244  0.70323788 -1.85302157]', '[ 1.54835695 -2.29852825 -0.62191464 -0.36347038]', '[ 1.28922281 -2.19185675 -1.9499368   1.47371554]', '[ 0.78183018 -1.68361201 -3.0800747   3.68957098]', '[ 0.07510218 -0.68649233 -3.92574039  6.23524741]', '[-0.71325729  0.63892122 -3.68547243  6.37041037]', '[-1.32542542  1.70429056 -2.39999527  4.29168722]', '[-1.67421595  2.40040422 -1.09388001  2.75384971]', '[-1.76681697  2.82218046  0.15624844  1.47301302]', '[-1.60914677  2.96691106  1.4167304  -0.03901625]', '[-1.20216214  2.80054244  2.63043057 -1.64339614]', '[-0.58057383  2.29889525  3.48602181 -3.40943186]', '[ 0.14547089  1.42527121  3.68997172 -5.32339635]', '[ 0.86871302  0.21318263  3.41618363 -6.46194549]', '[ 1.42948555 -0.95919236  2.05445893 -4.98142713]', '[ 1.67483529 -1.77445984  0.39854924 -3.22775735]', '[ 1.59180912 -2.25844942 -1.2121145  -1.59112553]', '[ 1.19575826 -2.37316929 -2.6968554   0.49051754]', '[ 0.54540729 -2.04516465 -3.69231026  2.82243988]', '[-0.22927511 -1.24202884 -3.95631523  5.16342557]', '[-1.00267137 -0.05059515 -3.63330797  6.34739025]', '[-1.60638339  1.1024858  -2.30189154  4.97483052]', '[-1.91612295  1.95275299 -0.79979998  3.60222769]', '[-1.92939296  2.55603743  0.65069186  2.42014853]', '[-1.65883861  2.88835368  2.03354161  0.87190478]', '[-1.12300634  2.89650846  3.29119304 -0.79585088]', '[-0.3730975   2.57330311  4.07251217 -2.41727616]', '[ 0.43397564  1.94678789  3.83527911 -3.76498396]', '[ 1.11772579  1.1197079   2.95254049 -4.34637414]', '[ 1.60322882  0.27624163  1.87266108 -3.94256972]', '[ 1.85568026 -0.42076513  0.63192448 -2.99412334]', '[ 1.84758645 -0.91530252 -0.74252689 -1.91218232]', '[ 1.53516785 -1.1243353  -2.39895985 -0.06030483]', '[ 0.89193164 -0.88387501 -3.98223624  2.56461701]', '[-0.01384101 -0.1158549  -4.87798893  4.75920085]', '[-0.95033159  0.77136377 -4.26719273  3.64732508]', '[-1.67751612  1.28509502 -2.97730961  1.57638688]', '[-2.14758868  1.46595762 -1.76286104  0.39353309]', '[-2.40184707  1.49633464 -0.82547345  0.01251784]', '[-2.48208403  1.47238404  0.00374772 -0.21626992]', '[-2.40139649  1.41119303  0.81624496 -0.42310954]', '[-2.14425245  1.27918363  1.79576061 -0.99245103]', '[-1.66439175  0.96290081  3.04666914 -2.32103748]', '[-0.91679668  0.30191174  4.38781168 -4.24719816]', '[ 0.02796732 -0.59149018  4.82079022 -4.13187618]', '[ 0.9168387  -1.1642839   3.8906271  -1.43157984]', '[ 1.53346857 -1.17688959  2.21330178  1.17627657]', '[ 1.79959754 -0.75411058  0.48349433  2.9218081 ]', '[ 1.73523538 -0.01140089 -1.07012768  4.43846869]', '[ 1.40007919  0.97983558 -2.21311607  5.33605975]', '[ 0.86398843  2.07425611 -3.14813764  5.54392445]', '[ 0.1511617  -3.08627824 -3.85949493  5.7596688 ]', '[-0.60808892 -1.85242675 -3.64223551  6.72312879]', '[-1.31092723 -0.36359682 -3.34667928  8.01574176]', '[-1.84787359  1.14240911 -1.78440253  6.64891652]', '[-1.98581422  2.28614584  0.40066578  4.85550362]', '[-1.72263882  3.09930369  2.08305206  3.32328864]', '[-1.20031246 -2.64959604  3.03672258  2.18307333]', '[-0.55304589 -2.217815    3.26827061  2.44240369]', '[ 0.00828018 -1.53472363  2.06801222  4.71222351]', '[ 1.96590841e-01 -2.52081953e-01  2.40087418e-03  7.80262076e+00]', '[0.24447994 1.2281764  0.92403583 6.27487685]', '[0.58449703 2.25684857 2.27483329 4.32886369]', '[1.05218844 3.11398249 2.10149525 4.64405463]', '[ 1.29466003 -2.0494021  -0.02152631  6.85743506]', '[ 0.95338351 -0.28233632 -3.19454981 10.71351327]', '[ 0.3249783   1.76394691 -2.57328417  8.95553835]', '[-0.10809695 -2.85159196 -2.03572363  8.19973512]', '[-0.6114119  -1.04459352 -3.18273673 10.3513075 ]', '[-1.22504678  1.08669654 -2.17394505  9.75571331]', '[-1.31042606  2.67902884  1.11384275  6.51540765]', '[-0.96161487 -2.43232768  1.86493616  5.67342452]', '[-0.70937098 -1.16019941  0.4777811   7.43658481]', '[-0.71186902  0.53516089  0.24798302  8.45959266]', '[-0.328153    1.8067182   3.60360744  4.08077786]', '[0.58414026 2.2583573  5.07965736 0.84384527]', '[ 1.57442492  2.29835374  4.65217765 -0.13543327]', '[ 2.4335507   2.27180658  4.00619125 -0.08030387]', '[-3.05664039  2.24047267  4.07786358 -0.39411539]', '[-2.15846123  2.01857652  5.02913328 -2.14761815]', '[-1.01870207  1.23546432  6.38661169 -6.01981279]', '[ 0.36584077 -0.34764383  7.08540126 -8.56692552]', '[ 1.65748525 -1.65364547  5.73296664 -4.26111922]', '[ 2.68088255 -2.19370122  4.59142629 -1.53160831]', '[-2.73328869 -2.3940907   4.26996069 -0.72931243]', '[-1.82864616 -2.5507512   4.91052988 -0.91738732]', '[-0.74440279 -2.75430038  5.88260781 -1.00140348]', '[ 0.45631503 -2.87876318  5.88070318 -0.00641608]', '[ 1.50924739 -2.66681405  4.42247914  2.30956078]', '[ 2.14405699 -1.92091581  1.75214597  5.14278682]', '[ 2.19486473 -0.62771438 -1.09736099  7.70412888]', '[ 1.84291596  1.03908215 -1.99826202  8.45530009]']</t>
+  </si>
+  <si>
+    <t>[0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50, 51, 52, 53, 54, 55, 56, 57, 58, 59, 60, 61, 62, 63, 64, 65, 66, 67, 68, 69, 70, 71, 72, 73, 74, 75, 76, 77, 78, 79, 80, 81, 82, 83, 84, 85, 86, 87, 88, 89, 90, 91, 92, 93, 94, 95, 96, 97, 98, 99, 100, 101, 102, 103, 104, 105, 106, 107, 108, 109, 110, 111, 112, 113, 114, 115, 116, 117, 118, 119, 120, 121, 122, 123, 124, 125, 126, 127, 128, 129, 130, 131, 132, 133, 134, 135, 136, 137, 138, 139, 140, 141, 142, 143, 144, 145, 146, 147, 148, 149, 150, 151, 152, 153, 154, 155, 156, 157, 158, 159, 160, 161, 162, 163, 164, 165, 166, 167, 168, 169, 170, 171, 172, 173, 174, 175, 176, 177, 178, 179, 180, 181, 182]</t>
+  </si>
+  <si>
+    <t>[array([-0.03763371, -0.01533471,  0.06554052, -0.01816017], dtype=float32), array([-0.0208055 , -0.02030166,  0.09914155, -0.02801351]), array([ 0.00031733, -0.02489487,  0.10765546, -0.0138725 ]), array([ 0.02044082, -0.02428802,  0.08954248,  0.02288616]), array([ 0.03470698, -0.01491644,  0.05056501,  0.07132823]), array([ 0.02674144,  0.03818636, -0.12667052,  0.44879208]), array([-0.01270905,  0.15667936, -0.25571586,  0.70881747]), array([-0.06940829,  0.30836147, -0.29491305,  0.77301892]), array([-0.12394901,  0.4517198 , -0.23590169,  0.62988145]), array([-0.15876359,  0.5498143 , -0.10369689,  0.33260441]), array([-0.16331677,  0.57991751,  0.05921824, -0.03571874]), array([-0.12364641,  0.50409537,  0.32874453, -0.70766221]), array([-0.03775164,  0.30783049,  0.50916352, -1.21389118]), array([ 0.06909397,  0.04061776,  0.52882372, -1.39480458]), array([ 0.16087913, -0.22270668,  0.3614133 , -1.17772404]), array([ 0.20472536, -0.40990137,  0.06420388, -0.6597987 ]), array([ 0.18455416, -0.47825444, -0.26212436, -0.01817226]), array([ 0.09156532, -0.38679677, -0.64742279,  0.90761115]), array([-0.06271277, -0.13292697, -0.85786545,  1.56672789]), array([-0.23333411,  0.20632363, -0.80133675,  1.73587805]), array([-0.36498881,  0.52600302, -0.4801429 ,  1.39142644]), array([-0.41539568,  0.74217732, -0.01227622,  0.7395642 ]), array([-0.36944782,  0.81527715,  0.46213933, -0.01083091]), array([-0.22642744,  0.71066606,  0.93936783, -1.01021577]), array([-0.00892589,  0.42883145,  1.18897233, -1.74077443]), array([ 0.22660096,  0.0517002 ,  1.1068182 , -1.92405165]), array([ 0.41005532, -0.29693012,  0.6808143 , -1.47495926]), array([ 0.48521772, -0.51258559,  0.05370639, -0.64539491]), array([ 0.417663  , -0.51547329, -0.71588293,  0.61057794]), array([ 0.20989945, -0.2789723 , -1.31808193,  1.6972301 ]), array([-0.08492151,  0.12510753, -1.555619  ,  2.21640575]), array([-0.37963177,  0.55019577, -1.32030983,  1.91504598]), array([-0.58989289,  0.85617843, -0.74359286,  1.09612783]), array([-0.66706415,  0.97859659, -0.01685984,  0.11844472]), array([-0.58535204,  0.87309513,  0.82205171, -1.16698164]), array([-0.34814683,  0.51985272,  1.50786441, -2.31349921]), array([-0.00845867, -0.01084392,  1.80187214, -2.83660639]), array([ 0.33251678, -0.53972913,  1.5220548 , -2.29877877]), array([ 0.57395443, -0.88909757,  0.8506743 , -1.14546192]), array([ 0.66227792, -0.9897414 ,  0.02017728,  0.14415152]), array([ 0.56997838, -0.80175587, -0.93344798,  1.72881771]), array([ 0.29908242, -0.30913141, -1.72312117,  3.11534711]), array([-0.08315313,  0.37699688, -1.98491703,  3.51987652]), array([-0.44967675,  1.01119311, -1.6016925 ,  2.68937509]), array([-0.70314623,  1.42828109, -0.90116783,  1.46392917]), array([-0.80177252,  1.59623253, -0.07487256,  0.2180398 ]), array([-0.72394184,  1.49081901,  0.8443507 , -1.27627909]), array([-0.47088945,  1.08272659,  1.65970504, -2.80278718]), array([-0.07741763,  0.38520798,  2.19752525, -4.04435356]), array([ 0.35720396, -0.43419659,  2.00983042, -3.86699684]), array([ 0.68247785, -1.07790494,  1.18689067, -2.48691537]), array([ 0.8218953 , -1.42254632,  0.19968977, -0.96426762]), array([ 0.75459258, -1.43976003, -0.85807324,  0.79326183]), array([ 0.48761236, -1.10140602, -1.78195125,  2.59637368]), array([ 0.05897502, -0.41058711, -2.42976401,  4.19816012]), array([-0.4314646 ,  0.47314784, -2.31833387,  4.31615657]), array([-0.81672247,  1.21668414, -1.46858326,  3.02633097]), array([-1.00690155,  1.67989017, -0.42147508,  1.61848727]), array([-0.98493444,  1.86772757,  0.63078134,  0.26001653]), array([-0.75610554,  1.75789692,  1.62055782, -1.36967148]), array([-0.35595715,  1.31549434,  2.3275385 , -3.05204563]), array([ 0.15035756,  0.55372516,  2.65209298, -4.43210369]), array([ 0.65139012, -0.34680402,  2.2070832 , -4.25226899]), array([ 0.985684  , -1.05481891,  1.0818817 , -2.7503158 ]), array([ 1.07698896, -1.44506632, -0.16850092, -1.15785884]), array([ 0.91472109, -1.49041281, -1.42578234,  0.72126271]), array([ 0.52287851, -1.1461743 , -2.44221275,  2.73697075]), array([-0.0361505 , -0.40732268, -3.04996577,  4.50173997]), array([-0.63332802,  0.52271794, -2.74921409,  4.43041987]), array([-1.08521394,  1.26868163, -1.71335421,  2.97168385]), array([-1.30937357,  1.72013613, -0.51800962,  1.57270265]), array([-1.29116306,  1.90318794,  0.69559698,  0.25067901]), array([-1.02953854,  1.78773441,  1.89146013, -1.44270084]), array([-0.55192063,  1.30869456,  2.83147306, -3.37840682]), array([ 0.07603713,  0.44640653,  3.34164683, -5.06850996]), array([ 0.71210682, -0.56024523,  2.83323751, -4.58992558]), array([ 1.16215327, -1.30108095,  1.62634935, -2.79800121]), array([ 1.35782358, -1.69718345,  0.32701124, -1.20027476]), array([ 1.29357522, -1.78600472, -0.96168782,  0.32617383]), array([ 0.97175376, -1.52812432, -2.22977299,  2.30896536]), array([ 0.41597596, -0.83828934, -3.27848897,  4.59869571]), array([-0.29589598,  0.23917885, -3.63462951,  5.7170532 ]), array([-0.94771759,  1.24507869, -2.7652793 ,  4.12809826]), array([-1.3858772 ,  1.8946614 , -1.59986594,  2.43902533]), array([-1.58385127,  2.24551268, -0.37549195,  1.10482016]), array([-1.53593163,  2.34055771,  0.85171873, -0.16574769]), array([-1.24009148,  2.1465686 ,  2.08624736, -1.82154505]), array([-0.71580124,  1.58642695,  3.11066757, -3.85121969]), array([-0.01649641,  0.58958886,  3.7980246 , -6.00223423]), array([ 0.72271584, -0.63022441,  3.35288458, -5.6346347 ]), array([ 1.26589318, -1.54531652,  2.04677077, -3.52825443]), array([ 1.54074324, -2.07682244,  0.70323788, -1.85302157]), array([ 1.54835695, -2.29852825, -0.62191464, -0.36347038]), array([ 1.28922281, -2.19185675, -1.9499368 ,  1.47371554]), array([ 0.78183018, -1.68361201, -3.0800747 ,  3.68957098]), array([ 0.07510218, -0.68649233, -3.92574039,  6.23524741]), array([-0.71325729,  0.63892122, -3.68547243,  6.37041037]), array([-1.32542542,  1.70429056, -2.39999527,  4.29168722]), array([-1.67421595,  2.40040422, -1.09388001,  2.75384971]), array([-1.76681697,  2.82218046,  0.15624844,  1.47301302]), array([-1.60914677,  2.96691106,  1.4167304 , -0.03901625]), array([-1.20216214,  2.80054244,  2.63043057, -1.64339614]), array([-0.58057383,  2.29889525,  3.48602181, -3.40943186]), array([ 0.14547089,  1.42527121,  3.68997172, -5.32339635]), array([ 0.86871302,  0.21318263,  3.41618363, -6.46194549]), array([ 1.42948555, -0.95919236,  2.05445893, -4.98142713]), array([ 1.67483529, -1.77445984,  0.39854924, -3.22775735]), array([ 1.59180912, -2.25844942, -1.2121145 , -1.59112553]), array([ 1.19575826, -2.37316929, -2.6968554 ,  0.49051754]), array([ 0.54540729, -2.04516465, -3.69231026,  2.82243988]), array([-0.22927511, -1.24202884, -3.95631523,  5.16342557]), array([-1.00267137, -0.05059515, -3.63330797,  6.34739025]), array([-1.60638339,  1.1024858 , -2.30189154,  4.97483052]), array([-1.91612295,  1.95275299, -0.79979998,  3.60222769]), array([-1.92939296,  2.55603743,  0.65069186,  2.42014853]), array([-1.65883861,  2.88835368,  2.03354161,  0.87190478]), array([-1.12300634,  2.89650846,  3.29119304, -0.79585088]), array([-0.3730975 ,  2.57330311,  4.07251217, -2.41727616]), array([ 0.43397564,  1.94678789,  3.83527911, -3.76498396]), array([ 1.11772579,  1.1197079 ,  2.95254049, -4.34637414]), array([ 1.60322882,  0.27624163,  1.87266108, -3.94256972]), array([ 1.85568026, -0.42076513,  0.63192448, -2.99412334]), array([ 1.84758645, -0.91530252, -0.74252689, -1.91218232]), array([ 1.53516785, -1.1243353 , -2.39895985, -0.06030483]), array([ 0.89193164, -0.88387501, -3.98223624,  2.56461701]), array([-0.01384101, -0.1158549 , -4.87798893,  4.75920085]), array([-0.95033159,  0.77136377, -4.26719273,  3.64732508]), array([-1.67751612,  1.28509502, -2.97730961,  1.57638688]), array([-2.14758868,  1.46595762, -1.76286104,  0.39353309]), array([-2.40184707,  1.49633464, -0.82547345,  0.01251784]), array([-2.48208403,  1.47238404,  0.00374772, -0.21626992]), array([-2.40139649,  1.41119303,  0.81624496, -0.42310954]), array([-2.14425245,  1.27918363,  1.79576061, -0.99245103]), array([-1.66439175,  0.96290081,  3.04666914, -2.32103748]), array([-0.91679668,  0.30191174,  4.38781168, -4.24719816]), array([ 0.02796732, -0.59149018,  4.82079022, -4.13187618]), array([ 0.9168387 , -1.1642839 ,  3.8906271 , -1.43157984]), array([ 1.53346857, -1.17688959,  2.21330178,  1.17627657]), array([ 1.79959754, -0.75411058,  0.48349433,  2.9218081 ]), array([ 1.73523538, -0.01140089, -1.07012768,  4.43846869]), array([ 1.40007919,  0.97983558, -2.21311607,  5.33605975]), array([ 0.86398843,  2.07425611, -3.14813764,  5.54392445]), array([ 0.1511617 , -3.08627824, -3.85949493,  5.7596688 ]), array([-0.60808892, -1.85242675, -3.64223551,  6.72312879]), array([-1.31092723, -0.36359682, -3.34667928,  8.01574176]), array([-1.84787359,  1.14240911, -1.78440253,  6.64891652]), array([-1.98581422,  2.28614584,  0.40066578,  4.85550362]), array([-1.72263882,  3.09930369,  2.08305206,  3.32328864]), array([-1.20031246, -2.64959604,  3.03672258,  2.18307333]), array([-0.55304589, -2.217815  ,  3.26827061,  2.44240369]), array([ 0.00828018, -1.53472363,  2.06801222,  4.71222351]), array([ 1.96590841e-01, -2.52081953e-01,  2.40087418e-03,  7.80262076e+00]), array([0.24447994, 1.2281764 , 0.92403583, 6.27487685]), array([0.58449703, 2.25684857, 2.27483329, 4.32886369]), array([1.05218844, 3.11398249, 2.10149525, 4.64405463]), array([ 1.29466003, -2.0494021 , -0.02152631,  6.85743506]), array([ 0.95338351, -0.28233632, -3.19454981, 10.71351327]), array([ 0.3249783 ,  1.76394691, -2.57328417,  8.95553835]), array([-0.10809695, -2.85159196, -2.03572363,  8.19973512]), array([-0.6114119 , -1.04459352, -3.18273673, 10.3513075 ]), array([-1.22504678,  1.08669654, -2.17394505,  9.75571331]), array([-1.31042606,  2.67902884,  1.11384275,  6.51540765]), array([-0.96161487, -2.43232768,  1.86493616,  5.67342452]), array([-0.70937098, -1.16019941,  0.4777811 ,  7.43658481]), array([-0.71186902,  0.53516089,  0.24798302,  8.45959266]), array([-0.328153  ,  1.8067182 ,  3.60360744,  4.08077786]), array([0.58414026, 2.2583573 , 5.07965736, 0.84384527]), array([ 1.57442492,  2.29835374,  4.65217765, -0.13543327]), array([ 2.4335507 ,  2.27180658,  4.00619125, -0.08030387]), array([-3.05664039,  2.24047267,  4.07786358, -0.39411539]), array([-2.15846123,  2.01857652,  5.02913328, -2.14761815]), array([-1.01870207,  1.23546432,  6.38661169, -6.01981279]), array([ 0.36584077, -0.34764383,  7.08540126, -8.56692552]), array([ 1.65748525, -1.65364547,  5.73296664, -4.26111922]), array([ 2.68088255, -2.19370122,  4.59142629, -1.53160831]), array([-2.73328869, -2.3940907 ,  4.26996069, -0.72931243]), array([-1.82864616, -2.5507512 ,  4.91052988, -0.91738732]), array([-0.74440279, -2.75430038,  5.88260781, -1.00140348]), array([ 0.45631503, -2.87876318,  5.88070318, -0.00641608]), array([ 1.50924739, -2.66681405,  4.42247914,  2.30956078]), array([ 2.14405699, -1.92091581,  1.75214597,  5.14278682]), array([ 2.19486473, -0.62771438, -1.09736099,  7.70412888]), array([ 1.84291596,  1.03908215, -1.99826202,  8.45530009])]</t>
+  </si>
+  <si>
+    <t>['[0,1,1]', '[2,0,1]', '[2,1,0]', '[0,0,0]', '[1,0,2]', '[2,2,2]', '[1,2,0]', '[1,1,2]', '[0,2,1]', '[1,1,1]']</t>
+  </si>
+  <si>
+    <t>[0,1,1]</t>
+  </si>
+  <si>
+    <t>[20, 30, 35, 45, 46, 62, 79, 80, 81, 85, 88]</t>
+  </si>
+  <si>
+    <t>[0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 1, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 1, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 0, 1, 1, 1, 1, 1, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 0, 0]</t>
+  </si>
+  <si>
+    <t>['[-0.03763371 -0.01533471  0.06554052 -0.01816017]', '[-0.00754409 -0.05458322  0.2277812  -0.36241836]', '[ 0.04879627 -0.15231473  0.32089719 -0.5887683 ]', '[ 0.11397169 -0.27767857  0.31375488 -0.63332862]', '[ 0.16759438 -0.39312519  0.2086893  -0.49480525]', '[ 0.1930193  -0.46685036  0.03906408 -0.22816919]', '[ 0.15689524 -0.41528579 -0.3922057   0.73207416]', '[ 0.04309269 -0.18588535 -0.71796191  1.51055937]', '[-0.1147829   0.15904975 -0.81547211  1.84906375]', '[-0.26363568  0.51494657 -0.63159042  1.62703318]', '[-0.35418658  0.78351571 -0.2539271   1.01663306]', '[-0.36122763  0.91144819  0.18313112  0.25239067]', '[-0.26190848  0.82452699  0.79137833 -1.10754289]', '[-0.05546354  0.48017359  1.23429726 -2.2781243 ]', '[ 0.20909957 -0.04617758  1.33805656 -2.84269804]', '[ 0.4464647  -0.59077472  0.966733   -2.46825376]', '[ 0.57603342 -0.99637145  0.30429255 -1.53991243]', '[ 0.56516121 -1.19760706 -0.40558213 -0.46475241]', '[ 0.40174223 -1.12742398 -1.19611308  1.15628906]', '[ 0.10260264 -0.74319691 -1.74734194  2.63891225]', '[-0.25807383 -0.1452152  -1.77061623  3.17399322]', '[-0.57803325  0.47992713 -1.33914933  2.90253669]', '[-0.76654767  0.96661355 -0.50946131  1.90351124]', '[-0.77569311  1.23009447  0.41548215  0.7177946 ]', '[-0.58806109  1.19602136  1.42512484 -1.05939455]', '[-0.22419017  0.80911508  2.15666013 -2.77219944]', '[ 0.24351216  0.12832591  2.41195464 -3.83615437]', '[ 0.68605805 -0.61539644  1.89713079 -3.37488714]', '[ 0.97114586 -1.17076883  0.91547062 -2.14026622]', '[ 1.04530152 -1.46977464 -0.17735917 -0.84855231]', '[ 0.89477831 -1.48139615 -1.30452838  0.74744522]', '[ 0.52853054 -1.13632691 -2.31243256  2.7180926 ]', '[-0.00622285 -0.40478327 -2.94168387  4.45563061]', '[-0.58612351  0.51898622 -2.68641416  4.4200075 ]', '[-1.02946155  1.26562112 -1.6880404   2.98147388]', '[-1.24242816  1.69323781 -0.43565571  1.33054958]', '[-1.21182289  1.82771613  0.73601439  0.0067021 ]', '[-0.93891834  1.63962643  1.9636951  -1.92759976]', '[-0.44168666  1.03722575  2.96374159 -4.12268742]', '[ 0.21591193  0.02466871  3.45241902 -5.66837193]', '[ 0.84836729 -1.02581088  2.71422753 -4.51370957]', '[ 1.27571152 -1.75406603  1.5388616  -2.81668488]', '[ 1.46006414 -2.17482048  0.30043993 -1.42329069]', '[ 1.38980612 -2.30547508 -0.99335974  0.12738976]', '[ 1.06358236 -2.09161958 -2.23581524  2.0560564 ]', '[ 0.52220739 -1.48275237 -3.12369363  4.08301653]', '[-0.16205146 -0.45877502 -3.61507363  5.9709291 ]', '[-0.85114125  0.74161377 -3.05382728  5.53102681]', '[-1.33398237  1.6630836  -1.74736228  3.70937293]', '[-1.54893837  2.25471242 -0.40453803  2.25327623]', '[-1.49853577  2.56982702  0.89743448  0.8897805 ]', '[-1.18476057  2.56325555  2.20820926 -0.97780077]', '[-0.63763759  2.16756446  3.17864675 -3.01347746]', '[ 0.04763391  1.34499139  3.60234545 -5.22326618]', '[ 0.77769988  0.11581909  3.55436928 -6.70549147]', '[ 1.37511117 -1.11416463  2.26855616 -5.29353241]', '[ 1.66901485 -2.00185204  0.67150329 -3.654969  ]', '[ 1.64898222 -2.59064389 -0.84624381 -2.23311428]', '[ 1.3376853  -2.87023818 -2.23088287 -0.55819507]', '[ 0.76844987 -2.79841638 -3.38707181  1.25163477]', '[ 0.03214189 -2.38322131 -3.81509527  2.85546939]', '[-0.69216251 -1.6842459  -3.31841119  4.03529743]', '[-1.26437374 -0.84583794 -2.37443982  4.20085939]', '[-1.64311833 -0.02683747 -1.38268863  3.88883841]', '[-1.80225972  0.6810347  -0.16589945  3.13651581]', '[-1.68953145  1.20180705  1.34310917  1.97235398]', '[-1.23602846  1.36488578  3.16439353 -0.47813493]', '[-0.45499551  0.9621599   4.52618159 -3.5756089 ]', '[ 0.50746543  0.00891283  4.86389701 -5.4365829 ]', '[ 1.38892815 -0.95305065  3.81349134 -3.86990229]', '[ 2.02667789 -1.5491763   2.59821945 -2.24813705]', '[ 2.44772722 -1.91680222  1.66451387 -1.56139225]', '[ 2.71122554 -2.21203949  1.01129872 -1.45597189]', '[ 2.86466063 -2.51382917  0.54886305 -1.57808861]', '[ 2.93281362 -2.82270549  0.15269739 -1.49941578]', '[ 2.93208693 -3.10476878 -0.14746305 -1.29364612]', '[ 2.87623148  2.95623851 -0.41251997 -0.89344417]', '[ 2.76285032  2.83575041 -0.7415756  -0.27477734]', '[ 2.56771962  2.86102521 -1.24976293  0.56417732]', '[ 2.2435186   3.07643993 -2.04813039  1.63297856]', '[ 1.7270624  -2.74656633 -3.15150121  3.05585952]', '[ 0.98351602 -1.93153035 -4.25268287  5.28308   ]', '[ 0.02446784 -0.52661454 -5.28997308  8.70478415]', '[-0.99243135  1.17284667 -4.52758794  7.37280859]', '[-1.75960679  2.37434836 -3.19327709  4.89734033]', '[-2.28057554 -3.08819753 -2.07333755  3.43597032]', '[-2.62186651 -2.49007844 -1.41021359  2.57730299]', '[-2.86722901 -2.04980156 -1.09067299  1.8437913 ]', '[-3.06521369 -1.76772904 -0.92298669  0.99852011]', '[ 3.02456596 -1.6143193  -1.05226153  0.58054211]', '[ 2.77838113 -1.51248806 -1.46560367  0.51528611]', '[ 2.41285798 -1.36798452 -2.26245575  1.06473089]', '[ 1.84297094 -1.01866796 -3.51063534  2.6309546 ]', '[ 0.98760711 -0.24557174 -5.01691815  5.05119857]', '[-0.09053382  0.79886437 -5.48535159  4.67449353]', '[-1.10577937  1.42040353 -4.47556696  1.42555639]', '[-1.82617272  1.41113985 -2.67500271 -1.31568865]', '[-2.18437951  0.98208979 -0.97977569 -2.78244071]', '[-2.22784997  0.28865841  0.47975814 -4.09613256]', '[-2.01645458 -0.64301816  1.57453158 -5.16947744]']</t>
+  </si>
+  <si>
+    <t>[0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50, 51, 52, 53, 54, 55, 56, 57, 58, 59, 60, 61, 62, 63, 64, 65, 66, 67, 68, 69, 70, 71, 72, 73, 74, 75, 76, 77, 78, 79, 80, 81, 82, 83, 84, 85, 86, 87, 88, 89, 90, 91, 92, 93, 94, 95, 96, 97, 98, 99]</t>
+  </si>
+  <si>
+    <t>[array([-0.03763371, -0.01533471,  0.06554052, -0.01816017], dtype=float32), array([-0.00754409, -0.05458322,  0.2277812 , -0.36241836]), array([ 0.04879627, -0.15231473,  0.32089719, -0.5887683 ]), array([ 0.11397169, -0.27767857,  0.31375488, -0.63332862]), array([ 0.16759438, -0.39312519,  0.2086893 , -0.49480525]), array([ 0.1930193 , -0.46685036,  0.03906408, -0.22816919]), array([ 0.15689524, -0.41528579, -0.3922057 ,  0.73207416]), array([ 0.04309269, -0.18588535, -0.71796191,  1.51055937]), array([-0.1147829 ,  0.15904975, -0.81547211,  1.84906375]), array([-0.26363568,  0.51494657, -0.63159042,  1.62703318]), array([-0.35418658,  0.78351571, -0.2539271 ,  1.01663306]), array([-0.36122763,  0.91144819,  0.18313112,  0.25239067]), array([-0.26190848,  0.82452699,  0.79137833, -1.10754289]), array([-0.05546354,  0.48017359,  1.23429726, -2.2781243 ]), array([ 0.20909957, -0.04617758,  1.33805656, -2.84269804]), array([ 0.4464647 , -0.59077472,  0.966733  , -2.46825376]), array([ 0.57603342, -0.99637145,  0.30429255, -1.53991243]), array([ 0.56516121, -1.19760706, -0.40558213, -0.46475241]), array([ 0.40174223, -1.12742398, -1.19611308,  1.15628906]), array([ 0.10260264, -0.74319691, -1.74734194,  2.63891225]), array([-0.25807383, -0.1452152 , -1.77061623,  3.17399322]), array([-0.57803325,  0.47992713, -1.33914933,  2.90253669]), array([-0.76654767,  0.96661355, -0.50946131,  1.90351124]), array([-0.77569311,  1.23009447,  0.41548215,  0.7177946 ]), array([-0.58806109,  1.19602136,  1.42512484, -1.05939455]), array([-0.22419017,  0.80911508,  2.15666013, -2.77219944]), array([ 0.24351216,  0.12832591,  2.41195464, -3.83615437]), array([ 0.68605805, -0.61539644,  1.89713079, -3.37488714]), array([ 0.97114586, -1.17076883,  0.91547062, -2.14026622]), array([ 1.04530152, -1.46977464, -0.17735917, -0.84855231]), array([ 0.89477831, -1.48139615, -1.30452838,  0.74744522]), array([ 0.52853054, -1.13632691, -2.31243256,  2.7180926 ]), array([-0.00622285, -0.40478327, -2.94168387,  4.45563061]), array([-0.58612351,  0.51898622, -2.68641416,  4.4200075 ]), array([-1.02946155,  1.26562112, -1.6880404 ,  2.98147388]), array([-1.24242816,  1.69323781, -0.43565571,  1.33054958]), array([-1.21182289,  1.82771613,  0.73601439,  0.0067021 ]), array([-0.93891834,  1.63962643,  1.9636951 , -1.92759976]), array([-0.44168666,  1.03722575,  2.96374159, -4.12268742]), array([ 0.21591193,  0.02466871,  3.45241902, -5.66837193]), array([ 0.84836729, -1.02581088,  2.71422753, -4.51370957]), array([ 1.27571152, -1.75406603,  1.5388616 , -2.81668488]), array([ 1.46006414, -2.17482048,  0.30043993, -1.42329069]), array([ 1.38980612, -2.30547508, -0.99335974,  0.12738976]), array([ 1.06358236, -2.09161958, -2.23581524,  2.0560564 ]), array([ 0.52220739, -1.48275237, -3.12369363,  4.08301653]), array([-0.16205146, -0.45877502, -3.61507363,  5.9709291 ]), array([-0.85114125,  0.74161377, -3.05382728,  5.53102681]), array([-1.33398237,  1.6630836 , -1.74736228,  3.70937293]), array([-1.54893837,  2.25471242, -0.40453803,  2.25327623]), array([-1.49853577,  2.56982702,  0.89743448,  0.8897805 ]), array([-1.18476057,  2.56325555,  2.20820926, -0.97780077]), array([-0.63763759,  2.16756446,  3.17864675, -3.01347746]), array([ 0.04763391,  1.34499139,  3.60234545, -5.22326618]), array([ 0.77769988,  0.11581909,  3.55436928, -6.70549147]), array([ 1.37511117, -1.11416463,  2.26855616, -5.29353241]), array([ 1.66901485, -2.00185204,  0.67150329, -3.654969  ]), array([ 1.64898222, -2.59064389, -0.84624381, -2.23311428]), array([ 1.3376853 , -2.87023818, -2.23088287, -0.55819507]), array([ 0.76844987, -2.79841638, -3.38707181,  1.25163477]), array([ 0.03214189, -2.38322131, -3.81509527,  2.85546939]), array([-0.69216251, -1.6842459 , -3.31841119,  4.03529743]), array([-1.26437374, -0.84583794, -2.37443982,  4.20085939]), array([-1.64311833, -0.02683747, -1.38268863,  3.88883841]), array([-1.80225972,  0.6810347 , -0.16589945,  3.13651581]), array([-1.68953145,  1.20180705,  1.34310917,  1.97235398]), array([-1.23602846,  1.36488578,  3.16439353, -0.47813493]), array([-0.45499551,  0.9621599 ,  4.52618159, -3.5756089 ]), array([ 0.50746543,  0.00891283,  4.86389701, -5.4365829 ]), array([ 1.38892815, -0.95305065,  3.81349134, -3.86990229]), array([ 2.02667789, -1.5491763 ,  2.59821945, -2.24813705]), array([ 2.44772722, -1.91680222,  1.66451387, -1.56139225]), array([ 2.71122554, -2.21203949,  1.01129872, -1.45597189]), array([ 2.86466063, -2.51382917,  0.54886305, -1.57808861]), array([ 2.93281362, -2.82270549,  0.15269739, -1.49941578]), array([ 2.93208693, -3.10476878, -0.14746305, -1.29364612]), array([ 2.87623148,  2.95623851, -0.41251997, -0.89344417]), array([ 2.76285032,  2.83575041, -0.7415756 , -0.27477734]), array([ 2.56771962,  2.86102521, -1.24976293,  0.56417732]), array([ 2.2435186 ,  3.07643993, -2.04813039,  1.63297856]), array([ 1.7270624 , -2.74656633, -3.15150121,  3.05585952]), array([ 0.98351602, -1.93153035, -4.25268287,  5.28308   ]), array([ 0.02446784, -0.52661454, -5.28997308,  8.70478415]), array([-0.99243135,  1.17284667, -4.52758794,  7.37280859]), array([-1.75960679,  2.37434836, -3.19327709,  4.89734033]), array([-2.28057554, -3.08819753, -2.07333755,  3.43597032]), array([-2.62186651, -2.49007844, -1.41021359,  2.57730299]), array([-2.86722901, -2.04980156, -1.09067299,  1.8437913 ]), array([-3.06521369, -1.76772904, -0.92298669,  0.99852011]), array([ 3.02456596, -1.6143193 , -1.05226153,  0.58054211]), array([ 2.77838113, -1.51248806, -1.46560367,  0.51528611]), array([ 2.41285798, -1.36798452, -2.26245575,  1.06473089]), array([ 1.84297094, -1.01866796, -3.51063534,  2.6309546 ]), array([ 0.98760711, -0.24557174, -5.01691815,  5.05119857]), array([-0.09053382,  0.79886437, -5.48535159,  4.67449353]), array([-1.10577937,  1.42040353, -4.47556696,  1.42555639]), array([-1.82617272,  1.41113985, -2.67500271, -1.31568865]), array([-2.18437951,  0.98208979, -0.97977569, -2.78244071]), array([-2.22784997,  0.28865841,  0.47975814, -4.09613256]), array([-2.01645458, -0.64301816,  1.57453158, -5.16947744])]</t>
+  </si>
+  <si>
+    <t>['[2,2,2]', '[1,2,0]', '[0,2,1]', '[1,0,2]', '[2,1,0]', '[1,1,2]', '[2,0,1]', '[0,0,0]', '[0,1,1]', '[1,1,1]']</t>
+  </si>
+  <si>
+    <t>[8, 18, 23, 31, 36, 47, 58, 60, 62, 64, 74, 81, 92, 94, 95, 98, 100, 101]</t>
+  </si>
+  <si>
+    <t>[0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 1, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 1, 1, 2, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 1, 2, 2, 2, 2, 2, 2, 2, 2, 2, 1, 2, 2, 2, 0, 0, 0]</t>
+  </si>
+  <si>
+    <t>['[-0.03763371 -0.01533471  0.06554052 -0.01816017]', '[-0.00754409 -0.05458322  0.2277812  -0.36241836]', '[ 0.04879627 -0.15231473  0.32089719 -0.5887683 ]', '[ 0.11397169 -0.27767857  0.31375488 -0.63332862]', '[ 0.16759438 -0.39312519  0.2086893  -0.49480525]', '[ 0.1930193  -0.46685036  0.03906408 -0.22816919]', '[ 0.15689524 -0.41528579 -0.3922057   0.73207416]', '[ 0.04309269 -0.18588535 -0.71796191  1.51055937]', '[-0.10156356  0.12486504 -0.68790627  1.51697551]', '[-0.22927161  0.42348907 -0.55357165  1.39819937]', '[-0.31090932  0.65984646 -0.24293606  0.92318871]', '[-0.32187145  0.78154289  0.13516303  0.28054481]', '[-0.23584819  0.70921086  0.7080842  -0.98918522]', '[-0.0490822   0.39857798  1.12159951 -2.05785564]', '[ 0.19121042 -0.07513787  1.21472891 -2.55061341]', '[ 0.40736477 -0.56371893  0.88570962 -2.21595125]', '[ 0.52742041 -0.92731447  0.29092255 -1.37281403]', '[ 0.52026319 -1.10307428 -0.35718941 -0.37601845]', '[ 0.38078573 -1.04969914 -1.00966352  0.89742565]', '[ 0.11982675 -0.72393616 -1.55616388  2.31665167]', '[-0.21808542 -0.15771215 -1.7435872   3.20034189]', '[-0.53763473  0.47750108 -1.35965403  2.9710476 ]', '[-0.7335312   0.97873624 -0.56074333  1.97669848]', '[-0.74532914  1.22888041  0.43575859  0.51969426]', '[-0.55762671  1.15798271  1.40751448 -1.22822949]', '[-0.19987373  0.74159332  2.11433808 -2.89133393]', '[ 0.25621145  0.04786928  2.33452877 -3.83409026]', '[ 0.67971194 -0.68291439  1.79096234 -3.26502541]', '[ 0.94438666 -1.21433263  0.82171613 -2.01789506]', '[ 1.00240578 -1.4887737  -0.24293637 -0.72496804]', '[ 0.83397838 -1.45048557 -1.41482271  1.12279308]', '[ 0.46079208 -1.05862045 -2.26825986  2.79184567]', '[-0.05830476 -0.32506263 -2.82356625  4.3803936 ]', '[-0.60638976  0.56555233 -2.49795946  4.19441485]', '[-1.01180757  1.26945683 -1.50345724  2.79135538]', '[-1.19834906  1.68704574 -0.35201531  1.40431828]', '[-1.14435838  1.81068665  0.88029715 -0.17490364]', '[-0.84725788  1.58375577  2.05710869 -2.13252421]', '[-0.33826718  0.94126431  2.98316292 -4.29793115]', '[ 0.30989627 -0.08287143  3.32445905 -5.56946979]', '[ 0.90441643 -1.09350752  2.48642081 -4.27764831]', '[ 1.28396209 -1.78060198  1.29223105 -2.6415233 ]', '[ 1.4181963  -2.16859989  0.0480973  -1.26072747]', '[ 1.29838176 -2.26370005 -1.23135255  0.32573783]', '[ 0.92972081 -2.00473394 -2.41220524  2.30885261]', '[ 0.35565597 -1.31808922 -3.27684367  4.60566633]', '[-0.3567189  -0.17709846 -3.70313653  6.49175574]', '[-1.01171644  1.0098533  -2.66916798  4.99923804]', '[-1.41239776  1.83087569 -1.32783295  3.27453906]', '[-1.54293208  2.34314915  0.01757477  1.87350053]', '[-1.40933434  2.57969048  1.30322334  0.47647324]', '[-1.01968371  2.48547123  2.54569231 -1.44133519]', '[-0.42200684  1.99278496  3.33267047 -3.51269108]', '[ 0.27591291  1.07478088  3.58574996 -5.63459768]', '[ 0.97696908 -0.17803572  3.24011211 -6.4331605 ]', '[ 1.48887662 -1.31462378  1.78732219 -4.79482374]', '[ 1.68503897 -2.11528677  0.17792998 -3.26108332]', '[ 1.56664404 -2.62283912 -1.33258754 -1.8000322 ]', '[ 1.16074957 -2.80953142 -2.68020287 -0.06708078]', '[ 0.51610692 -2.63694675 -3.65531844  1.76199969]', '[-0.23278645 -2.14360256 -3.66964702  3.09738752]', '[-0.90532614 -1.41889891 -2.9837492   4.02606507]', '[-1.40300067 -0.61591181 -1.96635994  3.86241285]', '[-1.69398292  0.11545251 -0.91782992  3.38572982]', '[-1.74489032  0.68669     0.44049041  2.28638947]', '[-1.51453144  1.03301012  1.89971487  1.0627469 ]', '[-0.96175732  1.00105357  3.58023446 -1.49227482]', '[-0.12264012  0.42363698  4.64917965 -4.09856064]', '[ 0.80349045 -0.45108482  4.3711098  -4.11339947]', '[ 1.56147994 -1.0890613   3.15459061 -2.24124692]', '[ 2.06810919 -1.39568269  1.94587959 -0.97650954]', '[ 2.35728741 -1.53340655  0.9882419  -0.50519685]', '[ 2.46711835 -1.60078335  0.12883209 -0.20793205]', '[ 2.4098045  -1.61910635 -0.71478824  0.04970025]', '[ 2.17024157 -1.55787416 -1.7193412   0.65597442]', '[ 1.69606468 -1.27925355 -3.06256975  2.30055691]', '[ 0.93430807 -0.566752   -4.54065002  4.88950059]', '[-0.06518143  0.55263865 -5.18623772  5.61040933]', '[-1.03652871  1.42338667 -4.3732442   2.90187468]', '[-1.77832723  1.7431851  -3.00098531  0.46783088]', '[-2.2382424   1.68718831 -1.63706567 -0.84957379]', '[-2.44568571  1.43766439 -0.48870724 -1.53824996]', '[-2.43940206  1.07014069  0.53312394 -2.12289392]', '[-2.23099453  0.57602493  1.5757872  -2.88799877]', '[-1.79354886 -0.11814572  2.82988468 -4.08466225]', '[-1.10043116 -1.01607304  4.05909404 -4.64047416]', '[-0.19634822 -1.84869455  4.86612531 -3.40030901]', '[ 0.77039523 -2.29899258  4.56873781 -1.00274407]', '[ 1.54777079 -2.24235671  3.05861867  1.5251329 ]', '[ 1.95045418 -1.70241236  0.92749037  3.77522643]', '[ 1.91382362 -0.73419089 -1.24528314  5.89086209]', '[ 1.50110283  0.61094185 -2.6779545   7.24186099]', '[ 0.91489616  2.01219404 -3.18517211  6.7377631 ]', '[ 0.2089309  -2.91229492 -3.81086778  7.04034261]', '[-0.56771904 -1.37271642 -3.97260538  8.62460828]', '[-1.35725011  0.49756136 -3.52127545  9.24086527]', '[-1.82551185  2.07802229 -1.09088185  6.61937474]', '[-1.8417077  -3.05534002  0.68676565  5.02522485]', '[-1.63692921 -2.16360362  1.22686326  4.02928826]', '[-1.37443209 -1.38311067  1.36508477  3.93565841]', '[-1.1011816  -0.53126404  1.39423559  4.61381668]', '[-0.75565511  0.37234406  2.28627025  3.9940085 ]', '[-0.13178539  0.92474143  3.90492951  1.35173659]', '[ 0.74078368  0.87734915  4.54356693 -1.55356405]', '[ 1.59462142  0.44180811  3.8634311  -2.48176111]', '[ 2.2693473  -0.03089216  2.91063321 -2.17421304]']</t>
+  </si>
+  <si>
+    <t>[0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50, 51, 52, 53, 54, 55, 56, 57, 58, 59, 60, 61, 62, 63, 64, 65, 66, 67, 68, 69, 70, 71, 72, 73, 74, 75, 76, 77, 78, 79, 80, 81, 82, 83, 84, 85, 86, 87, 88, 89, 90, 91, 92, 93, 94, 95, 96, 97, 98, 99, 100, 101, 102, 103, 104, 105]</t>
+  </si>
+  <si>
+    <t>[array([-0.03763371, -0.01533471,  0.06554052, -0.01816017], dtype=float32), array([-0.00754409, -0.05458322,  0.2277812 , -0.36241836]), array([ 0.04879627, -0.15231473,  0.32089719, -0.5887683 ]), array([ 0.11397169, -0.27767857,  0.31375488, -0.63332862]), array([ 0.16759438, -0.39312519,  0.2086893 , -0.49480525]), array([ 0.1930193 , -0.46685036,  0.03906408, -0.22816919]), array([ 0.15689524, -0.41528579, -0.3922057 ,  0.73207416]), array([ 0.04309269, -0.18588535, -0.71796191,  1.51055937]), array([-0.10156356,  0.12486504, -0.68790627,  1.51697551]), array([-0.22927161,  0.42348907, -0.55357165,  1.39819937]), array([-0.31090932,  0.65984646, -0.24293606,  0.92318871]), array([-0.32187145,  0.78154289,  0.13516303,  0.28054481]), array([-0.23584819,  0.70921086,  0.7080842 , -0.98918522]), array([-0.0490822 ,  0.39857798,  1.12159951, -2.05785564]), array([ 0.19121042, -0.07513787,  1.21472891, -2.55061341]), array([ 0.40736477, -0.56371893,  0.88570962, -2.21595125]), array([ 0.52742041, -0.92731447,  0.29092255, -1.37281403]), array([ 0.52026319, -1.10307428, -0.35718941, -0.37601845]), array([ 0.38078573, -1.04969914, -1.00966352,  0.89742565]), array([ 0.11982675, -0.72393616, -1.55616388,  2.31665167]), array([-0.21808542, -0.15771215, -1.7435872 ,  3.20034189]), array([-0.53763473,  0.47750108, -1.35965403,  2.9710476 ]), array([-0.7335312 ,  0.97873624, -0.56074333,  1.97669848]), array([-0.74532914,  1.22888041,  0.43575859,  0.51969426]), array([-0.55762671,  1.15798271,  1.40751448, -1.22822949]), array([-0.19987373,  0.74159332,  2.11433808, -2.89133393]), array([ 0.25621145,  0.04786928,  2.33452877, -3.83409026]), array([ 0.67971194, -0.68291439,  1.79096234, -3.26502541]), array([ 0.94438666, -1.21433263,  0.82171613, -2.01789506]), array([ 1.00240578, -1.4887737 , -0.24293637, -0.72496804]), array([ 0.83397838, -1.45048557, -1.41482271,  1.12279308]), array([ 0.46079208, -1.05862045, -2.26825986,  2.79184567]), array([-0.05830476, -0.32506263, -2.82356625,  4.3803936 ]), array([-0.60638976,  0.56555233, -2.49795946,  4.19441485]), array([-1.01180757,  1.26945683, -1.50345724,  2.79135538]), array([-1.19834906,  1.68704574, -0.35201531,  1.40431828]), array([-1.14435838,  1.81068665,  0.88029715, -0.17490364]), array([-0.84725788,  1.58375577,  2.05710869, -2.13252421]), array([-0.33826718,  0.94126431,  2.98316292, -4.29793115]), array([ 0.30989627, -0.08287143,  3.32445905, -5.56946979]), array([ 0.90441643, -1.09350752,  2.48642081, -4.27764831]), array([ 1.28396209, -1.78060198,  1.29223105, -2.6415233 ]), array([ 1.4181963 , -2.16859989,  0.0480973 , -1.26072747]), array([ 1.29838176, -2.26370005, -1.23135255,  0.32573783]), array([ 0.92972081, -2.00473394, -2.41220524,  2.30885261]), array([ 0.35565597, -1.31808922, -3.27684367,  4.60566633]), array([-0.3567189 , -0.17709846, -3.70313653,  6.49175574]), array([-1.01171644,  1.0098533 , -2.66916798,  4.99923804]), array([-1.41239776,  1.83087569, -1.32783295,  3.27453906]), array([-1.54293208,  2.34314915,  0.01757477,  1.87350053]), array([-1.40933434,  2.57969048,  1.30322334,  0.47647324]), array([-1.01968371,  2.48547123,  2.54569231, -1.44133519]), array([-0.42200684,  1.99278496,  3.33267047, -3.51269108]), array([ 0.27591291,  1.07478088,  3.58574996, -5.63459768]), array([ 0.97696908, -0.17803572,  3.24011211, -6.4331605 ]), array([ 1.48887662, -1.31462378,  1.78732219, -4.79482374]), array([ 1.68503897, -2.11528677,  0.17792998, -3.26108332]), array([ 1.56664404, -2.62283912, -1.33258754, -1.8000322 ]), array([ 1.16074957, -2.80953142, -2.68020287, -0.06708078]), array([ 0.51610692, -2.63694675, -3.65531844,  1.76199969]), array([-0.23278645, -2.14360256, -3.66964702,  3.09738752]), array([-0.90532614, -1.41889891, -2.9837492 ,  4.02606507]), array([-1.40300067, -0.61591181, -1.96635994,  3.86241285]), array([-1.69398292,  0.11545251, -0.91782992,  3.38572982]), array([-1.74489032,  0.68669   ,  0.44049041,  2.28638947]), array([-1.51453144,  1.03301012,  1.89971487,  1.0627469 ]), array([-0.96175732,  1.00105357,  3.58023446, -1.49227482]), array([-0.12264012,  0.42363698,  4.64917965, -4.09856064]), array([ 0.80349045, -0.45108482,  4.3711098 , -4.11339947]), array([ 1.56147994, -1.0890613 ,  3.15459061, -2.24124692]), array([ 2.06810919, -1.39568269,  1.94587959, -0.97650954]), array([ 2.35728741, -1.53340655,  0.9882419 , -0.50519685]), array([ 2.46711835, -1.60078335,  0.12883209, -0.20793205]), array([ 2.4098045 , -1.61910635, -0.71478824,  0.04970025]), array([ 2.17024157, -1.55787416, -1.7193412 ,  0.65597442]), array([ 1.69606468, -1.27925355, -3.06256975,  2.30055691]), array([ 0.93430807, -0.566752  , -4.54065002,  4.88950059]), array([-0.06518143,  0.55263865, -5.18623772,  5.61040933]), array([-1.03652871,  1.42338667, -4.3732442 ,  2.90187468]), array([-1.77832723,  1.7431851 , -3.00098531,  0.46783088]), array([-2.2382424 ,  1.68718831, -1.63706567, -0.84957379]), array([-2.44568571,  1.43766439, -0.48870724, -1.53824996]), array([-2.43940206,  1.07014069,  0.53312394, -2.12289392]), array([-2.23099453,  0.57602493,  1.5757872 , -2.88799877]), array([-1.79354886, -0.11814572,  2.82988468, -4.08466225]), array([-1.10043116, -1.01607304,  4.05909404, -4.64047416]), array([-0.19634822, -1.84869455,  4.86612531, -3.40030901]), array([ 0.77039523, -2.29899258,  4.56873781, -1.00274407]), array([ 1.54777079, -2.24235671,  3.05861867,  1.5251329 ]), array([ 1.95045418, -1.70241236,  0.92749037,  3.77522643]), array([ 1.91382362, -0.73419089, -1.24528314,  5.89086209]), array([ 1.50110283,  0.61094185, -2.6779545 ,  7.24186099]), array([ 0.91489616,  2.01219404, -3.18517211,  6.7377631 ]), array([ 0.2089309 , -2.91229492, -3.81086778,  7.04034261]), array([-0.56771904, -1.37271642, -3.97260538,  8.62460828]), array([-1.35725011,  0.49756136, -3.52127545,  9.24086527]), array([-1.82551185,  2.07802229, -1.09088185,  6.61937474]), array([-1.8417077 , -3.05534002,  0.68676565,  5.02522485]), array([-1.63692921, -2.16360362,  1.22686326,  4.02928826]), array([-1.37443209, -1.38311067,  1.36508477,  3.93565841]), array([-1.1011816 , -0.53126404,  1.39423559,  4.61381668]), array([-0.75565511,  0.37234406,  2.28627025,  3.9940085 ]), array([-0.13178539,  0.92474143,  3.90492951,  1.35173659]), array([ 0.74078368,  0.87734915,  4.54356693, -1.55356405]), array([ 1.59462142,  0.44180811,  3.8634311 , -2.48176111]), array([ 2.2693473 , -0.03089216,  2.91063321, -2.17421304])]</t>
+  </si>
+  <si>
+    <t>['[1,1,2]', '[0,0,0]', '[2,1,0]', '[1,0,2]', '[2,2,2]', '[1,1,1]', '[0,1,1]', '[1,2,0]', '[0,2,1]', '[2,0,1]']</t>
+  </si>
+  <si>
+    <t>[6, 7, 8, 9, 11, 18, 20, 22, 23, 30, 31, 32, 33, 34, 35, 42, 43, 45, 46, 47, 48, 55, 60, 70, 71, 74, 75, 76, 85, 86, 87, 88, 89, 90, 91, 100, 101, 102, 103]</t>
+  </si>
+  <si>
+    <t>[0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 1, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 1, 1, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 1, 2, 2, 2, 2, 2, 2, 2]</t>
+  </si>
+  <si>
+    <t>['[-0.03763371 -0.01533471  0.06554052 -0.01816017]', '[-0.00754409 -0.05458322  0.2277812  -0.36241836]', '[ 0.04879627 -0.15231473  0.32089719 -0.5887683 ]', '[ 0.11397169 -0.27767857  0.31375488 -0.63332862]', '[ 0.16759438 -0.39312519  0.2086893  -0.49480525]', '[ 0.1930193  -0.46685036  0.03906408 -0.22816919]', '[ 0.16956871 -0.44830261 -0.26820417  0.40739083]', '[ 0.09055011 -0.31127879 -0.50323119  0.93116007]', '[-0.02165415 -0.09380121 -0.58952709  1.1892161 ]', '[-0.13228272  0.13968862 -0.48657385  1.08703787]', '[-0.21842905  0.35335821 -0.35084306  1.00036988]', '[-0.25195003  0.48960053  0.02384951  0.33984609]', '[-0.19642111  0.45311714  0.51937854 -0.69256597]', '[-0.05307561  0.22491996  0.88091359 -1.53539268]', '[ 0.13802188 -0.12918667  0.97826521 -1.90895317]', '[ 0.31605351 -0.49658808  0.75465775 -1.67554103]', '[ 0.42468334 -0.77124123  0.30822734 -1.02677713]', '[ 0.43446136 -0.89671866 -0.21095426 -0.21717049]', '[ 0.33260677 -0.82796451 -0.7878784   0.89095935]', '[ 0.11895536 -0.52014693 -1.30899108  2.13554748]', '[-0.15506189 -0.04523277 -1.35957979  2.48102867]', '[-0.40691623  0.44686407 -1.08935977  2.30736054]', '[-0.5564256   0.80512411 -0.37787988  1.22668507]', '[-0.5537129   0.92864525  0.40116417  0.00228018]', '[-0.39080819  0.77698019  1.20046194 -1.50281488]', '[-0.08999453  0.34390987  1.74701155 -2.7385827 ]', '[ 0.27317466 -0.25633786  1.78355809 -3.07071984]', '[ 0.58381965 -0.80979964  1.25275733 -2.34462057]', '[ 0.75625447 -1.16954501  0.44849885 -1.22960907]', '[ 0.75951625 -1.29827451 -0.41255534 -0.05405852]', '[ 0.58721868 -1.16293685 -1.28442211  1.40677667]', '[ 0.26062646 -0.74059903 -1.93007964  2.76947897]', '[-0.15455451 -0.09997029 -2.1187961   3.44680983]', '[-0.53832222  0.54281118 -1.61923427  2.79320592]', '[-0.77515416  0.97344559 -0.7144475   1.47289343]', '[-0.81781851  1.12775092  0.2893512   0.06754646]', '[-0.65265505  0.97025693  1.34137983 -1.64601959]', '[-0.29504341  0.47397839  2.17667958 -3.2498051 ]', '[ 0.17851251 -0.26140617  2.42570577 -3.84182313]', '[ 0.62007723 -0.95414925  1.8948333  -2.92440573]', '[ 0.91323312 -1.40615516  1.00424535 -1.58868856]', '[ 1.0140886  -1.59337681 -0.00368105 -0.29095715]', '[ 0.90377872 -1.49733625 -1.08699828  1.26266421]', '[ 0.58806273 -1.08075213 -2.03765882  2.91285899]', '[ 0.09740728 -0.31435836 -2.7787139   4.60552365]', '[-0.44641784  0.59653397 -2.49509314  4.16201215]', '[-0.8555011   1.26875197 -1.54432101  2.51233737]', '[-1.05422086  1.60746709 -0.43068434  0.89779489]', '[-1.02624063  1.63274173  0.70515713 -0.64786431]', '[-0.76897872  1.31596704  1.8464915  -2.55194347]', '[-0.29973655  0.60200961  2.78982478 -4.53839163]', '[ 0.2961404  -0.40320984  2.97780305 -5.10401646]', '[ 0.82020823 -1.29165304  2.17295204 -3.6414326 ]', '[ 1.14971312 -1.86035241  1.10163347 -2.08347611]', '[ 1.2558649  -2.13780578 -0.04434794 -0.70625533]', '[ 1.12695891 -2.12113439 -1.22819019  0.88665259]', '[ 0.7687793  -1.7498437  -2.31568493  2.8699482 ]', '[ 0.21716124 -0.95313572 -3.15786491  5.10909962]', '[-0.45473437  0.22469162 -3.3503157   6.19775683]', '[-1.02812904  1.318461   -2.27070847  4.54510444]', '[-1.34409922  2.03119242 -0.89208004  2.66036124]', '[-1.39396312  2.42178651  0.38673363  1.25594608]', '[-1.18284725  2.49060831  1.6961625  -0.58052741]', '[-0.73350468  2.18138333  2.73020548 -2.53925451]', '[-0.12381008  1.46260449  3.29739573 -4.67114052]', '[ 0.5625372   0.32833802  3.45894209 -6.42793939]', '[ 1.17173089 -0.90146277  2.44167017 -5.46268963]', '[ 1.50629498 -1.81541935  0.89173535 -3.72861395]', '[ 1.53074035 -2.4112497  -0.62928002 -2.24039833]', '[ 1.26032451 -2.68790409 -2.03452905 -0.51838221]', '[ 0.73803547 -2.6192127  -3.10826083  1.19065836]', '[ 0.06496644 -2.22359794 -3.47735889  2.71654573]', '[-0.60304683 -1.54129798 -3.10746239  4.01037434]', '[-1.1576297  -0.66671993 -2.40505407  4.59807879]', '[-1.53171342  0.19760886 -1.27317218  3.89498411]', '[-1.64610974  0.85585636  0.16677345  2.63804772]', '[-1.45300147  1.22949337  1.78095107  1.00880651]', '[-0.92964641  1.18781181  3.39495467 -1.52616484]', '[-0.134735    0.60139854  4.414561   -4.21772503]', '[ 0.75460177 -0.34378006  4.24572391 -4.69444278]', '[ 1.49336249 -1.11559181  3.0790644  -2.94645499]', '[ 1.98722874 -1.56074951  1.88478106 -1.63875332]', '[ 2.25937116 -1.81722113  0.8634832  -1.00864546]', '[ 2.33150035 -1.96014526 -0.13613652 -0.43593431]', '[ 2.2018257  -1.9842338  -1.17983477  0.24599317]', '[ 1.84874187 -1.82842312 -2.37884676  1.43037609]', '[ 1.24264327 -1.35272049 -3.68606602  3.49173455]', '[ 0.38301923 -0.38631887 -4.81229778  6.0208793 ]', '[-0.58151251  0.80398371 -4.55904687  5.20308023]', '[-1.37951337  1.57189049 -3.36573839  2.52021203]', '[-1.91934271  1.87196189 -2.03468262  0.63752368]', '[-2.20113508  1.88063767 -0.80979795 -0.44740933]', '[-2.24399096  1.69709309  0.37046035 -1.35912738]', '[-2.05165607  1.33149418  1.57109181 -2.35730058]', '[-1.60241354  0.71206486  2.96004875 -3.96073747]', '[-0.86534031 -0.26307132  4.31683035 -5.5220172 ]', '[ 0.05149804 -1.28499711  4.67241182 -4.24594906]', '[ 0.94017466 -1.87028407  4.04900175 -1.55541802]', '[ 1.61252904 -1.92903664  2.58348426  0.85373807]', '[ 1.94981868 -1.55996937  0.78901782  2.71482652]', '[ 1.93909305 -0.87764998 -0.85951417  4.07050475]', '[ 1.62166138  0.0624168  -2.26011332  5.26295229]', '[ 1.06609053  1.15658725 -3.23283595  5.46353308]', '[ 0.33821527  2.18111698 -4.01275652  4.67848009]', '[-0.50006013  3.03223394 -4.17554079  3.8497766 ]', '[-1.25116764 -2.54825191 -3.20827451  3.1854462 ]', '[-1.76612252 -1.99122996 -1.94990897  2.32970093]']</t>
+  </si>
+  <si>
+    <t>[0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50, 51, 52, 53, 54, 55, 56, 57, 58, 59, 60, 61, 62, 63, 64, 65, 66, 67, 68, 69, 70, 71, 72, 73, 74, 75, 76, 77, 78, 79, 80, 81, 82, 83, 84, 85, 86, 87, 88, 89, 90, 91, 92, 93, 94, 95, 96, 97, 98, 99, 100, 101, 102, 103, 104, 105, 106]</t>
+  </si>
+  <si>
+    <t>[array([-0.03763371, -0.01533471,  0.06554052, -0.01816017], dtype=float32), array([-0.00754409, -0.05458322,  0.2277812 , -0.36241836]), array([ 0.04879627, -0.15231473,  0.32089719, -0.5887683 ]), array([ 0.11397169, -0.27767857,  0.31375488, -0.63332862]), array([ 0.16759438, -0.39312519,  0.2086893 , -0.49480525]), array([ 0.1930193 , -0.46685036,  0.03906408, -0.22816919]), array([ 0.16956871, -0.44830261, -0.26820417,  0.40739083]), array([ 0.09055011, -0.31127879, -0.50323119,  0.93116007]), array([-0.02165415, -0.09380121, -0.58952709,  1.1892161 ]), array([-0.13228272,  0.13968862, -0.48657385,  1.08703787]), array([-0.21842905,  0.35335821, -0.35084306,  1.00036988]), array([-0.25195003,  0.48960053,  0.02384951,  0.33984609]), array([-0.19642111,  0.45311714,  0.51937854, -0.69256597]), array([-0.05307561,  0.22491996,  0.88091359, -1.53539268]), array([ 0.13802188, -0.12918667,  0.97826521, -1.90895317]), array([ 0.31605351, -0.49658808,  0.75465775, -1.67554103]), array([ 0.42468334, -0.77124123,  0.30822734, -1.02677713]), array([ 0.43446136, -0.89671866, -0.21095426, -0.21717049]), array([ 0.33260677, -0.82796451, -0.7878784 ,  0.89095935]), array([ 0.11895536, -0.52014693, -1.30899108,  2.13554748]), array([-0.15506189, -0.04523277, -1.35957979,  2.48102867]), array([-0.40691623,  0.44686407, -1.08935977,  2.30736054]), array([-0.5564256 ,  0.80512411, -0.37787988,  1.22668507]), array([-0.5537129 ,  0.92864525,  0.40116417,  0.00228018]), array([-0.39080819,  0.77698019,  1.20046194, -1.50281488]), array([-0.08999453,  0.34390987,  1.74701155, -2.7385827 ]), array([ 0.27317466, -0.25633786,  1.78355809, -3.07071984]), array([ 0.58381965, -0.80979964,  1.25275733, -2.34462057]), array([ 0.75625447, -1.16954501,  0.44849885, -1.22960907]), array([ 0.75951625, -1.29827451, -0.41255534, -0.05405852]), array([ 0.58721868, -1.16293685, -1.28442211,  1.40677667]), array([ 0.26062646, -0.74059903, -1.93007964,  2.76947897]), array([-0.15455451, -0.09997029, -2.1187961 ,  3.44680983]), array([-0.53832222,  0.54281118, -1.61923427,  2.79320592]), array([-0.77515416,  0.97344559, -0.7144475 ,  1.47289343]), array([-0.81781851,  1.12775092,  0.2893512 ,  0.06754646]), array([-0.65265505,  0.97025693,  1.34137983, -1.64601959]), array([-0.29504341,  0.47397839,  2.17667958, -3.2498051 ]), array([ 0.17851251, -0.26140617,  2.42570577, -3.84182313]), array([ 0.62007723, -0.95414925,  1.8948333 , -2.92440573]), array([ 0.91323312, -1.40615516,  1.00424535, -1.58868856]), array([ 1.0140886 , -1.59337681, -0.00368105, -0.29095715]), array([ 0.90377872, -1.49733625, -1.08699828,  1.26266421]), array([ 0.58806273, -1.08075213, -2.03765882,  2.91285899]), array([ 0.09740728, -0.31435836, -2.7787139 ,  4.60552365]), array([-0.44641784,  0.59653397, -2.49509314,  4.16201215]), array([-0.8555011 ,  1.26875197, -1.54432101,  2.51233737]), array([-1.05422086,  1.60746709, -0.43068434,  0.89779489]), array([-1.02624063,  1.63274173,  0.70515713, -0.64786431]), array([-0.76897872,  1.31596704,  1.8464915 , -2.55194347]), array([-0.29973655,  0.60200961,  2.78982478, -4.53839163]), array([ 0.2961404 , -0.40320984,  2.97780305, -5.10401646]), array([ 0.82020823, -1.29165304,  2.17295204, -3.6414326 ]), array([ 1.14971312, -1.86035241,  1.10163347, -2.08347611]), array([ 1.2558649 , -2.13780578, -0.04434794, -0.70625533]), array([ 1.12695891, -2.12113439, -1.22819019,  0.88665259]), array([ 0.7687793 , -1.7498437 , -2.31568493,  2.8699482 ]), array([ 0.21716124, -0.95313572, -3.15786491,  5.10909962]), array([-0.45473437,  0.22469162, -3.3503157 ,  6.19775683]), array([-1.02812904,  1.318461  , -2.27070847,  4.54510444]), array([-1.34409922,  2.03119242, -0.89208004,  2.66036124]), array([-1.39396312,  2.42178651,  0.38673363,  1.25594608]), array([-1.18284725,  2.49060831,  1.6961625 , -0.58052741]), array([-0.73350468,  2.18138333,  2.73020548, -2.53925451]), array([-0.12381008,  1.46260449,  3.29739573, -4.67114052]), array([ 0.5625372 ,  0.32833802,  3.45894209, -6.42793939]), array([ 1.17173089, -0.90146277,  2.44167017, -5.46268963]), array([ 1.50629498, -1.81541935,  0.89173535, -3.72861395]), array([ 1.53074035, -2.4112497 , -0.62928002, -2.24039833]), array([ 1.26032451, -2.68790409, -2.03452905, -0.51838221]), array([ 0.73803547, -2.6192127 , -3.10826083,  1.19065836]), array([ 0.06496644, -2.22359794, -3.47735889,  2.71654573]), array([-0.60304683, -1.54129798, -3.10746239,  4.01037434]), array([-1.1576297 , -0.66671993, -2.40505407,  4.59807879]), array([-1.53171342,  0.19760886, -1.27317218,  3.89498411]), array([-1.64610974,  0.85585636,  0.16677345,  2.63804772]), array([-1.45300147,  1.22949337,  1.78095107,  1.00880651]), array([-0.92964641,  1.18781181,  3.39495467, -1.52616484]), array([-0.134735  ,  0.60139854,  4.414561  , -4.21772503]), array([ 0.75460177, -0.34378006,  4.24572391, -4.69444278]), array([ 1.49336249, -1.11559181,  3.0790644 , -2.94645499]), array([ 1.98722874, -1.56074951,  1.88478106, -1.63875332]), array([ 2.25937116, -1.81722113,  0.8634832 , -1.00864546]), array([ 2.33150035, -1.96014526, -0.13613652, -0.43593431]), array([ 2.2018257 , -1.9842338 , -1.17983477,  0.24599317]), array([ 1.84874187, -1.82842312, -2.37884676,  1.43037609]), array([ 1.24264327, -1.35272049, -3.68606602,  3.49173455]), array([ 0.38301923, -0.38631887, -4.81229778,  6.0208793 ]), array([-0.58151251,  0.80398371, -4.55904687,  5.20308023]), array([-1.37951337,  1.57189049, -3.36573839,  2.52021203]), array([-1.91934271,  1.87196189, -2.03468262,  0.63752368]), array([-2.20113508,  1.88063767, -0.80979795, -0.44740933]), array([-2.24399096,  1.69709309,  0.37046035, -1.35912738]), array([-2.05165607,  1.33149418,  1.57109181, -2.35730058]), array([-1.60241354,  0.71206486,  2.96004875, -3.96073747]), array([-0.86534031, -0.26307132,  4.31683035, -5.5220172 ]), array([ 0.05149804, -1.28499711,  4.67241182, -4.24594906]), array([ 0.94017466, -1.87028407,  4.04900175, -1.55541802]), array([ 1.61252904, -1.92903664,  2.58348426,  0.85373807]), array([ 1.94981868, -1.55996937,  0.78901782,  2.71482652]), array([ 1.93909305, -0.87764998, -0.85951417,  4.07050475]), array([ 1.62166138,  0.0624168 , -2.26011332,  5.26295229]), array([ 1.06609053,  1.15658725, -3.23283595,  5.46353308]), array([ 0.33821527,  2.18111698, -4.01275652,  4.67848009]), array([-0.50006013,  3.03223394, -4.17554079,  3.8497766 ]), array([-1.25116764, -2.54825191, -3.20827451,  3.1854462 ]), array([-1.76612252, -1.99122996, -1.94990897,  2.32970093])]</t>
+  </si>
+  <si>
+    <t>['[1,0,2]', '[1,2,0]', '[0,2,1]', '[0,1,1]', '[2,0,1]', '[0,0,0]', '[2,2,2]', '[1,1,1]', '[2,1,0]', '[1,1,2]']</t>
+  </si>
+  <si>
+    <t>[6, 7, 8, 9, 10, 11, 19, 20, 21, 22, 29, 32, 33, 34, 41, 42, 43, 44, 45, 47, 55, 56, 57, 58, 59, 60, 68, 69, 70, 71, 72, 74, 83, 85, 86, 87, 88, 89, 97, 98, 99, 100, 101, 102, 103, 104, 111, 112, 113, 114, 115, 116, 117, 127, 128, 129, 130, 131]</t>
+  </si>
+  <si>
+    <t>[0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 1, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 1, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2]</t>
+  </si>
+  <si>
+    <t>['[-0.03763371 -0.01533471  0.06554052 -0.01816017]', '[-0.00754409 -0.05458322  0.2277812  -0.36241836]', '[ 0.04879627 -0.15231473  0.32089719 -0.5887683 ]', '[ 0.11397169 -0.27767857  0.31375488 -0.63332862]', '[ 0.16759438 -0.39312519  0.2086893  -0.49480525]', '[ 0.1930193  -0.46685036  0.03906408 -0.22816919]', '[ 0.16956871 -0.44830261 -0.26820417  0.40739083]', '[ 0.09055011 -0.31127879 -0.50323119  0.93116007]', '[-0.02165415 -0.09380121 -0.58952709  1.1892161 ]', '[-0.13228272  0.13968862 -0.48657385  1.08703787]', '[-0.20542731  0.31962025 -0.22562708  0.67289162]', '[-0.21756752  0.39782756  0.10766541  0.09689063]', '[-0.15109606  0.32490126  0.54216963 -0.80657469]', '[-0.01068619  0.09081112  0.82714324 -1.47439182]', '[ 0.16212513 -0.23279107  0.85391345 -1.67375883]', '[ 0.3120332  -0.54339537  0.60708552 -1.36152952]', '[ 0.39322683 -0.75586146  0.18779451 -0.73014827]', '[ 0.38412465 -0.82793881 -0.27624305  0.01454459]', '[ 0.26384544 -0.69033685 -0.90484238  1.34113963]', '[ 0.04812306 -0.34154272 -1.20443244  2.06892924]', '[-0.19334691  0.0931444  -1.14461952  2.15461365]', '[-0.38415987  0.47206772 -0.71565145  1.54616118]', '[-0.4664302   0.68796397 -0.09144519  0.5827317 ]', '[-0.40763805  0.66863188  0.66756212 -0.76948417]', '[-0.20903609  0.3896402   1.27902287 -1.96704333]', '[ 0.08044428 -0.07977731  1.54000573 -2.58987186]', '[ 0.37233894 -0.58152686  1.30355715 -2.29099442]', '[ 0.57811065 -0.95699839  0.71677374 -1.41124549]', '[ 0.65007991 -1.13567333 -0.00570882 -0.36529173]', '[ 0.56626986 -1.07361105 -0.81866928  0.98274739]', '[ 0.32092708 -0.71683294 -1.59981757  2.55638341]', '[-0.05052645 -0.08385897 -2.02340723  3.60592802]', '[-0.42682416  0.5956482  -1.63582065  2.98961684]', '[-0.67640133  1.06440262 -0.82320547  1.65389271]', '[-0.74893843  1.2529176   0.10212691  0.23070725]', '[-0.62782939  1.12879971  1.09333305 -1.47498797]', '[-0.32171617  0.66365598  1.92614149 -3.14041463]', '[ 0.11256128 -0.07988052  2.29777145 -4.06372421]', '[ 0.5395609  -0.84478217  1.86106345 -3.37564886]', '[ 0.82955928 -1.39024061  1.0046487  -2.05636433]', '[ 0.93426067 -1.66895919  0.03651735 -0.7374327 ]', '[ 0.83776612 -1.66167204 -0.98439247  0.81521505]', '[ 0.55134775 -1.33831067 -1.84427115  2.42714019]', '[ 0.11812534 -0.69508014 -2.42490915  3.93346013]', '[-0.37618732  0.15759761 -2.37316387  4.29389395]', '[-0.77323758  0.90481255 -1.51137151  3.02755628]', '[-0.97485837  1.37979655 -0.48521681  1.71428401]', '[-0.95660528  1.56580608  0.65630773  0.1457577 ]', '[-0.71280365  1.40854323  1.74731302 -1.73665551]', '[-0.27500041  0.86506489  2.5772111  -3.67722815]', '[ 0.28363686 -0.01243029  2.86616205 -4.80755194]', '[ 0.79962399 -0.90518938  2.16561088 -3.87279608]', '[ 1.12398252 -1.52966558  1.0524708  -2.38107374]', '[ 1.21628266 -1.86724018 -0.13093504 -1.00609137]', '[ 1.06013894 -1.88475755 -1.40611274  0.84931811]', '[ 0.67617726 -1.53802401 -2.38677159  2.64893273]', '[ 0.12784629 -0.82001984 -3.0277071   4.47575338]', '[-0.48761749  0.16500981 -2.95110855  4.99084177]', '[-0.98232098  1.02617649 -1.90366385  3.46241202]', '[-1.23603381  1.54741209 -0.62469004  1.7833769 ]', '[-1.23207636  1.74837726  0.65722677  0.22512287]', '[-0.97173961  1.60459746  1.91753729 -1.70287067]', '[-0.48057557  1.04771559  2.9473733  -3.89365544]', '[ 0.17704574  0.07650042  3.47803596 -5.51124508]', '[ 0.822024   -0.95755385  2.80686819 -4.48618262]', '[ 1.27024136 -1.68126237  1.65105781 -2.79107679]', '[ 1.47795174 -2.09714899  0.42039879 -1.4050344 ]', '[ 1.43136411 -2.22673243 -0.87932026  0.1181179 ]', '[ 1.13201031 -2.03844343 -2.08757262  1.80949651]', '[ 0.61306273 -1.48030352 -3.05179182  3.82724055]', '[-0.06548584 -0.50331058 -3.63576642  5.78414069]', '[-0.76000902  0.64869084 -3.09139957  5.24003617]', '[-1.25158697  1.49632185 -1.79399991  3.24849096]', '[-1.48397975  2.00002894 -0.52533619  1.83200365]', '[-1.45480344  2.21407614  0.80909464  0.30201025]', '[-1.15977455  2.08834142  2.11243749 -1.60516892]', '[-0.62750365  1.54743968  3.15896053 -3.87272979]', '[ 0.08292501  0.52356052  3.85943699 -6.2361673 ]', '[ 0.83037017 -0.74624255  3.36871673 -5.88822175]', '[ 1.37534679 -1.72513599  2.05722925 -3.94009343]', '[ 1.65383509 -2.36050248  0.73257133 -2.47724247]', '[ 1.67166416 -2.72604081 -0.54454248 -1.17682867]', '[ 1.42778267 -2.78604161 -1.88169624  0.59591535]', '[ 0.93529547 -2.49782835 -2.98739781  2.31782843]', '[ 0.26322532 -1.82262258 -3.63421356  4.47764906]', '[-0.4790098  -0.72841465 -3.71827925  6.33664727]', '[-1.15879183  0.54457408 -2.86909087  5.89075546]', '[-1.57376898  1.52632974 -1.25754193  3.950029  ]', '[-1.66406552  2.1516764   0.3431489   2.32903484]', '[-1.44374937  2.45210244  1.83292156  0.64060217]', '[-0.94146731  2.37215166  3.11950538 -1.47607447]', '[-0.23888273  1.85060374  3.78133758 -3.75135973]', '[ 0.52750147  0.88216931  3.80967332 -5.8234095 ]', '[ 1.23948623 -0.35167445  3.1333994  -6.05163443]', '[ 1.72174251 -1.40854976  1.64426924 -4.48379364]', '[ 1.89523975 -2.17120458  0.09400876 -3.18009586]', '[ 1.76453176 -2.67801419 -1.37749794 -1.85778078]', '[ 1.34906393 -2.88220174 -2.74693777 -0.16777064]', '[ 0.68445832 -2.74613126 -3.81000227  1.50901687]', '[-0.1163657  -2.29305009 -4.02014898  2.96175394]', '[-0.85715988 -1.60223021 -3.28340169  3.80569618]', '[-1.40958499 -0.83517402 -2.2174589   3.71430039]', '[-1.73744253 -0.16339262 -1.04875239  2.93774604]', '[-1.82555504  0.33115611  0.17911129  1.99934242]', '[-1.65767664  0.62572949  1.52739457  0.88484031]', '[-1.19367376  0.61617552  3.10753232 -1.06953176]', '[-0.43544667  0.18717164  4.34754777 -3.06717715]', '[ 0.460757   -0.45886001  4.37790116 -2.95321885]', '[ 1.2358795  -0.86562624  3.25793861 -1.03661624]', '[ 1.74493266 -0.90142581  1.83674604  0.5490425 ]', '[ 1.97105639 -0.66657306  0.45993073  1.70695602]', '[ 1.94025109 -0.23741307 -0.75371639  2.57712508]', '[ 1.67032699  0.36859978 -1.9452526   3.47233462]', '[ 1.16565756  1.12336519 -3.08110634  3.93433824]', '[ 0.45097764  1.86783419 -3.99881708  3.31043622]', '[-0.38310354  2.37839528 -4.15958156  1.66607647]', '[-1.13471031  2.50281101 -3.19721406 -0.45843449]', '[-1.61536827  2.19397602 -1.52411134 -2.60354667]', '[-1.71289225  1.45352213  0.58163629 -4.80259355]', '[-1.38434425  0.25473148  2.6180504  -7.12381035]', '[-0.76017032 -1.22631167  3.40394241 -7.21025513]', '[-0.04915927 -2.55876868  3.68949829 -6.18069257]', '[ 0.67154126  2.5299894   3.37310938 -5.91751427]', '[ 1.27502603  1.31484939  2.69420515 -6.30159598]', '[ 1.75613515  0.01659369  2.0300983  -6.49959535]', '[ 2.01715426 -1.17505914  0.42634668 -5.24697175]', '[ 1.88663807 -2.05448865 -1.77359928 -3.46916335]', '[ 1.31500494 -2.50809421 -3.84106014 -1.00769253]', '[ 0.40682314 -2.45309289 -5.0460466   1.52111389]', '[-0.60489319 -1.93540165 -4.84005162  3.50407418]', '[-1.46905701 -1.13546972 -3.74736863  4.26007396]', '[-2.10387826 -0.31505731 -2.62281375  3.81054959]']</t>
+  </si>
+  <si>
+    <t>[0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50, 51, 52, 53, 54, 55, 56, 57, 58, 59, 60, 61, 62, 63, 64, 65, 66, 67, 68, 69, 70, 71, 72, 73, 74, 75, 76, 77, 78, 79, 80, 81, 82, 83, 84, 85, 86, 87, 88, 89, 90, 91, 92, 93, 94, 95, 96, 97, 98, 99, 100, 101, 102, 103, 104, 105, 106, 107, 108, 109, 110, 111, 112, 113, 114, 115, 116, 117, 118, 119, 120, 121, 122, 123, 124, 125, 126, 127, 128, 129, 130, 131]</t>
+  </si>
+  <si>
+    <t>[array([-0.03763371, -0.01533471,  0.06554052, -0.01816017], dtype=float32), array([-0.00754409, -0.05458322,  0.2277812 , -0.36241836]), array([ 0.04879627, -0.15231473,  0.32089719, -0.5887683 ]), array([ 0.11397169, -0.27767857,  0.31375488, -0.63332862]), array([ 0.16759438, -0.39312519,  0.2086893 , -0.49480525]), array([ 0.1930193 , -0.46685036,  0.03906408, -0.22816919]), array([ 0.16956871, -0.44830261, -0.26820417,  0.40739083]), array([ 0.09055011, -0.31127879, -0.50323119,  0.93116007]), array([-0.02165415, -0.09380121, -0.58952709,  1.1892161 ]), array([-0.13228272,  0.13968862, -0.48657385,  1.08703787]), array([-0.20542731,  0.31962025, -0.22562708,  0.67289162]), array([-0.21756752,  0.39782756,  0.10766541,  0.09689063]), array([-0.15109606,  0.32490126,  0.54216963, -0.80657469]), array([-0.01068619,  0.09081112,  0.82714324, -1.47439182]), array([ 0.16212513, -0.23279107,  0.85391345, -1.67375883]), array([ 0.3120332 , -0.54339537,  0.60708552, -1.36152952]), array([ 0.39322683, -0.75586146,  0.18779451, -0.73014827]), array([ 0.38412465, -0.82793881, -0.27624305,  0.01454459]), array([ 0.26384544, -0.69033685, -0.90484238,  1.34113963]), array([ 0.04812306, -0.34154272, -1.20443244,  2.06892924]), array([-0.19334691,  0.0931444 , -1.14461952,  2.15461365]), array([-0.38415987,  0.47206772, -0.71565145,  1.54616118]), array([-0.4664302 ,  0.68796397, -0.09144519,  0.5827317 ]), array([-0.40763805,  0.66863188,  0.66756212, -0.76948417]), array([-0.20903609,  0.3896402 ,  1.27902287, -1.96704333]), array([ 0.08044428, -0.07977731,  1.54000573, -2.58987186]), array([ 0.37233894, -0.58152686,  1.30355715, -2.29099442]), array([ 0.57811065, -0.95699839,  0.71677374, -1.41124549]), array([ 0.65007991, -1.13567333, -0.00570882, -0.36529173]), array([ 0.56626986, -1.07361105, -0.81866928,  0.98274739]), array([ 0.32092708, -0.71683294, -1.59981757,  2.55638341]), array([-0.05052645, -0.08385897, -2.02340723,  3.60592802]), array([-0.42682416,  0.5956482 , -1.63582065,  2.98961684]), array([-0.67640133,  1.06440262, -0.82320547,  1.65389271]), array([-0.74893843,  1.2529176 ,  0.10212691,  0.23070725]), array([-0.62782939,  1.12879971,  1.09333305, -1.47498797]), array([-0.32171617,  0.66365598,  1.92614149, -3.14041463]), array([ 0.11256128, -0.07988052,  2.29777145, -4.06372421]), array([ 0.5395609 , -0.84478217,  1.86106345, -3.37564886]), array([ 0.82955928, -1.39024061,  1.0046487 , -2.05636433]), array([ 0.93426067, -1.66895919,  0.03651735, -0.7374327 ]), array([ 0.83776612, -1.66167204, -0.98439247,  0.81521505]), array([ 0.55134775, -1.33831067, -1.84427115,  2.42714019]), array([ 0.11812534, -0.69508014, -2.42490915,  3.93346013]), array([-0.37618732,  0.15759761, -2.37316387,  4.29389395]), array([-0.77323758,  0.90481255, -1.51137151,  3.02755628]), array([-0.97485837,  1.37979655, -0.48521681,  1.71428401]), array([-0.95660528,  1.56580608,  0.65630773,  0.1457577 ]), array([-0.71280365,  1.40854323,  1.74731302, -1.73665551]), array([-0.27500041,  0.86506489,  2.5772111 , -3.67722815]), array([ 0.28363686, -0.01243029,  2.86616205, -4.80755194]), array([ 0.79962399, -0.90518938,  2.16561088, -3.87279608]), array([ 1.12398252, -1.52966558,  1.0524708 , -2.38107374]), array([ 1.21628266, -1.86724018, -0.13093504, -1.00609137]), array([ 1.06013894, -1.88475755, -1.40611274,  0.84931811]), array([ 0.67617726, -1.53802401, -2.38677159,  2.64893273]), array([ 0.12784629, -0.82001984, -3.0277071 ,  4.47575338]), array([-0.48761749,  0.16500981, -2.95110855,  4.99084177]), array([-0.98232098,  1.02617649, -1.90366385,  3.46241202]), array([-1.23603381,  1.54741209, -0.62469004,  1.7833769 ]), array([-1.23207636,  1.74837726,  0.65722677,  0.22512287]), array([-0.97173961,  1.60459746,  1.91753729, -1.70287067]), array([-0.48057557,  1.04771559,  2.9473733 , -3.89365544]), array([ 0.17704574,  0.07650042,  3.47803596, -5.51124508]), array([ 0.822024  , -0.95755385,  2.80686819, -4.48618262]), array([ 1.27024136, -1.68126237,  1.65105781, -2.79107679]), array([ 1.47795174, -2.09714899,  0.42039879, -1.4050344 ]), array([ 1.43136411, -2.22673243, -0.87932026,  0.1181179 ]), array([ 1.13201031, -2.03844343, -2.08757262,  1.80949651]), array([ 0.61306273, -1.48030352, -3.05179182,  3.82724055]), array([-0.06548584, -0.50331058, -3.63576642,  5.78414069]), array([-0.76000902,  0.64869084, -3.09139957,  5.24003617]), array([-1.25158697,  1.49632185, -1.79399991,  3.24849096]), array([-1.48397975,  2.00002894, -0.52533619,  1.83200365]), array([-1.45480344,  2.21407614,  0.80909464,  0.30201025]), array([-1.15977455,  2.08834142,  2.11243749, -1.60516892]), array([-0.62750365,  1.54743968,  3.15896053, -3.87272979]), array([ 0.08292501,  0.52356052,  3.85943699, -6.2361673 ]), array([ 0.83037017, -0.74624255,  3.36871673, -5.88822175]), array([ 1.37534679, -1.72513599,  2.05722925, -3.94009343]), array([ 1.65383509, -2.36050248,  0.73257133, -2.47724247]), array([ 1.67166416, -2.72604081, -0.54454248, -1.17682867]), array([ 1.42778267, -2.78604161, -1.88169624,  0.59591535]), array([ 0.93529547, -2.49782835, -2.98739781,  2.31782843]), array([ 0.26322532, -1.82262258, -3.63421356,  4.47764906]), array([-0.4790098 , -0.72841465, -3.71827925,  6.33664727]), array([-1.15879183,  0.54457408, -2.86909087,  5.89075546]), array([-1.57376898,  1.52632974, -1.25754193,  3.950029  ]), array([-1.66406552,  2.1516764 ,  0.3431489 ,  2.32903484]), array([-1.44374937,  2.45210244,  1.83292156,  0.64060217]), array([-0.94146731,  2.37215166,  3.11950538, -1.47607447]), array([-0.23888273,  1.85060374,  3.78133758, -3.75135973]), array([ 0.52750147,  0.88216931,  3.80967332, -5.8234095 ]), array([ 1.23948623, -0.35167445,  3.1333994 , -6.05163443]), array([ 1.72174251, -1.40854976,  1.64426924, -4.48379364]), array([ 1.89523975, -2.17120458,  0.09400876, -3.18009586]), array([ 1.76453176, -2.67801419, -1.37749794, -1.85778078]), array([ 1.34906393, -2.88220174, -2.74693777, -0.16777064]), array([ 0.68445832, -2.74613126, -3.81000227,  1.50901687]), array([-0.1163657 , -2.29305009, -4.02014898,  2.96175394]), array([-0.85715988, -1.60223021, -3.28340169,  3.80569618]), array([-1.40958499, -0.83517402, -2.2174589 ,  3.71430039]), array([-1.73744253, -0.16339262, -1.04875239,  2.93774604]), array([-1.82555504,  0.33115611,  0.17911129,  1.99934242]), array([-1.65767664,  0.62572949,  1.52739457,  0.88484031]), array([-1.19367376,  0.61617552,  3.10753232, -1.06953176]), array([-0.43544667,  0.18717164,  4.34754777, -3.06717715]), array([ 0.460757  , -0.45886001,  4.37790116, -2.95321885]), array([ 1.2358795 , -0.86562624,  3.25793861, -1.03661624]), array([ 1.74493266, -0.90142581,  1.83674604,  0.5490425 ]), array([ 1.97105639, -0.66657306,  0.45993073,  1.70695602]), array([ 1.94025109, -0.23741307, -0.75371639,  2.57712508]), array([ 1.67032699,  0.36859978, -1.9452526 ,  3.47233462]), array([ 1.16565756,  1.12336519, -3.08110634,  3.93433824]), array([ 0.45097764,  1.86783419, -3.99881708,  3.31043622]), array([-0.38310354,  2.37839528, -4.15958156,  1.66607647]), array([-1.13471031,  2.50281101, -3.19721406, -0.45843449]), array([-1.61536827,  2.19397602, -1.52411134, -2.60354667]), array([-1.71289225,  1.45352213,  0.58163629, -4.80259355]), array([-1.38434425,  0.25473148,  2.6180504 , -7.12381035]), array([-0.76017032, -1.22631167,  3.40394241, -7.21025513]), array([-0.04915927, -2.55876868,  3.68949829, -6.18069257]), array([ 0.67154126,  2.5299894 ,  3.37310938, -5.91751427]), array([ 1.27502603,  1.31484939,  2.69420515, -6.30159598]), array([ 1.75613515,  0.01659369,  2.0300983 , -6.49959535]), array([ 2.01715426, -1.17505914,  0.42634668, -5.24697175]), array([ 1.88663807, -2.05448865, -1.77359928, -3.46916335]), array([ 1.31500494, -2.50809421, -3.84106014, -1.00769253]), array([ 0.40682314, -2.45309289, -5.0460466 ,  1.52111389]), array([-0.60489319, -1.93540165, -4.84005162,  3.50407418]), array([-1.46905701, -1.13546972, -3.74736863,  4.26007396]), array([-2.10387826, -0.31505731, -2.62281375,  3.81054959])]</t>
+  </si>
+  <si>
+    <t>['[0,2,1]', '[1,2,0]', '[2,2,2]', '[0,1,1]', '[1,0,2]', '[0,0,0]', '[2,0,1]', '[1,1,2]', '[1,1,1]', '[2,1,0]']</t>
+  </si>
+  <si>
+    <t>[6, 7, 8, 9, 10, 11, 18, 19, 20, 21, 22, 23, 29, 30, 31, 32, 33, 34, 41, 42, 43, 44, 45, 46, 47, 54, 55, 56, 57, 58, 59, 60, 67, 68, 69, 70, 71, 72, 73, 81, 82, 83, 84, 85, 86, 87, 96, 97, 98, 99, 100, 101, 102, 111, 112, 113, 114, 115, 116, 117, 118, 137, 138]</t>
+  </si>
+  <si>
+    <t>[0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 1, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 1, 2, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 1, 2, 2]</t>
+  </si>
+  <si>
+    <t>['[-0.03763371 -0.01533471  0.06554052 -0.01816017]', '[-0.00754409 -0.05458322  0.2277812  -0.36241836]', '[ 0.04879627 -0.15231473  0.32089719 -0.5887683 ]', '[ 0.11397169 -0.27767857  0.31375488 -0.63332862]', '[ 0.16759438 -0.39312519  0.2086893  -0.49480525]', '[ 0.1930193  -0.46685036  0.03906408 -0.22816919]', '[ 0.16956871 -0.44830261 -0.26820417  0.40739083]', '[ 0.09055011 -0.31127879 -0.50323119  0.93116007]', '[-0.02165415 -0.09380121 -0.58952709  1.1892161 ]', '[-0.13228272  0.13968862 -0.48657385  1.08703787]', '[-0.20542731  0.31962025 -0.22562708  0.67289162]', '[-0.21756752  0.39782756  0.10766541  0.09689063]', '[-0.15109606  0.32490126  0.54216963 -0.80657469]', '[-0.01068619  0.09081112  0.82714324 -1.47439182]', '[ 0.16212513 -0.23279107  0.85391345 -1.67375883]', '[ 0.3120332  -0.54339537  0.60708552 -1.36152952]', '[ 0.39322683 -0.75586146  0.18779451 -0.73014827]', '[ 0.38412465 -0.82793881 -0.27624305  0.01454459]', '[ 0.27552572 -0.72135137 -0.78884754  1.03160865]', '[ 0.08086773 -0.43032213 -1.11647003  1.81675029]', '[-0.14966877 -0.03109877 -1.12879696  2.06540623]', '[-0.3455444   0.34863759 -0.7784691   1.63534647]', '[-0.44544803  0.59424237 -0.19906427  0.77949316]', '[-0.4218337   0.6519398   0.43007126 -0.20572333]', '[-0.26769146  0.484052    1.08142007 -1.44055859]', '[-0.00742761  0.10113176  1.45927884 -2.28595201]', '[ 0.28490347 -0.37428385  1.38589424 -2.32532176]', '[ 0.5187101  -0.77937684  0.90230152 -1.64619583]', '[ 0.63240836 -1.01433747  0.21740989 -0.68198512]', '[ 0.59278756 -1.01958166 -0.60566507  0.62852481]', '[ 0.39752784 -0.7660208  -1.31595743  1.88179849]', '[ 0.08542661 -0.29020757 -1.73661998  2.76615566]', '[-0.26054486  0.27360101 -1.62803895  2.69265107]', '[-0.53183224  0.72525907 -1.02799868  1.73308445]', '[-0.65747495  0.94866122 -0.21116234  0.48419472]', '[-0.60316944  0.88713812  0.74646124 -1.09703619]', '[-0.3667148   0.51448679  1.5802398  -2.58584684]', '[ 2.25515542e-03 -1.04226788e-01  2.01052042e+00 -3.41515113e+00]', '[ 0.38981745 -0.75816996  1.76540261 -2.93947302]', '[ 0.67971886 -1.23563438  1.09061136 -1.79181237]', '[ 0.81522073 -1.47040276  0.25012952 -0.55613563]', '[ 0.76893557 -1.43299403 -0.70634091  0.93217091]', '[ 0.53890731 -1.09497955 -1.5685075   2.44803386]', '[ 0.15769536 -0.46498696 -2.17507038  3.75054866]', '[-0.28566374  0.31885175 -2.12308403  3.81427092]', '[-0.64333931  0.96714913 -1.38377582  2.55626676]', '[-0.82476188  1.32821982 -0.41497441  1.0541805 ]', '[-0.80769438  1.39053182  0.57925977 -0.43113385]', '[-0.58966747  1.12643161  1.57705339 -2.21920745]', '[-0.19115743  0.50615398  2.34648211 -3.90612928]', '[ 0.30339761 -0.35080814  2.44609663 -4.34908803]', '[ 0.72926902 -1.11787821  1.72849028 -3.18529002]', '[ 0.97784646 -1.61271142  0.7372731  -1.77273591]', '[ 1.02063975 -1.83229792 -0.30765192 -0.42827287]', '[ 0.8520877  -1.75909807 -1.35222299  1.17222519]', '[ 0.49438686 -1.35658722 -2.18080855  2.86380021]', '[ 1.00762334e-03 -6.20843848e-01 -2.67811907e+00  4.39175692e+00]', '[-0.52543841  0.29807699 -2.42518508  4.45563686]', '[-0.91358233  1.05045396 -1.38833549  2.96371659]', '[-1.07068508  1.48053778 -0.17760768  1.35120727]', '[-0.98698022  1.59293246  0.99771813 -0.2363293 ]', '[-0.67458429  1.35277557  2.08591422 -2.1902737 ]', '[-0.17257945  0.7121893   2.86826583 -4.16299452]', '[ 0.42654616 -0.22986762  2.95103072 -4.89035041]', '[ 0.93778312 -1.09635369  2.06289939 -3.60682875]', '[ 1.23512506 -1.66554553  0.89403237 -2.11536181]', '[ 1.2925874  -1.95282627 -0.31874559 -0.76398106]', '[ 1.10434513 -1.94410117 -1.53992148  0.87663865]', '[ 0.69181453 -1.5878337  -2.53506175  2.72222862]', '[ 0.1141862  -0.84811196 -3.17077399  4.62247333]', '[-0.52819058  0.17080839 -3.07026003  5.16081708]', '[-1.04130142  1.05893    -1.96969821  3.56491538]', '[-1.30452454  1.59874429 -0.65598023  1.87444291]', '[-1.30385453  1.81885452  0.65610727  0.32547074]', '[-1.0405206   1.6957045   1.9492216  -1.60077881]', '[-0.53981694  1.15624497  3.01179277 -3.83696118]', '[ 0.1372115   0.17699716  3.62003771 -5.68231063]', '[ 0.81714379 -0.90901082  2.9941466  -4.77727736]', '[ 1.30077933 -1.68444311  1.81783839 -3.01937746]', '[ 1.54044333 -2.14395201  0.57410527 -1.62162767]', '[ 1.53015478 -2.34022436 -0.67386049 -0.3349864 ]', '[ 1.26794035 -2.24754766 -1.92783573  1.30056457]', '[ 0.77398019 -1.79920792 -2.95822207  3.24300749]', '[ 0.10912329 -0.93053956 -3.62675865  5.42116516]', '[-0.62545765  0.26611029 -3.49608951  6.01988262]', '[-1.20465197  1.28709304 -2.21592237  4.06698629]', '[-1.50797598  1.91807846 -0.82066615  2.31676317]', '[-1.53477864  2.2293726   0.54577611  0.80013611]', '[-1.2877879   2.20842304  1.90129391 -1.04971139]', '[-0.78963194  1.78691254  3.02687444 -3.23448346]', '[-0.10030915  0.88843882  3.80956796 -5.74461357]', '[ 0.6800303  -0.39674343  3.7435005  -6.50465385]', '[ 1.30715153 -1.50997221  2.45867409 -4.5409428 ]', '[ 1.66295011 -2.25180565  1.10659453 -2.9676307 ]', '[ 1.75378095 -2.71564871 -0.18565107 -1.68161197]', '[ 1.58719261 -2.90109289 -1.4723594  -0.1570594 ]', '[ 1.16856593 -2.77159888 -2.68682871  1.47067408]', '[ 0.53803373 -2.30375458 -3.51328481  3.23512206]', '[-0.18689025 -1.47171807 -3.64264476  5.06600075]', '[-0.89191829 -0.32040404 -3.30370334  6.16212656]', '[-1.43738497  0.81560486 -2.01541372  4.90941679]', '[-1.67729527  1.62358431 -0.37474765  3.2087413 ]', '[-1.58743078  2.10406514  1.26274863  1.56657122]', '[-1.17686802  2.20715638  2.7876195  -0.59672218]', '[-0.50730587  1.84271979  3.79246475 -3.08863666]', '[ 0.29147201  0.97119874  4.10085764 -5.54206842]', '[ 1.08414599 -0.25378944  3.63499511 -6.19286979]', '[ 1.67640522 -1.3365948   2.23652426 -4.56246495]', '[ 1.9814544  -2.11437006  0.82705999 -3.29460719]', '[ 2.01269692 -2.66619774 -0.49620149 -2.21383358]', '[ 1.78409404 -2.96809523 -1.77965027 -0.77249303]', '[ 1.30149129 -2.96441766 -3.03533588  0.82631458]', '[ 0.58890924 -2.63390153 -3.98354262  2.48567983]', '[-0.22631846 -1.97283376 -4.00376081  4.08524298]', '[-0.96558336 -1.03796571 -3.33240076  5.11323848]', '[-1.53922556 -0.01454682 -2.33370838  4.88332683]', '[-1.87187423  0.84815259 -0.95576384  3.69536389]', '[-1.91165507  1.46323511  0.58512333  2.43051425]', '[-1.62770799  1.79176562  2.26273466  0.74152557]', '[-1.00988905  1.68362849  3.84148013 -1.95309403]', '[-0.13585858  0.9738579   4.77819076 -5.12142974]', '[ 0.83565798 -0.2398631   4.68927476 -6.34985101]', '[ 1.65142165 -1.3228547   3.41257782 -4.35839551]', '[ 2.21520709 -2.04128122  2.27602432 -2.99811286]', '[ 2.58160112 -2.57359675  1.43950076 -2.41030312]', '[ 2.81131759 -3.02440586  0.91146434 -2.12231163]', '[ 2.96620913  2.85763281  0.68571764 -1.891342  ]', '[ 3.10182854  2.50290167  0.70700839 -1.65836682]', '[-3.02153244  2.19152507  0.92343942 -1.47303363]', '[-2.79824568  1.90164466  1.35072441 -1.47546205]', '[-2.46165889  1.57209735  2.07478658 -1.92730454]', '[-1.94100647  1.07275137  3.20807492 -3.25194534]', '[-1.15137198  0.20163219  4.68919384 -5.4342263 ]', '[-0.12448895 -0.91571373  5.34175489 -5.06561134]', '[ 0.89800185 -1.62986529  4.68648726 -1.92490485]', '[ 1.68031081 -1.7067368   3.02854483  0.99907813]', '[ 2.08617254 -1.28248348  1.05430359  3.06795616]', '[ 2.1281456  -0.53224006 -0.55713409  4.35210695]', '[ 1.89410325  0.43386325 -1.71041519  5.23147326]']</t>
+  </si>
+  <si>
+    <t>[0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50, 51, 52, 53, 54, 55, 56, 57, 58, 59, 60, 61, 62, 63, 64, 65, 66, 67, 68, 69, 70, 71, 72, 73, 74, 75, 76, 77, 78, 79, 80, 81, 82, 83, 84, 85, 86, 87, 88, 89, 90, 91, 92, 93, 94, 95, 96, 97, 98, 99, 100, 101, 102, 103, 104, 105, 106, 107, 108, 109, 110, 111, 112, 113, 114, 115, 116, 117, 118, 119, 120, 121, 122, 123, 124, 125, 126, 127, 128, 129, 130, 131, 132, 133, 134, 135, 136, 137, 138]</t>
+  </si>
+  <si>
+    <t>[array([-0.03763371, -0.01533471,  0.06554052, -0.01816017], dtype=float32), array([-0.00754409, -0.05458322,  0.2277812 , -0.36241836]), array([ 0.04879627, -0.15231473,  0.32089719, -0.5887683 ]), array([ 0.11397169, -0.27767857,  0.31375488, -0.63332862]), array([ 0.16759438, -0.39312519,  0.2086893 , -0.49480525]), array([ 0.1930193 , -0.46685036,  0.03906408, -0.22816919]), array([ 0.16956871, -0.44830261, -0.26820417,  0.40739083]), array([ 0.09055011, -0.31127879, -0.50323119,  0.93116007]), array([-0.02165415, -0.09380121, -0.58952709,  1.1892161 ]), array([-0.13228272,  0.13968862, -0.48657385,  1.08703787]), array([-0.20542731,  0.31962025, -0.22562708,  0.67289162]), array([-0.21756752,  0.39782756,  0.10766541,  0.09689063]), array([-0.15109606,  0.32490126,  0.54216963, -0.80657469]), array([-0.01068619,  0.09081112,  0.82714324, -1.47439182]), array([ 0.16212513, -0.23279107,  0.85391345, -1.67375883]), array([ 0.3120332 , -0.54339537,  0.60708552, -1.36152952]), array([ 0.39322683, -0.75586146,  0.18779451, -0.73014827]), array([ 0.38412465, -0.82793881, -0.27624305,  0.01454459]), array([ 0.27552572, -0.72135137, -0.78884754,  1.03160865]), array([ 0.08086773, -0.43032213, -1.11647003,  1.81675029]), array([-0.14966877, -0.03109877, -1.12879696,  2.06540623]), array([-0.3455444 ,  0.34863759, -0.7784691 ,  1.63534647]), array([-0.44544803,  0.59424237, -0.19906427,  0.77949316]), array([-0.4218337 ,  0.6519398 ,  0.43007126, -0.20572333]), array([-0.26769146,  0.484052  ,  1.08142007, -1.44055859]), array([-0.00742761,  0.10113176,  1.45927884, -2.28595201]), array([ 0.28490347, -0.37428385,  1.38589424, -2.32532176]), array([ 0.5187101 , -0.77937684,  0.90230152, -1.64619583]), array([ 0.63240836, -1.01433747,  0.21740989, -0.68198512]), array([ 0.59278756, -1.01958166, -0.60566507,  0.62852481]), array([ 0.39752784, -0.7660208 , -1.31595743,  1.88179849]), array([ 0.08542661, -0.29020757, -1.73661998,  2.76615566]), array([-0.26054486,  0.27360101, -1.62803895,  2.69265107]), array([-0.53183224,  0.72525907, -1.02799868,  1.73308445]), array([-0.65747495,  0.94866122, -0.21116234,  0.48419472]), array([-0.60316944,  0.88713812,  0.74646124, -1.09703619]), array([-0.3667148 ,  0.51448679,  1.5802398 , -2.58584684]), array([ 2.25515542e-03, -1.04226788e-01,  2.01052042e+00, -3.41515113e+00]), array([ 0.38981745, -0.75816996,  1.76540261, -2.93947302]), array([ 0.67971886, -1.23563438,  1.09061136, -1.79181237]), array([ 0.81522073, -1.47040276,  0.25012952, -0.55613563]), array([ 0.76893557, -1.43299403, -0.70634091,  0.93217091]), array([ 0.53890731, -1.09497955, -1.5685075 ,  2.44803386]), array([ 0.15769536, -0.46498696, -2.17507038,  3.75054866]), array([-0.28566374,  0.31885175, -2.12308403,  3.81427092]), array([-0.64333931,  0.96714913, -1.38377582,  2.55626676]), array([-0.82476188,  1.32821982, -0.41497441,  1.0541805 ]), array([-0.80769438,  1.39053182,  0.57925977, -0.43113385]), array([-0.58966747,  1.12643161,  1.57705339, -2.21920745]), array([-0.19115743,  0.50615398,  2.34648211, -3.90612928]), array([ 0.30339761, -0.35080814,  2.44609663, -4.34908803]), array([ 0.72926902, -1.11787821,  1.72849028, -3.18529002]), array([ 0.97784646, -1.61271142,  0.7372731 , -1.77273591]), array([ 1.02063975, -1.83229792, -0.30765192, -0.42827287]), array([ 0.8520877 , -1.75909807, -1.35222299,  1.17222519]), array([ 0.49438686, -1.35658722, -2.18080855,  2.86380021]), array([ 1.00762334e-03, -6.20843848e-01, -2.67811907e+00,  4.39175692e+00]), array([-0.52543841,  0.29807699, -2.42518508,  4.45563686]), array([-0.91358233,  1.05045396, -1.38833549,  2.96371659]), array([-1.07068508,  1.48053778, -0.17760768,  1.35120727]), array([-0.98698022,  1.59293246,  0.99771813, -0.2363293 ]), array([-0.67458429,  1.35277557,  2.08591422, -2.1902737 ]), array([-0.17257945,  0.7121893 ,  2.86826583, -4.16299452]), array([ 0.42654616, -0.22986762,  2.95103072, -4.89035041]), array([ 0.93778312, -1.09635369,  2.06289939, -3.60682875]), array([ 1.23512506, -1.66554553,  0.89403237, -2.11536181]), array([ 1.2925874 , -1.95282627, -0.31874559, -0.76398106]), array([ 1.10434513, -1.94410117, -1.53992148,  0.87663865]), array([ 0.69181453, -1.5878337 , -2.53506175,  2.72222862]), array([ 0.1141862 , -0.84811196, -3.17077399,  4.62247333]), array([-0.52819058,  0.17080839, -3.07026003,  5.16081708]), array([-1.04130142,  1.05893   , -1.96969821,  3.56491538]), array([-1.30452454,  1.59874429, -0.65598023,  1.87444291]), array([-1.30385453,  1.81885452,  0.65610727,  0.32547074]), array([-1.0405206 ,  1.6957045 ,  1.9492216 , -1.60077881]), array([-0.53981694,  1.15624497,  3.01179277, -3.83696118]), array([ 0.1372115 ,  0.17699716,  3.62003771, -5.68231063]), array([ 0.81714379, -0.90901082,  2.9941466 , -4.77727736]), array([ 1.30077933, -1.68444311,  1.81783839, -3.01937746]), array([ 1.54044333, -2.14395201,  0.57410527, -1.62162767]), array([ 1.53015478, -2.34022436, -0.67386049, -0.3349864 ]), array([ 1.26794035, -2.24754766, -1.92783573,  1.30056457]), array([ 0.77398019, -1.79920792, -2.95822207,  3.24300749]), array([ 0.10912329, -0.93053956, -3.62675865,  5.42116516]), array([-0.62545765,  0.26611029, -3.49608951,  6.01988262]), array([-1.20465197,  1.28709304, -2.21592237,  4.06698629]), array([-1.50797598,  1.91807846, -0.82066615,  2.31676317]), array([-1.53477864,  2.2293726 ,  0.54577611,  0.80013611]), array([-1.2877879 ,  2.20842304,  1.90129391, -1.04971139]), array([-0.78963194,  1.78691254,  3.02687444, -3.23448346]), array([-0.10030915,  0.88843882,  3.80956796, -5.74461357]), array([ 0.6800303 , -0.39674343,  3.7435005 , -6.50465385]), array([ 1.30715153, -1.50997221,  2.45867409, -4.5409428 ]), array([ 1.66295011, -2.25180565,  1.10659453, -2.9676307 ]), array([ 1.75378095, -2.71564871, -0.18565107, -1.68161197]), array([ 1.58719261, -2.90109289, -1.4723594 , -0.1570594 ]), array([ 1.16856593, -2.77159888, -2.68682871,  1.47067408]), array([ 0.53803373, -2.30375458, -3.51328481,  3.23512206]), array([-0.18689025, -1.47171807, -3.64264476,  5.06600075]), array([-0.89191829, -0.32040404, -3.30370334,  6.16212656]), array([-1.43738497,  0.81560486, -2.01541372,  4.90941679]), array([-1.67729527,  1.62358431, -0.37474765,  3.2087413 ]), array([-1.58743078,  2.10406514,  1.26274863,  1.56657122]), array([-1.17686802,  2.20715638,  2.7876195 , -0.59672218]), array([-0.50730587,  1.84271979,  3.79246475, -3.08863666]), array([ 0.29147201,  0.97119874,  4.10085764, -5.54206842]), array([ 1.08414599, -0.25378944,  3.63499511, -6.19286979]), array([ 1.67640522, -1.3365948 ,  2.23652426, -4.56246495]), array([ 1.9814544 , -2.11437006,  0.82705999, -3.29460719]), array([ 2.01269692, -2.66619774, -0.49620149, -2.21383358]), array([ 1.78409404, -2.96809523, -1.77965027, -0.77249303]), array([ 1.30149129, -2.96441766, -3.03533588,  0.82631458]), array([ 0.58890924, -2.63390153, -3.98354262,  2.48567983]), array([-0.22631846, -1.97283376, -4.00376081,  4.08524298]), array([-0.96558336, -1.03796571, -3.33240076,  5.11323848]), array([-1.53922556, -0.01454682, -2.33370838,  4.88332683]), array([-1.87187423,  0.84815259, -0.95576384,  3.69536389]), array([-1.91165507,  1.46323511,  0.58512333,  2.43051425]), array([-1.62770799,  1.79176562,  2.26273466,  0.74152557]), array([-1.00988905,  1.68362849,  3.84148013, -1.95309403]), array([-0.13585858,  0.9738579 ,  4.77819076, -5.12142974]), array([ 0.83565798, -0.2398631 ,  4.68927476, -6.34985101]), array([ 1.65142165, -1.3228547 ,  3.41257782, -4.35839551]), array([ 2.21520709, -2.04128122,  2.27602432, -2.99811286]), array([ 2.58160112, -2.57359675,  1.43950076, -2.41030312]), array([ 2.81131759, -3.02440586,  0.91146434, -2.12231163]), array([ 2.96620913,  2.85763281,  0.68571764, -1.891342  ]), array([ 3.10182854,  2.50290167,  0.70700839, -1.65836682]), array([-3.02153244,  2.19152507,  0.92343942, -1.47303363]), array([-2.79824568,  1.90164466,  1.35072441, -1.47546205]), array([-2.46165889,  1.57209735,  2.07478658, -1.92730454]), array([-1.94100647,  1.07275137,  3.20807492, -3.25194534]), array([-1.15137198,  0.20163219,  4.68919384, -5.4342263 ]), array([-0.12448895, -0.91571373,  5.34175489, -5.06561134]), array([ 0.89800185, -1.62986529,  4.68648726, -1.92490485]), array([ 1.68031081, -1.7067368 ,  3.02854483,  0.99907813]), array([ 2.08617254, -1.28248348,  1.05430359,  3.06795616]), array([ 2.1281456 , -0.53224006, -0.55713409,  4.35210695]), array([ 1.89410325,  0.43386325, -1.71041519,  5.23147326])]</t>
+  </si>
+  <si>
+    <t>['[2,2,2]', '[1,2,0]', '[1,1,2]', '[0,0,0]', '[2,1,0]', '[0,1,1]', '[2,0,1]', '[1,0,2]', '[0,2,1]', '[1,1,1]']</t>
+  </si>
+  <si>
+    <t>[0,2,1]</t>
+  </si>
+  <si>
+    <t>[8, 11, 19, 49, 81]</t>
+  </si>
+  <si>
+    <t>[0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 1, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 1, 2, 2, 2, 2, 2, 2, 2, 2]</t>
+  </si>
+  <si>
+    <t>['[-0.03763371 -0.01533471  0.06554052 -0.01816017]', '[-0.00754409 -0.05458322  0.2277812  -0.36241836]', '[ 0.04879627 -0.15231473  0.32089719 -0.5887683 ]', '[ 0.11397169 -0.27767857  0.31375488 -0.63332862]', '[ 0.16759438 -0.39312519  0.2086893  -0.49480525]', '[ 0.1930193  -0.46685036  0.03906408 -0.22816919]', '[ 0.15689524 -0.41528579 -0.3922057   0.73207416]', '[ 0.04309269 -0.18588535 -0.71796191  1.51055937]', '[-0.10156356  0.12486504 -0.68790627  1.51697551]', '[-0.22927161  0.42348907 -0.55357165  1.39819937]', '[-0.31090932  0.65984646 -0.24293606  0.92318871]', '[-0.31014687  0.75044756  0.2486755  -0.02372896]', '[-0.20366105  0.62121032  0.79599893 -1.24647654]', '[-0.00411788  0.26942411  1.15489481 -2.19549786]', '[ 0.23392956 -0.21131539  1.15674844 -2.47741296]', '[ 0.43096425 -0.66762183  0.76173917 -1.986265  ]', '[ 0.52458578 -0.9796545   0.15820524 -1.10009687]', '[ 0.4930839  -1.1011094  -0.46380341 -0.11075199]', '[ 0.32589057 -0.96862421 -1.17826925  1.42078016]', '[ 0.04894834 -0.57676061 -1.53869505  2.4260482 ]', '[-0.27489665 -0.01149737 -1.61623004  3.06802964]', '[-0.55945103  0.5756583  -1.15065073  2.65270956]', '[-0.71288953  1.01000952 -0.35583386  1.64294581]', '[-0.69808217  1.22385838  0.49692877  0.48560128]', '[-0.50287533  1.14784598  1.41869689 -1.24158671]', '[-0.14900383  0.73341372  2.06329024 -2.85295241]', '[ 0.29084568  0.05384361  2.22735475 -3.73810785]', '[ 0.69044425 -0.6585127   1.66461254 -3.18721047]', '[ 0.92961455 -1.17809972  0.6945577  -1.97409212]', '[ 0.96296101 -1.44497717 -0.35997969 -0.68946073]', '[ 0.77351961 -1.39864484 -1.50344078  1.16654626]', '[ 0.37811844 -0.97203993 -2.39985579  3.09342205]', '[-0.15765015 -0.1910167  -2.84206179  4.50453462]', '[-0.6921189   0.69002473 -2.35483635  4.00508677]', '[-1.06248704  1.34995229 -1.30862257  2.5701969 ]', '[-1.20839901  1.72552608 -0.14388277  1.2017002 ]', '[-1.12091592  1.83108977  1.00594216 -0.1597045 ]', '[-0.80072729  1.60454421  2.15604673 -2.14203903]', '[-0.27785721  0.95988728  3.01836009 -4.30313643]', '[ 0.37001256 -0.0624663   3.28947047 -5.55100751]', '[ 0.95247305 -1.07094443  2.40312497 -4.27892571]', '[ 1.31139858 -1.76096256  1.1713296  -2.66773437]', '[ 1.41874113 -2.15499272 -0.09777892 -1.28993425]', '[ 1.26852643 -2.25376428 -1.38554064  0.32183657]', '[ 0.87089962 -1.99198599 -2.54010382  2.33963295]', '[ 0.277876   -1.29815694 -3.33218293  4.63468626]', '[-0.43542605 -0.16061033 -3.6545583   6.41500876]', '[-1.08500329  1.03644671 -2.66409948  5.18042474]', '[-1.47782361  1.89132943 -1.25912823  3.44216102]', '[-1.58379664  2.41622554  0.18516663  1.83524217]', '[-1.4162227   2.64455043  1.47395128  0.430476  ]', '[-0.99301098  2.54079809  2.70705194 -1.48770356]', '[-0.36734514  2.04096511  3.44078708 -3.53135915]', '[ 0.34195898  1.12624437  3.58865734 -5.57753079]', '[ 1.0370162  -0.11374862  3.19630518 -6.39724983]', '[ 1.54070842 -1.25374011  1.74373069 -4.84984492]', '[ 1.72528114 -2.06821172  0.10154403 -3.33755992]', '[ 1.58697783 -2.590101   -1.45480487 -1.86074434]', '[ 1.14771547 -2.76476414 -2.88375568  0.11840648]', '[ 0.46492783 -2.547014   -3.82055788  2.03604324]', '[-0.31362117 -1.96663064 -3.8042126   3.699351  ]', '[-1.0117947  -1.10941178 -3.12832596  4.74046968]', '[-1.55328748 -0.13554602 -2.24205416  4.81933802]', '[-1.88473896  0.75702691 -1.02167175  4.02881652]', '[-1.94362624  1.46260479  0.480283    2.98203456]', '[-1.67580164  1.91692664  2.21652388  1.44254881]', '[-1.05404077  1.94352837  3.91122854 -1.29583555]', '[-0.16753135  1.3644695   4.80215646 -4.50823068]', '[ 0.81085737  0.19853686  4.8080617  -6.68305723]', '[ 1.6630718  -1.03119087  3.5916421  -5.25627834]', '[ 2.25495594 -1.9241427   2.38867153 -3.84923336]', '[ 2.64176881 -2.62737364  1.54116842 -3.27477388]', '[ 2.89839441  3.03028362  1.10387863 -3.00405866]', '[ 3.1132312   2.45041911  1.11249185 -2.80714997]', '[-2.91843432  1.89967211  1.45082655 -2.73929224]', '[-2.57026411  1.32929404  2.08992603 -3.06527812]', '[-2.05342979  0.61824775  3.16214964 -4.20322967]', '[-1.28222054 -0.37860427  4.52096716 -5.5536819 ]', '[-0.28926921 -1.41460972  5.26602771 -4.33630605]', '[ 0.75260202 -1.99304108  4.90882451 -1.30956949]', '[ 1.57720383 -1.93765036  3.16443057  1.77081702]', '[ 1.96343732 -1.29357067  0.67672625  4.54641942]', '[ 1.87345071 -0.15594353 -1.4236511   6.6841618 ]', '[ 1.49145113  1.2532678  -2.20159453  7.137893  ]', '[ 1.01164807  2.68707725 -2.66936386  7.36338532]', '[ 0.37689106 -1.97857613 -3.81745202  9.24103091]', '[-0.56893083  0.29124598 -5.06526881 12.38729091]', '[-1.32995505  2.39029187 -2.39442465  8.55136325]', '[-1.65836399 -2.35024614 -1.28097179  7.23239486]', '[-1.93636796 -0.88779556 -1.53925358  7.59411258]']</t>
+  </si>
+  <si>
+    <t>[0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50, 51, 52, 53, 54, 55, 56, 57, 58, 59, 60, 61, 62, 63, 64, 65, 66, 67, 68, 69, 70, 71, 72, 73, 74, 75, 76, 77, 78, 79, 80, 81, 82, 83, 84, 85, 86, 87, 88, 89]</t>
+  </si>
+  <si>
+    <t>[array([-0.03763371, -0.01533471,  0.06554052, -0.01816017], dtype=float32), array([-0.00754409, -0.05458322,  0.2277812 , -0.36241836]), array([ 0.04879627, -0.15231473,  0.32089719, -0.5887683 ]), array([ 0.11397169, -0.27767857,  0.31375488, -0.63332862]), array([ 0.16759438, -0.39312519,  0.2086893 , -0.49480525]), array([ 0.1930193 , -0.46685036,  0.03906408, -0.22816919]), array([ 0.15689524, -0.41528579, -0.3922057 ,  0.73207416]), array([ 0.04309269, -0.18588535, -0.71796191,  1.51055937]), array([-0.10156356,  0.12486504, -0.68790627,  1.51697551]), array([-0.22927161,  0.42348907, -0.55357165,  1.39819937]), array([-0.31090932,  0.65984646, -0.24293606,  0.92318871]), array([-0.31014687,  0.75044756,  0.2486755 , -0.02372896]), array([-0.20366105,  0.62121032,  0.79599893, -1.24647654]), array([-0.00411788,  0.26942411,  1.15489481, -2.19549786]), array([ 0.23392956, -0.21131539,  1.15674844, -2.47741296]), array([ 0.43096425, -0.66762183,  0.76173917, -1.986265  ]), array([ 0.52458578, -0.9796545 ,  0.15820524, -1.10009687]), array([ 0.4930839 , -1.1011094 , -0.46380341, -0.11075199]), array([ 0.32589057, -0.96862421, -1.17826925,  1.42078016]), array([ 0.04894834, -0.57676061, -1.53869505,  2.4260482 ]), array([-0.27489665, -0.01149737, -1.61623004,  3.06802964]), array([-0.55945103,  0.5756583 , -1.15065073,  2.65270956]), array([-0.71288953,  1.01000952, -0.35583386,  1.64294581]), array([-0.69808217,  1.22385838,  0.49692877,  0.48560128]), array([-0.50287533,  1.14784598,  1.41869689, -1.24158671]), array([-0.14900383,  0.73341372,  2.06329024, -2.85295241]), array([ 0.29084568,  0.05384361,  2.22735475, -3.73810785]), array([ 0.69044425, -0.6585127 ,  1.66461254, -3.18721047]), array([ 0.92961455, -1.17809972,  0.6945577 , -1.97409212]), array([ 0.96296101, -1.44497717, -0.35997969, -0.68946073]), array([ 0.77351961, -1.39864484, -1.50344078,  1.16654626]), array([ 0.37811844, -0.97203993, -2.39985579,  3.09342205]), array([-0.15765015, -0.1910167 , -2.84206179,  4.50453462]), array([-0.6921189 ,  0.69002473, -2.35483635,  4.00508677]), array([-1.06248704,  1.34995229, -1.30862257,  2.5701969 ]), array([-1.20839901,  1.72552608, -0.14388277,  1.2017002 ]), array([-1.12091592,  1.83108977,  1.00594216, -0.1597045 ]), array([-0.80072729,  1.60454421,  2.15604673, -2.14203903]), array([-0.27785721,  0.95988728,  3.01836009, -4.30313643]), array([ 0.37001256, -0.0624663 ,  3.28947047, -5.55100751]), array([ 0.95247305, -1.07094443,  2.40312497, -4.27892571]), array([ 1.31139858, -1.76096256,  1.1713296 , -2.66773437]), array([ 1.41874113, -2.15499272, -0.09777892, -1.28993425]), array([ 1.26852643, -2.25376428, -1.38554064,  0.32183657]), array([ 0.87089962, -1.99198599, -2.54010382,  2.33963295]), array([ 0.277876  , -1.29815694, -3.33218293,  4.63468626]), array([-0.43542605, -0.16061033, -3.6545583 ,  6.41500876]), array([-1.08500329,  1.03644671, -2.66409948,  5.18042474]), array([-1.47782361,  1.89132943, -1.25912823,  3.44216102]), array([-1.58379664,  2.41622554,  0.18516663,  1.83524217]), array([-1.4162227 ,  2.64455043,  1.47395128,  0.430476  ]), array([-0.99301098,  2.54079809,  2.70705194, -1.48770356]), array([-0.36734514,  2.04096511,  3.44078708, -3.53135915]), array([ 0.34195898,  1.12624437,  3.58865734, -5.57753079]), array([ 1.0370162 , -0.11374862,  3.19630518, -6.39724983]), array([ 1.54070842, -1.25374011,  1.74373069, -4.84984492]), array([ 1.72528114, -2.06821172,  0.10154403, -3.33755992]), array([ 1.58697783, -2.590101  , -1.45480487, -1.86074434]), array([ 1.14771547, -2.76476414, -2.88375568,  0.11840648]), array([ 0.46492783, -2.547014  , -3.82055788,  2.03604324]), array([-0.31362117, -1.96663064, -3.8042126 ,  3.699351  ]), array([-1.0117947 , -1.10941178, -3.12832596,  4.74046968]), array([-1.55328748, -0.13554602, -2.24205416,  4.81933802]), array([-1.88473896,  0.75702691, -1.02167175,  4.02881652]), array([-1.94362624,  1.46260479,  0.480283  ,  2.98203456]), array([-1.67580164,  1.91692664,  2.21652388,  1.44254881]), array([-1.05404077,  1.94352837,  3.91122854, -1.29583555]), array([-0.16753135,  1.3644695 ,  4.80215646, -4.50823068]), array([ 0.81085737,  0.19853686,  4.8080617 , -6.68305723]), array([ 1.6630718 , -1.03119087,  3.5916421 , -5.25627834]), array([ 2.25495594, -1.9241427 ,  2.38867153, -3.84923336]), array([ 2.64176881, -2.62737364,  1.54116842, -3.27477388]), array([ 2.89839441,  3.03028362,  1.10387863, -3.00405866]), array([ 3.1132312 ,  2.45041911,  1.11249185, -2.80714997]), array([-2.91843432,  1.89967211,  1.45082655, -2.73929224]), array([-2.57026411,  1.32929404,  2.08992603, -3.06527812]), array([-2.05342979,  0.61824775,  3.16214964, -4.20322967]), array([-1.28222054, -0.37860427,  4.52096716, -5.5536819 ]), array([-0.28926921, -1.41460972,  5.26602771, -4.33630605]), array([ 0.75260202, -1.99304108,  4.90882451, -1.30956949]), array([ 1.57720383, -1.93765036,  3.16443057,  1.77081702]), array([ 1.96343732, -1.29357067,  0.67672625,  4.54641942]), array([ 1.87345071, -0.15594353, -1.4236511 ,  6.6841618 ]), array([ 1.49145113,  1.2532678 , -2.20159453,  7.137893  ]), array([ 1.01164807,  2.68707725, -2.66936386,  7.36338532]), array([ 0.37689106, -1.97857613, -3.81745202,  9.24103091]), array([-0.56893083,  0.29124598, -5.06526881, 12.38729091]), array([-1.32995505,  2.39029187, -2.39442465,  8.55136325]), array([-1.65836399, -2.35024614, -1.28097179,  7.23239486]), array([-1.93636796, -0.88779556, -1.53925358,  7.59411258])]</t>
+  </si>
+  <si>
+    <t>['[0,0,0]', '[0,2,1]', '[0,1,1]', '[1,1,1]', '[1,1,2]', '[2,1,0]', '[2,2,2]', '[1,2,0]', '[1,0,2]', '[2,0,1]']</t>
+  </si>
+  <si>
+    <t>[6, 9, 10, 11, 18, 20, 22, 23, 30, 32, 33, 43, 44, 45, 48, 58, 59, 62, 70, 71, 73, 88, 89, 90, 95, 104, 111, 116]</t>
+  </si>
+  <si>
+    <t>[0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 1, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 2, 2, 1, 1, 0, 0, 0, 1, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 1, 1, 1, 1]</t>
+  </si>
+  <si>
+    <t>['[-0.03763371 -0.01533471  0.06554052 -0.01816017]', '[-0.00754409 -0.05458322  0.2277812  -0.36241836]', '[ 0.04879627 -0.15231473  0.32089719 -0.5887683 ]', '[ 0.11397169 -0.27767857  0.31375488 -0.63332862]', '[ 0.16759438 -0.39312519  0.2086893  -0.49480525]', '[ 0.1930193  -0.46685036  0.03906408 -0.22816919]', '[ 0.16956871 -0.44830261 -0.26820417  0.40739083]', '[ 0.07764819 -0.2777752  -0.62973474  1.26105599]', '[-0.06966349  0.03261704 -0.80302667  1.76452698]', '[-0.21167982  0.35689841 -0.57807865  1.40055574]', '[-0.28871224  0.56859039 -0.17470055  0.67947281]', '[-0.27847355  0.62063701  0.27437479 -0.16244055]', '[-0.1710445   0.47507147  0.77816367 -1.26464565]', '[ 0.01936374  0.13588643  1.07947728 -2.04484795]', '[ 0.23695357 -0.29798889  1.03442289 -2.17421786]', '[ 0.40969848 -0.68898776  0.65040294 -1.6559087 ]', '[ 0.48567883 -0.93929998  0.09638582 -0.81950146]', '[ 0.44760168 -1.01153796 -0.4678144   0.09822009]', '[ 0.29504844 -0.87386654 -1.02972873  1.25757659]', '[ 0.03870067 -0.49258951 -1.48588004  2.48827445]', '[-0.25905405  0.04017398 -1.41075917  2.68448888]', '[-0.50582279  0.55145131 -0.99024773  2.30158705]', '[-0.62435918  0.89527013 -0.17637506  1.10177013]', '[-0.57550103  0.98647487  0.65295216 -0.19225139]', '[-0.36160409  0.7907017   1.45022715 -1.74520153]', '[-0.01566966  0.30909466  1.93748553 -2.96158392]', '[ 0.37375694 -0.32144045  1.84888201 -3.13624084]', '[ 0.68468172 -0.87280671  1.19616501 -2.27435607]', '[ 0.8368613  -1.21277711  0.30766939 -1.11037131]', '[ 0.80584052 -1.31456546 -0.610222    0.09723123]', '[ 0.59076698 -1.14469713 -1.50905331  1.60239345]', '[ 0.20856653 -0.64964114 -2.25536993  3.29450224]', '[-0.26159298  0.07929518 -2.31927689  3.74606082]', '[-0.66590931  0.74309583 -1.63196796  2.72863944]', '[-0.90399964  1.17257644 -0.71865935  1.54245644]', '[-0.94756561  1.35840171  0.28485439  0.31305372]', '[-0.7748463   1.24152227  1.42040514 -1.49640193]', '[-0.39220369  0.75425975  2.35868776 -3.35528725]', '[ 0.1353928  -0.05314326  2.78066973 -4.45081048]', '[ 0.65212333 -0.88475059  2.2593891  -3.62296384]', '[ 1.01000736 -1.46411132  1.28424828 -2.16669395]', '[ 1.15804276 -1.75999983  0.18702306 -0.80897796]', '[ 1.06891707 -1.74234424 -1.06629431  0.99763346]', '[ 0.7482387  -1.37332749 -2.11032064  2.72485082]', '[ 0.24145184 -0.64663717 -2.89029671  4.47397646]', '[-0.35537968  0.3165223  -2.8957684   4.76801614]', '[-0.86192333  1.15338828 -2.07647931  3.44998987]', '[-1.16910993  1.69077168 -0.97565887  1.95291318]', '[-1.24035095  1.92230591  0.26208181  0.37625344]', '[-1.06042531  1.81562582  1.51775438 -1.4701685 ]', '[-0.64455186  1.31615453  2.60784093 -3.57559854]', '[-0.03493803  0.37988818  3.39258481 -5.63124627]', '[ 0.63074695 -0.75656785  3.04815608 -5.25690487]', '[ 1.13291809 -1.62822893  1.93376576 -3.45969788]', '[ 1.39843645 -2.16514524  0.71378692 -1.95881928]', '[ 1.41762289 -2.42132026 -0.51793772 -0.60520968]', '[ 1.18325636 -2.36124021 -1.80061286  1.23014679]', '[ 0.71409172 -1.91412022 -2.83462816  3.29276818]', '[ 0.08186135 -1.04782395 -3.43130685  5.36508432]', '[-0.61678703  0.15345969 -3.3494747   6.16993994]', '[-1.17880626  1.24844411 -2.15867086  4.58284853]', '[-1.46977316  1.99734563 -0.74958468  2.96835571]', '[-1.47453964  2.42820311  0.68480421  1.34796394]', '[-1.19882255  2.51121817  2.0378538  -0.53773224]', '[-0.68118864  2.20349943  3.05657829 -2.5664252 ]', '[-0.01674834  1.47553708  3.50334821 -4.71911956]', '[ 0.69429308  0.34033316  3.50395996 -6.37929907]', '[ 1.3034389  -0.87722729  2.41243614 -5.41734511]', '[ 1.62933847 -1.79064829  0.83441247 -3.76817607]', '[ 1.63859175 -2.40034231 -0.72600898 -2.33014211]', '[ 1.33848093 -2.67464474 -2.23264984 -0.39495227]', '[ 0.77268866 -2.573605   -3.34307192  1.40571663]', '[ 0.04620896 -2.09772103 -3.76903656  3.32201672]', '[-0.67198808 -1.29514855 -3.32633675  4.5844563 ]', '[-1.2733002  -0.30226166 -2.62781829  5.1351081 ]', '[-1.68794417  0.66393343 -1.44154607  4.37248315]', '[-1.82843527  1.42374978  0.0765114   3.19942855]', '[-1.64426372  1.92342319  1.77911333  1.71089778]', '[-1.11241273  2.02316556  3.46209939 -0.81006244]', '[-0.30879193  1.56918442  4.42757295 -3.75957955]', '[ 0.6034108   0.54500602  4.56645255 -6.21754252]', '[ 1.4397607  -0.69203329  3.61909013 -5.64933061]', '[ 2.0266638  -1.65400286  2.27859957 -4.08044985]', '[ 2.36658145 -2.37681402  1.15697411 -3.23400524]', '[ 2.50450659 -2.96166896  0.26713518 -2.61577032]', '[ 2.48971706  2.8685222  -0.38654014 -1.88531522]', '[ 2.35215783  2.58078371 -1.00451622 -0.96104197]', '[ 2.06083532  2.53508915 -1.96007396  0.51974895]', '[ 1.55356772  2.76880583 -3.15152361  1.80517945]', '[ 0.80022819 -3.03041688 -4.30885003  3.04264472]', '[-0.10434283 -2.28376168 -4.53173274  4.45721025]', '[-0.95531753 -1.23330324 -3.92717984  5.97072941]', '[-1.66841751  0.0328387  -3.12960492  6.38494838]', '[-2.16298229  1.20503271 -1.76003544  5.26360323]', '[-2.36447441  2.15909163 -0.24820565  4.31941063]', '[-2.26584537  2.9117104   1.16562135  3.18492931]', '[-1.92610546 -2.86065523  2.19169561  1.91778336]', '[-1.39171801 -2.59348016  3.15226669  0.83307502]', '[-0.66964981 -2.49211395  3.98717673  0.39141784]', '[ 0.14043567 -2.33340954  3.8860729   1.48737082]', '[ 0.77338905 -1.79040081  2.1695741   4.14268371]', '[ 0.92242361 -0.6068578  -0.63740518  7.61055306]', '[ 0.68272228  1.02759107 -1.22941098  7.94000124]', '[ 0.53083157  2.46710988 -0.38022138  6.72648301]', '[ 0.4316556  -2.43758182 -0.97641348  7.46119725]', '[ 8.66442083e-03 -6.25631531e-01 -3.27521770e+00  1.09183842e+01]', '[-0.57964815  1.475958   -1.87708599  8.93158184]', '[-0.70516772  2.98083308  0.31326194  6.56121907]', '[-0.62317841 -2.01341845  0.13309607  6.76311551]', '[-0.74458938 -0.4289118  -1.2380761   9.10944136]', '[-0.84914806  1.25798336  0.80301422  6.82993583]', '[-0.37120854  2.22299749  3.70668121  3.0237894 ]', '[0.49228738 2.57124821 4.59108444 0.83146675]', '[1.36946716 2.6867731  4.0413508  0.58914821]', '[2.09041054 2.870578   3.1788251  1.32260628]', '[ 2.64882771 -3.0478184   2.43334626  2.27324792]', '[ 3.0577573  -2.51397514  1.6460895   2.9759511 ]', '[-2.96668204 -1.91323078  0.990401    2.94197686]', '[-2.80003516 -1.36675103  0.759813    2.46144454]']</t>
+  </si>
+  <si>
+    <t>[0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50, 51, 52, 53, 54, 55, 56, 57, 58, 59, 60, 61, 62, 63, 64, 65, 66, 67, 68, 69, 70, 71, 72, 73, 74, 75, 76, 77, 78, 79, 80, 81, 82, 83, 84, 85, 86, 87, 88, 89, 90, 91, 92, 93, 94, 95, 96, 97, 98, 99, 100, 101, 102, 103, 104, 105, 106, 107, 108, 109, 110, 111, 112, 113, 114, 115, 116, 117, 118]</t>
+  </si>
+  <si>
+    <t>[array([-0.03763371, -0.01533471,  0.06554052, -0.01816017], dtype=float32), array([-0.00754409, -0.05458322,  0.2277812 , -0.36241836]), array([ 0.04879627, -0.15231473,  0.32089719, -0.5887683 ]), array([ 0.11397169, -0.27767857,  0.31375488, -0.63332862]), array([ 0.16759438, -0.39312519,  0.2086893 , -0.49480525]), array([ 0.1930193 , -0.46685036,  0.03906408, -0.22816919]), array([ 0.16956871, -0.44830261, -0.26820417,  0.40739083]), array([ 0.07764819, -0.2777752 , -0.62973474,  1.26105599]), array([-0.06966349,  0.03261704, -0.80302667,  1.76452698]), array([-0.21167982,  0.35689841, -0.57807865,  1.40055574]), array([-0.28871224,  0.56859039, -0.17470055,  0.67947281]), array([-0.27847355,  0.62063701,  0.27437479, -0.16244055]), array([-0.1710445 ,  0.47507147,  0.77816367, -1.26464565]), array([ 0.01936374,  0.13588643,  1.07947728, -2.04484795]), array([ 0.23695357, -0.29798889,  1.03442289, -2.17421786]), array([ 0.40969848, -0.68898776,  0.65040294, -1.6559087 ]), array([ 0.48567883, -0.93929998,  0.09638582, -0.81950146]), array([ 0.44760168, -1.01153796, -0.4678144 ,  0.09822009]), array([ 0.29504844, -0.87386654, -1.02972873,  1.25757659]), array([ 0.03870067, -0.49258951, -1.48588004,  2.48827445]), array([-0.25905405,  0.04017398, -1.41075917,  2.68448888]), array([-0.50582279,  0.55145131, -0.99024773,  2.30158705]), array([-0.62435918,  0.89527013, -0.17637506,  1.10177013]), array([-0.57550103,  0.98647487,  0.65295216, -0.19225139]), array([-0.36160409,  0.7907017 ,  1.45022715, -1.74520153]), array([-0.01566966,  0.30909466,  1.93748553, -2.96158392]), array([ 0.37375694, -0.32144045,  1.84888201, -3.13624084]), array([ 0.68468172, -0.87280671,  1.19616501, -2.27435607]), array([ 0.8368613 , -1.21277711,  0.30766939, -1.11037131]), array([ 0.80584052, -1.31456546, -0.610222  ,  0.09723123]), array([ 0.59076698, -1.14469713, -1.50905331,  1.60239345]), array([ 0.20856653, -0.64964114, -2.25536993,  3.29450224]), array([-0.26159298,  0.07929518, -2.31927689,  3.74606082]), array([-0.66590931,  0.74309583, -1.63196796,  2.72863944]), array([-0.90399964,  1.17257644, -0.71865935,  1.54245644]), array([-0.94756561,  1.35840171,  0.28485439,  0.31305372]), array([-0.7748463 ,  1.24152227,  1.42040514, -1.49640193]), array([-0.39220369,  0.75425975,  2.35868776, -3.35528725]), array([ 0.1353928 , -0.05314326,  2.78066973, -4.45081048]), array([ 0.65212333, -0.88475059,  2.2593891 , -3.62296384]), array([ 1.01000736, -1.46411132,  1.28424828, -2.16669395]), array([ 1.15804276, -1.75999983,  0.18702306, -0.80897796]), array([ 1.06891707, -1.74234424, -1.06629431,  0.99763346]), array([ 0.7482387 , -1.37332749, -2.11032064,  2.72485082]), array([ 0.24145184, -0.64663717, -2.89029671,  4.47397646]), array([-0.35537968,  0.3165223 , -2.8957684 ,  4.76801614]), array([-0.86192333,  1.15338828, -2.07647931,  3.44998987]), array([-1.16910993,  1.69077168, -0.97565887,  1.95291318]), array([-1.24035095,  1.92230591,  0.26208181,  0.37625344]), array([-1.06042531,  1.81562582,  1.51775438, -1.4701685 ]), array([-0.64455186,  1.31615453,  2.60784093, -3.57559854]), array([-0.03493803,  0.37988818,  3.39258481, -5.63124627]), array([ 0.63074695, -0.75656785,  3.04815608, -5.25690487]), array([ 1.13291809, -1.62822893,  1.93376576, -3.45969788]), array([ 1.39843645, -2.16514524,  0.71378692, -1.95881928]), array([ 1.41762289, -2.42132026, -0.51793772, -0.60520968]), array([ 1.18325636, -2.36124021, -1.80061286,  1.23014679]), array([ 0.71409172, -1.91412022, -2.83462816,  3.29276818]), array([ 0.08186135, -1.04782395, -3.43130685,  5.36508432]), array([-0.61678703,  0.15345969, -3.3494747 ,  6.16993994]), array([-1.17880626,  1.24844411, -2.15867086,  4.58284853]), array([-1.46977316,  1.99734563, -0.74958468,  2.96835571]), array([-1.47453964,  2.42820311,  0.68480421,  1.34796394]), array([-1.19882255,  2.51121817,  2.0378538 , -0.53773224]), array([-0.68118864,  2.20349943,  3.05657829, -2.5664252 ]), array([-0.01674834,  1.47553708,  3.50334821, -4.71911956]), array([ 0.69429308,  0.34033316,  3.50395996, -6.37929907]), array([ 1.3034389 , -0.87722729,  2.41243614, -5.41734511]), array([ 1.62933847, -1.79064829,  0.83441247, -3.76817607]), array([ 1.63859175, -2.40034231, -0.72600898, -2.33014211]), array([ 1.33848093, -2.67464474, -2.23264984, -0.39495227]), array([ 0.77268866, -2.573605  , -3.34307192,  1.40571663]), array([ 0.04620896, -2.09772103, -3.76903656,  3.32201672]), array([-0.67198808, -1.29514855, -3.32633675,  4.5844563 ]), array([-1.2733002 , -0.30226166, -2.62781829,  5.1351081 ]), array([-1.68794417,  0.66393343, -1.44154607,  4.37248315]), array([-1.82843527,  1.42374978,  0.0765114 ,  3.19942855]), array([-1.64426372,  1.92342319,  1.77911333,  1.71089778]), array([-1.11241273,  2.02316556,  3.46209939, -0.81006244]), array([-0.30879193,  1.56918442,  4.42757295, -3.75957955]), array([ 0.6034108 ,  0.54500602,  4.56645255, -6.21754252]), array([ 1.4397607 , -0.69203329,  3.61909013, -5.64933061]), array([ 2.0266638 , -1.65400286,  2.27859957, -4.08044985]), array([ 2.36658145, -2.37681402,  1.15697411, -3.23400524]), array([ 2.50450659, -2.96166896,  0.26713518, -2.61577032]), array([ 2.48971706,  2.8685222 , -0.38654014, -1.88531522]), array([ 2.35215783,  2.58078371, -1.00451622, -0.96104197]), array([ 2.06083532,  2.53508915, -1.96007396,  0.51974895]), array([ 1.55356772,  2.76880583, -3.15152361,  1.80517945]), array([ 0.80022819, -3.03041688, -4.30885003,  3.04264472]), array([-0.10434283, -2.28376168, -4.53173274,  4.45721025]), array([-0.95531753, -1.23330324, -3.92717984,  5.97072941]), array([-1.66841751,  0.0328387 , -3.12960492,  6.38494838]), array([-2.16298229,  1.20503271, -1.76003544,  5.26360323]), array([-2.36447441,  2.15909163, -0.24820565,  4.31941063]), array([-2.26584537,  2.9117104 ,  1.16562135,  3.18492931]), array([-1.92610546, -2.86065523,  2.19169561,  1.91778336]), array([-1.39171801, -2.59348016,  3.15226669,  0.83307502]), array([-0.66964981, -2.49211395,  3.98717673,  0.39141784]), array([ 0.14043567, -2.33340954,  3.8860729 ,  1.48737082]), array([ 0.77338905, -1.79040081,  2.1695741 ,  4.14268371]), array([ 0.92242361, -0.6068578 , -0.63740518,  7.61055306]), array([ 0.68272228,  1.02759107, -1.22941098,  7.94000124]), array([ 0.53083157,  2.46710988, -0.38022138,  6.72648301]), array([ 0.4316556 , -2.43758182, -0.97641348,  7.46119725]), array([ 8.66442083e-03, -6.25631531e-01, -3.27521770e+00,  1.09183842e+01]), array([-0.57964815,  1.475958  , -1.87708599,  8.93158184]), array([-0.70516772,  2.98083308,  0.31326194,  6.56121907]), array([-0.62317841, -2.01341845,  0.13309607,  6.76311551]), array([-0.74458938, -0.4289118 , -1.2380761 ,  9.10944136]), array([-0.84914806,  1.25798336,  0.80301422,  6.82993583]), array([-0.37120854,  2.22299749,  3.70668121,  3.0237894 ]), array([0.49228738, 2.57124821, 4.59108444, 0.83146675]), array([1.36946716, 2.6867731 , 4.0413508 , 0.58914821]), array([2.09041054, 2.870578  , 3.1788251 , 1.32260628]), array([ 2.64882771, -3.0478184 ,  2.43334626,  2.27324792]), array([ 3.0577573 , -2.51397514,  1.6460895 ,  2.9759511 ]), array([-2.96668204, -1.91323078,  0.990401  ,  2.94197686]), array([-2.80003516, -1.36675103,  0.759813  ,  2.46144454])]</t>
+  </si>
+  <si>
+    <t>['[1,0,2]', '[2,0,1]', '[0,2,1]', '[1,2,0]', '[0,0,0]', '[2,2,2]', '[1,1,2]', '[1,1,1]', '[0,1,1]', '[2,1,0]']</t>
+  </si>
+  <si>
+    <t>[6, 7, 10, 11, 18, 20, 21, 22, 23, 31, 33, 43, 44, 46, 56, 58, 59, 60, 61, 72, 75, 87, 90, 91, 93, 115, 116]</t>
+  </si>
+  <si>
+    <t>[0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 1, 2]</t>
+  </si>
+  <si>
+    <t>['[-0.03763371 -0.01533471  0.06554052 -0.01816017]', '[-0.00754409 -0.05458322  0.2277812  -0.36241836]', '[ 0.04879627 -0.15231473  0.32089719 -0.5887683 ]', '[ 0.11397169 -0.27767857  0.31375488 -0.63332862]', '[ 0.16759438 -0.39312519  0.2086893  -0.49480525]', '[ 0.1930193  -0.46685036  0.03906408 -0.22816919]', '[ 0.16956871 -0.44830261 -0.26820417  0.40739083]', '[ 0.09055011 -0.31127879 -0.50323119  0.93116007]', '[-0.03483507 -0.05969969 -0.71793241  1.5230623 ]', '[-0.18039446  0.26629635 -0.69574778  1.65343328]', '[-0.28434539  0.53634675 -0.31832408  0.99491968]', '[-0.30187474  0.65121841  0.14588946  0.1405248 ]', '[-0.21625946  0.56068727  0.69308128 -1.02717928]', '[-0.03581705  0.25602337  1.07063553 -1.95170192]', '[ 0.18983261 -0.17944421  1.12254236 -2.28166283]', '[ 0.38705788 -0.60627424  0.79784549 -1.88839787]', '[ 0.49384505 -0.90711289  0.24974902 -1.08137931]', '[ 0.48392205 -1.03070599 -0.34439937 -0.14811263]', '[ 0.35111717 -0.93839535 -0.95874347  1.05644279]', '[ 0.10236466 -0.58897241 -1.4851611   2.38460568]', '[-0.20497122 -0.05899707 -1.50825708  2.76530806]', '[-0.46626337  0.4500858  -1.03514934  2.19356727]', '[-0.59948738  0.78340461 -0.27275816  1.09648574]', '[-0.57228673  0.88079816  0.53763126 -0.1275029 ]', '[-0.38067583  0.70365255  1.34585614 -1.62262011]', '[-0.05341741  0.25292846  1.85668413 -2.77703773]', '[ 0.32373181 -0.3381208   1.81183669 -2.93923585]', '[ 0.633655   -0.85439707  1.22348698 -2.12305461]', '[ 0.7969282  -1.16817092  0.38836994 -0.99796535]', '[ 0.78576796 -1.2511562  -0.49592701  0.17144049]', '[ 0.58434776 -1.04263716 -1.4928037   1.91756884]', '[ 0.21572281 -0.52133442 -2.12918583  3.21355068]', '[-0.24064973  0.20707362 -2.30668212  3.81906468]', '[-0.64140383  0.86941162 -1.61627077  2.66165844]', '[-0.87868641  1.27972335 -0.72847465  1.4267804 ]', '[-0.92711361  1.44026686  0.24651391  0.17889557]', '[-0.76485826  1.29704898  1.35700101 -1.62525239]', '[-0.39547775  0.78387439  2.2946346  -3.49082431]', '[ 0.12154395 -0.05404257  2.73873316 -4.61753663]', '[ 0.63037863 -0.91755905  2.22036528 -3.76925879]', '[ 0.98097548 -1.5238406   1.25215041 -2.29131944]', '[ 1.12393404 -1.84274942  0.16937401 -0.91428574]', '[ 1.03399187 -1.84547404 -1.05423464  0.89624088]', '[ 0.71991137 -1.49780793 -2.05332296  2.60905839]', '[ 0.22951341 -0.79466765 -2.79233359  4.38016019]', '[-0.36564231  0.20885371 -2.98140777  5.27423599]', '[-0.87417176  1.12024523 -2.00530102  3.6701814 ]', '[-1.16311481  1.7007373  -0.86707841  2.16173928]', '[-1.21822534  1.9946434   0.31417883  0.78490858]', '[-1.02804579  1.96719492  1.55951365 -1.08005657]', '[-0.61056398  1.54895027  2.56783182 -3.14239943]', '[-0.02101678  0.6999854   3.26263308 -5.28408077]', '[ 0.63623715 -0.44292367  3.09349597 -5.65817088]', '[ 1.14389338 -1.41289673  1.91525319 -3.95986679]', '[ 1.39583196 -2.04557566  0.60102498 -2.41707824]', '[ 1.38553068 -2.38910207 -0.69404527 -1.01798769]', '[ 1.11953642 -2.42690603 -1.93191953  0.6580526 ]', '[ 0.62847827 -2.09669816 -2.89965205  2.66841448]', '[ 3.96381473e-03 -1.37579041e+00 -3.26634345e+00  4.52386826e+00]', '[-0.64845831 -0.3262826  -3.14437181  5.70653677]', '[-1.18156559  0.73644069 -2.04149289  4.61198482]', '[-1.43891006  1.48273638 -0.51845396  2.87187359]', '[-1.39705371  1.91565844  0.93266022  1.4357822 ]', '[-1.0610939   1.99652701  2.37309493 -0.67168517]', '[-0.47937828  1.629154    3.3488345  -3.03175507]', '[ 0.23939097  0.78756108  3.74754119 -5.27634227]', '[ 0.96283039 -0.35020337  3.29305062 -5.62408281]', '[ 1.49370106 -1.32158779  1.96393525 -4.03054044]', '[ 1.74625394 -1.98751725  0.56334834 -2.68360389]', '[ 1.72016195 -2.40127005 -0.81828069 -1.43588525]', '[ 1.41121354 -2.5062241  -2.24702907  0.43138093]', '[ 0.8384986  -2.20806705 -3.40454144  2.60795357]', '[ 0.09850298 -1.46564545 -3.89729261  4.82694953]', '[-0.69788874 -0.28239687 -3.9433392   6.69129385]', '[-1.38810126  0.97748462 -2.78859685  5.51822654]', '[-1.78532508  1.88454087 -1.20076109  3.66508461]', '[-1.88223908  2.49399403  0.21721324  2.44239267]', '[-1.7057045   2.85449813  1.53122097  1.13523015]', '[-1.26360452  2.89958921  2.86694628 -0.69803946]', '[-0.58054882  2.57214757  3.85530788 -2.58474841]', '[ 0.21532369  1.86549206  3.95551354 -4.45832935]', '[ 0.96474895  0.81632834  3.49740336 -5.89521597]', '[ 1.58316272 -0.380222    2.56280451 -5.73669851]', '[ 1.9485309  -1.39880065  1.04720182 -4.43458762]', '[ 1.99237196 -2.16401552 -0.62135983 -3.20526667]', '[ 1.70396854 -2.6624594  -2.2308583  -1.72528494]', '[ 1.1059387  -2.80029995 -3.68654804  0.35489071]', '[ 0.27542422 -2.54688648 -4.46004446  2.13964667]', '[-0.60270668 -1.95219673 -4.14132328  3.69696776]', '[-1.33795282 -1.12778732 -3.1777561   4.3843711 ]', '[-1.86085846 -0.29090759 -2.04669902  3.86040242]', '[-2.15735819  0.39641118 -0.92704108  3.02620404]', '[-2.24389637  0.96266507  0.08770946  2.62823242]', '[-2.09337458  1.39909025  1.47081301  1.64108863]', '[-1.62845299  1.53653395  3.19423892 -0.44819847]', '[-0.82629156  1.14207127  4.75763928 -3.64481898]', '[ 0.22622666  0.09370999  5.53866558 -6.32684284]', '[ 1.26063368 -1.03973841  4.59883988 -4.49401228]', '[ 2.05259207 -1.70124448  3.35562003 -2.32289283]', '[ 2.62792089 -2.05670922  2.47888167 -1.42594173]', '[ 3.07929141 -2.33317559  2.12820003 -1.46320977]', '[-2.76739779 -2.68055692  2.33312697 -2.09357793]', '[-2.23246175  3.08199879  3.10778701 -3.20669191]', '[-1.49779384  2.2654648   4.26677575 -5.17967892]', '[-0.51635732  0.88669341  5.60122974 -8.86774683]', '[ 0.6464256  -1.01021262  5.57653688 -8.83057457]', '[ 1.63470794 -2.42603901  4.360252   -5.63268224]', '[ 2.40265605  2.88982737  3.36868364 -4.27522617]', '[ 3.0210953   2.08438131  2.94516858 -3.90780796]', '[-2.65069699  1.27087942  3.30760697 -4.41080695]', '[-1.88320914  0.23616468  4.47582695 -6.04138734]', '[-0.86503288 -1.03731864  5.59784792 -6.11399131]', '[ 0.30971031 -2.00316005  5.95960078 -3.25390128]', '[ 1.41184905 -2.30960069  4.81360288  0.13396842]', '[ 2.17273047 -2.00010645  2.72333081  2.78697257]', '[ 2.48388557 -1.22026514  0.44198068  4.8787107 ]', '[ 2.40749461 -0.11499328 -1.04178058  6.05524941]']</t>
   </si>
   <si>
     <t>[0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50, 51, 52, 53, 54, 55, 56, 57, 58, 59, 60, 61, 62, 63, 64, 65, 66, 67, 68, 69, 70, 71, 72, 73, 74, 75, 76, 77, 78, 79, 80, 81, 82, 83, 84, 85, 86, 87, 88, 89, 90, 91, 92, 93, 94, 95, 96, 97, 98, 99, 100, 101, 102, 103, 104, 105, 106, 107, 108, 109, 110, 111, 112, 113, 114, 115, 116]</t>
   </si>
   <si>
-    <t>[array([-0.03763371, -0.01533471,  0.06554052, -0.01816017], dtype=float32), array([-0.00754409, -0.05458322,  0.2277812 , -0.36241836]), array([ 0.03557041, -0.11811661,  0.19275289, -0.25552579]), array([ 0.07892797, -0.1849336 ,  0.22986116, -0.39424827]), array([ 0.12271824, -0.267417  ,  0.19671429, -0.40996627]), array([ 0.15338212, -0.34091394,  0.10180504, -0.30861109]), array([ 0.16107551, -0.38557729, -0.0273968 , -0.13010444]), array([ 0.11689442, -0.32478194, -0.40419263,  0.72290359]), array([ 0.00699758, -0.10946448, -0.66682387,  1.37864006]), array([-0.13518691,  0.19851722, -0.71460523,  1.62157325]), array([-0.26216055,  0.50605306, -0.52049404,  1.38437545]), array([-0.33248769,  0.73016948, -0.16679196,  0.82126441]), array([-0.32601137,  0.82598862,  0.22935372,  0.12936813]), array([-0.23310864,  0.75237898,  0.68098455, -0.84867834]), array([-0.05199092,  0.4669668 ,  1.09481076, -1.9534796 ]), array([ 0.17177326,  0.03966882,  1.08297445, -2.20563548]), array([ 0.35604853, -0.36621616,  0.70891984, -1.75321128]), array([ 0.45270788, -0.66444852,  0.23325569, -1.17687632]), array([ 0.4445464 , -0.82360354, -0.31342495, -0.39921041]), array([ 0.30954221, -0.76187415, -1.0094624 ,  1.00035337]), array([ 0.05595999, -0.43759942, -1.47573908,  2.17481945]), array([-0.25360483,  0.06316573, -1.53948539,  2.68467845]), array([-0.52539341,  0.57112116, -1.10888983,  2.26738845]), array([-0.67705457,  0.93606471, -0.3804693 ,  1.3384434 ]), array([-0.67304307,  1.09772826,  0.41729355,  0.26857392]), array([-0.49553157,  0.98500559,  1.32807675, -1.39027622]), array([-0.17004724,  0.58165138,  1.86742313, -2.57337335]), array([ 0.23160718, -0.02572826,  2.04685411, -3.31076392]), array([ 0.60240398, -0.65297327,  1.568263  , -2.79140887]), array([ 0.82248658, -1.07361519,  0.60517813, -1.38992621]), array([ 0.84025911, -1.20743645, -0.42515924,  0.05322303]), array([ 0.64735119, -1.02204979, -1.48009051,  1.80706959]), array([ 0.26309435, -0.48863013, -2.30098295,  3.45598492]), array([-0.23082223,  0.2857871 , -2.49686718,  4.00553376]), array([-0.67884917,  1.0010593 , -1.89057012,  2.99253081]), array([-0.96567402,  1.46252668, -0.9489651 ,  1.62299375]), array([-1.05195817,  1.65531974,  0.09162765,  0.31232484]), array([-0.9138075 ,  1.53738981,  1.27509378, -1.50955901]), array([-0.56057132,  1.06626713,  2.2219813 , -3.21263214]), array([-0.04814964,  0.27117236,  2.79661727, -4.55414132]), array([ 0.49165791, -0.61781215,  2.44337951, -4.01042004]), array([ 0.89795444, -1.28784675,  1.56423359, -2.6337518 ]), array([ 1.09700996, -1.64909104,  0.41613217, -1.00493376]), array([ 1.06353494, -1.69505132, -0.74409615,  0.54889826]), array([ 0.79718856, -1.39700237, -1.8960272 ,  2.46639721]), array([ 0.31763711, -0.69551535, -2.84822387,  4.51929882]), array([-0.29540514,  0.32593323, -3.09010244,  5.28132737]), array([-0.84138707,  1.25356408, -2.26936097,  3.828653  ]), array([-1.18685648,  1.85640639, -1.16591782,  2.24214184]), array([-1.30314298,  2.16490622,  0.00699825,  0.86028355]), array([-1.17901679,  2.17921702,  1.21844396, -0.73086459]), array([-0.82708377,  1.86187882,  2.25947341, -2.47841034]), array([-0.28672542,  1.146977  ,  3.09949128, -4.70095926]), array([ 0.38427971,  0.01597864,  3.44165403, -6.2384889 ]), array([ 0.97985671, -1.09641616,  2.36933346, -4.59934022]), array([ 1.32513565, -1.84502254,  1.07255557, -2.93946594]), array([ 1.40825385, -2.28950136, -0.23645068, -1.52120098]), array([ 1.22933591, -2.43098018, -1.52785603,  0.12073893]), array([ 0.80695634, -2.2122894 , -2.63255035,  2.09187231]), array([ 0.20980735, -1.58336507, -3.25927539,  4.21779605]), array([-0.4711149 , -0.53306286, -3.46898415,  6.12251142]), array([-1.10476081,  0.68997325, -2.66353943,  5.6494184 ]), array([-1.48884843,  1.64497887, -1.15020417,  3.9217163 ]), array([-1.56452636,  2.27926454,  0.38272279,  2.43942766]), array([-1.34463095,  2.61711625,  1.78380245,  0.92262504]), array([-0.86307794,  2.62498259,  2.96218674, -0.83811695]), array([-0.1965416 ,  2.26962954,  3.56223723, -2.68283291]), array([ 0.4952368 ,  1.59758385,  3.24435793, -3.93955144]), array([ 1.08388237,  0.71888727,  2.60286174, -4.70386025]), array([ 1.50128026, -0.1766842 ,  1.50181667, -4.07716378]), array([ 1.66198199, -0.87073788,  0.0679292 , -2.81724414]), array([ 1.51685823, -1.28520154, -1.53805584, -1.24995426]), array([ 1.04010155, -1.30215696, -3.18243568,  1.18847199]), array([ 0.27854307, -0.7796659 , -4.31298482,  3.9922082 ]), array([-0.61501349,  0.18167305, -4.39136286,  5.09001453]), array([-1.39297551,  1.05124991, -3.29227865,  3.42916171]), array([-1.92801688,  1.57820859, -2.07923664,  1.97305114]), array([-2.23622675,  1.88957903, -1.03036261,  1.2318007 ]), array([-2.34785835,  2.09273442, -0.09477685,  0.82071748]), array([-2.26565423,  2.19226117,  0.93024602,  0.13695917]), array([-1.96658518,  2.12112596,  2.08706002, -0.94412254]), array([-1.42257474,  1.76477828,  3.35764437, -2.77358848]), array([-0.62062808,  0.92007883,  4.63443003, -5.78254431]), array([ 0.37973262, -0.4449266 ,  5.06712084, -7.06527338]), array([ 1.28349934, -1.58197478,  3.89474652, -4.19821241]), array([ 1.93800669, -2.19256355,  2.66258737, -2.09673869]), array([ 2.36659525, -2.50278792,  1.6644645 , -1.11988117]), array([ 2.62131847, -2.67380743,  0.92489652, -0.65045076]), array([ 2.74342423, -2.75909027,  0.320519  , -0.22883456]), array([ 2.75448876, -2.77046746, -0.20707014,  0.11285619]), array([ 2.65723331, -2.71026158, -0.78424932,  0.51010337]), array([ 2.42294339, -2.53253372, -1.59813361,  1.32166245]), array([ 1.9997098 , -2.14953934, -2.68045203,  2.62891539]), array([ 1.33433935, -1.41317451, -4.01352231,  4.95793719]), array([ 0.38372467, -0.09705747, -5.36444202,  7.87457265]), array([-0.67285286,  1.34644041, -4.93960617,  5.86666758]), array([-1.56537514,  2.22912695, -3.94825256,  3.13716903]), array([-2.24588245,  2.68138626, -2.883646  ,  1.56513058]), array([-2.74358869,  2.91366401, -2.17547116,  0.88122774]), array([ 3.13353088,  3.07550793, -1.97382122,  0.83426715]), array([ 2.71570835, -2.99965033, -2.29488383,  1.34157439]), array([ 2.18053306, -2.62916961, -3.13771747,  2.49697153]), array([ 1.43746715, -1.9310796 , -4.32409067,  4.72501156]), array([ 0.43970763, -0.62732747, -5.65461045,  8.38641137]), array([-0.70464203,  1.07789067, -5.40345368,  7.56955661]), array([-1.6714284 ,  2.26453498, -4.28865508,  4.53859207]), array([-2.42972838,  3.00407911, -3.34565323,  3.08469265]), array([-3.04596742, -2.71614054, -2.93560918,  2.69057028]), array([ 2.63042613, -2.14593971, -3.2572678 ,  3.18432724]), array([ 1.88695847, -1.35470735, -4.30111778,  5.0147983 ]), array([ 0.86607329, -0.03831953, -5.85377283,  7.88275853]), array([-0.33719614,  1.40000356, -5.90585695,  5.68229485]), array([-1.44304788,  2.16876411, -5.01363961,  2.13277705]), array([-2.30810625,  2.34191173, -3.63727848, -0.15358126]), array([-2.92264319,  2.19884207, -2.60385542, -1.06656161]), array([ 2.89050277,  1.98534337, -2.21440842, -0.92167265]), array([ 2.42870866,  1.87284022, -2.51559029, -0.13490451])]</t>
-  </si>
-  <si>
-    <t>['[1,1,2]', '[1,1,1]', '[2,1,0]', '[1,2,0]', '[0,0,0]', '[2,0,1]', '[2,2,2]', '[1,0,2]', '[0,1,1]', '[0,2,1]']</t>
-  </si>
-  <si>
-    <t>[1, 3, 4, 11, 12, 14, 15, 16, 23, 24, 25, 26, 28, 35, 36, 37, 38, 39, 40, 47, 48, 49, 50, 51, 52, 60, 61, 62, 63, 64, 74, 75, 76, 77, 78, 79, 89, 90, 91, 92, 93, 94, 105, 106, 107, 108]</t>
-  </si>
-  <si>
-    <t>[0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 1, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 1, 2, 2, 2, 2, 2, 2, 2, 2, 1, 0, 0, 0, 0, 0]</t>
-  </si>
-  <si>
-    <t>['[-0.03763371 -0.01533471  0.06554052 -0.01816017]', '[-0.0208055  -0.02030166  0.09914155 -0.02801351]', '[ 0.013578   -0.05917353  0.23628798 -0.34824344]', '[ 0.05569493 -0.11750576  0.17467028 -0.21881458]', '[ 0.08000939 -0.1414547   0.06300338 -0.0132271 ]', '[ 0.06657137 -0.08758677 -0.19283697  0.54032615]', '[ 0.00731296  0.06492895 -0.38251373  0.94850147]', '[-0.07746096  0.27319091 -0.44079182  1.08370966]', '[-0.15888768  0.47769873 -0.35165449  0.91660574]', '[-0.21076339  0.6247122  -0.15481124  0.52721898]', '[-0.21786653  0.68164744  0.08517     0.03521468]', '[-0.16600201  0.60761759  0.42274412 -0.76087299]', '[-0.05580611  0.38860384  0.65426274 -1.38478298]', '[ 0.0956853   0.04470926  0.81953581 -1.97208953]', '[ 0.23897176 -0.32545144  0.57075454 -1.6404927 ]', '[ 0.31082626 -0.58329541  0.1300411  -0.89480725]', '[ 0.28854808 -0.6738532  -0.34729328 -0.00519497]', '[ 0.16561334 -0.55662251 -0.85713256  1.1511933 ]', '[-0.04013912 -0.23282112 -1.15349174  2.00948864]', '[-0.27184803  0.20359494 -1.09952911  2.23265767]', '[-0.45489788  0.61236481 -0.68395514  1.76617058]', '[-0.53254708  0.88586594 -0.07769622  0.93589032]', '[-0.48521224  0.9800007   0.54041636  0.00193093]', '[-0.31393268  0.85973219  1.1399975  -1.18325198]', '[-0.0463749   0.5234024   1.48183551 -2.10800116]', '[ 0.25173876  0.06065508  1.42435304 -2.38393486]', '[ 0.49264598 -0.37283111  0.92415958 -1.83960284]', '[ 0.61641383 -0.67690596  0.2862465  -1.150905  ]', '[ 0.59034061 -0.79003686 -0.54118729  0.02784974]', '[ 0.39582786 -0.63579979 -1.36971977  1.49191887]', '[ 0.06301046 -0.21549704 -1.88602619  2.60236595]', '[-0.32020638  0.33770894 -1.84496764  2.74422719]', '[-0.63800372  0.81715001 -1.26870854  1.95332207]', '[-0.81076874  1.1000733  -0.43583786  0.85916348]', '[-0.80817411  1.15849981  0.46006214 -0.27766825]', '[-0.6212991   0.95950176  1.38404633 -1.70958957]', '[-0.2704879   0.48441976  2.0617477  -2.96337639]', '[ 0.16535436 -0.16135831  2.17931015 -3.27197905]', '[ 0.5536822  -0.7342766   1.61851815 -2.31486065]', '[ 0.79054609 -1.06046886  0.71900933 -0.92876785]', '[ 0.83445703 -1.10536693 -0.28473295  0.47816123]', '[ 0.66780558 -0.83942264 -1.36563368  2.18150781]', '[ 0.30220796 -0.24406782 -2.21964136  3.66141312]', '[-0.17196334  0.53234671 -2.38277492  3.82229869]', '[-0.60228899  1.19284624 -1.84445857  2.67456063]', '[-0.89019239  1.58995071 -1.00243753  1.30033509]', '[-0.99447196  1.71768707 -0.02937823 -0.01469416]', '[-0.89300399  1.55992237  1.03579238 -1.57439872]', '[-0.58691417  1.0797985   1.99817692 -3.23927693]', '[-0.11329809  0.27932772  2.64020328 -4.59658461]', '[ 0.40434373 -0.62560839  2.37687947 -4.12441185]', '[ 0.79426777 -1.29284936  1.47295282 -2.50094146]', '[ 0.98373762 -1.63052907  0.40958836 -0.89551447]', '[ 0.95662001 -1.65536347 -0.67494058  0.64882176]', '[ 0.71090515 -1.34021306 -1.76088457  2.5295718 ]', '[ 0.26411249 -0.63530706 -2.65431245  4.47370544]', '[-0.30323883  0.3604135  -2.83486611  5.09202886]', '[-0.79863381  1.25425636 -2.02685537  3.69780825]', '[-1.09846275  1.83669851 -0.95346646  2.1585851 ]', '[-1.17628166  2.12855909  0.17583403  0.77215012]', '[-1.02503536  2.12350717  1.31362519 -0.8336964 ]', '[-0.66552169  1.78718978  2.23312528 -2.55292606]', '[-0.1538701   1.09504761  2.82805102 -4.35373031]', '[ 0.43320308  0.09464438  2.89742791 -5.33980039]', '[ 0.9280553  -0.87273469  1.92069157 -4.07694319]', '[ 1.18960109 -1.53809163  0.67433785 -2.58239255]', '[ 1.19617722 -1.9113529  -0.60052956 -1.1490787 ]', '[ 0.94422955 -1.94691603 -1.87322444  0.81418009]', '[ 0.47186129 -1.57536118 -2.77898116  2.92145884]', '[-0.13828227 -0.77993966 -3.24818022  4.95216595]', '[-0.7768836   0.29873561 -2.95299943  5.41058379]', '[-1.25197854  1.24129558 -1.72419285  3.90834685]', '[-1.458254    1.8718869  -0.33418752  2.43225411]', '[-1.38692131  2.21764855  1.03492603  1.00947729]', '[-1.04829434  2.24306837  2.30364062 -0.78642615]', '[-0.49475045  1.89216695  3.1369166  -2.73748956]', '[ 0.16516832  1.15333272  3.37499311 -4.58568842]', '[ 0.81786652  0.12924802  3.01736108 -5.32571931]', '[ 1.30742373 -0.82480946  1.77803069 -4.01440128]', '[ 1.5146647  -1.46537005  0.28666996 -2.41428738]', '[ 1.42976506 -1.81540212 -1.13429535 -1.04871224]', '[ 1.05416263 -1.8162659  -2.57089784  1.10342404]', '[ 0.43151476 -1.34945315 -3.56847325  3.59970586]', '[-0.33549966 -0.39375906 -3.9735238   5.71374334]', '[-1.0737705   0.73119563 -3.21848224  5.08379104]', '[-1.58709803  1.5744898  -1.90337992  3.40184534]', '[-1.8372799   2.1266066  -0.60371365  2.17463688]', '[-1.83010966  2.45066627  0.67270345  1.05020239]', '[-1.5568929   2.49138083  2.05018959 -0.6938422 ]', '[-1.02533598  2.16789948  3.21618303 -2.61730174]', '[-0.30137498  1.41378673  3.9459133  -4.97537237]', '[ 0.520961    0.20410924  4.12003489 -6.74156701]', '[ 1.24300791 -1.02169824  2.93212243 -5.13359132]', '[ 1.68097675 -1.84761018  1.46154552 -3.23839364]', '[ 1.83323711 -2.35020533  0.0725274  -1.82097015]', '[ 1.71362234 -2.57401665 -1.26192114 -0.38847068]', '[ 1.32567633 -2.46833544 -2.59540552  1.50064848]', '[ 0.69525696 -1.94637957 -3.63266257  3.80090645]', '[-0.09620738 -0.91827296 -4.22466971  6.47049571]', '[-0.93576651  0.49809105 -3.89858254  7.00133153]', '[-1.57003313  1.68683284 -2.41111051  4.88913558]', '[-1.90916075  2.51002147 -1.00832578  3.44064587]', '[-1.98696924  3.07905479  0.19382064  2.25434701]', '[-1.84104105 -2.87548476  1.26025957  1.0238981 ]', '[-1.47248382 -2.8130893   2.44006931 -0.37822957]', '[-0.86579543 -3.01016548  3.58550433 -1.53396641]', '[-0.07876824  2.88091138  4.12715322 -2.32755778]', '[ 0.70889408  2.3692331   3.58538902 -2.69751874]', '[ 1.31149321  1.85046158  2.3901811  -2.35869981]', '[ 1.66773114  1.44749146  1.17554518 -1.59258071]']</t>
+    <t>[array([-0.03763371, -0.01533471,  0.06554052, -0.01816017], dtype=float32), array([-0.00754409, -0.05458322,  0.2277812 , -0.36241836]), array([ 0.04879627, -0.15231473,  0.32089719, -0.5887683 ]), array([ 0.11397169, -0.27767857,  0.31375488, -0.63332862]), array([ 0.16759438, -0.39312519,  0.2086893 , -0.49480525]), array([ 0.1930193 , -0.46685036,  0.03906408, -0.22816919]), array([ 0.16956871, -0.44830261, -0.26820417,  0.40739083]), array([ 0.09055011, -0.31127879, -0.50323119,  0.93116007]), array([-0.03483507, -0.05969969, -0.71793241,  1.5230623 ]), array([-0.18039446,  0.26629635, -0.69574778,  1.65343328]), array([-0.28434539,  0.53634675, -0.31832408,  0.99491968]), array([-0.30187474,  0.65121841,  0.14588946,  0.1405248 ]), array([-0.21625946,  0.56068727,  0.69308128, -1.02717928]), array([-0.03581705,  0.25602337,  1.07063553, -1.95170192]), array([ 0.18983261, -0.17944421,  1.12254236, -2.28166283]), array([ 0.38705788, -0.60627424,  0.79784549, -1.88839787]), array([ 0.49384505, -0.90711289,  0.24974902, -1.08137931]), array([ 0.48392205, -1.03070599, -0.34439937, -0.14811263]), array([ 0.35111717, -0.93839535, -0.95874347,  1.05644279]), array([ 0.10236466, -0.58897241, -1.4851611 ,  2.38460568]), array([-0.20497122, -0.05899707, -1.50825708,  2.76530806]), array([-0.46626337,  0.4500858 , -1.03514934,  2.19356727]), array([-0.59948738,  0.78340461, -0.27275816,  1.09648574]), array([-0.57228673,  0.88079816,  0.53763126, -0.1275029 ]), array([-0.38067583,  0.70365255,  1.34585614, -1.62262011]), array([-0.05341741,  0.25292846,  1.85668413, -2.77703773]), array([ 0.32373181, -0.3381208 ,  1.81183669, -2.93923585]), array([ 0.633655  , -0.85439707,  1.22348698, -2.12305461]), array([ 0.7969282 , -1.16817092,  0.38836994, -0.99796535]), array([ 0.78576796, -1.2511562 , -0.49592701,  0.17144049]), array([ 0.58434776, -1.04263716, -1.4928037 ,  1.91756884]), array([ 0.21572281, -0.52133442, -2.12918583,  3.21355068]), array([-0.24064973,  0.20707362, -2.30668212,  3.81906468]), array([-0.64140383,  0.86941162, -1.61627077,  2.66165844]), array([-0.87868641,  1.27972335, -0.72847465,  1.4267804 ]), array([-0.92711361,  1.44026686,  0.24651391,  0.17889557]), array([-0.76485826,  1.29704898,  1.35700101, -1.62525239]), array([-0.39547775,  0.78387439,  2.2946346 , -3.49082431]), array([ 0.12154395, -0.05404257,  2.73873316, -4.61753663]), array([ 0.63037863, -0.91755905,  2.22036528, -3.76925879]), array([ 0.98097548, -1.5238406 ,  1.25215041, -2.29131944]), array([ 1.12393404, -1.84274942,  0.16937401, -0.91428574]), array([ 1.03399187, -1.84547404, -1.05423464,  0.89624088]), array([ 0.71991137, -1.49780793, -2.05332296,  2.60905839]), array([ 0.22951341, -0.79466765, -2.79233359,  4.38016019]), array([-0.36564231,  0.20885371, -2.98140777,  5.27423599]), array([-0.87417176,  1.12024523, -2.00530102,  3.6701814 ]), array([-1.16311481,  1.7007373 , -0.86707841,  2.16173928]), array([-1.21822534,  1.9946434 ,  0.31417883,  0.78490858]), array([-1.02804579,  1.96719492,  1.55951365, -1.08005657]), array([-0.61056398,  1.54895027,  2.56783182, -3.14239943]), array([-0.02101678,  0.6999854 ,  3.26263308, -5.28408077]), array([ 0.63623715, -0.44292367,  3.09349597, -5.65817088]), array([ 1.14389338, -1.41289673,  1.91525319, -3.95986679]), array([ 1.39583196, -2.04557566,  0.60102498, -2.41707824]), array([ 1.38553068, -2.38910207, -0.69404527, -1.01798769]), array([ 1.11953642, -2.42690603, -1.93191953,  0.6580526 ]), array([ 0.62847827, -2.09669816, -2.89965205,  2.66841448]), array([ 3.96381473e-03, -1.37579041e+00, -3.26634345e+00,  4.52386826e+00]), array([-0.64845831, -0.3262826 , -3.14437181,  5.70653677]), array([-1.18156559,  0.73644069, -2.04149289,  4.61198482]), array([-1.43891006,  1.48273638, -0.51845396,  2.87187359]), array([-1.39705371,  1.91565844,  0.93266022,  1.4357822 ]), array([-1.0610939 ,  1.99652701,  2.37309493, -0.67168517]), array([-0.47937828,  1.629154  ,  3.3488345 , -3.03175507]), array([ 0.23939097,  0.78756108,  3.74754119, -5.27634227]), array([ 0.96283039, -0.35020337,  3.29305062, -5.62408281]), array([ 1.49370106, -1.32158779,  1.96393525, -4.03054044]), array([ 1.74625394, -1.98751725,  0.56334834, -2.68360389]), array([ 1.72016195, -2.40127005, -0.81828069, -1.43588525]), array([ 1.41121354, -2.5062241 , -2.24702907,  0.43138093]), array([ 0.8384986 , -2.20806705, -3.40454144,  2.60795357]), array([ 0.09850298, -1.46564545, -3.89729261,  4.82694953]), array([-0.69788874, -0.28239687, -3.9433392 ,  6.69129385]), array([-1.38810126,  0.97748462, -2.78859685,  5.51822654]), array([-1.78532508,  1.88454087, -1.20076109,  3.66508461]), array([-1.88223908,  2.49399403,  0.21721324,  2.44239267]), array([-1.7057045 ,  2.85449813,  1.53122097,  1.13523015]), array([-1.26360452,  2.89958921,  2.86694628, -0.69803946]), array([-0.58054882,  2.57214757,  3.85530788, -2.58474841]), array([ 0.21532369,  1.86549206,  3.95551354, -4.45832935]), array([ 0.96474895,  0.81632834,  3.49740336, -5.89521597]), array([ 1.58316272, -0.380222  ,  2.56280451, -5.73669851]), array([ 1.9485309 , -1.39880065,  1.04720182, -4.43458762]), array([ 1.99237196, -2.16401552, -0.62135983, -3.20526667]), array([ 1.70396854, -2.6624594 , -2.2308583 , -1.72528494]), array([ 1.1059387 , -2.80029995, -3.68654804,  0.35489071]), array([ 0.27542422, -2.54688648, -4.46004446,  2.13964667]), array([-0.60270668, -1.95219673, -4.14132328,  3.69696776]), array([-1.33795282, -1.12778732, -3.1777561 ,  4.3843711 ]), array([-1.86085846, -0.29090759, -2.04669902,  3.86040242]), array([-2.15735819,  0.39641118, -0.92704108,  3.02620404]), array([-2.24389637,  0.96266507,  0.08770946,  2.62823242]), array([-2.09337458,  1.39909025,  1.47081301,  1.64108863]), array([-1.62845299,  1.53653395,  3.19423892, -0.44819847]), array([-0.82629156,  1.14207127,  4.75763928, -3.64481898]), array([ 0.22622666,  0.09370999,  5.53866558, -6.32684284]), array([ 1.26063368, -1.03973841,  4.59883988, -4.49401228]), array([ 2.05259207, -1.70124448,  3.35562003, -2.32289283]), array([ 2.62792089, -2.05670922,  2.47888167, -1.42594173]), array([ 3.07929141, -2.33317559,  2.12820003, -1.46320977]), array([-2.76739779, -2.68055692,  2.33312697, -2.09357793]), array([-2.23246175,  3.08199879,  3.10778701, -3.20669191]), array([-1.49779384,  2.2654648 ,  4.26677575, -5.17967892]), array([-0.51635732,  0.88669341,  5.60122974, -8.86774683]), array([ 0.6464256 , -1.01021262,  5.57653688, -8.83057457]), array([ 1.63470794, -2.42603901,  4.360252  , -5.63268224]), array([ 2.40265605,  2.88982737,  3.36868364, -4.27522617]), array([ 3.0210953 ,  2.08438131,  2.94516858, -3.90780796]), array([-2.65069699,  1.27087942,  3.30760697, -4.41080695]), array([-1.88320914,  0.23616468,  4.47582695, -6.04138734]), array([-0.86503288, -1.03731864,  5.59784792, -6.11399131]), array([ 0.30971031, -2.00316005,  5.95960078, -3.25390128]), array([ 1.41184905, -2.30960069,  4.81360288,  0.13396842]), array([ 2.17273047, -2.00010645,  2.72333081,  2.78697257]), array([ 2.48388557, -1.22026514,  0.44198068,  4.8787107 ]), array([ 2.40749461, -0.11499328, -1.04178058,  6.05524941])]</t>
+  </si>
+  <si>
+    <t>['[2,0,1]', '[2,1,0]', '[0,2,1]', '[1,2,0]', '[1,1,2]', '[1,0,2]', '[0,0,0]', '[2,2,2]', '[0,1,1]', '[1,1,1]']</t>
+  </si>
+  <si>
+    <t>[6, 7, 8, 9, 10, 11, 19, 20, 22, 23, 30, 31, 32, 33, 34, 41, 42, 43, 44, 45, 47, 54, 55, 56, 57, 59, 68, 69, 71, 73, 74, 82, 83, 84, 85, 86, 87, 88, 89, 97, 99, 101, 102, 103, 104, 105, 114, 115, 117, 118, 119]</t>
+  </si>
+  <si>
+    <t>[0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 1, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 1, 2, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+  </si>
+  <si>
+    <t>['[-0.03763371 -0.01533471  0.06554052 -0.01816017]', '[-0.00754409 -0.05458322  0.2277812  -0.36241836]', '[ 0.04879627 -0.15231473  0.32089719 -0.5887683 ]', '[ 0.11397169 -0.27767857  0.31375488 -0.63332862]', '[ 0.16759438 -0.39312519  0.2086893  -0.49480525]', '[ 0.1930193  -0.46685036  0.03906408 -0.22816919]', '[ 0.16956871 -0.44830261 -0.26820417  0.40739083]', '[ 0.09055011 -0.31127879 -0.50323119  0.93116007]', '[-0.02165415 -0.09380121 -0.58952709  1.1892161 ]', '[-0.13228272  0.13968862 -0.48657385  1.08703787]', '[-0.20542731  0.31962025 -0.22562708  0.67289162]', '[-0.21756752  0.39782756  0.10766541  0.09689063]', '[-0.15109606  0.32490126  0.54216963 -0.80657469]', '[-0.01068619  0.09081112  0.82714324 -1.47439182]', '[ 0.16212513 -0.23279107  0.85391345 -1.67375883]', '[ 0.3120332  -0.54339537  0.60708552 -1.36152952]', '[ 0.39322683 -0.75586146  0.18779451 -0.73014827]', '[ 0.38412465 -0.82793881 -0.27624305  0.01454459]', '[ 0.26384544 -0.69033685 -0.90484238  1.34113963]', '[ 0.04812306 -0.34154272 -1.20443244  2.06892924]', '[-0.19334691  0.0931444  -1.14461952  2.15461365]', '[-0.39695754  0.5053154  -0.8375582   1.86591421]', '[-0.49989841  0.77779812 -0.17339874  0.82423532]', '[-0.46447437  0.82889034  0.51931751 -0.31386703]', '[-0.28805572  0.62547325  1.21365089 -1.69091958]', '[ 2.21524878e-03  1.77421278e-01  1.62247552e+00 -2.67839388e+00]', '[ 0.32582768 -0.38073979  1.52349886 -2.7322232 ]', '[ 0.57960549 -0.85729663  0.96089882 -1.94671753]', '[ 0.69692098 -1.14155954  0.19699003 -0.87752907]', '[ 0.63713961 -1.14984138 -0.7822067   0.79415754]', '[ 0.40350114 -0.85357079 -1.51951514  2.14628853]', '[ 0.0501135  -0.31521661 -1.93860578  3.11442572]', '[-0.33056178  0.31470881 -1.76154814  2.97926903]', '[-0.61806588  0.80981738 -1.0569195   1.88375576]', '[-0.74035324  1.05347358 -0.15209565  0.54215003]', '[-0.66753519  0.99656421  0.86977043 -1.11174267]', '[-0.40101507  0.61047269  1.75705196 -2.71558197]', '[ 0.0081067  -0.04906218  2.2282976  -3.68199244]', '[ 0.43718034 -0.75693977  1.95050409 -3.18592549]', '[ 0.75703577 -1.27506064  1.20325425 -1.95474765]', '[ 0.90754287 -1.53690554  0.28747381 -0.66869583]', '[ 0.86151228 -1.51877561 -0.74069232  0.85302859]', '[ 0.61777583 -1.19130089 -1.67087853  2.43086559]', '[ 0.20881993 -0.55167387 -2.35332279  3.88122985]', '[-0.27783307  0.27614635 -2.36622764  4.09713916]', '[-0.68284965  0.97840237 -1.60389079  2.79444328]', '[-0.91311699  1.40754377 -0.67518083  1.49202968]', '[-0.93973981  1.55204259  0.40576228 -0.04284332]', '[-0.74693779  1.36218166  1.5007336  -1.87378421]', '[-0.35130105  0.79497482  2.41218815 -3.78177945]', '[ 0.18426765 -0.09910264  2.79486401 -4.85689386]', '[ 0.69364916 -0.99404855  2.1737503  -3.85549868]', '[ 1.02859766 -1.61250432  1.14851234 -2.33973481]', '[ 1.14746823 -1.94012038  0.03570949 -0.95207706]', '[ 1.03761021 -1.9717987  -1.11615736  0.64469965]', '[ 0.71311577 -1.6740905  -2.08754988  2.35731299]', '[ 0.22240169 -1.02116436 -2.76446618  4.15447474]', '[-0.35834304 -0.06358177 -2.89563194  5.11257482]', '[-0.87280665  0.89269674 -2.11196825  4.17935867]', '[-1.16716344  1.54795668 -0.81841606  2.40054968]', '[-1.20808324  1.88853816  0.40553842  1.0089592 ]', '[-0.99662209  1.90165792  1.67427933 -0.89968019]', '[-0.55786673  1.51574645  2.65623412 -2.99151378]', '[ 0.04159478  0.70087751  3.2656337  -5.078329  ]', '[ 0.69178386 -0.39687841  3.03461015 -5.44337939]', '[ 1.18696352 -1.33369127  1.84894895 -3.83711418]', '[ 1.42418721 -1.94673044  0.519335   -2.33715132]', '[ 1.39560508 -2.27576951 -0.79557963 -0.94675212]', '[ 1.10751477 -2.29608582 -2.0480961   0.77064116]', '[ 0.6000502  -1.95605103 -2.94582027  2.65361326]', '[-0.04245381 -1.20680426 -3.40674196  4.82263411]', '[-0.71889294 -0.11100349 -3.20976787  5.78090413]', '[-1.26076989  0.9563431  -2.07932196  4.63297313]', '[-1.52193826  1.70080611 -0.53110756  2.8634779 ]', '[-1.47576238  2.112079    0.97932663  1.23796727]', '[-1.13393269  2.16038951  2.39207953 -0.800678  ]', '[-0.54754549  1.77238546  3.38070347 -3.12090823]', '[ 0.18061411  0.90645416  3.82066635 -5.47163055]', '[ 0.9297066  -0.29975106  3.46559557 -6.07871698]', '[ 1.49271133 -1.35546165  2.10159223 -4.39395706]', '[ 1.76891313 -2.0864227   0.6663522  -2.98258977]', '[ 1.7625886  -2.5580326  -0.71725849 -1.72280998]', '[ 1.4759997  -2.72449106 -2.12874348  0.08926591]', '[ 0.92924487 -2.5295158  -3.2769024   1.89210972]', '[ 0.20824954 -1.95750792 -3.80228109  3.83687643]', '[-0.54506888 -1.00854805 -3.65518702  5.54267162]', '[-1.21565058  0.15144053 -2.90371     5.66139458]', '[-1.65184226  1.13093911 -1.40486731  4.06210458]', '[-1.77303636  1.79086665  0.19713705  2.55733862]', '[-1.57301089  2.14389385  1.79101969  0.91321893]', '[-1.06330837  2.10465792  3.23976979 -1.38349977]', '[-0.31797111  1.56389794  4.09755593 -4.06120562]', '[ 0.53345981  0.49636513  4.30270594 -6.37188791]', '[ 1.32051783 -0.76030984  3.37412457 -5.69474458]', '[ 1.85295689 -1.72244486  1.96178544 -4.02280532]', '[ 2.11401903 -2.41291513  0.67054555 -2.94215889]', '[ 2.1305447  -2.90439876 -0.48128614 -1.95652131]', '[ 1.91512372  3.13873233 -1.67643365 -0.41336355]', '[ 1.45309519 -3.05879714 -2.95391865  1.29360127]', '[ 0.74980428 -2.63571158 -3.99009474  2.97725127]', '[-0.08939105 -1.83015389 -4.25897677  5.10773867]', '[-0.91074029 -0.6325607  -3.893107    6.66900415]', '[-1.58744136  0.65625266 -2.71300961  5.80854488]', '[-1.96654719  1.64291079 -1.07726805  4.13203396]', '[-2.02121679  2.33414066  0.51863898  2.78665988]', '[-1.76714328  2.74405831  1.99840012  1.26515991]', '[-1.22491218  2.80382912  3.38862967 -0.69646993]', '[-0.44194303  2.45839838  4.30252368 -2.76895975]', '[ 0.42275727  1.70145291  4.19459836 -4.74406778]', '[ 1.20437865  0.60768485  3.58073877 -5.99141186]', '[ 1.82157537 -0.56680573  2.49520795 -5.48182334]', '[ 2.18031417 -1.54898328  1.07534611 -4.38009833]', '[ 2.24610516 -2.33324409 -0.42125282 -3.45406292]', '[ 2.02021944 -2.91435806 -1.79761319 -2.31134955]', '[ 1.53493966  3.05619679 -3.0360293  -0.82118618]', '[ 0.81378366  3.0211867  -4.1226503   0.37303977]', '[-0.07609906 -3.11049058 -4.61664502  0.98657122]', '[-0.95468444 -2.94674187 -4.02301197  0.50791904]', '[-1.65056158 -2.95339413 -2.90657936 -0.65374412]', '[-2.11899577  3.0611325  -1.78373285 -2.02802642]', '[-2.35101655  2.51127207 -0.4922312  -3.42911475]', '[-2.29545138  1.70061587  1.07978767 -4.69409875]', '[-1.91053859  0.59900183  2.7806579  -6.43377956]', '[-1.2109645  -0.82866562  4.05455256 -7.41659437]', '[-0.32733182 -2.21062717  4.77287782 -6.28640337]', '[ 0.65280535  2.91149312  4.77865296 -5.49898659]', '[ 1.49856648  1.8178976   3.63124669 -5.48382219]', '[ 2.12817772  0.72347486  2.73679312 -5.43261633]']</t>
+  </si>
+  <si>
+    <t>[0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50, 51, 52, 53, 54, 55, 56, 57, 58, 59, 60, 61, 62, 63, 64, 65, 66, 67, 68, 69, 70, 71, 72, 73, 74, 75, 76, 77, 78, 79, 80, 81, 82, 83, 84, 85, 86, 87, 88, 89, 90, 91, 92, 93, 94, 95, 96, 97, 98, 99, 100, 101, 102, 103, 104, 105, 106, 107, 108, 109, 110, 111, 112, 113, 114, 115, 116, 117, 118, 119, 120, 121, 122, 123, 124, 125, 126, 127]</t>
+  </si>
+  <si>
+    <t>[array([-0.03763371, -0.01533471,  0.06554052, -0.01816017], dtype=float32), array([-0.00754409, -0.05458322,  0.2277812 , -0.36241836]), array([ 0.04879627, -0.15231473,  0.32089719, -0.5887683 ]), array([ 0.11397169, -0.27767857,  0.31375488, -0.63332862]), array([ 0.16759438, -0.39312519,  0.2086893 , -0.49480525]), array([ 0.1930193 , -0.46685036,  0.03906408, -0.22816919]), array([ 0.16956871, -0.44830261, -0.26820417,  0.40739083]), array([ 0.09055011, -0.31127879, -0.50323119,  0.93116007]), array([-0.02165415, -0.09380121, -0.58952709,  1.1892161 ]), array([-0.13228272,  0.13968862, -0.48657385,  1.08703787]), array([-0.20542731,  0.31962025, -0.22562708,  0.67289162]), array([-0.21756752,  0.39782756,  0.10766541,  0.09689063]), array([-0.15109606,  0.32490126,  0.54216963, -0.80657469]), array([-0.01068619,  0.09081112,  0.82714324, -1.47439182]), array([ 0.16212513, -0.23279107,  0.85391345, -1.67375883]), array([ 0.3120332 , -0.54339537,  0.60708552, -1.36152952]), array([ 0.39322683, -0.75586146,  0.18779451, -0.73014827]), array([ 0.38412465, -0.82793881, -0.27624305,  0.01454459]), array([ 0.26384544, -0.69033685, -0.90484238,  1.34113963]), array([ 0.04812306, -0.34154272, -1.20443244,  2.06892924]), array([-0.19334691,  0.0931444 , -1.14461952,  2.15461365]), array([-0.39695754,  0.5053154 , -0.8375582 ,  1.86591421]), array([-0.49989841,  0.77779812, -0.17339874,  0.82423532]), array([-0.46447437,  0.82889034,  0.51931751, -0.31386703]), array([-0.28805572,  0.62547325,  1.21365089, -1.69091958]), array([ 2.21524878e-03,  1.77421278e-01,  1.62247552e+00, -2.67839388e+00]), array([ 0.32582768, -0.38073979,  1.52349886, -2.7322232 ]), array([ 0.57960549, -0.85729663,  0.96089882, -1.94671753]), array([ 0.69692098, -1.14155954,  0.19699003, -0.87752907]), array([ 0.63713961, -1.14984138, -0.7822067 ,  0.79415754]), array([ 0.40350114, -0.85357079, -1.51951514,  2.14628853]), array([ 0.0501135 , -0.31521661, -1.93860578,  3.11442572]), array([-0.33056178,  0.31470881, -1.76154814,  2.97926903]), array([-0.61806588,  0.80981738, -1.0569195 ,  1.88375576]), array([-0.74035324,  1.05347358, -0.15209565,  0.54215003]), array([-0.66753519,  0.99656421,  0.86977043, -1.11174267]), array([-0.40101507,  0.61047269,  1.75705196, -2.71558197]), array([ 0.0081067 , -0.04906218,  2.2282976 , -3.68199244]), array([ 0.43718034, -0.75693977,  1.95050409, -3.18592549]), array([ 0.75703577, -1.27506064,  1.20325425, -1.95474765]), array([ 0.90754287, -1.53690554,  0.28747381, -0.66869583]), array([ 0.86151228, -1.51877561, -0.74069232,  0.85302859]), array([ 0.61777583, -1.19130089, -1.67087853,  2.43086559]), array([ 0.20881993, -0.55167387, -2.35332279,  3.88122985]), array([-0.27783307,  0.27614635, -2.36622764,  4.09713916]), array([-0.68284965,  0.97840237, -1.60389079,  2.79444328]), array([-0.91311699,  1.40754377, -0.67518083,  1.49202968]), array([-0.93973981,  1.55204259,  0.40576228, -0.04284332]), array([-0.74693779,  1.36218166,  1.5007336 , -1.87378421]), array([-0.35130105,  0.79497482,  2.41218815, -3.78177945]), array([ 0.18426765, -0.09910264,  2.79486401, -4.85689386]), array([ 0.69364916, -0.99404855,  2.1737503 , -3.85549868]), array([ 1.02859766, -1.61250432,  1.14851234, -2.33973481]), array([ 1.14746823, -1.94012038,  0.03570949, -0.95207706]), array([ 1.03761021, -1.9717987 , -1.11615736,  0.64469965]), array([ 0.71311577, -1.6740905 , -2.08754988,  2.35731299]), array([ 0.22240169, -1.02116436, -2.76446618,  4.15447474]), array([-0.35834304, -0.06358177, -2.89563194,  5.11257482]), array([-0.87280665,  0.89269674, -2.11196825,  4.17935867]), array([-1.16716344,  1.54795668, -0.81841606,  2.40054968]), array([-1.20808324,  1.88853816,  0.40553842,  1.0089592 ]), array([-0.99662209,  1.90165792,  1.67427933, -0.89968019]), array([-0.55786673,  1.51574645,  2.65623412, -2.99151378]), array([ 0.04159478,  0.70087751,  3.2656337 , -5.078329  ]), array([ 0.69178386, -0.39687841,  3.03461015, -5.44337939]), array([ 1.18696352, -1.33369127,  1.84894895, -3.83711418]), array([ 1.42418721, -1.94673044,  0.519335  , -2.33715132]), array([ 1.39560508, -2.27576951, -0.79557963, -0.94675212]), array([ 1.10751477, -2.29608582, -2.0480961 ,  0.77064116]), array([ 0.6000502 , -1.95605103, -2.94582027,  2.65361326]), array([-0.04245381, -1.20680426, -3.40674196,  4.82263411]), array([-0.71889294, -0.11100349, -3.20976787,  5.78090413]), array([-1.26076989,  0.9563431 , -2.07932196,  4.63297313]), array([-1.52193826,  1.70080611, -0.53110756,  2.8634779 ]), array([-1.47576238,  2.112079  ,  0.97932663,  1.23796727]), array([-1.13393269,  2.16038951,  2.39207953, -0.800678  ]), array([-0.54754549,  1.77238546,  3.38070347, -3.12090823]), array([ 0.18061411,  0.90645416,  3.82066635, -5.47163055]), array([ 0.9297066 , -0.29975106,  3.46559557, -6.07871698]), array([ 1.49271133, -1.35546165,  2.10159223, -4.39395706]), array([ 1.76891313, -2.0864227 ,  0.6663522 , -2.98258977]), array([ 1.7625886 , -2.5580326 , -0.71725849, -1.72280998]), array([ 1.4759997 , -2.72449106, -2.12874348,  0.08926591]), array([ 0.92924487, -2.5295158 , -3.2769024 ,  1.89210972]), array([ 0.20824954, -1.95750792, -3.80228109,  3.83687643]), array([-0.54506888, -1.00854805, -3.65518702,  5.54267162]), array([-1.21565058,  0.15144053, -2.90371   ,  5.66139458]), array([-1.65184226,  1.13093911, -1.40486731,  4.06210458]), array([-1.77303636,  1.79086665,  0.19713705,  2.55733862]), array([-1.57301089,  2.14389385,  1.79101969,  0.91321893]), array([-1.06330837,  2.10465792,  3.23976979, -1.38349977]), array([-0.31797111,  1.56389794,  4.09755593, -4.06120562]), array([ 0.53345981,  0.49636513,  4.30270594, -6.37188791]), array([ 1.32051783, -0.76030984,  3.37412457, -5.69474458]), array([ 1.85295689, -1.72244486,  1.96178544, -4.02280532]), array([ 2.11401903, -2.41291513,  0.67054555, -2.94215889]), array([ 2.1305447 , -2.90439876, -0.48128614, -1.95652131]), array([ 1.91512372,  3.13873233, -1.67643365, -0.41336355]), array([ 1.45309519, -3.05879714, -2.95391865,  1.29360127]), array([ 0.74980428, -2.63571158, -3.99009474,  2.97725127]), array([-0.08939105, -1.83015389, -4.25897677,  5.10773867]), array([-0.91074029, -0.6325607 , -3.893107  ,  6.66900415]), array([-1.58744136,  0.65625266, -2.71300961,  5.80854488]), array([-1.96654719,  1.64291079, -1.07726805,  4.13203396]), array([-2.02121679,  2.33414066,  0.51863898,  2.78665988]), array([-1.76714328,  2.74405831,  1.99840012,  1.26515991]), array([-1.22491218,  2.80382912,  3.38862967, -0.69646993]), array([-0.44194303,  2.45839838,  4.30252368, -2.76895975]), array([ 0.42275727,  1.70145291,  4.19459836, -4.74406778]), array([ 1.20437865,  0.60768485,  3.58073877, -5.99141186]), array([ 1.82157537, -0.56680573,  2.49520795, -5.48182334]), array([ 2.18031417, -1.54898328,  1.07534611, -4.38009833]), array([ 2.24610516, -2.33324409, -0.42125282, -3.45406292]), array([ 2.02021944, -2.91435806, -1.79761319, -2.31134955]), array([ 1.53493966,  3.05619679, -3.0360293 , -0.82118618]), array([ 0.81378366,  3.0211867 , -4.1226503 ,  0.37303977]), array([-0.07609906, -3.11049058, -4.61664502,  0.98657122]), array([-0.95468444, -2.94674187, -4.02301197,  0.50791904]), array([-1.65056158, -2.95339413, -2.90657936, -0.65374412]), array([-2.11899577,  3.0611325 , -1.78373285, -2.02802642]), array([-2.35101655,  2.51127207, -0.4922312 , -3.42911475]), array([-2.29545138,  1.70061587,  1.07978767, -4.69409875]), array([-1.91053859,  0.59900183,  2.7806579 , -6.43377956]), array([-1.2109645 , -0.82866562,  4.05455256, -7.41659437]), array([-0.32733182, -2.21062717,  4.77287782, -6.28640337]), array([ 0.65280535,  2.91149312,  4.77865296, -5.49898659]), array([ 1.49856648,  1.8178976 ,  3.63124669, -5.48382219]), array([ 2.12817772,  0.72347486,  2.73679312, -5.43261633])]</t>
+  </si>
+  <si>
+    <t>['[2,1,0]', '[2,0,1]', '[1,0,2]', '[0,2,1]', '[0,1,1]', '[0,0,0]', '[1,2,0]', '[2,2,2]', '[1,1,1]', '[1,1,2]']</t>
+  </si>
+  <si>
+    <t>[6, 7, 8, 9, 10, 11, 18, 19, 20, 21, 22, 23, 29, 30, 31, 32, 33, 34, 41, 42, 43, 44, 45, 46, 47, 54, 55, 56, 57, 58, 59, 60, 67, 68, 69, 70, 71, 72, 73, 81, 82, 83, 84, 85, 86, 87, 95, 96, 97, 98, 99, 100, 101, 102, 110, 111, 112, 113, 114, 115, 116, 117, 131, 132, 133, 134, 135, 136, 137, 138, 139, 140, 141, 142, 157, 158, 159]</t>
+  </si>
+  <si>
+    <t>[0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 1, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 1, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 1, 1, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2]</t>
+  </si>
+  <si>
+    <t>['[-0.03763371 -0.01533471  0.06554052 -0.01816017]', '[-0.00754409 -0.05458322  0.2277812  -0.36241836]', '[ 0.04879627 -0.15231473  0.32089719 -0.5887683 ]', '[ 0.11397169 -0.27767857  0.31375488 -0.63332862]', '[ 0.16759438 -0.39312519  0.2086893  -0.49480525]', '[ 0.1930193  -0.46685036  0.03906408 -0.22816919]', '[ 0.16956871 -0.44830261 -0.26820417  0.40739083]', '[ 0.09055011 -0.31127879 -0.50323119  0.93116007]', '[-0.02165415 -0.09380121 -0.58952709  1.1892161 ]', '[-0.13228272  0.13968862 -0.48657385  1.08703787]', '[-0.20542731  0.31962025 -0.22562708  0.67289162]', '[-0.21756752  0.39782756  0.10766541  0.09689063]', '[-0.15109606  0.32490126  0.54216963 -0.80657469]', '[-0.01068619  0.09081112  0.82714324 -1.47439182]', '[ 0.16212513 -0.23279107  0.85391345 -1.67375883]', '[ 0.3120332  -0.54339537  0.60708552 -1.36152952]', '[ 0.39322683 -0.75586146  0.18779451 -0.73014827]', '[ 0.38412465 -0.82793881 -0.27624305  0.01454459]', '[ 0.27552572 -0.72135137 -0.78884754  1.03160865]', '[ 0.08086773 -0.43032213 -1.11647003  1.81675029]', '[-0.14966877 -0.03109877 -1.12879696  2.06540623]', '[-0.3455444   0.34863759 -0.7784691   1.63534647]', '[-0.44544803  0.59424237 -0.19906427  0.77949316]', '[-0.4218337   0.6519398   0.43007126 -0.20572333]', '[-0.26769146  0.484052    1.08142007 -1.44055859]', '[-0.00742761  0.10113176  1.45927884 -2.28595201]', '[ 0.28490347 -0.37428385  1.38589424 -2.32532176]', '[ 0.5187101  -0.77937684  0.90230152 -1.64619583]', '[ 0.63240836 -1.01433747  0.21740989 -0.68198512]', '[ 0.59278756 -1.01958166 -0.60566507  0.62852481]', '[ 0.39752784 -0.7660208  -1.31595743  1.88179849]', '[ 0.08542661 -0.29020757 -1.73661998  2.76615566]', '[-0.26054486  0.27360101 -1.62803895  2.69265107]', '[-0.53183224  0.72525907 -1.02799868  1.73308445]', '[-0.65747495  0.94866122 -0.21116234  0.48419472]', '[-0.60316944  0.88713812  0.74646124 -1.09703619]', '[-0.3667148   0.51448679  1.5802398  -2.58584684]', '[ 2.25515542e-03 -1.04226788e-01  2.01052042e+00 -3.41515113e+00]', '[ 0.38981745 -0.75816996  1.76540261 -2.93947302]', '[ 0.67971886 -1.23563438  1.09061136 -1.79181237]', '[ 0.81522073 -1.47040276  0.25012952 -0.55613563]', '[ 0.76893557 -1.43299403 -0.70634091  0.93217091]', '[ 0.53890731 -1.09497955 -1.5685075   2.44803386]', '[ 0.15769536 -0.46498696 -2.17507038  3.75054866]', '[-0.28566374  0.31885175 -2.12308403  3.81427092]', '[-0.64333931  0.96714913 -1.38377582  2.55626676]', '[-0.82476188  1.32821982 -0.41497441  1.0541805 ]', '[-0.80769438  1.39053182  0.57925977 -0.43113385]', '[-0.58966747  1.12643161  1.57705339 -2.21920745]', '[-0.19115743  0.50615398  2.34648211 -3.90612928]', '[ 0.30339761 -0.35080814  2.44609663 -4.34908803]', '[ 0.72926902 -1.11787821  1.72849028 -3.18529002]', '[ 0.97784646 -1.61271142  0.7372731  -1.77273591]', '[ 1.02063975 -1.83229792 -0.30765192 -0.42827287]', '[ 0.8520877  -1.75909807 -1.35222299  1.17222519]', '[ 0.49438686 -1.35658722 -2.18080855  2.86380021]', '[ 1.00762334e-03 -6.20843848e-01 -2.67811907e+00  4.39175692e+00]', '[-0.52543841  0.29807699 -2.42518508  4.45563686]', '[-0.91358233  1.05045396 -1.38833549  2.96371659]', '[-1.07068508  1.48053778 -0.17760768  1.35120727]', '[-0.98698022  1.59293246  0.99771813 -0.2363293 ]', '[-0.67458429  1.35277557  2.08591422 -2.1902737 ]', '[-0.17257945  0.7121893   2.86826583 -4.16299452]', '[ 0.42654616 -0.22986762  2.95103072 -4.89035041]', '[ 0.93778312 -1.09635369  2.06289939 -3.60682875]', '[ 1.23512506 -1.66554553  0.89403237 -2.11536181]', '[ 1.2925874  -1.95282627 -0.31874559 -0.76398106]', '[ 1.10434513 -1.94410117 -1.53992148  0.87663865]', '[ 0.69181453 -1.5878337  -2.53506175  2.72222862]', '[ 0.1141862  -0.84811196 -3.17077399  4.62247333]', '[-0.52819058  0.17080839 -3.07026003  5.16081708]', '[-1.04130142  1.05893    -1.96969821  3.56491538]', '[-1.30452454  1.59874429 -0.65598023  1.87444291]', '[-1.30385453  1.81885452  0.65610727  0.32547074]', '[-1.0405206   1.6957045   1.9492216  -1.60077881]', '[-0.53981694  1.15624497  3.01179277 -3.83696118]', '[ 0.1372115   0.17699716  3.62003771 -5.68231063]', '[ 0.81714379 -0.90901082  2.9941466  -4.77727736]', '[ 1.30077933 -1.68444311  1.81783839 -3.01937746]', '[ 1.54044333 -2.14395201  0.57410527 -1.62162767]', '[ 1.53015478 -2.34022436 -0.67386049 -0.3349864 ]', '[ 1.26794035 -2.24754766 -1.92783573  1.30056457]', '[ 0.77398019 -1.79920792 -2.95822207  3.24300749]', '[ 0.10912329 -0.93053956 -3.62675865  5.42116516]', '[-0.62545765  0.26611029 -3.49608951  6.01988262]', '[-1.20465197  1.28709304 -2.21592237  4.06698629]', '[-1.50797598  1.91807846 -0.82066615  2.31676317]', '[-1.53477864  2.2293726   0.54577611  0.80013611]', '[-1.2877879   2.20842304  1.90129391 -1.04971139]', '[-0.78963194  1.78691254  3.02687444 -3.23448346]', '[-0.10030915  0.88843882  3.80956796 -5.74461357]', '[ 0.6800303  -0.39674343  3.7435005  -6.50465385]', '[ 1.30715153 -1.50997221  2.45867409 -4.5409428 ]', '[ 1.66295011 -2.25180565  1.10659453 -2.9676307 ]', '[ 1.75378095 -2.71564871 -0.18565107 -1.68161197]', '[ 1.5813519  -2.88137073 -1.52983951  0.04045167]', '[ 1.1519438  -2.7111456  -2.73434768  1.6862411 ]', '[ 0.51469557 -2.19454948 -3.53385774  3.51577218]', '[-0.21605975 -1.29637768 -3.69530472  5.44381948]', '[-0.93347479 -0.07890334 -3.33155425  6.34278847]', '[-1.46815164  1.04914056 -1.90369944  4.72496493]', '[-1.68504663  1.8186261  -0.26686772  3.02286773]', '[-1.57790214  2.26289729  1.32157282  1.3925168 ]', '[-1.16230252  2.33628647  2.78098167 -0.70872357]', '[-0.49937378  1.96104263  3.73305796 -3.07862305]', '[ 0.28168801  1.10328838  3.98778248 -5.43912807]', '[ 1.05641581 -0.12139406  3.58807581 -6.33965149]', '[ 1.64197964 -1.24799698  2.19153353 -4.79346573]', '[ 1.93110596 -2.06554328  0.70796954 -3.45572032]', '[ 1.9298668  -2.64055422 -0.70059025 -2.28138   ]', '[ 1.64798507 -2.92647169 -2.10001467 -0.54933263]', '[ 1.10113438 -2.87141254 -3.33487859  1.1106115 ]', '[ 0.34697668 -2.48153264 -4.06563526  2.78224148]', '[-0.45449675 -1.77188397 -3.80453306  4.23624619]', '[-1.14036848 -0.83961199 -3.00985396  4.9119112 ]', '[-1.63827553  0.10748742 -1.91032936  4.37331902]', '[-1.88581424  0.8697594  -0.53732323  3.22693025]', '[-1.84250576  1.39232548  1.00128781  1.94585667]', '[-1.46792407  1.58397786  2.73695626 -0.1591014 ]', '[-0.76574103  1.27166851  4.20293413 -3.0762577 ]', '[ 0.16720186  0.35309345  4.95605261 -5.8105889 ]', '[ 1.11001304 -0.78239843  4.24571007 -4.96871473]', '[ 1.83243961 -1.56549641  2.99112398 -2.9780063 ]', '[ 2.32227254 -2.04212274  1.95471592 -1.9392754 ]', '[ 2.63327895 -2.38572334  1.20117266 -1.57380137]', '[ 2.81833741 -2.69021329  0.68507069 -1.49642129]', '[ 2.91927563 -2.98722699  0.35267656 -1.47057386]', '[ 2.96921892  3.00967473  0.1693663  -1.37645824]', '[ 2.99422643  2.75310207  0.09508466 -1.17065374]', '[ 3.01106998  2.54879278  0.07969731 -0.85696437]', '[ 3.02756577  2.41548615  0.08795807 -0.46735169]', '[ 3.03377925  2.40510353 -0.02459955  0.36300865]', '[ 3.01827787  2.5577791  -0.13006699  1.14990759]', '[ 2.9864113   2.83764122 -0.1997427   1.62844096]', '[ 2.93073389 -3.08293415 -0.38523736  1.97693621]', '[ 2.81830541 -2.66191764 -0.77868654  2.22498429]', '[ 2.60316735 -2.19099131 -1.41413499  2.51324944]', '[ 2.23515129 -1.63261367 -2.31658838  3.17520518]', '[ 1.65288255 -0.8611259  -3.56832895  4.70760047]', '[ 0.8015193   0.26241492 -4.82676116  6.16024713]', '[-0.19149596  1.34193963 -4.91208833  4.16421567]', '[-1.0982578   1.85892141 -3.98458959  1.00780127]', '[-1.72830921  1.78285216 -2.23609115 -1.62970826]', '[-1.97371022  1.23925332 -0.22988789 -3.70518026]', '[-1.83583303  0.3201441   1.54885412 -5.45056978]', '[-1.395785   -0.885842    2.72841253 -6.36930281]', '[-0.77045381 -2.15027896  3.53177566 -6.22290519]', '[ 4.95699164e-03  2.88670206e+00  4.07794122e+00 -6.38852897e+00]', '[ 0.79647085  1.50207057  3.81763177 -7.63972274]', '[ 1.53948774 -0.17230282  3.41042481 -8.62058517]', '[ 2.02871491 -1.70080075  1.3321221  -6.53848522]', '[ 2.07921905 -2.84284003 -0.69206813 -4.97970055]', '[ 1.8356673   2.56044989 -1.55110255 -3.92136947]', '[ 1.50268517  1.81961282 -1.71693449 -3.64940056]', '[ 1.1743514   1.0217513  -1.50659192 -4.51840734]', '[ 0.89517673 -0.00957279 -1.49166253 -5.48667645]', '[ 0.43439719 -0.91862526 -3.29640123 -3.12260905]', '[-0.39598026 -1.16901903 -4.71684721  0.45931427]', '[-1.32700473 -0.85921825 -4.37367202  2.2629972 ]', '[-2.10096419 -0.39503362 -3.34549019  2.17212666]']</t>
+  </si>
+  <si>
+    <t>[0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50, 51, 52, 53, 54, 55, 56, 57, 58, 59, 60, 61, 62, 63, 64, 65, 66, 67, 68, 69, 70, 71, 72, 73, 74, 75, 76, 77, 78, 79, 80, 81, 82, 83, 84, 85, 86, 87, 88, 89, 90, 91, 92, 93, 94, 95, 96, 97, 98, 99, 100, 101, 102, 103, 104, 105, 106, 107, 108, 109, 110, 111, 112, 113, 114, 115, 116, 117, 118, 119, 120, 121, 122, 123, 124, 125, 126, 127, 128, 129, 130, 131, 132, 133, 134, 135, 136, 137, 138, 139, 140, 141, 142, 143, 144, 145, 146, 147, 148, 149, 150, 151, 152, 153, 154, 155, 156, 157, 158, 159]</t>
+  </si>
+  <si>
+    <t>[array([-0.03763371, -0.01533471,  0.06554052, -0.01816017], dtype=float32), array([-0.00754409, -0.05458322,  0.2277812 , -0.36241836]), array([ 0.04879627, -0.15231473,  0.32089719, -0.5887683 ]), array([ 0.11397169, -0.27767857,  0.31375488, -0.63332862]), array([ 0.16759438, -0.39312519,  0.2086893 , -0.49480525]), array([ 0.1930193 , -0.46685036,  0.03906408, -0.22816919]), array([ 0.16956871, -0.44830261, -0.26820417,  0.40739083]), array([ 0.09055011, -0.31127879, -0.50323119,  0.93116007]), array([-0.02165415, -0.09380121, -0.58952709,  1.1892161 ]), array([-0.13228272,  0.13968862, -0.48657385,  1.08703787]), array([-0.20542731,  0.31962025, -0.22562708,  0.67289162]), array([-0.21756752,  0.39782756,  0.10766541,  0.09689063]), array([-0.15109606,  0.32490126,  0.54216963, -0.80657469]), array([-0.01068619,  0.09081112,  0.82714324, -1.47439182]), array([ 0.16212513, -0.23279107,  0.85391345, -1.67375883]), array([ 0.3120332 , -0.54339537,  0.60708552, -1.36152952]), array([ 0.39322683, -0.75586146,  0.18779451, -0.73014827]), array([ 0.38412465, -0.82793881, -0.27624305,  0.01454459]), array([ 0.27552572, -0.72135137, -0.78884754,  1.03160865]), array([ 0.08086773, -0.43032213, -1.11647003,  1.81675029]), array([-0.14966877, -0.03109877, -1.12879696,  2.06540623]), array([-0.3455444 ,  0.34863759, -0.7784691 ,  1.63534647]), array([-0.44544803,  0.59424237, -0.19906427,  0.77949316]), array([-0.4218337 ,  0.6519398 ,  0.43007126, -0.20572333]), array([-0.26769146,  0.484052  ,  1.08142007, -1.44055859]), array([-0.00742761,  0.10113176,  1.45927884, -2.28595201]), array([ 0.28490347, -0.37428385,  1.38589424, -2.32532176]), array([ 0.5187101 , -0.77937684,  0.90230152, -1.64619583]), array([ 0.63240836, -1.01433747,  0.21740989, -0.68198512]), array([ 0.59278756, -1.01958166, -0.60566507,  0.62852481]), array([ 0.39752784, -0.7660208 , -1.31595743,  1.88179849]), array([ 0.08542661, -0.29020757, -1.73661998,  2.76615566]), array([-0.26054486,  0.27360101, -1.62803895,  2.69265107]), array([-0.53183224,  0.72525907, -1.02799868,  1.73308445]), array([-0.65747495,  0.94866122, -0.21116234,  0.48419472]), array([-0.60316944,  0.88713812,  0.74646124, -1.09703619]), array([-0.3667148 ,  0.51448679,  1.5802398 , -2.58584684]), array([ 2.25515542e-03, -1.04226788e-01,  2.01052042e+00, -3.41515113e+00]), array([ 0.38981745, -0.75816996,  1.76540261, -2.93947302]), array([ 0.67971886, -1.23563438,  1.09061136, -1.79181237]), array([ 0.81522073, -1.47040276,  0.25012952, -0.55613563]), array([ 0.76893557, -1.43299403, -0.70634091,  0.93217091]), array([ 0.53890731, -1.09497955, -1.5685075 ,  2.44803386]), array([ 0.15769536, -0.46498696, -2.17507038,  3.75054866]), array([-0.28566374,  0.31885175, -2.12308403,  3.81427092]), array([-0.64333931,  0.96714913, -1.38377582,  2.55626676]), array([-0.82476188,  1.32821982, -0.41497441,  1.0541805 ]), array([-0.80769438,  1.39053182,  0.57925977, -0.43113385]), array([-0.58966747,  1.12643161,  1.57705339, -2.21920745]), array([-0.19115743,  0.50615398,  2.34648211, -3.90612928]), array([ 0.30339761, -0.35080814,  2.44609663, -4.34908803]), array([ 0.72926902, -1.11787821,  1.72849028, -3.18529002]), array([ 0.97784646, -1.61271142,  0.7372731 , -1.77273591]), array([ 1.02063975, -1.83229792, -0.30765192, -0.42827287]), array([ 0.8520877 , -1.75909807, -1.35222299,  1.17222519]), array([ 0.49438686, -1.35658722, -2.18080855,  2.86380021]), array([ 1.00762334e-03, -6.20843848e-01, -2.67811907e+00,  4.39175692e+00]), array([-0.52543841,  0.29807699, -2.42518508,  4.45563686]), array([-0.91358233,  1.05045396, -1.38833549,  2.96371659]), array([-1.07068508,  1.48053778, -0.17760768,  1.35120727]), array([-0.98698022,  1.59293246,  0.99771813, -0.2363293 ]), array([-0.67458429,  1.35277557,  2.08591422, -2.1902737 ]), array([-0.17257945,  0.7121893 ,  2.86826583, -4.16299452]), array([ 0.42654616, -0.22986762,  2.95103072, -4.89035041]), array([ 0.93778312, -1.09635369,  2.06289939, -3.60682875]), array([ 1.23512506, -1.66554553,  0.89403237, -2.11536181]), array([ 1.2925874 , -1.95282627, -0.31874559, -0.76398106]), array([ 1.10434513, -1.94410117, -1.53992148,  0.87663865]), array([ 0.69181453, -1.5878337 , -2.53506175,  2.72222862]), array([ 0.1141862 , -0.84811196, -3.17077399,  4.62247333]), array([-0.52819058,  0.17080839, -3.07026003,  5.16081708]), array([-1.04130142,  1.05893   , -1.96969821,  3.56491538]), array([-1.30452454,  1.59874429, -0.65598023,  1.87444291]), array([-1.30385453,  1.81885452,  0.65610727,  0.32547074]), array([-1.0405206 ,  1.6957045 ,  1.9492216 , -1.60077881]), array([-0.53981694,  1.15624497,  3.01179277, -3.83696118]), array([ 0.1372115 ,  0.17699716,  3.62003771, -5.68231063]), array([ 0.81714379, -0.90901082,  2.9941466 , -4.77727736]), array([ 1.30077933, -1.68444311,  1.81783839, -3.01937746]), array([ 1.54044333, -2.14395201,  0.57410527, -1.62162767]), array([ 1.53015478, -2.34022436, -0.67386049, -0.3349864 ]), array([ 1.26794035, -2.24754766, -1.92783573,  1.30056457]), array([ 0.77398019, -1.79920792, -2.95822207,  3.24300749]), array([ 0.10912329, -0.93053956, -3.62675865,  5.42116516]), array([-0.62545765,  0.26611029, -3.49608951,  6.01988262]), array([-1.20465197,  1.28709304, -2.21592237,  4.06698629]), array([-1.50797598,  1.91807846, -0.82066615,  2.31676317]), array([-1.53477864,  2.2293726 ,  0.54577611,  0.80013611]), array([-1.2877879 ,  2.20842304,  1.90129391, -1.04971139]), array([-0.78963194,  1.78691254,  3.02687444, -3.23448346]), array([-0.10030915,  0.88843882,  3.80956796, -5.74461357]), array([ 0.6800303 , -0.39674343,  3.7435005 , -6.50465385]), array([ 1.30715153, -1.50997221,  2.45867409, -4.5409428 ]), array([ 1.66295011, -2.25180565,  1.10659453, -2.9676307 ]), array([ 1.75378095, -2.71564871, -0.18565107, -1.68161197]), array([ 1.5813519 , -2.88137073, -1.52983951,  0.04045167]), array([ 1.1519438 , -2.7111456 , -2.73434768,  1.6862411 ]), array([ 0.51469557, -2.19454948, -3.53385774,  3.51577218]), array([-0.21605975, -1.29637768, -3.69530472,  5.44381948]), array([-0.93347479, -0.07890334, -3.33155425,  6.34278847]), array([-1.46815164,  1.04914056, -1.90369944,  4.72496493]), array([-1.68504663,  1.8186261 , -0.26686772,  3.02286773]), array([-1.57790214,  2.26289729,  1.32157282,  1.3925168 ]), array([-1.16230252,  2.33628647,  2.78098167, -0.70872357]), array([-0.49937378,  1.96104263,  3.73305796, -3.07862305]), array([ 0.28168801,  1.10328838,  3.98778248, -5.43912807]), array([ 1.05641581, -0.12139406,  3.58807581, -6.33965149]), array([ 1.64197964, -1.24799698,  2.19153353, -4.79346573]), array([ 1.93110596, -2.06554328,  0.70796954, -3.45572032]), array([ 1.9298668 , -2.64055422, -0.70059025, -2.28138   ]), array([ 1.64798507, -2.92647169, -2.10001467, -0.54933263]), array([ 1.10113438, -2.87141254, -3.33487859,  1.1106115 ]), array([ 0.34697668, -2.48153264, -4.06563526,  2.78224148]), array([-0.45449675, -1.77188397, -3.80453306,  4.23624619]), array([-1.14036848, -0.83961199, -3.00985396,  4.9119112 ]), array([-1.63827553,  0.10748742, -1.91032936,  4.37331902]), array([-1.88581424,  0.8697594 , -0.53732323,  3.22693025]), array([-1.84250576,  1.39232548,  1.00128781,  1.94585667]), array([-1.46792407,  1.58397786,  2.73695626, -0.1591014 ]), array([-0.76574103,  1.27166851,  4.20293413, -3.0762577 ]), array([ 0.16720186,  0.35309345,  4.95605261, -5.8105889 ]), array([ 1.11001304, -0.78239843,  4.24571007, -4.96871473]), array([ 1.83243961, -1.56549641,  2.99112398, -2.9780063 ]), array([ 2.32227254, -2.04212274,  1.95471592, -1.9392754 ]), array([ 2.63327895, -2.38572334,  1.20117266, -1.57380137]), array([ 2.81833741, -2.69021329,  0.68507069, -1.49642129]), array([ 2.91927563, -2.98722699,  0.35267656, -1.47057386]), array([ 2.96921892,  3.00967473,  0.1693663 , -1.37645824]), array([ 2.99422643,  2.75310207,  0.09508466, -1.17065374]), array([ 3.01106998,  2.54879278,  0.07969731, -0.85696437]), array([ 3.02756577,  2.41548615,  0.08795807, -0.46735169]), array([ 3.03377925,  2.40510353, -0.02459955,  0.36300865]), array([ 3.01827787,  2.5577791 , -0.13006699,  1.14990759]), array([ 2.9864113 ,  2.83764122, -0.1997427 ,  1.62844096]), array([ 2.93073389, -3.08293415, -0.38523736,  1.97693621]), array([ 2.81830541, -2.66191764, -0.77868654,  2.22498429]), array([ 2.60316735, -2.19099131, -1.41413499,  2.51324944]), array([ 2.23515129, -1.63261367, -2.31658838,  3.17520518]), array([ 1.65288255, -0.8611259 , -3.56832895,  4.70760047]), array([ 0.8015193 ,  0.26241492, -4.82676116,  6.16024713]), array([-0.19149596,  1.34193963, -4.91208833,  4.16421567]), array([-1.0982578 ,  1.85892141, -3.98458959,  1.00780127]), array([-1.72830921,  1.78285216, -2.23609115, -1.62970826]), array([-1.97371022,  1.23925332, -0.22988789, -3.70518026]), array([-1.83583303,  0.3201441 ,  1.54885412, -5.45056978]), array([-1.395785  , -0.885842  ,  2.72841253, -6.36930281]), array([-0.77045381, -2.15027896,  3.53177566, -6.22290519]), array([ 4.95699164e-03,  2.88670206e+00,  4.07794122e+00, -6.38852897e+00]), array([ 0.79647085,  1.50207057,  3.81763177, -7.63972274]), array([ 1.53948774, -0.17230282,  3.41042481, -8.62058517]), array([ 2.02871491, -1.70080075,  1.3321221 , -6.53848522]), array([ 2.07921905, -2.84284003, -0.69206813, -4.97970055]), array([ 1.8356673 ,  2.56044989, -1.55110255, -3.92136947]), array([ 1.50268517,  1.81961282, -1.71693449, -3.64940056]), array([ 1.1743514 ,  1.0217513 , -1.50659192, -4.51840734]), array([ 0.89517673, -0.00957279, -1.49166253, -5.48667645]), array([ 0.43439719, -0.91862526, -3.29640123, -3.12260905]), array([-0.39598026, -1.16901903, -4.71684721,  0.45931427]), array([-1.32700473, -0.85921825, -4.37367202,  2.2629972 ]), array([-2.10096419, -0.39503362, -3.34549019,  2.17212666])]</t>
+  </si>
+  <si>
+    <t>['[2,0,1]', '[1,0,2]', '[2,2,2]', '[0,2,1]', '[1,1,1]', '[1,2,0]', '[0,0,0]', '[1,1,2]', '[0,1,1]', '[2,1,0]']</t>
+  </si>
+  <si>
+    <t>[1,0,2]</t>
+  </si>
+  <si>
+    <t>[16, 68]</t>
+  </si>
+  <si>
+    <t>[0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 1, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 1, 0, 0, 0, 0, 0]</t>
+  </si>
+  <si>
+    <t>['[-0.03763371 -0.01533471  0.06554052 -0.01816017]', '[-0.00754409 -0.05458322  0.2277812  -0.36241836]', '[ 0.04879627 -0.15231473  0.32089719 -0.5887683 ]', '[ 0.11397169 -0.27767857  0.31375488 -0.63332862]', '[ 0.16759438 -0.39312519  0.2086893  -0.49480525]', '[ 0.1930193  -0.46685036  0.03906408 -0.22816919]', '[ 0.15689524 -0.41528579 -0.3922057   0.73207416]', '[ 0.04309269 -0.18588535 -0.71796191  1.51055937]', '[-0.1147829   0.15904975 -0.81547211  1.84906375]', '[-0.26363568  0.51494657 -0.63159042  1.62703318]', '[-0.35418658  0.78351571 -0.2539271   1.01663306]', '[-0.36122763  0.91144819  0.18313112  0.25239067]', '[-0.26190848  0.82452699  0.79137833 -1.10754289]', '[-0.05546354  0.48017359  1.23429726 -2.2781243 ]', '[ 0.20909957 -0.04617758  1.33805656 -2.84269804]', '[ 0.4464647  -0.59077472  0.966733   -2.46825376]', '[ 0.56484782 -0.96631335  0.19941509 -1.25172843]', '[ 0.53630986 -1.11483074 -0.4758274  -0.22742363]', '[ 0.36187725 -1.00146604 -1.23637201  1.34791736]', '[ 0.0580978  -0.58722668 -1.74863438  2.72971679]', '[-0.30763456  0.04008799 -1.81210934  3.35722424]', '[-0.62370801  0.67078191 -1.26505938  2.79267149]', '[-0.79176675  1.12101918 -0.38985662  1.67263015]', '[-0.77662467  1.33379438  0.53348258  0.44747497]', '[-0.56821474  1.24461177  1.51371348 -1.34090431]', '[-0.18963826  0.80017986  2.21570035 -3.06285926]', '[ 0.28602229  0.0657226   2.42534545 -4.05955899]', '[ 0.72332666 -0.70672227  1.83326158 -3.44408135]', '[ 0.99097693 -1.26824034  0.81099898 -2.14498322]', '[ 1.04249779 -1.56487607 -0.29557831 -0.82053342]', '[ 0.86098448 -1.54334595 -1.48971493  1.05248141]', '[ 0.46277681 -1.13424648 -2.44427921  3.05107493]', '[-0.09153592 -0.33840064 -2.99635574  4.73417722]', '[-0.66837987  0.6169185  -2.60150514  4.45773663]', '[-1.08631471  1.36171957 -1.53072348  2.95405826]', '[-1.27307294  1.80880139 -0.329348    1.54218224]', '[-1.21816192  1.98175115  0.86884768  0.17725331]', '[-0.91983498  1.82518555  2.0756177  -1.77907706]', '[-0.40802487  1.25265874  2.99002247 -3.97839585]', '[ 0.25025761  0.24961359  3.46683796 -5.80140085]', '[ 0.89086489 -0.86790723  2.75267861 -4.97108418]', '[ 1.31639248 -1.68657652  1.48160378 -3.25291153]', '[ 1.48148984 -2.19211541  0.16971851 -1.83405892]', '[ 1.38030206 -2.40106675 -1.16599368 -0.2427649 ]', '[ 1.01908541 -2.25832355 -2.40158696  1.70546053]', '[ 0.44630971 -1.70169712 -3.25166245  3.90592236]', '[-0.25533447 -0.68733341 -3.69553351  6.14174768]', '[-0.96312663  0.59122361 -3.14780405  6.0939836 ]', '[-1.45075757  1.62403316 -1.69363758  4.24055084]', '[-1.6414465   2.31967581 -0.22363782  2.76416164]', '[-1.54714264  2.73383629  1.14478563  1.36839781]', '[-1.1814243   2.82317085  2.47848257 -0.47893915]', '[-0.57911947  2.54296114  3.44408922 -2.31946399]', '[ 0.13995721  1.89960469  3.61167234 -4.08663145]', '[ 0.82853437  0.93244748  3.22933929 -5.47617692]', '[ 1.40547438 -0.20242071  2.42305286 -5.56529744]', '[ 1.74897822 -1.19538745  0.94401846 -4.28695899]', '[ 1.7680138  -1.91436049 -0.775375   -2.87580225]', '[ 1.43952091 -2.32245266 -2.47681548 -1.13483154]', '[ 0.79261032 -2.30417614 -3.87433194  1.35181249]', '[-0.04465723 -1.78070915 -4.32444956  3.84281981]', '[-0.88232768 -0.80891755 -3.97149825  5.681597  ]', '[-1.59568424  0.35604882 -3.04638118  5.60302364]', '[-2.07000376  1.35443462 -1.68567609  4.39983656]', '[-2.27101805  2.14391752 -0.32536811  3.53121497]', '[-2.20361839  2.76289424  0.97408865  2.62024885]', '[-1.88736985 -3.12897394  2.17184318  1.25922438]', '[-1.32773663 -3.04145749  3.42705423 -0.36866634]', '[-0.53508313  3.04281999  4.40535921 -1.55661515]', '[ 0.37401246  2.62801276  4.48478802 -2.5110522 ]', '[ 1.18488663  2.07883682  3.51066626 -2.8518207 ]', '[ 1.76251542  1.54089153  2.27216323 -2.41072233]']</t>
+  </si>
+  <si>
+    <t>[0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50, 51, 52, 53, 54, 55, 56, 57, 58, 59, 60, 61, 62, 63, 64, 65, 66, 67, 68, 69, 70, 71]</t>
+  </si>
+  <si>
+    <t>[array([-0.03763371, -0.01533471,  0.06554052, -0.01816017], dtype=float32), array([-0.00754409, -0.05458322,  0.2277812 , -0.36241836]), array([ 0.04879627, -0.15231473,  0.32089719, -0.5887683 ]), array([ 0.11397169, -0.27767857,  0.31375488, -0.63332862]), array([ 0.16759438, -0.39312519,  0.2086893 , -0.49480525]), array([ 0.1930193 , -0.46685036,  0.03906408, -0.22816919]), array([ 0.15689524, -0.41528579, -0.3922057 ,  0.73207416]), array([ 0.04309269, -0.18588535, -0.71796191,  1.51055937]), array([-0.1147829 ,  0.15904975, -0.81547211,  1.84906375]), array([-0.26363568,  0.51494657, -0.63159042,  1.62703318]), array([-0.35418658,  0.78351571, -0.2539271 ,  1.01663306]), array([-0.36122763,  0.91144819,  0.18313112,  0.25239067]), array([-0.26190848,  0.82452699,  0.79137833, -1.10754289]), array([-0.05546354,  0.48017359,  1.23429726, -2.2781243 ]), array([ 0.20909957, -0.04617758,  1.33805656, -2.84269804]), array([ 0.4464647 , -0.59077472,  0.966733  , -2.46825376]), array([ 0.56484782, -0.96631335,  0.19941509, -1.25172843]), array([ 0.53630986, -1.11483074, -0.4758274 , -0.22742363]), array([ 0.36187725, -1.00146604, -1.23637201,  1.34791736]), array([ 0.0580978 , -0.58722668, -1.74863438,  2.72971679]), array([-0.30763456,  0.04008799, -1.81210934,  3.35722424]), array([-0.62370801,  0.67078191, -1.26505938,  2.79267149]), array([-0.79176675,  1.12101918, -0.38985662,  1.67263015]), array([-0.77662467,  1.33379438,  0.53348258,  0.44747497]), array([-0.56821474,  1.24461177,  1.51371348, -1.34090431]), array([-0.18963826,  0.80017986,  2.21570035, -3.06285926]), array([ 0.28602229,  0.0657226 ,  2.42534545, -4.05955899]), array([ 0.72332666, -0.70672227,  1.83326158, -3.44408135]), array([ 0.99097693, -1.26824034,  0.81099898, -2.14498322]), array([ 1.04249779, -1.56487607, -0.29557831, -0.82053342]), array([ 0.86098448, -1.54334595, -1.48971493,  1.05248141]), array([ 0.46277681, -1.13424648, -2.44427921,  3.05107493]), array([-0.09153592, -0.33840064, -2.99635574,  4.73417722]), array([-0.66837987,  0.6169185 , -2.60150514,  4.45773663]), array([-1.08631471,  1.36171957, -1.53072348,  2.95405826]), array([-1.27307294,  1.80880139, -0.329348  ,  1.54218224]), array([-1.21816192,  1.98175115,  0.86884768,  0.17725331]), array([-0.91983498,  1.82518555,  2.0756177 , -1.77907706]), array([-0.40802487,  1.25265874,  2.99002247, -3.97839585]), array([ 0.25025761,  0.24961359,  3.46683796, -5.80140085]), array([ 0.89086489, -0.86790723,  2.75267861, -4.97108418]), array([ 1.31639248, -1.68657652,  1.48160378, -3.25291153]), array([ 1.48148984, -2.19211541,  0.16971851, -1.83405892]), array([ 1.38030206, -2.40106675, -1.16599368, -0.2427649 ]), array([ 1.01908541, -2.25832355, -2.40158696,  1.70546053]), array([ 0.44630971, -1.70169712, -3.25166245,  3.90592236]), array([-0.25533447, -0.68733341, -3.69553351,  6.14174768]), array([-0.96312663,  0.59122361, -3.14780405,  6.0939836 ]), array([-1.45075757,  1.62403316, -1.69363758,  4.24055084]), array([-1.6414465 ,  2.31967581, -0.22363782,  2.76416164]), array([-1.54714264,  2.73383629,  1.14478563,  1.36839781]), array([-1.1814243 ,  2.82317085,  2.47848257, -0.47893915]), array([-0.57911947,  2.54296114,  3.44408922, -2.31946399]), array([ 0.13995721,  1.89960469,  3.61167234, -4.08663145]), array([ 0.82853437,  0.93244748,  3.22933929, -5.47617692]), array([ 1.40547438, -0.20242071,  2.42305286, -5.56529744]), array([ 1.74897822, -1.19538745,  0.94401846, -4.28695899]), array([ 1.7680138 , -1.91436049, -0.775375  , -2.87580225]), array([ 1.43952091, -2.32245266, -2.47681548, -1.13483154]), array([ 0.79261032, -2.30417614, -3.87433194,  1.35181249]), array([-0.04465723, -1.78070915, -4.32444956,  3.84281981]), array([-0.88232768, -0.80891755, -3.97149825,  5.681597  ]), array([-1.59568424,  0.35604882, -3.04638118,  5.60302364]), array([-2.07000376,  1.35443462, -1.68567609,  4.39983656]), array([-2.27101805,  2.14391752, -0.32536811,  3.53121497]), array([-2.20361839,  2.76289424,  0.97408865,  2.62024885]), array([-1.88736985, -3.12897394,  2.17184318,  1.25922438]), array([-1.32773663, -3.04145749,  3.42705423, -0.36866634]), array([-0.53508313,  3.04281999,  4.40535921, -1.55661515]), array([ 0.37401246,  2.62801276,  4.48478802, -2.5110522 ]), array([ 1.18488663,  2.07883682,  3.51066626, -2.8518207 ]), array([ 1.76251542,  1.54089153,  2.27216323, -2.41072233])]</t>
+  </si>
+  <si>
+    <t>['[0,2,1]', '[2,2,2]', '[2,0,1]', '[0,0,0]', '[2,1,0]', '[1,2,0]', '[1,0,2]', '[1,1,2]', '[0,1,1]', '[1,1,1]']</t>
+  </si>
+  <si>
+    <t>[1, 3, 18, 19, 26, 27, 30, 39, 41, 43, 44, 52, 56, 66, 67, 68, 69, 70, 72, 73, 81, 82, 85, 100, 103]</t>
+  </si>
+  <si>
+    <t>[0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 1, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 1, 2, 2, 2, 2, 2, 2, 2, 2, 1, 1, 2, 2, 2, 0, 0, 1, 1, 2, 2, 2, 2, 2, 2, 2, 2, 2]</t>
+  </si>
+  <si>
+    <t>['[-0.03763371 -0.01533471  0.06554052 -0.01816017]', '[-0.0208055  -0.02030166  0.09914155 -0.02801351]', '[ 0.013578   -0.05917353  0.23628798 -0.34824344]', '[ 0.05569493 -0.11750576  0.17467028 -0.21881458]', '[ 0.09321032 -0.17559542  0.19101534 -0.34617425]', '[ 0.12806655 -0.2487453   0.14829789 -0.36762724]', '[ 0.1491768  -0.31577516  0.05671487 -0.2885846 ]', '[ 0.1491399  -0.35962956 -0.05812126 -0.14310744]', '[ 0.10078417 -0.30482088 -0.41429757  0.67590713]', '[-0.00877971 -0.1021336  -0.65366711  1.30105491]', '[-0.14649189  0.18875387 -0.68486519  1.53261151]', '[-0.26689266  0.47967206 -0.48629038  1.31072239]', '[-0.33065524  0.69184444 -0.13627269  0.77654458]', '[-0.31882631  0.78190662  0.2516868   0.1168993 ]', '[-0.2107277   0.67776786  0.80835085 -1.13859974]', '[-0.00774104  0.34216336  1.17853631 -2.14819372]', '[ 0.23708876 -0.13839981  1.20085028 -2.52383641]', '[ 0.44380933 -0.61103662  0.81004486 -2.09377148]', '[ 0.5340185  -0.91593505  0.07902348 -0.9264767 ]', '[ 0.47602959 -0.97735533 -0.64487557  0.31091151]', '[ 0.27460327 -0.7658559  -1.33496247  1.77820953]', '[-0.03879617 -0.2886872  -1.73221501  2.88532626]', '[-0.38189075  0.32032361 -1.60126553  3.01568407]', '[-0.64406386  0.85152768 -0.96311508  2.19914442]', '[-0.75376899  1.18086762 -0.1207509   1.07537743]', '[-0.69260222  1.27822641  0.71880945 -0.10556321]', '[-0.46665395  1.11129633  1.50334868 -1.55481306]', '[-0.11074029  0.66792547  1.99359308 -2.80786895]', '[ 0.30985506  0.00937551  2.10646642 -3.57585264]', '[ 0.68334953 -0.66613583  1.53306445 -3.00026753]', '[ 0.88747402 -1.12272148  0.48530942 -1.54463845]', '[ 0.88504679 -1.31011533 -0.50571022 -0.32127981]', '[ 0.67272943 -1.19336847 -1.58597571  1.49934464]', '[ 0.267722   -0.70961391 -2.40590159  3.29633826]', '[-0.25275786  0.06877213 -2.66325624  4.22043675]', '[-0.73476602  0.84972453 -2.04326591  3.37878657]', '[-1.04427181  1.38774942 -1.02156629  1.99653254]', '[-1.13747193  1.65409864  0.09380119  0.67494678]', '[-0.99246287  1.60735013  1.33745648 -1.16205055]', '[-0.62279034  1.20167746  2.32010445 -2.91670045]', '[-0.07505087  0.41744652  3.06857725 -4.79499017]', '[ 0.52563813 -0.54574902  2.75697053 -4.44945813]', '[ 0.98798611 -1.2954571   1.80503338 -2.9810824 ]', '[ 1.22770781 -1.72061123  0.58311947 -1.30985187]', '[ 1.22022521 -1.82794431 -0.65309871  0.23729113]', '[ 0.9638374  -1.59350879 -1.88861628  2.14887026]', '[ 0.47654386 -0.94714159 -2.94598998  4.34155929]', '[-0.18154036  0.09915184 -3.45654521  5.74027846]', '[-0.81345855  1.1419236  -2.71823912  4.40351366]', '[-1.24652439  1.8457379  -1.59104913  2.68890137]', '[-1.44473534  2.2398988  -0.38430159  1.28614564]', '[-1.39995784  2.36445221  0.82661936 -0.04809416]', '[-1.11323595  2.19125767  2.01235024 -1.71829519]', '[-0.60567711  1.6357532   3.01284418 -3.89985425]', '[ 0.07304121  0.61237534  3.7048127  -6.24591029]', '[ 0.79762123 -0.68271131  3.28597163 -6.11790387]', '[ 1.31372501 -1.68242492  1.85429894 -3.92012335]', '[ 1.54938898 -2.31203832  0.50604989 -2.42942758]', '[ 1.51948496 -2.66172704 -0.79309196 -1.06412416]', '[ 1.22655224 -2.69299027 -2.10930517  0.76596662]', '[ 0.69525179 -2.34809393 -3.12227849  2.70771759]', '[ 0.02022658 -1.59946376 -3.53822799  4.79509048]', '[-0.69609843 -0.44405351 -3.54193642  6.55179952]', '[-1.31790427  0.82603757 -2.48315815  5.72538786]', '[-1.65236909  1.79591875 -0.84583857  4.02364386]', '[-1.65829024  2.45328658  0.76530846  2.5550301 ]', '[-1.34879779  2.772113    2.2828389   0.62418598]', '[-0.77195962  2.72366265  3.40690394 -1.0899576 ]', '[-0.03608024  2.35056242  3.79146419 -2.58495168]', '[ 0.6785069   1.72561953  3.23461562 -3.5401204 ]', '[ 1.23016002  0.99407242  2.24749527 -3.62846473]', '[ 1.58088715  0.29185433  1.24561597 -3.31827454]', '[ 1.70798668 -0.27981501  0.00498028 -2.36848399]', '[ 1.57314847 -0.64156658 -1.38104354 -1.18668206]', '[ 1.13607141 -0.68650905 -2.97879022  0.82607079]', '[ 0.40418187 -0.29591024 -4.21605859  2.95838221]', '[-0.46983357  0.36146143 -4.29335077  3.18026282]', '[-1.23379121  0.83683611 -3.23261734  1.46486077]', '[-1.74484861  0.96724153 -1.88014212 -0.0440307 ]', '[-1.99690074  0.86829759 -0.67560123 -0.84715338]', '[-2.00191903  0.58902382  0.61783184 -1.93905456]', '[-1.76021196  0.11528893  1.81073043 -2.8278549 ]', '[-1.27600906 -0.5379119   3.00904848 -3.59957668]', '[-0.56742779 -1.26912106  3.98269271 -3.42450482]', '[ 0.26402667 -1.79590418  4.14934172 -1.62800867]', '[ 0.99704882 -1.84639213  2.9765928   1.16228577]', '[ 1.39085112 -1.3398965   0.88081265  3.8439423 ]', '[ 1.33826126 -0.30693162 -1.3052421   6.35123774]', '[ 0.96617362  1.05155939 -2.17491388  6.8318041 ]', '[ 0.51005975  2.36088058 -2.40137373  6.33937783]', '[-2.04781984e-03 -2.63526827e+00 -2.71609853e+00  6.72842039e+00]', '[-0.58635706 -1.13486205 -3.19462847  8.52574864]', '[-1.22167448  0.68752483 -2.67580359  8.83799421]', '[-1.49329128e+00  2.16555368e+00  2.81902940e-03  6.02430662e+00]', '[-1.27975889 -3.11353281  1.87852346  4.20424433]', '[-0.83417896 -2.3605711   2.36967226  3.62347853]', '[-0.41606873 -1.53015457  1.60055613  5.01162528]', '[-0.26521977 -0.23140833  0.08435073  7.73066412]', '[-0.14162269  1.1842265   1.58092842  5.68067708]', '[0.37208822 2.01487101 3.30762679 2.88123935]', '[1.07305103 2.45377426 3.47194455 1.86055093]', '[1.71115107 2.85077584 2.82361439 2.3114345 ]', '[ 2.17209396 -2.83976019  1.69158528  3.66679619]', '[ 2.34777319 -1.98466007 -0.01174011  4.86280663]', '[ 2.14341394 -0.8415599  -2.01619015  6.65559565]', '[ 1.5786897   0.65998267 -3.42236834  7.9892388 ]', '[ 0.8340188   2.206252   -4.04609573  7.43483267]', '[-0.03992189 -2.57803525 -4.56218222  7.86814634]', '[-0.9641765  -0.78425852 -4.74388611 10.28516447]', '[-1.80835375  1.22849551 -3.250163    8.93810686]', '[-2.21594829  2.77505324 -1.01183064  6.84990407]', '[-2.34012949 -2.23284446 -0.55064012  6.05911448]', '[-2.48922258 -1.03261051 -0.93516011  6.05084063]']</t>
+  </si>
+  <si>
+    <t>[array([-0.03763371, -0.01533471,  0.06554052, -0.01816017], dtype=float32), array([-0.0208055 , -0.02030166,  0.09914155, -0.02801351]), array([ 0.013578  , -0.05917353,  0.23628798, -0.34824344]), array([ 0.05569493, -0.11750576,  0.17467028, -0.21881458]), array([ 0.09321032, -0.17559542,  0.19101534, -0.34617425]), array([ 0.12806655, -0.2487453 ,  0.14829789, -0.36762724]), array([ 0.1491768 , -0.31577516,  0.05671487, -0.2885846 ]), array([ 0.1491399 , -0.35962956, -0.05812126, -0.14310744]), array([ 0.10078417, -0.30482088, -0.41429757,  0.67590713]), array([-0.00877971, -0.1021336 , -0.65366711,  1.30105491]), array([-0.14649189,  0.18875387, -0.68486519,  1.53261151]), array([-0.26689266,  0.47967206, -0.48629038,  1.31072239]), array([-0.33065524,  0.69184444, -0.13627269,  0.77654458]), array([-0.31882631,  0.78190662,  0.2516868 ,  0.1168993 ]), array([-0.2107277 ,  0.67776786,  0.80835085, -1.13859974]), array([-0.00774104,  0.34216336,  1.17853631, -2.14819372]), array([ 0.23708876, -0.13839981,  1.20085028, -2.52383641]), array([ 0.44380933, -0.61103662,  0.81004486, -2.09377148]), array([ 0.5340185 , -0.91593505,  0.07902348, -0.9264767 ]), array([ 0.47602959, -0.97735533, -0.64487557,  0.31091151]), array([ 0.27460327, -0.7658559 , -1.33496247,  1.77820953]), array([-0.03879617, -0.2886872 , -1.73221501,  2.88532626]), array([-0.38189075,  0.32032361, -1.60126553,  3.01568407]), array([-0.64406386,  0.85152768, -0.96311508,  2.19914442]), array([-0.75376899,  1.18086762, -0.1207509 ,  1.07537743]), array([-0.69260222,  1.27822641,  0.71880945, -0.10556321]), array([-0.46665395,  1.11129633,  1.50334868, -1.55481306]), array([-0.11074029,  0.66792547,  1.99359308, -2.80786895]), array([ 0.30985506,  0.00937551,  2.10646642, -3.57585264]), array([ 0.68334953, -0.66613583,  1.53306445, -3.00026753]), array([ 0.88747402, -1.12272148,  0.48530942, -1.54463845]), array([ 0.88504679, -1.31011533, -0.50571022, -0.32127981]), array([ 0.67272943, -1.19336847, -1.58597571,  1.49934464]), array([ 0.267722  , -0.70961391, -2.40590159,  3.29633826]), array([-0.25275786,  0.06877213, -2.66325624,  4.22043675]), array([-0.73476602,  0.84972453, -2.04326591,  3.37878657]), array([-1.04427181,  1.38774942, -1.02156629,  1.99653254]), array([-1.13747193,  1.65409864,  0.09380119,  0.67494678]), array([-0.99246287,  1.60735013,  1.33745648, -1.16205055]), array([-0.62279034,  1.20167746,  2.32010445, -2.91670045]), array([-0.07505087,  0.41744652,  3.06857725, -4.79499017]), array([ 0.52563813, -0.54574902,  2.75697053, -4.44945813]), array([ 0.98798611, -1.2954571 ,  1.80503338, -2.9810824 ]), array([ 1.22770781, -1.72061123,  0.58311947, -1.30985187]), array([ 1.22022521, -1.82794431, -0.65309871,  0.23729113]), array([ 0.9638374 , -1.59350879, -1.88861628,  2.14887026]), array([ 0.47654386, -0.94714159, -2.94598998,  4.34155929]), array([-0.18154036,  0.09915184, -3.45654521,  5.74027846]), array([-0.81345855,  1.1419236 , -2.71823912,  4.40351366]), array([-1.24652439,  1.8457379 , -1.59104913,  2.68890137]), array([-1.44473534,  2.2398988 , -0.38430159,  1.28614564]), array([-1.39995784,  2.36445221,  0.82661936, -0.04809416]), array([-1.11323595,  2.19125767,  2.01235024, -1.71829519]), array([-0.60567711,  1.6357532 ,  3.01284418, -3.89985425]), array([ 0.07304121,  0.61237534,  3.7048127 , -6.24591029]), array([ 0.79762123, -0.68271131,  3.28597163, -6.11790387]), array([ 1.31372501, -1.68242492,  1.85429894, -3.92012335]), array([ 1.54938898, -2.31203832,  0.50604989, -2.42942758]), array([ 1.51948496, -2.66172704, -0.79309196, -1.06412416]), array([ 1.22655224, -2.69299027, -2.10930517,  0.76596662]), array([ 0.69525179, -2.34809393, -3.12227849,  2.70771759]), array([ 0.02022658, -1.59946376, -3.53822799,  4.79509048]), array([-0.69609843, -0.44405351, -3.54193642,  6.55179952]), array([-1.31790427,  0.82603757, -2.48315815,  5.72538786]), array([-1.65236909,  1.79591875, -0.84583857,  4.02364386]), array([-1.65829024,  2.45328658,  0.76530846,  2.5550301 ]), array([-1.34879779,  2.772113  ,  2.2828389 ,  0.62418598]), array([-0.77195962,  2.72366265,  3.40690394, -1.0899576 ]), array([-0.03608024,  2.35056242,  3.79146419, -2.58495168]), array([ 0.6785069 ,  1.72561953,  3.23461562, -3.5401204 ]), array([ 1.23016002,  0.99407242,  2.24749527, -3.62846473]), array([ 1.58088715,  0.29185433,  1.24561597, -3.31827454]), array([ 1.70798668, -0.27981501,  0.00498028, -2.36848399]), array([ 1.57314847, -0.64156658, -1.38104354, -1.18668206]), array([ 1.13607141, -0.68650905, -2.97879022,  0.82607079]), array([ 0.40418187, -0.29591024, -4.21605859,  2.95838221]), array([-0.46983357,  0.36146143, -4.29335077,  3.18026282]), array([-1.23379121,  0.83683611, -3.23261734,  1.46486077]), array([-1.74484861,  0.96724153, -1.88014212, -0.0440307 ]), array([-1.99690074,  0.86829759, -0.67560123, -0.84715338]), array([-2.00191903,  0.58902382,  0.61783184, -1.93905456]), array([-1.76021196,  0.11528893,  1.81073043, -2.8278549 ]), array([-1.27600906, -0.5379119 ,  3.00904848, -3.59957668]), array([-0.56742779, -1.26912106,  3.98269271, -3.42450482]), array([ 0.26402667, -1.79590418,  4.14934172, -1.62800867]), array([ 0.99704882, -1.84639213,  2.9765928 ,  1.16228577]), array([ 1.39085112, -1.3398965 ,  0.88081265,  3.8439423 ]), array([ 1.33826126, -0.30693162, -1.3052421 ,  6.35123774]), array([ 0.96617362,  1.05155939, -2.17491388,  6.8318041 ]), array([ 0.51005975,  2.36088058, -2.40137373,  6.33937783]), array([-2.04781984e-03, -2.63526827e+00, -2.71609853e+00,  6.72842039e+00]), array([-0.58635706, -1.13486205, -3.19462847,  8.52574864]), array([-1.22167448,  0.68752483, -2.67580359,  8.83799421]), array([-1.49329128e+00,  2.16555368e+00,  2.81902940e-03,  6.02430662e+00]), array([-1.27975889, -3.11353281,  1.87852346,  4.20424433]), array([-0.83417896, -2.3605711 ,  2.36967226,  3.62347853]), array([-0.41606873, -1.53015457,  1.60055613,  5.01162528]), array([-0.26521977, -0.23140833,  0.08435073,  7.73066412]), array([-0.14162269,  1.1842265 ,  1.58092842,  5.68067708]), array([0.37208822, 2.01487101, 3.30762679, 2.88123935]), array([1.07305103, 2.45377426, 3.47194455, 1.86055093]), array([1.71115107, 2.85077584, 2.82361439, 2.3114345 ]), array([ 2.17209396, -2.83976019,  1.69158528,  3.66679619]), array([ 2.34777319, -1.98466007, -0.01174011,  4.86280663]), array([ 2.14341394, -0.8415599 , -2.01619015,  6.65559565]), array([ 1.5786897 ,  0.65998267, -3.42236834,  7.9892388 ]), array([ 0.8340188 ,  2.206252  , -4.04609573,  7.43483267]), array([-0.03992189, -2.57803525, -4.56218222,  7.86814634]), array([-0.9641765 , -0.78425852, -4.74388611, 10.28516447]), array([-1.80835375,  1.22849551, -3.250163  ,  8.93810686]), array([-2.21594829,  2.77505324, -1.01183064,  6.84990407]), array([-2.34012949, -2.23284446, -0.55064012,  6.05911448]), array([-2.48922258, -1.03261051, -0.93516011,  6.05084063])]</t>
+  </si>
+  <si>
+    <t>['[2,1,0]', '[2,2,2]', '[0,0,0]', '[2,0,1]', '[0,2,1]', '[0,1,1]', '[1,1,1]', '[1,1,2]', '[1,2,0]', '[1,0,2]']</t>
+  </si>
+  <si>
+    <t>[1, 4, 5, 14, 16, 23, 24, 25, 26, 28, 35, 36, 37, 39, 40, 48, 50, 51, 52, 62, 64, 65, 66, 67, 68, 76, 77, 80, 82, 83, 92, 94, 95, 98]</t>
+  </si>
+  <si>
+    <t>[0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 1, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 2, 1, 0, 0, 0, 0, 0, 1, 2, 2, 2, 2, 2, 2, 2, 2]</t>
+  </si>
+  <si>
+    <t>['[-0.03763371 -0.01533471  0.06554052 -0.01816017]', '[-0.0208055  -0.02030166  0.09914155 -0.02801351]', '[ 0.013578   -0.05917353  0.23628798 -0.34824344]', '[ 0.06892075 -0.15170277  0.30283362 -0.5520916 ]', '[ 0.11515941 -0.23443406  0.14815184 -0.25506525]', '[ 0.12516455 -0.24852371 -0.05021307  0.11741394]', '[ 0.08294831 -0.1554863  -0.36084386  0.79144629]', '[-0.0115013   0.05308243 -0.55745024  1.24253891]', '[-0.12720547  0.31605297 -0.56683333  1.32180305]', '[-0.22549382  0.55647218 -0.39075074  1.03179137]', '[-0.27576109  0.7130825  -0.10096431  0.50987643]', '[-0.26413272  0.75498001  0.21439249 -0.09305547]', '[-0.16966369  0.61579754  0.71283704 -1.2767982 ]', '[ 0.00997798  0.26147124  1.04273335 -2.19268002]', '[ 0.21151091 -0.18299059  0.91306497 -2.1328163 ]', '[ 0.3660878  -0.58109161  0.58945938 -1.76067488]', '[ 0.42351369 -0.83113972 -0.02390919 -0.71368888]', '[ 0.3467972  -0.8326786  -0.72608284  0.69048514]', '[ 0.14367971 -0.56332387 -1.26765311  1.95833071]', '[-0.13903229 -0.08230847 -1.48933705  2.72471756]', '[-0.41798943  0.4610808  -1.22159487  2.55808794]', '[-0.6022921   0.89454202 -0.58351282  1.71149063]', '[-0.64357437  1.13230262  0.17381159  0.65177929]', '[-0.52645409  1.12517142  0.97399063 -0.71888222]', '[-0.26748644  0.85001831  1.57169712 -1.9988221 ]', '[ 0.07903208  0.35357746  1.81898851 -2.84496019]', '[ 0.422692   -0.21862818  1.52488155 -2.69938579]', '[ 0.66969302 -0.699921    0.88926339 -2.01671206]', '[ 0.75339007 -0.97353553 -0.06147539 -0.70246719]', '[ 0.63635564 -0.94857319 -1.08887736  0.95279875]', '[ 0.33081884 -0.59578929 -1.91724047  2.53284219]', '[-0.1000162   0.02080831 -2.28360653  3.43816818]', '[-0.53111322  0.67963565 -1.91944228  2.95201496]', '[-0.83731531  1.15561409 -1.09917697  1.76819293]', '[-0.96079488  1.38461268 -0.12433534  0.52451357]', '[-0.87735311  1.33899546  0.948029   -0.98792618]', '[-0.58992021  0.98439622  1.89326484 -2.55916472]', '[-0.14130006  0.3320562   2.50475919 -3.82600986]', '[ 0.37102934 -0.47469007  2.46924347 -3.93898345]', '[ 0.78511229 -1.11983726  1.60810946 -2.43369016]', '[ 1.00103218 -1.44666156  0.5339712  -0.85091426]', '[ 1.00469928 -1.49034771 -0.49643411  0.41445217]', '[ 0.78800238 -1.22444767 -1.65262627  2.26952238]', '[ 0.35508965 -0.57531964 -2.62207024  4.17326543]', '[-0.21422215  0.35975706 -2.89600457  4.8092666 ]', '[-0.73458991  1.20602234 -2.21017733  3.4938544 ]', '[-1.0789926   1.74867412 -1.20709871  1.95958178]', '[-1.21050078  2.00174156 -0.09975676  0.58835723]', '[-1.11189888  1.96282832  1.07405911 -0.98966003]', '[-0.78175723  1.57129649  2.19950598 -2.97241994]', '[-0.25530331  0.78309131  3.00963735 -4.87587895]', '[ 0.37244401 -0.28595197  3.06740006 -5.3768596 ]', '[ 0.89467918 -1.20393942  2.06450754 -3.65709172]', '[ 1.19525092 -1.77899562  0.92498816 -2.12843854]', '[ 1.2616474  -2.06649355 -0.26057099 -0.75611187]', '[ 1.08105915 -2.03500342 -1.52053199  1.09199859]', '[ 0.66820844 -1.61517845 -2.56322412  3.15214131]', '[ 0.07459795 -0.75881031 -3.31478024  5.37149526]', '[-0.60198419  0.4188076  -3.22557792  5.8940197 ]', '[-1.13662852  1.43181493 -2.04732214  4.14181226]', '[-1.41461933  2.096889   -0.73013892  2.5673652 ]', '[-1.42994488  2.47059977  0.56770861  1.1739029 ]', '[-1.18786254  2.54226915  1.82495066 -0.4717687 ]', '[-0.71273363  2.25449146  2.85209911 -2.42801706]', '[-0.09220019  1.58550368  3.26470158 -4.25883283]', '[ 0.56409641  0.57324037  3.21419567 -5.68295316]', '[ 1.13087571 -0.53558116  2.28655715 -5.0292217 ]', '[ 1.43802844 -1.36642157  0.75683059 -3.27378551]', '[ 1.43227703 -1.85432299 -0.80633751 -1.59919569]', '[ 1.11778399 -1.96972937 -2.29008249  0.49304943]', '[ 0.54567258 -1.63672935 -3.33865246  2.87485936]', '[-0.1782722  -0.81956464 -3.80778698  5.20126854]', '[-0.92101839  0.31728628 -3.42210682  5.678747  ]', '[-1.48052862  1.2997974  -2.11652885  4.07237543]', '[-1.76578531  1.97262868 -0.73943337  2.72028054]', '[-1.77760456  2.39793541  0.61643348  1.52170556]', '[-1.5101164   2.52709595  2.04132073 -0.27458829]', '[-0.97917771  2.28722284  3.20999219 -2.18252632]', '[-0.2565819   1.60993129  3.91903764 -4.63715414]', '[ 0.55779757  0.4389494   4.12363153 -6.83704709]', '[ 1.28982674 -0.85572796  2.99808192 -5.6332865 ]', '[ 1.74113063 -1.80500086  1.51690042 -3.94585488]', '[ 1.89472418 -2.44502765  0.04011504 -2.49368906]', '[ 1.76537473 -2.80075234 -1.3172783  -1.0385932 ]', '[ 1.36605294 -2.82876415 -2.66029368  0.78712831]', '[ 0.71829303 -2.47432775 -3.72552523  2.79301775]', '[-0.06978288 -1.69830349 -4.03333928  4.98112086]', '[-0.86567112 -0.5005154  -3.85530464  6.78296821]', '[-1.54109083  0.81686491 -2.72117393  5.96838878]', '[-1.92317413  1.84535083 -1.09533877  4.39479952]', '[-1.98381134  2.59913142  0.45876347  3.15432391]', '[-1.75769596  3.10088088  1.75923392  1.85092229]', '[-1.27864221 -2.97920944  3.0150331   0.22088589]', '[-0.56539506 -3.06463398  4.03832962 -0.96989771]', '[ 0.27627882  2.98231599  4.21081138 -1.26594437]', '[ 1.05277023  2.76263124  3.43565171 -0.8079233 ]', '[1.63136954 2.68119571 2.33486115 0.07134226]', '[1.99235194 2.80913382 1.29866384 1.22448225]', '[ 2.15707461 -3.11396386  0.34535595  2.35878275]', '[ 2.10662286 -2.49875835 -0.9026687   3.79414951]', '[ 1.77148033 -1.57613897 -2.50737886  5.57041214]', '[ 1.08097122 -0.19007189 -4.34197625  8.21488092]', '[ 0.15060487  1.41829596 -4.71495641  7.17672937]', '[-0.77908089  2.62092022 -4.49175799  4.96122609]', '[-1.5852461  -2.81839701 -3.46029138  3.60190199]', '[-2.15677103 -2.19947111 -2.2994509   2.59779132]', '[-2.52936089 -1.77967141 -1.48656919  1.60278609]']</t>
+  </si>
+  <si>
+    <t>[array([-0.03763371, -0.01533471,  0.06554052, -0.01816017], dtype=float32), array([-0.0208055 , -0.02030166,  0.09914155, -0.02801351]), array([ 0.013578  , -0.05917353,  0.23628798, -0.34824344]), array([ 0.06892075, -0.15170277,  0.30283362, -0.5520916 ]), array([ 0.11515941, -0.23443406,  0.14815184, -0.25506525]), array([ 0.12516455, -0.24852371, -0.05021307,  0.11741394]), array([ 0.08294831, -0.1554863 , -0.36084386,  0.79144629]), array([-0.0115013 ,  0.05308243, -0.55745024,  1.24253891]), array([-0.12720547,  0.31605297, -0.56683333,  1.32180305]), array([-0.22549382,  0.55647218, -0.39075074,  1.03179137]), array([-0.27576109,  0.7130825 , -0.10096431,  0.50987643]), array([-0.26413272,  0.75498001,  0.21439249, -0.09305547]), array([-0.16966369,  0.61579754,  0.71283704, -1.2767982 ]), array([ 0.00997798,  0.26147124,  1.04273335, -2.19268002]), array([ 0.21151091, -0.18299059,  0.91306497, -2.1328163 ]), array([ 0.3660878 , -0.58109161,  0.58945938, -1.76067488]), array([ 0.42351369, -0.83113972, -0.02390919, -0.71368888]), array([ 0.3467972 , -0.8326786 , -0.72608284,  0.69048514]), array([ 0.14367971, -0.56332387, -1.26765311,  1.95833071]), array([-0.13903229, -0.08230847, -1.48933705,  2.72471756]), array([-0.41798943,  0.4610808 , -1.22159487,  2.55808794]), array([-0.6022921 ,  0.89454202, -0.58351282,  1.71149063]), array([-0.64357437,  1.13230262,  0.17381159,  0.65177929]), array([-0.52645409,  1.12517142,  0.97399063, -0.71888222]), array([-0.26748644,  0.85001831,  1.57169712, -1.9988221 ]), array([ 0.07903208,  0.35357746,  1.81898851, -2.84496019]), array([ 0.422692  , -0.21862818,  1.52488155, -2.69938579]), array([ 0.66969302, -0.699921  ,  0.88926339, -2.01671206]), array([ 0.75339007, -0.97353553, -0.06147539, -0.70246719]), array([ 0.63635564, -0.94857319, -1.08887736,  0.95279875]), array([ 0.33081884, -0.59578929, -1.91724047,  2.53284219]), array([-0.1000162 ,  0.02080831, -2.28360653,  3.43816818]), array([-0.53111322,  0.67963565, -1.91944228,  2.95201496]), array([-0.83731531,  1.15561409, -1.09917697,  1.76819293]), array([-0.96079488,  1.38461268, -0.12433534,  0.52451357]), array([-0.87735311,  1.33899546,  0.948029  , -0.98792618]), array([-0.58992021,  0.98439622,  1.89326484, -2.55916472]), array([-0.14130006,  0.3320562 ,  2.50475919, -3.82600986]), array([ 0.37102934, -0.47469007,  2.46924347, -3.93898345]), array([ 0.78511229, -1.11983726,  1.60810946, -2.43369016]), array([ 1.00103218, -1.44666156,  0.5339712 , -0.85091426]), array([ 1.00469928, -1.49034771, -0.49643411,  0.41445217]), array([ 0.78800238, -1.22444767, -1.65262627,  2.26952238]), array([ 0.35508965, -0.57531964, -2.62207024,  4.17326543]), array([-0.21422215,  0.35975706, -2.89600457,  4.8092666 ]), array([-0.73458991,  1.20602234, -2.21017733,  3.4938544 ]), array([-1.0789926 ,  1.74867412, -1.20709871,  1.95958178]), array([-1.21050078,  2.00174156, -0.09975676,  0.58835723]), array([-1.11189888,  1.96282832,  1.07405911, -0.98966003]), array([-0.78175723,  1.57129649,  2.19950598, -2.97241994]), array([-0.25530331,  0.78309131,  3.00963735, -4.87587895]), array([ 0.37244401, -0.28595197,  3.06740006, -5.3768596 ]), array([ 0.89467918, -1.20393942,  2.06450754, -3.65709172]), array([ 1.19525092, -1.77899562,  0.92498816, -2.12843854]), array([ 1.2616474 , -2.06649355, -0.26057099, -0.75611187]), array([ 1.08105915, -2.03500342, -1.52053199,  1.09199859]), array([ 0.66820844, -1.61517845, -2.56322412,  3.15214131]), array([ 0.07459795, -0.75881031, -3.31478024,  5.37149526]), array([-0.60198419,  0.4188076 , -3.22557792,  5.8940197 ]), array([-1.13662852,  1.43181493, -2.04732214,  4.14181226]), array([-1.41461933,  2.096889  , -0.73013892,  2.5673652 ]), array([-1.42994488,  2.47059977,  0.56770861,  1.1739029 ]), array([-1.18786254,  2.54226915,  1.82495066, -0.4717687 ]), array([-0.71273363,  2.25449146,  2.85209911, -2.42801706]), array([-0.09220019,  1.58550368,  3.26470158, -4.25883283]), array([ 0.56409641,  0.57324037,  3.21419567, -5.68295316]), array([ 1.13087571, -0.53558116,  2.28655715, -5.0292217 ]), array([ 1.43802844, -1.36642157,  0.75683059, -3.27378551]), array([ 1.43227703, -1.85432299, -0.80633751, -1.59919569]), array([ 1.11778399, -1.96972937, -2.29008249,  0.49304943]), array([ 0.54567258, -1.63672935, -3.33865246,  2.87485936]), array([-0.1782722 , -0.81956464, -3.80778698,  5.20126854]), array([-0.92101839,  0.31728628, -3.42210682,  5.678747  ]), array([-1.48052862,  1.2997974 , -2.11652885,  4.07237543]), array([-1.76578531,  1.97262868, -0.73943337,  2.72028054]), array([-1.77760456,  2.39793541,  0.61643348,  1.52170556]), array([-1.5101164 ,  2.52709595,  2.04132073, -0.27458829]), array([-0.97917771,  2.28722284,  3.20999219, -2.18252632]), array([-0.2565819 ,  1.60993129,  3.91903764, -4.63715414]), array([ 0.55779757,  0.4389494 ,  4.12363153, -6.83704709]), array([ 1.28982674, -0.85572796,  2.99808192, -5.6332865 ]), array([ 1.74113063, -1.80500086,  1.51690042, -3.94585488]), array([ 1.89472418, -2.44502765,  0.04011504, -2.49368906]), array([ 1.76537473, -2.80075234, -1.3172783 , -1.0385932 ]), array([ 1.36605294, -2.82876415, -2.66029368,  0.78712831]), array([ 0.71829303, -2.47432775, -3.72552523,  2.79301775]), array([-0.06978288, -1.69830349, -4.03333928,  4.98112086]), array([-0.86567112, -0.5005154 , -3.85530464,  6.78296821]), array([-1.54109083,  0.81686491, -2.72117393,  5.96838878]), array([-1.92317413,  1.84535083, -1.09533877,  4.39479952]), array([-1.98381134,  2.59913142,  0.45876347,  3.15432391]), array([-1.75769596,  3.10088088,  1.75923392,  1.85092229]), array([-1.27864221, -2.97920944,  3.0150331 ,  0.22088589]), array([-0.56539506, -3.06463398,  4.03832962, -0.96989771]), array([ 0.27627882,  2.98231599,  4.21081138, -1.26594437]), array([ 1.05277023,  2.76263124,  3.43565171, -0.8079233 ]), array([1.63136954, 2.68119571, 2.33486115, 0.07134226]), array([1.99235194, 2.80913382, 1.29866384, 1.22448225]), array([ 2.15707461, -3.11396386,  0.34535595,  2.35878275]), array([ 2.10662286, -2.49875835, -0.9026687 ,  3.79414951]), array([ 1.77148033, -1.57613897, -2.50737886,  5.57041214]), array([ 1.08097122, -0.19007189, -4.34197625,  8.21488092]), array([ 0.15060487,  1.41829596, -4.71495641,  7.17672937]), array([-0.77908089,  2.62092022, -4.49175799,  4.96122609]), array([-1.5852461 , -2.81839701, -3.46029138,  3.60190199]), array([-2.15677103, -2.19947111, -2.2994509 ,  2.59779132]), array([-2.52936089, -1.77967141, -1.48656919,  1.60278609])]</t>
+  </si>
+  <si>
+    <t>['[1,0,2]', '[1,1,2]', '[0,2,1]', '[2,1,0]', '[1,2,0]', '[0,0,0]', '[0,1,1]', '[2,0,1]', '[1,1,1]', '[2,2,2]']</t>
+  </si>
+  <si>
+    <t>[1, 2, 3, 5, 6, 12, 13, 14, 15, 16, 17, 25, 27, 29, 36, 37, 38, 39, 41, 48, 49, 51, 52, 54, 62, 63, 64, 65, 66, 67, 68, 76, 78, 79, 80, 81, 90, 91, 92, 94, 95, 96, 97, 107, 108, 109, 111, 112, 113]</t>
+  </si>
+  <si>
+    <t>[0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 1, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 2, 1, 0, 0, 0, 0, 0, 0, 1, 2, 2, 2, 2, 2, 2, 2]</t>
+  </si>
+  <si>
+    <t>['[-0.03763371 -0.01533471  0.06554052 -0.01816017]', '[-0.0208055  -0.02030166  0.09914155 -0.02801351]', '[ 0.00031733 -0.02489487  0.10765546 -0.0138725 ]', '[ 0.02044082 -0.02428802  0.08954248  0.02288616]', '[ 0.0479687  -0.04919805  0.17922331 -0.26311843]', '[ 0.07526888 -0.08935819  0.08715243 -0.12765022]', '[ 0.08105487 -0.09736072 -0.03054921  0.04959891]', '[ 0.05039934 -0.03628321 -0.26767248  0.5455682 ]', '[-0.02025468  0.10992046 -0.41951797  0.87931856]', '[-0.1080623   0.29740141 -0.43460356  0.94904975]', '[-0.18459285  0.47113603 -0.3110179   0.74993262]', '[-0.2260921   0.58480915 -0.09414718  0.36614175]', '[-0.20808653  0.58061472  0.270049   -0.40458673]', '[-0.12257754  0.42942846  0.56608003 -1.07616477]', '[ 0.0075959   0.16914581  0.70234525 -1.4644143 ]', '[ 0.1427952  -0.1262605   0.61171509 -1.41461516]', '[ 0.23823302 -0.36855793  0.31712125 -0.95552421]', '[ 0.26282029 -0.49337494 -0.07738101 -0.2734523 ]', '[ 0.19573046 -0.44295423 -0.57908578  0.76253121]', '[ 0.0411469  -0.20223856 -0.93073075  1.58608238]', '[-0.15749798  0.15770539 -1.00200138  1.91366674]', '[-0.33720105  0.5210456  -0.74824228  1.63263075]', '[-0.44212474  0.78407481 -0.2790133   0.95679808]', '[-0.44449006  0.894249    0.25452535  0.13607006]', '[-0.32178397  0.77856061  0.95058837 -1.27722357]', '[-0.08981792  0.42997024  1.32079495 -2.13643331]', '[ 0.19411911 -0.06592872  1.44285859 -2.68091684]', '[ 0.44119278 -0.54524606  0.96541457 -1.99689123]', '[ 0.57516326 -0.86692034  0.34839759 -1.17572169]', '[ 0.56496599 -0.97662845 -0.44490772  0.08281464]', '[ 0.39268147 -0.805333   -1.24989538  1.61443003]', '[ 0.08174204 -0.3473967  -1.79725021  2.87212264]', '[-0.29002453  0.27802698 -1.81540418  3.17946531]', '[-0.60390492  0.84777256 -1.25364095  2.40004291]', '[-0.77410505  1.21502908 -0.42685437  1.25246733]', '[-0.77151428  1.34607515  0.4481349   0.05481784]', '[-0.59158069  1.20898042  1.32389639 -1.4261041 ]', '[-0.25721082  0.77994502  1.96831992 -2.81992369]', '[ 0.1656801   0.12479732  2.15709127 -3.54014509]', '[ 0.5559792  -0.5379552   1.64326572 -2.89182815]', '[ 0.80665036 -1.01655035  0.82220897 -1.84006252]', '[ 0.86634761 -1.23856567 -0.22650173 -0.37900217]', '[ 0.71011606 -1.13885797 -1.31415599  1.38430656]', '[ 0.35367717 -0.6833823  -2.20114816  3.13693861]', '[-0.13710551  0.06653302 -2.57875207  4.11527824]', '[-0.61615841  0.83732512 -2.09397261  3.37243001]', '[-0.94593824  1.37631818 -1.16718273  2.0024142 ]', '[-1.07494438  1.64298465 -0.1141187   0.6752337 ]', '[-0.98359178  1.62267474  1.01513599 -0.88861305]', '[-0.67789333  1.27891601  2.00962936 -2.57035372]', '[-0.18653489  0.56495045  2.83706493 -4.49553924]', '[ 0.39017877 -0.38140686  2.7517527  -4.58912411]', '[ 0.85394946 -1.1497439   1.81232586 -2.9899753 ]', '[ 1.11182329 -1.60437541  0.74742048 -1.57520818]', '[ 1.14119089 -1.76271912 -0.45064423 -0.01405073]', '[ 0.92821352 -1.58104656 -1.65780557  1.86145202]', '[ 0.48962113 -1.00129123 -2.69134434  3.96080734]', '[-0.12052184 -0.02675333 -3.26028007  5.48063357]', '[-0.72732527  0.99915579 -2.64810485  4.45378266]', '[-1.15036195  1.71885495 -1.55503399  2.77407682]', '[-1.34348856  2.12807877 -0.36863281  1.34966885]', '[-1.29754526  2.26304695  0.82073988 -0.0062372 ]', '[-1.01566326  2.09672911  1.96520343 -1.68697045]', '[-0.53088471  1.57305374  2.82655053 -3.58625723]', '[ 0.09134781  0.65978034  3.31683254 -5.43815781]', '[ 0.73098222 -0.46031041  2.87299963 -5.29771428]', '[ 1.18027589 -1.33800549  1.57147214 -3.43539503]', '[ 1.35642318 -1.85336967  0.19242584 -1.75690261]', '[ 1.26054506 -2.04466396 -1.13441565 -0.14130194]', '[ 0.90754871 -1.87524166 -2.34836127  1.87754889]', '[ 0.3455849  -1.27541617 -3.20970834  4.14986778]', '[-0.34788325 -0.23596566 -3.59229583  5.96736293]', '[-1.00127152  0.90169427 -2.76031149  5.01499904]', '[-1.42156406  1.72858463 -1.42852947  3.30647123]', '[-1.57217633  2.24864509 -0.08044348  1.92299442]', '[-1.45669448  2.49746973  1.22257459  0.54643112]', '[-1.08579861  2.43629515  2.44504487 -1.18735897]', '[-0.50024052  1.98949222  3.31644913 -3.31297524]', '[ 0.19397038  1.12922676  3.5501207  -5.24185748]', '[ 0.88231364 -0.02708643  3.16980599 -5.91295364]', '[ 1.3869284  -1.06316223  1.78337774 -4.2804976 ]', '[ 1.58750373 -1.74763734  0.22300178 -2.60744455]', '[ 1.48533903 -2.13114808 -1.23630412 -1.19456537]', '[ 1.0903179  -2.16348559 -2.65814516  0.92205351]', '[ 0.45578762 -1.74300795 -3.5835367   3.31747267]', '[-0.30211009 -0.83770043 -3.90964382  5.63551737]', '[-1.05276309  0.37504364 -3.39561396  5.9794661 ]', '[-1.59577482  1.40776441 -1.99016978  4.308169  ]', '[-1.84951376  2.13051132 -0.55442592  2.98034692]', '[-1.821323    2.60618197  0.82282485  1.75901701]', '[-1.51439817  2.78152651  2.22904115 -0.03859418]', '[-0.94627013  2.59795387  3.39271587 -1.82713624]', '[-0.20133133  2.0412724   3.9159291  -3.7471466 ]', '[ 0.57692315  1.08771392  3.79693592 -5.70709012]', '[ 1.27491545 -0.11542172  3.04105886 -5.92132742]', '[ 1.73678709 -1.14698396  1.52286377 -4.31843094]', '[ 1.880239   -1.86140113 -0.09168284 -2.85524762]', '[ 1.69997006 -2.28116242 -1.70098128 -1.28566242]', '[ 1.20406943 -2.32608269 -3.20388288  0.91081928]', '[ 0.45564425 -1.89020435 -4.15252491  3.49806748]', '[-0.40506681 -0.92554017 -4.36271044  6.04796097]', '[-1.23689665  0.38194354 -3.75296625  6.45553393]', '[-1.84384036  1.5006385  -2.29573037  4.73102957]', '[-2.16494079  2.32349257 -0.94324686  3.58710285]', '[-2.23443021  2.94852303  0.20554544  2.65835618]', '[-2.09728512 -2.90593847  1.14807482  1.60416553]', '[-1.76592542 -2.71966339  2.19196366  0.25826534]', '[-1.20984107 -2.79303935  3.37416489 -0.93777747]', '[-0.43262098 -3.06460087  4.2945737  -1.68731945]', '[ 0.44161412  2.85096992  4.26180307 -1.89709795]', '[ 1.21149555  2.47991547  3.33139899 -1.70674425]', '[ 1.75102007  2.22967187  2.06788281 -0.70841251]', '[2.04940978 2.22004456 0.95031164 0.64358018]', '[2.14971684 2.47010645 0.07087992 1.85501269]', '[ 2.06604989  2.99872405 -0.92903439  3.42167552]', '[ 1.75643999 -2.43877827 -2.23826533  5.107155  ]', '[ 1.14012846 -1.17042435 -4.00864176  7.86912056]', '[ 0.17815812  0.68265714 -5.17351929  9.61233904]', '[-0.78323559  2.30390569 -4.41302593  6.63263053]', '[-1.56984538 -2.83403766 -3.37737828  5.03754381]', '[-2.13192056 -1.92033701 -2.30097257  4.13928395]']</t>
+  </si>
+  <si>
+    <t>[0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50, 51, 52, 53, 54, 55, 56, 57, 58, 59, 60, 61, 62, 63, 64, 65, 66, 67, 68, 69, 70, 71, 72, 73, 74, 75, 76, 77, 78, 79, 80, 81, 82, 83, 84, 85, 86, 87, 88, 89, 90, 91, 92, 93, 94, 95, 96, 97, 98, 99, 100, 101, 102, 103, 104, 105, 106, 107, 108, 109, 110, 111, 112, 113, 114, 115, 116, 117, 118, 119, 120]</t>
+  </si>
+  <si>
+    <t>[array([-0.03763371, -0.01533471,  0.06554052, -0.01816017], dtype=float32), array([-0.0208055 , -0.02030166,  0.09914155, -0.02801351]), array([ 0.00031733, -0.02489487,  0.10765546, -0.0138725 ]), array([ 0.02044082, -0.02428802,  0.08954248,  0.02288616]), array([ 0.0479687 , -0.04919805,  0.17922331, -0.26311843]), array([ 0.07526888, -0.08935819,  0.08715243, -0.12765022]), array([ 0.08105487, -0.09736072, -0.03054921,  0.04959891]), array([ 0.05039934, -0.03628321, -0.26767248,  0.5455682 ]), array([-0.02025468,  0.10992046, -0.41951797,  0.87931856]), array([-0.1080623 ,  0.29740141, -0.43460356,  0.94904975]), array([-0.18459285,  0.47113603, -0.3110179 ,  0.74993262]), array([-0.2260921 ,  0.58480915, -0.09414718,  0.36614175]), array([-0.20808653,  0.58061472,  0.270049  , -0.40458673]), array([-0.12257754,  0.42942846,  0.56608003, -1.07616477]), array([ 0.0075959 ,  0.16914581,  0.70234525, -1.4644143 ]), array([ 0.1427952 , -0.1262605 ,  0.61171509, -1.41461516]), array([ 0.23823302, -0.36855793,  0.31712125, -0.95552421]), array([ 0.26282029, -0.49337494, -0.07738101, -0.2734523 ]), array([ 0.19573046, -0.44295423, -0.57908578,  0.76253121]), array([ 0.0411469 , -0.20223856, -0.93073075,  1.58608238]), array([-0.15749798,  0.15770539, -1.00200138,  1.91366674]), array([-0.33720105,  0.5210456 , -0.74824228,  1.63263075]), array([-0.44212474,  0.78407481, -0.2790133 ,  0.95679808]), array([-0.44449006,  0.894249  ,  0.25452535,  0.13607006]), array([-0.32178397,  0.77856061,  0.95058837, -1.27722357]), array([-0.08981792,  0.42997024,  1.32079495, -2.13643331]), array([ 0.19411911, -0.06592872,  1.44285859, -2.68091684]), array([ 0.44119278, -0.54524606,  0.96541457, -1.99689123]), array([ 0.57516326, -0.86692034,  0.34839759, -1.17572169]), array([ 0.56496599, -0.97662845, -0.44490772,  0.08281464]), array([ 0.39268147, -0.805333  , -1.24989538,  1.61443003]), array([ 0.08174204, -0.3473967 , -1.79725021,  2.87212264]), array([-0.29002453,  0.27802698, -1.81540418,  3.17946531]), array([-0.60390492,  0.84777256, -1.25364095,  2.40004291]), array([-0.77410505,  1.21502908, -0.42685437,  1.25246733]), array([-0.77151428,  1.34607515,  0.4481349 ,  0.05481784]), array([-0.59158069,  1.20898042,  1.32389639, -1.4261041 ]), array([-0.25721082,  0.77994502,  1.96831992, -2.81992369]), array([ 0.1656801 ,  0.12479732,  2.15709127, -3.54014509]), array([ 0.5559792 , -0.5379552 ,  1.64326572, -2.89182815]), array([ 0.80665036, -1.01655035,  0.82220897, -1.84006252]), array([ 0.86634761, -1.23856567, -0.22650173, -0.37900217]), array([ 0.71011606, -1.13885797, -1.31415599,  1.38430656]), array([ 0.35367717, -0.6833823 , -2.20114816,  3.13693861]), array([-0.13710551,  0.06653302, -2.57875207,  4.11527824]), array([-0.61615841,  0.83732512, -2.09397261,  3.37243001]), array([-0.94593824,  1.37631818, -1.16718273,  2.0024142 ]), array([-1.07494438,  1.64298465, -0.1141187 ,  0.6752337 ]), array([-0.98359178,  1.62267474,  1.01513599, -0.88861305]), array([-0.67789333,  1.27891601,  2.00962936, -2.57035372]), array([-0.18653489,  0.56495045,  2.83706493, -4.49553924]), array([ 0.39017877, -0.38140686,  2.7517527 , -4.58912411]), array([ 0.85394946, -1.1497439 ,  1.81232586, -2.9899753 ]), array([ 1.11182329, -1.60437541,  0.74742048, -1.57520818]), array([ 1.14119089, -1.76271912, -0.45064423, -0.01405073]), array([ 0.92821352, -1.58104656, -1.65780557,  1.86145202]), array([ 0.48962113, -1.00129123, -2.69134434,  3.96080734]), array([-0.12052184, -0.02675333, -3.26028007,  5.48063357]), array([-0.72732527,  0.99915579, -2.64810485,  4.45378266]), array([-1.15036195,  1.71885495, -1.55503399,  2.77407682]), array([-1.34348856,  2.12807877, -0.36863281,  1.34966885]), array([-1.29754526,  2.26304695,  0.82073988, -0.0062372 ]), array([-1.01566326,  2.09672911,  1.96520343, -1.68697045]), array([-0.53088471,  1.57305374,  2.82655053, -3.58625723]), array([ 0.09134781,  0.65978034,  3.31683254, -5.43815781]), array([ 0.73098222, -0.46031041,  2.87299963, -5.29771428]), array([ 1.18027589, -1.33800549,  1.57147214, -3.43539503]), array([ 1.35642318, -1.85336967,  0.19242584, -1.75690261]), array([ 1.26054506, -2.04466396, -1.13441565, -0.14130194]), array([ 0.90754871, -1.87524166, -2.34836127,  1.87754889]), array([ 0.3455849 , -1.27541617, -3.20970834,  4.14986778]), array([-0.34788325, -0.23596566, -3.59229583,  5.96736293]), array([-1.00127152,  0.90169427, -2.76031149,  5.01499904]), array([-1.42156406,  1.72858463, -1.42852947,  3.30647123]), array([-1.57217633,  2.24864509, -0.08044348,  1.92299442]), array([-1.45669448,  2.49746973,  1.22257459,  0.54643112]), array([-1.08579861,  2.43629515,  2.44504487, -1.18735897]), array([-0.50024052,  1.98949222,  3.31644913, -3.31297524]), array([ 0.19397038,  1.12922676,  3.5501207 , -5.24185748]), array([ 0.88231364, -0.02708643,  3.16980599, -5.91295364]), array([ 1.3869284 , -1.06316223,  1.78337774, -4.2804976 ]), array([ 1.58750373, -1.74763734,  0.22300178, -2.60744455]), array([ 1.48533903, -2.13114808, -1.23630412, -1.19456537]), array([ 1.0903179 , -2.16348559, -2.65814516,  0.92205351]), array([ 0.45578762, -1.74300795, -3.5835367 ,  3.31747267]), array([-0.30211009, -0.83770043, -3.90964382,  5.63551737]), array([-1.05276309,  0.37504364, -3.39561396,  5.9794661 ]), array([-1.59577482,  1.40776441, -1.99016978,  4.308169  ]), array([-1.84951376,  2.13051132, -0.55442592,  2.98034692]), array([-1.821323  ,  2.60618197,  0.82282485,  1.75901701]), array([-1.51439817,  2.78152651,  2.22904115, -0.03859418]), array([-0.94627013,  2.59795387,  3.39271587, -1.82713624]), array([-0.20133133,  2.0412724 ,  3.9159291 , -3.7471466 ]), array([ 0.57692315,  1.08771392,  3.79693592, -5.70709012]), array([ 1.27491545, -0.11542172,  3.04105886, -5.92132742]), array([ 1.73678709, -1.14698396,  1.52286377, -4.31843094]), array([ 1.880239  , -1.86140113, -0.09168284, -2.85524762]), array([ 1.69997006, -2.28116242, -1.70098128, -1.28566242]), array([ 1.20406943, -2.32608269, -3.20388288,  0.91081928]), array([ 0.45564425, -1.89020435, -4.15252491,  3.49806748]), array([-0.40506681, -0.92554017, -4.36271044,  6.04796097]), array([-1.23689665,  0.38194354, -3.75296625,  6.45553393]), array([-1.84384036,  1.5006385 , -2.29573037,  4.73102957]), array([-2.16494079,  2.32349257, -0.94324686,  3.58710285]), array([-2.23443021,  2.94852303,  0.20554544,  2.65835618]), array([-2.09728512, -2.90593847,  1.14807482,  1.60416553]), array([-1.76592542, -2.71966339,  2.19196366,  0.25826534]), array([-1.20984107, -2.79303935,  3.37416489, -0.93777747]), array([-0.43262098, -3.06460087,  4.2945737 , -1.68731945]), array([ 0.44161412,  2.85096992,  4.26180307, -1.89709795]), array([ 1.21149555,  2.47991547,  3.33139899, -1.70674425]), array([ 1.75102007,  2.22967187,  2.06788281, -0.70841251]), array([2.04940978, 2.22004456, 0.95031164, 0.64358018]), array([2.14971684, 2.47010645, 0.07087992, 1.85501269]), array([ 2.06604989,  2.99872405, -0.92903439,  3.42167552]), array([ 1.75643999, -2.43877827, -2.23826533,  5.107155  ]), array([ 1.14012846, -1.17042435, -4.00864176,  7.86912056]), array([ 0.17815812,  0.68265714, -5.17351929,  9.61233904]), array([-0.78323559,  2.30390569, -4.41302593,  6.63263053]), array([-1.56984538, -2.83403766, -3.37737828,  5.03754381]), array([-2.13192056, -1.92033701, -2.30097257,  4.13928395])]</t>
+  </si>
+  <si>
+    <t>['[2,2,2]', '[1,0,2]', '[1,1,1]', '[0,1,1]', '[2,0,1]', '[0,2,1]', '[2,1,0]', '[1,1,2]', '[1,2,0]', '[0,0,0]']</t>
+  </si>
+  <si>
+    <t>[1, 2, 3, 4, 11, 12, 13, 14, 15, 16, 23, 24, 25, 26, 27, 34, 35, 36, 37, 38, 39, 46, 47, 48, 49, 50, 51, 59, 60, 61, 62, 63, 64, 72, 73, 74, 75, 76, 77, 78, 86, 87, 88, 89, 90, 91, 92, 100, 101, 102, 103, 104, 105, 106, 107, 115, 116, 117, 118, 119, 120, 121, 122, 133, 134, 135, 136, 137, 138, 139, 140, 141, 142, 143, 144, 145, 146]</t>
+  </si>
+  <si>
+    <t>[0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 1, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 1, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 1, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 1, 1, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 1, 1, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2]</t>
+  </si>
+  <si>
+    <t>['[-0.03763371 -0.01533471  0.06554052 -0.01816017]', '[-0.0208055  -0.02030166  0.09914155 -0.02801351]', '[ 0.00031733 -0.02489487  0.10765546 -0.0138725 ]', '[ 0.02044082 -0.02428802  0.08954248  0.02288616]', '[ 0.03470698 -0.01491644  0.05056501  0.07132823]', '[ 0.02674144  0.03818636 -0.12667052  0.44879208]', '[-0.01270905  0.15667936 -0.25571586  0.70881747]', '[-0.06940829  0.30836147 -0.29491305  0.77301892]', '[-0.12394901  0.4517198  -0.23590169  0.62988145]', '[-0.15876359  0.5498143  -0.10369689  0.33260441]', '[-0.16331677  0.57991751  0.05921824 -0.03571874]', '[-0.12364641  0.50409537  0.32874453 -0.70766221]', '[-0.03775164  0.30783049  0.50916352 -1.21389118]', '[ 0.06909397  0.04061776  0.52882372 -1.39480458]', '[ 0.16087913 -0.22270668  0.3614133  -1.17772404]', '[ 0.20472536 -0.40990137  0.06420388 -0.6597987 ]', '[ 0.18455416 -0.47825444 -0.26212436 -0.01817226]', '[ 0.09156532 -0.38679677 -0.64742279  0.90761115]', '[-0.06271277 -0.13292697 -0.85786545  1.56672789]', '[-0.23333411  0.20632363 -0.80133675  1.73587805]', '[-0.36498881  0.52600302 -0.4801429   1.39142644]', '[-0.41539568  0.74217732 -0.01227622  0.7395642 ]', '[-0.36944782  0.81527715  0.46213933 -0.01083091]', '[-0.22642744  0.71066606  0.93936783 -1.01021577]', '[-0.00892589  0.42883145  1.18897233 -1.74077443]', '[ 0.22660096  0.0517002   1.1068182  -1.92405165]', '[ 0.41005532 -0.29693012  0.6808143  -1.47495926]', '[ 0.48521772 -0.51258559  0.05370639 -0.64539491]', '[ 0.417663   -0.51547329 -0.71588293  0.61057794]', '[ 0.20989945 -0.2789723  -1.31808193  1.6972301 ]', '[-0.08492151  0.12510753 -1.555619    2.21640575]', '[-0.37963177  0.55019577 -1.32030983  1.91504598]', '[-0.58989289  0.85617843 -0.74359286  1.09612783]', '[-0.66706415  0.97859659 -0.01685984  0.11844472]', '[-0.58535204  0.87309513  0.82205171 -1.16698164]', '[-0.34814683  0.51985272  1.50786441 -2.31349921]', '[-0.00845867 -0.01084392  1.80187214 -2.83660639]', '[ 0.33251678 -0.53972913  1.5220548  -2.29877877]', '[ 0.57395443 -0.88909757  0.8506743  -1.14546192]', '[ 0.66227792 -0.9897414   0.02017728  0.14415152]', '[ 0.56997838 -0.80175587 -0.93344798  1.72881771]', '[ 0.29908242 -0.30913141 -1.72312117  3.11534711]', '[-0.08315313  0.37699688 -1.98491703  3.51987652]', '[-0.44967675  1.01119311 -1.6016925   2.68937509]', '[-0.70314623  1.42828109 -0.90116783  1.46392917]', '[-0.80177252  1.59623253 -0.07487256  0.2180398 ]', '[-0.72394184  1.49081901  0.8443507  -1.27627909]', '[-0.47088945  1.08272659  1.65970504 -2.80278718]', '[-0.07741763  0.38520798  2.19752525 -4.04435356]', '[ 0.35720396 -0.43419659  2.00983042 -3.86699684]', '[ 0.68247785 -1.07790494  1.18689067 -2.48691537]', '[ 0.8218953  -1.42254632  0.19968977 -0.96426762]', '[ 0.75459258 -1.43976003 -0.85807324  0.79326183]', '[ 0.48761236 -1.10140602 -1.78195125  2.59637368]', '[ 0.05897502 -0.41058711 -2.42976401  4.19816012]', '[-0.4314646   0.47314784 -2.31833387  4.31615657]', '[-0.81672247  1.21668414 -1.46858326  3.02633097]', '[-1.00690155  1.67989017 -0.42147508  1.61848727]', '[-0.98493444  1.86772757  0.63078134  0.26001653]', '[-0.75610554  1.75789692  1.62055782 -1.36967148]', '[-0.35595715  1.31549434  2.3275385  -3.05204563]', '[ 0.15035756  0.55372516  2.65209298 -4.43210369]', '[ 0.65139012 -0.34680402  2.2070832  -4.25226899]', '[ 0.985684   -1.05481891  1.0818817  -2.7503158 ]', '[ 1.07698896 -1.44506632 -0.16850092 -1.15785884]', '[ 0.91472109 -1.49041281 -1.42578234  0.72126271]', '[ 0.52287851 -1.1461743  -2.44221275  2.73697075]', '[-0.0361505  -0.40732268 -3.04996577  4.50173997]', '[-0.63332802  0.52271794 -2.74921409  4.43041987]', '[-1.08521394  1.26868163 -1.71335421  2.97168385]', '[-1.30937357  1.72013613 -0.51800962  1.57270265]', '[-1.29116306  1.90318794  0.69559698  0.25067901]', '[-1.02953854  1.78773441  1.89146013 -1.44270084]', '[-0.55192063  1.30869456  2.83147306 -3.37840682]', '[ 0.07603713  0.44640653  3.34164683 -5.06850996]', '[ 0.71210682 -0.56024523  2.83323751 -4.58992558]', '[ 1.16215327 -1.30108095  1.62634935 -2.79800121]', '[ 1.35782358 -1.69718345  0.32701124 -1.20027476]', '[ 1.30144266 -1.80944427 -0.88549401  0.09265836]', '[ 0.99400401 -1.59936647 -2.16048181  2.0609052 ]', '[ 0.45252281 -0.96102535 -3.20685487  4.34885667]', '[-0.25244304  0.09156171 -3.65778063  5.77314362]', '[-0.91661372  1.13370092 -2.84149586  4.36606722]', '[-1.36878347  1.82860103 -1.66344369  2.65004852]', '[-1.57850251  2.21982629 -0.42967068  1.30072406]', '[-1.5405753   2.35359044  0.8058149   0.02656021]', '[-1.25317949  2.19845399  2.04745347 -1.62236049]', '[-0.73653364  1.68088959  3.06882828 -3.62086887]', '[-0.0477877   0.73109595  3.74656433 -5.8081108 ]', '[ 0.69354275 -0.49023316  3.4252725  -5.83763954]', '[ 1.25185642 -1.45301411  2.11107446 -3.75903698]', '[ 1.53705783 -2.02758588  0.74397487 -2.05720434]', '[ 1.55104324 -2.28919955 -0.59805463 -0.55966798]', '[ 1.29547026 -2.22135375 -1.93692724  1.279967  ]', '[ 0.79061624 -1.75322035 -3.06269786  3.47692178]', '[ 0.09089764 -0.80168826 -3.87853789  6.02093093]', '[-0.69741674  0.5149997  -3.73831066  6.50690418]', '[-1.32045812  1.61520414 -2.4407719   4.45914839]', '[-1.67462079  2.34218287 -1.10847324  2.8997805 ]', '[-1.76815669  2.79281948  0.15998958  1.61679382]', '[-1.6029545   2.94643857  1.48609456 -0.09452293]', '[-1.18230305  2.76783546  2.69502195 -1.71300589]', '[-0.55016829  2.24939377  3.52428904 -3.50965378]', '[ 0.18136183  1.35288664  3.71109857 -5.44534145]', '[ 0.90612574  0.12465753  3.39498322 -6.4625698 ]', '[ 1.45594573 -1.03225026  1.98044985 -4.86581396]', '[ 1.68684443 -1.82657166  0.33063116 -3.13510082]', '[ 1.5916107  -2.29295399 -1.26529319 -1.50542563]', '[ 1.18664015 -2.39097767 -2.73298415  0.57118435]', '[ 0.5309742  -2.04772769 -3.70855831  2.89376443]', '[-0.24506756 -1.23143077 -3.95570213  5.22298451]', '[-1.01714361 -0.03100536 -3.61851786  6.37112832]', '[-1.61614472  1.12337344 -2.27213091  4.97315001]', '[-1.91925411  1.97355762 -0.76347825  3.60240829]', '[-1.92492648  2.57624902  0.68896904  2.41293315]', '[-1.6413515   2.8865666   2.12389129  0.66031887]', '[-1.08846     2.85099205  3.36773225 -1.02679203]', '[-0.32846545  2.47603458  4.08853382 -2.71222607]', '[ 0.47542966  1.78201064  3.80351195 -4.14302619]', '[ 1.15770037  0.87349878  2.97543297 -4.76827692]', '[ 1.64787089 -0.04458396  1.87569526 -4.24106039]', '[ 1.89167472 -0.78577978  0.5369341  -3.14819288]', '[ 1.85221976 -1.2976897  -0.96355732 -1.91879435]', '[ 1.48692181 -1.48855962 -2.68848191  0.14152842]', '[ 0.79155997 -1.18253063 -4.19035462  3.03199758]', '[-0.14349073 -0.2799125  -4.97815382  5.66345249]', '[-1.09002765  0.80867125 -4.26479466  4.67470096]', '[-1.81705093  1.53032135 -3.01260358  2.65933112]', '[-2.3096281   1.9414232  -1.96072211  1.6079987 ]', '[-2.62089397  2.22139443 -1.19852491  1.27827528]', '[-2.80422995  2.47491944 -0.66672102  1.28955961]', '[-2.89708388  2.74208234 -0.28205853  1.38025187]', '[-2.92352738e+00  3.02131725e+00  2.77850998e-03  1.39049145e+00]', '[-2.88848059 -3.03520941  0.34435169  0.84566862]', '[-2.78262066 -2.93707759  0.73314671  0.10164881]', '[-2.58337424 -3.0084998   1.30021428 -0.85204317]', '[-2.24850283  3.00872707  2.10450703 -1.85926233]', '[-1.72090363  2.50207774  3.20458643 -3.31976978]', '[-0.9644246   1.61582144  4.35639025 -5.7563139 ]', '[ 0.0197627   0.13976522  5.31880935 -8.58550195]', '[ 1.00503618 -1.39138164  4.29261139 -6.11308541]', '[ 1.7366414  -2.34427631  3.04413759 -3.63881148]', '[ 2.23043987 -2.91552348  1.92860321 -2.18618931]', '[ 2.52669359  3.03760132  1.08400971 -1.15534145]', '[ 2.68045183  2.89547379  0.48616479 -0.28522888]', '[2.73514781 2.89820781 0.07221868 0.30036711]', '[ 2.7098547   3.01215952 -0.33277863  0.83352219]', '[ 2.58297282 -3.01307381 -0.96679868  1.75143018]', '[ 2.30590089 -2.56302617 -1.85571192  2.79413777]', '[ 1.8190061  -1.860393   -3.06848272  4.38895447]', '[ 1.05284341 -0.71585754 -4.64466718  7.23856997]', '[ 0.02169612  0.87140274 -5.33268474  7.69181303]', '[-0.99190082  2.10738134 -4.7382387   4.66354363]', '[-1.84419513  2.81014065 -3.73169851  2.56363582]', '[-2.49043923 -3.08411406 -2.80018755  1.46060746]', '[-3.00170396 -2.84333    -2.41922994  1.05809328]', '[ 2.78343741 -2.61604647 -2.66855816  1.34373156]', '[ 2.1740265  -2.24611917 -3.5159178   2.54714711]', '[ 1.35002321 -1.50236105 -4.77654843  5.18142257]', '[ 0.24906592 -0.08548319 -6.08536087  8.55137322]', '[-0.92594079  1.43615601 -5.39438753  5.90908248]', '[-1.89816059  2.30355891 -4.32484934  3.0353748 ]', '[-2.66973057  2.7580251  -3.47852836  1.75071226]', '[ 2.94493924  3.08430764 -3.34925149  1.69892097]', '[ 2.21855346 -2.7744956  -4.03681021  2.74949413]', '[ 1.30047452 -2.00186766 -5.16228066  5.29281588]', '[ 0.14869954 -0.52433709 -6.33314372  9.45071091]', '[-1.07585326  1.28915273 -5.53311621  7.55064023]', '[-2.0614779   2.47841525 -4.40187839  4.71285984]', '[-2.86635554 -2.97876261 -3.75331907  3.81349974]', '[ 2.66624946 -2.18924188 -3.90662461  4.32347849]', '[ 1.79197189 -1.13162488 -5.01045896  6.6139771 ]', '[ 0.62395337  0.49661066 -6.44410795  8.78814013]', '[-0.66358597  1.92730029 -6.27793956  5.11155575]', '[-1.83366105  2.60081256 -5.30081181  1.90331644]', '[-2.78608803  2.80328153 -4.33714816  0.40528819]', '[ 2.6517429   2.85973064 -4.29776463  0.38596051]', '[ 1.71153236  3.02858568 -5.23467776  1.45123673]', '[ 0.54313103 -2.79572246 -6.33063033  3.26673991]', '[-0.71403843 -1.90372268 -5.98579588  5.68024618]', '[-1.81628127 -0.5635191  -5.08296603  7.46769096]', '[-2.74622303  0.90323243 -4.22958763  6.90280737]']</t>
+  </si>
+  <si>
+    <t>[0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50, 51, 52, 53, 54, 55, 56, 57, 58, 59, 60, 61, 62, 63, 64, 65, 66, 67, 68, 69, 70, 71, 72, 73, 74, 75, 76, 77, 78, 79, 80, 81, 82, 83, 84, 85, 86, 87, 88, 89, 90, 91, 92, 93, 94, 95, 96, 97, 98, 99, 100, 101, 102, 103, 104, 105, 106, 107, 108, 109, 110, 111, 112, 113, 114, 115, 116, 117, 118, 119, 120, 121, 122, 123, 124, 125, 126, 127, 128, 129, 130, 131, 132, 133, 134, 135, 136, 137, 138, 139, 140, 141, 142, 143, 144, 145, 146, 147, 148, 149, 150, 151, 152, 153, 154, 155, 156, 157, 158, 159, 160, 161, 162, 163, 164, 165, 166, 167, 168, 169, 170, 171, 172, 173, 174, 175, 176, 177, 178, 179, 180, 181]</t>
+  </si>
+  <si>
+    <t>[array([-0.03763371, -0.01533471,  0.06554052, -0.01816017], dtype=float32), array([-0.0208055 , -0.02030166,  0.09914155, -0.02801351]), array([ 0.00031733, -0.02489487,  0.10765546, -0.0138725 ]), array([ 0.02044082, -0.02428802,  0.08954248,  0.02288616]), array([ 0.03470698, -0.01491644,  0.05056501,  0.07132823]), array([ 0.02674144,  0.03818636, -0.12667052,  0.44879208]), array([-0.01270905,  0.15667936, -0.25571586,  0.70881747]), array([-0.06940829,  0.30836147, -0.29491305,  0.77301892]), array([-0.12394901,  0.4517198 , -0.23590169,  0.62988145]), array([-0.15876359,  0.5498143 , -0.10369689,  0.33260441]), array([-0.16331677,  0.57991751,  0.05921824, -0.03571874]), array([-0.12364641,  0.50409537,  0.32874453, -0.70766221]), array([-0.03775164,  0.30783049,  0.50916352, -1.21389118]), array([ 0.06909397,  0.04061776,  0.52882372, -1.39480458]), array([ 0.16087913, -0.22270668,  0.3614133 , -1.17772404]), array([ 0.20472536, -0.40990137,  0.06420388, -0.6597987 ]), array([ 0.18455416, -0.47825444, -0.26212436, -0.01817226]), array([ 0.09156532, -0.38679677, -0.64742279,  0.90761115]), array([-0.06271277, -0.13292697, -0.85786545,  1.56672789]), array([-0.23333411,  0.20632363, -0.80133675,  1.73587805]), array([-0.36498881,  0.52600302, -0.4801429 ,  1.39142644]), array([-0.41539568,  0.74217732, -0.01227622,  0.7395642 ]), array([-0.36944782,  0.81527715,  0.46213933, -0.01083091]), array([-0.22642744,  0.71066606,  0.93936783, -1.01021577]), array([-0.00892589,  0.42883145,  1.18897233, -1.74077443]), array([ 0.22660096,  0.0517002 ,  1.1068182 , -1.92405165]), array([ 0.41005532, -0.29693012,  0.6808143 , -1.47495926]), array([ 0.48521772, -0.51258559,  0.05370639, -0.64539491]), array([ 0.417663  , -0.51547329, -0.71588293,  0.61057794]), array([ 0.20989945, -0.2789723 , -1.31808193,  1.6972301 ]), array([-0.08492151,  0.12510753, -1.555619  ,  2.21640575]), array([-0.37963177,  0.55019577, -1.32030983,  1.91504598]), array([-0.58989289,  0.85617843, -0.74359286,  1.09612783]), array([-0.66706415,  0.97859659, -0.01685984,  0.11844472]), array([-0.58535204,  0.87309513,  0.82205171, -1.16698164]), array([-0.34814683,  0.51985272,  1.50786441, -2.31349921]), array([-0.00845867, -0.01084392,  1.80187214, -2.83660639]), array([ 0.33251678, -0.53972913,  1.5220548 , -2.29877877]), array([ 0.57395443, -0.88909757,  0.8506743 , -1.14546192]), array([ 0.66227792, -0.9897414 ,  0.02017728,  0.14415152]), array([ 0.56997838, -0.80175587, -0.93344798,  1.72881771]), array([ 0.29908242, -0.30913141, -1.72312117,  3.11534711]), array([-0.08315313,  0.37699688, -1.98491703,  3.51987652]), array([-0.44967675,  1.01119311, -1.6016925 ,  2.68937509]), array([-0.70314623,  1.42828109, -0.90116783,  1.46392917]), array([-0.80177252,  1.59623253, -0.07487256,  0.2180398 ]), array([-0.72394184,  1.49081901,  0.8443507 , -1.27627909]), array([-0.47088945,  1.08272659,  1.65970504, -2.80278718]), array([-0.07741763,  0.38520798,  2.19752525, -4.04435356]), array([ 0.35720396, -0.43419659,  2.00983042, -3.86699684]), array([ 0.68247785, -1.07790494,  1.18689067, -2.48691537]), array([ 0.8218953 , -1.42254632,  0.19968977, -0.96426762]), array([ 0.75459258, -1.43976003, -0.85807324,  0.79326183]), array([ 0.48761236, -1.10140602, -1.78195125,  2.59637368]), array([ 0.05897502, -0.41058711, -2.42976401,  4.19816012]), array([-0.4314646 ,  0.47314784, -2.31833387,  4.31615657]), array([-0.81672247,  1.21668414, -1.46858326,  3.02633097]), array([-1.00690155,  1.67989017, -0.42147508,  1.61848727]), array([-0.98493444,  1.86772757,  0.63078134,  0.26001653]), array([-0.75610554,  1.75789692,  1.62055782, -1.36967148]), array([-0.35595715,  1.31549434,  2.3275385 , -3.05204563]), array([ 0.15035756,  0.55372516,  2.65209298, -4.43210369]), array([ 0.65139012, -0.34680402,  2.2070832 , -4.25226899]), array([ 0.985684  , -1.05481891,  1.0818817 , -2.7503158 ]), array([ 1.07698896, -1.44506632, -0.16850092, -1.15785884]), array([ 0.91472109, -1.49041281, -1.42578234,  0.72126271]), array([ 0.52287851, -1.1461743 , -2.44221275,  2.73697075]), array([-0.0361505 , -0.40732268, -3.04996577,  4.50173997]), array([-0.63332802,  0.52271794, -2.74921409,  4.43041987]), array([-1.08521394,  1.26868163, -1.71335421,  2.97168385]), array([-1.30937357,  1.72013613, -0.51800962,  1.57270265]), array([-1.29116306,  1.90318794,  0.69559698,  0.25067901]), array([-1.02953854,  1.78773441,  1.89146013, -1.44270084]), array([-0.55192063,  1.30869456,  2.83147306, -3.37840682]), array([ 0.07603713,  0.44640653,  3.34164683, -5.06850996]), array([ 0.71210682, -0.56024523,  2.83323751, -4.58992558]), array([ 1.16215327, -1.30108095,  1.62634935, -2.79800121]), array([ 1.35782358, -1.69718345,  0.32701124, -1.20027476]), array([ 1.30144266, -1.80944427, -0.88549401,  0.09265836]), array([ 0.99400401, -1.59936647, -2.16048181,  2.0609052 ]), array([ 0.45252281, -0.96102535, -3.20685487,  4.34885667]), array([-0.25244304,  0.09156171, -3.65778063,  5.77314362]), array([-0.91661372,  1.13370092, -2.84149586,  4.36606722]), array([-1.36878347,  1.82860103, -1.66344369,  2.65004852]), array([-1.57850251,  2.21982629, -0.42967068,  1.30072406]), array([-1.5405753 ,  2.35359044,  0.8058149 ,  0.02656021]), array([-1.25317949,  2.19845399,  2.04745347, -1.62236049]), array([-0.73653364,  1.68088959,  3.06882828, -3.62086887]), array([-0.0477877 ,  0.73109595,  3.74656433, -5.8081108 ]), array([ 0.69354275, -0.49023316,  3.4252725 , -5.83763954]), array([ 1.25185642, -1.45301411,  2.11107446, -3.75903698]), array([ 1.53705783, -2.02758588,  0.74397487, -2.05720434]), array([ 1.55104324, -2.28919955, -0.59805463, -0.55966798]), array([ 1.29547026, -2.22135375, -1.93692724,  1.279967  ]), array([ 0.79061624, -1.75322035, -3.06269786,  3.47692178]), array([ 0.09089764, -0.80168826, -3.87853789,  6.02093093]), array([-0.69741674,  0.5149997 , -3.73831066,  6.50690418]), array([-1.32045812,  1.61520414, -2.4407719 ,  4.45914839]), array([-1.67462079,  2.34218287, -1.10847324,  2.8997805 ]), array([-1.76815669,  2.79281948,  0.15998958,  1.61679382]), array([-1.6029545 ,  2.94643857,  1.48609456, -0.09452293]), array([-1.18230305,  2.76783546,  2.69502195, -1.71300589]), array([-0.55016829,  2.24939377,  3.52428904, -3.50965378]), array([ 0.18136183,  1.35288664,  3.71109857, -5.44534145]), array([ 0.90612574,  0.12465753,  3.39498322, -6.4625698 ]), array([ 1.45594573, -1.03225026,  1.98044985, -4.86581396]), array([ 1.68684443, -1.82657166,  0.33063116, -3.13510082]), array([ 1.5916107 , -2.29295399, -1.26529319, -1.50542563]), array([ 1.18664015, -2.39097767, -2.73298415,  0.57118435]), array([ 0.5309742 , -2.04772769, -3.70855831,  2.89376443]), array([-0.24506756, -1.23143077, -3.95570213,  5.22298451]), array([-1.01714361, -0.03100536, -3.61851786,  6.37112832]), array([-1.61614472,  1.12337344, -2.27213091,  4.97315001]), array([-1.91925411,  1.97355762, -0.76347825,  3.60240829]), array([-1.92492648,  2.57624902,  0.68896904,  2.41293315]), array([-1.6413515 ,  2.8865666 ,  2.12389129,  0.66031887]), array([-1.08846   ,  2.85099205,  3.36773225, -1.02679203]), array([-0.32846545,  2.47603458,  4.08853382, -2.71222607]), array([ 0.47542966,  1.78201064,  3.80351195, -4.14302619]), array([ 1.15770037,  0.87349878,  2.97543297, -4.76827692]), array([ 1.64787089, -0.04458396,  1.87569526, -4.24106039]), array([ 1.89167472, -0.78577978,  0.5369341 , -3.14819288]), array([ 1.85221976, -1.2976897 , -0.96355732, -1.91879435]), array([ 1.48692181, -1.48855962, -2.68848191,  0.14152842]), array([ 0.79155997, -1.18253063, -4.19035462,  3.03199758]), array([-0.14349073, -0.2799125 , -4.97815382,  5.66345249]), array([-1.09002765,  0.80867125, -4.26479466,  4.67470096]), array([-1.81705093,  1.53032135, -3.01260358,  2.65933112]), array([-2.3096281 ,  1.9414232 , -1.96072211,  1.6079987 ]), array([-2.62089397,  2.22139443, -1.19852491,  1.27827528]), array([-2.80422995,  2.47491944, -0.66672102,  1.28955961]), array([-2.89708388,  2.74208234, -0.28205853,  1.38025187]), array([-2.92352738e+00,  3.02131725e+00,  2.77850998e-03,  1.39049145e+00]), array([-2.88848059, -3.03520941,  0.34435169,  0.84566862]), array([-2.78262066, -2.93707759,  0.73314671,  0.10164881]), array([-2.58337424, -3.0084998 ,  1.30021428, -0.85204317]), array([-2.24850283,  3.00872707,  2.10450703, -1.85926233]), array([-1.72090363,  2.50207774,  3.20458643, -3.31976978]), array([-0.9644246 ,  1.61582144,  4.35639025, -5.7563139 ]), array([ 0.0197627 ,  0.13976522,  5.31880935, -8.58550195]), array([ 1.00503618, -1.39138164,  4.29261139, -6.11308541]), array([ 1.7366414 , -2.34427631,  3.04413759, -3.63881148]), array([ 2.23043987, -2.91552348,  1.92860321, -2.18618931]), array([ 2.52669359,  3.03760132,  1.08400971, -1.15534145]), array([ 2.68045183,  2.89547379,  0.48616479, -0.28522888]), array([2.73514781, 2.89820781, 0.07221868, 0.30036711]), array([ 2.7098547 ,  3.01215952, -0.33277863,  0.83352219]), array([ 2.58297282, -3.01307381, -0.96679868,  1.75143018]), array([ 2.30590089, -2.56302617, -1.85571192,  2.79413777]), array([ 1.8190061 , -1.860393  , -3.06848272,  4.38895447]), array([ 1.05284341, -0.71585754, -4.64466718,  7.23856997]), array([ 0.02169612,  0.87140274, -5.33268474,  7.69181303]), array([-0.99190082,  2.10738134, -4.7382387 ,  4.66354363]), array([-1.84419513,  2.81014065, -3.73169851,  2.56363582]), array([-2.49043923, -3.08411406, -2.80018755,  1.46060746]), array([-3.00170396, -2.84333   , -2.41922994,  1.05809328]), array([ 2.78343741, -2.61604647, -2.66855816,  1.34373156]), array([ 2.1740265 , -2.24611917, -3.5159178 ,  2.54714711]), array([ 1.35002321, -1.50236105, -4.77654843,  5.18142257]), array([ 0.24906592, -0.08548319, -6.08536087,  8.55137322]), array([-0.92594079,  1.43615601, -5.39438753,  5.90908248]), array([-1.89816059,  2.30355891, -4.32484934,  3.0353748 ]), array([-2.66973057,  2.7580251 , -3.47852836,  1.75071226]), array([ 2.94493924,  3.08430764, -3.34925149,  1.69892097]), array([ 2.21855346, -2.7744956 , -4.03681021,  2.74949413]), array([ 1.30047452, -2.00186766, -5.16228066,  5.29281588]), array([ 0.14869954, -0.52433709, -6.33314372,  9.45071091]), array([-1.07585326,  1.28915273, -5.53311621,  7.55064023]), array([-2.0614779 ,  2.47841525, -4.40187839,  4.71285984]), array([-2.86635554, -2.97876261, -3.75331907,  3.81349974]), array([ 2.66624946, -2.18924188, -3.90662461,  4.32347849]), array([ 1.79197189, -1.13162488, -5.01045896,  6.6139771 ]), array([ 0.62395337,  0.49661066, -6.44410795,  8.78814013]), array([-0.66358597,  1.92730029, -6.27793956,  5.11155575]), array([-1.83366105,  2.60081256, -5.30081181,  1.90331644]), array([-2.78608803,  2.80328153, -4.33714816,  0.40528819]), array([ 2.6517429 ,  2.85973064, -4.29776463,  0.38596051]), array([ 1.71153236,  3.02858568, -5.23467776,  1.45123673]), array([ 0.54313103, -2.79572246, -6.33063033,  3.26673991]), array([-0.71403843, -1.90372268, -5.98579588,  5.68024618]), array([-1.81628127, -0.5635191 , -5.08296603,  7.46769096]), array([-2.74622303,  0.90323243, -4.22958763,  6.90280737])]</t>
+  </si>
+  <si>
+    <t>['[1,1,2]', '[0,1,1]', '[2,1,0]', '[1,1,1]', '[1,0,2]', '[2,0,1]', '[2,2,2]', '[0,2,1]', '[1,2,0]', '[0,0,0]']</t>
+  </si>
+  <si>
+    <t>[1,2,0]</t>
+  </si>
+  <si>
+    <t>[19, 20, 21, 24, 34, 50, 53, 63, 64, 83, 85, 96, 97, 98]</t>
+  </si>
+  <si>
+    <t>[0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 1, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 1, 2, 2, 2, 2, 2, 2, 2, 2, 1, 0, 0, 0, 0, 1, 2, 2, 2, 2, 2, 2, 2, 2, 1, 2, 2, 2, 0, 0, 0]</t>
+  </si>
+  <si>
+    <t>['[-0.03763371 -0.01533471  0.06554052 -0.01816017]', '[-0.00754409 -0.05458322  0.2277812  -0.36241836]', '[ 0.04879627 -0.15231473  0.32089719 -0.5887683 ]', '[ 0.11397169 -0.27767857  0.31375488 -0.63332862]', '[ 0.16759438 -0.39312519  0.2086893  -0.49480525]', '[ 0.1930193  -0.46685036  0.03906408 -0.22816919]', '[ 0.15689524 -0.41528579 -0.3922057   0.73207416]', '[ 0.04309269 -0.18588535 -0.71796191  1.51055937]', '[-0.1147829   0.15904975 -0.81547211  1.84906375]', '[-0.26363568  0.51494657 -0.63159042  1.62703318]', '[-0.35418658  0.78351571 -0.2539271   1.01663306]', '[-0.36122763  0.91144819  0.18313112  0.25239067]', '[-0.26190848  0.82452699  0.79137833 -1.10754289]', '[-0.05546354  0.48017359  1.23429726 -2.2781243 ]', '[ 0.20909957 -0.04617758  1.33805656 -2.84269804]', '[ 0.4464647  -0.59077472  0.966733   -2.46825376]', '[ 0.57603342 -0.99637145  0.30429255 -1.53991243]', '[ 0.56516121 -1.19760706 -0.40558213 -0.46475241]', '[ 0.40174223 -1.12742398 -1.19611308  1.15628906]', '[ 0.12468571 -0.80293681 -1.52283222  2.03079276]', '[-0.18217998 -0.35191871 -1.47504924  2.35734041]', '[-0.43470748  0.08303025 -0.98464581  1.867767  ]', '[-0.5817114   0.42450509 -0.44787668  1.4739004 ]', '[-0.60388599  0.65110485  0.23506479  0.75953166]', '[-0.47776744  0.68939336  1.00314287 -0.37404036]', '[-0.20561504  0.47776889  1.66446085 -1.69065932]', '[ 0.15919797  0.05131234  1.89694547 -2.43413717]', '[ 0.51436743 -0.42807718  1.56922561 -2.21264335]', '[ 0.75959541 -0.79099918  0.83971197 -1.36055766]', '[ 0.83987915 -0.9617938  -0.0473906  -0.33651921]', '[ 0.71906799 -0.86365319 -1.14514988  1.31993417]', '[ 0.39369819 -0.43791295 -2.05578387  2.88001213]', '[-0.0674174   0.2296699  -2.43213322  3.56106318]', '[-0.52528108  0.88200445 -2.04419348  2.78748533]', '[-0.83622703  1.25593534 -1.03033084  0.95322675]', '[-0.94779263  1.32250713 -0.07169325 -0.28023566]', '[-0.84326329  1.09006103  1.11350203 -2.05570953]', '[-0.50859901  0.4965919   2.19021618 -3.83491246]', '[-0.00683289 -0.37252453  2.67404852 -4.54012252]', '[ 0.49741517 -1.18790108  2.26642989 -3.43618764]', '[ 0.87543328 -1.72543057  1.47338468 -1.94387829]', '[ 1.07422384 -1.97347887  0.49370768 -0.55447229]', '[ 1.06106035 -1.92864197 -0.6252488   1.00512794]', '[ 0.81956839 -1.54062234 -1.77656247  2.91508194]', '[ 0.35743955 -0.74305069 -2.80816495  5.05640183]', '[-0.25637383  0.39484123 -3.11183299  5.85150465]', '[-0.80211533  1.41753772 -2.24994748  4.22392096]', '[-1.14362336  2.09334249 -1.14967128  2.58765987]', '[-1.25805661  2.46814087  0.00760454  1.17950062]', '[-1.14294084  2.56731062  1.12785145 -0.18901701]', '[-0.81268537  2.3704952   2.12494281 -1.78662898]', '[-0.31422415  1.82671303  2.78643539 -3.66964039]', '[ 0.27791047  0.89825248  3.08902234 -5.5729603 ]', '[ 0.8660903  -0.27456375  2.60091865 -5.72248619]', '[ 1.25793783 -1.27659738  1.23360876 -4.17846789]', '[ 1.34987884 -1.94954754 -0.31229337 -2.5667557 ]', '[ 1.14137037 -2.3013719  -1.73156283 -0.93748835]', '[ 0.67085362 -2.27967992 -2.876467    1.14824605]', '[ 0.04034462 -1.85107679 -3.29989278  3.09447294]', '[-0.60506095 -1.07103822 -3.08300008  4.59802201]', '[-1.16700115 -0.08260152 -2.4445068   5.03529461]', '[-1.53792008  0.84006946 -1.18450092  4.05039801]', '[-1.62172832  1.51920429  0.37560878  2.71207435]', '[-1.36795497  1.85697999  2.13306967  0.60061739]', '[-0.79965925  1.75029195  3.4580646  -1.7353615 ]', '[-0.02609599  1.12699725  4.15437697 -4.45448993]', '[ 0.81050928  0.04958212  4.03667933 -5.87621453]', '[ 1.50900968 -1.01432149  2.84739661 -4.5293363 ]', '[ 1.94602536 -1.77510358  1.54075062 -3.18285335]', '[ 2.13120334 -2.31782079  0.3215775  -2.27529933]', '[ 2.07758935 -2.68208179 -0.85357564 -1.33398797]', '[ 1.78295772 -2.81267322 -2.09952784  0.08083681]', '[ 1.23104976 -2.60739905 -3.39277037  2.03861354]', '[ 0.45651635 -1.966091   -4.23942453  4.46039508]', '[-0.42516554 -0.80056469 -4.51663109  7.11843556]', '[-1.27962424  0.67930413 -3.76775796  6.9912101 ]', '[-1.8734577   1.86744666 -2.18314449  4.99975463]', '[-2.16952586  2.73890942 -0.83254201  3.79816751]', '[-2.23325886 -2.88637972  0.12978371  2.77917426]', '[-2.13190449 -2.43778193  0.87945175  1.69633174]', '[-1.86583978 -2.2295763   1.81820778  0.40092848]', '[-1.38295387 -2.28066577  3.03295962 -0.82403228]', '[-0.65819123 -2.50756585  4.14416406 -1.27562387]', '[ 0.21265269 -2.69849172  4.37668041 -0.44872702]', '[ 1.01862099 -2.63971588  3.5054854   1.17385792]', '[ 1.5390562  -2.15392684  1.54677364  3.72842434]', '[ 1.59246165 -1.13892406 -1.04858835  6.47433134]', '[ 1.16043303  0.41616262 -2.92772942  8.55906988]', '[ 0.5640299   2.03420356 -2.95212671  7.50601978]', '[-0.04062301 -2.78051694 -3.1196449   7.4575861 ]', '[-0.70058448 -1.13953708 -3.57360842  9.27945054]', '[-1.3995825   0.8208936  -2.87074559  9.35935321]', '[-1.68472301e+00  2.38728173e+00 -5.96432255e-03  6.49715955e+00]', '[-1.50019303 -2.7704709   1.49554683  4.99330266]', '[-1.18974008 -1.81391382  1.44683399  4.8470988 ]', '[-0.97756444 -0.69505724  0.66253054  6.48355121]', '[-0.78709207  0.57213241  1.68776504  5.46500939]', '[-0.19639885  1.27084281  4.10585705  1.40299146]', '[ 0.72042592  1.21334527  4.74223636 -1.67814222]', '[ 1.61285268  0.71565363  4.0527259  -2.96313463]', '[ 2.32838975  0.12470637  3.13692778 -2.83975638]']</t>
+  </si>
+  <si>
+    <t>[0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50, 51, 52, 53, 54, 55, 56, 57, 58, 59, 60, 61, 62, 63, 64, 65, 66, 67, 68, 69, 70, 71, 72, 73, 74, 75, 76, 77, 78, 79, 80, 81, 82, 83, 84, 85, 86, 87, 88, 89, 90, 91, 92, 93, 94, 95, 96, 97, 98, 99, 100]</t>
+  </si>
+  <si>
+    <t>[array([-0.03763371, -0.01533471,  0.06554052, -0.01816017], dtype=float32), array([-0.00754409, -0.05458322,  0.2277812 , -0.36241836]), array([ 0.04879627, -0.15231473,  0.32089719, -0.5887683 ]), array([ 0.11397169, -0.27767857,  0.31375488, -0.63332862]), array([ 0.16759438, -0.39312519,  0.2086893 , -0.49480525]), array([ 0.1930193 , -0.46685036,  0.03906408, -0.22816919]), array([ 0.15689524, -0.41528579, -0.3922057 ,  0.73207416]), array([ 0.04309269, -0.18588535, -0.71796191,  1.51055937]), array([-0.1147829 ,  0.15904975, -0.81547211,  1.84906375]), array([-0.26363568,  0.51494657, -0.63159042,  1.62703318]), array([-0.35418658,  0.78351571, -0.2539271 ,  1.01663306]), array([-0.36122763,  0.91144819,  0.18313112,  0.25239067]), array([-0.26190848,  0.82452699,  0.79137833, -1.10754289]), array([-0.05546354,  0.48017359,  1.23429726, -2.2781243 ]), array([ 0.20909957, -0.04617758,  1.33805656, -2.84269804]), array([ 0.4464647 , -0.59077472,  0.966733  , -2.46825376]), array([ 0.57603342, -0.99637145,  0.30429255, -1.53991243]), array([ 0.56516121, -1.19760706, -0.40558213, -0.46475241]), array([ 0.40174223, -1.12742398, -1.19611308,  1.15628906]), array([ 0.12468571, -0.80293681, -1.52283222,  2.03079276]), array([-0.18217998, -0.35191871, -1.47504924,  2.35734041]), array([-0.43470748,  0.08303025, -0.98464581,  1.867767  ]), array([-0.5817114 ,  0.42450509, -0.44787668,  1.4739004 ]), array([-0.60388599,  0.65110485,  0.23506479,  0.75953166]), array([-0.47776744,  0.68939336,  1.00314287, -0.37404036]), array([-0.20561504,  0.47776889,  1.66446085, -1.69065932]), array([ 0.15919797,  0.05131234,  1.89694547, -2.43413717]), array([ 0.51436743, -0.42807718,  1.56922561, -2.21264335]), array([ 0.75959541, -0.79099918,  0.83971197, -1.36055766]), array([ 0.83987915, -0.9617938 , -0.0473906 , -0.33651921]), array([ 0.71906799, -0.86365319, -1.14514988,  1.31993417]), array([ 0.39369819, -0.43791295, -2.05578387,  2.88001213]), array([-0.0674174 ,  0.2296699 , -2.43213322,  3.56106318]), array([-0.52528108,  0.88200445, -2.04419348,  2.78748533]), array([-0.83622703,  1.25593534, -1.03033084,  0.95322675]), array([-0.94779263,  1.32250713, -0.07169325, -0.28023566]), array([-0.84326329,  1.09006103,  1.11350203, -2.05570953]), array([-0.50859901,  0.4965919 ,  2.19021618, -3.83491246]), array([-0.00683289, -0.37252453,  2.67404852, -4.54012252]), array([ 0.49741517, -1.18790108,  2.26642989, -3.43618764]), array([ 0.87543328, -1.72543057,  1.47338468, -1.94387829]), array([ 1.07422384, -1.97347887,  0.49370768, -0.55447229]), array([ 1.06106035, -1.92864197, -0.6252488 ,  1.00512794]), array([ 0.81956839, -1.54062234, -1.77656247,  2.91508194]), array([ 0.35743955, -0.74305069, -2.80816495,  5.05640183]), array([-0.25637383,  0.39484123, -3.11183299,  5.85150465]), array([-0.80211533,  1.41753772, -2.24994748,  4.22392096]), array([-1.14362336,  2.09334249, -1.14967128,  2.58765987]), array([-1.25805661,  2.46814087,  0.00760454,  1.17950062]), array([-1.14294084,  2.56731062,  1.12785145, -0.18901701]), array([-0.81268537,  2.3704952 ,  2.12494281, -1.78662898]), array([-0.31422415,  1.82671303,  2.78643539, -3.66964039]), array([ 0.27791047,  0.89825248,  3.08902234, -5.5729603 ]), array([ 0.8660903 , -0.27456375,  2.60091865, -5.72248619]), array([ 1.25793783, -1.27659738,  1.23360876, -4.17846789]), array([ 1.34987884, -1.94954754, -0.31229337, -2.5667557 ]), array([ 1.14137037, -2.3013719 , -1.73156283, -0.93748835]), array([ 0.67085362, -2.27967992, -2.876467  ,  1.14824605]), array([ 0.04034462, -1.85107679, -3.29989278,  3.09447294]), array([-0.60506095, -1.07103822, -3.08300008,  4.59802201]), array([-1.16700115, -0.08260152, -2.4445068 ,  5.03529461]), array([-1.53792008,  0.84006946, -1.18450092,  4.05039801]), array([-1.62172832,  1.51920429,  0.37560878,  2.71207435]), array([-1.36795497,  1.85697999,  2.13306967,  0.60061739]), array([-0.79965925,  1.75029195,  3.4580646 , -1.7353615 ]), array([-0.02609599,  1.12699725,  4.15437697, -4.45448993]), array([ 0.81050928,  0.04958212,  4.03667933, -5.87621453]), array([ 1.50900968, -1.01432149,  2.84739661, -4.5293363 ]), array([ 1.94602536, -1.77510358,  1.54075062, -3.18285335]), array([ 2.13120334, -2.31782079,  0.3215775 , -2.27529933]), array([ 2.07758935, -2.68208179, -0.85357564, -1.33398797]), array([ 1.78295772, -2.81267322, -2.09952784,  0.08083681]), array([ 1.23104976, -2.60739905, -3.39277037,  2.03861354]), array([ 0.45651635, -1.966091  , -4.23942453,  4.46039508]), array([-0.42516554, -0.80056469, -4.51663109,  7.11843556]), array([-1.27962424,  0.67930413, -3.76775796,  6.9912101 ]), array([-1.8734577 ,  1.86744666, -2.18314449,  4.99975463]), array([-2.16952586,  2.73890942, -0.83254201,  3.79816751]), array([-2.23325886, -2.88637972,  0.12978371,  2.77917426]), array([-2.13190449, -2.43778193,  0.87945175,  1.69633174]), array([-1.86583978, -2.2295763 ,  1.81820778,  0.40092848]), array([-1.38295387, -2.28066577,  3.03295962, -0.82403228]), array([-0.65819123, -2.50756585,  4.14416406, -1.27562387]), array([ 0.21265269, -2.69849172,  4.37668041, -0.44872702]), array([ 1.01862099, -2.63971588,  3.5054854 ,  1.17385792]), array([ 1.5390562 , -2.15392684,  1.54677364,  3.72842434]), array([ 1.59246165, -1.13892406, -1.04858835,  6.47433134]), array([ 1.16043303,  0.41616262, -2.92772942,  8.55906988]), array([ 0.5640299 ,  2.03420356, -2.95212671,  7.50601978]), array([-0.04062301, -2.78051694, -3.1196449 ,  7.4575861 ]), array([-0.70058448, -1.13953708, -3.57360842,  9.27945054]), array([-1.3995825 ,  0.8208936 , -2.87074559,  9.35935321]), array([-1.68472301e+00,  2.38728173e+00, -5.96432255e-03,  6.49715955e+00]), array([-1.50019303, -2.7704709 ,  1.49554683,  4.99330266]), array([-1.18974008, -1.81391382,  1.44683399,  4.8470988 ]), array([-0.97756444, -0.69505724,  0.66253054,  6.48355121]), array([-0.78709207,  0.57213241,  1.68776504,  5.46500939]), array([-0.19639885,  1.27084281,  4.10585705,  1.40299146]), array([ 0.72042592,  1.21334527,  4.74223636, -1.67814222]), array([ 1.61285268,  0.71565363,  4.0527259 , -2.96313463]), array([ 2.32838975,  0.12470637,  3.13692778, -2.83975638])]</t>
+  </si>
+  <si>
+    <t>['[1,1,2]', '[1,1,1]', '[2,1,0]', '[0,1,1]', '[1,2,0]', '[0,2,1]', '[2,2,2]', '[2,0,1]', '[0,0,0]', '[1,0,2]']</t>
+  </si>
+  <si>
+    <t>[1, 2, 4, 9, 10, 14, 17, 19, 22, 29, 36, 44, 47, 48, 50, 51, 53, 55, 58, 59, 63, 64, 70, 71, 75, 76, 77, 78, 80, 81, 85, 88, 91, 92, 95, 97, 101, 103, 104, 106, 107, 114, 115, 116, 117, 122, 124, 125, 126, 130, 133, 135, 136, 137, 144, 153, 156, 159, 162, 163, 164, 166, 167]</t>
+  </si>
+  <si>
+    <t>[0, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 1, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 1, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 1, 2, 2, 2, 2, 2, 2, 2, 1, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 1, 0, 0, 0, 0, 0, 0, 0, 1, 2, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 1, 2, 2]</t>
+  </si>
+  <si>
+    <t>['[-0.03763371 -0.01533471  0.06554052 -0.01816017]', '[-0.0208055  -0.02030166  0.09914155 -0.02801351]', '[ 0.00031733 -0.02489487  0.10765546 -0.0138725 ]', '[ 0.0337014  -0.05856607  0.21818034 -0.31149513]', '[ 0.06996561 -0.10814788  0.13572986 -0.17050685]', '[ 0.09852821 -0.15685011  0.14254113 -0.30361614]', '[ 0.1238476  -0.22355539  0.10347568 -0.34817045]', '[ 0.13732446 -0.29000983  0.02665489 -0.30329561]', '[ 0.13332581 -0.34042543 -0.06714561 -0.19335867]', '[ 0.11111995 -0.36559315 -0.15096966 -0.05777012]', '[ 0.07529972 -0.36462705 -0.19983367  0.06167435]', '[ 0.00879744 -0.2771006  -0.44978527  0.7905486 ]', '[-0.09587055 -0.06364127 -0.5696234   1.29212478]', '[-0.20613018  0.21390629 -0.50056622  1.4158688 ]', '[-0.25813801  0.40941612 -0.00636887  0.50544445]', '[-0.23345875  0.47680191  0.2495623   0.16182281]', '[-0.13686313  0.40889189  0.69549142 -0.81880514]', '[ 0.01943064  0.19990927  0.83040016 -1.21311703]', '[ 0.1918386  -0.08274725  0.84942024 -1.53521311]', '[ 0.32785439 -0.34690595  0.47679202 -1.04410417]', '[ 0.38573214 -0.51566509  0.08734339 -0.61207739]', '[ 0.36037281 -0.58382726 -0.33693299 -0.0633068 ]', '[ 0.25602517 -0.54296453 -0.68532592  0.45421191]', '[ 0.07264224 -0.34819049 -1.10900315  1.44274713]', '[-0.16700597  0.00261168 -1.22793255  1.9636187 ]', '[-0.39246586  0.3905643  -0.96882579  1.8119019 ]', '[-0.5353307   0.69370778 -0.4287709   1.16592062]', '[-0.55686913  0.84378412  0.21704557  0.31937341]', '[-0.4288283   0.75860584  1.04042946 -1.15942197]', '[-0.16747389  0.42525134  1.52000716 -2.10275734]', '[ 0.16384585 -0.07059995  1.70815599 -2.70345904]', '[ 0.47825708 -0.58650568  1.35763383 -2.31625427]', '[ 0.68335885 -0.95980389  0.65829965 -1.37070655]', '[ 0.73387279 -1.12639867 -0.15824092 -0.28686126]', '[ 0.60175708 -1.01618638 -1.1438718   1.38924099]', '[ 0.28847066 -0.57461764 -1.94043838  2.97662553]', '[-0.11577746  0.05413702 -1.992633    3.1044147 ]', '[-0.48944063  0.64816227 -1.65034839  2.66676023]', '[-0.74852854  1.07867709 -0.9002457   1.5940655 ]', '[-0.84028752  1.27998834 -0.00824144  0.41545862]', '[-0.73294401  1.18950651  1.0679587  -1.32655846]', '[-0.42232133  0.74643829  2.00053996 -3.0852529 ]', '[ 0.03963163 -0.00623713  2.50116334 -4.21735665]', '[ 0.51598092 -0.81336504  2.13494417 -3.60721246]', '[ 0.85112943 -1.37276013  1.18216307 -1.97516013]', '[ 0.99028469 -1.63479424  0.19814721 -0.65452425]', '[ 0.91294619 -1.58710126 -0.96133876  1.13973184]', '[ 0.63155594 -1.22235582 -1.82029924  2.51315503]', '[ 0.20380125 -0.59125851 -2.38449846  3.70201738]', '[-0.30237978  0.24177118 -2.52965919  4.32707481]', '[-0.72412672  0.95598728 -1.61000747  2.69061575]', '[-0.93266455  1.31099062 -0.46166321  0.8743596 ]', '[-0.92618124  1.36316081  0.52413434 -0.35467998]', '[-0.71836675  1.13905112  1.53057471 -1.89630067]', '[-0.3172984   0.57607803  2.42404983 -3.68067031]', '[ 0.19649455 -0.22718036  2.56696368 -4.05592951]', '[ 0.66288851 -0.96021119  1.99590235 -3.09969416]', '[ 0.97127263 -1.44221261  1.0563647  -1.71880258]', '[ 1.06941686 -1.62878076 -0.07982499 -0.16022466]', '[ 0.94941159 -1.53038809 -1.10690694  1.15587006]', '[ 0.61725531 -1.10616098 -2.18586792  3.11307882]', '[ 0.09377097 -0.29189887 -2.95238599  4.86937919]', '[-0.49350161  0.69431764 -2.73850266  4.60813692]', '[-0.93227328  1.40764511 -1.61244653  2.5211056 ]', '[-1.132064    1.72059339 -0.3767454   0.64436085]', '[-1.08182414  1.67121637  0.87481718 -1.14639311]', '[-0.78654819  1.24994121  2.06084585 -3.10977034]', '[-0.26928796  0.41760447  3.03760677 -5.11326138]', '[ 0.36027366 -0.65377883  3.04955456 -5.14690772]', '[ 0.88973885 -1.52069654  2.18140952 -3.46076107]', '[ 1.21244777 -2.02934505  1.02927271 -1.68043814]', '[ 1.29709542 -2.20689928 -0.18592    -0.10907153]', '[ 1.13312817 -2.0496399  -1.43969708  1.70611976]', '[ 0.73020339 -1.50580309 -2.56405497  3.79794991]', '[ 0.11897885 -0.50859375 -3.47699296  6.08261795]', '[-0.55335533  0.68275944 -3.01321626  5.31320154]', '[-1.03445388  1.51870597 -1.76721655  3.05902865]', '[-1.25745299  1.93395826 -0.45996471  1.14395415]', '[-1.2189222   1.9849518   0.83760497 -0.63810973]', '[-0.92864774  1.66793019  2.04192479 -2.57919295]', '[-0.42334913  0.95690422  2.9673672  -4.54167405]', '[ 0.22127232 -0.09300508  3.29701165 -5.56761215]', '[ 0.81925845 -1.10668492  2.54386521 -4.29958407]', '[ 1.21645508 -1.79591058  1.40731264 -2.63761301]', '[ 1.37763807 -2.1807326   0.19960961 -1.23707798]', '[ 1.28384483 -2.25065645 -1.12377162  0.54855873]', '[ 0.93762399 -1.94952902 -2.3024704   2.50940945]', '[ 0.38068522 -1.22245585 -3.22620295  4.81482019]', '[-0.30289961 -0.11080831 -3.44056848  5.9349181 ]', '[-0.92514815  0.99945734 -2.61331412  4.81751471]', '[-1.32175607  1.78702601 -1.33781626  3.10959235]', '[-1.44474828  2.22120456  0.09696522  1.26892907]', '[-1.2948159   2.31662757  1.38470311 -0.33382237]', '[-0.89671858  2.05393688  2.54667114 -2.33673026]', '[-0.30170232  1.36143374  3.34507632 -4.63121806]', '[ 0.40471773  0.24801637  3.58050127 -6.20006352]', '[ 1.0490922  -0.93106354  2.67791116 -5.19028734]', '[ 1.43727732 -1.7651777   1.20284754 -3.22675003]', '[ 1.54024344 -2.26960331 -0.16830535 -1.8360855 ]', '[ 1.3682144  -2.47590819 -1.530471   -0.20649717]', '[ 0.93552652 -2.320629   -2.73819     1.79179295]', '[ 0.32102679 -1.79047654 -3.30653024  3.51441382]', '[-0.3672287  -0.87633985 -3.50805423  5.54298982]', '[-1.01013525  0.24694491 -2.74492978  5.26138656]', '[-1.41063446  1.11115196 -1.21745076  3.33169396]', '[-1.51403328  1.64655515  0.19330959  2.02150496]', '[-1.31821793  1.86242455  1.73985234  0.09358154]', '[-0.84293685  1.68220792  2.94889281 -1.95572706]', '[-0.16422561  1.03950525  3.74932252 -4.45503971]', '[ 0.61079205 -0.02901872  3.81653499 -5.7963951 ]', '[ 1.27611088 -1.07075742  2.71970496 -4.38085377]', '[ 1.6881676  -1.78700754  1.40337675 -2.86635069]', '[ 1.83926643 -2.24288139  0.11090094 -1.71726437]', '[ 1.7271679  -2.44969967 -1.22733803 -0.31954703]', '[ 1.35705356 -2.37164334 -2.45666757  1.16048988]', '[ 0.76185381 -1.95948634 -3.42110476  3.02321091]', '[ 0.02638239 -1.14861892 -3.84397709  5.04779452]', '[-0.7298065  -0.02630971 -3.53752326  5.72953373]', '[-1.33360939  1.01438003 -2.38821913  4.44828624]', '[-1.67275685  1.75255921 -1.00079671  2.99615538]', '[-1.73406566  2.22862887  0.3858229   1.76566663]', '[-1.51460008  2.42691396  1.79300615  0.17416926]', '[-1.02824024  2.27768208  3.01644129 -1.72118078]', '[-0.33671028  1.69652961  3.79688548 -4.132041  ]', '[ 0.44523269  0.65578354  3.92949011 -6.10091614]', '[ 1.16440239 -0.56046342  3.06388074 -5.57003472]', '[ 1.62672256 -1.48316203  1.54691122 -3.69608647]', '[ 1.79428161 -2.09408593  0.12961378 -2.44365639]', '[ 1.67990454 -2.45722486 -1.26518472 -1.15288989]', '[ 1.2824571  -2.49619818 -2.67461723  0.81228739]', '[ 0.64728575 -2.15426986 -3.57926687  2.64321303]', '[-0.11369297 -1.38941935 -3.92851967  4.98783159]', '[-0.89266468 -0.20688613 -3.73716544  6.49370316]', '[-1.50434763  0.9373924  -2.26515145  4.69537657]', '[-1.81201999  1.73523532 -0.80672642  3.3375817 ]', '[-1.81245319  2.23929512  0.78843358  1.70108792]', '[-1.51472838  2.44083083  2.17487624  0.25273616]', '[-0.94986051  2.2954772   3.40372354 -1.76292344]', '[-0.19142239  1.69703065  4.05594142 -4.2431211 ]', '[ 0.63213856  0.61359926  4.09321694 -6.40007833]', '[ 1.37719991 -0.6694766   3.16724988 -5.94051409]', '[ 1.86080059 -1.68767451  1.66672817 -4.31167727]', '[ 2.04949177 -2.43043336  0.23921991 -3.15740787]', '[ 1.96735922 -2.94948645 -1.03012733 -2.00995747]', '[ 1.63315506  3.0977564  -2.30933726 -0.33645502]', '[ 1.04347929 -3.08527141 -3.56060969  1.31956431]', '[ 0.24301736 -2.66652462 -4.2898761   2.8481368 ]', '[-0.59370454 -1.95908828 -3.9165869   4.15809548]', '[-1.28968739 -1.04705782 -3.02477826  4.83202127]', '[-1.80127481 -0.08261238 -2.0695644   4.68170836]', '[-2.10391598  0.78961262 -0.92225601  4.00580615]', '[-2.15277495  1.51191621  0.48957865  3.17009735]', '[-1.88578459  2.02172394  2.21559243  1.79770776]', '[-1.26251555  2.1523038   3.95381653 -0.62978654]', '[-0.34836697  1.70468224  5.01448092 -3.90744624]', '[ 0.67767963  0.60730652  5.11678588 -6.79217282]', '[ 1.60554808 -0.71715469  3.98538278 -5.8809124 ]', '[ 2.2718797  -1.72460038  2.74367923 -4.35037606]', '[ 2.73240629 -2.52579744  1.93787852 -3.78839482]', '[ 3.07446794  3.03221588  1.58486569 -3.5158242 ]', '[-2.87091635  2.31586847  1.8893867  -3.70431566]', '[-2.41927846  1.51506025  2.71335509 -4.45070098]', '[-1.75858618  0.48671345  3.96760403 -5.96622478]', '[-0.84321596 -0.79985495  5.04786123 -6.36571724]', '[ 0.20641483 -1.84695385  5.31296232 -3.82302957]', '[ 1.21233861 -2.31835532  4.53942173 -0.91867549]', '[ 1.95705311 -2.2325237   2.83129656  1.64152205]', '[ 2.32597721 -1.69827537  0.86255356  3.57207961]', '[ 2.31721652 -0.8363463  -0.89527379  5.02403434]', '[ 1.99372123  0.30820593 -2.24403544  6.32401856]']</t>
+  </si>
+  <si>
+    <t>[0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50, 51, 52, 53, 54, 55, 56, 57, 58, 59, 60, 61, 62, 63, 64, 65, 66, 67, 68, 69, 70, 71, 72, 73, 74, 75, 76, 77, 78, 79, 80, 81, 82, 83, 84, 85, 86, 87, 88, 89, 90, 91, 92, 93, 94, 95, 96, 97, 98, 99, 100, 101, 102, 103, 104, 105, 106, 107, 108, 109, 110, 111, 112, 113, 114, 115, 116, 117, 118, 119, 120, 121, 122, 123, 124, 125, 126, 127, 128, 129, 130, 131, 132, 133, 134, 135, 136, 137, 138, 139, 140, 141, 142, 143, 144, 145, 146, 147, 148, 149, 150, 151, 152, 153, 154, 155, 156, 157, 158, 159, 160, 161, 162, 163, 164, 165, 166, 167, 168, 169]</t>
+  </si>
+  <si>
+    <t>[array([-0.03763371, -0.01533471,  0.06554052, -0.01816017], dtype=float32), array([-0.0208055 , -0.02030166,  0.09914155, -0.02801351]), array([ 0.00031733, -0.02489487,  0.10765546, -0.0138725 ]), array([ 0.0337014 , -0.05856607,  0.21818034, -0.31149513]), array([ 0.06996561, -0.10814788,  0.13572986, -0.17050685]), array([ 0.09852821, -0.15685011,  0.14254113, -0.30361614]), array([ 0.1238476 , -0.22355539,  0.10347568, -0.34817045]), array([ 0.13732446, -0.29000983,  0.02665489, -0.30329561]), array([ 0.13332581, -0.34042543, -0.06714561, -0.19335867]), array([ 0.11111995, -0.36559315, -0.15096966, -0.05777012]), array([ 0.07529972, -0.36462705, -0.19983367,  0.06167435]), array([ 0.00879744, -0.2771006 , -0.44978527,  0.7905486 ]), array([-0.09587055, -0.06364127, -0.5696234 ,  1.29212478]), array([-0.20613018,  0.21390629, -0.50056622,  1.4158688 ]), array([-0.25813801,  0.40941612, -0.00636887,  0.50544445]), array([-0.23345875,  0.47680191,  0.2495623 ,  0.16182281]), array([-0.13686313,  0.40889189,  0.69549142, -0.81880514]), array([ 0.01943064,  0.19990927,  0.83040016, -1.21311703]), array([ 0.1918386 , -0.08274725,  0.84942024, -1.53521311]), array([ 0.32785439, -0.34690595,  0.47679202, -1.04410417]), array([ 0.38573214, -0.51566509,  0.08734339, -0.61207739]), array([ 0.36037281, -0.58382726, -0.33693299, -0.0633068 ]), array([ 0.25602517, -0.54296453, -0.68532592,  0.45421191]), array([ 0.07264224, -0.34819049, -1.10900315,  1.44274713]), array([-0.16700597,  0.00261168, -1.22793255,  1.9636187 ]), array([-0.39246586,  0.3905643 , -0.96882579,  1.8119019 ]), array([-0.5353307 ,  0.69370778, -0.4287709 ,  1.16592062]), array([-0.55686913,  0.84378412,  0.21704557,  0.31937341]), array([-0.4288283 ,  0.75860584,  1.04042946, -1.15942197]), array([-0.16747389,  0.42525134,  1.52000716, -2.10275734]), array([ 0.16384585, -0.07059995,  1.70815599, -2.70345904]), array([ 0.47825708, -0.58650568,  1.35763383, -2.31625427]), array([ 0.68335885, -0.95980389,  0.65829965, -1.37070655]), array([ 0.73387279, -1.12639867, -0.15824092, -0.28686126]), array([ 0.60175708, -1.01618638, -1.1438718 ,  1.38924099]), array([ 0.28847066, -0.57461764, -1.94043838,  2.97662553]), array([-0.11577746,  0.05413702, -1.992633  ,  3.1044147 ]), array([-0.48944063,  0.64816227, -1.65034839,  2.66676023]), array([-0.74852854,  1.07867709, -0.9002457 ,  1.5940655 ]), array([-0.84028752,  1.27998834, -0.00824144,  0.41545862]), array([-0.73294401,  1.18950651,  1.0679587 , -1.32655846]), array([-0.42232133,  0.74643829,  2.00053996, -3.0852529 ]), array([ 0.03963163, -0.00623713,  2.50116334, -4.21735665]), array([ 0.51598092, -0.81336504,  2.13494417, -3.60721246]), array([ 0.85112943, -1.37276013,  1.18216307, -1.97516013]), array([ 0.99028469, -1.63479424,  0.19814721, -0.65452425]), array([ 0.91294619, -1.58710126, -0.96133876,  1.13973184]), array([ 0.63155594, -1.22235582, -1.82029924,  2.51315503]), array([ 0.20380125, -0.59125851, -2.38449846,  3.70201738]), array([-0.30237978,  0.24177118, -2.52965919,  4.32707481]), array([-0.72412672,  0.95598728, -1.61000747,  2.69061575]), array([-0.93266455,  1.31099062, -0.46166321,  0.8743596 ]), array([-0.92618124,  1.36316081,  0.52413434, -0.35467998]), array([-0.71836675,  1.13905112,  1.53057471, -1.89630067]), array([-0.3172984 ,  0.57607803,  2.42404983, -3.68067031]), array([ 0.19649455, -0.22718036,  2.56696368, -4.05592951]), array([ 0.66288851, -0.96021119,  1.99590235, -3.09969416]), array([ 0.97127263, -1.44221261,  1.0563647 , -1.71880258]), array([ 1.06941686, -1.62878076, -0.07982499, -0.16022466]), array([ 0.94941159, -1.53038809, -1.10690694,  1.15587006]), array([ 0.61725531, -1.10616098, -2.18586792,  3.11307882]), array([ 0.09377097, -0.29189887, -2.95238599,  4.86937919]), array([-0.49350161,  0.69431764, -2.73850266,  4.60813692]), array([-0.93227328,  1.40764511, -1.61244653,  2.5211056 ]), array([-1.132064  ,  1.72059339, -0.3767454 ,  0.64436085]), array([-1.08182414,  1.67121637,  0.87481718, -1.14639311]), array([-0.78654819,  1.24994121,  2.06084585, -3.10977034]), array([-0.26928796,  0.41760447,  3.03760677, -5.11326138]), array([ 0.36027366, -0.65377883,  3.04955456, -5.14690772]), array([ 0.88973885, -1.52069654,  2.18140952, -3.46076107]), array([ 1.21244777, -2.02934505,  1.02927271, -1.68043814]), array([ 1.29709542, -2.20689928, -0.18592   , -0.10907153]), array([ 1.13312817, -2.0496399 , -1.43969708,  1.70611976]), array([ 0.73020339, -1.50580309, -2.56405497,  3.79794991]), array([ 0.11897885, -0.50859375, -3.47699296,  6.08261795]), array([-0.55335533,  0.68275944, -3.01321626,  5.31320154]), array([-1.03445388,  1.51870597, -1.76721655,  3.05902865]), array([-1.25745299,  1.93395826, -0.45996471,  1.14395415]), array([-1.2189222 ,  1.9849518 ,  0.83760497, -0.63810973]), array([-0.92864774,  1.66793019,  2.04192479, -2.57919295]), array([-0.42334913,  0.95690422,  2.9673672 , -4.54167405]), array([ 0.22127232, -0.09300508,  3.29701165, -5.56761215]), array([ 0.81925845, -1.10668492,  2.54386521, -4.29958407]), array([ 1.21645508, -1.79591058,  1.40731264, -2.63761301]), array([ 1.37763807, -2.1807326 ,  0.19960961, -1.23707798]), array([ 1.28384483, -2.25065645, -1.12377162,  0.54855873]), array([ 0.93762399, -1.94952902, -2.3024704 ,  2.50940945]), array([ 0.38068522, -1.22245585, -3.22620295,  4.81482019]), array([-0.30289961, -0.11080831, -3.44056848,  5.9349181 ]), array([-0.92514815,  0.99945734, -2.61331412,  4.81751471]), array([-1.32175607,  1.78702601, -1.33781626,  3.10959235]), array([-1.44474828,  2.22120456,  0.09696522,  1.26892907]), array([-1.2948159 ,  2.31662757,  1.38470311, -0.33382237]), array([-0.89671858,  2.05393688,  2.54667114, -2.33673026]), array([-0.30170232,  1.36143374,  3.34507632, -4.63121806]), array([ 0.40471773,  0.24801637,  3.58050127, -6.20006352]), array([ 1.0490922 , -0.93106354,  2.67791116, -5.19028734]), array([ 1.43727732, -1.7651777 ,  1.20284754, -3.22675003]), array([ 1.54024344, -2.26960331, -0.16830535, -1.8360855 ]), array([ 1.3682144 , -2.47590819, -1.530471  , -0.20649717]), array([ 0.93552652, -2.320629  , -2.73819   ,  1.79179295]), array([ 0.32102679, -1.79047654, -3.30653024,  3.51441382]), array([-0.3672287 , -0.87633985, -3.50805423,  5.54298982]), array([-1.01013525,  0.24694491, -2.74492978,  5.26138656]), array([-1.41063446,  1.11115196, -1.21745076,  3.33169396]), array([-1.51403328,  1.64655515,  0.19330959,  2.02150496]), array([-1.31821793,  1.86242455,  1.73985234,  0.09358154]), array([-0.84293685,  1.68220792,  2.94889281, -1.95572706]), array([-0.16422561,  1.03950525,  3.74932252, -4.45503971]), array([ 0.61079205, -0.02901872,  3.81653499, -5.7963951 ]), array([ 1.27611088, -1.07075742,  2.71970496, -4.38085377]), array([ 1.6881676 , -1.78700754,  1.40337675, -2.86635069]), array([ 1.83926643, -2.24288139,  0.11090094, -1.71726437]), array([ 1.7271679 , -2.44969967, -1.22733803, -0.31954703]), array([ 1.35705356, -2.37164334, -2.45666757,  1.16048988]), array([ 0.76185381, -1.95948634, -3.42110476,  3.02321091]), array([ 0.02638239, -1.14861892, -3.84397709,  5.04779452]), array([-0.7298065 , -0.02630971, -3.53752326,  5.72953373]), array([-1.33360939,  1.01438003, -2.38821913,  4.44828624]), array([-1.67275685,  1.75255921, -1.00079671,  2.99615538]), array([-1.73406566,  2.22862887,  0.3858229 ,  1.76566663]), array([-1.51460008,  2.42691396,  1.79300615,  0.17416926]), array([-1.02824024,  2.27768208,  3.01644129, -1.72118078]), array([-0.33671028,  1.69652961,  3.79688548, -4.132041  ]), array([ 0.44523269,  0.65578354,  3.92949011, -6.10091614]), array([ 1.16440239, -0.56046342,  3.06388074, -5.57003472]), array([ 1.62672256, -1.48316203,  1.54691122, -3.69608647]), array([ 1.79428161, -2.09408593,  0.12961378, -2.44365639]), array([ 1.67990454, -2.45722486, -1.26518472, -1.15288989]), array([ 1.2824571 , -2.49619818, -2.67461723,  0.81228739]), array([ 0.64728575, -2.15426986, -3.57926687,  2.64321303]), array([-0.11369297, -1.38941935, -3.92851967,  4.98783159]), array([-0.89266468, -0.20688613, -3.73716544,  6.49370316]), array([-1.50434763,  0.9373924 , -2.26515145,  4.69537657]), array([-1.81201999,  1.73523532, -0.80672642,  3.3375817 ]), array([-1.81245319,  2.23929512,  0.78843358,  1.70108792]), array([-1.51472838,  2.44083083,  2.17487624,  0.25273616]), array([-0.94986051,  2.2954772 ,  3.40372354, -1.76292344]), array([-0.19142239,  1.69703065,  4.05594142, -4.2431211 ]), array([ 0.63213856,  0.61359926,  4.09321694, -6.40007833]), array([ 1.37719991, -0.6694766 ,  3.16724988, -5.94051409]), array([ 1.86080059, -1.68767451,  1.66672817, -4.31167727]), array([ 2.04949177, -2.43043336,  0.23921991, -3.15740787]), array([ 1.96735922, -2.94948645, -1.03012733, -2.00995747]), array([ 1.63315506,  3.0977564 , -2.30933726, -0.33645502]), array([ 1.04347929, -3.08527141, -3.56060969,  1.31956431]), array([ 0.24301736, -2.66652462, -4.2898761 ,  2.8481368 ]), array([-0.59370454, -1.95908828, -3.9165869 ,  4.15809548]), array([-1.28968739, -1.04705782, -3.02477826,  4.83202127]), array([-1.80127481, -0.08261238, -2.0695644 ,  4.68170836]), array([-2.10391598,  0.78961262, -0.92225601,  4.00580615]), array([-2.15277495,  1.51191621,  0.48957865,  3.17009735]), array([-1.88578459,  2.02172394,  2.21559243,  1.79770776]), array([-1.26251555,  2.1523038 ,  3.95381653, -0.62978654]), array([-0.34836697,  1.70468224,  5.01448092, -3.90744624]), array([ 0.67767963,  0.60730652,  5.11678588, -6.79217282]), array([ 1.60554808, -0.71715469,  3.98538278, -5.8809124 ]), array([ 2.2718797 , -1.72460038,  2.74367923, -4.35037606]), array([ 2.73240629, -2.52579744,  1.93787852, -3.78839482]), array([ 3.07446794,  3.03221588,  1.58486569, -3.5158242 ]), array([-2.87091635,  2.31586847,  1.8893867 , -3.70431566]), array([-2.41927846,  1.51506025,  2.71335509, -4.45070098]), array([-1.75858618,  0.48671345,  3.96760403, -5.96622478]), array([-0.84321596, -0.79985495,  5.04786123, -6.36571724]), array([ 0.20641483, -1.84695385,  5.31296232, -3.82302957]), array([ 1.21233861, -2.31835532,  4.53942173, -0.91867549]), array([ 1.95705311, -2.2325237 ,  2.83129656,  1.64152205]), array([ 2.32597721, -1.69827537,  0.86255356,  3.57207961]), array([ 2.31721652, -0.8363463 , -0.89527379,  5.02403434]), array([ 1.99372123,  0.30820593, -2.24403544,  6.32401856])]</t>
+  </si>
+  <si>
+    <t>['[0,0,0]', '[2,1,0]', '[0,1,1]', '[2,2,2]', '[2,0,1]', '[1,2,0]', '[1,1,2]', '[1,0,2]', '[0,2,1]', '[1,1,1]']</t>
+  </si>
+  <si>
+    <t>[2, 3, 4, 5, 7, 8, 9, 12, 14, 15, 16, 19, 22, 25, 27, 28, 32, 34, 37, 39, 40, 41, 45, 49, 50, 51, 52, 53, 55, 57, 58, 59, 60, 63, 64, 65, 66, 67, 68, 69, 72, 73, 78, 79, 80, 81, 83, 84, 85, 86, 87, 88, 89, 91, 93, 95, 97, 98, 100, 101, 104, 106, 108, 109, 110, 111, 112, 114, 115, 117, 118, 120, 122, 123, 124, 125, 126, 127, 128, 130, 131, 132, 133, 139, 141, 143, 144, 146, 147, 148, 149, 150, 151, 152, 153, 154, 157, 159, 160, 164, 170, 171, 172, 173, 174, 175, 178, 180, 181, 182, 183, 187, 188, 189, 191, 192, 194, 195, 196, 197]</t>
+  </si>
+  <si>
+    <t>[0, 0, 0, 0, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2]</t>
+  </si>
+  <si>
+    <t>['[-0.03763371 -0.01533471  0.06554052 -0.01816017]', '[-0.00754409 -0.05458322  0.2277812  -0.36241836]', '[ 0.03557041 -0.11811661  0.19275289 -0.25552579]', '[ 0.06573284 -0.15080759  0.10193248 -0.0615216 ]', '[ 0.074488   -0.14056792 -0.01570518  0.16324094]', '[ 0.07329543 -0.12208375  0.0045646   0.01832801]', '[ 0.0498401  -0.06504108 -0.23241544  0.538389  ]', '[ 0.01196863  0.01441307 -0.13626441  0.23682794]', '[-0.00177963  0.02458025  0.00166247 -0.13858628]', '[-0.00096817 -0.00485241  0.00537069 -0.15053382]', '[ 0.01315386 -0.0677344   0.13077331 -0.46477989]', '[ 0.04795348 -0.18252585  0.20624227 -0.65736369]', '[ 0.07745902 -0.28496781  0.08037706 -0.34645635]', '[ 0.0910353  -0.34929612  0.05091132 -0.28436374]', '[ 0.08352579 -0.36098776 -0.12438919  0.16751256]', '[ 0.05652741 -0.31934798 -0.13898592  0.23798714]', '[ 0.03076392 -0.27070399 -0.11206922  0.23645985]', '[-0.01211695 -0.16149099 -0.30529229  0.83167604]', '[-0.08447864  0.04708233 -0.39663179  1.20602288]', '[-0.13442393  0.23019122 -0.08787744  0.58785697]', '[-0.14298371  0.34110501  0.00728824  0.50153774]', '[-0.13044203  0.42421223  0.11755274  0.31853804]', '[-0.08467274  0.43297292  0.33031381 -0.22456991]', '[ 0.00869117  0.30754334  0.58217521 -0.99809482]', '[ 0.13700397  0.0530512   0.66772137 -1.48403803]', '[ 0.24742914 -0.2218096   0.40521205 -1.19961873]', '[ 0.30230624 -0.43910619  0.12629419 -0.93040424]', '[ 0.28151163 -0.54836113 -0.33059155 -0.15162769]', '[ 0.1877539  -0.53394946 -0.58766779  0.28116369]', '[ 0.03138406 -0.37986795 -0.94208301  1.21714818]', '[-0.17184224 -0.07305378 -1.04065166  1.76674914]', '[-0.36287289  0.2869237  -0.81892484  1.73822404]', '[-0.45665991  0.52336003 -0.09969314  0.58828971]', '[-0.42588882  0.58129182  0.40249691 -0.01381665]', '[-0.28923165  0.48811001  0.93657693 -0.89220834]', '[-0.05421892  0.2097033   1.36097272 -1.81618979]', '[ 0.22834422 -0.19439475  1.39228945 -2.09893807]', '[ 0.46121946 -0.54680927  0.88505365 -1.34349784]', '[ 0.58026735 -0.74364043  0.28331073 -0.59491333]', '[ 0.57034628 -0.77863026 -0.38051811  0.24767659]', '[ 0.43327627 -0.6476467  -0.96498345  1.0391884 ]', '[ 0.19954041 -0.38013764 -1.3222068   1.56811772]', '[-0.09695842  0.01006767 -1.57020198  2.21378285]', '[-0.39565531  0.44772013 -1.34250709  2.03450158]', '[-0.6092356   0.78414669 -0.7520066   1.27178596]', '[-0.66333836  0.88375856  0.21662085 -0.27920912]', '[-0.52479267  0.67322227  1.14956893 -1.81128479]', '[-0.21870785  0.17757755  1.84496427 -3.03650254]', '[ 0.17326173 -0.46642367  1.96369666 -3.18894394]', '[ 0.51481595 -0.99376297  1.38955967 -1.99631291]', '[ 0.71273321 -1.25150349  0.56430912 -0.57425083]', '[ 0.73433818 -1.22364109 -0.35314752  0.85202767]', '[ 0.58409417 -0.93942377 -1.12958026  1.9753336 ]', '[ 0.29679118 -0.44923318 -1.68579962  2.83958929]', '[-0.08253229  0.20393414 -1.99981406  3.48406881]', '[-0.43146788  0.78847578 -1.41450096  2.23404256]', '[-0.65195149  1.13386887 -0.75652902  1.18735551]', '[-0.70547738  1.20368164  0.2267813  -0.48720778]', '[-0.57286755  0.96676599  1.08432172 -1.87556347]', '[-0.28354115  0.46386192  1.75626748 -3.0777491 ]', '[ 0.09505594 -0.20223937  1.91988516 -3.36925582]', '[ 0.45190656 -0.82879543  1.56181471 -2.74054498]', '[ 0.69623495 -1.26456465  0.84769556 -1.5863747 ]', '[ 0.7737797  -1.4343303  -0.07696068 -0.11524414]', '[ 0.67645028 -1.33679018 -0.88240499  1.09049224]', '[ 0.43047701 -0.99999212 -1.54183747  2.2560348 ]', '[ 0.08026709 -0.45690523 -1.88791282  3.06112974]', '[-0.28552338  0.15218264 -1.66752306  2.83191698]', '[-0.55077465  0.60855887 -0.92836965  1.63730898]', '[-0.64406708  0.78973973  0.00753145  0.16091815]', '[-0.54813216  0.67212686  0.93717521 -1.32698205]', '[-0.28136088  0.27162424  1.6772059  -2.59964285]', '[ 0.07650084 -0.27559453  1.80534141 -2.69467939]', '[ 0.40325443 -0.73872313  1.39158065 -1.8259143 ]', '[ 0.62380609 -1.01087234  0.777082   -0.86172707]', '[ 0.7042504  -1.07766331  0.01551784  0.19690855]', '[ 0.60743982 -0.87421728 -0.97519796  1.83446218]', '[ 0.32361982 -0.35225444 -1.81145443  3.30737311]', '[-0.05349696  0.31120936 -1.84963138  3.11184281]', '[-0.37705463  0.81897135 -1.32095362  1.86355964]', '[-0.56446987  1.03799452 -0.52551817  0.31130215]', '[-0.59086967  0.9707216   0.2685505  -0.98213156]', '[-0.44681694  0.61801864  1.15407089 -2.51949106]', '[-0.16012989  0.02680474  1.6337645  -3.24206427]', '[ 0.1660358  -0.59813495  1.53625073 -2.82899232]', '[ 0.42619794 -1.05506341  1.02159754 -1.67948179]', '[ 0.56306484 -1.25957177  0.32942665 -0.35713428]', '[ 0.56394851 -1.22394728 -0.32179419  0.71240819]', '[ 0.43732453 -0.97705923 -0.92660257  1.73905938]', '[ 0.2054359  -0.54340123 -1.34576352  2.52476416]', '[-0.10042164  0.05274169 -1.62716297  3.27098824]', '[-0.37916126  0.61783679 -1.08922327  2.24596175]', '[-0.54192379  0.98364433 -0.50903226  1.36579586]', '[-0.55591755  1.09824192  0.36479618 -0.21919795]', '[-0.40107504  0.89705827  1.16183841 -1.78171449]', '[-0.11714755  0.43094302  1.62061991 -2.79195648]', '[ 0.22760799 -0.19430878  1.72776118 -3.2674239 ]', '[ 0.52035129 -0.7635574   1.13197877 -2.30473817]', '[ 0.66462814 -1.09329857  0.29390073 -0.9738787 ]', '[ 0.64667659 -1.17889916 -0.46767008  0.12084116]', '[ 0.48410857 -1.04577413 -1.13075886  1.19834667]', '[ 0.2098624  -0.71104616 -1.56086854  2.09154514]', '[-0.13915541 -0.18163766 -1.84946726  3.06452877]', '[-0.48934912  0.43710896 -1.55543704  2.93612302]', '[-0.70669298  0.87501303 -0.58544326  1.39814878]', '[-0.74064086  1.05040136  0.24942066  0.34418563]', '[-0.59982365  0.98144839  1.13597474 -1.03141994]', '[-0.28901226  0.6131387   1.92178105 -2.60688562]', '[ 0.12515342  0.01746435  2.11535351 -3.16013979]', '[ 0.51038256 -0.5620466   1.64307548 -2.46720021]', '[ 0.75617954 -0.93042505  0.77824239 -1.17983978]', '[ 0.8138541  -1.03005772 -0.207236    0.18473445]', '[ 0.68637417 -0.8858768  -1.04972264  1.2500458 ]', '[ 0.3827787  -0.4754508  -1.93747604  2.80224977]', '[-0.0292267   0.11379919 -2.07450918  2.89158481]', '[-0.40294639  0.60052512 -1.57881826  1.84104914]', '[-0.66031493  0.88247069 -0.95008528  0.93450069]', '[-0.74827532  0.90750242  0.0839769  -0.68274465]', '[-0.63779072  0.64223907  1.00537986 -1.94882641]', '[-0.34733683  0.11489148  1.83499379 -3.21391876]', '[ 0.04272307 -0.53157638  1.95900813 -3.04368696]', '[ 0.41051298 -1.06562939  1.64697983 -2.18967963]', '[ 0.66963024 -1.35893614  0.90762659 -0.73194342]', '[ 0.76230598 -1.35810883  0.00168221  0.73903506]', '[ 0.67736607 -1.09031365 -0.84397855  1.93219631]', '[ 0.43324447 -0.59350992 -1.55471249  2.97675287]', '[ 0.08471771  0.04985933 -1.83149171  3.26720833]', '[-0.25583128  0.62822836 -1.48959305  2.36194065]', '[-0.48745354  0.95877084 -0.79023324  0.90630883]', '[-0.58405365  1.04328287 -0.15986424 -0.06984314]', '[-0.53778079  0.90125957  0.61816674 -1.34309663]', '[-0.34352186  0.51437568  1.28948144 -2.47359114]', '[-0.04582934 -0.04667766  1.60485078 -2.98004219]', '[ 0.26016713 -0.60318793  1.3747831  -2.43475866]', '[ 0.49138804 -1.01060263  0.8947058  -1.57853759]', '[ 0.60667555 -1.22226208  0.24282053 -0.5256174 ]', '[ 0.56610626 -1.16431627 -0.64364642  1.10498361]', '[ 0.35418935 -0.78064723 -1.45093959  2.71291037]', '[ 0.00498747 -0.10695492 -1.9536541   3.86055809]', '[-0.35136011  0.59594655 -1.50763044  2.96822858]', '[-0.59475084  1.09592737 -0.8834908   1.96913463]', '[-0.67582524  1.31998237  0.07345673  0.27713509]', '[-0.56820504  1.20762107  0.98805036 -1.40198259]', '[-0.30060321  0.78939772  1.64953189 -2.74501834]', '[ 0.06704991  0.14596021  1.93545404 -3.51991167]', '[ 0.43952936 -0.55886842  1.67897875 -3.31155231]', '[ 0.69395719 -1.08902997  0.8273487  -1.94003521]', '[ 0.76414849 -1.33079168 -0.12652354 -0.4783765 ]', '[ 0.65658495 -1.3068565  -0.93038658  0.71789047]', '[ 0.40387731 -1.04586683 -1.5561963   1.87035541]', '[ 0.05554362 -0.57902454 -1.85877034  2.70184642]', '[-0.3045243  -0.02586512 -1.64787426  2.65305149]', '[-0.56816512  0.41551243 -0.92746883  1.65285651]', '[-0.66066725  0.61179601  0.01701777  0.28746274]', '[-0.57395398  0.56068997  0.8354337  -0.78975491]', '[-0.32558986  0.27359795  1.59938843 -2.01913616]', '[ 0.03653272 -0.20099053  1.93013014 -2.56714253]', '[ 0.39363248 -0.64958139  1.56122021 -1.79484007]', '[ 0.64829654 -0.91948072  0.94139718 -0.86359975]', '[ 0.74693936 -0.95893813  0.03025011  0.46881993]', '[ 0.67064308 -0.76435687 -0.78144467  1.46026199]', '[ 0.41989967 -0.32290796 -1.68072058  2.88795838]', '[ 0.03088821  0.33235016 -2.09923235  3.4497201 ]', '[-0.37282421  0.96545863 -1.84841886  2.72706584]', '[-0.66248441  1.33673122 -1.01279966  0.97815793]', '[-0.7860697   1.41051248 -0.20410576 -0.2393945 ]', '[-0.72075839  1.18803212  0.85980712 -1.9942859 ]', '[-0.44535904  0.60941375  1.8627704  -3.76108701]', '[-0.0084601  -0.25889893  2.36387186 -4.63377618]', '[ 0.4356231  -1.11115299  1.97075432 -3.69129557]', '[ 0.74787048 -1.68308813  1.12737856 -2.03858277]', '[ 0.87973624 -1.93461282  0.1817867  -0.49097559]', '[ 0.82763869 -1.90416716 -0.69424236  0.79664256]', '[ 0.60957521 -1.61381935 -1.45850624  2.11226641]', '[ 0.2585713  -1.05980359 -2.00737607  3.4002897 ]', '[-0.16711811 -0.29032287 -2.14846361  4.10258273]', '[-0.57230674  0.53668544 -1.77244737  3.90187286]', '[-0.83702342  1.19884125 -0.82874643  2.65383566]', '[-0.8795061   1.5417942   0.38885003  0.79125583]', '[-0.69196756  1.51654727  1.44996805 -1.04914228]', '[-0.32727515  1.14615123  2.14279306 -2.63804249]', '[ 0.13875709  0.48513043  2.43070514 -3.832701  ]', '[ 0.5961512  -0.28984651  2.01467439 -3.65288059]', '[ 0.90325547 -0.89688935  1.00253715 -2.33462644]', '[ 0.99829907 -1.2435247  -0.06175778 -1.11901569]', '[ 0.86132661 -1.28603343 -1.2842887   0.7067575 ]', '[ 0.49876111 -0.95335461 -2.2936653   2.62201868]', '[-0.00431904 -0.32367526 -2.62928435  3.49831484]', '[-0.4975331   0.33970012 -2.17524918  2.89124076]', '[-0.83646621  0.76904478 -1.16160875  1.34367294]', '[-0.97409127  0.93397466 -0.19886477  0.30170595]', '[-0.90297958  0.85927056  0.90256667 -1.05089613]', '[-0.62111255  0.51451487  1.87652185 -2.36475799]', '[-0.16702692 -0.08232686  2.55789174 -3.41488612]', '[ 0.33430065 -0.71245338  2.33614131 -2.67538519]', '[ 0.7307232  -1.10242104  1.56537332 -1.18059073]', '[ 0.94225943 -1.18349189  0.5209079   0.3574459 ]', '[ 0.94333707 -0.99302914 -0.51071712  1.53434303]', '[ 0.71888233 -0.51285067 -1.70885085  3.24327466]', '[ 0.28624315  0.2602315  -2.49854267  4.24930248]']</t>
+  </si>
+  <si>
+    <t>[0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50, 51, 52, 53, 54, 55, 56, 57, 58, 59, 60, 61, 62, 63, 64, 65, 66, 67, 68, 69, 70, 71, 72, 73, 74, 75, 76, 77, 78, 79, 80, 81, 82, 83, 84, 85, 86, 87, 88, 89, 90, 91, 92, 93, 94, 95, 96, 97, 98, 99, 100, 101, 102, 103, 104, 105, 106, 107, 108, 109, 110, 111, 112, 113, 114, 115, 116, 117, 118, 119, 120, 121, 122, 123, 124, 125, 126, 127, 128, 129, 130, 131, 132, 133, 134, 135, 136, 137, 138, 139, 140, 141, 142, 143, 144, 145, 146, 147, 148, 149, 150, 151, 152, 153, 154, 155, 156, 157, 158, 159, 160, 161, 162, 163, 164, 165, 166, 167, 168, 169, 170, 171, 172, 173, 174, 175, 176, 177, 178, 179, 180, 181, 182, 183, 184, 185, 186, 187, 188, 189, 190, 191, 192, 193, 194, 195, 196, 197, 198, 199]</t>
+  </si>
+  <si>
+    <t>[array([-0.03763371, -0.01533471,  0.06554052, -0.01816017], dtype=float32), array([-0.00754409, -0.05458322,  0.2277812 , -0.36241836]), array([ 0.03557041, -0.11811661,  0.19275289, -0.25552579]), array([ 0.06573284, -0.15080759,  0.10193248, -0.0615216 ]), array([ 0.074488  , -0.14056792, -0.01570518,  0.16324094]), array([ 0.07329543, -0.12208375,  0.0045646 ,  0.01832801]), array([ 0.0498401 , -0.06504108, -0.23241544,  0.538389  ]), array([ 0.01196863,  0.01441307, -0.13626441,  0.23682794]), array([-0.00177963,  0.02458025,  0.00166247, -0.13858628]), array([-0.00096817, -0.00485241,  0.00537069, -0.15053382]), array([ 0.01315386, -0.0677344 ,  0.13077331, -0.46477989]), array([ 0.04795348, -0.18252585,  0.20624227, -0.65736369]), array([ 0.07745902, -0.28496781,  0.08037706, -0.34645635]), array([ 0.0910353 , -0.34929612,  0.05091132, -0.28436374]), array([ 0.08352579, -0.36098776, -0.12438919,  0.16751256]), array([ 0.05652741, -0.31934798, -0.13898592,  0.23798714]), array([ 0.03076392, -0.27070399, -0.11206922,  0.23645985]), array([-0.01211695, -0.16149099, -0.30529229,  0.83167604]), array([-0.08447864,  0.04708233, -0.39663179,  1.20602288]), array([-0.13442393,  0.23019122, -0.08787744,  0.58785697]), array([-0.14298371,  0.34110501,  0.00728824,  0.50153774]), array([-0.13044203,  0.42421223,  0.11755274,  0.31853804]), array([-0.08467274,  0.43297292,  0.33031381, -0.22456991]), array([ 0.00869117,  0.30754334,  0.58217521, -0.99809482]), array([ 0.13700397,  0.0530512 ,  0.66772137, -1.48403803]), array([ 0.24742914, -0.2218096 ,  0.40521205, -1.19961873]), array([ 0.30230624, -0.43910619,  0.12629419, -0.93040424]), array([ 0.28151163, -0.54836113, -0.33059155, -0.15162769]), array([ 0.1877539 , -0.53394946, -0.58766779,  0.28116369]), array([ 0.03138406, -0.37986795, -0.94208301,  1.21714818]), array([-0.17184224, -0.07305378, -1.04065166,  1.76674914]), array([-0.36287289,  0.2869237 , -0.81892484,  1.73822404]), array([-0.45665991,  0.52336003, -0.09969314,  0.58828971]), array([-0.42588882,  0.58129182,  0.40249691, -0.01381665]), array([-0.28923165,  0.48811001,  0.93657693, -0.89220834]), array([-0.05421892,  0.2097033 ,  1.36097272, -1.81618979]), array([ 0.22834422, -0.19439475,  1.39228945, -2.09893807]), array([ 0.46121946, -0.54680927,  0.88505365, -1.34349784]), array([ 0.58026735, -0.74364043,  0.28331073, -0.59491333]), array([ 0.57034628, -0.77863026, -0.38051811,  0.24767659]), array([ 0.43327627, -0.6476467 , -0.96498345,  1.0391884 ]), array([ 0.19954041, -0.38013764, -1.3222068 ,  1.56811772]), array([-0.09695842,  0.01006767, -1.57020198,  2.21378285]), array([-0.39565531,  0.44772013, -1.34250709,  2.03450158]), array([-0.6092356 ,  0.78414669, -0.7520066 ,  1.27178596]), array([-0.66333836,  0.88375856,  0.21662085, -0.27920912]), array([-0.52479267,  0.67322227,  1.14956893, -1.81128479]), array([-0.21870785,  0.17757755,  1.84496427, -3.03650254]), array([ 0.17326173, -0.46642367,  1.96369666, -3.18894394]), array([ 0.51481595, -0.99376297,  1.38955967, -1.99631291]), array([ 0.71273321, -1.25150349,  0.56430912, -0.57425083]), array([ 0.73433818, -1.22364109, -0.35314752,  0.85202767]), array([ 0.58409417, -0.93942377, -1.12958026,  1.9753336 ]), array([ 0.29679118, -0.44923318, -1.68579962,  2.83958929]), array([-0.08253229,  0.20393414, -1.99981406,  3.48406881]), array([-0.43146788,  0.78847578, -1.41450096,  2.23404256]), array([-0.65195149,  1.13386887, -0.75652902,  1.18735551]), array([-0.70547738,  1.20368164,  0.2267813 , -0.48720778]), array([-0.57286755,  0.96676599,  1.08432172, -1.87556347]), array([-0.28354115,  0.46386192,  1.75626748, -3.0777491 ]), array([ 0.09505594, -0.20223937,  1.91988516, -3.36925582]), array([ 0.45190656, -0.82879543,  1.56181471, -2.74054498]), array([ 0.69623495, -1.26456465,  0.84769556, -1.5863747 ]), array([ 0.7737797 , -1.4343303 , -0.07696068, -0.11524414]), array([ 0.67645028, -1.33679018, -0.88240499,  1.09049224]), array([ 0.43047701, -0.99999212, -1.54183747,  2.2560348 ]), array([ 0.08026709, -0.45690523, -1.88791282,  3.06112974]), array([-0.28552338,  0.15218264, -1.66752306,  2.83191698]), array([-0.55077465,  0.60855887, -0.92836965,  1.63730898]), array([-0.64406708,  0.78973973,  0.00753145,  0.16091815]), array([-0.54813216,  0.67212686,  0.93717521, -1.32698205]), array([-0.28136088,  0.27162424,  1.6772059 , -2.59964285]), array([ 0.07650084, -0.27559453,  1.80534141, -2.69467939]), array([ 0.40325443, -0.73872313,  1.39158065, -1.8259143 ]), array([ 0.62380609, -1.01087234,  0.777082  , -0.86172707]), array([ 0.7042504 , -1.07766331,  0.01551784,  0.19690855]), array([ 0.60743982, -0.87421728, -0.97519796,  1.83446218]), array([ 0.32361982, -0.35225444, -1.81145443,  3.30737311]), array([-0.05349696,  0.31120936, -1.84963138,  3.11184281]), array([-0.37705463,  0.81897135, -1.32095362,  1.86355964]), array([-0.56446987,  1.03799452, -0.52551817,  0.31130215]), array([-0.59086967,  0.9707216 ,  0.2685505 , -0.98213156]), array([-0.44681694,  0.61801864,  1.15407089, -2.51949106]), array([-0.16012989,  0.02680474,  1.6337645 , -3.24206427]), array([ 0.1660358 , -0.59813495,  1.53625073, -2.82899232]), array([ 0.42619794, -1.05506341,  1.02159754, -1.67948179]), array([ 0.56306484, -1.25957177,  0.32942665, -0.35713428]), array([ 0.56394851, -1.22394728, -0.32179419,  0.71240819]), array([ 0.43732453, -0.97705923, -0.92660257,  1.73905938]), array([ 0.2054359 , -0.54340123, -1.34576352,  2.52476416]), array([-0.10042164,  0.05274169, -1.62716297,  3.27098824]), array([-0.37916126,  0.61783679, -1.08922327,  2.24596175]), array([-0.54192379,  0.98364433, -0.50903226,  1.36579586]), array([-0.55591755,  1.09824192,  0.36479618, -0.21919795]), array([-0.40107504,  0.89705827,  1.16183841, -1.78171449]), array([-0.11714755,  0.43094302,  1.62061991, -2.79195648]), array([ 0.22760799, -0.19430878,  1.72776118, -3.2674239 ]), array([ 0.52035129, -0.7635574 ,  1.13197877, -2.30473817]), array([ 0.66462814, -1.09329857,  0.29390073, -0.9738787 ]), array([ 0.64667659, -1.17889916, -0.46767008,  0.12084116]), array([ 0.48410857, -1.04577413, -1.13075886,  1.19834667]), array([ 0.2098624 , -0.71104616, -1.56086854,  2.09154514]), array([-0.13915541, -0.18163766, -1.84946726,  3.06452877]), array([-0.48934912,  0.43710896, -1.55543704,  2.93612302]), array([-0.70669298,  0.87501303, -0.58544326,  1.39814878]), array([-0.74064086,  1.05040136,  0.24942066,  0.34418563]), array([-0.59982365,  0.98144839,  1.13597474, -1.03141994]), array([-0.28901226,  0.6131387 ,  1.92178105, -2.60688562]), array([ 0.12515342,  0.01746435,  2.11535351, -3.16013979]), array([ 0.51038256, -0.5620466 ,  1.64307548, -2.46720021]), array([ 0.75617954, -0.93042505,  0.77824239, -1.17983978]), array([ 0.8138541 , -1.03005772, -0.207236  ,  0.18473445]), array([ 0.68637417, -0.8858768 , -1.04972264,  1.2500458 ]), array([ 0.3827787 , -0.4754508 , -1.93747604,  2.80224977]), array([-0.0292267 ,  0.11379919, -2.07450918,  2.89158481]), array([-0.40294639,  0.60052512, -1.57881826,  1.84104914]), array([-0.66031493,  0.88247069, -0.95008528,  0.93450069]), array([-0.74827532,  0.90750242,  0.0839769 , -0.68274465]), array([-0.63779072,  0.64223907,  1.00537986, -1.94882641]), array([-0.34733683,  0.11489148,  1.83499379, -3.21391876]), array([ 0.04272307, -0.53157638,  1.95900813, -3.04368696]), array([ 0.41051298, -1.06562939,  1.64697983, -2.18967963]), array([ 0.66963024, -1.35893614,  0.90762659, -0.73194342]), array([ 0.76230598, -1.35810883,  0.00168221,  0.73903506]), array([ 0.67736607, -1.09031365, -0.84397855,  1.93219631]), array([ 0.43324447, -0.59350992, -1.55471249,  2.97675287]), array([ 0.08471771,  0.04985933, -1.83149171,  3.26720833]), array([-0.25583128,  0.62822836, -1.48959305,  2.36194065]), array([-0.48745354,  0.95877084, -0.79023324,  0.90630883]), array([-0.58405365,  1.04328287, -0.15986424, -0.06984314]), array([-0.53778079,  0.90125957,  0.61816674, -1.34309663]), array([-0.34352186,  0.51437568,  1.28948144, -2.47359114]), array([-0.04582934, -0.04667766,  1.60485078, -2.98004219]), array([ 0.26016713, -0.60318793,  1.3747831 , -2.43475866]), array([ 0.49138804, -1.01060263,  0.8947058 , -1.57853759]), array([ 0.60667555, -1.22226208,  0.24282053, -0.5256174 ]), array([ 0.56610626, -1.16431627, -0.64364642,  1.10498361]), array([ 0.35418935, -0.78064723, -1.45093959,  2.71291037]), array([ 0.00498747, -0.10695492, -1.9536541 ,  3.86055809]), array([-0.35136011,  0.59594655, -1.50763044,  2.96822858]), array([-0.59475084,  1.09592737, -0.8834908 ,  1.96913463]), array([-0.67582524,  1.31998237,  0.07345673,  0.27713509]), array([-0.56820504,  1.20762107,  0.98805036, -1.40198259]), array([-0.30060321,  0.78939772,  1.64953189, -2.74501834]), array([ 0.06704991,  0.14596021,  1.93545404, -3.51991167]), array([ 0.43952936, -0.55886842,  1.67897875, -3.31155231]), array([ 0.69395719, -1.08902997,  0.8273487 , -1.94003521]), array([ 0.76414849, -1.33079168, -0.12652354, -0.4783765 ]), array([ 0.65658495, -1.3068565 , -0.93038658,  0.71789047]), array([ 0.40387731, -1.04586683, -1.5561963 ,  1.87035541]), array([ 0.05554362, -0.57902454, -1.85877034,  2.70184642]), array([-0.3045243 , -0.02586512, -1.64787426,  2.65305149]), array([-0.56816512,  0.41551243, -0.92746883,  1.65285651]), array([-0.66066725,  0.61179601,  0.01701777,  0.28746274]), array([-0.57395398,  0.56068997,  0.8354337 , -0.78975491]), array([-0.32558986,  0.27359795,  1.59938843, -2.01913616]), array([ 0.03653272, -0.20099053,  1.93013014, -2.56714253]), array([ 0.39363248, -0.64958139,  1.56122021, -1.79484007]), array([ 0.64829654, -0.91948072,  0.94139718, -0.86359975]), array([ 0.74693936, -0.95893813,  0.03025011,  0.46881993]), array([ 0.67064308, -0.76435687, -0.78144467,  1.46026199]), array([ 0.41989967, -0.32290796, -1.68072058,  2.88795838]), array([ 0.03088821,  0.33235016, -2.09923235,  3.4497201 ]), array([-0.37282421,  0.96545863, -1.84841886,  2.72706584]), array([-0.66248441,  1.33673122, -1.01279966,  0.97815793]), array([-0.7860697 ,  1.41051248, -0.20410576, -0.2393945 ]), array([-0.72075839,  1.18803212,  0.85980712, -1.9942859 ]), array([-0.44535904,  0.60941375,  1.8627704 , -3.76108701]), array([-0.0084601 , -0.25889893,  2.36387186, -4.63377618]), array([ 0.4356231 , -1.11115299,  1.97075432, -3.69129557]), array([ 0.74787048, -1.68308813,  1.12737856, -2.03858277]), array([ 0.87973624, -1.93461282,  0.1817867 , -0.49097559]), array([ 0.82763869, -1.90416716, -0.69424236,  0.79664256]), array([ 0.60957521, -1.61381935, -1.45850624,  2.11226641]), array([ 0.2585713 , -1.05980359, -2.00737607,  3.4002897 ]), array([-0.16711811, -0.29032287, -2.14846361,  4.10258273]), array([-0.57230674,  0.53668544, -1.77244737,  3.90187286]), array([-0.83702342,  1.19884125, -0.82874643,  2.65383566]), array([-0.8795061 ,  1.5417942 ,  0.38885003,  0.79125583]), array([-0.69196756,  1.51654727,  1.44996805, -1.04914228]), array([-0.32727515,  1.14615123,  2.14279306, -2.63804249]), array([ 0.13875709,  0.48513043,  2.43070514, -3.832701  ]), array([ 0.5961512 , -0.28984651,  2.01467439, -3.65288059]), array([ 0.90325547, -0.89688935,  1.00253715, -2.33462644]), array([ 0.99829907, -1.2435247 , -0.06175778, -1.11901569]), array([ 0.86132661, -1.28603343, -1.2842887 ,  0.7067575 ]), array([ 0.49876111, -0.95335461, -2.2936653 ,  2.62201868]), array([-0.00431904, -0.32367526, -2.62928435,  3.49831484]), array([-0.4975331 ,  0.33970012, -2.17524918,  2.89124076]), array([-0.83646621,  0.76904478, -1.16160875,  1.34367294]), array([-0.97409127,  0.93397466, -0.19886477,  0.30170595]), array([-0.90297958,  0.85927056,  0.90256667, -1.05089613]), array([-0.62111255,  0.51451487,  1.87652185, -2.36475799]), array([-0.16702692, -0.08232686,  2.55789174, -3.41488612]), array([ 0.33430065, -0.71245338,  2.33614131, -2.67538519]), array([ 0.7307232 , -1.10242104,  1.56537332, -1.18059073]), array([ 0.94225943, -1.18349189,  0.5209079 ,  0.3574459 ]), array([ 0.94333707, -0.99302914, -0.51071712,  1.53434303]), array([ 0.71888233, -0.51285067, -1.70885085,  3.24327466]), array([ 0.28624315,  0.2602315 , -2.49854267,  4.24930248])]</t>
+  </si>
+  <si>
+    <t>['[2,0,1]', '[1,0,2]', '[1,2,0]', '[2,2,2]', '[1,1,2]', '[1,1,1]', '[0,1,1]', '[0,2,1]', '[0,0,0]', '[2,1,0]']</t>
+  </si>
+  <si>
+    <t>[2, 3, 6, 7, 8, 9, 10, 11, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 24, 26, 27, 28, 29, 31, 33, 34, 36, 37, 38, 39, 40, 41, 43, 45, 47, 48, 49, 50, 51, 52, 53, 55, 56, 57, 58, 59, 60, 61, 62, 63, 64, 65, 67, 68, 69, 71, 72, 73, 75, 76, 77, 78, 79, 83, 85, 86, 87, 88, 89, 90, 91, 92, 93, 94, 95, 96, 97, 98, 99, 101, 104, 105, 106, 107, 108, 109, 110, 111, 112, 113, 115, 117, 118, 119, 123, 124, 125, 126, 127, 128, 129, 130, 132, 133, 134, 135, 138, 139, 140, 143, 145, 148, 149, 150, 151, 152, 153, 155, 156, 158, 159, 160, 161, 162, 163, 164, 165, 166, 167, 168, 169, 170, 171, 172, 173, 174, 175, 177, 178, 179, 180, 181, 182, 183, 185, 186, 187, 188, 189, 190, 191, 192, 193, 195, 197, 198]</t>
+  </si>
+  <si>
+    <t>[0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 0, 0, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 2, 2, 2, 2, 0, 0, 0, 2, 0, 2, 0, 2, 2, 2, 2, 0, 0, 0, 0, 2, 2, 2, 2, 0, 2, 0, 0, 0, 0, 0, 2, 2, 2, 2, 0, 0, 0, 0, 2, 0, 2, 2, 0, 2, 2, 0, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 2, 0, 0, 0, 2, 2, 0, 2, 2, 0, 0, 2, 2, 2, 2, 2, 2, 0, 2, 2, 2, 2, 2, 0, 0]</t>
+  </si>
+  <si>
+    <t>['[-0.03763371 -0.01533471  0.06554052 -0.01816017]', '[-0.00754409 -0.05458322  0.2277812  -0.36241836]', '[ 0.03557041 -0.11811661  0.19275289 -0.25552579]', '[ 0.06573284 -0.15080759  0.10193248 -0.0615216 ]', '[ 0.08768179 -0.17469111  0.11234335 -0.16976787]', '[ 0.10838977 -0.21494739  0.08931875 -0.22276025]', '[ 0.10828241 -0.22568195 -0.09040326  0.11669965]', '[ 0.08706594 -0.20484991 -0.11683835  0.084879  ]', '[ 0.06367806 -0.19436317 -0.11202438  0.01469992]', '[ 0.04413984 -0.20059304 -0.07966117 -0.07881951]', '[ 0.03293322 -0.22582194 -0.03098382 -0.17077825]', '[ 0.03184047 -0.26696479  0.01898849 -0.23379861]', '[ 0.03966376 -0.31594688  0.05624057 -0.24669522]', '[ 0.03994165 -0.3281348  -0.05356836  0.12630472]', '[ 0.03231072 -0.30127162 -0.02049291  0.13681076]', '[ 0.032399   -0.27549569  0.02203268  0.11679475]', '[ 0.04103963 -0.25584976  0.06313712  0.07782357]', '[ 0.05680443 -0.24462687  0.09161022  0.03502406]', '[ 0.07626355 -0.24116807  0.09913715  0.00198524]', '[ 0.09483524 -0.24262391  0.08280658 -0.01350601]', '[ 0.1079922  -0.24535953  0.0460726  -0.01147104]', '[ 0.11247577 -0.24648294 -0.00212208  0.00102613]', '[ 0.10717225 -0.24497803 -0.04975712  0.01291971]', '[ 0.06718922 -0.17416826 -0.33996372  0.67753301]', '[ 0.00467567 -0.055485   -0.26874477  0.47900256]', '[-0.06108861  0.0756855  -0.37118029  0.79925315]', '[-0.10917576  0.17990345 -0.0975127   0.21924811]', '[-0.09797516  0.15923209  0.20633229 -0.42025959]', '[-0.04412165  0.05399896  0.31797462 -0.60563557]', '[ 0.02242121 -0.0704892   0.3300093  -0.60727271]', '[ 0.09405152 -0.21027285  0.36714522 -0.75481638]', '[ 0.14828098 -0.32353349  0.16172983 -0.35246913]', '[ 0.16831547 -0.37841705  0.0333236  -0.18498879]', '[ 0.16066125 -0.3947358  -0.10855509  0.0229766 ]', '[ 0.12668788 -0.37074215 -0.2236102   0.20805531]', '[ 0.0493945  -0.24957652 -0.53116208  0.97423927]', '[-0.04877893 -0.06825935 -0.42477171  0.79162314]', '[-0.11130552  0.05013325 -0.18441926  0.36263213]', '[-0.11855417  0.06935023  0.11355297 -0.17407456]', '[-0.08136525  0.0184686   0.24911504 -0.32009856]', '[-0.02380275 -0.05109336  0.31262719 -0.35451962]', '[ 0.03762341 -0.11438492  0.28728963 -0.25814669]', '[ 0.09891897 -0.1812505   0.31111403 -0.38939161]', '[ 0.14284551 -0.2268758   0.11832184 -0.05339696]', '[ 0.13099075 -0.16638885 -0.23265428  0.64629249]', '[ 0.08142862 -0.04808667 -0.2491019   0.50854262]', '[ 0.0102972   0.09517913 -0.44286673  0.88741864]', '[-0.05972682  0.22045047 -0.24018433  0.33483188]', '[-0.08109692  0.22178569  0.03056013 -0.3242223 ]', '[-0.06172106  0.12920877  0.15647137 -0.58289561]', '[-0.02252424 -0.00137954  0.22329029 -0.69414569]', '[ 0.02205861 -0.13576275  0.20925386 -0.61957329]', '[ 0.05616844 -0.23796745  0.12221515 -0.38062309]', '[ 0.06809914 -0.28146726 -0.00616617 -0.04610873]', '[ 0.04061982 -0.22198863 -0.26151635  0.62724801]', '[-0.00461111 -0.11001301 -0.17810762  0.4661661 ]', '[-0.02640271 -0.04448633 -0.03348061  0.17466084]', '[-0.01695323 -0.04311582  0.12587358 -0.15930333]', '[ 0.00824152 -0.07017155  0.12015404 -0.102774  ]', '[ 0.02885817 -0.08125744  0.08155174 -0.00313373]', '[ 0.03949359 -0.07032739  0.02305761  0.11204746]', '[ 0.05122073 -0.07194505  0.09167226 -0.12589562]', '[ 0.06110282 -0.08355677  0.00491173  0.01306721]', '[ 0.06635842 -0.10104372  0.04593236 -0.18389731]', '[ 0.0650328  -0.11978061 -0.05933049 -0.0007524 ]', '[ 0.05679596 -0.13622576 -0.02198826 -0.16192634]', '[ 0.02979694 -0.11427254 -0.24157933  0.37312046]', '[-0.00852525 -0.06349767 -0.13241849  0.12014908]', '[-0.02063825 -0.06966158  0.01332943 -0.182198  ]', '[-0.01708958 -0.09947308  0.02055479 -0.11033747]', '[ 1.90104577e-04 -1.46194954e-01  1.47061230e-01 -3.45742608e-01]', '[ 0.02527314 -0.19701396  0.09734704 -0.15035095]', '[ 0.03716122 -0.20306     0.01906631  0.09246616]', '[ 0.04592196 -0.19501532  0.06695014 -0.01191608]', '[ 0.036477   -0.138697   -0.15779365  0.5640758 ]', '[ 0.01313989 -0.04733873 -0.06797798  0.33014894]', '[ 0.01131645 -0.01224423  0.05103894  0.01478914]', '[ 0.01952084 -0.00676237  0.02953672  0.04030496]', '[ 0.03600372 -0.03059152  0.13103463 -0.27159387]', '[ 0.05584361 -0.0757059   0.06205273 -0.1689227 ]', '[ 0.0725911  -0.12921918  0.10022181 -0.35413323]', '[ 0.09334345 -0.21109876  0.10043853 -0.44722416]', '[ 0.10994426 -0.30060592  0.05952487 -0.43026816]', '[ 0.10225474 -0.34315804 -0.13538781  0.00944334]', '[ 0.04506835 -0.26486107 -0.42307097  0.7531465 ]', '[-0.03233238 -0.12459328 -0.33086223  0.61316708]', '[-0.08013594 -0.03267259 -0.1347886   0.28297744]', '[-0.08323803 -0.017203    0.10455427 -0.13085223]', '[-0.05357805 -0.04766869  0.18502077 -0.16387419]', '[-0.01268932 -0.07811957  0.21461658 -0.1290636 ]', '[ 0.0283918  -0.09475441  0.18739315 -0.02820183]', '[ 0.05908435 -0.08661305  0.11365503  0.11273295]', '[ 0.08549293 -0.08401964  0.14512486 -0.08306769]', '[ 0.10130813 -0.08265395  0.01004686  0.09859056]', '[ 0.10281357 -0.08003552  0.00475395 -0.07252022]', '[ 0.10294405 -0.11059489 -0.00450215 -0.22762203]', '[ 0.08728015 -0.13376282 -0.1494675  -0.00281713]', '[ 0.05878219 -0.1476521  -0.13028901 -0.13784238]', '[ 0.03694116 -0.18859816 -0.0851218  -0.26769578]', '[ 0.0123501  -0.21811671 -0.1563876  -0.02677724]', '[-0.03619921 -0.16691531 -0.31766154  0.52264116]', '[-0.0818986  -0.08837055 -0.12780174  0.24235409]', '[-0.11104198 -0.00658785 -0.15519537  0.55686037]', '[-0.13997552  0.12461498 -0.12387429  0.72761494]', '[-0.13027604  0.20447354  0.22044717  0.06037743]', '[-0.06841451  0.18458728  0.38485726 -0.24632252]', '[ 0.01675437  0.11404419  0.4473441  -0.43379359]', '[ 0.10204645  0.02284031  0.38553049 -0.44925204]', '[ 0.16345883 -0.05441026  0.21406373 -0.30092317]', '[ 0.18339035 -0.09065512 -0.01954412 -0.05287427]', '[ 0.16901516 -0.1092291  -0.12190114 -0.13178967]', '[ 0.13622308 -0.14295042 -0.20059144 -0.20433358]', '[ 0.09145259 -0.19045377 -0.23976    -0.26895826]', '[ 0.04349186 -0.24965095 -0.2321376  -0.31998004]', '[-0.02435792 -0.249411   -0.43177944  0.31090695]', '[-0.09515778 -0.20278255 -0.26055577  0.13618323]', '[-0.15019251 -0.13224518 -0.27673603  0.54894942]', '[-0.17358918 -0.06253335  0.04927584  0.1331695 ]', '[-0.14413437 -0.04603959  0.23963952  0.03386432]', '[-0.08155381 -0.04643467  0.37336242 -0.02782183]', '[ 0.01224873 -0.08627417  0.54412281 -0.3484857 ]', '[ 0.12621259 -0.17390013  0.56962612 -0.49468386]', '[ 0.22951011 -0.27011109  0.44005969 -0.43632296]', '[ 0.28112861 -0.30385041  0.06567573  0.11003848]', '[ 0.26793567 -0.2605057  -0.19350318  0.31412879]', '[ 0.20750695 -0.18448855 -0.39646724  0.42464127]', '[ 0.11677321 -0.10117005 -0.49009276  0.38063387]', '[ 0.02048578 -0.04376128 -0.45158534  0.16878854]', '[-0.05593859 -0.0418602  -0.29736042 -0.16148062]', '[-0.09395929 -0.10990459 -0.07777257 -0.51236912]', '[-0.10027934 -0.20654557  0.01304187 -0.43901243]', '[-0.07685014 -0.31344092  0.2131264  -0.60802347]', '[-0.03271559 -0.40561276  0.21757341 -0.2934546 ]', '[ 0.00610425 -0.42453525  0.16220951  0.11311447]', '[ 0.04226466 -0.39252754  0.19252738  0.20814393]', '[ 0.08026074 -0.34130107  0.18095245  0.30194938]', '[ 0.08614189 -0.20585194 -0.12042007  1.03265279]', '[ 0.03638362  0.0566849  -0.3570351   1.53730363]', '[-0.01957971  0.31348945 -0.18391396  0.98007167]', '[-0.03262349  0.43481503  0.05670544  0.21660063]', '[-0.01057696  0.43194636  0.1588405  -0.24087399]', '[ 0.04087102  0.30969146  0.34357711 -0.95734382]', '[ 0.11979192  0.06453497  0.4226478  -1.44142199]', '[ 0.18552021 -0.20640775  0.21146494 -1.20946192]', '[ 0.21031676 -0.4331104   0.02398394 -1.01553529]', '[ 0.18005535 -0.56679676 -0.32097855 -0.30956231]', '[ 0.07512051 -0.52542973 -0.70520091  0.70249821]', '[-0.08985671 -0.30085432 -0.90781567  1.48702052]', '[-0.24393465 -0.02964811 -0.59304445  1.15156692]', '[-0.31426118  0.13559099 -0.09205237  0.46385352]', '[-0.27816234  0.14859986  0.44576073 -0.32999197]', '[-0.15690589  0.0470525   0.73945993 -0.64995968]', '[ 0.00390779 -0.09288767  0.83152395 -0.69915253]', '[ 0.16011315 -0.21175702  0.69551512 -0.44544961]', '[ 0.28279377 -0.29043155  0.50511914 -0.31142716]', '[ 0.34045702 -0.29310017  0.06089968  0.2912036 ]', '[ 0.31984069 -0.21086026 -0.26026765  0.51442557]', '[ 0.21521621 -0.02865769 -0.75981427  1.26180252]', '[ 0.05791748  0.19810496 -0.77460081  0.94179623]', '[-0.07971457  0.32529124 -0.5709511   0.28968286]', '[-0.16027515  0.30328971 -0.21858512 -0.5176079 ]', '[-0.17736724  0.15573946  0.04629962 -0.93508445]', '[-0.14508191 -0.05703447  0.26209036 -1.14942791]', '[-0.08015934 -0.28414889  0.36675915 -1.07271232]', '[-0.00669032 -0.46747496  0.34968455 -0.72260123]', '[ 0.05314637 -0.5609158   0.23573057 -0.19134934]', '[ 0.08339349 -0.53901391  0.06025918  0.41270624]', '[ 0.08889535 -0.43162243 -0.00440866  0.64677076]', '[ 0.08288899 -0.28825342 -0.05037866  0.76275259]', '[ 0.07156052 -0.13765669 -0.05543463  0.71509176]', '[ 0.06371197 -0.01328183 -0.01723478  0.50556882]', '[0.06634662 0.05710963 0.04510159 0.18695175]', '[ 0.08148201  0.05945092  0.10310186 -0.16126649]', '[ 0.0922518   0.03036606  0.00163714 -0.12309633]', '[ 0.08178145  0.01197162 -0.10467226 -0.05948246]', '[ 0.0652015  -0.0281824  -0.05916031 -0.33739472]', '[ 0.05819538 -0.1189701  -0.0126775  -0.55529578]', '[ 0.04565418 -0.20845935 -0.1126608  -0.32674643]', '[ 0.01425701 -0.24669579 -0.1956688  -0.05466778]', '[-0.01639327 -0.26600545 -0.10524156 -0.13995949]', '[-0.02639323 -0.30223405  0.00617061 -0.21786578]', '[-0.027429   -0.31664825 -0.01649665  0.07546654]', '[-0.01960006 -0.30683664  0.09330963  0.02254894]', '[ 0.008395   -0.30667927  0.18079234 -0.01628488]', '[ 0.04966734 -0.31074279  0.22332544 -0.01705376]', '[ 0.08094605 -0.27670459  0.08391575  0.35667568]', '[ 0.0956284  -0.20546126  0.0622238   0.34576106]', '[ 0.10574109 -0.14250099  0.03896269  0.27439368]', '[ 0.11132642 -0.09913461  0.01719492  0.15258297]', '[ 0.11275204 -0.08343487 -0.00273121  0.0019757 ]', '[ 0.11028671 -0.098421   -0.02193501 -0.14950945]', '[ 0.10393516 -0.14139966 -0.04173886 -0.27364657]', '[ 0.08037533 -0.17042928 -0.18972101 -0.01567515]', '[ 0.0442759  -0.18385269 -0.16448285 -0.12161956]', '[-0.00929475 -0.15136342 -0.35909659  0.43242148]', '[-0.06602141 -0.08959505 -0.19491399  0.16595736]', '[-0.1100637  -0.0214003  -0.23446276  0.49736199]', '[-0.12818623  0.03092545  0.05811502  0.01483332]', '[-0.10093212  0.01922839  0.20840566 -0.12538145]', '[-0.03527918 -0.04917756  0.43238219 -0.53609008]']</t>
+  </si>
+  <si>
+    <t>[array([-0.03763371, -0.01533471,  0.06554052, -0.01816017], dtype=float32), array([-0.00754409, -0.05458322,  0.2277812 , -0.36241836]), array([ 0.03557041, -0.11811661,  0.19275289, -0.25552579]), array([ 0.06573284, -0.15080759,  0.10193248, -0.0615216 ]), array([ 0.08768179, -0.17469111,  0.11234335, -0.16976787]), array([ 0.10838977, -0.21494739,  0.08931875, -0.22276025]), array([ 0.10828241, -0.22568195, -0.09040326,  0.11669965]), array([ 0.08706594, -0.20484991, -0.11683835,  0.084879  ]), array([ 0.06367806, -0.19436317, -0.11202438,  0.01469992]), array([ 0.04413984, -0.20059304, -0.07966117, -0.07881951]), array([ 0.03293322, -0.22582194, -0.03098382, -0.17077825]), array([ 0.03184047, -0.26696479,  0.01898849, -0.23379861]), array([ 0.03966376, -0.31594688,  0.05624057, -0.24669522]), array([ 0.03994165, -0.3281348 , -0.05356836,  0.12630472]), array([ 0.03231072, -0.30127162, -0.02049291,  0.13681076]), array([ 0.032399  , -0.27549569,  0.02203268,  0.11679475]), array([ 0.04103963, -0.25584976,  0.06313712,  0.07782357]), array([ 0.05680443, -0.24462687,  0.09161022,  0.03502406]), array([ 0.07626355, -0.24116807,  0.09913715,  0.00198524]), array([ 0.09483524, -0.24262391,  0.08280658, -0.01350601]), array([ 0.1079922 , -0.24535953,  0.0460726 , -0.01147104]), array([ 0.11247577, -0.24648294, -0.00212208,  0.00102613]), array([ 0.10717225, -0.24497803, -0.04975712,  0.01291971]), array([ 0.06718922, -0.17416826, -0.33996372,  0.67753301]), array([ 0.00467567, -0.055485  , -0.26874477,  0.47900256]), array([-0.06108861,  0.0756855 , -0.37118029,  0.79925315]), array([-0.10917576,  0.17990345, -0.0975127 ,  0.21924811]), array([-0.09797516,  0.15923209,  0.20633229, -0.42025959]), array([-0.04412165,  0.05399896,  0.31797462, -0.60563557]), array([ 0.02242121, -0.0704892 ,  0.3300093 , -0.60727271]), array([ 0.09405152, -0.21027285,  0.36714522, -0.75481638]), array([ 0.14828098, -0.32353349,  0.16172983, -0.35246913]), array([ 0.16831547, -0.37841705,  0.0333236 , -0.18498879]), array([ 0.16066125, -0.3947358 , -0.10855509,  0.0229766 ]), array([ 0.12668788, -0.37074215, -0.2236102 ,  0.20805531]), array([ 0.0493945 , -0.24957652, -0.53116208,  0.97423927]), array([-0.04877893, -0.06825935, -0.42477171,  0.79162314]), array([-0.11130552,  0.05013325, -0.18441926,  0.36263213]), array([-0.11855417,  0.06935023,  0.11355297, -0.17407456]), array([-0.08136525,  0.0184686 ,  0.24911504, -0.32009856]), array([-0.02380275, -0.05109336,  0.31262719, -0.35451962]), array([ 0.03762341, -0.11438492,  0.28728963, -0.25814669]), array([ 0.09891897, -0.1812505 ,  0.31111403, -0.38939161]), array([ 0.14284551, -0.2268758 ,  0.11832184, -0.05339696]), array([ 0.13099075, -0.16638885, -0.23265428,  0.64629249]), array([ 0.08142862, -0.04808667, -0.2491019 ,  0.50854262]), array([ 0.0102972 ,  0.09517913, -0.44286673,  0.88741864]), array([-0.05972682,  0.22045047, -0.24018433,  0.33483188]), array([-0.08109692,  0.22178569,  0.03056013, -0.3242223 ]), array([-0.06172106,  0.12920877,  0.15647137, -0.58289561]), array([-0.02252424, -0.00137954,  0.22329029, -0.69414569]), array([ 0.02205861, -0.13576275,  0.20925386, -0.61957329]), array([ 0.05616844, -0.23796745,  0.12221515, -0.38062309]), array([ 0.06809914, -0.28146726, -0.00616617, -0.04610873]), array([ 0.04061982, -0.22198863, -0.26151635,  0.62724801]), array([-0.00461111, -0.11001301, -0.17810762,  0.4661661 ]), array([-0.02640271, -0.04448633, -0.03348061,  0.17466084]), array([-0.01695323, -0.04311582,  0.12587358, -0.15930333]), array([ 0.00824152, -0.07017155,  0.12015404, -0.102774  ]), array([ 0.02885817, -0.08125744,  0.08155174, -0.00313373]), array([ 0.03949359, -0.07032739,  0.02305761,  0.11204746]), array([ 0.05122073, -0.07194505,  0.09167226, -0.12589562]), array([ 0.06110282, -0.08355677,  0.00491173,  0.01306721]), array([ 0.06635842, -0.10104372,  0.04593236, -0.18389731]), array([ 0.0650328 , -0.11978061, -0.05933049, -0.0007524 ]), array([ 0.05679596, -0.13622576, -0.02198826, -0.16192634]), array([ 0.02979694, -0.11427254, -0.24157933,  0.37312046]), array([-0.00852525, -0.06349767, -0.13241849,  0.12014908]), array([-0.02063825, -0.06966158,  0.01332943, -0.182198  ]), array([-0.01708958, -0.09947308,  0.02055479, -0.11033747]), array([ 1.90104577e-04, -1.46194954e-01,  1.47061230e-01, -3.45742608e-01]), array([ 0.02527314, -0.19701396,  0.09734704, -0.15035095]), array([ 0.03716122, -0.20306   ,  0.01906631,  0.09246616]), array([ 0.04592196, -0.19501532,  0.06695014, -0.01191608]), array([ 0.036477  , -0.138697  , -0.15779365,  0.5640758 ]), array([ 0.01313989, -0.04733873, -0.06797798,  0.33014894]), array([ 0.01131645, -0.01224423,  0.05103894,  0.01478914]), array([ 0.01952084, -0.00676237,  0.02953672,  0.04030496]), array([ 0.03600372, -0.03059152,  0.13103463, -0.27159387]), array([ 0.05584361, -0.0757059 ,  0.06205273, -0.1689227 ]), array([ 0.0725911 , -0.12921918,  0.10022181, -0.35413323]), array([ 0.09334345, -0.21109876,  0.10043853, -0.44722416]), array([ 0.10994426, -0.30060592,  0.05952487, -0.43026816]), array([ 0.10225474, -0.34315804, -0.13538781,  0.00944334]), array([ 0.04506835, -0.26486107, -0.42307097,  0.7531465 ]), array([-0.03233238, -0.12459328, -0.33086223,  0.61316708]), array([-0.08013594, -0.03267259, -0.1347886 ,  0.28297744]), array([-0.08323803, -0.017203  ,  0.10455427, -0.13085223]), array([-0.05357805, -0.04766869,  0.18502077, -0.16387419]), array([-0.01268932, -0.07811957,  0.21461658, -0.1290636 ]), array([ 0.0283918 , -0.09475441,  0.18739315, -0.02820183]), array([ 0.05908435, -0.08661305,  0.11365503,  0.11273295]), array([ 0.08549293, -0.08401964,  0.14512486, -0.08306769]), array([ 0.10130813, -0.08265395,  0.01004686,  0.09859056]), array([ 0.10281357, -0.08003552,  0.00475395, -0.07252022]), array([ 0.10294405, -0.11059489, -0.00450215, -0.22762203]), array([ 0.08728015, -0.13376282, -0.1494675 , -0.00281713]), array([ 0.05878219, -0.1476521 , -0.13028901, -0.13784238]), array([ 0.03694116, -0.18859816, -0.0851218 , -0.26769578]), array([ 0.0123501 , -0.21811671, -0.1563876 , -0.02677724]), array([-0.03619921, -0.16691531, -0.31766154,  0.52264116]), array([-0.0818986 , -0.08837055, -0.12780174,  0.24235409]), array([-0.11104198, -0.00658785, -0.15519537,  0.55686037]), array([-0.13997552,  0.12461498, -0.12387429,  0.72761494]), array([-0.13027604,  0.20447354,  0.22044717,  0.06037743]), array([-0.06841451,  0.18458728,  0.38485726, -0.24632252]), array([ 0.01675437,  0.11404419,  0.4473441 , -0.43379359]), array([ 0.10204645,  0.02284031,  0.38553049, -0.44925204]), array([ 0.16345883, -0.05441026,  0.21406373, -0.30092317]), array([ 0.18339035, -0.09065512, -0.01954412, -0.05287427]), array([ 0.16901516, -0.1092291 , -0.12190114, -0.13178967]), array([ 0.13622308, -0.14295042, -0.20059144, -0.20433358]), array([ 0.09145259, -0.19045377, -0.23976   , -0.26895826]), array([ 0.04349186, -0.24965095, -0.2321376 , -0.31998004]), array([-0.02435792, -0.249411  , -0.43177944,  0.31090695]), array([-0.09515778, -0.20278255, -0.26055577,  0.13618323]), array([-0.15019251, -0.13224518, -0.27673603,  0.54894942]), array([-0.17358918, -0.06253335,  0.04927584,  0.1331695 ]), array([-0.14413437, -0.04603959,  0.23963952,  0.03386432]), array([-0.08155381, -0.04643467,  0.37336242, -0.02782183]), array([ 0.01224873, -0.08627417,  0.54412281, -0.3484857 ]), array([ 0.12621259, -0.17390013,  0.56962612, -0.49468386]), array([ 0.22951011, -0.27011109,  0.44005969, -0.43632296]), array([ 0.28112861, -0.30385041,  0.06567573,  0.11003848]), array([ 0.26793567, -0.2605057 , -0.19350318,  0.31412879]), array([ 0.20750695, -0.18448855, -0.39646724,  0.42464127]), array([ 0.11677321, -0.10117005, -0.49009276,  0.38063387]), array([ 0.02048578, -0.04376128, -0.45158534,  0.16878854]), array([-0.05593859, -0.0418602 , -0.29736042, -0.16148062]), array([-0.09395929, -0.10990459, -0.07777257, -0.51236912]), array([-0.10027934, -0.20654557,  0.01304187, -0.43901243]), array([-0.07685014, -0.31344092,  0.2131264 , -0.60802347]), array([-0.03271559, -0.40561276,  0.21757341, -0.2934546 ]), array([ 0.00610425, -0.42453525,  0.16220951,  0.11311447]), array([ 0.04226466, -0.39252754,  0.19252738,  0.20814393]), array([ 0.08026074, -0.34130107,  0.18095245,  0.30194938]), array([ 0.08614189, -0.20585194, -0.12042007,  1.03265279]), array([ 0.03638362,  0.0566849 , -0.3570351 ,  1.53730363]), array([-0.01957971,  0.31348945, -0.18391396,  0.98007167]), array([-0.03262349,  0.43481503,  0.05670544,  0.21660063]), array([-0.01057696,  0.43194636,  0.1588405 , -0.24087399]), array([ 0.04087102,  0.30969146,  0.34357711, -0.95734382]), array([ 0.11979192,  0.06453497,  0.4226478 , -1.44142199]), array([ 0.18552021, -0.20640775,  0.21146494, -1.20946192]), array([ 0.21031676, -0.4331104 ,  0.02398394, -1.01553529]), array([ 0.18005535, -0.56679676, -0.32097855, -0.30956231]), array([ 0.07512051, -0.52542973, -0.70520091,  0.70249821]), array([-0.08985671, -0.30085432, -0.90781567,  1.48702052]), array([-0.24393465, -0.02964811, -0.59304445,  1.15156692]), array([-0.31426118,  0.13559099, -0.09205237,  0.46385352]), array([-0.27816234,  0.14859986,  0.44576073, -0.32999197]), array([-0.15690589,  0.0470525 ,  0.73945993, -0.64995968]), array([ 0.00390779, -0.09288767,  0.83152395, -0.69915253]), array([ 0.16011315, -0.21175702,  0.69551512, -0.44544961]), array([ 0.28279377, -0.29043155,  0.50511914, -0.31142716]), array([ 0.34045702, -0.29310017,  0.06089968,  0.2912036 ]), array([ 0.31984069, -0.21086026, -0.26026765,  0.51442557]), array([ 0.21521621, -0.02865769, -0.75981427,  1.26180252]), array([ 0.05791748,  0.19810496, -0.77460081,  0.94179623]), array([-0.07971457,  0.32529124, -0.5709511 ,  0.28968286]), array([-0.16027515,  0.30328971, -0.21858512, -0.5176079 ]), array([-0.17736724,  0.15573946,  0.04629962, -0.93508445]), array([-0.14508191, -0.05703447,  0.26209036, -1.14942791]), array([-0.08015934, -0.28414889,  0.36675915, -1.07271232]), array([-0.00669032, -0.46747496,  0.34968455, -0.72260123]), array([ 0.05314637, -0.5609158 ,  0.23573057, -0.19134934]), array([ 0.08339349, -0.53901391,  0.06025918,  0.41270624]), array([ 0.08889535, -0.43162243, -0.00440866,  0.64677076]), array([ 0.08288899, -0.28825342, -0.05037866,  0.76275259]), array([ 0.07156052, -0.13765669, -0.05543463,  0.71509176]), array([ 0.06371197, -0.01328183, -0.01723478,  0.50556882]), array([0.06634662, 0.05710963, 0.04510159, 0.18695175]), array([ 0.08148201,  0.05945092,  0.10310186, -0.16126649]), array([ 0.0922518 ,  0.03036606,  0.00163714, -0.12309633]), array([ 0.08178145,  0.01197162, -0.10467226, -0.05948246]), array([ 0.0652015 , -0.0281824 , -0.05916031, -0.33739472]), array([ 0.05819538, -0.1189701 , -0.0126775 , -0.55529578]), array([ 0.04565418, -0.20845935, -0.1126608 , -0.32674643]), array([ 0.01425701, -0.24669579, -0.1956688 , -0.05466778]), array([-0.01639327, -0.26600545, -0.10524156, -0.13995949]), array([-0.02639323, -0.30223405,  0.00617061, -0.21786578]), array([-0.027429  , -0.31664825, -0.01649665,  0.07546654]), array([-0.01960006, -0.30683664,  0.09330963,  0.02254894]), array([ 0.008395  , -0.30667927,  0.18079234, -0.01628488]), array([ 0.04966734, -0.31074279,  0.22332544, -0.01705376]), array([ 0.08094605, -0.27670459,  0.08391575,  0.35667568]), array([ 0.0956284 , -0.20546126,  0.0622238 ,  0.34576106]), array([ 0.10574109, -0.14250099,  0.03896269,  0.27439368]), array([ 0.11132642, -0.09913461,  0.01719492,  0.15258297]), array([ 0.11275204, -0.08343487, -0.00273121,  0.0019757 ]), array([ 0.11028671, -0.098421  , -0.02193501, -0.14950945]), array([ 0.10393516, -0.14139966, -0.04173886, -0.27364657]), array([ 0.08037533, -0.17042928, -0.18972101, -0.01567515]), array([ 0.0442759 , -0.18385269, -0.16448285, -0.12161956]), array([-0.00929475, -0.15136342, -0.35909659,  0.43242148]), array([-0.06602141, -0.08959505, -0.19491399,  0.16595736]), array([-0.1100637 , -0.0214003 , -0.23446276,  0.49736199]), array([-0.12818623,  0.03092545,  0.05811502,  0.01483332]), array([-0.10093212,  0.01922839,  0.20840566, -0.12538145]), array([-0.03527918, -0.04917756,  0.43238219, -0.53609008])]</t>
+  </si>
+  <si>
+    <t>['[2,2,2]', '[2,1,0]', '[0,2,1]', '[2,0,1]', '[1,2,0]', '[1,1,1]', '[0,0,0]', '[0,1,1]', '[1,1,2]', '[1,0,2]']</t>
+  </si>
+  <si>
+    <t>[1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50, 51, 52, 53, 54, 55, 56, 57, 58, 59, 60, 61, 62, 63, 64, 65, 66, 67, 68, 69, 70, 71, 72, 73, 74, 75, 76, 77, 78, 79, 80, 81, 82, 83, 84, 85, 86, 87, 88, 89, 90, 91, 92, 93, 94, 95, 96, 97, 98, 99, 100, 101, 102, 103, 104, 105, 106, 107, 108, 109, 110, 111, 112, 113, 114, 115, 116, 117, 118, 119, 120, 121, 122, 123, 124, 125, 126, 127, 128, 129, 130, 131, 132, 133, 134, 135, 136, 137, 138, 139, 140, 141, 142, 143, 144, 145, 146, 147, 148, 149, 150, 151, 152, 153, 154, 155, 156, 157, 158, 159, 160, 161, 162, 163, 164, 165, 166, 167, 168, 169, 170, 171, 172, 173, 174, 175, 176, 177, 178, 179, 180, 181, 182, 183, 184, 185, 186, 187, 188, 189, 190, 191, 192, 193, 194, 195, 196, 197, 198, 199]</t>
+  </si>
+  <si>
+    <t>[0, 0, 0, 0, 2, 0, 0, 2, 0, 2, 0, 2, 0, 2, 0, 2, 2, 0, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2]</t>
+  </si>
+  <si>
+    <t>['[-0.03763371 -0.01533471  0.06554052 -0.01816017]', '[-0.0208055  -0.02030166  0.09914155 -0.02801351]', '[ 0.00031733 -0.02489487  0.10765546 -0.0138725 ]', '[ 0.02044082 -0.02428802  0.08954248  0.02288616]', '[ 0.03470698 -0.01491644  0.05056501  0.07132823]', '[ 0.05326751 -0.03038784  0.13065223 -0.22021077]', '[ 0.07101291 -0.0640307   0.04229076 -0.10791836]', '[ 0.06919594 -0.07148833 -0.06018897  0.03411905]', '[ 0.06123949 -0.0858309  -0.01832924 -0.17605239]', '[ 0.04848925 -0.10546764 -0.10705552 -0.01913256]', '[ 0.03334023 -0.12873715 -0.04224633 -0.21160413]', '[ 0.01856077 -0.15355978 -0.1031453  -0.03494141]', '[ 0.00687968 -0.17764366 -0.01219475 -0.20332606]', '[ 0.00024918 -0.19823055 -0.05320561 -0.00041555]', '[-0.00038196 -0.21249406  0.04645807 -0.13967612]', '[ 0.00462703 -0.21766377  0.00256154  0.08939976]', '[ 0.01391452 -0.21184382  0.0884936  -0.03053848]', '[ 0.03850047 -0.22834148  0.15179103 -0.12764898]', '[ 0.05871339 -0.22531591  0.04642174  0.1602345 ]', '[ 0.06975736 -0.19972822  0.06255754  0.09301244]', '[ 0.08295526 -0.18863935  0.06709485  0.01801994]', '[ 0.0955466  -0.19194963  0.05618073 -0.04863014]', '[ 0.10438266 -0.20672312  0.02995667 -0.09524718]', '[ 0.10679076 -0.22835209 -0.00700287 -0.1170154 ]', '[ 0.10139245 -0.251988   -0.04658216 -0.11618468]', '[ 0.08862558 -0.27379536 -0.07912951 -0.10019242]', '[ 0.07079541 -0.2916811  -0.09605709 -0.07844699]', '[ 0.05160586 -0.30533224 -0.09231221 -0.05881123]', '[ 0.03527347 -0.31561531 -0.06796943 -0.04491109]', '[ 0.02545877 -0.32360191 -0.02840871 -0.03520182]', '[ 0.02431678 -0.32962124  0.01702803 -0.0241677 ]', '[ 0.03194057 -0.33273766  0.0575287  -0.00523763]', '[ 0.04635922 -0.33089406  0.08372791  0.02568935]', '[ 0.06409062 -0.32170512  0.09020522  0.06748616]', '[ 0.08108895 -0.30362649  0.07683704  0.11292955]', '[ 0.09381032 -0.27706452  0.04859846  0.15016487]', '[ 0.10008474 -0.24498455  0.01387843  0.16612946]', '[ 0.099545   -0.21272175 -0.0181427   0.15089341]', '[ 0.09350925 -0.18694889 -0.04018141  0.10151107]', '[ 0.08439395 -0.17403958 -0.04874136  0.02402904]', '[ 0.0748759  -0.17828815 -0.04468765 -0.06714713]', '[ 0.06707968 -0.2005238  -0.03244224 -0.15248501]', '[ 0.06204155 -0.23757011 -0.01810026 -0.2123621 ]', '[ 0.0596084  -0.28277818 -0.00709475 -0.23248464]', '[ 0.0587725  -0.32752505 -0.00232775 -0.20781714]', '[ 0.05826257 -0.3632139  -0.00355436 -0.1435367 ]', '[ 0.05712088 -0.38315408 -0.00807237 -0.05302107]', '[ 0.05506565 -0.38385601 -0.01204958  0.04571899]', '[ 0.05258562 -0.36558361 -0.01179826  0.13373731]', '[ 0.05080563 -0.3322004  -0.0047971   0.19451381]', '[ 0.05116333 -0.29036678  0.00943036  0.21708422]', '[ 0.05492846 -0.24815416  0.02866925  0.1986191 ]', '[ 0.06265333 -0.2132846   0.04805764  0.14539356]', '[ 0.0737392  -0.1914255   0.06122493  0.07119519]', '[ 0.08632927 -0.18505144  0.06232775 -0.0065993 ]', '[ 0.09763559 -0.19320967  0.04820618 -0.07185489]', '[ 0.1046364  -0.21219823  0.01981793 -0.11373169]', '[ 0.10494239 -0.23687371 -0.01755309 -0.12880179]', '[ 0.09757088 -0.26214836 -0.05540839 -0.12082367]', '[ 0.08338498 -0.28422734 -0.084203   -0.09846705]', '[ 0.06503934 -0.30125202 -0.09599606 -0.07181621]', '[ 0.04641147 -0.31321516 -0.08681408 -0.04877953]', '[ 0.03165341 -0.32124755 -0.05798066 -0.03256881]', '[ 0.02412308 -0.32658523 -0.01595187 -0.02112032]', '[ 0.02550179 -0.32964056  0.02933688 -0.00867761]', '[ 0.03535467 -0.32956213  0.06713802  0.01106326]', '[ 0.05126215 -0.32448023  0.08879534  0.04147042]', '[ 0.06948414 -0.31236544  0.09003875  0.0805337 ]', '[ 0.08596321 -0.29218207  0.07199708  0.12046316]', '[ 0.09737325 -0.26489006  0.04063242  0.14957341]', '[ 0.10190935 -0.23388285  0.00479206  0.15588881]', '[ 0.09960108 -0.20462479 -0.02647608  0.13132678]', '[ 0.09208836 -0.18350913 -0.04647049  0.07508745]', '[ 0.08196904 -0.17622141 -0.05247261 -0.00494006]', '[ 0.07194826 -0.1860764  -0.04606129 -0.09335229]', '[ 0.0640607  -0.21283993 -0.03210001 -0.17081162]', '[ 0.05920229 -0.25243865 -0.01674109 -0.2191429 ]', '[ 0.0571035  -0.29771672 -0.00514729 -0.22641302]', '[ 5.67079806e-02 -3.40049845e-01  1.40509559e-04 -1.90152289e-01]', '[ 0.0567542  -0.37130947 -0.00044065 -0.1175718 ]', '[ 0.05630704 -0.38559301 -0.00424585 -0.02319697]', '[ 0.05508019 -0.38034455 -0.00762881  0.0746204 ]', '[ 0.05352152 -0.35676725 -0.00706294  0.15719537]', '[ 5.26889742e-02 -3.19556780e-01 -1.32505029e-04  2.08826291e-01]', '[ 0.05393115 -0.2759787   0.01350876  0.22000939]', '[ 0.05839564 -0.23435582  0.03145057  0.18995248]', '[ 0.06647515 -0.20222884  0.04868101  0.12712705]', '[ 0.07740249 -0.18468121  0.0589193   0.04705174]', '[ 0.08920474 -0.18334652  0.05675805 -0.03210605]', '[ 0.09909535 -0.19637959  0.03975234 -0.09447618]', '[ 0.10420937 -0.21932955  0.00966234 -0.13033698]', '[ 0.10246404 -0.24658161 -0.02757142 -0.13784684]', '[ 0.09328114 -0.27290276 -0.06315946 -0.12236486]', '[ 0.07793604 -0.29463867 -0.08778553 -0.09376129]', '[ 0.0593946  -0.31024783 -0.09427901 -0.06266294]', '[ 0.04164872 -0.32007965 -0.07982525 -0.03685256]', '[ 0.02871865 -0.32554868 -0.04699358 -0.01899582]', '[ 0.02360262 -0.32805697 -0.00321876 -0.00646596]', '[ 0.02747827 -0.32810149  0.04113818  0.00669675]', '[ 0.03938956 -0.32492763  0.0755836   0.02646753]', '[ 0.0565101  -0.31687384  0.0923231   0.05547315]', '[ 0.07490627 -0.30227879  0.08830434  0.09091934]', '[ 0.09057649 -0.28059671  0.06587143  0.12465308]', '[ 0.10046354 -0.25327641  0.03185408  0.14539966]', '[ 0.10315103 -0.22403115 -0.00458867  0.14244801]', '[ 0.09906173 -0.19832456 -0.03465823  0.1095913 ]', '[ 0.090136   -0.18215254 -0.05229431  0.04802964]', '[ 0.07912538 -0.18043834 -0.05556224 -0.03278709]', '[ 0.06873857 -0.19550748 -0.0467223  -0.1168093 ]', '[ 0.06090465 -0.22612413 -0.03102421 -0.18524267]', '[ 0.05637446 -0.26744124 -0.01462964 -0.22160895]', '[ 0.05476245 -0.31195043 -0.00243303 -0.21638607]', '[ 0.05495737 -0.35116801  0.00332542 -0.16950281]', '[ 0.05568737 -0.37752895  0.0032086  -0.08993096]', '[ 5.60120148e-02 -3.85961900e-01 -1.99426156e-04  6.88577345e-03]', '[ 0.05562006 -0.37485205 -0.00336396  0.10238374]', '[ 0.05491675 -0.34632881 -0.00281815  0.17823062]', '[ 0.05490846 -0.30588436  0.00380835  0.21968852]', '[ 0.05687536 -0.26131719  0.01672642  0.2189266 ]', '[ 0.06185878 -0.22108772  0.03329702  0.17737189]', '[ 0.07010297 -0.1924189   0.04835125  0.10572158]', '[ 0.08068633 -0.17968709  0.0557311   0.02106819]', '[ 0.09154199 -0.18360664  0.05050737 -0.05790659]', '[ 0.09991338 -0.20142098  0.03096826 -0.11590096]', '[ 0.1031209  -0.22796893 -0.00034305 -0.14457436]', '[ 0.09940889 -0.25724729 -0.03689008 -0.14384494]', '[ 0.08860779 -0.28398315 -0.06969503 -0.12071965]', '[ 0.07238558 -0.30476413 -0.08980074 -0.08618494]', '[ 0.053974   -0.31844045 -0.09092666 -0.05123801]', '[ 0.03741523 -0.32575622 -0.0714764  -0.02335558]', '[ 0.02653095 -0.3284175  -0.03523065 -0.00454442]', '[ 0.02390923 -0.32798743  0.0095238   0.00839929]', '[ 0.03020552 -0.32504777  0.05218353  0.02158279]', '[ 0.04396167 -0.31895319  0.08269304  0.04059812]', '[ 0.06199569 -0.30826712  0.09424795  0.06735185]', '[ 0.08024809 -0.29169783  0.08504662  0.09839758]', '[ 0.09483717 -0.26915531  0.05858188  0.12543454]', '[ 0.10301802 -0.24249826  0.0224198   0.13781555]', '[ 0.10377826 -0.21564543 -0.01410806  0.12621646]', '[ 0.09792482 -0.19393613 -0.04255291  0.08627243]', '[ 0.08767477 -0.18286809 -0.0575417   0.02099345]', '[ 0.07590541 -0.18655146 -0.05792259 -0.05890949]', '[ 0.06530491 -0.20633731 -0.04660131 -0.13708618]', '[ 0.05768201 -0.24007046 -0.02916026 -0.19560079]', '[ 0.05363739 -0.28226425 -0.01173496 -0.21985746]', '[ 0.05266638 -0.32520851  0.0010306  -0.20272093]', '[ 0.05359128 -0.36068612  0.00713647 -0.14630965]', '[ 0.05510701 -0.38177224  0.00723029 -0.06109619]', '[ 0.0562436  -0.38425748  0.00386662  0.03674448]', '[ 0.0566538  -0.36747063  0.00056143  0.12854072]', '[ 0.05670863 -0.33445047  0.00081213  0.1964189 ]', '[ 0.05738383 -0.29144034  0.00697313  0.22678809]', '[ 0.05991129 -0.24668346  0.019088    0.21372085]', '[ 0.06523806 -0.2086492   0.03425028  0.16101479]', '[ 0.07346816 -0.18410168  0.04713803  0.08155666]', '[ 0.08353885 -0.17659553  0.05175852 -0.00620498]', '[ 0.09331176 -0.18586558  0.04370315 -0.08338381]', '[ 0.10008853 -0.20824698  0.02200651 -0.13555758]', '[ 0.10140207 -0.23792825 -0.01003113 -0.15601687]', '[ 0.09584132 -0.26861749 -0.04534776 -0.14657816]', '[ 0.08364422 -0.29511506 -0.07489216 -0.11589105]', '[ 0.0668445  -0.31434892 -0.09020274 -0.07592226]', '[ 0.04888729 -0.32562439 -0.08599892 -0.03783852]', '[ 0.03379772 -0.33010452 -0.06193576 -0.00863452]', '[ 0.02513479 -0.32978443 -0.02293809  0.01042693]', '[ 0.02503494 -0.32637922  0.02200748  0.02311183]', '[ 0.03362506 -0.32055551  0.0622461   0.03560982]', '[ 0.04897573 -0.31178877  0.08833123  0.05309252]', '[ 0.0676078  -0.29887794  0.09454709  0.07680051]', '[ 0.08540429 -0.28088981  0.0803421   0.10279361]', '[ 0.09866221 -0.25814068  0.05026789  0.12283631]', '[ 0.10498439 -0.23280889  0.01249125  0.12708833]', '[ 0.10377068 -0.20890319 -0.02361189  0.1076759 ]', '[ 0.09619874 -0.19152544 -0.05002788  0.06198729]', '[ 0.08473696 -0.18559403 -0.06210636 -0.00538117]', '[ 0.07236021 -0.19437892 -0.05947148 -0.08276543]', '[ 0.06171276 -0.21829461 -0.04563574 -0.15384494]', '[ 0.05446894 -0.25436617 -0.02646529 -0.20181367]', '[ 0.05107278 -0.29660697 -0.00804791 -0.2140739 ]', '[ 0.05089334 -0.33724733  0.00519376 -0.18578769]', '[ 0.05267033 -0.36844501  0.01144903 -0.12103312]', '[ 0.05504228 -0.38397531  0.01143998 -0.03155138]', '[ 0.05699176 -0.38051242  0.00775358  0.0658985 ]', '[ 0.05813473 -0.35832758  0.00398721  0.15263031]', '[ 0.05882524 -0.32134641  0.00373793  0.21136315]', '[ 0.06003229 -0.27650529  0.00934041  0.22987307]', '[ 0.06295692 -0.2323867   0.02061899  0.20436843]', '[ 0.06845962 -0.19732792  0.03436439  0.14111977]', '[ 0.07651005 -0.17749343  0.04511943  0.0550965 ]', '[ 0.08591764 -0.17551461  0.04710647 -0.03416791]', '[ 0.09449538 -0.1901073   0.03647786 -0.10791535]', '[ 0.09963108 -0.21672435  0.01302232 -0.15291381]', '[ 0.09909552 -0.24898478 -0.01923623 -0.1643131 ]', '[ 0.09183623 -0.28042156 -0.05279286 -0.1459218 ]', '[ 0.07849122 -0.30602506 -0.07865026 -0.10796961]', '[ 0.06142526 -0.32315462 -0.0889805  -0.06322103]', '[ 0.04423814 -0.33162027 -0.07959606 -0.02279592]', '[ 0.03086916 -0.33301485 -0.05140538  0.00695212]', '[ 0.02455586 -0.32961189 -0.01037788  0.02555682]', '[ 0.02695213 -0.32326726  0.03397195  0.03730786]']</t>
+  </si>
+  <si>
+    <t>[array([-0.03763371, -0.01533471,  0.06554052, -0.01816017], dtype=float32), array([-0.0208055 , -0.02030166,  0.09914155, -0.02801351]), array([ 0.00031733, -0.02489487,  0.10765546, -0.0138725 ]), array([ 0.02044082, -0.02428802,  0.08954248,  0.02288616]), array([ 0.03470698, -0.01491644,  0.05056501,  0.07132823]), array([ 0.05326751, -0.03038784,  0.13065223, -0.22021077]), array([ 0.07101291, -0.0640307 ,  0.04229076, -0.10791836]), array([ 0.06919594, -0.07148833, -0.06018897,  0.03411905]), array([ 0.06123949, -0.0858309 , -0.01832924, -0.17605239]), array([ 0.04848925, -0.10546764, -0.10705552, -0.01913256]), array([ 0.03334023, -0.12873715, -0.04224633, -0.21160413]), array([ 0.01856077, -0.15355978, -0.1031453 , -0.03494141]), array([ 0.00687968, -0.17764366, -0.01219475, -0.20332606]), array([ 0.00024918, -0.19823055, -0.05320561, -0.00041555]), array([-0.00038196, -0.21249406,  0.04645807, -0.13967612]), array([ 0.00462703, -0.21766377,  0.00256154,  0.08939976]), array([ 0.01391452, -0.21184382,  0.0884936 , -0.03053848]), array([ 0.03850047, -0.22834148,  0.15179103, -0.12764898]), array([ 0.05871339, -0.22531591,  0.04642174,  0.1602345 ]), array([ 0.06975736, -0.19972822,  0.06255754,  0.09301244]), array([ 0.08295526, -0.18863935,  0.06709485,  0.01801994]), array([ 0.0955466 , -0.19194963,  0.05618073, -0.04863014]), array([ 0.10438266, -0.20672312,  0.02995667, -0.09524718]), array([ 0.10679076, -0.22835209, -0.00700287, -0.1170154 ]), array([ 0.10139245, -0.251988  , -0.04658216, -0.11618468]), array([ 0.08862558, -0.27379536, -0.07912951, -0.10019242]), array([ 0.07079541, -0.2916811 , -0.09605709, -0.07844699]), array([ 0.05160586, -0.30533224, -0.09231221, -0.05881123]), array([ 0.03527347, -0.31561531, -0.06796943, -0.04491109]), array([ 0.02545877, -0.32360191, -0.02840871, -0.03520182]), array([ 0.02431678, -0.32962124,  0.01702803, -0.0241677 ]), array([ 0.03194057, -0.33273766,  0.0575287 , -0.00523763]), array([ 0.04635922, -0.33089406,  0.08372791,  0.02568935]), array([ 0.06409062, -0.32170512,  0.09020522,  0.06748616]), array([ 0.08108895, -0.30362649,  0.07683704,  0.11292955]), array([ 0.09381032, -0.27706452,  0.04859846,  0.15016487]), array([ 0.10008474, -0.24498455,  0.01387843,  0.16612946]), array([ 0.099545  , -0.21272175, -0.0181427 ,  0.15089341]), array([ 0.09350925, -0.18694889, -0.04018141,  0.10151107]), array([ 0.08439395, -0.17403958, -0.04874136,  0.02402904]), array([ 0.0748759 , -0.17828815, -0.04468765, -0.06714713]), array([ 0.06707968, -0.2005238 , -0.03244224, -0.15248501]), array([ 0.06204155, -0.23757011, -0.01810026, -0.2123621 ]), array([ 0.0596084 , -0.28277818, -0.00709475, -0.23248464]), array([ 0.0587725 , -0.32752505, -0.00232775, -0.20781714]), array([ 0.05826257, -0.3632139 , -0.00355436, -0.1435367 ]), array([ 0.05712088, -0.38315408, -0.00807237, -0.05302107]), array([ 0.05506565, -0.38385601, -0.01204958,  0.04571899]), array([ 0.05258562, -0.36558361, -0.01179826,  0.13373731]), array([ 0.05080563, -0.3322004 , -0.0047971 ,  0.19451381]), array([ 0.05116333, -0.29036678,  0.00943036,  0.21708422]), array([ 0.05492846, -0.24815416,  0.02866925,  0.1986191 ]), array([ 0.06265333, -0.2132846 ,  0.04805764,  0.14539356]), array([ 0.0737392 , -0.1914255 ,  0.06122493,  0.07119519]), array([ 0.08632927, -0.18505144,  0.06232775, -0.0065993 ]), array([ 0.09763559, -0.19320967,  0.04820618, -0.07185489]), array([ 0.1046364 , -0.21219823,  0.01981793, -0.11373169]), array([ 0.10494239, -0.23687371, -0.01755309, -0.12880179]), array([ 0.09757088, -0.26214836, -0.05540839, -0.12082367]), array([ 0.08338498, -0.28422734, -0.084203  , -0.09846705]), array([ 0.06503934, -0.30125202, -0.09599606, -0.07181621]), array([ 0.04641147, -0.31321516, -0.08681408, -0.04877953]), array([ 0.03165341, -0.32124755, -0.05798066, -0.03256881]), array([ 0.02412308, -0.32658523, -0.01595187, -0.02112032]), array([ 0.02550179, -0.32964056,  0.02933688, -0.00867761]), array([ 0.03535467, -0.32956213,  0.06713802,  0.01106326]), array([ 0.05126215, -0.32448023,  0.08879534,  0.04147042]), array([ 0.06948414, -0.31236544,  0.09003875,  0.0805337 ]), array([ 0.08596321, -0.29218207,  0.07199708,  0.12046316]), array([ 0.09737325, -0.26489006,  0.04063242,  0.14957341]), array([ 0.10190935, -0.23388285,  0.00479206,  0.15588881]), array([ 0.09960108, -0.20462479, -0.02647608,  0.13132678]), array([ 0.09208836, -0.18350913, -0.04647049,  0.07508745]), array([ 0.08196904, -0.17622141, -0.05247261, -0.00494006]), array([ 0.07194826, -0.1860764 , -0.04606129, -0.09335229]), array([ 0.0640607 , -0.21283993, -0.03210001, -0.17081162]), array([ 0.05920229, -0.25243865, -0.01674109, -0.2191429 ]), array([ 0.0571035 , -0.29771672, -0.00514729, -0.22641302]), array([ 5.67079806e-02, -3.40049845e-01,  1.40509559e-04, -1.90152289e-01]), array([ 0.0567542 , -0.37130947, -0.00044065, -0.1175718 ]), array([ 0.05630704, -0.38559301, -0.00424585, -0.02319697]), array([ 0.05508019, -0.38034455, -0.00762881,  0.0746204 ]), array([ 0.05352152, -0.35676725, -0.00706294,  0.15719537]), array([ 5.26889742e-02, -3.19556780e-01, -1.32505029e-04,  2.08826291e-01]), array([ 0.05393115, -0.2759787 ,  0.01350876,  0.22000939]), array([ 0.05839564, -0.23435582,  0.03145057,  0.18995248]), array([ 0.06647515, -0.20222884,  0.04868101,  0.12712705]), array([ 0.07740249, -0.18468121,  0.0589193 ,  0.04705174]), array([ 0.08920474, -0.18334652,  0.05675805, -0.03210605]), array([ 0.09909535, -0.19637959,  0.03975234, -0.09447618]), array([ 0.10420937, -0.21932955,  0.00966234, -0.13033698]), array([ 0.10246404, -0.24658161, -0.02757142, -0.13784684]), array([ 0.09328114, -0.27290276, -0.06315946, -0.12236486]), array([ 0.07793604, -0.29463867, -0.08778553, -0.09376129]), array([ 0.0593946 , -0.31024783, -0.09427901, -0.06266294]), array([ 0.04164872, -0.32007965, -0.07982525, -0.03685256]), array([ 0.02871865, -0.32554868, -0.04699358, -0.01899582]), array([ 0.02360262, -0.32805697, -0.00321876, -0.00646596]), array([ 0.02747827, -0.32810149,  0.04113818,  0.00669675]), array([ 0.03938956, -0.32492763,  0.0755836 ,  0.02646753]), array([ 0.0565101 , -0.31687384,  0.0923231 ,  0.05547315]), array([ 0.07490627, -0.30227879,  0.08830434,  0.09091934]), array([ 0.09057649, -0.28059671,  0.06587143,  0.12465308]), array([ 0.10046354, -0.25327641,  0.03185408,  0.14539966]), array([ 0.10315103, -0.22403115, -0.00458867,  0.14244801]), array([ 0.09906173, -0.19832456, -0.03465823,  0.1095913 ]), array([ 0.090136  , -0.18215254, -0.05229431,  0.04802964]), array([ 0.07912538, -0.18043834, -0.05556224, -0.03278709]), array([ 0.06873857, -0.19550748, -0.0467223 , -0.1168093 ]), array([ 0.06090465, -0.22612413, -0.03102421, -0.18524267]), array([ 0.05637446, -0.26744124, -0.01462964, -0.22160895]), array([ 0.05476245, -0.31195043, -0.00243303, -0.21638607]), array([ 0.05495737, -0.35116801,  0.00332542, -0.16950281]), array([ 0.05568737, -0.37752895,  0.0032086 , -0.08993096]), array([ 5.60120148e-02, -3.85961900e-01, -1.99426156e-04,  6.88577345e-03]), array([ 0.05562006, -0.37485205, -0.00336396,  0.10238374]), array([ 0.05491675, -0.34632881, -0.00281815,  0.17823062]), array([ 0.05490846, -0.30588436,  0.00380835,  0.21968852]), array([ 0.05687536, -0.26131719,  0.01672642,  0.2189266 ]), array([ 0.06185878, -0.22108772,  0.03329702,  0.17737189]), array([ 0.07010297, -0.1924189 ,  0.04835125,  0.10572158]), array([ 0.08068633, -0.17968709,  0.0557311 ,  0.02106819]), array([ 0.09154199, -0.18360664,  0.05050737, -0.05790659]), array([ 0.09991338, -0.20142098,  0.03096826, -0.11590096]), array([ 0.1031209 , -0.22796893, -0.00034305, -0.14457436]), array([ 0.09940889, -0.25724729, -0.03689008, -0.14384494]), array([ 0.08860779, -0.28398315, -0.06969503, -0.12071965]), array([ 0.07238558, -0.30476413, -0.08980074, -0.08618494]), array([ 0.053974  , -0.31844045, -0.09092666, -0.05123801]), array([ 0.03741523, -0.32575622, -0.0714764 , -0.02335558]), array([ 0.02653095, -0.3284175 , -0.03523065, -0.00454442]), array([ 0.02390923, -0.32798743,  0.0095238 ,  0.00839929]), array([ 0.03020552, -0.32504777,  0.05218353,  0.02158279]), array([ 0.04396167, -0.31895319,  0.08269304,  0.04059812]), array([ 0.06199569, -0.30826712,  0.09424795,  0.06735185]), array([ 0.08024809, -0.29169783,  0.08504662,  0.09839758]), array([ 0.09483717, -0.26915531,  0.05858188,  0.12543454]), array([ 0.10301802, -0.24249826,  0.0224198 ,  0.13781555]), array([ 0.10377826, -0.21564543, -0.01410806,  0.12621646]), array([ 0.09792482, -0.19393613, -0.04255291,  0.08627243]), array([ 0.08767477, -0.18286809, -0.0575417 ,  0.02099345]), array([ 0.07590541, -0.18655146, -0.05792259, -0.05890949]), array([ 0.06530491, -0.20633731, -0.04660131, -0.13708618]), array([ 0.05768201, -0.24007046, -0.02916026, -0.19560079]), array([ 0.05363739, -0.28226425, -0.01173496, -0.21985746]), array([ 0.05266638, -0.32520851,  0.0010306 , -0.20272093]), array([ 0.05359128, -0.36068612,  0.00713647, -0.14630965]), array([ 0.05510701, -0.38177224,  0.00723029, -0.06109619]), array([ 0.0562436 , -0.38425748,  0.00386662,  0.03674448]), array([ 0.0566538 , -0.36747063,  0.00056143,  0.12854072]), array([ 0.05670863, -0.33445047,  0.00081213,  0.1964189 ]), array([ 0.05738383, -0.29144034,  0.00697313,  0.22678809]), array([ 0.05991129, -0.24668346,  0.019088  ,  0.21372085]), array([ 0.06523806, -0.2086492 ,  0.03425028,  0.16101479]), array([ 0.07346816, -0.18410168,  0.04713803,  0.08155666]), array([ 0.08353885, -0.17659553,  0.05175852, -0.00620498]), array([ 0.09331176, -0.18586558,  0.04370315, -0.08338381]), array([ 0.10008853, -0.20824698,  0.02200651, -0.13555758]), array([ 0.10140207, -0.23792825, -0.01003113, -0.15601687]), array([ 0.09584132, -0.26861749, -0.04534776, -0.14657816]), array([ 0.08364422, -0.29511506, -0.07489216, -0.11589105]), array([ 0.0668445 , -0.31434892, -0.09020274, -0.07592226]), array([ 0.04888729, -0.32562439, -0.08599892, -0.03783852]), array([ 0.03379772, -0.33010452, -0.06193576, -0.00863452]), array([ 0.02513479, -0.32978443, -0.02293809,  0.01042693]), array([ 0.02503494, -0.32637922,  0.02200748,  0.02311183]), array([ 0.03362506, -0.32055551,  0.0622461 ,  0.03560982]), array([ 0.04897573, -0.31178877,  0.08833123,  0.05309252]), array([ 0.0676078 , -0.29887794,  0.09454709,  0.07680051]), array([ 0.08540429, -0.28088981,  0.0803421 ,  0.10279361]), array([ 0.09866221, -0.25814068,  0.05026789,  0.12283631]), array([ 0.10498439, -0.23280889,  0.01249125,  0.12708833]), array([ 0.10377068, -0.20890319, -0.02361189,  0.1076759 ]), array([ 0.09619874, -0.19152544, -0.05002788,  0.06198729]), array([ 0.08473696, -0.18559403, -0.06210636, -0.00538117]), array([ 0.07236021, -0.19437892, -0.05947148, -0.08276543]), array([ 0.06171276, -0.21829461, -0.04563574, -0.15384494]), array([ 0.05446894, -0.25436617, -0.02646529, -0.20181367]), array([ 0.05107278, -0.29660697, -0.00804791, -0.2140739 ]), array([ 0.05089334, -0.33724733,  0.00519376, -0.18578769]), array([ 0.05267033, -0.36844501,  0.01144903, -0.12103312]), array([ 0.05504228, -0.38397531,  0.01143998, -0.03155138]), array([ 0.05699176, -0.38051242,  0.00775358,  0.0658985 ]), array([ 0.05813473, -0.35832758,  0.00398721,  0.15263031]), array([ 0.05882524, -0.32134641,  0.00373793,  0.21136315]), array([ 0.06003229, -0.27650529,  0.00934041,  0.22987307]), array([ 0.06295692, -0.2323867 ,  0.02061899,  0.20436843]), array([ 0.06845962, -0.19732792,  0.03436439,  0.14111977]), array([ 0.07651005, -0.17749343,  0.04511943,  0.0550965 ]), array([ 0.08591764, -0.17551461,  0.04710647, -0.03416791]), array([ 0.09449538, -0.1901073 ,  0.03647786, -0.10791535]), array([ 0.09963108, -0.21672435,  0.01302232, -0.15291381]), array([ 0.09909552, -0.24898478, -0.01923623, -0.1643131 ]), array([ 0.09183623, -0.28042156, -0.05279286, -0.1459218 ]), array([ 0.07849122, -0.30602506, -0.07865026, -0.10796961]), array([ 0.06142526, -0.32315462, -0.0889805 , -0.06322103]), array([ 0.04423814, -0.33162027, -0.07959606, -0.02279592]), array([ 0.03086916, -0.33301485, -0.05140538,  0.00695212]), array([ 0.02455586, -0.32961189, -0.01037788,  0.02555682]), array([ 0.02695213, -0.32326726,  0.03397195,  0.03730786])]</t>
+  </si>
+  <si>
+    <t>['[1,2,0]', '[2,0,1]', '[2,2,2]', '[0,1,1]', '[0,0,0]', '[1,0,2]', '[2,1,0]', '[1,1,2]', '[1,1,1]', '[0,2,1]']</t>
+  </si>
+  <si>
+    <t>[2,0,1]</t>
+  </si>
+  <si>
+    <t>[5, 8, 17, 18, 27, 31, 37, 39, 52, 56, 59, 63, 64, 68, 77]</t>
+  </si>
+  <si>
+    <t>[0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 1, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 1, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2]</t>
+  </si>
+  <si>
+    <t>['[-0.03763371 -0.01533471  0.06554052 -0.01816017]', '[-0.00754409 -0.05458322  0.2277812  -0.36241836]', '[ 0.04879627 -0.15231473  0.32089719 -0.5887683 ]', '[ 0.11397169 -0.27767857  0.31375488 -0.63332862]', '[ 0.16759438 -0.39312519  0.2086893  -0.49480525]', '[ 0.16756229 -0.40059886 -0.20854687  0.42010337]', '[ 0.08785953 -0.23163826 -0.56914473  1.23330318]', '[-0.04819891  0.06972415 -0.75317192  1.70451308]', '[-0.1825679   0.38074165 -0.55386931  1.33242358]', '[-0.27067484  0.6123869  -0.30529147  0.93926837]', '[-0.29880959  0.7436722   0.02971823  0.35624477]', '[-0.2357675   0.68993463  0.58803663 -0.88217723]', '[-0.07222277  0.40183661  1.0141725  -1.94561861]', '[ 0.15044135 -0.05298063  1.15055964 -2.48221462]', '[ 0.35979437 -0.53511526  0.88225786 -2.21916858]', '[ 0.48469833 -0.9047363   0.340802   -1.42553112]', '[ 0.49172355 -1.09431605 -0.26770384 -0.45977575]', '[ 0.37269186 -1.06018729 -0.89789799  0.78985481]', '[ 0.14569511 -0.78734889 -1.33151039  1.89658554]', '[-0.15180892 -0.29766251 -1.57995565  2.89101882]', '[-0.4526142   0.30414847 -1.34005039  2.95238516]', '[-0.65651148  0.82290379 -0.6498545   2.14440904]', '[-0.70227015  1.14274147  0.19698349  1.03243414]', '[-0.56253402  1.17678756  1.16903828 -0.68890514]', '[-0.25130795  0.87055229  1.89258512 -2.34391308]', '[ 0.16824417  0.26922641  2.21387742 -3.51824844]', '[ 0.58679809 -0.44380681  1.85565607 -3.38273915]', '[ 0.85128157 -0.95776777  0.75418643 -1.71549167]', '[ 0.90478669 -1.18573004 -0.22386806 -0.55444672]', '[ 0.74483209 -1.12020996 -1.35249496  1.21953959]', '[ 0.37774129 -0.69562071 -2.26691186  2.99583657]', '[-1.15497096e-01 -2.42314357e-03 -2.54131320e+00  3.70394526e+00]', '[-0.59402966  0.7049429  -2.12569251  3.14960626]', '[-0.93387062  1.21047427 -1.2293769   1.87495373]', '[-1.0760604   1.45668227 -0.18110407  0.59628678]', '[-0.98744331  1.39828072  1.05806834 -1.19301357]', '[-0.65958193  0.96812013  2.1934693  -3.13166589]', '[-0.15572528  0.22506762  2.73538088 -4.10747105]', '[ 0.39768626 -0.6145756   2.64120958 -3.9681263 ]', '[ 0.83124124 -1.21935246  1.6423928  -2.0442145 ]', '[ 1.06204074 -1.49264266  0.64309239 -0.70432271]', '[ 1.07458855 -1.48115137 -0.51942012  0.81733944]', '[ 0.84710551 -1.13316662 -1.74325681  2.69391199]', '[ 0.38776129 -0.39713676 -2.78381836  4.58124538]', '[-0.2080086   0.58271596 -2.9860389   4.8147285 ]', '[-0.74489088  1.40413181 -2.30324366  3.29591537]', '[-1.11128858  1.90327299 -1.32937194  1.73073768]', '[-1.26758646  2.10961981 -0.22115959  0.35294896]', '[-1.18404861  2.00295301  1.05105605 -1.43379331]', '[-0.85215996  1.52085487  2.25133475 -3.44831354]', '[-0.2916609   0.59803929  3.30095083 -5.74068753]', '[ 0.39917185 -0.63169021  3.35555555 -5.99307843]', '[ 0.95620967 -1.59135307  2.1745071  -3.59656423]', '[ 1.28054847 -2.14888756  1.05209256 -2.03118509]', '[ 1.37295521 -2.41700956 -0.13059824 -0.66285736]', '[ 1.21768906 -2.37200812 -1.40558826  1.12840605]', '[ 0.82917693 -1.97466976 -2.43577653  2.88639178]', '[ 0.25542169 -1.17284852 -3.26248043  5.17752674]', '[-0.44777236  0.05968006 -3.57602474  6.71141393]', '[-1.05542209  1.23835545 -2.36371701  4.81637504]', '[-1.39230545  2.02466029 -1.00218417  3.11764422]', '[-1.45802464  2.50397529  0.33436468  1.69115792]', '[-1.25918531  2.68019121  1.62921751  0.06435607]', '[-0.82717228  2.54740227  2.63061692 -1.39287192]', '[-0.24422562  2.1265905   3.08404281 -2.79096284]', '[ 0.37515627  1.40423756  3.03171432 -4.37589978]', '[ 0.94759381  0.41631558  2.62634516 -5.31836538]', '[ 1.37805699 -0.60740329  1.55647019 -4.66976652]', '[ 1.51675908 -1.34605607 -0.18569885 -2.7142092 ]', '[ 1.32096259 -1.73486111 -1.76455924 -1.10605935]', '[ 0.81380339 -1.71203478 -3.21521911  1.39381174]', '[ 0.08352747 -1.16578969 -3.96400029  4.03144555]', '[-0.7212031  -0.1667425  -3.92394603  5.5815729 ]', '[-1.40903821  0.86834795 -2.83490397  4.48853175]', '[-1.8435105   1.62033227 -1.51829112  3.11460466]', '[-2.02000229  2.14273479 -0.25067167  2.13969409]', '[-1.94383822  2.47242196  1.01408706  1.11862645]', '[-1.61319166  2.56773057  2.29121267 -0.23076982]', '[-1.02297124  2.31182659  3.5526465  -2.40726288]', '[-0.23172498  1.57323858  4.25889827 -5.04100466]', '[ 0.6496519   0.30592139  4.42991619 -7.30421556]', '[ 1.43569666 -1.06635597  3.23918044 -5.95156178]', '[ 1.93288166 -2.07128423  1.76283297 -4.24459042]', '[ 2.15456895 -2.80573943  0.49820724 -3.14439036]', '[ 2.15109246  2.95290565 -0.49490186 -2.087504  ]', '[ 1.96186492  2.64948755 -1.40733009 -0.93700597]', '[ 1.56456586  2.61622855 -2.59821518  0.57600646]', '[ 0.91714577  2.85850032 -3.84606376  1.77237834]', '[ 0.06555595 -2.98633801 -4.50226966  2.55368882]', '[-0.79964721 -2.42366121 -3.96834205  3.00381137]', '[-1.47674103 -1.82557453 -2.76482325  2.85806274]', '[-1.90832289 -1.32230595 -1.57301992  2.09840264]']</t>
+  </si>
+  <si>
+    <t>[0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50, 51, 52, 53, 54, 55, 56, 57, 58, 59, 60, 61, 62, 63, 64, 65, 66, 67, 68, 69, 70, 71, 72, 73, 74, 75, 76, 77, 78, 79, 80, 81, 82, 83, 84, 85, 86, 87, 88, 89, 90, 91]</t>
+  </si>
+  <si>
+    <t>[array([-0.03763371, -0.01533471,  0.06554052, -0.01816017], dtype=float32), array([-0.00754409, -0.05458322,  0.2277812 , -0.36241836]), array([ 0.04879627, -0.15231473,  0.32089719, -0.5887683 ]), array([ 0.11397169, -0.27767857,  0.31375488, -0.63332862]), array([ 0.16759438, -0.39312519,  0.2086893 , -0.49480525]), array([ 0.16756229, -0.40059886, -0.20854687,  0.42010337]), array([ 0.08785953, -0.23163826, -0.56914473,  1.23330318]), array([-0.04819891,  0.06972415, -0.75317192,  1.70451308]), array([-0.1825679 ,  0.38074165, -0.55386931,  1.33242358]), array([-0.27067484,  0.6123869 , -0.30529147,  0.93926837]), array([-0.29880959,  0.7436722 ,  0.02971823,  0.35624477]), array([-0.2357675 ,  0.68993463,  0.58803663, -0.88217723]), array([-0.07222277,  0.40183661,  1.0141725 , -1.94561861]), array([ 0.15044135, -0.05298063,  1.15055964, -2.48221462]), array([ 0.35979437, -0.53511526,  0.88225786, -2.21916858]), array([ 0.48469833, -0.9047363 ,  0.340802  , -1.42553112]), array([ 0.49172355, -1.09431605, -0.26770384, -0.45977575]), array([ 0.37269186, -1.06018729, -0.89789799,  0.78985481]), array([ 0.14569511, -0.78734889, -1.33151039,  1.89658554]), array([-0.15180892, -0.29766251, -1.57995565,  2.89101882]), array([-0.4526142 ,  0.30414847, -1.34005039,  2.95238516]), array([-0.65651148,  0.82290379, -0.6498545 ,  2.14440904]), array([-0.70227015,  1.14274147,  0.19698349,  1.03243414]), array([-0.56253402,  1.17678756,  1.16903828, -0.68890514]), array([-0.25130795,  0.87055229,  1.89258512, -2.34391308]), array([ 0.16824417,  0.26922641,  2.21387742, -3.51824844]), array([ 0.58679809, -0.44380681,  1.85565607, -3.38273915]), array([ 0.85128157, -0.95776777,  0.75418643, -1.71549167]), array([ 0.90478669, -1.18573004, -0.22386806, -0.55444672]), array([ 0.74483209, -1.12020996, -1.35249496,  1.21953959]), array([ 0.37774129, -0.69562071, -2.26691186,  2.99583657]), array([-1.15497096e-01, -2.42314357e-03, -2.54131320e+00,  3.70394526e+00]), array([-0.59402966,  0.7049429 , -2.12569251,  3.14960626]), array([-0.93387062,  1.21047427, -1.2293769 ,  1.87495373]), array([-1.0760604 ,  1.45668227, -0.18110407,  0.59628678]), array([-0.98744331,  1.39828072,  1.05806834, -1.19301357]), array([-0.65958193,  0.96812013,  2.1934693 , -3.13166589]), array([-0.15572528,  0.22506762,  2.73538088, -4.10747105]), array([ 0.39768626, -0.6145756 ,  2.64120958, -3.9681263 ]), array([ 0.83124124, -1.21935246,  1.6423928 , -2.0442145 ]), array([ 1.06204074, -1.49264266,  0.64309239, -0.70432271]), array([ 1.07458855, -1.48115137, -0.51942012,  0.81733944]), array([ 0.84710551, -1.13316662, -1.74325681,  2.69391199]), array([ 0.38776129, -0.39713676, -2.78381836,  4.58124538]), array([-0.2080086 ,  0.58271596, -2.9860389 ,  4.8147285 ]), array([-0.74489088,  1.40413181, -2.30324366,  3.29591537]), array([-1.11128858,  1.90327299, -1.32937194,  1.73073768]), array([-1.26758646,  2.10961981, -0.22115959,  0.35294896]), array([-1.18404861,  2.00295301,  1.05105605, -1.43379331]), array([-0.85215996,  1.52085487,  2.25133475, -3.44831354]), array([-0.2916609 ,  0.59803929,  3.30095083, -5.74068753]), array([ 0.39917185, -0.63169021,  3.35555555, -5.99307843]), array([ 0.95620967, -1.59135307,  2.1745071 , -3.59656423]), array([ 1.28054847, -2.14888756,  1.05209256, -2.03118509]), array([ 1.37295521, -2.41700956, -0.13059824, -0.66285736]), array([ 1.21768906, -2.37200812, -1.40558826,  1.12840605]), array([ 0.82917693, -1.97466976, -2.43577653,  2.88639178]), array([ 0.25542169, -1.17284852, -3.26248043,  5.17752674]), array([-0.44777236,  0.05968006, -3.57602474,  6.71141393]), array([-1.05542209,  1.23835545, -2.36371701,  4.81637504]), array([-1.39230545,  2.02466029, -1.00218417,  3.11764422]), array([-1.45802464,  2.50397529,  0.33436468,  1.69115792]), array([-1.25918531,  2.68019121,  1.62921751,  0.06435607]), array([-0.82717228,  2.54740227,  2.63061692, -1.39287192]), array([-0.24422562,  2.1265905 ,  3.08404281, -2.79096284]), array([ 0.37515627,  1.40423756,  3.03171432, -4.37589978]), array([ 0.94759381,  0.41631558,  2.62634516, -5.31836538]), array([ 1.37805699, -0.60740329,  1.55647019, -4.66976652]), array([ 1.51675908, -1.34605607, -0.18569885, -2.7142092 ]), array([ 1.32096259, -1.73486111, -1.76455924, -1.10605935]), array([ 0.81380339, -1.71203478, -3.21521911,  1.39381174]), array([ 0.08352747, -1.16578969, -3.96400029,  4.03144555]), array([-0.7212031 , -0.1667425 , -3.92394603,  5.5815729 ]), array([-1.40903821,  0.86834795, -2.83490397,  4.48853175]), array([-1.8435105 ,  1.62033227, -1.51829112,  3.11460466]), array([-2.02000229,  2.14273479, -0.25067167,  2.13969409]), array([-1.94383822,  2.47242196,  1.01408706,  1.11862645]), array([-1.61319166,  2.56773057,  2.29121267, -0.23076982]), array([-1.02297124,  2.31182659,  3.5526465 , -2.40726288]), array([-0.23172498,  1.57323858,  4.25889827, -5.04100466]), array([ 0.6496519 ,  0.30592139,  4.42991619, -7.30421556]), array([ 1.43569666, -1.06635597,  3.23918044, -5.95156178]), array([ 1.93288166, -2.07128423,  1.76283297, -4.24459042]), array([ 2.15456895, -2.80573943,  0.49820724, -3.14439036]), array([ 2.15109246,  2.95290565, -0.49490186, -2.087504  ]), array([ 1.96186492,  2.64948755, -1.40733009, -0.93700597]), array([ 1.56456586,  2.61622855, -2.59821518,  0.57600646]), array([ 0.91714577,  2.85850032, -3.84606376,  1.77237834]), array([ 0.06555595, -2.98633801, -4.50226966,  2.55368882]), array([-0.79964721, -2.42366121, -3.96834205,  3.00381137]), array([-1.47674103, -1.82557453, -2.76482325,  2.85806274]), array([-1.90832289, -1.32230595, -1.57301992,  2.09840264])]</t>
+  </si>
+  <si>
+    <t>['[2,2,2]', '[2,0,1]', '[0,1,1]', '[1,1,2]', '[0,0,0]', '[0,2,1]', '[1,0,2]', '[1,2,0]', '[2,1,0]', '[1,1,1]']</t>
+  </si>
+  <si>
+    <t>[1, 4, 5, 8, 13, 14, 16, 23, 25, 31, 35, 41, 44, 46, 47, 48, 51, 56, 57, 58, 59, 63, 64, 65, 67, 70, 71, 72, 74, 80, 82, 90, 92, 96, 98, 99, 100, 102, 104, 105, 111, 115, 117, 119, 122, 125, 126, 128, 129, 131, 132, 137, 139, 140, 146, 147, 148, 151, 153, 154, 155, 156, 158, 159, 163, 168, 169, 171, 175, 177, 178, 185]</t>
+  </si>
+  <si>
+    <t>[0, 2, 2, 2, 2, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 1, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 1, 2, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 0, 0, 1, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 1, 1, 0, 0, 0, 0, 0, 0, 0, 0, 1, 1, 2, 2, 2, 2, 2, 2, 2, 2, 2, 1, 1, 1, 1, 2, 0, 0, 0]</t>
+  </si>
+  <si>
+    <t>['[-0.03763371 -0.01533471  0.06554052 -0.01816017]', '[-0.03406929  0.01398622 -0.02953871  0.30651903]', '[-0.04818188  0.10262173 -0.10566927  0.56184435]', '[-0.07305261  0.22936701 -0.13369446  0.67944384]', '[-0.08471207  0.32956689  0.02155914  0.30562945]', '[-0.06426935  0.34812641  0.17870967 -0.11914196]', '[-0.00340699  0.25183341  0.41547866 -0.82011948]', '[ 0.09360006  0.03546661  0.52847245 -1.29175873]', '[ 0.16926484 -0.17115921  0.20674635 -0.72801741]', '[ 0.19733869 -0.311245    0.06398557 -0.64496288]', '[ 0.19216768 -0.41959877 -0.11745588 -0.42216696]', '[ 0.12613052 -0.40998822 -0.52841548  0.50679343]', '[-0.00992823 -0.22836713 -0.8008212   1.26180348]', '[-0.16510499  0.03359919 -0.7109692   1.28647327]', '[-0.27911439  0.2584836  -0.39998769  0.9080588 ]', '[-0.32955916  0.41396917 -0.09058411  0.61574063]', '[-0.29998127  0.46310717  0.38073515 -0.12681434]', '[-0.17067837  0.33482679  0.88450134 -1.12199   ]', '[ 0.03773497  0.03789136  1.14866477 -1.76343303]', '[ 0.2646821  -0.32838888  1.0618532  -1.79476801]', '[ 0.44085617 -0.64241825  0.66008786 -1.27943431]', '[ 0.51757116 -0.82253054  0.09309348 -0.49838853]', '[ 0.45386198 -0.7765031  -0.7186184   0.9522818 ]', '[ 0.2517247  -0.48230696 -1.26330827  1.93683976]', '[-0.04175975 -0.00417769 -1.59704838  2.71111161]', '[-0.33808948  0.50064546 -1.28976878  2.1975962 ]', '[-0.54621418  0.86749236 -0.75086158  1.41077933]', '[-0.62814763  1.05198778 -0.05711646  0.42018251]', '[-0.54750632  0.97581252  0.85130042 -1.17918461]', '[-0.29668199  0.58486763  1.61803126 -2.68759975]', '[ 0.07307157 -0.05652007  1.98009317 -3.5377056 ]', '[ 0.42212975 -0.66996962  1.42580926 -2.44259498]', '[ 0.64509303 -1.06304735  0.76734931 -1.44394305]', '[ 0.7205435  -1.24021346 -0.02078455 -0.32167835]', '[ 0.61778714 -1.13585896 -0.9931069   1.36710528]', '[ 0.34371273 -0.72423562 -1.70680836  2.71087431]', '[-0.05143972 -0.05718807 -2.14626548  3.77718986]', '[-0.46226715  0.68166509 -1.84586711  3.38580784]', '[-0.75716294  1.24256191 -1.06007547  2.17519469]', '[-0.87727025  1.54846333 -0.13256392  0.88645795]', '[-0.79401259  1.54819016  0.9488408  -0.8924333 ]', '[-0.52605121  1.23889007  1.6942977  -2.19576532]', '[-0.11352816  0.6216479   2.37197222 -3.91013922]', '[ 0.38070481 -0.24796589  2.42090932 -4.47704241]', '[ 0.77138832 -0.98626477  1.41470734 -2.79122848]', '[ 0.95584969 -1.41430978  0.41315152 -1.48568908]', '[ 0.91772932 -1.53088611 -0.78006118  0.31897182]', '[ 0.66222879 -1.3072681  -1.74167374  1.92934862]', '[ 0.23900222 -0.76005264 -2.42962229  3.4910072 ]', '[-0.28422844  0.06099296 -2.66463741  4.44262818]', '[-0.76181075  0.88198562 -1.996041    3.55162783]', '[-1.04796787  1.42385541 -0.84577527  1.87978882]', '[-1.10611948  1.66715763  0.26509017  0.55696461]', '[-0.92938512  1.59485317  1.4785886  -1.30154906]', '[-0.52783784  1.13328214  2.49684034 -3.33953229]', '[ 0.04621848  0.27152121  3.13374025 -5.08335726]', '[ 0.62516456 -0.67289137  2.49197403 -4.01899701]', '[ 1.0076142  -1.27931999  1.30072129 -2.04553261]', '[ 1.14039219 -1.50508223  0.022812   -0.23603617]', '[ 1.02662319 -1.40005511 -1.15083551  1.30249675]', '[ 0.67748325 -0.94521341 -2.31317102  3.27242244]', '[ 0.12347069 -0.10757794 -3.10761398  4.88498877]', '[-0.4893577   0.84558507 -2.85059905  4.29318301]', '[-0.96515318  1.51568496 -1.86330739  2.40800734]', '[-1.22359672  1.82589695 -0.70272618  0.7336522 ]', '[-1.2420747   1.81848319  0.52009264 -0.80476094]', '[-1.00915358  1.47222249  1.80017192 -2.70458083]', '[-0.549195    0.77091995  2.75101269 -4.28664691]', '[ 0.07470834 -0.23856978  3.30547948 -5.41947479]', '[ 0.68814423 -1.21075361  2.70117928 -4.06440002]', '[ 1.11403468 -1.80158046  1.53542776 -1.90830996]', '[ 1.29482036 -1.99640584  0.26017198 -0.07281212]', '[ 1.22362239 -1.85681769 -0.96947816  1.48119494]', '[ 0.90224435 -1.36529353 -2.23366822  3.49793205]', '[ 0.34952317 -0.46639093 -3.21912713  5.394904  ]', '[-0.32581706  0.67347565 -3.30622469  5.49622528]', '[-0.90691235  1.59676634 -2.44010271  3.67859722]', '[-1.28914494  2.16476905 -1.35877019  2.06041551]', '[-1.44397966  2.43763761 -0.18205811  0.68928872]', '[-1.34908266  2.40113916  1.12341255 -1.06603022]', '[-1.01469398  2.04171919  2.18961336 -2.5682733 ]', '[-0.47395435  1.30476718  3.18506299 -4.87451415]', '[ 0.21513704  0.16210558  3.54409109 -6.2093318 ]', '[ 0.86668079 -1.01127315  2.78107694 -5.12081956]', '[ 1.29783729 -1.85020243  1.51559226 -3.32782814]', '[ 1.471508   -2.36808346  0.22267065 -1.88530744]', '[ 1.38967011 -2.60758536 -1.02898187 -0.50283757]', '[ 1.05610325 -2.52381658 -2.2674083   1.35793153]', '[ 0.50883732 -2.05498181 -3.11847296  3.36026067]', '[-0.15649769 -1.16930587 -3.47767475  5.49142018]', '[-0.83947618  0.04744944 -3.17706849  6.24985012]', '[-1.35390261  1.17083561 -1.85046882  4.77839716]', '[-1.55862686  1.93920382 -0.20409037  2.96368672]', '[-1.44827408  2.38449322  1.28669939  1.47031946]', '[-1.04636014  2.47617869  2.67139414 -0.57319765]', '[-0.41581944  2.15033421  3.51221873 -2.68666514]', '[ 0.28931006  1.45830318  3.4256414  -4.14476285]', '[ 0.94100121  0.49565901  3.01966061 -5.27922038]', '[ 1.42682861 -0.46553749  1.73917286 -4.10033195]', '[ 1.6180962  -1.11543777  0.16150995 -2.40414069]', '[ 1.48971203 -1.42415905 -1.4440306  -0.63407148]', '[ 1.04684108 -1.3356208  -2.94589455  1.61573675]', '[ 0.34792411 -0.77745676 -3.9450366   3.92599175]', '[-0.48183714  0.1679249  -4.13747719  5.04917178]', '[-1.20931609  1.01288168 -3.03104835  3.21654177]', '[-1.6832515   1.47042492 -1.70963327  1.46482879]', '[-1.90627314  1.66277166 -0.53036482  0.5223107 ]', '[-1.88051549  1.64299066  0.78948175 -0.72882764]', '[-1.58676155  1.35046889  2.16230635 -2.29070383]', '[-1.01013477  0.67816182  3.59928113 -4.51333493]', '[-0.18058127 -0.3959971   4.48819125 -5.72025834]', '[ 0.66575321 -1.31411892  3.82861117 -3.21843752]', '[ 1.33068519 -1.72996474  2.74370707 -1.00785133]', '[ 1.74492872 -1.76020252  1.38492588  0.5938918 ]', '[ 1.87823019 -1.50669165 -0.04133421  1.88050032]', '[ 1.73210772 -1.01544836 -1.41812108  3.05726097]', '[ 1.29724635 -0.23186241 -2.91896433  4.78127162]', '[ 0.6102679   0.78265777 -3.81764436  4.99938455]', '[-0.18883559  1.65382389 -4.05125602  3.48142489]', '[-0.94635112  2.11098814 -3.37648944  1.07702824]', '[-1.49694486  2.11981547 -2.05108658 -0.92487302]', '[-1.75066352  1.77278213 -0.47484912 -2.47078699]', '[-1.69040873  1.15251765  1.05892096 -3.71547134]', '[-1.31147028  0.2197767   2.69489751 -5.5846431 ]', '[-0.6605723  -0.97581101  3.65987854 -5.96670847]', '[ 0.09360104 -1.99521412  3.82635087 -4.13688511]', '[ 0.82746963 -2.62249913  3.37372483 -2.14638158]', '[ 1.40774113 -2.90028668  2.35947975 -0.64911284]', '[ 1.74765425 -2.85003209  1.02869765  1.1322257 ]', '[ 1.82760263 -2.49528287 -0.24197761  2.39803162]', '[ 1.62954198 -1.84674267 -1.76617806  4.15006344]', '[ 1.11805008 -0.81001063 -3.35953403  6.3309867 ]', '[ 0.32944972  0.60627624 -4.25585001  7.18237158]', '[-0.50069712  1.84910219 -3.95548161  5.07487125]', '[-1.22569228  2.65911814 -3.2065514   3.12479026]', '[-1.7561106   3.13321642 -2.07276994  1.67350828]', '[-2.05863522 -2.94175293 -0.97590996  0.42721254]', '[-2.14891759 -2.99355605  0.06224683 -0.93395129]', '[-2.02588588  2.95145029  1.18826232 -2.44989007]', '[-1.67404027  2.33906907  2.35325909 -3.73806531]', '[-1.07878211  1.40911992  3.61280379 -5.72619919]', '[-0.2102876  -0.04563889  4.8749034  -8.35857269]', '[ 0.71899543 -1.54612687  4.20680328 -6.13536529]', '[ 1.46203947 -2.5301277   3.19719524 -3.88187565]', '[ 1.98828344  3.12773329  2.07002329 -2.46096128]', '[ 2.30260177  2.74971449  1.11470349 -1.34228089]', '[2.4358686  2.62646072 0.24220093 0.10278277]', '[ 2.41573633  2.74814183 -0.4470137   1.1078727 ]', '[ 2.24396692  3.08815558 -1.30231934  2.29604766]', '[ 1.87196521 -2.5883204  -2.46148253  3.83411423]', '[ 1.24403542 -1.60804494 -3.86285123  6.20089963]', '[ 0.31924776 -0.04734268 -5.21120762  8.99167856]', '[-0.68468569  1.57940247 -4.57857715  6.63469034]', '[-1.49789759  2.62452066 -3.52926166  4.04428619]', '[-2.08615317 -3.01813295 -2.36495681  2.46604714]', '[-2.46182637 -2.6493644  -1.44958943  1.25509116]', '[-2.68700997 -2.50634043 -0.84940054  0.20032485]', '[-2.82276687 -2.53841827 -0.53959236 -0.49128809]', '[-2.90016407 -2.73040634 -0.25343164 -1.39144076]', '[-2.92636897e+00 -3.07951481e+00  4.65324835e-04 -2.06087208e+00]', '[-2.88978296  2.7428902   0.40226012 -2.51839541]', '[-2.74915069  2.20322129  1.04354768 -2.88284391]', '[-2.45701902  1.57601674  1.92199553 -3.46842133]', '[-1.97855142  0.82195992  2.91483736 -4.19271236]', '[-1.24972285 -0.19548975  4.3426108  -5.82132949]', '[-0.2934196  -1.31598357  5.06941605 -4.8840644 ]', '[ 0.71825388 -2.02685158  4.84876147 -2.09990603]', '[ 1.56369896 -2.1596232   3.45666246  0.67974241]', '[ 2.06992565 -1.80956411  1.58953656  2.66648995]', '[ 2.21333756 -1.15096069 -0.09007755  3.80941625]', '[ 2.03658864 -0.24639688 -1.63091292  5.22998762]', '[ 1.60044769  0.87645477 -2.66369501  5.85405964]', '[ 0.97036114  2.06989352 -3.65293661  6.00273255]', '[ 0.14659583 -3.00082827 -4.43713811  6.24440154]', '[-0.72115291 -1.63986504 -4.16932076  7.55431699]', '[-1.51956855e+00  6.19949099e-03 -3.67175597e+00  8.48576377e+00]', '[-2.08500815  1.53759127 -1.82713225  6.63358296]', '[-2.24428928  2.69148708  0.13208372  5.02461995]', '[-2.09966462 -2.71410624  1.14146817  3.79688741]', '[-1.82297251 -2.053693    1.60638525  2.87131877]', '[-1.45654916 -1.5281958   2.04521374  2.51507736]', '[-1.02354082 -0.98043327  2.21208439  3.13408812]', '[-0.59419871 -0.23555043  2.12797447  4.18825028]', '[-0.11390714  0.56738398  2.83847033  3.39942586]', '[0.57219013 0.96149488 3.84514445 0.61859274]', '[ 1.31328564  0.96540243  3.40082843 -0.30928674]', '[ 1.91418137  0.87298952  2.56634982 -0.44558842]']</t>
+  </si>
+  <si>
+    <t>[0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50, 51, 52, 53, 54, 55, 56, 57, 58, 59, 60, 61, 62, 63, 64, 65, 66, 67, 68, 69, 70, 71, 72, 73, 74, 75, 76, 77, 78, 79, 80, 81, 82, 83, 84, 85, 86, 87, 88, 89, 90, 91, 92, 93, 94, 95, 96, 97, 98, 99, 100, 101, 102, 103, 104, 105, 106, 107, 108, 109, 110, 111, 112, 113, 114, 115, 116, 117, 118, 119, 120, 121, 122, 123, 124, 125, 126, 127, 128, 129, 130, 131, 132, 133, 134, 135, 136, 137, 138, 139, 140, 141, 142, 143, 144, 145, 146, 147, 148, 149, 150, 151, 152, 153, 154, 155, 156, 157, 158, 159, 160, 161, 162, 163, 164, 165, 166, 167, 168, 169, 170, 171, 172, 173, 174, 175, 176, 177, 178, 179, 180, 181, 182, 183, 184, 185, 186]</t>
+  </si>
+  <si>
+    <t>[array([-0.03763371, -0.01533471,  0.06554052, -0.01816017], dtype=float32), array([-0.03406929,  0.01398622, -0.02953871,  0.30651903]), array([-0.04818188,  0.10262173, -0.10566927,  0.56184435]), array([-0.07305261,  0.22936701, -0.13369446,  0.67944384]), array([-0.08471207,  0.32956689,  0.02155914,  0.30562945]), array([-0.06426935,  0.34812641,  0.17870967, -0.11914196]), array([-0.00340699,  0.25183341,  0.41547866, -0.82011948]), array([ 0.09360006,  0.03546661,  0.52847245, -1.29175873]), array([ 0.16926484, -0.17115921,  0.20674635, -0.72801741]), array([ 0.19733869, -0.311245  ,  0.06398557, -0.64496288]), array([ 0.19216768, -0.41959877, -0.11745588, -0.42216696]), array([ 0.12613052, -0.40998822, -0.52841548,  0.50679343]), array([-0.00992823, -0.22836713, -0.8008212 ,  1.26180348]), array([-0.16510499,  0.03359919, -0.7109692 ,  1.28647327]), array([-0.27911439,  0.2584836 , -0.39998769,  0.9080588 ]), array([-0.32955916,  0.41396917, -0.09058411,  0.61574063]), array([-0.29998127,  0.46310717,  0.38073515, -0.12681434]), array([-0.17067837,  0.33482679,  0.88450134, -1.12199   ]), array([ 0.03773497,  0.03789136,  1.14866477, -1.76343303]), array([ 0.2646821 , -0.32838888,  1.0618532 , -1.79476801]), array([ 0.44085617, -0.64241825,  0.66008786, -1.27943431]), array([ 0.51757116, -0.82253054,  0.09309348, -0.49838853]), array([ 0.45386198, -0.7765031 , -0.7186184 ,  0.9522818 ]), array([ 0.2517247 , -0.48230696, -1.26330827,  1.93683976]), array([-0.04175975, -0.00417769, -1.59704838,  2.71111161]), array([-0.33808948,  0.50064546, -1.28976878,  2.1975962 ]), array([-0.54621418,  0.86749236, -0.75086158,  1.41077933]), array([-0.62814763,  1.05198778, -0.05711646,  0.42018251]), array([-0.54750632,  0.97581252,  0.85130042, -1.17918461]), array([-0.29668199,  0.58486763,  1.61803126, -2.68759975]), array([ 0.07307157, -0.05652007,  1.98009317, -3.5377056 ]), array([ 0.42212975, -0.66996962,  1.42580926, -2.44259498]), array([ 0.64509303, -1.06304735,  0.76734931, -1.44394305]), array([ 0.7205435 , -1.24021346, -0.02078455, -0.32167835]), array([ 0.61778714, -1.13585896, -0.9931069 ,  1.36710528]), array([ 0.34371273, -0.72423562, -1.70680836,  2.71087431]), array([-0.05143972, -0.05718807, -2.14626548,  3.77718986]), array([-0.46226715,  0.68166509, -1.84586711,  3.38580784]), array([-0.75716294,  1.24256191, -1.06007547,  2.17519469]), array([-0.87727025,  1.54846333, -0.13256392,  0.88645795]), array([-0.79401259,  1.54819016,  0.9488408 , -0.8924333 ]), array([-0.52605121,  1.23889007,  1.6942977 , -2.19576532]), array([-0.11352816,  0.6216479 ,  2.37197222, -3.91013922]), array([ 0.38070481, -0.24796589,  2.42090932, -4.47704241]), array([ 0.77138832, -0.98626477,  1.41470734, -2.79122848]), array([ 0.95584969, -1.41430978,  0.41315152, -1.48568908]), array([ 0.91772932, -1.53088611, -0.78006118,  0.31897182]), array([ 0.66222879, -1.3072681 , -1.74167374,  1.92934862]), array([ 0.23900222, -0.76005264, -2.42962229,  3.4910072 ]), array([-0.28422844,  0.06099296, -2.66463741,  4.44262818]), array([-0.76181075,  0.88198562, -1.996041  ,  3.55162783]), array([-1.04796787,  1.42385541, -0.84577527,  1.87978882]), array([-1.10611948,  1.66715763,  0.26509017,  0.55696461]), array([-0.92938512,  1.59485317,  1.4785886 , -1.30154906]), array([-0.52783784,  1.13328214,  2.49684034, -3.33953229]), array([ 0.04621848,  0.27152121,  3.13374025, -5.08335726]), array([ 0.62516456, -0.67289137,  2.49197403, -4.01899701]), array([ 1.0076142 , -1.27931999,  1.30072129, -2.04553261]), array([ 1.14039219, -1.50508223,  0.022812  , -0.23603617]), array([ 1.02662319, -1.40005511, -1.15083551,  1.30249675]), array([ 0.67748325, -0.94521341, -2.31317102,  3.27242244]), array([ 0.12347069, -0.10757794, -3.10761398,  4.88498877]), array([-0.4893577 ,  0.84558507, -2.85059905,  4.29318301]), array([-0.96515318,  1.51568496, -1.86330739,  2.40800734]), array([-1.22359672,  1.82589695, -0.70272618,  0.7336522 ]), array([-1.2420747 ,  1.81848319,  0.52009264, -0.80476094]), array([-1.00915358,  1.47222249,  1.80017192, -2.70458083]), array([-0.549195  ,  0.77091995,  2.75101269, -4.28664691]), array([ 0.07470834, -0.23856978,  3.30547948, -5.41947479]), array([ 0.68814423, -1.21075361,  2.70117928, -4.06440002]), array([ 1.11403468, -1.80158046,  1.53542776, -1.90830996]), array([ 1.29482036, -1.99640584,  0.26017198, -0.07281212]), array([ 1.22362239, -1.85681769, -0.96947816,  1.48119494]), array([ 0.90224435, -1.36529353, -2.23366822,  3.49793205]), array([ 0.34952317, -0.46639093, -3.21912713,  5.394904  ]), array([-0.32581706,  0.67347565, -3.30622469,  5.49622528]), array([-0.90691235,  1.59676634, -2.44010271,  3.67859722]), array([-1.28914494,  2.16476905, -1.35877019,  2.06041551]), array([-1.44397966,  2.43763761, -0.18205811,  0.68928872]), array([-1.34908266,  2.40113916,  1.12341255, -1.06603022]), array([-1.01469398,  2.04171919,  2.18961336, -2.5682733 ]), array([-0.47395435,  1.30476718,  3.18506299, -4.87451415]), array([ 0.21513704,  0.16210558,  3.54409109, -6.2093318 ]), array([ 0.86668079, -1.01127315,  2.78107694, -5.12081956]), array([ 1.29783729, -1.85020243,  1.51559226, -3.32782814]), array([ 1.471508  , -2.36808346,  0.22267065, -1.88530744]), array([ 1.38967011, -2.60758536, -1.02898187, -0.50283757]), array([ 1.05610325, -2.52381658, -2.2674083 ,  1.35793153]), array([ 0.50883732, -2.05498181, -3.11847296,  3.36026067]), array([-0.15649769, -1.16930587, -3.47767475,  5.49142018]), array([-0.83947618,  0.04744944, -3.17706849,  6.24985012]), array([-1.35390261,  1.17083561, -1.85046882,  4.77839716]), array([-1.55862686,  1.93920382, -0.20409037,  2.96368672]), array([-1.44827408,  2.38449322,  1.28669939,  1.47031946]), array([-1.04636014,  2.47617869,  2.67139414, -0.57319765]), array([-0.41581944,  2.15033421,  3.51221873, -2.68666514]), array([ 0.28931006,  1.45830318,  3.4256414 , -4.14476285]), array([ 0.94100121,  0.49565901,  3.01966061, -5.27922038]), array([ 1.42682861, -0.46553749,  1.73917286, -4.10033195]), array([ 1.6180962 , -1.11543777,  0.16150995, -2.40414069]), array([ 1.48971203, -1.42415905, -1.4440306 , -0.63407148]), array([ 1.04684108, -1.3356208 , -2.94589455,  1.61573675]), array([ 0.34792411, -0.77745676, -3.9450366 ,  3.92599175]), array([-0.48183714,  0.1679249 , -4.13747719,  5.04917178]), array([-1.20931609,  1.01288168, -3.03104835,  3.21654177]), array([-1.6832515 ,  1.47042492, -1.70963327,  1.46482879]), array([-1.90627314,  1.66277166, -0.53036482,  0.5223107 ]), array([-1.88051549,  1.64299066,  0.78948175, -0.72882764]), array([-1.58676155,  1.35046889,  2.16230635, -2.29070383]), array([-1.01013477,  0.67816182,  3.59928113, -4.51333493]), array([-0.18058127, -0.3959971 ,  4.48819125, -5.72025834]), array([ 0.66575321, -1.31411892,  3.82861117, -3.21843752]), array([ 1.33068519, -1.72996474,  2.74370707, -1.00785133]), array([ 1.74492872, -1.76020252,  1.38492588,  0.5938918 ]), array([ 1.87823019, -1.50669165, -0.04133421,  1.88050032]), array([ 1.73210772, -1.01544836, -1.41812108,  3.05726097]), array([ 1.29724635, -0.23186241, -2.91896433,  4.78127162]), array([ 0.6102679 ,  0.78265777, -3.81764436,  4.99938455]), array([-0.18883559,  1.65382389, -4.05125602,  3.48142489]), array([-0.94635112,  2.11098814, -3.37648944,  1.07702824]), array([-1.49694486,  2.11981547, -2.05108658, -0.92487302]), array([-1.75066352,  1.77278213, -0.47484912, -2.47078699]), array([-1.69040873,  1.15251765,  1.05892096, -3.71547134]), array([-1.31147028,  0.2197767 ,  2.69489751, -5.5846431 ]), array([-0.6605723 , -0.97581101,  3.65987854, -5.96670847]), array([ 0.09360104, -1.99521412,  3.82635087, -4.13688511]), array([ 0.82746963, -2.62249913,  3.37372483, -2.14638158]), array([ 1.40774113, -2.90028668,  2.35947975, -0.64911284]), array([ 1.74765425, -2.85003209,  1.02869765,  1.1322257 ]), array([ 1.82760263, -2.49528287, -0.24197761,  2.39803162]), array([ 1.62954198, -1.84674267, -1.76617806,  4.15006344]), array([ 1.11805008, -0.81001063, -3.35953403,  6.3309867 ]), array([ 0.32944972,  0.60627624, -4.25585001,  7.18237158]), array([-0.50069712,  1.84910219, -3.95548161,  5.07487125]), array([-1.22569228,  2.65911814, -3.2065514 ,  3.12479026]), array([-1.7561106 ,  3.13321642, -2.07276994,  1.67350828]), array([-2.05863522, -2.94175293, -0.97590996,  0.42721254]), array([-2.14891759, -2.99355605,  0.06224683, -0.93395129]), array([-2.02588588,  2.95145029,  1.18826232, -2.44989007]), array([-1.67404027,  2.33906907,  2.35325909, -3.73806531]), array([-1.07878211,  1.40911992,  3.61280379, -5.72619919]), array([-0.2102876 , -0.04563889,  4.8749034 , -8.35857269]), array([ 0.71899543, -1.54612687,  4.20680328, -6.13536529]), array([ 1.46203947, -2.5301277 ,  3.19719524, -3.88187565]), array([ 1.98828344,  3.12773329,  2.07002329, -2.46096128]), array([ 2.30260177,  2.74971449,  1.11470349, -1.34228089]), array([2.4358686 , 2.62646072, 0.24220093, 0.10278277]), array([ 2.41573633,  2.74814183, -0.4470137 ,  1.1078727 ]), array([ 2.24396692,  3.08815558, -1.30231934,  2.29604766]), array([ 1.87196521, -2.5883204 , -2.46148253,  3.83411423]), array([ 1.24403542, -1.60804494, -3.86285123,  6.20089963]), array([ 0.31924776, -0.04734268, -5.21120762,  8.99167856]), array([-0.68468569,  1.57940247, -4.57857715,  6.63469034]), array([-1.49789759,  2.62452066, -3.52926166,  4.04428619]), array([-2.08615317, -3.01813295, -2.36495681,  2.46604714]), array([-2.46182637, -2.6493644 , -1.44958943,  1.25509116]), array([-2.68700997, -2.50634043, -0.84940054,  0.20032485]), array([-2.82276687, -2.53841827, -0.53959236, -0.49128809]), array([-2.90016407, -2.73040634, -0.25343164, -1.39144076]), array([-2.92636897e+00, -3.07951481e+00,  4.65324835e-04, -2.06087208e+00]), array([-2.88978296,  2.7428902 ,  0.40226012, -2.51839541]), array([-2.74915069,  2.20322129,  1.04354768, -2.88284391]), array([-2.45701902,  1.57601674,  1.92199553, -3.46842133]), array([-1.97855142,  0.82195992,  2.91483736, -4.19271236]), array([-1.24972285, -0.19548975,  4.3426108 , -5.82132949]), array([-0.2934196 , -1.31598357,  5.06941605, -4.8840644 ]), array([ 0.71825388, -2.02685158,  4.84876147, -2.09990603]), array([ 1.56369896, -2.1596232 ,  3.45666246,  0.67974241]), array([ 2.06992565, -1.80956411,  1.58953656,  2.66648995]), array([ 2.21333756, -1.15096069, -0.09007755,  3.80941625]), array([ 2.03658864, -0.24639688, -1.63091292,  5.22998762]), array([ 1.60044769,  0.87645477, -2.66369501,  5.85405964]), array([ 0.97036114,  2.06989352, -3.65293661,  6.00273255]), array([ 0.14659583, -3.00082827, -4.43713811,  6.24440154]), array([-0.72115291, -1.63986504, -4.16932076,  7.55431699]), array([-1.51956855e+00,  6.19949099e-03, -3.67175597e+00,  8.48576377e+00]), array([-2.08500815,  1.53759127, -1.82713225,  6.63358296]), array([-2.24428928,  2.69148708,  0.13208372,  5.02461995]), array([-2.09966462, -2.71410624,  1.14146817,  3.79688741]), array([-1.82297251, -2.053693  ,  1.60638525,  2.87131877]), array([-1.45654916, -1.5281958 ,  2.04521374,  2.51507736]), array([-1.02354082, -0.98043327,  2.21208439,  3.13408812]), array([-0.59419871, -0.23555043,  2.12797447,  4.18825028]), array([-0.11390714,  0.56738398,  2.83847033,  3.39942586]), array([0.57219013, 0.96149488, 3.84514445, 0.61859274]), array([ 1.31328564,  0.96540243,  3.40082843, -0.30928674]), array([ 1.91418137,  0.87298952,  2.56634982, -0.44558842])]</t>
+  </si>
+  <si>
+    <t>['[2,2,2]', '[0,2,1]', '[1,0,2]', '[1,2,0]', '[0,1,1]', '[1,1,2]', '[1,1,1]', '[2,0,1]', '[2,1,0]', '[0,0,0]']</t>
+  </si>
+  <si>
+    <t>[5, 7, 9, 10, 11, 12, 15, 16, 20, 21, 22, 26, 27, 29, 33, 34, 35, 37, 38, 39, 41, 42, 43, 44, 46, 47, 48, 49, 50, 51, 53, 55, 56, 58, 59, 60, 61, 62, 64, 65, 69, 70, 73, 74, 75, 76, 77, 79, 80, 82, 83, 84, 90, 91, 93, 95, 96, 97, 100, 102, 103, 108, 109, 110, 111, 114, 115, 117, 119, 124, 125, 127, 128, 129, 130, 131, 133, 134, 135, 136, 137, 138, 140, 141, 144, 146, 148, 149, 151, 152, 153, 155, 157, 158, 159, 162, 165, 166, 167, 169, 170, 172, 173, 174, 175, 176, 177, 178, 179, 181, 183, 185, 187, 190, 191, 193, 194, 196, 197, 198, 199]</t>
+  </si>
+  <si>
+    <t>[0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 1, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 2]</t>
+  </si>
+  <si>
+    <t>['[-0.03763371 -0.01533471  0.06554052 -0.01816017]', '[-0.00754409 -0.05458322  0.2277812  -0.36241836]', '[ 0.04879627 -0.15231473  0.32089719 -0.5887683 ]', '[ 0.11397169 -0.27767857  0.31375488 -0.63332862]', '[ 0.16759438 -0.39312519  0.2086893  -0.49480525]', '[ 0.16756229 -0.40059886 -0.20854687  0.42010337]', '[ 0.08785953 -0.23163826 -0.56914473  1.23330318]', '[-0.03496308  0.03550642 -0.62492445  1.37100342]', '[-0.16086758  0.32239077 -0.59829402  1.42632207]', '[-0.24821629  0.54624438 -0.25469228  0.77043444]', '[-0.2581729   0.62047788  0.15657145 -0.03641898]', '[-0.20045827  0.5657268   0.40809078 -0.4962178 ]', '[-0.10215641  0.4318351   0.55243466 -0.80905558]', '[ 0.03585965  0.19163324  0.79478601 -1.53578676]', '[ 0.198972   -0.15108812  0.79060749 -1.80207488]', '[ 0.3078316  -0.42539481  0.2713019  -0.88648234]', '[ 0.30242235 -0.49387728 -0.32368128  0.20766446]', '[ 0.18360005 -0.34709493 -0.83908972  1.22610838]', '[-0.01785413 -0.02736485 -1.12510567  1.8845045 ]', '[-0.24214039  0.36271199 -1.05788189  1.90689269]', '[-0.4068205   0.66428367 -0.55449804  1.0527991 ]', '[-0.45549179  0.77123043  0.0753671   0.00492952]', '[-0.38963746  0.69783482  0.57034218 -0.72545518]', '[-0.21164669  0.42700804  1.1749769  -1.93504057]', '[ 0.05906424 -0.04099989  1.46095587 -2.61446122]', '[ 0.33907314 -0.55474349  1.26366267 -2.38222915]', '[ 0.51727182 -0.89112338  0.49165093 -0.9469629 ]', '[ 0.5308362  -0.92895671 -0.35648363  0.56931409]', '[ 0.37830696 -0.66571443 -1.1467149   2.0400303 ]', '[ 0.10152289 -0.17031155 -1.55385174  2.79476443]', '[-0.22090524  0.41862481 -1.57667277  2.91321218]', '[-0.49506616  0.93173813 -1.10716579  2.12325684]', '[-0.64886905  1.24874506 -0.41106509  1.02834179]', '[-0.64649883  1.31389602  0.43031573 -0.37573693]', '[-0.49197875  1.12633674  1.09153129 -1.489019  ]', '[-0.22356022  0.72886428  1.54546402 -2.42889097]', '[ 0.12555293  0.12940436  1.86171616 -3.41203226]', '[ 0.45123515 -0.48206909  1.30660379 -2.53270993]', '[ 0.62542102 -0.84472711  0.40925149 -1.05710243]', '[ 0.61156874 -0.90043064 -0.54255589  0.5009012 ]', '[ 0.41493415 -0.64652754 -1.39341543  2.01363934]', '[ 0.08734706 -0.15466736 -1.80571897  2.77584844]', '[-0.26831362  0.39192473 -1.65651843  2.51642572]', '[-0.54338358  0.79760376 -1.04139767  1.46647266]', '[-0.67115509  0.96478388 -0.21825715  0.19424766]', '[-0.61672874  0.84456875  0.75723531 -1.39261261]', '[-0.40029807  0.47863867  1.3647862  -2.2062435 ]', '[-0.09600966  0.00347406  1.60003623 -2.40676234]', '[ 0.20538141 -0.42205806  1.34024049 -1.72346296]', '[ 0.41619057 -0.65048056  0.72704906 -0.51405386]', '[ 0.48497504 -0.61893447 -0.05251378  0.83103306]', '[ 0.4080302  -0.35723903 -0.69841199  1.74421279]', '[ 0.20678012  0.08441116 -1.25782065  2.56188963]', '[-0.0525349   0.57544068 -1.26751337  2.21908999]', '[-0.28875179  0.96226564 -1.04704003  1.57563666]', '[-0.44555152  1.1587048  -0.49620823  0.3701808 ]', '[-0.47989357  1.10665259  0.16265242 -0.89285285]', '[-0.36844282  0.77331348  0.94382936 -2.42692106]', '[-0.13978783  0.22287239  1.27888994 -2.95376404]', '[ 0.10979111 -0.34128395  1.13870706 -2.52990378]', '[ 0.29083069 -0.74049021  0.63513285 -1.39556006]', '[ 0.35571043 -0.88647949  0.00590574 -0.05313236]', '[ 0.30474842 -0.79199378 -0.50696348  0.98681731]', '[ 0.14761943 -0.46982443 -1.03547468  2.18728829]', '[-0.07694228  0.01300518 -1.14547736  2.51356585]', '[-0.28216729  0.47888212 -0.84870247  2.03010721]', '[-0.41126628  0.82364722 -0.41370586  1.36195738]', '[-0.44141472  1.01048742  0.11497515  0.4917175 ]', '[-0.34664187  0.96084845  0.81386537 -0.97855781]', '[-0.14972416  0.68900128  1.11678576 -1.68981036]', '[ 0.08062219  0.31497171  1.13142466 -1.95460649]', '[ 0.30517207 -0.11675697  1.05308424 -2.2455098 ]', '[ 0.47731111 -0.53524711  0.6209553  -1.84577378]', '[ 0.51696303 -0.76588848 -0.22801111 -0.44133583]', '[ 0.40217498 -0.74169492 -0.89757301  0.67282654]', '[ 0.17168718 -0.50791221 -1.3607326   1.61139539]', '[-0.11801414 -0.13153358 -1.46692464  2.03922902]', '[-0.38496169  0.25559529 -1.13661663  1.71813231]', '[-0.56385532  0.55315158 -0.61332307  1.1947074 ]', '[-0.60791183  0.68534235  0.17976529  0.11281586]', '[-0.50636712  0.62953515  0.81778083 -0.659361  ]', '[-0.26802266  0.36695659  1.51904067 -1.91132846]', '[ 0.04774245 -0.02586162  1.56045908 -1.88763285]', '[ 0.32468681 -0.33642313  1.14538955 -1.12261485]', '[ 0.4860787  -0.44947966  0.43776036  0.02115478]', '[ 0.49318717 -0.32513347 -0.36582767  1.20598086]', '[ 0.34695823  0.01631252 -1.05782483  2.13191453]', '[ 0.09351726  0.48173453 -1.40780506  2.3894974 ]', '[-0.18772998  0.91938835 -1.34426195  1.88727992]', '[-0.42348706  1.20870798 -0.97216373  0.9651981 ]', '[-0.55275541  1.26921098 -0.29592067 -0.36851589]', '[-0.54538719  1.08740799  0.37379049 -1.44390094]', '[-0.38287013  0.63721541  1.23357373 -3.03017672]', '[-0.09898304 -0.01906569  1.51441948 -3.3525079 ]', '[ 0.207131   -0.68666325  1.45291961 -3.13669548]', '[ 0.43256411 -1.16452738  0.77503615 -1.60921565]', '[ 0.51199757 -1.32817919  0.01420953 -0.02870202]', '[ 0.44804723 -1.20308022 -0.64698558  1.27675348]', '[ 0.24772962 -0.79172842 -1.33462944  2.81536802]', '[-0.06791057 -0.10583838 -1.73805297  3.88099573]', '[-0.38622058  0.62889872 -1.34209634  3.26019964]', '[-0.58914814  1.179051   -0.65216479  2.18417457]', '[-0.63273152  1.46919469  0.2080228   0.72256694]', '[-0.52206892  1.49589847  0.87332528 -0.44847421]', '[-0.27853921  1.2423978   1.52455703 -2.07458846]', '[ 0.07142813  0.67660382  1.92484041 -3.51646418]', '[ 0.4594029  -0.10431658  1.8416024  -4.05997243]', '[ 0.75801784 -0.84631     1.05919381 -3.19957142]', '[ 0.84555022 -1.30033769 -0.1789152  -1.34337769]', '[ 0.70434871 -1.41131975 -1.20089833  0.23675911]', '[ 0.38374391 -1.20577478 -1.94806941  1.80332521]', '[-0.04796034 -0.70748619 -2.29219815  3.08600024]', '[-0.50748041 -0.00421836 -2.19111327  3.72406706]', '[-0.8765674   0.68528688 -1.4128244   3.00909719]', '[-1.04118542  1.1395524  -0.21799109  1.52059853]', '[-0.9640096   1.29119119  0.9759216  -0.0178035 ]', '[-0.65216019  1.09668342  2.10013229 -1.94493307]', '[-0.17010224  0.57929023  2.63279695 -3.1245109 ]', '[ 0.37872175 -0.13899051  2.71413718 -3.78325405]', '[ 0.83361415 -0.75721231  1.7511066  -2.26812683]', '[ 1.0846674  -1.09398337  0.73346791 -1.09529975]', '[ 1.12192146 -1.19771396 -0.36369911  0.05849822]', '[ 0.92098488 -1.00934617 -1.62992731  1.85006923]', '[ 0.48184387 -0.45166624 -2.70190702  3.67099816]', '[-0.10010126  0.3428221  -2.95884639  3.95265217]', '[-0.64011149  1.00813638 -2.33883578  2.54735029]', '[-1.01976089  1.37255423 -1.41294558  1.10261664]', '[-1.18400009  1.4338894  -0.21343469 -0.46384349]', '[-1.11227543  1.21754455  0.92626457 -1.70207358]', '[-0.81908359  0.74914147  1.97590629 -2.97351848]', '[-0.34600397  0.05775721  2.65054282 -3.75346841]', '[ 0.18422893 -0.63881141  2.51994231 -2.96251918]', '[ 0.6430985  -1.12190646  1.98728093 -1.78006004]', '[ 0.93395786 -1.28609486  0.88006835  0.12245177]', '[ 0.99383702 -1.10700397 -0.29370158  1.65679688]', '[ 0.81680926 -0.62597126 -1.45633972  3.13151984]', '[ 0.43277573  0.11183606 -2.28414375  4.05378275]', '[-0.04376595  0.88500783 -2.36594069  3.44621587]', '[-0.47894196  1.43321272 -1.92101693  1.97520055]', '[-0.79787305  1.69148337 -1.21746852  0.60169389]', '[-0.9408622   1.65166036 -0.18402035 -0.99468156]', '[-0.87401001  1.31813253  0.85298836 -2.34345394]', '[-0.58230242  0.65462339  2.03951586 -4.28070546]', '[-0.09352269 -0.33326545  2.67912067 -5.24993571]', '[ 0.39320106 -1.23085756  2.09972545 -3.56934316]', '[ 0.74827897 -1.80263647  1.41365688 -2.14821001]', '[ 0.93103989 -2.05113452  0.39573102 -0.35653113]', '[ 0.90224405 -1.94769681 -0.68498354  1.39804888]', '[ 0.66784397 -1.50679557 -1.64364066  3.03768283]', '[ 0.25387903 -0.72387886 -2.44997333  4.75144854]', '[-0.27864103  0.34088415 -2.68183443  5.49056383]', '[-0.72989891  1.28332664 -1.74595606  3.79762239]', '[-0.96729978  1.86404799 -0.6234159   2.04777669]', '[-0.98038807  2.11328307  0.48095806  0.45701175]', '[-0.77692866  2.0256711   1.51796551 -1.33959713]', '[-0.40722621  1.61901149  2.12430622 -2.72328306]', '[ 0.06925998  0.89078568  2.59149389 -4.51868092]', '[ 0.56845211 -0.05515058  2.2521476  -4.62141508]', '[ 0.91117188 -0.83533847  1.09647733 -3.03701189]', '[ 0.99684521 -1.25811428 -0.23692872 -1.19328475]', '[ 0.82359327 -1.3109681  -1.46424031  0.67936958]', '[ 0.42909963 -0.9796618  -2.42364121  2.62913942]', '[-0.10324306 -0.31709629 -2.78870894  3.8126715 ]', '[-0.64072971  0.46229407 -2.44381859  3.6937405 ]', '[-1.03795486  1.08326448 -1.47316468  2.45280461]', '[-1.20964459  1.41713634 -0.2365592   0.90705478]', '[-1.14174529  1.4738879   0.90904343 -0.35425836]', '[-0.85288327  1.26461345  1.94910987 -1.76568373]', '[-0.35953969  0.70490705  2.92180968 -3.80014227]', '[ 0.24565549 -0.11732796  2.9673789  -4.09118226]', '[ 0.76248288 -0.79948097  2.09888637 -2.56199062]', '[ 1.08564869 -1.18385785  1.09907771 -1.28030779]', '[ 1.17475979 -1.26430099 -0.21335295  0.46028481]', '[ 1.01089861 -1.0250622  -1.41513904  1.94966616]', '[ 0.61801873 -0.48005085 -2.46327283  3.45446898]', '[ 0.06553354  0.28868469 -2.91636003  3.94231741]', '[-0.48634223  0.97193653 -2.48816842  2.70264339]', '[-0.89789303  1.34051915 -1.57192026  0.97944538]', '[-1.09877094  1.37252167 -0.41135207 -0.63500366]', '[-1.06733472  1.11981691  0.72400805 -1.88374424]', '[-0.7910394   0.5591882   2.01506926 -3.71217218]', '[-0.3169442  -0.24878109  2.59768218 -4.10872918]', '[ 0.21530769 -1.02775437  2.60336165 -3.44591563]', '[ 0.668545   -1.52388849  1.86816844 -1.49717668]', '[ 0.95806075 -1.67852219  0.98235793 -0.05936489]', '[ 1.04896262 -1.55334285 -0.08975201  1.30080989]', '[ 0.90035145 -1.10507348 -1.39994451  3.20966736]', '[ 0.5075623  -0.29704128 -2.4540646   4.75502678]', '[-0.03344433  0.70743547 -2.77639098  4.9061992 ]', '[-0.5476934   1.55364416 -2.29499588  3.46338067]', '[-0.92424226  2.06927403 -1.43291692  1.72434788]', '[-1.10763655  2.25370705 -0.37918722  0.13582877]', '[-1.06455377  2.10414955  0.81115879 -1.64156578]', '[-0.80166926  1.63161669  1.79742067 -3.11364253]', '[-0.35693161  0.84779879  2.60255566 -4.69787744]', '[ 0.22172289 -0.23851668  2.99174036 -5.75870336]', '[ 0.72999555 -1.21117437  1.99510573 -3.8039179 ]', '[ 1.00984635 -1.76668109  0.79753468 -1.80026433]', '[ 1.04859931 -1.94479425 -0.40438866  0.00661487]', '[ 0.86129121 -1.78453089 -1.44509191  1.61255663]']</t>
+  </si>
+  <si>
+    <t>[array([-0.03763371, -0.01533471,  0.06554052, -0.01816017], dtype=float32), array([-0.00754409, -0.05458322,  0.2277812 , -0.36241836]), array([ 0.04879627, -0.15231473,  0.32089719, -0.5887683 ]), array([ 0.11397169, -0.27767857,  0.31375488, -0.63332862]), array([ 0.16759438, -0.39312519,  0.2086893 , -0.49480525]), array([ 0.16756229, -0.40059886, -0.20854687,  0.42010337]), array([ 0.08785953, -0.23163826, -0.56914473,  1.23330318]), array([-0.03496308,  0.03550642, -0.62492445,  1.37100342]), array([-0.16086758,  0.32239077, -0.59829402,  1.42632207]), array([-0.24821629,  0.54624438, -0.25469228,  0.77043444]), array([-0.2581729 ,  0.62047788,  0.15657145, -0.03641898]), array([-0.20045827,  0.5657268 ,  0.40809078, -0.4962178 ]), array([-0.10215641,  0.4318351 ,  0.55243466, -0.80905558]), array([ 0.03585965,  0.19163324,  0.79478601, -1.53578676]), array([ 0.198972  , -0.15108812,  0.79060749, -1.80207488]), array([ 0.3078316 , -0.42539481,  0.2713019 , -0.88648234]), array([ 0.30242235, -0.49387728, -0.32368128,  0.20766446]), array([ 0.18360005, -0.34709493, -0.83908972,  1.22610838]), array([-0.01785413, -0.02736485, -1.12510567,  1.8845045 ]), array([-0.24214039,  0.36271199, -1.05788189,  1.90689269]), array([-0.4068205 ,  0.66428367, -0.55449804,  1.0527991 ]), array([-0.45549179,  0.77123043,  0.0753671 ,  0.00492952]), array([-0.38963746,  0.69783482,  0.57034218, -0.72545518]), array([-0.21164669,  0.42700804,  1.1749769 , -1.93504057]), array([ 0.05906424, -0.04099989,  1.46095587, -2.61446122]), array([ 0.33907314, -0.55474349,  1.26366267, -2.38222915]), array([ 0.51727182, -0.89112338,  0.49165093, -0.9469629 ]), array([ 0.5308362 , -0.92895671, -0.35648363,  0.56931409]), array([ 0.37830696, -0.66571443, -1.1467149 ,  2.0400303 ]), array([ 0.10152289, -0.17031155, -1.55385174,  2.79476443]), array([-0.22090524,  0.41862481, -1.57667277,  2.91321218]), array([-0.49506616,  0.93173813, -1.10716579,  2.12325684]), array([-0.64886905,  1.24874506, -0.41106509,  1.02834179]), array([-0.64649883,  1.31389602,  0.43031573, -0.37573693]), array([-0.49197875,  1.12633674,  1.09153129, -1.489019  ]), array([-0.22356022,  0.72886428,  1.54546402, -2.42889097]), array([ 0.12555293,  0.12940436,  1.86171616, -3.41203226]), array([ 0.45123515, -0.48206909,  1.30660379, -2.53270993]), array([ 0.62542102, -0.84472711,  0.40925149, -1.05710243]), array([ 0.61156874, -0.90043064, -0.54255589,  0.5009012 ]), array([ 0.41493415, -0.64652754, -1.39341543,  2.01363934]), array([ 0.08734706, -0.15466736, -1.80571897,  2.77584844]), array([-0.26831362,  0.39192473, -1.65651843,  2.51642572]), array([-0.54338358,  0.79760376, -1.04139767,  1.46647266]), array([-0.67115509,  0.96478388, -0.21825715,  0.19424766]), array([-0.61672874,  0.84456875,  0.75723531, -1.39261261]), array([-0.40029807,  0.47863867,  1.3647862 , -2.2062435 ]), array([-0.09600966,  0.00347406,  1.60003623, -2.40676234]), array([ 0.20538141, -0.42205806,  1.34024049, -1.72346296]), array([ 0.41619057, -0.65048056,  0.72704906, -0.51405386]), array([ 0.48497504, -0.61893447, -0.05251378,  0.83103306]), array([ 0.4080302 , -0.35723903, -0.69841199,  1.74421279]), array([ 0.20678012,  0.08441116, -1.25782065,  2.56188963]), array([-0.0525349 ,  0.57544068, -1.26751337,  2.21908999]), array([-0.28875179,  0.96226564, -1.04704003,  1.57563666]), array([-0.44555152,  1.1587048 , -0.49620823,  0.3701808 ]), array([-0.47989357,  1.10665259,  0.16265242, -0.89285285]), array([-0.36844282,  0.77331348,  0.94382936, -2.42692106]), array([-0.13978783,  0.22287239,  1.27888994, -2.95376404]), array([ 0.10979111, -0.34128395,  1.13870706, -2.52990378]), array([ 0.29083069, -0.74049021,  0.63513285, -1.39556006]), array([ 0.35571043, -0.88647949,  0.00590574, -0.05313236]), array([ 0.30474842, -0.79199378, -0.50696348,  0.98681731]), array([ 0.14761943, -0.46982443, -1.03547468,  2.18728829]), array([-0.07694228,  0.01300518, -1.14547736,  2.51356585]), array([-0.28216729,  0.47888212, -0.84870247,  2.03010721]), array([-0.41126628,  0.82364722, -0.41370586,  1.36195738]), array([-0.44141472,  1.01048742,  0.11497515,  0.4917175 ]), array([-0.34664187,  0.96084845,  0.81386537, -0.97855781]), array([-0.14972416,  0.68900128,  1.11678576, -1.68981036]), array([ 0.08062219,  0.31497171,  1.13142466, -1.95460649]), array([ 0.30517207, -0.11675697,  1.05308424, -2.2455098 ]), array([ 0.47731111, -0.53524711,  0.6209553 , -1.84577378]), array([ 0.51696303, -0.76588848, -0.22801111, -0.44133583]), array([ 0.40217498, -0.74169492, -0.89757301,  0.67282654]), array([ 0.17168718, -0.50791221, -1.3607326 ,  1.61139539]), array([-0.11801414, -0.13153358, -1.46692464,  2.03922902]), array([-0.38496169,  0.25559529, -1.13661663,  1.71813231]), array([-0.56385532,  0.55315158, -0.61332307,  1.1947074 ]), array([-0.60791183,  0.68534235,  0.17976529,  0.11281586]), array([-0.50636712,  0.62953515,  0.81778083, -0.659361  ]), array([-0.26802266,  0.36695659,  1.51904067, -1.91132846]), array([ 0.04774245, -0.02586162,  1.56045908, -1.88763285]), array([ 0.32468681, -0.33642313,  1.14538955, -1.12261485]), array([ 0.4860787 , -0.44947966,  0.43776036,  0.02115478]), array([ 0.49318717, -0.32513347, -0.36582767,  1.20598086]), array([ 0.34695823,  0.01631252, -1.05782483,  2.13191453]), array([ 0.09351726,  0.48173453, -1.40780506,  2.3894974 ]), array([-0.18772998,  0.91938835, -1.34426195,  1.88727992]), array([-0.42348706,  1.20870798, -0.97216373,  0.9651981 ]), array([-0.55275541,  1.26921098, -0.29592067, -0.36851589]), array([-0.54538719,  1.08740799,  0.37379049, -1.44390094]), array([-0.38287013,  0.63721541,  1.23357373, -3.03017672]), array([-0.09898304, -0.01906569,  1.51441948, -3.3525079 ]), array([ 0.207131  , -0.68666325,  1.45291961, -3.13669548]), array([ 0.43256411, -1.16452738,  0.77503615, -1.60921565]), array([ 0.51199757, -1.32817919,  0.01420953, -0.02870202]), array([ 0.44804723, -1.20308022, -0.64698558,  1.27675348]), array([ 0.24772962, -0.79172842, -1.33462944,  2.81536802]), array([-0.06791057, -0.10583838, -1.73805297,  3.88099573]), array([-0.38622058,  0.62889872, -1.34209634,  3.26019964]), array([-0.58914814,  1.179051  , -0.65216479,  2.18417457]), array([-0.63273152,  1.46919469,  0.2080228 ,  0.72256694]), array([-0.52206892,  1.49589847,  0.87332528, -0.44847421]), array([-0.27853921,  1.2423978 ,  1.52455703, -2.07458846]), array([ 0.07142813,  0.67660382,  1.92484041, -3.51646418]), array([ 0.4594029 , -0.10431658,  1.8416024 , -4.05997243]), array([ 0.75801784, -0.84631   ,  1.05919381, -3.19957142]), array([ 0.84555022, -1.30033769, -0.1789152 , -1.34337769]), array([ 0.70434871, -1.41131975, -1.20089833,  0.23675911]), array([ 0.38374391, -1.20577478, -1.94806941,  1.80332521]), array([-0.04796034, -0.70748619, -2.29219815,  3.08600024]), array([-0.50748041, -0.00421836, -2.19111327,  3.72406706]), array([-0.8765674 ,  0.68528688, -1.4128244 ,  3.00909719]), array([-1.04118542,  1.1395524 , -0.21799109,  1.52059853]), array([-0.9640096 ,  1.29119119,  0.9759216 , -0.0178035 ]), array([-0.65216019,  1.09668342,  2.10013229, -1.94493307]), array([-0.17010224,  0.57929023,  2.63279695, -3.1245109 ]), array([ 0.37872175, -0.13899051,  2.71413718, -3.78325405]), array([ 0.83361415, -0.75721231,  1.7511066 , -2.26812683]), array([ 1.0846674 , -1.09398337,  0.73346791, -1.09529975]), array([ 1.12192146, -1.19771396, -0.36369911,  0.05849822]), array([ 0.92098488, -1.00934617, -1.62992731,  1.85006923]), array([ 0.48184387, -0.45166624, -2.70190702,  3.67099816]), array([-0.10010126,  0.3428221 , -2.95884639,  3.95265217]), array([-0.64011149,  1.00813638, -2.33883578,  2.54735029]), array([-1.01976089,  1.37255423, -1.41294558,  1.10261664]), array([-1.18400009,  1.4338894 , -0.21343469, -0.46384349]), array([-1.11227543,  1.21754455,  0.92626457, -1.70207358]), array([-0.81908359,  0.74914147,  1.97590629, -2.97351848]), array([-0.34600397,  0.05775721,  2.65054282, -3.75346841]), array([ 0.18422893, -0.63881141,  2.51994231, -2.96251918]), array([ 0.6430985 , -1.12190646,  1.98728093, -1.78006004]), array([ 0.93395786, -1.28609486,  0.88006835,  0.12245177]), array([ 0.99383702, -1.10700397, -0.29370158,  1.65679688]), array([ 0.81680926, -0.62597126, -1.45633972,  3.13151984]), array([ 0.43277573,  0.11183606, -2.28414375,  4.05378275]), array([-0.04376595,  0.88500783, -2.36594069,  3.44621587]), array([-0.47894196,  1.43321272, -1.92101693,  1.97520055]), array([-0.79787305,  1.69148337, -1.21746852,  0.60169389]), array([-0.9408622 ,  1.65166036, -0.18402035, -0.99468156]), array([-0.87401001,  1.31813253,  0.85298836, -2.34345394]), array([-0.58230242,  0.65462339,  2.03951586, -4.28070546]), array([-0.09352269, -0.33326545,  2.67912067, -5.24993571]), array([ 0.39320106, -1.23085756,  2.09972545, -3.56934316]), array([ 0.74827897, -1.80263647,  1.41365688, -2.14821001]), array([ 0.93103989, -2.05113452,  0.39573102, -0.35653113]), array([ 0.90224405, -1.94769681, -0.68498354,  1.39804888]), array([ 0.66784397, -1.50679557, -1.64364066,  3.03768283]), array([ 0.25387903, -0.72387886, -2.44997333,  4.75144854]), array([-0.27864103,  0.34088415, -2.68183443,  5.49056383]), array([-0.72989891,  1.28332664, -1.74595606,  3.79762239]), array([-0.96729978,  1.86404799, -0.6234159 ,  2.04777669]), array([-0.98038807,  2.11328307,  0.48095806,  0.45701175]), array([-0.77692866,  2.0256711 ,  1.51796551, -1.33959713]), array([-0.40722621,  1.61901149,  2.12430622, -2.72328306]), array([ 0.06925998,  0.89078568,  2.59149389, -4.51868092]), array([ 0.56845211, -0.05515058,  2.2521476 , -4.62141508]), array([ 0.91117188, -0.83533847,  1.09647733, -3.03701189]), array([ 0.99684521, -1.25811428, -0.23692872, -1.19328475]), array([ 0.82359327, -1.3109681 , -1.46424031,  0.67936958]), array([ 0.42909963, -0.9796618 , -2.42364121,  2.62913942]), array([-0.10324306, -0.31709629, -2.78870894,  3.8126715 ]), array([-0.64072971,  0.46229407, -2.44381859,  3.6937405 ]), array([-1.03795486,  1.08326448, -1.47316468,  2.45280461]), array([-1.20964459,  1.41713634, -0.2365592 ,  0.90705478]), array([-1.14174529,  1.4738879 ,  0.90904343, -0.35425836]), array([-0.85288327,  1.26461345,  1.94910987, -1.76568373]), array([-0.35953969,  0.70490705,  2.92180968, -3.80014227]), array([ 0.24565549, -0.11732796,  2.9673789 , -4.09118226]), array([ 0.76248288, -0.79948097,  2.09888637, -2.56199062]), array([ 1.08564869, -1.18385785,  1.09907771, -1.28030779]), array([ 1.17475979, -1.26430099, -0.21335295,  0.46028481]), array([ 1.01089861, -1.0250622 , -1.41513904,  1.94966616]), array([ 0.61801873, -0.48005085, -2.46327283,  3.45446898]), array([ 0.06553354,  0.28868469, -2.91636003,  3.94231741]), array([-0.48634223,  0.97193653, -2.48816842,  2.70264339]), array([-0.89789303,  1.34051915, -1.57192026,  0.97944538]), array([-1.09877094,  1.37252167, -0.41135207, -0.63500366]), array([-1.06733472,  1.11981691,  0.72400805, -1.88374424]), array([-0.7910394 ,  0.5591882 ,  2.01506926, -3.71217218]), array([-0.3169442 , -0.24878109,  2.59768218, -4.10872918]), array([ 0.21530769, -1.02775437,  2.60336165, -3.44591563]), array([ 0.668545  , -1.52388849,  1.86816844, -1.49717668]), array([ 0.95806075, -1.67852219,  0.98235793, -0.05936489]), array([ 1.04896262, -1.55334285, -0.08975201,  1.30080989]), array([ 0.90035145, -1.10507348, -1.39994451,  3.20966736]), array([ 0.5075623 , -0.29704128, -2.4540646 ,  4.75502678]), array([-0.03344433,  0.70743547, -2.77639098,  4.9061992 ]), array([-0.5476934 ,  1.55364416, -2.29499588,  3.46338067]), array([-0.92424226,  2.06927403, -1.43291692,  1.72434788]), array([-1.10763655,  2.25370705, -0.37918722,  0.13582877]), array([-1.06455377,  2.10414955,  0.81115879, -1.64156578]), array([-0.80166926,  1.63161669,  1.79742067, -3.11364253]), array([-0.35693161,  0.84779879,  2.60255566, -4.69787744]), array([ 0.22172289, -0.23851668,  2.99174036, -5.75870336]), array([ 0.72999555, -1.21117437,  1.99510573, -3.8039179 ]), array([ 1.00984635, -1.76668109,  0.79753468, -1.80026433]), array([ 1.04859931, -1.94479425, -0.40438866,  0.00661487]), array([ 0.86129121, -1.78453089, -1.44509191,  1.61255663])]</t>
+  </si>
+  <si>
+    <t>['[2,0,1]', '[0,2,1]', '[2,1,0]', '[1,1,2]', '[1,2,0]', '[1,0,2]', '[1,1,1]', '[0,1,1]', '[0,0,0]', '[2,2,2]']</t>
+  </si>
+  <si>
+    <t>[1, 2, 3, 4, 5, 8, 9, 10, 13, 14, 15, 16, 17, 18, 19, 20, 21, 23, 24, 25, 27, 28, 30, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50, 53, 54, 56, 57, 58, 59, 60, 61, 62, 64, 65, 66, 67, 69, 70, 71, 72, 73, 74, 76, 77, 78, 79, 80, 81, 82, 83, 85, 86, 87, 89, 90, 92, 93, 94, 96, 98, 99, 101, 102, 103, 104, 105, 106, 107, 108, 109, 110, 112, 113, 116, 117, 118, 119, 120, 121, 122, 126, 127, 128, 129, 130, 131, 132, 133, 135, 136, 137, 138, 139, 140, 141, 143, 145, 146, 147, 148, 151, 152, 153, 154, 155, 156, 159, 160, 162, 165, 166, 167, 169, 171, 172, 173, 177, 181, 183, 184, 185, 186, 187, 189, 190, 191, 192, 193, 194, 196, 197, 198, 199]</t>
+  </si>
+  <si>
+    <t>[0, 2, 2, 0, 2, 0, 0, 0, 0, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 0, 0, 0, 0, 2, 2, 2, 2, 2, 0, 0, 2, 0, 0, 2, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 0, 2, 2, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 2, 2, 2, 0, 2, 0, 2, 0, 0, 0, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2]</t>
+  </si>
+  <si>
+    <t>['[-0.03763371 -0.01533471  0.06554052 -0.01816017]', '[-0.03406929  0.01398622 -0.02953871  0.30651903]', '[-0.03493773  0.06836613  0.02265481  0.22789337]', '[-0.02479211  0.10222584  0.07768516  0.10663031]', '[-0.01808581  0.14469195 -0.0104571   0.31140101]', '[-0.01484609  0.18823383  0.0432976   0.11751461]', '[ 0.01194358  0.15658508  0.21806051 -0.4242783 ]', '[ 0.0678951   0.02679956  0.32611908 -0.842647  ]', '[ 0.10833315 -0.09598004  0.06661274 -0.35846568]', '[ 0.09253129 -0.1107569  -0.22143012  0.21004927]', '[ 0.03708618 -0.05169622 -0.31988112  0.36175619]', '[-0.0424962   0.05911995 -0.45609523  0.71434439]', '[-0.13593202  0.218015   -0.45416786  0.83221759]', '[-0.20159779  0.34111104 -0.18676049  0.37078898]', '[-0.20692198  0.35964782  0.13453837 -0.18817803]', '[-0.16316795  0.3031075   0.29261487 -0.36170901]', '[-0.09544353  0.22321674  0.36860886 -0.41365115]', '[-0.02280964  0.1479752   0.34073583 -0.3146744 ]', '[ 0.0343875   0.10619347  0.21847948 -0.0872298 ]', '[0.06071131 0.11719764 0.04002032 0.19907824]', '[ 0.06340743  0.14947491 -0.01266858  0.11874504]', '[ 0.05611954  0.16293569 -0.05833146  0.01250149]', '[ 0.0278894   0.18763465 -0.21726166  0.22540446]', '[-0.0135069   0.21319018 -0.18759951  0.01961953]', '[-0.04394829  0.19276054 -0.11122735 -0.22507727]', '[-0.06982987  0.15882953 -0.14341484 -0.11240385]', '[-0.0728237   0.07927496  0.11153339 -0.66975014]', '[-0.05521114 -0.0299149   0.05754565 -0.40058548]', '[-0.05180276 -0.07457874 -0.02530196 -0.03832665]', '[-0.06502872 -0.04498725 -0.103254    0.32686837]', '[-0.077351    0.01609943 -0.01567102  0.27173056]', '[-0.08356918  0.09393305 -0.04261112  0.49184131]', '[-0.07917379  0.17117229  0.08781687  0.26842389]', '[-0.04923481  0.19869616  0.20605149  0.00714886]', '[-0.01327081  0.21052343  0.14675499  0.11453721]', '[0.00731565 0.24484452 0.05607611 0.22594086]', '[ 0.02178471  0.26479149  0.08597305 -0.0270246 ]', '[ 0.02714725  0.26934659 -0.03318409  0.07249461]', '[ 0.00921004  0.29240876 -0.14174895  0.15123896]', '[-0.01385711  0.29229138 -0.08421935 -0.15588616]', '[-0.03637451  0.26464439 -0.13709124 -0.11966476]', '[-0.06671755  0.24429515 -0.16076438 -0.08514522]', '[-0.09824828  0.22974197 -0.14864543 -0.06266969]', '[-0.1239008   0.21826715 -0.10314425 -0.05385943]', '[-0.13795914  0.20769341 -0.03503467 -0.05203625]', '[-0.13747092  0.19774649  0.0394371  -0.04557123]', '[-0.12293157  0.19056248  0.10277867 -0.0228489 ]', '[-0.0980822   0.19016399  0.1407091   0.02262481]', '[-0.06888396  0.20102437  0.1457621   0.08846102]', '[-0.04194329  0.22614174  0.11903107  0.16245593]', '[-0.02283177  0.26528905  0.06944227  0.22530159]', '[ 0.01123673  0.24657393  0.26347413 -0.40370371]', '[ 0.07750298  0.11206078  0.38214363 -0.90917372]', '[ 0.12909472 -0.03125369  0.11897374 -0.4914324 ]', '[ 0.12181062 -0.07603485 -0.19126166  0.0493746 ]', '[ 0.05578697 -0.01442815 -0.4534121   0.54544558]', '[-0.03747011  0.0945057  -0.45684832  0.51048471]', '[-0.11811135  0.17678774 -0.33100285  0.28646   ]', '[-0.16373325  0.2011036  -0.11565511 -0.05346138]', '[-0.17573045  0.18873704 -0.0024546  -0.06963751]', '[-0.16484146  0.17417288  0.10862484 -0.07181057]', '[-0.13420461  0.16228723  0.19121497 -0.04047292]', '[-0.09155472  0.1608538   0.22670217  0.03269654]', '[-0.02079354  0.109444    0.46474786 -0.52691003]', '[ 0.05894636  0.03164513  0.31420962 -0.22539763]', '[0.09907406 0.0265747  0.07911812 0.18120376]', '[ 0.10295939  0.06841814 -0.03965063  0.23051882]', '[ 0.08441829  0.11511875 -0.14052701  0.22557937]', '[ 0.03640562  0.18788769 -0.32731739  0.4814773 ]', '[-0.02679899  0.26286396 -0.28993901  0.24641437]', '[-0.07420151  0.27950582 -0.17410017 -0.08960531]', '[-0.10674407  0.25974428 -0.14538266 -0.10954247]', '[-0.1302407   0.23540335 -0.08569132 -0.13310225]', '[-0.13995724  0.20730429 -0.01049688 -0.14439362]', '[-0.1346345   0.17952318  0.06171461 -0.12778246]', '[-0.09019943  0.09041715  0.37087232 -0.74134412]', '[-0.02066041 -0.03370116  0.3065757  -0.46765826]', '[ 0.02615083 -0.08613489  0.15072167 -0.04105559]', '[ 0.03698146 -0.04756558 -0.04320639  0.42134236]', '[ 0.02385986  0.04178865 -0.08245774  0.45461069]', '[ 0.00653799  0.12684296 -0.08465038  0.37873804]', '[-0.00767279  0.18698641 -0.05294198  0.21064165]', '[-0.01327928  0.20758608 -0.00153677 -0.00865712]', '[-0.02140441  0.21759261 -0.07766016  0.10557611]', '[-0.04280947  0.24738367 -0.13107986  0.18383771]', '[-0.05816827  0.2531289  -0.01938035 -0.12933901]', '[-0.06357604  0.23094311 -0.03424897 -0.08964586]', '[-0.07153273  0.21808389 -0.04408587 -0.03801734]', '[-0.05427366  0.14765041  0.21115372 -0.65193598]', '[-0.01847478  0.03707675  0.13604384 -0.42908421]', '[-0.00327247 -0.01610618  0.01142529 -0.09158691]', '[ 0.0121596  -0.06662696  0.13795839 -0.40207481]', '[ 0.02215196 -0.10113027 -0.04076409  0.06380943]', '[ 0.00987846 -0.07664404 -0.07868377  0.17487156]', '[-0.0075934  -0.03459204 -0.09117781  0.23568466]', '[-0.03775112  0.04746517 -0.20150804  0.56564428]', '[-0.07016643  0.14692224 -0.11315533  0.4071646 ]', '[-0.0932724   0.23731756 -0.11032123  0.4775992 ]', '[-0.09826713  0.29624744  0.06251134  0.10218325]', '[-0.08207889  0.31132672  0.09647077  0.04866301]', '[-0.03517508  0.24883079  0.36144487 -0.65677069]', '[ 0.02899656  0.1294676   0.26357616 -0.50629552]', '[ 0.06452321  0.05696179  0.0824029  -0.20099883]', '[ 0.06002553  0.05304363 -0.12630908  0.16128913]', '[ 0.02970227  0.08342661 -0.16981286  0.13260758]', '[-0.00476092  0.10207373 -0.16727348  0.04540381]', '[-0.03431527  0.0988121  -0.12243015 -0.08187782]', '[-0.06513964  0.1031136  -0.17935713  0.11922148]', '[-0.08958665  0.10840205 -0.06016666 -0.07066028]', '[-0.10159922  0.10925453 -0.05749006  0.07713063]', '[-0.09822116  0.103271    0.09022448 -0.13512488]', '[-0.05404286  0.0238739   0.33992499 -0.63802702]', '[ 0.00404865 -0.07022621  0.2265018  -0.27817589]', '[ 0.0320937  -0.08061217  0.04820645  0.17984987]', '[ 2.29105013e-02 -4.94118708e-05 -1.35426237e-01  6.10032670e-01]', '[-0.01823691  0.15307822 -0.26225999  0.88731946]', '[-0.06215527  0.3049912  -0.16405666  0.60064235]', '[-0.08000129  0.38372541 -0.00955023  0.17294841]', '[-0.07837717  0.4053228   0.02588131  0.04010659]', '[-0.07000149  0.39958904  0.05597226 -0.09514699]', '[-0.05709209  0.36914554  0.06973676 -0.20249524]', '[-0.04366847  0.32204871  0.06055644 -0.25886547]', '[-0.034446    0.26977615  0.02836089 -0.25388106]', '[-0.00713584  0.15635904  0.2363557  -0.85799892]', '[ 0.05425467 -0.05900447  0.35756435 -1.24773725]', '[ 0.12613514 -0.31967185  0.33692525 -1.30072597]', '[ 0.15480144 -0.49128613 -0.05684633 -0.39095504]', '[ 0.11694132 -0.50597862 -0.31346067  0.23952635]', '[ 0.03489429 -0.40168435 -0.48851808  0.77661859]', '[-0.06922869 -0.21054403 -0.52690027  1.08818452]', '[-0.16456769  0.01188943 -0.40008724  1.0824354 ]', '[-0.2196661   0.20182028 -0.13402142  0.77645084]', '[-0.21404422  0.31028936  0.19158155  0.29226487]', '[-0.15840267  0.35062416  0.35481301  0.11236961]', '[-0.051904    0.29077301  0.68664515 -0.68572917]', '[ 0.07741988  0.16137298  0.5763803  -0.56519   ]', '[ 0.16759269  0.0804711   0.30488191 -0.21583278]', '[ 0.19375515  0.08215674 -0.04801543  0.23581746]', '[ 0.16292299  0.13683954 -0.25233211  0.29676403]', '[ 0.0976433   0.19356885 -0.38547663  0.25045189]', '[ 0.01572324  0.22851292 -0.41591721  0.08006626]', '[-0.06154072  0.21902122 -0.34119416 -0.18526698]', '[-0.12864975  0.18658345 -0.31753707 -0.1434258 ]', '[-0.17057865  0.1257569  -0.09548534 -0.46011631]', '[-0.15317929 -0.02654368  0.26054542 -1.03311292]', '[-0.09986181 -0.20120594  0.25688545 -0.67637558]', '[-0.05600947 -0.28511705  0.17118199 -0.1436908 ]', '[-0.03454964 -0.25462075  0.03952848  0.44743955]', '[-0.02704226 -0.14496404  0.03708392  0.63221009]', '[-0.03197612  0.024247   -0.07949212  1.02908408]', '[-0.05432743  0.25046028 -0.1304706   1.18786767]', '[-0.06569672  0.44734594  0.02317713  0.75009658]', '[-0.04467137  0.54268423  0.18269774  0.19596282]', '[-0.00823232  0.55894661  0.17398146 -0.02884561]', '[ 0.02184133  0.53399689  0.12007357 -0.21206026]', '[ 0.03750983  0.4780961   0.0326462  -0.33685579]', '[ 0.03391176  0.40345177 -0.06912462 -0.3997123 ]', '[ 0.03633022  0.25490171  0.09074976 -1.06494645]', '[ 0.06666369 -0.00807976  0.1968511  -1.51352334]', '[ 0.080356   -0.25689012 -0.07109991 -0.92953613]', '[ 0.03746053 -0.36876573 -0.3500626  -0.18088074]', '[-0.05373307 -0.33185041 -0.54161206  0.52939951]', '[-0.15622901 -0.20421726 -0.45928981  0.70974777]', '[-0.2415178  -0.0293185  -0.37166156  0.99698885]', '[-0.29624189  0.17603065 -0.15775141  1.01268039]', '[-0.28606861  0.32565282  0.26139839  0.46118945]', '[-0.20757297  0.39057695  0.51000983  0.18767701]', '[-0.089807    0.40378232  0.64402527 -0.04044147]', '[ 0.06468229  0.31632894  0.86649825 -0.79620347]', '[ 0.21470232  0.1746412   0.5991511  -0.57114224]', '[ 0.31948048  0.03572675  0.42422233 -0.77892561]', '[ 0.3492289  -0.0525838  -0.13447011 -0.08632361]', '[ 0.28074174 -0.03334565 -0.53624304  0.26512628]', '[ 0.14385924  0.04343391 -0.80267625  0.46798885]', '[-0.03917194  0.17091352 -0.98594237  0.75385398]', '[-0.23218939  0.32103267 -0.9009534   0.69211637]', '[-0.3835145   0.42811845 -0.58108076  0.34413104]', '[-0.44238989  0.41632831  0.00240935 -0.46487757]', '[-0.37012337  0.21354079  0.70258447 -1.52584629]', '[-0.17560566 -0.16669345  1.18968756 -2.17557055]', '[ 0.07926217 -0.60613772  1.29343292 -2.09810836]', '[ 0.29455501 -0.90443715  0.82169704 -0.83900419]', '[ 0.41838608 -0.99066344  0.39296906 -0.00538273]', '[ 0.43387445 -0.87394323 -0.24490454  1.16879845]', '[ 0.32209165 -0.52997261 -0.8521801   2.22808841]', '[ 0.10975275 -0.01573624 -1.20780971  2.78706878]', '[-0.12967999  0.52130681 -1.11606926  2.44235352]', '[-0.31450386  0.91916513 -0.6979683   1.47781317]', '[-0.41104085  1.12897855 -0.25330144  0.60117868]', '[-0.40283141  1.12823174  0.33326064 -0.60740628]', '[-0.29202208  0.9179995   0.75704161 -1.47280548]', '[-0.11083322  0.55491987  1.01696499 -2.0938347 ]', '[ 0.09443011  0.11822221  0.97807847 -2.16025332]', '[ 0.25664041 -0.2616346   0.59760898 -1.54417788]', '[ 0.32043862 -0.47257377  0.02575029 -0.53038873]', '[ 0.26633847 -0.4684581  -0.55514416  0.5638284 ]', '[ 0.12047816 -0.29138039 -0.87058336  1.1601865 ]', '[-0.06520359 -0.03039369 -0.94027604  1.37392829]', '[-0.23628961  0.22547542 -0.72827298  1.11355416]', '[-0.34220783  0.39147017 -0.3071372   0.50846616]']</t>
+  </si>
+  <si>
+    <t>[array([-0.03763371, -0.01533471,  0.06554052, -0.01816017], dtype=float32), array([-0.03406929,  0.01398622, -0.02953871,  0.30651903]), array([-0.03493773,  0.06836613,  0.02265481,  0.22789337]), array([-0.02479211,  0.10222584,  0.07768516,  0.10663031]), array([-0.01808581,  0.14469195, -0.0104571 ,  0.31140101]), array([-0.01484609,  0.18823383,  0.0432976 ,  0.11751461]), array([ 0.01194358,  0.15658508,  0.21806051, -0.4242783 ]), array([ 0.0678951 ,  0.02679956,  0.32611908, -0.842647  ]), array([ 0.10833315, -0.09598004,  0.06661274, -0.35846568]), array([ 0.09253129, -0.1107569 , -0.22143012,  0.21004927]), array([ 0.03708618, -0.05169622, -0.31988112,  0.36175619]), array([-0.0424962 ,  0.05911995, -0.45609523,  0.71434439]), array([-0.13593202,  0.218015  , -0.45416786,  0.83221759]), array([-0.20159779,  0.34111104, -0.18676049,  0.37078898]), array([-0.20692198,  0.35964782,  0.13453837, -0.18817803]), array([-0.16316795,  0.3031075 ,  0.29261487, -0.36170901]), array([-0.09544353,  0.22321674,  0.36860886, -0.41365115]), array([-0.02280964,  0.1479752 ,  0.34073583, -0.3146744 ]), array([ 0.0343875 ,  0.10619347,  0.21847948, -0.0872298 ]), array([0.06071131, 0.11719764, 0.04002032, 0.19907824]), array([ 0.06340743,  0.14947491, -0.01266858,  0.11874504]), array([ 0.05611954,  0.16293569, -0.05833146,  0.01250149]), array([ 0.0278894 ,  0.18763465, -0.21726166,  0.22540446]), array([-0.0135069 ,  0.21319018, -0.18759951,  0.01961953]), array([-0.04394829,  0.19276054, -0.11122735, -0.22507727]), array([-0.06982987,  0.15882953, -0.14341484, -0.11240385]), array([-0.0728237 ,  0.07927496,  0.11153339, -0.66975014]), array([-0.05521114, -0.0299149 ,  0.05754565, -0.40058548]), array([-0.05180276, -0.07457874, -0.02530196, -0.03832665]), array([-0.06502872, -0.04498725, -0.103254  ,  0.32686837]), array([-0.077351  ,  0.01609943, -0.01567102,  0.27173056]), array([-0.08356918,  0.09393305, -0.04261112,  0.49184131]), array([-0.07917379,  0.17117229,  0.08781687,  0.26842389]), array([-0.04923481,  0.19869616,  0.20605149,  0.00714886]), array([-0.01327081,  0.21052343,  0.14675499,  0.11453721]), array([0.00731565, 0.24484452, 0.05607611, 0.22594086]), array([ 0.02178471,  0.26479149,  0.08597305, -0.0270246 ]), array([ 0.02714725,  0.26934659, -0.03318409,  0.07249461]), array([ 0.00921004,  0.29240876, -0.14174895,  0.15123896]), array([-0.01385711,  0.29229138, -0.08421935, -0.15588616]), array([-0.03637451,  0.26464439, -0.13709124, -0.11966476]), array([-0.06671755,  0.24429515, -0.16076438, -0.08514522]), array([-0.09824828,  0.22974197, -0.14864543, -0.06266969]), array([-0.1239008 ,  0.21826715, -0.10314425, -0.05385943]), array([-0.13795914,  0.20769341, -0.03503467, -0.05203625]), array([-0.13747092,  0.19774649,  0.0394371 , -0.04557123]), array([-0.12293157,  0.19056248,  0.10277867, -0.0228489 ]), array([-0.0980822 ,  0.19016399,  0.1407091 ,  0.02262481]), array([-0.06888396,  0.20102437,  0.1457621 ,  0.08846102]), array([-0.04194329,  0.22614174,  0.11903107,  0.16245593]), array([-0.02283177,  0.26528905,  0.06944227,  0.22530159]), array([ 0.01123673,  0.24657393,  0.26347413, -0.40370371]), array([ 0.07750298,  0.11206078,  0.38214363, -0.90917372]), array([ 0.12909472, -0.03125369,  0.11897374, -0.4914324 ]), array([ 0.12181062, -0.07603485, -0.19126166,  0.0493746 ]), array([ 0.05578697, -0.01442815, -0.4534121 ,  0.54544558]), array([-0.03747011,  0.0945057 , -0.45684832,  0.51048471]), array([-0.11811135,  0.17678774, -0.33100285,  0.28646   ]), array([-0.16373325,  0.2011036 , -0.11565511, -0.05346138]), array([-0.17573045,  0.18873704, -0.0024546 , -0.06963751]), array([-0.16484146,  0.17417288,  0.10862484, -0.07181057]), array([-0.13420461,  0.16228723,  0.19121497, -0.04047292]), array([-0.09155472,  0.1608538 ,  0.22670217,  0.03269654]), array([-0.02079354,  0.109444  ,  0.46474786, -0.52691003]), array([ 0.05894636,  0.03164513,  0.31420962, -0.22539763]), array([0.09907406, 0.0265747 , 0.07911812, 0.18120376]), array([ 0.10295939,  0.06841814, -0.03965063,  0.23051882]), array([ 0.08441829,  0.11511875, -0.14052701,  0.22557937]), array([ 0.03640562,  0.18788769, -0.32731739,  0.4814773 ]), array([-0.02679899,  0.26286396, -0.28993901,  0.24641437]), array([-0.07420151,  0.27950582, -0.17410017, -0.08960531]), array([-0.10674407,  0.25974428, -0.14538266, -0.10954247]), array([-0.1302407 ,  0.23540335, -0.08569132, -0.13310225]), array([-0.13995724,  0.20730429, -0.01049688, -0.14439362]), array([-0.1346345 ,  0.17952318,  0.06171461, -0.12778246]), array([-0.09019943,  0.09041715,  0.37087232, -0.74134412]), array([-0.02066041, -0.03370116,  0.3065757 , -0.46765826]), array([ 0.02615083, -0.08613489,  0.15072167, -0.04105559]), array([ 0.03698146, -0.04756558, -0.04320639,  0.42134236]), array([ 0.02385986,  0.04178865, -0.08245774,  0.45461069]), array([ 0.00653799,  0.12684296, -0.08465038,  0.37873804]), array([-0.00767279,  0.18698641, -0.05294198,  0.21064165]), array([-0.01327928,  0.20758608, -0.00153677, -0.00865712]), array([-0.02140441,  0.21759261, -0.07766016,  0.10557611]), array([-0.04280947,  0.24738367, -0.13107986,  0.18383771]), array([-0.05816827,  0.2531289 , -0.01938035, -0.12933901]), array([-0.06357604,  0.23094311, -0.03424897, -0.08964586]), array([-0.07153273,  0.21808389, -0.04408587, -0.03801734]), array([-0.05427366,  0.14765041,  0.21115372, -0.65193598]), array([-0.01847478,  0.03707675,  0.13604384, -0.42908421]), array([-0.00327247, -0.01610618,  0.01142529, -0.09158691]), array([ 0.0121596 , -0.06662696,  0.13795839, -0.40207481]), array([ 0.02215196, -0.10113027, -0.04076409,  0.06380943]), array([ 0.00987846, -0.07664404, -0.07868377,  0.17487156]), array([-0.0075934 , -0.03459204, -0.09117781,  0.23568466]), array([-0.03775112,  0.04746517, -0.20150804,  0.56564428]), array([-0.07016643,  0.14692224, -0.11315533,  0.4071646 ]), array([-0.0932724 ,  0.23731756, -0.11032123,  0.4775992 ]), array([-0.09826713,  0.29624744,  0.06251134,  0.10218325]), array([-0.08207889,  0.31132672,  0.09647077,  0.04866301]), array([-0.03517508,  0.24883079,  0.36144487, -0.65677069]), array([ 0.02899656,  0.1294676 ,  0.26357616, -0.50629552]), array([ 0.06452321,  0.05696179,  0.0824029 , -0.20099883]), array([ 0.06002553,  0.05304363, -0.12630908,  0.16128913]), array([ 0.02970227,  0.08342661, -0.16981286,  0.13260758]), array([-0.00476092,  0.10207373, -0.16727348,  0.04540381]), array([-0.03431527,  0.0988121 , -0.12243015, -0.08187782]), array([-0.06513964,  0.1031136 , -0.17935713,  0.11922148]), array([-0.08958665,  0.10840205, -0.06016666, -0.07066028]), array([-0.10159922,  0.10925453, -0.05749006,  0.07713063]), array([-0.09822116,  0.103271  ,  0.09022448, -0.13512488]), array([-0.05404286,  0.0238739 ,  0.33992499, -0.63802702]), array([ 0.00404865, -0.07022621,  0.2265018 , -0.27817589]), array([ 0.0320937 , -0.08061217,  0.04820645,  0.17984987]), array([ 2.29105013e-02, -4.94118708e-05, -1.35426237e-01,  6.10032670e-01]), array([-0.01823691,  0.15307822, -0.26225999,  0.88731946]), array([-0.06215527,  0.3049912 , -0.16405666,  0.60064235]), array([-0.08000129,  0.38372541, -0.00955023,  0.17294841]), array([-0.07837717,  0.4053228 ,  0.02588131,  0.04010659]), array([-0.07000149,  0.39958904,  0.05597226, -0.09514699]), array([-0.05709209,  0.36914554,  0.06973676, -0.20249524]), array([-0.04366847,  0.32204871,  0.06055644, -0.25886547]), array([-0.034446  ,  0.26977615,  0.02836089, -0.25388106]), array([-0.00713584,  0.15635904,  0.2363557 , -0.85799892]), array([ 0.05425467, -0.05900447,  0.35756435, -1.24773725]), array([ 0.12613514, -0.31967185,  0.33692525, -1.30072597]), array([ 0.15480144, -0.49128613, -0.05684633, -0.39095504]), array([ 0.11694132, -0.50597862, -0.31346067,  0.23952635]), array([ 0.03489429, -0.40168435, -0.48851808,  0.77661859]), array([-0.06922869, -0.21054403, -0.52690027,  1.08818452]), array([-0.16456769,  0.01188943, -0.40008724,  1.0824354 ]), array([-0.2196661 ,  0.20182028, -0.13402142,  0.77645084]), array([-0.21404422,  0.31028936,  0.19158155,  0.29226487]), array([-0.15840267,  0.35062416,  0.35481301,  0.11236961]), array([-0.051904  ,  0.29077301,  0.68664515, -0.68572917]), array([ 0.07741988,  0.16137298,  0.5763803 , -0.56519   ]), array([ 0.16759269,  0.0804711 ,  0.30488191, -0.21583278]), array([ 0.19375515,  0.08215674, -0.04801543,  0.23581746]), array([ 0.16292299,  0.13683954, -0.25233211,  0.29676403]), array([ 0.0976433 ,  0.19356885, -0.38547663,  0.25045189]), array([ 0.01572324,  0.22851292, -0.41591721,  0.08006626]), array([-0.06154072,  0.21902122, -0.34119416, -0.18526698]), array([-0.12864975,  0.18658345, -0.31753707, -0.1434258 ]), array([-0.17057865,  0.1257569 , -0.09548534, -0.46011631]), array([-0.15317929, -0.02654368,  0.26054542, -1.03311292]), array([-0.09986181, -0.20120594,  0.25688545, -0.67637558]), array([-0.05600947, -0.28511705,  0.17118199, -0.1436908 ]), array([-0.03454964, -0.25462075,  0.03952848,  0.44743955]), array([-0.02704226, -0.14496404,  0.03708392,  0.63221009]), array([-0.03197612,  0.024247  , -0.07949212,  1.02908408]), array([-0.05432743,  0.25046028, -0.1304706 ,  1.18786767]), array([-0.06569672,  0.44734594,  0.02317713,  0.75009658]), array([-0.04467137,  0.54268423,  0.18269774,  0.19596282]), array([-0.00823232,  0.55894661,  0.17398146, -0.02884561]), array([ 0.02184133,  0.53399689,  0.12007357, -0.21206026]), array([ 0.03750983,  0.4780961 ,  0.0326462 , -0.33685579]), array([ 0.03391176,  0.40345177, -0.06912462, -0.3997123 ]), array([ 0.03633022,  0.25490171,  0.09074976, -1.06494645]), array([ 0.06666369, -0.00807976,  0.1968511 , -1.51352334]), array([ 0.080356  , -0.25689012, -0.07109991, -0.92953613]), array([ 0.03746053, -0.36876573, -0.3500626 , -0.18088074]), array([-0.05373307, -0.33185041, -0.54161206,  0.52939951]), array([-0.15622901, -0.20421726, -0.45928981,  0.70974777]), array([-0.2415178 , -0.0293185 , -0.37166156,  0.99698885]), array([-0.29624189,  0.17603065, -0.15775141,  1.01268039]), array([-0.28606861,  0.32565282,  0.26139839,  0.46118945]), array([-0.20757297,  0.39057695,  0.51000983,  0.18767701]), array([-0.089807  ,  0.40378232,  0.64402527, -0.04044147]), array([ 0.06468229,  0.31632894,  0.86649825, -0.79620347]), array([ 0.21470232,  0.1746412 ,  0.5991511 , -0.57114224]), array([ 0.31948048,  0.03572675,  0.42422233, -0.77892561]), array([ 0.3492289 , -0.0525838 , -0.13447011, -0.08632361]), array([ 0.28074174, -0.03334565, -0.53624304,  0.26512628]), array([ 0.14385924,  0.04343391, -0.80267625,  0.46798885]), array([-0.03917194,  0.17091352, -0.98594237,  0.75385398]), array([-0.23218939,  0.32103267, -0.9009534 ,  0.69211637]), array([-0.3835145 ,  0.42811845, -0.58108076,  0.34413104]), array([-0.44238989,  0.41632831,  0.00240935, -0.46487757]), array([-0.37012337,  0.21354079,  0.70258447, -1.52584629]), array([-0.17560566, -0.16669345,  1.18968756, -2.17557055]), array([ 0.07926217, -0.60613772,  1.29343292, -2.09810836]), array([ 0.29455501, -0.90443715,  0.82169704, -0.83900419]), array([ 0.41838608, -0.99066344,  0.39296906, -0.00538273]), array([ 0.43387445, -0.87394323, -0.24490454,  1.16879845]), array([ 0.32209165, -0.52997261, -0.8521801 ,  2.22808841]), array([ 0.10975275, -0.01573624, -1.20780971,  2.78706878]), array([-0.12967999,  0.52130681, -1.11606926,  2.44235352]), array([-0.31450386,  0.91916513, -0.6979683 ,  1.47781317]), array([-0.41104085,  1.12897855, -0.25330144,  0.60117868]), array([-0.40283141,  1.12823174,  0.33326064, -0.60740628]), array([-0.29202208,  0.9179995 ,  0.75704161, -1.47280548]), array([-0.11083322,  0.55491987,  1.01696499, -2.0938347 ]), array([ 0.09443011,  0.11822221,  0.97807847, -2.16025332]), array([ 0.25664041, -0.2616346 ,  0.59760898, -1.54417788]), array([ 0.32043862, -0.47257377,  0.02575029, -0.53038873]), array([ 0.26633847, -0.4684581 , -0.55514416,  0.5638284 ]), array([ 0.12047816, -0.29138039, -0.87058336,  1.1601865 ]), array([-0.06520359, -0.03039369, -0.94027604,  1.37392829]), array([-0.23628961,  0.22547542, -0.72827298,  1.11355416]), array([-0.34220783,  0.39147017, -0.3071372 ,  0.50846616])]</t>
+  </si>
+  <si>
+    <t>['[1,1,1]', '[1,1,2]', '[2,2,2]', '[0,1,1]', '[2,1,0]', '[1,0,2]', '[0,0,0]', '[0,2,1]', '[1,2,0]', '[2,0,1]']</t>
+  </si>
+  <si>
+    <t>[0, 2, 2, 0, 2, 0, 2, 0, 0, 2, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 2, 0, 0, 0, 2, 0, 0, 0, 2, 0, 0, 0, 0, 2, 0, 0, 0, 2, 0, 0, 2, 0, 0, 2, 0, 0, 2, 0, 0, 2, 0, 0, 2, 0, 0, 2, 0, 0, 0, 2, 0, 0, 0, 0, 2, 0, 0, 0, 2, 0, 0, 2, 0, 0, 2, 0, 0, 2, 0, 0, 0, 2, 0, 0, 0, 2, 0, 0, 0, 2, 0, 0, 0, 2, 0, 0, 0, 2, 0, 0, 2, 0, 0, 2, 0, 0, 2, 0, 0, 0, 2, 0, 0, 0, 2, 0, 0, 0, 2, 0, 0, 0, 2, 0, 0, 0, 0, 2, 0, 0, 0, 0, 2, 0, 0, 0, 2, 0, 0, 0, 2, 0, 0, 0, 0, 2, 0, 0, 0, 0, 2, 0, 0, 0, 2, 0, 0, 0, 2, 0, 0, 0, 2, 0, 0, 0, 2, 0, 0, 0, 2, 0, 0, 0, 2, 0, 0, 0, 2, 0, 0, 0, 2, 0]</t>
+  </si>
+  <si>
+    <t>['[-0.03763371 -0.01533471  0.06554052 -0.01816017]', '[-0.03406929  0.01398622 -0.02953871  0.30651903]', '[-0.03493773  0.06836613  0.02265481  0.22789337]', '[-0.02479211  0.10222584  0.07768516  0.10663031]', '[-0.01808581  0.14469195 -0.0104571   0.31140101]', '[-0.01484609  0.18823383  0.0432976   0.11751461]', '[-0.01434726  0.22467153 -0.03717771  0.24054013]', '[-0.01545278  0.24682047  0.02676029 -0.02247913]', '[-0.01721181  0.25018444 -0.04380907  0.05514087]', '[-0.03213003  0.26757856 -0.10176092  0.11343711]', '[-0.04292178  0.2589368  -0.00427078 -0.19989973]', '[-0.04724582  0.22400641 -0.03910061 -0.1442553 ]', '[-0.05828925  0.20274667 -0.06971448 -0.06649573]', '[-0.07416359  0.19747218 -0.0859609   0.01216736]', '[-0.0912366   0.20638244 -0.08104733  0.07279687]', '[-0.10506889  0.22457911 -0.0539522   0.10400424]', '[-0.11166695  0.24587804 -0.010094    0.10444057]', '[-0.10867284  0.26478582  0.03995039  0.08196904]', '[-0.09613136  0.27802333  0.08328201  0.05013698]', '[-0.07660094  0.2851802   0.10825155  0.02324806]', '[-0.0545593   0.2883646   0.10777726  0.01147603]', '[-0.03525161  0.29099778  0.08146314  0.01741678]', '[-0.02329543  0.29616619  0.03584343  0.03525702]', '[-0.0214414   0.30511627 -0.01738635  0.05301171]', '[-0.02985137  0.31645556 -0.06464183  0.05714453]', '[-0.04610073  0.32638407 -0.09423766  0.03793816]', '[-0.06589513  0.32991089 -0.09957126 -0.0063193 ]', '[-0.08428464  0.32265766 -0.08080209 -0.06781655]', '[-0.09702234  0.30264881 -0.04459147 -0.13085587]', '[-0.10168093  0.27149627 -0.00200248 -0.17612255]', '[-0.09820986  0.23455768  0.03486443 -0.1864638 ]', '[-0.0887719   0.19991036  0.05652747 -0.1526692 ]', '[-0.076919    0.17632476  0.05888771 -0.07738584]', '[-0.06638826  0.1707868   0.04416262  0.02447002]', '[-0.05992123  0.18633723  0.01974774  0.1292307 ]', '[-0.0584844   0.22093296 -0.00454223  0.21092628]', '[-0.04805938  0.23384537  0.10680343 -0.08193806]', '[-0.03080471  0.22450229  0.06202129 -0.00733249]', '[-0.02430606  0.23182975  0.00194388  0.08025297]', '[-0.02987406  0.25554917 -0.05571698  0.1519643 ]', '[-0.03226718  0.25603978  0.03214881 -0.14722185]', '[-0.03092284  0.23283646 -0.01960446 -0.08080664]', '[-0.03999585  0.22459335 -0.06946922 -0.00175473]', '[-0.05757792  0.23128942 -0.10254152  0.0647801 ]', '[-0.06605782  0.21440088  0.01888208 -0.23192227]', '[-0.06398042  0.17583314  0.00028999 -0.14688162]', '[-0.06633966  0.15773225 -0.02393686 -0.03146107]', '[-0.07325426  0.16341223 -0.04358916  0.08612216]', '[-0.0828409   0.19044139 -0.04946038  0.17797922]', '[-0.07864045  0.19750911  0.09060325 -0.10746977]', '[-0.06146966  0.1840293   0.07725441 -0.02247667]', '[-0.04907293  0.18981812  0.04445008  0.08115296]', '[-0.0442206   0.21593689  0.00396872  0.17619258]', '[-0.0340252   0.22400041  0.09594658 -0.09498212]', '[-0.02075128  0.2143682   0.03388699  0.00222931]', '[-0.02104003  0.22532354 -0.03629256  0.10526593]', '[-0.02132272  0.22066204  0.03329065 -0.15093594]', '[-0.02172504  0.20133409 -0.03773268 -0.03927642]', '[-0.03590812  0.20503959 -0.10102303  0.07333768]', '[-0.04715656  0.19439332 -0.00957467 -0.17953506]', '[-0.0531357   0.16954638 -0.04973417 -0.06569152]', '[-0.06641635  0.16843644 -0.08037468  0.05264093]', '[-0.07065933  0.15478558  0.03826249 -0.18722535]', '[-0.06537071  0.13069535  0.01283817 -0.04881322]', '[-0.06587487  0.13613518 -0.01753718  0.10204491]', '[-0.05864396  0.1357341   0.08821968 -0.10462186]', '[-0.04548709  0.13096902  0.0406286   0.05963551]', '[-0.04291628  0.15928652 -0.01443372  0.21883176]', '[-0.03731008  0.18120939  0.06982108 -0.00211053]', '[-0.02929538  0.19339059  0.00917428  0.12290951]', '[-0.03349002  0.22880302 -0.04909788  0.22438117]', '[-0.03450974  0.2455827   0.03936722 -0.05911149]', '[-0.03159904  0.24030656 -0.01094568  0.00758765]', '[-0.03869893  0.24839084 -0.05831173  0.07068777]', '[-0.05379571  0.26688344 -0.08901105  0.10873581]', '[-0.05952816  0.25548823  0.03243166 -0.22145423]', '[-0.05489462  0.21545832  0.01177921 -0.17140764]', '[-0.05545332  0.18946482 -0.01801811 -0.08425214]', '[-0.06203264  0.18272624 -0.04661029  0.01691807]', '[-0.07329597  0.19542728 -0.06331667  0.10611252]', '[-0.07291285  0.18890039  0.06671518 -0.16992223]', '[-0.06124858  0.1646186   0.04684919 -0.0670246 ]', '[-0.05512685  0.16363989  0.01316512  0.05821198]', '[-0.0560562   0.1872715  -0.0214586   0.17375768]', '[-0.04978711  0.19645649  0.08295617 -0.08215295]', '[-0.03756886  0.19056932  0.0366416   0.02604427]', '[-0.03567973  0.20700006 -0.01754356  0.13560046]', '[-0.03085252  0.20876406  0.06473776 -0.11723264]', '[-0.02424847  0.196482   -0.00032713 -0.00261782]', '[-0.03100005  0.20777645 -0.06538222  0.11242368]', '[-0.0359292   0.20511167  0.0169028  -0.1391461 ]', '[-0.03796388  0.18818858 -0.03728875 -0.02764034]', '[-0.05031463  0.19399173 -0.08347089  0.08264107]', '[-0.05662994  0.18503831  0.02121658 -0.17138809]', '[-0.0557285   0.1620654  -0.01305608 -0.05435543]', '[-0.06179154  0.1639193  -0.04623193  0.07152106]', '[-0.07328392  0.18910806 -0.06553354  0.17417505]', '[-0.07335166  0.19634492  0.06487831 -0.10266275]', '[-0.06177017  0.18423969  0.04825838 -0.01462708]', '[-0.05488602  0.19131999  0.01946897  0.08515879]', '[-0.05409083  0.21737568 -0.01081564  0.17096106]', '[-0.0455179   0.22329134  0.09477424 -0.11112369]', '[-0.03110464  0.20954516  0.04608388 -0.02188119]', '[-0.02791325  0.21545438 -0.01455441  0.08032165]', '[-0.03649726  0.24040015 -0.06871848  0.16345142]', '[-0.04080527  0.24387915  0.02645818 -0.12958454]', '[-0.0397104   0.22448553 -0.01626015 -0.06100079]', '[-0.04720324  0.22012961 -0.05722677  0.01691987]', '[-0.06162359  0.23030853 -0.08370973  0.08084752]', '[-0.06600717  0.2163849   0.04024637 -0.2181857 ]', '[-0.05979725  0.1804201   0.01950769 -0.13441852]', '[-0.05888347  0.16476469 -0.01099665 -0.01940731]', '[-0.06407603  0.17281273 -0.0395712   0.09758891]', '[-0.06065386  0.1678865   0.07280166 -0.14522098]', '[-0.04966623  0.15169303  0.03440973 -0.01236959]', '[-0.04750035  0.16357179 -0.01272862  0.12927392]', '[-0.04105973  0.16737522  0.07579271 -0.09062643]', '[-0.03181692  0.16358967  0.01474012  0.05467468]', '[-0.03527926  0.18869417 -0.04777651  0.19133535]', '[-0.0365353   0.20287936  0.03571079 -0.051725  ]', '[-0.03483137  0.20313934 -0.01893185  0.05440579]', '[-0.0436698   0.22366711 -0.06696449  0.145884  ]', '[-0.04706184  0.22473147  0.03361301 -0.13563625]', '[-0.04418538  0.20557604 -0.00596334 -0.05231351]', '[-0.04949228  0.20447588 -0.04600717  0.04057067]', '[-0.06173633  0.2206755  -0.07341547  0.116697  ]', '[-0.06425486  0.2146904   0.0484192  -0.17563926]', '[-0.05668024  0.18734092  0.02498423 -0.0920928 ]', '[-0.05491882  0.17947298 -0.00791746  0.01492437]', '[-0.0596878   0.19302134 -0.03832988  0.11739016]', '[-0.05619001  0.19031439  0.07236123 -0.14318035]', '[-0.0454138   0.17261945  0.03273101 -0.02919417]', '[-0.04372408  0.17948352 -0.01588161  0.09676409]', '[-0.05126569  0.20979208 -0.05699667  0.19983639]', '[-0.05198527  0.22200654  0.0500947  -0.07945891]', '[-0.04533753  0.21363571  0.01483222 -0.0018944 ]', '[-0.0463109   0.22148048 -0.02407281  0.0787548 ]', '[-0.05438047  0.24375967 -0.05427245  0.13894306]', '[-0.05372026  0.2406193   0.06049358 -0.16942006]', '[-0.04463697  0.21288262  0.02770161 -0.10192129]', '[-0.04336373  0.20163234 -0.0155124  -0.00857866]', '[-0.05061889  0.2093934  -0.05527231  0.08363345]', '[-0.06435839  0.23324163 -0.07857756  0.14861028]', '[-0.06730651  0.23192304  0.04948398 -0.16168937]', '[-0.05883162  0.20524499  0.03276134 -0.09931012]', '[-0.05500133  0.19400643  0.00446478 -0.01065727]', '[-0.05715497  0.20120397 -0.02529162  0.08096931]', '[-0.0645019   0.22496316 -0.04592316  0.15136883]', '[-0.06130255  0.22518156  0.0770882  -0.14839335]', '[-0.04837349  0.20248298  0.04893301 -0.07281919]', '[-0.04273031  0.19770393  0.00627284  0.02659696]', '[-0.04591053  0.21285164 -0.03689892  0.12168229]', '[-0.04347258  0.21028651  0.06056486 -0.1462549 ]', '[-0.03614087  0.1910518   0.01074203 -0.04179718]', '[-0.03947321  0.19431122 -0.04321122  0.07317264]', '[-0.05253773  0.21877441 -0.08397342  0.16515061]', '[-0.05817197  0.2231173   0.02872709 -0.12296549]', '[-0.05489845  0.20552316  0.00284485 -0.04955296]', '[-0.05721498  0.20403602 -0.02554212  0.03448932]', '[-0.0646143   0.21853204 -0.04647194  0.10678867]', '[-0.07477389  0.24469845 -0.05226096  0.14885243]', '[-0.07122742  0.24152634  0.086726   -0.17916281]', '[-0.05498818  0.21037193  0.07145947 -0.12465497]', '[-0.04414385  0.19431106  0.03434931 -0.03164432]', '[-0.04190616  0.19861129 -0.01222167  0.07412546]', '[-0.04865249  0.22279494 -0.05307019  0.16243211]', '[-0.04876946  0.22677321  0.05186349 -0.1229961 ]', '[-0.04213859  0.20981456  0.01263879 -0.04278132]', '[-0.04404101  0.21043339 -0.03119619  0.04845499]', '[-0.05398993  0.22814664 -0.065687    0.12403651]', '[-0.05583566  0.22360832  0.04732925 -0.16865855]', '[-0.04932204  0.19746509  0.015729   -0.08739938]', '[-0.05003684  0.19008374 -0.02290332  0.0146265 ]', '[-0.05807878  0.20284165 -0.0554402   0.10942639]', '[-0.05790075  0.19766104  0.05688596 -0.16005493]', '[-0.04976802  0.17569977  0.0221649  -0.05464645]', '[-0.0495524   0.17686995 -0.01994654  0.06604468]', '[-0.05725766  0.20096191 -0.05473457  0.16943631]', '[-0.0570025   0.20764109  0.05724175 -0.10337722]', '[-0.0486632   0.19569477  0.02414707 -0.01286173]', '[-0.04778381  0.20299982 -0.0152429   0.08468107]', '[-0.0543024   0.22821443 -0.04779902  0.16207112]', '[-0.05263416  0.23110656  0.0640425  -0.13303324]', '[-0.04313379  0.21149034  0.02848912 -0.05842022]', '[-0.04186596  0.2089284  -0.01608281  0.03331756]', '[-0.04922772  0.22416994 -0.05552064  0.11526221]', '[-0.04977785  0.21882787  0.04984121 -0.16760659]', '[-0.04360366  0.19394719  0.00993861 -0.07610417]', '[-0.0461728   0.18959435 -0.03517878  0.03279826]', '[-0.05702251  0.20618426 -0.07055258  0.12848178]', '[-0.05979159  0.20435551  0.04321498 -0.14658365]', '[-0.05391177  0.18405248  0.01380909 -0.05215954]', '[-0.05463957  0.18441447 -0.02087051  0.05548924]', '[-0.06178226  0.20522765 -0.04841424  0.14787871]', '[-0.05972167  0.20694652  0.06847341 -0.13033408]', '[-0.04894413  0.18968478  0.03663804 -0.03777247]', '[-0.0457767   0.19284761 -0.00543932  0.06921977]', '[-0.05086272  0.21635844 -0.04360406  0.16097351]', '[-0.04900321  0.22054227  0.06176369 -0.1192147 ]', '[-0.04055416  0.20498766  0.02059695 -0.03248258]']</t>
+  </si>
+  <si>
+    <t>[array([-0.03763371, -0.01533471,  0.06554052, -0.01816017], dtype=float32), array([-0.03406929,  0.01398622, -0.02953871,  0.30651903]), array([-0.03493773,  0.06836613,  0.02265481,  0.22789337]), array([-0.02479211,  0.10222584,  0.07768516,  0.10663031]), array([-0.01808581,  0.14469195, -0.0104571 ,  0.31140101]), array([-0.01484609,  0.18823383,  0.0432976 ,  0.11751461]), array([-0.01434726,  0.22467153, -0.03717771,  0.24054013]), array([-0.01545278,  0.24682047,  0.02676029, -0.02247913]), array([-0.01721181,  0.25018444, -0.04380907,  0.05514087]), array([-0.03213003,  0.26757856, -0.10176092,  0.11343711]), array([-0.04292178,  0.2589368 , -0.00427078, -0.19989973]), array([-0.04724582,  0.22400641, -0.03910061, -0.1442553 ]), array([-0.05828925,  0.20274667, -0.06971448, -0.06649573]), array([-0.07416359,  0.19747218, -0.0859609 ,  0.01216736]), array([-0.0912366 ,  0.20638244, -0.08104733,  0.07279687]), array([-0.10506889,  0.22457911, -0.0539522 ,  0.10400424]), array([-0.11166695,  0.24587804, -0.010094  ,  0.10444057]), array([-0.10867284,  0.26478582,  0.03995039,  0.08196904]), array([-0.09613136,  0.27802333,  0.08328201,  0.05013698]), array([-0.07660094,  0.2851802 ,  0.10825155,  0.02324806]), array([-0.0545593 ,  0.2883646 ,  0.10777726,  0.01147603]), array([-0.03525161,  0.29099778,  0.08146314,  0.01741678]), array([-0.02329543,  0.29616619,  0.03584343,  0.03525702]), array([-0.0214414 ,  0.30511627, -0.01738635,  0.05301171]), array([-0.02985137,  0.31645556, -0.06464183,  0.05714453]), array([-0.04610073,  0.32638407, -0.09423766,  0.03793816]), array([-0.06589513,  0.32991089, -0.09957126, -0.0063193 ]), array([-0.08428464,  0.32265766, -0.08080209, -0.06781655]), array([-0.09702234,  0.30264881, -0.04459147, -0.13085587]), array([-0.10168093,  0.27149627, -0.00200248, -0.17612255]), array([-0.09820986,  0.23455768,  0.03486443, -0.1864638 ]), array([-0.0887719 ,  0.19991036,  0.05652747, -0.1526692 ]), array([-0.076919  ,  0.17632476,  0.05888771, -0.07738584]), array([-0.06638826,  0.1707868 ,  0.04416262,  0.02447002]), array([-0.05992123,  0.18633723,  0.01974774,  0.1292307 ]), array([-0.0584844 ,  0.22093296, -0.00454223,  0.21092628]), array([-0.04805938,  0.23384537,  0.10680343, -0.08193806]), array([-0.03080471,  0.22450229,  0.06202129, -0.00733249]), array([-0.02430606,  0.23182975,  0.00194388,  0.08025297]), array([-0.02987406,  0.25554917, -0.05571698,  0.1519643 ]), array([-0.03226718,  0.25603978,  0.03214881, -0.14722185]), array([-0.03092284,  0.23283646, -0.01960446, -0.08080664]), array([-0.03999585,  0.22459335, -0.06946922, -0.00175473]), array([-0.05757792,  0.23128942, -0.10254152,  0.0647801 ]), array([-0.06605782,  0.21440088,  0.01888208, -0.23192227]), array([-0.06398042,  0.17583314,  0.00028999, -0.14688162]), array([-0.06633966,  0.15773225, -0.02393686, -0.03146107]), array([-0.07325426,  0.16341223, -0.04358916,  0.08612216]), array([-0.0828409 ,  0.19044139, -0.04946038,  0.17797922]), array([-0.07864045,  0.19750911,  0.09060325, -0.10746977]), array([-0.06146966,  0.1840293 ,  0.07725441, -0.02247667]), array([-0.04907293,  0.18981812,  0.04445008,  0.08115296]), array([-0.0442206 ,  0.21593689,  0.00396872,  0.17619258]), array([-0.0340252 ,  0.22400041,  0.09594658, -0.09498212]), array([-0.02075128,  0.2143682 ,  0.03388699,  0.00222931]), array([-0.02104003,  0.22532354, -0.03629256,  0.10526593]), array([-0.02132272,  0.22066204,  0.03329065, -0.15093594]), array([-0.02172504,  0.20133409, -0.03773268, -0.03927642]), array([-0.03590812,  0.20503959, -0.10102303,  0.07333768]), array([-0.04715656,  0.19439332, -0.00957467, -0.17953506]), array([-0.0531357 ,  0.16954638, -0.04973417, -0.06569152]), array([-0.06641635,  0.16843644, -0.08037468,  0.05264093]), array([-0.07065933,  0.15478558,  0.03826249, -0.18722535]), array([-0.06537071,  0.13069535,  0.01283817, -0.04881322]), array([-0.06587487,  0.13613518, -0.01753718,  0.10204491]), array([-0.05864396,  0.1357341 ,  0.08821968, -0.10462186]), array([-0.04548709,  0.13096902,  0.0406286 ,  0.05963551]), array([-0.04291628,  0.15928652, -0.01443372,  0.21883176]), array([-0.03731008,  0.18120939,  0.06982108, -0.00211053]), array([-0.02929538,  0.19339059,  0.00917428,  0.12290951]), array([-0.03349002,  0.22880302, -0.04909788,  0.22438117]), array([-0.03450974,  0.2455827 ,  0.03936722, -0.05911149]), array([-0.03159904,  0.24030656, -0.01094568,  0.00758765]), array([-0.03869893,  0.24839084, -0.05831173,  0.07068777]), array([-0.05379571,  0.26688344, -0.08901105,  0.10873581]), array([-0.05952816,  0.25548823,  0.03243166, -0.22145423]), array([-0.05489462,  0.21545832,  0.01177921, -0.17140764]), array([-0.05545332,  0.18946482, -0.01801811, -0.08425214]), array([-0.06203264,  0.18272624, -0.04661029,  0.01691807]), array([-0.07329597,  0.19542728, -0.06331667,  0.10611252]), array([-0.07291285,  0.18890039,  0.06671518, -0.16992223]), array([-0.06124858,  0.1646186 ,  0.04684919, -0.0670246 ]), array([-0.05512685,  0.16363989,  0.01316512,  0.05821198]), array([-0.0560562 ,  0.1872715 , -0.0214586 ,  0.17375768]), array([-0.04978711,  0.19645649,  0.08295617, -0.08215295]), array([-0.03756886,  0.19056932,  0.0366416 ,  0.02604427]), array([-0.03567973,  0.20700006, -0.01754356,  0.13560046]), array([-0.03085252,  0.20876406,  0.06473776, -0.11723264]), array([-0.02424847,  0.196482  , -0.00032713, -0.00261782]), array([-0.03100005,  0.20777645, -0.06538222,  0.11242368]), array([-0.0359292 ,  0.20511167,  0.0169028 , -0.1391461 ]), array([-0.03796388,  0.18818858, -0.03728875, -0.02764034]), array([-0.05031463,  0.19399173, -0.08347089,  0.08264107]), array([-0.05662994,  0.18503831,  0.02121658, -0.17138809]), array([-0.0557285 ,  0.1620654 , -0.01305608, -0.05435543]), array([-0.06179154,  0.1639193 , -0.04623193,  0.07152106]), array([-0.07328392,  0.18910806, -0.06553354,  0.17417505]), array([-0.07335166,  0.19634492,  0.06487831, -0.10266275]), array([-0.06177017,  0.18423969,  0.04825838, -0.01462708]), array([-0.05488602,  0.19131999,  0.01946897,  0.08515879]), array([-0.05409083,  0.21737568, -0.01081564,  0.17096106]), array([-0.0455179 ,  0.22329134,  0.09477424, -0.11112369]), array([-0.03110464,  0.20954516,  0.04608388, -0.02188119]), array([-0.02791325,  0.21545438, -0.01455441,  0.08032165]), array([-0.03649726,  0.24040015, -0.06871848,  0.16345142]), array([-0.04080527,  0.24387915,  0.02645818, -0.12958454]), array([-0.0397104 ,  0.22448553, -0.01626015, -0.06100079]), array([-0.04720324,  0.22012961, -0.05722677,  0.01691987]), array([-0.06162359,  0.23030853, -0.08370973,  0.08084752]), array([-0.06600717,  0.2163849 ,  0.04024637, -0.2181857 ]), array([-0.05979725,  0.1804201 ,  0.01950769, -0.13441852]), array([-0.05888347,  0.16476469, -0.01099665, -0.01940731]), array([-0.06407603,  0.17281273, -0.0395712 ,  0.09758891]), array([-0.06065386,  0.1678865 ,  0.07280166, -0.14522098]), array([-0.04966623,  0.15169303,  0.03440973, -0.01236959]), array([-0.04750035,  0.16357179, -0.01272862,  0.12927392]), array([-0.04105973,  0.16737522,  0.07579271, -0.09062643]), array([-0.03181692,  0.16358967,  0.01474012,  0.05467468]), array([-0.03527926,  0.18869417, -0.04777651,  0.19133535]), array([-0.0365353 ,  0.20287936,  0.03571079, -0.051725  ]), array([-0.03483137,  0.20313934, -0.01893185,  0.05440579]), array([-0.0436698 ,  0.22366711, -0.06696449,  0.145884  ]), array([-0.04706184,  0.22473147,  0.03361301, -0.13563625]), array([-0.04418538,  0.20557604, -0.00596334, -0.05231351]), array([-0.04949228,  0.20447588, -0.04600717,  0.04057067]), array([-0.06173633,  0.2206755 , -0.07341547,  0.116697  ]), array([-0.06425486,  0.2146904 ,  0.0484192 , -0.17563926]), array([-0.05668024,  0.18734092,  0.02498423, -0.0920928 ]), array([-0.05491882,  0.17947298, -0.00791746,  0.01492437]), array([-0.0596878 ,  0.19302134, -0.03832988,  0.11739016]), array([-0.05619001,  0.19031439,  0.07236123, -0.14318035]), array([-0.0454138 ,  0.17261945,  0.03273101, -0.02919417]), array([-0.04372408,  0.17948352, -0.01588161,  0.09676409]), array([-0.05126569,  0.20979208, -0.05699667,  0.19983639]), array([-0.05198527,  0.22200654,  0.0500947 , -0.07945891]), array([-0.04533753,  0.21363571,  0.01483222, -0.0018944 ]), array([-0.0463109 ,  0.22148048, -0.02407281,  0.0787548 ]), array([-0.05438047,  0.24375967, -0.05427245,  0.13894306]), array([-0.05372026,  0.2406193 ,  0.06049358, -0.16942006]), array([-0.04463697,  0.21288262,  0.02770161, -0.10192129]), array([-0.04336373,  0.20163234, -0.0155124 , -0.00857866]), array([-0.05061889,  0.2093934 , -0.05527231,  0.08363345]), array([-0.06435839,  0.23324163, -0.07857756,  0.14861028]), array([-0.06730651,  0.23192304,  0.04948398, -0.16168937]), array([-0.05883162,  0.20524499,  0.03276134, -0.09931012]), array([-0.05500133,  0.19400643,  0.00446478, -0.01065727]), array([-0.05715497,  0.20120397, -0.02529162,  0.08096931]), array([-0.0645019 ,  0.22496316, -0.04592316,  0.15136883]), array([-0.06130255,  0.22518156,  0.0770882 , -0.14839335]), array([-0.04837349,  0.20248298,  0.04893301, -0.07281919]), array([-0.04273031,  0.19770393,  0.00627284,  0.02659696]), array([-0.04591053,  0.21285164, -0.03689892,  0.12168229]), array([-0.04347258,  0.21028651,  0.06056486, -0.1462549 ]), array([-0.03614087,  0.1910518 ,  0.01074203, -0.04179718]), array([-0.03947321,  0.19431122, -0.04321122,  0.07317264]), array([-0.05253773,  0.21877441, -0.08397342,  0.16515061]), array([-0.05817197,  0.2231173 ,  0.02872709, -0.12296549]), array([-0.05489845,  0.20552316,  0.00284485, -0.04955296]), array([-0.05721498,  0.20403602, -0.02554212,  0.03448932]), array([-0.0646143 ,  0.21853204, -0.04647194,  0.10678867]), array([-0.07477389,  0.24469845, -0.05226096,  0.14885243]), array([-0.07122742,  0.24152634,  0.086726  , -0.17916281]), array([-0.05498818,  0.21037193,  0.07145947, -0.12465497]), array([-0.04414385,  0.19431106,  0.03434931, -0.03164432]), array([-0.04190616,  0.19861129, -0.01222167,  0.07412546]), array([-0.04865249,  0.22279494, -0.05307019,  0.16243211]), array([-0.04876946,  0.22677321,  0.05186349, -0.1229961 ]), array([-0.04213859,  0.20981456,  0.01263879, -0.04278132]), array([-0.04404101,  0.21043339, -0.03119619,  0.04845499]), array([-0.05398993,  0.22814664, -0.065687  ,  0.12403651]), array([-0.05583566,  0.22360832,  0.04732925, -0.16865855]), array([-0.04932204,  0.19746509,  0.015729  , -0.08739938]), array([-0.05003684,  0.19008374, -0.02290332,  0.0146265 ]), array([-0.05807878,  0.20284165, -0.0554402 ,  0.10942639]), array([-0.05790075,  0.19766104,  0.05688596, -0.16005493]), array([-0.04976802,  0.17569977,  0.0221649 , -0.05464645]), array([-0.0495524 ,  0.17686995, -0.01994654,  0.06604468]), array([-0.05725766,  0.20096191, -0.05473457,  0.16943631]), array([-0.0570025 ,  0.20764109,  0.05724175, -0.10337722]), array([-0.0486632 ,  0.19569477,  0.02414707, -0.01286173]), array([-0.04778381,  0.20299982, -0.0152429 ,  0.08468107]), array([-0.0543024 ,  0.22821443, -0.04779902,  0.16207112]), array([-0.05263416,  0.23110656,  0.0640425 , -0.13303324]), array([-0.04313379,  0.21149034,  0.02848912, -0.05842022]), array([-0.04186596,  0.2089284 , -0.01608281,  0.03331756]), array([-0.04922772,  0.22416994, -0.05552064,  0.11526221]), array([-0.04977785,  0.21882787,  0.04984121, -0.16760659]), array([-0.04360366,  0.19394719,  0.00993861, -0.07610417]), array([-0.0461728 ,  0.18959435, -0.03517878,  0.03279826]), array([-0.05702251,  0.20618426, -0.07055258,  0.12848178]), array([-0.05979159,  0.20435551,  0.04321498, -0.14658365]), array([-0.05391177,  0.18405248,  0.01380909, -0.05215954]), array([-0.05463957,  0.18441447, -0.02087051,  0.05548924]), array([-0.06178226,  0.20522765, -0.04841424,  0.14787871]), array([-0.05972167,  0.20694652,  0.06847341, -0.13033408]), array([-0.04894413,  0.18968478,  0.03663804, -0.03777247]), array([-0.0457767 ,  0.19284761, -0.00543932,  0.06921977]), array([-0.05086272,  0.21635844, -0.04360406,  0.16097351]), array([-0.04900321,  0.22054227,  0.06176369, -0.1192147 ]), array([-0.04055416,  0.20498766,  0.02059695, -0.03248258])]</t>
+  </si>
+  <si>
+    <t>['[2,0,1]', '[1,0,2]', '[1,2,0]', '[0,0,0]', '[0,2,1]', '[2,2,2]', '[1,1,1]', '[2,1,0]', '[0,1,1]', '[1,1,2]']</t>
+  </si>
+  <si>
+    <t>[2,1,0]</t>
+  </si>
+  <si>
+    <t>[5, 7, 10, 24, 25, 26, 27, 31, 52, 55, 58, 63, 65, 67, 68, 70, 71, 74, 76, 82, 83, 88, 97, 100, 106, 110, 112, 123, 130, 132, 134, 138, 141, 142, 145]</t>
+  </si>
+  <si>
+    <t>[0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 1, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 1, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 1, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+  </si>
+  <si>
+    <t>['[-0.03763371 -0.01533471  0.06554052 -0.01816017]', '[-0.00754409 -0.05458322  0.2277812  -0.36241836]', '[ 0.04879627 -0.15231473  0.32089719 -0.5887683 ]', '[ 0.11397169 -0.27767857  0.31375488 -0.63332862]', '[ 0.16759438 -0.39312519  0.2086893  -0.49480525]', '[ 0.16756229 -0.40059886 -0.20854687  0.42010337]', '[ 0.08785953 -0.23163826 -0.56914473  1.23330318]', '[-0.02173155  0.0012969  -0.49647049  1.03705522]', '[-0.12599545  0.22998299 -0.51700189  1.19236199]', '[-0.21674083  0.45476869 -0.3659157   1.00562048]', '[-0.23975321  0.55094429  0.13950864 -0.0556623 ]', '[-0.16322163  0.43427234  0.60971722 -1.08769998]', '[-0.00665149  0.13383501  0.91712346 -1.84578778]', '[ 0.18326135 -0.26503786  0.92719184 -2.03560795]', '[ 0.34268416 -0.63836451  0.62585129 -1.61799004]', '[ 0.42188579 -0.88977803  0.15130649 -0.86450518]', '[ 0.40150893 -0.97764641 -0.34897943 -0.01084619]', '[ 0.26596452 -0.8371339  -0.98277486  1.39829792]', '[ 0.02161826 -0.4329412  -1.41359144  2.57118095]', '[-0.27207736  0.14125966 -1.4391099   3.00542624]', '[-0.5184697   0.6991813  -0.95809196  2.4466727 ]', '[-0.63798471  1.08913405 -0.21809108  1.4174412 ]', '[-0.60462679  1.25997233  0.54011568  0.28648879]', '[-0.4118727   1.15002391  1.35165319 -1.37664477]', '[-0.10336556  0.77766962  1.67645089 -2.28074761]', '[ 0.2305376   0.28077965  1.58334663 -2.546737  ]', '[ 0.4963933  -0.17744984  1.00696301 -1.90633284]', '[ 0.61367844 -0.44574844  0.14162874 -0.73122349]', '[ 0.57554197 -0.52788387 -0.51870189 -0.08053454]', '[ 0.38783024 -0.4132435  -1.32316272  1.19832655]', '[ 0.06789041 -0.07380443 -1.80337232  2.08909485]', '[-0.27123255  0.29566089 -1.50714279  1.47933034]', '[-0.53354609  0.54656961 -1.06234691  0.96241101]', '[-0.6800311   0.66370068 -0.37821299  0.18992135]', '[-0.65543019  0.55618446  0.62074811 -1.2551682 ]', '[-0.43980085  0.17348988  1.491308   -2.49971775]', '[-0.0884314  -0.38997672  1.92788422 -2.95463996]', '[ 0.29105034 -0.93255017  1.78418868 -2.33404928]', '[ 0.59872551 -1.29007464  1.2429939  -1.2031083 ]', '[ 0.77256029 -1.40823975  0.46830957  0.02287473]', '[ 0.75957544 -1.22857331 -0.60770821  1.77998051]', '[ 0.52965886 -0.69203431 -1.67093017  3.57103665]', '[ 0.11695015  0.15770717 -2.32730174  4.6702035 ]', '[-0.33529347  1.03934062 -2.0747076   3.9111534 ]', '[-0.68560799  1.68303358 -1.39211622  2.51223869]', '[-0.88160248  2.04911766 -0.54949286  1.16313823]', '[-0.90130497  2.15206877  0.35174297 -0.12944283]', '[-0.73136359  1.9530597   1.32582574 -1.87286604]', '[-0.38203199  1.39330688  2.14122845 -3.75493067]', '[ 0.11281462  0.44896476  2.73245181 -5.56415787]', '[ 0.63903262 -0.68177436  2.32200409 -5.31104839]', '[ 0.9867145  -1.57779131  1.11310984 -3.62171023]', '[ 1.0678486  -2.09925836 -0.27707075 -1.63751051]', '[ 0.89534325 -2.2615765  -1.40798283  0.00847068]', '[ 0.52070315 -2.07668127 -2.26489417  1.83338906]', '[ 0.03806588 -1.58029099 -2.48029642  3.08589092]', '[-0.46233571 -0.8167249  -2.469587    4.46000595]', '[-0.91715461  0.12989126 -1.95762059  4.7367773 ]', '[-1.17031331  0.91199113 -0.51627351  2.98670596]', '[-1.13757797  1.37103164  0.84867832  1.56451602]', '[-0.82228876  1.47003546  2.24425503 -0.60660002]', '[-0.27361746  1.12005803  3.14522186 -2.87339094]', '[ 0.39209768  0.3600433   3.38198886 -4.49441906]', '[ 0.98713431 -0.46431839  2.43432897 -3.46020956]', '[ 1.36169997 -1.03970541  1.27946844 -2.27435831]', '[ 1.47406293 -1.32718334 -0.15328334 -0.62480335]', '[ 1.30164238 -1.28525723 -1.5648497   1.08897749]', '[ 0.8740592  -0.92231649 -2.67782019  2.57678753]', '[ 0.2567114  -0.26823526 -3.37957433  3.78547539]', '[-0.43487975  0.52355446 -3.35337626  3.76214622]', '[-1.00263131  1.07200521 -2.24836898  1.6722167 ]', '[-1.3170401   1.20768695 -0.87224897 -0.25954856]', '[-1.34676476  0.98482106  0.57950296 -1.95600847]', '[-1.08576553  0.42108845  2.01307521 -3.67634004]', '[-0.59242425 -0.37469887  2.81207166 -4.04906587]', '[ 0.01255076 -1.14651056  3.11523832 -3.416738  ]', '[ 0.59017029 -1.62584159  2.56050385 -1.32275441]', '[ 1.01414355 -1.71796302  1.60009531  0.39152952]', '[ 1.19826192 -1.45574884  0.2056432   2.20623289]', '[ 1.07923233 -0.81095952 -1.39688703  4.25362086]', '[ 0.65881299  0.22147962 -2.66604803  5.7991679 ]', '[ 0.09063798  1.33968698 -2.88639404  5.09432768]', '[-0.45450054  2.17324709 -2.52177863  3.26035129]', '[-0.89031414  2.65315259 -1.76424506  1.55497071]', '[-1.14953659  2.83656507 -0.792778    0.27684424]', '[-1.20009673  2.76235396  0.29264193 -1.02292844]', '[-1.02179211  2.38407929  1.47821421 -2.78410569]', '[-0.61607205  1.62773376  2.56675047 -4.86791452]', '[-0.0210494   0.4617889   3.28610873 -6.63718235]', '[ 0.62154072 -0.87515791  2.86960062 -6.15839672]', '[ 1.06962127 -1.90460558  1.58820659 -4.17948092]', '[ 1.25780098 -2.57960434  0.30365901 -2.62384097]', '[ 1.19767466 -2.96563911 -0.88447193 -1.25784069]', '[ 0.90213793 -3.05440159 -2.0354732   0.33156669]', '[ 0.40677793 -2.85226917 -2.82810372  1.63599627]', '[-0.17969488 -2.42227926 -2.90423288  2.60427123]', '[-0.70752428 -1.83930553 -2.29802854  3.14680621]', '[-1.06503703 -1.24685846 -1.25032571  2.68590048]', '[-1.22364328 -0.73280662 -0.33743847  2.43688891]', '[-1.20086536 -0.27375944  0.56617719  2.14812718]', '[-0.96748274  0.04792645  1.76732683  1.03768623]', '[-0.50326195  0.13267629  2.81332783 -0.17014882]', '[ 0.11649761  0.01075167  3.24886271 -0.91096794]', '[ 0.73642387 -0.1629111   2.82351245 -0.68637759]', '[ 1.20828222 -0.22810089  1.84360341  0.06046617]', '[ 1.46522735 -0.14237799  0.72231396  0.77555483]', '[ 1.49844659  0.0752064  -0.38638346  1.39048289]', '[ 1.28577627  0.47805676 -1.72420046  2.5905852 ]', '[ 0.82262099  1.06788588 -2.8516033   3.13550712]', '[ 0.17638903  1.64725455 -3.50340873  2.44932349]', '[-0.50318447  1.93186063 -3.11843584  0.28394941]', '[-1.01732937  1.77877731 -1.88899792 -1.83308449]', '[-1.22238253  1.20632825 -0.12881953 -3.8517606 ]', '[-1.0541739   0.19895284  1.71468709 -6.08272535]', '[-0.62307243 -1.07510666  2.39358465 -6.26992505]', '[-0.13271933 -2.23994206  2.49804037 -5.3993567 ]', '[ 0.3624783   3.01833242  2.37864148 -4.93960028]', '[ 0.78902296  2.03578386  1.86337907 -4.95808454]', '[ 1.1148543   1.01047574  1.41775714 -5.34039815]', '[ 1.34341535 -0.08263658  0.74223266 -5.39269656]', '[ 1.33624586 -1.02926278 -0.95977523 -3.83760439]', '[ 0.9359768  -1.55442173 -2.99534756 -1.30612701]', '[ 0.1828138  -1.48465963 -4.31596012  1.95532678]', '[-0.68129236 -0.88719984 -4.14042016  3.73716085]', '[-1.43872557 -0.06825906 -3.33292871  4.13649672]', '[-1.99271603  0.68539499 -2.20679058  3.36175069]', '[-2.33197172  1.29875175 -1.21151454  2.84596496]', '[-2.48062021  1.84213999 -0.26618751  2.59720555]', '[-2.43009896  2.32638873  0.79501309  2.18582285]', '[-2.14899509  2.66408057  2.02948773  1.1012955 ]', '[-1.61777839  2.74977799  3.29338683 -0.3335335 ]', '[-0.82896672  2.45920155  4.50333873 -2.65314995]', '[ 0.10651029  1.70817796  4.68543972 -4.8438067 ]', '[ 1.01788836  0.51553446  4.3520303  -6.81360035]', '[ 1.76101033 -0.74297971  2.95768766 -5.40652457]', '[ 2.21745947 -1.69691449  1.62843452 -4.23209709]', '[ 2.42034607 -2.46901044  0.42533    -3.52362218]', '[ 2.40360355 -3.10344997 -0.53868081 -2.79373008]', '[ 2.20901293  2.75010431 -1.40138134 -1.46979119]', '[ 1.83143692  2.60137564 -2.42053691 -0.01512056]', '[ 1.22407763  2.73363753 -3.6673034   1.27848411]', '[ 0.39364346  3.04221124 -4.52334271  1.71674627]', '[-0.51489678 -2.90017226 -4.37469569  1.59092982]', '[-1.3046685  -2.60818011 -3.42926145  1.22452316]', '[-1.87493774 -2.4446546  -2.29007921  0.34948416]', '[-2.22499811 -2.52170562 -1.26357607 -1.12316328]', '[-2.40312299 -2.86710117 -0.5372413  -2.30225425]', '[-2.42828759  2.83361325  0.33582437 -3.4966372 ]', '[-2.23886245  2.01853343  1.6301526  -4.70374389]', '[-1.75027294  0.8997193   3.31802964 -6.68360764]', '[-0.9227049  -0.64265202  4.73548507 -8.14207855]', '[ 0.06340808 -2.09209976  5.07219955 -6.14755874]', '[ 1.06115293 -3.13626254  4.69738057 -4.46961832]', '[ 1.87897603  2.34630242  3.44589758 -3.60358379]', '[ 2.46098183  1.69947024  2.4606336  -2.86790923]']</t>
+  </si>
+  <si>
+    <t>[0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50, 51, 52, 53, 54, 55, 56, 57, 58, 59, 60, 61, 62, 63, 64, 65, 66, 67, 68, 69, 70, 71, 72, 73, 74, 75, 76, 77, 78, 79, 80, 81, 82, 83, 84, 85, 86, 87, 88, 89, 90, 91, 92, 93, 94, 95, 96, 97, 98, 99, 100, 101, 102, 103, 104, 105, 106, 107, 108, 109, 110, 111, 112, 113, 114, 115, 116, 117, 118, 119, 120, 121, 122, 123, 124, 125, 126, 127, 128, 129, 130, 131, 132, 133, 134, 135, 136, 137, 138, 139, 140, 141, 142, 143, 144, 145, 146, 147, 148, 149, 150, 151, 152, 153, 154]</t>
+  </si>
+  <si>
+    <t>[array([-0.03763371, -0.01533471,  0.06554052, -0.01816017], dtype=float32), array([-0.00754409, -0.05458322,  0.2277812 , -0.36241836]), array([ 0.04879627, -0.15231473,  0.32089719, -0.5887683 ]), array([ 0.11397169, -0.27767857,  0.31375488, -0.63332862]), array([ 0.16759438, -0.39312519,  0.2086893 , -0.49480525]), array([ 0.16756229, -0.40059886, -0.20854687,  0.42010337]), array([ 0.08785953, -0.23163826, -0.56914473,  1.23330318]), array([-0.02173155,  0.0012969 , -0.49647049,  1.03705522]), array([-0.12599545,  0.22998299, -0.51700189,  1.19236199]), array([-0.21674083,  0.45476869, -0.3659157 ,  1.00562048]), array([-0.23975321,  0.55094429,  0.13950864, -0.0556623 ]), array([-0.16322163,  0.43427234,  0.60971722, -1.08769998]), array([-0.00665149,  0.13383501,  0.91712346, -1.84578778]), array([ 0.18326135, -0.26503786,  0.92719184, -2.03560795]), array([ 0.34268416, -0.63836451,  0.62585129, -1.61799004]), array([ 0.42188579, -0.88977803,  0.15130649, -0.86450518]), array([ 0.40150893, -0.97764641, -0.34897943, -0.01084619]), array([ 0.26596452, -0.8371339 , -0.98277486,  1.39829792]), array([ 0.02161826, -0.4329412 , -1.41359144,  2.57118095]), array([-0.27207736,  0.14125966, -1.4391099 ,  3.00542624]), array([-0.5184697 ,  0.6991813 , -0.95809196,  2.4466727 ]), array([-0.63798471,  1.08913405, -0.21809108,  1.4174412 ]), array([-0.60462679,  1.25997233,  0.54011568,  0.28648879]), array([-0.4118727 ,  1.15002391,  1.35165319, -1.37664477]), array([-0.10336556,  0.77766962,  1.67645089, -2.28074761]), array([ 0.2305376 ,  0.28077965,  1.58334663, -2.546737  ]), array([ 0.4963933 , -0.17744984,  1.00696301, -1.90633284]), array([ 0.61367844, -0.44574844,  0.14162874, -0.73122349]), array([ 0.57554197, -0.52788387, -0.51870189, -0.08053454]), array([ 0.38783024, -0.4132435 , -1.32316272,  1.19832655]), array([ 0.06789041, -0.07380443, -1.80337232,  2.08909485]), array([-0.27123255,  0.29566089, -1.50714279,  1.47933034]), array([-0.53354609,  0.54656961, -1.06234691,  0.96241101]), array([-0.6800311 ,  0.66370068, -0.37821299,  0.18992135]), array([-0.65543019,  0.55618446,  0.62074811, -1.2551682 ]), array([-0.43980085,  0.17348988,  1.491308  , -2.49971775]), array([-0.0884314 , -0.38997672,  1.92788422, -2.95463996]), array([ 0.29105034, -0.93255017,  1.78418868, -2.33404928]), array([ 0.59872551, -1.29007464,  1.2429939 , -1.2031083 ]), array([ 0.77256029, -1.40823975,  0.46830957,  0.02287473]), array([ 0.75957544, -1.22857331, -0.60770821,  1.77998051]), array([ 0.52965886, -0.69203431, -1.67093017,  3.57103665]), array([ 0.11695015,  0.15770717, -2.32730174,  4.6702035 ]), array([-0.33529347,  1.03934062, -2.0747076 ,  3.9111534 ]), array([-0.68560799,  1.68303358, -1.39211622,  2.51223869]), array([-0.88160248,  2.04911766, -0.54949286,  1.16313823]), array([-0.90130497,  2.15206877,  0.35174297, -0.12944283]), array([-0.73136359,  1.9530597 ,  1.32582574, -1.87286604]), array([-0.38203199,  1.39330688,  2.14122845, -3.75493067]), array([ 0.11281462,  0.44896476,  2.73245181, -5.56415787]), array([ 0.63903262, -0.68177436,  2.32200409, -5.31104839]), array([ 0.9867145 , -1.57779131,  1.11310984, -3.62171023]), array([ 1.0678486 , -2.09925836, -0.27707075, -1.63751051]), array([ 0.89534325, -2.2615765 , -1.40798283,  0.00847068]), array([ 0.52070315, -2.07668127, -2.26489417,  1.83338906]), array([ 0.03806588, -1.58029099, -2.48029642,  3.08589092]), array([-0.46233571, -0.8167249 , -2.469587  ,  4.46000595]), array([-0.91715461,  0.12989126, -1.95762059,  4.7367773 ]), array([-1.17031331,  0.91199113, -0.51627351,  2.98670596]), array([-1.13757797,  1.37103164,  0.84867832,  1.56451602]), array([-0.82228876,  1.47003546,  2.24425503, -0.60660002]), array([-0.27361746,  1.12005803,  3.14522186, -2.87339094]), array([ 0.39209768,  0.3600433 ,  3.38198886, -4.49441906]), array([ 0.98713431, -0.46431839,  2.43432897, -3.46020956]), array([ 1.36169997, -1.03970541,  1.27946844, -2.27435831]), array([ 1.47406293, -1.32718334, -0.15328334, -0.62480335]), array([ 1.30164238, -1.28525723, -1.5648497 ,  1.08897749]), array([ 0.8740592 , -0.92231649, -2.67782019,  2.57678753]), array([ 0.2567114 , -0.26823526, -3.37957433,  3.78547539]), array([-0.43487975,  0.52355446, -3.35337626,  3.76214622]), array([-1.00263131,  1.07200521, -2.24836898,  1.6722167 ]), array([-1.3170401 ,  1.20768695, -0.87224897, -0.25954856]), array([-1.34676476,  0.98482106,  0.57950296, -1.95600847]), array([-1.08576553,  0.42108845,  2.01307521, -3.67634004]), array([-0.59242425, -0.37469887,  2.81207166, -4.04906587]), array([ 0.01255076, -1.14651056,  3.11523832, -3.416738  ]), array([ 0.59017029, -1.62584159,  2.56050385, -1.32275441]), array([ 1.01414355, -1.71796302,  1.60009531,  0.39152952]), array([ 1.19826192, -1.45574884,  0.2056432 ,  2.20623289]), array([ 1.07923233, -0.81095952, -1.39688703,  4.25362086]), array([ 0.65881299,  0.22147962, -2.66604803,  5.7991679 ]), array([ 0.09063798,  1.33968698, -2.88639404,  5.09432768]), array([-0.45450054,  2.17324709, -2.52177863,  3.26035129]), array([-0.89031414,  2.65315259, -1.76424506,  1.55497071]), array([-1.14953659,  2.83656507, -0.792778  ,  0.27684424]), array([-1.20009673,  2.76235396,  0.29264193, -1.02292844]), array([-1.02179211,  2.38407929,  1.47821421, -2.78410569]), array([-0.61607205,  1.62773376,  2.56675047, -4.86791452]), array([-0.0210494 ,  0.4617889 ,  3.28610873, -6.63718235]), array([ 0.62154072, -0.87515791,  2.86960062, -6.15839672]), array([ 1.06962127, -1.90460558,  1.58820659, -4.17948092]), array([ 1.25780098, -2.57960434,  0.30365901, -2.62384097]), array([ 1.19767466, -2.96563911, -0.88447193, -1.25784069]), array([ 0.90213793, -3.05440159, -2.0354732 ,  0.33156669]), array([ 0.40677793, -2.85226917, -2.82810372,  1.63599627]), array([-0.17969488, -2.42227926, -2.90423288,  2.60427123]), array([-0.70752428, -1.83930553, -2.29802854,  3.14680621]), array([-1.06503703, -1.24685846, -1.25032571,  2.68590048]), array([-1.22364328, -0.73280662, -0.33743847,  2.43688891]), array([-1.20086536, -0.27375944,  0.56617719,  2.14812718]), array([-0.96748274,  0.04792645,  1.76732683,  1.03768623]), array([-0.50326195,  0.13267629,  2.81332783, -0.17014882]), array([ 0.11649761,  0.01075167,  3.24886271, -0.91096794]), array([ 0.73642387, -0.1629111 ,  2.82351245, -0.68637759]), array([ 1.20828222, -0.22810089,  1.84360341,  0.06046617]), array([ 1.46522735, -0.14237799,  0.72231396,  0.77555483]), array([ 1.49844659,  0.0752064 , -0.38638346,  1.39048289]), array([ 1.28577627,  0.47805676, -1.72420046,  2.5905852 ]), array([ 0.82262099,  1.06788588, -2.8516033 ,  3.13550712]), array([ 0.17638903,  1.64725455, -3.50340873,  2.44932349]), array([-0.50318447,  1.93186063, -3.11843584,  0.28394941]), array([-1.01732937,  1.77877731, -1.88899792, -1.83308449]), array([-1.22238253,  1.20632825, -0.12881953, -3.8517606 ]), array([-1.0541739 ,  0.19895284,  1.71468709, -6.08272535]), array([-0.62307243, -1.07510666,  2.39358465, -6.26992505]), array([-0.13271933, -2.23994206,  2.49804037, -5.3993567 ]), array([ 0.3624783 ,  3.01833242,  2.37864148, -4.93960028]), array([ 0.78902296,  2.03578386,  1.86337907, -4.95808454]), array([ 1.1148543 ,  1.01047574,  1.41775714, -5.34039815]), array([ 1.34341535, -0.08263658,  0.74223266, -5.39269656]), array([ 1.33624586, -1.02926278, -0.95977523, -3.83760439]), array([ 0.9359768 , -1.55442173, -2.99534756, -1.30612701]), array([ 0.1828138 , -1.48465963, -4.31596012,  1.95532678]), array([-0.68129236, -0.88719984, -4.14042016,  3.73716085]), array([-1.43872557, -0.06825906, -3.33292871,  4.13649672]), array([-1.99271603,  0.68539499, -2.20679058,  3.36175069]), array([-2.33197172,  1.29875175, -1.21151454,  2.84596496]), array([-2.48062021,  1.84213999, -0.26618751,  2.59720555]), array([-2.43009896,  2.32638873,  0.79501309,  2.18582285]), array([-2.14899509,  2.66408057,  2.02948773,  1.1012955 ]), array([-1.61777839,  2.74977799,  3.29338683, -0.3335335 ]), array([-0.82896672,  2.45920155,  4.50333873, -2.65314995]), array([ 0.10651029,  1.70817796,  4.68543972, -4.8438067 ]), array([ 1.01788836,  0.51553446,  4.3520303 , -6.81360035]), array([ 1.76101033, -0.74297971,  2.95768766, -5.40652457]), array([ 2.21745947, -1.69691449,  1.62843452, -4.23209709]), array([ 2.42034607, -2.46901044,  0.42533   , -3.52362218]), array([ 2.40360355, -3.10344997, -0.53868081, -2.79373008]), array([ 2.20901293,  2.75010431, -1.40138134, -1.46979119]), array([ 1.83143692,  2.60137564, -2.42053691, -0.01512056]), array([ 1.22407763,  2.73363753, -3.6673034 ,  1.27848411]), array([ 0.39364346,  3.04221124, -4.52334271,  1.71674627]), array([-0.51489678, -2.90017226, -4.37469569,  1.59092982]), array([-1.3046685 , -2.60818011, -3.42926145,  1.22452316]), array([-1.87493774, -2.4446546 , -2.29007921,  0.34948416]), array([-2.22499811, -2.52170562, -1.26357607, -1.12316328]), array([-2.40312299, -2.86710117, -0.5372413 , -2.30225425]), array([-2.42828759,  2.83361325,  0.33582437, -3.4966372 ]), array([-2.23886245,  2.01853343,  1.6301526 , -4.70374389]), array([-1.75027294,  0.8997193 ,  3.31802964, -6.68360764]), array([-0.9227049 , -0.64265202,  4.73548507, -8.14207855]), array([ 0.06340808, -2.09209976,  5.07219955, -6.14755874]), array([ 1.06115293, -3.13626254,  4.69738057, -4.46961832]), array([ 1.87897603,  2.34630242,  3.44589758, -3.60358379]), array([ 2.46098183,  1.69947024,  2.4606336 , -2.86790923])]</t>
+  </si>
+  <si>
+    <t>['[2,1,0]', '[0,0,0]', '[0,1,1]', '[1,0,2]', '[1,2,0]', '[2,2,2]', '[1,1,1]', '[1,1,2]', '[2,0,1]', '[0,2,1]']</t>
+  </si>
+  <si>
+    <t>[4, 5, 8, 11, 12, 13, 24, 25, 28, 31, 33, 35, 38, 42, 43, 45, 47, 50, 54, 56, 58, 59, 60, 61, 62, 63, 64, 66, 67, 68, 69, 74, 75, 77, 78, 83, 86, 89, 92, 93, 94, 101, 102, 103, 105, 116, 117, 121, 124, 126, 130, 133, 134, 138, 140, 148, 149, 153, 155, 158, 161, 163, 164, 165, 166, 167, 174, 175, 178, 180, 181, 185, 189, 193, 195, 197, 199]</t>
+  </si>
+  <si>
+    <t>[0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 1, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 1, 2, 2, 2, 2, 2, 2, 2, 1, 0, 0, 0, 0, 0, 0, 0, 1, 2]</t>
+  </si>
+  <si>
+    <t>['[-0.03763371 -0.01533471  0.06554052 -0.01816017]', '[-0.00754409 -0.05458322  0.2277812  -0.36241836]', '[ 0.04879627 -0.15231473  0.32089719 -0.5887683 ]', '[ 0.11397169 -0.27767857  0.31375488 -0.63332862]', '[ 0.14175109 -0.32605932 -0.04191742  0.15948612]', '[ 0.12408355 -0.28359622 -0.12991716  0.25542587]', '[ 0.06628156 -0.1609925  -0.4332554   0.94238688]', '[-0.03997183  0.07536271 -0.59955244  1.36223188]', '[-0.13347965  0.28830272 -0.31134893  0.71916536]', '[-0.18392678  0.41746954 -0.17971715  0.54476058]', '[-0.20135815  0.49730862  0.01027918  0.23990637]', '[-0.17960152  0.5107326   0.20286864 -0.10413804]', '[-0.12367496  0.4591226   0.34390883 -0.39617737]', '[-0.04837934  0.3611809   0.39136792 -0.556458  ]', '[ 0.05128842  0.18116446  0.58106138 -1.20070672]', '[ 0.17173109 -0.09552311  0.58938555 -1.49765887]', '[ 0.272735   -0.38816445  0.39021647 -1.36263387]', '[ 0.31809462 -0.61814284  0.04979373 -0.89875229]', '[ 0.29081563 -0.73779218 -0.31736498 -0.28790243]', '[ 0.17295151 -0.67148998 -0.83645619  0.93047757]', '[-0.03041486 -0.38107376 -1.15448665  1.90971619]', '[-0.26685451  0.05406794 -1.14725647  2.32320254]', '[-0.46279339  0.4967239  -0.7579657   1.99775086]', '[-0.55403823  0.82199184 -0.13398103  1.20949258]', '[-0.49218933  0.91081433  0.73597288 -0.32030153]', '[-0.29362168  0.75958902  1.21152544 -1.15984968]', '[-0.00283143  0.40409859  1.63698883 -2.31393249]', '[ 0.33040959 -0.11429168  1.60900133 -2.71033821]', '[ 0.58057182 -0.54911047  0.83871716 -1.54659023]', '[ 0.67785985 -0.77854932  0.11636301 -0.71858287]', '[ 0.60221093 -0.76891109 -0.85948861  0.81312561]', '[ 0.36916884 -0.52359588 -1.42694954  1.59221376]', '[ 0.0298536  -0.0972408  -1.88800066  2.5476114 ]', '[-0.32064774  0.35878596 -1.53115643  1.8671078 ]', '[-0.58047394  0.67394426 -1.01511311  1.21521919]', '[-0.68827248  0.76706947 -0.04711342 -0.2903242 ]', '[-0.59804575  0.55903455  0.93686624 -1.77241678]', '[-0.32660438  0.07737809  1.71571916 -2.93662542]', '[ 0.02504663 -0.47764301  1.71019468 -2.44488272]', '[ 0.35006477 -0.91005053  1.47206763 -1.77857192]', '[ 0.5918488  -1.16426295  0.90531366 -0.7341114 ]', '[ 0.70007829 -1.1988848   0.15883606  0.38957219]', '[ 0.65220855 -1.009555   -0.63312249  1.49466502]', '[ 0.45379361 -0.60933072 -1.31598258  2.45870344]', '[ 1.23083995e-01  2.99678791e-03 -1.90522181e+00  3.50439057e+00]', '[-0.23644371  0.63446648 -1.59719929  2.63521525]', '[-0.51258746  1.07561634 -1.11485922  1.71101948]', '[-0.6483764   1.2521287  -0.22708632  0.05426094]', '[-0.59984502  1.09703379  0.71254194 -1.60766009]', '[-0.36733011  0.60989071  1.58293319 -3.22865278]', '[-0.0198321  -0.07989726  1.78635748 -3.46187985]', '[ 0.32714773 -0.75021455  1.58715394 -3.05648109]', '[ 0.58749647 -1.25646567  0.97701768 -1.95828784]', '[ 0.7086426  -1.52758117  0.22348887 -0.7510771 ]', '[ 0.67618143 -1.55722704 -0.54000164  0.45342344]', '[ 0.48118422 -1.29509777 -1.3882316   2.17386079]', '[ 0.1542685  -0.74800937 -1.82794413  3.22955123]', '[-0.24363461  0.00766025 -2.04178531  4.11063409]', '[-0.58317962  0.72068533 -1.26528327  2.85120759]', '[-0.732835    1.12230918 -0.22024311  1.15457375]', '[-0.67300305  1.1831618   0.80307617 -0.54557227]', '[-0.44265372  0.96138966  1.46290881 -1.65158547]', '[-0.10848935  0.54185032  1.81184906 -2.45301697]', '[ 0.24799389  0.03672657  1.66191429 -2.43374984]', '[ 0.52141151 -0.36834984  1.00936403 -1.51037562]', '[ 0.66032359 -0.60806364  0.35249687 -0.84563748]', '[ 0.63261513 -0.63337324 -0.62417772  0.59328653]', '[ 0.44356936 -0.44178622 -1.23075893  1.28368537]', '[ 0.16074011 -0.14622054 -1.53387227  1.58034742]', '[-0.14038898  0.14545833 -1.40603227  1.23050374]', '[-0.40153047  0.37687145 -1.14782399  1.00665   ]', '[-0.58013246  0.52427727 -0.60460963  0.43212332]', '[-0.63464498  0.5421699   0.06777785 -0.25683382]', '[-0.52882216  0.35826738  0.97113146 -1.55468031]', '[-0.28845981  0.01325595  1.37599183 -1.80174616]', '[-0.00546246 -0.31718617  1.38672182 -1.39586378]', '[ 0.2658565  -0.57341535  1.26558264 -1.08349257]', '[ 0.45442429 -0.66146834  0.58339149  0.22801596]', '[ 0.51455871 -0.54457159  0.01008753  0.92834899]', '[ 0.43416631 -0.23384937 -0.7933758   2.12883278]', '[ 0.21505608  0.26993792 -1.33148023  2.77451831]', '[-0.06692344  0.81252463 -1.41786331  2.51624637]', '[-0.32858446  1.23651327 -1.15451941  1.66493663]', '[-0.49486793  1.41297557 -0.48322794  0.09233619]', '[-0.51296152  1.27037446  0.31820176 -1.5273664 ]', '[-0.36403409  0.79841885  1.16412801 -3.18260614]', '[-0.08907126  0.09241473  1.49510934 -3.69832162]', '[ 0.21388883 -0.65418349  1.42689731 -3.54887483]', '[ 0.44980034 -1.26631424  0.89251976 -2.50735489]', '[ 0.54633967 -1.59947118  0.07954009 -0.84053729]', '[ 0.48623097 -1.6073156  -0.66468847  0.75568543]', '[ 0.28815559 -1.29773758 -1.29543911  2.33949024]', '[ 2.76246475e-05 -7.35380636e-01 -1.53816961e+00  3.21041134e+00]', '[-0.2984104  -0.06796958 -1.35610813  3.27976989]', '[-0.50504998  0.49954787 -0.64714745  2.26434891]', '[-0.56748033  0.87133341  0.04010847  1.40438948]', '[-0.48924423  1.0507656   0.72484781  0.38175518]', '[-0.26928757  0.96858663  1.42828585 -1.18038667]', '[ 0.06015201  0.59582509  1.80374552 -2.4707841 ]', '[ 0.42157391  0.03038091  1.72253519 -3.01765649]', '[ 0.71183906 -0.53849413  1.10667906 -2.53267376]', '[ 0.82123254 -0.88654582 -0.02439309 -0.92659634]', '[ 0.72608844 -0.96515163 -0.91315619  0.1507867 ]', '[ 0.46731372 -0.8256879  -1.6306137   1.22481891]', '[ 0.07430265 -0.4312519  -2.22179693  2.62626975]', '[-0.35411872  0.09022941 -1.95470194  2.39654934]', '[-0.69563492  0.5290857  -1.38826536  1.87780713]', '[-0.8892093   0.81449054 -0.51884381  0.94698219]', '[-0.89749595  0.902716    0.43725452 -0.07198268]', '[-0.69559062  0.72213337  1.556736   -1.73296487]', '[-0.29285244  0.2225355   2.39334788 -3.15316416]', '[ 0.21420896 -0.45291111  2.54167923 -3.34152156]', '[ 0.67413173 -1.02450016  1.97258787 -2.25921563]', '[ 0.98045843 -1.34174541  1.05465932 -0.91724546]', '[ 1.08688658e+00 -1.39779760e+00 -1.11939604e-03  3.44274797e-01]', '[ 0.95974711 -1.15095884 -1.26642737  2.14370568]', '[ 0.60926803 -0.59292951 -2.19027788  3.39024019]', '[ 0.11952124  0.1462485  -2.57791222  3.75042338]', '[-0.38940102  0.85694664 -2.38930179  3.13219601]', '[-0.80090102  1.35000139 -1.66804787  1.7626339 ]', '[-1.0400806   1.56383005 -0.69657018  0.3926776 ]', '[-1.07308046  1.51300616  0.37154725 -0.89543201]', '[-0.87383565  1.14986065  1.61377194 -2.76645667]', '[-0.43586238  0.3986219   2.70437019 -4.66781874]', '[ 0.1246717  -0.53624923  2.72835694 -4.31701559]', '[ 0.62457772 -1.28249471  2.18581489 -3.02302051]', '[ 0.95957201 -1.68682115  1.13354702 -1.05295431]', '[ 1.0850024  -1.76188946  0.10581544  0.28979979]', '[ 0.98280577 -1.52325186 -1.12748222  2.11771541]', '[ 0.63650918 -0.89882376 -2.31753862  4.15608486]', '[ 0.106704    0.04127943 -2.83007508  4.94449159]', '[-0.44435251  0.98159689 -2.53285125  4.16220127]', '[-0.87290301  1.65777691 -1.70951541  2.59312281]', '[-1.10035528  1.98415759 -0.54968365  0.70714949]', '[-1.08921511  1.9473326   0.66136892 -1.07795048]', '[-0.83872788  1.54374145  1.83079188 -3.00126475]', '[-0.36366723  0.72572637  2.88242714 -5.17392049]', '[ 0.2641935  -0.43202306  3.17049513 -5.91313981]', '[ 0.7989747  -1.40462576  2.10827008 -3.72195837]', '[ 1.11724188 -1.9885037   1.05532343 -2.15734842]', '[ 1.20242339 -2.23698034 -0.20176662 -0.34724204]', '[ 1.04033075 -2.12716277 -1.39961555  1.46228496]', '[ 0.65466243 -1.63864639 -2.4221078   3.47146808]', '[ 0.08522293 -0.71942041 -3.22188603  5.68616431]', '[-0.57354962  0.5102354  -3.12322362  6.07149704]', '[-1.08467499  1.5471734  -1.92305688  4.23083151]', '[-1.33811815  2.22745841 -0.61165886  2.6295464 ]', '[-1.33210008  2.61048653  0.65820947  1.20901365]', '[-1.0828675   2.7113084   1.80389689 -0.1981535 ]', '[-0.63018364  2.53485446  2.6469774  -1.54927618]', '[-0.0539396   2.06072462  3.00012549 -3.16146834]', '[ 0.53027831  1.28848365  2.7842231  -4.49833063]', '[ 1.04318492  0.30387973  2.27720295 -5.16187915]', '[ 1.36947985 -0.6051369   0.89352123 -3.7511142 ]', '[ 1.40304638 -1.2287178  -0.59370058 -2.4214479 ]', '[ 1.11080894 -1.4946626  -2.28959529 -0.17276499]', '[ 0.5176027  -1.2712983  -3.53709379  2.43734444]', '[-0.25367415 -0.53844292 -4.03351839  4.68712654]', '[-0.99539273  0.37097736 -3.20926625  3.99780079]', '[-1.52224971  1.04222557 -2.02573987  2.69087279]', '[-1.80509072  1.46990204 -0.80741885  1.64518072]', '[-1.82843338  1.66377153  0.57297461  0.29504938]', '[-1.57405737  1.57092268  1.97582252 -1.30606893]', '[-1.05669698  1.14944023  3.17932973 -3.00337132]', '[-0.32251449  0.3594482   4.04786957 -4.72297371]', '[ 0.48000796 -0.56119971  3.76037957 -4.01149464]', '[ 1.1205557  -1.13571503  2.56731429 -1.69840184]', '[ 1.49062657 -1.26715808  1.11454011  0.29996105]', '[ 1.57485695 -1.07010213 -0.26800183  1.63339832]', '[ 1.37345328 -0.58438865 -1.74484357  3.24897306]', '[ 0.88587355  0.22184586 -3.05432067  4.64665728]', '[ 0.20426421  1.14274231 -3.62856604  4.23311727]', '[-0.51873993  1.82407755 -3.48235878  2.46886248]', '[-1.13785635  2.11729437 -2.59961741  0.48282452]', '[-1.51087485  1.99255841 -1.07449126 -1.67700098]', '[-1.57215177  1.51055251  0.46317613 -3.11270857]', '[-1.30736014  0.68928318  2.18023389 -5.14517337]', '[-0.72848854 -0.5071273   3.4306018  -6.42849387]', '[-0.02954232 -1.64220247  3.48669531 -4.73913809]', '[ 0.65852048 -2.43341002  3.29110367 -3.16723713]', '[ 1.22736222 -2.87796794  2.30937565 -1.30743958]', '[ 1.56306512 -2.96198403  1.02858955  0.45987983]', '[ 1.6414336  -2.71616719 -0.25412176  1.99434293]', '[ 1.44924608 -2.13985741 -1.68662858  3.81796339]', '[ 0.95753502 -1.14419936 -3.25866184  6.30434034]', '[ 0.19069384  0.30644691 -4.13211676  7.58626575]', '[-0.59063055  1.64882309 -3.54422234  5.55360437]', '[-1.21295398  2.55414517 -2.63555765  3.61398734]', '[-1.62758675  3.12851004 -1.48949755  2.17665352]', '[-1.79687514 -2.89078177 -0.20935865  0.4634606 ]', '[-1.71804942 -2.95021163  1.00187948 -1.05678597]', '[-1.38784561  2.95012011  2.29525291 -2.7848522 ]', '[-0.81255995  2.20039239  3.40121961 -4.8113725 ]', '[-0.06332719  1.01865017  4.05460391 -7.05861491]', '[ 0.77231769 -0.55091738  3.96618454 -7.83757028]', '[ 1.39302423 -1.82497059  2.22913011 -4.97175996]', '[ 1.69329681 -2.65304398  0.80010699 -3.3971761 ]', '[ 1.71464777  3.12405392 -0.55593232 -1.675045  ]', '[ 1.48175773  2.93934697 -1.77192455 -0.18389447]', '[ 1.01353463  3.01980495 -2.88487448  0.94275971]']</t>
+  </si>
+  <si>
+    <t>[array([-0.03763371, -0.01533471,  0.06554052, -0.01816017], dtype=float32), array([-0.00754409, -0.05458322,  0.2277812 , -0.36241836]), array([ 0.04879627, -0.15231473,  0.32089719, -0.5887683 ]), array([ 0.11397169, -0.27767857,  0.31375488, -0.63332862]), array([ 0.14175109, -0.32605932, -0.04191742,  0.15948612]), array([ 0.12408355, -0.28359622, -0.12991716,  0.25542587]), array([ 0.06628156, -0.1609925 , -0.4332554 ,  0.94238688]), array([-0.03997183,  0.07536271, -0.59955244,  1.36223188]), array([-0.13347965,  0.28830272, -0.31134893,  0.71916536]), array([-0.18392678,  0.41746954, -0.17971715,  0.54476058]), array([-0.20135815,  0.49730862,  0.01027918,  0.23990637]), array([-0.17960152,  0.5107326 ,  0.20286864, -0.10413804]), array([-0.12367496,  0.4591226 ,  0.34390883, -0.39617737]), array([-0.04837934,  0.3611809 ,  0.39136792, -0.556458  ]), array([ 0.05128842,  0.18116446,  0.58106138, -1.20070672]), array([ 0.17173109, -0.09552311,  0.58938555, -1.49765887]), array([ 0.272735  , -0.38816445,  0.39021647, -1.36263387]), array([ 0.31809462, -0.61814284,  0.04979373, -0.89875229]), array([ 0.29081563, -0.73779218, -0.31736498, -0.28790243]), array([ 0.17295151, -0.67148998, -0.83645619,  0.93047757]), array([-0.03041486, -0.38107376, -1.15448665,  1.90971619]), array([-0.26685451,  0.05406794, -1.14725647,  2.32320254]), array([-0.46279339,  0.4967239 , -0.7579657 ,  1.99775086]), array([-0.55403823,  0.82199184, -0.13398103,  1.20949258]), array([-0.49218933,  0.91081433,  0.73597288, -0.32030153]), array([-0.29362168,  0.75958902,  1.21152544, -1.15984968]), array([-0.00283143,  0.40409859,  1.63698883, -2.31393249]), array([ 0.33040959, -0.11429168,  1.60900133, -2.71033821]), array([ 0.58057182, -0.54911047,  0.83871716, -1.54659023]), array([ 0.67785985, -0.77854932,  0.11636301, -0.71858287]), array([ 0.60221093, -0.76891109, -0.85948861,  0.81312561]), array([ 0.36916884, -0.52359588, -1.42694954,  1.59221376]), array([ 0.0298536 , -0.0972408 , -1.88800066,  2.5476114 ]), array([-0.32064774,  0.35878596, -1.53115643,  1.8671078 ]), array([-0.58047394,  0.67394426, -1.01511311,  1.21521919]), array([-0.68827248,  0.76706947, -0.04711342, -0.2903242 ]), array([-0.59804575,  0.55903455,  0.93686624, -1.77241678]), array([-0.32660438,  0.07737809,  1.71571916, -2.93662542]), array([ 0.02504663, -0.47764301,  1.71019468, -2.44488272]), array([ 0.35006477, -0.91005053,  1.47206763, -1.77857192]), array([ 0.5918488 , -1.16426295,  0.90531366, -0.7341114 ]), array([ 0.70007829, -1.1988848 ,  0.15883606,  0.38957219]), array([ 0.65220855, -1.009555  , -0.63312249,  1.49466502]), array([ 0.45379361, -0.60933072, -1.31598258,  2.45870344]), array([ 1.23083995e-01,  2.99678791e-03, -1.90522181e+00,  3.50439057e+00]), array([-0.23644371,  0.63446648, -1.59719929,  2.63521525]), array([-0.51258746,  1.07561634, -1.11485922,  1.71101948]), array([-0.6483764 ,  1.2521287 , -0.22708632,  0.05426094]), array([-0.59984502,  1.09703379,  0.71254194, -1.60766009]), array([-0.36733011,  0.60989071,  1.58293319, -3.22865278]), array([-0.0198321 , -0.07989726,  1.78635748, -3.46187985]), array([ 0.32714773, -0.75021455,  1.58715394, -3.05648109]), array([ 0.58749647, -1.25646567,  0.97701768, -1.95828784]), array([ 0.7086426 , -1.52758117,  0.22348887, -0.7510771 ]), array([ 0.67618143, -1.55722704, -0.54000164,  0.45342344]), array([ 0.48118422, -1.29509777, -1.3882316 ,  2.17386079]), array([ 0.1542685 , -0.74800937, -1.82794413,  3.22955123]), array([-0.24363461,  0.00766025, -2.04178531,  4.11063409]), array([-0.58317962,  0.72068533, -1.26528327,  2.85120759]), array([-0.732835  ,  1.12230918, -0.22024311,  1.15457375]), array([-0.67300305,  1.1831618 ,  0.80307617, -0.54557227]), array([-0.44265372,  0.96138966,  1.46290881, -1.65158547]), array([-0.10848935,  0.54185032,  1.81184906, -2.45301697]), array([ 0.24799389,  0.03672657,  1.66191429, -2.43374984]), array([ 0.52141151, -0.36834984,  1.00936403, -1.51037562]), array([ 0.66032359, -0.60806364,  0.35249687, -0.84563748]), array([ 0.63261513, -0.63337324, -0.62417772,  0.59328653]), array([ 0.44356936, -0.44178622, -1.23075893,  1.28368537]), array([ 0.16074011, -0.14622054, -1.53387227,  1.58034742]), array([-0.14038898,  0.14545833, -1.40603227,  1.23050374]), array([-0.40153047,  0.37687145, -1.14782399,  1.00665   ]), array([-0.58013246,  0.52427727, -0.60460963,  0.43212332]), array([-0.63464498,  0.5421699 ,  0.06777785, -0.25683382]), array([-0.52882216,  0.35826738,  0.97113146, -1.55468031]), array([-0.28845981,  0.01325595,  1.37599183, -1.80174616]), array([-0.00546246, -0.31718617,  1.38672182, -1.39586378]), array([ 0.2658565 , -0.57341535,  1.26558264, -1.08349257]), array([ 0.45442429, -0.66146834,  0.58339149,  0.22801596]), array([ 0.51455871, -0.54457159,  0.01008753,  0.92834899]), array([ 0.43416631, -0.23384937, -0.7933758 ,  2.12883278]), array([ 0.21505608,  0.26993792, -1.33148023,  2.77451831]), array([-0.06692344,  0.81252463, -1.41786331,  2.51624637]), array([-0.32858446,  1.23651327, -1.15451941,  1.66493663]), array([-0.49486793,  1.41297557, -0.48322794,  0.09233619]), array([-0.51296152,  1.27037446,  0.31820176, -1.5273664 ]), array([-0.36403409,  0.79841885,  1.16412801, -3.18260614]), array([-0.08907126,  0.09241473,  1.49510934, -3.69832162]), array([ 0.21388883, -0.65418349,  1.42689731, -3.54887483]), array([ 0.44980034, -1.26631424,  0.89251976, -2.50735489]), array([ 0.54633967, -1.59947118,  0.07954009, -0.84053729]), array([ 0.48623097, -1.6073156 , -0.66468847,  0.75568543]), array([ 0.28815559, -1.29773758, -1.29543911,  2.33949024]), array([ 2.76246475e-05, -7.35380636e-01, -1.53816961e+00,  3.21041134e+00]), array([-0.2984104 , -0.06796958, -1.35610813,  3.27976989]), array([-0.50504998,  0.49954787, -0.64714745,  2.26434891]), array([-0.56748033,  0.87133341,  0.04010847,  1.40438948]), array([-0.48924423,  1.0507656 ,  0.72484781,  0.38175518]), array([-0.26928757,  0.96858663,  1.42828585, -1.18038667]), array([ 0.06015201,  0.59582509,  1.80374552, -2.4707841 ]), array([ 0.42157391,  0.03038091,  1.72253519, -3.01765649]), array([ 0.71183906, -0.53849413,  1.10667906, -2.53267376]), array([ 0.82123254, -0.88654582, -0.02439309, -0.92659634]), array([ 0.72608844, -0.96515163, -0.91315619,  0.1507867 ]), array([ 0.46731372, -0.8256879 , -1.6306137 ,  1.22481891]), array([ 0.07430265, -0.4312519 , -2.22179693,  2.62626975]), array([-0.35411872,  0.09022941, -1.95470194,  2.39654934]), array([-0.69563492,  0.5290857 , -1.38826536,  1.87780713]), array([-0.8892093 ,  0.81449054, -0.51884381,  0.94698219]), array([-0.89749595,  0.902716  ,  0.43725452, -0.07198268]), array([-0.69559062,  0.72213337,  1.556736  , -1.73296487]), array([-0.29285244,  0.2225355 ,  2.39334788, -3.15316416]), array([ 0.21420896, -0.45291111,  2.54167923, -3.34152156]), array([ 0.67413173, -1.02450016,  1.97258787, -2.25921563]), array([ 0.98045843, -1.34174541,  1.05465932, -0.91724546]), array([ 1.08688658e+00, -1.39779760e+00, -1.11939604e-03,  3.44274797e-01]), array([ 0.95974711, -1.15095884, -1.26642737,  2.14370568]), array([ 0.60926803, -0.59292951, -2.19027788,  3.39024019]), array([ 0.11952124,  0.1462485 , -2.57791222,  3.75042338]), array([-0.38940102,  0.85694664, -2.38930179,  3.13219601]), array([-0.80090102,  1.35000139, -1.66804787,  1.7626339 ]), array([-1.0400806 ,  1.56383005, -0.69657018,  0.3926776 ]), array([-1.07308046,  1.51300616,  0.37154725, -0.89543201]), array([-0.87383565,  1.14986065,  1.61377194, -2.76645667]), array([-0.43586238,  0.3986219 ,  2.70437019, -4.66781874]), array([ 0.1246717 , -0.53624923,  2.72835694, -4.31701559]), array([ 0.62457772, -1.28249471,  2.18581489, -3.02302051]), array([ 0.95957201, -1.68682115,  1.13354702, -1.05295431]), array([ 1.0850024 , -1.76188946,  0.10581544,  0.28979979]), array([ 0.98280577, -1.52325186, -1.12748222,  2.11771541]), array([ 0.63650918, -0.89882376, -2.31753862,  4.15608486]), array([ 0.106704  ,  0.04127943, -2.83007508,  4.94449159]), array([-0.44435251,  0.98159689, -2.53285125,  4.16220127]), array([-0.87290301,  1.65777691, -1.70951541,  2.59312281]), array([-1.10035528,  1.98415759, -0.54968365,  0.70714949]), array([-1.08921511,  1.9473326 ,  0.66136892, -1.07795048]), array([-0.83872788,  1.54374145,  1.83079188, -3.00126475]), array([-0.36366723,  0.72572637,  2.88242714, -5.17392049]), array([ 0.2641935 , -0.43202306,  3.17049513, -5.91313981]), array([ 0.7989747 , -1.40462576,  2.10827008, -3.72195837]), array([ 1.11724188, -1.9885037 ,  1.05532343, -2.15734842]), array([ 1.20242339, -2.23698034, -0.20176662, -0.34724204]), array([ 1.04033075, -2.12716277, -1.39961555,  1.46228496]), array([ 0.65466243, -1.63864639, -2.4221078 ,  3.47146808]), array([ 0.08522293, -0.71942041, -3.22188603,  5.68616431]), array([-0.57354962,  0.5102354 , -3.12322362,  6.07149704]), array([-1.08467499,  1.5471734 , -1.92305688,  4.23083151]), array([-1.33811815,  2.22745841, -0.61165886,  2.6295464 ]), array([-1.33210008,  2.61048653,  0.65820947,  1.20901365]), array([-1.0828675 ,  2.7113084 ,  1.80389689, -0.1981535 ]), array([-0.63018364,  2.53485446,  2.6469774 , -1.54927618]), array([-0.0539396 ,  2.06072462,  3.00012549, -3.16146834]), array([ 0.53027831,  1.28848365,  2.7842231 , -4.49833063]), array([ 1.04318492,  0.30387973,  2.27720295, -5.16187915]), array([ 1.36947985, -0.6051369 ,  0.89352123, -3.7511142 ]), array([ 1.40304638, -1.2287178 , -0.59370058, -2.4214479 ]), array([ 1.11080894, -1.4946626 , -2.28959529, -0.17276499]), array([ 0.5176027 , -1.2712983 , -3.53709379,  2.43734444]), array([-0.25367415, -0.53844292, -4.03351839,  4.68712654]), array([-0.99539273,  0.37097736, -3.20926625,  3.99780079]), array([-1.52224971,  1.04222557, -2.02573987,  2.69087279]), array([-1.80509072,  1.46990204, -0.80741885,  1.64518072]), array([-1.82843338,  1.66377153,  0.57297461,  0.29504938]), array([-1.57405737,  1.57092268,  1.97582252, -1.30606893]), array([-1.05669698,  1.14944023,  3.17932973, -3.00337132]), array([-0.32251449,  0.3594482 ,  4.04786957, -4.72297371]), array([ 0.48000796, -0.56119971,  3.76037957, -4.01149464]), array([ 1.1205557 , -1.13571503,  2.56731429, -1.69840184]), array([ 1.49062657, -1.26715808,  1.11454011,  0.29996105]), array([ 1.57485695, -1.07010213, -0.26800183,  1.63339832]), array([ 1.37345328, -0.58438865, -1.74484357,  3.24897306]), array([ 0.88587355,  0.22184586, -3.05432067,  4.64665728]), array([ 0.20426421,  1.14274231, -3.62856604,  4.23311727]), array([-0.51873993,  1.82407755, -3.48235878,  2.46886248]), array([-1.13785635,  2.11729437, -2.59961741,  0.48282452]), array([-1.51087485,  1.99255841, -1.07449126, -1.67700098]), array([-1.57215177,  1.51055251,  0.46317613, -3.11270857]), array([-1.30736014,  0.68928318,  2.18023389, -5.14517337]), array([-0.72848854, -0.5071273 ,  3.4306018 , -6.42849387]), array([-0.02954232, -1.64220247,  3.48669531, -4.73913809]), array([ 0.65852048, -2.43341002,  3.29110367, -3.16723713]), array([ 1.22736222, -2.87796794,  2.30937565, -1.30743958]), array([ 1.56306512, -2.96198403,  1.02858955,  0.45987983]), array([ 1.6414336 , -2.71616719, -0.25412176,  1.99434293]), array([ 1.44924608, -2.13985741, -1.68662858,  3.81796339]), array([ 0.95753502, -1.14419936, -3.25866184,  6.30434034]), array([ 0.19069384,  0.30644691, -4.13211676,  7.58626575]), array([-0.59063055,  1.64882309, -3.54422234,  5.55360437]), array([-1.21295398,  2.55414517, -2.63555765,  3.61398734]), array([-1.62758675,  3.12851004, -1.48949755,  2.17665352]), array([-1.79687514, -2.89078177, -0.20935865,  0.4634606 ]), array([-1.71804942, -2.95021163,  1.00187948, -1.05678597]), array([-1.38784561,  2.95012011,  2.29525291, -2.7848522 ]), array([-0.81255995,  2.20039239,  3.40121961, -4.8113725 ]), array([-0.06332719,  1.01865017,  4.05460391, -7.05861491]), array([ 0.77231769, -0.55091738,  3.96618454, -7.83757028]), array([ 1.39302423, -1.82497059,  2.22913011, -4.97175996]), array([ 1.69329681, -2.65304398,  0.80010699, -3.3971761 ]), array([ 1.71464777,  3.12405392, -0.55593232, -1.675045  ]), array([ 1.48175773,  2.93934697, -1.77192455, -0.18389447]), array([ 1.01353463,  3.01980495, -2.88487448,  0.94275971])]</t>
+  </si>
+  <si>
+    <t>['[0,1,1]', '[2,2,2]', '[2,1,0]', '[0,0,0]', '[2,0,1]', '[0,2,1]', '[1,2,0]', '[1,1,2]', '[1,1,1]', '[1,0,2]']</t>
+  </si>
+  <si>
+    <t>[1, 2, 4, 5, 6, 7, 13, 14, 15, 16, 17, 18, 20, 21, 22, 23, 26, 30, 34, 38, 39, 40, 41, 42, 43, 46, 49, 50, 51, 52, 53, 54, 55, 57, 60, 61, 64, 65, 66, 67, 68, 69, 72, 73, 74, 75, 76, 77, 80, 81, 82, 83, 85, 87, 88, 89, 90, 93, 94, 95, 98, 100, 101, 102, 103, 106, 107, 108, 110, 111, 113, 115, 117, 118, 119, 122, 123, 126, 127, 128, 129, 131, 133, 134, 139, 142, 143, 144, 145, 147, 151, 153, 154, 157, 158, 163, 164, 165, 166, 167, 169, 173, 174, 176, 177, 178, 179, 180, 181, 182, 183, 184, 188, 190, 191, 193, 195, 198, 199]</t>
+  </si>
+  <si>
+    <t>[0, 2, 0, 0, 2, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 0, 0, 2, 2, 2, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 0, 0, 2, 2, 2, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 2, 2, 2, 0, 0, 0, 2, 2, 0, 0, 0, 2, 0, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0]</t>
+  </si>
+  <si>
+    <t>['[-0.03763371 -0.01533471  0.06554052 -0.01816017]', '[-0.03406929  0.01398622 -0.02953871  0.30651903]', '[-0.02168374  0.03409236  0.1512214  -0.10649158]', '[ 0.02369474 -0.02529386  0.2912986  -0.46969041]', '[ 0.06234371 -0.07501275  0.08617182 -0.01368346]', '[ 0.08315347 -0.09791055  0.11692115 -0.20796639]', '[ 0.08020517 -0.08541727 -0.14509226  0.32970125]', '[ 0.05475411 -0.0408008  -0.10294581  0.10501779]', '[ 0.01449316  0.02233479 -0.28927767  0.50874422]', '[-0.05487888  0.15185714 -0.38598361  0.75260807]', '[-0.13151596  0.30774377 -0.36003007  0.76779475]', '[-0.19114455  0.44419858 -0.22099032  0.56691754]', '[-0.21526437  0.52504421 -0.01414536  0.22715205]', '[-0.19624212  0.53230986  0.20037684 -0.15248762]', '[-0.13856969  0.46793798  0.36335797 -0.47364979]', '[-0.05765003  0.35281933  0.42663124 -0.64732946]', '[ 0.02361446  0.22294473  0.36576462 -0.61687994]', '[ 0.08100934  0.11949787  0.19346517 -0.39089043]', '[ 0.09673497  0.07469937 -0.04051456 -0.04738656]', '[ 0.06529448  0.10077525 -0.26640357  0.29816719]', '[ 0.02174139  0.11805472 -0.15992568 -0.13463117]', '[ 0.00373492  0.04659715 -0.01879236 -0.57020119]', '[-0.01343128 -0.03376743 -0.15181649 -0.22243195]', '[-0.05508596 -0.04110871 -0.25629302  0.14345238]', '[-0.11137827  0.01841433 -0.29330998  0.43262042]', '[-0.16648497  0.12218393 -0.24336812  0.5786436 ]', '[-0.17688994  0.17056828  0.14213579 -0.10321362]', '[-0.11208787  0.08377522  0.49005844 -0.74011237]', '[ 0.00932659 -0.10918538  0.69286939 -1.13569258]', '[ 0.15044987 -0.34486996  0.68217902 -1.15775539]', '[ 0.2430498  -0.48264441  0.22456727 -0.19160053]', '[ 0.23640195 -0.41727039 -0.2891476   0.83621406]', '[ 0.1326104  -0.15962309 -0.72203482  1.68609983]', '[-0.03605212  0.22428323 -0.91439343  2.05194947]', '[-0.1862075   0.55212426 -0.55244029  1.16045202]', '[-0.27212815  0.73592922 -0.28845374  0.64520891]', '[-0.29681783  0.80189765  0.04590269  0.00593279]', '[-0.23091786  0.67648442  0.60236024 -1.24512251]', '[-0.08959853  0.38335365  0.77664197 -1.62360097]', '[ 0.06302085  0.05887253  0.70682565 -1.53768717]', '[ 0.17668615 -0.19923704  0.39879561 -0.98134896]', '[ 0.21384752 -0.31592643 -0.0363296  -0.164071  ]', '[ 0.18839874 -0.33059151 -0.2133716   0.01606951]', '[ 0.13194109 -0.31208056 -0.33929525  0.15776596]', '[ 0.03254011 -0.20601665 -0.63181305  0.87124589]', '[-0.10855632  0.01708382 -0.74349148  1.2984699 ]', '[-0.22268677  0.21673721 -0.36968422  0.64838071]', '[-0.27518616  0.3314042  -0.14187202  0.47249182]', '[-0.27604484  0.39791974  0.13496786  0.18238315]', '[-0.22287951  0.40330373  0.38619664 -0.1222587 ]', '[-0.127967    0.35468656  0.54256554 -0.34258431]', '[-0.01549536  0.27734425  0.55708803 -0.40052093]', '[ 0.0846301   0.2073117   0.42175387 -0.27178474]', '[ 0.14547563  0.17817331  0.17371894 -0.00505677]', '[ 0.15117333  0.2078243  -0.1166798   0.29702965]', '[ 0.12759754  0.22364033 -0.11393935 -0.14491404]', '[ 0.10733917  0.14996377 -0.08616047 -0.58358686]', '[ 0.06679144  0.06518941 -0.31375354 -0.25608039]', '[-0.01376899  0.04730064 -0.47592357  0.06748539]', '[-0.11558336  0.08523573 -0.5203374   0.2893527 ]', '[-0.18614684  0.08405342 -0.17161474 -0.31057516]', '[-0.20866362  0.03164677 -0.05092505 -0.20762666]', '[-0.17968922 -0.06533234  0.33135983 -0.740314  ]', '[-0.08344532 -0.24983686  0.60526858 -1.05631854]', '[ 0.02400808 -0.39827254  0.4450017  -0.39057494]', '[ 0.08651432 -0.39602898  0.16689486  0.42207173]', '[ 0.11409855 -0.29879214  0.10617643  0.53847807]', '[ 0.12860637 -0.18670005  0.03981207  0.56504664]', '[ 0.13097199 -0.0803708  -0.01290662  0.4797865 ]', '[ 0.1249936  -0.00182054 -0.0431256   0.29123404]', '[ 0.08867151  0.10003875 -0.30912352  0.70337618]', '[ 0.00830054  0.26555686 -0.47268468  0.90973038]', '[-0.06457305  0.3783891  -0.23967901  0.19233869]', '[-0.08322564  0.33728544  0.05644646 -0.60029584]', '[-0.06977596  0.21336203  0.07146777 -0.6159098 ]', '[-0.05748547  0.10051041  0.04518916 -0.4910084 ]', '[-0.05382222  0.0245961  -0.01169596 -0.2544975 ]', '[-0.06266549  0.00221034 -0.07552165  0.03287217]', '[-0.08272294  0.03637665 -0.1198227   0.29957252]', '[-0.1078512   0.1163352  -0.12373807  0.48208978]', '[-0.10254922  0.1526298   0.17620262 -0.12350564]', '[-0.06690665  0.13898429  0.17265896 -0.00529455]', '[-0.03633798  0.15276324  0.12739474  0.14518847]', '[-0.01767076  0.19664551  0.05701914  0.28873288]', '[-0.01373302  0.26497852 -0.01624319  0.3834572 ]', '[ 0.00297107  0.27724028  0.17963631 -0.25929735]', '[ 0.05475413  0.16655685  0.32497328 -0.82200974]', '[ 0.09931224  0.03190881  0.10738795 -0.49430596]', '[ 0.09456282 -0.022693   -0.15528948 -0.04364382]', '[ 0.0660997  -0.05535088 -0.12475814 -0.28135734]', '[ 0.01950147 -0.06435112 -0.33170451  0.18517283]', '[-0.06067467  0.01203031 -0.45123355  0.55263803]', '[-0.15213452  0.14315933 -0.44066911  0.72153153]', '[-0.20159435  0.21706636 -0.04275564 -0.00026383]', '[-0.19476177  0.21051407  0.10938411 -0.06297999]', '[-0.15972858  0.19397308  0.2333991  -0.09447461]', '[-0.07906478  0.10856252  0.55427052 -0.73299233]', '[ 0.05114369 -0.0822546   0.71500391 -1.12056135]', '[ 0.16580694 -0.2462081   0.40458582 -0.47579796]', '[ 0.23149564 -0.32928001  0.23712745 -0.33232213]', '[ 0.23022435 -0.30501519 -0.24871558  0.57049542]', '[ 0.16304453 -0.17834945 -0.40571713  0.66489197]', '[ 0.0762591  -0.05332184 -0.44064986  0.55037408]', '[-0.00449991  0.02834127 -0.3481691   0.2398771 ]', '[-0.08311866  0.10327867 -0.4195856   0.48397862]', '[-0.16417184  0.20978194 -0.37132394  0.55038471]', '[-0.19805947  0.24360902  0.03946446 -0.22106913]', '[-0.17563682  0.19248285  0.17859335 -0.27810849]', '[-0.13020613  0.1383304   0.26488026 -0.24734889]', '[-0.04818225  0.0318112   0.5353029  -0.78670812]', '[ 0.04660899 -0.08999604  0.38983787 -0.39599305]', '[ 0.10030261 -0.11612036  0.13580825  0.14656917]', '[ 0.09895402 -0.03155019 -0.14611397  0.6838951 ]', '[ 0.07249739  0.07755695 -0.10978274  0.38457286]', '[ 0.031377    0.18392292 -0.28938956  0.65364553]', '[-0.01066795  0.25842763 -0.12112045  0.07404205]', '[-0.04102713  0.27871417 -0.17563646  0.12055601]', '[-0.05161573  0.2351928   0.07089013 -0.55040367]', '[-0.04117753  0.1344419   0.028128   -0.43809073]', '[-0.04204566  0.06659143 -0.03877316 -0.22886823]', '[-0.03016422 -0.0228507   0.15208303 -0.6477503 ]', '[ 0.01454199 -0.18138256  0.28027326 -0.9021175 ]', '[ 0.04884659 -0.29978487  0.05372178 -0.25951644]', '[ 0.03475193 -0.28142608 -0.19110773  0.43766823]', '[-0.02381352 -0.13219693 -0.37882275  1.02165073]', '[-0.10804918  0.10845588 -0.43785054  1.32839339]', '[-0.16166111  0.30640477 -0.08293491  0.61261689]', '[-0.13892644  0.34522949  0.30551395 -0.22550094]', '[-0.07076147  0.28969587  0.36076795 -0.31038922]', '[-0.00130494  0.22982701  0.31795796 -0.26739579]', '[ 0.07677064  0.12247852  0.44395039 -0.77620752]', '[ 0.14063978  0.00408282  0.17837079 -0.37767515]', '[ 0.17067749 -0.08949736  0.11299576 -0.53734509]', '[ 0.15614931 -0.13354393 -0.25608589  0.10117657]', '[ 0.09902638 -0.12175541 -0.30334882  0.00621426]', '[ 0.01336543 -0.06649735 -0.53390713  0.52331934]', '[-0.10444232  0.07352358 -0.61569276  0.83360284]', '[-0.22056965  0.24714443 -0.51686254  0.85497938]', '[-0.30069223  0.39764521 -0.26479153  0.61536457]', '[-0.29562651  0.41663054  0.31391808 -0.42619635]', '[-0.18036679  0.23437525  0.81240487 -1.35468531]', '[ 0.01336731 -0.09788123  1.07393412 -1.87593471]', '[ 0.19976029 -0.40569271  0.74531984 -1.1255078 ]', '[ 0.29811513 -0.52747097  0.21864148 -0.06735353]', '[ 0.30872866 -0.495406   -0.11364591  0.38416567]', '[ 0.25499187 -0.37926087 -0.41038334  0.75278164]', '[ 0.12651198 -0.14054324 -0.84299359  1.57873696]', '[-0.03789811  0.15095317 -0.75773254  1.25725512]', '[-0.18694157  0.40234355 -0.6948861   1.19052415]', '[-0.30202644  0.60356402 -0.42984013  0.77858654]', '[-0.35123707  0.70155404 -0.05241604  0.18523763]', '[-0.32205347  0.6754826   0.33808745 -0.43949648]', '[-0.19684929  0.46810226  0.88963843 -1.59919552]', '[-0.00797283  0.1296963   0.94971602 -1.69531561]', '[ 0.16213792 -0.17154559  0.70680019 -1.23583942]', '[ 0.28618425 -0.4062553   0.50220949 -1.05443061]', '[ 0.35279964 -0.5745569   0.14815307 -0.59734244]', '[ 0.31794278 -0.57323    -0.48902227  0.6059197 ]', '[ 0.19009269 -0.40721243 -0.76092768  1.01346924]', '[ 0.00182637 -0.12191351 -1.07661676  1.76503244]', '[-0.21796094  0.25863899 -1.06226279  1.93240235]', '[-0.40022364  0.6093772  -0.71636875  1.49707223]', '[-0.49169789  0.83565986 -0.18103517  0.73517151]', '[-0.4475589   0.83678355  0.61283651 -0.72039906]', '[-0.27845168  0.61667229  1.04491274 -1.43978134]', '[-0.04767068  0.28678999  1.20856714 -1.77178659]', '[ 0.18021928 -0.04974772  1.01214846 -1.49272089]', '[ 0.33653266 -0.27519136  0.5149303  -0.70385041]', '[ 0.40280684 -0.3846477   0.13285609 -0.36634729]', '[ 0.38683034 -0.41586118 -0.29015805  0.0569028 ]', '[ 0.26546143 -0.29798617 -0.89790559  1.09110561]', '[ 0.04374751 -0.00245406 -1.26557614  1.77802416]', '[-0.21462743  0.3686741  -1.25257094  1.82093916]', '[-0.40787355  0.62099571 -0.64206014  0.65288244]', '[-0.46169882  0.62036582  0.11376253 -0.66232318]', '[-0.36340456  0.36119899  0.84925243 -1.89048521]', '[-0.16474788 -0.03675556  1.08245359 -1.98475754]', '[ 0.04575222 -0.38801201  0.97014496 -1.43467465]', '[ 0.20530908 -0.58170443  0.59223921 -0.45784336]', '[ 0.27259478 -0.5609095   0.066383    0.67176645]', '[ 0.25586097 -0.38370436 -0.22594584  1.07114999]', '[ 0.18838744 -0.14896065 -0.42712788  1.22572477]', '[ 0.09558978  0.08351773 -0.47403613  1.04332504]', '[ 0.00927772  0.24762848 -0.36745893  0.55809674]', '[-0.04423661  0.29504459 -0.15600514 -0.09861504]', '[-0.05050411  0.20718436  0.09267364 -0.76726545]', '[-1.02164303e-02 -8.92084159e-04  2.94957544e-01 -1.27079706e+00]', '[ 0.05866648 -0.27855701  0.36876266 -1.44357372]', '[ 0.1017143  -0.48696724  0.05112975 -0.60790966]', '[ 0.10310341 -0.58071766 -0.03859837 -0.3172804 ]', '[ 0.08669448 -0.61117559 -0.12205169  0.01337796]', '[ 0.05640425 -0.57713196 -0.17407556  0.3177277 ]', '[-0.00485483 -0.42417963 -0.42587965  1.18596459]', '[-0.0797806  -0.18793414 -0.30081602  1.12460016]', '[-0.14339836  0.07391565 -0.31296195  1.43712113]', '[-0.16902427  0.29365927  0.06779774  0.72113855]', '[-0.14171362  0.42108726  0.20342405  0.53639859]', '[-0.06479414  0.43797622  0.54872071 -0.3568267 ]', '[ 0.0424496   0.3557501   0.49960539 -0.43484694]', '[ 0.12571068  0.27665003  0.31393445 -0.32935871]']</t>
+  </si>
+  <si>
+    <t>[array([-0.03763371, -0.01533471,  0.06554052, -0.01816017], dtype=float32), array([-0.03406929,  0.01398622, -0.02953871,  0.30651903]), array([-0.02168374,  0.03409236,  0.1512214 , -0.10649158]), array([ 0.02369474, -0.02529386,  0.2912986 , -0.46969041]), array([ 0.06234371, -0.07501275,  0.08617182, -0.01368346]), array([ 0.08315347, -0.09791055,  0.11692115, -0.20796639]), array([ 0.08020517, -0.08541727, -0.14509226,  0.32970125]), array([ 0.05475411, -0.0408008 , -0.10294581,  0.10501779]), array([ 0.01449316,  0.02233479, -0.28927767,  0.50874422]), array([-0.05487888,  0.15185714, -0.38598361,  0.75260807]), array([-0.13151596,  0.30774377, -0.36003007,  0.76779475]), array([-0.19114455,  0.44419858, -0.22099032,  0.56691754]), array([-0.21526437,  0.52504421, -0.01414536,  0.22715205]), array([-0.19624212,  0.53230986,  0.20037684, -0.15248762]), array([-0.13856969,  0.46793798,  0.36335797, -0.47364979]), array([-0.05765003,  0.35281933,  0.42663124, -0.64732946]), array([ 0.02361446,  0.22294473,  0.36576462, -0.61687994]), array([ 0.08100934,  0.11949787,  0.19346517, -0.39089043]), array([ 0.09673497,  0.07469937, -0.04051456, -0.04738656]), array([ 0.06529448,  0.10077525, -0.26640357,  0.29816719]), array([ 0.02174139,  0.11805472, -0.15992568, -0.13463117]), array([ 0.00373492,  0.04659715, -0.01879236, -0.57020119]), array([-0.01343128, -0.03376743, -0.15181649, -0.22243195]), array([-0.05508596, -0.04110871, -0.25629302,  0.14345238]), array([-0.11137827,  0.01841433, -0.29330998,  0.43262042]), array([-0.16648497,  0.12218393, -0.24336812,  0.5786436 ]), array([-0.17688994,  0.17056828,  0.14213579, -0.10321362]), array([-0.11208787,  0.08377522,  0.49005844, -0.74011237]), array([ 0.00932659, -0.10918538,  0.69286939, -1.13569258]), array([ 0.15044987, -0.34486996,  0.68217902, -1.15775539]), array([ 0.2430498 , -0.48264441,  0.22456727, -0.19160053]), array([ 0.23640195, -0.41727039, -0.2891476 ,  0.83621406]), array([ 0.1326104 , -0.15962309, -0.72203482,  1.68609983]), array([-0.03605212,  0.22428323, -0.91439343,  2.05194947]), array([-0.1862075 ,  0.55212426, -0.55244029,  1.16045202]), array([-0.27212815,  0.73592922, -0.28845374,  0.64520891]), array([-0.29681783,  0.80189765,  0.04590269,  0.00593279]), array([-0.23091786,  0.67648442,  0.60236024, -1.24512251]), array([-0.08959853,  0.38335365,  0.77664197, -1.62360097]), array([ 0.06302085,  0.05887253,  0.70682565, -1.53768717]), array([ 0.17668615, -0.19923704,  0.39879561, -0.98134896]), array([ 0.21384752, -0.31592643, -0.0363296 , -0.164071  ]), array([ 0.18839874, -0.33059151, -0.2133716 ,  0.01606951]), array([ 0.13194109, -0.31208056, -0.33929525,  0.15776596]), array([ 0.03254011, -0.20601665, -0.63181305,  0.87124589]), array([-0.10855632,  0.01708382, -0.74349148,  1.2984699 ]), array([-0.22268677,  0.21673721, -0.36968422,  0.64838071]), array([-0.27518616,  0.3314042 , -0.14187202,  0.47249182]), array([-0.27604484,  0.39791974,  0.13496786,  0.18238315]), array([-0.22287951,  0.40330373,  0.38619664, -0.1222587 ]), array([-0.127967  ,  0.35468656,  0.54256554, -0.34258431]), array([-0.01549536,  0.27734425,  0.55708803, -0.40052093]), array([ 0.0846301 ,  0.2073117 ,  0.42175387, -0.27178474]), array([ 0.14547563,  0.17817331,  0.17371894, -0.00505677]), array([ 0.15117333,  0.2078243 , -0.1166798 ,  0.29702965]), array([ 0.12759754,  0.22364033, -0.11393935, -0.14491404]), array([ 0.10733917,  0.14996377, -0.08616047, -0.58358686]), array([ 0.06679144,  0.06518941, -0.31375354, -0.25608039]), array([-0.01376899,  0.04730064, -0.47592357,  0.06748539]), array([-0.11558336,  0.08523573, -0.5203374 ,  0.2893527 ]), array([-0.18614684,  0.08405342, -0.17161474, -0.31057516]), array([-0.20866362,  0.03164677, -0.05092505, -0.20762666]), array([-0.17968922, -0.06533234,  0.33135983, -0.740314  ]), array([-0.08344532, -0.24983686,  0.60526858, -1.05631854]), array([ 0.02400808, -0.39827254,  0.4450017 , -0.39057494]), array([ 0.08651432, -0.39602898,  0.16689486,  0.42207173]), array([ 0.11409855, -0.29879214,  0.10617643,  0.53847807]), array([ 0.12860637, -0.18670005,  0.03981207,  0.56504664]), array([ 0.13097199, -0.0803708 , -0.01290662,  0.4797865 ]), array([ 0.1249936 , -0.00182054, -0.0431256 ,  0.29123404]), array([ 0.08867151,  0.10003875, -0.30912352,  0.70337618]), array([ 0.00830054,  0.26555686, -0.47268468,  0.90973038]), array([-0.06457305,  0.3783891 , -0.23967901,  0.19233869]), array([-0.08322564,  0.33728544,  0.05644646, -0.60029584]), array([-0.06977596,  0.21336203,  0.07146777, -0.6159098 ]), array([-0.05748547,  0.10051041,  0.04518916, -0.4910084 ]), array([-0.05382222,  0.0245961 , -0.01169596, -0.2544975 ]), array([-0.06266549,  0.00221034, -0.07552165,  0.03287217]), array([-0.08272294,  0.03637665, -0.1198227 ,  0.29957252]), array([-0.1078512 ,  0.1163352 , -0.12373807,  0.48208978]), array([-0.10254922,  0.1526298 ,  0.17620262, -0.12350564]), array([-0.06690665,  0.13898429,  0.17265896, -0.00529455]), array([-0.03633798,  0.15276324,  0.12739474,  0.14518847]), array([-0.01767076,  0.19664551,  0.05701914,  0.28873288]), array([-0.01373302,  0.26497852, -0.01624319,  0.3834572 ]), array([ 0.00297107,  0.27724028,  0.17963631, -0.25929735]), array([ 0.05475413,  0.16655685,  0.32497328, -0.82200974]), array([ 0.09931224,  0.03190881,  0.10738795, -0.49430596]), array([ 0.09456282, -0.022693  , -0.15528948, -0.04364382]), array([ 0.0660997 , -0.05535088, -0.12475814, -0.28135734]), array([ 0.01950147, -0.06435112, -0.33170451,  0.18517283]), array([-0.06067467,  0.01203031, -0.45123355,  0.55263803]), array([-0.15213452,  0.14315933, -0.44066911,  0.72153153]), array([-0.20159435,  0.21706636, -0.04275564, -0.00026383]), array([-0.19476177,  0.21051407,  0.10938411, -0.06297999]), array([-0.15972858,  0.19397308,  0.2333991 , -0.09447461]), array([-0.07906478,  0.10856252,  0.55427052, -0.73299233]), array([ 0.05114369, -0.0822546 ,  0.71500391, -1.12056135]), array([ 0.16580694, -0.2462081 ,  0.40458582, -0.47579796]), array([ 0.23149564, -0.32928001,  0.23712745, -0.33232213]), array([ 0.23022435, -0.30501519, -0.24871558,  0.57049542]), array([ 0.16304453, -0.17834945, -0.40571713,  0.66489197]), array([ 0.0762591 , -0.05332184, -0.44064986,  0.55037408]), array([-0.00449991,  0.02834127, -0.3481691 ,  0.2398771 ]), array([-0.08311866,  0.10327867, -0.4195856 ,  0.48397862]), array([-0.16417184,  0.20978194, -0.37132394,  0.55038471]), array([-0.19805947,  0.24360902,  0.03946446, -0.22106913]), array([-0.17563682,  0.19248285,  0.17859335, -0.27810849]), array([-0.13020613,  0.1383304 ,  0.26488026, -0.24734889]), array([-0.04818225,  0.0318112 ,  0.5353029 , -0.78670812]), array([ 0.04660899, -0.08999604,  0.38983787, -0.39599305]), array([ 0.10030261, -0.11612036,  0.13580825,  0.14656917]), array([ 0.09895402, -0.03155019, -0.14611397,  0.6838951 ]), array([ 0.07249739,  0.07755695, -0.10978274,  0.38457286]), array([ 0.031377  ,  0.18392292, -0.28938956,  0.65364553]), array([-0.01066795,  0.25842763, -0.12112045,  0.07404205]), array([-0.04102713,  0.27871417, -0.17563646,  0.12055601]), array([-0.05161573,  0.2351928 ,  0.07089013, -0.55040367]), array([-0.04117753,  0.1344419 ,  0.028128  , -0.43809073]), array([-0.04204566,  0.06659143, -0.03877316, -0.22886823]), array([-0.03016422, -0.0228507 ,  0.15208303, -0.6477503 ]), array([ 0.01454199, -0.18138256,  0.28027326, -0.9021175 ]), array([ 0.04884659, -0.29978487,  0.05372178, -0.25951644]), array([ 0.03475193, -0.28142608, -0.19110773,  0.43766823]), array([-0.02381352, -0.13219693, -0.37882275,  1.02165073]), array([-0.10804918,  0.10845588, -0.43785054,  1.32839339]), array([-0.16166111,  0.30640477, -0.08293491,  0.61261689]), array([-0.13892644,  0.34522949,  0.30551395, -0.22550094]), array([-0.07076147,  0.28969587,  0.36076795, -0.31038922]), array([-0.00130494,  0.22982701,  0.31795796, -0.26739579]), array([ 0.07677064,  0.12247852,  0.44395039, -0.77620752]), array([ 0.14063978,  0.00408282,  0.17837079, -0.37767515]), array([ 0.17067749, -0.08949736,  0.11299576, -0.53734509]), array([ 0.15614931, -0.13354393, -0.25608589,  0.10117657]), array([ 0.09902638, -0.12175541, -0.30334882,  0.00621426]), array([ 0.01336543, -0.06649735, -0.53390713,  0.52331934]), array([-0.10444232,  0.07352358, -0.61569276,  0.83360284]), array([-0.22056965,  0.24714443, -0.51686254,  0.85497938]), array([-0.30069223,  0.39764521, -0.26479153,  0.61536457]), array([-0.29562651,  0.41663054,  0.31391808, -0.42619635]), array([-0.18036679,  0.23437525,  0.81240487, -1.35468531]), array([ 0.01336731, -0.09788123,  1.07393412, -1.87593471]), array([ 0.19976029, -0.40569271,  0.74531984, -1.1255078 ]), array([ 0.29811513, -0.52747097,  0.21864148, -0.06735353]), array([ 0.30872866, -0.495406  , -0.11364591,  0.38416567]), array([ 0.25499187, -0.37926087, -0.41038334,  0.75278164]), array([ 0.12651198, -0.14054324, -0.84299359,  1.57873696]), array([-0.03789811,  0.15095317, -0.75773254,  1.25725512]), array([-0.18694157,  0.40234355, -0.6948861 ,  1.19052415]), array([-0.30202644,  0.60356402, -0.42984013,  0.77858654]), array([-0.35123707,  0.70155404, -0.05241604,  0.18523763]), array([-0.32205347,  0.6754826 ,  0.33808745, -0.43949648]), array([-0.19684929,  0.46810226,  0.88963843, -1.59919552]), array([-0.00797283,  0.1296963 ,  0.94971602, -1.69531561]), array([ 0.16213792, -0.17154559,  0.70680019, -1.23583942]), array([ 0.28618425, -0.4062553 ,  0.50220949, -1.05443061]), array([ 0.35279964, -0.5745569 ,  0.14815307, -0.59734244]), array([ 0.31794278, -0.57323   , -0.48902227,  0.6059197 ]), array([ 0.19009269, -0.40721243, -0.76092768,  1.01346924]), array([ 0.00182637, -0.12191351, -1.07661676,  1.76503244]), array([-0.21796094,  0.25863899, -1.06226279,  1.93240235]), array([-0.40022364,  0.6093772 , -0.71636875,  1.49707223]), array([-0.49169789,  0.83565986, -0.18103517,  0.73517151]), array([-0.4475589 ,  0.83678355,  0.61283651, -0.72039906]), array([-0.27845168,  0.61667229,  1.04491274, -1.43978134]), array([-0.04767068,  0.28678999,  1.20856714, -1.77178659]), array([ 0.18021928, -0.04974772,  1.01214846, -1.49272089]), array([ 0.33653266, -0.27519136,  0.5149303 , -0.70385041]), array([ 0.40280684, -0.3846477 ,  0.13285609, -0.36634729]), array([ 0.38683034, -0.41586118, -0.29015805,  0.0569028 ]), array([ 0.26546143, -0.29798617, -0.89790559,  1.09110561]), array([ 0.04374751, -0.00245406, -1.26557614,  1.77802416]), array([-0.21462743,  0.3686741 , -1.25257094,  1.82093916]), array([-0.40787355,  0.62099571, -0.64206014,  0.65288244]), array([-0.46169882,  0.62036582,  0.11376253, -0.66232318]), array([-0.36340456,  0.36119899,  0.84925243, -1.89048521]), array([-0.16474788, -0.03675556,  1.08245359, -1.98475754]), array([ 0.04575222, -0.38801201,  0.97014496, -1.43467465]), array([ 0.20530908, -0.58170443,  0.59223921, -0.45784336]), array([ 0.27259478, -0.5609095 ,  0.066383  ,  0.67176645]), array([ 0.25586097, -0.38370436, -0.22594584,  1.07114999]), array([ 0.18838744, -0.14896065, -0.42712788,  1.22572477]), array([ 0.09558978,  0.08351773, -0.47403613,  1.04332504]), array([ 0.00927772,  0.24762848, -0.36745893,  0.55809674]), array([-0.04423661,  0.29504459, -0.15600514, -0.09861504]), array([-0.05050411,  0.20718436,  0.09267364, -0.76726545]), array([-1.02164303e-02, -8.92084159e-04,  2.94957544e-01, -1.27079706e+00]), array([ 0.05866648, -0.27855701,  0.36876266, -1.44357372]), array([ 0.1017143 , -0.48696724,  0.05112975, -0.60790966]), array([ 0.10310341, -0.58071766, -0.03859837, -0.3172804 ]), array([ 0.08669448, -0.61117559, -0.12205169,  0.01337796]), array([ 0.05640425, -0.57713196, -0.17407556,  0.3177277 ]), array([-0.00485483, -0.42417963, -0.42587965,  1.18596459]), array([-0.0797806 , -0.18793414, -0.30081602,  1.12460016]), array([-0.14339836,  0.07391565, -0.31296195,  1.43712113]), array([-0.16902427,  0.29365927,  0.06779774,  0.72113855]), array([-0.14171362,  0.42108726,  0.20342405,  0.53639859]), array([-0.06479414,  0.43797622,  0.54872071, -0.3568267 ]), array([ 0.0424496 ,  0.3557501 ,  0.49960539, -0.43484694]), array([ 0.12571068,  0.27665003,  0.31393445, -0.32935871])]</t>
+  </si>
+  <si>
+    <t>['[1,1,2]', '[2,0,1]', '[2,2,2]', '[1,1,1]', '[0,0,0]', '[2,1,0]', '[0,1,1]', '[0,2,1]', '[1,2,0]', '[1,0,2]']</t>
+  </si>
+  <si>
+    <t>[1, 2, 3, 6, 7, 8, 9, 10, 11, 12, 13, 15, 16, 17, 18, 19, 20, 21, 22, 23, 25, 26, 28, 30, 31, 32, 33, 34, 35, 36, 38, 40, 42, 43, 44, 45, 46, 48, 49, 51, 52, 53, 54, 55, 56, 57, 59, 60, 61, 62, 63, 64, 65, 66, 68, 69, 70, 71, 73, 75, 76, 77, 78, 79, 83, 84, 85, 87, 88, 89, 90, 92, 93, 94, 95, 96, 97, 98, 99, 100, 101, 102, 103, 105, 106, 107, 108, 109, 110, 112, 113, 115, 116, 117, 118, 121, 122, 123, 125, 126, 127, 128, 129, 130, 131, 132, 133, 134, 135, 136, 137, 138, 139, 140, 141, 142, 143, 144, 145, 146, 149, 150, 151, 152, 153, 154, 155, 156, 157, 158, 159, 160, 161, 163, 164, 166, 167, 169, 170, 173, 174, 175, 176, 177, 178, 180, 181, 182, 183, 184, 187, 188, 189, 191, 192, 193, 194, 195, 197, 198]</t>
+  </si>
+  <si>
+    <t>[0, 2, 0, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 2, 0, 2, 0, 2, 0, 2, 2, 0, 2, 2, 0, 0, 0, 2, 2, 0, 2, 2, 0, 0, 2, 2, 2, 2, 0, 2, 0, 0, 2, 2, 0, 0, 0, 0, 2, 0, 2, 0, 2, 0, 0, 2, 2, 2, 0, 2, 2, 2, 0, 0, 2, 2, 2, 0, 0, 2, 2, 2, 0, 2, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 0, 2, 0, 0, 0, 2, 2, 2, 2, 0, 2, 2, 0, 2, 0, 2, 2, 0, 2, 0, 0, 2, 0, 0, 2, 0, 0, 2, 0, 2, 2, 2, 2, 0, 0, 2, 2, 0, 0, 2, 0, 2, 0, 0, 2, 0, 0, 2, 0, 0, 2, 0, 2, 0, 2, 0, 2, 0, 2, 2, 2, 0, 0, 0, 0, 2, 0, 2, 0, 2, 2, 0, 2, 2, 2, 0, 2, 2, 0, 0, 0, 0, 2, 2, 2, 2, 0, 0, 0, 0, 2, 2, 0, 0, 0, 0, 2, 2, 2, 0, 0, 0, 0, 0, 2, 2, 0, 2, 2, 0, 2]</t>
+  </si>
+  <si>
+    <t>['[-0.03763371 -0.01533471  0.06554052 -0.01816017]', '[-0.03406929  0.01398622 -0.02953871  0.30651903]', '[-0.02168374  0.03409236  0.1512214  -0.10649158]', '[-0.00282652  0.04327343  0.03401407  0.19924661]', '[-0.00814034  0.11145621 -0.08365717  0.46948189]', '[-0.03365186  0.22334811 -0.16249273  0.62574953]', '[-0.04285076  0.2835192   0.07310173 -0.03359517]', '[-0.03176865  0.27882203  0.03536798 -0.01091686]', '[-0.02932458  0.27976972 -0.01134823  0.02054779]', '[-0.03608027  0.28663083 -0.05459109  0.04579883]', '[-0.0501551   0.29677884 -0.08297669  0.05176831]', '[-0.06777844  0.30558506 -0.08942408  0.03212042]', '[-0.08436899  0.30806041 -0.0730686  -0.01026882]', '[-0.09581655  0.30068774 -0.03933726 -0.06390967]', '[-0.07347318  0.21521875  0.25624669 -0.77411808]', '[-0.02549141  0.07242505  0.20913951 -0.62142584]', '[ 0.005005   -0.02174213  0.08680366 -0.29949166]', '[ 0.00699615 -0.04200657 -0.06766405  0.10014684]', '[ 0.0057884  -0.05241753  0.05530831 -0.2022683 ]', '[ 0.00121612 -0.05090957 -0.09981119  0.21591138]', '[-0.00547005 -0.03879613  0.03448463 -0.09752754]', '[-0.01229102 -0.01962781 -0.1005132   0.28445644]', '[-0.01680487  0.00123477  0.05670342 -0.07968184]', '[-0.01723611  0.01883435 -0.06018765  0.25219462]', '[-0.03925736  0.09784876 -0.15284015  0.52043503]', '[-0.04810444  0.14945678  0.06720622 -0.01353452]', '[-0.03987919  0.16168461  0.0138649   0.13478559]', '[-0.04244576  0.20167637 -0.03766341  0.25769045]', '[-0.02745532  0.19278766  0.18394505 -0.34225122]', '[ 0.02745265  0.07138497  0.3504006  -0.84280025]', '[ 0.07830451 -0.05964028  0.14388227 -0.43725698]', '[ 0.08149146 -0.09554643 -0.11332034  0.08403858]', '[ 0.06147297 -0.09697159 -0.08295858 -0.10090843]', '[ 0.04941064 -0.13554367 -0.03659042 -0.27971852]', '[ 0.02035788 -0.13715479 -0.24769427  0.2587894 ]', '[-0.0185623  -0.10697522 -0.1328243   0.03199534]', '[-0.03046514 -0.12657087  0.01537186 -0.22604563]', '[-0.01323273 -0.19406343  0.15112098 -0.43418513]', '[ 2.16344362e-04 -2.24462179e-01 -1.97646682e-02  1.36388564e-01]', '[-0.02062911 -0.14134474 -0.1822367   0.67798016]', '[-0.04165264 -0.033105   -0.02035014  0.38252035]', '[-0.05387789  0.07444784 -0.09572739  0.67198247]', '[-0.05015103  0.15660509  0.13416518  0.13717571]', '[-0.02844668  0.1973133   0.0798914   0.2660323 ]', '[ 0.0073629   0.19240938  0.27036143 -0.30810314]', '[ 0.04821631  0.14971785  0.12871898 -0.10528688]', '[ 0.05641385  0.15351306 -0.0480613   0.14350513]', '[ 0.03011995  0.20454807 -0.20774363  0.35356295]', '[ 0.0038217   0.21954728 -0.04970803 -0.20951367]', '[-0.01559179  0.19073805 -0.1412619  -0.07691308]', '[-0.02417625  0.11987612  0.05511404 -0.62104914]', '[-0.02240481  0.01991038 -0.04099207 -0.36098654]', '[-0.04089841 -0.01984411 -0.1412743  -0.03287604]', '[-0.05017263 -0.06307824  0.04874821 -0.39288613]', '[-0.04964863 -0.10247576 -0.0445339   0.00516335]', '[-0.04079197 -0.13004076  0.1301919  -0.27423497]', '[-0.0267818  -0.13845147  0.00703011  0.19323707]', '[-0.01125664 -0.1235447   0.1453659  -0.04398948]', '[ 0.02887994 -0.15361091  0.24676827 -0.24494018]', '[ 0.05639592 -0.14679317  0.02323185  0.31561532]', '[ 0.06489294 -0.09959999  0.06150652  0.14951446]', '[ 0.0804065  -0.0883744   0.09080158 -0.03669922]', '[ 0.09963978 -0.11265479  0.09683773 -0.1988487 ]', '[ 0.09060477 -0.09555016 -0.18450052  0.36500044]', '[ 0.05619341 -0.04236247 -0.15104827  0.15254933]', '[ 0.03308856 -0.03863092 -0.07535096 -0.11913768]', '[ 0.02700272 -0.0893307   0.013914   -0.37962725]', '[ 0.03740861 -0.18492786  0.08473625 -0.55775526]', '[ 0.03189263 -0.23573597 -0.13945514  0.05593224]', '[ 0.01026862 -0.23290407 -0.07238627 -0.03135546]', '[ 0.00407733 -0.24881733  0.01116323 -0.12592688]', '[ 0.01426195 -0.28144496  0.08758004 -0.19317591]', '[ 0.03721748 -0.32237225  0.13611635 -0.20570991]', '[ 0.0400804  -0.29209233 -0.10740364  0.50418501]', '[-0.0033212  -0.12781653 -0.31355086  1.10553754]', '[-0.05088216  0.06239806 -0.14595318  0.75566731]', '[-0.05724766  0.16187341  0.08604794  0.2221972 ]', '[-0.04368195  0.21747783  0.04872457  0.32618569]', '[-0.01160895  0.22066918  0.26505794 -0.28910685]', '[ 0.03107296  0.17695397  0.15187858 -0.13403674]', '[ 0.07264182  0.10268309  0.25321127 -0.58972643]', '[ 0.12680949 -0.04774379  0.27264711 -0.87993656]', '[ 0.17474255 -0.23321361  0.19057143 -0.93467239]', '[ 0.17152281 -0.33894949 -0.22335582 -0.10878821]', '[ 0.11478036 -0.34515576 -0.33271776  0.03931809]', '[ 0.04398779 -0.32778713 -0.36027616  0.12056204]', '[-0.04900172 -0.23575106 -0.54833765  0.77101189]', '[-0.13838645 -0.10455097 -0.32348978  0.50418026]', '[-0.1717028  -0.045523   -0.00152064  0.0713898 ]', '[-0.16524649 -0.00855417  0.06588049  0.29299227]', '[-1.19149541e-01 -1.34303737e-04  3.85679162e-01 -2.02474985e-01]', '[-0.01776908 -0.08191157  0.60468577 -0.58457113]', '[ 0.08479167 -0.14956897  0.39839988 -0.06548097]', '[ 0.13475422 -0.10215487  0.09283022  0.53839063]', '[ 0.14820469 -0.00894954  0.04218062  0.37931962]', '[ 0.15194776  0.04474809 -0.00387246  0.14920894]', '[ 0.1470812   0.04862963 -0.04372076 -0.11166848]', '[ 0.13491458  0.00102089 -0.07697001 -0.35807386]', '[ 0.0901097  -0.02200851 -0.36238654  0.1242428 ]', '[ 0.02270652 -0.02404969 -0.29822413 -0.15433615]', '[-0.0246614  -0.08534945 -0.16818062 -0.45468039]', '[-0.06940329 -0.13327542 -0.27118886 -0.02406635]', '[-0.10228018 -0.16647505 -0.05224672 -0.30702747]', '[-0.11644031 -0.1845648  -0.08668043  0.12627344]', '[-0.13528274 -0.11865686 -0.09622871  0.51915868]', '[-0.12567433 -0.05352839  0.19212587  0.1229898 ]', '[-8.77245909e-02 -2.86856104e-04  1.81452350e-01  4.05893942e-01]', '[-0.02849592  0.03684135  0.39971827 -0.03144634]', '[0.03901826 0.0610819  0.26279474 0.27955546]', '[0.07304059 0.14804982 0.07381343 0.57959697]', '[0.09507145 0.21778325 0.14330893 0.11089704]', '[ 0.12812185  0.19295211  0.17968739 -0.34968524]', '[ 0.13689546  0.15294854 -0.0946212  -0.04269484]', '[ 0.11810798  0.10697207 -0.09063051 -0.41250347]', '[ 0.1012111  -0.00773571 -0.07868424 -0.71721201]', '[ 0.05943336 -0.10213756 -0.33334528 -0.21736251]', '[-0.00082766 -0.16406618 -0.25939255 -0.39989391]', '[-0.06732464 -0.19173764 -0.39217197  0.11645654]', '[-0.12455704 -0.19231389 -0.16877669 -0.13109615]', '[-0.15856304 -0.17673541 -0.16381937  0.27862004]', '[-0.18684037 -0.0865212  -0.11093234  0.6045227 ]', '[-0.17315698 -0.01302887  0.24696997  0.12060771]', '[-0.11821077  0.03158297  0.2929629   0.32595506]', '[-0.05983122  0.11629767  0.28225192  0.51454403]', '[-0.00837145  0.23334601  0.22634923  0.64261071]', '[0.05459284 0.29980858 0.39084785 0.0231519 ]', '[0.11529916 0.31515154 0.20424257 0.13803244]', '[ 0.13308146  0.35628545 -0.02890918  0.26984455]', '[ 0.13037952  0.35268394  0.00236331 -0.3056332 ]', '[ 0.10775698  0.30449147 -0.22481849 -0.17322135]', '[ 0.07004314  0.21483674 -0.14606156 -0.71633164]', '[ 0.02390531  0.09344094 -0.31019123 -0.48351883]', '[-0.05042798  0.02466732 -0.42042877 -0.20351837]', '[-0.11145469 -0.0587631  -0.18080716 -0.62460859]', '[-0.14791145 -0.15022676 -0.17887377 -0.28086504]', '[-0.18059312 -0.16983998 -0.1415968   0.08217231]', '[-0.17563603 -0.18855993  0.18922494 -0.26480563]', '[-0.13488903 -0.20171743  0.2095596   0.14183551]', '[-0.09514354 -0.13064791  0.18150441  0.56382041]', '[-0.03747868 -0.04987902  0.38607869  0.23891353]', '[0.02714888 0.03478192 0.25030414 0.60200457]', '[0.0866758  0.11693842 0.33524494 0.2150276 ]', '[0.12983609 0.19046312 0.09037148 0.51389199]', '[0.14870843 0.24896785 0.09537609 0.06606211]', '[ 0.1402882   0.28521028 -0.17657512  0.28862009]', '[ 0.10761049  0.29091047 -0.14326277 -0.23780196]', '[ 0.05898426  0.25840663 -0.33368991 -0.0904923 ]', '[-0.02053236  0.25142577 -0.44528805  0.00877804]', '[-0.11173196  0.25602672 -0.44810838  0.02247984]', '[-0.16609464  0.18681106 -0.08647518 -0.71078578]', '[-0.17295583  0.04849614  0.01409213 -0.64854144]', '[-0.16253408 -0.06313321  0.08443438 -0.44702644]', '[-0.14164532 -0.12314402  0.11863617 -0.14015725]', '[-0.11735756 -0.11577061  0.11952163  0.21637792]', '[-0.06886487 -0.10632221  0.3555938  -0.11531686]', '[-0.00772679 -0.08734149  0.24400914  0.31105532]', '[ 0.05193699 -0.0515555   0.34163457  0.04991728]', '[0.09694763 0.00469317 0.10152452 0.50901412]', '[0.11869062 0.07768025 0.11367182 0.21198179]', '[ 0.14104536  0.08803938  0.10554153 -0.10636178]', '[ 0.13242667  0.10640997 -0.1890456   0.2849246 ]', '[ 0.09563781  0.12733784 -0.17085952 -0.08464048]', '[ 0.04030355  0.13977565 -0.37060607  0.19761166]', '[-0.01957558  0.13059331 -0.2163511  -0.29677189]', '[-0.06976258  0.09069831 -0.2766527  -0.10299021]', '[-0.12600313  0.08745724 -0.27454613  0.06257736]', '[-0.14844109  0.0429935   0.05292645 -0.50226499]', '[-0.13343343 -0.03735408  0.09162085 -0.28522375]', '[-0.08751451 -0.13447875  0.35483376 -0.66133584]', '[-0.02531694 -0.22001252  0.25253082 -0.17106739]', '[ 0.00887954 -0.19737305  0.08302991  0.39889523]', '[ 0.00720629 -0.06438393 -0.0953459   0.90806204]', '[-0.02519009  0.15175941 -0.21365988  1.20860512]', '[-0.04507228  0.33112487  0.02253753  0.5551697 ]', '[-0.0159151   0.367824    0.26271889 -0.18751725]', '[ 0.02946319  0.32873693  0.18079481 -0.18976199]', '[ 0.0529455   0.29687707  0.0484953  -0.12000677]', '[ 0.04775965  0.28300861 -0.09949342 -0.01755456]', '[ 0.01475191  0.28875933 -0.22349962  0.0684577 ]', '[-0.03776261  0.30649902 -0.29031944  0.09747359]', '[-0.07024382  0.25527396 -0.02882033 -0.60674023]', '[-0.07618529  0.13901268 -0.0333443  -0.53643461]', '[-0.08457128  0.04802687 -0.05188614 -0.35875037]', '[-9.70835949e-02  1.45545885e-05 -7.21800855e-02 -1.15139835e-01]', '[-0.11256576  0.00270827 -0.07936847  0.139058  ]', '[-0.12718292  0.05272748 -0.0622465   0.35014595]', '[-0.13551053  0.13705194 -0.01655177  0.47703275]', '[-0.10592808  0.16841115  0.30670966 -0.16333527]', '[-0.04457559  0.14583765  0.29378729 -0.04926621]', '[0.00661366 0.15313808 0.2081169  0.12869562]', '[ 0.06188084  0.13000039  0.33235495 -0.34714389]', '[ 0.10680276  0.09163826  0.10684081 -0.02320763]', '[ 0.10274431  0.122525   -0.1453049   0.32556324]', '[ 0.07824938  0.14725823 -0.09412842 -0.0857747 ]', '[ 0.06652748  0.08802939 -0.02241012 -0.49834552]', '[ 0.04195031  0.02294808 -0.22028185 -0.14534319]', '[-0.01838799  0.0292469  -0.37044976  0.1974959 ]', '[-0.07311157  0.02597129 -0.16608629 -0.2375189 ]', '[-0.109168    0.00396024 -0.18782689  0.01551503]', '[-0.14513093  0.02963068 -0.16374786  0.23118016]']</t>
+  </si>
+  <si>
+    <t>[array([-0.03763371, -0.01533471,  0.06554052, -0.01816017], dtype=float32), array([-0.03406929,  0.01398622, -0.02953871,  0.30651903]), array([-0.02168374,  0.03409236,  0.1512214 , -0.10649158]), array([-0.00282652,  0.04327343,  0.03401407,  0.19924661]), array([-0.00814034,  0.11145621, -0.08365717,  0.46948189]), array([-0.03365186,  0.22334811, -0.16249273,  0.62574953]), array([-0.04285076,  0.2835192 ,  0.07310173, -0.03359517]), array([-0.03176865,  0.27882203,  0.03536798, -0.01091686]), array([-0.02932458,  0.27976972, -0.01134823,  0.02054779]), array([-0.03608027,  0.28663083, -0.05459109,  0.04579883]), array([-0.0501551 ,  0.29677884, -0.08297669,  0.05176831]), array([-0.06777844,  0.30558506, -0.08942408,  0.03212042]), array([-0.08436899,  0.30806041, -0.0730686 , -0.01026882]), array([-0.09581655,  0.30068774, -0.03933726, -0.06390967]), array([-0.07347318,  0.21521875,  0.25624669, -0.77411808]), array([-0.02549141,  0.07242505,  0.20913951, -0.62142584]), array([ 0.005005  , -0.02174213,  0.08680366, -0.29949166]), array([ 0.00699615, -0.04200657, -0.06766405,  0.10014684]), array([ 0.0057884 , -0.05241753,  0.05530831, -0.2022683 ]), array([ 0.00121612, -0.05090957, -0.09981119,  0.21591138]), array([-0.00547005, -0.03879613,  0.03448463, -0.09752754]), array([-0.01229102, -0.01962781, -0.1005132 ,  0.28445644]), array([-0.01680487,  0.00123477,  0.05670342, -0.07968184]), array([-0.01723611,  0.01883435, -0.06018765,  0.25219462]), array([-0.03925736,  0.09784876, -0.15284015,  0.52043503]), array([-0.04810444,  0.14945678,  0.06720622, -0.01353452]), array([-0.03987919,  0.16168461,  0.0138649 ,  0.13478559]), array([-0.04244576,  0.20167637, -0.03766341,  0.25769045]), array([-0.02745532,  0.19278766,  0.18394505, -0.34225122]), array([ 0.02745265,  0.07138497,  0.3504006 , -0.84280025]), array([ 0.07830451, -0.05964028,  0.14388227, -0.43725698]), array([ 0.08149146, -0.09554643, -0.11332034,  0.08403858]), array([ 0.06147297, -0.09697159, -0.08295858, -0.10090843]), array([ 0.04941064, -0.13554367, -0.03659042, -0.27971852]), array([ 0.02035788, -0.13715479, -0.24769427,  0.2587894 ]), array([-0.0185623 , -0.10697522, -0.1328243 ,  0.03199534]), array([-0.03046514, -0.12657087,  0.01537186, -0.22604563]), array([-0.01323273, -0.19406343,  0.15112098, -0.43418513]), array([ 2.16344362e-04, -2.24462179e-01, -1.97646682e-02,  1.36388564e-01]), array([-0.02062911, -0.14134474, -0.1822367 ,  0.67798016]), array([-0.04165264, -0.033105  , -0.02035014,  0.38252035]), array([-0.05387789,  0.07444784, -0.09572739,  0.67198247]), array([-0.05015103,  0.15660509,  0.13416518,  0.13717571]), array([-0.02844668,  0.1973133 ,  0.0798914 ,  0.2660323 ]), array([ 0.0073629 ,  0.19240938,  0.27036143, -0.30810314]), array([ 0.04821631,  0.14971785,  0.12871898, -0.10528688]), array([ 0.05641385,  0.15351306, -0.0480613 ,  0.14350513]), array([ 0.03011995,  0.20454807, -0.20774363,  0.35356295]), array([ 0.0038217 ,  0.21954728, -0.04970803, -0.20951367]), array([-0.01559179,  0.19073805, -0.1412619 , -0.07691308]), array([-0.02417625,  0.11987612,  0.05511404, -0.62104914]), array([-0.02240481,  0.01991038, -0.04099207, -0.36098654]), array([-0.04089841, -0.01984411, -0.1412743 , -0.03287604]), array([-0.05017263, -0.06307824,  0.04874821, -0.39288613]), array([-0.04964863, -0.10247576, -0.0445339 ,  0.00516335]), array([-0.04079197, -0.13004076,  0.1301919 , -0.27423497]), array([-0.0267818 , -0.13845147,  0.00703011,  0.19323707]), array([-0.01125664, -0.1235447 ,  0.1453659 , -0.04398948]), array([ 0.02887994, -0.15361091,  0.24676827, -0.24494018]), array([ 0.05639592, -0.14679317,  0.02323185,  0.31561532]), array([ 0.06489294, -0.09959999,  0.06150652,  0.14951446]), array([ 0.0804065 , -0.0883744 ,  0.09080158, -0.03669922]), array([ 0.09963978, -0.11265479,  0.09683773, -0.1988487 ]), array([ 0.09060477, -0.09555016, -0.18450052,  0.36500044]), array([ 0.05619341, -0.04236247, -0.15104827,  0.15254933]), array([ 0.03308856, -0.03863092, -0.07535096, -0.11913768]), array([ 0.02700272, -0.0893307 ,  0.013914  , -0.37962725]), array([ 0.03740861, -0.18492786,  0.08473625, -0.55775526]), array([ 0.03189263, -0.23573597, -0.13945514,  0.05593224]), array([ 0.01026862, -0.23290407, -0.07238627, -0.03135546]), array([ 0.00407733, -0.24881733,  0.01116323, -0.12592688]), array([ 0.01426195, -0.28144496,  0.08758004, -0.19317591]), array([ 0.03721748, -0.32237225,  0.13611635, -0.20570991]), array([ 0.0400804 , -0.29209233, -0.10740364,  0.50418501]), array([-0.0033212 , -0.12781653, -0.31355086,  1.10553754]), array([-0.05088216,  0.06239806, -0.14595318,  0.75566731]), array([-0.05724766,  0.16187341,  0.08604794,  0.2221972 ]), array([-0.04368195,  0.21747783,  0.04872457,  0.32618569]), array([-0.01160895,  0.22066918,  0.26505794, -0.28910685]), array([ 0.03107296,  0.17695397,  0.15187858, -0.13403674]), array([ 0.07264182,  0.10268309,  0.25321127, -0.58972643]), array([ 0.12680949, -0.04774379,  0.27264711, -0.87993656]), array([ 0.17474255, -0.23321361,  0.19057143, -0.93467239]), array([ 0.17152281, -0.33894949, -0.22335582, -0.10878821]), array([ 0.11478036, -0.34515576, -0.33271776,  0.03931809]), array([ 0.04398779, -0.32778713, -0.36027616,  0.12056204]), array([-0.04900172, -0.23575106, -0.54833765,  0.77101189]), array([-0.13838645, -0.10455097, -0.32348978,  0.50418026]), array([-0.1717028 , -0.045523  , -0.00152064,  0.0713898 ]), array([-0.16524649, -0.00855417,  0.06588049,  0.29299227]), array([-1.19149541e-01, -1.34303737e-04,  3.85679162e-01, -2.02474985e-01]), array([-0.01776908, -0.08191157,  0.60468577, -0.58457113]), array([ 0.08479167, -0.14956897,  0.39839988, -0.06548097]), array([ 0.13475422, -0.10215487,  0.09283022,  0.53839063]), array([ 0.14820469, -0.00894954,  0.04218062,  0.37931962]), array([ 0.15194776,  0.04474809, -0.00387246,  0.14920894]), array([ 0.1470812 ,  0.04862963, -0.04372076, -0.11166848]), array([ 0.13491458,  0.00102089, -0.07697001, -0.35807386]), array([ 0.0901097 , -0.02200851, -0.36238654,  0.1242428 ]), array([ 0.02270652, -0.02404969, -0.29822413, -0.15433615]), array([-0.0246614 , -0.08534945, -0.16818062, -0.45468039]), array([-0.06940329, -0.13327542, -0.27118886, -0.02406635]), array([-0.10228018, -0.16647505, -0.05224672, -0.30702747]), array([-0.11644031, -0.1845648 , -0.08668043,  0.12627344]), array([-0.13528274, -0.11865686, -0.09622871,  0.51915868]), array([-0.12567433, -0.05352839,  0.19212587,  0.1229898 ]), array([-8.77245909e-02, -2.86856104e-04,  1.81452350e-01,  4.05893942e-01]), array([-0.02849592,  0.03684135,  0.39971827, -0.03144634]), array([0.03901826, 0.0610819 , 0.26279474, 0.27955546]), array([0.07304059, 0.14804982, 0.07381343, 0.57959697]), array([0.09507145, 0.21778325, 0.14330893, 0.11089704]), array([ 0.12812185,  0.19295211,  0.17968739, -0.34968524]), array([ 0.13689546,  0.15294854, -0.0946212 , -0.04269484]), array([ 0.11810798,  0.10697207, -0.09063051, -0.41250347]), array([ 0.1012111 , -0.00773571, -0.07868424, -0.71721201]), array([ 0.05943336, -0.10213756, -0.33334528, -0.21736251]), array([-0.00082766, -0.16406618, -0.25939255, -0.39989391]), array([-0.06732464, -0.19173764, -0.39217197,  0.11645654]), array([-0.12455704, -0.19231389, -0.16877669, -0.13109615]), array([-0.15856304, -0.17673541, -0.16381937,  0.27862004]), array([-0.18684037, -0.0865212 , -0.11093234,  0.6045227 ]), array([-0.17315698, -0.01302887,  0.24696997,  0.12060771]), array([-0.11821077,  0.03158297,  0.2929629 ,  0.32595506]), array([-0.05983122,  0.11629767,  0.28225192,  0.51454403]), array([-0.00837145,  0.23334601,  0.22634923,  0.64261071]), array([0.05459284, 0.29980858, 0.39084785, 0.0231519 ]), array([0.11529916, 0.31515154, 0.20424257, 0.13803244]), array([ 0.13308146,  0.35628545, -0.02890918,  0.26984455]), array([ 0.13037952,  0.35268394,  0.00236331, -0.3056332 ]), array([ 0.10775698,  0.30449147, -0.22481849, -0.17322135]), array([ 0.07004314,  0.21483674, -0.14606156, -0.71633164]), array([ 0.02390531,  0.09344094, -0.31019123, -0.48351883]), array([-0.05042798,  0.02466732, -0.42042877, -0.20351837]), array([-0.11145469, -0.0587631 , -0.18080716, -0.62460859]), array([-0.14791145, -0.15022676, -0.17887377, -0.28086504]), array([-0.18059312, -0.16983998, -0.1415968 ,  0.08217231]), array([-0.17563603, -0.18855993,  0.18922494, -0.26480563]), array([-0.13488903, -0.20171743,  0.2095596 ,  0.14183551]), array([-0.09514354, -0.13064791,  0.18150441,  0.56382041]), array([-0.03747868, -0.04987902,  0.38607869,  0.23891353]), array([0.02714888, 0.03478192, 0.25030414, 0.60200457]), array([0.0866758 , 0.11693842, 0.33524494, 0.2150276 ]), array([0.12983609, 0.19046312, 0.09037148, 0.51389199]), array([0.14870843, 0.24896785, 0.09537609, 0.06606211]), array([ 0.1402882 ,  0.28521028, -0.17657512,  0.28862009]), array([ 0.10761049,  0.29091047, -0.14326277, -0.23780196]), array([ 0.05898426,  0.25840663, -0.33368991, -0.0904923 ]), array([-0.02053236,  0.25142577, -0.44528805,  0.00877804]), array([-0.11173196,  0.25602672, -0.44810838,  0.02247984]), array([-0.16609464,  0.18681106, -0.08647518, -0.71078578]), array([-0.17295583,  0.04849614,  0.01409213, -0.64854144]), array([-0.16253408, -0.06313321,  0.08443438, -0.44702644]), array([-0.14164532, -0.12314402,  0.11863617, -0.14015725]), array([-0.11735756, -0.11577061,  0.11952163,  0.21637792]), array([-0.06886487, -0.10632221,  0.3555938 , -0.11531686]), array([-0.00772679, -0.08734149,  0.24400914,  0.31105532]), array([ 0.05193699, -0.0515555 ,  0.34163457,  0.04991728]), array([0.09694763, 0.00469317, 0.10152452, 0.50901412]), array([0.11869062, 0.07768025, 0.11367182, 0.21198179]), array([ 0.14104536,  0.08803938,  0.10554153, -0.10636178]), array([ 0.13242667,  0.10640997, -0.1890456 ,  0.2849246 ]), array([ 0.09563781,  0.12733784, -0.17085952, -0.08464048]), array([ 0.04030355,  0.13977565, -0.37060607,  0.19761166]), array([-0.01957558,  0.13059331, -0.2163511 , -0.29677189]), array([-0.06976258,  0.09069831, -0.2766527 , -0.10299021]), array([-0.12600313,  0.08745724, -0.27454613,  0.06257736]), array([-0.14844109,  0.0429935 ,  0.05292645, -0.50226499]), array([-0.13343343, -0.03735408,  0.09162085, -0.28522375]), array([-0.08751451, -0.13447875,  0.35483376, -0.66133584]), array([-0.02531694, -0.22001252,  0.25253082, -0.17106739]), array([ 0.00887954, -0.19737305,  0.08302991,  0.39889523]), array([ 0.00720629, -0.06438393, -0.0953459 ,  0.90806204]), array([-0.02519009,  0.15175941, -0.21365988,  1.20860512]), array([-0.04507228,  0.33112487,  0.02253753,  0.5551697 ]), array([-0.0159151 ,  0.367824  ,  0.26271889, -0.18751725]), array([ 0.02946319,  0.32873693,  0.18079481, -0.18976199]), array([ 0.0529455 ,  0.29687707,  0.0484953 , -0.12000677]), array([ 0.04775965,  0.28300861, -0.09949342, -0.01755456]), array([ 0.01475191,  0.28875933, -0.22349962,  0.0684577 ]), array([-0.03776261,  0.30649902, -0.29031944,  0.09747359]), array([-0.07024382,  0.25527396, -0.02882033, -0.60674023]), array([-0.07618529,  0.13901268, -0.0333443 , -0.53643461]), array([-0.08457128,  0.04802687, -0.05188614, -0.35875037]), array([-9.70835949e-02,  1.45545885e-05, -7.21800855e-02, -1.15139835e-01]), array([-0.11256576,  0.00270827, -0.07936847,  0.139058  ]), array([-0.12718292,  0.05272748, -0.0622465 ,  0.35014595]), array([-0.13551053,  0.13705194, -0.01655177,  0.47703275]), array([-0.10592808,  0.16841115,  0.30670966, -0.16333527]), array([-0.04457559,  0.14583765,  0.29378729, -0.04926621]), array([0.00661366, 0.15313808, 0.2081169 , 0.12869562]), array([ 0.06188084,  0.13000039,  0.33235495, -0.34714389]), array([ 0.10680276,  0.09163826,  0.10684081, -0.02320763]), array([ 0.10274431,  0.122525  , -0.1453049 ,  0.32556324]), array([ 0.07824938,  0.14725823, -0.09412842, -0.0857747 ]), array([ 0.06652748,  0.08802939, -0.02241012, -0.49834552]), array([ 0.04195031,  0.02294808, -0.22028185, -0.14534319]), array([-0.01838799,  0.0292469 , -0.37044976,  0.1974959 ]), array([-0.07311157,  0.02597129, -0.16608629, -0.2375189 ]), array([-0.109168  ,  0.00396024, -0.18782689,  0.01551503]), array([-0.14513093,  0.02963068, -0.16374786,  0.23118016])]</t>
+  </si>
+  <si>
+    <t>['[0,2,1]', '[2,0,1]', '[1,0,2]', '[2,2,2]', '[1,2,0]', '[1,1,2]', '[2,1,0]', '[1,1,1]', '[0,0,0]', '[0,1,1]']</t>
+  </si>
+  <si>
+    <t>[0, 2, 0, 2, 0, 2, 0, 2, 0, 2, 0, 2, 0, 2, 0, 2, 0, 2, 0, 2, 2, 0, 2, 0, 2, 2, 0, 2, 0, 2, 0, 2, 0, 2, 0, 2, 0, 2, 0, 2, 0, 2, 0, 2, 0, 2, 0, 2, 0, 2, 0, 2, 2, 0, 2, 0, 2, 2, 0, 2, 0, 2, 0, 2, 0, 2, 0, 2, 0, 2, 0, 2, 0, 2, 0, 2, 0, 2, 0, 2, 0, 2, 0, 2, 2, 0, 2, 0, 2, 2, 0, 2, 0, 2, 0, 2, 0, 2, 0, 2, 0, 2, 0, 2, 0, 2, 0, 2, 0, 2, 0, 2, 0, 2, 0, 2, 2, 0, 2, 0, 2, 2, 0, 2, 0, 2, 0, 2, 0, 2, 0, 2, 0, 2, 0, 2, 0, 2, 0, 2, 0, 2, 0, 2, 0, 2, 0, 2, 2, 0, 2, 0, 2, 0, 2, 0, 2, 0, 0, 2, 0, 2, 0, 2, 0, 2, 0, 2, 0, 2, 0, 2, 0, 0, 2, 0, 2, 0, 2, 0, 2, 0, 2, 0, 2, 0, 2, 0, 2, 0, 2, 0, 2, 2, 0, 2, 2, 0, 2]</t>
+  </si>
+  <si>
+    <t>['[-0.03763371 -0.01533471  0.06554052 -0.01816017]', '[-0.03406929  0.01398622 -0.02953871  0.30651903]', '[-0.02168374  0.03409236  0.1512214  -0.10649158]', '[-0.00282652  0.04327343  0.03401407  0.19924661]', '[ 0.01834705  0.04294749  0.17317668 -0.19873753]', '[0.03659766 0.0372359  0.00569586 0.14498695]', '[ 0.04737447  0.03050982  0.09950876 -0.20907803]', '[ 0.04773513  0.02629209 -0.09583188  0.16718432]', '[ 0.03752505  0.02534768 -0.00439201 -0.17769188]', '[ 0.01910665  0.02614969 -0.17578652  0.18226832]', '[-0.00293854  0.02498097 -0.04044017 -0.19672323]', '[-0.02338561  0.01819528 -0.15991175  0.1265223 ]', '[-0.03744461  0.00328053  0.02144561 -0.27476369]', '[-0.04234133 -0.01910231 -0.06994388  0.05368665]', '[-0.03763269 -0.04539758  0.11498126 -0.31087136]', '[-0.02550263 -0.06918706  0.00335501  0.07846404]', '[-0.00968282 -0.08350681  0.15097012 -0.21632696]', '[ 0.0053941  -0.08236633 -0.00300315  0.22938636]', '[ 0.0161822  -0.06338321  0.10914378 -0.04087513]', '[ 0.02066644 -0.02828874 -0.063904    0.38603243]', '[0.01913681 0.01633736 0.05013034 0.05264949]', '[ 0.0400551  -0.0073938   0.15390054 -0.28229442]', '[ 0.05094132 -0.02216557 -0.04740575  0.1382459 ]', '[ 0.04870162 -0.02310954  0.02529389 -0.14757537]', '[ 0.03376547 -0.01028918 -0.17094986  0.2707556 ]', '[ 0.0103118   0.01075104 -0.05836816 -0.0672164 ]', '[ 0.01124463 -0.0370396   0.06579493 -0.4018725 ]', '[ 0.00803486 -0.07504962 -0.09809813  0.02722039]', '[ 1.51338775e-04 -9.62015886e-02  1.99960523e-02 -2.35938240e-01]', '[-0.01132378 -0.09750196 -0.13218554  0.22087768]', '[-0.02355496 -0.08096771  0.01267429 -0.05993836]', '[-0.0330696  -0.05205256 -0.10484912  0.34234137]', '[-0.03642324 -0.01860412  0.07279953 -0.01371334]', '[-0.03166866  0.01206933 -0.02509297  0.31554307]', '[-0.01874523  0.03436217  0.15211703 -0.09394883]', '[-5.13230523e-05  4.62105789e-02  3.16075962e-02  2.12883305e-01]', '[ 0.02039466  0.04845639  0.16853114 -0.18720539]', '[0.03762326 0.04455931 0.00038545 0.1511327 ]', '[ 0.04739711  0.03833294  0.09500645 -0.210463  ]', '[ 0.04703493  0.03301412 -0.09845059  0.15764597]', '[ 0.03651771  0.02945918 -0.00486237 -0.19385638]', '[ 0.01818744  0.02662077 -0.17457023  0.1626772 ]', '[-0.00352862  0.02154485 -0.03855204 -0.21548247]', '[-0.02362984  0.01145217 -0.1585124   0.11283283]', '[-0.03753204 -0.00542412  0.02151977 -0.28032934]', '[-0.0425714  -0.02799292 -0.07141092  0.05738308]', '[-0.03827598 -0.05268781  0.11245074 -0.2989076 ]', '[-0.02666782 -0.07350228  0.00086365  0.09565699]', '[-0.01124264 -0.08418115  0.14971078 -0.19780414]', '[ 0.00379227 -0.07954607 -0.00205983  0.24522416]', '[ 0.01502732 -0.05793824  0.11266026 -0.0308478 ]', '[ 0.02043587 -0.0215465  -0.05831989  0.38888924]', '[0.0201345  0.02294776 0.05656633 0.04870431]', '[ 0.04228153 -0.00209186  0.15946475 -0.29102339]', '[ 0.05405053 -0.01885364 -0.04438103  0.12755362]', '[ 0.05206131 -0.02189818  0.02466117 -0.15749228]', '[ 0.03660591 -0.01081184 -0.17545328  0.26354381]', '[ 0.01192537  0.0091228  -0.06591528 -0.07106547]', '[ 0.01118009 -0.03914202  0.05688384 -0.40293856]', '[ 0.00622896 -0.0772038  -0.10624534  0.02750459]', '[-0.00303788 -0.09829433  0.01458906 -0.23583011]', '[-0.01519879 -0.09969145 -0.13350175  0.21971518]', '[-0.0272538  -0.08352116  0.01570042 -0.06232006]', '[-0.03578703 -0.0551298  -0.09828338  0.33973714]', '[-0.03761326 -0.02207353  0.08118663 -0.01472797]', '[-0.03117157  0.0087054  -0.0169494   0.3178561 ]', '[-0.01680571  0.03188745  0.15813818 -0.08731009]', '[0.00277007 0.04548881 0.03428665 0.22359811]', '[ 0.02338839  0.05015225  0.16761522 -0.17413231]', '[ 0.04012653  0.04887202 -0.00341795  0.16369621]', '[ 0.04896058  0.04483812  0.08966857 -0.20161924]', '[ 0.04751718  0.04066462 -0.1036719   0.15989458]', '[ 0.03608145  0.03677286 -0.00864944 -0.19955532]', '[ 0.01720728  0.03201352 -0.17617777  0.14942282]', '[-0.00461583  0.02372424 -0.03809184 -0.23382355]', '[-0.02447932  0.00976918 -0.15676744  0.09325948]', '[-0.03799968 -0.01077833  0.02339896 -0.29677434]', '[-0.04274161 -0.03600156 -0.07044923  0.04776911]', '[-0.03840229 -0.06173394  0.11188697 -0.29948506]', '[-0.02704815 -0.08175761 -0.00103029  0.10395188]', '[-0.01208312 -0.09002918  0.14717567 -0.18251961]', '[ 0.00248328 -0.08194469 -0.00402095  0.26378905]', '[ 0.01347812 -0.05663598  0.11238667 -0.01308476]', '[ 0.01906687 -0.01709075 -0.05618284  0.40214629]', '[0.01944171 0.02938882 0.06110738 0.05507872]', '[ 0.0426691   0.00488294  0.16552386 -0.29198549]', '[ 0.05567946 -0.01270791 -0.03830676  0.12056844]', '[ 0.05476185 -0.01754592  0.02903159 -0.16796849]', '[ 0.03988309 -0.00865282 -0.17423833  0.25254733]', '[ 0.01506354  0.0092458  -0.06855153 -0.08010439]', '[ 0.01342235 -0.040504    0.05069643 -0.40863199]', '[ 0.00697918 -0.07935649 -0.11469307  0.02518724]', '[-0.00404282 -0.10065344  0.0058336  -0.23581411]', '[-0.01780205 -0.1019573  -0.14040012  0.22036821]', '[-0.03090464 -0.08571047  0.01233408 -0.06238079]', '[-0.03967834 -0.05746832 -0.09728464  0.33830588]', '[-0.04088649 -0.02479813  0.0862282  -0.01699021]', '[-0.03313408  0.00555571 -0.00916788  0.31615044]', '[-0.01709824  0.0286016   0.16671648 -0.08669091]', '[0.00409761 0.0426896  0.04159804 0.2280058 ]', '[ 0.02591234  0.04865704  0.1720678  -0.16554347]', '[ 0.04318138  0.04944889 -0.00259859  0.17554405]', '[ 0.05182717  0.04793017  0.08708201 -0.18877447]', '[ 0.04961378  0.04616405 -0.10855157  0.17058545]', '[ 0.03710027  0.04393717 -0.01427681 -0.19404838]', '[ 0.0171644   0.03955664 -0.18094415  0.14747835]', '[-0.00543206  0.03008287 -0.04093621 -0.24363824]', '[-0.02563501  0.01348145 -0.15733974  0.07702875]', '[-0.03907693 -0.0106912   0.02462454 -0.31615271]', '[-0.04347682 -0.03975416 -0.06843994  0.0294576 ]', '[-0.03875691 -0.06868657  0.11350382 -0.31255978]', '[-0.02718902 -0.09055323 -0.0005972   0.09892028]', '[-0.01229391 -0.09889691  0.14605862 -0.17821307]', '[ 0.00193427 -0.08911365 -0.00617459  0.27613969]', '[ 0.01246219 -0.0607399   0.11006833  0.00460279]', '[ 0.01767613 -0.01746661 -0.05742591  0.42104822]', '[0.01799889 0.03256356 0.06194914 0.07106617]', '[ 0.04164095  0.01069004  0.16882221 -0.28203346]', '[ 0.05552767 -0.00565132 -0.03298584  0.12304419]', '[ 0.05578172 -0.01071831  0.0351817  -0.17251072]', '[ 0.04207756 -0.00327057 -0.16892467  0.24306336]', '[ 0.01809734  0.01247845 -0.06570728 -0.09161583]', '[ 0.0166784  -0.03952956  0.04996191 -0.41928328]', '[ 0.00970175 -0.08024085 -0.11923689  0.0174798 ]', '[-0.00255012 -0.1027089  -0.00170788 -0.23980761]', '[-0.01797844 -0.10448545 -0.14921732  0.21944907]', '[-0.03279817 -0.08822614  0.00432766 -0.06160815]', '[-0.0429199  -0.05980691 -0.10248424  0.3390746 ]', '[-0.04477409 -0.02707825  0.08509623 -0.01727879]', '[-0.03680915  0.00308939 -0.00596657  0.31465325]', '[-0.01976107  0.02578306  0.17342083 -0.08849873]', '[0.00298872 0.03961152 0.05010813 0.22750325]', '[ 0.026514    0.04574731  0.18032288 -0.16312637]', '[0.04524209 0.0474135  0.00347248 0.18193809]', '[ 0.0547737   0.04756446  0.089742   -0.1786232 ]', '[ 0.052719    0.04808358 -0.10958037  0.182909  ]', '[ 0.03968097  0.04832029 -0.01831026 -0.18224004]', '[ 0.01875532  0.04597667 -0.18654323  0.15553006]', '[-0.00498113  0.03750945 -0.04647087 -0.24197424]', '[-0.02615815  0.02046471 -0.16137018  0.07087075]', '[-0.04018818 -0.00569015  0.02283148 -0.32956194]', '[-0.04472263 -0.03796813 -0.06807105  0.0112597 ]', '[-0.03977193 -0.0707079   0.11527201 -0.33173448]', '[-0.02780187 -0.0961543   0.00147775  0.08294848]', '[-0.01255879 -0.10704514  0.14731344 -0.1872195 ]', '[ 0.00179073 -0.09820019 -0.00627177  0.27594249]', '[ 0.01214555 -0.06893478  0.10850376  0.01352591]', '[ 0.0169596  -0.02313884 -0.05971152  0.43687334]', '[0.01684516 0.03045181 0.06007176 0.0901481 ]', '[ 0.04025325  0.01235965  0.16851984 -0.26398233]', '[ 0.05430388 -0.00079913 -0.030983    0.13630429]', '[ 0.0551963  -0.00390572  0.03949108 -0.16640006]', '[ 0.04252198  0.00399475 -0.1631329   0.24156304]', '[ 0.01972951  0.01878404 -0.05989374 -0.09935726]', '[-0.00719077  0.03338913 -0.20317714  0.23831098]', '[-0.03109278  0.03970184 -0.03105751 -0.17943795]', '[-0.04602812  0.03220258 -0.11536638  0.10315408]', '[-0.04857485  0.00954666  0.08942957 -0.32567426]', '[-0.03903633 -0.02389749  0.00315131 -0.00188288]', '[-0.04739862  0.00891768 -0.08390808  0.32277384]', '[-0.04389416  0.03111565  0.11862509 -0.10351861]', '[-0.02864332  0.03893335  0.03120107  0.18236794]', '[-0.00497513  0.0334018   0.2002452  -0.23260361]', '[0.02107596 0.02016769 0.05479172 0.10615778]', '[ 0.04279093  0.00657729  0.15735704 -0.23601811]', '[ 0.05432279 -0.00042662 -0.04430346  0.16843264]', '[ 0.05270667  0.0025464   0.02841883 -0.13915784]', '[ 0.03836449  0.0147418  -0.16827479  0.25628195]', '[ 0.01530575  0.03085196 -0.05733159 -0.10110943]', '[-0.01036427  0.04347995 -0.19356254  0.22084265]', '[-0.03187717  0.04515792 -0.01740894 -0.20714614]', '[-0.04403382  0.03176144 -0.10197892  0.07334333]', '[-0.04430096  0.00366435  0.09821205 -0.34899642]', '[-0.03373534 -0.03322643  0.0043413  -0.01230537]', '[-0.04269608 -0.00097066 -0.0909752   0.32760099]', '[-0.04129243  0.02356253  0.10519625 -0.08574262]', '[-0.0290492   0.03574529  0.01530273  0.2070179 ]', '[-0.00840644  0.03516068  0.18665023 -0.20909091]', '[0.01551767 0.02588013 0.04766478 0.12118061]', '[ 0.03666441  0.01404583  0.15895883 -0.23385199]', '[ 0.04938654  0.006138   -0.03428356  0.15758913]', '[ 0.05039664  0.00595369  0.04402447 -0.15892806]', '[ 0.03936407  0.01386988 -0.15158915  0.23451048]', '[ 0.01933942  0.0260666  -0.0444065  -0.11734339]', '[-0.00445233  0.03651128 -0.18814468  0.21589742]', '[-0.02577642  0.03852623 -0.02095712 -0.1988815 ]', '[-0.03946704  0.027949   -0.11335767  0.09252509]', '[-0.04251502  0.00429218  0.08248658 -0.3249713 ]', '[-0.03513879 -0.02796251 -0.01104114  0.00874986]', '[-0.02023327 -0.06097559  0.15578729 -0.3303973 ]', '[-0.00269428 -0.08508483  0.01557024  0.09560047]', '[ 0.01242213 -0.09227187  0.13213142 -0.16355619]', '[ 0.02111218 -0.07814076 -0.04633684  0.30331765]', '[ 0.02185659 -0.04415853  0.05456546  0.03100886]', '[ 0.04214847 -0.06553987  0.14341803 -0.23768561]', '[ 0.0497783  -0.06563303 -0.06836522  0.23735732]', '[ 0.04297833 -0.04319393  0.00232915 -0.01764589]', '[ 0.0506473  -0.07245873  0.07174425 -0.26846855]', '[ 0.04334158 -0.07746957 -0.14314117  0.21749326]', '[ 0.02274164 -0.0586999  -0.05823584 -0.03594645]']</t>
+  </si>
+  <si>
+    <t>[array([-0.03763371, -0.01533471,  0.06554052, -0.01816017], dtype=float32), array([-0.03406929,  0.01398622, -0.02953871,  0.30651903]), array([-0.02168374,  0.03409236,  0.1512214 , -0.10649158]), array([-0.00282652,  0.04327343,  0.03401407,  0.19924661]), array([ 0.01834705,  0.04294749,  0.17317668, -0.19873753]), array([0.03659766, 0.0372359 , 0.00569586, 0.14498695]), array([ 0.04737447,  0.03050982,  0.09950876, -0.20907803]), array([ 0.04773513,  0.02629209, -0.09583188,  0.16718432]), array([ 0.03752505,  0.02534768, -0.00439201, -0.17769188]), array([ 0.01910665,  0.02614969, -0.17578652,  0.18226832]), array([-0.00293854,  0.02498097, -0.04044017, -0.19672323]), array([-0.02338561,  0.01819528, -0.15991175,  0.1265223 ]), array([-0.03744461,  0.00328053,  0.02144561, -0.27476369]), array([-0.04234133, -0.01910231, -0.06994388,  0.05368665]), array([-0.03763269, -0.04539758,  0.11498126, -0.31087136]), array([-0.02550263, -0.06918706,  0.00335501,  0.07846404]), array([-0.00968282, -0.08350681,  0.15097012, -0.21632696]), array([ 0.0053941 , -0.08236633, -0.00300315,  0.22938636]), array([ 0.0161822 , -0.06338321,  0.10914378, -0.04087513]), array([ 0.02066644, -0.02828874, -0.063904  ,  0.38603243]), array([0.01913681, 0.01633736, 0.05013034, 0.05264949]), array([ 0.0400551 , -0.0073938 ,  0.15390054, -0.28229442]), array([ 0.05094132, -0.02216557, -0.04740575,  0.1382459 ]), array([ 0.04870162, -0.02310954,  0.02529389, -0.14757537]), array([ 0.03376547, -0.01028918, -0.17094986,  0.2707556 ]), array([ 0.0103118 ,  0.01075104, -0.05836816, -0.0672164 ]), array([ 0.01124463, -0.0370396 ,  0.06579493, -0.4018725 ]), array([ 0.00803486, -0.07504962, -0.09809813,  0.02722039]), array([ 1.51338775e-04, -9.62015886e-02,  1.99960523e-02, -2.35938240e-01]), array([-0.01132378, -0.09750196, -0.13218554,  0.22087768]), array([-0.02355496, -0.08096771,  0.01267429, -0.05993836]), array([-0.0330696 , -0.05205256, -0.10484912,  0.34234137]), array([-0.03642324, -0.01860412,  0.07279953, -0.01371334]), array([-0.03166866,  0.01206933, -0.02509297,  0.31554307]), array([-0.01874523,  0.03436217,  0.15211703, -0.09394883]), array([-5.13230523e-05,  4.62105789e-02,  3.16075962e-02,  2.12883305e-01]), array([ 0.02039466,  0.04845639,  0.16853114, -0.18720539]), array([0.03762326, 0.04455931, 0.00038545, 0.1511327 ]), array([ 0.04739711,  0.03833294,  0.09500645, -0.210463  ]), array([ 0.04703493,  0.03301412, -0.09845059,  0.15764597]), array([ 0.03651771,  0.02945918, -0.00486237, -0.19385638]), array([ 0.01818744,  0.02662077, -0.17457023,  0.1626772 ]), array([-0.00352862,  0.02154485, -0.03855204, -0.21548247]), array([-0.02362984,  0.01145217, -0.1585124 ,  0.11283283]), array([-0.03753204, -0.00542412,  0.02151977, -0.28032934]), array([-0.0425714 , -0.02799292, -0.07141092,  0.05738308]), array([-0.03827598, -0.05268781,  0.11245074, -0.2989076 ]), array([-0.02666782, -0.07350228,  0.00086365,  0.09565699]), array([-0.01124264, -0.08418115,  0.14971078, -0.19780414]), array([ 0.00379227, -0.07954607, -0.00205983,  0.24522416]), array([ 0.01502732, -0.05793824,  0.11266026, -0.0308478 ]), array([ 0.02043587, -0.0215465 , -0.05831989,  0.38888924]), array([0.0201345 , 0.02294776, 0.05656633, 0.04870431]), array([ 0.04228153, -0.00209186,  0.15946475, -0.29102339]), array([ 0.05405053, -0.01885364, -0.04438103,  0.12755362]), array([ 0.05206131, -0.02189818,  0.02466117, -0.15749228]), array([ 0.03660591, -0.01081184, -0.17545328,  0.26354381]), array([ 0.01192537,  0.0091228 , -0.06591528, -0.07106547]), array([ 0.01118009, -0.03914202,  0.05688384, -0.40293856]), array([ 0.00622896, -0.0772038 , -0.10624534,  0.02750459]), array([-0.00303788, -0.09829433,  0.01458906, -0.23583011]), array([-0.01519879, -0.09969145, -0.13350175,  0.21971518]), array([-0.0272538 , -0.08352116,  0.01570042, -0.06232006]), array([-0.03578703, -0.0551298 , -0.09828338,  0.33973714]), array([-0.03761326, -0.02207353,  0.08118663, -0.01472797]), array([-0.03117157,  0.0087054 , -0.0169494 ,  0.3178561 ]), array([-0.01680571,  0.03188745,  0.15813818, -0.08731009]), array([0.00277007, 0.04548881, 0.03428665, 0.22359811]), array([ 0.02338839,  0.05015225,  0.16761522, -0.17413231]), array([ 0.04012653,  0.04887202, -0.00341795,  0.16369621]), array([ 0.04896058,  0.04483812,  0.08966857, -0.20161924]), array([ 0.04751718,  0.04066462, -0.1036719 ,  0.15989458]), array([ 0.03608145,  0.03677286, -0.00864944, -0.19955532]), array([ 0.01720728,  0.03201352, -0.17617777,  0.14942282]), array([-0.00461583,  0.02372424, -0.03809184, -0.23382355]), array([-0.02447932,  0.00976918, -0.15676744,  0.09325948]), array([-0.03799968, -0.01077833,  0.02339896, -0.29677434]), array([-0.04274161, -0.03600156, -0.07044923,  0.04776911]), array([-0.03840229, -0.06173394,  0.11188697, -0.29948506]), array([-0.02704815, -0.08175761, -0.00103029,  0.10395188]), array([-0.01208312, -0.09002918,  0.14717567, -0.18251961]), array([ 0.00248328, -0.08194469, -0.00402095,  0.26378905]), array([ 0.01347812, -0.05663598,  0.11238667, -0.01308476]), array([ 0.01906687, -0.01709075, -0.05618284,  0.40214629]), array([0.01944171, 0.02938882, 0.06110738, 0.05507872]), array([ 0.0426691 ,  0.00488294,  0.16552386, -0.29198549]), array([ 0.05567946, -0.01270791, -0.03830676,  0.12056844]), array([ 0.05476185, -0.01754592,  0.02903159, -0.16796849]), array([ 0.03988309, -0.00865282, -0.17423833,  0.25254733]), array([ 0.01506354,  0.0092458 , -0.06855153, -0.08010439]), array([ 0.01342235, -0.040504  ,  0.05069643, -0.40863199]), array([ 0.00697918, -0.07935649, -0.11469307,  0.02518724]), array([-0.00404282, -0.10065344,  0.0058336 , -0.23581411]), array([-0.01780205, -0.1019573 , -0.14040012,  0.22036821]), array([-0.03090464, -0.08571047,  0.01233408, -0.06238079]), array([-0.03967834, -0.05746832, -0.09728464,  0.33830588]), array([-0.04088649, -0.02479813,  0.0862282 , -0.01699021]), array([-0.03313408,  0.00555571, -0.00916788,  0.31615044]), array([-0.01709824,  0.0286016 ,  0.16671648, -0.08669091]), array([0.00409761, 0.0426896 , 0.04159804, 0.2280058 ]), array([ 0.02591234,  0.04865704,  0.1720678 , -0.16554347]), array([ 0.04318138,  0.04944889, -0.00259859,  0.17554405]), array([ 0.05182717,  0.04793017,  0.08708201, -0.18877447]), array([ 0.04961378,  0.04616405, -0.10855157,  0.17058545]), array([ 0.03710027,  0.04393717, -0.01427681, -0.19404838]), array([ 0.0171644 ,  0.03955664, -0.18094415,  0.14747835]), array([-0.00543206,  0.03008287, -0.04093621, -0.24363824]), array([-0.02563501,  0.01348145, -0.15733974,  0.07702875]), array([-0.03907693, -0.0106912 ,  0.02462454, -0.31615271]), array([-0.04347682, -0.03975416, -0.06843994,  0.0294576 ]), array([-0.03875691, -0.06868657,  0.11350382, -0.31255978]), array([-0.02718902, -0.09055323, -0.0005972 ,  0.09892028]), array([-0.01229391, -0.09889691,  0.14605862, -0.17821307]), array([ 0.00193427, -0.08911365, -0.00617459,  0.27613969]), array([ 0.01246219, -0.0607399 ,  0.11006833,  0.00460279]), array([ 0.01767613, -0.01746661, -0.05742591,  0.42104822]), array([0.01799889, 0.03256356, 0.06194914, 0.07106617]), array([ 0.04164095,  0.01069004,  0.16882221, -0.28203346]), array([ 0.05552767, -0.00565132, -0.03298584,  0.12304419]), array([ 0.05578172, -0.01071831,  0.0351817 , -0.17251072]), array([ 0.04207756, -0.00327057, -0.16892467,  0.24306336]), array([ 0.01809734,  0.01247845, -0.06570728, -0.09161583]), array([ 0.0166784 , -0.03952956,  0.04996191, -0.41928328]), array([ 0.00970175, -0.08024085, -0.11923689,  0.0174798 ]), array([-0.00255012, -0.1027089 , -0.00170788, -0.23980761]), array([-0.01797844, -0.10448545, -0.14921732,  0.21944907]), array([-0.03279817, -0.08822614,  0.00432766, -0.06160815]), array([-0.0429199 , -0.05980691, -0.10248424,  0.3390746 ]), array([-0.04477409, -0.02707825,  0.08509623, -0.01727879]), array([-0.03680915,  0.00308939, -0.00596657,  0.31465325]), array([-0.01976107,  0.02578306,  0.17342083, -0.08849873]), array([0.00298872, 0.03961152, 0.05010813, 0.22750325]), array([ 0.026514  ,  0.04574731,  0.18032288, -0.16312637]), array([0.04524209, 0.0474135 , 0.00347248, 0.18193809]), array([ 0.0547737 ,  0.04756446,  0.089742  , -0.1786232 ]), array([ 0.052719  ,  0.04808358, -0.10958037,  0.182909  ]), array([ 0.03968097,  0.04832029, -0.01831026, -0.18224004]), array([ 0.01875532,  0.04597667, -0.18654323,  0.15553006]), array([-0.00498113,  0.03750945, -0.04647087, -0.24197424]), array([-0.02615815,  0.02046471, -0.16137018,  0.07087075]), array([-0.04018818, -0.00569015,  0.02283148, -0.32956194]), array([-0.04472263, -0.03796813, -0.06807105,  0.0112597 ]), array([-0.03977193, -0.0707079 ,  0.11527201, -0.33173448]), array([-0.02780187, -0.0961543 ,  0.00147775,  0.08294848]), array([-0.01255879, -0.10704514,  0.14731344, -0.1872195 ]), array([ 0.00179073, -0.09820019, -0.00627177,  0.27594249]), array([ 0.01214555, -0.06893478,  0.10850376,  0.01352591]), array([ 0.0169596 , -0.02313884, -0.05971152,  0.43687334]), array([0.01684516, 0.03045181, 0.06007176, 0.0901481 ]), array([ 0.04025325,  0.01235965,  0.16851984, -0.26398233]), array([ 0.05430388, -0.00079913, -0.030983  ,  0.13630429]), array([ 0.0551963 , -0.00390572,  0.03949108, -0.16640006]), array([ 0.04252198,  0.00399475, -0.1631329 ,  0.24156304]), array([ 0.01972951,  0.01878404, -0.05989374, -0.09935726]), array([-0.00719077,  0.03338913, -0.20317714,  0.23831098]), array([-0.03109278,  0.03970184, -0.03105751, -0.17943795]), array([-0.04602812,  0.03220258, -0.11536638,  0.10315408]), array([-0.04857485,  0.00954666,  0.08942957, -0.32567426]), array([-0.03903633, -0.02389749,  0.00315131, -0.00188288]), array([-0.04739862,  0.00891768, -0.08390808,  0.32277384]), array([-0.04389416,  0.03111565,  0.11862509, -0.10351861]), array([-0.02864332,  0.03893335,  0.03120107,  0.18236794]), array([-0.00497513,  0.0334018 ,  0.2002452 , -0.23260361]), array([0.02107596, 0.02016769, 0.05479172, 0.10615778]), array([ 0.04279093,  0.00657729,  0.15735704, -0.23601811]), array([ 0.05432279, -0.00042662, -0.04430346,  0.16843264]), array([ 0.05270667,  0.0025464 ,  0.02841883, -0.13915784]), array([ 0.03836449,  0.0147418 , -0.16827479,  0.25628195]), array([ 0.01530575,  0.03085196, -0.05733159, -0.10110943]), array([-0.01036427,  0.04347995, -0.19356254,  0.22084265]), array([-0.03187717,  0.04515792, -0.01740894, -0.20714614]), array([-0.04403382,  0.03176144, -0.10197892,  0.07334333]), array([-0.04430096,  0.00366435,  0.09821205, -0.34899642]), array([-0.03373534, -0.03322643,  0.0043413 , -0.01230537]), array([-0.04269608, -0.00097066, -0.0909752 ,  0.32760099]), array([-0.04129243,  0.02356253,  0.10519625, -0.08574262]), array([-0.0290492 ,  0.03574529,  0.01530273,  0.2070179 ]), array([-0.00840644,  0.03516068,  0.18665023, -0.20909091]), array([0.01551767, 0.02588013, 0.04766478, 0.12118061]), array([ 0.03666441,  0.01404583,  0.15895883, -0.23385199]), array([ 0.04938654,  0.006138  , -0.03428356,  0.15758913]), array([ 0.05039664,  0.00595369,  0.04402447, -0.15892806]), array([ 0.03936407,  0.01386988, -0.15158915,  0.23451048]), array([ 0.01933942,  0.0260666 , -0.0444065 , -0.11734339]), array([-0.00445233,  0.03651128, -0.18814468,  0.21589742]), array([-0.02577642,  0.03852623, -0.02095712, -0.1988815 ]), array([-0.03946704,  0.027949  , -0.11335767,  0.09252509]), array([-0.04251502,  0.00429218,  0.08248658, -0.3249713 ]), array([-0.03513879, -0.02796251, -0.01104114,  0.00874986]), array([-0.02023327, -0.06097559,  0.15578729, -0.3303973 ]), array([-0.00269428, -0.08508483,  0.01557024,  0.09560047]), array([ 0.01242213, -0.09227187,  0.13213142, -0.16355619]), array([ 0.02111218, -0.07814076, -0.04633684,  0.30331765]), array([ 0.02185659, -0.04415853,  0.05456546,  0.03100886]), array([ 0.04214847, -0.06553987,  0.14341803, -0.23768561]), array([ 0.0497783 , -0.06563303, -0.06836522,  0.23735732]), array([ 0.04297833, -0.04319393,  0.00232915, -0.01764589]), array([ 0.0506473 , -0.07245873,  0.07174425, -0.26846855]), array([ 0.04334158, -0.07746957, -0.14314117,  0.21749326]), array([ 0.02274164, -0.0586999 , -0.05823584, -0.03594645])]</t>
+  </si>
+  <si>
+    <t>['[1,1,2]', '[1,2,0]', '[1,0,2]', '[2,1,0]', '[1,1,1]', '[0,0,0]', '[2,0,1]', '[0,2,1]', '[2,2,2]', '[0,1,1]']</t>
+  </si>
+  <si>
+    <t>[0,0,0]</t>
+  </si>
+  <si>
+    <t>[8, 34, 45, 47, 63, 73, 77]</t>
+  </si>
+  <si>
+    <t>[0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 1, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 2, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+  </si>
+  <si>
+    <t>['[-0.03763371 -0.01533471  0.06554052 -0.01816017]', '[-0.00754409 -0.05458322  0.2277812  -0.36241836]', '[ 0.04879627 -0.15231473  0.32089719 -0.5887683 ]', '[ 0.11397169 -0.27767857  0.31375488 -0.63332862]', '[ 0.16759438 -0.39312519  0.2086893  -0.49480525]', '[ 0.1930193  -0.46685036  0.03906408 -0.22816919]', '[ 0.15689524 -0.41528579 -0.3922057   0.73207416]', '[ 0.04309269 -0.18588535 -0.71796191  1.51055937]', '[-0.08833617  0.09066275 -0.55988174  1.1839315 ]', '[-0.19460404  0.3314577  -0.47333723  1.1656441 ]', '[-0.2670624   0.53551493 -0.23226808  0.83448453]', '[-0.28253496  0.65340003  0.0815849   0.32814701]', '[-0.21144388  0.60081983  0.6145284  -0.8401734 ]', '[-0.04645421  0.3300048   0.9997152  -1.81097325]', '[ 0.16869588 -0.08813379  1.09267552 -2.25742492]', '[ 0.36480578 -0.52268033  0.81394168 -1.98220406]', '[ 0.47749612 -0.84905976  0.28918449 -1.23434024]', '[ 0.47638235 -1.00585569 -0.29746498 -0.32340467]', '[ 0.34226325 -0.92003681 -1.01833061  1.16859442]', '[ 0.08277994 -0.54958257 -1.53003992  2.47635479]', '[-0.24311848  0.02582745 -1.64265914  3.11335998]', '[-0.53505882  0.61885443 -1.19689843  2.66513343]', '[-0.69959443  1.05324151 -0.42043748  1.63398971]', '[-0.6992366   1.26461646  0.41860287  0.47181808]', '[-0.52016686  1.18655453  1.33929365 -1.24961954]', '[-0.18014593  0.76926921  2.0091675  -2.88133359]', '[ 0.25392031  0.07719768  2.22571455 -3.83892195]', '[ 0.65745132 -0.66000022  1.70021104 -3.32185677]', '[ 0.90525742 -1.20486101  0.74365341 -2.08951996]', '[ 0.94937002 -1.49293131 -0.3016355  -0.78796185]', '[ 0.77284694 -1.46663208 -1.43255459  1.06204289]', '[ 0.39274252 -1.06207329 -2.31988111  2.98322662]', '[-0.12921538 -0.29512335 -2.79684459  4.50707858]', '[-0.66235483  0.60791394 -2.37883616  4.20033782]', '[-1.01724128  1.25337291 -1.14035295  2.2469769 ]', '[-1.13379141  1.57027642 -0.01875281  0.92981886]', '[-1.00936867  1.5747652   1.24464069 -0.90129083]', '[-0.64701094  1.19681427  2.34290451 -2.91088278]', '[-0.09228153  0.41159861  3.11477347 -4.81004429]', '[ 0.53172839 -0.58730032  2.9338936  -4.76533473]', '[ 1.02563402 -1.38705935  1.94582662 -3.17620213]', '[ 1.29991828 -1.87066225  0.7838472  -1.70070749]', '[ 1.33666532 -2.0772122  -0.41548899 -0.36874729]', '[ 1.12338211 -1.96859963 -1.6951431   1.48741687]', '[ 0.67180094 -1.46186569 -2.78242933  3.64082988]', '[ 0.04995988 -0.55822341 -3.34143928  5.25396657]', '[-0.61847638  0.55091029 -3.12785763  5.35575188]', '[-1.11688351  1.40026663 -1.81824194  3.12811707]', '[-1.36048616  1.8780604  -0.60863513  1.68900673]', '[-1.3591107   2.08341817  0.61872691  0.36121868]', '[-1.10414811  1.97013407  1.90331541 -1.53262594]', '[-0.61385303  1.44866557  2.95397919 -3.7414322 ]', '[ 0.05724236  0.46373892  3.66487287 -5.96147017]', '[ 0.76783835 -0.74390531  3.20972259 -5.5888534 ]', '[ 1.28823418 -1.67208479  1.96365663 -3.71496527]', '[ 1.55124703 -2.26185432  0.66610534 -2.23881694]', '[ 1.55611401 -2.57674719 -0.6104529  -0.90837444]', '[ 1.29930081 -2.57888194 -1.93632915  0.91062595]', '[ 0.79749144 -2.1991213  -3.01589225  2.93302445]', '[ 0.12595936 -1.38423786 -3.63513664  5.25895259]', '[-0.63252303 -0.11905254 -3.79491319  7.01649398]', '[-1.28473446  1.16766729 -2.55650283  5.50028679]', '[-1.64036136  2.0853955  -1.00785995  3.77286619]', '[-1.68278131  2.6586417   0.54969559  1.98315864]', '[-1.4374758   2.89630239  1.88266878  0.38271192]', '[-0.93442555  2.79059867  3.09502997 -1.4373823 ]', '[-0.23909866  2.32300801  3.71798349 -3.2322712 ]', '[ 0.4939028   1.5078573   3.51748458 -4.86399095]', '[ 1.14899447  0.42021293  2.97833681 -5.81105259]', '[ 1.63918079 -0.69178591  1.80781711 -5.06541564]', '[ 1.8426583  -1.57108583  0.18778203 -3.7206612 ]', '[ 1.70451708 -2.17102794 -1.57135428 -2.22050242]', '[ 1.21399523 -2.38923252 -3.26188157  0.09921346]', '[ 0.45494295 -2.15644316 -4.18058454  2.23532284]', '[-0.39962467 -1.46923606 -4.21505836  4.5395452 ]', '[-1.19339056 -0.41066914 -3.64635848  5.7666148 ]', '[-1.81552833  0.69249991 -2.49389855  5.03367952]', '[-2.16065614  1.53540796 -0.98061959  3.49662539]', '[-2.22657798  2.16071559  0.33537889  2.73922726]', '[-2.02297049  2.61002342  1.70071232  1.68197696]', '[-1.54247816e+00  2.78457758e+00  3.09210616e+00  1.02053027e-03]', '[-0.79410331  2.57118097  4.29994413 -2.17730056]', '[ 0.11290685  1.90287361  4.59126736 -4.49982148]', '[ 0.99226337  0.79999191  4.1479839  -6.35436232]', '[ 1.7364473  -0.49076324  3.16652009 -6.1482712 ]', '[ 2.22824098 -1.58646881  1.75368593 -4.87164434]', '[ 2.44459363 -2.47721855  0.44054438 -4.08487096]', '[ 2.42886744  3.06166175 -0.50958574 -3.34203982]', '[ 2.26936194  2.47834332 -1.05353527 -2.4750735 ]', '[ 2.00389836  2.07414074 -1.63181196 -1.57965856]']</t>
+  </si>
+  <si>
+    <t>[array([-0.03763371, -0.01533471,  0.06554052, -0.01816017], dtype=float32), array([-0.00754409, -0.05458322,  0.2277812 , -0.36241836]), array([ 0.04879627, -0.15231473,  0.32089719, -0.5887683 ]), array([ 0.11397169, -0.27767857,  0.31375488, -0.63332862]), array([ 0.16759438, -0.39312519,  0.2086893 , -0.49480525]), array([ 0.1930193 , -0.46685036,  0.03906408, -0.22816919]), array([ 0.15689524, -0.41528579, -0.3922057 ,  0.73207416]), array([ 0.04309269, -0.18588535, -0.71796191,  1.51055937]), array([-0.08833617,  0.09066275, -0.55988174,  1.1839315 ]), array([-0.19460404,  0.3314577 , -0.47333723,  1.1656441 ]), array([-0.2670624 ,  0.53551493, -0.23226808,  0.83448453]), array([-0.28253496,  0.65340003,  0.0815849 ,  0.32814701]), array([-0.21144388,  0.60081983,  0.6145284 , -0.8401734 ]), array([-0.04645421,  0.3300048 ,  0.9997152 , -1.81097325]), array([ 0.16869588, -0.08813379,  1.09267552, -2.25742492]), array([ 0.36480578, -0.52268033,  0.81394168, -1.98220406]), array([ 0.47749612, -0.84905976,  0.28918449, -1.23434024]), array([ 0.47638235, -1.00585569, -0.29746498, -0.32340467]), array([ 0.34226325, -0.92003681, -1.01833061,  1.16859442]), array([ 0.08277994, -0.54958257, -1.53003992,  2.47635479]), array([-0.24311848,  0.02582745, -1.64265914,  3.11335998]), array([-0.53505882,  0.61885443, -1.19689843,  2.66513343]), array([-0.69959443,  1.05324151, -0.42043748,  1.63398971]), array([-0.6992366 ,  1.26461646,  0.41860287,  0.47181808]), array([-0.52016686,  1.18655453,  1.33929365, -1.24961954]), array([-0.18014593,  0.76926921,  2.0091675 , -2.88133359]), array([ 0.25392031,  0.07719768,  2.22571455, -3.83892195]), array([ 0.65745132, -0.66000022,  1.70021104, -3.32185677]), array([ 0.90525742, -1.20486101,  0.74365341, -2.08951996]), array([ 0.94937002, -1.49293131, -0.3016355 , -0.78796185]), array([ 0.77284694, -1.46663208, -1.43255459,  1.06204289]), array([ 0.39274252, -1.06207329, -2.31988111,  2.98322662]), array([-0.12921538, -0.29512335, -2.79684459,  4.50707858]), array([-0.66235483,  0.60791394, -2.37883616,  4.20033782]), array([-1.01724128,  1.25337291, -1.14035295,  2.2469769 ]), array([-1.13379141,  1.57027642, -0.01875281,  0.92981886]), array([-1.00936867,  1.5747652 ,  1.24464069, -0.90129083]), array([-0.64701094,  1.19681427,  2.34290451, -2.91088278]), array([-0.09228153,  0.41159861,  3.11477347, -4.81004429]), array([ 0.53172839, -0.58730032,  2.9338936 , -4.76533473]), array([ 1.02563402, -1.38705935,  1.94582662, -3.17620213]), array([ 1.29991828, -1.87066225,  0.7838472 , -1.70070749]), array([ 1.33666532, -2.0772122 , -0.41548899, -0.36874729]), array([ 1.12338211, -1.96859963, -1.6951431 ,  1.48741687]), array([ 0.67180094, -1.46186569, -2.78242933,  3.64082988]), array([ 0.04995988, -0.55822341, -3.34143928,  5.25396657]), array([-0.61847638,  0.55091029, -3.12785763,  5.35575188]), array([-1.11688351,  1.40026663, -1.81824194,  3.12811707]), array([-1.36048616,  1.8780604 , -0.60863513,  1.68900673]), array([-1.3591107 ,  2.08341817,  0.61872691,  0.36121868]), array([-1.10414811,  1.97013407,  1.90331541, -1.53262594]), array([-0.61385303,  1.44866557,  2.95397919, -3.7414322 ]), array([ 0.05724236,  0.46373892,  3.66487287, -5.96147017]), array([ 0.76783835, -0.74390531,  3.20972259, -5.5888534 ]), array([ 1.28823418, -1.67208479,  1.96365663, -3.71496527]), array([ 1.55124703, -2.26185432,  0.66610534, -2.23881694]), array([ 1.55611401, -2.57674719, -0.6104529 , -0.90837444]), array([ 1.29930081, -2.57888194, -1.93632915,  0.91062595]), array([ 0.79749144, -2.1991213 , -3.01589225,  2.93302445]), array([ 0.12595936, -1.38423786, -3.63513664,  5.25895259]), array([-0.63252303, -0.11905254, -3.79491319,  7.01649398]), array([-1.28473446,  1.16766729, -2.55650283,  5.50028679]), array([-1.64036136,  2.0853955 , -1.00785995,  3.77286619]), array([-1.68278131,  2.6586417 ,  0.54969559,  1.98315864]), array([-1.4374758 ,  2.89630239,  1.88266878,  0.38271192]), array([-0.93442555,  2.79059867,  3.09502997, -1.4373823 ]), array([-0.23909866,  2.32300801,  3.71798349, -3.2322712 ]), array([ 0.4939028 ,  1.5078573 ,  3.51748458, -4.86399095]), array([ 1.14899447,  0.42021293,  2.97833681, -5.81105259]), array([ 1.63918079, -0.69178591,  1.80781711, -5.06541564]), array([ 1.8426583 , -1.57108583,  0.18778203, -3.7206612 ]), array([ 1.70451708, -2.17102794, -1.57135428, -2.22050242]), array([ 1.21399523, -2.38923252, -3.26188157,  0.09921346]), array([ 0.45494295, -2.15644316, -4.18058454,  2.23532284]), array([-0.39962467, -1.46923606, -4.21505836,  4.5395452 ]), array([-1.19339056, -0.41066914, -3.64635848,  5.7666148 ]), array([-1.81552833,  0.69249991, -2.49389855,  5.03367952]), array([-2.16065614,  1.53540796, -0.98061959,  3.49662539]), array([-2.22657798,  2.16071559,  0.33537889,  2.73922726]), array([-2.02297049,  2.61002342,  1.70071232,  1.68197696]), array([-1.54247816e+00,  2.78457758e+00,  3.09210616e+00,  1.02053027e-03]), array([-0.79410331,  2.57118097,  4.29994413, -2.17730056]), array([ 0.11290685,  1.90287361,  4.59126736, -4.49982148]), array([ 0.99226337,  0.79999191,  4.1479839 , -6.35436232]), array([ 1.7364473 , -0.49076324,  3.16652009, -6.1482712 ]), array([ 2.22824098, -1.58646881,  1.75368593, -4.87164434]), array([ 2.44459363, -2.47721855,  0.44054438, -4.08487096]), array([ 2.42886744,  3.06166175, -0.50958574, -3.34203982]), array([ 2.26936194,  2.47834332, -1.05353527, -2.4750735 ]), array([ 2.00389836,  2.07414074, -1.63181196, -1.57965856])]</t>
+  </si>
+  <si>
+    <t>['[0,2,1]', '[0,1,1]', '[0,0,0]', '[2,2,2]', '[1,0,2]', '[1,1,2]', '[2,1,0]', '[1,2,0]', '[2,0,1]', '[1,1,1]']</t>
+  </si>
+  <si>
+    <t>[7, 8, 22, 23, 31, 34, 42, 45, 47, 57, 60, 70, 73, 74, 84, 88, 89, 90, 101, 106]</t>
+  </si>
+  <si>
+    <t>[0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 1, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 1, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 1, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 1, 2, 2, 2, 2, 2, 2, 2, 2, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+  </si>
+  <si>
+    <t>['[-0.03763371 -0.01533471  0.06554052 -0.01816017]', '[-0.00754409 -0.05458322  0.2277812  -0.36241836]', '[ 0.04879627 -0.15231473  0.32089719 -0.5887683 ]', '[ 0.11397169 -0.27767857  0.31375488 -0.63332862]', '[ 0.16759438 -0.39312519  0.2086893  -0.49480525]', '[ 0.1930193  -0.46685036  0.03906408 -0.22816919]', '[ 0.15689524 -0.41528579 -0.3922057   0.73207416]', '[ 0.06912431 -0.2533688  -0.46320736  0.84724268]', '[-0.01860077 -0.09405544 -0.39115728  0.70438893]', '[-0.10545168  0.08172492 -0.45391444  1.00879274]', '[-0.18986196  0.28911204 -0.36628196  1.01600317]', '[-0.24335408  0.46975101 -0.15337892  0.75465706]', '[-0.24733499  0.58016849  0.11589752  0.33425395]', '[-0.1740036   0.53661102  0.60167266 -0.75519424]', '[-0.01665944  0.29117218  0.9366974  -1.64334085]', '[ 0.1820328  -0.08758353  0.99640406 -2.04237684]', '[ 0.35882125 -0.48111665  0.72271169 -1.79803256]', '[ 0.455889   -0.77723617  0.22614365 -1.11753753]', '[ 0.44557276 -0.91744837 -0.32586708 -0.27414406]', '[ 0.30877283 -0.82728764 -1.0158762   1.15971739]', '[ 0.05368593 -0.46718153 -1.48597077  2.37394348]', '[-0.25833433  0.07564064 -1.55072277  2.89599791]', '[-0.50521312  0.5556418  -0.859951    1.79847698]', '[-0.58924919  0.77376208  0.03059389  0.36389618]', '[-0.49412298  0.69953204  0.90435333 -1.09721091]', '[-0.23969589  0.3461743   1.59011613 -2.36852316]', '[ 0.11184781 -0.19738308  1.83110307 -2.89320279]', '[ 0.45231675 -0.73569405  1.49303979 -2.35130729]', '[ 0.68557382 -1.1044708   0.80351381 -1.30030284]', '[ 0.764998   -1.2505531  -0.01821658 -0.15711698]', '[ 0.65866333 -1.11160637 -1.03363324  1.55058198]', '[ 0.38305275 -0.69148231 -1.67717429  2.60102774]', '[-0.01012484 -0.04661379 -2.1574021   3.66988329]', '[-0.4282025   0.67393773 -1.90748199  3.31201849]', '[-0.71809221  1.16512583 -0.95809891  1.57642188]', '[-0.82434305  1.36034486 -0.09335078  0.37451961]', '[-0.736005    1.26153106  0.96684138 -1.36875098]', '[-0.44488208  0.80881171  1.91305581 -3.1483066 ]', '[ 0.0047178   0.03461529  2.46951515 -4.37859729]', '[ 0.47929313 -0.8117225   2.14181236 -3.81936964]', '[ 0.82750168 -1.43920792  1.29884148 -2.42672381]', '[ 0.98968513 -1.7861879   0.3118309  -1.05684879]', '[ 0.95155545 -1.86469197 -0.68387266  0.27311384]', '[ 0.70858305 -1.62646332 -1.71590277  2.13017505]', '[ 0.27929295 -1.00233464 -2.53749694  4.11472765]', '[-0.25276975 -0.08512622 -2.64022734  4.76586042]', '[-0.73168316  0.82061361 -2.01281998  4.02224444]', '[-1.00817373  1.42513736 -0.74020925  2.04429678]', '[-1.04569441  1.69897268  0.36208609  0.69572512]', '[-0.85332481  1.65242198  1.53025983 -1.17776337]', '[-0.45015835  1.2180526   2.45437527 -3.18255329]', '[ 0.10510472  0.3906718   3.00242807 -4.93122598]', '[ 0.68325012 -0.61041686  2.60018922 -4.69707168]', '[ 1.09677346 -1.39906341  1.48820898 -3.15290657]', '[ 1.27180657 -1.88285495  0.2569567  -1.71083858]', '[ 1.20078118 -2.08623079 -0.95399697 -0.31307338]', '[ 0.88716796 -1.95585608 -2.13576446  1.64620473]', '[ 0.38663658 -1.4626706  -2.79911931  3.28677964]', '[-0.22296391 -0.60156074 -3.21487943  5.20002096]', '[-0.83828974  0.48216067 -2.74909527  5.2122819 ]', '[-1.24494907  1.31517611 -1.28719097  3.10996932]', '[-1.37086447  1.79684922  0.03160074  1.72114621]', '[-1.23432576  2.00040296  1.31668149  0.28815467]', '[-0.84399933  1.85302959  2.52769576 -1.80214255]', '[-0.25310715  1.26499922  3.30699868 -4.08937071]', '[ 0.44653743  0.24708491  3.55739742 -5.80699892]', '[ 1.08554029 -0.85893375  2.66478924 -4.88639621]', '[ 1.4838664  -1.66849755  1.30494205 -3.25669264]', '[ 1.60698147 -2.18312718 -0.07138056 -1.91054863]', '[ 1.45198002 -2.40818888 -1.46123333 -0.31384862]', '[ 1.03973413 -2.31467968 -2.61478127  1.28700685]', '[ 0.42383296 -1.83707101 -3.44616681  3.52067218]', '[-0.30178538 -0.90380255 -3.74006373  5.74168625]', '[-0.99766494  0.27364439 -3.0254376   5.55303213]', '[-1.45237132  1.18590995 -1.48137704  3.52938727]', '[-1.60875507  1.75988041 -0.07526116  2.22828881]', '[-1.48141936  2.07192524  1.34188131  0.85121536]', '[-1.06823575  2.03434632  2.73593023 -1.28883879]', '[-0.4193122   1.53243654  3.66084594 -3.77210916]', '[ 0.36016627  0.53247608  4.02849163 -6.03648658]', '[ 1.11257101 -0.6824746   3.28730649 -5.60366441]', '[ 1.63198721 -1.62380995  1.89571227 -3.86150425]', '[ 1.87446742 -2.26429987  0.53873999 -2.59884896]', '[ 1.8516124  -2.66824052 -0.75667692 -1.4235738 ]', '[ 1.57473067 -2.82129045 -2.0064331  -0.07323788]', '[ 1.04346071 -2.64557167 -3.25906847  1.86392708]', '[ 0.30938556 -2.06072302 -3.95255626  4.02220803]', '[-0.49104166 -1.03186613 -3.99015363  6.21051194]', '[-1.2233016   0.24535818 -3.14824108  6.06543427]', '[-1.69066299  1.25719113 -1.49292997  4.03163739]', '[-1.82445072  1.89018367  0.14482259  2.34122518]', '[-1.64908268  2.23188512  1.60663422  1.01605253]', '[-1.17692516  2.22565822  3.06330742 -1.15382017]', '[-0.45850942  1.74178893  4.00949301 -3.74069443]', '[ 0.38392881  0.72736176  4.32286713 -6.26609116]', '[ 1.20101542 -0.57714333  3.62672814 -6.19371648]', '[ 1.78224133 -1.63051014  2.18044991 -4.39387532]', '[ 2.08241948 -2.38331096  0.84575097 -3.21231723]', '[ 2.13151491 -2.9255896  -0.32416402 -2.20228353]', '[ 1.95525531  3.04835684 -1.43537771 -0.86450673]', '[ 1.54531199  3.03916974 -2.68313542  0.78119357]', '[ 0.89473267 -2.96126064 -3.77058899  2.04457487]', '[ 0.07433434 -2.38604154 -4.25685975  3.71182426]', '[-0.73877984 -1.4867178  -3.78166471  5.21093499]', '[-1.42638553 -0.35283563 -3.05634957  5.91710189]', '[-1.92520441  0.7690137  -1.84830191  5.12478405]', '[-2.12735636  1.63075816 -0.16683078  3.54724171]', '[-2.0012943   2.23248435  1.44698732  2.3971111 ]', '[-1.54446861  2.53310594  3.08925761  0.52306551]', '[-0.78359405  2.39346063  4.40530259 -1.97477056]', '[ 0.14753533  1.73358502  4.72609983 -4.59874463]', '[ 1.05804955  0.59797522  4.30760471 -6.504445  ]', '[ 1.82158394 -0.68276088  3.20852513 -5.91902402]', '[ 2.32758534 -1.73477366  1.88230983 -4.71407599]', '[ 2.58852241 -2.61118986  0.7781594  -4.10762347]', '[ 2.6708444   2.90057178  0.14821639 -3.59921622]', '[ 2.67988411  2.24027094 -0.0181051  -2.98364808]', '[ 2.6631949   1.71595321 -0.17259036 -2.23871961]']</t>
+  </si>
+  <si>
+    <t>[0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50, 51, 52, 53, 54, 55, 56, 57, 58, 59, 60, 61, 62, 63, 64, 65, 66, 67, 68, 69, 70, 71, 72, 73, 74, 75, 76, 77, 78, 79, 80, 81, 82, 83, 84, 85, 86, 87, 88, 89, 90, 91, 92, 93, 94, 95, 96, 97, 98, 99, 100, 101, 102, 103, 104, 105, 106, 107, 108, 109, 110, 111, 112, 113, 114, 115, 116, 117]</t>
+  </si>
+  <si>
+    <t>[array([-0.03763371, -0.01533471,  0.06554052, -0.01816017], dtype=float32), array([-0.00754409, -0.05458322,  0.2277812 , -0.36241836]), array([ 0.04879627, -0.15231473,  0.32089719, -0.5887683 ]), array([ 0.11397169, -0.27767857,  0.31375488, -0.63332862]), array([ 0.16759438, -0.39312519,  0.2086893 , -0.49480525]), array([ 0.1930193 , -0.46685036,  0.03906408, -0.22816919]), array([ 0.15689524, -0.41528579, -0.3922057 ,  0.73207416]), array([ 0.06912431, -0.2533688 , -0.46320736,  0.84724268]), array([-0.01860077, -0.09405544, -0.39115728,  0.70438893]), array([-0.10545168,  0.08172492, -0.45391444,  1.00879274]), array([-0.18986196,  0.28911204, -0.36628196,  1.01600317]), array([-0.24335408,  0.46975101, -0.15337892,  0.75465706]), array([-0.24733499,  0.58016849,  0.11589752,  0.33425395]), array([-0.1740036 ,  0.53661102,  0.60167266, -0.75519424]), array([-0.01665944,  0.29117218,  0.9366974 , -1.64334085]), array([ 0.1820328 , -0.08758353,  0.99640406, -2.04237684]), array([ 0.35882125, -0.48111665,  0.72271169, -1.79803256]), array([ 0.455889  , -0.77723617,  0.22614365, -1.11753753]), array([ 0.44557276, -0.91744837, -0.32586708, -0.27414406]), array([ 0.30877283, -0.82728764, -1.0158762 ,  1.15971739]), array([ 0.05368593, -0.46718153, -1.48597077,  2.37394348]), array([-0.25833433,  0.07564064, -1.55072277,  2.89599791]), array([-0.50521312,  0.5556418 , -0.859951  ,  1.79847698]), array([-0.58924919,  0.77376208,  0.03059389,  0.36389618]), array([-0.49412298,  0.69953204,  0.90435333, -1.09721091]), array([-0.23969589,  0.3461743 ,  1.59011613, -2.36852316]), array([ 0.11184781, -0.19738308,  1.83110307, -2.89320279]), array([ 0.45231675, -0.73569405,  1.49303979, -2.35130729]), array([ 0.68557382, -1.1044708 ,  0.80351381, -1.30030284]), array([ 0.764998  , -1.2505531 , -0.01821658, -0.15711698]), array([ 0.65866333, -1.11160637, -1.03363324,  1.55058198]), array([ 0.38305275, -0.69148231, -1.67717429,  2.60102774]), array([-0.01012484, -0.04661379, -2.1574021 ,  3.66988329]), array([-0.4282025 ,  0.67393773, -1.90748199,  3.31201849]), array([-0.71809221,  1.16512583, -0.95809891,  1.57642188]), array([-0.82434305,  1.36034486, -0.09335078,  0.37451961]), array([-0.736005  ,  1.26153106,  0.96684138, -1.36875098]), array([-0.44488208,  0.80881171,  1.91305581, -3.1483066 ]), array([ 0.0047178 ,  0.03461529,  2.46951515, -4.37859729]), array([ 0.47929313, -0.8117225 ,  2.14181236, -3.81936964]), array([ 0.82750168, -1.43920792,  1.29884148, -2.42672381]), array([ 0.98968513, -1.7861879 ,  0.3118309 , -1.05684879]), array([ 0.95155545, -1.86469197, -0.68387266,  0.27311384]), array([ 0.70858305, -1.62646332, -1.71590277,  2.13017505]), array([ 0.27929295, -1.00233464, -2.53749694,  4.11472765]), array([-0.25276975, -0.08512622, -2.64022734,  4.76586042]), array([-0.73168316,  0.82061361, -2.01281998,  4.02224444]), array([-1.00817373,  1.42513736, -0.74020925,  2.04429678]), array([-1.04569441,  1.69897268,  0.36208609,  0.69572512]), array([-0.85332481,  1.65242198,  1.53025983, -1.17776337]), array([-0.45015835,  1.2180526 ,  2.45437527, -3.18255329]), array([ 0.10510472,  0.3906718 ,  3.00242807, -4.93122598]), array([ 0.68325012, -0.61041686,  2.60018922, -4.69707168]), array([ 1.09677346, -1.39906341,  1.48820898, -3.15290657]), array([ 1.27180657, -1.88285495,  0.2569567 , -1.71083858]), array([ 1.20078118, -2.08623079, -0.95399697, -0.31307338]), array([ 0.88716796, -1.95585608, -2.13576446,  1.64620473]), array([ 0.38663658, -1.4626706 , -2.79911931,  3.28677964]), array([-0.22296391, -0.60156074, -3.21487943,  5.20002096]), array([-0.83828974,  0.48216067, -2.74909527,  5.2122819 ]), array([-1.24494907,  1.31517611, -1.28719097,  3.10996932]), array([-1.37086447,  1.79684922,  0.03160074,  1.72114621]), array([-1.23432576,  2.00040296,  1.31668149,  0.28815467]), array([-0.84399933,  1.85302959,  2.52769576, -1.80214255]), array([-0.25310715,  1.26499922,  3.30699868, -4.08937071]), array([ 0.44653743,  0.24708491,  3.55739742, -5.80699892]), array([ 1.08554029, -0.85893375,  2.66478924, -4.88639621]), array([ 1.4838664 , -1.66849755,  1.30494205, -3.25669264]), array([ 1.60698147, -2.18312718, -0.07138056, -1.91054863]), array([ 1.45198002, -2.40818888, -1.46123333, -0.31384862]), array([ 1.03973413, -2.31467968, -2.61478127,  1.28700685]), array([ 0.42383296, -1.83707101, -3.44616681,  3.52067218]), array([-0.30178538, -0.90380255, -3.74006373,  5.74168625]), array([-0.99766494,  0.27364439, -3.0254376 ,  5.55303213]), array([-1.45237132,  1.18590995, -1.48137704,  3.52938727]), array([-1.60875507,  1.75988041, -0.07526116,  2.22828881]), array([-1.48141936,  2.07192524,  1.34188131,  0.85121536]), array([-1.06823575,  2.03434632,  2.73593023, -1.28883879]), array([-0.4193122 ,  1.53243654,  3.66084594, -3.77210916]), array([ 0.36016627,  0.53247608,  4.02849163, -6.03648658]), array([ 1.11257101, -0.6824746 ,  3.28730649, -5.60366441]), array([ 1.63198721, -1.62380995,  1.89571227, -3.86150425]), array([ 1.87446742, -2.26429987,  0.53873999, -2.59884896]), array([ 1.8516124 , -2.66824052, -0.75667692, -1.4235738 ]), array([ 1.57473067, -2.82129045, -2.0064331 , -0.07323788]), array([ 1.04346071, -2.64557167, -3.25906847,  1.86392708]), array([ 0.30938556, -2.06072302, -3.95255626,  4.02220803]), array([-0.49104166, -1.03186613, -3.99015363,  6.21051194]), array([-1.2233016 ,  0.24535818, -3.14824108,  6.06543427]), array([-1.69066299,  1.25719113, -1.49292997,  4.03163739]), array([-1.82445072,  1.89018367,  0.14482259,  2.34122518]), array([-1.64908268,  2.23188512,  1.60663422,  1.01605253]), array([-1.17692516,  2.22565822,  3.06330742, -1.15382017]), array([-0.45850942,  1.74178893,  4.00949301, -3.74069443]), array([ 0.38392881,  0.72736176,  4.32286713, -6.26609116]), array([ 1.20101542, -0.57714333,  3.62672814, -6.19371648]), array([ 1.78224133, -1.63051014,  2.18044991, -4.39387532]), array([ 2.08241948, -2.38331096,  0.84575097, -3.21231723]), array([ 2.13151491, -2.9255896 , -0.32416402, -2.20228353]), array([ 1.95525531,  3.04835684, -1.43537771, -0.86450673]), array([ 1.54531199,  3.03916974, -2.68313542,  0.78119357]), array([ 0.89473267, -2.96126064, -3.77058899,  2.04457487]), array([ 0.07433434, -2.38604154, -4.25685975,  3.71182426]), array([-0.73877984, -1.4867178 , -3.78166471,  5.21093499]), array([-1.42638553, -0.35283563, -3.05634957,  5.91710189]), array([-1.92520441,  0.7690137 , -1.84830191,  5.12478405]), array([-2.12735636,  1.63075816, -0.16683078,  3.54724171]), array([-2.0012943 ,  2.23248435,  1.44698732,  2.3971111 ]), array([-1.54446861,  2.53310594,  3.08925761,  0.52306551]), array([-0.78359405,  2.39346063,  4.40530259, -1.97477056]), array([ 0.14753533,  1.73358502,  4.72609983, -4.59874463]), array([ 1.05804955,  0.59797522,  4.30760471, -6.504445  ]), array([ 1.82158394, -0.68276088,  3.20852513, -5.91902402]), array([ 2.32758534, -1.73477366,  1.88230983, -4.71407599]), array([ 2.58852241, -2.61118986,  0.7781594 , -4.10762347]), array([ 2.6708444 ,  2.90057178,  0.14821639, -3.59921622]), array([ 2.67988411,  2.24027094, -0.0181051 , -2.98364808]), array([ 2.6631949 ,  1.71595321, -0.17259036, -2.23871961])]</t>
+  </si>
+  <si>
+    <t>['[2,1,0]', '[1,0,2]', '[0,2,1]', '[1,2,0]', '[2,0,1]', '[2,2,2]', '[1,1,1]', '[0,0,0]', '[0,1,1]', '[1,1,2]']</t>
+  </si>
+  <si>
+    <t>[6, 7, 9, 10, 11, 21, 22, 28, 30, 31, 33, 34, 40, 41, 43, 44, 53, 54, 57, 58, 67, 71, 72, 81, 82, 83, 84, 85, 92, 94, 95, 96, 109, 110, 112, 114, 123, 125]</t>
+  </si>
+  <si>
+    <t>[0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 1, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 1, 2, 2, 2, 2, 2, 2, 2, 1, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+  </si>
+  <si>
+    <t>['[-0.03763371 -0.01533471  0.06554052 -0.01816017]', '[-0.00754409 -0.05458322  0.2277812  -0.36241836]', '[ 0.04879627 -0.15231473  0.32089719 -0.5887683 ]', '[ 0.11397169 -0.27767857  0.31375488 -0.63332862]', '[ 0.16759438 -0.39312519  0.2086893  -0.49480525]', '[ 0.1930193  -0.46685036  0.03906408 -0.22816919]', '[ 0.18217995 -0.48119372 -0.14531723  0.08492936]', '[ 0.13737799 -0.43548032 -0.29255645  0.35879992]', '[ 0.0448411  -0.27859812 -0.61146179  1.17448612]', '[-0.06860641 -0.05622008 -0.49256054  0.99183019]', '[-0.14124543  0.09729776 -0.21467558  0.50620575]', '[-0.14968433  0.13659429  0.13257963 -0.120111  ]', '[-0.0905776   0.05231674  0.44376485 -0.69898246]', '[ 0.01880609 -0.12769834  0.62170324 -1.05159645]', '[ 0.14493442 -0.34499409  0.60714543 -1.06399616]', '[ 0.2492602  -0.53163849  0.41137671 -0.7601214 ]', '[ 0.30177805 -0.63610881  0.10256253 -0.26547779]', '[ 0.26401674 -0.57024939 -0.47283708  0.91356453]', '[ 0.11991419 -0.28235468 -0.93593667  1.90832825]', '[-0.09085923  0.15628831 -1.11091308  2.35896477]', '[-0.29761807  0.60847034 -0.90020751  2.05390538]', '[-0.41069544  0.88510218 -0.21555102  0.68736841]', '[-0.38248204  0.88034003  0.49131012 -0.73169907]', '[-0.22011253  0.59777265  1.10565551 -2.05912033]', '[ 0.04198696  0.08588341  1.44821645 -2.9337883 ]', '[ 0.32381283 -0.50597909  1.28487283 -2.81704938]', '[ 0.52817405 -0.98902677  0.71746561 -1.94274586]', '[ 0.60205781 -1.26965447  0.01563191 -0.85127352]', '[ 0.53665857 -1.32822334 -0.65356945  0.26267136]', '[ 0.33107242 -1.11337428 -1.37083846  1.87505763]', '[ 0.02672801 -0.65051049 -1.61491464  2.6696507 ]', '[-0.28497233 -0.09844566 -1.41912857  2.69088609]', '[-0.53420411  0.42904373 -1.00314221  2.44710891]', '[-0.6409175   0.77642315 -0.04741911  0.99110737]', '[-0.55414419  0.82054184  0.89737643 -0.54934066]', '[-0.29440684  0.56195104  1.65355245 -1.99489777]', '[ 0.08038864  0.05872726  2.0048716  -2.88578608]', '[ 0.46437983 -0.51259627  1.73704928 -2.64951159]', '[ 0.74425899 -0.95075812  1.01379778 -1.67177504]', '[ 0.85843732 -1.17196712  0.11500361 -0.5333711 ]', '[ 0.78962215 -1.16252654 -0.79303772  0.63121642]', '[ 0.54995088 -0.91926188 -1.56832114  1.78676992]', '[ 0.15915896 -0.40223389 -2.26826114  3.28861648]', '[-0.28715876  0.24943393 -2.07331002  2.99513889]', '[-0.62862829  0.72107427 -1.27640378  1.6282928 ]', '[-0.80521144  0.94772876 -0.46395491  0.62006415]', '[-0.80916431  0.96669553  0.42451037 -0.43121672]', '[-0.6170793   0.71522591  1.47274641 -2.07517611]', '[-0.23803471  0.15495792  2.23808476 -3.39877346]', '[ 0.22987034 -0.55207553  2.31149819 -3.41906642]', '[ 0.64225818 -1.13335625  1.74033385 -2.29967333]', '[ 0.90675886 -1.46055646  0.87359505 -0.97451644]', '[ 0.98370315 -1.52701012 -0.11277244  0.30374935]', '[ 0.86214299 -1.33851269 -1.0910309   1.58815843]', '[ 0.55647916 -0.88952347 -1.92746095  2.88382265]', '[ 0.09171146 -0.15033652 -2.61846151  4.32828249]', '[-0.42773828  0.71246604 -2.42525879  3.9943164 ]', '[-0.81571045  1.31982822 -1.41510183  2.06376843]', '[-0.98510433  1.54761665 -0.26624589  0.23584613]', '[-0.91993672  1.41685458  0.91574724 -1.55400589]', '[-0.62254293  0.91601464  2.03762476 -3.471856  ]', '[-0.12555443  0.04900021  2.81205084 -4.97054508]', '[ 0.42727303 -0.91333982  2.55736859 -4.3279059 ]', '[ 0.86018856 -1.62335278  1.72726089 -2.75786999]', '[ 1.10656782 -2.0271457   0.71674349 -1.30761758]', '[ 1.14239982 -2.15319713 -0.35935458  0.04215541]', '[ 0.95250797 -1.96403932 -1.51903624  1.87217332]', '[ 0.56287258 -1.43731059 -2.33646351  3.41642527]', '[ 0.01635347 -0.54292712 -3.05861136  5.43245557]', '[-0.59313802  0.59333823 -2.81954932  5.45895377]', '[-1.04843197  1.51848961 -1.67960161  3.74674003]', '[-1.24413149  2.06426228 -0.28725581  1.76897343]', '[-1.16860964  2.2355082   1.02231734 -0.05702219]', '[-0.84773317  2.03501351  2.14108511 -1.97455245]', '[-0.33523891  1.43201691  2.92865716 -4.08697117]', '[ 0.30211814  0.40567329  3.34773335 -5.99076774]', '[ 0.92154366 -0.7772247   2.64045186 -5.39044928]', '[ 1.31399416 -1.67743423  1.25886426 -3.6351397 ]', '[ 1.42444284 -2.25248702 -0.14665541 -2.14165023]', '[ 1.26197901 -2.53458517 -1.45190042 -0.67000827]', '[ 0.84769032 -2.47666089 -2.6252117   1.25324357]', '[ 0.2626396  -2.07627416 -3.11091292  2.72668697]', '[-0.3494054  -1.40838582 -2.91624636  3.85832955]', '[-0.87354551 -0.59079377 -2.25144995  4.12819787]', '[-1.21601519  0.15676389 -1.10072346  3.18145308]', '[-1.29491653  0.64448622  0.33303095  1.65126051]', '[-1.10306949  0.86327316  1.58633846  0.47563194]', '[-0.64781423  0.75072295  2.90291173 -1.61990724]', '[ 0.01730848  0.23936588  3.60353476 -3.29217529]', '[ 0.72015939 -0.43136361  3.25552602 -3.09424467]', '[ 1.27124549 -0.91906129  2.1959282  -1.74209091]', '[ 1.58994006 -1.14497286  0.98853238 -0.57938177]', '[ 1.6683853  -1.17112369 -0.20055864  0.29457717]', '[ 1.48840354 -0.96628382 -1.6052063   1.80271154]', '[ 1.04884024 -0.4877698  -2.76702913  2.99049828]', '[ 0.40918863  0.18887187 -3.50175663  3.52462411]', '[-0.28381998  0.78532968 -3.26761634  2.17601745]', '[-0.86531329  1.05787189 -2.44079899  0.49825989]', '[-1.23064972  0.99322448 -1.17745458 -1.08367881]', '[-1.30889885  0.59001877  0.39078845 -2.90316584]', '[-1.08529282 -0.14703886  1.78390087 -4.35366902]', '[-0.63339372 -1.06882734  2.64264089 -4.63628101]', '[-0.05563873 -1.92869321  3.0748061  -3.85038826]', '[ 0.5616523  -2.58402659  2.98266904 -2.67634418]', '[ 1.08902061 -2.99575272  2.19951828 -1.43823841]', '[ 1.41949207  3.12722889  1.08058497 -0.15390108]', '[ 1.51203765 -3.03467653 -0.15831776  1.3709807 ]', '[ 1.34887494 -2.58547509 -1.47649314  3.144024  ]', '[ 0.92119857 -1.75213378 -2.80505186  5.31356177]', '[ 0.24346509 -0.45555168 -3.88288463  7.53209786]', '[-0.50899138  0.98967509 -3.34718883  6.26379399]', '[-1.07045044  2.02818399 -2.2455005   4.18825347]', '[-1.38934032  2.66276979 -0.94017659  2.2309988 ]', '[-1.45813213  2.97255108  0.25116458  0.87504614]', '[-1.27894076  2.97477546  1.53005418 -0.85047847]', '[-0.85675923  2.63208236  2.63648992 -2.58794751]', '[-0.258913    1.92842127  3.25298651 -4.49115445]', '[ 0.42016139  0.82090495  3.49892512 -6.54068228]', '[ 1.08316002 -0.5485711   2.88410326 -6.59619917]', '[ 1.49701336 -1.67557649  1.20549962 -4.66702748]', '[ 1.56702979 -2.44380634 -0.47743381 -3.0515095 ]', '[ 1.32448905 -2.90039801 -1.89466749 -1.52889464]', '[ 0.81926083 -3.03120471 -3.09162613  0.15443693]', '[ 0.13723206 -2.9133052  -3.60239563  0.91344861]', '[-0.5724218  -2.67563075 -3.34780957  1.3358681 ]', '[-1.14296557 -2.47001771 -2.28920995  0.59784249]', '[-1.48783318 -2.43645009 -1.14901735 -0.33611303]', '[-1.60305098 -2.6231932  -0.00611182 -1.55607033]', '[-1.4780053  -3.10219286  1.26152262 -3.23909121]', '[-1.09531396  2.35292656  2.56880672 -5.12771148]', '[-0.44484791  1.05957831  3.97067178 -8.02402403]', '[ 0.4292361  -0.74176765  4.30870228 -8.96384792]', '[ 1.1421188  -2.24328617  2.81559095 -6.1813491 ]', '[ 1.5728107   2.97562297  1.53988336 -4.60073516]', '[ 1.77996734  2.17281554  0.57565423 -3.4620925 ]', '[ 1.81078235  1.58042324 -0.26468711 -2.49248512]']</t>
+  </si>
+  <si>
+    <t>[array([-0.03763371, -0.01533471,  0.06554052, -0.01816017], dtype=float32), array([-0.00754409, -0.05458322,  0.2277812 , -0.36241836]), array([ 0.04879627, -0.15231473,  0.32089719, -0.5887683 ]), array([ 0.11397169, -0.27767857,  0.31375488, -0.63332862]), array([ 0.16759438, -0.39312519,  0.2086893 , -0.49480525]), array([ 0.1930193 , -0.46685036,  0.03906408, -0.22816919]), array([ 0.18217995, -0.48119372, -0.14531723,  0.08492936]), array([ 0.13737799, -0.43548032, -0.29255645,  0.35879992]), array([ 0.0448411 , -0.27859812, -0.61146179,  1.17448612]), array([-0.06860641, -0.05622008, -0.49256054,  0.99183019]), array([-0.14124543,  0.09729776, -0.21467558,  0.50620575]), array([-0.14968433,  0.13659429,  0.13257963, -0.120111  ]), array([-0.0905776 ,  0.05231674,  0.44376485, -0.69898246]), array([ 0.01880609, -0.12769834,  0.62170324, -1.05159645]), array([ 0.14493442, -0.34499409,  0.60714543, -1.06399616]), array([ 0.2492602 , -0.53163849,  0.41137671, -0.7601214 ]), array([ 0.30177805, -0.63610881,  0.10256253, -0.26547779]), array([ 0.26401674, -0.57024939, -0.47283708,  0.91356453]), array([ 0.11991419, -0.28235468, -0.93593667,  1.90832825]), array([-0.09085923,  0.15628831, -1.11091308,  2.35896477]), array([-0.29761807,  0.60847034, -0.90020751,  2.05390538]), array([-0.41069544,  0.88510218, -0.21555102,  0.68736841]), array([-0.38248204,  0.88034003,  0.49131012, -0.73169907]), array([-0.22011253,  0.59777265,  1.10565551, -2.05912033]), array([ 0.04198696,  0.08588341,  1.44821645, -2.9337883 ]), array([ 0.32381283, -0.50597909,  1.28487283, -2.81704938]), array([ 0.52817405, -0.98902677,  0.71746561, -1.94274586]), array([ 0.60205781, -1.26965447,  0.01563191, -0.85127352]), array([ 0.53665857, -1.32822334, -0.65356945,  0.26267136]), array([ 0.33107242, -1.11337428, -1.37083846,  1.87505763]), array([ 0.02672801, -0.65051049, -1.61491464,  2.6696507 ]), array([-0.28497233, -0.09844566, -1.41912857,  2.69088609]), array([-0.53420411,  0.42904373, -1.00314221,  2.44710891]), array([-0.6409175 ,  0.77642315, -0.04741911,  0.99110737]), array([-0.55414419,  0.82054184,  0.89737643, -0.54934066]), array([-0.29440684,  0.56195104,  1.65355245, -1.99489777]), array([ 0.08038864,  0.05872726,  2.0048716 , -2.88578608]), array([ 0.46437983, -0.51259627,  1.73704928, -2.64951159]), array([ 0.74425899, -0.95075812,  1.01379778, -1.67177504]), array([ 0.85843732, -1.17196712,  0.11500361, -0.5333711 ]), array([ 0.78962215, -1.16252654, -0.79303772,  0.63121642]), array([ 0.54995088, -0.91926188, -1.56832114,  1.78676992]), array([ 0.15915896, -0.40223389, -2.26826114,  3.28861648]), array([-0.28715876,  0.24943393, -2.07331002,  2.99513889]), array([-0.62862829,  0.72107427, -1.27640378,  1.6282928 ]), array([-0.80521144,  0.94772876, -0.46395491,  0.62006415]), array([-0.80916431,  0.96669553,  0.42451037, -0.43121672]), array([-0.6170793 ,  0.71522591,  1.47274641, -2.07517611]), array([-0.23803471,  0.15495792,  2.23808476, -3.39877346]), array([ 0.22987034, -0.55207553,  2.31149819, -3.41906642]), array([ 0.64225818, -1.13335625,  1.74033385, -2.29967333]), array([ 0.90675886, -1.46055646,  0.87359505, -0.97451644]), array([ 0.98370315, -1.52701012, -0.11277244,  0.30374935]), array([ 0.86214299, -1.33851269, -1.0910309 ,  1.58815843]), array([ 0.55647916, -0.88952347, -1.92746095,  2.88382265]), array([ 0.09171146, -0.15033652, -2.61846151,  4.32828249]), array([-0.42773828,  0.71246604, -2.42525879,  3.9943164 ]), array([-0.81571045,  1.31982822, -1.41510183,  2.06376843]), array([-0.98510433,  1.54761665, -0.26624589,  0.23584613]), array([-0.91993672,  1.41685458,  0.91574724, -1.55400589]), array([-0.62254293,  0.91601464,  2.03762476, -3.471856  ]), array([-0.12555443,  0.04900021,  2.81205084, -4.97054508]), array([ 0.42727303, -0.91333982,  2.55736859, -4.3279059 ]), array([ 0.86018856, -1.62335278,  1.72726089, -2.75786999]), array([ 1.10656782, -2.0271457 ,  0.71674349, -1.30761758]), array([ 1.14239982, -2.15319713, -0.35935458,  0.04215541]), array([ 0.95250797, -1.96403932, -1.51903624,  1.87217332]), array([ 0.56287258, -1.43731059, -2.33646351,  3.41642527]), array([ 0.01635347, -0.54292712, -3.05861136,  5.43245557]), array([-0.59313802,  0.59333823, -2.81954932,  5.45895377]), array([-1.04843197,  1.51848961, -1.67960161,  3.74674003]), array([-1.24413149,  2.06426228, -0.28725581,  1.76897343]), array([-1.16860964,  2.2355082 ,  1.02231734, -0.05702219]), array([-0.84773317,  2.03501351,  2.14108511, -1.97455245]), array([-0.33523891,  1.43201691,  2.92865716, -4.08697117]), array([ 0.30211814,  0.40567329,  3.34773335, -5.99076774]), array([ 0.92154366, -0.7772247 ,  2.64045186, -5.39044928]), array([ 1.31399416, -1.67743423,  1.25886426, -3.6351397 ]), array([ 1.42444284, -2.25248702, -0.14665541, -2.14165023]), array([ 1.26197901, -2.53458517, -1.45190042, -0.67000827]), array([ 0.84769032, -2.47666089, -2.6252117 ,  1.25324357]), array([ 0.2626396 , -2.07627416, -3.11091292,  2.72668697]), array([-0.3494054 , -1.40838582, -2.91624636,  3.85832955]), array([-0.87354551, -0.59079377, -2.25144995,  4.12819787]), array([-1.21601519,  0.15676389, -1.10072346,  3.18145308]), array([-1.29491653,  0.64448622,  0.33303095,  1.65126051]), array([-1.10306949,  0.86327316,  1.58633846,  0.47563194]), array([-0.64781423,  0.75072295,  2.90291173, -1.61990724]), array([ 0.01730848,  0.23936588,  3.60353476, -3.29217529]), array([ 0.72015939, -0.43136361,  3.25552602, -3.09424467]), array([ 1.27124549, -0.91906129,  2.1959282 , -1.74209091]), array([ 1.58994006, -1.14497286,  0.98853238, -0.57938177]), array([ 1.6683853 , -1.17112369, -0.20055864,  0.29457717]), array([ 1.48840354, -0.96628382, -1.6052063 ,  1.80271154]), array([ 1.04884024, -0.4877698 , -2.76702913,  2.99049828]), array([ 0.40918863,  0.18887187, -3.50175663,  3.52462411]), array([-0.28381998,  0.78532968, -3.26761634,  2.17601745]), array([-0.86531329,  1.05787189, -2.44079899,  0.49825989]), array([-1.23064972,  0.99322448, -1.17745458, -1.08367881]), array([-1.30889885,  0.59001877,  0.39078845, -2.90316584]), array([-1.08529282, -0.14703886,  1.78390087, -4.35366902]), array([-0.63339372, -1.06882734,  2.64264089, -4.63628101]), array([-0.05563873, -1.92869321,  3.0748061 , -3.85038826]), array([ 0.5616523 , -2.58402659,  2.98266904, -2.67634418]), array([ 1.08902061, -2.99575272,  2.19951828, -1.43823841]), array([ 1.41949207,  3.12722889,  1.08058497, -0.15390108]), array([ 1.51203765, -3.03467653, -0.15831776,  1.3709807 ]), array([ 1.34887494, -2.58547509, -1.47649314,  3.144024  ]), array([ 0.92119857, -1.75213378, -2.80505186,  5.31356177]), array([ 0.24346509, -0.45555168, -3.88288463,  7.53209786]), array([-0.50899138,  0.98967509, -3.34718883,  6.26379399]), array([-1.07045044,  2.02818399, -2.2455005 ,  4.18825347]), array([-1.38934032,  2.66276979, -0.94017659,  2.2309988 ]), array([-1.45813213,  2.97255108,  0.25116458,  0.87504614]), array([-1.27894076,  2.97477546,  1.53005418, -0.85047847]), array([-0.85675923,  2.63208236,  2.63648992, -2.58794751]), array([-0.258913  ,  1.92842127,  3.25298651, -4.49115445]), array([ 0.42016139,  0.82090495,  3.49892512, -6.54068228]), array([ 1.08316002, -0.5485711 ,  2.88410326, -6.59619917]), array([ 1.49701336, -1.67557649,  1.20549962, -4.66702748]), array([ 1.56702979, -2.44380634, -0.47743381, -3.0515095 ]), array([ 1.32448905, -2.90039801, -1.89466749, -1.52889464]), array([ 0.81926083, -3.03120471, -3.09162613,  0.15443693]), array([ 0.13723206, -2.9133052 , -3.60239563,  0.91344861]), array([-0.5724218 , -2.67563075, -3.34780957,  1.3358681 ]), array([-1.14296557, -2.47001771, -2.28920995,  0.59784249]), array([-1.48783318, -2.43645009, -1.14901735, -0.33611303]), array([-1.60305098, -2.6231932 , -0.00611182, -1.55607033]), array([-1.4780053 , -3.10219286,  1.26152262, -3.23909121]), array([-1.09531396,  2.35292656,  2.56880672, -5.12771148]), array([-0.44484791,  1.05957831,  3.97067178, -8.02402403]), array([ 0.4292361 , -0.74176765,  4.30870228, -8.96384792]), array([ 1.1421188 , -2.24328617,  2.81559095, -6.1813491 ]), array([ 1.5728107 ,  2.97562297,  1.53988336, -4.60073516]), array([ 1.77996734,  2.17281554,  0.57565423, -3.4620925 ]), array([ 1.81078235,  1.58042324, -0.26468711, -2.49248512])]</t>
+  </si>
+  <si>
+    <t>['[1,0,2]', '[1,1,2]', '[2,1,0]', '[1,2,0]', '[1,1,1]', '[0,1,1]', '[2,0,1]', '[0,2,1]', '[2,2,2]', '[0,0,0]']</t>
+  </si>
+  <si>
+    <t>[6, 8, 9, 10, 11, 19, 20, 21, 27, 28, 29, 30, 31, 32, 33, 39, 41, 42, 43, 44, 50, 51, 52, 54, 55, 62, 63, 64, 65, 66, 67, 74, 75, 76, 77, 78, 79, 86, 87, 88, 89, 91, 98, 99, 100, 101, 102, 103, 110, 111, 112, 113, 114, 115, 122, 123, 125, 126, 127, 135, 136, 137, 138, 139, 146, 147, 148, 149, 150, 151, 158, 159, 160, 162, 163, 171, 172, 174, 175, 176, 177, 183, 184, 186, 187, 188, 195, 197, 198, 199]</t>
+  </si>
+  <si>
+    <t>[0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 1, 2, 2, 2, 2]</t>
+  </si>
+  <si>
+    <t>['[-0.03763371 -0.01533471  0.06554052 -0.01816017]', '[-0.00754409 -0.05458322  0.2277812  -0.36241836]', '[ 0.04879627 -0.15231473  0.32089719 -0.5887683 ]', '[ 0.11397169 -0.27767857  0.31375488 -0.63332862]', '[ 0.16759438 -0.39312519  0.2086893  -0.49480525]', '[ 0.1930193  -0.46685036  0.03906408 -0.22816919]', '[ 0.18217995 -0.48119372 -0.14531723  0.08492936]', '[ 0.11196576 -0.36927962 -0.54130528  1.01009116]', '[ 0.00196683 -0.16269792 -0.52993942  1.00304703]', '[-0.08846848  0.01055114 -0.35053458  0.68491803]', '[-0.13062525  0.09702055 -0.06034533  0.15941132]', '[-0.11117591  0.07128848  0.2497702  -0.40878217]', '[-0.03575223 -0.05786526  0.48480694 -0.84806298]', '[ 0.07246632 -0.24951705  0.56892694 -1.0172209 ]', '[ 0.17980565 -0.44321283  0.4776381  -0.87229334]', '[ 0.25409616 -0.58210371  0.24836546 -0.48780854]', '[ 0.2745924  -0.63058041 -0.0476133   0.01100174]', '[ 0.21114115 -0.5137247  -0.57453463  1.1385484 ]', '[ 0.05428383 -0.1913682  -0.95618274  2.01493815]', '[-0.12369599  0.18275324 -0.7730874   1.62733728]', '[-0.23806646  0.4270883  -0.34365534  0.76524208]', '[-0.25497724  0.47737266  0.17745132 -0.26918973]', '[-0.16995971  0.32351375  0.65378169 -1.23797005]', '[-0.00600072  0.00443977  0.94247022 -1.87179089]', '[ 0.1855285  -0.3839758   0.91897209 -1.90876426]', '[ 0.34167951 -0.72155856  0.60600911 -1.40045725]', '[ 0.41772505 -0.92625585  0.14140843 -0.6224063 ]', '[ 0.39669685 -0.96597315 -0.34625698  0.22527182]', '[ 0.28455048 -0.83987342 -0.75391715  1.01433798]', '[ 0.10692348 -0.57475295 -0.98511774  1.58228918]', '[-0.09115468 -0.23722682 -0.9460368   1.70439368]', '[-0.25094377  0.0688145  -0.60911934  1.27490219]', '[-0.32151183  0.24711914 -0.07869018  0.47095481]', '[-0.28024953  0.25044022  0.48270169 -0.43204985]', '[-0.13679173  0.08461305  0.91853854 -1.17772706]', '[ 0.0691619  -0.19220267  1.08938002 -1.50545189]', '[ 0.27678232 -0.48074536  0.93725641 -1.30050515]', '[ 0.42689322 -0.68656343  0.53305709 -0.71567715]', '[ 0.48150949 -0.75659003  0.00335343  0.02602657]', '[ 0.42811198 -0.67624274 -0.52688589  0.76446632]', '[ 0.25414104 -0.39627225 -1.17891512  1.98673236]', '[ 0.00455216  0.01391655 -1.25110358  1.99672428]', '[-0.21939047  0.35415706 -0.93367419  1.31299103]', '[-0.3518592   0.51303631 -0.36440709  0.24195061]', '[-0.35918066  0.44553135  0.29212347 -0.90942741]', '[-0.24002407  0.16064108  0.86975573 -1.8812177 ]', '[-0.03043812 -0.2696147   1.16545881 -2.30266549]', '[ 0.19947594 -0.70885356  1.07622065 -1.9840391 ]', '[ 0.38125817 -1.03197679  0.7087626  -1.20077212]', '[ 0.47355851 -1.17847732  0.20028971 -0.25176912]', '[ 0.45868778 -1.13082236 -0.34732319  0.72555302]', '[ 0.33841461 -0.89235154 -0.8365189   1.63569009]', '[ 0.13616352 -0.49416586 -1.14232899  2.27226964]', '[-0.12111115  0.04065304 -1.35768142  2.93349384]', '[-0.34699218  0.54411151 -0.84146326  1.98483349]', '[-0.44350217  0.80847359 -0.11007211  0.63266911]', '[-0.39086541  0.79412614  0.62545173 -0.77056176]', '[-0.20179956  0.50783229  1.2306385  -2.04749233]', '[ 0.0800856   0.00973915  1.51499485 -2.79832145]', '[ 0.36862137 -0.54284955  1.28988294 -2.57438849]', '[ 0.57059255 -0.97489239  0.69155301 -1.68570199]', '[ 0.63682164 -1.20549743 -0.03536624 -0.60903972]', '[ 0.55843628 -1.21699151 -0.73269713  0.49160476]', '[ 0.35402886 -1.01273113 -1.2761663   1.52727704]', '[ 0.0663389  -0.62446687 -1.54394479  2.27727955]', '[-0.23525534 -0.14884599 -1.39562308  2.33915316]', '[-0.46157326  0.25411419 -0.8104234   1.58446898]', '[-0.54403784  0.4572509   0.00241451  0.41462424]', '[-0.46032649  0.41589667  0.81890091 -0.81634996]', '[-0.22923466  0.14512902  1.44173108 -1.81990495]', '[ 0.08845577 -0.26697174  1.65473907 -2.16404973]', '[ 0.39914826 -0.66379924  1.38223606 -1.6966382 ]', '[ 0.61894833 -0.91666767  0.77762589 -0.79528664]', '[ 0.70001559 -0.97531997  0.02092088  0.21237912]', '[ 0.62680417 -0.8328837  -0.741872    1.20014529]', '[ 0.4129947  -0.50572124 -1.35566661  2.01790161]', '[ 0.10851142 -0.06291765 -1.61398364  2.28170935]', '[-0.19864859  0.34714828 -1.38201288  1.69188788]', '[-0.41896136  0.57590184 -0.77715638  0.54340318]', '[-0.49738885  0.55435521  0.00730602 -0.76147914]', '[-0.41589643  0.27743868  0.78861168 -1.96419276]', '[-0.19847189 -0.19815255  1.32242916 -2.66598775]', '[ 0.08183611 -0.72684988  1.40788352 -2.4819039 ]', '[ 0.33985072 -1.14804784  1.12623014 -1.66584627]', '[ 0.51764752 -1.37851068  0.62424756 -0.62065352]', '[ 0.58114656 -1.39262701 -0.00157519  0.48289867]', '[ 0.51515843 -1.18520056 -0.65332679  1.58588169]', '[ 0.32593933 -0.76481187 -1.20887673  2.57614696]', '[ 0.05213245 -0.18949137 -1.45486906  3.03602445]', '[-0.21935151  0.37691037 -1.17917353  2.46814232]', '[-0.41929644  0.81528823 -0.77408054  1.83229096]', '[-0.49540319  1.03169551  0.01794452  0.32401165]', '[-0.41389401  0.9449443   0.78404316 -1.1849418 ]', '[-0.19067124  0.56485413  1.41154057 -2.56805407]', '[ 0.12645598 -0.04087675  1.67202488 -3.32004391]', '[ 0.43587447 -0.67923839  1.33411661 -2.89419098]', '[ 0.63546318 -1.15601578  0.62998306 -1.82765843]', '[ 0.68233508 -1.40369889 -0.16081474 -0.6450771 ]', '[ 0.57573839 -1.41394478 -0.88302437  0.53899545]', '[ 0.34188397 -1.19185239 -1.41560372  1.66020865]', '[ 0.0289233  -0.7667852  -1.65702805  2.51646456]', '[-0.29266935 -0.23225004 -1.47978399  2.6796371 ]', '[-0.53020788  0.24073503 -0.83253847  1.92655879]', '[-0.60896175  0.50588014  0.06174808  0.68613047]', '[-0.50597576  0.50913743  0.94958053 -0.64765305]', '[-0.2431393   0.25828095  1.62493208 -1.79551888]', '[ 0.11402314 -0.16419561  1.85813617 -2.28228159]', '[ 0.46237012 -0.59064839  1.54598147 -1.85787529]', '[ 0.70741009 -0.87418653  0.86322417 -0.93753206]', '[ 0.7971144  -0.95919034  0.0217347   0.09082592]', '[ 0.7157599  -0.83843201 -0.82367454  1.10894483]', '[ 0.47763756 -0.52366291 -1.51560034  1.99095047]', '[ 0.13473125 -0.07828596 -1.83226187  2.32938588]', '[-0.21766498  0.34330081 -1.60599437  1.74574831]', '[-0.47849454  0.57783721 -0.95086356  0.54286701]', '[-0.58357932  0.55001041 -0.08161244 -0.82287243]', '[-0.50996002  0.25513169  0.79974318 -2.08141195]', '[-0.28060147 -0.2480841   1.42758949 -2.81789893]', '[ 0.02822072 -0.80610627  1.58405213 -2.61552173]', '[ 0.32660726 -1.24942723  1.34826943 -1.75028652]', '[ 0.54982368 -1.49064132  0.84761349 -0.64218559]', '[ 0.65354898 -1.50219928  0.16889903  0.53104884]', '[ 0.61248051 -1.27724897 -0.58099903  1.71731601]', '[ 0.42502974 -0.81879512 -1.26748431  2.83419402]', '[ 0.10030175 -0.11052277 -1.8952496   4.08842912]', '[-0.25514381  0.64402625 -1.55081028  3.24058171]', '[-0.49354835  1.13887485 -0.80387542  1.67189878]', '[-0.57136514  1.31088214  0.02964707  0.05078926]', '[-0.48249144  1.15942147  0.85048509 -1.56577159]', '[-0.23760613  0.68656786  1.56744694 -3.12821403]', '[ 0.11959934 -0.04933651  1.89960969 -4.02313104]', '[ 0.46900023 -0.81471434  1.48980398 -3.4275119 ]', '[ 0.68993529 -1.37819361  0.6921412  -2.17665541]', '[ 0.74230131 -1.68449553 -0.16400336 -0.89121334]', '[ 0.61458358 -1.68904674 -1.08314118  0.8406976 ]', '[ 0.34118432 -1.39877144 -1.6070387   2.04440863]', '[-0.00822277 -0.88600874 -1.83076908  3.01295487]', '[-0.36227444 -0.2432148  -1.62251262  3.24211167]', '[-0.61906247  0.33281185 -0.87251971  2.37044565]', '[-0.69337061  0.66907908  0.14394682  0.95288016]', '[-0.56377984  0.7074543   1.12852097 -0.56895402]', '[-0.2579008   0.44908043  1.87195762 -1.95829329]', '[ 0.15254862 -0.03102656  2.13278721 -2.67634213]', '[ 0.55110972 -0.54310149  1.75972899 -2.28752783]', '[ 0.82826205 -0.90563073  0.9683953  -1.29396857]', '[ 0.92814571 -1.05500614  0.01916212 -0.19684144]', '[ 0.83576339 -0.98333792 -0.93178245  0.91585611]', '[ 0.56499768 -0.69015265 -1.73533353  1.98831975]', '[ 0.16682405 -0.21722208 -2.15916462  2.60697076]', '[-0.25508495  0.27737376 -1.95457778  2.1582989 ]', '[-0.57865579  0.58973254 -1.21834897  0.89095099]', '[-0.72533387  0.62113736 -0.22545639 -0.58095228]', '[-0.66572804  0.36132468  0.8098716  -1.98682226]', '[-0.41550252 -0.14667996  1.62795754 -2.96858832]', '[-0.05045341 -0.75423526  1.93055197 -2.92690988]', '[ 0.32337746 -1.25833987  1.74100691 -2.02366289]', '[ 0.62256015 -1.54342158  1.20137888 -0.80424189]', '[ 0.78701681 -1.57652863  0.41280881  0.47425349]', '[ 0.77975845 -1.35384106 -0.4924043   1.75227726]', '[ 0.5920733  -0.87652251 -1.36249656  3.00048136]', '[ 0.25437379 -0.18210505 -1.92693206  3.78381174]', '[-0.15508596  0.60529727 -2.03803366  3.82786937]', '[-0.49706822  1.21193881 -1.33557094  2.18288971]', '[-0.67846657  1.47618472 -0.46040625  0.46598522]', '[-0.6761785   1.39958986  0.48864763 -1.2356849 ]', '[-0.48346171  0.97753973  1.42728759 -2.99032868]', '[-0.11848327  0.21738283  2.14007301 -4.46286143]', '[ 0.31380949 -0.68841158  2.03183801 -4.28739716]', '[ 0.65150445 -1.4190633   1.29669809 -2.96002277]', '[ 0.82362259 -1.87265156  0.41557568 -1.59039447]', '[ 0.81764229 -2.06008535 -0.46531026 -0.29180085]', '[ 0.64590258 -1.99124693 -1.21960433  0.97530732]', '[ 0.34710666 -1.67289863 -1.71945117  2.19426585]', '[-0.04023589 -1.0708942  -2.1149696   3.80224729]', '[-0.45261212 -0.25076468 -1.90732339  4.18854424]', '[-0.75277021  0.49866267 -0.99866504  3.11113211]', '[-0.83166779  0.95442556  0.21968051  1.41420965]', '[-0.67058978  1.0591123   1.35829227 -0.37448421]', '[-0.30801113  0.80533345  2.20363945 -2.13201843]', '[ 0.17769883  0.24112767  2.54766416 -3.33962357]', '[ 0.65898372 -0.43136405  2.14506805 -3.15453579]', '[ 0.99954871 -0.95882277  1.21047957 -2.06052026]', '[ 1.13276453 -1.25112253  0.11054727 -0.86295955]', '[ 1.04323851 -1.30153251 -0.99681138  0.37564318]', '[ 0.74249391 -1.091539   -1.97439678  1.73885146]', '[ 0.25300793 -0.55047984 -2.84418488  3.59945201]', '[-0.31957269  0.195427   -2.72799871  3.55488242]', '[-0.78290076  0.7661359  -1.82044919  2.02918672]', '[-1.02886215  0.99613531 -0.61491549  0.28227568]', '[-1.02397659  0.88456371  0.66596879 -1.3949324 ]', '[-0.76584835  0.43717799  1.88616132 -3.05340234]', '[-0.29711217 -0.29154112  2.68301155 -3.99783729]', '[ 0.24924201 -1.04046993  2.65961747 -3.26439555]', '[ 0.7297557  -1.54809468  2.07412876 -1.77262483]', '[ 1.05478075 -1.75046987  1.13113941 -0.2713687 ]', '[ 1.16986891 -1.66591032  0.00362313  1.10058503]', '[ 1.03530073 -1.26009219 -1.35471208  2.98945112]', '[ 0.65369946 -0.51651385 -2.40703787  4.38436902]', '[ 0.11992066  0.4048501  -2.76852954  4.4888578 ]', '[-0.39426741  1.15553486 -2.28284573  2.87209629]']</t>
+  </si>
+  <si>
+    <t>[array([-0.03763371, -0.01533471,  0.06554052, -0.01816017], dtype=float32), array([-0.00754409, -0.05458322,  0.2277812 , -0.36241836]), array([ 0.04879627, -0.15231473,  0.32089719, -0.5887683 ]), array([ 0.11397169, -0.27767857,  0.31375488, -0.63332862]), array([ 0.16759438, -0.39312519,  0.2086893 , -0.49480525]), array([ 0.1930193 , -0.46685036,  0.03906408, -0.22816919]), array([ 0.18217995, -0.48119372, -0.14531723,  0.08492936]), array([ 0.11196576, -0.36927962, -0.54130528,  1.01009116]), array([ 0.00196683, -0.16269792, -0.52993942,  1.00304703]), array([-0.08846848,  0.01055114, -0.35053458,  0.68491803]), array([-0.13062525,  0.09702055, -0.06034533,  0.15941132]), array([-0.11117591,  0.07128848,  0.2497702 , -0.40878217]), array([-0.03575223, -0.05786526,  0.48480694, -0.84806298]), array([ 0.07246632, -0.24951705,  0.56892694, -1.0172209 ]), array([ 0.17980565, -0.44321283,  0.4776381 , -0.87229334]), array([ 0.25409616, -0.58210371,  0.24836546, -0.48780854]), array([ 0.2745924 , -0.63058041, -0.0476133 ,  0.01100174]), array([ 0.21114115, -0.5137247 , -0.57453463,  1.1385484 ]), array([ 0.05428383, -0.1913682 , -0.95618274,  2.01493815]), array([-0.12369599,  0.18275324, -0.7730874 ,  1.62733728]), array([-0.23806646,  0.4270883 , -0.34365534,  0.76524208]), array([-0.25497724,  0.47737266,  0.17745132, -0.26918973]), array([-0.16995971,  0.32351375,  0.65378169, -1.23797005]), array([-0.00600072,  0.00443977,  0.94247022, -1.87179089]), array([ 0.1855285 , -0.3839758 ,  0.91897209, -1.90876426]), array([ 0.34167951, -0.72155856,  0.60600911, -1.40045725]), array([ 0.41772505, -0.92625585,  0.14140843, -0.6224063 ]), array([ 0.39669685, -0.96597315, -0.34625698,  0.22527182]), array([ 0.28455048, -0.83987342, -0.75391715,  1.01433798]), array([ 0.10692348, -0.57475295, -0.98511774,  1.58228918]), array([-0.09115468, -0.23722682, -0.9460368 ,  1.70439368]), array([-0.25094377,  0.0688145 , -0.60911934,  1.27490219]), array([-0.32151183,  0.24711914, -0.07869018,  0.47095481]), array([-0.28024953,  0.25044022,  0.48270169, -0.43204985]), array([-0.13679173,  0.08461305,  0.91853854, -1.17772706]), array([ 0.0691619 , -0.19220267,  1.08938002, -1.50545189]), array([ 0.27678232, -0.48074536,  0.93725641, -1.30050515]), array([ 0.42689322, -0.68656343,  0.53305709, -0.71567715]), array([ 0.48150949, -0.75659003,  0.00335343,  0.02602657]), array([ 0.42811198, -0.67624274, -0.52688589,  0.76446632]), array([ 0.25414104, -0.39627225, -1.17891512,  1.98673236]), array([ 0.00455216,  0.01391655, -1.25110358,  1.99672428]), array([-0.21939047,  0.35415706, -0.93367419,  1.31299103]), array([-0.3518592 ,  0.51303631, -0.36440709,  0.24195061]), array([-0.35918066,  0.44553135,  0.29212347, -0.90942741]), array([-0.24002407,  0.16064108,  0.86975573, -1.8812177 ]), array([-0.03043812, -0.2696147 ,  1.16545881, -2.30266549]), array([ 0.19947594, -0.70885356,  1.07622065, -1.9840391 ]), array([ 0.38125817, -1.03197679,  0.7087626 , -1.20077212]), array([ 0.47355851, -1.17847732,  0.20028971, -0.25176912]), array([ 0.45868778, -1.13082236, -0.34732319,  0.72555302]), array([ 0.33841461, -0.89235154, -0.8365189 ,  1.63569009]), array([ 0.13616352, -0.49416586, -1.14232899,  2.27226964]), array([-0.12111115,  0.04065304, -1.35768142,  2.93349384]), array([-0.34699218,  0.54411151, -0.84146326,  1.98483349]), array([-0.44350217,  0.80847359, -0.11007211,  0.63266911]), array([-0.39086541,  0.79412614,  0.62545173, -0.77056176]), array([-0.20179956,  0.50783229,  1.2306385 , -2.04749233]), array([ 0.0800856 ,  0.00973915,  1.51499485, -2.79832145]), array([ 0.36862137, -0.54284955,  1.28988294, -2.57438849]), array([ 0.57059255, -0.97489239,  0.69155301, -1.68570199]), array([ 0.63682164, -1.20549743, -0.03536624, -0.60903972]), array([ 0.55843628, -1.21699151, -0.73269713,  0.49160476]), array([ 0.35402886, -1.01273113, -1.2761663 ,  1.52727704]), array([ 0.0663389 , -0.62446687, -1.54394479,  2.27727955]), array([-0.23525534, -0.14884599, -1.39562308,  2.33915316]), array([-0.46157326,  0.25411419, -0.8104234 ,  1.58446898]), array([-0.54403784,  0.4572509 ,  0.00241451,  0.41462424]), array([-0.46032649,  0.41589667,  0.81890091, -0.81634996]), array([-0.22923466,  0.14512902,  1.44173108, -1.81990495]), array([ 0.08845577, -0.26697174,  1.65473907, -2.16404973]), array([ 0.39914826, -0.66379924,  1.38223606, -1.6966382 ]), array([ 0.61894833, -0.91666767,  0.77762589, -0.79528664]), array([ 0.70001559, -0.97531997,  0.02092088,  0.21237912]), array([ 0.62680417, -0.8328837 , -0.741872  ,  1.20014529]), array([ 0.4129947 , -0.50572124, -1.35566661,  2.01790161]), array([ 0.10851142, -0.06291765, -1.61398364,  2.28170935]), array([-0.19864859,  0.34714828, -1.38201288,  1.69188788]), array([-0.41896136,  0.57590184, -0.77715638,  0.54340318]), array([-0.49738885,  0.55435521,  0.00730602, -0.76147914]), array([-0.41589643,  0.27743868,  0.78861168, -1.96419276]), array([-0.19847189, -0.19815255,  1.32242916, -2.66598775]), array([ 0.08183611, -0.72684988,  1.40788352, -2.4819039 ]), array([ 0.33985072, -1.14804784,  1.12623014, -1.66584627]), array([ 0.51764752, -1.37851068,  0.62424756, -0.62065352]), array([ 0.58114656, -1.39262701, -0.00157519,  0.48289867]), array([ 0.51515843, -1.18520056, -0.65332679,  1.58588169]), array([ 0.32593933, -0.76481187, -1.20887673,  2.57614696]), array([ 0.05213245, -0.18949137, -1.45486906,  3.03602445]), array([-0.21935151,  0.37691037, -1.17917353,  2.46814232]), array([-0.41929644,  0.81528823, -0.77408054,  1.83229096]), array([-0.49540319,  1.03169551,  0.01794452,  0.32401165]), array([-0.41389401,  0.9449443 ,  0.78404316, -1.1849418 ]), array([-0.19067124,  0.56485413,  1.41154057, -2.56805407]), array([ 0.12645598, -0.04087675,  1.67202488, -3.32004391]), array([ 0.43587447, -0.67923839,  1.33411661, -2.89419098]), array([ 0.63546318, -1.15601578,  0.62998306, -1.82765843]), array([ 0.68233508, -1.40369889, -0.16081474, -0.6450771 ]), array([ 0.57573839, -1.41394478, -0.88302437,  0.53899545]), array([ 0.34188397, -1.19185239, -1.41560372,  1.66020865]), array([ 0.0289233 , -0.7667852 , -1.65702805,  2.51646456]), array([-0.29266935, -0.23225004, -1.47978399,  2.6796371 ]), array([-0.53020788,  0.24073503, -0.83253847,  1.92655879]), array([-0.60896175,  0.50588014,  0.06174808,  0.68613047]), array([-0.50597576,  0.50913743,  0.94958053, -0.64765305]), array([-0.2431393 ,  0.25828095,  1.62493208, -1.79551888]), array([ 0.11402314, -0.16419561,  1.85813617, -2.28228159]), array([ 0.46237012, -0.59064839,  1.54598147, -1.85787529]), array([ 0.70741009, -0.87418653,  0.86322417, -0.93753206]), array([ 0.7971144 , -0.95919034,  0.0217347 ,  0.09082592]), array([ 0.7157599 , -0.83843201, -0.82367454,  1.10894483]), array([ 0.47763756, -0.52366291, -1.51560034,  1.99095047]), array([ 0.13473125, -0.07828596, -1.83226187,  2.32938588]), array([-0.21766498,  0.34330081, -1.60599437,  1.74574831]), array([-0.47849454,  0.57783721, -0.95086356,  0.54286701]), array([-0.58357932,  0.55001041, -0.08161244, -0.82287243]), array([-0.50996002,  0.25513169,  0.79974318, -2.08141195]), array([-0.28060147, -0.2480841 ,  1.42758949, -2.81789893]), array([ 0.02822072, -0.80610627,  1.58405213, -2.61552173]), array([ 0.32660726, -1.24942723,  1.34826943, -1.75028652]), array([ 0.54982368, -1.49064132,  0.84761349, -0.64218559]), array([ 0.65354898, -1.50219928,  0.16889903,  0.53104884]), array([ 0.61248051, -1.27724897, -0.58099903,  1.71731601]), array([ 0.42502974, -0.81879512, -1.26748431,  2.83419402]), array([ 0.10030175, -0.11052277, -1.8952496 ,  4.08842912]), array([-0.25514381,  0.64402625, -1.55081028,  3.24058171]), array([-0.49354835,  1.13887485, -0.80387542,  1.67189878]), array([-0.57136514,  1.31088214,  0.02964707,  0.05078926]), array([-0.48249144,  1.15942147,  0.85048509, -1.56577159]), array([-0.23760613,  0.68656786,  1.56744694, -3.12821403]), array([ 0.11959934, -0.04933651,  1.89960969, -4.02313104]), array([ 0.46900023, -0.81471434,  1.48980398, -3.4275119 ]), array([ 0.68993529, -1.37819361,  0.6921412 , -2.17665541]), array([ 0.74230131, -1.68449553, -0.16400336, -0.89121334]), array([ 0.61458358, -1.68904674, -1.08314118,  0.8406976 ]), array([ 0.34118432, -1.39877144, -1.6070387 ,  2.04440863]), array([-0.00822277, -0.88600874, -1.83076908,  3.01295487]), array([-0.36227444, -0.2432148 , -1.62251262,  3.24211167]), array([-0.61906247,  0.33281185, -0.87251971,  2.37044565]), array([-0.69337061,  0.66907908,  0.14394682,  0.95288016]), array([-0.56377984,  0.7074543 ,  1.12852097, -0.56895402]), array([-0.2579008 ,  0.44908043,  1.87195762, -1.95829329]), array([ 0.15254862, -0.03102656,  2.13278721, -2.67634213]), array([ 0.55110972, -0.54310149,  1.75972899, -2.28752783]), array([ 0.82826205, -0.90563073,  0.9683953 , -1.29396857]), array([ 0.92814571, -1.05500614,  0.01916212, -0.19684144]), array([ 0.83576339, -0.98333792, -0.93178245,  0.91585611]), array([ 0.56499768, -0.69015265, -1.73533353,  1.98831975]), array([ 0.16682405, -0.21722208, -2.15916462,  2.60697076]), array([-0.25508495,  0.27737376, -1.95457778,  2.1582989 ]), array([-0.57865579,  0.58973254, -1.21834897,  0.89095099]), array([-0.72533387,  0.62113736, -0.22545639, -0.58095228]), array([-0.66572804,  0.36132468,  0.8098716 , -1.98682226]), array([-0.41550252, -0.14667996,  1.62795754, -2.96858832]), array([-0.05045341, -0.75423526,  1.93055197, -2.92690988]), array([ 0.32337746, -1.25833987,  1.74100691, -2.02366289]), array([ 0.62256015, -1.54342158,  1.20137888, -0.80424189]), array([ 0.78701681, -1.57652863,  0.41280881,  0.47425349]), array([ 0.77975845, -1.35384106, -0.4924043 ,  1.75227726]), array([ 0.5920733 , -0.87652251, -1.36249656,  3.00048136]), array([ 0.25437379, -0.18210505, -1.92693206,  3.78381174]), array([-0.15508596,  0.60529727, -2.03803366,  3.82786937]), array([-0.49706822,  1.21193881, -1.33557094,  2.18288971]), array([-0.67846657,  1.47618472, -0.46040625,  0.46598522]), array([-0.6761785 ,  1.39958986,  0.48864763, -1.2356849 ]), array([-0.48346171,  0.97753973,  1.42728759, -2.99032868]), array([-0.11848327,  0.21738283,  2.14007301, -4.46286143]), array([ 0.31380949, -0.68841158,  2.03183801, -4.28739716]), array([ 0.65150445, -1.4190633 ,  1.29669809, -2.96002277]), array([ 0.82362259, -1.87265156,  0.41557568, -1.59039447]), array([ 0.81764229, -2.06008535, -0.46531026, -0.29180085]), array([ 0.64590258, -1.99124693, -1.21960433,  0.97530732]), array([ 0.34710666, -1.67289863, -1.71945117,  2.19426585]), array([-0.04023589, -1.0708942 , -2.1149696 ,  3.80224729]), array([-0.45261212, -0.25076468, -1.90732339,  4.18854424]), array([-0.75277021,  0.49866267, -0.99866504,  3.11113211]), array([-0.83166779,  0.95442556,  0.21968051,  1.41420965]), array([-0.67058978,  1.0591123 ,  1.35829227, -0.37448421]), array([-0.30801113,  0.80533345,  2.20363945, -2.13201843]), array([ 0.17769883,  0.24112767,  2.54766416, -3.33962357]), array([ 0.65898372, -0.43136405,  2.14506805, -3.15453579]), array([ 0.99954871, -0.95882277,  1.21047957, -2.06052026]), array([ 1.13276453, -1.25112253,  0.11054727, -0.86295955]), array([ 1.04323851, -1.30153251, -0.99681138,  0.37564318]), array([ 0.74249391, -1.091539  , -1.97439678,  1.73885146]), array([ 0.25300793, -0.55047984, -2.84418488,  3.59945201]), array([-0.31957269,  0.195427  , -2.72799871,  3.55488242]), array([-0.78290076,  0.7661359 , -1.82044919,  2.02918672]), array([-1.02886215,  0.99613531, -0.61491549,  0.28227568]), array([-1.02397659,  0.88456371,  0.66596879, -1.3949324 ]), array([-0.76584835,  0.43717799,  1.88616132, -3.05340234]), array([-0.29711217, -0.29154112,  2.68301155, -3.99783729]), array([ 0.24924201, -1.04046993,  2.65961747, -3.26439555]), array([ 0.7297557 , -1.54809468,  2.07412876, -1.77262483]), array([ 1.05478075, -1.75046987,  1.13113941, -0.2713687 ]), array([ 1.16986891, -1.66591032,  0.00362313,  1.10058503]), array([ 1.03530073, -1.26009219, -1.35471208,  2.98945112]), array([ 0.65369946, -0.51651385, -2.40703787,  4.38436902]), array([ 0.11992066,  0.4048501 , -2.76852954,  4.4888578 ]), array([-0.39426741,  1.15553486, -2.28284573,  2.87209629])]</t>
+  </si>
+  <si>
+    <t>['[0,1,1]', '[0,0,0]', '[1,0,2]', '[1,2,0]', '[0,2,1]', '[1,1,2]', '[2,0,1]', '[2,2,2]', '[2,1,0]', '[1,1,1]']</t>
+  </si>
+  <si>
+    <t>[6, 7, 8, 9, 10, 11, 12, 17, 18, 19, 20, 21, 22, 23, 29, 30, 31, 32, 33, 34, 40, 41, 42, 43, 44, 45, 46, 51, 52, 53, 54, 55, 56, 57, 63, 64, 65, 66, 67, 68, 74, 75, 76, 77, 78, 79, 85, 86, 87, 88, 89, 90, 91, 96, 97, 98, 99, 100, 101, 102, 108, 109, 110, 111, 112, 113, 119, 120, 121, 122, 123, 124, 130, 131, 132, 133, 134, 135, 136, 142, 143, 144, 145, 146, 147, 153, 154, 155, 156, 157, 158, 164, 165, 166, 167, 168, 169, 170, 176, 177, 178, 179, 180, 181, 187, 188, 189, 190, 191, 192, 198, 199]</t>
+  </si>
+  <si>
+    <t>[0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 2, 2]</t>
+  </si>
+  <si>
+    <t>['[-0.03763371 -0.01533471  0.06554052 -0.01816017]', '[-0.00754409 -0.05458322  0.2277812  -0.36241836]', '[ 0.04879627 -0.15231473  0.32089719 -0.5887683 ]', '[ 0.11397169 -0.27767857  0.31375488 -0.63332862]', '[ 0.16759438 -0.39312519  0.2086893  -0.49480525]', '[ 0.1930193  -0.46685036  0.03906408 -0.22816919]', '[ 0.18217995 -0.48119372 -0.14531723  0.08492936]', '[ 0.13737799 -0.43548032 -0.29255645  0.35879992]', '[ 0.07059687 -0.34553749 -0.35944697  0.51636187]', '[ 0.00066518 -0.24025206 -0.32266973  0.50804924]', '[-0.05184718 -0.15356453 -0.18924715  0.33585339]', '[-0.07099568 -0.11316     0.00267821  0.05860212]', '[-0.0506235  -0.13098626  0.19609592 -0.23012254]', '[ 0.00363944 -0.19947979  0.33317766 -0.43407441]', '[ 0.07604673 -0.29425756  0.37330708 -0.48624983]', '[ 0.14566012 -0.38269974  0.30650217 -0.37362319]', '[ 0.19284616 -0.43524651  0.15487527 -0.13746415]', '[ 0.20480978 -0.43420274 -0.03738189  0.14899985]', '[ 0.17872861 -0.37781944 -0.21671607  0.40226469]', '[ 0.12244395 -0.28089207 -0.33207824  0.54289906]', '[ 0.05262627 -0.17207597 -0.34864539  0.51601465]', '[-0.00991093 -0.08621824 -0.26142967  0.31808955]', '[-0.04676022 -0.05276175 -0.09876284  0.00534115]', '[-0.04773189 -0.08549506  0.08793289 -0.326671  ]', '[-0.01386808 -0.17774148  0.24064044 -0.5740393 ]', '[ 0.04305734 -0.30394484  0.31308665 -0.65740151]', '[ 0.10464298 -0.42784083  0.2871402  -0.55250711]', '[ 0.15213765 -0.51456341  0.17665722 -0.29545229]', '[ 0.17195601 -0.54054882  0.01729499  0.04161741]', '[ 0.15877658 -0.49810034 -0.14558791  0.37488532]', '[ 0.11662491 -0.39653924 -0.26514127  0.61927065]', '[ 0.05830606 -0.26143591 -0.30243069  0.70071627]', '[ 0.00240191 -0.12975114 -0.241122    0.58472722]', '[-0.03255824 -0.03901385 -0.09863914  0.30169722]', '[-0.03459084 -0.01467301  0.07923617 -0.06234707]', '[-0.00228999 -0.06214743  0.23549293 -0.3987235 ]', '[ 0.05469493 -0.16555079  0.31932445 -0.60811377]', '[ 0.11857421 -0.29274507  0.30262565 -0.63232462]', '[ 0.16925182 -0.40618487  0.19109743 -0.47671256]', '[ 0.19093562 -0.47518295  0.02014588 -0.20033382]', '[ 0.17663487 -0.48368374 -0.16020096  0.11418666]', '[ 0.12963404 -0.4326335  -0.2991053   0.38177157]', '[ 0.06259366 -0.33924046 -0.35533189  0.52721541]', '[-0.00545982 -0.23320565 -0.30834707  0.50479686]', '[-0.05435734 -0.14835926 -0.16821515  0.32158817]', '[-0.0690908  -0.1113463   0.02479252  0.04024292]', '[-0.04470101 -0.1325791   0.21323988 -0.24461353]', '[ 0.01207873 -0.20303341  0.340642   -0.43848531]', '[ 0.08482177 -0.29746838  0.36917508 -0.47850826]', '[ 0.1525418  -0.38334874  0.2921883  -0.35655192]', '[ 0.19617153 -0.4320439   0.13444274 -0.11715048]', '[ 0.20388778 -0.42720707 -0.05849114  0.16546952]', '[ 0.17398796 -0.36847879 -0.23295603  0.40829353]', '[ 0.1153207  -0.27180171 -0.33916027  0.53394423]', '[ 0.04516552 -0.16633744 -0.34496401  0.4919154 ]', '[-0.0156794  -0.08639963 -0.2487325   0.28429739]', '[-0.04944028 -0.05989949 -0.0814285  -0.02873616]', '[-0.04694202 -0.0986057   0.1044044  -0.35075043]', '[-0.01029722 -0.19395393  0.25133512 -0.58004048]', '[ 0.04794467 -0.31925892  0.31539355 -0.64253249]', '[ 0.10916681 -0.4383569   0.28149033 -0.52044648]', '[ 0.15494366 -0.5175889   0.16566025 -0.25405374]', '[ 0.17232096 -0.53511424  0.00449839  0.08332966]', '[ 0.15672589 -0.48504811 -0.15630978  0.40789288]', '[ 0.11295623 -0.37847862 -0.27006623  0.63512111]', '[ 0.05445207 -0.24243394 -0.29919459  0.6938453 ]', '[-8.55415035e-06 -1.14387117e-01 -2.30313400e-01  5.56016231e-01]', '[-0.03234316 -0.03095466 -0.08398241  0.2590858 ]', '[-0.03149599 -0.01555775  0.09251092 -0.10717874]', '[ 0.00289903 -0.07121941  0.24247762 -0.4340178 ]', '[ 0.06036847 -0.17995142  0.31692464 -0.62513263]', '[ 0.12280364 -0.3084402   0.29089975 -0.62842443]', '[ 0.17046561 -0.41930362  0.17342852 -0.45592275]', '[ 0.18845389 -0.48309582  0.00175629 -0.17045621]', '[ 0.17085017 -0.48542883 -0.17405849  0.14463445]', '[ 0.12188749 -0.42889481 -0.30435303  0.40502489]', '[ 0.05485204 -0.33207856 -0.3499268   0.53755427]', '[-0.01109282 -0.22545104 -0.29306061  0.50055708]', '[-0.0562388  -0.14265631 -0.1468137   0.30626435]', '[-0.06655496 -0.1092283   0.04655432  0.02103969]', '[-0.03828739 -0.13400489  0.22936268 -0.25963315]', '[ 0.02075592 -0.2065006   0.34664538 -0.44320477]', '[ 0.09352759 -0.30065256  0.36349482 -0.4710981 ]', '[ 0.15906701 -0.38405907  0.27660445 -0.34005201]', '[ 0.19893847 -0.42904752  0.11329493 -0.09771185]', '[ 0.20233283 -0.42061863 -0.07962023  0.18082312]', '[ 0.16867979 -0.35978016 -0.24854041  0.41313049]', '[ 0.10781346 -0.26357345 -0.34510867  0.52404886]', '[ 0.03756826 -0.16158606 -0.33999876  0.46757617]', '[-0.02134095 -0.08751632 -0.23493228  0.25129289]', '[-0.05183159 -0.06770688 -0.06340633 -0.06096496]', '[-0.04577688 -0.11192892  0.12105164 -0.37217439]', '[-0.00636211 -0.20981062  0.2617703  -0.58312574]', '[ 0.05311776 -0.33366903  0.31720956 -0.62520875]', '[ 0.11387031 -0.44757142  0.27528967 -0.48691928]', '[ 0.15782037 -0.51913462  0.15413599 -0.2123491 ]', '[ 0.17266067 -0.5282575  -0.00871049  0.12415312]', '[ 0.15459095 -0.47087552 -0.16718667  0.43876966]', '[ 0.10920671 -0.35984165 -0.27480368  0.647718  ]', '[ 0.05058    -0.22357198 -0.29556036  0.68321036]', '[-0.00236243 -0.09988256 -0.21920677  0.52403854]', '[-0.03204327 -0.02428592 -0.06936301  0.21452605]', '[-0.02836262 -0.01805683  0.10536514 -0.15227442]', '[ 0.00801015 -0.08178725  0.24874348 -0.46789726]', '[ 0.06580799 -0.19542955  0.31373207 -0.63949376]', '[ 0.1266619  -0.32462508  0.27865082 -0.62144791]', '[ 0.1712551  -0.4323224   0.15577799 -0.43240974]', '[ 0.18561176 -0.49043688 -0.0160227  -0.13862512]', '[ 0.1648761  -0.48630309 -0.186849    0.1761045 ]', '[ 0.11419159 -0.42417757 -0.308311    0.4283408 ]', '[ 0.04741783 -0.32401123 -0.34329362  0.54714212]', '[-0.01620478 -0.21699361 -0.27691391  0.4951125 ]', '[-0.05748608 -0.13650046 -0.12517129  0.28970765]', '[-0.06340893 -0.10688041  0.06783391  0.0008713 ]', '[-0.03142722 -0.1353568   0.24435981 -0.27524853]', '[ 0.02961009 -0.20998313  0.35113223 -0.44825277]', '[ 0.1020983  -0.30391169  0.35627322 -0.46399804]', '[ 0.16517746 -0.3849238   0.25981792 -0.32405857]', '[ 0.20110697 -0.42633289  0.09154393 -0.07903781]', '[ 0.20012989 -0.41448666 -0.10063599  0.19521183]', '[ 0.16281552 -0.35173902 -0.26334201  0.41696046]', '[ 0.09995635 -0.25618315 -0.34982669  0.51342118]', '[ 0.02988365 -0.1577558  -0.33369746  0.44320173]', '[-0.02684079 -0.08946497 -0.22002454  0.21923835]', '[-0.05388292 -0.07605512 -0.04473508 -0.09125745]', '[-0.04419617 -0.12532797  0.13780688 -0.39095496]', '[-0.00203736 -0.22518866  0.27186677 -0.58342076]', '[ 0.05858556 -0.34708685  0.31844918 -0.60564263]', '[ 0.11874462 -0.45544268  0.26844706 -0.45217168]', '[ 0.16074156 -0.5192091   0.14200673 -0.17059402]', '[ 0.17293733 -0.52003962 -0.02236528  0.16381812]', '[ 0.15233307 -0.45569821 -0.17819456  0.4672458 ]', '[ 0.10534655 -0.34079236 -0.27929557  0.65686383]', '[ 0.04667114 -0.2050374  -0.29148118  0.6687885 ]', '[-0.0046721  -0.0864086  -0.20778504  0.48897506]', '[-0.0316693  -0.01912683 -0.05477854  0.16834437]', '[-0.02520125 -0.02221553  0.11779981 -0.197232  ]', '[ 0.01303363 -0.09381422  0.25429981 -0.49995888]', '[ 0.07100818 -0.21187623  0.30978509 -0.65089385]', '[ 0.13015534 -0.34114643  0.26595612 -0.61125905]', '[ 0.17164421 -0.44507679  0.13823839 -0.40619118]', '[ 0.18245006 -0.49705658 -0.03312004 -0.10496463]', '[ 0.15876336 -0.4861893  -0.19854713  0.20840241]', '[ 0.10659692 -0.41840818 -0.31100554  0.45148228]', '[ 0.04033156 -0.31501379 -0.33550506  0.55573312]', '[-0.02077351 -0.20785551 -0.26001576  0.48824559]', '[-0.05810099 -0.12995242 -0.10341573  0.27175288]', '[-0.05968004 -0.10439027  0.08850812 -0.02036604]', '[-0.02416987 -0.13673713  0.25813825 -0.29150291]', '[ 0.03857817 -0.21358663  0.35406158 -0.45362142]', '[ 0.11046888 -0.3073455   0.34753208 -0.45715734]', '[ 0.17081847 -0.3860283   0.24190825 -0.30847886]', '[ 0.20264264 -0.42396272  0.06930968 -0.06099569]', '[ 0.19727061 -0.40884405 -0.12140226  0.20879956]', '[ 0.15641341 -0.34435319 -0.27723535  0.41996889]', '[ 0.09178962 -0.24959024 -0.35322333  0.50225676]', '[ 0.02216544 -0.15476795 -0.32601707  0.41897253]', '[-0.03212161 -0.09213518 -0.2040166   0.18826462]', '[-0.05554302 -0.08481494 -0.02546602 -0.11955956]', '[-0.04216203 -0.13867226  0.15459085 -0.40713579]', '[ 0.00269779 -0.23997684  0.28153481 -0.58107401]', '[ 0.0643504  -0.35943905  0.31901832 -0.58405638]', '[ 0.12377317 -0.46194498  0.26086964 -0.41645205]', '[ 0.16367404 -0.5178372   0.12920383 -0.12904522]', '[ 0.17310891 -0.51053798 -0.03648228  0.20205679]', '[ 0.14991297 -0.43964671 -0.18929197  0.49306636]', '[ 0.10134809 -0.32150445 -0.28347477  0.66239937]', '[ 0.04270985 -0.18701762 -0.28690959  0.6506117 ]', '[-0.00694698 -0.0741256  -0.19603172  0.45105675]', '[-0.03122902 -0.0155774  -0.0402261   0.12090059]', '[-0.0220194  -0.028055    0.1298159  -0.24163438]', '[ 0.01796282 -0.10723881  0.25915707 -0.52980885]', '[ 0.07596735 -0.22916227  0.30512621 -0.65906496]', '[ 0.13329477 -0.35783934  0.25289537 -0.59776936]', '[ 0.17166109 -0.45739992  0.12089713 -0.37732755]', '[ 0.17901197 -0.50281049 -0.04947757 -0.06963127]', '[ 0.15256201 -0.4849809  -0.20914358  0.24131059]', '[ 0.09915037 -0.41152754 -0.31247672  0.47419686]', '[ 0.03362784 -0.30507832 -0.32664237  0.56307452]', '[-0.02478393 -0.19807613 -0.2424778   0.47974174]', '[-0.05809247 -0.1230885  -0.08167209  0.25224745]', '[-0.05540165 -0.1018578   0.1084618  -0.04275511]', '[-0.01656868 -0.1382555   0.27061726 -0.30841242]', '[ 0.04759589 -0.21741834  0.35540701 -0.45927273]', '[ 0.11857601 -0.31104923  0.33730726 -0.45049543]', '[ 0.17593961 -0.38744781  0.22296617 -0.29319402]', '[ 0.20351716 -0.42198514  0.04671887 -0.0434345 ]', '[ 0.19375359 -0.40370649 -0.14178097  0.22175745]', '[ 0.14949857 -0.33760306 -0.29009763  0.42233593]', '[ 0.08335935 -0.24373903 -0.35521449  0.49073359]', '[ 0.0144715  -0.15253321 -0.31692507  0.3950417 ]', '[-0.03712438 -0.09541205 -0.18692865  0.1584704 ]', '[-0.05676153 -0.09385909 -0.00566356 -0.14584965]', '[-0.03963997 -0.15183938  0.17131257 -0.42078886]', '[ 0.00785856 -0.25407691  0.29067472 -0.57625252]', '[ 0.07040739 -0.37066773  0.31881646 -0.56067911]', '[ 0.12893159 -0.46706878  0.2524664  -0.38000974]', '[ 0.16657823 -0.51505995  0.11567108 -0.08795928]', '[ 0.17313027 -0.49984576 -0.05105896  0.23860635]', '[ 0.14729192 -0.42286497 -0.20042114  0.51599725]']</t>
+  </si>
+  <si>
+    <t>[array([-0.03763371, -0.01533471,  0.06554052, -0.01816017], dtype=float32), array([-0.00754409, -0.05458322,  0.2277812 , -0.36241836]), array([ 0.04879627, -0.15231473,  0.32089719, -0.5887683 ]), array([ 0.11397169, -0.27767857,  0.31375488, -0.63332862]), array([ 0.16759438, -0.39312519,  0.2086893 , -0.49480525]), array([ 0.1930193 , -0.46685036,  0.03906408, -0.22816919]), array([ 0.18217995, -0.48119372, -0.14531723,  0.08492936]), array([ 0.13737799, -0.43548032, -0.29255645,  0.35879992]), array([ 0.07059687, -0.34553749, -0.35944697,  0.51636187]), array([ 0.00066518, -0.24025206, -0.32266973,  0.50804924]), array([-0.05184718, -0.15356453, -0.18924715,  0.33585339]), array([-0.07099568, -0.11316   ,  0.00267821,  0.05860212]), array([-0.0506235 , -0.13098626,  0.19609592, -0.23012254]), array([ 0.00363944, -0.19947979,  0.33317766, -0.43407441]), array([ 0.07604673, -0.29425756,  0.37330708, -0.48624983]), array([ 0.14566012, -0.38269974,  0.30650217, -0.37362319]), array([ 0.19284616, -0.43524651,  0.15487527, -0.13746415]), array([ 0.20480978, -0.43420274, -0.03738189,  0.14899985]), array([ 0.17872861, -0.37781944, -0.21671607,  0.40226469]), array([ 0.12244395, -0.28089207, -0.33207824,  0.54289906]), array([ 0.05262627, -0.17207597, -0.34864539,  0.51601465]), array([-0.00991093, -0.08621824, -0.26142967,  0.31808955]), array([-0.04676022, -0.05276175, -0.09876284,  0.00534115]), array([-0.04773189, -0.08549506,  0.08793289, -0.326671  ]), array([-0.01386808, -0.17774148,  0.24064044, -0.5740393 ]), array([ 0.04305734, -0.30394484,  0.31308665, -0.65740151]), array([ 0.10464298, -0.42784083,  0.2871402 , -0.55250711]), array([ 0.15213765, -0.51456341,  0.17665722, -0.29545229]), array([ 0.17195601, -0.54054882,  0.01729499,  0.04161741]), array([ 0.15877658, -0.49810034, -0.14558791,  0.37488532]), array([ 0.11662491, -0.39653924, -0.26514127,  0.61927065]), array([ 0.05830606, -0.26143591, -0.30243069,  0.70071627]), array([ 0.00240191, -0.12975114, -0.241122  ,  0.58472722]), array([-0.03255824, -0.03901385, -0.09863914,  0.30169722]), array([-0.03459084, -0.01467301,  0.07923617, -0.06234707]), array([-0.00228999, -0.06214743,  0.23549293, -0.3987235 ]), array([ 0.05469493, -0.16555079,  0.31932445, -0.60811377]), array([ 0.11857421, -0.29274507,  0.30262565, -0.63232462]), array([ 0.16925182, -0.40618487,  0.19109743, -0.47671256]), array([ 0.19093562, -0.47518295,  0.02014588, -0.20033382]), array([ 0.17663487, -0.48368374, -0.16020096,  0.11418666]), array([ 0.12963404, -0.4326335 , -0.2991053 ,  0.38177157]), array([ 0.06259366, -0.33924046, -0.35533189,  0.52721541]), array([-0.00545982, -0.23320565, -0.30834707,  0.50479686]), array([-0.05435734, -0.14835926, -0.16821515,  0.32158817]), array([-0.0690908 , -0.1113463 ,  0.02479252,  0.04024292]), array([-0.04470101, -0.1325791 ,  0.21323988, -0.24461353]), array([ 0.01207873, -0.20303341,  0.340642  , -0.43848531]), array([ 0.08482177, -0.29746838,  0.36917508, -0.47850826]), array([ 0.1525418 , -0.38334874,  0.2921883 , -0.35655192]), array([ 0.19617153, -0.4320439 ,  0.13444274, -0.11715048]), array([ 0.20388778, -0.42720707, -0.05849114,  0.16546952]), array([ 0.17398796, -0.36847879, -0.23295603,  0.40829353]), array([ 0.1153207 , -0.27180171, -0.33916027,  0.53394423]), array([ 0.04516552, -0.16633744, -0.34496401,  0.4919154 ]), array([-0.0156794 , -0.08639963, -0.2487325 ,  0.28429739]), array([-0.04944028, -0.05989949, -0.0814285 , -0.02873616]), array([-0.04694202, -0.0986057 ,  0.1044044 , -0.35075043]), array([-0.01029722, -0.19395393,  0.25133512, -0.58004048]), array([ 0.04794467, -0.31925892,  0.31539355, -0.64253249]), array([ 0.10916681, -0.4383569 ,  0.28149033, -0.52044648]), array([ 0.15494366, -0.5175889 ,  0.16566025, -0.25405374]), array([ 0.17232096, -0.53511424,  0.00449839,  0.08332966]), array([ 0.15672589, -0.48504811, -0.15630978,  0.40789288]), array([ 0.11295623, -0.37847862, -0.27006623,  0.63512111]), array([ 0.05445207, -0.24243394, -0.29919459,  0.6938453 ]), array([-8.55415035e-06, -1.14387117e-01, -2.30313400e-01,  5.56016231e-01]), array([-0.03234316, -0.03095466, -0.08398241,  0.2590858 ]), array([-0.03149599, -0.01555775,  0.09251092, -0.10717874]), array([ 0.00289903, -0.07121941,  0.24247762, -0.4340178 ]), array([ 0.06036847, -0.17995142,  0.31692464, -0.62513263]), array([ 0.12280364, -0.3084402 ,  0.29089975, -0.62842443]), array([ 0.17046561, -0.41930362,  0.17342852, -0.45592275]), array([ 0.18845389, -0.48309582,  0.00175629, -0.17045621]), array([ 0.17085017, -0.48542883, -0.17405849,  0.14463445]), array([ 0.12188749, -0.42889481, -0.30435303,  0.40502489]), array([ 0.05485204, -0.33207856, -0.3499268 ,  0.53755427]), array([-0.01109282, -0.22545104, -0.29306061,  0.50055708]), array([-0.0562388 , -0.14265631, -0.1468137 ,  0.30626435]), array([-0.06655496, -0.1092283 ,  0.04655432,  0.02103969]), array([-0.03828739, -0.13400489,  0.22936268, -0.25963315]), array([ 0.02075592, -0.2065006 ,  0.34664538, -0.44320477]), array([ 0.09352759, -0.30065256,  0.36349482, -0.4710981 ]), array([ 0.15906701, -0.38405907,  0.27660445, -0.34005201]), array([ 0.19893847, -0.42904752,  0.11329493, -0.09771185]), array([ 0.20233283, -0.42061863, -0.07962023,  0.18082312]), array([ 0.16867979, -0.35978016, -0.24854041,  0.41313049]), array([ 0.10781346, -0.26357345, -0.34510867,  0.52404886]), array([ 0.03756826, -0.16158606, -0.33999876,  0.46757617]), array([-0.02134095, -0.08751632, -0.23493228,  0.25129289]), array([-0.05183159, -0.06770688, -0.06340633, -0.06096496]), array([-0.04577688, -0.11192892,  0.12105164, -0.37217439]), array([-0.00636211, -0.20981062,  0.2617703 , -0.58312574]), array([ 0.05311776, -0.33366903,  0.31720956, -0.62520875]), array([ 0.11387031, -0.44757142,  0.27528967, -0.48691928]), array([ 0.15782037, -0.51913462,  0.15413599, -0.2123491 ]), array([ 0.17266067, -0.5282575 , -0.00871049,  0.12415312]), array([ 0.15459095, -0.47087552, -0.16718667,  0.43876966]), array([ 0.10920671, -0.35984165, -0.27480368,  0.647718  ]), array([ 0.05058   , -0.22357198, -0.29556036,  0.68321036]), array([-0.00236243, -0.09988256, -0.21920677,  0.52403854]), array([-0.03204327, -0.02428592, -0.06936301,  0.21452605]), array([-0.02836262, -0.01805683,  0.10536514, -0.15227442]), array([ 0.00801015, -0.08178725,  0.24874348, -0.46789726]), array([ 0.06580799, -0.19542955,  0.31373207, -0.63949376]), array([ 0.1266619 , -0.32462508,  0.27865082, -0.62144791]), array([ 0.1712551 , -0.4323224 ,  0.15577799, -0.43240974]), array([ 0.18561176, -0.49043688, -0.0160227 , -0.13862512]), array([ 0.1648761 , -0.48630309, -0.186849  ,  0.1761045 ]), array([ 0.11419159, -0.42417757, -0.308311  ,  0.4283408 ]), array([ 0.04741783, -0.32401123, -0.34329362,  0.54714212]), array([-0.01620478, -0.21699361, -0.27691391,  0.4951125 ]), array([-0.05748608, -0.13650046, -0.12517129,  0.28970765]), array([-0.06340893, -0.10688041,  0.06783391,  0.0008713 ]), array([-0.03142722, -0.1353568 ,  0.24435981, -0.27524853]), array([ 0.02961009, -0.20998313,  0.35113223, -0.44825277]), array([ 0.1020983 , -0.30391169,  0.35627322, -0.46399804]), array([ 0.16517746, -0.3849238 ,  0.25981792, -0.32405857]), array([ 0.20110697, -0.42633289,  0.09154393, -0.07903781]), array([ 0.20012989, -0.41448666, -0.10063599,  0.19521183]), array([ 0.16281552, -0.35173902, -0.26334201,  0.41696046]), array([ 0.09995635, -0.25618315, -0.34982669,  0.51342118]), array([ 0.02988365, -0.1577558 , -0.33369746,  0.44320173]), array([-0.02684079, -0.08946497, -0.22002454,  0.21923835]), array([-0.05388292, -0.07605512, -0.04473508, -0.09125745]), array([-0.04419617, -0.12532797,  0.13780688, -0.39095496]), array([-0.00203736, -0.22518866,  0.27186677, -0.58342076]), array([ 0.05858556, -0.34708685,  0.31844918, -0.60564263]), array([ 0.11874462, -0.45544268,  0.26844706, -0.45217168]), array([ 0.16074156, -0.5192091 ,  0.14200673, -0.17059402]), array([ 0.17293733, -0.52003962, -0.02236528,  0.16381812]), array([ 0.15233307, -0.45569821, -0.17819456,  0.4672458 ]), array([ 0.10534655, -0.34079236, -0.27929557,  0.65686383]), array([ 0.04667114, -0.2050374 , -0.29148118,  0.6687885 ]), array([-0.0046721 , -0.0864086 , -0.20778504,  0.48897506]), array([-0.0316693 , -0.01912683, -0.05477854,  0.16834437]), array([-0.02520125, -0.02221553,  0.11779981, -0.197232  ]), array([ 0.01303363, -0.09381422,  0.25429981, -0.49995888]), array([ 0.07100818, -0.21187623,  0.30978509, -0.65089385]), array([ 0.13015534, -0.34114643,  0.26595612, -0.61125905]), array([ 0.17164421, -0.44507679,  0.13823839, -0.40619118]), array([ 0.18245006, -0.49705658, -0.03312004, -0.10496463]), array([ 0.15876336, -0.4861893 , -0.19854713,  0.20840241]), array([ 0.10659692, -0.41840818, -0.31100554,  0.45148228]), array([ 0.04033156, -0.31501379, -0.33550506,  0.55573312]), array([-0.02077351, -0.20785551, -0.26001576,  0.48824559]), array([-0.05810099, -0.12995242, -0.10341573,  0.27175288]), array([-0.05968004, -0.10439027,  0.08850812, -0.02036604]), array([-0.02416987, -0.13673713,  0.25813825, -0.29150291]), array([ 0.03857817, -0.21358663,  0.35406158, -0.45362142]), array([ 0.11046888, -0.3073455 ,  0.34753208, -0.45715734]), array([ 0.17081847, -0.3860283 ,  0.24190825, -0.30847886]), array([ 0.20264264, -0.42396272,  0.06930968, -0.06099569]), array([ 0.19727061, -0.40884405, -0.12140226,  0.20879956]), array([ 0.15641341, -0.34435319, -0.27723535,  0.41996889]), array([ 0.09178962, -0.24959024, -0.35322333,  0.50225676]), array([ 0.02216544, -0.15476795, -0.32601707,  0.41897253]), array([-0.03212161, -0.09213518, -0.2040166 ,  0.18826462]), array([-0.05554302, -0.08481494, -0.02546602, -0.11955956]), array([-0.04216203, -0.13867226,  0.15459085, -0.40713579]), array([ 0.00269779, -0.23997684,  0.28153481, -0.58107401]), array([ 0.0643504 , -0.35943905,  0.31901832, -0.58405638]), array([ 0.12377317, -0.46194498,  0.26086964, -0.41645205]), array([ 0.16367404, -0.5178372 ,  0.12920383, -0.12904522]), array([ 0.17310891, -0.51053798, -0.03648228,  0.20205679]), array([ 0.14991297, -0.43964671, -0.18929197,  0.49306636]), array([ 0.10134809, -0.32150445, -0.28347477,  0.66239937]), array([ 0.04270985, -0.18701762, -0.28690959,  0.6506117 ]), array([-0.00694698, -0.0741256 , -0.19603172,  0.45105675]), array([-0.03122902, -0.0155774 , -0.0402261 ,  0.12090059]), array([-0.0220194 , -0.028055  ,  0.1298159 , -0.24163438]), array([ 0.01796282, -0.10723881,  0.25915707, -0.52980885]), array([ 0.07596735, -0.22916227,  0.30512621, -0.65906496]), array([ 0.13329477, -0.35783934,  0.25289537, -0.59776936]), array([ 0.17166109, -0.45739992,  0.12089713, -0.37732755]), array([ 0.17901197, -0.50281049, -0.04947757, -0.06963127]), array([ 0.15256201, -0.4849809 , -0.20914358,  0.24131059]), array([ 0.09915037, -0.41152754, -0.31247672,  0.47419686]), array([ 0.03362784, -0.30507832, -0.32664237,  0.56307452]), array([-0.02478393, -0.19807613, -0.2424778 ,  0.47974174]), array([-0.05809247, -0.1230885 , -0.08167209,  0.25224745]), array([-0.05540165, -0.1018578 ,  0.1084618 , -0.04275511]), array([-0.01656868, -0.1382555 ,  0.27061726, -0.30841242]), array([ 0.04759589, -0.21741834,  0.35540701, -0.45927273]), array([ 0.11857601, -0.31104923,  0.33730726, -0.45049543]), array([ 0.17593961, -0.38744781,  0.22296617, -0.29319402]), array([ 0.20351716, -0.42198514,  0.04671887, -0.0434345 ]), array([ 0.19375359, -0.40370649, -0.14178097,  0.22175745]), array([ 0.14949857, -0.33760306, -0.29009763,  0.42233593]), array([ 0.08335935, -0.24373903, -0.35521449,  0.49073359]), array([ 0.0144715 , -0.15253321, -0.31692507,  0.3950417 ]), array([-0.03712438, -0.09541205, -0.18692865,  0.1584704 ]), array([-0.05676153, -0.09385909, -0.00566356, -0.14584965]), array([-0.03963997, -0.15183938,  0.17131257, -0.42078886]), array([ 0.00785856, -0.25407691,  0.29067472, -0.57625252]), array([ 0.07040739, -0.37066773,  0.31881646, -0.56067911]), array([ 0.12893159, -0.46706878,  0.2524664 , -0.38000974]), array([ 0.16657823, -0.51505995,  0.11567108, -0.08795928]), array([ 0.17313027, -0.49984576, -0.05105896,  0.23860635]), array([ 0.14729192, -0.42286497, -0.20042114,  0.51599725])]</t>
+  </si>
+  <si>
+    <t>['[2,1,0]', '[2,0,1]', '[1,2,0]', '[0,2,1]', '[0,0,0]', '[1,1,1]', '[0,1,1]', '[1,1,2]', '[2,2,2]', '[1,0,2]']</t>
+  </si>
+  <si>
+    <t>[1,1,1]</t>
+  </si>
+  <si>
+    <t>[2, 6, 23, 29, 31, 35, 48, 51, 54, 64, 80, 85, 87, 88]</t>
+  </si>
+  <si>
+    <t>[0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 1, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 1, 0, 0, 0, 0, 0, 0, 0, 1, 2, 2, 2, 2, 2, 2, 2, 1, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+  </si>
+  <si>
+    <t>['[-0.03763371 -0.01533471  0.06554052 -0.01816017]', '[-0.00754409 -0.05458322  0.2277812  -0.36241836]', '[ 0.03557041 -0.11811661  0.19275289 -0.25552579]', '[ 0.07892797 -0.1849336   0.22986116 -0.39424827]', '[ 0.12271824 -0.267417    0.19671429 -0.40996627]', '[ 0.15338212 -0.34091394  0.10180504 -0.30861109]', '[ 0.14821295 -0.35214844 -0.15231642  0.19659226]', '[ 0.08221469 -0.23257051 -0.49175499  0.97158045]', '[-0.03852789  0.01808886 -0.68300946  1.472231  ]', '[-0.17530395  0.32553648 -0.64578239  1.52482289]', '[-0.28221181  0.59893637 -0.39589606  1.15382079]', '[-0.32593922  0.77085441 -0.03233943  0.54190511]', '[-0.27157263  0.74958069  0.56429783 -0.74659547]', '[-0.10832682  0.48111058  1.03689058 -1.89239283]', '[ 0.1246281   0.02471156  1.23090806 -2.55404706]', '[ 0.35437564 -0.48207916  0.99898591 -2.38068657]', '[ 0.50248271 -0.88601078  0.45006796 -1.59779011]', '[ 0.52818459 -1.10802866 -0.19344758 -0.60874898]', '[ 0.40907771 -1.07197637 -0.97290555  0.96058655]', '[ 0.15191774 -0.73064751 -1.55748153  2.41249618]', '[-0.19065347 -0.1413636  -1.7864479   3.32940069]', '[-0.52060907  0.51787183 -1.41640259  3.07328476]', '[-0.72797853  1.03498197 -0.61850669  2.03553899]', '[-0.75167288  1.2947263   0.37497486  0.55961386]', '[-0.57620782  1.23129111  1.34770643 -1.19437445]', '[-0.22901394  0.81916333  2.07325181 -2.89324903]', '[ 0.22398916  0.11366419  2.34972534 -3.96128981]', '[ 0.65552412 -0.65301677  1.84758721 -3.47500973]', '[ 0.93183048 -1.22530822  0.87838779 -2.21031504]', '[ 0.99146954 -1.51000408 -0.27856296 -0.64312319]', '[ 0.81743073 -1.45541302 -1.43490757  1.20400086]', '[ 0.44189342 -1.04766574 -2.27162163  2.86736332]', '[-0.07604823 -0.30147574 -2.80667999  4.42354493]', '[-0.6177266   0.59141483 -2.45241985  4.17844205]', '[-1.01289826  1.29068265 -1.44918929  2.76663926]', '[-1.17978227  1.67861233 -0.21584309  1.13935845]', '[-1.10870908  1.77334273  0.91591961 -0.20335979]', '[-0.80642726  1.54008891  2.0716244  -2.16506095]', '[-0.29746887  0.89308029  2.96529537 -4.29876284]', '[ 0.34116542 -0.11933287  3.24515732 -5.44653759]', '[ 0.91685189 -1.1016887   2.38648635 -4.14156323]', '[ 1.2764865  -1.76512432  1.19337872 -2.53754865]', '[ 1.39120249 -2.13325376 -0.04757127 -1.16204134]', '[ 1.25306151 -2.20739118 -1.31660929  0.4389184 ]', '[ 0.86984793 -1.92317795 -2.46956479  2.44891116]', '[ 0.28764001 -1.20665986 -3.30124664  4.7522638 ]', '[-0.42222039 -0.05350896 -3.63031963  6.40474169]', '[-1.06310351  1.1212205  -2.61669872  5.01133077]', '[-1.44176858  1.91882759 -1.17446655  3.05618798]', '[-1.54275267  2.3901657   0.15894752  1.67519001]', '[-1.3823675   2.58660822  1.42894564  0.27206315]', '[-0.97600903  2.47076932  2.58456463 -1.45110433]', '[-0.3747293   1.97721588  3.32652075 -3.5050573 ]', '[ 0.31663614  1.06666389  3.52582399 -5.55863844]', '[ 0.98816081 -0.1300981   3.01690714 -5.97893836]', '[ 1.46225863 -1.19441209  1.6332534  -4.51972999]', '[ 1.63077818 -1.94551799  0.04651072 -3.02080161]', '[ 1.48374451 -2.40116328 -1.49410164 -1.5077312 ]', '[ 1.03715406 -2.49529041 -2.90472468  0.58834721]', '[ 0.36171235 -2.16154722 -3.7152513   2.74549855]', '[-0.39007637 -1.40998716 -3.69545443  4.69909427]', '[-1.08900091 -0.3377468  -3.2141408   5.76900511]', '[-1.62395839  0.75583383 -2.02765775  4.92794008]', '[-1.87835181  1.61049799 -0.49275628  3.63919897]', '[-1.80759862  2.18906044  1.1968646   2.11366253]', '[-1.40696285  2.43118299  2.77237541  0.23829073]', '[-0.7192305   2.23988443  3.99103385 -2.19896094]', '[ 0.12724112  1.54422499  4.33148582 -4.72925662]', '[ 0.9740072   0.39586689  4.03977626 -6.45457826]', '[ 1.67691207 -0.83716878  2.85930812 -5.53262823]', '[ 2.10390469 -1.8012222   1.42494105 -4.20631938]', '[ 2.25338595 -2.54894907  0.09524365 -3.29282247]', '[ 2.15737338 -3.11193593 -1.01333592 -2.30802056]', '[ 1.85119222  2.8415598  -2.05238431 -0.97665284]', '[ 1.32198929  2.79575644 -3.25476895  0.47400271]', '[ 0.55776444  3.00154429 -4.30655107  1.48520911]', '[-0.34058905 -2.93274824 -4.49004616  1.90786856]', '[-1.16552552 -2.55625642 -3.63573958  1.75650136]', '[-1.7730405  -2.26888376 -2.43933885  1.0339091 ]', '[-2.15365196 -2.16518505 -1.41008292 -0.02757566]', '[-2.34776903 -2.30475022 -0.57273031 -1.35919413]', '[-2.39412608 -2.7014313   0.100081   -2.58442016]', '[-2.29250654  2.932979    0.9768485  -3.89664359]', '[-1.96794444  2.0109066   2.35774483 -5.43303504]', '[-1.31409303  0.67201547  4.24107016 -8.16833123]', '[-0.36017097 -1.04600971  4.96792764 -8.1275243 ]', '[ 0.62171219 -2.41573451  4.80001962 -5.622931  ]', '[ 1.49869035  2.93424783  3.8305997  -3.88383122]', '[ 2.13626879  2.27855397  2.58052373 -2.69683505]', '[ 2.56410571  1.83254469  1.7693157  -1.77255596]']</t>
+  </si>
+  <si>
+    <t>[array([-0.03763371, -0.01533471,  0.06554052, -0.01816017], dtype=float32), array([-0.00754409, -0.05458322,  0.2277812 , -0.36241836]), array([ 0.03557041, -0.11811661,  0.19275289, -0.25552579]), array([ 0.07892797, -0.1849336 ,  0.22986116, -0.39424827]), array([ 0.12271824, -0.267417  ,  0.19671429, -0.40996627]), array([ 0.15338212, -0.34091394,  0.10180504, -0.30861109]), array([ 0.14821295, -0.35214844, -0.15231642,  0.19659226]), array([ 0.08221469, -0.23257051, -0.49175499,  0.97158045]), array([-0.03852789,  0.01808886, -0.68300946,  1.472231  ]), array([-0.17530395,  0.32553648, -0.64578239,  1.52482289]), array([-0.28221181,  0.59893637, -0.39589606,  1.15382079]), array([-0.32593922,  0.77085441, -0.03233943,  0.54190511]), array([-0.27157263,  0.74958069,  0.56429783, -0.74659547]), array([-0.10832682,  0.48111058,  1.03689058, -1.89239283]), array([ 0.1246281 ,  0.02471156,  1.23090806, -2.55404706]), array([ 0.35437564, -0.48207916,  0.99898591, -2.38068657]), array([ 0.50248271, -0.88601078,  0.45006796, -1.59779011]), array([ 0.52818459, -1.10802866, -0.19344758, -0.60874898]), array([ 0.40907771, -1.07197637, -0.97290555,  0.96058655]), array([ 0.15191774, -0.73064751, -1.55748153,  2.41249618]), array([-0.19065347, -0.1413636 , -1.7864479 ,  3.32940069]), array([-0.52060907,  0.51787183, -1.41640259,  3.07328476]), array([-0.72797853,  1.03498197, -0.61850669,  2.03553899]), array([-0.75167288,  1.2947263 ,  0.37497486,  0.55961386]), array([-0.57620782,  1.23129111,  1.34770643, -1.19437445]), array([-0.22901394,  0.81916333,  2.07325181, -2.89324903]), array([ 0.22398916,  0.11366419,  2.34972534, -3.96128981]), array([ 0.65552412, -0.65301677,  1.84758721, -3.47500973]), array([ 0.93183048, -1.22530822,  0.87838779, -2.21031504]), array([ 0.99146954, -1.51000408, -0.27856296, -0.64312319]), array([ 0.81743073, -1.45541302, -1.43490757,  1.20400086]), array([ 0.44189342, -1.04766574, -2.27162163,  2.86736332]), array([-0.07604823, -0.30147574, -2.80667999,  4.42354493]), array([-0.6177266 ,  0.59141483, -2.45241985,  4.17844205]), array([-1.01289826,  1.29068265, -1.44918929,  2.76663926]), array([-1.17978227,  1.67861233, -0.21584309,  1.13935845]), array([-1.10870908,  1.77334273,  0.91591961, -0.20335979]), array([-0.80642726,  1.54008891,  2.0716244 , -2.16506095]), array([-0.29746887,  0.89308029,  2.96529537, -4.29876284]), array([ 0.34116542, -0.11933287,  3.24515732, -5.44653759]), array([ 0.91685189, -1.1016887 ,  2.38648635, -4.14156323]), array([ 1.2764865 , -1.76512432,  1.19337872, -2.53754865]), array([ 1.39120249, -2.13325376, -0.04757127, -1.16204134]), array([ 1.25306151, -2.20739118, -1.31660929,  0.4389184 ]), array([ 0.86984793, -1.92317795, -2.46956479,  2.44891116]), array([ 0.28764001, -1.20665986, -3.30124664,  4.7522638 ]), array([-0.42222039, -0.05350896, -3.63031963,  6.40474169]), array([-1.06310351,  1.1212205 , -2.61669872,  5.01133077]), array([-1.44176858,  1.91882759, -1.17446655,  3.05618798]), array([-1.54275267,  2.3901657 ,  0.15894752,  1.67519001]), array([-1.3823675 ,  2.58660822,  1.42894564,  0.27206315]), array([-0.97600903,  2.47076932,  2.58456463, -1.45110433]), array([-0.3747293 ,  1.97721588,  3.32652075, -3.5050573 ]), array([ 0.31663614,  1.06666389,  3.52582399, -5.55863844]), array([ 0.98816081, -0.1300981 ,  3.01690714, -5.97893836]), array([ 1.46225863, -1.19441209,  1.6332534 , -4.51972999]), array([ 1.63077818, -1.94551799,  0.04651072, -3.02080161]), array([ 1.48374451, -2.40116328, -1.49410164, -1.5077312 ]), array([ 1.03715406, -2.49529041, -2.90472468,  0.58834721]), array([ 0.36171235, -2.16154722, -3.7152513 ,  2.74549855]), array([-0.39007637, -1.40998716, -3.69545443,  4.69909427]), array([-1.08900091, -0.3377468 , -3.2141408 ,  5.76900511]), array([-1.62395839,  0.75583383, -2.02765775,  4.92794008]), array([-1.87835181,  1.61049799, -0.49275628,  3.63919897]), array([-1.80759862,  2.18906044,  1.1968646 ,  2.11366253]), array([-1.40696285,  2.43118299,  2.77237541,  0.23829073]), array([-0.7192305 ,  2.23988443,  3.99103385, -2.19896094]), array([ 0.12724112,  1.54422499,  4.33148582, -4.72925662]), array([ 0.9740072 ,  0.39586689,  4.03977626, -6.45457826]), array([ 1.67691207, -0.83716878,  2.85930812, -5.53262823]), array([ 2.10390469, -1.8012222 ,  1.42494105, -4.20631938]), array([ 2.25338595, -2.54894907,  0.09524365, -3.29282247]), array([ 2.15737338, -3.11193593, -1.01333592, -2.30802056]), array([ 1.85119222,  2.8415598 , -2.05238431, -0.97665284]), array([ 1.32198929,  2.79575644, -3.25476895,  0.47400271]), array([ 0.55776444,  3.00154429, -4.30655107,  1.48520911]), array([-0.34058905, -2.93274824, -4.49004616,  1.90786856]), array([-1.16552552, -2.55625642, -3.63573958,  1.75650136]), array([-1.7730405 , -2.26888376, -2.43933885,  1.0339091 ]), array([-2.15365196, -2.16518505, -1.41008292, -0.02757566]), array([-2.34776903, -2.30475022, -0.57273031, -1.35919413]), array([-2.39412608, -2.7014313 ,  0.100081  , -2.58442016]), array([-2.29250654,  2.932979  ,  0.9768485 , -3.89664359]), array([-1.96794444,  2.0109066 ,  2.35774483, -5.43303504]), array([-1.31409303,  0.67201547,  4.24107016, -8.16833123]), array([-0.36017097, -1.04600971,  4.96792764, -8.1275243 ]), array([ 0.62171219, -2.41573451,  4.80001962, -5.622931  ]), array([ 1.49869035,  2.93424783,  3.8305997 , -3.88383122]), array([ 2.13626879,  2.27855397,  2.58052373, -2.69683505]), array([ 2.56410571,  1.83254469,  1.7693157 , -1.77255596])]</t>
+  </si>
+  <si>
+    <t>['[1,1,1]', '[1,2,0]', '[1,1,2]', '[2,2,2]', '[1,0,2]', '[2,0,1]', '[0,1,1]', '[2,1,0]', '[0,2,1]', '[0,0,0]']</t>
+  </si>
+  <si>
+    <t>[1, 5, 8, 11, 14, 16, 17, 20, 25, 27, 28, 33, 35, 36, 37, 38, 39, 40, 42, 43, 44, 45, 46, 47, 49, 53, 54, 55, 57, 58, 59, 60, 64, 69, 73, 74, 76, 81, 82, 87, 88, 90, 100, 102, 108, 109]</t>
+  </si>
+  <si>
+    <t>[0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 1, 2, 2, 2, 2, 2, 2, 2, 2, 1, 0, 0, 0, 0, 0]</t>
+  </si>
+  <si>
+    <t>['[-0.03763371 -0.01533471  0.06554052 -0.01816017]', '[-0.0208055  -0.02030166  0.09914155 -0.02801351]', '[ 0.013578   -0.05917353  0.23628798 -0.34824344]', '[ 0.06892075 -0.15170277  0.30283362 -0.5520916 ]', '[ 0.12827063 -0.26838081  0.27505366 -0.58564774]', '[ 0.16005875 -0.34102171  0.03515865 -0.12569461]', '[ 0.12853775 -0.28300606 -0.34263689  0.69246565]', '[ 0.02967829 -0.07631626 -0.62005388  1.32504849]', '[-0.09246068  0.18592321 -0.56754814  1.23120791]', '[-0.1976969   0.42525518 -0.45641363  1.1061965 ]', '[-0.26530513  0.60912674 -0.20326561  0.69842509]', '[-0.26302958  0.66372753  0.2246754  -0.15656325]', '[-0.16680371  0.51765705  0.71872155 -1.27833   ]', '[ 0.0124048   0.17197175  1.02997135 -2.0994731 ]', '[ 0.2090163  -0.24365488  0.87971357 -1.94585788]', '[ 0.35704713 -0.600544    0.56171405 -1.54674072]', '[ 0.41110979 -0.80959286 -0.02920943 -0.52168299]', '[ 0.34662659 -0.80649065 -0.60190911  0.54576576]', '[ 0.1675692  -0.56771434 -1.15559225  1.80278521]', '[-0.09650255 -0.1145736  -1.42064778  2.61316666]', '[-0.35550054  0.3823065  -1.09801968  2.21941658]', '[-0.52565236  0.76452727 -0.56548069  1.53514494]', '[-0.57276171  0.9803314   0.10102203  0.60374824]', '[-0.46589531  0.94458041  0.9469516  -0.95497077]', '[-0.20633833  0.60538674  1.60448403 -2.39024761]', '[ 0.13673026  0.06212475  1.73897486 -2.8835563 ]', '[ 0.46300931 -0.50695129  1.43635223 -2.64338708]', '[ 0.67239452 -0.9176374   0.62344881 -1.41645785]', '[ 0.70617916 -1.06671357 -0.28644978 -0.06947851]', '[ 0.55119775 -0.91569372 -1.24134589  1.57602388]', '[ 0.22379676 -0.4449935  -1.97531981  3.05757966]', '[-0.20191144  0.24272702 -2.1617158   3.58599373]', '[-0.59138034  0.89327617 -1.64573111  2.7698439 ]', '[-0.82816075  1.29640938 -0.69802256  1.2564462 ]', '[-0.87533873  1.42445164  0.22928548  0.02449156]', '[-0.72993849  1.27863076  1.20687977 -1.48988228]', '[-0.40394683  0.82715945  2.0102243  -2.99974762]', '[ 0.04604846  0.1166174   2.38032189 -3.90382345]', '[ 0.49156105 -0.62063731  1.95480293 -3.23656349]', '[ 0.79596223 -1.1263714   1.04855096 -1.78290436]', '[ 0.90266398 -1.33339035  0.01086897 -0.2927491 ]', '[ 0.7914319  -1.21648025 -1.11146929  1.4714899 ]', '[ 0.47746951 -0.76939455 -1.98793128  2.97579577]', '[ 0.02437494 -0.06447944 -2.4314289   3.86762506]', '[-0.43778372  0.66295326 -2.06916611  3.17557942]', '[-0.77041651  1.15456347 -1.21203373  1.70295306]', '[-0.91195946  1.3441739  -0.18975495  0.2011394 ]', '[-0.84464094  1.23614923  0.85701946 -1.2857466 ]', '[-0.56471341  0.79765424  1.91514825 -3.0973971 ]', '[-0.11456627  0.05883346  2.47547463 -4.08536032]', '[ 0.37801179 -0.74707082  2.31338395 -3.70255992]', '[ 0.77217797 -1.35790731  1.57443466 -2.35731442]', '[ 0.99423847 -1.69060125  0.62517191 -0.98395324]', '[ 1.00946225 -1.73226703 -0.47294926  0.56479236]', '[ 0.80867095 -1.46024161 -1.51695346  2.17615987]', '[ 0.41353488 -0.85359911 -2.39215024  3.8750556 ]', '[-0.12769257  0.07298444 -2.87081496  5.08797985]', '[-0.64540244  0.98592404 -2.18075613  3.80197666]', '[-0.97709446  1.56973278 -1.11306582  2.05547506]', '[-1.08591433  1.81993959  0.02816082  0.4638776 ]', '[-0.96793597  1.75584168  1.13638061 -1.11724118]', '[-0.63277206  1.33856196  2.18558769 -3.09060594]', '[-0.10899746  0.51365785  2.98025191 -5.06419517]', '[ 0.49564492 -0.55578318  2.86200774 -5.18795066]', '[ 0.9629674  -1.41020849  1.7587789  -3.30896619]', '[ 1.20101365 -1.91990345  0.61075352 -1.82171043]', '[ 1.2060078  -2.14643589 -0.55498379 -0.44571563]', '[ 0.97212336 -2.05067595 -1.75093197  1.42552786]', '[ 0.52397513 -1.56271995 -2.68011614  3.49297322]', '[-0.06934615 -0.67431691 -3.17789272  5.29138282]', '[-0.69867503  0.45567204 -2.90708131  5.5436131 ]', '[-1.16423318  1.40568238 -1.68529403  3.88464787]', '[-1.36668088  2.02560116 -0.3379525   2.35432163]', '[-1.295708    2.33200922  1.0272971   0.70707241]', '[-0.96822394  2.30225359  2.19945986 -1.02342426]', '[-0.4380737   1.89415934  3.01345166 -3.07366675]', '[ 0.19334588  1.09816487  3.2272589  -4.82673954]', '[ 8.29378637e-01  4.01164662e-03  2.98799436e+00 -5.76588438e+00]', '[ 1.3145159  -1.04229337  1.75092929 -4.49128183]', '[ 1.5132586  -1.78505239  0.22593452 -2.96148528]', '[ 1.40592442 -2.22790777 -1.28157845 -1.4440446 ]', '[ 1.00902494 -2.32881044 -2.62410867  0.46152442]', '[ 0.39382805 -2.03806661 -3.40588578  2.43796958]', '[-0.30739433 -1.34636262 -3.50299033  4.40709469]', '[-0.97685262 -0.33118135 -3.10232705  5.49371604]', '[-1.49501961  0.71235004 -1.96818966  4.69838163]', '[-1.74054     1.51872125 -0.46167481  3.3733284 ]', '[-1.66600549  2.03692929  1.20380638  1.77600803]', '[-1.26691007  2.20411494  2.7429661  -0.17677638]', '[-0.59420716  1.91865651  3.86557669 -2.72681254]', '[ 0.21672742  1.13534693  4.12824362 -5.02174508]', '[ 1.02262582 -0.02221172  3.77006264 -6.10700031]', '[ 1.65337421 -1.11947875  2.45904735 -4.69965657]', '[ 2.00523742 -1.92472315  1.07213238 -3.44079221]', '[ 2.08613518 -2.51357619 -0.25064955 -2.44712623]', '[ 1.90504199 -2.8717143  -1.54778965 -1.09455165]', '[ 1.46201603 -2.91557314 -2.87871753  0.69162683]', '[ 0.76575314 -2.58186104 -3.99634448  2.68486531]', '[-0.0774133  -1.82672331 -4.28766369  4.88280943]', '[-0.91262075 -0.64561797 -4.01113216  6.75112092]', '[-1.61294763  0.66190075 -2.83051472  5.89938268]', '[-2.0261753   1.69286496 -1.29413005  4.47401818]', '[-2.12604633  2.45611485  0.27047117  3.18263339]', '[-1.93792895  2.97785388  1.57557708  2.0012405 ]', '[-1.49908496 -3.05461804  2.80321767  0.510942  ]', '[-0.81665643 -3.10600319  3.97097674 -0.95645739]', '[ 0.04464072  2.87916409  4.47375187 -1.93228598]', '[ 0.89432013  2.44225312  3.86046148 -2.32669258]', '[ 1.54292189  2.01925109  2.59148688 -1.77440705]', '[ 1.93310203  1.77499294  1.33175827 -0.59235752]']</t>
   </si>
   <si>
     <t>[0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50, 51, 52, 53, 54, 55, 56, 57, 58, 59, 60, 61, 62, 63, 64, 65, 66, 67, 68, 69, 70, 71, 72, 73, 74, 75, 76, 77, 78, 79, 80, 81, 82, 83, 84, 85, 86, 87, 88, 89, 90, 91, 92, 93, 94, 95, 96, 97, 98, 99, 100, 101, 102, 103, 104, 105, 106, 107, 108, 109]</t>
   </si>
   <si>
-    <t>[array([-0.03763371, -0.01533471,  0.06554052, -0.01816017], dtype=float32), array([-0.0208055 , -0.02030166,  0.09914155, -0.02801351]), array([ 0.013578  , -0.05917353,  0.23628798, -0.34824344]), array([ 0.05569493, -0.11750576,  0.17467028, -0.21881458]), array([ 0.08000939, -0.1414547 ,  0.06300338, -0.0132271 ]), array([ 0.06657137, -0.08758677, -0.19283697,  0.54032615]), array([ 0.00731296,  0.06492895, -0.38251373,  0.94850147]), array([-0.07746096,  0.27319091, -0.44079182,  1.08370966]), array([-0.15888768,  0.47769873, -0.35165449,  0.91660574]), array([-0.21076339,  0.6247122 , -0.15481124,  0.52721898]), array([-0.21786653,  0.68164744,  0.08517   ,  0.03521468]), array([-0.16600201,  0.60761759,  0.42274412, -0.76087299]), array([-0.05580611,  0.38860384,  0.65426274, -1.38478298]), array([ 0.0956853 ,  0.04470926,  0.81953581, -1.97208953]), array([ 0.23897176, -0.32545144,  0.57075454, -1.6404927 ]), array([ 0.31082626, -0.58329541,  0.1300411 , -0.89480725]), array([ 0.28854808, -0.6738532 , -0.34729328, -0.00519497]), array([ 0.16561334, -0.55662251, -0.85713256,  1.1511933 ]), array([-0.04013912, -0.23282112, -1.15349174,  2.00948864]), array([-0.27184803,  0.20359494, -1.09952911,  2.23265767]), array([-0.45489788,  0.61236481, -0.68395514,  1.76617058]), array([-0.53254708,  0.88586594, -0.07769622,  0.93589032]), array([-0.48521224,  0.9800007 ,  0.54041636,  0.00193093]), array([-0.31393268,  0.85973219,  1.1399975 , -1.18325198]), array([-0.0463749 ,  0.5234024 ,  1.48183551, -2.10800116]), array([ 0.25173876,  0.06065508,  1.42435304, -2.38393486]), array([ 0.49264598, -0.37283111,  0.92415958, -1.83960284]), array([ 0.61641383, -0.67690596,  0.2862465 , -1.150905  ]), array([ 0.59034061, -0.79003686, -0.54118729,  0.02784974]), array([ 0.39582786, -0.63579979, -1.36971977,  1.49191887]), array([ 0.06301046, -0.21549704, -1.88602619,  2.60236595]), array([-0.32020638,  0.33770894, -1.84496764,  2.74422719]), array([-0.63800372,  0.81715001, -1.26870854,  1.95332207]), array([-0.81076874,  1.1000733 , -0.43583786,  0.85916348]), array([-0.80817411,  1.15849981,  0.46006214, -0.27766825]), array([-0.6212991 ,  0.95950176,  1.38404633, -1.70958957]), array([-0.2704879 ,  0.48441976,  2.0617477 , -2.96337639]), array([ 0.16535436, -0.16135831,  2.17931015, -3.27197905]), array([ 0.5536822 , -0.7342766 ,  1.61851815, -2.31486065]), array([ 0.79054609, -1.06046886,  0.71900933, -0.92876785]), array([ 0.83445703, -1.10536693, -0.28473295,  0.47816123]), array([ 0.66780558, -0.83942264, -1.36563368,  2.18150781]), array([ 0.30220796, -0.24406782, -2.21964136,  3.66141312]), array([-0.17196334,  0.53234671, -2.38277492,  3.82229869]), array([-0.60228899,  1.19284624, -1.84445857,  2.67456063]), array([-0.89019239,  1.58995071, -1.00243753,  1.30033509]), array([-0.99447196,  1.71768707, -0.02937823, -0.01469416]), array([-0.89300399,  1.55992237,  1.03579238, -1.57439872]), array([-0.58691417,  1.0797985 ,  1.99817692, -3.23927693]), array([-0.11329809,  0.27932772,  2.64020328, -4.59658461]), array([ 0.40434373, -0.62560839,  2.37687947, -4.12441185]), array([ 0.79426777, -1.29284936,  1.47295282, -2.50094146]), array([ 0.98373762, -1.63052907,  0.40958836, -0.89551447]), array([ 0.95662001, -1.65536347, -0.67494058,  0.64882176]), array([ 0.71090515, -1.34021306, -1.76088457,  2.5295718 ]), array([ 0.26411249, -0.63530706, -2.65431245,  4.47370544]), array([-0.30323883,  0.3604135 , -2.83486611,  5.09202886]), array([-0.79863381,  1.25425636, -2.02685537,  3.69780825]), array([-1.09846275,  1.83669851, -0.95346646,  2.1585851 ]), array([-1.17628166,  2.12855909,  0.17583403,  0.77215012]), array([-1.02503536,  2.12350717,  1.31362519, -0.8336964 ]), array([-0.66552169,  1.78718978,  2.23312528, -2.55292606]), array([-0.1538701 ,  1.09504761,  2.82805102, -4.35373031]), array([ 0.43320308,  0.09464438,  2.89742791, -5.33980039]), array([ 0.9280553 , -0.87273469,  1.92069157, -4.07694319]), array([ 1.18960109, -1.53809163,  0.67433785, -2.58239255]), array([ 1.19617722, -1.9113529 , -0.60052956, -1.1490787 ]), array([ 0.94422955, -1.94691603, -1.87322444,  0.81418009]), array([ 0.47186129, -1.57536118, -2.77898116,  2.92145884]), array([-0.13828227, -0.77993966, -3.24818022,  4.95216595]), array([-0.7768836 ,  0.29873561, -2.95299943,  5.41058379]), array([-1.25197854,  1.24129558, -1.72419285,  3.90834685]), array([-1.458254  ,  1.8718869 , -0.33418752,  2.43225411]), array([-1.38692131,  2.21764855,  1.03492603,  1.00947729]), array([-1.04829434,  2.24306837,  2.30364062, -0.78642615]), array([-0.49475045,  1.89216695,  3.1369166 , -2.73748956]), array([ 0.16516832,  1.15333272,  3.37499311, -4.58568842]), array([ 0.81786652,  0.12924802,  3.01736108, -5.32571931]), array([ 1.30742373, -0.82480946,  1.77803069, -4.01440128]), array([ 1.5146647 , -1.46537005,  0.28666996, -2.41428738]), array([ 1.42976506, -1.81540212, -1.13429535, -1.04871224]), array([ 1.05416263, -1.8162659 , -2.57089784,  1.10342404]), array([ 0.43151476, -1.34945315, -3.56847325,  3.59970586]), array([-0.33549966, -0.39375906, -3.9735238 ,  5.71374334]), array([-1.0737705 ,  0.73119563, -3.21848224,  5.08379104]), array([-1.58709803,  1.5744898 , -1.90337992,  3.40184534]), array([-1.8372799 ,  2.1266066 , -0.60371365,  2.17463688]), array([-1.83010966,  2.45066627,  0.67270345,  1.05020239]), array([-1.5568929 ,  2.49138083,  2.05018959, -0.6938422 ]), array([-1.02533598,  2.16789948,  3.21618303, -2.61730174]), array([-0.30137498,  1.41378673,  3.9459133 , -4.97537237]), array([ 0.520961  ,  0.20410924,  4.12003489, -6.74156701]), array([ 1.24300791, -1.02169824,  2.93212243, -5.13359132]), array([ 1.68097675, -1.84761018,  1.46154552, -3.23839364]), array([ 1.83323711, -2.35020533,  0.0725274 , -1.82097015]), array([ 1.71362234, -2.57401665, -1.26192114, -0.38847068]), array([ 1.32567633, -2.46833544, -2.59540552,  1.50064848]), array([ 0.69525696, -1.94637957, -3.63266257,  3.80090645]), array([-0.09620738, -0.91827296, -4.22466971,  6.47049571]), array([-0.93576651,  0.49809105, -3.89858254,  7.00133153]), array([-1.57003313,  1.68683284, -2.41111051,  4.88913558]), array([-1.90916075,  2.51002147, -1.00832578,  3.44064587]), array([-1.98696924,  3.07905479,  0.19382064,  2.25434701]), array([-1.84104105, -2.87548476,  1.26025957,  1.0238981 ]), array([-1.47248382, -2.8130893 ,  2.44006931, -0.37822957]), array([-0.86579543, -3.01016548,  3.58550433, -1.53396641]), array([-0.07876824,  2.88091138,  4.12715322, -2.32755778]), array([ 0.70889408,  2.3692331 ,  3.58538902, -2.69751874]), array([ 1.31149321,  1.85046158,  2.3901811 , -2.35869981]), array([ 1.66773114,  1.44749146,  1.17554518, -1.59258071])]</t>
-  </si>
-  <si>
-    <t>['[1,1,2]', '[1,2,0]', '[1,1,1]', '[2,2,2]', '[1,0,2]', '[0,2,1]', '[2,1,0]', '[2,0,1]', '[0,1,1]', '[0,0,0]']</t>
-  </si>
-  <si>
-    <t>[1, 2, 3, 4, 11, 12, 13, 14, 15, 16, 23, 24, 25, 26, 27, 34, 35, 36, 37, 38, 39, 46, 47, 48, 49, 50, 51, 59, 60, 61, 62, 63, 64, 72, 73, 74, 75, 76, 77, 86, 87, 88, 89, 90, 91, 92, 101, 102, 103, 104, 105, 106, 107, 116, 117, 118, 119, 120, 121, 122, 130, 131, 132, 133, 134, 135, 136, 137, 149, 166, 167, 168, 169, 170, 171, 172, 173, 174, 175, 176, 177, 178, 179]</t>
-  </si>
-  <si>
-    <t>[0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 1, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 1, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 1, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 0, 1, 2, 2, 2, 2, 2, 2, 2, 2, 2, 1, 0, 1, 1, 2, 2, 2, 1, 2, 2, 2, 2, 2, 2, 2, 1, 2, 2, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 1, 1, 2]</t>
-  </si>
-  <si>
-    <t>['[-0.03763371 -0.01533471  0.06554052 -0.01816017]', '[-0.0208055  -0.02030166  0.09914155 -0.02801351]', '[ 0.00031733 -0.02489487  0.10765546 -0.0138725 ]', '[ 0.02044082 -0.02428802  0.08954248  0.02288616]', '[ 0.03470698 -0.01491644  0.05056501  0.07132823]', '[ 0.02674144  0.03818636 -0.12667052  0.44879208]', '[-0.01270905  0.15667936 -0.25571586  0.70881747]', '[-0.06940829  0.30836147 -0.29491305  0.77301892]', '[-0.12394901  0.4517198  -0.23590169  0.62988145]', '[-0.15876359  0.5498143  -0.10369689  0.33260441]', '[-0.16331677  0.57991751  0.05921824 -0.03571874]', '[-0.12364641  0.50409537  0.32874453 -0.70766221]', '[-0.03775164  0.30783049  0.50916352 -1.21389118]', '[ 0.06909397  0.04061776  0.52882372 -1.39480458]', '[ 0.16087913 -0.22270668  0.3614133  -1.17772404]', '[ 0.20472536 -0.40990137  0.06420388 -0.6597987 ]', '[ 0.18455416 -0.47825444 -0.26212436 -0.01817226]', '[ 0.09156532 -0.38679677 -0.64742279  0.90761115]', '[-0.06271277 -0.13292697 -0.85786545  1.56672789]', '[-0.23333411  0.20632363 -0.80133675  1.73587805]', '[-0.36498881  0.52600302 -0.4801429   1.39142644]', '[-0.41539568  0.74217732 -0.01227622  0.7395642 ]', '[-0.36944782  0.81527715  0.46213933 -0.01083091]', '[-0.22642744  0.71066606  0.93936783 -1.01021577]', '[-0.00892589  0.42883145  1.18897233 -1.74077443]', '[ 0.22660096  0.0517002   1.1068182  -1.92405165]', '[ 0.41005532 -0.29693012  0.6808143  -1.47495926]', '[ 0.48521772 -0.51258559  0.05370639 -0.64539491]', '[ 0.417663   -0.51547329 -0.71588293  0.61057794]', '[ 0.20989945 -0.2789723  -1.31808193  1.6972301 ]', '[-0.08492151  0.12510753 -1.555619    2.21640575]', '[-0.37963177  0.55019577 -1.32030983  1.91504598]', '[-0.58989289  0.85617843 -0.74359286  1.09612783]', '[-0.66706415  0.97859659 -0.01685984  0.11844472]', '[-0.58535204  0.87309513  0.82205171 -1.16698164]', '[-0.34814683  0.51985272  1.50786441 -2.31349921]', '[-0.00845867 -0.01084392  1.80187214 -2.83660639]', '[ 0.33251678 -0.53972913  1.5220548  -2.29877877]', '[ 0.57395443 -0.88909757  0.8506743  -1.14546192]', '[ 0.66227792 -0.9897414   0.02017728  0.14415152]', '[ 0.56997838 -0.80175587 -0.93344798  1.72881771]', '[ 0.29908242 -0.30913141 -1.72312117  3.11534711]', '[-0.08315313  0.37699688 -1.98491703  3.51987652]', '[-0.44967675  1.01119311 -1.6016925   2.68937509]', '[-0.70314623  1.42828109 -0.90116783  1.46392917]', '[-0.80177252  1.59623253 -0.07487256  0.2180398 ]', '[-0.72394184  1.49081901  0.8443507  -1.27627909]', '[-0.47088945  1.08272659  1.65970504 -2.80278718]', '[-0.07741763  0.38520798  2.19752525 -4.04435356]', '[ 0.35720396 -0.43419659  2.00983042 -3.86699684]', '[ 0.68247785 -1.07790494  1.18689067 -2.48691537]', '[ 0.8218953  -1.42254632  0.19968977 -0.96426762]', '[ 0.75459258 -1.43976003 -0.85807324  0.79326183]', '[ 0.48761236 -1.10140602 -1.78195125  2.59637368]', '[ 0.05897502 -0.41058711 -2.42976401  4.19816012]', '[-0.4314646   0.47314784 -2.31833387  4.31615657]', '[-0.81672247  1.21668414 -1.46858326  3.02633097]', '[-1.00690155  1.67989017 -0.42147508  1.61848727]', '[-0.98493444  1.86772757  0.63078134  0.26001653]', '[-0.75610554  1.75789692  1.62055782 -1.36967148]', '[-0.35595715  1.31549434  2.3275385  -3.05204563]', '[ 0.15035756  0.55372516  2.65209298 -4.43210369]', '[ 0.65139012 -0.34680402  2.2070832  -4.25226899]', '[ 0.985684   -1.05481891  1.0818817  -2.7503158 ]', '[ 1.07698896 -1.44506632 -0.16850092 -1.15785884]', '[ 0.91472109 -1.49041281 -1.42578234  0.72126271]', '[ 0.52287851 -1.1461743  -2.44221275  2.73697075]', '[-0.0361505  -0.40732268 -3.04996577  4.50173997]', '[-0.63332802  0.52271794 -2.74921409  4.43041987]', '[-1.08521394  1.26868163 -1.71335421  2.97168385]', '[-1.30937357  1.72013613 -0.51800962  1.57270265]', '[-1.29116306  1.90318794  0.69559698  0.25067901]', '[-1.02953854  1.78773441  1.89146013 -1.44270084]', '[-0.55192063  1.30869456  2.83147306 -3.37840682]', '[ 0.07603713  0.44640653  3.34164683 -5.06850996]', '[ 0.71210682 -0.56024523  2.83323751 -4.58992558]', '[ 1.16215327 -1.30108095  1.62634935 -2.79800121]', '[ 1.35782358 -1.69718345  0.32701124 -1.20027476]', '[ 1.29357522 -1.78600472 -0.96168782  0.32617383]', '[ 0.97175376 -1.52812432 -2.22977299  2.30896536]', '[ 0.41597596 -0.83828934 -3.27848897  4.59869571]', '[-0.29589598  0.23917885 -3.63462951  5.7170532 ]', '[-0.94771759  1.24507869 -2.7652793   4.12809826]', '[-1.3858772   1.8946614  -1.59986594  2.43902533]', '[-1.58385127  2.24551268 -0.37549195  1.10482016]', '[-1.53593163  2.34055771  0.85171873 -0.16574769]', '[-1.24009148  2.1465686   2.08624736 -1.82154505]', '[-0.71580124  1.58642695  3.11066757 -3.85121969]', '[-0.01649641  0.58958886  3.7980246  -6.00223423]', '[ 0.72271584 -0.63022441  3.35288458 -5.6346347 ]', '[ 1.26589318 -1.54531652  2.04677077 -3.52825443]', '[ 1.54074324 -2.07682244  0.70323788 -1.85302157]', '[ 1.54835695 -2.29852825 -0.62191464 -0.36347038]', '[ 1.28922281 -2.19185675 -1.9499368   1.47371554]', '[ 0.78183018 -1.68361201 -3.0800747   3.68957098]', '[ 0.07510218 -0.68649233 -3.92574039  6.23524741]', '[-0.71325729  0.63892122 -3.68547243  6.37041037]', '[-1.32542542  1.70429056 -2.39999527  4.29168722]', '[-1.67421595  2.40040422 -1.09388001  2.75384971]', '[-1.76681697  2.82218046  0.15624844  1.47301302]', '[-1.60914677  2.96691106  1.4167304  -0.03901625]', '[-1.20216214  2.80054244  2.63043057 -1.64339614]', '[-0.58057383  2.29889525  3.48602181 -3.40943186]', '[ 0.14547089  1.42527121  3.68997172 -5.32339635]', '[ 0.86871302  0.21318263  3.41618363 -6.46194549]', '[ 1.42948555 -0.95919236  2.05445893 -4.98142713]', '[ 1.67483529 -1.77445984  0.39854924 -3.22775735]', '[ 1.59180912 -2.25844942 -1.2121145  -1.59112553]', '[ 1.19575826 -2.37316929 -2.6968554   0.49051754]', '[ 0.54540729 -2.04516465 -3.69231026  2.82243988]', '[-0.22927511 -1.24202884 -3.95631523  5.16342557]', '[-1.00267137 -0.05059515 -3.63330797  6.34739025]', '[-1.60638339  1.1024858  -2.30189154  4.97483052]', '[-1.91612295  1.95275299 -0.79979998  3.60222769]', '[-1.92939296  2.55603743  0.65069186  2.42014853]', '[-1.65883861  2.88835368  2.03354161  0.87190478]', '[-1.12300634  2.89650846  3.29119304 -0.79585088]', '[-0.3730975   2.57330311  4.07251217 -2.41727616]', '[ 0.43397564  1.94678789  3.83527911 -3.76498396]', '[ 1.11772579  1.1197079   2.95254049 -4.34637414]', '[ 1.60322882  0.27624163  1.87266108 -3.94256972]', '[ 1.85568026 -0.42076513  0.63192448 -2.99412334]', '[ 1.84758645 -0.91530252 -0.74252689 -1.91218232]', '[ 1.53516785 -1.1243353  -2.39895985 -0.06030483]', '[ 0.89193164 -0.88387501 -3.98223624  2.56461701]', '[-0.01384101 -0.1158549  -4.87798893  4.75920085]', '[-0.95033159  0.77136377 -4.26719273  3.64732508]', '[-1.67751612  1.28509502 -2.97730961  1.57638688]', '[-2.14758868  1.46595762 -1.76286104  0.39353309]', '[-2.40184707  1.49633464 -0.82547345  0.01251784]', '[-2.48208403  1.47238404  0.00374772 -0.21626992]', '[-2.40139649  1.41119303  0.81624496 -0.42310954]', '[-2.14425245  1.27918363  1.79576061 -0.99245103]', '[-1.66439175  0.96290081  3.04666914 -2.32103748]', '[-0.91679668  0.30191174  4.38781168 -4.24719816]', '[ 0.02796732 -0.59149018  4.82079022 -4.13187618]', '[ 0.9168387  -1.1642839   3.8906271  -1.43157984]', '[ 1.53346857 -1.17688959  2.21330178  1.17627657]', '[ 1.79959754 -0.75411058  0.48349433  2.9218081 ]', '[ 1.73523538 -0.01140089 -1.07012768  4.43846869]', '[ 1.40007919  0.97983558 -2.21311607  5.33605975]', '[ 0.86398843  2.07425611 -3.14813764  5.54392445]', '[ 0.1511617  -3.08627824 -3.85949493  5.7596688 ]', '[-0.60808892 -1.85242675 -3.64223551  6.72312879]', '[-1.31092723 -0.36359682 -3.34667928  8.01574176]', '[-1.84787359  1.14240911 -1.78440253  6.64891652]', '[-1.98581422  2.28614584  0.40066578  4.85550362]', '[-1.72263882  3.09930369  2.08305206  3.32328864]', '[-1.20031246 -2.64959604  3.03672258  2.18307333]', '[-0.55304589 -2.217815    3.26827061  2.44240369]', '[ 0.00828018 -1.53472363  2.06801222  4.71222351]', '[ 1.96590841e-01 -2.52081953e-01  2.40087418e-03  7.80262076e+00]', '[0.24447994 1.2281764  0.92403583 6.27487685]', '[0.58449703 2.25684857 2.27483329 4.32886369]', '[1.05218844 3.11398249 2.10149525 4.64405463]', '[ 1.29466003 -2.0494021  -0.02152631  6.85743506]', '[ 0.95338351 -0.28233632 -3.19454981 10.71351327]', '[ 0.3249783   1.76394691 -2.57328417  8.95553835]', '[-0.10809695 -2.85159196 -2.03572363  8.19973512]', '[-0.6114119  -1.04459352 -3.18273673 10.3513075 ]', '[-1.22504678  1.08669654 -2.17394505  9.75571331]', '[-1.31042606  2.67902884  1.11384275  6.51540765]', '[-0.96161487 -2.43232768  1.86493616  5.67342452]', '[-0.70937098 -1.16019941  0.4777811   7.43658481]', '[-0.71186902  0.53516089  0.24798302  8.45959266]', '[-0.328153    1.8067182   3.60360744  4.08077786]', '[0.58414026 2.2583573  5.07965736 0.84384527]', '[ 1.57442492  2.29835374  4.65217765 -0.13543327]', '[ 2.4335507   2.27180658  4.00619125 -0.08030387]', '[-3.05664039  2.24047267  4.07786358 -0.39411539]', '[-2.15846123  2.01857652  5.02913328 -2.14761815]', '[-1.01870207  1.23546432  6.38661169 -6.01981279]', '[ 0.36584077 -0.34764383  7.08540126 -8.56692552]', '[ 1.65748525 -1.65364547  5.73296664 -4.26111922]', '[ 2.68088255 -2.19370122  4.59142629 -1.53160831]', '[-2.73328869 -2.3940907   4.26996069 -0.72931243]', '[-1.82864616 -2.5507512   4.91052988 -0.91738732]', '[-0.74440279 -2.75430038  5.88260781 -1.00140348]', '[ 0.45631503 -2.87876318  5.88070318 -0.00641608]', '[ 1.50924739 -2.66681405  4.42247914  2.30956078]', '[ 2.14405699 -1.92091581  1.75214597  5.14278682]', '[ 2.19486473 -0.62771438 -1.09736099  7.70412888]', '[ 1.84291596  1.03908215 -1.99826202  8.45530009]']</t>
-  </si>
-  <si>
-    <t>[0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50, 51, 52, 53, 54, 55, 56, 57, 58, 59, 60, 61, 62, 63, 64, 65, 66, 67, 68, 69, 70, 71, 72, 73, 74, 75, 76, 77, 78, 79, 80, 81, 82, 83, 84, 85, 86, 87, 88, 89, 90, 91, 92, 93, 94, 95, 96, 97, 98, 99, 100, 101, 102, 103, 104, 105, 106, 107, 108, 109, 110, 111, 112, 113, 114, 115, 116, 117, 118, 119, 120, 121, 122, 123, 124, 125, 126, 127, 128, 129, 130, 131, 132, 133, 134, 135, 136, 137, 138, 139, 140, 141, 142, 143, 144, 145, 146, 147, 148, 149, 150, 151, 152, 153, 154, 155, 156, 157, 158, 159, 160, 161, 162, 163, 164, 165, 166, 167, 168, 169, 170, 171, 172, 173, 174, 175, 176, 177, 178, 179, 180, 181, 182]</t>
-  </si>
-  <si>
-    <t>[array([-0.03763371, -0.01533471,  0.06554052, -0.01816017], dtype=float32), array([-0.0208055 , -0.02030166,  0.09914155, -0.02801351]), array([ 0.00031733, -0.02489487,  0.10765546, -0.0138725 ]), array([ 0.02044082, -0.02428802,  0.08954248,  0.02288616]), array([ 0.03470698, -0.01491644,  0.05056501,  0.07132823]), array([ 0.02674144,  0.03818636, -0.12667052,  0.44879208]), array([-0.01270905,  0.15667936, -0.25571586,  0.70881747]), array([-0.06940829,  0.30836147, -0.29491305,  0.77301892]), array([-0.12394901,  0.4517198 , -0.23590169,  0.62988145]), array([-0.15876359,  0.5498143 , -0.10369689,  0.33260441]), array([-0.16331677,  0.57991751,  0.05921824, -0.03571874]), array([-0.12364641,  0.50409537,  0.32874453, -0.70766221]), array([-0.03775164,  0.30783049,  0.50916352, -1.21389118]), array([ 0.06909397,  0.04061776,  0.52882372, -1.39480458]), array([ 0.16087913, -0.22270668,  0.3614133 , -1.17772404]), array([ 0.20472536, -0.40990137,  0.06420388, -0.6597987 ]), array([ 0.18455416, -0.47825444, -0.26212436, -0.01817226]), array([ 0.09156532, -0.38679677, -0.64742279,  0.90761115]), array([-0.06271277, -0.13292697, -0.85786545,  1.56672789]), array([-0.23333411,  0.20632363, -0.80133675,  1.73587805]), array([-0.36498881,  0.52600302, -0.4801429 ,  1.39142644]), array([-0.41539568,  0.74217732, -0.01227622,  0.7395642 ]), array([-0.36944782,  0.81527715,  0.46213933, -0.01083091]), array([-0.22642744,  0.71066606,  0.93936783, -1.01021577]), array([-0.00892589,  0.42883145,  1.18897233, -1.74077443]), array([ 0.22660096,  0.0517002 ,  1.1068182 , -1.92405165]), array([ 0.41005532, -0.29693012,  0.6808143 , -1.47495926]), array([ 0.48521772, -0.51258559,  0.05370639, -0.64539491]), array([ 0.417663  , -0.51547329, -0.71588293,  0.61057794]), array([ 0.20989945, -0.2789723 , -1.31808193,  1.6972301 ]), array([-0.08492151,  0.12510753, -1.555619  ,  2.21640575]), array([-0.37963177,  0.55019577, -1.32030983,  1.91504598]), array([-0.58989289,  0.85617843, -0.74359286,  1.09612783]), array([-0.66706415,  0.97859659, -0.01685984,  0.11844472]), array([-0.58535204,  0.87309513,  0.82205171, -1.16698164]), array([-0.34814683,  0.51985272,  1.50786441, -2.31349921]), array([-0.00845867, -0.01084392,  1.80187214, -2.83660639]), array([ 0.33251678, -0.53972913,  1.5220548 , -2.29877877]), array([ 0.57395443, -0.88909757,  0.8506743 , -1.14546192]), array([ 0.66227792, -0.9897414 ,  0.02017728,  0.14415152]), array([ 0.56997838, -0.80175587, -0.93344798,  1.72881771]), array([ 0.29908242, -0.30913141, -1.72312117,  3.11534711]), array([-0.08315313,  0.37699688, -1.98491703,  3.51987652]), array([-0.44967675,  1.01119311, -1.6016925 ,  2.68937509]), array([-0.70314623,  1.42828109, -0.90116783,  1.46392917]), array([-0.80177252,  1.59623253, -0.07487256,  0.2180398 ]), array([-0.72394184,  1.49081901,  0.8443507 , -1.27627909]), array([-0.47088945,  1.08272659,  1.65970504, -2.80278718]), array([-0.07741763,  0.38520798,  2.19752525, -4.04435356]), array([ 0.35720396, -0.43419659,  2.00983042, -3.86699684]), array([ 0.68247785, -1.07790494,  1.18689067, -2.48691537]), array([ 0.8218953 , -1.42254632,  0.19968977, -0.96426762]), array([ 0.75459258, -1.43976003, -0.85807324,  0.79326183]), array([ 0.48761236, -1.10140602, -1.78195125,  2.59637368]), array([ 0.05897502, -0.41058711, -2.42976401,  4.19816012]), array([-0.4314646 ,  0.47314784, -2.31833387,  4.31615657]), array([-0.81672247,  1.21668414, -1.46858326,  3.02633097]), array([-1.00690155,  1.67989017, -0.42147508,  1.61848727]), array([-0.98493444,  1.86772757,  0.63078134,  0.26001653]), array([-0.75610554,  1.75789692,  1.62055782, -1.36967148]), array([-0.35595715,  1.31549434,  2.3275385 , -3.05204563]), array([ 0.15035756,  0.55372516,  2.65209298, -4.43210369]), array([ 0.65139012, -0.34680402,  2.2070832 , -4.25226899]), array([ 0.985684  , -1.05481891,  1.0818817 , -2.7503158 ]), array([ 1.07698896, -1.44506632, -0.16850092, -1.15785884]), array([ 0.91472109, -1.49041281, -1.42578234,  0.72126271]), array([ 0.52287851, -1.1461743 , -2.44221275,  2.73697075]), array([-0.0361505 , -0.40732268, -3.04996577,  4.50173997]), array([-0.63332802,  0.52271794, -2.74921409,  4.43041987]), array([-1.08521394,  1.26868163, -1.71335421,  2.97168385]), array([-1.30937357,  1.72013613, -0.51800962,  1.57270265]), array([-1.29116306,  1.90318794,  0.69559698,  0.25067901]), array([-1.02953854,  1.78773441,  1.89146013, -1.44270084]), array([-0.55192063,  1.30869456,  2.83147306, -3.37840682]), array([ 0.07603713,  0.44640653,  3.34164683, -5.06850996]), array([ 0.71210682, -0.56024523,  2.83323751, -4.58992558]), array([ 1.16215327, -1.30108095,  1.62634935, -2.79800121]), array([ 1.35782358, -1.69718345,  0.32701124, -1.20027476]), array([ 1.29357522, -1.78600472, -0.96168782,  0.32617383]), array([ 0.97175376, -1.52812432, -2.22977299,  2.30896536]), array([ 0.41597596, -0.83828934, -3.27848897,  4.59869571]), array([-0.29589598,  0.23917885, -3.63462951,  5.7170532 ]), array([-0.94771759,  1.24507869, -2.7652793 ,  4.12809826]), array([-1.3858772 ,  1.8946614 , -1.59986594,  2.43902533]), array([-1.58385127,  2.24551268, -0.37549195,  1.10482016]), array([-1.53593163,  2.34055771,  0.85171873, -0.16574769]), array([-1.24009148,  2.1465686 ,  2.08624736, -1.82154505]), array([-0.71580124,  1.58642695,  3.11066757, -3.85121969]), array([-0.01649641,  0.58958886,  3.7980246 , -6.00223423]), array([ 0.72271584, -0.63022441,  3.35288458, -5.6346347 ]), array([ 1.26589318, -1.54531652,  2.04677077, -3.52825443]), array([ 1.54074324, -2.07682244,  0.70323788, -1.85302157]), array([ 1.54835695, -2.29852825, -0.62191464, -0.36347038]), array([ 1.28922281, -2.19185675, -1.9499368 ,  1.47371554]), array([ 0.78183018, -1.68361201, -3.0800747 ,  3.68957098]), array([ 0.07510218, -0.68649233, -3.92574039,  6.23524741]), array([-0.71325729,  0.63892122, -3.68547243,  6.37041037]), array([-1.32542542,  1.70429056, -2.39999527,  4.29168722]), array([-1.67421595,  2.40040422, -1.09388001,  2.75384971]), array([-1.76681697,  2.82218046,  0.15624844,  1.47301302]), array([-1.60914677,  2.96691106,  1.4167304 , -0.03901625]), array([-1.20216214,  2.80054244,  2.63043057, -1.64339614]), array([-0.58057383,  2.29889525,  3.48602181, -3.40943186]), array([ 0.14547089,  1.42527121,  3.68997172, -5.32339635]), array([ 0.86871302,  0.21318263,  3.41618363, -6.46194549]), array([ 1.42948555, -0.95919236,  2.05445893, -4.98142713]), array([ 1.67483529, -1.77445984,  0.39854924, -3.22775735]), array([ 1.59180912, -2.25844942, -1.2121145 , -1.59112553]), array([ 1.19575826, -2.37316929, -2.6968554 ,  0.49051754]), array([ 0.54540729, -2.04516465, -3.69231026,  2.82243988]), array([-0.22927511, -1.24202884, -3.95631523,  5.16342557]), array([-1.00267137, -0.05059515, -3.63330797,  6.34739025]), array([-1.60638339,  1.1024858 , -2.30189154,  4.97483052]), array([-1.91612295,  1.95275299, -0.79979998,  3.60222769]), array([-1.92939296,  2.55603743,  0.65069186,  2.42014853]), array([-1.65883861,  2.88835368,  2.03354161,  0.87190478]), array([-1.12300634,  2.89650846,  3.29119304, -0.79585088]), array([-0.3730975 ,  2.57330311,  4.07251217, -2.41727616]), array([ 0.43397564,  1.94678789,  3.83527911, -3.76498396]), array([ 1.11772579,  1.1197079 ,  2.95254049, -4.34637414]), array([ 1.60322882,  0.27624163,  1.87266108, -3.94256972]), array([ 1.85568026, -0.42076513,  0.63192448, -2.99412334]), array([ 1.84758645, -0.91530252, -0.74252689, -1.91218232]), array([ 1.53516785, -1.1243353 , -2.39895985, -0.06030483]), array([ 0.89193164, -0.88387501, -3.98223624,  2.56461701]), array([-0.01384101, -0.1158549 , -4.87798893,  4.75920085]), array([-0.95033159,  0.77136377, -4.26719273,  3.64732508]), array([-1.67751612,  1.28509502, -2.97730961,  1.57638688]), array([-2.14758868,  1.46595762, -1.76286104,  0.39353309]), array([-2.40184707,  1.49633464, -0.82547345,  0.01251784]), array([-2.48208403,  1.47238404,  0.00374772, -0.21626992]), array([-2.40139649,  1.41119303,  0.81624496, -0.42310954]), array([-2.14425245,  1.27918363,  1.79576061, -0.99245103]), array([-1.66439175,  0.96290081,  3.04666914, -2.32103748]), array([-0.91679668,  0.30191174,  4.38781168, -4.24719816]), array([ 0.02796732, -0.59149018,  4.82079022, -4.13187618]), array([ 0.9168387 , -1.1642839 ,  3.8906271 , -1.43157984]), array([ 1.53346857, -1.17688959,  2.21330178,  1.17627657]), array([ 1.79959754, -0.75411058,  0.48349433,  2.9218081 ]), array([ 1.73523538, -0.01140089, -1.07012768,  4.43846869]), array([ 1.40007919,  0.97983558, -2.21311607,  5.33605975]), array([ 0.86398843,  2.07425611, -3.14813764,  5.54392445]), array([ 0.1511617 , -3.08627824, -3.85949493,  5.7596688 ]), array([-0.60808892, -1.85242675, -3.64223551,  6.72312879]), array([-1.31092723, -0.36359682, -3.34667928,  8.01574176]), array([-1.84787359,  1.14240911, -1.78440253,  6.64891652]), array([-1.98581422,  2.28614584,  0.40066578,  4.85550362]), array([-1.72263882,  3.09930369,  2.08305206,  3.32328864]), array([-1.20031246, -2.64959604,  3.03672258,  2.18307333]), array([-0.55304589, -2.217815  ,  3.26827061,  2.44240369]), array([ 0.00828018, -1.53472363,  2.06801222,  4.71222351]), array([ 1.96590841e-01, -2.52081953e-01,  2.40087418e-03,  7.80262076e+00]), array([0.24447994, 1.2281764 , 0.92403583, 6.27487685]), array([0.58449703, 2.25684857, 2.27483329, 4.32886369]), array([1.05218844, 3.11398249, 2.10149525, 4.64405463]), array([ 1.29466003, -2.0494021 , -0.02152631,  6.85743506]), array([ 0.95338351, -0.28233632, -3.19454981, 10.71351327]), array([ 0.3249783 ,  1.76394691, -2.57328417,  8.95553835]), array([-0.10809695, -2.85159196, -2.03572363,  8.19973512]), array([-0.6114119 , -1.04459352, -3.18273673, 10.3513075 ]), array([-1.22504678,  1.08669654, -2.17394505,  9.75571331]), array([-1.31042606,  2.67902884,  1.11384275,  6.51540765]), array([-0.96161487, -2.43232768,  1.86493616,  5.67342452]), array([-0.70937098, -1.16019941,  0.4777811 ,  7.43658481]), array([-0.71186902,  0.53516089,  0.24798302,  8.45959266]), array([-0.328153  ,  1.8067182 ,  3.60360744,  4.08077786]), array([0.58414026, 2.2583573 , 5.07965736, 0.84384527]), array([ 1.57442492,  2.29835374,  4.65217765, -0.13543327]), array([ 2.4335507 ,  2.27180658,  4.00619125, -0.08030387]), array([-3.05664039,  2.24047267,  4.07786358, -0.39411539]), array([-2.15846123,  2.01857652,  5.02913328, -2.14761815]), array([-1.01870207,  1.23546432,  6.38661169, -6.01981279]), array([ 0.36584077, -0.34764383,  7.08540126, -8.56692552]), array([ 1.65748525, -1.65364547,  5.73296664, -4.26111922]), array([ 2.68088255, -2.19370122,  4.59142629, -1.53160831]), array([-2.73328869, -2.3940907 ,  4.26996069, -0.72931243]), array([-1.82864616, -2.5507512 ,  4.91052988, -0.91738732]), array([-0.74440279, -2.75430038,  5.88260781, -1.00140348]), array([ 0.45631503, -2.87876318,  5.88070318, -0.00641608]), array([ 1.50924739, -2.66681405,  4.42247914,  2.30956078]), array([ 2.14405699, -1.92091581,  1.75214597,  5.14278682]), array([ 2.19486473, -0.62771438, -1.09736099,  7.70412888]), array([ 1.84291596,  1.03908215, -1.99826202,  8.45530009])]</t>
-  </si>
-  <si>
-    <t>['[1,2,0]', '[2,0,1]', '[0,1,1]', '[1,0,2]', '[2,1,0]', '[1,1,1]', '[1,1,2]', '[2,2,2]', '[0,2,1]', '[0,0,0]']</t>
-  </si>
-  <si>
-    <t>[0,1,1]</t>
-  </si>
-  <si>
-    <t>[8, 18, 21, 30, 32, 34, 46, 49, 61, 62, 78, 94, 95, 100, 104, 110]</t>
-  </si>
-  <si>
-    <t>[0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 1, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 1, 2, 2, 2, 2, 2, 2, 2, 1, 1, 0, 0, 0, 0, 0, 1, 1, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2]</t>
-  </si>
-  <si>
-    <t>['[-0.03763371 -0.01533471  0.06554052 -0.01816017]', '[-0.00754409 -0.05458322  0.2277812  -0.36241836]', '[ 0.04879627 -0.15231473  0.32089719 -0.5887683 ]', '[ 0.11397169 -0.27767857  0.31375488 -0.63332862]', '[ 0.16759438 -0.39312519  0.2086893  -0.49480525]', '[ 0.1930193  -0.46685036  0.03906408 -0.22816919]', '[ 0.15689524 -0.41528579 -0.3922057   0.73207416]', '[ 0.04309269 -0.18588535 -0.71796191  1.51055937]', '[-0.10156356  0.12486504 -0.68790627  1.51697551]', '[-0.22927161  0.42348907 -0.55357165  1.39819937]', '[-0.31090932  0.65984646 -0.24293606  0.92318871]', '[-0.32187145  0.78154289  0.13516303  0.28054481]', '[-0.23584819  0.70921086  0.7080842  -0.98918522]', '[-0.0490822   0.39857798  1.12159951 -2.05785564]', '[ 0.19121042 -0.07513787  1.21472891 -2.55061341]', '[ 0.40736477 -0.56371893  0.88570962 -2.21595125]', '[ 0.52742041 -0.92731447  0.29092255 -1.37281403]', '[ 0.52026319 -1.10307428 -0.35718941 -0.37601845]', '[ 0.38078573 -1.04969914 -1.00966352  0.89742565]', '[ 0.11982675 -0.72393616 -1.55616388  2.31665167]', '[-0.21808542 -0.15771215 -1.7435872   3.20034189]', '[-0.52473451  0.44405853 -1.23760999  2.65133904]', '[-0.70083265  0.89038295 -0.48724101  1.74910443]', '[-0.71301301  1.13089705  0.36457626  0.64092806]', '[-0.54088115  1.08771811  1.32429401 -1.07017388]', '[-0.20061789  0.70811136  2.02267457 -2.67930499]', '[ 0.23692927  0.06077769  2.24655498 -3.5977058 ]', '[ 0.64704566 -0.63007913  1.74894327 -3.11075169]', '[ 0.90788821 -1.13795851  0.82293642 -1.9292381 ]', '[ 0.96938889 -1.3983941  -0.2108514  -0.67160322]', '[ 0.81804898 -1.37742833 -1.27915787  0.89289558]', '[ 0.46201796 -1.00864495 -2.23627198  2.79727202]', '[-0.03891106 -0.31097657 -2.6697091   4.00567617]', '[-0.56025657  0.5094458  -2.39638796  3.89845968]', '[-0.94163091  1.13768495 -1.36789914  2.33382181]', '[-1.10828122  1.47312239 -0.28633231  1.02993218]', '[-1.05519803  1.55059531  0.80932414 -0.26462627]', '[-0.77436597  1.30808796  1.96907046 -2.1918109 ]', '[-0.28373137  0.66503385  2.87616274 -4.19440812]', '[ 0.32879671 -0.28534001  3.06925465 -4.9259302 ]', '[ 0.87163667 -1.15274623  2.25813528 -3.57937425]', '[ 1.21421804 -1.71138441  1.14681498 -2.04318207]', '[ 1.32570263 -1.98377668 -0.03620591 -0.69693647]', '[ 1.18661607 -1.94444646 -1.33955614  1.11254041]', '[ 0.79961171 -1.52126378 -2.49932018  3.17844822]', '[ 0.20145473 -0.65203914 -3.42185721  5.46756156]', '[-0.49224265  0.49918232 -3.28470342  5.52416623]', '[-1.05276824  1.43842245 -2.25022486  3.78498464]', '[-1.38333822  2.03266451 -1.04480857  2.21737486]', '[-1.46179562  2.31922062  0.25727503  0.66329217]', '[-1.27718863  2.27415404  1.57160013 -1.1395652 ]', '[-0.84499962  1.84571494  2.70870624 -3.20775213]', '[-0.21165118  0.96196129  3.58276613 -5.65808066]', '[ 0.54274279 -0.33108501  3.71262584 -6.69077168]', '[ 1.1725771  -1.48802472  2.49396994 -4.73891648]', '[ 1.53677522 -2.26022     1.15174214 -3.07373099]', '[ 1.63630053 -2.73761654 -0.14485535 -1.71618483]', '[ 1.47772371 -2.9260729  -1.42998909 -0.16120796]', '[ 1.0645403  -2.77971253 -2.6657666   1.63321725]', '[ 0.44110032 -2.26662219 -3.45848363  3.52272555]', '[-0.27243498 -1.36220884 -3.6067924   5.51918017]', '[-0.96847824 -0.13324362 -3.22135829  6.41758965]', '[-1.48095562  1.01687807 -1.78114828  4.85244235]', '[-1.67561001  1.83361103 -0.15146687  3.34127036]', '[-1.54196083  2.352328    1.46826898  1.81470979]', '[-1.09243502  2.50377975  2.95840263 -0.32625824]', '[-0.39861184  2.21675993  3.84097326 -2.54029466]', '[ 0.38002607  1.50145455  3.82179788 -4.53770069]', '[ 1.09980298  0.45622653  3.3087385  -5.68343925]', '[ 1.6592705  -0.63865897  2.18279255 -5.0147566 ]', '[ 1.9501262  -1.51872308  0.70157995 -3.80586511]', '[ 1.93181086 -2.16418073 -0.89739451 -2.61422161]', '[ 1.58726434 -2.51858579 -2.5196177  -0.8617246 ]', '[ 0.93691028 -2.46454064 -3.8976598   1.45082099]', '[ 0.08459381 -1.92688664 -4.454587    3.9240608 ]', '[-0.7871099  -0.91938727 -4.18432254  5.99802159]', '[-1.55269338  0.33709581 -3.33452806  6.13180265]', '[-2.07942689  1.42642985 -1.91951422  4.77589372]', '[-2.31835592  2.26234708 -0.49504391  3.65447717]', '[-2.29598934  2.91268124  0.67612298  2.82230738]', '[-2.05852738 -2.92595736  1.67940366  1.59463899]', '[-1.61993551 -2.73784673  2.73098915  0.30233561]', '[-0.95410971 -2.80424756  3.90620485 -0.87290914]', '[-0.09053503 -3.04006526  4.58509326 -1.35176121]', '[ 0.80606138  2.98832859  4.21378077 -1.07940185]', '[ 1.54901634  2.8506663   3.16828868 -0.22226883]', '[2.07536309 2.91540209 2.12742696 0.87502886]', '[ 2.40789274 -3.0721043   1.21882283  2.03717762]', '[ 2.56037874 -2.57424748  0.28328635  2.88638336]', '[ 2.50296413 -1.91354722 -0.88162534  3.71376532]', '[ 2.19880286 -1.07093788 -2.19139701  4.8191036 ]', '[ 1.61140147  0.06180006 -3.6674898   6.45511869]', '[ 0.77142539  1.37066036 -4.64141113  6.21964487]', '[-0.22699821  2.45324033 -5.22691501  4.52509809]', '[-1.22635797 -3.10299066 -4.56416665  2.85343166]', '[-2.01442108 -2.65808839 -3.32567047  1.64020885]', '[-2.59059034 -2.41176195 -2.53287182  0.87377966]', '[-3.06806865 -2.28071471 -2.34874652  0.53120205]', '[ 2.71171802 -2.15232915 -2.79138758  0.90394807]', '[ 2.05911525 -1.8449361  -3.82182384  2.40659826]', '[ 1.16571415 -1.10560413 -5.15020654  5.23519085]', '[ 4.30758585e-03  2.66788680e-01 -6.18704718e+00  7.66780232e+00]', '[-1.16214099  1.5183044  -5.29474469  4.43478032]', '[-2.09845615  2.10158124 -4.06748784  1.67262493]', '[-2.80234365  2.27414917 -3.06562422  0.29825285]', '[ 2.90541057  2.32099733 -2.8194619   0.33439324]', '[ 2.30144265  2.45685796 -3.34904973  1.11241446]', '[ 1.52082101  2.78625326 -4.53156538  2.20580424]', '[ 0.49195665 -2.93324228 -5.6215132   3.4927215 ]', '[-0.6262016  -2.06816994 -5.31729886  5.1920255 ]', '[-1.58156145 -0.90913366 -4.24624657  6.21778173]', '[-2.34387642  0.34902387 -3.37209672  6.13888752]']</t>
-  </si>
-  <si>
-    <t>[0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50, 51, 52, 53, 54, 55, 56, 57, 58, 59, 60, 61, 62, 63, 64, 65, 66, 67, 68, 69, 70, 71, 72, 73, 74, 75, 76, 77, 78, 79, 80, 81, 82, 83, 84, 85, 86, 87, 88, 89, 90, 91, 92, 93, 94, 95, 96, 97, 98, 99, 100, 101, 102, 103, 104, 105, 106, 107, 108, 109, 110, 111]</t>
-  </si>
-  <si>
-    <t>[array([-0.03763371, -0.01533471,  0.06554052, -0.01816017], dtype=float32), array([-0.00754409, -0.05458322,  0.2277812 , -0.36241836]), array([ 0.04879627, -0.15231473,  0.32089719, -0.5887683 ]), array([ 0.11397169, -0.27767857,  0.31375488, -0.63332862]), array([ 0.16759438, -0.39312519,  0.2086893 , -0.49480525]), array([ 0.1930193 , -0.46685036,  0.03906408, -0.22816919]), array([ 0.15689524, -0.41528579, -0.3922057 ,  0.73207416]), array([ 0.04309269, -0.18588535, -0.71796191,  1.51055937]), array([-0.10156356,  0.12486504, -0.68790627,  1.51697551]), array([-0.22927161,  0.42348907, -0.55357165,  1.39819937]), array([-0.31090932,  0.65984646, -0.24293606,  0.92318871]), array([-0.32187145,  0.78154289,  0.13516303,  0.28054481]), array([-0.23584819,  0.70921086,  0.7080842 , -0.98918522]), array([-0.0490822 ,  0.39857798,  1.12159951, -2.05785564]), array([ 0.19121042, -0.07513787,  1.21472891, -2.55061341]), array([ 0.40736477, -0.56371893,  0.88570962, -2.21595125]), array([ 0.52742041, -0.92731447,  0.29092255, -1.37281403]), array([ 0.52026319, -1.10307428, -0.35718941, -0.37601845]), array([ 0.38078573, -1.04969914, -1.00966352,  0.89742565]), array([ 0.11982675, -0.72393616, -1.55616388,  2.31665167]), array([-0.21808542, -0.15771215, -1.7435872 ,  3.20034189]), array([-0.52473451,  0.44405853, -1.23760999,  2.65133904]), array([-0.70083265,  0.89038295, -0.48724101,  1.74910443]), array([-0.71301301,  1.13089705,  0.36457626,  0.64092806]), array([-0.54088115,  1.08771811,  1.32429401, -1.07017388]), array([-0.20061789,  0.70811136,  2.02267457, -2.67930499]), array([ 0.23692927,  0.06077769,  2.24655498, -3.5977058 ]), array([ 0.64704566, -0.63007913,  1.74894327, -3.11075169]), array([ 0.90788821, -1.13795851,  0.82293642, -1.9292381 ]), array([ 0.96938889, -1.3983941 , -0.2108514 , -0.67160322]), array([ 0.81804898, -1.37742833, -1.27915787,  0.89289558]), array([ 0.46201796, -1.00864495, -2.23627198,  2.79727202]), array([-0.03891106, -0.31097657, -2.6697091 ,  4.00567617]), array([-0.56025657,  0.5094458 , -2.39638796,  3.89845968]), array([-0.94163091,  1.13768495, -1.36789914,  2.33382181]), array([-1.10828122,  1.47312239, -0.28633231,  1.02993218]), array([-1.05519803,  1.55059531,  0.80932414, -0.26462627]), array([-0.77436597,  1.30808796,  1.96907046, -2.1918109 ]), array([-0.28373137,  0.66503385,  2.87616274, -4.19440812]), array([ 0.32879671, -0.28534001,  3.06925465, -4.9259302 ]), array([ 0.87163667, -1.15274623,  2.25813528, -3.57937425]), array([ 1.21421804, -1.71138441,  1.14681498, -2.04318207]), array([ 1.32570263, -1.98377668, -0.03620591, -0.69693647]), array([ 1.18661607, -1.94444646, -1.33955614,  1.11254041]), array([ 0.79961171, -1.52126378, -2.49932018,  3.17844822]), array([ 0.20145473, -0.65203914, -3.42185721,  5.46756156]), array([-0.49224265,  0.49918232, -3.28470342,  5.52416623]), array([-1.05276824,  1.43842245, -2.25022486,  3.78498464]), array([-1.38333822,  2.03266451, -1.04480857,  2.21737486]), array([-1.46179562,  2.31922062,  0.25727503,  0.66329217]), array([-1.27718863,  2.27415404,  1.57160013, -1.1395652 ]), array([-0.84499962,  1.84571494,  2.70870624, -3.20775213]), array([-0.21165118,  0.96196129,  3.58276613, -5.65808066]), array([ 0.54274279, -0.33108501,  3.71262584, -6.69077168]), array([ 1.1725771 , -1.48802472,  2.49396994, -4.73891648]), array([ 1.53677522, -2.26022   ,  1.15174214, -3.07373099]), array([ 1.63630053, -2.73761654, -0.14485535, -1.71618483]), array([ 1.47772371, -2.9260729 , -1.42998909, -0.16120796]), array([ 1.0645403 , -2.77971253, -2.6657666 ,  1.63321725]), array([ 0.44110032, -2.26662219, -3.45848363,  3.52272555]), array([-0.27243498, -1.36220884, -3.6067924 ,  5.51918017]), array([-0.96847824, -0.13324362, -3.22135829,  6.41758965]), array([-1.48095562,  1.01687807, -1.78114828,  4.85244235]), array([-1.67561001,  1.83361103, -0.15146687,  3.34127036]), array([-1.54196083,  2.352328  ,  1.46826898,  1.81470979]), array([-1.09243502,  2.50377975,  2.95840263, -0.32625824]), array([-0.39861184,  2.21675993,  3.84097326, -2.54029466]), array([ 0.38002607,  1.50145455,  3.82179788, -4.53770069]), array([ 1.09980298,  0.45622653,  3.3087385 , -5.68343925]), array([ 1.6592705 , -0.63865897,  2.18279255, -5.0147566 ]), array([ 1.9501262 , -1.51872308,  0.70157995, -3.80586511]), array([ 1.93181086, -2.16418073, -0.89739451, -2.61422161]), array([ 1.58726434, -2.51858579, -2.5196177 , -0.8617246 ]), array([ 0.93691028, -2.46454064, -3.8976598 ,  1.45082099]), array([ 0.08459381, -1.92688664, -4.454587  ,  3.9240608 ]), array([-0.7871099 , -0.91938727, -4.18432254,  5.99802159]), array([-1.55269338,  0.33709581, -3.33452806,  6.13180265]), array([-2.07942689,  1.42642985, -1.91951422,  4.77589372]), array([-2.31835592,  2.26234708, -0.49504391,  3.65447717]), array([-2.29598934,  2.91268124,  0.67612298,  2.82230738]), array([-2.05852738, -2.92595736,  1.67940366,  1.59463899]), array([-1.61993551, -2.73784673,  2.73098915,  0.30233561]), array([-0.95410971, -2.80424756,  3.90620485, -0.87290914]), array([-0.09053503, -3.04006526,  4.58509326, -1.35176121]), array([ 0.80606138,  2.98832859,  4.21378077, -1.07940185]), array([ 1.54901634,  2.8506663 ,  3.16828868, -0.22226883]), array([2.07536309, 2.91540209, 2.12742696, 0.87502886]), array([ 2.40789274, -3.0721043 ,  1.21882283,  2.03717762]), array([ 2.56037874, -2.57424748,  0.28328635,  2.88638336]), array([ 2.50296413, -1.91354722, -0.88162534,  3.71376532]), array([ 2.19880286, -1.07093788, -2.19139701,  4.8191036 ]), array([ 1.61140147,  0.06180006, -3.6674898 ,  6.45511869]), array([ 0.77142539,  1.37066036, -4.64141113,  6.21964487]), array([-0.22699821,  2.45324033, -5.22691501,  4.52509809]), array([-1.22635797, -3.10299066, -4.56416665,  2.85343166]), array([-2.01442108, -2.65808839, -3.32567047,  1.64020885]), array([-2.59059034, -2.41176195, -2.53287182,  0.87377966]), array([-3.06806865, -2.28071471, -2.34874652,  0.53120205]), array([ 2.71171802, -2.15232915, -2.79138758,  0.90394807]), array([ 2.05911525, -1.8449361 , -3.82182384,  2.40659826]), array([ 1.16571415, -1.10560413, -5.15020654,  5.23519085]), array([ 4.30758585e-03,  2.66788680e-01, -6.18704718e+00,  7.66780232e+00]), array([-1.16214099,  1.5183044 , -5.29474469,  4.43478032]), array([-2.09845615,  2.10158124, -4.06748784,  1.67262493]), array([-2.80234365,  2.27414917, -3.06562422,  0.29825285]), array([ 2.90541057,  2.32099733, -2.8194619 ,  0.33439324]), array([ 2.30144265,  2.45685796, -3.34904973,  1.11241446]), array([ 1.52082101,  2.78625326, -4.53156538,  2.20580424]), array([ 0.49195665, -2.93324228, -5.6215132 ,  3.4927215 ]), array([-0.6262016 , -2.06816994, -5.31729886,  5.1920255 ]), array([-1.58156145, -0.90913366, -4.24624657,  6.21778173]), array([-2.34387642,  0.34902387, -3.37209672,  6.13888752])]</t>
-  </si>
-  <si>
-    <t>['[1,1,1]', '[1,1,2]', '[2,2,2]', '[0,2,1]', '[0,1,1]', '[2,1,0]', '[1,0,2]', '[1,2,0]', '[2,0,1]', '[0,0,0]']</t>
-  </si>
-  <si>
-    <t>[8, 9, 19, 22, 32, 33, 34, 35, 44, 45, 46, 56, 60, 61, 62, 71, 72, 73, 74, 87, 88, 90, 94, 96, 98, 99, 102, 107, 108]</t>
-  </si>
-  <si>
-    <t>[0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 1, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 1, 1, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2]</t>
-  </si>
-  <si>
-    <t>['[-0.03763371 -0.01533471  0.06554052 -0.01816017]', '[-0.00754409 -0.05458322  0.2277812  -0.36241836]', '[ 0.04879627 -0.15231473  0.32089719 -0.5887683 ]', '[ 0.11397169 -0.27767857  0.31375488 -0.63332862]', '[ 0.16759438 -0.39312519  0.2086893  -0.49480525]', '[ 0.1930193  -0.46685036  0.03906408 -0.22816919]', '[ 0.15689524 -0.41528579 -0.3922057   0.73207416]', '[ 0.04309269 -0.18588535 -0.71796191  1.51055937]', '[-0.10156356  0.12486504 -0.68790627  1.51697551]', '[-0.21636795  0.38996412 -0.42995154  1.07414568]', '[-0.27725576  0.56952638 -0.16350655  0.68794418]', '[-0.27828103  0.65602489  0.15390405  0.16684646]', '[-0.19386239  0.57232276  0.67314696 -0.98563643]', '[-0.01986345  0.27688231  1.02794642 -1.90403547]', '[ 0.1962186  -0.15057152  1.07222081 -2.25351289]', '[ 0.38369622 -0.57517123  0.75172958 -1.89412559]', '[ 0.48199952 -0.87984738  0.21163869 -1.11221155]', '[ 0.46566981 -1.01139552 -0.36921323 -0.19628544]', '[ 0.3189943  -0.90094464 -1.07053627  1.28562506]', '[ 0.06389667 -0.54167087 -1.43061779  2.23806616]', '[-0.24018981 -0.01580509 -1.53215776  2.87439573]', '[-0.51332601  0.53877086 -1.12384468  2.52715897]', '[-0.65613602  0.92473602 -0.28160894  1.29357161]', '[-0.63464466  1.07894236  0.4903698   0.23923503]', '[-0.4464642   0.96225666  1.35863771 -1.39699428]', '[-0.10889473  0.53123704  1.95694686 -2.84108296]', '[ 0.30160076 -0.11605032  2.03856495 -3.42198772]', '[ 0.66008863 -0.74723524  1.46083772 -2.73699967]', '[ 0.86432554 -1.17986713  0.55485628 -1.56346745]', '[ 0.8777485  -1.36954208 -0.41796628 -0.3281795 ]', '[ 0.68432745 -1.25514904 -1.48777001  1.48245813]', '[ 0.29797157 -0.77418139 -2.3240886   3.29733447]', '[-0.19911914 -0.01810638 -2.51899208  4.01556416]', '[-0.65037485  0.71169845 -1.88379843  3.07735331]', '[-0.92689343  1.17716794 -0.85159481  1.56296943]', '[-0.98571982  1.33983894  0.26510292  0.06802451]', '[-0.81419598  1.17482031  1.4329052  -1.73555827]', '[-0.42373784  0.63958651  2.423381   -3.58587843]', '[ 0.11742573 -0.19880352  2.83754576 -4.49355981]', '[ 0.64302564 -1.01614962  2.3019764  -3.46940765]', '[ 1.01220318 -1.55971821  1.35472581 -1.97395163]', '[ 1.17604117 -1.81606984  0.27160201 -0.60932131]', '[ 1.10377105 -1.75960718 -0.98737371  1.18555697]', '[ 0.78666095 -1.32831735 -2.16430661  3.17582838]', '[ 0.26125456 -0.50653587 -3.01475673  4.94520803]', '[-0.35521443  0.51944092 -2.95108475  4.88437502]', '[-0.85824     1.32521522 -2.01261169  3.09649857]', '[-1.15716293  1.79244279 -0.95539175  1.60800734]', '[-1.23535392  1.97869323  0.17723677  0.26484336]', '[-1.07347004  1.85111665  1.42586653 -1.56553101]', '[-0.67447359  1.33450478  2.53637998 -3.65548791]', '[-0.07417857  0.37986794  3.37427177 -5.74271487]', '[ 0.59194431 -0.77999974  3.06468659 -5.36661849]', '[ 1.09935568 -1.67037489  1.96975262 -3.53937414]', '[ 1.37373979 -2.2211895   0.76539003 -2.019456  ]', '[ 1.40438862 -2.48834608 -0.45542047 -0.65686089]', '[ 1.1895879  -2.46024418 -1.67020401  0.95491176]', '[ 0.74583513 -2.07505393 -2.70835689  2.9365772 ]', '[ 0.1330954  -1.26644317 -3.36799763  5.18462184]', '[-0.57570519 -0.03370881 -3.54956347  6.74717861]', '[-1.17053146  1.16369042 -2.25374505  4.94575822]', '[-1.46671821  1.95469937 -0.71607206  3.04471016]', '[-1.46234226  2.39915582  0.74120665  1.40682738]', '[-1.17422352  2.4917169   2.10167121 -0.50115722]', '[-0.64534595  2.18962714  3.10020015 -2.54321161]', '[ 0.02350373  1.46789841  3.5007231  -4.67077748]', '[ 0.72837844  0.34943369  3.44791849 -6.26379571]', '[ 1.32548513 -0.84771192  2.35520293 -5.34350355]', '[ 1.64038239 -1.75074358  0.77887103 -3.73048146]', '[ 1.63731843 -2.35337268 -0.79605831 -2.29201344]', '[ 1.32683845 -2.63755735 -2.26747676 -0.52696755]', '[ 0.75269849 -2.55931529 -3.3865734   1.30665993]', '[ 0.02488661 -2.12378985 -3.735201    3.00080154]', '[-0.68264671 -1.39451545 -3.24395281  4.16379342]', '[-1.24922667 -0.52458468 -2.37257734  4.35031091]', '[-1.62249408  0.30854214 -1.30889685  3.85917771]', '[-1.75414478  0.99050266  0.03481224  2.91206333]', '[-1.59176447  1.44748867  1.62094387  1.55898907]', '[-1.08933857  1.51520264  3.34683256 -1.00180208]', '[-0.29360309  1.00965347  4.48357813 -4.05038991]', '[ 0.63977234 -0.01942376  4.628308   -5.71315025]', '[ 1.46412768 -1.02983624  3.50363335 -4.13016241]', '[ 2.04120182 -1.69278232  2.30315515 -2.64946915]', '[ 2.40151028 -2.14400154  1.33817213 -1.96215321]', '[ 2.58902599 -2.50152375  0.56320579 -1.64152273]', '[ 2.62799693 -2.78157754 -0.16072999 -1.14516523]', '[ 2.52521805 -2.94779222 -0.87782065 -0.47741887]', '[ 2.26714522 -2.95306227 -1.73940064  0.48163384]', '[ 1.81249902 -2.72840647 -2.8428591   1.84968963]', '[ 1.12048943 -2.14866961 -4.04460312  4.10316478]', '[ 0.22346352 -1.04012159 -4.88853742  7.07893303]', '[-0.78755127  0.56841115 -4.87521111  8.062488  ]', '[-1.61929641  1.90714761 -3.43952933  5.38257504]', '[-2.1849416   2.81660907 -2.2703276   3.8872701 ]', '[-2.54709199 -2.80141019 -1.42558171  2.81322215]', '[-2.78657894 -2.31320292 -1.02259999  2.08286865]', '[-2.96406555 -1.98590219 -0.78139538  1.19963997]', '[-3.11717532 -1.80474688 -0.77914478  0.63722467]', '[ 3.0025843  -1.74158391 -0.89463914  0.03730037]', '[ 2.78950383 -1.76722592 -1.29282306 -0.21735564]', '[ 2.45228609 -1.76559967 -2.14738317  0.36448395]', '[ 1.90345175 -1.55515734 -3.40158413  1.94955318]', '[ 1.08417001 -0.91967545 -4.79998048  4.57887866]', '[ 3.62205162e-03  2.64537454e-01 -5.74363170e+00  6.56043729e+00]', '[-1.08072354  1.33893222 -4.9056248   3.79702945]', '[-1.93010507  1.81097882 -3.5659475   1.13898102]', '[-2.51778123  1.88910285 -2.37697715 -0.13786317]', '[-2.90596411  1.80674146 -1.5917305  -0.53329399]', '[ 3.09571621  1.72316613 -1.30267003 -0.2063579 ]', '[ 2.81857981  1.77736346 -1.54095729  0.80574758]']</t>
-  </si>
-  <si>
-    <t>[array([-0.03763371, -0.01533471,  0.06554052, -0.01816017], dtype=float32), array([-0.00754409, -0.05458322,  0.2277812 , -0.36241836]), array([ 0.04879627, -0.15231473,  0.32089719, -0.5887683 ]), array([ 0.11397169, -0.27767857,  0.31375488, -0.63332862]), array([ 0.16759438, -0.39312519,  0.2086893 , -0.49480525]), array([ 0.1930193 , -0.46685036,  0.03906408, -0.22816919]), array([ 0.15689524, -0.41528579, -0.3922057 ,  0.73207416]), array([ 0.04309269, -0.18588535, -0.71796191,  1.51055937]), array([-0.10156356,  0.12486504, -0.68790627,  1.51697551]), array([-0.21636795,  0.38996412, -0.42995154,  1.07414568]), array([-0.27725576,  0.56952638, -0.16350655,  0.68794418]), array([-0.27828103,  0.65602489,  0.15390405,  0.16684646]), array([-0.19386239,  0.57232276,  0.67314696, -0.98563643]), array([-0.01986345,  0.27688231,  1.02794642, -1.90403547]), array([ 0.1962186 , -0.15057152,  1.07222081, -2.25351289]), array([ 0.38369622, -0.57517123,  0.75172958, -1.89412559]), array([ 0.48199952, -0.87984738,  0.21163869, -1.11221155]), array([ 0.46566981, -1.01139552, -0.36921323, -0.19628544]), array([ 0.3189943 , -0.90094464, -1.07053627,  1.28562506]), array([ 0.06389667, -0.54167087, -1.43061779,  2.23806616]), array([-0.24018981, -0.01580509, -1.53215776,  2.87439573]), array([-0.51332601,  0.53877086, -1.12384468,  2.52715897]), array([-0.65613602,  0.92473602, -0.28160894,  1.29357161]), array([-0.63464466,  1.07894236,  0.4903698 ,  0.23923503]), array([-0.4464642 ,  0.96225666,  1.35863771, -1.39699428]), array([-0.10889473,  0.53123704,  1.95694686, -2.84108296]), array([ 0.30160076, -0.11605032,  2.03856495, -3.42198772]), array([ 0.66008863, -0.74723524,  1.46083772, -2.73699967]), array([ 0.86432554, -1.17986713,  0.55485628, -1.56346745]), array([ 0.8777485 , -1.36954208, -0.41796628, -0.3281795 ]), array([ 0.68432745, -1.25514904, -1.48777001,  1.48245813]), array([ 0.29797157, -0.77418139, -2.3240886 ,  3.29733447]), array([-0.19911914, -0.01810638, -2.51899208,  4.01556416]), array([-0.65037485,  0.71169845, -1.88379843,  3.07735331]), array([-0.92689343,  1.17716794, -0.85159481,  1.56296943]), array([-0.98571982,  1.33983894,  0.26510292,  0.06802451]), array([-0.81419598,  1.17482031,  1.4329052 , -1.73555827]), array([-0.42373784,  0.63958651,  2.423381  , -3.58587843]), array([ 0.11742573, -0.19880352,  2.83754576, -4.49355981]), array([ 0.64302564, -1.01614962,  2.3019764 , -3.46940765]), array([ 1.01220318, -1.55971821,  1.35472581, -1.97395163]), array([ 1.17604117, -1.81606984,  0.27160201, -0.60932131]), array([ 1.10377105, -1.75960718, -0.98737371,  1.18555697]), array([ 0.78666095, -1.32831735, -2.16430661,  3.17582838]), array([ 0.26125456, -0.50653587, -3.01475673,  4.94520803]), array([-0.35521443,  0.51944092, -2.95108475,  4.88437502]), array([-0.85824   ,  1.32521522, -2.01261169,  3.09649857]), array([-1.15716293,  1.79244279, -0.95539175,  1.60800734]), array([-1.23535392,  1.97869323,  0.17723677,  0.26484336]), array([-1.07347004,  1.85111665,  1.42586653, -1.56553101]), array([-0.67447359,  1.33450478,  2.53637998, -3.65548791]), array([-0.07417857,  0.37986794,  3.37427177, -5.74271487]), array([ 0.59194431, -0.77999974,  3.06468659, -5.36661849]), array([ 1.09935568, -1.67037489,  1.96975262, -3.53937414]), array([ 1.37373979, -2.2211895 ,  0.76539003, -2.019456  ]), array([ 1.40438862, -2.48834608, -0.45542047, -0.65686089]), array([ 1.1895879 , -2.46024418, -1.67020401,  0.95491176]), array([ 0.74583513, -2.07505393, -2.70835689,  2.9365772 ]), array([ 0.1330954 , -1.26644317, -3.36799763,  5.18462184]), array([-0.57570519, -0.03370881, -3.54956347,  6.74717861]), array([-1.17053146,  1.16369042, -2.25374505,  4.94575822]), array([-1.46671821,  1.95469937, -0.71607206,  3.04471016]), array([-1.46234226,  2.39915582,  0.74120665,  1.40682738]), array([-1.17422352,  2.4917169 ,  2.10167121, -0.50115722]), array([-0.64534595,  2.18962714,  3.10020015, -2.54321161]), array([ 0.02350373,  1.46789841,  3.5007231 , -4.67077748]), array([ 0.72837844,  0.34943369,  3.44791849, -6.26379571]), array([ 1.32548513, -0.84771192,  2.35520293, -5.34350355]), array([ 1.64038239, -1.75074358,  0.77887103, -3.73048146]), array([ 1.63731843, -2.35337268, -0.79605831, -2.29201344]), array([ 1.32683845, -2.63755735, -2.26747676, -0.52696755]), array([ 0.75269849, -2.55931529, -3.3865734 ,  1.30665993]), array([ 0.02488661, -2.12378985, -3.735201  ,  3.00080154]), array([-0.68264671, -1.39451545, -3.24395281,  4.16379342]), array([-1.24922667, -0.52458468, -2.37257734,  4.35031091]), array([-1.62249408,  0.30854214, -1.30889685,  3.85917771]), array([-1.75414478,  0.99050266,  0.03481224,  2.91206333]), array([-1.59176447,  1.44748867,  1.62094387,  1.55898907]), array([-1.08933857,  1.51520264,  3.34683256, -1.00180208]), array([-0.29360309,  1.00965347,  4.48357813, -4.05038991]), array([ 0.63977234, -0.01942376,  4.628308  , -5.71315025]), array([ 1.46412768, -1.02983624,  3.50363335, -4.13016241]), array([ 2.04120182, -1.69278232,  2.30315515, -2.64946915]), array([ 2.40151028, -2.14400154,  1.33817213, -1.96215321]), array([ 2.58902599, -2.50152375,  0.56320579, -1.64152273]), array([ 2.62799693, -2.78157754, -0.16072999, -1.14516523]), array([ 2.52521805, -2.94779222, -0.87782065, -0.47741887]), array([ 2.26714522, -2.95306227, -1.73940064,  0.48163384]), array([ 1.81249902, -2.72840647, -2.8428591 ,  1.84968963]), array([ 1.12048943, -2.14866961, -4.04460312,  4.10316478]), array([ 0.22346352, -1.04012159, -4.88853742,  7.07893303]), array([-0.78755127,  0.56841115, -4.87521111,  8.062488  ]), array([-1.61929641,  1.90714761, -3.43952933,  5.38257504]), array([-2.1849416 ,  2.81660907, -2.2703276 ,  3.8872701 ]), array([-2.54709199, -2.80141019, -1.42558171,  2.81322215]), array([-2.78657894, -2.31320292, -1.02259999,  2.08286865]), array([-2.96406555, -1.98590219, -0.78139538,  1.19963997]), array([-3.11717532, -1.80474688, -0.77914478,  0.63722467]), array([ 3.0025843 , -1.74158391, -0.89463914,  0.03730037]), array([ 2.78950383, -1.76722592, -1.29282306, -0.21735564]), array([ 2.45228609, -1.76559967, -2.14738317,  0.36448395]), array([ 1.90345175, -1.55515734, -3.40158413,  1.94955318]), array([ 1.08417001, -0.91967545, -4.79998048,  4.57887866]), array([ 3.62205162e-03,  2.64537454e-01, -5.74363170e+00,  6.56043729e+00]), array([-1.08072354,  1.33893222, -4.9056248 ,  3.79702945]), array([-1.93010507,  1.81097882, -3.5659475 ,  1.13898102]), array([-2.51778123,  1.88910285, -2.37697715, -0.13786317]), array([-2.90596411,  1.80674146, -1.5917305 , -0.53329399]), array([ 3.09571621,  1.72316613, -1.30267003, -0.2063579 ]), array([ 2.81857981,  1.77736346, -1.54095729,  0.80574758])]</t>
-  </si>
-  <si>
-    <t>['[1,0,2]', '[0,2,1]', '[2,1,0]', '[1,2,0]', '[0,0,0]', '[2,0,1]', '[0,1,1]', '[1,1,2]', '[2,2,2]', '[1,1,1]']</t>
-  </si>
-  <si>
-    <t>[6, 7, 8, 10, 12, 19, 20, 22, 30, 31, 32, 33, 35, 44, 46, 71, 73, 74, 76, 77, 90, 91, 92, 93, 94, 95, 96]</t>
-  </si>
-  <si>
-    <t>[0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 1, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 1, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 1, 0, 0, 0, 0, 0]</t>
-  </si>
-  <si>
-    <t>['[-0.03763371 -0.01533471  0.06554052 -0.01816017]', '[-0.00754409 -0.05458322  0.2277812  -0.36241836]', '[ 0.04879627 -0.15231473  0.32089719 -0.5887683 ]', '[ 0.11397169 -0.27767857  0.31375488 -0.63332862]', '[ 0.16759438 -0.39312519  0.2086893  -0.49480525]', '[ 0.1930193  -0.46685036  0.03906408 -0.22816919]', '[ 0.16956871 -0.44830261 -0.26820417  0.40739083]', '[ 0.09055011 -0.31127879 -0.50323119  0.93116007]', '[-0.02165415 -0.09380121 -0.58952709  1.1892161 ]', '[-0.14550206  0.17387773 -0.61422386  1.41936009]', '[-0.24020309  0.41196422 -0.30815479  0.91099128]', '[-0.27488985  0.55703731 -0.02927682  0.51487191]', '[-0.23853097  0.57976184  0.3849129  -0.28484504]', '[-0.1148168   0.41682334  0.82624975 -1.30917304]', '[ 0.07706097  0.08005865  1.04448622 -1.97246274]', '[ 0.27977967 -0.32836906  0.92574093 -2.00219668]', '[ 0.42677148 -0.68151065  0.50831031 -1.46081935]', '[ 0.47402744 -0.89476941 -0.0439214  -0.64855501]', '[ 0.38827378 -0.87741839 -0.79558816  0.81424623]', '[ 0.178675   -0.60860655 -1.2606086   1.82621508]', '[-0.09448414 -0.17923063 -1.40501544  2.35299432]', '[-0.36606817  0.31025054 -1.23635701  2.40094896]', '[-0.55018582  0.6998434  -0.56624612  1.42814616]', '[-0.59597148  0.89828076  0.11597578  0.53611006]', '[-0.48344191  0.85100829  0.98864863 -1.00216112]', '[-0.21359233  0.50599696  1.66123327 -2.39188783]', '[ 0.15217693 -0.06024306  1.9016523  -3.09648649]', '[ 0.5039099  -0.65017195  1.52673731 -2.64120207]', '[ 0.73727952 -1.07668054  0.77046946 -1.58101022]', '[ 0.80425917 -1.27640594 -0.10625184 -0.41114311]', '[ 0.6872759  -1.2126082  -1.04557564  1.05174119]', '[ 0.39754678 -0.8563643  -1.81006318  2.48667754]', '[-0.01185732 -0.24755915 -2.19294212  3.44654931]', '[-0.43114516  0.42859674 -1.88447116  3.09135008]', '[-0.74171486  0.95702773 -1.16423906  2.11113022]', '[-0.87339499  1.23296604 -0.14196197  0.64827664]', '[-0.78882043  1.1890023   0.97580801 -1.09354698]', '[-0.49156949  0.79159911  1.96188169 -2.87095732]', '[-0.02901229  0.07048711  2.55455307 -4.14105045]', '[ 0.46878175 -0.73974322  2.28646558 -3.69126304]', '[ 0.84836812 -1.34550368  1.46030339 -2.32670048]', '[ 1.04146499 -1.67302558  0.45484161 -0.96354868]', '[ 1.01959005 -1.71065195 -0.6683051   0.58874627]', '[ 0.77131664 -1.4064329  -1.79330507  2.4847305 ]', '[ 0.32448303 -0.73403247 -2.6211858   4.19896812]', '[-0.24708766  0.23151627 -2.92197881  5.09366673]', '[-0.75745051  1.1142536  -2.08053288  3.5587749 ]', '[-1.07199492  1.6737619  -1.04157824  2.05703864]', '[-1.16899425  1.94707554  0.07516339  0.68875185]', '[-1.02961166  1.90372891  1.29928407 -1.13821505]', '[-0.66089905  1.47871844  2.35303356 -3.15432724]', '[-0.10419153  0.62983588  3.15068076 -5.26935217]', '[ 0.53813769 -0.50262214  3.05321797 -5.56994472]', '[ 1.04625595 -1.45341391  1.96144014 -3.86163733]', '[ 1.3150941  -2.06503446  0.72037304 -2.30445446]', '[ 1.33429379 -2.38595748 -0.52150458 -0.91006521]', '[ 1.10035355 -2.38469821 -1.78593065  0.93846788]', '[ 0.63994612 -2.00075383 -2.75096768  2.93304462]', '[ 0.02888805 -1.19819429 -3.30456239  5.10310541]', '[-6.53225596e-01 -4.88829005e-03 -3.34906838e+00  6.43878177e+00]', '[-1.21515313  1.16230004 -2.12926364  4.9672715 ]', '[-1.48962665  1.98282688 -0.61421094  3.2986766 ]', '[-1.46498354  2.49485845  0.83966338  1.82467437]', '[-1.15984203  2.68923587  2.17011314  0.11524992]', '[-0.61519013  2.52306143  3.18217054 -1.76374841]', '[ 0.06066113  1.99307049  3.43992967 -3.49725766]', '[ 0.71734497  1.15045018  3.06906837 -4.8339665 ]', '[ 1.26985253  0.12131346  2.37796986 -5.22839841]', '[ 1.62487098 -0.84160745  1.08663136 -4.25629341]', '[ 1.68211267 -1.55975962 -0.55081022 -2.88533986]', '[ 1.39786759 -1.96967678 -2.27555753 -1.12661193]', '[ 0.78960005 -1.95474767 -3.69341286  1.33457119]', '[-0.02457871 -1.40710439 -4.29278335  4.09479151]', '[-0.86438212 -0.40874053 -3.97391179  5.55195224]', '[-1.55097547  0.62974404 -2.78374105  4.53540381]', '[-1.97822008  1.41515031 -1.49654911  3.38121918]', '[-2.14462319  1.98431428 -0.17305839  2.34553026]', '[-2.04633749  2.34800912  1.16180305  1.24115256]', '[-1.67133939  2.43050903  2.58601692 -0.50663537]', '[-1.02058333  2.10425332  3.862433   -2.87243201]', '[-0.16328724  1.23749971  4.63046413 -5.85749953]', '[ 0.79196876 -0.17015832  4.68075592 -7.55028124]', '[ 1.59655163 -1.48117095  3.28134115 -5.37704639]', '[ 2.11993675 -2.38785253  2.00110877 -3.86015269]', '[ 2.41700714 -3.06612897  1.03016572 -2.97055488]', '[ 2.55523944  2.70253256  0.40016624 -2.17007981]', '[ 2.58737433  2.35499109 -0.07080584 -1.2881046 ]', '[ 2.52375491  2.19491922 -0.58419364 -0.29476708]', '[ 2.32789493  2.28591219 -1.41377997  1.21290515]', '[ 1.93980837  2.68024819 -2.51741442  2.72951169]', '[ 1.31223867 -2.91792407 -3.74867808  4.18909175]', '[ 0.47060522 -1.87254865 -4.58066257  6.46118814]', '[-0.50630491 -0.27254302 -5.05801232  9.19566092]', '[-1.39194808  1.38703708 -3.54485359  6.80146733]', '[-1.93556296  2.51107266 -1.96260442  4.67092819]', '[-2.2049319  -2.97725331 -0.80809319  3.32696604]', '[-2.28164627 -2.43886232  0.01290427  2.04690053]', '[-2.20596173 -2.1436606   0.76171223  0.89586464]', '[-1.95721081 -2.10281575  1.76564514 -0.47297196]', '[-1.47636336 -2.33882393  3.07349302 -1.81550065]', '[-0.72813918 -2.79274674  4.34656127 -2.6298105 ]', '[ 0.2027636   2.91662558  4.74874611 -3.08302617]', '[ 1.08148024  2.26846167  3.88499554 -3.33425178]', '[ 1.73203384  1.62310823  2.62545604 -3.0108994 ]']</t>
-  </si>
-  <si>
-    <t>[array([-0.03763371, -0.01533471,  0.06554052, -0.01816017], dtype=float32), array([-0.00754409, -0.05458322,  0.2277812 , -0.36241836]), array([ 0.04879627, -0.15231473,  0.32089719, -0.5887683 ]), array([ 0.11397169, -0.27767857,  0.31375488, -0.63332862]), array([ 0.16759438, -0.39312519,  0.2086893 , -0.49480525]), array([ 0.1930193 , -0.46685036,  0.03906408, -0.22816919]), array([ 0.16956871, -0.44830261, -0.26820417,  0.40739083]), array([ 0.09055011, -0.31127879, -0.50323119,  0.93116007]), array([-0.02165415, -0.09380121, -0.58952709,  1.1892161 ]), array([-0.14550206,  0.17387773, -0.61422386,  1.41936009]), array([-0.24020309,  0.41196422, -0.30815479,  0.91099128]), array([-0.27488985,  0.55703731, -0.02927682,  0.51487191]), array([-0.23853097,  0.57976184,  0.3849129 , -0.28484504]), array([-0.1148168 ,  0.41682334,  0.82624975, -1.30917304]), array([ 0.07706097,  0.08005865,  1.04448622, -1.97246274]), array([ 0.27977967, -0.32836906,  0.92574093, -2.00219668]), array([ 0.42677148, -0.68151065,  0.50831031, -1.46081935]), array([ 0.47402744, -0.89476941, -0.0439214 , -0.64855501]), array([ 0.38827378, -0.87741839, -0.79558816,  0.81424623]), array([ 0.178675  , -0.60860655, -1.2606086 ,  1.82621508]), array([-0.09448414, -0.17923063, -1.40501544,  2.35299432]), array([-0.36606817,  0.31025054, -1.23635701,  2.40094896]), array([-0.55018582,  0.6998434 , -0.56624612,  1.42814616]), array([-0.59597148,  0.89828076,  0.11597578,  0.53611006]), array([-0.48344191,  0.85100829,  0.98864863, -1.00216112]), array([-0.21359233,  0.50599696,  1.66123327, -2.39188783]), array([ 0.15217693, -0.06024306,  1.9016523 , -3.09648649]), array([ 0.5039099 , -0.65017195,  1.52673731, -2.64120207]), array([ 0.73727952, -1.07668054,  0.77046946, -1.58101022]), array([ 0.80425917, -1.27640594, -0.10625184, -0.41114311]), array([ 0.6872759 , -1.2126082 , -1.04557564,  1.05174119]), array([ 0.39754678, -0.8563643 , -1.81006318,  2.48667754]), array([-0.01185732, -0.24755915, -2.19294212,  3.44654931]), array([-0.43114516,  0.42859674, -1.88447116,  3.09135008]), array([-0.74171486,  0.95702773, -1.16423906,  2.11113022]), array([-0.87339499,  1.23296604, -0.14196197,  0.64827664]), array([-0.78882043,  1.1890023 ,  0.97580801, -1.09354698]), array([-0.49156949,  0.79159911,  1.96188169, -2.87095732]), array([-0.02901229,  0.07048711,  2.55455307, -4.14105045]), array([ 0.46878175, -0.73974322,  2.28646558, -3.69126304]), array([ 0.84836812, -1.34550368,  1.46030339, -2.32670048]), array([ 1.04146499, -1.67302558,  0.45484161, -0.96354868]), array([ 1.01959005, -1.71065195, -0.6683051 ,  0.58874627]), array([ 0.77131664, -1.4064329 , -1.79330507,  2.4847305 ]), array([ 0.32448303, -0.73403247, -2.6211858 ,  4.19896812]), array([-0.24708766,  0.23151627, -2.92197881,  5.09366673]), array([-0.75745051,  1.1142536 , -2.08053288,  3.5587749 ]), array([-1.07199492,  1.6737619 , -1.04157824,  2.05703864]), array([-1.16899425,  1.94707554,  0.07516339,  0.68875185]), array([-1.02961166,  1.90372891,  1.29928407, -1.13821505]), array([-0.66089905,  1.47871844,  2.35303356, -3.15432724]), array([-0.10419153,  0.62983588,  3.15068076, -5.26935217]), array([ 0.53813769, -0.50262214,  3.05321797, -5.56994472]), array([ 1.04625595, -1.45341391,  1.96144014, -3.86163733]), array([ 1.3150941 , -2.06503446,  0.72037304, -2.30445446]), array([ 1.33429379, -2.38595748, -0.52150458, -0.91006521]), array([ 1.10035355, -2.38469821, -1.78593065,  0.93846788]), array([ 0.63994612, -2.00075383, -2.75096768,  2.93304462]), array([ 0.02888805, -1.19819429, -3.30456239,  5.10310541]), array([-6.53225596e-01, -4.88829005e-03, -3.34906838e+00,  6.43878177e+00]), array([-1.21515313,  1.16230004, -2.12926364,  4.9672715 ]), array([-1.48962665,  1.98282688, -0.61421094,  3.2986766 ]), array([-1.46498354,  2.49485845,  0.83966338,  1.82467437]), array([-1.15984203,  2.68923587,  2.17011314,  0.11524992]), array([-0.61519013,  2.52306143,  3.18217054, -1.76374841]), array([ 0.06066113,  1.99307049,  3.43992967, -3.49725766]), array([ 0.71734497,  1.15045018,  3.06906837, -4.8339665 ]), array([ 1.26985253,  0.12131346,  2.37796986, -5.22839841]), array([ 1.62487098, -0.84160745,  1.08663136, -4.25629341]), array([ 1.68211267, -1.55975962, -0.55081022, -2.88533986]), array([ 1.39786759, -1.96967678, -2.27555753, -1.12661193]), array([ 0.78960005, -1.95474767, -3.69341286,  1.33457119]), array([-0.02457871, -1.40710439, -4.29278335,  4.09479151]), array([-0.86438212, -0.40874053, -3.97391179,  5.55195224]), array([-1.55097547,  0.62974404, -2.78374105,  4.53540381]), array([-1.97822008,  1.41515031, -1.49654911,  3.38121918]), array([-2.14462319,  1.98431428, -0.17305839,  2.34553026]), array([-2.04633749,  2.34800912,  1.16180305,  1.24115256]), array([-1.67133939,  2.43050903,  2.58601692, -0.50663537]), array([-1.02058333,  2.10425332,  3.862433  , -2.87243201]), array([-0.16328724,  1.23749971,  4.63046413, -5.85749953]), array([ 0.79196876, -0.17015832,  4.68075592, -7.55028124]), array([ 1.59655163, -1.48117095,  3.28134115, -5.37704639]), array([ 2.11993675, -2.38785253,  2.00110877, -3.86015269]), array([ 2.41700714, -3.06612897,  1.03016572, -2.97055488]), array([ 2.55523944,  2.70253256,  0.40016624, -2.17007981]), array([ 2.58737433,  2.35499109, -0.07080584, -1.2881046 ]), array([ 2.52375491,  2.19491922, -0.58419364, -0.29476708]), array([ 2.32789493,  2.28591219, -1.41377997,  1.21290515]), array([ 1.93980837,  2.68024819, -2.51741442,  2.72951169]), array([ 1.31223867, -2.91792407, -3.74867808,  4.18909175]), array([ 0.47060522, -1.87254865, -4.58066257,  6.46118814]), array([-0.50630491, -0.27254302, -5.05801232,  9.19566092]), array([-1.39194808,  1.38703708, -3.54485359,  6.80146733]), array([-1.93556296,  2.51107266, -1.96260442,  4.67092819]), array([-2.2049319 , -2.97725331, -0.80809319,  3.32696604]), array([-2.28164627, -2.43886232,  0.01290427,  2.04690053]), array([-2.20596173, -2.1436606 ,  0.76171223,  0.89586464]), array([-1.95721081, -2.10281575,  1.76564514, -0.47297196]), array([-1.47636336, -2.33882393,  3.07349302, -1.81550065]), array([-0.72813918, -2.79274674,  4.34656127, -2.6298105 ]), array([ 0.2027636 ,  2.91662558,  4.74874611, -3.08302617]), array([ 1.08148024,  2.26846167,  3.88499554, -3.33425178]), array([ 1.73203384,  1.62310823,  2.62545604, -3.0108994 ])]</t>
-  </si>
-  <si>
-    <t>['[2,1,0]', '[0,1,1]', '[0,0,0]', '[1,1,2]', '[1,2,0]', '[2,2,2]', '[1,0,2]', '[0,2,1]', '[1,1,1]', '[2,0,1]']</t>
-  </si>
-  <si>
-    <t>[6, 7, 9, 10, 11, 18, 19, 20, 21, 22, 23, 29, 30, 31, 32, 33, 34, 41, 42, 43, 44, 45, 46, 47, 54, 57, 58, 60, 68, 69, 72, 73, 74, 82, 85, 86, 87, 88, 98, 99, 100, 101, 102]</t>
-  </si>
-  <si>
-    <t>[0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 1, 0, 0, 0, 0, 0, 0, 0, 1, 2, 2, 2, 2, 2]</t>
-  </si>
-  <si>
-    <t>['[-0.03763371 -0.01533471  0.06554052 -0.01816017]', '[-0.00754409 -0.05458322  0.2277812  -0.36241836]', '[ 0.04879627 -0.15231473  0.32089719 -0.5887683 ]', '[ 0.11397169 -0.27767857  0.31375488 -0.63332862]', '[ 0.16759438 -0.39312519  0.2086893  -0.49480525]', '[ 0.1930193  -0.46685036  0.03906408 -0.22816919]', '[ 0.16956871 -0.44830261 -0.26820417  0.40739083]', '[ 0.09055011 -0.31127879 -0.50323119  0.93116007]', '[-0.03483507 -0.05969969 -0.71793241  1.5230623 ]', '[-0.16724813  0.23226042 -0.56936916  1.32372037]', '[-0.24997128  0.44471277 -0.23709198  0.7579718 ]', '[-0.25729563  0.52450869  0.16549558  0.02988042]', '[-0.17385533  0.42508154  0.65118359 -1.00143825]', '[-0.008281    0.14158157  0.9644314  -1.76410525]', '[ 0.19122701 -0.24238614  0.97513251 -1.97008608]', '[ 0.35981153 -0.60474891  0.66794073 -1.57347469]', '[ 0.44590609 -0.84884015  0.17627235 -0.83453479]', '[ 0.42796192 -0.93156217 -0.35071064  0.01149131]', '[ 0.30002245 -0.81654025 -0.90475407  1.11957906]', '[ 0.07954589 -0.49854112 -1.25541626  1.99672911]', '[-0.17883542 -0.05699426 -1.26166819  2.29611422]', '[-0.39690661  0.36642278 -0.86142478  1.82932209]', '[-0.50630532  0.64324762 -0.20980928  0.89547613]', '[-0.47759262  0.71585994  0.4906629  -0.17354122]', '[-0.30526712  0.54566943  1.20040785 -1.498047  ]', '[-0.01677696  0.14175363  1.61784543 -2.43361548]', '[ 0.30782059 -0.36677596  1.5416169  -2.49326066]', '[ 0.56870335 -0.80086594  1.01283646 -1.7630818 ]', '[ 0.69854201 -1.05357695  0.26683356 -0.74411152]', '[ 0.66232905 -1.06662312 -0.62170356  0.61382329]', '[ 0.45703968 -0.80967285 -1.40047279  1.93580715]', '[ 0.12133252 -0.31363982 -1.88550199  2.91343826]', '[-0.25796625  0.28431256 -1.80330187  2.8687948 ]', '[-0.56260653  0.76601931 -1.18084481  1.85137376]', '[-0.71466721  1.00690979 -0.3197434   0.5431738 ]', '[-0.67648952  0.95258561  0.69691776 -1.08579134]', '[-0.44219626  0.57468713  1.61254842 -2.66028476]', '[-0.05677644 -0.07255426  2.14047109 -3.62231807]', '[ 0.36267249 -0.7724087   1.94406004 -3.16833062]', '[ 0.68924274 -1.2902043   1.27418867 -1.96395878]', '[ 0.85994567 -1.55450536  0.41453787 -0.68273796]', '[ 0.84285157 -1.53999995 -0.58297497  0.82870771]', '[ 0.63128396 -1.21946336 -1.51213743  2.38584643]', '[ 0.25118832 -0.58884842 -2.23105742  3.84952368]', '[-0.21871715  0.24275335 -2.32375697  4.17315591]', '[-0.62188736  0.96729341 -1.62286904  2.9265575 ]', '[-0.8505054   1.39641472 -0.64382957  1.36694823]', '[-0.87626981  1.517873    0.3838726  -0.14872296]', '[-0.69242736  1.30900978  1.43487236 -1.95463439]', '[-0.31349453  0.73094971  2.3104291  -3.79808982]', '[ 0.19658939 -0.15264478  2.64185276 -4.73513999]', '[ 0.67389677 -1.01897018  2.01623275 -3.71550348]', '[ 0.97990131 -1.6133157   1.01834722 -2.2356677 ]', '[ 1.0762173  -1.92138948 -0.05766747 -0.85733635]', '[ 0.95257064 -1.93416676 -1.15746113  0.73757465]', '[ 0.61877456 -1.59608658 -2.13965102  2.67002624]', '[ 0.11434239 -0.85690914 -2.85436928  4.69695115]', '[-0.46921847  0.17493279 -2.80264532  5.23436922]', '[-0.93313733  1.08156325 -1.74208408  3.66896073]', '[-1.16276388  1.66525743 -0.54130972  2.18650428]', '[-1.14180406  1.93876593  0.73603802  0.55123035]', '[-0.87192505  1.857699    1.91975687 -1.38560672]', '[-0.39620654  1.37292503  2.77847009 -3.48324892]', '[ 0.21446978  0.4729183   3.23577407 -5.35977977]', '[ 0.82800329 -0.61510973  2.70722697 -5.09656235]', '[ 1.24731262 -1.4728879   1.44554729 -3.46280147]', '[ 1.40212652 -2.01696458  0.10209569 -2.00591897]', '[ 1.29105703 -2.27621459 -1.19548883 -0.57093522]', '[ 0.93020734 -2.2148907  -2.35913931  1.2083971 ]', '[ 0.37871959 -1.78513202 -3.0633687   3.09509602]', '[-0.2677959  -0.95962453 -3.33211141  5.09281902]', '[-0.91425122  0.16321556 -2.96591496  5.73429659]', '[-1.37249198  1.15010798 -1.54228298  4.02011445]', '[-1.52537412  1.78330233  0.01159691  2.34431296]', '[-1.37153119  2.0865292   1.50599722  0.65510107]', '[-0.93201383  2.0045282   2.82282567 -1.52594196]', '[-0.27890591  1.45882683  3.61262829 -3.94989164]', '[ 0.47728268  0.4445934   3.8377844  -5.96274431]', '[ 1.17749573 -0.72899003  2.97861512 -5.33216748]', '[ 1.63329513 -1.62600548  1.56831263 -3.68951725]', '[ 1.80638819 -2.23380973  0.16799092 -2.4226468 ]', '[ 1.70362452 -2.59329676 -1.18514359 -1.14424757]', '[ 1.33164356 -2.65686106 -2.51067584  0.5452172 ]', '[ 0.71321876 -2.34112288 -3.58126034  2.64954401]', '[-0.05002562 -1.58540956 -3.94062496  4.91308723]', '[-0.82258884 -0.43243416 -3.68747792  6.34768764]', '[-1.45304887  0.7603379  -2.46614363  5.22536654]', '[-1.78661818  1.62936183 -0.86810431  3.52906831]', '[-1.80184172  2.18964012  0.70961918  2.06830367]', '[-1.50783411  2.44019741  2.20783716  0.37972674]', '[-0.92909762  2.29735791  3.50229557 -1.86543662]', '[-0.15428028  1.67606642  4.11914029 -4.36684348]', '[ 0.67864377  0.56897959  4.12122221 -6.4928291 ]', '[ 1.42298791 -0.71864903  3.13708354 -5.90636029]', '[ 1.90010575 -1.73119862  1.63755954 -4.30182234]', '[ 2.08444034 -2.47560416  0.22769932 -3.1815075 ]', '[ 2.00344193 -3.00210268 -1.00462885 -2.06047659]', '[ 1.68431609  3.01237271 -2.18568832 -0.61672586]', '[ 1.12696871  3.02990777 -3.37517375  0.75481588]', '[ 0.35741032 -2.99130655 -4.20181338  1.79593597]', '[-0.4835481  -2.56479606 -4.02223662  2.37961804]', '[-1.1897366  -2.08579555 -2.94966461  2.27441206]', '[-1.64922665 -1.708417   -1.64084041  1.38840623]']</t>
-  </si>
-  <si>
-    <t>[0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50, 51, 52, 53, 54, 55, 56, 57, 58, 59, 60, 61, 62, 63, 64, 65, 66, 67, 68, 69, 70, 71, 72, 73, 74, 75, 76, 77, 78, 79, 80, 81, 82, 83, 84, 85, 86, 87, 88, 89, 90, 91, 92, 93, 94, 95, 96, 97, 98, 99, 100, 101, 102]</t>
-  </si>
-  <si>
-    <t>[array([-0.03763371, -0.01533471,  0.06554052, -0.01816017], dtype=float32), array([-0.00754409, -0.05458322,  0.2277812 , -0.36241836]), array([ 0.04879627, -0.15231473,  0.32089719, -0.5887683 ]), array([ 0.11397169, -0.27767857,  0.31375488, -0.63332862]), array([ 0.16759438, -0.39312519,  0.2086893 , -0.49480525]), array([ 0.1930193 , -0.46685036,  0.03906408, -0.22816919]), array([ 0.16956871, -0.44830261, -0.26820417,  0.40739083]), array([ 0.09055011, -0.31127879, -0.50323119,  0.93116007]), array([-0.03483507, -0.05969969, -0.71793241,  1.5230623 ]), array([-0.16724813,  0.23226042, -0.56936916,  1.32372037]), array([-0.24997128,  0.44471277, -0.23709198,  0.7579718 ]), array([-0.25729563,  0.52450869,  0.16549558,  0.02988042]), array([-0.17385533,  0.42508154,  0.65118359, -1.00143825]), array([-0.008281  ,  0.14158157,  0.9644314 , -1.76410525]), array([ 0.19122701, -0.24238614,  0.97513251, -1.97008608]), array([ 0.35981153, -0.60474891,  0.66794073, -1.57347469]), array([ 0.44590609, -0.84884015,  0.17627235, -0.83453479]), array([ 0.42796192, -0.93156217, -0.35071064,  0.01149131]), array([ 0.30002245, -0.81654025, -0.90475407,  1.11957906]), array([ 0.07954589, -0.49854112, -1.25541626,  1.99672911]), array([-0.17883542, -0.05699426, -1.26166819,  2.29611422]), array([-0.39690661,  0.36642278, -0.86142478,  1.82932209]), array([-0.50630532,  0.64324762, -0.20980928,  0.89547613]), array([-0.47759262,  0.71585994,  0.4906629 , -0.17354122]), array([-0.30526712,  0.54566943,  1.20040785, -1.498047  ]), array([-0.01677696,  0.14175363,  1.61784543, -2.43361548]), array([ 0.30782059, -0.36677596,  1.5416169 , -2.49326066]), array([ 0.56870335, -0.80086594,  1.01283646, -1.7630818 ]), array([ 0.69854201, -1.05357695,  0.26683356, -0.74411152]), array([ 0.66232905, -1.06662312, -0.62170356,  0.61382329]), array([ 0.45703968, -0.80967285, -1.40047279,  1.93580715]), array([ 0.12133252, -0.31363982, -1.88550199,  2.91343826]), array([-0.25796625,  0.28431256, -1.80330187,  2.8687948 ]), array([-0.56260653,  0.76601931, -1.18084481,  1.85137376]), array([-0.71466721,  1.00690979, -0.3197434 ,  0.5431738 ]), array([-0.67648952,  0.95258561,  0.69691776, -1.08579134]), array([-0.44219626,  0.57468713,  1.61254842, -2.66028476]), array([-0.05677644, -0.07255426,  2.14047109, -3.62231807]), array([ 0.36267249, -0.7724087 ,  1.94406004, -3.16833062]), array([ 0.68924274, -1.2902043 ,  1.27418867, -1.96395878]), array([ 0.85994567, -1.55450536,  0.41453787, -0.68273796]), array([ 0.84285157, -1.53999995, -0.58297497,  0.82870771]), array([ 0.63128396, -1.21946336, -1.51213743,  2.38584643]), array([ 0.25118832, -0.58884842, -2.23105742,  3.84952368]), array([-0.21871715,  0.24275335, -2.32375697,  4.17315591]), array([-0.62188736,  0.96729341, -1.62286904,  2.9265575 ]), array([-0.8505054 ,  1.39641472, -0.64382957,  1.36694823]), array([-0.87626981,  1.517873  ,  0.3838726 , -0.14872296]), array([-0.69242736,  1.30900978,  1.43487236, -1.95463439]), array([-0.31349453,  0.73094971,  2.3104291 , -3.79808982]), array([ 0.19658939, -0.15264478,  2.64185276, -4.73513999]), array([ 0.67389677, -1.01897018,  2.01623275, -3.71550348]), array([ 0.97990131, -1.6133157 ,  1.01834722, -2.2356677 ]), array([ 1.0762173 , -1.92138948, -0.05766747, -0.85733635]), array([ 0.95257064, -1.93416676, -1.15746113,  0.73757465]), array([ 0.61877456, -1.59608658, -2.13965102,  2.67002624]), array([ 0.11434239, -0.85690914, -2.85436928,  4.69695115]), array([-0.46921847,  0.17493279, -2.80264532,  5.23436922]), array([-0.93313733,  1.08156325, -1.74208408,  3.66896073]), array([-1.16276388,  1.66525743, -0.54130972,  2.18650428]), array([-1.14180406,  1.93876593,  0.73603802,  0.55123035]), array([-0.87192505,  1.857699  ,  1.91975687, -1.38560672]), array([-0.39620654,  1.37292503,  2.77847009, -3.48324892]), array([ 0.21446978,  0.4729183 ,  3.23577407, -5.35977977]), array([ 0.82800329, -0.61510973,  2.70722697, -5.09656235]), array([ 1.24731262, -1.4728879 ,  1.44554729, -3.46280147]), array([ 1.40212652, -2.01696458,  0.10209569, -2.00591897]), array([ 1.29105703, -2.27621459, -1.19548883, -0.57093522]), array([ 0.93020734, -2.2148907 , -2.35913931,  1.2083971 ]), array([ 0.37871959, -1.78513202, -3.0633687 ,  3.09509602]), array([-0.2677959 , -0.95962453, -3.33211141,  5.09281902]), array([-0.91425122,  0.16321556, -2.96591496,  5.73429659]), array([-1.37249198,  1.15010798, -1.54228298,  4.02011445]), array([-1.52537412,  1.78330233,  0.01159691,  2.34431296]), array([-1.37153119,  2.0865292 ,  1.50599722,  0.65510107]), array([-0.93201383,  2.0045282 ,  2.82282567, -1.52594196]), array([-0.27890591,  1.45882683,  3.61262829, -3.94989164]), array([ 0.47728268,  0.4445934 ,  3.8377844 , -5.96274431]), array([ 1.17749573, -0.72899003,  2.97861512, -5.33216748]), array([ 1.63329513, -1.62600548,  1.56831263, -3.68951725]), array([ 1.80638819, -2.23380973,  0.16799092, -2.4226468 ]), array([ 1.70362452, -2.59329676, -1.18514359, -1.14424757]), array([ 1.33164356, -2.65686106, -2.51067584,  0.5452172 ]), array([ 0.71321876, -2.34112288, -3.58126034,  2.64954401]), array([-0.05002562, -1.58540956, -3.94062496,  4.91308723]), array([-0.82258884, -0.43243416, -3.68747792,  6.34768764]), array([-1.45304887,  0.7603379 , -2.46614363,  5.22536654]), array([-1.78661818,  1.62936183, -0.86810431,  3.52906831]), array([-1.80184172,  2.18964012,  0.70961918,  2.06830367]), array([-1.50783411,  2.44019741,  2.20783716,  0.37972674]), array([-0.92909762,  2.29735791,  3.50229557, -1.86543662]), array([-0.15428028,  1.67606642,  4.11914029, -4.36684348]), array([ 0.67864377,  0.56897959,  4.12122221, -6.4928291 ]), array([ 1.42298791, -0.71864903,  3.13708354, -5.90636029]), array([ 1.90010575, -1.73119862,  1.63755954, -4.30182234]), array([ 2.08444034, -2.47560416,  0.22769932, -3.1815075 ]), array([ 2.00344193, -3.00210268, -1.00462885, -2.06047659]), array([ 1.68431609,  3.01237271, -2.18568832, -0.61672586]), array([ 1.12696871,  3.02990777, -3.37517375,  0.75481588]), array([ 0.35741032, -2.99130655, -4.20181338,  1.79593597]), array([-0.4835481 , -2.56479606, -4.02223662,  2.37961804]), array([-1.1897366 , -2.08579555, -2.94966461,  2.27441206]), array([-1.64922665, -1.708417  , -1.64084041,  1.38840623])]</t>
-  </si>
-  <si>
-    <t>['[0,1,1]', '[0,0,0]', '[1,1,1]', '[2,0,1]', '[0,2,1]', '[1,2,0]', '[1,0,2]', '[1,1,2]', '[2,1,0]', '[2,2,2]']</t>
-  </si>
-  <si>
-    <t>[6, 7, 8, 9, 10, 11, 18, 19, 20, 21, 22, 23, 29, 30, 31, 32, 33, 34, 41, 42, 43, 44, 45, 46, 47, 54, 55, 56, 57, 58, 59, 60, 67, 68, 69, 70, 71, 72, 73, 81, 82, 83, 84, 85, 86, 87, 96, 97, 98, 99, 100, 101, 102, 111, 112, 113, 114, 115, 116, 117, 118, 137, 138]</t>
-  </si>
-  <si>
-    <t>[0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 1, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 1, 2, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 1, 2, 2]</t>
-  </si>
-  <si>
-    <t>['[-0.03763371 -0.01533471  0.06554052 -0.01816017]', '[-0.00754409 -0.05458322  0.2277812  -0.36241836]', '[ 0.04879627 -0.15231473  0.32089719 -0.5887683 ]', '[ 0.11397169 -0.27767857  0.31375488 -0.63332862]', '[ 0.16759438 -0.39312519  0.2086893  -0.49480525]', '[ 0.1930193  -0.46685036  0.03906408 -0.22816919]', '[ 0.16956871 -0.44830261 -0.26820417  0.40739083]', '[ 0.09055011 -0.31127879 -0.50323119  0.93116007]', '[-0.02165415 -0.09380121 -0.58952709  1.1892161 ]', '[-0.13228272  0.13968862 -0.48657385  1.08703787]', '[-0.20542731  0.31962025 -0.22562708  0.67289162]', '[-0.21756752  0.39782756  0.10766541  0.09689063]', '[-0.15109606  0.32490126  0.54216963 -0.80657469]', '[-0.01068619  0.09081112  0.82714324 -1.47439182]', '[ 0.16212513 -0.23279107  0.85391345 -1.67375883]', '[ 0.3120332  -0.54339537  0.60708552 -1.36152952]', '[ 0.39322683 -0.75586146  0.18779451 -0.73014827]', '[ 0.38412465 -0.82793881 -0.27624305  0.01454459]', '[ 0.27552572 -0.72135137 -0.78884754  1.03160865]', '[ 0.08086773 -0.43032213 -1.11647003  1.81675029]', '[-0.14966877 -0.03109877 -1.12879696  2.06540623]', '[-0.3455444   0.34863759 -0.7784691   1.63534647]', '[-0.44544803  0.59424237 -0.19906427  0.77949316]', '[-0.4218337   0.6519398   0.43007126 -0.20572333]', '[-0.26769146  0.484052    1.08142007 -1.44055859]', '[-0.00742761  0.10113176  1.45927884 -2.28595201]', '[ 0.28490347 -0.37428385  1.38589424 -2.32532176]', '[ 0.5187101  -0.77937684  0.90230152 -1.64619583]', '[ 0.63240836 -1.01433747  0.21740989 -0.68198512]', '[ 0.59278756 -1.01958166 -0.60566507  0.62852481]', '[ 0.39752784 -0.7660208  -1.31595743  1.88179849]', '[ 0.08542661 -0.29020757 -1.73661998  2.76615566]', '[-0.26054486  0.27360101 -1.62803895  2.69265107]', '[-0.53183224  0.72525907 -1.02799868  1.73308445]', '[-0.65747495  0.94866122 -0.21116234  0.48419472]', '[-0.60316944  0.88713812  0.74646124 -1.09703619]', '[-0.3667148   0.51448679  1.5802398  -2.58584684]', '[ 2.25515542e-03 -1.04226788e-01  2.01052042e+00 -3.41515113e+00]', '[ 0.38981745 -0.75816996  1.76540261 -2.93947302]', '[ 0.67971886 -1.23563438  1.09061136 -1.79181237]', '[ 0.81522073 -1.47040276  0.25012952 -0.55613563]', '[ 0.76893557 -1.43299403 -0.70634091  0.93217091]', '[ 0.53890731 -1.09497955 -1.5685075   2.44803386]', '[ 0.15769536 -0.46498696 -2.17507038  3.75054866]', '[-0.28566374  0.31885175 -2.12308403  3.81427092]', '[-0.64333931  0.96714913 -1.38377582  2.55626676]', '[-0.82476188  1.32821982 -0.41497441  1.0541805 ]', '[-0.80769438  1.39053182  0.57925977 -0.43113385]', '[-0.58966747  1.12643161  1.57705339 -2.21920745]', '[-0.19115743  0.50615398  2.34648211 -3.90612928]', '[ 0.30339761 -0.35080814  2.44609663 -4.34908803]', '[ 0.72926902 -1.11787821  1.72849028 -3.18529002]', '[ 0.97784646 -1.61271142  0.7372731  -1.77273591]', '[ 1.02063975 -1.83229792 -0.30765192 -0.42827287]', '[ 0.8520877  -1.75909807 -1.35222299  1.17222519]', '[ 0.49438686 -1.35658722 -2.18080855  2.86380021]', '[ 1.00762334e-03 -6.20843848e-01 -2.67811907e+00  4.39175692e+00]', '[-0.52543841  0.29807699 -2.42518508  4.45563686]', '[-0.91358233  1.05045396 -1.38833549  2.96371659]', '[-1.07068508  1.48053778 -0.17760768  1.35120727]', '[-0.98698022  1.59293246  0.99771813 -0.2363293 ]', '[-0.67458429  1.35277557  2.08591422 -2.1902737 ]', '[-0.17257945  0.7121893   2.86826583 -4.16299452]', '[ 0.42654616 -0.22986762  2.95103072 -4.89035041]', '[ 0.93778312 -1.09635369  2.06289939 -3.60682875]', '[ 1.23512506 -1.66554553  0.89403237 -2.11536181]', '[ 1.2925874  -1.95282627 -0.31874559 -0.76398106]', '[ 1.10434513 -1.94410117 -1.53992148  0.87663865]', '[ 0.69181453 -1.5878337  -2.53506175  2.72222862]', '[ 0.1141862  -0.84811196 -3.17077399  4.62247333]', '[-0.52819058  0.17080839 -3.07026003  5.16081708]', '[-1.04130142  1.05893    -1.96969821  3.56491538]', '[-1.30452454  1.59874429 -0.65598023  1.87444291]', '[-1.30385453  1.81885452  0.65610727  0.32547074]', '[-1.0405206   1.6957045   1.9492216  -1.60077881]', '[-0.53981694  1.15624497  3.01179277 -3.83696118]', '[ 0.1372115   0.17699716  3.62003771 -5.68231063]', '[ 0.81714379 -0.90901082  2.9941466  -4.77727736]', '[ 1.30077933 -1.68444311  1.81783839 -3.01937746]', '[ 1.54044333 -2.14395201  0.57410527 -1.62162767]', '[ 1.53015478 -2.34022436 -0.67386049 -0.3349864 ]', '[ 1.26794035 -2.24754766 -1.92783573  1.30056457]', '[ 0.77398019 -1.79920792 -2.95822207  3.24300749]', '[ 0.10912329 -0.93053956 -3.62675865  5.42116516]', '[-0.62545765  0.26611029 -3.49608951  6.01988262]', '[-1.20465197  1.28709304 -2.21592237  4.06698629]', '[-1.50797598  1.91807846 -0.82066615  2.31676317]', '[-1.53477864  2.2293726   0.54577611  0.80013611]', '[-1.2877879   2.20842304  1.90129391 -1.04971139]', '[-0.78963194  1.78691254  3.02687444 -3.23448346]', '[-0.10030915  0.88843882  3.80956796 -5.74461357]', '[ 0.6800303  -0.39674343  3.7435005  -6.50465385]', '[ 1.30715153 -1.50997221  2.45867409 -4.5409428 ]', '[ 1.66295011 -2.25180565  1.10659453 -2.9676307 ]', '[ 1.75378095 -2.71564871 -0.18565107 -1.68161197]', '[ 1.58719261 -2.90109289 -1.4723594  -0.1570594 ]', '[ 1.16856593 -2.77159888 -2.68682871  1.47067408]', '[ 0.53803373 -2.30375458 -3.51328481  3.23512206]', '[-0.18689025 -1.47171807 -3.64264476  5.06600075]', '[-0.89191829 -0.32040404 -3.30370334  6.16212656]', '[-1.43738497  0.81560486 -2.01541372  4.90941679]', '[-1.67729527  1.62358431 -0.37474765  3.2087413 ]', '[-1.58743078  2.10406514  1.26274863  1.56657122]', '[-1.17686802  2.20715638  2.7876195  -0.59672218]', '[-0.50730587  1.84271979  3.79246475 -3.08863666]', '[ 0.29147201  0.97119874  4.10085764 -5.54206842]', '[ 1.08414599 -0.25378944  3.63499511 -6.19286979]', '[ 1.67640522 -1.3365948   2.23652426 -4.56246495]', '[ 1.9814544  -2.11437006  0.82705999 -3.29460719]', '[ 2.01269692 -2.66619774 -0.49620149 -2.21383358]', '[ 1.78409404 -2.96809523 -1.77965027 -0.77249303]', '[ 1.30149129 -2.96441766 -3.03533588  0.82631458]', '[ 0.58890924 -2.63390153 -3.98354262  2.48567983]', '[-0.22631846 -1.97283376 -4.00376081  4.08524298]', '[-0.96558336 -1.03796571 -3.33240076  5.11323848]', '[-1.53922556 -0.01454682 -2.33370838  4.88332683]', '[-1.87187423  0.84815259 -0.95576384  3.69536389]', '[-1.91165507  1.46323511  0.58512333  2.43051425]', '[-1.62770799  1.79176562  2.26273466  0.74152557]', '[-1.00988905  1.68362849  3.84148013 -1.95309403]', '[-0.13585858  0.9738579   4.77819076 -5.12142974]', '[ 0.83565798 -0.2398631   4.68927476 -6.34985101]', '[ 1.65142165 -1.3228547   3.41257782 -4.35839551]', '[ 2.21520709 -2.04128122  2.27602432 -2.99811286]', '[ 2.58160112 -2.57359675  1.43950076 -2.41030312]', '[ 2.81131759 -3.02440586  0.91146434 -2.12231163]', '[ 2.96620913  2.85763281  0.68571764 -1.891342  ]', '[ 3.10182854  2.50290167  0.70700839 -1.65836682]', '[-3.02153244  2.19152507  0.92343942 -1.47303363]', '[-2.79824568  1.90164466  1.35072441 -1.47546205]', '[-2.46165889  1.57209735  2.07478658 -1.92730454]', '[-1.94100647  1.07275137  3.20807492 -3.25194534]', '[-1.15137198  0.20163219  4.68919384 -5.4342263 ]', '[-0.12448895 -0.91571373  5.34175489 -5.06561134]', '[ 0.89800185 -1.62986529  4.68648726 -1.92490485]', '[ 1.68031081 -1.7067368   3.02854483  0.99907813]', '[ 2.08617254 -1.28248348  1.05430359  3.06795616]', '[ 2.1281456  -0.53224006 -0.55713409  4.35210695]', '[ 1.89410325  0.43386325 -1.71041519  5.23147326]']</t>
-  </si>
-  <si>
-    <t>[0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50, 51, 52, 53, 54, 55, 56, 57, 58, 59, 60, 61, 62, 63, 64, 65, 66, 67, 68, 69, 70, 71, 72, 73, 74, 75, 76, 77, 78, 79, 80, 81, 82, 83, 84, 85, 86, 87, 88, 89, 90, 91, 92, 93, 94, 95, 96, 97, 98, 99, 100, 101, 102, 103, 104, 105, 106, 107, 108, 109, 110, 111, 112, 113, 114, 115, 116, 117, 118, 119, 120, 121, 122, 123, 124, 125, 126, 127, 128, 129, 130, 131, 132, 133, 134, 135, 136, 137, 138]</t>
-  </si>
-  <si>
-    <t>[array([-0.03763371, -0.01533471,  0.06554052, -0.01816017], dtype=float32), array([-0.00754409, -0.05458322,  0.2277812 , -0.36241836]), array([ 0.04879627, -0.15231473,  0.32089719, -0.5887683 ]), array([ 0.11397169, -0.27767857,  0.31375488, -0.63332862]), array([ 0.16759438, -0.39312519,  0.2086893 , -0.49480525]), array([ 0.1930193 , -0.46685036,  0.03906408, -0.22816919]), array([ 0.16956871, -0.44830261, -0.26820417,  0.40739083]), array([ 0.09055011, -0.31127879, -0.50323119,  0.93116007]), array([-0.02165415, -0.09380121, -0.58952709,  1.1892161 ]), array([-0.13228272,  0.13968862, -0.48657385,  1.08703787]), array([-0.20542731,  0.31962025, -0.22562708,  0.67289162]), array([-0.21756752,  0.39782756,  0.10766541,  0.09689063]), array([-0.15109606,  0.32490126,  0.54216963, -0.80657469]), array([-0.01068619,  0.09081112,  0.82714324, -1.47439182]), array([ 0.16212513, -0.23279107,  0.85391345, -1.67375883]), array([ 0.3120332 , -0.54339537,  0.60708552, -1.36152952]), array([ 0.39322683, -0.75586146,  0.18779451, -0.73014827]), array([ 0.38412465, -0.82793881, -0.27624305,  0.01454459]), array([ 0.27552572, -0.72135137, -0.78884754,  1.03160865]), array([ 0.08086773, -0.43032213, -1.11647003,  1.81675029]), array([-0.14966877, -0.03109877, -1.12879696,  2.06540623]), array([-0.3455444 ,  0.34863759, -0.7784691 ,  1.63534647]), array([-0.44544803,  0.59424237, -0.19906427,  0.77949316]), array([-0.4218337 ,  0.6519398 ,  0.43007126, -0.20572333]), array([-0.26769146,  0.484052  ,  1.08142007, -1.44055859]), array([-0.00742761,  0.10113176,  1.45927884, -2.28595201]), array([ 0.28490347, -0.37428385,  1.38589424, -2.32532176]), array([ 0.5187101 , -0.77937684,  0.90230152, -1.64619583]), array([ 0.63240836, -1.01433747,  0.21740989, -0.68198512]), array([ 0.59278756, -1.01958166, -0.60566507,  0.62852481]), array([ 0.39752784, -0.7660208 , -1.31595743,  1.88179849]), array([ 0.08542661, -0.29020757, -1.73661998,  2.76615566]), array([-0.26054486,  0.27360101, -1.62803895,  2.69265107]), array([-0.53183224,  0.72525907, -1.02799868,  1.73308445]), array([-0.65747495,  0.94866122, -0.21116234,  0.48419472]), array([-0.60316944,  0.88713812,  0.74646124, -1.09703619]), array([-0.3667148 ,  0.51448679,  1.5802398 , -2.58584684]), array([ 2.25515542e-03, -1.04226788e-01,  2.01052042e+00, -3.41515113e+00]), array([ 0.38981745, -0.75816996,  1.76540261, -2.93947302]), array([ 0.67971886, -1.23563438,  1.09061136, -1.79181237]), array([ 0.81522073, -1.47040276,  0.25012952, -0.55613563]), array([ 0.76893557, -1.43299403, -0.70634091,  0.93217091]), array([ 0.53890731, -1.09497955, -1.5685075 ,  2.44803386]), array([ 0.15769536, -0.46498696, -2.17507038,  3.75054866]), array([-0.28566374,  0.31885175, -2.12308403,  3.81427092]), array([-0.64333931,  0.96714913, -1.38377582,  2.55626676]), array([-0.82476188,  1.32821982, -0.41497441,  1.0541805 ]), array([-0.80769438,  1.39053182,  0.57925977, -0.43113385]), array([-0.58966747,  1.12643161,  1.57705339, -2.21920745]), array([-0.19115743,  0.50615398,  2.34648211, -3.90612928]), array([ 0.30339761, -0.35080814,  2.44609663, -4.34908803]), array([ 0.72926902, -1.11787821,  1.72849028, -3.18529002]), array([ 0.97784646, -1.61271142,  0.7372731 , -1.77273591]), array([ 1.02063975, -1.83229792, -0.30765192, -0.42827287]), array([ 0.8520877 , -1.75909807, -1.35222299,  1.17222519]), array([ 0.49438686, -1.35658722, -2.18080855,  2.86380021]), array([ 1.00762334e-03, -6.20843848e-01, -2.67811907e+00,  4.39175692e+00]), array([-0.52543841,  0.29807699, -2.42518508,  4.45563686]), array([-0.91358233,  1.05045396, -1.38833549,  2.96371659]), array([-1.07068508,  1.48053778, -0.17760768,  1.35120727]), array([-0.98698022,  1.59293246,  0.99771813, -0.2363293 ]), array([-0.67458429,  1.35277557,  2.08591422, -2.1902737 ]), array([-0.17257945,  0.7121893 ,  2.86826583, -4.16299452]), array([ 0.42654616, -0.22986762,  2.95103072, -4.89035041]), array([ 0.93778312, -1.09635369,  2.06289939, -3.60682875]), array([ 1.23512506, -1.66554553,  0.89403237, -2.11536181]), array([ 1.2925874 , -1.95282627, -0.31874559, -0.76398106]), array([ 1.10434513, -1.94410117, -1.53992148,  0.87663865]), array([ 0.69181453, -1.5878337 , -2.53506175,  2.72222862]), array([ 0.1141862 , -0.84811196, -3.17077399,  4.62247333]), array([-0.52819058,  0.17080839, -3.07026003,  5.16081708]), array([-1.04130142,  1.05893   , -1.96969821,  3.56491538]), array([-1.30452454,  1.59874429, -0.65598023,  1.87444291]), array([-1.30385453,  1.81885452,  0.65610727,  0.32547074]), array([-1.0405206 ,  1.6957045 ,  1.9492216 , -1.60077881]), array([-0.53981694,  1.15624497,  3.01179277, -3.83696118]), array([ 0.1372115 ,  0.17699716,  3.62003771, -5.68231063]), array([ 0.81714379, -0.90901082,  2.9941466 , -4.77727736]), array([ 1.30077933, -1.68444311,  1.81783839, -3.01937746]), array([ 1.54044333, -2.14395201,  0.57410527, -1.62162767]), array([ 1.53015478, -2.34022436, -0.67386049, -0.3349864 ]), array([ 1.26794035, -2.24754766, -1.92783573,  1.30056457]), array([ 0.77398019, -1.79920792, -2.95822207,  3.24300749]), array([ 0.10912329, -0.93053956, -3.62675865,  5.42116516]), array([-0.62545765,  0.26611029, -3.49608951,  6.01988262]), array([-1.20465197,  1.28709304, -2.21592237,  4.06698629]), array([-1.50797598,  1.91807846, -0.82066615,  2.31676317]), array([-1.53477864,  2.2293726 ,  0.54577611,  0.80013611]), array([-1.2877879 ,  2.20842304,  1.90129391, -1.04971139]), array([-0.78963194,  1.78691254,  3.02687444, -3.23448346]), array([-0.10030915,  0.88843882,  3.80956796, -5.74461357]), array([ 0.6800303 , -0.39674343,  3.7435005 , -6.50465385]), array([ 1.30715153, -1.50997221,  2.45867409, -4.5409428 ]), array([ 1.66295011, -2.25180565,  1.10659453, -2.9676307 ]), array([ 1.75378095, -2.71564871, -0.18565107, -1.68161197]), array([ 1.58719261, -2.90109289, -1.4723594 , -0.1570594 ]), array([ 1.16856593, -2.77159888, -2.68682871,  1.47067408]), array([ 0.53803373, -2.30375458, -3.51328481,  3.23512206]), array([-0.18689025, -1.47171807, -3.64264476,  5.06600075]), array([-0.89191829, -0.32040404, -3.30370334,  6.16212656]), array([-1.43738497,  0.81560486, -2.01541372,  4.90941679]), array([-1.67729527,  1.62358431, -0.37474765,  3.2087413 ]), array([-1.58743078,  2.10406514,  1.26274863,  1.56657122]), array([-1.17686802,  2.20715638,  2.7876195 , -0.59672218]), array([-0.50730587,  1.84271979,  3.79246475, -3.08863666]), array([ 0.29147201,  0.97119874,  4.10085764, -5.54206842]), array([ 1.08414599, -0.25378944,  3.63499511, -6.19286979]), array([ 1.67640522, -1.3365948 ,  2.23652426, -4.56246495]), array([ 1.9814544 , -2.11437006,  0.82705999, -3.29460719]), array([ 2.01269692, -2.66619774, -0.49620149, -2.21383358]), array([ 1.78409404, -2.96809523, -1.77965027, -0.77249303]), array([ 1.30149129, -2.96441766, -3.03533588,  0.82631458]), array([ 0.58890924, -2.63390153, -3.98354262,  2.48567983]), array([-0.22631846, -1.97283376, -4.00376081,  4.08524298]), array([-0.96558336, -1.03796571, -3.33240076,  5.11323848]), array([-1.53922556, -0.01454682, -2.33370838,  4.88332683]), array([-1.87187423,  0.84815259, -0.95576384,  3.69536389]), array([-1.91165507,  1.46323511,  0.58512333,  2.43051425]), array([-1.62770799,  1.79176562,  2.26273466,  0.74152557]), array([-1.00988905,  1.68362849,  3.84148013, -1.95309403]), array([-0.13585858,  0.9738579 ,  4.77819076, -5.12142974]), array([ 0.83565798, -0.2398631 ,  4.68927476, -6.34985101]), array([ 1.65142165, -1.3228547 ,  3.41257782, -4.35839551]), array([ 2.21520709, -2.04128122,  2.27602432, -2.99811286]), array([ 2.58160112, -2.57359675,  1.43950076, -2.41030312]), array([ 2.81131759, -3.02440586,  0.91146434, -2.12231163]), array([ 2.96620913,  2.85763281,  0.68571764, -1.891342  ]), array([ 3.10182854,  2.50290167,  0.70700839, -1.65836682]), array([-3.02153244,  2.19152507,  0.92343942, -1.47303363]), array([-2.79824568,  1.90164466,  1.35072441, -1.47546205]), array([-2.46165889,  1.57209735,  2.07478658, -1.92730454]), array([-1.94100647,  1.07275137,  3.20807492, -3.25194534]), array([-1.15137198,  0.20163219,  4.68919384, -5.4342263 ]), array([-0.12448895, -0.91571373,  5.34175489, -5.06561134]), array([ 0.89800185, -1.62986529,  4.68648726, -1.92490485]), array([ 1.68031081, -1.7067368 ,  3.02854483,  0.99907813]), array([ 2.08617254, -1.28248348,  1.05430359,  3.06795616]), array([ 2.1281456 , -0.53224006, -0.55713409,  4.35210695]), array([ 1.89410325,  0.43386325, -1.71041519,  5.23147326])]</t>
-  </si>
-  <si>
-    <t>['[0,0,0]', '[1,1,2]', '[0,2,1]', '[2,1,0]', '[0,1,1]', '[1,1,1]', '[2,2,2]', '[1,2,0]', '[2,0,1]', '[1,0,2]']</t>
-  </si>
-  <si>
-    <t>[0,2,1]</t>
-  </si>
-  <si>
-    <t>[6, 34, 35, 48, 49, 62]</t>
-  </si>
-  <si>
-    <t>[0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 1, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 1, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 1, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2]</t>
-  </si>
-  <si>
-    <t>['[-0.03763371 -0.01533471  0.06554052 -0.01816017]', '[-0.00754409 -0.05458322  0.2277812  -0.36241836]', '[ 0.04879627 -0.15231473  0.32089719 -0.5887683 ]', '[ 0.11397169 -0.27767857  0.31375488 -0.63332862]', '[ 0.16759438 -0.39312519  0.2086893  -0.49480525]', '[ 0.1930193  -0.46685036  0.03906408 -0.22816919]', '[ 0.16956871 -0.44830261 -0.26820417  0.40739083]', '[ 0.07764819 -0.2777752  -0.62973474  1.26105599]', '[-0.06966349  0.03261704 -0.80302667  1.76452698]', '[-0.22465905  0.39058523 -0.70217906  1.72562277]', '[-0.33473527  0.69134317 -0.37152277  1.22661262]', '[-0.3665604   0.86641223  0.05855316  0.50502011]', '[-0.2902422   0.83034492  0.68874955 -0.85560583]', '[-0.10067244  0.53350339  1.17222386 -2.06518635]', '[ 0.15834837  0.03861766  1.35020622 -2.75501467]', '[ 0.4067969  -0.50420448  1.06115475 -2.52952059]', '[ 0.56001777 -0.93015548  0.43912923 -1.67046011]', '[ 0.57684927 -1.1602767  -0.26889077 -0.61879139]', '[ 0.43815341 -1.12120884 -1.08950026  1.00133178]', '[ 0.15556883 -0.76623271 -1.6914747   2.50835845]', '[-0.21367349 -0.15336851 -1.91436095  3.46094303]', '[-0.56562576  0.52965607 -1.50364495  3.17033497]', '[-0.78506524  1.06113145 -0.65170231  2.08510542]', '[-0.81974624  1.35479505  0.30379744  0.84259963]', '[-0.65145106  1.34335605  1.34587039 -0.95988568]', '[-0.29856385  0.97014979  2.13223916 -2.75416186]', '[ 0.17475072  0.26993715  2.50281365 -4.07576894]', '[ 0.64662107 -0.54619651  2.08107881 -3.81260201]', '[ 0.96851549 -1.18658407  1.09123658 -2.53710897]', '[ 1.07493688 -1.55948432 -0.03211188 -1.19515589]', '[ 0.94189396 -1.61393901 -1.27311138  0.66271178]', '[ 0.58014371 -1.2845204  -2.29983374  2.65488467]', '[ 0.04378738 -0.55352356 -2.98440023  4.55503349]', '[-0.55630483  0.42239481 -2.83426284  4.80991392]', '[-1.01824872  1.21927104 -1.7241359   3.08509956]', '[-1.23793145  1.66688577 -0.4665406   1.42692631]', '[-1.21301205  1.820428    0.71028108  0.10147076]', '[-0.94470344  1.65139982  1.94285309 -1.83058136]', '[-0.45165306  1.06913829  2.94197727 -4.01997875]', '[ 0.20265191  0.0727603   3.44927862 -5.63110578]', '[ 0.83812351 -0.98106875  2.74099813 -4.56619269]', '[ 1.27077046 -1.72016525  1.56372263 -2.86810438]', '[ 1.4597383  -2.1507919   0.32169822 -1.47173161]', '[ 1.39328765 -2.29117741 -0.97658599  0.07822893]', '[ 1.06989096 -2.08718186 -2.22449971  2.00663144]', '[ 0.52236784 -1.46438794 -3.20191077  4.28710752]', '[-0.19081657 -0.36482212 -3.82173024  6.50214143]', '[-0.90798411  0.90556884 -3.12008527  5.68375696]', '[-1.3898581   1.81988264 -1.69611729  3.54767743]', '[-1.58955987  2.36154811 -0.30919107  1.91809333]', '[-1.52349933  2.6123691   0.96101826  0.5790714 ]', '[-1.19873432  2.54491459  2.25731508 -1.280937  ]', '[-0.64218806  2.08542571  3.22847051 -3.36103865]', '[ 0.05830557  1.18158409  3.71833731 -5.6931722 ]', '[ 0.81293998 -0.12909372  3.62656527 -6.91427975]', '[ 1.40809581 -1.35314302  2.21240104 -5.1338422 ]', '[ 1.69345826 -2.21066645  0.65341741 -3.52429511]', '[ 1.67824092 -2.77724949 -0.77488816 -2.14483717]', '[ 1.38958215 -3.04681793 -2.08680692 -0.5550934 ]', '[ 0.84895845 -2.98800584 -3.26541031  1.10647519]', '[ 0.12441076 -2.62186002 -3.82916437  2.50666858]', '[-0.61248442 -2.01035227 -3.39868979  3.52062283]', '[-1.1934481  -1.28393268 -2.37484053  3.61077144]', '[-1.56788939 -0.58290237 -1.36628026  3.32854045]', '[-1.73747137  0.0311827  -0.3167569   2.78960276]', '[-1.68479174  0.52168866  0.88167515  2.05913589]', '[-1.34456341  0.75415913  2.53576843  0.16050148]', '[-0.67919187  0.54568774  4.03763673 -2.25494735]', '[ 0.20840851 -0.07875288  4.61295619 -3.58625162]', '[ 1.06737632 -0.69336852  3.80322888 -2.27730055]', '[ 1.6955749  -0.96774515  2.46135418 -0.55744704]', '[ 2.06086781 -0.97096756  1.23248152  0.3959363 ]', '[ 2.19358694 -0.81835083  0.12449486  1.07256311]', '[ 2.10342847 -0.51564071 -1.03431083  1.98449278]', '[ 1.77053805e+00 -2.35126596e-03 -2.31994873e+00  3.18975726e+00]', '[ 1.17397064  0.74304079 -3.60833445  4.07954913]', '[ 0.35727908  1.51099122 -4.44462756  3.28567603]', '[-0.53675978  1.95439178 -4.27500555  0.97994995]', '[-1.26061945  1.87436657 -2.78124631 -1.76559293]', '[-1.60369524  1.27778876 -0.62189875 -4.10007353]', '[-1.50499699  0.21357524  1.49084229 -6.40388612]', '[-1.09936672 -1.14530966  2.36129135 -6.84146425]', '[-0.58886524 -2.47598411  2.76726437 -6.55112487]', '[ 0.0093572   2.45275794  3.19147338 -7.22278373]', '[ 0.69904547  0.80436561  3.75014686 -9.45552219]', '[ 1.37564088 -1.07906433  2.51632034 -8.48332981]', '[ 1.61091799 -2.49690773 -0.08548142 -5.90785626]', '[ 1.42910416  2.7665055  -1.45449198 -4.48233305]', '[ 1.11548888  1.90267728 -1.52770984 -4.41609308]', '[ 0.87280636  0.88731498 -0.82626923 -5.9418341 ]', '[ 0.72747456 -0.41385031 -1.062419   -6.3891903 ]', '[ 0.27722809 -1.37255202 -3.4713141  -2.93451198]', '[-0.57107798 -1.57533452 -4.6505434   0.62674746]', '[-1.46232026 -1.25586419 -4.08801042  2.24225898]', '[-2.1820141  -0.78101121 -3.12269413  2.34700042]']</t>
-  </si>
-  <si>
-    <t>[0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50, 51, 52, 53, 54, 55, 56, 57, 58, 59, 60, 61, 62, 63, 64, 65, 66, 67, 68, 69, 70, 71, 72, 73, 74, 75, 76, 77, 78, 79, 80, 81, 82, 83, 84, 85, 86, 87, 88, 89, 90, 91, 92, 93, 94]</t>
-  </si>
-  <si>
-    <t>[array([-0.03763371, -0.01533471,  0.06554052, -0.01816017], dtype=float32), array([-0.00754409, -0.05458322,  0.2277812 , -0.36241836]), array([ 0.04879627, -0.15231473,  0.32089719, -0.5887683 ]), array([ 0.11397169, -0.27767857,  0.31375488, -0.63332862]), array([ 0.16759438, -0.39312519,  0.2086893 , -0.49480525]), array([ 0.1930193 , -0.46685036,  0.03906408, -0.22816919]), array([ 0.16956871, -0.44830261, -0.26820417,  0.40739083]), array([ 0.07764819, -0.2777752 , -0.62973474,  1.26105599]), array([-0.06966349,  0.03261704, -0.80302667,  1.76452698]), array([-0.22465905,  0.39058523, -0.70217906,  1.72562277]), array([-0.33473527,  0.69134317, -0.37152277,  1.22661262]), array([-0.3665604 ,  0.86641223,  0.05855316,  0.50502011]), array([-0.2902422 ,  0.83034492,  0.68874955, -0.85560583]), array([-0.10067244,  0.53350339,  1.17222386, -2.06518635]), array([ 0.15834837,  0.03861766,  1.35020622, -2.75501467]), array([ 0.4067969 , -0.50420448,  1.06115475, -2.52952059]), array([ 0.56001777, -0.93015548,  0.43912923, -1.67046011]), array([ 0.57684927, -1.1602767 , -0.26889077, -0.61879139]), array([ 0.43815341, -1.12120884, -1.08950026,  1.00133178]), array([ 0.15556883, -0.76623271, -1.6914747 ,  2.50835845]), array([-0.21367349, -0.15336851, -1.91436095,  3.46094303]), array([-0.56562576,  0.52965607, -1.50364495,  3.17033497]), array([-0.78506524,  1.06113145, -0.65170231,  2.08510542]), array([-0.81974624,  1.35479505,  0.30379744,  0.84259963]), array([-0.65145106,  1.34335605,  1.34587039, -0.95988568]), array([-0.29856385,  0.97014979,  2.13223916, -2.75416186]), array([ 0.17475072,  0.26993715,  2.50281365, -4.07576894]), array([ 0.64662107, -0.54619651,  2.08107881, -3.81260201]), array([ 0.96851549, -1.18658407,  1.09123658, -2.53710897]), array([ 1.07493688, -1.55948432, -0.03211188, -1.19515589]), array([ 0.94189396, -1.61393901, -1.27311138,  0.66271178]), array([ 0.58014371, -1.2845204 , -2.29983374,  2.65488467]), array([ 0.04378738, -0.55352356, -2.98440023,  4.55503349]), array([-0.55630483,  0.42239481, -2.83426284,  4.80991392]), array([-1.01824872,  1.21927104, -1.7241359 ,  3.08509956]), array([-1.23793145,  1.66688577, -0.4665406 ,  1.42692631]), array([-1.21301205,  1.820428  ,  0.71028108,  0.10147076]), array([-0.94470344,  1.65139982,  1.94285309, -1.83058136]), array([-0.45165306,  1.06913829,  2.94197727, -4.01997875]), array([ 0.20265191,  0.0727603 ,  3.44927862, -5.63110578]), array([ 0.83812351, -0.98106875,  2.74099813, -4.56619269]), array([ 1.27077046, -1.72016525,  1.56372263, -2.86810438]), array([ 1.4597383 , -2.1507919 ,  0.32169822, -1.47173161]), array([ 1.39328765, -2.29117741, -0.97658599,  0.07822893]), array([ 1.06989096, -2.08718186, -2.22449971,  2.00663144]), array([ 0.52236784, -1.46438794, -3.20191077,  4.28710752]), array([-0.19081657, -0.36482212, -3.82173024,  6.50214143]), array([-0.90798411,  0.90556884, -3.12008527,  5.68375696]), array([-1.3898581 ,  1.81988264, -1.69611729,  3.54767743]), array([-1.58955987,  2.36154811, -0.30919107,  1.91809333]), array([-1.52349933,  2.6123691 ,  0.96101826,  0.5790714 ]), array([-1.19873432,  2.54491459,  2.25731508, -1.280937  ]), array([-0.64218806,  2.08542571,  3.22847051, -3.36103865]), array([ 0.05830557,  1.18158409,  3.71833731, -5.6931722 ]), array([ 0.81293998, -0.12909372,  3.62656527, -6.91427975]), array([ 1.40809581, -1.35314302,  2.21240104, -5.1338422 ]), array([ 1.69345826, -2.21066645,  0.65341741, -3.52429511]), array([ 1.67824092, -2.77724949, -0.77488816, -2.14483717]), array([ 1.38958215, -3.04681793, -2.08680692, -0.5550934 ]), array([ 0.84895845, -2.98800584, -3.26541031,  1.10647519]), array([ 0.12441076, -2.62186002, -3.82916437,  2.50666858]), array([-0.61248442, -2.01035227, -3.39868979,  3.52062283]), array([-1.1934481 , -1.28393268, -2.37484053,  3.61077144]), array([-1.56788939, -0.58290237, -1.36628026,  3.32854045]), array([-1.73747137,  0.0311827 , -0.3167569 ,  2.78960276]), array([-1.68479174,  0.52168866,  0.88167515,  2.05913589]), array([-1.34456341,  0.75415913,  2.53576843,  0.16050148]), array([-0.67919187,  0.54568774,  4.03763673, -2.25494735]), array([ 0.20840851, -0.07875288,  4.61295619, -3.58625162]), array([ 1.06737632, -0.69336852,  3.80322888, -2.27730055]), array([ 1.6955749 , -0.96774515,  2.46135418, -0.55744704]), array([ 2.06086781, -0.97096756,  1.23248152,  0.3959363 ]), array([ 2.19358694, -0.81835083,  0.12449486,  1.07256311]), array([ 2.10342847, -0.51564071, -1.03431083,  1.98449278]), array([ 1.77053805e+00, -2.35126596e-03, -2.31994873e+00,  3.18975726e+00]), array([ 1.17397064,  0.74304079, -3.60833445,  4.07954913]), array([ 0.35727908,  1.51099122, -4.44462756,  3.28567603]), array([-0.53675978,  1.95439178, -4.27500555,  0.97994995]), array([-1.26061945,  1.87436657, -2.78124631, -1.76559293]), array([-1.60369524,  1.27778876, -0.62189875, -4.10007353]), array([-1.50499699,  0.21357524,  1.49084229, -6.40388612]), array([-1.09936672, -1.14530966,  2.36129135, -6.84146425]), array([-0.58886524, -2.47598411,  2.76726437, -6.55112487]), array([ 0.0093572 ,  2.45275794,  3.19147338, -7.22278373]), array([ 0.69904547,  0.80436561,  3.75014686, -9.45552219]), array([ 1.37564088, -1.07906433,  2.51632034, -8.48332981]), array([ 1.61091799, -2.49690773, -0.08548142, -5.90785626]), array([ 1.42910416,  2.7665055 , -1.45449198, -4.48233305]), array([ 1.11548888,  1.90267728, -1.52770984, -4.41609308]), array([ 0.87280636,  0.88731498, -0.82626923, -5.9418341 ]), array([ 0.72747456, -0.41385031, -1.062419  , -6.3891903 ]), array([ 0.27722809, -1.37255202, -3.4713141 , -2.93451198]), array([-0.57107798, -1.57533452, -4.6505434 ,  0.62674746]), array([-1.46232026, -1.25586419, -4.08801042,  2.24225898]), array([-2.1820141 , -0.78101121, -3.12269413,  2.34700042])]</t>
-  </si>
-  <si>
-    <t>['[1,2,0]', '[0,2,1]', '[1,0,2]', '[1,1,2]', '[0,0,0]', '[2,2,2]', '[2,0,1]', '[2,1,0]', '[1,1,1]', '[0,1,1]']</t>
-  </si>
-  <si>
-    <t>[6, 7, 12, 20, 23, 30, 34, 35, 36, 47, 49, 58, 59, 61, 72, 73, 75, 76, 82, 83]</t>
-  </si>
-  <si>
-    <t>[0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 1, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 1, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 1, 1, 2, 2, 2, 2, 2, 2, 2, 2, 2, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
-  </si>
-  <si>
-    <t>['[-0.03763371 -0.01533471  0.06554052 -0.01816017]', '[-0.00754409 -0.05458322  0.2277812  -0.36241836]', '[ 0.04879627 -0.15231473  0.32089719 -0.5887683 ]', '[ 0.11397169 -0.27767857  0.31375488 -0.63332862]', '[ 0.16759438 -0.39312519  0.2086893  -0.49480525]', '[ 0.1930193  -0.46685036  0.03906408 -0.22816919]', '[ 0.16956871 -0.44830261 -0.26820417  0.40739083]', '[ 0.09055011 -0.31127879 -0.50323119  0.93116007]', '[-0.03483507 -0.05969969 -0.71793241  1.5230623 ]', '[-0.18039446  0.26629635 -0.69574778  1.65343328]', '[-0.29690327  0.56916291 -0.43821183  1.31167254]', '[-0.34675453  0.77201171 -0.04953222  0.68864755]', '[-0.30454825  0.80815644  0.46136288 -0.32415858]', '[-0.1577012   0.61699714  0.97996208 -1.55618873]', '[ 0.07189896  0.20877574  1.26272334 -2.43181387]', '[ 0.31951943 -0.30233783  1.14071473 -2.53610943]', '[ 0.50143374 -0.75374181  0.63319299 -1.89176887]', '[ 0.56204381 -1.03841441 -0.03565408 -0.93030011]', '[ 0.46846348 -1.06492529 -0.87795383  0.65932004]', '[ 0.22323207 -0.77974914 -1.53433452  2.16055548]', '[-0.11064823 -0.26209874 -1.72810082  2.88401003]', '[-0.4436498   0.33658689 -1.50842414  2.92152293]', '[-0.68143749  0.84582736 -0.8181079   2.0835892 ]', '[-0.7489734   1.12403387  0.14624354  0.68865402]', '[-0.61674061  1.09145388  1.15243818 -1.01525746]', '[-0.30171748  0.72000998  1.95002269 -2.66498792]', '[ 0.13441193  0.06485292  2.30569491 -3.6937826 ]', '[ 0.56718069 -0.65161158  1.90724686 -3.25159442]', '[ 0.86554577 -1.18467201  1.03459225 -2.03679624]', '[ 0.97240624 -1.4641066   0.02650409 -0.75946142]', '[ 0.86864796 -1.46206211 -1.04752773  0.78836081]', '[ 0.55472175 -1.11609645 -2.05654674  2.68577663]', '[ 0.06588662 -0.39583146 -2.74719899  4.38993625]', '[-0.48504557  0.520763   -2.59333775  4.42222075]', '[-0.90799323  1.24388983 -1.58129312  2.75057524]', '[-1.108508    1.62804582 -0.41464979  1.11751444]', '[-1.07341002  1.69624045  0.75780993 -0.43936711]', '[-0.80380505  1.41972277  1.91276486 -2.36037614]', '[-0.32166503  0.73882551  2.85796208 -4.4261218 ]', '[ 0.29517277 -0.27314385  3.12279614 -5.29010335]', '[ 0.84871591 -1.2087579   2.3056435  -3.88165657]', '[ 1.20012743 -1.82183509  1.18908214 -2.29120468]', '[ 1.31990166 -2.14024749  0.00485939 -0.91111561]', '[ 1.1969423  -2.16484316 -1.21890649  0.6796917 ]', '[ 0.83638461 -1.83477553 -2.34700992  2.66610612]', '[ 0.27636732 -1.07678546 -3.21008263  4.94375909]', '[-0.41498976  0.09524226 -3.5102475   6.34360111]', '[-1.01594208  1.20504754 -2.37303262  4.51733841]', '[-1.36206987  1.9366542  -1.08044966  2.86106515]', '[-1.44107016  2.34597328  0.2815531   1.25211817]', '[-1.24879741  2.41517793  1.61698535 -0.57831904]', '[-0.80989724  2.10281314  2.71315858 -2.58502416]', '[-0.19265367  1.36303326  3.39778356 -4.84755792]', '[ 0.52462263  0.18446891  3.63534652 -6.61748949]', '[ 1.16167421 -1.04989134  2.55514889 -5.34851531]', '[ 1.5239594  -1.93788661  1.06555337 -3.60775684]', '[ 1.59139133 -2.51518719 -0.3746532  -2.18233851]', '[ 1.37721442 -2.78884006 -1.7399199  -0.54597329]', '[ 0.90883338 -2.73236177 -2.88821801  1.10503285]', '[ 0.25985399 -2.35267441 -3.47013543  2.66666653]', '[-0.42767433 -1.66273387 -3.29633643  4.16608063]', '[-1.02361742 -0.75386387 -2.616005    4.76650082]', '[-1.461127    0.19607917 -1.68012365  4.53892089]', '[-1.66377692  1.00384202 -0.28736692  3.46364176]', '[-1.55791283  1.55859783  1.3744002   2.00452636]', '[-1.10118042  1.71766641  3.12825756 -0.51168242]', '[-0.3507874   1.32177895  4.24103084 -3.46940817]', '[ 0.53823956  0.36859124  4.48724725 -5.73059982]', '[ 1.35755227 -0.74003201  3.54133828 -4.92251238]', '[ 1.9356818  -1.56043297  2.26262665 -3.38641051]', '[ 2.27551595 -2.14423709  1.16358508 -2.53985815]', '[ 2.40964518 -2.59360256  0.19605283 -1.96111799]', '[ 2.34706192 -2.88129989 -0.81658284 -0.88268683]', '[ 2.07812672 -2.92808406 -1.89917472  0.46981156]', '[ 1.57523168 -2.66736509 -3.14411152  2.22272773]', '[ 0.83643658 -2.0148482  -4.17776329  4.44024509]', '[-0.06693134 -0.84080115 -4.79910538  7.28557062]', '[-1.01390022  0.71380837 -4.35154619  7.41129474]', '[-1.73366011  1.94713096 -2.86553413  5.04871852]', '[-2.1797433   2.81168863 -1.6490489   3.72372731]', '[-2.41808175 -2.82299913 -0.79979917  2.78095358]', '[-2.518304   -2.36013515 -0.22858395  1.83755285]', '[-2.50382636 -2.11552053  0.38692063  0.59044715]', '[-2.36159154 -2.10815648  1.06577493 -0.52636313]', '[-2.04760817 -2.37003537  2.12064378 -2.08182385]', '[-1.49479123 -2.93545583  3.4327894  -3.57589683]', '[-0.68954562  2.45881698  4.50256284 -5.45839503]', '[ 0.25898095  1.08551827  4.96887676 -8.42695301]', '[ 1.23910934 -0.74115143  4.45008832 -8.83708405]', '[ 1.93883555 -2.23022044  2.60461095 -6.28159903]', '[ 2.32699552  2.93035521  1.433187   -5.08071651]', '[ 2.56914155  1.99479864  1.08225931 -4.31766297]', '[ 2.77389967  1.19042003  0.9748834  -3.7606138 ]']</t>
-  </si>
-  <si>
-    <t>[0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50, 51, 52, 53, 54, 55, 56, 57, 58, 59, 60, 61, 62, 63, 64, 65, 66, 67, 68, 69, 70, 71, 72, 73, 74, 75, 76, 77, 78, 79, 80, 81, 82, 83, 84, 85, 86, 87, 88, 89, 90, 91, 92]</t>
-  </si>
-  <si>
-    <t>[array([-0.03763371, -0.01533471,  0.06554052, -0.01816017], dtype=float32), array([-0.00754409, -0.05458322,  0.2277812 , -0.36241836]), array([ 0.04879627, -0.15231473,  0.32089719, -0.5887683 ]), array([ 0.11397169, -0.27767857,  0.31375488, -0.63332862]), array([ 0.16759438, -0.39312519,  0.2086893 , -0.49480525]), array([ 0.1930193 , -0.46685036,  0.03906408, -0.22816919]), array([ 0.16956871, -0.44830261, -0.26820417,  0.40739083]), array([ 0.09055011, -0.31127879, -0.50323119,  0.93116007]), array([-0.03483507, -0.05969969, -0.71793241,  1.5230623 ]), array([-0.18039446,  0.26629635, -0.69574778,  1.65343328]), array([-0.29690327,  0.56916291, -0.43821183,  1.31167254]), array([-0.34675453,  0.77201171, -0.04953222,  0.68864755]), array([-0.30454825,  0.80815644,  0.46136288, -0.32415858]), array([-0.1577012 ,  0.61699714,  0.97996208, -1.55618873]), array([ 0.07189896,  0.20877574,  1.26272334, -2.43181387]), array([ 0.31951943, -0.30233783,  1.14071473, -2.53610943]), array([ 0.50143374, -0.75374181,  0.63319299, -1.89176887]), array([ 0.56204381, -1.03841441, -0.03565408, -0.93030011]), array([ 0.46846348, -1.06492529, -0.87795383,  0.65932004]), array([ 0.22323207, -0.77974914, -1.53433452,  2.16055548]), array([-0.11064823, -0.26209874, -1.72810082,  2.88401003]), array([-0.4436498 ,  0.33658689, -1.50842414,  2.92152293]), array([-0.68143749,  0.84582736, -0.8181079 ,  2.0835892 ]), array([-0.7489734 ,  1.12403387,  0.14624354,  0.68865402]), array([-0.61674061,  1.09145388,  1.15243818, -1.01525746]), array([-0.30171748,  0.72000998,  1.95002269, -2.66498792]), array([ 0.13441193,  0.06485292,  2.30569491, -3.6937826 ]), array([ 0.56718069, -0.65161158,  1.90724686, -3.25159442]), array([ 0.86554577, -1.18467201,  1.03459225, -2.03679624]), array([ 0.97240624, -1.4641066 ,  0.02650409, -0.75946142]), array([ 0.86864796, -1.46206211, -1.04752773,  0.78836081]), array([ 0.55472175, -1.11609645, -2.05654674,  2.68577663]), array([ 0.06588662, -0.39583146, -2.74719899,  4.38993625]), array([-0.48504557,  0.520763  , -2.59333775,  4.42222075]), array([-0.90799323,  1.24388983, -1.58129312,  2.75057524]), array([-1.108508  ,  1.62804582, -0.41464979,  1.11751444]), array([-1.07341002,  1.69624045,  0.75780993, -0.43936711]), array([-0.80380505,  1.41972277,  1.91276486, -2.36037614]), array([-0.32166503,  0.73882551,  2.85796208, -4.4261218 ]), array([ 0.29517277, -0.27314385,  3.12279614, -5.29010335]), array([ 0.84871591, -1.2087579 ,  2.3056435 , -3.88165657]), array([ 1.20012743, -1.82183509,  1.18908214, -2.29120468]), array([ 1.31990166, -2.14024749,  0.00485939, -0.91111561]), array([ 1.1969423 , -2.16484316, -1.21890649,  0.6796917 ]), array([ 0.83638461, -1.83477553, -2.34700992,  2.66610612]), array([ 0.27636732, -1.07678546, -3.21008263,  4.94375909]), array([-0.41498976,  0.09524226, -3.5102475 ,  6.34360111]), array([-1.01594208,  1.20504754, -2.37303262,  4.51733841]), array([-1.36206987,  1.9366542 , -1.08044966,  2.86106515]), array([-1.44107016,  2.34597328,  0.2815531 ,  1.25211817]), array([-1.24879741,  2.41517793,  1.61698535, -0.57831904]), array([-0.80989724,  2.10281314,  2.71315858, -2.58502416]), array([-0.19265367,  1.36303326,  3.39778356, -4.84755792]), array([ 0.52462263,  0.18446891,  3.63534652, -6.61748949]), array([ 1.16167421, -1.04989134,  2.55514889, -5.34851531]), array([ 1.5239594 , -1.93788661,  1.06555337, -3.60775684]), array([ 1.59139133, -2.51518719, -0.3746532 , -2.18233851]), array([ 1.37721442, -2.78884006, -1.7399199 , -0.54597329]), array([ 0.90883338, -2.73236177, -2.88821801,  1.10503285]), array([ 0.25985399, -2.35267441, -3.47013543,  2.66666653]), array([-0.42767433, -1.66273387, -3.29633643,  4.16608063]), array([-1.02361742, -0.75386387, -2.616005  ,  4.76650082]), array([-1.461127  ,  0.19607917, -1.68012365,  4.53892089]), array([-1.66377692,  1.00384202, -0.28736692,  3.46364176]), array([-1.55791283,  1.55859783,  1.3744002 ,  2.00452636]), array([-1.10118042,  1.71766641,  3.12825756, -0.51168242]), array([-0.3507874 ,  1.32177895,  4.24103084, -3.46940817]), array([ 0.53823956,  0.36859124,  4.48724725, -5.73059982]), array([ 1.35755227, -0.74003201,  3.54133828, -4.92251238]), array([ 1.9356818 , -1.56043297,  2.26262665, -3.38641051]), array([ 2.27551595, -2.14423709,  1.16358508, -2.53985815]), array([ 2.40964518, -2.59360256,  0.19605283, -1.96111799]), array([ 2.34706192, -2.88129989, -0.81658284, -0.88268683]), array([ 2.07812672, -2.92808406, -1.89917472,  0.46981156]), array([ 1.57523168, -2.66736509, -3.14411152,  2.22272773]), array([ 0.83643658, -2.0148482 , -4.17776329,  4.44024509]), array([-0.06693134, -0.84080115, -4.79910538,  7.28557062]), array([-1.01390022,  0.71380837, -4.35154619,  7.41129474]), array([-1.73366011,  1.94713096, -2.86553413,  5.04871852]), array([-2.1797433 ,  2.81168863, -1.6490489 ,  3.72372731]), array([-2.41808175, -2.82299913, -0.79979917,  2.78095358]), array([-2.518304  , -2.36013515, -0.22858395,  1.83755285]), array([-2.50382636, -2.11552053,  0.38692063,  0.59044715]), array([-2.36159154, -2.10815648,  1.06577493, -0.52636313]), array([-2.04760817, -2.37003537,  2.12064378, -2.08182385]), array([-1.49479123, -2.93545583,  3.4327894 , -3.57589683]), array([-0.68954562,  2.45881698,  4.50256284, -5.45839503]), array([ 0.25898095,  1.08551827,  4.96887676, -8.42695301]), array([ 1.23910934, -0.74115143,  4.45008832, -8.83708405]), array([ 1.93883555, -2.23022044,  2.60461095, -6.28159903]), array([ 2.32699552,  2.93035521,  1.433187  , -5.08071651]), array([ 2.56914155,  1.99479864,  1.08225931, -4.31766297]), array([ 2.77389967,  1.19042003,  0.9748834 , -3.7606138 ])]</t>
-  </si>
-  <si>
-    <t>['[0,1,1]', '[1,2,0]', '[1,1,1]', '[2,0,1]', '[2,2,2]', '[0,0,0]', '[1,0,2]', '[2,1,0]', '[1,1,2]', '[0,2,1]']</t>
-  </si>
-  <si>
-    <t>[6, 7, 8, 9, 10, 11, 19, 21, 30, 31, 32, 33, 35, 42, 43, 45, 46, 47, 48, 55, 56, 58, 59, 60, 70, 71, 72, 73, 74, 75, 83, 88, 89, 91, 101, 103, 114, 121, 124, 126, 128, 129, 130, 132, 135, 136, 138, 139, 141, 145, 146, 147, 148, 149, 151, 153, 154, 155]</t>
-  </si>
-  <si>
-    <t>[0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 1, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 1, 2, 2, 2, 2, 2, 2, 2, 1, 0, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 0, 0, 2, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2]</t>
-  </si>
-  <si>
-    <t>['[-0.03763371 -0.01533471  0.06554052 -0.01816017]', '[-0.00754409 -0.05458322  0.2277812  -0.36241836]', '[ 0.04879627 -0.15231473  0.32089719 -0.5887683 ]', '[ 0.11397169 -0.27767857  0.31375488 -0.63332862]', '[ 0.16759438 -0.39312519  0.2086893  -0.49480525]', '[ 0.1930193  -0.46685036  0.03906408 -0.22816919]', '[ 0.16956871 -0.44830261 -0.26820417  0.40739083]', '[ 0.09055011 -0.31127879 -0.50323119  0.93116007]', '[-0.02165415 -0.09380121 -0.58952709  1.1892161 ]', '[-0.13228272  0.13968862 -0.48657385  1.08703787]', '[-0.20542731  0.31962025 -0.22562708  0.67289162]', '[-0.21756752  0.39782756  0.10766541  0.09689063]', '[-0.15109606  0.32490126  0.54216963 -0.80657469]', '[-0.01068619  0.09081112  0.82714324 -1.47439182]', '[ 0.16212513 -0.23279107  0.85391345 -1.67375883]', '[ 0.3120332  -0.54339537  0.60708552 -1.36152952]', '[ 0.39322683 -0.75586146  0.18779451 -0.73014827]', '[ 0.38412465 -0.82793881 -0.27624305  0.01454459]', '[ 0.26384544 -0.69033685 -0.90484238  1.34113963]', '[ 0.04812306 -0.34154272 -1.20443244  2.06892924]', '[-0.20653981  0.12725783 -1.27222972  2.48633127]', '[-0.41852719  0.56318458 -0.79486767  1.77490087]', '[-0.522427    0.84395802 -0.2236329   0.99447792]', '[-0.50486371  0.95264153  0.39443013  0.08553845]', '[-0.34860375  0.81961377  1.14063297 -1.39950412]', '[-0.06430234  0.40798991  1.64675929 -2.63693307]', '[ 0.27836775 -0.17919914  1.68510071 -3.05326233]', '[ 0.57098808 -0.73907917  1.16996325 -2.41826742]', '[ 0.72783428 -1.11797385  0.3757934  -1.34074134]', '[ 0.71827332 -1.2703979  -0.46548837 -0.17828038]', '[ 0.53892599 -1.16115036 -1.2980151   1.26702377]', '[ 0.2154031  -0.77022273 -1.88412902  2.59367549]', '[-0.18541883 -0.1658562  -2.02834522  3.2766552 ]', '[-0.55072321  0.45240117 -1.52882431  2.72358014]', '[-0.78149557  0.90827613 -0.73710577  1.77370914]', '[-0.8263472   1.12237072  0.28948508  0.36143443]', '[-0.65986944  1.02214329  1.35108519 -1.36831392]', '[-0.30062106  0.5776505   2.18541475 -3.0248181 ]', '[ 0.17807207 -0.13057463  2.47450871 -3.81330594]', '[ 0.63237026 -0.83490973  1.96309792 -3.04178284]', '[ 0.93701153 -1.31375837  1.04819383 -1.73150498]', '[ 1.04382431 -1.53052824  0.01207142 -0.44328464]', '[ 0.93378462 -1.46527139 -1.09936875  1.1079906 ]', '[ 0.61330619 -1.07926903 -2.07120471  2.76314892]', '[ 0.11459929 -0.34095891 -2.82705063  4.48283178]', '[-0.44206373  0.55334501 -2.5744405   4.11703507]', '[-0.86795545  1.21922999 -1.62828627  2.48529377]', '[-1.08229703  1.55259187 -0.50100937  0.87252435]', '[-1.06609837  1.57386527  0.6598207  -0.66177534]', '[-0.81389768  1.25478993  1.84393616 -2.56300242]', '[-0.3401283   0.53871359  2.83436319 -4.53955854]', '[ 0.26619158 -0.45776133  3.03636171 -5.01153974]', '[ 0.8055366  -1.32333928  2.26992727 -3.5160867 ]', '[ 1.15766359 -1.8659089   1.2269471  -1.94889864]', '[ 1.28981664 -2.11673435  0.0869289  -0.57786813]', '[ 1.18575397 -2.07623601 -1.11643397  0.99650128]', '[ 0.85189171 -1.70622415 -2.19064913  2.74589556]', '[ 0.31533665 -0.93293513 -3.13530262  5.00682555]', '[-0.35001334  0.19728011 -3.31224172  5.83998389]', '[-0.92043036  1.20732521 -2.28341035  4.06894899]', '[-1.25136402  1.83174013 -1.01819666  2.23538514]', '[-1.33395977  2.14061236  0.19266388  0.86566583]', '[-1.16393516  2.1326817   1.48567148 -0.96594898]', '[-0.75345348  1.73922352  2.57443776 -3.01906396]', '[-0.15335708  0.90435834  3.3768666  -5.32826798]', '[ 0.55102549 -0.30351652  3.44162308 -6.23386432]', '[ 1.13190517 -1.38837035  2.27312149 -4.46735474]', '[ 1.45314056 -2.1119819   0.93804167 -2.84021583]', '[ 1.50862775 -2.54049485 -0.3743288  -1.45519946]', '[ 1.3027601  -2.67140207 -1.66348888  0.15820759]', '[ 0.85704222 -2.47164615 -2.73318208  1.85419147]', '[ 0.24662185 -1.92473015 -3.26494455  3.61809489]', '[-0.41104431 -1.03441776 -3.24481437  5.20333338]', '[-1.01555989  0.06933016 -2.6554254   5.47673714]', '[-1.41184936  1.02263698 -1.22972424  3.92987998]', '[-1.4975554   1.64081522  0.37699527  2.25684706]', '[-1.27171419  1.93789127  1.85950755  0.6587885 ]', '[-0.76088093  1.83633997  3.15723822 -1.72052972]', '[-0.05486076  1.24112657  3.79272678 -4.20216   ]', '[ 0.71335663  0.21165978  3.74725064 -5.7515278 ]', '[ 1.36746164 -0.86480771  2.66296556 -4.71334929]', '[ 1.76194661 -1.65728276  1.28160022 -3.27931357]', '[ 1.88120679 -2.1987431  -0.08759545 -2.149387  ]', '[ 1.71564165 -2.46694661 -1.55595189 -0.49184139]', '[ 1.2649275  -2.37226601 -2.91887818  1.50893978]', '[ 0.57411266 -1.83239154 -3.89835383  3.96951687]', '[-0.25945193 -0.76453957 -4.36384663  6.62560749]', '[-1.09865014  0.62695806 -3.77047678  6.6246043 ]', '[-1.69517904  1.7191326  -2.20047587  4.38600765]', '[-1.99150406  2.4392427  -0.7918182   2.90182321]', '[-2.02866677  2.91123633  0.39801907  1.81007175]', '[-1.83716526 -3.12888559  1.51801952  0.59734293]', '[-1.40551177  3.10423133  2.80317997 -1.10825716]', '[-0.72711046  2.7067454   3.89250561 -2.88991746]', '[ 0.09138759  1.93536529  4.14146996 -4.84544451]', '[ 0.89239834  0.7781053   3.83041328 -6.60369324]', '[ 1.57933607 -0.55984169  2.86710004 -6.33284438]', '[ 1.99192876 -1.66882625  1.23304236 -4.79611892]', '[ 2.07290947 -2.50461786 -0.39894729 -3.57938914]', '[ 1.8529538  -3.09468185 -1.74005515 -2.30827007]', '[ 1.38127472  2.89046395 -2.95731091 -0.71879591]', '[ 0.6868341   2.84542101 -3.92120164  0.12513233]', '[-0.14539501  2.88916078 -4.24125063  0.10765586]', '[-0.93207066  2.79059354 -3.4573851  -1.2707769 ]', '[-1.47551554  2.34957975 -1.84070483 -3.20919851]', '[-1.60756664  1.453812    0.59447577 -5.79737352]', '[-1.24277462e+00  7.05860263e-03  2.84031007e+00 -8.41613007e+00]', '[-0.62838085 -1.64041313  3.08267959 -7.65053364]', '[-6.67762538e-03 -3.08614920e+00  3.15041431e+00 -7.03868161e+00]', '[ 0.62450126  1.72589683  3.201952   -7.95828237]', '[ 1.29543735 -0.05958223  3.25923063 -9.45338532]', '[ 1.72968972 -1.72278011  0.81341323 -6.8814287 ]', '[ 1.63204091 -2.87446387 -1.59399184 -4.78368264]', '[ 1.19912788  2.57721793 -2.48525089 -3.7851053 ]', '[ 0.71566744  1.78972662 -2.14678404 -4.43657061]', '[ 0.43360942  0.64090559 -0.63194289 -7.15925657]', '[ 0.29850142 -0.82810059 -1.31516278 -6.54703333]', '[-0.20876959 -1.77467449 -3.58205764 -3.01493914]', '[-1.01327203 -2.11719203 -4.15131937 -0.78628616]', '[-1.79277748 -2.21337587 -3.56790082 -0.39567354]', '[-2.44596315 -2.3205252  -3.03191802 -0.70106208]', '[-3.03817885 -2.49566993 -3.00682979 -0.94359055]', '[ 2.58393906 -2.6195782  -3.71464892 -0.10976384]', '[ 1.72038477 -2.45510932 -4.97712001  2.00796269]', '[ 0.61143439 -1.73169962 -6.00482024  5.47480416]', '[-0.64967917 -0.20492502 -6.42929555  9.21473584]', '[-1.8008438   1.41014386 -4.92116597  6.33613668]', '[-2.68266462  2.46385295 -4.04881933  4.55736062]', '[ 2.81135213 -2.95417255 -3.99232034  4.36297943]', '[ 1.94927743 -1.9642078  -4.75660048  5.88614416]', '[ 0.85230288 -0.4353803  -6.27428304  9.4659884 ]', '[-0.43334403  1.38667335 -6.19932777  7.54626957]', '[-1.59082146  2.49575925 -5.32336094  3.85166597]', '[-2.55709835  3.07904184 -4.4031806   2.2880717 ]', '[ 2.87505553 -2.76650104 -4.28243264  2.3562081 ]', '[ 1.95561651 -2.16890626 -5.03299445  3.95972467]', '[ 0.83278337 -1.03220449 -6.25864748  7.72000432]', '[-0.50674142  0.76979068 -6.70646826  8.86876721]', '[-1.72430017  2.09892211 -5.49667899  4.6137115 ]', '[-2.7276978   2.77877951 -4.63473626  2.57415016]', '[ 2.63595143 -3.00542422 -4.74524549  2.733304  ]', '[ 1.60325806 -2.30170466 -5.65311706  4.69473066]', '[ 0.36497735 -0.93871481 -6.77059099  9.22664019]', '[-1.0032156   1.03454843 -6.461581    8.99065805]', '[-2.1654101   2.43487109 -5.2990905   5.47000928]', '[ 3.11927738 -2.89110617 -4.82192211  4.53222591]', '[ 2.12480459 -1.88013057 -5.30123126  6.01135138]', '[ 0.92119722 -0.30048799 -6.80039587  9.73161487]', '[-0.4534956   1.47392907 -6.58346893  6.81008282]', '[-1.68477018  2.4004745  -5.62904432  2.74867575]', '[-2.69999236  2.72769693 -4.61142319  0.85628317]', '[ 2.69781768  2.8343745  -4.42923807  0.46352995]', '[ 1.73601639  3.00958712 -5.32838117  1.44759417]', '[ 0.5542125  -2.84105581 -6.38116436  2.99819541]', '[-0.71258726 -2.03769447 -6.01217187  5.04431393]', '[-1.79788921 -0.87081494 -4.86758138  6.39894519]']</t>
-  </si>
-  <si>
-    <t>[0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50, 51, 52, 53, 54, 55, 56, 57, 58, 59, 60, 61, 62, 63, 64, 65, 66, 67, 68, 69, 70, 71, 72, 73, 74, 75, 76, 77, 78, 79, 80, 81, 82, 83, 84, 85, 86, 87, 88, 89, 90, 91, 92, 93, 94, 95, 96, 97, 98, 99, 100, 101, 102, 103, 104, 105, 106, 107, 108, 109, 110, 111, 112, 113, 114, 115, 116, 117, 118, 119, 120, 121, 122, 123, 124, 125, 126, 127, 128, 129, 130, 131, 132, 133, 134, 135, 136, 137, 138, 139, 140, 141, 142, 143, 144, 145, 146, 147, 148, 149, 150, 151, 152, 153, 154, 155]</t>
-  </si>
-  <si>
-    <t>[array([-0.03763371, -0.01533471,  0.06554052, -0.01816017], dtype=float32), array([-0.00754409, -0.05458322,  0.2277812 , -0.36241836]), array([ 0.04879627, -0.15231473,  0.32089719, -0.5887683 ]), array([ 0.11397169, -0.27767857,  0.31375488, -0.63332862]), array([ 0.16759438, -0.39312519,  0.2086893 , -0.49480525]), array([ 0.1930193 , -0.46685036,  0.03906408, -0.22816919]), array([ 0.16956871, -0.44830261, -0.26820417,  0.40739083]), array([ 0.09055011, -0.31127879, -0.50323119,  0.93116007]), array([-0.02165415, -0.09380121, -0.58952709,  1.1892161 ]), array([-0.13228272,  0.13968862, -0.48657385,  1.08703787]), array([-0.20542731,  0.31962025, -0.22562708,  0.67289162]), array([-0.21756752,  0.39782756,  0.10766541,  0.09689063]), array([-0.15109606,  0.32490126,  0.54216963, -0.80657469]), array([-0.01068619,  0.09081112,  0.82714324, -1.47439182]), array([ 0.16212513, -0.23279107,  0.85391345, -1.67375883]), array([ 0.3120332 , -0.54339537,  0.60708552, -1.36152952]), array([ 0.39322683, -0.75586146,  0.18779451, -0.73014827]), array([ 0.38412465, -0.82793881, -0.27624305,  0.01454459]), array([ 0.26384544, -0.69033685, -0.90484238,  1.34113963]), array([ 0.04812306, -0.34154272, -1.20443244,  2.06892924]), array([-0.20653981,  0.12725783, -1.27222972,  2.48633127]), array([-0.41852719,  0.56318458, -0.79486767,  1.77490087]), array([-0.522427  ,  0.84395802, -0.2236329 ,  0.99447792]), array([-0.50486371,  0.95264153,  0.39443013,  0.08553845]), array([-0.34860375,  0.81961377,  1.14063297, -1.39950412]), array([-0.06430234,  0.40798991,  1.64675929, -2.63693307]), array([ 0.27836775, -0.17919914,  1.68510071, -3.05326233]), array([ 0.57098808, -0.73907917,  1.16996325, -2.41826742]), array([ 0.72783428, -1.11797385,  0.3757934 , -1.34074134]), array([ 0.71827332, -1.2703979 , -0.46548837, -0.17828038]), array([ 0.53892599, -1.16115036, -1.2980151 ,  1.26702377]), array([ 0.2154031 , -0.77022273, -1.88412902,  2.59367549]), array([-0.18541883, -0.1658562 , -2.02834522,  3.2766552 ]), array([-0.55072321,  0.45240117, -1.52882431,  2.72358014]), array([-0.78149557,  0.90827613, -0.73710577,  1.77370914]), array([-0.8263472 ,  1.12237072,  0.28948508,  0.36143443]), array([-0.65986944,  1.02214329,  1.35108519, -1.36831392]), array([-0.30062106,  0.5776505 ,  2.18541475, -3.0248181 ]), array([ 0.17807207, -0.13057463,  2.47450871, -3.81330594]), array([ 0.63237026, -0.83490973,  1.96309792, -3.04178284]), array([ 0.93701153, -1.31375837,  1.04819383, -1.73150498]), array([ 1.04382431, -1.53052824,  0.01207142, -0.44328464]), array([ 0.93378462, -1.46527139, -1.09936875,  1.1079906 ]), array([ 0.61330619, -1.07926903, -2.07120471,  2.76314892]), array([ 0.11459929, -0.34095891, -2.82705063,  4.48283178]), array([-0.44206373,  0.55334501, -2.5744405 ,  4.11703507]), array([-0.86795545,  1.21922999, -1.62828627,  2.48529377]), array([-1.08229703,  1.55259187, -0.50100937,  0.87252435]), array([-1.06609837,  1.57386527,  0.6598207 , -0.66177534]), array([-0.81389768,  1.25478993,  1.84393616, -2.56300242]), array([-0.3401283 ,  0.53871359,  2.83436319, -4.53955854]), array([ 0.26619158, -0.45776133,  3.03636171, -5.01153974]), array([ 0.8055366 , -1.32333928,  2.26992727, -3.5160867 ]), array([ 1.15766359, -1.8659089 ,  1.2269471 , -1.94889864]), array([ 1.28981664, -2.11673435,  0.0869289 , -0.57786813]), array([ 1.18575397, -2.07623601, -1.11643397,  0.99650128]), array([ 0.85189171, -1.70622415, -2.19064913,  2.74589556]), array([ 0.31533665, -0.93293513, -3.13530262,  5.00682555]), array([-0.35001334,  0.19728011, -3.31224172,  5.83998389]), array([-0.92043036,  1.20732521, -2.28341035,  4.06894899]), array([-1.25136402,  1.83174013, -1.01819666,  2.23538514]), array([-1.33395977,  2.14061236,  0.19266388,  0.86566583]), array([-1.16393516,  2.1326817 ,  1.48567148, -0.96594898]), array([-0.75345348,  1.73922352,  2.57443776, -3.01906396]), array([-0.15335708,  0.90435834,  3.3768666 , -5.32826798]), array([ 0.55102549, -0.30351652,  3.44162308, -6.23386432]), array([ 1.13190517, -1.38837035,  2.27312149, -4.46735474]), array([ 1.45314056, -2.1119819 ,  0.93804167, -2.84021583]), array([ 1.50862775, -2.54049485, -0.3743288 , -1.45519946]), array([ 1.3027601 , -2.67140207, -1.66348888,  0.15820759]), array([ 0.85704222, -2.47164615, -2.73318208,  1.85419147]), array([ 0.24662185, -1.92473015, -3.26494455,  3.61809489]), array([-0.41104431, -1.03441776, -3.24481437,  5.20333338]), array([-1.01555989,  0.06933016, -2.6554254 ,  5.47673714]), array([-1.41184936,  1.02263698, -1.22972424,  3.92987998]), array([-1.4975554 ,  1.64081522,  0.37699527,  2.25684706]), array([-1.27171419,  1.93789127,  1.85950755,  0.6587885 ]), array([-0.76088093,  1.83633997,  3.15723822, -1.72052972]), array([-0.05486076,  1.24112657,  3.79272678, -4.20216   ]), array([ 0.71335663,  0.21165978,  3.74725064, -5.7515278 ]), array([ 1.36746164, -0.86480771,  2.66296556, -4.71334929]), array([ 1.76194661, -1.65728276,  1.28160022, -3.27931357]), array([ 1.88120679, -2.1987431 , -0.08759545, -2.149387  ]), array([ 1.71564165, -2.46694661, -1.55595189, -0.49184139]), array([ 1.2649275 , -2.37226601, -2.91887818,  1.50893978]), array([ 0.57411266, -1.83239154, -3.89835383,  3.96951687]), array([-0.25945193, -0.76453957, -4.36384663,  6.62560749]), array([-1.09865014,  0.62695806, -3.77047678,  6.6246043 ]), array([-1.69517904,  1.7191326 , -2.20047587,  4.38600765]), array([-1.99150406,  2.4392427 , -0.7918182 ,  2.90182321]), array([-2.02866677,  2.91123633,  0.39801907,  1.81007175]), array([-1.83716526, -3.12888559,  1.51801952,  0.59734293]), array([-1.40551177,  3.10423133,  2.80317997, -1.10825716]), array([-0.72711046,  2.7067454 ,  3.89250561, -2.88991746]), array([ 0.09138759,  1.93536529,  4.14146996, -4.84544451]), array([ 0.89239834,  0.7781053 ,  3.83041328, -6.60369324]), array([ 1.57933607, -0.55984169,  2.86710004, -6.33284438]), array([ 1.99192876, -1.66882625,  1.23304236, -4.79611892]), array([ 2.07290947, -2.50461786, -0.39894729, -3.57938914]), array([ 1.8529538 , -3.09468185, -1.74005515, -2.30827007]), array([ 1.38127472,  2.89046395, -2.95731091, -0.71879591]), array([ 0.6868341 ,  2.84542101, -3.92120164,  0.12513233]), array([-0.14539501,  2.88916078, -4.24125063,  0.10765586]), array([-0.93207066,  2.79059354, -3.4573851 , -1.2707769 ]), array([-1.47551554,  2.34957975, -1.84070483, -3.20919851]), array([-1.60756664,  1.453812  ,  0.59447577, -5.79737352]), array([-1.24277462e+00,  7.05860263e-03,  2.84031007e+00, -8.41613007e+00]), array([-0.62838085, -1.64041313,  3.08267959, -7.65053364]), array([-6.67762538e-03, -3.08614920e+00,  3.15041431e+00, -7.03868161e+00]), array([ 0.62450126,  1.72589683,  3.201952  , -7.95828237]), array([ 1.29543735, -0.05958223,  3.25923063, -9.45338532]), array([ 1.72968972, -1.72278011,  0.81341323, -6.8814287 ]), array([ 1.63204091, -2.87446387, -1.59399184, -4.78368264]), array([ 1.19912788,  2.57721793, -2.48525089, -3.7851053 ]), array([ 0.71566744,  1.78972662, -2.14678404, -4.43657061]), array([ 0.43360942,  0.64090559, -0.63194289, -7.15925657]), array([ 0.29850142, -0.82810059, -1.31516278, -6.54703333]), array([-0.20876959, -1.77467449, -3.58205764, -3.01493914]), array([-1.01327203, -2.11719203, -4.15131937, -0.78628616]), array([-1.79277748, -2.21337587, -3.56790082, -0.39567354]), array([-2.44596315, -2.3205252 , -3.03191802, -0.70106208]), array([-3.03817885, -2.49566993, -3.00682979, -0.94359055]), array([ 2.58393906, -2.6195782 , -3.71464892, -0.10976384]), array([ 1.72038477, -2.45510932, -4.97712001,  2.00796269]), array([ 0.61143439, -1.73169962, -6.00482024,  5.47480416]), array([-0.64967917, -0.20492502, -6.42929555,  9.21473584]), array([-1.8008438 ,  1.41014386, -4.92116597,  6.33613668]), array([-2.68266462,  2.46385295, -4.04881933,  4.55736062]), array([ 2.81135213, -2.95417255, -3.99232034,  4.36297943]), array([ 1.94927743, -1.9642078 , -4.75660048,  5.88614416]), array([ 0.85230288, -0.4353803 , -6.27428304,  9.4659884 ]), array([-0.43334403,  1.38667335, -6.19932777,  7.54626957]), array([-1.59082146,  2.49575925, -5.32336094,  3.85166597]), array([-2.55709835,  3.07904184, -4.4031806 ,  2.2880717 ]), array([ 2.87505553, -2.76650104, -4.28243264,  2.3562081 ]), array([ 1.95561651, -2.16890626, -5.03299445,  3.95972467]), array([ 0.83278337, -1.03220449, -6.25864748,  7.72000432]), array([-0.50674142,  0.76979068, -6.70646826,  8.86876721]), array([-1.72430017,  2.09892211, -5.49667899,  4.6137115 ]), array([-2.7276978 ,  2.77877951, -4.63473626,  2.57415016]), array([ 2.63595143, -3.00542422, -4.74524549,  2.733304  ]), array([ 1.60325806, -2.30170466, -5.65311706,  4.69473066]), array([ 0.36497735, -0.93871481, -6.77059099,  9.22664019]), array([-1.0032156 ,  1.03454843, -6.461581  ,  8.99065805]), array([-2.1654101 ,  2.43487109, -5.2990905 ,  5.47000928]), array([ 3.11927738, -2.89110617, -4.82192211,  4.53222591]), array([ 2.12480459, -1.88013057, -5.30123126,  6.01135138]), array([ 0.92119722, -0.30048799, -6.80039587,  9.73161487]), array([-0.4534956 ,  1.47392907, -6.58346893,  6.81008282]), array([-1.68477018,  2.4004745 , -5.62904432,  2.74867575]), array([-2.69999236,  2.72769693, -4.61142319,  0.85628317]), array([ 2.69781768,  2.8343745 , -4.42923807,  0.46352995]), array([ 1.73601639,  3.00958712, -5.32838117,  1.44759417]), array([ 0.5542125 , -2.84105581, -6.38116436,  2.99819541]), array([-0.71258726, -2.03769447, -6.01217187,  5.04431393]), array([-1.79788921, -0.87081494, -4.86758138,  6.39894519])]</t>
-  </si>
-  <si>
-    <t>['[2,0,1]', '[1,1,2]', '[1,2,0]', '[0,0,0]', '[1,1,1]', '[0,1,1]', '[0,2,1]', '[1,0,2]', '[2,1,0]', '[2,2,2]']</t>
-  </si>
-  <si>
-    <t>[6, 7, 8, 9, 10, 11, 18, 19, 20, 21, 22, 23, 30, 31, 32, 34, 41, 42, 43, 45, 46, 47, 54, 55, 56, 58, 59, 68, 69, 70, 71, 72, 73, 83, 85, 86, 87, 88, 89, 97, 98, 99, 100, 101, 102, 104, 109, 111, 113, 114, 115, 116, 117, 119, 120, 121, 122, 129, 130, 131, 132, 133, 134, 135]</t>
-  </si>
-  <si>
-    <t>[0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 1, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 1, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 0]</t>
-  </si>
-  <si>
-    <t>['[-0.03763371 -0.01533471  0.06554052 -0.01816017]', '[-0.00754409 -0.05458322  0.2277812  -0.36241836]', '[ 0.04879627 -0.15231473  0.32089719 -0.5887683 ]', '[ 0.11397169 -0.27767857  0.31375488 -0.63332862]', '[ 0.16759438 -0.39312519  0.2086893  -0.49480525]', '[ 0.1930193  -0.46685036  0.03906408 -0.22816919]', '[ 0.16956871 -0.44830261 -0.26820417  0.40739083]', '[ 0.09055011 -0.31127879 -0.50323119  0.93116007]', '[-0.02165415 -0.09380121 -0.58952709  1.1892161 ]', '[-0.13228272  0.13968862 -0.48657385  1.08703787]', '[-0.20542731  0.31962025 -0.22562708  0.67289162]', '[-0.21756752  0.39782756  0.10766541  0.09689063]', '[-0.15109606  0.32490126  0.54216963 -0.80657469]', '[-0.01068619  0.09081112  0.82714324 -1.47439182]', '[ 0.16212513 -0.23279107  0.85391345 -1.67375883]', '[ 0.3120332  -0.54339537  0.60708552 -1.36152952]', '[ 0.39322683 -0.75586146  0.18779451 -0.73014827]', '[ 0.38412465 -0.82793881 -0.27624305  0.01454459]', '[ 0.27552572 -0.72135137 -0.78884754  1.03160865]', '[ 0.08086773 -0.43032213 -1.11647003  1.81675029]', '[-0.14966877 -0.03109877 -1.12879696  2.06540623]', '[-0.3455444   0.34863759 -0.7784691   1.63534647]', '[-0.44544803  0.59424237 -0.19906427  0.77949316]', '[-0.4218337   0.6519398   0.43007126 -0.20572333]', '[-0.26769146  0.484052    1.08142007 -1.44055859]', '[-0.00742761  0.10113176  1.45927884 -2.28595201]', '[ 0.28490347 -0.37428385  1.38589424 -2.32532176]', '[ 0.5187101  -0.77937684  0.90230152 -1.64619583]', '[ 0.63240836 -1.01433747  0.21740989 -0.68198512]', '[ 0.58206264 -0.99063291 -0.71189282  0.91746391]', '[ 0.36681234 -0.68097529 -1.40575041  2.14420403]', '[ 0.04159544 -0.16374689 -1.76892118  2.89401986]', '[-0.30147311  0.40276889 -1.56856425  2.59619163]', '[-0.56722524  0.85273137 -1.0345985   1.8196755 ]', '[-0.69032682  1.084332   -0.18208987  0.48616486]', '[-0.62824805  1.01752684  0.7944636  -1.15384725]', '[-0.3800221   0.62483041  1.65269834 -2.74012714]', '[ 0.00720557 -0.03923131  2.11746131 -3.70795602]', '[ 0.41500717 -0.75479796  1.85057805 -3.23807742]', '[ 0.71685207 -1.28565093  1.12515326 -2.02792903]', '[ 0.8549872  -1.56314504  0.24390184 -0.75031589]', '[ 0.8048585  -1.56201668 -0.73579793  0.76329224]', '[ 0.56805638 -1.25459393 -1.60503614  2.31711443]', '[ 0.17813345 -0.63996063 -2.23521717  3.7586311 ]', '[-0.29836231  0.20893449 -2.38641402  4.43746304]', '[-0.70364774  0.98022879 -1.57930762  3.12400331]', '[-0.91432405  1.44400635 -0.51375289  1.52161562]', '[-0.90851305  1.59332735  0.56295467 -0.02604444]', '[-0.68808027  1.40543405  1.61277985 -1.86895171]', '[-0.27788057  0.8399148   2.44208328 -3.76608041]', '[ 0.25551789 -0.0506448   2.74819722 -4.8471174 ]', '[ 0.74961013 -0.94763338  2.06735784 -3.88349979]', '[ 1.05742564 -1.57379789  0.98622685 -2.38608363]', '[ 1.14008664 -1.91078837 -0.15952378 -0.99489953]', '[ 0.99057574 -1.94832377 -1.31016288  0.63147604]', '[ 0.63166569 -1.65028703 -2.22833513  2.36842343]', '[ 0.12270839 -0.99797152 -2.79850887  4.119234  ]', '[-0.46398222 -0.02811732 -2.92321638  5.26900993]', '[-0.95897148  0.91373686 -1.90756258  3.92024436]', '[-1.20869784  1.52282371 -0.58005103  2.1960462 ]', '[-1.19990017  1.82421104  0.66126905  0.81161141]', '[-0.93740166  1.79313317  1.92241774 -1.15150975]', '[-0.45322559  1.34959204  2.85717882 -3.30887099]', '[ 0.17809969  0.47788691  3.35856892 -5.24913942]', '[ 0.8197509  -0.59338201  2.86536694 -5.0334679 ]', '[ 1.27379155 -1.43939879  1.63381144 -3.40710105]', '[ 1.46889473 -1.97520522  0.31442469 -1.98628896]', '[ 1.40057572 -2.23695012 -0.9878709  -0.61568316]', '[ 1.07562901 -2.18859234 -2.22156428  1.13540513]', '[ 0.53705513 -1.76775967 -3.08437556  3.102807  ]', '[-0.12422539 -0.94654906 -3.44987324  5.0387937 ]', '[-0.79578311  0.14858912 -3.08674835  5.48691033]', '[-1.2891931   1.09262057 -1.76991547  3.8252249 ]', '[-1.49711862  1.68915834 -0.30964532  2.18174644]', '[-1.42218874  1.99232632  1.0528921   0.82373384]', '[-1.07029994  1.95670561  2.42006472 -1.23336252]', '[-0.48108348  1.47619739  3.39456955 -3.61602526]', '[ 0.25565165  0.51377139  3.86910644 -5.8322724 ]', '[ 0.98737983 -0.66681951  3.23656781 -5.47177611]', '[ 1.50287008 -1.58217897  1.89657876 -3.7123968 ]', '[ 1.74699912 -2.18536108  0.54942673 -2.37378651]', '[ 1.72497246 -2.53773813 -0.76264461 -1.13606302]', '[ 1.4332936  -2.58751049 -2.13705319  0.67694505]', '[ 0.88988362 -2.2686499  -3.23213838  2.56467512]', '[ 0.17150249 -1.51869222 -3.86505529  4.97828542]', '[-0.61768727 -0.3226962  -3.90052977  6.67109763]', '[-1.29555755  0.9141597  -2.70343234  5.29949066]', '[-1.67953696  1.77907729 -1.14448961  3.4416358 ]', '[-1.75819454  2.31727728  0.3454926   1.95696356]', '[-1.54688735  2.55423913  1.75100175  0.37583435]', '[-1.06218754  2.43024298  3.04411664 -1.66278923]', '[-0.36492481  1.8700886   3.81767417 -3.98104952]', '[ 0.42580062  0.83374344  4.02121863 -6.2911993 ]', '[ 1.18697988 -0.49365671  3.37183406 -6.42300646]', '[ 1.71052458 -1.59770662  1.8346465  -4.63029728]', '[ 1.92502936 -2.38514789  0.32923702 -3.30111548]', '[ 1.85357592 -2.92183813 -1.01022558 -2.05187554]', '[ 1.51888374  3.12259037 -2.3255732  -0.3331218 ]', '[ 0.93387974 -3.08068917 -3.48427757  1.0976473 ]', '[ 0.16260132 -2.73984474 -4.07847858  2.25698766]', '[-0.62299311 -2.20610804 -3.61352539  2.97987434]', '[-1.23845033 -1.6013922  -2.48932963  2.92298857]', '[-1.61181909 -1.08811027 -1.24066074  2.11694136]', '[-1.74681543 -0.74415769 -0.11640173  1.31597038]', '[-1.64814139 -0.58780271  1.10011949  0.27627472]', '[-1.29712177 -0.64628845  2.3871119  -0.77230175]', '[-0.71541484 -0.83702125  3.32963263 -0.9269326 ]', '[-0.02658804 -0.9173628   3.37594009  0.33449779]', '[ 0.55931635 -0.64680655  2.36591062  2.36228504]', '[0.89504461 0.00754331 1.07101736 3.93088683]', '[1.02947729 0.84687545 0.37996553 4.27897234]', '[1.07561807 1.67399454 0.06263943 4.0715605 ]', '[ 1.03345725  2.54141837 -0.52497857  4.71009379]', '[ 0.84372994 -2.69772621 -1.4735932   5.87746906]', '[ 0.40139256 -1.30857519 -3.03363297  8.2926628 ]', '[-0.32401848  0.58785073 -3.66301006  9.63967126]', '[-0.8672922   2.19897997 -1.73747809  6.56838254]', '[-1.0652977  -2.95664453 -0.38527135  4.89996128]', '[-1.07868487 -2.0438034   0.15379306  4.38111375]', '[-1.02434587 -1.1639588   0.34595279  4.55376609]', '[-0.94015899 -0.19829595  0.59533473  4.97253244]', '[-0.7025074   0.68210606  1.95186182  3.46829369]', '[-0.14400214  1.09826131  3.50697667  0.66476823]', '[ 0.62152558  0.96596945  3.91721242 -1.75182899]', '[ 1.34773025  0.51284072  3.22551426 -2.50951752]', '[ 1.88826528  0.04053974  2.17004116 -2.12338512]', '[ 2.22447585 -0.33526621  1.22729876 -1.67980707]', '[ 2.39196854 -0.65334749  0.46943166 -1.54805247]', '[ 2.41381546 -0.96359904 -0.26679248 -1.54755513]', '[ 2.25063911 -1.19828614 -1.40655925 -0.72526733]', '[ 1.84030861 -1.23268775 -2.74891246  0.54806852]', '[ 1.1388338  -0.90420297 -4.25636673  2.88934914]', '[ 0.16873759 -0.07987973 -5.25048174  4.97129314]', '[-0.84275363  0.80351309 -4.61384961  3.34593915]', '[-1.62146815  1.19674824 -3.11835375  0.68368982]', '[-2.08941669  1.14813797 -1.59695352 -0.99156776]', '[-2.26930309  0.82717361 -0.24549857 -2.13402263]', '[-2.19875582  0.30490591  0.94274554 -3.10878202]', '[-1.88945297 -0.43174684  2.15580806 -4.26008882]', '[-1.33791287 -1.36935384  3.35601494 -4.97350817]', '[-0.54552923 -2.35913653  4.53355057 -4.7991364 ]', '[ 0.41654042  3.00736755  4.83650208 -4.43136927]', '[ 1.29045036  2.12451795  3.77758959 -4.40269553]', '[ 1.92426601  1.26807537  2.60872527 -4.09546719]']</t>
-  </si>
-  <si>
-    <t>[0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50, 51, 52, 53, 54, 55, 56, 57, 58, 59, 60, 61, 62, 63, 64, 65, 66, 67, 68, 69, 70, 71, 72, 73, 74, 75, 76, 77, 78, 79, 80, 81, 82, 83, 84, 85, 86, 87, 88, 89, 90, 91, 92, 93, 94, 95, 96, 97, 98, 99, 100, 101, 102, 103, 104, 105, 106, 107, 108, 109, 110, 111, 112, 113, 114, 115, 116, 117, 118, 119, 120, 121, 122, 123, 124, 125, 126, 127, 128, 129, 130, 131, 132, 133, 134, 135, 136, 137, 138, 139, 140, 141, 142, 143]</t>
-  </si>
-  <si>
-    <t>[array([-0.03763371, -0.01533471,  0.06554052, -0.01816017], dtype=float32), array([-0.00754409, -0.05458322,  0.2277812 , -0.36241836]), array([ 0.04879627, -0.15231473,  0.32089719, -0.5887683 ]), array([ 0.11397169, -0.27767857,  0.31375488, -0.63332862]), array([ 0.16759438, -0.39312519,  0.2086893 , -0.49480525]), array([ 0.1930193 , -0.46685036,  0.03906408, -0.22816919]), array([ 0.16956871, -0.44830261, -0.26820417,  0.40739083]), array([ 0.09055011, -0.31127879, -0.50323119,  0.93116007]), array([-0.02165415, -0.09380121, -0.58952709,  1.1892161 ]), array([-0.13228272,  0.13968862, -0.48657385,  1.08703787]), array([-0.20542731,  0.31962025, -0.22562708,  0.67289162]), array([-0.21756752,  0.39782756,  0.10766541,  0.09689063]), array([-0.15109606,  0.32490126,  0.54216963, -0.80657469]), array([-0.01068619,  0.09081112,  0.82714324, -1.47439182]), array([ 0.16212513, -0.23279107,  0.85391345, -1.67375883]), array([ 0.3120332 , -0.54339537,  0.60708552, -1.36152952]), array([ 0.39322683, -0.75586146,  0.18779451, -0.73014827]), array([ 0.38412465, -0.82793881, -0.27624305,  0.01454459]), array([ 0.27552572, -0.72135137, -0.78884754,  1.03160865]), array([ 0.08086773, -0.43032213, -1.11647003,  1.81675029]), array([-0.14966877, -0.03109877, -1.12879696,  2.06540623]), array([-0.3455444 ,  0.34863759, -0.7784691 ,  1.63534647]), array([-0.44544803,  0.59424237, -0.19906427,  0.77949316]), array([-0.4218337 ,  0.6519398 ,  0.43007126, -0.20572333]), array([-0.26769146,  0.484052  ,  1.08142007, -1.44055859]), array([-0.00742761,  0.10113176,  1.45927884, -2.28595201]), array([ 0.28490347, -0.37428385,  1.38589424, -2.32532176]), array([ 0.5187101 , -0.77937684,  0.90230152, -1.64619583]), array([ 0.63240836, -1.01433747,  0.21740989, -0.68198512]), array([ 0.58206264, -0.99063291, -0.71189282,  0.91746391]), array([ 0.36681234, -0.68097529, -1.40575041,  2.14420403]), array([ 0.04159544, -0.16374689, -1.76892118,  2.89401986]), array([-0.30147311,  0.40276889, -1.56856425,  2.59619163]), array([-0.56722524,  0.85273137, -1.0345985 ,  1.8196755 ]), array([-0.69032682,  1.084332  , -0.18208987,  0.48616486]), array([-0.62824805,  1.01752684,  0.7944636 , -1.15384725]), array([-0.3800221 ,  0.62483041,  1.65269834, -2.74012714]), array([ 0.00720557, -0.03923131,  2.11746131, -3.70795602]), array([ 0.41500717, -0.75479796,  1.85057805, -3.23807742]), array([ 0.71685207, -1.28565093,  1.12515326, -2.02792903]), array([ 0.8549872 , -1.56314504,  0.24390184, -0.75031589]), array([ 0.8048585 , -1.56201668, -0.73579793,  0.76329224]), array([ 0.56805638, -1.25459393, -1.60503614,  2.31711443]), array([ 0.17813345, -0.63996063, -2.23521717,  3.7586311 ]), array([-0.29836231,  0.20893449, -2.38641402,  4.43746304]), array([-0.70364774,  0.98022879, -1.57930762,  3.12400331]), array([-0.91432405,  1.44400635, -0.51375289,  1.52161562]), array([-0.90851305,  1.59332735,  0.56295467, -0.02604444]), array([-0.68808027,  1.40543405,  1.61277985, -1.86895171]), array([-0.27788057,  0.8399148 ,  2.44208328, -3.76608041]), array([ 0.25551789, -0.0506448 ,  2.74819722, -4.8471174 ]), array([ 0.74961013, -0.94763338,  2.06735784, -3.88349979]), array([ 1.05742564, -1.57379789,  0.98622685, -2.38608363]), array([ 1.14008664, -1.91078837, -0.15952378, -0.99489953]), array([ 0.99057574, -1.94832377, -1.31016288,  0.63147604]), array([ 0.63166569, -1.65028703, -2.22833513,  2.36842343]), array([ 0.12270839, -0.99797152, -2.79850887,  4.119234  ]), array([-0.46398222, -0.02811732, -2.92321638,  5.26900993]), array([-0.95897148,  0.91373686, -1.90756258,  3.92024436]), array([-1.20869784,  1.52282371, -0.58005103,  2.1960462 ]), array([-1.19990017,  1.82421104,  0.66126905,  0.81161141]), array([-0.93740166,  1.79313317,  1.92241774, -1.15150975]), array([-0.45322559,  1.34959204,  2.85717882, -3.30887099]), array([ 0.17809969,  0.47788691,  3.35856892, -5.24913942]), array([ 0.8197509 , -0.59338201,  2.86536694, -5.0334679 ]), array([ 1.27379155, -1.43939879,  1.63381144, -3.40710105]), array([ 1.46889473, -1.97520522,  0.31442469, -1.98628896]), array([ 1.40057572, -2.23695012, -0.9878709 , -0.61568316]), array([ 1.07562901, -2.18859234, -2.22156428,  1.13540513]), array([ 0.53705513, -1.76775967, -3.08437556,  3.102807  ]), array([-0.12422539, -0.94654906, -3.44987324,  5.0387937 ]), array([-0.79578311,  0.14858912, -3.08674835,  5.48691033]), array([-1.2891931 ,  1.09262057, -1.76991547,  3.8252249 ]), array([-1.49711862,  1.68915834, -0.30964532,  2.18174644]), array([-1.42218874,  1.99232632,  1.0528921 ,  0.82373384]), array([-1.07029994,  1.95670561,  2.42006472, -1.23336252]), array([-0.48108348,  1.47619739,  3.39456955, -3.61602526]), array([ 0.25565165,  0.51377139,  3.86910644, -5.8322724 ]), array([ 0.98737983, -0.66681951,  3.23656781, -5.47177611]), array([ 1.50287008, -1.58217897,  1.89657876, -3.7123968 ]), array([ 1.74699912, -2.18536108,  0.54942673, -2.37378651]), array([ 1.72497246, -2.53773813, -0.76264461, -1.13606302]), array([ 1.4332936 , -2.58751049, -2.13705319,  0.67694505]), array([ 0.88988362, -2.2686499 , -3.23213838,  2.56467512]), array([ 0.17150249, -1.51869222, -3.86505529,  4.97828542]), array([-0.61768727, -0.3226962 , -3.90052977,  6.67109763]), array([-1.29555755,  0.9141597 , -2.70343234,  5.29949066]), array([-1.67953696,  1.77907729, -1.14448961,  3.4416358 ]), array([-1.75819454,  2.31727728,  0.3454926 ,  1.95696356]), array([-1.54688735,  2.55423913,  1.75100175,  0.37583435]), array([-1.06218754,  2.43024298,  3.04411664, -1.66278923]), array([-0.36492481,  1.8700886 ,  3.81767417, -3.98104952]), array([ 0.42580062,  0.83374344,  4.02121863, -6.2911993 ]), array([ 1.18697988, -0.49365671,  3.37183406, -6.42300646]), array([ 1.71052458, -1.59770662,  1.8346465 , -4.63029728]), array([ 1.92502936, -2.38514789,  0.32923702, -3.30111548]), array([ 1.85357592, -2.92183813, -1.01022558, -2.05187554]), array([ 1.51888374,  3.12259037, -2.3255732 , -0.3331218 ]), array([ 0.93387974, -3.08068917, -3.48427757,  1.0976473 ]), array([ 0.16260132, -2.73984474, -4.07847858,  2.25698766]), array([-0.62299311, -2.20610804, -3.61352539,  2.97987434]), array([-1.23845033, -1.6013922 , -2.48932963,  2.92298857]), array([-1.61181909, -1.08811027, -1.24066074,  2.11694136]), array([-1.74681543, -0.74415769, -0.11640173,  1.31597038]), array([-1.64814139, -0.58780271,  1.10011949,  0.27627472]), array([-1.29712177, -0.64628845,  2.3871119 , -0.77230175]), array([-0.71541484, -0.83702125,  3.32963263, -0.9269326 ]), array([-0.02658804, -0.9173628 ,  3.37594009,  0.33449779]), array([ 0.55931635, -0.64680655,  2.36591062,  2.36228504]), array([0.89504461, 0.00754331, 1.07101736, 3.93088683]), array([1.02947729, 0.84687545, 0.37996553, 4.27897234]), array([1.07561807, 1.67399454, 0.06263943, 4.0715605 ]), array([ 1.03345725,  2.54141837, -0.52497857,  4.71009379]), array([ 0.84372994, -2.69772621, -1.4735932 ,  5.87746906]), array([ 0.40139256, -1.30857519, -3.03363297,  8.2926628 ]), array([-0.32401848,  0.58785073, -3.66301006,  9.63967126]), array([-0.8672922 ,  2.19897997, -1.73747809,  6.56838254]), array([-1.0652977 , -2.95664453, -0.38527135,  4.89996128]), array([-1.07868487, -2.0438034 ,  0.15379306,  4.38111375]), array([-1.02434587, -1.1639588 ,  0.34595279,  4.55376609]), array([-0.94015899, -0.19829595,  0.59533473,  4.97253244]), array([-0.7025074 ,  0.68210606,  1.95186182,  3.46829369]), array([-0.14400214,  1.09826131,  3.50697667,  0.66476823]), array([ 0.62152558,  0.96596945,  3.91721242, -1.75182899]), array([ 1.34773025,  0.51284072,  3.22551426, -2.50951752]), array([ 1.88826528,  0.04053974,  2.17004116, -2.12338512]), array([ 2.22447585, -0.33526621,  1.22729876, -1.67980707]), array([ 2.39196854, -0.65334749,  0.46943166, -1.54805247]), array([ 2.41381546, -0.96359904, -0.26679248, -1.54755513]), array([ 2.25063911, -1.19828614, -1.40655925, -0.72526733]), array([ 1.84030861, -1.23268775, -2.74891246,  0.54806852]), array([ 1.1388338 , -0.90420297, -4.25636673,  2.88934914]), array([ 0.16873759, -0.07987973, -5.25048174,  4.97129314]), array([-0.84275363,  0.80351309, -4.61384961,  3.34593915]), array([-1.62146815,  1.19674824, -3.11835375,  0.68368982]), array([-2.08941669,  1.14813797, -1.59695352, -0.99156776]), array([-2.26930309,  0.82717361, -0.24549857, -2.13402263]), array([-2.19875582,  0.30490591,  0.94274554, -3.10878202]), array([-1.88945297, -0.43174684,  2.15580806, -4.26008882]), array([-1.33791287, -1.36935384,  3.35601494, -4.97350817]), array([-0.54552923, -2.35913653,  4.53355057, -4.7991364 ]), array([ 0.41654042,  3.00736755,  4.83650208, -4.43136927]), array([ 1.29045036,  2.12451795,  3.77758959, -4.40269553]), array([ 1.92426601,  1.26807537,  2.60872527, -4.09546719])]</t>
-  </si>
-  <si>
-    <t>['[2,0,1]', '[0,1,1]', '[0,2,1]', '[1,1,2]', '[2,2,2]', '[2,1,0]', '[1,0,2]', '[1,1,1]', '[0,0,0]', '[1,2,0]']</t>
-  </si>
-  <si>
-    <t>[6, 7, 8, 9, 10, 11, 18, 19, 20, 21, 22, 23, 29, 30, 31, 32, 33, 34, 41, 42, 43, 44, 45, 46, 47, 54, 55, 56, 57, 58, 59, 60, 67, 68, 69, 70, 71, 72, 73, 81, 82, 83, 84, 85, 86, 87, 95, 96, 97, 98, 99, 100, 101, 102, 110, 111, 112, 113, 114, 115, 116, 117, 131, 132, 133, 134, 135, 136, 137, 138, 139, 140, 141, 142, 157, 158, 159]</t>
-  </si>
-  <si>
-    <t>[0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 1, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 1, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 1, 1, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2]</t>
-  </si>
-  <si>
-    <t>['[-0.03763371 -0.01533471  0.06554052 -0.01816017]', '[-0.00754409 -0.05458322  0.2277812  -0.36241836]', '[ 0.04879627 -0.15231473  0.32089719 -0.5887683 ]', '[ 0.11397169 -0.27767857  0.31375488 -0.63332862]', '[ 0.16759438 -0.39312519  0.2086893  -0.49480525]', '[ 0.1930193  -0.46685036  0.03906408 -0.22816919]', '[ 0.16956871 -0.44830261 -0.26820417  0.40739083]', '[ 0.09055011 -0.31127879 -0.50323119  0.93116007]', '[-0.02165415 -0.09380121 -0.58952709  1.1892161 ]', '[-0.13228272  0.13968862 -0.48657385  1.08703787]', '[-0.20542731  0.31962025 -0.22562708  0.67289162]', '[-0.21756752  0.39782756  0.10766541  0.09689063]', '[-0.15109606  0.32490126  0.54216963 -0.80657469]', '[-0.01068619  0.09081112  0.82714324 -1.47439182]', '[ 0.16212513 -0.23279107  0.85391345 -1.67375883]', '[ 0.3120332  -0.54339537  0.60708552 -1.36152952]', '[ 0.39322683 -0.75586146  0.18779451 -0.73014827]', '[ 0.38412465 -0.82793881 -0.27624305  0.01454459]', '[ 0.27552572 -0.72135137 -0.78884754  1.03160865]', '[ 0.08086773 -0.43032213 -1.11647003  1.81675029]', '[-0.14966877 -0.03109877 -1.12879696  2.06540623]', '[-0.3455444   0.34863759 -0.7784691   1.63534647]', '[-0.44544803  0.59424237 -0.19906427  0.77949316]', '[-0.4218337   0.6519398   0.43007126 -0.20572333]', '[-0.26769146  0.484052    1.08142007 -1.44055859]', '[-0.00742761  0.10113176  1.45927884 -2.28595201]', '[ 0.28490347 -0.37428385  1.38589424 -2.32532176]', '[ 0.5187101  -0.77937684  0.90230152 -1.64619583]', '[ 0.63240836 -1.01433747  0.21740989 -0.68198512]', '[ 0.59278756 -1.01958166 -0.60566507  0.62852481]', '[ 0.39752784 -0.7660208  -1.31595743  1.88179849]', '[ 0.08542661 -0.29020757 -1.73661998  2.76615566]', '[-0.26054486  0.27360101 -1.62803895  2.69265107]', '[-0.53183224  0.72525907 -1.02799868  1.73308445]', '[-0.65747495  0.94866122 -0.21116234  0.48419472]', '[-0.60316944  0.88713812  0.74646124 -1.09703619]', '[-0.3667148   0.51448679  1.5802398  -2.58584684]', '[ 2.25515542e-03 -1.04226788e-01  2.01052042e+00 -3.41515113e+00]', '[ 0.38981745 -0.75816996  1.76540261 -2.93947302]', '[ 0.67971886 -1.23563438  1.09061136 -1.79181237]', '[ 0.81522073 -1.47040276  0.25012952 -0.55613563]', '[ 0.76893557 -1.43299403 -0.70634091  0.93217091]', '[ 0.53890731 -1.09497955 -1.5685075   2.44803386]', '[ 0.15769536 -0.46498696 -2.17507038  3.75054866]', '[-0.28566374  0.31885175 -2.12308403  3.81427092]', '[-0.64333931  0.96714913 -1.38377582  2.55626676]', '[-0.82476188  1.32821982 -0.41497441  1.0541805 ]', '[-0.80769438  1.39053182  0.57925977 -0.43113385]', '[-0.58966747  1.12643161  1.57705339 -2.21920745]', '[-0.19115743  0.50615398  2.34648211 -3.90612928]', '[ 0.30339761 -0.35080814  2.44609663 -4.34908803]', '[ 0.72926902 -1.11787821  1.72849028 -3.18529002]', '[ 0.97784646 -1.61271142  0.7372731  -1.77273591]', '[ 1.02063975 -1.83229792 -0.30765192 -0.42827287]', '[ 0.8520877  -1.75909807 -1.35222299  1.17222519]', '[ 0.49438686 -1.35658722 -2.18080855  2.86380021]', '[ 1.00762334e-03 -6.20843848e-01 -2.67811907e+00  4.39175692e+00]', '[-0.52543841  0.29807699 -2.42518508  4.45563686]', '[-0.91358233  1.05045396 -1.38833549  2.96371659]', '[-1.07068508  1.48053778 -0.17760768  1.35120727]', '[-0.98698022  1.59293246  0.99771813 -0.2363293 ]', '[-0.67458429  1.35277557  2.08591422 -2.1902737 ]', '[-0.17257945  0.7121893   2.86826583 -4.16299452]', '[ 0.42654616 -0.22986762  2.95103072 -4.89035041]', '[ 0.93778312 -1.09635369  2.06289939 -3.60682875]', '[ 1.23512506 -1.66554553  0.89403237 -2.11536181]', '[ 1.2925874  -1.95282627 -0.31874559 -0.76398106]', '[ 1.10434513 -1.94410117 -1.53992148  0.87663865]', '[ 0.69181453 -1.5878337  -2.53506175  2.72222862]', '[ 0.1141862  -0.84811196 -3.17077399  4.62247333]', '[-0.52819058  0.17080839 -3.07026003  5.16081708]', '[-1.04130142  1.05893    -1.96969821  3.56491538]', '[-1.30452454  1.59874429 -0.65598023  1.87444291]', '[-1.30385453  1.81885452  0.65610727  0.32547074]', '[-1.0405206   1.6957045   1.9492216  -1.60077881]', '[-0.53981694  1.15624497  3.01179277 -3.83696118]', '[ 0.1372115   0.17699716  3.62003771 -5.68231063]', '[ 0.81714379 -0.90901082  2.9941466  -4.77727736]', '[ 1.30077933 -1.68444311  1.81783839 -3.01937746]', '[ 1.54044333 -2.14395201  0.57410527 -1.62162767]', '[ 1.53015478 -2.34022436 -0.67386049 -0.3349864 ]', '[ 1.26794035 -2.24754766 -1.92783573  1.30056457]', '[ 0.77398019 -1.79920792 -2.95822207  3.24300749]', '[ 0.10912329 -0.93053956 -3.62675865  5.42116516]', '[-0.62545765  0.26611029 -3.49608951  6.01988262]', '[-1.20465197  1.28709304 -2.21592237  4.06698629]', '[-1.50797598  1.91807846 -0.82066615  2.31676317]', '[-1.53477864  2.2293726   0.54577611  0.80013611]', '[-1.2877879   2.20842304  1.90129391 -1.04971139]', '[-0.78963194  1.78691254  3.02687444 -3.23448346]', '[-0.10030915  0.88843882  3.80956796 -5.74461357]', '[ 0.6800303  -0.39674343  3.7435005  -6.50465385]', '[ 1.30715153 -1.50997221  2.45867409 -4.5409428 ]', '[ 1.66295011 -2.25180565  1.10659453 -2.9676307 ]', '[ 1.75378095 -2.71564871 -0.18565107 -1.68161197]', '[ 1.5813519  -2.88137073 -1.52983951  0.04045167]', '[ 1.1519438  -2.7111456  -2.73434768  1.6862411 ]', '[ 0.51469557 -2.19454948 -3.53385774  3.51577218]', '[-0.21605975 -1.29637768 -3.69530472  5.44381948]', '[-0.93347479 -0.07890334 -3.33155425  6.34278847]', '[-1.46815164  1.04914056 -1.90369944  4.72496493]', '[-1.68504663  1.8186261  -0.26686772  3.02286773]', '[-1.57790214  2.26289729  1.32157282  1.3925168 ]', '[-1.16230252  2.33628647  2.78098167 -0.70872357]', '[-0.49937378  1.96104263  3.73305796 -3.07862305]', '[ 0.28168801  1.10328838  3.98778248 -5.43912807]', '[ 1.05641581 -0.12139406  3.58807581 -6.33965149]', '[ 1.64197964 -1.24799698  2.19153353 -4.79346573]', '[ 1.93110596 -2.06554328  0.70796954 -3.45572032]', '[ 1.9298668  -2.64055422 -0.70059025 -2.28138   ]', '[ 1.64798507 -2.92647169 -2.10001467 -0.54933263]', '[ 1.10113438 -2.87141254 -3.33487859  1.1106115 ]', '[ 0.34697668 -2.48153264 -4.06563526  2.78224148]', '[-0.45449675 -1.77188397 -3.80453306  4.23624619]', '[-1.14036848 -0.83961199 -3.00985396  4.9119112 ]', '[-1.63827553  0.10748742 -1.91032936  4.37331902]', '[-1.88581424  0.8697594  -0.53732323  3.22693025]', '[-1.84250576  1.39232548  1.00128781  1.94585667]', '[-1.46792407  1.58397786  2.73695626 -0.1591014 ]', '[-0.76574103  1.27166851  4.20293413 -3.0762577 ]', '[ 0.16720186  0.35309345  4.95605261 -5.8105889 ]', '[ 1.11001304 -0.78239843  4.24571007 -4.96871473]', '[ 1.83243961 -1.56549641  2.99112398 -2.9780063 ]', '[ 2.32227254 -2.04212274  1.95471592 -1.9392754 ]', '[ 2.63327895 -2.38572334  1.20117266 -1.57380137]', '[ 2.81833741 -2.69021329  0.68507069 -1.49642129]', '[ 2.91927563 -2.98722699  0.35267656 -1.47057386]', '[ 2.96921892  3.00967473  0.1693663  -1.37645824]', '[ 2.99422643  2.75310207  0.09508466 -1.17065374]', '[ 3.01106998  2.54879278  0.07969731 -0.85696437]', '[ 3.02756577  2.41548615  0.08795807 -0.46735169]', '[ 3.03377925  2.40510353 -0.02459955  0.36300865]', '[ 3.01827787  2.5577791  -0.13006699  1.14990759]', '[ 2.9864113   2.83764122 -0.1997427   1.62844096]', '[ 2.93073389 -3.08293415 -0.38523736  1.97693621]', '[ 2.81830541 -2.66191764 -0.77868654  2.22498429]', '[ 2.60316735 -2.19099131 -1.41413499  2.51324944]', '[ 2.23515129 -1.63261367 -2.31658838  3.17520518]', '[ 1.65288255 -0.8611259  -3.56832895  4.70760047]', '[ 0.8015193   0.26241492 -4.82676116  6.16024713]', '[-0.19149596  1.34193963 -4.91208833  4.16421567]', '[-1.0982578   1.85892141 -3.98458959  1.00780127]', '[-1.72830921  1.78285216 -2.23609115 -1.62970826]', '[-1.97371022  1.23925332 -0.22988789 -3.70518026]', '[-1.83583303  0.3201441   1.54885412 -5.45056978]', '[-1.395785   -0.885842    2.72841253 -6.36930281]', '[-0.77045381 -2.15027896  3.53177566 -6.22290519]', '[ 4.95699164e-03  2.88670206e+00  4.07794122e+00 -6.38852897e+00]', '[ 0.79647085  1.50207057  3.81763177 -7.63972274]', '[ 1.53948774 -0.17230282  3.41042481 -8.62058517]', '[ 2.02871491 -1.70080075  1.3321221  -6.53848522]', '[ 2.07921905 -2.84284003 -0.69206813 -4.97970055]', '[ 1.8356673   2.56044989 -1.55110255 -3.92136947]', '[ 1.50268517  1.81961282 -1.71693449 -3.64940056]', '[ 1.1743514   1.0217513  -1.50659192 -4.51840734]', '[ 0.89517673 -0.00957279 -1.49166253 -5.48667645]', '[ 0.43439719 -0.91862526 -3.29640123 -3.12260905]', '[-0.39598026 -1.16901903 -4.71684721  0.45931427]', '[-1.32700473 -0.85921825 -4.37367202  2.2629972 ]', '[-2.10096419 -0.39503362 -3.34549019  2.17212666]']</t>
-  </si>
-  <si>
-    <t>[0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50, 51, 52, 53, 54, 55, 56, 57, 58, 59, 60, 61, 62, 63, 64, 65, 66, 67, 68, 69, 70, 71, 72, 73, 74, 75, 76, 77, 78, 79, 80, 81, 82, 83, 84, 85, 86, 87, 88, 89, 90, 91, 92, 93, 94, 95, 96, 97, 98, 99, 100, 101, 102, 103, 104, 105, 106, 107, 108, 109, 110, 111, 112, 113, 114, 115, 116, 117, 118, 119, 120, 121, 122, 123, 124, 125, 126, 127, 128, 129, 130, 131, 132, 133, 134, 135, 136, 137, 138, 139, 140, 141, 142, 143, 144, 145, 146, 147, 148, 149, 150, 151, 152, 153, 154, 155, 156, 157, 158, 159]</t>
-  </si>
-  <si>
-    <t>[array([-0.03763371, -0.01533471,  0.06554052, -0.01816017], dtype=float32), array([-0.00754409, -0.05458322,  0.2277812 , -0.36241836]), array([ 0.04879627, -0.15231473,  0.32089719, -0.5887683 ]), array([ 0.11397169, -0.27767857,  0.31375488, -0.63332862]), array([ 0.16759438, -0.39312519,  0.2086893 , -0.49480525]), array([ 0.1930193 , -0.46685036,  0.03906408, -0.22816919]), array([ 0.16956871, -0.44830261, -0.26820417,  0.40739083]), array([ 0.09055011, -0.31127879, -0.50323119,  0.93116007]), array([-0.02165415, -0.09380121, -0.58952709,  1.1892161 ]), array([-0.13228272,  0.13968862, -0.48657385,  1.08703787]), array([-0.20542731,  0.31962025, -0.22562708,  0.67289162]), array([-0.21756752,  0.39782756,  0.10766541,  0.09689063]), array([-0.15109606,  0.32490126,  0.54216963, -0.80657469]), array([-0.01068619,  0.09081112,  0.82714324, -1.47439182]), array([ 0.16212513, -0.23279107,  0.85391345, -1.67375883]), array([ 0.3120332 , -0.54339537,  0.60708552, -1.36152952]), array([ 0.39322683, -0.75586146,  0.18779451, -0.73014827]), array([ 0.38412465, -0.82793881, -0.27624305,  0.01454459]), array([ 0.27552572, -0.72135137, -0.78884754,  1.03160865]), array([ 0.08086773, -0.43032213, -1.11647003,  1.81675029]), array([-0.14966877, -0.03109877, -1.12879696,  2.06540623]), array([-0.3455444 ,  0.34863759, -0.7784691 ,  1.63534647]), array([-0.44544803,  0.59424237, -0.19906427,  0.77949316]), array([-0.4218337 ,  0.6519398 ,  0.43007126, -0.20572333]), array([-0.26769146,  0.484052  ,  1.08142007, -1.44055859]), array([-0.00742761,  0.10113176,  1.45927884, -2.28595201]), array([ 0.28490347, -0.37428385,  1.38589424, -2.32532176]), array([ 0.5187101 , -0.77937684,  0.90230152, -1.64619583]), array([ 0.63240836, -1.01433747,  0.21740989, -0.68198512]), array([ 0.59278756, -1.01958166, -0.60566507,  0.62852481]), array([ 0.39752784, -0.7660208 , -1.31595743,  1.88179849]), array([ 0.08542661, -0.29020757, -1.73661998,  2.76615566]), array([-0.26054486,  0.27360101, -1.62803895,  2.69265107]), array([-0.53183224,  0.72525907, -1.02799868,  1.73308445]), array([-0.65747495,  0.94866122, -0.21116234,  0.48419472]), array([-0.60316944,  0.88713812,  0.74646124, -1.09703619]), array([-0.3667148 ,  0.51448679,  1.5802398 , -2.58584684]), array([ 2.25515542e-03, -1.04226788e-01,  2.01052042e+00, -3.41515113e+00]), array([ 0.38981745, -0.75816996,  1.76540261, -2.93947302]), array([ 0.67971886, -1.23563438,  1.09061136, -1.79181237]), array([ 0.81522073, -1.47040276,  0.25012952, -0.55613563]), array([ 0.76893557, -1.43299403, -0.70634091,  0.93217091]), array([ 0.53890731, -1.09497955, -1.5685075 ,  2.44803386]), array([ 0.15769536, -0.46498696, -2.17507038,  3.75054866]), array([-0.28566374,  0.31885175, -2.12308403,  3.81427092]), array([-0.64333931,  0.96714913, -1.38377582,  2.55626676]), array([-0.82476188,  1.32821982, -0.41497441,  1.0541805 ]), array([-0.80769438,  1.39053182,  0.57925977, -0.43113385]), array([-0.58966747,  1.12643161,  1.57705339, -2.21920745]), array([-0.19115743,  0.50615398,  2.34648211, -3.90612928]), array([ 0.30339761, -0.35080814,  2.44609663, -4.34908803]), array([ 0.72926902, -1.11787821,  1.72849028, -3.18529002]), array([ 0.97784646, -1.61271142,  0.7372731 , -1.77273591]), array([ 1.02063975, -1.83229792, -0.30765192, -0.42827287]), array([ 0.8520877 , -1.75909807, -1.35222299,  1.17222519]), array([ 0.49438686, -1.35658722, -2.18080855,  2.86380021]), array([ 1.00762334e-03, -6.20843848e-01, -2.67811907e+00,  4.39175692e+00]), array([-0.52543841,  0.29807699, -2.42518508,  4.45563686]), array([-0.91358233,  1.05045396, -1.38833549,  2.96371659]), array([-1.07068508,  1.48053778, -0.17760768,  1.35120727]), array([-0.98698022,  1.59293246,  0.99771813, -0.2363293 ]), array([-0.67458429,  1.35277557,  2.08591422, -2.1902737 ]), array([-0.17257945,  0.7121893 ,  2.86826583, -4.16299452]), array([ 0.42654616, -0.22986762,  2.95103072, -4.89035041]), array([ 0.93778312, -1.09635369,  2.06289939, -3.60682875]), array([ 1.23512506, -1.66554553,  0.89403237, -2.11536181]), array([ 1.2925874 , -1.95282627, -0.31874559, -0.76398106]), array([ 1.10434513, -1.94410117, -1.53992148,  0.87663865]), array([ 0.69181453, -1.5878337 , -2.53506175,  2.72222862]), array([ 0.1141862 , -0.84811196, -3.17077399,  4.62247333]), array([-0.52819058,  0.17080839, -3.07026003,  5.16081708]), array([-1.04130142,  1.05893   , -1.96969821,  3.56491538]), array([-1.30452454,  1.59874429, -0.65598023,  1.87444291]), array([-1.30385453,  1.81885452,  0.65610727,  0.32547074]), array([-1.0405206 ,  1.6957045 ,  1.9492216 , -1.60077881]), array([-0.53981694,  1.15624497,  3.01179277, -3.83696118]), array([ 0.1372115 ,  0.17699716,  3.62003771, -5.68231063]), array([ 0.81714379, -0.90901082,  2.9941466 , -4.77727736]), array([ 1.30077933, -1.68444311,  1.81783839, -3.01937746]), array([ 1.54044333, -2.14395201,  0.57410527, -1.62162767]), array([ 1.53015478, -2.34022436, -0.67386049, -0.3349864 ]), array([ 1.26794035, -2.24754766, -1.92783573,  1.30056457]), array([ 0.77398019, -1.79920792, -2.95822207,  3.24300749]), array([ 0.10912329, -0.93053956, -3.62675865,  5.42116516]), array([-0.62545765,  0.26611029, -3.49608951,  6.01988262]), array([-1.20465197,  1.28709304, -2.21592237,  4.06698629]), array([-1.50797598,  1.91807846, -0.82066615,  2.31676317]), array([-1.53477864,  2.2293726 ,  0.54577611,  0.80013611]), array([-1.2877879 ,  2.20842304,  1.90129391, -1.04971139]), array([-0.78963194,  1.78691254,  3.02687444, -3.23448346]), array([-0.10030915,  0.88843882,  3.80956796, -5.74461357]), array([ 0.6800303 , -0.39674343,  3.7435005 , -6.50465385]), array([ 1.30715153, -1.50997221,  2.45867409, -4.5409428 ]), array([ 1.66295011, -2.25180565,  1.10659453, -2.9676307 ]), array([ 1.75378095, -2.71564871, -0.18565107, -1.68161197]), array([ 1.5813519 , -2.88137073, -1.52983951,  0.04045167]), array([ 1.1519438 , -2.7111456 , -2.73434768,  1.6862411 ]), array([ 0.51469557, -2.19454948, -3.53385774,  3.51577218]), array([-0.21605975, -1.29637768, -3.69530472,  5.44381948]), array([-0.93347479, -0.07890334, -3.33155425,  6.34278847]), array([-1.46815164,  1.04914056, -1.90369944,  4.72496493]), array([-1.68504663,  1.8186261 , -0.26686772,  3.02286773]), array([-1.57790214,  2.26289729,  1.32157282,  1.3925168 ]), array([-1.16230252,  2.33628647,  2.78098167, -0.70872357]), array([-0.49937378,  1.96104263,  3.73305796, -3.07862305]), array([ 0.28168801,  1.10328838,  3.98778248, -5.43912807]), array([ 1.05641581, -0.12139406,  3.58807581, -6.33965149]), array([ 1.64197964, -1.24799698,  2.19153353, -4.79346573]), array([ 1.93110596, -2.06554328,  0.70796954, -3.45572032]), array([ 1.9298668 , -2.64055422, -0.70059025, -2.28138   ]), array([ 1.64798507, -2.92647169, -2.10001467, -0.54933263]), array([ 1.10113438, -2.87141254, -3.33487859,  1.1106115 ]), array([ 0.34697668, -2.48153264, -4.06563526,  2.78224148]), array([-0.45449675, -1.77188397, -3.80453306,  4.23624619]), array([-1.14036848, -0.83961199, -3.00985396,  4.9119112 ]), array([-1.63827553,  0.10748742, -1.91032936,  4.37331902]), array([-1.88581424,  0.8697594 , -0.53732323,  3.22693025]), array([-1.84250576,  1.39232548,  1.00128781,  1.94585667]), array([-1.46792407,  1.58397786,  2.73695626, -0.1591014 ]), array([-0.76574103,  1.27166851,  4.20293413, -3.0762577 ]), array([ 0.16720186,  0.35309345,  4.95605261, -5.8105889 ]), array([ 1.11001304, -0.78239843,  4.24571007, -4.96871473]), array([ 1.83243961, -1.56549641,  2.99112398, -2.9780063 ]), array([ 2.32227254, -2.04212274,  1.95471592, -1.9392754 ]), array([ 2.63327895, -2.38572334,  1.20117266, -1.57380137]), array([ 2.81833741, -2.69021329,  0.68507069, -1.49642129]), array([ 2.91927563, -2.98722699,  0.35267656, -1.47057386]), array([ 2.96921892,  3.00967473,  0.1693663 , -1.37645824]), array([ 2.99422643,  2.75310207,  0.09508466, -1.17065374]), array([ 3.01106998,  2.54879278,  0.07969731, -0.85696437]), array([ 3.02756577,  2.41548615,  0.08795807, -0.46735169]), array([ 3.03377925,  2.40510353, -0.02459955,  0.36300865]), array([ 3.01827787,  2.5577791 , -0.13006699,  1.14990759]), array([ 2.9864113 ,  2.83764122, -0.1997427 ,  1.62844096]), array([ 2.93073389, -3.08293415, -0.38523736,  1.97693621]), array([ 2.81830541, -2.66191764, -0.77868654,  2.22498429]), array([ 2.60316735, -2.19099131, -1.41413499,  2.51324944]), array([ 2.23515129, -1.63261367, -2.31658838,  3.17520518]), array([ 1.65288255, -0.8611259 , -3.56832895,  4.70760047]), array([ 0.8015193 ,  0.26241492, -4.82676116,  6.16024713]), array([-0.19149596,  1.34193963, -4.91208833,  4.16421567]), array([-1.0982578 ,  1.85892141, -3.98458959,  1.00780127]), array([-1.72830921,  1.78285216, -2.23609115, -1.62970826]), array([-1.97371022,  1.23925332, -0.22988789, -3.70518026]), array([-1.83583303,  0.3201441 ,  1.54885412, -5.45056978]), array([-1.395785  , -0.885842  ,  2.72841253, -6.36930281]), array([-0.77045381, -2.15027896,  3.53177566, -6.22290519]), array([ 4.95699164e-03,  2.88670206e+00,  4.07794122e+00, -6.38852897e+00]), array([ 0.79647085,  1.50207057,  3.81763177, -7.63972274]), array([ 1.53948774, -0.17230282,  3.41042481, -8.62058517]), array([ 2.02871491, -1.70080075,  1.3321221 , -6.53848522]), array([ 2.07921905, -2.84284003, -0.69206813, -4.97970055]), array([ 1.8356673 ,  2.56044989, -1.55110255, -3.92136947]), array([ 1.50268517,  1.81961282, -1.71693449, -3.64940056]), array([ 1.1743514 ,  1.0217513 , -1.50659192, -4.51840734]), array([ 0.89517673, -0.00957279, -1.49166253, -5.48667645]), array([ 0.43439719, -0.91862526, -3.29640123, -3.12260905]), array([-0.39598026, -1.16901903, -4.71684721,  0.45931427]), array([-1.32700473, -0.85921825, -4.37367202,  2.2629972 ]), array([-2.10096419, -0.39503362, -3.34549019,  2.17212666])]</t>
-  </si>
-  <si>
-    <t>['[1,0,2]', '[0,0,0]', '[0,1,1]', '[1,1,1]', '[2,0,1]', '[2,2,2]', '[0,2,1]', '[1,1,2]', '[1,2,0]', '[2,1,0]']</t>
-  </si>
-  <si>
-    <t>[1,0,2]</t>
-  </si>
-  <si>
-    <t>[27, 38, 39, 51, 73, 75]</t>
-  </si>
-  <si>
-    <t>[0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 1, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 1, 2, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 1, 1, 1, 1, 1, 1, 2, 2, 2, 2, 2, 2, 2, 2, 2]</t>
-  </si>
-  <si>
-    <t>['[-0.03763371 -0.01533471  0.06554052 -0.01816017]', '[-0.00754409 -0.05458322  0.2277812  -0.36241836]', '[ 0.04879627 -0.15231473  0.32089719 -0.5887683 ]', '[ 0.11397169 -0.27767857  0.31375488 -0.63332862]', '[ 0.16759438 -0.39312519  0.2086893  -0.49480525]', '[ 0.1930193  -0.46685036  0.03906408 -0.22816919]', '[ 0.15689524 -0.41528579 -0.3922057   0.73207416]', '[ 0.04309269 -0.18588535 -0.71796191  1.51055937]', '[-0.1147829   0.15904975 -0.81547211  1.84906375]', '[-0.26363568  0.51494657 -0.63159042  1.62703318]', '[-0.35418658  0.78351571 -0.2539271   1.01663306]', '[-0.36122763  0.91144819  0.18313112  0.25239067]', '[-0.26190848  0.82452699  0.79137833 -1.10754289]', '[-0.05546354  0.48017359  1.23429726 -2.2781243 ]', '[ 0.20909957 -0.04617758  1.33805656 -2.84269804]', '[ 0.4464647  -0.59077472  0.966733   -2.46825376]', '[ 0.57603342 -0.99637145  0.30429255 -1.53991243]', '[ 0.56516121 -1.19760706 -0.40558213 -0.46475241]', '[ 0.40174223 -1.12742398 -1.19611308  1.15628906]', '[ 0.10260264 -0.74319691 -1.74734194  2.63891225]', '[-0.2709061  -0.11181674 -1.89757953  3.50473183]', '[-0.61163409  0.5691586  -1.41246159  3.11532725]', '[-0.80839131  1.08597374 -0.52123819  2.00121872]', '[-0.81524764  1.36167033  0.4476147   0.74644332]', '[-0.61908766  1.32941944  1.47593314 -1.07166988]', '[-0.24402049  0.93362994  2.21913634 -2.8599763 ]', '[ 0.2394916   0.21984858  2.51157673 -4.08763472]', '[ 0.69117549 -0.55210898  1.88433378 -3.39149782]', '[ 0.97378379 -1.11552571  0.90102326 -2.1956991 ]', '[ 1.04419898 -1.42674025 -0.20054365 -0.91250673]', '[ 0.87935589 -1.4251424  -1.42147869  0.94525911]', '[ 0.49056418 -1.03896838 -2.41895626  2.92595422]', '[-0.06157144 -0.27409082 -2.99344712  4.53697084]', '[-0.63932259  0.63460465 -2.62042342  4.20877364]', '[-1.06601557  1.33235717 -1.59831797  2.73355774]', '[-1.26992966  1.73769947 -0.43061853  1.34631183]', '[-1.23719918  1.87514574  0.7521603   0.02017078]', '[-0.9602765   1.68970035  1.98736844 -1.91591938]', '[-0.46710179  1.11484621  2.89400545 -3.85056917]', '[ 0.16670215  0.17965745  3.30449621 -5.22537317]', '[ 0.78528785 -0.82611467  2.7120754  -4.47596769]', '[ 1.21613184 -1.55671397  1.56592881 -2.84540498]', '[ 1.40663091 -1.98324135  0.33342507 -1.45204147]', '[ 1.34259995 -2.11920378 -0.96375294  0.10341853]', '[ 1.02197929 -1.90777777 -2.20939662  2.05912968]', '[ 0.47661807 -1.27096433 -3.19864402  4.36438853]', '[-0.23319436 -0.17332372 -3.7554337   6.31038521]', '[-0.9240712   1.01680905 -2.96035101  5.17185051]', '[-1.38912881  1.8622755  -1.6789453   3.35541314]', '[-1.59502026  2.38884253 -0.38199468  1.95090149]', '[-1.54420905  2.64672507  0.88204683  0.6190267 ]', '[-1.24092265  2.60920147  2.127103   -1.01751026]', '[-0.70612578  2.20764344  3.14368537 -3.03838617]', '[-0.02058128  1.37644623  3.64282007 -5.30161188]', '[ 0.72662365  0.11729849  3.68021032 -6.91787913]', '[ 1.35018457 -1.1505516   2.39440044 -5.43678072]', '[ 1.66934416 -2.06126879  0.80287593 -3.75524271]', '[ 1.67830176 -2.6710728  -0.68430683 -2.35051585]', '[ 1.4029606  -2.9791265  -2.03839052 -0.73051129]', '[ 0.86999203 -2.95012239 -3.23621143  0.98781982]', '[ 0.14886518 -2.60077393 -3.82606394  2.45770138]', '[-0.59050056 -1.99230144 -3.42555643  3.53824237]', '[-1.18772007 -1.23104698 -2.51705411  3.95657208]', '[-1.59431307 -0.45199684 -1.54119637  3.75116786]', '[-1.79785704  0.24637251 -0.46917077  3.19285987]', '[-1.76680173  0.80743149  0.83027325  2.344908  ]', '[-1.44462744  1.13951376  2.42502012  0.8308947 ]', '[-0.7832569   1.02392276  4.10517576 -2.08390577]', '[ 0.14118719  0.31783249  4.93740896 -4.66688146]', '[ 1.08623645 -0.60535333  4.29319363 -4.05238732]', '[ 1.8179651  -1.2233258   3.01939547 -2.200789  ]', '[ 2.30942866 -1.55006742  1.95018819 -1.22921241]', '[ 2.62063665 -1.76797434  1.21392598 -1.05112238]', '[ 2.81114346 -1.99794394  0.72103989 -1.29180927]', '[ 2.90888888 -2.2708514   0.26759059 -1.44170081]', '[ 2.92597964 -2.58978714 -0.09795686 -1.71791065]', '[ 2.86353166 -2.92192531 -0.52518014 -1.55690468]', '[ 2.71473714  3.09211119 -0.97471377 -1.07777785]', '[ 2.46380183  2.95379181 -1.57432624 -0.24702041]', '[ 2.05809226  3.03530866 -2.5431108   1.11687906]', '[ 1.4263361  -2.85904205 -3.786426    2.85361015]', '[ 0.56609229 -2.05879239 -4.70655843  5.30893371]', '[-0.42264311 -0.67720764 -5.1361755   8.44042765]', '[-1.38140194  1.00435923 -4.14022978  7.54038583]', '[-2.04572591  2.27299592 -2.5781627   5.39296602]', '[-2.44716726 -3.04467068 -1.54701437  4.36688224]', '[-2.70840208 -2.24501447 -1.15412138  3.65590772]', '[-2.92838665 -1.57538964 -1.07397005  3.06168284]']</t>
-  </si>
-  <si>
-    <t>[0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50, 51, 52, 53, 54, 55, 56, 57, 58, 59, 60, 61, 62, 63, 64, 65, 66, 67, 68, 69, 70, 71, 72, 73, 74, 75, 76, 77, 78, 79, 80, 81, 82, 83, 84, 85, 86, 87]</t>
-  </si>
-  <si>
-    <t>[array([-0.03763371, -0.01533471,  0.06554052, -0.01816017], dtype=float32), array([-0.00754409, -0.05458322,  0.2277812 , -0.36241836]), array([ 0.04879627, -0.15231473,  0.32089719, -0.5887683 ]), array([ 0.11397169, -0.27767857,  0.31375488, -0.63332862]), array([ 0.16759438, -0.39312519,  0.2086893 , -0.49480525]), array([ 0.1930193 , -0.46685036,  0.03906408, -0.22816919]), array([ 0.15689524, -0.41528579, -0.3922057 ,  0.73207416]), array([ 0.04309269, -0.18588535, -0.71796191,  1.51055937]), array([-0.1147829 ,  0.15904975, -0.81547211,  1.84906375]), array([-0.26363568,  0.51494657, -0.63159042,  1.62703318]), array([-0.35418658,  0.78351571, -0.2539271 ,  1.01663306]), array([-0.36122763,  0.91144819,  0.18313112,  0.25239067]), array([-0.26190848,  0.82452699,  0.79137833, -1.10754289]), array([-0.05546354,  0.48017359,  1.23429726, -2.2781243 ]), array([ 0.20909957, -0.04617758,  1.33805656, -2.84269804]), array([ 0.4464647 , -0.59077472,  0.966733  , -2.46825376]), array([ 0.57603342, -0.99637145,  0.30429255, -1.53991243]), array([ 0.56516121, -1.19760706, -0.40558213, -0.46475241]), array([ 0.40174223, -1.12742398, -1.19611308,  1.15628906]), array([ 0.10260264, -0.74319691, -1.74734194,  2.63891225]), array([-0.2709061 , -0.11181674, -1.89757953,  3.50473183]), array([-0.61163409,  0.5691586 , -1.41246159,  3.11532725]), array([-0.80839131,  1.08597374, -0.52123819,  2.00121872]), array([-0.81524764,  1.36167033,  0.4476147 ,  0.74644332]), array([-0.61908766,  1.32941944,  1.47593314, -1.07166988]), array([-0.24402049,  0.93362994,  2.21913634, -2.8599763 ]), array([ 0.2394916 ,  0.21984858,  2.51157673, -4.08763472]), array([ 0.69117549, -0.55210898,  1.88433378, -3.39149782]), array([ 0.97378379, -1.11552571,  0.90102326, -2.1956991 ]), array([ 1.04419898, -1.42674025, -0.20054365, -0.91250673]), array([ 0.87935589, -1.4251424 , -1.42147869,  0.94525911]), array([ 0.49056418, -1.03896838, -2.41895626,  2.92595422]), array([-0.06157144, -0.27409082, -2.99344712,  4.53697084]), array([-0.63932259,  0.63460465, -2.62042342,  4.20877364]), array([-1.06601557,  1.33235717, -1.59831797,  2.73355774]), array([-1.26992966,  1.73769947, -0.43061853,  1.34631183]), array([-1.23719918,  1.87514574,  0.7521603 ,  0.02017078]), array([-0.9602765 ,  1.68970035,  1.98736844, -1.91591938]), array([-0.46710179,  1.11484621,  2.89400545, -3.85056917]), array([ 0.16670215,  0.17965745,  3.30449621, -5.22537317]), array([ 0.78528785, -0.82611467,  2.7120754 , -4.47596769]), array([ 1.21613184, -1.55671397,  1.56592881, -2.84540498]), array([ 1.40663091, -1.98324135,  0.33342507, -1.45204147]), array([ 1.34259995, -2.11920378, -0.96375294,  0.10341853]), array([ 1.02197929, -1.90777777, -2.20939662,  2.05912968]), array([ 0.47661807, -1.27096433, -3.19864402,  4.36438853]), array([-0.23319436, -0.17332372, -3.7554337 ,  6.31038521]), array([-0.9240712 ,  1.01680905, -2.96035101,  5.17185051]), array([-1.38912881,  1.8622755 , -1.6789453 ,  3.35541314]), array([-1.59502026,  2.38884253, -0.38199468,  1.95090149]), array([-1.54420905,  2.64672507,  0.88204683,  0.6190267 ]), array([-1.24092265,  2.60920147,  2.127103  , -1.01751026]), array([-0.70612578,  2.20764344,  3.14368537, -3.03838617]), array([-0.02058128,  1.37644623,  3.64282007, -5.30161188]), array([ 0.72662365,  0.11729849,  3.68021032, -6.91787913]), array([ 1.35018457, -1.1505516 ,  2.39440044, -5.43678072]), array([ 1.66934416, -2.06126879,  0.80287593, -3.75524271]), array([ 1.67830176, -2.6710728 , -0.68430683, -2.35051585]), array([ 1.4029606 , -2.9791265 , -2.03839052, -0.73051129]), array([ 0.86999203, -2.95012239, -3.23621143,  0.98781982]), array([ 0.14886518, -2.60077393, -3.82606394,  2.45770138]), array([-0.59050056, -1.99230144, -3.42555643,  3.53824237]), array([-1.18772007, -1.23104698, -2.51705411,  3.95657208]), array([-1.59431307, -0.45199684, -1.54119637,  3.75116786]), array([-1.79785704,  0.24637251, -0.46917077,  3.19285987]), array([-1.76680173,  0.80743149,  0.83027325,  2.344908  ]), array([-1.44462744,  1.13951376,  2.42502012,  0.8308947 ]), array([-0.7832569 ,  1.02392276,  4.10517576, -2.08390577]), array([ 0.14118719,  0.31783249,  4.93740896, -4.66688146]), array([ 1.08623645, -0.60535333,  4.29319363, -4.05238732]), array([ 1.8179651 , -1.2233258 ,  3.01939547, -2.200789  ]), array([ 2.30942866, -1.55006742,  1.95018819, -1.22921241]), array([ 2.62063665, -1.76797434,  1.21392598, -1.05112238]), array([ 2.81114346, -1.99794394,  0.72103989, -1.29180927]), array([ 2.90888888, -2.2708514 ,  0.26759059, -1.44170081]), array([ 2.92597964, -2.58978714, -0.09795686, -1.71791065]), array([ 2.86353166, -2.92192531, -0.52518014, -1.55690468]), array([ 2.71473714,  3.09211119, -0.97471377, -1.07777785]), array([ 2.46380183,  2.95379181, -1.57432624, -0.24702041]), array([ 2.05809226,  3.03530866, -2.5431108 ,  1.11687906]), array([ 1.4263361 , -2.85904205, -3.786426  ,  2.85361015]), array([ 0.56609229, -2.05879239, -4.70655843,  5.30893371]), array([-0.42264311, -0.67720764, -5.1361755 ,  8.44042765]), array([-1.38140194,  1.00435923, -4.14022978,  7.54038583]), array([-2.04572591,  2.27299592, -2.5781627 ,  5.39296602]), array([-2.44716726, -3.04467068, -1.54701437,  4.36688224]), array([-2.70840208, -2.24501447, -1.15412138,  3.65590772]), array([-2.92838665, -1.57538964, -1.07397005,  3.06168284])]</t>
-  </si>
-  <si>
-    <t>['[0,2,1]', '[2,0,1]', '[1,1,1]', '[1,0,2]', '[2,1,0]', '[2,2,2]', '[0,0,0]', '[1,1,2]', '[1,2,0]', '[0,1,1]']</t>
-  </si>
-  <si>
-    <t>[4, 23, 28, 37, 40, 42, 56, 57, 66, 67, 68, 72, 82, 84, 88, 91, 104, 107, 109, 112, 113, 117, 118, 121, 122, 124, 125, 129]</t>
-  </si>
-  <si>
-    <t>[0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 1, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 1, 2, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 1, 1, 2, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 0, 0, 1, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
-  </si>
-  <si>
-    <t>['[-0.03763371 -0.01533471  0.06554052 -0.01816017]', '[-0.00754409 -0.05458322  0.2277812  -0.36241836]', '[ 0.04879627 -0.15231473  0.32089719 -0.5887683 ]', '[ 0.11397169 -0.27767857  0.31375488 -0.63332862]', '[ 0.15469752 -0.35964331  0.08386034 -0.16862923]', '[ 0.1328986  -0.30852175 -0.29631136  0.66902399]', '[ 0.04193434 -0.10322104 -0.58935853  1.33680279]', '[-0.0895624   0.19970356 -0.68735485  1.61532039]', '[-0.21671213  0.51005343 -0.54911684  1.41746405]', '[-0.29775335  0.74363137 -0.24311842  0.88008455]', '[-0.3099396   0.85242745  0.12252104  0.19753864]', '[-0.22805628  0.7615075   0.68124181 -1.09272869]', '[-0.04681936  0.42734149  1.09559275 -2.19100247]', '[ 0.1890354  -0.07558709  1.19523955 -2.70411161]', '[ 0.40083096 -0.59317051  0.86004853 -2.34670125]', '[ 0.51503476 -0.97919856  0.25973082 -1.46695327]', '[ 0.50222831 -1.17086038 -0.37993929 -0.44268219]', '[ 0.35054191 -1.10163677 -1.10615567  1.12233487]', '[ 0.07460813 -0.73093941 -1.60864212  2.53748392]', '[-0.26861178 -0.12448947 -1.74059878  3.36983165]', '[-0.58016521  0.5340796  -1.28298101  3.03481604]', '[-0.75500166  1.04058322 -0.43201198  1.9731889 ]', '[-0.74847174  1.31351942  0.49031062  0.74540217]', '[-0.55852521  1.3101156   1.37034616 -0.77637724]', '[-0.21046837  0.98011731  2.05346592 -2.49410136]', '[ 0.23563297  0.3420203   2.31862639 -3.73514795]', '[ 0.66871365 -0.41722741  1.89138947 -3.61279591]', '[ 0.95446017 -1.03363271  0.91630455 -2.47903128]', '[ 1.01664259 -1.37353874 -0.29268251 -0.92026149]', '[ 0.83425561 -1.37227369 -1.50107115  0.94945177]', '[ 0.43300511 -0.98571852 -2.4585572   2.91542003]', '[-0.11976547 -0.2323834  -2.9544336   4.41640071]', '[-0.68221417  0.64186726 -2.51657809  4.01073119]', '[-1.08632928  1.30374446 -1.47988845  2.57814048]', '[-1.26602191  1.68167393 -0.30798227  1.22279167]', '[-1.20897661  1.79514794  0.87098101 -0.10044487]', '[-0.90921304  1.58285848  2.09481759 -2.06622468]', '[-0.39721042  0.9769489   2.96943623 -3.99108653]', '[ 2.54335267e-01  3.09008382e-03  3.38536543e+00 -5.41161312e+00]', '[ 0.87101647 -0.99607114  2.63408194 -4.28387821]', '[ 1.27341138 -1.65919983  1.37559781 -2.40346802]', '[ 1.42679309 -2.00287151  0.15343162 -1.05829672]', '[ 1.33517194 -2.08330214 -1.06134429  0.27190274]', '[ 0.99565086 -1.83601128 -2.30044585  2.25422778]', '[ 0.43234857 -1.1556199  -3.2880399   4.59891353]', '[-0.29073487 -0.02462929 -3.76887536  6.32810552]', '[-0.97154641  1.13461081 -2.87372174  4.91925595]', '[-1.42036246  1.93282376 -1.60621413  3.14436746]', '[-1.61327604  2.42050639 -0.32460961  1.76834607]', '[-1.55221226  2.64305945  0.9282952   0.44641982]', '[-1.2344243   2.55082357  2.22426278 -1.39811687]', '[-0.68216637  2.0673751   3.22473524 -3.49183473]', '[ 0.02419428  1.13030897  3.78685539 -5.90369811]', '[ 0.79650149 -0.22098826  3.70857675 -7.04968156]', '[ 1.40387594 -1.45389397  2.26708615 -5.12657561]', '[ 1.70283846 -2.30923277  0.7394663  -3.51688167]', '[ 1.70398913 -2.85641638 -0.69408119 -1.96398679]', '[ 1.44118683 -3.11286281 -1.91763357 -0.60346702]', '[ 0.93276882 -3.06668444 -3.12562103  1.02882671]', '[ 0.22552547 -2.7188232  -3.80801275  2.40423   ]', '[-0.52036997 -2.12647701 -3.49660458  3.44394778]', '[-1.13291609 -1.38265518 -2.58979199  3.88115358]', '[-1.55302417 -0.61558131 -1.60839976  3.70820427]', '[-1.77256899  0.07828102 -0.56885565  3.194343  ]', '[-1.76816263  0.6476292   0.65838739  2.43855069]', '[-1.48786696  1.01399644  2.18745379  1.08907281]', '[-0.88110328  0.99458267  3.82096078 -1.39189694]', '[-0.00902251  0.45512285  4.71369048 -3.78289658]', '[ 0.9069687  -0.33136924  4.21832854 -3.59019972]', '[ 1.63314349 -0.8953631   2.99749729 -2.01706246]', '[ 2.11195251 -1.17950643  1.83171963 -0.96214909]', '[ 2.38471191 -1.32947243  0.93891154 -0.63363185]', '[ 2.49968307 -1.45807628  0.2267804  -0.68568172]', '[ 2.46591714 -1.57958966 -0.58008833 -0.50462988]', '[ 2.24714748 -1.61257394 -1.64683684  0.2673443 ]', '[ 1.78936316 -1.42036786 -2.97322115  1.82645009]', '[ 1.04617219 -0.80471929 -4.46049994  4.47230639]', '[ 0.03999966  0.31474723 -5.35370196  6.08359968]', '[-0.9751945   1.31396261 -4.61279022  3.56617459]', '[-1.77012105  1.75468538 -3.2952984   1.01394755]', '[-2.29503608  1.80073126 -1.9955449  -0.36073383]', '[-2.59272974  1.67614538 -1.04777857 -0.75158448]', '[-2.72849536  1.51520253 -0.35495361 -0.78878169]', '[-2.73690391  1.35083735  0.25794455 -0.84110277]', '[-2.63439787  1.20213459  0.78183703 -0.67336582]', '[-2.40200201  1.03264093  1.58657702 -1.10520185]', '[-1.97729857  0.7148625   2.72422316 -2.21102614]', '[-1.29056034  0.09988137  4.14881536 -3.92681647]', '[-0.36852553 -0.70941323  4.88676076 -3.69332112]', '[ 0.58289578 -1.22030548  4.39061633 -1.15151847]', '[ 1.30145282 -1.14281027  2.66534244  1.83324583]', '[ 1.63506024 -0.55487743  0.73458798  3.84370477]', '[ 1.61863209  0.37986903 -0.75177471  5.30229566]', '[ 1.39072015  1.49329121 -1.45219126  5.75935406]', '[ 1.04037217  2.69578898 -2.10014777  6.37192583]', '[ 0.51834152 -2.17208276 -3.21753069  8.07452932]', '[-0.29607527 -0.1888234  -4.73237064 11.50474799]', '[-1.07894775  1.86666579 -2.65408084  8.30797851]', '[-1.40969403 -2.98265991 -0.90437792  6.35319168]', '[-1.53917548 -1.78635789 -0.5435135   5.80319561]', '[-1.64861773 -0.59375113 -0.50663142  6.18866402]', '[-1.66330679  0.61225522  0.66474823  5.47043777]', '[-1.27658695  1.43944959  3.28782852  2.52843362]', '[-0.38033405  1.50888601  5.39730311 -1.86573687]', '[ 0.74491338  0.77225616  5.59666322 -5.12259109]', '[ 1.78888772 -0.33171956  4.70774829 -5.35304509]', '[ 2.62280372 -1.26726011  3.7398656  -4.09856103]', '[-2.94898646 -2.02272736  3.53563784 -3.65306721]', '[-2.1774661  -2.80909864  4.31794488 -4.35554068]', '[-1.19868929  2.45739569  5.43277461 -6.13821038]', '[ -0.01969445   0.83381961   6.40194953 -10.3630489 ]', '[ 1.2208657  -1.24839803  5.54493937 -9.09801881]', '[ 2.17198528 -2.71746663  4.12386449 -6.09933194]', '[ 2.91729144  2.4515103   3.4712095  -5.2903262 ]', '[-2.6514002   1.34347477  3.85977798 -6.05033428]', '[-1.75196971 -0.07126478  5.18986075 -7.9957386 ]', '[-0.6165462  -1.60380395  6.08241021 -6.71472992]', '[ 0.65086488 -2.65517811  6.3736642  -3.84266857]', '[ 1.83159569  3.07383136  5.32107134 -1.91550066]', '[ 2.80540246  2.76654688  4.57050676 -1.36979458]', '[-2.55049959  2.4293046   4.88673622 -2.30844127]', '[-1.47508538  1.72152772  5.94660342 -5.18525441]', '[-0.1540111   0.22140395  7.13922005 -9.37533117]', '[ 1.21250364 -1.43669583  6.19712398 -6.18211005]', '[ 2.32954314 -2.29100132  5.03672346 -2.7774128 ]', '[-3.01087327 -2.69759696  4.56156252 -1.62320708]', '[-2.04688949 -3.06670578  5.25242975 -2.32164929]', '[-0.8751224   2.55714666  6.38693572 -4.58575417]', '[ 0.42547491  1.26626569  6.51318622 -8.47867529]', '[ 1.68175296 -0.61998252  5.77141168 -9.2188202 ]', '[ 2.6886751  -2.18334924  4.50140308 -6.7354607 ]', '[-2.71179414  2.79856934  4.52411153 -6.68459538]', '[-1.70661644  1.24248036  5.79431142 -9.48542661]', '[ -0.36990242  -0.97446379   7.12791068 -11.12233232]', '[ 1.02807644 -2.75732307  6.82282145 -7.09076558]', '[ 2.27957676  2.22960018  5.61857373 -6.3736555 ]', '[-2.93213389  0.8409323   5.42030906 -7.79155589]']</t>
-  </si>
-  <si>
-    <t>[0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50, 51, 52, 53, 54, 55, 56, 57, 58, 59, 60, 61, 62, 63, 64, 65, 66, 67, 68, 69, 70, 71, 72, 73, 74, 75, 76, 77, 78, 79, 80, 81, 82, 83, 84, 85, 86, 87, 88, 89, 90, 91, 92, 93, 94, 95, 96, 97, 98, 99, 100, 101, 102, 103, 104, 105, 106, 107, 108, 109, 110, 111, 112, 113, 114, 115, 116, 117, 118, 119, 120, 121, 122, 123, 124, 125, 126, 127, 128, 129, 130, 131, 132, 133, 134, 135, 136]</t>
-  </si>
-  <si>
-    <t>[array([-0.03763371, -0.01533471,  0.06554052, -0.01816017], dtype=float32), array([-0.00754409, -0.05458322,  0.2277812 , -0.36241836]), array([ 0.04879627, -0.15231473,  0.32089719, -0.5887683 ]), array([ 0.11397169, -0.27767857,  0.31375488, -0.63332862]), array([ 0.15469752, -0.35964331,  0.08386034, -0.16862923]), array([ 0.1328986 , -0.30852175, -0.29631136,  0.66902399]), array([ 0.04193434, -0.10322104, -0.58935853,  1.33680279]), array([-0.0895624 ,  0.19970356, -0.68735485,  1.61532039]), array([-0.21671213,  0.51005343, -0.54911684,  1.41746405]), array([-0.29775335,  0.74363137, -0.24311842,  0.88008455]), array([-0.3099396 ,  0.85242745,  0.12252104,  0.19753864]), array([-0.22805628,  0.7615075 ,  0.68124181, -1.09272869]), array([-0.04681936,  0.42734149,  1.09559275, -2.19100247]), array([ 0.1890354 , -0.07558709,  1.19523955, -2.70411161]), array([ 0.40083096, -0.59317051,  0.86004853, -2.34670125]), array([ 0.51503476, -0.97919856,  0.25973082, -1.46695327]), array([ 0.50222831, -1.17086038, -0.37993929, -0.44268219]), array([ 0.35054191, -1.10163677, -1.10615567,  1.12233487]), array([ 0.07460813, -0.73093941, -1.60864212,  2.53748392]), array([-0.26861178, -0.12448947, -1.74059878,  3.36983165]), array([-0.58016521,  0.5340796 , -1.28298101,  3.03481604]), array([-0.75500166,  1.04058322, -0.43201198,  1.9731889 ]), array([-0.74847174,  1.31351942,  0.49031062,  0.74540217]), array([-0.55852521,  1.3101156 ,  1.37034616, -0.77637724]), array([-0.21046837,  0.98011731,  2.05346592, -2.49410136]), array([ 0.23563297,  0.3420203 ,  2.31862639, -3.73514795]), array([ 0.66871365, -0.41722741,  1.89138947, -3.61279591]), array([ 0.95446017, -1.03363271,  0.91630455, -2.47903128]), array([ 1.01664259, -1.37353874, -0.29268251, -0.92026149]), array([ 0.83425561, -1.37227369, -1.50107115,  0.94945177]), array([ 0.43300511, -0.98571852, -2.4585572 ,  2.91542003]), array([-0.11976547, -0.2323834 , -2.9544336 ,  4.41640071]), array([-0.68221417,  0.64186726, -2.51657809,  4.01073119]), array([-1.08632928,  1.30374446, -1.47988845,  2.57814048]), array([-1.26602191,  1.68167393, -0.30798227,  1.22279167]), array([-1.20897661,  1.79514794,  0.87098101, -0.10044487]), array([-0.90921304,  1.58285848,  2.09481759, -2.06622468]), array([-0.39721042,  0.9769489 ,  2.96943623, -3.99108653]), array([ 2.54335267e-01,  3.09008382e-03,  3.38536543e+00, -5.41161312e+00]), array([ 0.87101647, -0.99607114,  2.63408194, -4.28387821]), array([ 1.27341138, -1.65919983,  1.37559781, -2.40346802]), array([ 1.42679309, -2.00287151,  0.15343162, -1.05829672]), array([ 1.33517194, -2.08330214, -1.06134429,  0.27190274]), array([ 0.99565086, -1.83601128, -2.30044585,  2.25422778]), array([ 0.43234857, -1.1556199 , -3.2880399 ,  4.59891353]), array([-0.29073487, -0.02462929, -3.76887536,  6.32810552]), array([-0.97154641,  1.13461081, -2.87372174,  4.91925595]), array([-1.42036246,  1.93282376, -1.60621413,  3.14436746]), array([-1.61327604,  2.42050639, -0.32460961,  1.76834607]), array([-1.55221226,  2.64305945,  0.9282952 ,  0.44641982]), array([-1.2344243 ,  2.55082357,  2.22426278, -1.39811687]), array([-0.68216637,  2.0673751 ,  3.22473524, -3.49183473]), array([ 0.02419428,  1.13030897,  3.78685539, -5.90369811]), array([ 0.79650149, -0.22098826,  3.70857675, -7.04968156]), array([ 1.40387594, -1.45389397,  2.26708615, -5.12657561]), array([ 1.70283846, -2.30923277,  0.7394663 , -3.51688167]), array([ 1.70398913, -2.85641638, -0.69408119, -1.96398679]), array([ 1.44118683, -3.11286281, -1.91763357, -0.60346702]), array([ 0.93276882, -3.06668444, -3.12562103,  1.02882671]), array([ 0.22552547, -2.7188232 , -3.80801275,  2.40423   ]), array([-0.52036997, -2.12647701, -3.49660458,  3.44394778]), array([-1.13291609, -1.38265518, -2.58979199,  3.88115358]), array([-1.55302417, -0.61558131, -1.60839976,  3.70820427]), array([-1.77256899,  0.07828102, -0.56885565,  3.194343  ]), array([-1.76816263,  0.6476292 ,  0.65838739,  2.43855069]), array([-1.48786696,  1.01399644,  2.18745379,  1.08907281]), array([-0.88110328,  0.99458267,  3.82096078, -1.39189694]), array([-0.00902251,  0.45512285,  4.71369048, -3.78289658]), array([ 0.9069687 , -0.33136924,  4.21832854, -3.59019972]), array([ 1.63314349, -0.8953631 ,  2.99749729, -2.01706246]), array([ 2.11195251, -1.17950643,  1.83171963, -0.96214909]), array([ 2.38471191, -1.32947243,  0.93891154, -0.63363185]), array([ 2.49968307, -1.45807628,  0.2267804 , -0.68568172]), array([ 2.46591714, -1.57958966, -0.58008833, -0.50462988]), array([ 2.24714748, -1.61257394, -1.64683684,  0.2673443 ]), array([ 1.78936316, -1.42036786, -2.97322115,  1.82645009]), array([ 1.04617219, -0.80471929, -4.46049994,  4.47230639]), array([ 0.03999966,  0.31474723, -5.35370196,  6.08359968]), array([-0.9751945 ,  1.31396261, -4.61279022,  3.56617459]), array([-1.77012105,  1.75468538, -3.2952984 ,  1.01394755]), array([-2.29503608,  1.80073126, -1.9955449 , -0.36073383]), array([-2.59272974,  1.67614538, -1.04777857, -0.75158448]), array([-2.72849536,  1.51520253, -0.35495361, -0.78878169]), array([-2.73690391,  1.35083735,  0.25794455, -0.84110277]), array([-2.63439787,  1.20213459,  0.78183703, -0.67336582]), array([-2.40200201,  1.03264093,  1.58657702, -1.10520185]), array([-1.97729857,  0.7148625 ,  2.72422316, -2.21102614]), array([-1.29056034,  0.09988137,  4.14881536, -3.92681647]), array([-0.36852553, -0.70941323,  4.88676076, -3.69332112]), array([ 0.58289578, -1.22030548,  4.39061633, -1.15151847]), array([ 1.30145282, -1.14281027,  2.66534244,  1.83324583]), array([ 1.63506024, -0.55487743,  0.73458798,  3.84370477]), array([ 1.61863209,  0.37986903, -0.75177471,  5.30229566]), array([ 1.39072015,  1.49329121, -1.45219126,  5.75935406]), array([ 1.04037217,  2.69578898, -2.10014777,  6.37192583]), array([ 0.51834152, -2.17208276, -3.21753069,  8.07452932]), array([-0.29607527, -0.1888234 , -4.73237064, 11.50474799]), array([-1.07894775,  1.86666579, -2.65408084,  8.30797851]), array([-1.40969403, -2.98265991, -0.90437792,  6.35319168]), array([-1.53917548, -1.78635789, -0.5435135 ,  5.80319561]), array([-1.64861773, -0.59375113, -0.50663142,  6.18866402]), array([-1.66330679,  0.61225522,  0.66474823,  5.47043777]), array([-1.27658695,  1.43944959,  3.28782852,  2.52843362]), array([-0.38033405,  1.50888601,  5.39730311, -1.86573687]), array([ 0.74491338,  0.77225616,  5.59666322, -5.12259109]), array([ 1.78888772, -0.33171956,  4.70774829, -5.35304509]), array([ 2.62280372, -1.26726011,  3.7398656 , -4.09856103]), array([-2.94898646, -2.02272736,  3.53563784, -3.65306721]), array([-2.1774661 , -2.80909864,  4.31794488, -4.35554068]), array([-1.19868929,  2.45739569,  5.43277461, -6.13821038]), array([ -0.01969445,   0.83381961,   6.40194953, -10.3630489 ]), array([ 1.2208657 , -1.24839803,  5.54493937, -9.09801881]), array([ 2.17198528, -2.71746663,  4.12386449, -6.09933194]), array([ 2.91729144,  2.4515103 ,  3.4712095 , -5.2903262 ]), array([-2.6514002 ,  1.34347477,  3.85977798, -6.05033428]), array([-1.75196971, -0.07126478,  5.18986075, -7.9957386 ]), array([-0.6165462 , -1.60380395,  6.08241021, -6.71472992]), array([ 0.65086488, -2.65517811,  6.3736642 , -3.84266857]), array([ 1.83159569,  3.07383136,  5.32107134, -1.91550066]), array([ 2.80540246,  2.76654688,  4.57050676, -1.36979458]), array([-2.55049959,  2.4293046 ,  4.88673622, -2.30844127]), array([-1.47508538,  1.72152772,  5.94660342, -5.18525441]), array([-0.1540111 ,  0.22140395,  7.13922005, -9.37533117]), array([ 1.21250364, -1.43669583,  6.19712398, -6.18211005]), array([ 2.32954314, -2.29100132,  5.03672346, -2.7774128 ]), array([-3.01087327, -2.69759696,  4.56156252, -1.62320708]), array([-2.04688949, -3.06670578,  5.25242975, -2.32164929]), array([-0.8751224 ,  2.55714666,  6.38693572, -4.58575417]), array([ 0.42547491,  1.26626569,  6.51318622, -8.47867529]), array([ 1.68175296, -0.61998252,  5.77141168, -9.2188202 ]), array([ 2.6886751 , -2.18334924,  4.50140308, -6.7354607 ]), array([-2.71179414,  2.79856934,  4.52411153, -6.68459538]), array([-1.70661644,  1.24248036,  5.79431142, -9.48542661]), array([ -0.36990242,  -0.97446379,   7.12791068, -11.12233232]), array([ 1.02807644, -2.75732307,  6.82282145, -7.09076558]), array([ 2.27957676,  2.22960018,  5.61857373, -6.3736555 ]), array([-2.93213389,  0.8409323 ,  5.42030906, -7.79155589])]</t>
-  </si>
-  <si>
-    <t>['[2,1,0]', '[2,2,2]', '[0,1,1]', '[0,0,0]', '[1,1,2]', '[1,2,0]', '[1,1,1]', '[2,0,1]', '[0,2,1]', '[1,0,2]']</t>
-  </si>
-  <si>
-    <t>[1, 2, 3, 6, 7, 15, 17, 26, 27, 28, 29, 38, 41, 42, 50, 52, 53, 54, 55, 56, 65, 66, 67, 68, 70, 78, 80, 82, 83, 93, 97]</t>
-  </si>
-  <si>
-    <t>[0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 1, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 1, 2, 2, 2, 2, 2, 2, 2, 1, 0, 0, 0, 0, 0]</t>
-  </si>
-  <si>
-    <t>['[-0.03763371 -0.01533471  0.06554052 -0.01816017]', '[-0.0208055  -0.02030166  0.09914155 -0.02801351]', '[ 0.00031733 -0.02489487  0.10765546 -0.0138725 ]', '[ 0.02044082 -0.02428802  0.08954248  0.02288616]', '[ 0.0479687  -0.04919805  0.17922331 -0.26311843]', '[ 0.08850804 -0.12358959  0.21549919 -0.46142015]', '[ 0.11624667 -0.19048     0.05459375 -0.19254603]', '[ 0.10897736 -0.1973004  -0.12576083  0.12396431]', '[ 0.0550622  -0.10988033 -0.39981924  0.72728155]', '[-0.04266374  0.07870359 -0.55123823  1.10968785]', '[-0.1531927   0.31071666 -0.52388154  1.15234652]', '[-0.24074019  0.51744829 -0.32925961  0.87103957]', '[-0.27822793  0.64556832 -0.03696221  0.38960999]', '[-0.23050882  0.60555791  0.50419263 -0.77996162]', '[-0.08433427  0.34430059  0.92625857 -1.7810221 ]', '[ 0.10852319 -0.03937976  0.94904724 -1.95360451]', '[ 0.28627963 -0.42813198  0.77839617 -1.83591939]', '[ 0.39093331 -0.70925734  0.24672746 -0.93258053]', '[ 0.39313667 -0.82325453 -0.22445631 -0.1967451 ]', '[ 0.28173879 -0.72663633 -0.86843653  1.14620496]', '[ 0.05842322 -0.37920452 -1.31919841  2.2591992 ]', '[-0.22028054  0.13154951 -1.390728    2.70114477]', '[-0.46514883  0.63810968 -0.99353226  2.24389829]', '[-0.59954798  0.99744284 -0.32701777  1.30938985]', '[-0.59258996  1.15413665  0.39135772  0.25076448]', '[-0.42913454  1.04158726  1.2146805  -1.36799998]', '[-0.13328536  0.64641655  1.69115338 -2.52080369]', '[ 0.21843543  0.0796138   1.73689888 -2.98177255]', '[ 0.52220006 -0.47044046  1.22193282 -2.37100329]', '[ 0.68534903 -0.83140838  0.38206431 -1.19615994]', '[ 0.68206433 -0.97139301 -0.41346252 -0.19261661]', '[ 0.50358966 -0.84758623 -1.34227537  1.42270232]', '[ 0.16250827 -0.41445203 -2.00457097  2.82661324]', '[-0.26058656  0.21884633 -2.11206767  3.28944478]', '[-0.63621268  0.81406277 -1.5616381   2.52445098]', '[-0.86404295  1.20238326 -0.68799136  1.3397355 ]', '[-0.90563849  1.34878833  0.27422959  0.12284374]', '[-0.73849434  1.19564662  1.37778242 -1.66685871]', '[-0.37750383  0.708409    2.18115703 -3.16500358]', '[ 0.1129431  -0.05242268  2.59600495 -4.19760601]', '[ 0.59797748 -0.84198701  2.13270834 -3.46802638]', '[ 0.9262171  -1.37115166  1.11853215 -1.82163621]', '[ 1.03882441e+00 -1.57843208e+00  1.24349840e-03 -2.64963214e-01]', '[ 0.91880889 -1.4521878  -1.19048035  1.54394015]', '[ 0.56994142 -0.94900799 -2.26975607  3.50632092]', '[ 0.03420208 -0.07241165 -2.96183636  5.01988362]', '[-0.53753766  0.89395078 -2.59435695  4.31414494]', '[-0.96701144  1.59730959 -1.65963925  2.71463134]', '[-1.19180119  1.99306475 -0.57360646  1.27255186]', '[-1.19388521  2.112549    0.54972572 -0.0768638 ]', '[-0.97018807  1.93555762  1.66150981 -1.71756799]', '[-0.53576417  1.38725056  2.64546886 -3.81189883]', '[ 0.05904166  0.43718494  3.20508216 -5.52313175]', '[ 0.66901087 -0.65353562  2.69488649 -4.95052112]', '[ 1.08932686 -1.45613893  1.47327128 -3.06806886]', '[ 1.25510836 -1.89956986  0.18489543 -1.40040515]', '[ 1.17320311 -2.04251796 -0.99079061 -0.01797931]', '[ 0.85514582 -1.85332532 -2.14647387  1.9429784 ]', '[ 0.33620553 -1.24986728 -2.98936049  4.11727285]', '[-0.31457366 -0.22627626 -3.39009867  5.85553537]', '[-0.93199367  0.8928861  -2.60398449  4.95309558]', '[-1.32372662  1.70968448 -1.29480304  3.2536487 ]', '[-1.44859077  2.21488548  0.04308176  1.82256944]', '[-1.31045665  2.43828373  1.31989956  0.39611548]', '[-0.92109045  2.32406369  2.51737568 -1.56160187]', '[-0.34302257  1.82606205  3.16881596 -3.42830555]', '[ 0.31065295  0.96063389  3.29517971 -5.1398399 ]', '[ 0.93286621 -0.13285361  2.76652099 -5.40871048]', '[ 1.35439276 -1.06603857  1.37628812 -3.80788587]', '[ 1.48439973 -1.68612332 -0.08726539 -2.39743561]', '[ 1.31276879 -1.99471942 -1.60513801 -0.65221687]', '[ 0.85389969 -1.90511333 -2.9083387   1.59678468]', '[ 0.18891931 -1.34208998 -3.64233867  4.03313703]', '[-0.56476899 -0.32703516 -3.76706368  5.83465355]', '[-1.23849082  0.79332323 -2.80846867  4.99367339]', '[-1.66164432  1.63079846 -1.41604684  3.43890581]', '[-1.80587031  2.19395693 -0.02901178  2.2165699 ]', '[-1.67515558  2.51237235  1.32812171  0.9321854 ]', '[-1.27411071  2.52877808  2.65218473 -0.81467821]', '[-0.63240086  2.14760606  3.66484006 -3.04445883]', '[ 0.13614982  1.32260341  3.92386396 -5.17696511]', '[ 0.91450243  0.10863181  3.71842646 -6.57565765]', '[ 1.5277034  -1.06417741  2.30048825 -4.91570245]', '[ 1.82921843 -1.87375883  0.72586668 -3.26512546]', '[ 1.82860857 -2.40648514 -0.72501485 -2.04660896]', '[ 1.5385588  -2.65694304 -2.15455287 -0.41519863]', '[ 0.97359017 -2.53658114 -3.43098051  1.65601063]', '[ 0.2111125  -1.9821338  -4.05250889  3.90657204]', '[-0.59788768 -0.9822152  -3.96830031  5.99614423]', '[-1.33869181  0.29847003 -3.27303747  6.34383267]', '[-1.84661855  1.41606914 -1.7614625   4.7966872 ]', '[-2.04282911  2.24807442 -0.20942124  3.57083344]', '[-1.93957028  2.84415907  1.20450386  2.36537934]', '[-1.56291807 -3.13772935  2.54250809  0.6416335 ]', '[-0.92822148  3.10770687  3.76347874 -0.97627681]', '[-0.09693908  2.77729684  4.38793866 -2.26504893]', '[ 0.74675256  2.23089256  3.87669447 -3.09899126]', '[ 1.40392853  1.612695    2.65451773 -2.93347351]', '[ 1.81667838  1.08186868  1.4866066  -2.29611474]']</t>
-  </si>
-  <si>
-    <t>[0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50, 51, 52, 53, 54, 55, 56, 57, 58, 59, 60, 61, 62, 63, 64, 65, 66, 67, 68, 69, 70, 71, 72, 73, 74, 75, 76, 77, 78, 79, 80, 81, 82, 83, 84, 85, 86, 87, 88, 89, 90, 91, 92, 93, 94, 95, 96, 97, 98]</t>
-  </si>
-  <si>
-    <t>[array([-0.03763371, -0.01533471,  0.06554052, -0.01816017], dtype=float32), array([-0.0208055 , -0.02030166,  0.09914155, -0.02801351]), array([ 0.00031733, -0.02489487,  0.10765546, -0.0138725 ]), array([ 0.02044082, -0.02428802,  0.08954248,  0.02288616]), array([ 0.0479687 , -0.04919805,  0.17922331, -0.26311843]), array([ 0.08850804, -0.12358959,  0.21549919, -0.46142015]), array([ 0.11624667, -0.19048   ,  0.05459375, -0.19254603]), array([ 0.10897736, -0.1973004 , -0.12576083,  0.12396431]), array([ 0.0550622 , -0.10988033, -0.39981924,  0.72728155]), array([-0.04266374,  0.07870359, -0.55123823,  1.10968785]), array([-0.1531927 ,  0.31071666, -0.52388154,  1.15234652]), array([-0.24074019,  0.51744829, -0.32925961,  0.87103957]), array([-0.27822793,  0.64556832, -0.03696221,  0.38960999]), array([-0.23050882,  0.60555791,  0.50419263, -0.77996162]), array([-0.08433427,  0.34430059,  0.92625857, -1.7810221 ]), array([ 0.10852319, -0.03937976,  0.94904724, -1.95360451]), array([ 0.28627963, -0.42813198,  0.77839617, -1.83591939]), array([ 0.39093331, -0.70925734,  0.24672746, -0.93258053]), array([ 0.39313667, -0.82325453, -0.22445631, -0.1967451 ]), array([ 0.28173879, -0.72663633, -0.86843653,  1.14620496]), array([ 0.05842322, -0.37920452, -1.31919841,  2.2591992 ]), array([-0.22028054,  0.13154951, -1.390728  ,  2.70114477]), array([-0.46514883,  0.63810968, -0.99353226,  2.24389829]), array([-0.59954798,  0.99744284, -0.32701777,  1.30938985]), array([-0.59258996,  1.15413665,  0.39135772,  0.25076448]), array([-0.42913454,  1.04158726,  1.2146805 , -1.36799998]), array([-0.13328536,  0.64641655,  1.69115338, -2.52080369]), array([ 0.21843543,  0.0796138 ,  1.73689888, -2.98177255]), array([ 0.52220006, -0.47044046,  1.22193282, -2.37100329]), array([ 0.68534903, -0.83140838,  0.38206431, -1.19615994]), array([ 0.68206433, -0.97139301, -0.41346252, -0.19261661]), array([ 0.50358966, -0.84758623, -1.34227537,  1.42270232]), array([ 0.16250827, -0.41445203, -2.00457097,  2.82661324]), array([-0.26058656,  0.21884633, -2.11206767,  3.28944478]), array([-0.63621268,  0.81406277, -1.5616381 ,  2.52445098]), array([-0.86404295,  1.20238326, -0.68799136,  1.3397355 ]), array([-0.90563849,  1.34878833,  0.27422959,  0.12284374]), array([-0.73849434,  1.19564662,  1.37778242, -1.66685871]), array([-0.37750383,  0.708409  ,  2.18115703, -3.16500358]), array([ 0.1129431 , -0.05242268,  2.59600495, -4.19760601]), array([ 0.59797748, -0.84198701,  2.13270834, -3.46802638]), array([ 0.9262171 , -1.37115166,  1.11853215, -1.82163621]), array([ 1.03882441e+00, -1.57843208e+00,  1.24349840e-03, -2.64963214e-01]), array([ 0.91880889, -1.4521878 , -1.19048035,  1.54394015]), array([ 0.56994142, -0.94900799, -2.26975607,  3.50632092]), array([ 0.03420208, -0.07241165, -2.96183636,  5.01988362]), array([-0.53753766,  0.89395078, -2.59435695,  4.31414494]), array([-0.96701144,  1.59730959, -1.65963925,  2.71463134]), array([-1.19180119,  1.99306475, -0.57360646,  1.27255186]), array([-1.19388521,  2.112549  ,  0.54972572, -0.0768638 ]), array([-0.97018807,  1.93555762,  1.66150981, -1.71756799]), array([-0.53576417,  1.38725056,  2.64546886, -3.81189883]), array([ 0.05904166,  0.43718494,  3.20508216, -5.52313175]), array([ 0.66901087, -0.65353562,  2.69488649, -4.95052112]), array([ 1.08932686, -1.45613893,  1.47327128, -3.06806886]), array([ 1.25510836, -1.89956986,  0.18489543, -1.40040515]), array([ 1.17320311, -2.04251796, -0.99079061, -0.01797931]), array([ 0.85514582, -1.85332532, -2.14647387,  1.9429784 ]), array([ 0.33620553, -1.24986728, -2.98936049,  4.11727285]), array([-0.31457366, -0.22627626, -3.39009867,  5.85553537]), array([-0.93199367,  0.8928861 , -2.60398449,  4.95309558]), array([-1.32372662,  1.70968448, -1.29480304,  3.2536487 ]), array([-1.44859077,  2.21488548,  0.04308176,  1.82256944]), array([-1.31045665,  2.43828373,  1.31989956,  0.39611548]), array([-0.92109045,  2.32406369,  2.51737568, -1.56160187]), array([-0.34302257,  1.82606205,  3.16881596, -3.42830555]), array([ 0.31065295,  0.96063389,  3.29517971, -5.1398399 ]), array([ 0.93286621, -0.13285361,  2.76652099, -5.40871048]), array([ 1.35439276, -1.06603857,  1.37628812, -3.80788587]), array([ 1.48439973, -1.68612332, -0.08726539, -2.39743561]), array([ 1.31276879, -1.99471942, -1.60513801, -0.65221687]), array([ 0.85389969, -1.90511333, -2.9083387 ,  1.59678468]), array([ 0.18891931, -1.34208998, -3.64233867,  4.03313703]), array([-0.56476899, -0.32703516, -3.76706368,  5.83465355]), array([-1.23849082,  0.79332323, -2.80846867,  4.99367339]), array([-1.66164432,  1.63079846, -1.41604684,  3.43890581]), array([-1.80587031,  2.19395693, -0.02901178,  2.2165699 ]), array([-1.67515558,  2.51237235,  1.32812171,  0.9321854 ]), array([-1.27411071,  2.52877808,  2.65218473, -0.81467821]), array([-0.63240086,  2.14760606,  3.66484006, -3.04445883]), array([ 0.13614982,  1.32260341,  3.92386396, -5.17696511]), array([ 0.91450243,  0.10863181,  3.71842646, -6.57565765]), array([ 1.5277034 , -1.06417741,  2.30048825, -4.91570245]), array([ 1.82921843, -1.87375883,  0.72586668, -3.26512546]), array([ 1.82860857, -2.40648514, -0.72501485, -2.04660896]), array([ 1.5385588 , -2.65694304, -2.15455287, -0.41519863]), array([ 0.97359017, -2.53658114, -3.43098051,  1.65601063]), array([ 0.2111125 , -1.9821338 , -4.05250889,  3.90657204]), array([-0.59788768, -0.9822152 , -3.96830031,  5.99614423]), array([-1.33869181,  0.29847003, -3.27303747,  6.34383267]), array([-1.84661855,  1.41606914, -1.7614625 ,  4.7966872 ]), array([-2.04282911,  2.24807442, -0.20942124,  3.57083344]), array([-1.93957028,  2.84415907,  1.20450386,  2.36537934]), array([-1.56291807, -3.13772935,  2.54250809,  0.6416335 ]), array([-0.92822148,  3.10770687,  3.76347874, -0.97627681]), array([-0.09693908,  2.77729684,  4.38793866, -2.26504893]), array([ 0.74675256,  2.23089256,  3.87669447, -3.09899126]), array([ 1.40392853,  1.612695  ,  2.65451773, -2.93347351]), array([ 1.81667838,  1.08186868,  1.4866066 , -2.29611474])]</t>
-  </si>
-  <si>
-    <t>['[2,1,0]', '[1,0,2]', '[1,1,1]', '[1,2,0]', '[2,0,1]', '[1,1,2]', '[0,2,1]', '[0,0,0]', '[2,2,2]', '[0,1,1]']</t>
-  </si>
-  <si>
-    <t>[1, 5, 12, 13, 14, 17, 25, 27, 28, 29, 36, 37, 38, 39, 40, 41, 50, 51, 52, 53, 54, 55, 63, 64, 65, 66, 67, 68, 77, 78, 79, 80, 83, 93, 94, 95, 96, 97, 98, 106, 107, 108, 109, 110, 111, 112, 113, 115, 116]</t>
-  </si>
-  <si>
-    <t>[0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 1, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 2, 1, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2]</t>
-  </si>
-  <si>
-    <t>['[-0.03763371 -0.01533471  0.06554052 -0.01816017]', '[-0.0208055  -0.02030166  0.09914155 -0.02801351]', '[ 0.013578   -0.05917353  0.23628798 -0.34824344]', '[ 0.06892075 -0.15170277  0.30283362 -0.5520916 ]', '[ 0.12827063 -0.26838081  0.27505366 -0.58564774]', '[ 0.16005875 -0.34102171  0.03515865 -0.12569461]', '[ 0.12853775 -0.28300606 -0.34263689  0.69246565]', '[ 0.02967829 -0.07631626 -0.62005388  1.32504849]', '[-0.10564872  0.22004567 -0.69460559  1.56224911]', '[-0.23208332  0.51676422 -0.53579303  1.3377179 ]', '[-0.30900866  0.7334938  -0.21638168  0.7941777 ]', '[-0.31501811  0.82566317  0.156575    0.1190051 ]', '[-0.23750226  0.75099658  0.60325536 -0.85072398]', '[-0.08298687  0.49711852  0.91003804 -1.63907803]', '[ 0.10959228  0.12476418  0.96588618 -1.99073838]', '[ 0.29438331 -0.29003939  0.8278699  -2.04908492]', '[ 0.42099703 -0.65520693  0.40440457 -1.53212885]', '[ 0.43665329 -0.85356743 -0.2477276  -0.43571573]', '[ 0.3154454  -0.79850815 -0.93986314  0.97212164]', '[ 0.07452699 -0.47723299 -1.422634    2.17912061]', '[-0.22799074  0.03084872 -1.52387422  2.75572138]', '[-0.500157    0.55823624 -1.12548973  2.38276458]', '[-0.65694493  0.94691817 -0.413442    1.45623825]', '[-0.66061949  1.13123587  0.37393405  0.37680349]', '[-0.49295803  1.03984218  1.27327279 -1.28559214]', '[-0.17867106  0.65503304  1.81405849 -2.50189254]', '[ 0.21507452  0.05228576  2.02654814 -3.34800432]', '[ 0.57314126 -0.56127958  1.46378633 -2.61984193]', '[ 0.77686469 -0.95802629  0.54430753 -1.31302404]', '[ 0.78625774 -1.08227307 -0.44798834  0.0744522 ]', '[ 0.59243913 -0.89761134 -1.46425973  1.77126721]', '[ 0.21714336 -0.38361327 -2.22096965  3.2784941 ]', '[-0.25268978  0.33596787 -2.34482982  3.65685333]', '[-0.67009011  0.98210593 -1.74568348  2.6725537 ]', '[-0.93073491  1.38625431 -0.8325669   1.36555527]', '[-0.99682562  1.5313825   0.1762972   0.08982127]', '[-0.85335366  1.39508261  1.24266558 -1.4661766 ]', '[-0.51010105  0.93845348  2.15111743 -3.09553176]', '[-0.01888757  0.18530657  2.65049269 -4.23720654]', '[ 0.48730381 -0.62814562  2.27090776 -3.61697719]', '[ 0.85207599 -1.19925222  1.3306937  -2.05605659]', '[ 1.00992493 -1.45393198  0.23644734 -0.50524065]', '[ 0.93649688 -1.37768976 -0.96401787  1.27744641]', '[ 0.63003115 -0.93343506 -2.07563907  3.18197124]', '[ 0.12682855 -0.12224515 -2.84591612  4.72968552]', '[-0.43732554  0.80924937 -2.63270183  4.24982014]', '[-0.8846189   1.50780268 -1.78944842  2.70632329]', '[-1.14079196  1.90109127 -0.75234754  1.25538552]', '[-1.18105269  2.01751465  0.35128357 -0.08602443]', '[-0.98864644  1.81814343  1.5550764  -1.93607579]', '[-0.57776128  1.24999542  2.520105   -3.78000982]', '[-1.34353753e-03  3.14787916e-01  3.13383545e+00 -5.37488578e+00]', '[ 0.5961828  -0.7278749   2.65462677 -4.65388691]', '[ 1.01818217 -1.47367617  1.53010207 -2.80057591]', '[ 1.20294862 -1.86516269  0.31267236 -1.14746625]', '[ 1.15145594 -1.96025927 -0.81889236  0.20341211]', '[ 0.86844978 -1.73025106 -1.97878707  2.13195217]', '[ 0.37591125 -1.08986325 -2.90400995  4.29797904]', '[-0.26476043 -0.04281417 -3.3459133   5.8423843 ]', '[-0.87011053  1.04111717 -2.54777852  4.67280066]', '[-1.25883892  1.80127002 -1.32280067  2.97656987]', '[-1.39684822  2.25179095 -0.05739545  1.55378798]', '[-1.28448616  2.4238633   1.16615302  0.15580067]', '[-0.93508521  2.28626864  2.28022287 -1.55362922]', '[-0.40061151  1.79346596  2.98258231 -3.3903687 ]', '[ 0.22639926  0.93353763  3.21859452 -5.13408471]', '[ 0.84283022 -0.16362466  2.77486136 -5.43803222]', '[ 1.26968742 -1.09882534  1.41796245 -3.79386988]', '[ 1.40246756 -1.68640999 -0.08947721 -2.10435014]', '[ 1.24538815 -1.96108716 -1.46237567 -0.60815585]', '[ 0.82002506 -1.86813069 -2.71945874  1.57726542]', '[ 0.19436867 -1.31885262 -3.44526507  3.91240296]', '[-0.52180886 -0.33653014 -3.59398293  5.6485477 ]', '[-1.16666792  0.75466552 -2.69225024  4.89507214]', '[-1.56858779  1.57446473 -1.31228451  3.34226637]', '[-1.69083447  2.11240896  0.08928245  2.05540215]', '[-1.53467444  2.39048776  1.461113    0.68879346]', '[-1.10941117  2.34928479  2.74499246 -1.14735934]', '[-0.46827184  1.91496963  3.56024563 -3.22381644]', '[ 0.26995568  1.06298743  3.73356355 -5.21583107]', '[ 0.98249016 -0.07311     3.22845947 -5.72180154]', '[ 1.50633549 -1.09810106  1.92682699 -4.37962141]', '[ 1.74432117 -1.83342733  0.4473914  -3.01609406]', '[ 1.67804593 -2.28592207 -1.09838991 -1.48638107]', '[ 1.3069464  -2.38880071 -2.57485422  0.51247193]', '[ 0.67370942 -2.0582905  -3.65923946  2.84648041]', '[-0.10950668 -1.23693145 -4.08038645  5.35066726]', '[-0.92243996  0.0130462  -3.87834829  6.6846253 ]', '[-1.57264555  1.2131876  -2.51924477  5.10404197]', '[-1.92772441  2.08053718 -1.04688538  3.667746  ]', '[-1.99869888  2.69982411  0.3112158   2.52911002]', '[-1.813898    3.08411917  1.5189633   1.29099646]', '[-1.3870969  -3.09147392  2.74690099 -0.20902222]', '[-0.72407709  3.01054242  3.81460024 -1.56236136]', '[ 0.08586648  2.58546456  4.10736854 -2.63173987]', '[ 0.84516379  1.99197049  3.35333218 -3.18169228]', '[ 1.39902561  1.37085854  2.16004042 -2.89055373]', '[ 1.7069208   0.87909311  0.91943119 -1.960053  ]', '[ 1.76787352  0.59727372 -0.30713742 -0.86080119]', '[ 1.57182043  0.55944921 -1.65065644  0.44298451]', '[ 1.11399627  0.74360796 -2.88331063  1.26154628]', '[ 0.4541471   0.97998867 -3.57503918  0.85122531]', '[-0.23983733  0.98254523 -3.16807953 -0.99136054]', '[-0.74483435  0.55813456 -1.82055409 -3.15582811]', '[-0.96140272 -0.2584949  -0.49182132 -4.69812601]', '[-1.00999265 -1.20452311 -0.08136963 -4.64860113]', '[-1.00698678 -2.10905385  0.15532603 -4.52603494]', '[-0.92251367 -3.0709833   0.78118976 -5.23796406]', '[-0.64714756  2.01460888  2.09102393 -6.95700054]', '[-0.05025046  0.31860926  3.72956846 -9.86401767]', '[ 0.60829843 -1.49995944  2.43414325 -7.56972059]', '[ 0.9181712  -2.76288386  0.77053691 -5.30966246]', '[ 0.96658647  2.58819124 -0.16982836 -4.15776634]', '[ 0.88624642  1.79878372 -0.56070959 -3.89120855]', '[ 0.78184314  0.94039641 -0.42019568 -4.83496336]', '[ 0.69318338 -0.09434073 -0.653803   -5.1976498 ]', '[ 0.41914667 -0.95081922 -2.19073001 -3.07271145]', '[-0.16301882 -1.26671145 -3.42879782 -0.19259758]', '[-0.85892256 -1.10780985 -3.33864747  1.53379939]', '[-1.44495501 -0.7521322  -2.44718768  1.82304446]', '[-1.82527318 -0.43206732 -1.35166901  1.3095649 ]', '[-1.98930477 -0.23622376 -0.30022694  0.65278192]']</t>
-  </si>
-  <si>
-    <t>[0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50, 51, 52, 53, 54, 55, 56, 57, 58, 59, 60, 61, 62, 63, 64, 65, 66, 67, 68, 69, 70, 71, 72, 73, 74, 75, 76, 77, 78, 79, 80, 81, 82, 83, 84, 85, 86, 87, 88, 89, 90, 91, 92, 93, 94, 95, 96, 97, 98, 99, 100, 101, 102, 103, 104, 105, 106, 107, 108, 109, 110, 111, 112, 113, 114, 115, 116, 117, 118, 119, 120, 121]</t>
-  </si>
-  <si>
-    <t>[array([-0.03763371, -0.01533471,  0.06554052, -0.01816017], dtype=float32), array([-0.0208055 , -0.02030166,  0.09914155, -0.02801351]), array([ 0.013578  , -0.05917353,  0.23628798, -0.34824344]), array([ 0.06892075, -0.15170277,  0.30283362, -0.5520916 ]), array([ 0.12827063, -0.26838081,  0.27505366, -0.58564774]), array([ 0.16005875, -0.34102171,  0.03515865, -0.12569461]), array([ 0.12853775, -0.28300606, -0.34263689,  0.69246565]), array([ 0.02967829, -0.07631626, -0.62005388,  1.32504849]), array([-0.10564872,  0.22004567, -0.69460559,  1.56224911]), array([-0.23208332,  0.51676422, -0.53579303,  1.3377179 ]), array([-0.30900866,  0.7334938 , -0.21638168,  0.7941777 ]), array([-0.31501811,  0.82566317,  0.156575  ,  0.1190051 ]), array([-0.23750226,  0.75099658,  0.60325536, -0.85072398]), array([-0.08298687,  0.49711852,  0.91003804, -1.63907803]), array([ 0.10959228,  0.12476418,  0.96588618, -1.99073838]), array([ 0.29438331, -0.29003939,  0.8278699 , -2.04908492]), array([ 0.42099703, -0.65520693,  0.40440457, -1.53212885]), array([ 0.43665329, -0.85356743, -0.2477276 , -0.43571573]), array([ 0.3154454 , -0.79850815, -0.93986314,  0.97212164]), array([ 0.07452699, -0.47723299, -1.422634  ,  2.17912061]), array([-0.22799074,  0.03084872, -1.52387422,  2.75572138]), array([-0.500157  ,  0.55823624, -1.12548973,  2.38276458]), array([-0.65694493,  0.94691817, -0.413442  ,  1.45623825]), array([-0.66061949,  1.13123587,  0.37393405,  0.37680349]), array([-0.49295803,  1.03984218,  1.27327279, -1.28559214]), array([-0.17867106,  0.65503304,  1.81405849, -2.50189254]), array([ 0.21507452,  0.05228576,  2.02654814, -3.34800432]), array([ 0.57314126, -0.56127958,  1.46378633, -2.61984193]), array([ 0.77686469, -0.95802629,  0.54430753, -1.31302404]), array([ 0.78625774, -1.08227307, -0.44798834,  0.0744522 ]), array([ 0.59243913, -0.89761134, -1.46425973,  1.77126721]), array([ 0.21714336, -0.38361327, -2.22096965,  3.2784941 ]), array([-0.25268978,  0.33596787, -2.34482982,  3.65685333]), array([-0.67009011,  0.98210593, -1.74568348,  2.6725537 ]), array([-0.93073491,  1.38625431, -0.8325669 ,  1.36555527]), array([-0.99682562,  1.5313825 ,  0.1762972 ,  0.08982127]), array([-0.85335366,  1.39508261,  1.24266558, -1.4661766 ]), array([-0.51010105,  0.93845348,  2.15111743, -3.09553176]), array([-0.01888757,  0.18530657,  2.65049269, -4.23720654]), array([ 0.48730381, -0.62814562,  2.27090776, -3.61697719]), array([ 0.85207599, -1.19925222,  1.3306937 , -2.05605659]), array([ 1.00992493, -1.45393198,  0.23644734, -0.50524065]), array([ 0.93649688, -1.37768976, -0.96401787,  1.27744641]), array([ 0.63003115, -0.93343506, -2.07563907,  3.18197124]), array([ 0.12682855, -0.12224515, -2.84591612,  4.72968552]), array([-0.43732554,  0.80924937, -2.63270183,  4.24982014]), array([-0.8846189 ,  1.50780268, -1.78944842,  2.70632329]), array([-1.14079196,  1.90109127, -0.75234754,  1.25538552]), array([-1.18105269,  2.01751465,  0.35128357, -0.08602443]), array([-0.98864644,  1.81814343,  1.5550764 , -1.93607579]), array([-0.57776128,  1.24999542,  2.520105  , -3.78000982]), array([-1.34353753e-03,  3.14787916e-01,  3.13383545e+00, -5.37488578e+00]), array([ 0.5961828 , -0.7278749 ,  2.65462677, -4.65388691]), array([ 1.01818217, -1.47367617,  1.53010207, -2.80057591]), array([ 1.20294862, -1.86516269,  0.31267236, -1.14746625]), array([ 1.15145594, -1.96025927, -0.81889236,  0.20341211]), array([ 0.86844978, -1.73025106, -1.97878707,  2.13195217]), array([ 0.37591125, -1.08986325, -2.90400995,  4.29797904]), array([-0.26476043, -0.04281417, -3.3459133 ,  5.8423843 ]), array([-0.87011053,  1.04111717, -2.54777852,  4.67280066]), array([-1.25883892,  1.80127002, -1.32280067,  2.97656987]), array([-1.39684822,  2.25179095, -0.05739545,  1.55378798]), array([-1.28448616,  2.4238633 ,  1.16615302,  0.15580067]), array([-0.93508521,  2.28626864,  2.28022287, -1.55362922]), array([-0.40061151,  1.79346596,  2.98258231, -3.3903687 ]), array([ 0.22639926,  0.93353763,  3.21859452, -5.13408471]), array([ 0.84283022, -0.16362466,  2.77486136, -5.43803222]), array([ 1.26968742, -1.09882534,  1.41796245, -3.79386988]), array([ 1.40246756, -1.68640999, -0.08947721, -2.10435014]), array([ 1.24538815, -1.96108716, -1.46237567, -0.60815585]), array([ 0.82002506, -1.86813069, -2.71945874,  1.57726542]), array([ 0.19436867, -1.31885262, -3.44526507,  3.91240296]), array([-0.52180886, -0.33653014, -3.59398293,  5.6485477 ]), array([-1.16666792,  0.75466552, -2.69225024,  4.89507214]), array([-1.56858779,  1.57446473, -1.31228451,  3.34226637]), array([-1.69083447,  2.11240896,  0.08928245,  2.05540215]), array([-1.53467444,  2.39048776,  1.461113  ,  0.68879346]), array([-1.10941117,  2.34928479,  2.74499246, -1.14735934]), array([-0.46827184,  1.91496963,  3.56024563, -3.22381644]), array([ 0.26995568,  1.06298743,  3.73356355, -5.21583107]), array([ 0.98249016, -0.07311   ,  3.22845947, -5.72180154]), array([ 1.50633549, -1.09810106,  1.92682699, -4.37962141]), array([ 1.74432117, -1.83342733,  0.4473914 , -3.01609406]), array([ 1.67804593, -2.28592207, -1.09838991, -1.48638107]), array([ 1.3069464 , -2.38880071, -2.57485422,  0.51247193]), array([ 0.67370942, -2.0582905 , -3.65923946,  2.84648041]), array([-0.10950668, -1.23693145, -4.08038645,  5.35066726]), array([-0.92243996,  0.0130462 , -3.87834829,  6.6846253 ]), array([-1.57264555,  1.2131876 , -2.51924477,  5.10404197]), array([-1.92772441,  2.08053718, -1.04688538,  3.667746  ]), array([-1.99869888,  2.69982411,  0.3112158 ,  2.52911002]), array([-1.813898  ,  3.08411917,  1.5189633 ,  1.29099646]), array([-1.3870969 , -3.09147392,  2.74690099, -0.20902222]), array([-0.72407709,  3.01054242,  3.81460024, -1.56236136]), array([ 0.08586648,  2.58546456,  4.10736854, -2.63173987]), array([ 0.84516379,  1.99197049,  3.35333218, -3.18169228]), array([ 1.39902561,  1.37085854,  2.16004042, -2.89055373]), array([ 1.7069208 ,  0.87909311,  0.91943119, -1.960053  ]), array([ 1.76787352,  0.59727372, -0.30713742, -0.86080119]), array([ 1.57182043,  0.55944921, -1.65065644,  0.44298451]), array([ 1.11399627,  0.74360796, -2.88331063,  1.26154628]), array([ 0.4541471 ,  0.97998867, -3.57503918,  0.85122531]), array([-0.23983733,  0.98254523, -3.16807953, -0.99136054]), array([-0.74483435,  0.55813456, -1.82055409, -3.15582811]), array([-0.96140272, -0.2584949 , -0.49182132, -4.69812601]), array([-1.00999265, -1.20452311, -0.08136963, -4.64860113]), array([-1.00698678, -2.10905385,  0.15532603, -4.52603494]), array([-0.92251367, -3.0709833 ,  0.78118976, -5.23796406]), array([-0.64714756,  2.01460888,  2.09102393, -6.95700054]), array([-0.05025046,  0.31860926,  3.72956846, -9.86401767]), array([ 0.60829843, -1.49995944,  2.43414325, -7.56972059]), array([ 0.9181712 , -2.76288386,  0.77053691, -5.30966246]), array([ 0.96658647,  2.58819124, -0.16982836, -4.15776634]), array([ 0.88624642,  1.79878372, -0.56070959, -3.89120855]), array([ 0.78184314,  0.94039641, -0.42019568, -4.83496336]), array([ 0.69318338, -0.09434073, -0.653803  , -5.1976498 ]), array([ 0.41914667, -0.95081922, -2.19073001, -3.07271145]), array([-0.16301882, -1.26671145, -3.42879782, -0.19259758]), array([-0.85892256, -1.10780985, -3.33864747,  1.53379939]), array([-1.44495501, -0.7521322 , -2.44718768,  1.82304446]), array([-1.82527318, -0.43206732, -1.35166901,  1.3095649 ]), array([-1.98930477, -0.23622376, -0.30022694,  0.65278192])]</t>
-  </si>
-  <si>
-    <t>['[1,1,2]', '[2,2,2]', '[1,0,2]', '[1,2,0]', '[0,1,1]', '[0,0,0]', '[0,2,1]', '[1,1,1]', '[2,1,0]', '[2,0,1]']</t>
-  </si>
-  <si>
-    <t>[1, 2, 3, 4, 11, 12, 13, 14, 15, 16, 23, 24, 25, 26, 27, 34, 35, 36, 37, 38, 39, 46, 47, 48, 49, 50, 51, 59, 60, 61, 62, 63, 64, 72, 73, 74, 75, 76, 77, 78, 86, 87, 88, 89, 90, 91, 92, 100, 101, 102, 103, 104, 105, 106, 107, 115, 116, 117, 118, 119, 120, 121, 122, 133, 134, 135, 136, 137, 138, 139, 140, 141, 142, 143, 144, 145, 146]</t>
-  </si>
-  <si>
-    <t>[0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 1, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 1, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 1, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 1, 1, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 1, 1, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2]</t>
-  </si>
-  <si>
-    <t>['[-0.03763371 -0.01533471  0.06554052 -0.01816017]', '[-0.0208055  -0.02030166  0.09914155 -0.02801351]', '[ 0.00031733 -0.02489487  0.10765546 -0.0138725 ]', '[ 0.02044082 -0.02428802  0.08954248  0.02288616]', '[ 0.03470698 -0.01491644  0.05056501  0.07132823]', '[ 0.02674144  0.03818636 -0.12667052  0.44879208]', '[-0.01270905  0.15667936 -0.25571586  0.70881747]', '[-0.06940829  0.30836147 -0.29491305  0.77301892]', '[-0.12394901  0.4517198  -0.23590169  0.62988145]', '[-0.15876359  0.5498143  -0.10369689  0.33260441]', '[-0.16331677  0.57991751  0.05921824 -0.03571874]', '[-0.12364641  0.50409537  0.32874453 -0.70766221]', '[-0.03775164  0.30783049  0.50916352 -1.21389118]', '[ 0.06909397  0.04061776  0.52882372 -1.39480458]', '[ 0.16087913 -0.22270668  0.3614133  -1.17772404]', '[ 0.20472536 -0.40990137  0.06420388 -0.6597987 ]', '[ 0.18455416 -0.47825444 -0.26212436 -0.01817226]', '[ 0.09156532 -0.38679677 -0.64742279  0.90761115]', '[-0.06271277 -0.13292697 -0.85786545  1.56672789]', '[-0.23333411  0.20632363 -0.80133675  1.73587805]', '[-0.36498881  0.52600302 -0.4801429   1.39142644]', '[-0.41539568  0.74217732 -0.01227622  0.7395642 ]', '[-0.36944782  0.81527715  0.46213933 -0.01083091]', '[-0.22642744  0.71066606  0.93936783 -1.01021577]', '[-0.00892589  0.42883145  1.18897233 -1.74077443]', '[ 0.22660096  0.0517002   1.1068182  -1.92405165]', '[ 0.41005532 -0.29693012  0.6808143  -1.47495926]', '[ 0.48521772 -0.51258559  0.05370639 -0.64539491]', '[ 0.417663   -0.51547329 -0.71588293  0.61057794]', '[ 0.20989945 -0.2789723  -1.31808193  1.6972301 ]', '[-0.08492151  0.12510753 -1.555619    2.21640575]', '[-0.37963177  0.55019577 -1.32030983  1.91504598]', '[-0.58989289  0.85617843 -0.74359286  1.09612783]', '[-0.66706415  0.97859659 -0.01685984  0.11844472]', '[-0.58535204  0.87309513  0.82205171 -1.16698164]', '[-0.34814683  0.51985272  1.50786441 -2.31349921]', '[-0.00845867 -0.01084392  1.80187214 -2.83660639]', '[ 0.33251678 -0.53972913  1.5220548  -2.29877877]', '[ 0.57395443 -0.88909757  0.8506743  -1.14546192]', '[ 0.66227792 -0.9897414   0.02017728  0.14415152]', '[ 0.56997838 -0.80175587 -0.93344798  1.72881771]', '[ 0.29908242 -0.30913141 -1.72312117  3.11534711]', '[-0.08315313  0.37699688 -1.98491703  3.51987652]', '[-0.44967675  1.01119311 -1.6016925   2.68937509]', '[-0.70314623  1.42828109 -0.90116783  1.46392917]', '[-0.80177252  1.59623253 -0.07487256  0.2180398 ]', '[-0.72394184  1.49081901  0.8443507  -1.27627909]', '[-0.47088945  1.08272659  1.65970504 -2.80278718]', '[-0.07741763  0.38520798  2.19752525 -4.04435356]', '[ 0.35720396 -0.43419659  2.00983042 -3.86699684]', '[ 0.68247785 -1.07790494  1.18689067 -2.48691537]', '[ 0.8218953  -1.42254632  0.19968977 -0.96426762]', '[ 0.75459258 -1.43976003 -0.85807324  0.79326183]', '[ 0.48761236 -1.10140602 -1.78195125  2.59637368]', '[ 0.05897502 -0.41058711 -2.42976401  4.19816012]', '[-0.4314646   0.47314784 -2.31833387  4.31615657]', '[-0.81672247  1.21668414 -1.46858326  3.02633097]', '[-1.00690155  1.67989017 -0.42147508  1.61848727]', '[-0.98493444  1.86772757  0.63078134  0.26001653]', '[-0.75610554  1.75789692  1.62055782 -1.36967148]', '[-0.35595715  1.31549434  2.3275385  -3.05204563]', '[ 0.15035756  0.55372516  2.65209298 -4.43210369]', '[ 0.65139012 -0.34680402  2.2070832  -4.25226899]', '[ 0.985684   -1.05481891  1.0818817  -2.7503158 ]', '[ 1.07698896 -1.44506632 -0.16850092 -1.15785884]', '[ 0.91472109 -1.49041281 -1.42578234  0.72126271]', '[ 0.52287851 -1.1461743  -2.44221275  2.73697075]', '[-0.0361505  -0.40732268 -3.04996577  4.50173997]', '[-0.63332802  0.52271794 -2.74921409  4.43041987]', '[-1.08521394  1.26868163 -1.71335421  2.97168385]', '[-1.30937357  1.72013613 -0.51800962  1.57270265]', '[-1.29116306  1.90318794  0.69559698  0.25067901]', '[-1.02953854  1.78773441  1.89146013 -1.44270084]', '[-0.55192063  1.30869456  2.83147306 -3.37840682]', '[ 0.07603713  0.44640653  3.34164683 -5.06850996]', '[ 0.71210682 -0.56024523  2.83323751 -4.58992558]', '[ 1.16215327 -1.30108095  1.62634935 -2.79800121]', '[ 1.35782358 -1.69718345  0.32701124 -1.20027476]', '[ 1.30144266 -1.80944427 -0.88549401  0.09265836]', '[ 0.99400401 -1.59936647 -2.16048181  2.0609052 ]', '[ 0.45252281 -0.96102535 -3.20685487  4.34885667]', '[-0.25244304  0.09156171 -3.65778063  5.77314362]', '[-0.91661372  1.13370092 -2.84149586  4.36606722]', '[-1.36878347  1.82860103 -1.66344369  2.65004852]', '[-1.57850251  2.21982629 -0.42967068  1.30072406]', '[-1.5405753   2.35359044  0.8058149   0.02656021]', '[-1.25317949  2.19845399  2.04745347 -1.62236049]', '[-0.73653364  1.68088959  3.06882828 -3.62086887]', '[-0.0477877   0.73109595  3.74656433 -5.8081108 ]', '[ 0.69354275 -0.49023316  3.4252725  -5.83763954]', '[ 1.25185642 -1.45301411  2.11107446 -3.75903698]', '[ 1.53705783 -2.02758588  0.74397487 -2.05720434]', '[ 1.55104324 -2.28919955 -0.59805463 -0.55966798]', '[ 1.29547026 -2.22135375 -1.93692724  1.279967  ]', '[ 0.79061624 -1.75322035 -3.06269786  3.47692178]', '[ 0.09089764 -0.80168826 -3.87853789  6.02093093]', '[-0.69741674  0.5149997  -3.73831066  6.50690418]', '[-1.32045812  1.61520414 -2.4407719   4.45914839]', '[-1.67462079  2.34218287 -1.10847324  2.8997805 ]', '[-1.76815669  2.79281948  0.15998958  1.61679382]', '[-1.6029545   2.94643857  1.48609456 -0.09452293]', '[-1.18230305  2.76783546  2.69502195 -1.71300589]', '[-0.55016829  2.24939377  3.52428904 -3.50965378]', '[ 0.18136183  1.35288664  3.71109857 -5.44534145]', '[ 0.90612574  0.12465753  3.39498322 -6.4625698 ]', '[ 1.45594573 -1.03225026  1.98044985 -4.86581396]', '[ 1.68684443 -1.82657166  0.33063116 -3.13510082]', '[ 1.5916107  -2.29295399 -1.26529319 -1.50542563]', '[ 1.18664015 -2.39097767 -2.73298415  0.57118435]', '[ 0.5309742  -2.04772769 -3.70855831  2.89376443]', '[-0.24506756 -1.23143077 -3.95570213  5.22298451]', '[-1.01714361 -0.03100536 -3.61851786  6.37112832]', '[-1.61614472  1.12337344 -2.27213091  4.97315001]', '[-1.91925411  1.97355762 -0.76347825  3.60240829]', '[-1.92492648  2.57624902  0.68896904  2.41293315]', '[-1.6413515   2.8865666   2.12389129  0.66031887]', '[-1.08846     2.85099205  3.36773225 -1.02679203]', '[-0.32846545  2.47603458  4.08853382 -2.71222607]', '[ 0.47542966  1.78201064  3.80351195 -4.14302619]', '[ 1.15770037  0.87349878  2.97543297 -4.76827692]', '[ 1.64787089 -0.04458396  1.87569526 -4.24106039]', '[ 1.89167472 -0.78577978  0.5369341  -3.14819288]', '[ 1.85221976 -1.2976897  -0.96355732 -1.91879435]', '[ 1.48692181 -1.48855962 -2.68848191  0.14152842]', '[ 0.79155997 -1.18253063 -4.19035462  3.03199758]', '[-0.14349073 -0.2799125  -4.97815382  5.66345249]', '[-1.09002765  0.80867125 -4.26479466  4.67470096]', '[-1.81705093  1.53032135 -3.01260358  2.65933112]', '[-2.3096281   1.9414232  -1.96072211  1.6079987 ]', '[-2.62089397  2.22139443 -1.19852491  1.27827528]', '[-2.80422995  2.47491944 -0.66672102  1.28955961]', '[-2.89708388  2.74208234 -0.28205853  1.38025187]', '[-2.92352738e+00  3.02131725e+00  2.77850998e-03  1.39049145e+00]', '[-2.88848059 -3.03520941  0.34435169  0.84566862]', '[-2.78262066 -2.93707759  0.73314671  0.10164881]', '[-2.58337424 -3.0084998   1.30021428 -0.85204317]', '[-2.24850283  3.00872707  2.10450703 -1.85926233]', '[-1.72090363  2.50207774  3.20458643 -3.31976978]', '[-0.9644246   1.61582144  4.35639025 -5.7563139 ]', '[ 0.0197627   0.13976522  5.31880935 -8.58550195]', '[ 1.00503618 -1.39138164  4.29261139 -6.11308541]', '[ 1.7366414  -2.34427631  3.04413759 -3.63881148]', '[ 2.23043987 -2.91552348  1.92860321 -2.18618931]', '[ 2.52669359  3.03760132  1.08400971 -1.15534145]', '[ 2.68045183  2.89547379  0.48616479 -0.28522888]', '[2.73514781 2.89820781 0.07221868 0.30036711]', '[ 2.7098547   3.01215952 -0.33277863  0.83352219]', '[ 2.58297282 -3.01307381 -0.96679868  1.75143018]', '[ 2.30590089 -2.56302617 -1.85571192  2.79413777]', '[ 1.8190061  -1.860393   -3.06848272  4.38895447]', '[ 1.05284341 -0.71585754 -4.64466718  7.23856997]', '[ 0.02169612  0.87140274 -5.33268474  7.69181303]', '[-0.99190082  2.10738134 -4.7382387   4.66354363]', '[-1.84419513  2.81014065 -3.73169851  2.56363582]', '[-2.49043923 -3.08411406 -2.80018755  1.46060746]', '[-3.00170396 -2.84333    -2.41922994  1.05809328]', '[ 2.78343741 -2.61604647 -2.66855816  1.34373156]', '[ 2.1740265  -2.24611917 -3.5159178   2.54714711]', '[ 1.35002321 -1.50236105 -4.77654843  5.18142257]', '[ 0.24906592 -0.08548319 -6.08536087  8.55137322]', '[-0.92594079  1.43615601 -5.39438753  5.90908248]', '[-1.89816059  2.30355891 -4.32484934  3.0353748 ]', '[-2.66973057  2.7580251  -3.47852836  1.75071226]', '[ 2.94493924  3.08430764 -3.34925149  1.69892097]', '[ 2.21855346 -2.7744956  -4.03681021  2.74949413]', '[ 1.30047452 -2.00186766 -5.16228066  5.29281588]', '[ 0.14869954 -0.52433709 -6.33314372  9.45071091]', '[-1.07585326  1.28915273 -5.53311621  7.55064023]', '[-2.0614779   2.47841525 -4.40187839  4.71285984]', '[-2.86635554 -2.97876261 -3.75331907  3.81349974]', '[ 2.66624946 -2.18924188 -3.90662461  4.32347849]', '[ 1.79197189 -1.13162488 -5.01045896  6.6139771 ]', '[ 0.62395337  0.49661066 -6.44410795  8.78814013]', '[-0.66358597  1.92730029 -6.27793956  5.11155575]', '[-1.83366105  2.60081256 -5.30081181  1.90331644]', '[-2.78608803  2.80328153 -4.33714816  0.40528819]', '[ 2.6517429   2.85973064 -4.29776463  0.38596051]', '[ 1.71153236  3.02858568 -5.23467776  1.45123673]', '[ 0.54313103 -2.79572246 -6.33063033  3.26673991]', '[-0.71403843 -1.90372268 -5.98579588  5.68024618]', '[-1.81628127 -0.5635191  -5.08296603  7.46769096]', '[-2.74622303  0.90323243 -4.22958763  6.90280737]']</t>
-  </si>
-  <si>
-    <t>[0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50, 51, 52, 53, 54, 55, 56, 57, 58, 59, 60, 61, 62, 63, 64, 65, 66, 67, 68, 69, 70, 71, 72, 73, 74, 75, 76, 77, 78, 79, 80, 81, 82, 83, 84, 85, 86, 87, 88, 89, 90, 91, 92, 93, 94, 95, 96, 97, 98, 99, 100, 101, 102, 103, 104, 105, 106, 107, 108, 109, 110, 111, 112, 113, 114, 115, 116, 117, 118, 119, 120, 121, 122, 123, 124, 125, 126, 127, 128, 129, 130, 131, 132, 133, 134, 135, 136, 137, 138, 139, 140, 141, 142, 143, 144, 145, 146, 147, 148, 149, 150, 151, 152, 153, 154, 155, 156, 157, 158, 159, 160, 161, 162, 163, 164, 165, 166, 167, 168, 169, 170, 171, 172, 173, 174, 175, 176, 177, 178, 179, 180, 181]</t>
-  </si>
-  <si>
-    <t>[array([-0.03763371, -0.01533471,  0.06554052, -0.01816017], dtype=float32), array([-0.0208055 , -0.02030166,  0.09914155, -0.02801351]), array([ 0.00031733, -0.02489487,  0.10765546, -0.0138725 ]), array([ 0.02044082, -0.02428802,  0.08954248,  0.02288616]), array([ 0.03470698, -0.01491644,  0.05056501,  0.07132823]), array([ 0.02674144,  0.03818636, -0.12667052,  0.44879208]), array([-0.01270905,  0.15667936, -0.25571586,  0.70881747]), array([-0.06940829,  0.30836147, -0.29491305,  0.77301892]), array([-0.12394901,  0.4517198 , -0.23590169,  0.62988145]), array([-0.15876359,  0.5498143 , -0.10369689,  0.33260441]), array([-0.16331677,  0.57991751,  0.05921824, -0.03571874]), array([-0.12364641,  0.50409537,  0.32874453, -0.70766221]), array([-0.03775164,  0.30783049,  0.50916352, -1.21389118]), array([ 0.06909397,  0.04061776,  0.52882372, -1.39480458]), array([ 0.16087913, -0.22270668,  0.3614133 , -1.17772404]), array([ 0.20472536, -0.40990137,  0.06420388, -0.6597987 ]), array([ 0.18455416, -0.47825444, -0.26212436, -0.01817226]), array([ 0.09156532, -0.38679677, -0.64742279,  0.90761115]), array([-0.06271277, -0.13292697, -0.85786545,  1.56672789]), array([-0.23333411,  0.20632363, -0.80133675,  1.73587805]), array([-0.36498881,  0.52600302, -0.4801429 ,  1.39142644]), array([-0.41539568,  0.74217732, -0.01227622,  0.7395642 ]), array([-0.36944782,  0.81527715,  0.46213933, -0.01083091]), array([-0.22642744,  0.71066606,  0.93936783, -1.01021577]), array([-0.00892589,  0.42883145,  1.18897233, -1.74077443]), array([ 0.22660096,  0.0517002 ,  1.1068182 , -1.92405165]), array([ 0.41005532, -0.29693012,  0.6808143 , -1.47495926]), array([ 0.48521772, -0.51258559,  0.05370639, -0.64539491]), array([ 0.417663  , -0.51547329, -0.71588293,  0.61057794]), array([ 0.20989945, -0.2789723 , -1.31808193,  1.6972301 ]), array([-0.08492151,  0.12510753, -1.555619  ,  2.21640575]), array([-0.37963177,  0.55019577, -1.32030983,  1.91504598]), array([-0.58989289,  0.85617843, -0.74359286,  1.09612783]), array([-0.66706415,  0.97859659, -0.01685984,  0.11844472]), array([-0.58535204,  0.87309513,  0.82205171, -1.16698164]), array([-0.34814683,  0.51985272,  1.50786441, -2.31349921]), array([-0.00845867, -0.01084392,  1.80187214, -2.83660639]), array([ 0.33251678, -0.53972913,  1.5220548 , -2.29877877]), array([ 0.57395443, -0.88909757,  0.8506743 , -1.14546192]), array([ 0.66227792, -0.9897414 ,  0.02017728,  0.14415152]), array([ 0.56997838, -0.80175587, -0.93344798,  1.72881771]), array([ 0.29908242, -0.30913141, -1.72312117,  3.11534711]), array([-0.08315313,  0.37699688, -1.98491703,  3.51987652]), array([-0.44967675,  1.01119311, -1.6016925 ,  2.68937509]), array([-0.70314623,  1.42828109, -0.90116783,  1.46392917]), array([-0.80177252,  1.59623253, -0.07487256,  0.2180398 ]), array([-0.72394184,  1.49081901,  0.8443507 , -1.27627909]), array([-0.47088945,  1.08272659,  1.65970504, -2.80278718]), array([-0.07741763,  0.38520798,  2.19752525, -4.04435356]), array([ 0.35720396, -0.43419659,  2.00983042, -3.86699684]), array([ 0.68247785, -1.07790494,  1.18689067, -2.48691537]), array([ 0.8218953 , -1.42254632,  0.19968977, -0.96426762]), array([ 0.75459258, -1.43976003, -0.85807324,  0.79326183]), array([ 0.48761236, -1.10140602, -1.78195125,  2.59637368]), array([ 0.05897502, -0.41058711, -2.42976401,  4.19816012]), array([-0.4314646 ,  0.47314784, -2.31833387,  4.31615657]), array([-0.81672247,  1.21668414, -1.46858326,  3.02633097]), array([-1.00690155,  1.67989017, -0.42147508,  1.61848727]), array([-0.98493444,  1.86772757,  0.63078134,  0.26001653]), array([-0.75610554,  1.75789692,  1.62055782, -1.36967148]), array([-0.35595715,  1.31549434,  2.3275385 , -3.05204563]), array([ 0.15035756,  0.55372516,  2.65209298, -4.43210369]), array([ 0.65139012, -0.34680402,  2.2070832 , -4.25226899]), array([ 0.985684  , -1.05481891,  1.0818817 , -2.7503158 ]), array([ 1.07698896, -1.44506632, -0.16850092, -1.15785884]), array([ 0.91472109, -1.49041281, -1.42578234,  0.72126271]), array([ 0.52287851, -1.1461743 , -2.44221275,  2.73697075]), array([-0.0361505 , -0.40732268, -3.04996577,  4.50173997]), array([-0.63332802,  0.52271794, -2.74921409,  4.43041987]), array([-1.08521394,  1.26868163, -1.71335421,  2.97168385]), array([-1.30937357,  1.72013613, -0.51800962,  1.57270265]), array([-1.29116306,  1.90318794,  0.69559698,  0.25067901]), array([-1.02953854,  1.78773441,  1.89146013, -1.44270084]), array([-0.55192063,  1.30869456,  2.83147306, -3.37840682]), array([ 0.07603713,  0.44640653,  3.34164683, -5.06850996]), array([ 0.71210682, -0.56024523,  2.83323751, -4.58992558]), array([ 1.16215327, -1.30108095,  1.62634935, -2.79800121]), array([ 1.35782358, -1.69718345,  0.32701124, -1.20027476]), array([ 1.30144266, -1.80944427, -0.88549401,  0.09265836]), array([ 0.99400401, -1.59936647, -2.16048181,  2.0609052 ]), array([ 0.45252281, -0.96102535, -3.20685487,  4.34885667]), array([-0.25244304,  0.09156171, -3.65778063,  5.77314362]), array([-0.91661372,  1.13370092, -2.84149586,  4.36606722]), array([-1.36878347,  1.82860103, -1.66344369,  2.65004852]), array([-1.57850251,  2.21982629, -0.42967068,  1.30072406]), array([-1.5405753 ,  2.35359044,  0.8058149 ,  0.02656021]), array([-1.25317949,  2.19845399,  2.04745347, -1.62236049]), array([-0.73653364,  1.68088959,  3.06882828, -3.62086887]), array([-0.0477877 ,  0.73109595,  3.74656433, -5.8081108 ]), array([ 0.69354275, -0.49023316,  3.4252725 , -5.83763954]), array([ 1.25185642, -1.45301411,  2.11107446, -3.75903698]), array([ 1.53705783, -2.02758588,  0.74397487, -2.05720434]), array([ 1.55104324, -2.28919955, -0.59805463, -0.55966798]), array([ 1.29547026, -2.22135375, -1.93692724,  1.279967  ]), array([ 0.79061624, -1.75322035, -3.06269786,  3.47692178]), array([ 0.09089764, -0.80168826, -3.87853789,  6.02093093]), array([-0.69741674,  0.5149997 , -3.73831066,  6.50690418]), array([-1.32045812,  1.61520414, -2.4407719 ,  4.45914839]), array([-1.67462079,  2.34218287, -1.10847324,  2.8997805 ]), array([-1.76815669,  2.79281948,  0.15998958,  1.61679382]), array([-1.6029545 ,  2.94643857,  1.48609456, -0.09452293]), array([-1.18230305,  2.76783546,  2.69502195, -1.71300589]), array([-0.55016829,  2.24939377,  3.52428904, -3.50965378]), array([ 0.18136183,  1.35288664,  3.71109857, -5.44534145]), array([ 0.90612574,  0.12465753,  3.39498322, -6.4625698 ]), array([ 1.45594573, -1.03225026,  1.98044985, -4.86581396]), array([ 1.68684443, -1.82657166,  0.33063116, -3.13510082]), array([ 1.5916107 , -2.29295399, -1.26529319, -1.50542563]), array([ 1.18664015, -2.39097767, -2.73298415,  0.57118435]), array([ 0.5309742 , -2.04772769, -3.70855831,  2.89376443]), array([-0.24506756, -1.23143077, -3.95570213,  5.22298451]), array([-1.01714361, -0.03100536, -3.61851786,  6.37112832]), array([-1.61614472,  1.12337344, -2.27213091,  4.97315001]), array([-1.91925411,  1.97355762, -0.76347825,  3.60240829]), array([-1.92492648,  2.57624902,  0.68896904,  2.41293315]), array([-1.6413515 ,  2.8865666 ,  2.12389129,  0.66031887]), array([-1.08846   ,  2.85099205,  3.36773225, -1.02679203]), array([-0.32846545,  2.47603458,  4.08853382, -2.71222607]), array([ 0.47542966,  1.78201064,  3.80351195, -4.14302619]), array([ 1.15770037,  0.87349878,  2.97543297, -4.76827692]), array([ 1.64787089, -0.04458396,  1.87569526, -4.24106039]), array([ 1.89167472, -0.78577978,  0.5369341 , -3.14819288]), array([ 1.85221976, -1.2976897 , -0.96355732, -1.91879435]), array([ 1.48692181, -1.48855962, -2.68848191,  0.14152842]), array([ 0.79155997, -1.18253063, -4.19035462,  3.03199758]), array([-0.14349073, -0.2799125 , -4.97815382,  5.66345249]), array([-1.09002765,  0.80867125, -4.26479466,  4.67470096]), array([-1.81705093,  1.53032135, -3.01260358,  2.65933112]), array([-2.3096281 ,  1.9414232 , -1.96072211,  1.6079987 ]), array([-2.62089397,  2.22139443, -1.19852491,  1.27827528]), array([-2.80422995,  2.47491944, -0.66672102,  1.28955961]), array([-2.89708388,  2.74208234, -0.28205853,  1.38025187]), array([-2.92352738e+00,  3.02131725e+00,  2.77850998e-03,  1.39049145e+00]), array([-2.88848059, -3.03520941,  0.34435169,  0.84566862]), array([-2.78262066, -2.93707759,  0.73314671,  0.10164881]), array([-2.58337424, -3.0084998 ,  1.30021428, -0.85204317]), array([-2.24850283,  3.00872707,  2.10450703, -1.85926233]), array([-1.72090363,  2.50207774,  3.20458643, -3.31976978]), array([-0.9644246 ,  1.61582144,  4.35639025, -5.7563139 ]), array([ 0.0197627 ,  0.13976522,  5.31880935, -8.58550195]), array([ 1.00503618, -1.39138164,  4.29261139, -6.11308541]), array([ 1.7366414 , -2.34427631,  3.04413759, -3.63881148]), array([ 2.23043987, -2.91552348,  1.92860321, -2.18618931]), array([ 2.52669359,  3.03760132,  1.08400971, -1.15534145]), array([ 2.68045183,  2.89547379,  0.48616479, -0.28522888]), array([2.73514781, 2.89820781, 0.07221868, 0.30036711]), array([ 2.7098547 ,  3.01215952, -0.33277863,  0.83352219]), array([ 2.58297282, -3.01307381, -0.96679868,  1.75143018]), array([ 2.30590089, -2.56302617, -1.85571192,  2.79413777]), array([ 1.8190061 , -1.860393  , -3.06848272,  4.38895447]), array([ 1.05284341, -0.71585754, -4.64466718,  7.23856997]), array([ 0.02169612,  0.87140274, -5.33268474,  7.69181303]), array([-0.99190082,  2.10738134, -4.7382387 ,  4.66354363]), array([-1.84419513,  2.81014065, -3.73169851,  2.56363582]), array([-2.49043923, -3.08411406, -2.80018755,  1.46060746]), array([-3.00170396, -2.84333   , -2.41922994,  1.05809328]), array([ 2.78343741, -2.61604647, -2.66855816,  1.34373156]), array([ 2.1740265 , -2.24611917, -3.5159178 ,  2.54714711]), array([ 1.35002321, -1.50236105, -4.77654843,  5.18142257]), array([ 0.24906592, -0.08548319, -6.08536087,  8.55137322]), array([-0.92594079,  1.43615601, -5.39438753,  5.90908248]), array([-1.89816059,  2.30355891, -4.32484934,  3.0353748 ]), array([-2.66973057,  2.7580251 , -3.47852836,  1.75071226]), array([ 2.94493924,  3.08430764, -3.34925149,  1.69892097]), array([ 2.21855346, -2.7744956 , -4.03681021,  2.74949413]), array([ 1.30047452, -2.00186766, -5.16228066,  5.29281588]), array([ 0.14869954, -0.52433709, -6.33314372,  9.45071091]), array([-1.07585326,  1.28915273, -5.53311621,  7.55064023]), array([-2.0614779 ,  2.47841525, -4.40187839,  4.71285984]), array([-2.86635554, -2.97876261, -3.75331907,  3.81349974]), array([ 2.66624946, -2.18924188, -3.90662461,  4.32347849]), array([ 1.79197189, -1.13162488, -5.01045896,  6.6139771 ]), array([ 0.62395337,  0.49661066, -6.44410795,  8.78814013]), array([-0.66358597,  1.92730029, -6.27793956,  5.11155575]), array([-1.83366105,  2.60081256, -5.30081181,  1.90331644]), array([-2.78608803,  2.80328153, -4.33714816,  0.40528819]), array([ 2.6517429 ,  2.85973064, -4.29776463,  0.38596051]), array([ 1.71153236,  3.02858568, -5.23467776,  1.45123673]), array([ 0.54313103, -2.79572246, -6.33063033,  3.26673991]), array([-0.71403843, -1.90372268, -5.98579588,  5.68024618]), array([-1.81628127, -0.5635191 , -5.08296603,  7.46769096]), array([-2.74622303,  0.90323243, -4.22958763,  6.90280737])]</t>
-  </si>
-  <si>
-    <t>['[1,1,2]', '[0,2,1]', '[2,2,2]', '[2,1,0]', '[0,1,1]', '[0,0,0]', '[1,0,2]', '[1,1,1]', '[2,0,1]', '[1,2,0]']</t>
-  </si>
-  <si>
-    <t>[1,2,0]</t>
-  </si>
-  <si>
-    <t>[8, 11, 18, 28, 29, 33, 36, 39, 40, 42, 49, 60, 63, 68, 80, 83, 85, 90, 95, 97, 104, 113]</t>
-  </si>
-  <si>
-    <t>[0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 1, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 1, 0, 0, 0, 0, 0, 0, 0, 1, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 1, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 1, 2]</t>
-  </si>
-  <si>
-    <t>['[-0.03763371 -0.01533471  0.06554052 -0.01816017]', '[-0.00754409 -0.05458322  0.2277812  -0.36241836]', '[ 0.04879627 -0.15231473  0.32089719 -0.5887683 ]', '[ 0.11397169 -0.27767857  0.31375488 -0.63332862]', '[ 0.16759438 -0.39312519  0.2086893  -0.49480525]', '[ 0.1930193  -0.46685036  0.03906408 -0.22816919]', '[ 0.15689524 -0.41528579 -0.3922057   0.73207416]', '[ 0.04309269 -0.18588535 -0.71796191  1.51055937]', '[-0.08833617  0.09066275 -0.55988174  1.1839315 ]', '[-0.19460404  0.3314577  -0.47333723  1.1656441 ]', '[-0.2670624   0.53551493 -0.23226808  0.83448453]', '[-0.25813385  0.5892432   0.31842052 -0.29993036]', '[-0.14479216  0.42081771  0.79147863 -1.35065554]', '[ 0.0441876   0.07261958  1.05036241 -2.04391292]', '[ 0.25161682 -0.35143163  0.96480901 -2.08211344]', '[ 0.40862752 -0.71920374  0.56764403 -1.52484111]', '[ 0.46897685 -0.94310086  0.02606352 -0.69071794]', '[ 0.39771181 -0.93272785 -0.72330123  0.78802983]', '[ 0.21254615 -0.69636808 -1.0923829   1.5323607 ]', '[-0.04586502 -0.28067691 -1.43536108  2.53136619]', '[-0.33149752  0.26013203 -1.33943714  2.71852832]', '[-0.55082574  0.74779606 -0.80045364  2.06045225]', '[-0.63851854  1.06156915 -0.06359029  1.05066682]', '[-0.57675516  1.16316502  0.66687658 -0.037235  ]', '[-0.36152328  0.99201206  1.44864912 -1.66019691]', '[-0.01601426  0.51332788  1.94444975 -3.04341664]', '[ 0.38055854 -0.16180486  1.91172364 -3.49231095]', '[ 0.70416996 -0.79655028  1.2473567  -2.71748419]', '[ 0.85091301 -1.19415617  0.20734184 -1.24771155]', '[ 0.78800205 -1.29473673 -0.82154868  0.24594083]', '[ 0.52305653 -1.06570472 -1.79050475  2.04657543]', '[ 0.0919325  -0.48553085 -2.44717674  3.65974638]', '[-0.4091227   0.31171552 -2.41948576  4.0204088 ]', '[-0.79924091  0.95725787 -1.4181385   2.34473101]', '[-0.98583815  1.30220067 -0.42926566  1.10214787]', '[-0.96826411  1.39840947  0.60058776 -0.14506984]', '[-0.74232367  1.21287429  1.63138178 -1.72459384]', '[-0.32091457  0.67790948  2.52658795 -3.58632477]', '[ 0.22885645 -0.15822106  2.82050563 -4.4702325 ]', '[ 0.72810105 -0.93990057  2.06744853 -3.16326985]', '[ 1.03484668 -1.40552377  0.97538929 -1.50811478]', '[ 1.12211995 -1.57749452 -0.10845954 -0.21979109]', '[ 0.99279394 -1.49173967 -1.17124705  1.09242704]', '[ 0.64430798 -1.0781895  -2.2826548   3.07182432]', '[ 0.09991942 -0.27071063 -3.05962874  4.83370354]', '[-0.50793551  0.70427962 -2.83720017  4.53100606]', '[-0.98658498  1.4543064  -1.89599451  2.93349288]', '[-1.25551792  1.89061262 -0.77741414  1.46701159]', '[-1.29423674  2.05036526  0.39046254  0.13526902]', '[-1.09552389  1.91774253  1.57692627 -1.48958385]', '[-0.66765646  1.41341707  2.66730605 -3.61075697]', '[-0.04509971  0.4613782   3.47329389 -5.78365674]', '[ 0.64110363 -0.722221    3.15800653 -5.53620389]', '[ 1.161187   -1.64418634  2.00262976 -3.68253206]', '[ 1.43748734 -2.22323363  0.75504197 -2.16292232]', '[ 1.46311253 -2.51988507 -0.49383777 -0.80697515]', '[ 1.23208419 -2.50136653 -1.79328133  1.01207064]', '[ 0.76208675 -2.10257416 -2.8452418   3.02021349]', '[ 0.12240499 -1.27213879 -3.49850775  5.32298217]', '[-0.61098848 -0.00817598 -3.65675028  6.89361436]', '[-1.21059102  1.17914158 -2.21177861  4.73577944]', '[-1.50867933  1.95808142 -0.76730993  3.11657585]', '[-1.51991728  2.43973582  0.64156345  1.70286858]', '[-1.26018217  2.63362075  1.92699586  0.2199674 ]', '[-0.75579008  2.4836043   3.03764802 -1.72510332]', '[-0.0912597   1.94423543  3.48173787 -3.65494725]', '[ 0.59547711  1.03782142  3.32631488 -5.32335632]', '[ 1.21109791 -0.10346103  2.70111183 -5.75147147]', '[ 1.6055138  -1.10423254  1.17388475 -4.15834239]', '[ 1.67999453 -1.79739096 -0.44750835 -2.76163089]', '[ 1.42561732 -2.19173627 -2.07387128 -1.11889819]', '[ 0.85991814 -2.17828189 -3.48265038  1.29934238]', '[ 0.0882437  -1.6636906  -4.0865091   3.82889421]', '[-0.72569436 -0.68027713 -3.96045001  5.80327466]', '[-1.44205659  0.49713336 -3.05273646  5.55760095]', '[-1.91167273  1.46539267 -1.63263534  4.1583276 ]', '[-2.09697633  2.1897377  -0.22451399  3.11941484]', '[-2.00500898  2.70876467  1.12757021  2.0329795 ]', '[-1.64653074  2.96537165  2.44667013  0.49738258]', '[-1.02531602  2.87973312  3.72324536 -1.36233166]', '[-0.20394019  2.439779    4.32613767 -3.02755975]', '[ 0.63605889  1.66485317  3.94082937 -4.63628815]', '[ 1.34910545  0.63792562  3.16622383 -5.45731556]', '[ 1.86988674 -0.39363011  1.98359087 -4.6827815 ]', '[ 2.14022539 -1.24523183  0.69033453 -3.83471646]', '[ 2.12328437 -1.89947129 -0.8896648  -2.66773002]', '[ 1.77638455 -2.27838746 -2.57843757 -1.00783263]', '[ 1.09804528 -2.23465033 -4.1264691   1.55954217]', '[ 0.1799206  -1.61884135 -4.89830698  4.64101276]', '[-0.8103894  -0.40703723 -4.88068049  7.12868951]', '[-1.65973004  0.89011411 -3.46863373  5.40765756]', '[-2.22266284  1.81965423 -2.21145945  4.03922656]', '[-2.56375474  2.55735945 -1.25050678  3.4168274 ]', '[-2.74622161 -3.08395533 -0.64498693  3.00763927]', '[-2.84767593 -2.52744386 -0.42059816  2.54290134]', '[-2.91078153 -2.11640621 -0.21158439  1.54198759]', '[-2.94456769 -1.87492642 -0.12195223  0.86189772]', '[-2.94130431 -1.82141892  0.16069846 -0.33361684]', '[-2.8869942  -1.98550422  0.38455856 -1.30379426]', '[-2.78631026 -2.33999974  0.63018143 -2.23102674]', '[-2.62079503 -2.89358544  1.06549892 -3.29486113]', '[-2.33177904  2.62347432  1.91804096 -4.40718593]', '[-1.81528147  1.58361779  3.34209814 -6.21145145]', '[-0.95744365  0.03087473  5.14275857 -9.07918361]', '[ 0.09323898 -1.63013188  5.15004544 -6.86395732]', '[ 1.0940178  -2.74222218  4.73343807 -4.42861371]', '[ 1.93288913  2.8065319   3.60518792 -3.06054733]', '[ 2.55307376  2.28183795  2.68776808 -2.24604793]', '[ 3.04848862  1.88387373  2.37234964 -1.81156835]', '[-2.74055082  1.51675828  2.67551155 -1.99665812]', '[-2.12165668  1.01556015  3.62498974 -3.23016168]', '[-1.2519251   0.14710478  5.09056067 -5.41633365]', '[-0.1432818  -0.94540577  5.74555248 -4.7821921 ]', '[ 0.93478893 -1.53226766  4.7855712  -0.9389217 ]', '[ 1.69247666 -1.37251531  2.68235272  2.35008781]', '[ 1.9969893  -0.65284622  0.45383323  4.64389842]', '[ 1.925952    0.4374539  -0.96905959  6.03734874]']</t>
-  </si>
-  <si>
-    <t>[array([-0.03763371, -0.01533471,  0.06554052, -0.01816017], dtype=float32), array([-0.00754409, -0.05458322,  0.2277812 , -0.36241836]), array([ 0.04879627, -0.15231473,  0.32089719, -0.5887683 ]), array([ 0.11397169, -0.27767857,  0.31375488, -0.63332862]), array([ 0.16759438, -0.39312519,  0.2086893 , -0.49480525]), array([ 0.1930193 , -0.46685036,  0.03906408, -0.22816919]), array([ 0.15689524, -0.41528579, -0.3922057 ,  0.73207416]), array([ 0.04309269, -0.18588535, -0.71796191,  1.51055937]), array([-0.08833617,  0.09066275, -0.55988174,  1.1839315 ]), array([-0.19460404,  0.3314577 , -0.47333723,  1.1656441 ]), array([-0.2670624 ,  0.53551493, -0.23226808,  0.83448453]), array([-0.25813385,  0.5892432 ,  0.31842052, -0.29993036]), array([-0.14479216,  0.42081771,  0.79147863, -1.35065554]), array([ 0.0441876 ,  0.07261958,  1.05036241, -2.04391292]), array([ 0.25161682, -0.35143163,  0.96480901, -2.08211344]), array([ 0.40862752, -0.71920374,  0.56764403, -1.52484111]), array([ 0.46897685, -0.94310086,  0.02606352, -0.69071794]), array([ 0.39771181, -0.93272785, -0.72330123,  0.78802983]), array([ 0.21254615, -0.69636808, -1.0923829 ,  1.5323607 ]), array([-0.04586502, -0.28067691, -1.43536108,  2.53136619]), array([-0.33149752,  0.26013203, -1.33943714,  2.71852832]), array([-0.55082574,  0.74779606, -0.80045364,  2.06045225]), array([-0.63851854,  1.06156915, -0.06359029,  1.05066682]), array([-0.57675516,  1.16316502,  0.66687658, -0.037235  ]), array([-0.36152328,  0.99201206,  1.44864912, -1.66019691]), array([-0.01601426,  0.51332788,  1.94444975, -3.04341664]), array([ 0.38055854, -0.16180486,  1.91172364, -3.49231095]), array([ 0.70416996, -0.79655028,  1.2473567 , -2.71748419]), array([ 0.85091301, -1.19415617,  0.20734184, -1.24771155]), array([ 0.78800205, -1.29473673, -0.82154868,  0.24594083]), array([ 0.52305653, -1.06570472, -1.79050475,  2.04657543]), array([ 0.0919325 , -0.48553085, -2.44717674,  3.65974638]), array([-0.4091227 ,  0.31171552, -2.41948576,  4.0204088 ]), array([-0.79924091,  0.95725787, -1.4181385 ,  2.34473101]), array([-0.98583815,  1.30220067, -0.42926566,  1.10214787]), array([-0.96826411,  1.39840947,  0.60058776, -0.14506984]), array([-0.74232367,  1.21287429,  1.63138178, -1.72459384]), array([-0.32091457,  0.67790948,  2.52658795, -3.58632477]), array([ 0.22885645, -0.15822106,  2.82050563, -4.4702325 ]), array([ 0.72810105, -0.93990057,  2.06744853, -3.16326985]), array([ 1.03484668, -1.40552377,  0.97538929, -1.50811478]), array([ 1.12211995, -1.57749452, -0.10845954, -0.21979109]), array([ 0.99279394, -1.49173967, -1.17124705,  1.09242704]), array([ 0.64430798, -1.0781895 , -2.2826548 ,  3.07182432]), array([ 0.09991942, -0.27071063, -3.05962874,  4.83370354]), array([-0.50793551,  0.70427962, -2.83720017,  4.53100606]), array([-0.98658498,  1.4543064 , -1.89599451,  2.93349288]), array([-1.25551792,  1.89061262, -0.77741414,  1.46701159]), array([-1.29423674,  2.05036526,  0.39046254,  0.13526902]), array([-1.09552389,  1.91774253,  1.57692627, -1.48958385]), array([-0.66765646,  1.41341707,  2.66730605, -3.61075697]), array([-0.04509971,  0.4613782 ,  3.47329389, -5.78365674]), array([ 0.64110363, -0.722221  ,  3.15800653, -5.53620389]), array([ 1.161187  , -1.64418634,  2.00262976, -3.68253206]), array([ 1.43748734, -2.22323363,  0.75504197, -2.16292232]), array([ 1.46311253, -2.51988507, -0.49383777, -0.80697515]), array([ 1.23208419, -2.50136653, -1.79328133,  1.01207064]), array([ 0.76208675, -2.10257416, -2.8452418 ,  3.02021349]), array([ 0.12240499, -1.27213879, -3.49850775,  5.32298217]), array([-0.61098848, -0.00817598, -3.65675028,  6.89361436]), array([-1.21059102,  1.17914158, -2.21177861,  4.73577944]), array([-1.50867933,  1.95808142, -0.76730993,  3.11657585]), array([-1.51991728,  2.43973582,  0.64156345,  1.70286858]), array([-1.26018217,  2.63362075,  1.92699586,  0.2199674 ]), array([-0.75579008,  2.4836043 ,  3.03764802, -1.72510332]), array([-0.0912597 ,  1.94423543,  3.48173787, -3.65494725]), array([ 0.59547711,  1.03782142,  3.32631488, -5.32335632]), array([ 1.21109791, -0.10346103,  2.70111183, -5.75147147]), array([ 1.6055138 , -1.10423254,  1.17388475, -4.15834239]), array([ 1.67999453, -1.79739096, -0.44750835, -2.76163089]), array([ 1.42561732, -2.19173627, -2.07387128, -1.11889819]), array([ 0.85991814, -2.17828189, -3.48265038,  1.29934238]), array([ 0.0882437 , -1.6636906 , -4.0865091 ,  3.82889421]), array([-0.72569436, -0.68027713, -3.96045001,  5.80327466]), array([-1.44205659,  0.49713336, -3.05273646,  5.55760095]), array([-1.91167273,  1.46539267, -1.63263534,  4.1583276 ]), array([-2.09697633,  2.1897377 , -0.22451399,  3.11941484]), array([-2.00500898,  2.70876467,  1.12757021,  2.0329795 ]), array([-1.64653074,  2.96537165,  2.44667013,  0.49738258]), array([-1.02531602,  2.87973312,  3.72324536, -1.36233166]), array([-0.20394019,  2.439779  ,  4.32613767, -3.02755975]), array([ 0.63605889,  1.66485317,  3.94082937, -4.63628815]), array([ 1.34910545,  0.63792562,  3.16622383, -5.45731556]), array([ 1.86988674, -0.39363011,  1.98359087, -4.6827815 ]), array([ 2.14022539, -1.24523183,  0.69033453, -3.83471646]), array([ 2.12328437, -1.89947129, -0.8896648 , -2.66773002]), array([ 1.77638455, -2.27838746, -2.57843757, -1.00783263]), array([ 1.09804528, -2.23465033, -4.1264691 ,  1.55954217]), array([ 0.1799206 , -1.61884135, -4.89830698,  4.64101276]), array([-0.8103894 , -0.40703723, -4.88068049,  7.12868951]), array([-1.65973004,  0.89011411, -3.46863373,  5.40765756]), array([-2.22266284,  1.81965423, -2.21145945,  4.03922656]), array([-2.56375474,  2.55735945, -1.25050678,  3.4168274 ]), array([-2.74622161, -3.08395533, -0.64498693,  3.00763927]), array([-2.84767593, -2.52744386, -0.42059816,  2.54290134]), array([-2.91078153, -2.11640621, -0.21158439,  1.54198759]), array([-2.94456769, -1.87492642, -0.12195223,  0.86189772]), array([-2.94130431, -1.82141892,  0.16069846, -0.33361684]), array([-2.8869942 , -1.98550422,  0.38455856, -1.30379426]), array([-2.78631026, -2.33999974,  0.63018143, -2.23102674]), array([-2.62079503, -2.89358544,  1.06549892, -3.29486113]), array([-2.33177904,  2.62347432,  1.91804096, -4.40718593]), array([-1.81528147,  1.58361779,  3.34209814, -6.21145145]), array([-0.95744365,  0.03087473,  5.14275857, -9.07918361]), array([ 0.09323898, -1.63013188,  5.15004544, -6.86395732]), array([ 1.0940178 , -2.74222218,  4.73343807, -4.42861371]), array([ 1.93288913,  2.8065319 ,  3.60518792, -3.06054733]), array([ 2.55307376,  2.28183795,  2.68776808, -2.24604793]), array([ 3.04848862,  1.88387373,  2.37234964, -1.81156835]), array([-2.74055082,  1.51675828,  2.67551155, -1.99665812]), array([-2.12165668,  1.01556015,  3.62498974, -3.23016168]), array([-1.2519251 ,  0.14710478,  5.09056067, -5.41633365]), array([-0.1432818 , -0.94540577,  5.74555248, -4.7821921 ]), array([ 0.93478893, -1.53226766,  4.7855712 , -0.9389217 ]), array([ 1.69247666, -1.37251531,  2.68235272,  2.35008781]), array([ 1.9969893 , -0.65284622,  0.45383323,  4.64389842]), array([ 1.925952  ,  0.4374539 , -0.96905959,  6.03734874])]</t>
-  </si>
-  <si>
-    <t>['[0,0,0]', '[1,2,0]', '[2,2,2]', '[0,2,1]', '[1,1,2]', '[1,0,2]', '[2,0,1]', '[1,1,1]', '[2,1,0]', '[0,1,1]']</t>
-  </si>
-  <si>
-    <t>[2, 7, 8, 9, 12, 13, 14, 15, 16, 17, 22, 23, 25, 27, 29, 32, 33, 34, 36, 38, 39, 40, 48, 50, 51, 52, 53, 58, 60, 61, 64, 65, 66, 68, 70, 72, 75, 78, 79, 81, 91, 92, 93, 95, 98, 99, 100, 101, 102, 106, 107, 108, 109, 110, 112, 117, 120, 125, 126, 127, 128, 131, 140, 146, 147, 149, 151, 153, 154, 155, 156, 159, 160, 162, 163, 164, 166, 168, 170, 171, 177, 178, 180, 181, 182, 186, 190, 191, 192, 194]</t>
-  </si>
-  <si>
-    <t>[0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 1, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 2, 1, 0, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 1, 1, 2, 2, 2, 2, 2, 2, 2, 2, 2, 1, 1, 0, 0, 0, 0, 0, 0, 0]</t>
-  </si>
-  <si>
-    <t>['[-0.03763371 -0.01533471  0.06554052 -0.01816017]', '[-0.00754409 -0.05458322  0.2277812  -0.36241836]', '[ 0.03557041 -0.11811661  0.19275289 -0.25552579]', '[ 0.07892797 -0.1849336   0.22986116 -0.39424827]', '[ 0.12271824 -0.267417    0.19671429 -0.40996627]', '[ 0.15338212 -0.34091394  0.10180504 -0.30861109]', '[ 0.16107551 -0.38557729 -0.0273968  -0.13010444]', '[ 0.14258378 -0.39158197 -0.15378669  0.06807474]', '[ 0.1022     -0.36100556 -0.24101473  0.22671699]', '[ 0.05062109 -0.30678682 -0.26281254  0.29871133]', '[-0.02403093 -0.18110372 -0.4655087   0.92695417]', '[-0.12589896  0.04584632 -0.5250891   1.28673973]', '[-0.19544583  0.24011135 -0.15139978  0.61436426]', '[-0.18279216  0.28203161  0.27557174 -0.19862027]', '[-0.10308877  0.20002194  0.50304389 -0.59622521]', '[ 0.0088212   0.05774343  0.58895956 -0.78459825]', '[ 0.12073006 -0.09507966  0.50273749 -0.69964159]', '[ 0.19987599 -0.20598177  0.26998061 -0.37966868]', '[ 0.23654816 -0.27258837  0.08769904 -0.27038146]', '[ 0.20680966 -0.24186496 -0.37800971  0.56813749]', '[ 0.09241524 -0.05655722 -0.7374473   1.2365694 ]', '[-0.07276917  0.22557264 -0.87065722  1.50607249]', '[-0.21170649  0.44621003 -0.48761149  0.65011446]', '[-0.25932238  0.47377765  0.02078609 -0.38265415]', '[-0.20364025  0.2966798   0.52254252 -1.35732767]', '[-0.07442367 -0.01235199  0.73252255 -1.65772588]', '[ 0.08519429 -0.36572257  0.81756862 -1.78437309]', '[ 0.22218772 -0.65870302  0.52196489 -1.08951319]', '[ 0.29729799 -0.8181215   0.21447191 -0.47994719]', '[ 0.29321024 -0.8147959  -0.2541811   0.51194553]', '[ 0.18694294 -0.58671906 -0.79108875  1.74079129]', '[-0.01057443 -0.14130834 -1.13352413  2.61458448]', '[-0.21236432  0.33486888 -0.82372989  2.02388386]', '[-0.3224141   0.63286313 -0.25424804  0.90953997]', '[-0.31079212  0.69023306  0.36608528 -0.3375208 ]', '[-0.18159279  0.50295763  0.90084849 -1.50221934]', '[ 0.02115552  0.14753425  1.07589467 -1.96158934]', '[ 0.23828769 -0.27165869  1.03459086 -2.1141888 ]', '[ 0.39933364 -0.62155713  0.53899518 -1.31710911]', '[ 0.44516442 -0.78263441 -0.08743976 -0.27693951]', '[ 0.37768954 -0.76204057 -0.57402425  0.47469708]', '[ 0.20045733 -0.53739176 -1.16496896  1.73311586]', '[-0.06880709 -0.09791685 -1.46203867  2.54644039]', '[-0.3517817   0.41989775 -1.28913737  2.48285989]', '[-0.55767297  0.84668759 -0.72641089  1.71264936]', '[-0.63205709  1.08926912 -0.00804518  0.69578255]', '[-0.54131758  1.06559848  0.89791301 -0.92963106]', '[-0.28358096  0.72081644  1.64067802 -2.48624436]', '[ 0.07810167  0.13807672  1.88746398 -3.18119225]', '[ 0.44105459 -0.50139231  1.64027388 -3.01770028]', '[ 0.69051429 -0.98173318  0.81415598 -1.73120706]', '[ 0.75912306 -1.1873965  -0.13184387 -0.32246679]', '[ 0.65074533 -1.13781006 -0.93457911  0.81749734]', '[ 0.39692232 -0.8641383  -1.56178023  1.88891824]', '[ 0.02469386 -0.34377614 -2.08627627  3.20304579]', '[-0.39503475  0.33822706 -1.99292499  3.38602167]', '[-0.73004836  0.93120478 -1.29036977  2.43829526]', '[-0.89589954  1.29730046 -0.35064209  1.21313597]', '[-0.84988859  1.36295792  0.79850751 -0.55794729]', '[-0.58488562  1.06921946  1.82137864 -2.38989338]', '[-0.15110885  0.44573716  2.43798634 -3.7329311 ]', '[ 0.34088655 -0.33059967  2.34008924 -3.74489891]', '[ 0.74739807 -0.98870156  1.64589764 -2.71214813]', '[ 0.98131512 -1.40000842  0.67046987 -1.40094917]', '[ 1.00244361 -1.52655877 -0.45637805  0.13237276]', '[ 0.81266805 -1.36887547 -1.41836333  1.45674818]', '[ 0.44931641 -0.94146509 -2.16493735  2.79397982]', '[-0.04841148 -0.22073566 -2.70771022  4.23220808]', '[-0.5463286   0.55922311 -2.13804632  3.30347241]', '[-0.89284612  1.10643982 -1.27608161  2.11322524]', '[-1.02608199  1.34813156 -0.05069373  0.32110891]', '[-0.91393054  1.23573735  1.16222721 -1.45928986]', '[-0.57967201  0.78505052  2.14209164 -3.03612443]', '[-0.07240683  0.0231515   2.8106712  -4.36012379]', '[ 0.47718799 -0.81922328  2.54037448 -3.77686807]', '[ 0.89576544 -1.40237789  1.60052592 -2.04269414]', '[ 1.11495113 -1.67119362  0.5714533  -0.66665706]', '[ 1.11182384 -1.65044219 -0.60301219  0.87467368]', '[ 0.88597143 -1.33972624 -1.63594908  2.25295156]', '[ 0.47032856 -0.74473378 -2.46670775  3.65725716]', '[-0.08770158  0.12835395 -2.96254523  4.76852153]', '[-0.61716252  0.94503089 -2.21954201  3.1958199 ]', '[-0.97347126  1.44225206 -1.30535859  1.77317122]', '[-1.12975064  1.66185925 -0.24468304  0.43941926]', '[-1.05291825  1.57151757  1.00751438 -1.35601411]', '[-0.73155725  1.10591213  2.18683928 -3.33966424]', '[-0.1939038   0.23716645  3.08946978 -5.17722634]', '[ 0.42743603 -0.80083159  2.93187363 -4.79139821]', '[ 0.93063716 -1.59265865  2.0483019  -3.10192621]', '[ 1.23475661 -2.05726591  0.97214729 -1.58607278]', '[ 1.31438485 -2.23813384 -0.17983406 -0.23318806]', '[ 1.16467316 -2.14879548 -1.30246069  1.14358287]', '[ 0.80440369 -1.76951536 -2.26022383  2.68288357]', '[ 0.28068364 -1.06487481 -2.91888961  4.3478002 ]', '[-0.35116998 -0.02056817 -3.24105396  5.75631643]', '[-0.90358572  0.97980186 -2.15550948  3.99908659]', '[-1.21709924  1.62440251 -0.96065921  2.47077898]', '[-1.28513349  1.97915683  0.27881399  1.08570161]', '[-1.10304859  2.03287121  1.5155076  -0.56983712]', '[-0.6958137   1.73923997  2.4997484  -2.39630072]', '[-0.13019472  1.0676465   3.08735874 -4.291803  ]', '[ 0.50146553  0.08136796  3.07785859 -5.23949777]', '[ 1.02591909 -0.86057033  2.04528102 -3.93946123]', '[ 1.31033681 -1.50251161  0.77994925 -2.49400403]', '[ 1.33541228 -1.86513484 -0.52682926 -1.12885762]', '[ 1.09075006 -1.89949588 -1.88428337  0.8204828 ]', '[ 0.61796715 -1.56654541 -2.77658663  2.53368769]', '[ 0.01273532 -0.8910579  -3.18411561  4.12995568]', '[-0.60600353 -0.00627687 -2.84781631  4.37647027]', '[-1.06685323  0.7303139  -1.67849003  2.84070475]', '[-1.26525702  1.12218654 -0.29886617  1.09720955]', '[-1.20696065  1.22776118  0.87984831 -0.06151424]', '[-0.90810375  1.05605381  2.08171782 -1.69250782]', '[-0.38152736  0.51425049  3.10826569 -3.66292503]', '[ 0.2819929  -0.31718017  3.34736379 -4.28071341]', '[ 0.88777928 -1.05576078  2.60367452 -2.94147017]', '[ 1.30096333 -1.48638953  1.4991951  -1.40788084]', '[ 1.4723894  -1.61526411  0.20905008  0.07986584]', '[ 1.37487925 -1.43390387 -1.18520272  1.75870581]', '[ 0.99848097 -0.8887541  -2.5713268   3.75658705]', '[ 0.3891489  -0.00690142 -3.39273887  4.80720652]', '[-0.30705885  0.92811283 -3.39229086  4.16594096]', '[-0.91929375  1.58085892 -2.65215401  2.32833063]', '[-1.34426808  1.8745403  -1.55704869  0.66743164]', '[-1.5326826   1.87081958 -0.31707106 -0.66201219]', '[-1.46166539  1.59443103  1.02906079 -2.11483199]', '[-1.12091097  1.00648635  2.37429303 -3.82656933]', '[-0.52448253  0.06240541  3.47918028 -5.40234683]', '[ 0.19032962 -0.97001716  3.48610722 -4.5125547 ]', '[ 0.83352702 -1.68933332  2.86393435 -2.63720212]', '[ 1.30839368 -2.03746812  1.83291794 -0.90005855]', '[ 1.54582143 -2.05050343  0.52328489  0.72342792]', '[ 1.50598521 -1.73540157 -0.93073203  2.43926455]', '[ 1.16959531 -1.05273102 -2.44289514  4.47681816]', '[ 0.53715845  0.0657058  -3.74409698  6.42447655]', '[-0.22931294  1.28115727 -3.73593374  5.29554355]', '[-0.9222339   2.13359818 -3.12535296  3.25743615]', '[-1.45088288  2.61086761 -2.10788115  1.58127759]', '[-1.75508133  2.78651333 -0.92825059  0.21078278]', '[-1.82278494  2.70463992  0.25102486 -1.01706009]', '[-1.64665183  2.35867185  1.5172924  -2.47003426]', '[-1.20648839  1.66837018  2.89346739 -4.55942038]', '[-0.48359862  0.47131205  4.29055666 -7.38192442]', '[ 0.40116901 -1.02654273  4.23995773 -6.82239701]', '[ 1.15577687 -2.13829462  3.28002394 -4.3889663 ]', '[ 1.70179183 -2.83939155  2.15818148 -2.73024659]', '[ 2.01378734  3.04712437  0.97997264 -1.26606514]', '[ 2.10134067  2.93317619 -0.09368171  0.12354459]', '[ 1.96936175  3.11630222 -1.24075801  1.71210838]', '[ 1.60853283 -2.697458   -2.38019704  3.02488122]', '[ 1.00701098 -1.88131571 -3.62181726  5.29481985]', '[ 0.17910039 -0.55790013 -4.59124251  7.86097242]', '[-0.73065554  1.02473276 -4.16487299  7.13131546]', '[-1.41752373  2.1448718  -2.73059828  4.26641238]', '[-1.8293337   2.79958172 -1.39993991  2.37846452]', '[-1.98421857  3.11349381 -0.16403789  0.77311699]', '[-1.90876329 -3.13613359  0.92371315 -0.44582519]', '[-1.59815657  2.89050634  2.19133703 -2.14603177]', '[-1.03643729  2.26746603  3.38599281 -4.18237461]', '[-0.27131882  1.18487869  4.23690778 -6.75946389]', '[ 0.61843646 -0.36047098  4.34788966 -7.91576092]', '[ 1.35316452 -1.71325137  2.92208093 -5.50691455]', '[ 1.79031205 -2.61124735  1.4841508  -3.61886212]', '[ 1.96070467  3.09489453  0.25404525 -2.1717855 ]', '[ 1.8999521   2.80436892 -0.85973884 -0.72611352]', '[ 1.6049449   2.82513165 -2.11083868  0.92524552]', '[ 1.06437247  3.12864871 -3.26825561  2.09398639]', '[ 0.32007023 -2.58274118 -4.0260958   3.64082047]', '[-0.46273148 -1.73740385 -3.67307745  4.76399222]', '[-1.14184999 -0.66711327 -3.08949793  5.79357238]', '[-1.640783    0.40832601 -1.79946806  4.71702006]', '[-1.83890984  1.18509381 -0.16126993  3.05632675]', '[-1.71571601  1.67695571  1.4229505   1.77968836]', '[-1.25347978  1.80606384  3.15279071 -0.60677766]', '[-0.49071241  1.39023451  4.35636575 -3.61650119]', '[ 0.43700721  0.37946059  4.76045311 -6.16679079]', '[ 1.31634039 -0.81404734  3.84128083 -5.25684481]', '[ 1.94339966 -1.65365457  2.46707516 -3.28941925]', '[ 2.32084975 -2.1925768   1.34693979 -2.21252967]', '[ 2.50150889 -2.58474251  0.4848395  -1.73301044]', '[ 2.50983917 -2.84502159 -0.39090523 -0.85223766]', '[ 2.34291184 -2.91241433 -1.29928919  0.2219188 ]', '[ 1.98851099 -2.77367907 -2.2825769   1.23388618]', '[ 1.40719341 -2.34373073 -3.52790219  3.19159277]', '[ 0.59130194 -1.43184446 -4.59968577  6.11109068]', '[-0.41603753  0.10900948 -5.22032363  8.61601101]', '[-1.32372611  1.55160929 -3.73510107  5.52715599]', '[-1.944739    2.45339858 -2.5077234   3.68358306]', '[-2.34146068  3.07705742 -1.50917239  2.62704548]', '[-2.56966206 -2.76508321 -0.82318186  1.79812805]', '[-2.6723401  -2.52614596 -0.22403399  0.58785974]', '[-2.67521464 -2.49093087  0.19479118 -0.23783541]', '[-2.59118494 -2.62244497  0.66234711 -1.08070743]', '[-2.38719541 -2.96473382  1.41693406 -2.34946616]', '[-2.00986273  2.7316622   2.40996767 -3.57402296]', '[-1.39904486  1.8228875   3.74092821 -5.72500935]', '[-0.48935378  0.33082853  5.30661477 -9.10709481]', '[ 0.56532342 -1.40022853  4.89842119 -7.29828993]', '[ 1.4508575  -2.57128377  3.93914552 -4.65299331]', '[ 2.12850862  2.93734327  2.84579287 -3.23650721]']</t>
-  </si>
-  <si>
-    <t>[0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50, 51, 52, 53, 54, 55, 56, 57, 58, 59, 60, 61, 62, 63, 64, 65, 66, 67, 68, 69, 70, 71, 72, 73, 74, 75, 76, 77, 78, 79, 80, 81, 82, 83, 84, 85, 86, 87, 88, 89, 90, 91, 92, 93, 94, 95, 96, 97, 98, 99, 100, 101, 102, 103, 104, 105, 106, 107, 108, 109, 110, 111, 112, 113, 114, 115, 116, 117, 118, 119, 120, 121, 122, 123, 124, 125, 126, 127, 128, 129, 130, 131, 132, 133, 134, 135, 136, 137, 138, 139, 140, 141, 142, 143, 144, 145, 146, 147, 148, 149, 150, 151, 152, 153, 154, 155, 156, 157, 158, 159, 160, 161, 162, 163, 164, 165, 166, 167, 168, 169, 170, 171, 172, 173, 174, 175, 176, 177, 178, 179, 180, 181, 182, 183, 184, 185, 186, 187, 188, 189, 190, 191, 192, 193, 194, 195, 196, 197, 198, 199]</t>
-  </si>
-  <si>
-    <t>[array([-0.03763371, -0.01533471,  0.06554052, -0.01816017], dtype=float32), array([-0.00754409, -0.05458322,  0.2277812 , -0.36241836]), array([ 0.03557041, -0.11811661,  0.19275289, -0.25552579]), array([ 0.07892797, -0.1849336 ,  0.22986116, -0.39424827]), array([ 0.12271824, -0.267417  ,  0.19671429, -0.40996627]), array([ 0.15338212, -0.34091394,  0.10180504, -0.30861109]), array([ 0.16107551, -0.38557729, -0.0273968 , -0.13010444]), array([ 0.14258378, -0.39158197, -0.15378669,  0.06807474]), array([ 0.1022    , -0.36100556, -0.24101473,  0.22671699]), array([ 0.05062109, -0.30678682, -0.26281254,  0.29871133]), array([-0.02403093, -0.18110372, -0.4655087 ,  0.92695417]), array([-0.12589896,  0.04584632, -0.5250891 ,  1.28673973]), array([-0.19544583,  0.24011135, -0.15139978,  0.61436426]), array([-0.18279216,  0.28203161,  0.27557174, -0.19862027]), array([-0.10308877,  0.20002194,  0.50304389, -0.59622521]), array([ 0.0088212 ,  0.05774343,  0.58895956, -0.78459825]), array([ 0.12073006, -0.09507966,  0.50273749, -0.69964159]), array([ 0.19987599, -0.20598177,  0.26998061, -0.37966868]), array([ 0.23654816, -0.27258837,  0.08769904, -0.27038146]), array([ 0.20680966, -0.24186496, -0.37800971,  0.56813749]), array([ 0.09241524, -0.05655722, -0.7374473 ,  1.2365694 ]), array([-0.07276917,  0.22557264, -0.87065722,  1.50607249]), array([-0.21170649,  0.44621003, -0.48761149,  0.65011446]), array([-0.25932238,  0.47377765,  0.02078609, -0.38265415]), array([-0.20364025,  0.2966798 ,  0.52254252, -1.35732767]), array([-0.07442367, -0.01235199,  0.73252255, -1.65772588]), array([ 0.08519429, -0.36572257,  0.81756862, -1.78437309]), array([ 0.22218772, -0.65870302,  0.52196489, -1.08951319]), array([ 0.29729799, -0.8181215 ,  0.21447191, -0.47994719]), array([ 0.29321024, -0.8147959 , -0.2541811 ,  0.51194553]), array([ 0.18694294, -0.58671906, -0.79108875,  1.74079129]), array([-0.01057443, -0.14130834, -1.13352413,  2.61458448]), array([-0.21236432,  0.33486888, -0.82372989,  2.02388386]), array([-0.3224141 ,  0.63286313, -0.25424804,  0.90953997]), array([-0.31079212,  0.69023306,  0.36608528, -0.3375208 ]), array([-0.18159279,  0.50295763,  0.90084849, -1.50221934]), array([ 0.02115552,  0.14753425,  1.07589467, -1.96158934]), array([ 0.23828769, -0.27165869,  1.03459086, -2.1141888 ]), array([ 0.39933364, -0.62155713,  0.53899518, -1.31710911]), array([ 0.44516442, -0.78263441, -0.08743976, -0.27693951]), array([ 0.37768954, -0.76204057, -0.57402425,  0.47469708]), array([ 0.20045733, -0.53739176, -1.16496896,  1.73311586]), array([-0.06880709, -0.09791685, -1.46203867,  2.54644039]), array([-0.3517817 ,  0.41989775, -1.28913737,  2.48285989]), array([-0.55767297,  0.84668759, -0.72641089,  1.71264936]), array([-0.63205709,  1.08926912, -0.00804518,  0.69578255]), array([-0.54131758,  1.06559848,  0.89791301, -0.92963106]), array([-0.28358096,  0.72081644,  1.64067802, -2.48624436]), array([ 0.07810167,  0.13807672,  1.88746398, -3.18119225]), array([ 0.44105459, -0.50139231,  1.64027388, -3.01770028]), array([ 0.69051429, -0.98173318,  0.81415598, -1.73120706]), array([ 0.75912306, -1.1873965 , -0.13184387, -0.32246679]), array([ 0.65074533, -1.13781006, -0.93457911,  0.81749734]), array([ 0.39692232, -0.8641383 , -1.56178023,  1.88891824]), array([ 0.02469386, -0.34377614, -2.08627627,  3.20304579]), array([-0.39503475,  0.33822706, -1.99292499,  3.38602167]), array([-0.73004836,  0.93120478, -1.29036977,  2.43829526]), array([-0.89589954,  1.29730046, -0.35064209,  1.21313597]), array([-0.84988859,  1.36295792,  0.79850751, -0.55794729]), array([-0.58488562,  1.06921946,  1.82137864, -2.38989338]), array([-0.15110885,  0.44573716,  2.43798634, -3.7329311 ]), array([ 0.34088655, -0.33059967,  2.34008924, -3.74489891]), array([ 0.74739807, -0.98870156,  1.64589764, -2.71214813]), array([ 0.98131512, -1.40000842,  0.67046987, -1.40094917]), array([ 1.00244361, -1.52655877, -0.45637805,  0.13237276]), array([ 0.81266805, -1.36887547, -1.41836333,  1.45674818]), array([ 0.44931641, -0.94146509, -2.16493735,  2.79397982]), array([-0.04841148, -0.22073566, -2.70771022,  4.23220808]), array([-0.5463286 ,  0.55922311, -2.13804632,  3.30347241]), array([-0.89284612,  1.10643982, -1.27608161,  2.11322524]), array([-1.02608199,  1.34813156, -0.05069373,  0.32110891]), array([-0.91393054,  1.23573735,  1.16222721, -1.45928986]), array([-0.57967201,  0.78505052,  2.14209164, -3.03612443]), array([-0.07240683,  0.0231515 ,  2.8106712 , -4.36012379]), array([ 0.47718799, -0.81922328,  2.54037448, -3.77686807]), array([ 0.89576544, -1.40237789,  1.60052592, -2.04269414]), array([ 1.11495113, -1.67119362,  0.5714533 , -0.66665706]), array([ 1.11182384, -1.65044219, -0.60301219,  0.87467368]), array([ 0.88597143, -1.33972624, -1.63594908,  2.25295156]), array([ 0.47032856, -0.74473378, -2.46670775,  3.65725716]), array([-0.08770158,  0.12835395, -2.96254523,  4.76852153]), array([-0.61716252,  0.94503089, -2.21954201,  3.1958199 ]), array([-0.97347126,  1.44225206, -1.30535859,  1.77317122]), array([-1.12975064,  1.66185925, -0.24468304,  0.43941926]), array([-1.05291825,  1.57151757,  1.00751438, -1.35601411]), array([-0.73155725,  1.10591213,  2.18683928, -3.33966424]), array([-0.1939038 ,  0.23716645,  3.08946978, -5.17722634]), array([ 0.42743603, -0.80083159,  2.93187363, -4.79139821]), array([ 0.93063716, -1.59265865,  2.0483019 , -3.10192621]), array([ 1.23475661, -2.05726591,  0.97214729, -1.58607278]), array([ 1.31438485, -2.23813384, -0.17983406, -0.23318806]), array([ 1.16467316, -2.14879548, -1.30246069,  1.14358287]), array([ 0.80440369, -1.76951536, -2.26022383,  2.68288357]), array([ 0.28068364, -1.06487481, -2.91888961,  4.3478002 ]), array([-0.35116998, -0.02056817, -3.24105396,  5.75631643]), array([-0.90358572,  0.97980186, -2.15550948,  3.99908659]), array([-1.21709924,  1.62440251, -0.96065921,  2.47077898]), array([-1.28513349,  1.97915683,  0.27881399,  1.08570161]), array([-1.10304859,  2.03287121,  1.5155076 , -0.56983712]), array([-0.6958137 ,  1.73923997,  2.4997484 , -2.39630072]), array([-0.13019472,  1.0676465 ,  3.08735874, -4.291803  ]), array([ 0.50146553,  0.08136796,  3.07785859, -5.23949777]), array([ 1.02591909, -0.86057033,  2.04528102, -3.93946123]), array([ 1.31033681, -1.50251161,  0.77994925, -2.49400403]), array([ 1.33541228, -1.86513484, -0.52682926, -1.12885762]), array([ 1.09075006, -1.89949588, -1.88428337,  0.8204828 ]), array([ 0.61796715, -1.56654541, -2.77658663,  2.53368769]), array([ 0.01273532, -0.8910579 , -3.18411561,  4.12995568]), array([-0.60600353, -0.00627687, -2.84781631,  4.37647027]), array([-1.06685323,  0.7303139 , -1.67849003,  2.84070475]), array([-1.26525702,  1.12218654, -0.29886617,  1.09720955]), array([-1.20696065,  1.22776118,  0.87984831, -0.06151424]), array([-0.90810375,  1.05605381,  2.08171782, -1.69250782]), array([-0.38152736,  0.51425049,  3.10826569, -3.66292503]), array([ 0.2819929 , -0.31718017,  3.34736379, -4.28071341]), array([ 0.88777928, -1.05576078,  2.60367452, -2.94147017]), array([ 1.30096333, -1.48638953,  1.4991951 , -1.40788084]), array([ 1.4723894 , -1.61526411,  0.20905008,  0.07986584]), array([ 1.37487925, -1.43390387, -1.18520272,  1.75870581]), array([ 0.99848097, -0.8887541 , -2.5713268 ,  3.75658705]), array([ 0.3891489 , -0.00690142, -3.39273887,  4.80720652]), array([-0.30705885,  0.92811283, -3.39229086,  4.16594096]), array([-0.91929375,  1.58085892, -2.65215401,  2.32833063]), array([-1.34426808,  1.8745403 , -1.55704869,  0.66743164]), array([-1.5326826 ,  1.87081958, -0.31707106, -0.66201219]), array([-1.46166539,  1.59443103,  1.02906079, -2.11483199]), array([-1.12091097,  1.00648635,  2.37429303, -3.82656933]), array([-0.52448253,  0.06240541,  3.47918028, -5.40234683]), array([ 0.19032962, -0.97001716,  3.48610722, -4.5125547 ]), array([ 0.83352702, -1.68933332,  2.86393435, -2.63720212]), array([ 1.30839368, -2.03746812,  1.83291794, -0.90005855]), array([ 1.54582143, -2.05050343,  0.52328489,  0.72342792]), array([ 1.50598521, -1.73540157, -0.93073203,  2.43926455]), array([ 1.16959531, -1.05273102, -2.44289514,  4.47681816]), array([ 0.53715845,  0.0657058 , -3.74409698,  6.42447655]), array([-0.22931294,  1.28115727, -3.73593374,  5.29554355]), array([-0.9222339 ,  2.13359818, -3.12535296,  3.25743615]), array([-1.45088288,  2.61086761, -2.10788115,  1.58127759]), array([-1.75508133,  2.78651333, -0.92825059,  0.21078278]), array([-1.82278494,  2.70463992,  0.25102486, -1.01706009]), array([-1.64665183,  2.35867185,  1.5172924 , -2.47003426]), array([-1.20648839,  1.66837018,  2.89346739, -4.55942038]), array([-0.48359862,  0.47131205,  4.29055666, -7.38192442]), array([ 0.40116901, -1.02654273,  4.23995773, -6.82239701]), array([ 1.15577687, -2.13829462,  3.28002394, -4.3889663 ]), array([ 1.70179183, -2.83939155,  2.15818148, -2.73024659]), array([ 2.01378734,  3.04712437,  0.97997264, -1.26606514]), array([ 2.10134067,  2.93317619, -0.09368171,  0.12354459]), array([ 1.96936175,  3.11630222, -1.24075801,  1.71210838]), array([ 1.60853283, -2.697458  , -2.38019704,  3.02488122]), array([ 1.00701098, -1.88131571, -3.62181726,  5.29481985]), array([ 0.17910039, -0.55790013, -4.59124251,  7.86097242]), array([-0.73065554,  1.02473276, -4.16487299,  7.13131546]), array([-1.41752373,  2.1448718 , -2.73059828,  4.26641238]), array([-1.8293337 ,  2.79958172, -1.39993991,  2.37846452]), array([-1.98421857,  3.11349381, -0.16403789,  0.77311699]), array([-1.90876329, -3.13613359,  0.92371315, -0.44582519]), array([-1.59815657,  2.89050634,  2.19133703, -2.14603177]), array([-1.03643729,  2.26746603,  3.38599281, -4.18237461]), array([-0.27131882,  1.18487869,  4.23690778, -6.75946389]), array([ 0.61843646, -0.36047098,  4.34788966, -7.91576092]), array([ 1.35316452, -1.71325137,  2.92208093, -5.50691455]), array([ 1.79031205, -2.61124735,  1.4841508 , -3.61886212]), array([ 1.96070467,  3.09489453,  0.25404525, -2.1717855 ]), array([ 1.8999521 ,  2.80436892, -0.85973884, -0.72611352]), array([ 1.6049449 ,  2.82513165, -2.11083868,  0.92524552]), array([ 1.06437247,  3.12864871, -3.26825561,  2.09398639]), array([ 0.32007023, -2.58274118, -4.0260958 ,  3.64082047]), array([-0.46273148, -1.73740385, -3.67307745,  4.76399222]), array([-1.14184999, -0.66711327, -3.08949793,  5.79357238]), array([-1.640783  ,  0.40832601, -1.79946806,  4.71702006]), array([-1.83890984,  1.18509381, -0.16126993,  3.05632675]), array([-1.71571601,  1.67695571,  1.4229505 ,  1.77968836]), array([-1.25347978,  1.80606384,  3.15279071, -0.60677766]), array([-0.49071241,  1.39023451,  4.35636575, -3.61650119]), array([ 0.43700721,  0.37946059,  4.76045311, -6.16679079]), array([ 1.31634039, -0.81404734,  3.84128083, -5.25684481]), array([ 1.94339966, -1.65365457,  2.46707516, -3.28941925]), array([ 2.32084975, -2.1925768 ,  1.34693979, -2.21252967]), array([ 2.50150889, -2.58474251,  0.4848395 , -1.73301044]), array([ 2.50983917, -2.84502159, -0.39090523, -0.85223766]), array([ 2.34291184, -2.91241433, -1.29928919,  0.2219188 ]), array([ 1.98851099, -2.77367907, -2.2825769 ,  1.23388618]), array([ 1.40719341, -2.34373073, -3.52790219,  3.19159277]), array([ 0.59130194, -1.43184446, -4.59968577,  6.11109068]), array([-0.41603753,  0.10900948, -5.22032363,  8.61601101]), array([-1.32372611,  1.55160929, -3.73510107,  5.52715599]), array([-1.944739  ,  2.45339858, -2.5077234 ,  3.68358306]), array([-2.34146068,  3.07705742, -1.50917239,  2.62704548]), array([-2.56966206, -2.76508321, -0.82318186,  1.79812805]), array([-2.6723401 , -2.52614596, -0.22403399,  0.58785974]), array([-2.67521464, -2.49093087,  0.19479118, -0.23783541]), array([-2.59118494, -2.62244497,  0.66234711, -1.08070743]), array([-2.38719541, -2.96473382,  1.41693406, -2.34946616]), array([-2.00986273,  2.7316622 ,  2.40996767, -3.57402296]), array([-1.39904486,  1.8228875 ,  3.74092821, -5.72500935]), array([-0.48935378,  0.33082853,  5.30661477, -9.10709481]), array([ 0.56532342, -1.40022853,  4.89842119, -7.29828993]), array([ 1.4508575 , -2.57128377,  3.93914552, -4.65299331]), array([ 2.12850862,  2.93734327,  2.84579287, -3.23650721])]</t>
-  </si>
-  <si>
-    <t>['[1,1,1]', '[2,1,0]', '[2,2,2]', '[0,1,1]', '[0,0,0]', '[0,2,1]', '[1,0,2]', '[2,0,1]', '[1,2,0]', '[1,1,2]']</t>
-  </si>
-  <si>
-    <t>[1, 2, 3, 4, 7, 9, 11, 12, 13, 17, 19, 22, 23, 26, 27, 29, 30, 32, 36, 37, 38, 40, 41, 42, 43, 45, 47, 48, 50, 52, 53, 55, 58, 59, 60, 63, 65, 67, 68, 70, 71, 72, 73, 75, 79, 80, 82, 83, 85, 87, 88, 89, 90, 91, 93, 94, 98, 99, 101, 102, 103, 105, 106, 107, 108, 109, 112, 114, 115, 116, 117, 118, 120, 121, 122, 123, 125, 128, 130, 132, 134, 135, 136, 137, 138, 139, 141, 142, 143, 144, 145, 146, 147, 148, 149, 150, 151, 154, 157, 161, 163, 164, 166, 167, 168, 169, 171, 173, 174, 177, 181, 182, 183, 184, 186, 187, 192, 194, 195, 198, 199]</t>
-  </si>
-  <si>
-    <t>[0, 0, 0, 0, 2, 2, 2, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2]</t>
-  </si>
-  <si>
-    <t>['[-0.03763371 -0.01533471  0.06554052 -0.01816017]', '[-0.0208055  -0.02030166  0.09914155 -0.02801351]', '[ 0.00031733 -0.02489487  0.10765546 -0.0138725 ]', '[ 0.02044082 -0.02428802  0.08954248  0.02288616]', '[ 0.03470698 -0.01491644  0.05056501  0.07132823]', '[ 0.02674144  0.03818636 -0.12667052  0.44879208]', '[-0.01270905  0.15667936 -0.25571586  0.70881747]', '[-0.04326259  0.24058723 -0.04201128  0.11316277]', '[-0.02856994  0.19992338  0.1847616  -0.51074235]', '[ 0.01340206  0.07925064  0.22276409 -0.66890403]', '[ 0.06837074 -0.08967122  0.30996329 -0.98170941]', '[ 0.11635638 -0.26130066  0.1552225  -0.69872817]', '[ 0.12637466 -0.35809591 -0.0588444  -0.25356567]', '[ 0.10620827 -0.3937383  -0.13949123 -0.10047662]', '[ 0.04705976 -0.3320096  -0.43858013  0.69997673]', '[-0.06103436 -0.12714113 -0.61527401  1.29921437]', '[-0.18560692  0.16160376 -0.59476466  1.51610544]', '[-0.25883035  0.38253847 -0.11883307  0.65113982]', '[-0.25586305  0.47988365  0.14995175  0.3082916 ]', '[-0.18817957  0.47087101  0.51253773 -0.38767975]', '[-0.04690373  0.30127698  0.86882926 -1.26437406]', '[ 0.14281945 -0.00823878  0.98021643 -1.74592148]', '[ 0.31080465 -0.32406499  0.65652958 -1.3330903 ]', '[ 0.3923042  -0.5175331   0.1403688  -0.56691081]', '[ 0.37664003 -0.5763121  -0.29468048 -0.01495879]', '[ 0.25405437 -0.46042776 -0.90638924  1.14741265]', '[ 0.05540245 -0.20575117 -1.03289526  1.32613783]', '[-0.13844433  0.03690431 -0.8582082   1.02499997]', '[-0.29745415  0.24649073 -0.69382021  1.01060984]', '[-0.37663624  0.35249352 -0.08175228  0.02645803]', '[-0.34174846  0.28959648  0.42222737 -0.64138084]', '[-0.20227362  0.07391911  0.93916105 -1.4605323 ]', '[ 0.00166496 -0.22770056  1.04866727 -1.46747462]', '[ 0.20902374 -0.5114681   0.97535176 -1.2908149 ]', '[ 0.37392166 -0.71740996  0.63955138 -0.72371626]', '[ 0.45457929 -0.78932338  0.15220228  0.01775507]', '[ 0.43240548 -0.70943388 -0.36938957  0.77083698]', '[ 0.31265083 -0.49027366 -0.80238324  1.38012895]', '[ 0.12640346 -0.18192921 -1.01379803  1.62400992]', '[-0.09798857  0.19031223 -1.17041911  1.99059669]', '[-0.29093522  0.50222491 -0.71574823  1.05751691]', '[-0.37240828  0.59648595 -0.08393848 -0.13136604]', '[-0.3354437   0.48242344  0.44540019 -0.9914808 ]', '[-0.20217863  0.21437112  0.85465049 -1.63006639]', '[ 1.59182714e-03 -1.70532658e-01  1.12680833e+00 -2.11285007e+00]', '[ 0.21034902 -0.54951227  0.90952503 -1.58499874]', '[ 0.36118495 -0.80939214  0.56795079 -0.96664923]', '[ 0.41745631 -0.89422782 -0.01407163  0.12725405]', '[ 0.36694412 -0.78947886 -0.48179091  0.90660278]', '[ 0.20763131 -0.47829059 -1.08253447  2.16051387]', '[-0.02012915 -0.02837353 -1.13105374  2.21626192]', '[-0.24436986  0.42468349 -1.04752963  2.19119977]', '[-0.39268397  0.74296674 -0.40891739  0.94661447]', '[-0.40307487  0.7956552   0.30481724 -0.42217564]', '[-0.27467654  0.57772288  0.95718504 -1.72873883]', '[-0.04837551  0.16178026  1.2493931  -2.32914559]', '[ 0.21007724 -0.33466356  1.26066784 -2.49178383]', '[ 0.42764601 -0.78164631  0.86412213 -1.88756294]', '[ 0.53115487 -1.03842062  0.15855373 -0.66251508]', '[ 0.50108386 -1.07307397 -0.45214588  0.31546877]', '[ 0.35679573 -0.91566856 -0.965109    1.23744153]', '[ 0.10552686 -0.53070513 -1.50307737  2.55293618]', '[-0.21775947  0.05974054 -1.64150485  3.18162089]', '[-0.48595293  0.5977936  -0.97491436  2.07737942]', '[-0.61606954  0.92788642 -0.30266338  1.1837582 ]', '[-0.58205668  1.00513711  0.63191389 -0.41084489]', '[-0.37175268  0.76552332  1.43845371 -1.96458001]', '[-0.03904885  0.2747898   1.81482133 -2.8230313 ]', '[ 0.31579548 -0.29320701  1.63719316 -2.67546406]', '[ 0.59474268 -0.7675449   1.09197087 -1.96997632]', '[ 0.72575257 -1.03053297  0.20246556 -0.64590577]', '[ 0.68511424 -1.05290386 -0.60160125  0.42380917]', '[ 0.49255447 -0.86277686 -1.29273961  1.45850233]', '[ 0.18638974 -0.4870744  -1.70696164  2.21608119]', '[-0.18433754  0.04024375 -1.90693716  2.89073458]', '[-0.50931806  0.52582582 -1.26893103  1.84030842]', '[-0.6967485   0.81305631 -0.57263983  0.99163525]', '[-0.7309957   0.91446816  0.23473917  0.01468268]', '[-0.58291843  0.75754208  1.22523905 -1.57666247]', '[-0.26836384  0.32925931  1.85758013 -2.61732973]', '[ 0.12403703 -0.22761704  1.96296929 -2.76226106]', '[ 0.48852501 -0.73472373  1.59977249 -2.17535249]', '[ 0.72849421 -1.03707521  0.76568339 -0.82595692]', '[ 0.78653142 -1.06364212 -0.19335589  0.55847627]', '[ 0.64089552 -0.78457343 -1.24915593  2.22729638]', '[ 0.32595482 -0.25348174 -1.83049957  2.96846574]', '[-0.07851869  0.39829594 -2.10016605  3.32805201]', '[-0.44580267  0.93206411 -1.50500083  1.91278068]', '[-0.66217443  1.14888454 -0.62765406  0.24776501]', '[-0.69867795  1.05924565  0.27232186 -1.14160382]', '[-0.55398396  0.69491692  1.15594309 -2.47688758]', '[-0.25355609  0.09568163  1.77196343 -3.37493103]', '[ 0.12470858 -0.60355165  1.89858268 -3.39469953]', '[ 0.45708961 -1.16323815  1.3713321  -2.129178  ]', '[ 0.65880824 -1.44541663  0.62131729 -0.68868163]', '[ 0.7079543  -1.46442055 -0.13809245  0.49881547]', '[ 0.58442531 -1.1926143  -1.09189809  2.22922017]', '[ 0.27740864 -0.57182146 -1.93764711  3.92870415]', '[-0.1266987   0.24130677 -1.96851432  3.92933989]', '[-0.46060647  0.90138562 -1.30003487  2.54746152]', '[-0.65333965  1.29983448 -0.60251287  1.4135998 ]', '[-0.6781837   1.4123684   0.35024191 -0.28299147]', '[-0.52711857  1.2127615   1.14110107 -1.71123177]', '[-0.23327283  0.7329548   1.75397532 -3.03997698]', '[ 0.15911192  0.00940665  2.06473149 -3.9914332 ]', '[ 0.52632845 -0.7221519   1.50658886 -3.13034345]', '[ 0.73823602 -1.20538679  0.58836881 -1.67784771]', '[ 0.75902841 -1.39288573 -0.37441354 -0.199174  ]', '[ 0.60432166 -1.31105106 -1.14678762  1.01550632]', '[ 0.31504489 -0.99120895 -1.69873384  2.14992781]', '[-0.07469201 -0.41555456 -2.12518508  3.49296452]', '[-0.49204661  0.32352777 -1.9269497   3.65346444]', '[-0.77900321  0.90164075 -0.89516948  2.05624595]', '[-0.86419541  1.19774285  0.05210588  0.89142124]', '[-0.75023115  1.22729902  1.06726359 -0.60192066]', '[-0.45034114  0.95546469  1.88623196 -2.102171  ]', '[-0.02075131  0.40822337  2.32396092 -3.24377994]', '[ 0.43285723 -0.25682329  2.09069614 -3.17146335]', '[ 0.77396768 -0.7840171   1.25722647 -2.00596534]', '[ 0.93284811 -1.07561825  0.31232105 -0.89675111]', '[ 0.89624963 -1.14016557 -0.67299678  0.25847976]', '[ 0.67045187 -0.96891327 -1.55416384  1.45288866]', '[ 0.29365486 -0.56911584 -2.14561565  2.47095413]', '[-0.15012681 -0.03727677 -2.18242785  2.65700451]', '[-0.56027836  0.48040745 -1.82222643  2.35403331]', '[-0.82516152  0.79753497 -0.78929548  0.7881219 ]', '[-0.89149102  0.85573136  0.13383117 -0.2068969 ]', '[-0.74942163  0.65323792  1.27093537 -1.81248261]', '[-0.41027601  0.17786759  2.05338002 -2.83881748]', '[ 0.04488752 -0.44388518  2.37857178 -3.15194912]', '[ 0.48190513 -0.96623614  1.90705583 -1.95550551]', '[ 0.7930188  -1.23409312  1.15687293 -0.70655187]', '[ 0.92093669 -1.22305821  0.102461    0.80707543]', '[ 0.81958977 -0.88421991 -1.11475177  2.58552686]', '[ 0.50920506 -0.26219067 -1.92201541  3.5227479 ]', '[ 0.09286347  0.44389234 -2.12550233  3.30747932]', '[-0.29975419  0.98315873 -1.72734139  1.97708999]', '[-0.57506049  1.21418359 -0.97959507  0.31396062]', '[-0.6759151   1.10571131 -0.00162847 -1.40175569]', '[-0.58142256  0.68360745  0.93560215 -2.7917393 ]', '[-0.30494044 -0.01412393  1.74583382 -4.02196727]', '[ 0.05439309 -0.79011243  1.74131346 -3.52259586]', '[ 0.36318631 -1.37158329  1.30655856 -2.24234839]', '[ 0.56532871 -1.68113794  0.69140528 -0.85069182]', '[ 0.63187233 -1.7114554  -0.03868189  0.5498401 ]', '[ 0.55617127 -1.48357259 -0.71440869  1.73117273]', '[ 0.35090295 -1.01989875 -1.31513681  2.88567418]', '[ 0.04728125 -0.35416477 -1.64753642  3.63637021]', '[-0.26519012  0.34880349 -1.37164274  3.1786565 ]', '[-0.46938095  0.8545174  -0.63124508  1.80685709]', '[-0.51206749  1.06176141  0.20218557  0.26192264]', '[-0.40393605  0.9893011   0.85915479 -0.97637908]', '[-0.16851743  0.64949623  1.45647578 -2.37893105]', '[ 0.15559364  0.07378422  1.70294471 -3.22563213]', '[ 0.45894426 -0.52685886  1.24642509 -2.61866171]', '[ 0.64253325 -0.96345204  0.55456243 -1.69009505]', '[ 0.67416008 -1.19202012 -0.23891996 -0.58447505]', '[ 0.55165645 -1.1955482  -0.96248805  0.54600647]', '[ 0.28222538 -0.92141051 -1.68899157  2.17299285]', '[-0.10175114 -0.34940546 -2.07395042  3.42263677]', '[-0.50399049  0.36395854 -1.83235926  3.4794467 ]', '[-0.77176539  0.90633122 -0.80321915  1.88320294]', '[-0.8403786   1.16989939  0.12407543  0.73953808]', '[-0.71464434  1.17094652  1.11189507 -0.73408153]', '[-0.4091444   0.87624827  1.89588917 -2.19063023]', '[ 0.02963822  0.28945035  2.40186716 -3.53538483]', '[ 0.48807976 -0.40750494  2.0588238  -3.19308359]', '[ 0.81524533 -0.92120026  1.16036253 -1.87717351]', '[ 0.94134129 -1.15251075  0.08985248 -0.43728231]', '[ 0.86144667 -1.12375764 -0.8788037   0.73026716]', '[ 0.57685467 -0.7997579  -1.93324911  2.50695066]', '[ 0.13671095 -0.20971181 -2.37003907  3.23080942]', '[-0.34660409  0.46487589 -2.33329574  3.26708688]', '[-0.7288857   0.95857239 -1.43023493  1.60753841]', '[-0.90444696  1.10527811 -0.30507344 -0.13130253]', '[-0.84674808  0.90813694  0.88128091 -1.84114763]', '[-0.55795903  0.37112989  1.96298102 -3.47144577]', '[-0.11152806 -0.37905153  2.37446815 -3.77539407]', '[ 0.35267483 -1.06817765  2.16937423 -2.94576267]', '[ 0.72774431 -1.52429202  1.529293   -1.59173851]', '[ 0.94765488 -1.70562686  0.64014993 -0.23177873]', '[ 0.97622488 -1.62046554 -0.36147625  1.08093107]', '[ 0.80430108 -1.27093925 -1.34392738  2.42333053]', '[ 0.44959828 -0.65228383 -2.15132588  3.70724661]', '[-0.0175537   0.1452313  -2.38369089  3.99637366]', '[-0.47107322  0.89431502 -2.03980872  3.28712841]', '[-0.78450603  1.36621115 -1.06463354  1.43377757]', '[-0.88910424  1.47443659  0.029688   -0.34143943]', '[-0.77108064  1.22837758  1.14613703 -2.13376714]', '[-0.43639173  0.61496838  2.16297036 -3.9695605 ]', '[ 0.05677789 -0.29409168  2.61142123 -4.79796498]', '[ 0.53981121 -1.16245938  2.11273112 -3.69468444]', '[ 0.87090522 -1.72661378  1.17372039 -1.96889983]', '[ 1.01005216 -1.98331578  0.20594882 -0.6112929 ]', '[ 0.95244642 -1.97304096 -0.77284421  0.71699428]', '[ 0.7090887  -1.69264661 -1.62980227  2.09904181]', '[ 0.29763907 -1.07720751 -2.44955942  4.06742816]', '[-0.24654347 -0.09415044 -2.85838319  5.49251785]', '[-0.73943915  0.88092701 -1.93405408  3.9884894 ]', '[-0.99969494  1.47753625 -0.66038517  2.00422696]']</t>
-  </si>
-  <si>
-    <t>[array([-0.03763371, -0.01533471,  0.06554052, -0.01816017], dtype=float32), array([-0.0208055 , -0.02030166,  0.09914155, -0.02801351]), array([ 0.00031733, -0.02489487,  0.10765546, -0.0138725 ]), array([ 0.02044082, -0.02428802,  0.08954248,  0.02288616]), array([ 0.03470698, -0.01491644,  0.05056501,  0.07132823]), array([ 0.02674144,  0.03818636, -0.12667052,  0.44879208]), array([-0.01270905,  0.15667936, -0.25571586,  0.70881747]), array([-0.04326259,  0.24058723, -0.04201128,  0.11316277]), array([-0.02856994,  0.19992338,  0.1847616 , -0.51074235]), array([ 0.01340206,  0.07925064,  0.22276409, -0.66890403]), array([ 0.06837074, -0.08967122,  0.30996329, -0.98170941]), array([ 0.11635638, -0.26130066,  0.1552225 , -0.69872817]), array([ 0.12637466, -0.35809591, -0.0588444 , -0.25356567]), array([ 0.10620827, -0.3937383 , -0.13949123, -0.10047662]), array([ 0.04705976, -0.3320096 , -0.43858013,  0.69997673]), array([-0.06103436, -0.12714113, -0.61527401,  1.29921437]), array([-0.18560692,  0.16160376, -0.59476466,  1.51610544]), array([-0.25883035,  0.38253847, -0.11883307,  0.65113982]), array([-0.25586305,  0.47988365,  0.14995175,  0.3082916 ]), array([-0.18817957,  0.47087101,  0.51253773, -0.38767975]), array([-0.04690373,  0.30127698,  0.86882926, -1.26437406]), array([ 0.14281945, -0.00823878,  0.98021643, -1.74592148]), array([ 0.31080465, -0.32406499,  0.65652958, -1.3330903 ]), array([ 0.3923042 , -0.5175331 ,  0.1403688 , -0.56691081]), array([ 0.37664003, -0.5763121 , -0.29468048, -0.01495879]), array([ 0.25405437, -0.46042776, -0.90638924,  1.14741265]), array([ 0.05540245, -0.20575117, -1.03289526,  1.32613783]), array([-0.13844433,  0.03690431, -0.8582082 ,  1.02499997]), array([-0.29745415,  0.24649073, -0.69382021,  1.01060984]), array([-0.37663624,  0.35249352, -0.08175228,  0.02645803]), array([-0.34174846,  0.28959648,  0.42222737, -0.64138084]), array([-0.20227362,  0.07391911,  0.93916105, -1.4605323 ]), array([ 0.00166496, -0.22770056,  1.04866727, -1.46747462]), array([ 0.20902374, -0.5114681 ,  0.97535176, -1.2908149 ]), array([ 0.37392166, -0.71740996,  0.63955138, -0.72371626]), array([ 0.45457929, -0.78932338,  0.15220228,  0.01775507]), array([ 0.43240548, -0.70943388, -0.36938957,  0.77083698]), array([ 0.31265083, -0.49027366, -0.80238324,  1.38012895]), array([ 0.12640346, -0.18192921, -1.01379803,  1.62400992]), array([-0.09798857,  0.19031223, -1.17041911,  1.99059669]), array([-0.29093522,  0.50222491, -0.71574823,  1.05751691]), array([-0.37240828,  0.59648595, -0.08393848, -0.13136604]), array([-0.3354437 ,  0.48242344,  0.44540019, -0.9914808 ]), array([-0.20217863,  0.21437112,  0.85465049, -1.63006639]), array([ 1.59182714e-03, -1.70532658e-01,  1.12680833e+00, -2.11285007e+00]), array([ 0.21034902, -0.54951227,  0.90952503, -1.58499874]), array([ 0.36118495, -0.80939214,  0.56795079, -0.96664923]), array([ 0.41745631, -0.89422782, -0.01407163,  0.12725405]), array([ 0.36694412, -0.78947886, -0.48179091,  0.90660278]), array([ 0.20763131, -0.47829059, -1.08253447,  2.16051387]), array([-0.02012915, -0.02837353, -1.13105374,  2.21626192]), array([-0.24436986,  0.42468349, -1.04752963,  2.19119977]), array([-0.39268397,  0.74296674, -0.40891739,  0.94661447]), array([-0.40307487,  0.7956552 ,  0.30481724, -0.42217564]), array([-0.27467654,  0.57772288,  0.95718504, -1.72873883]), array([-0.04837551,  0.16178026,  1.2493931 , -2.32914559]), array([ 0.21007724, -0.33466356,  1.26066784, -2.49178383]), array([ 0.42764601, -0.78164631,  0.86412213, -1.88756294]), array([ 0.53115487, -1.03842062,  0.15855373, -0.66251508]), array([ 0.50108386, -1.07307397, -0.45214588,  0.31546877]), array([ 0.35679573, -0.91566856, -0.965109  ,  1.23744153]), array([ 0.10552686, -0.53070513, -1.50307737,  2.55293618]), array([-0.21775947,  0.05974054, -1.64150485,  3.18162089]), array([-0.48595293,  0.5977936 , -0.97491436,  2.07737942]), array([-0.61606954,  0.92788642, -0.30266338,  1.1837582 ]), array([-0.58205668,  1.00513711,  0.63191389, -0.41084489]), array([-0.37175268,  0.76552332,  1.43845371, -1.96458001]), array([-0.03904885,  0.2747898 ,  1.81482133, -2.8230313 ]), array([ 0.31579548, -0.29320701,  1.63719316, -2.67546406]), array([ 0.59474268, -0.7675449 ,  1.09197087, -1.96997632]), array([ 0.72575257, -1.03053297,  0.20246556, -0.64590577]), array([ 0.68511424, -1.05290386, -0.60160125,  0.42380917]), array([ 0.49255447, -0.86277686, -1.29273961,  1.45850233]), array([ 0.18638974, -0.4870744 , -1.70696164,  2.21608119]), array([-0.18433754,  0.04024375, -1.90693716,  2.89073458]), array([-0.50931806,  0.52582582, -1.26893103,  1.84030842]), array([-0.6967485 ,  0.81305631, -0.57263983,  0.99163525]), array([-0.7309957 ,  0.91446816,  0.23473917,  0.01468268]), array([-0.58291843,  0.75754208,  1.22523905, -1.57666247]), array([-0.26836384,  0.32925931,  1.85758013, -2.61732973]), array([ 0.12403703, -0.22761704,  1.96296929, -2.76226106]), array([ 0.48852501, -0.73472373,  1.59977249, -2.17535249]), array([ 0.72849421, -1.03707521,  0.76568339, -0.82595692]), array([ 0.78653142, -1.06364212, -0.19335589,  0.55847627]), array([ 0.64089552, -0.78457343, -1.24915593,  2.22729638]), array([ 0.32595482, -0.25348174, -1.83049957,  2.96846574]), array([-0.07851869,  0.39829594, -2.10016605,  3.32805201]), array([-0.44580267,  0.93206411, -1.50500083,  1.91278068]), array([-0.66217443,  1.14888454, -0.62765406,  0.24776501]), array([-0.69867795,  1.05924565,  0.27232186, -1.14160382]), array([-0.55398396,  0.69491692,  1.15594309, -2.47688758]), array([-0.25355609,  0.09568163,  1.77196343, -3.37493103]), array([ 0.12470858, -0.60355165,  1.89858268, -3.39469953]), array([ 0.45708961, -1.16323815,  1.3713321 , -2.129178  ]), array([ 0.65880824, -1.44541663,  0.62131729, -0.68868163]), array([ 0.7079543 , -1.46442055, -0.13809245,  0.49881547]), array([ 0.58442531, -1.1926143 , -1.09189809,  2.22922017]), array([ 0.27740864, -0.57182146, -1.93764711,  3.92870415]), array([-0.1266987 ,  0.24130677, -1.96851432,  3.92933989]), array([-0.46060647,  0.90138562, -1.30003487,  2.54746152]), array([-0.65333965,  1.29983448, -0.60251287,  1.4135998 ]), array([-0.6781837 ,  1.4123684 ,  0.35024191, -0.28299147]), array([-0.52711857,  1.2127615 ,  1.14110107, -1.71123177]), array([-0.23327283,  0.7329548 ,  1.75397532, -3.03997698]), array([ 0.15911192,  0.00940665,  2.06473149, -3.9914332 ]), array([ 0.52632845, -0.7221519 ,  1.50658886, -3.13034345]), array([ 0.73823602, -1.20538679,  0.58836881, -1.67784771]), array([ 0.75902841, -1.39288573, -0.37441354, -0.199174  ]), array([ 0.60432166, -1.31105106, -1.14678762,  1.01550632]), array([ 0.31504489, -0.99120895, -1.69873384,  2.14992781]), array([-0.07469201, -0.41555456, -2.12518508,  3.49296452]), array([-0.49204661,  0.32352777, -1.9269497 ,  3.65346444]), array([-0.77900321,  0.90164075, -0.89516948,  2.05624595]), array([-0.86419541,  1.19774285,  0.05210588,  0.89142124]), array([-0.75023115,  1.22729902,  1.06726359, -0.60192066]), array([-0.45034114,  0.95546469,  1.88623196, -2.102171  ]), array([-0.02075131,  0.40822337,  2.32396092, -3.24377994]), array([ 0.43285723, -0.25682329,  2.09069614, -3.17146335]), array([ 0.77396768, -0.7840171 ,  1.25722647, -2.00596534]), array([ 0.93284811, -1.07561825,  0.31232105, -0.89675111]), array([ 0.89624963, -1.14016557, -0.67299678,  0.25847976]), array([ 0.67045187, -0.96891327, -1.55416384,  1.45288866]), array([ 0.29365486, -0.56911584, -2.14561565,  2.47095413]), array([-0.15012681, -0.03727677, -2.18242785,  2.65700451]), array([-0.56027836,  0.48040745, -1.82222643,  2.35403331]), array([-0.82516152,  0.79753497, -0.78929548,  0.7881219 ]), array([-0.89149102,  0.85573136,  0.13383117, -0.2068969 ]), array([-0.74942163,  0.65323792,  1.27093537, -1.81248261]), array([-0.41027601,  0.17786759,  2.05338002, -2.83881748]), array([ 0.04488752, -0.44388518,  2.37857178, -3.15194912]), array([ 0.48190513, -0.96623614,  1.90705583, -1.95550551]), array([ 0.7930188 , -1.23409312,  1.15687293, -0.70655187]), array([ 0.92093669, -1.22305821,  0.102461  ,  0.80707543]), array([ 0.81958977, -0.88421991, -1.11475177,  2.58552686]), array([ 0.50920506, -0.26219067, -1.92201541,  3.5227479 ]), array([ 0.09286347,  0.44389234, -2.12550233,  3.30747932]), array([-0.29975419,  0.98315873, -1.72734139,  1.97708999]), array([-0.57506049,  1.21418359, -0.97959507,  0.31396062]), array([-0.6759151 ,  1.10571131, -0.00162847, -1.40175569]), array([-0.58142256,  0.68360745,  0.93560215, -2.7917393 ]), array([-0.30494044, -0.01412393,  1.74583382, -4.02196727]), array([ 0.05439309, -0.79011243,  1.74131346, -3.52259586]), array([ 0.36318631, -1.37158329,  1.30655856, -2.24234839]), array([ 0.56532871, -1.68113794,  0.69140528, -0.85069182]), array([ 0.63187233, -1.7114554 , -0.03868189,  0.5498401 ]), array([ 0.55617127, -1.48357259, -0.71440869,  1.73117273]), array([ 0.35090295, -1.01989875, -1.31513681,  2.88567418]), array([ 0.04728125, -0.35416477, -1.64753642,  3.63637021]), array([-0.26519012,  0.34880349, -1.37164274,  3.1786565 ]), array([-0.46938095,  0.8545174 , -0.63124508,  1.80685709]), array([-0.51206749,  1.06176141,  0.20218557,  0.26192264]), array([-0.40393605,  0.9893011 ,  0.85915479, -0.97637908]), array([-0.16851743,  0.64949623,  1.45647578, -2.37893105]), array([ 0.15559364,  0.07378422,  1.70294471, -3.22563213]), array([ 0.45894426, -0.52685886,  1.24642509, -2.61866171]), array([ 0.64253325, -0.96345204,  0.55456243, -1.69009505]), array([ 0.67416008, -1.19202012, -0.23891996, -0.58447505]), array([ 0.55165645, -1.1955482 , -0.96248805,  0.54600647]), array([ 0.28222538, -0.92141051, -1.68899157,  2.17299285]), array([-0.10175114, -0.34940546, -2.07395042,  3.42263677]), array([-0.50399049,  0.36395854, -1.83235926,  3.4794467 ]), array([-0.77176539,  0.90633122, -0.80321915,  1.88320294]), array([-0.8403786 ,  1.16989939,  0.12407543,  0.73953808]), array([-0.71464434,  1.17094652,  1.11189507, -0.73408153]), array([-0.4091444 ,  0.87624827,  1.89588917, -2.19063023]), array([ 0.02963822,  0.28945035,  2.40186716, -3.53538483]), array([ 0.48807976, -0.40750494,  2.0588238 , -3.19308359]), array([ 0.81524533, -0.92120026,  1.16036253, -1.87717351]), array([ 0.94134129, -1.15251075,  0.08985248, -0.43728231]), array([ 0.86144667, -1.12375764, -0.8788037 ,  0.73026716]), array([ 0.57685467, -0.7997579 , -1.93324911,  2.50695066]), array([ 0.13671095, -0.20971181, -2.37003907,  3.23080942]), array([-0.34660409,  0.46487589, -2.33329574,  3.26708688]), array([-0.7288857 ,  0.95857239, -1.43023493,  1.60753841]), array([-0.90444696,  1.10527811, -0.30507344, -0.13130253]), array([-0.84674808,  0.90813694,  0.88128091, -1.84114763]), array([-0.55795903,  0.37112989,  1.96298102, -3.47144577]), array([-0.11152806, -0.37905153,  2.37446815, -3.77539407]), array([ 0.35267483, -1.06817765,  2.16937423, -2.94576267]), array([ 0.72774431, -1.52429202,  1.529293  , -1.59173851]), array([ 0.94765488, -1.70562686,  0.64014993, -0.23177873]), array([ 0.97622488, -1.62046554, -0.36147625,  1.08093107]), array([ 0.80430108, -1.27093925, -1.34392738,  2.42333053]), array([ 0.44959828, -0.65228383, -2.15132588,  3.70724661]), array([-0.0175537 ,  0.1452313 , -2.38369089,  3.99637366]), array([-0.47107322,  0.89431502, -2.03980872,  3.28712841]), array([-0.78450603,  1.36621115, -1.06463354,  1.43377757]), array([-0.88910424,  1.47443659,  0.029688  , -0.34143943]), array([-0.77108064,  1.22837758,  1.14613703, -2.13376714]), array([-0.43639173,  0.61496838,  2.16297036, -3.9695605 ]), array([ 0.05677789, -0.29409168,  2.61142123, -4.79796498]), array([ 0.53981121, -1.16245938,  2.11273112, -3.69468444]), array([ 0.87090522, -1.72661378,  1.17372039, -1.96889983]), array([ 1.01005216, -1.98331578,  0.20594882, -0.6112929 ]), array([ 0.95244642, -1.97304096, -0.77284421,  0.71699428]), array([ 0.7090887 , -1.69264661, -1.62980227,  2.09904181]), array([ 0.29763907, -1.07720751, -2.44955942,  4.06742816]), array([-0.24654347, -0.09415044, -2.85838319,  5.49251785]), array([-0.73943915,  0.88092701, -1.93405408,  3.9884894 ]), array([-0.99969494,  1.47753625, -0.66038517,  2.00422696])]</t>
-  </si>
-  <si>
-    <t>['[2,0,1]', '[1,2,0]', '[0,1,1]', '[0,2,1]', '[1,0,2]', '[2,1,0]', '[1,1,1]', '[1,1,2]', '[2,2,2]', '[0,0,0]']</t>
-  </si>
-  <si>
-    <t>[1, 2, 3, 4, 5, 7, 8, 10, 11, 14, 15, 18, 19, 20, 22, 23, 25, 26, 27, 28, 32, 33, 34, 35, 36, 37, 38, 39, 40, 42, 43, 45, 46, 47, 49, 51, 52, 54, 55, 56, 57, 58, 61, 63, 65, 66, 68, 69, 70, 71, 74, 75, 77, 78, 80, 81, 82, 83, 84, 85, 86, 87, 88, 89, 90, 91, 92, 93, 95, 96, 97, 98, 99, 100, 102, 103, 104, 106, 108, 109, 110, 111, 112, 113, 114, 116, 117, 118, 121, 123, 124, 125, 126, 127, 128, 129, 130, 131, 132, 133, 134, 135, 136, 137, 138, 139, 140, 141, 142, 143, 144, 145, 146, 147, 149, 150, 151, 152, 153, 154, 155, 156, 157, 160, 161, 162, 164, 165, 166, 167, 169, 171, 173, 174, 176, 177, 178, 179, 180, 181, 182, 183, 185, 186, 187, 188, 190, 191, 192, 193, 194, 195, 196, 198]</t>
-  </si>
-  <si>
-    <t>[0, 0, 0, 0, 2, 0, 0, 0, 2, 2, 2, 0, 0, 0, 0, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 2, 0, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 0, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 2, 2, 0, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 2, 0, 0, 2, 2, 2, 2, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 0, 0, 0, 0, 2, 2, 2, 2, 2, 0, 0, 0, 2, 0, 0, 0]</t>
-  </si>
-  <si>
-    <t>['[-0.03763371 -0.01533471  0.06554052 -0.01816017]', '[-0.0208055  -0.02030166  0.09914155 -0.02801351]', '[ 0.00031733 -0.02489487  0.10765546 -0.0138725 ]', '[ 0.02044082 -0.02428802  0.08954248  0.02288616]', '[ 0.03470698 -0.01491644  0.05056501  0.07132823]', '[ 0.05326751 -0.03038784  0.13065223 -0.22021077]', '[ 0.08426237 -0.09828816  0.17075675 -0.44200317]', '[ 0.10440521 -0.16466942  0.02484734 -0.20792152]', '[ 0.09327439 -0.17827539 -0.1340662   0.07207783]', '[ 0.03992637 -0.1042478  -0.38626525  0.64738611]', '[-0.0268421  -0.00152039 -0.2647679   0.35189   ]', '[-0.0606613   0.0281044  -0.06594755 -0.06540149]', '[-0.05224593 -0.02769444  0.1463493  -0.48110843]', '[-0.00577245 -0.15572766  0.30448881 -0.76903781]', '[ 0.04939753 -0.28662006  0.23262498 -0.51030313]', '[ 0.08241209 -0.35040772  0.08967336 -0.11338368]', '[ 0.07059165 -0.2958437  -0.20440861  0.64914477]', '[ 0.00491815 -0.10078542 -0.43366229  1.25953608]', '[-0.06588522  0.11622637 -0.25273837  0.8613978 ]', '[-0.08981538  0.22863151  0.02070048  0.24180048]', '[-0.05747906  0.21007853  0.29521782 -0.41887946]', '[ 0.02261695  0.06998867  0.48535893 -0.94602274]', '[ 0.11301148 -0.11464291  0.39436583 -0.85399767]', '[ 0.17165839 -0.2546719   0.1766132  -0.5148719 ]', '[ 0.19261013 -0.34540995  0.02625045 -0.37478009]', '[ 0.16803648 -0.36592579 -0.26699537  0.16856492]', '[ 0.10335405 -0.31657775 -0.36539723  0.30730822]', '[ 0.0285775  -0.25159875 -0.36532484  0.32008522]', '[-0.03593222 -0.19768149 -0.26512344  0.19982685]', '[-0.09889333 -0.10976137 -0.34920962  0.6548952 ]', '[-0.16834386  0.05096444 -0.32619789  0.91376811]', '[-0.22148292  0.23858509 -0.18815641  0.92161744]', '[-0.2122001   0.3372767   0.28020648  0.05328863]', '[-0.12685835  0.29594302  0.55473464 -0.44771312]', '[-2.98366253e-04  1.70539290e-01  6.81581041e-01 -7.65906800e-01]', '[ 0.13264229  0.0090048   0.61588876 -0.80025932]', '[ 0.23385239 -0.13027463  0.37203249 -0.55386913]', '[ 0.27408942 -0.20052632  0.0209056  -0.13226197]', '[ 0.25465196 -0.21512345 -0.21179997 -0.01408469]', '[ 0.19261447 -0.20821522 -0.39611464  0.07330068]', '[ 0.10271022 -0.1913577  -0.48444885  0.0792228 ]', '[-0.01932229 -0.11542051 -0.7085067   0.64813015]', '[-0.14091986 -0.01867043 -0.48002679  0.28361575]', '[-0.20266008 -0.01223148 -0.12527776 -0.22900495]', '[-0.18951739 -0.10879006  0.25050398 -0.71716331]', '[-0.12151632 -0.25188547  0.41166945 -0.67919307]', '[-0.03306022 -0.36615865  0.4521985  -0.43157493]', '[ 0.05100574 -0.41318794  0.37011141 -0.0185481 ]', '[ 0.12140603 -0.40163553  0.31975409  0.14306974]', '[ 0.17386777 -0.35380784  0.19571002  0.33486525]', '[ 0.17109397 -0.2022636  -0.21939856  1.15673902]', '[ 0.11885841  0.02246099 -0.28400203  1.04191993]', '[ 0.06511836  0.19592021 -0.23755363  0.65555247]', '[ 0.00304197  0.34072043 -0.36610035  0.75787549]', '[-0.04805824  0.41798626 -0.13384471 -0.00241523]', '[-0.06095256  0.37123915  0.00683323 -0.46037612]', '[-0.0460241   0.23917566  0.13627311 -0.83738149]', '[-0.01059057  0.04909051  0.20453517 -1.02488743]', '[ 0.02943274 -0.15332255  0.18047965 -0.95707581]', '[ 0.06901002 -0.35171091  0.20054419 -0.98619339]', '[ 0.1039502  -0.53211556  0.13774632 -0.78558858]', '[ 0.10862082 -0.62353354 -0.09136539 -0.1190931 ]', '[ 0.05680718 -0.54782197 -0.41618443  0.86120009]', '[-0.02550709 -0.35758307 -0.38603062  0.99949879]', '[-0.11523071 -0.09832953 -0.48618741  1.53734895]', '[-0.18113265  0.16064751 -0.15053946  0.99664253]', '[-0.17042497  0.28479411  0.25778189  0.22793505]', '[-0.0818973   0.2519325   0.60816244 -0.53785863]', '[ 0.04861477  0.11795942  0.66643486 -0.75855204]', '[ 0.17174076 -0.0321245   0.53538774 -0.69697357]', '[ 0.25222596 -0.14426344  0.25049001 -0.39417381]', '[ 0.26694213 -0.18149338 -0.10684094  0.02932651]', '[ 0.19798087 -0.09981967 -0.56647393  0.76360887]', '[ 0.05128817  0.10671548 -0.86379462  1.24141527]', '[-0.10368667  0.29945938 -0.64985766  0.63135659]', '[-0.19674516  0.34354543 -0.26134741 -0.20905924]', '[-0.20398051  0.21506336  0.18747166 -1.05680102]', '[-0.14034109 -0.02901673  0.42716485 -1.33065916]', '[-0.04406961 -0.29232536  0.50736502 -1.24142575]', '[ 0.06416837 -0.53568613  0.54683704 -1.13662403]', '[ 0.15189986 -0.69542266  0.31283154 -0.43192842]', '[ 0.18416028 -0.70154925  0.0030247   0.37553629]', '[ 0.16481707 -0.57950215 -0.19161566  0.82777326]', '[ 0.11150884 -0.3813002  -0.32636107  1.11719246]', '[ 0.04221448 -0.15128213 -0.34476248  1.13231919]', '[-0.01731797  0.0506221  -0.23148755  0.8415638 ]', '[-0.04426108  0.17040274 -0.02937379  0.33272534]', '[-0.02785274  0.17890959  0.18993447 -0.24583155]', '[ 0.01488456  0.11174283  0.2267407  -0.40778844]', '[ 0.05809568  0.02431164  0.19394298 -0.44482257]', '[ 0.08810917 -0.05746479  0.09767876 -0.35440695]', '[ 0.09463297 -0.11123663 -0.03522759 -0.17342275]', '[ 0.08733981 -0.15899161 -0.03784399 -0.29678955]', '[ 0.06618655 -0.1921921  -0.17012509 -0.03324582]', '[ 0.00885221 -0.13983013 -0.38984257  0.53904846]', '[-0.05563044 -0.057175   -0.23946399  0.26332925]', '[-0.08224954 -0.04137598 -0.02114024 -0.11168504]', '[-0.07722742 -0.06637894  0.06949736 -0.13317956]', '[-0.05591475 -0.09193186  0.13847649 -0.11461184]', '[-0.02440446 -0.10886648  0.16969501 -0.04694646]', '[ 0.00903059 -0.10787562  0.15790936  0.06179547]', '[ 0.04952249 -0.11718445  0.23840292 -0.14678181]', '[ 0.08688513 -0.12737657  0.1275021   0.05198413]', '[ 0.11174843 -0.12966834  0.11605824 -0.0707091 ]', '[ 0.11801793 -0.11907878 -0.05410095  0.17538451]', '[ 0.07813632 -0.02827326 -0.33361664  0.71061946]', '[ 0.01834459  0.08254158 -0.24892008  0.36953763]', '[-0.0428247   0.17958069 -0.34710521  0.57410355]', '[-0.08709716  0.23189982 -0.08575137 -0.06501573]', '[-0.08888797  0.1872311   0.06683295 -0.37430673]', '[-0.06228836  0.08797466  0.19066023 -0.59714017]', '[-0.01728287 -0.0408995   0.24606799 -0.66211786]', '[ 0.03033474 -0.16437944  0.21670402 -0.54426719]', '[ 0.06450472 -0.24841518  0.11596525 -0.2774582 ]', '[ 0.07420526 -0.27027076 -0.02125374  0.06342605]', '[ 0.04333187 -0.19010896 -0.27916705  0.72070242]', '[-0.00492057 -0.06321945 -0.18950122  0.51863676]', '[-0.02790991  0.00747119 -0.03370879  0.17285747]', '[-0.0173633   0.00299299  0.13664342 -0.21476684]', '[ 0.02398012 -0.07376117  0.26576474 -0.53263384]', '[ 0.08315329 -0.19912644  0.30980545 -0.68975178]', '[ 0.12797657 -0.30231952  0.12703853 -0.31955627]', '[ 0.14418279 -0.35493569  0.03045732 -0.19590783]', '[ 0.13922157 -0.37774568 -0.07950747 -0.02953934]', '[ 0.11360529 -0.36729193 -0.1711003   0.1284572 ]', '[ 0.07385429 -0.33008483 -0.21731401  0.23152018]', '[ 0.03078193 -0.28046592 -0.20327803  0.24982351]', '[-0.00349057 -0.23616464 -0.13125332  0.18047519]', '[-0.01908099 -0.21249477 -0.02089872  0.04995763]', '[-0.01135488 -0.21718329  0.09629951 -0.09457466]', '[ 0.00451219 -0.21385465  0.05926316  0.12966282]', '[ 0.02477517 -0.20024488  0.13956949  0.00747105]', '[ 0.05806998 -0.2092076   0.18629556 -0.09029424]', '[ 0.08286666 -0.19879503  0.05706657  0.19615149]', '[ 0.09354389 -0.16669525  0.04858533  0.12093525]', '[ 0.10183021 -0.15153634  0.03310091  0.02930565]', '[ 0.10632329 -0.15498843  0.01081818 -0.06251933]', '[ 0.10581445 -0.17553489 -0.01646055 -0.13943627]', '[ 0.09963614 -0.20900382 -0.04514074 -0.19039391]', '[ 0.08799621 -0.24958488 -0.07016481 -0.2102482 ]', '[ 0.07219039 -0.29107525 -0.08591105 -0.20013322]', '[ 0.05457638 -0.32802574 -0.08765141 -0.16609783]', '[ 0.03822672 -0.35646953 -0.0732151  -0.11643604]', '[ 0.02628596 -0.3740826  -0.04415821 -0.05889987]', '[ 0.02120009 -0.37988735 -0.00580245  0.00091618]', '[ 0.02406923 -0.37380762  0.03401008  0.05943508]', '[ 0.03434697 -0.35639902  0.06703404  0.11362931]', '[ 0.04998794 -0.32891278  0.08685087  0.15936103]', '[ 0.04188218 -0.22609784 -0.16420631  0.8520789 ]', '[ 0.01512402 -0.06929061 -0.09257664  0.68420907]', '[0.00835508 0.03647242 0.02956126 0.35421803]', '[ 0.02740267  0.06774026  0.15774426 -0.04347105]', '[ 0.05550858  0.05589603  0.11727861 -0.06861194]', '[ 0.07219486  0.04275765  0.04587075 -0.05803023]', '[ 0.07294073  0.03409352 -0.03873948 -0.02713762]', '[ 0.07052001 -0.00247996  0.01377988 -0.33242869]', '[ 0.06412659 -0.05980127 -0.07811213 -0.23204493]', '[ 0.03994794 -0.09299486 -0.15968766 -0.09807588]', '[-0.01059994 -0.06541651 -0.33441875  0.36089872]', '[-0.08743645  0.04218642 -0.41487118  0.68426644]', '[-0.14148773  0.12496715 -0.11277227  0.12226407]', '[-0.13034716  0.08795526  0.22048184 -0.48383721]', '[-0.07126411 -0.02506343  0.35473234 -0.61752874]', '[ 0.01733312 -0.18001866  0.50794449 -0.89031675]', '[ 0.10814733 -0.32824709  0.37817764 -0.55467377]', '[ 0.16132767 -0.39036029  0.14196027 -0.05029734]', '[ 0.17531098 -0.37940596 -0.00448708  0.15981153]', '[ 0.15990354 -0.32847859 -0.14501711  0.338892  ]', '[ 0.09425926 -0.18227316 -0.4947351   1.09086661]', '[-0.00095436  0.01877091 -0.43132342  0.86902102]', '[-0.09518514  0.21562918 -0.48508274  1.04959495]', '[-0.1583334   0.3505138  -0.13165606  0.2713745 ]', '[-0.17108122  0.38646686  0.00746714  0.08095439]', '[-0.1424371   0.34853039  0.27217312 -0.45025047]', '[-0.06738081  0.21491789  0.45976155 -0.85330889]', '[ 0.045184   -0.0097994   0.63585677 -1.33713892]', '[ 0.15947888 -0.25808265  0.47613687 -1.08513828]', '[ 0.22536826 -0.42367076  0.16652709 -0.53755805]', '[ 0.22266277 -0.46519268 -0.19305573  0.12671613]', '[ 0.16411007 -0.40945895 -0.37936886  0.41389962]', '[ 0.07788287 -0.30921504 -0.46280426  0.5594798 ]', '[-0.01208595 -0.19902757 -0.41535907  0.50961611]', '[-0.08005633 -0.11798435 -0.24819175  0.27629163]', '[-0.10649927 -0.09572433 -0.01048728 -0.06120551]', '[-0.0841852  -0.14183531  0.22734863 -0.38788929]', '[-0.03342941 -0.20850256  0.26800373 -0.25975327]', '[ 0.01796903 -0.238769    0.23470638 -0.03006043]', '[ 0.05642761 -0.21704838  0.14266088  0.24946923]', '[ 0.0863596  -0.17450153  0.15198678  0.17321955]', '[ 0.08876013 -0.08001957 -0.12547207  0.75561677]', '[ 0.06663477  0.04719818 -0.08717902  0.49109981]', '[ 0.05659311  0.1084306  -0.00961683  0.1097895 ]', '[ 0.06321863  0.08946102  0.07383815 -0.29495825]', '[ 0.07098433  0.02960692  0.00048196 -0.29223008]', '[ 0.06264056 -0.02331757 -0.08379898 -0.22930673]', '[ 0.03823563 -0.05992284 -0.15636409 -0.1343126 ]', '[ 0.01554932 -0.11134263 -0.06777515 -0.37404465]', '[ 0.01122861 -0.205091    0.02217568 -0.54746051]', '[ 0.00960438 -0.28860553 -0.03997769 -0.27500458]', '[ 0.0083549  -0.34579349  0.02615559 -0.28779055]']</t>
-  </si>
-  <si>
-    <t>[array([-0.03763371, -0.01533471,  0.06554052, -0.01816017], dtype=float32), array([-0.0208055 , -0.02030166,  0.09914155, -0.02801351]), array([ 0.00031733, -0.02489487,  0.10765546, -0.0138725 ]), array([ 0.02044082, -0.02428802,  0.08954248,  0.02288616]), array([ 0.03470698, -0.01491644,  0.05056501,  0.07132823]), array([ 0.05326751, -0.03038784,  0.13065223, -0.22021077]), array([ 0.08426237, -0.09828816,  0.17075675, -0.44200317]), array([ 0.10440521, -0.16466942,  0.02484734, -0.20792152]), array([ 0.09327439, -0.17827539, -0.1340662 ,  0.07207783]), array([ 0.03992637, -0.1042478 , -0.38626525,  0.64738611]), array([-0.0268421 , -0.00152039, -0.2647679 ,  0.35189   ]), array([-0.0606613 ,  0.0281044 , -0.06594755, -0.06540149]), array([-0.05224593, -0.02769444,  0.1463493 , -0.48110843]), array([-0.00577245, -0.15572766,  0.30448881, -0.76903781]), array([ 0.04939753, -0.28662006,  0.23262498, -0.51030313]), array([ 0.08241209, -0.35040772,  0.08967336, -0.11338368]), array([ 0.07059165, -0.2958437 , -0.20440861,  0.64914477]), array([ 0.00491815, -0.10078542, -0.43366229,  1.25953608]), array([-0.06588522,  0.11622637, -0.25273837,  0.8613978 ]), array([-0.08981538,  0.22863151,  0.02070048,  0.24180048]), array([-0.05747906,  0.21007853,  0.29521782, -0.41887946]), array([ 0.02261695,  0.06998867,  0.48535893, -0.94602274]), array([ 0.11301148, -0.11464291,  0.39436583, -0.85399767]), array([ 0.17165839, -0.2546719 ,  0.1766132 , -0.5148719 ]), array([ 0.19261013, -0.34540995,  0.02625045, -0.37478009]), array([ 0.16803648, -0.36592579, -0.26699537,  0.16856492]), array([ 0.10335405, -0.31657775, -0.36539723,  0.30730822]), array([ 0.0285775 , -0.25159875, -0.36532484,  0.32008522]), array([-0.03593222, -0.19768149, -0.26512344,  0.19982685]), array([-0.09889333, -0.10976137, -0.34920962,  0.6548952 ]), array([-0.16834386,  0.05096444, -0.32619789,  0.91376811]), array([-0.22148292,  0.23858509, -0.18815641,  0.92161744]), array([-0.2122001 ,  0.3372767 ,  0.28020648,  0.05328863]), array([-0.12685835,  0.29594302,  0.55473464, -0.44771312]), array([-2.98366253e-04,  1.70539290e-01,  6.81581041e-01, -7.65906800e-01]), array([ 0.13264229,  0.0090048 ,  0.61588876, -0.80025932]), array([ 0.23385239, -0.13027463,  0.37203249, -0.55386913]), array([ 0.27408942, -0.20052632,  0.0209056 , -0.13226197]), array([ 0.25465196, -0.21512345, -0.21179997, -0.01408469]), array([ 0.19261447, -0.20821522, -0.39611464,  0.07330068]), array([ 0.10271022, -0.1913577 , -0.48444885,  0.0792228 ]), array([-0.01932229, -0.11542051, -0.7085067 ,  0.64813015]), array([-0.14091986, -0.01867043, -0.48002679,  0.28361575]), array([-0.20266008, -0.01223148, -0.12527776, -0.22900495]), array([-0.18951739, -0.10879006,  0.25050398, -0.71716331]), array([-0.12151632, -0.25188547,  0.41166945, -0.67919307]), array([-0.03306022, -0.36615865,  0.4521985 , -0.43157493]), array([ 0.05100574, -0.41318794,  0.37011141, -0.0185481 ]), array([ 0.12140603, -0.40163553,  0.31975409,  0.14306974]), array([ 0.17386777, -0.35380784,  0.19571002,  0.33486525]), array([ 0.17109397, -0.2022636 , -0.21939856,  1.15673902]), array([ 0.11885841,  0.02246099, -0.28400203,  1.04191993]), array([ 0.06511836,  0.19592021, -0.23755363,  0.65555247]), array([ 0.00304197,  0.34072043, -0.36610035,  0.75787549]), array([-0.04805824,  0.41798626, -0.13384471, -0.00241523]), array([-0.06095256,  0.37123915,  0.00683323, -0.46037612]), array([-0.0460241 ,  0.23917566,  0.13627311, -0.83738149]), array([-0.01059057,  0.04909051,  0.20453517, -1.02488743]), array([ 0.02943274, -0.15332255,  0.18047965, -0.95707581]), array([ 0.06901002, -0.35171091,  0.20054419, -0.98619339]), array([ 0.1039502 , -0.53211556,  0.13774632, -0.78558858]), array([ 0.10862082, -0.62353354, -0.09136539, -0.1190931 ]), array([ 0.05680718, -0.54782197, -0.41618443,  0.86120009]), array([-0.02550709, -0.35758307, -0.38603062,  0.99949879]), array([-0.11523071, -0.09832953, -0.48618741,  1.53734895]), array([-0.18113265,  0.16064751, -0.15053946,  0.99664253]), array([-0.17042497,  0.28479411,  0.25778189,  0.22793505]), array([-0.0818973 ,  0.2519325 ,  0.60816244, -0.53785863]), array([ 0.04861477,  0.11795942,  0.66643486, -0.75855204]), array([ 0.17174076, -0.0321245 ,  0.53538774, -0.69697357]), array([ 0.25222596, -0.14426344,  0.25049001, -0.39417381]), array([ 0.26694213, -0.18149338, -0.10684094,  0.02932651]), array([ 0.19798087, -0.09981967, -0.56647393,  0.76360887]), array([ 0.05128817,  0.10671548, -0.86379462,  1.24141527]), array([-0.10368667,  0.29945938, -0.64985766,  0.63135659]), array([-0.19674516,  0.34354543, -0.26134741, -0.20905924]), array([-0.20398051,  0.21506336,  0.18747166, -1.05680102]), array([-0.14034109, -0.02901673,  0.42716485, -1.33065916]), array([-0.04406961, -0.29232536,  0.50736502, -1.24142575]), array([ 0.06416837, -0.53568613,  0.54683704, -1.13662403]), array([ 0.15189986, -0.69542266,  0.31283154, -0.43192842]), array([ 0.18416028, -0.70154925,  0.0030247 ,  0.37553629]), array([ 0.16481707, -0.57950215, -0.19161566,  0.82777326]), array([ 0.11150884, -0.3813002 , -0.32636107,  1.11719246]), array([ 0.04221448, -0.15128213, -0.34476248,  1.13231919]), array([-0.01731797,  0.0506221 , -0.23148755,  0.8415638 ]), array([-0.04426108,  0.17040274, -0.02937379,  0.33272534]), array([-0.02785274,  0.17890959,  0.18993447, -0.24583155]), array([ 0.01488456,  0.11174283,  0.2267407 , -0.40778844]), array([ 0.05809568,  0.02431164,  0.19394298, -0.44482257]), array([ 0.08810917, -0.05746479,  0.09767876, -0.35440695]), array([ 0.09463297, -0.11123663, -0.03522759, -0.17342275]), array([ 0.08733981, -0.15899161, -0.03784399, -0.29678955]), array([ 0.06618655, -0.1921921 , -0.17012509, -0.03324582]), array([ 0.00885221, -0.13983013, -0.38984257,  0.53904846]), array([-0.05563044, -0.057175  , -0.23946399,  0.26332925]), array([-0.08224954, -0.04137598, -0.02114024, -0.11168504]), array([-0.07722742, -0.06637894,  0.06949736, -0.13317956]), array([-0.05591475, -0.09193186,  0.13847649, -0.11461184]), array([-0.02440446, -0.10886648,  0.16969501, -0.04694646]), array([ 0.00903059, -0.10787562,  0.15790936,  0.06179547]), array([ 0.04952249, -0.11718445,  0.23840292, -0.14678181]), array([ 0.08688513, -0.12737657,  0.1275021 ,  0.05198413]), array([ 0.11174843, -0.12966834,  0.11605824, -0.0707091 ]), array([ 0.11801793, -0.11907878, -0.05410095,  0.17538451]), array([ 0.07813632, -0.02827326, -0.33361664,  0.71061946]), array([ 0.01834459,  0.08254158, -0.24892008,  0.36953763]), array([-0.0428247 ,  0.17958069, -0.34710521,  0.57410355]), array([-0.08709716,  0.23189982, -0.08575137, -0.06501573]), array([-0.08888797,  0.1872311 ,  0.06683295, -0.37430673]), array([-0.06228836,  0.08797466,  0.19066023, -0.59714017]), array([-0.01728287, -0.0408995 ,  0.24606799, -0.66211786]), array([ 0.03033474, -0.16437944,  0.21670402, -0.54426719]), array([ 0.06450472, -0.24841518,  0.11596525, -0.2774582 ]), array([ 0.07420526, -0.27027076, -0.02125374,  0.06342605]), array([ 0.04333187, -0.19010896, -0.27916705,  0.72070242]), array([-0.00492057, -0.06321945, -0.18950122,  0.51863676]), array([-0.02790991,  0.00747119, -0.03370879,  0.17285747]), array([-0.0173633 ,  0.00299299,  0.13664342, -0.21476684]), array([ 0.02398012, -0.07376117,  0.26576474, -0.53263384]), array([ 0.08315329, -0.19912644,  0.30980545, -0.68975178]), array([ 0.12797657, -0.30231952,  0.12703853, -0.31955627]), array([ 0.14418279, -0.35493569,  0.03045732, -0.19590783]), array([ 0.13922157, -0.37774568, -0.07950747, -0.02953934]), array([ 0.11360529, -0.36729193, -0.1711003 ,  0.1284572 ]), array([ 0.07385429, -0.33008483, -0.21731401,  0.23152018]), array([ 0.03078193, -0.28046592, -0.20327803,  0.24982351]), array([-0.00349057, -0.23616464, -0.13125332,  0.18047519]), array([-0.01908099, -0.21249477, -0.02089872,  0.04995763]), array([-0.01135488, -0.21718329,  0.09629951, -0.09457466]), array([ 0.00451219, -0.21385465,  0.05926316,  0.12966282]), array([ 0.02477517, -0.20024488,  0.13956949,  0.00747105]), array([ 0.05806998, -0.2092076 ,  0.18629556, -0.09029424]), array([ 0.08286666, -0.19879503,  0.05706657,  0.19615149]), array([ 0.09354389, -0.16669525,  0.04858533,  0.12093525]), array([ 0.10183021, -0.15153634,  0.03310091,  0.02930565]), array([ 0.10632329, -0.15498843,  0.01081818, -0.06251933]), array([ 0.10581445, -0.17553489, -0.01646055, -0.13943627]), array([ 0.09963614, -0.20900382, -0.04514074, -0.19039391]), array([ 0.08799621, -0.24958488, -0.07016481, -0.2102482 ]), array([ 0.07219039, -0.29107525, -0.08591105, -0.20013322]), array([ 0.05457638, -0.32802574, -0.08765141, -0.16609783]), array([ 0.03822672, -0.35646953, -0.0732151 , -0.11643604]), array([ 0.02628596, -0.3740826 , -0.04415821, -0.05889987]), array([ 0.02120009, -0.37988735, -0.00580245,  0.00091618]), array([ 0.02406923, -0.37380762,  0.03401008,  0.05943508]), array([ 0.03434697, -0.35639902,  0.06703404,  0.11362931]), array([ 0.04998794, -0.32891278,  0.08685087,  0.15936103]), array([ 0.04188218, -0.22609784, -0.16420631,  0.8520789 ]), array([ 0.01512402, -0.06929061, -0.09257664,  0.68420907]), array([0.00835508, 0.03647242, 0.02956126, 0.35421803]), array([ 0.02740267,  0.06774026,  0.15774426, -0.04347105]), array([ 0.05550858,  0.05589603,  0.11727861, -0.06861194]), array([ 0.07219486,  0.04275765,  0.04587075, -0.05803023]), array([ 0.07294073,  0.03409352, -0.03873948, -0.02713762]), array([ 0.07052001, -0.00247996,  0.01377988, -0.33242869]), array([ 0.06412659, -0.05980127, -0.07811213, -0.23204493]), array([ 0.03994794, -0.09299486, -0.15968766, -0.09807588]), array([-0.01059994, -0.06541651, -0.33441875,  0.36089872]), array([-0.08743645,  0.04218642, -0.41487118,  0.68426644]), array([-0.14148773,  0.12496715, -0.11277227,  0.12226407]), array([-0.13034716,  0.08795526,  0.22048184, -0.48383721]), array([-0.07126411, -0.02506343,  0.35473234, -0.61752874]), array([ 0.01733312, -0.18001866,  0.50794449, -0.89031675]), array([ 0.10814733, -0.32824709,  0.37817764, -0.55467377]), array([ 0.16132767, -0.39036029,  0.14196027, -0.05029734]), array([ 0.17531098, -0.37940596, -0.00448708,  0.15981153]), array([ 0.15990354, -0.32847859, -0.14501711,  0.338892  ]), array([ 0.09425926, -0.18227316, -0.4947351 ,  1.09086661]), array([-0.00095436,  0.01877091, -0.43132342,  0.86902102]), array([-0.09518514,  0.21562918, -0.48508274,  1.04959495]), array([-0.1583334 ,  0.3505138 , -0.13165606,  0.2713745 ]), array([-0.17108122,  0.38646686,  0.00746714,  0.08095439]), array([-0.1424371 ,  0.34853039,  0.27217312, -0.45025047]), array([-0.06738081,  0.21491789,  0.45976155, -0.85330889]), array([ 0.045184  , -0.0097994 ,  0.63585677, -1.33713892]), array([ 0.15947888, -0.25808265,  0.47613687, -1.08513828]), array([ 0.22536826, -0.42367076,  0.16652709, -0.53755805]), array([ 0.22266277, -0.46519268, -0.19305573,  0.12671613]), array([ 0.16411007, -0.40945895, -0.37936886,  0.41389962]), array([ 0.07788287, -0.30921504, -0.46280426,  0.5594798 ]), array([-0.01208595, -0.19902757, -0.41535907,  0.50961611]), array([-0.08005633, -0.11798435, -0.24819175,  0.27629163]), array([-0.10649927, -0.09572433, -0.01048728, -0.06120551]), array([-0.0841852 , -0.14183531,  0.22734863, -0.38788929]), array([-0.03342941, -0.20850256,  0.26800373, -0.25975327]), array([ 0.01796903, -0.238769  ,  0.23470638, -0.03006043]), array([ 0.05642761, -0.21704838,  0.14266088,  0.24946923]), array([ 0.0863596 , -0.17450153,  0.15198678,  0.17321955]), array([ 0.08876013, -0.08001957, -0.12547207,  0.75561677]), array([ 0.06663477,  0.04719818, -0.08717902,  0.49109981]), array([ 0.05659311,  0.1084306 , -0.00961683,  0.1097895 ]), array([ 0.06321863,  0.08946102,  0.07383815, -0.29495825]), array([ 0.07098433,  0.02960692,  0.00048196, -0.29223008]), array([ 0.06264056, -0.02331757, -0.08379898, -0.22930673]), array([ 0.03823563, -0.05992284, -0.15636409, -0.1343126 ]), array([ 0.01554932, -0.11134263, -0.06777515, -0.37404465]), array([ 0.01122861, -0.205091  ,  0.02217568, -0.54746051]), array([ 0.00960438, -0.28860553, -0.03997769, -0.27500458]), array([ 0.0083549 , -0.34579349,  0.02615559, -0.28779055])]</t>
-  </si>
-  <si>
-    <t>['[1,0,2]', '[1,2,0]', '[0,0,0]', '[2,2,2]', '[1,1,1]', '[2,0,1]', '[0,2,1]', '[2,1,0]', '[1,1,2]', '[0,1,1]']</t>
-  </si>
-  <si>
-    <t>[1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50, 51, 52, 53, 54, 55, 56, 57, 58, 59, 60, 61, 62, 63, 64, 65, 66, 67, 68, 69, 70, 71, 72, 73, 74, 75, 76, 77, 78, 79, 80, 81, 82, 83, 84, 85, 86, 87, 88, 89, 90, 91, 92, 93, 94, 95, 96, 97, 98, 99, 100, 101, 102, 103, 104, 105, 106, 107, 108, 109, 110, 111, 112, 113, 114, 115, 116, 117, 118, 119, 120, 121, 122, 123, 124, 125, 126, 127, 128, 129, 130, 131, 132, 133, 134, 135, 136, 137, 138, 139, 140, 141, 142, 143, 144, 145, 146, 147, 148, 149, 150, 151, 152, 153, 154, 155, 156, 157, 158, 159, 160, 161, 162, 163, 164, 165, 166, 167, 168, 169, 170, 171, 172, 173, 174, 175, 176, 177, 178, 179, 180, 181, 182, 183, 184, 185, 186, 187, 188, 189, 190, 191, 192, 193, 194, 195, 196, 197, 198, 199]</t>
-  </si>
-  <si>
-    <t>[0, 0, 0, 0, 2, 0, 0, 2, 0, 2, 0, 2, 0, 2, 0, 2, 2, 0, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2]</t>
-  </si>
-  <si>
-    <t>['[-0.03763371 -0.01533471  0.06554052 -0.01816017]', '[-0.0208055  -0.02030166  0.09914155 -0.02801351]', '[ 0.00031733 -0.02489487  0.10765546 -0.0138725 ]', '[ 0.02044082 -0.02428802  0.08954248  0.02288616]', '[ 0.03470698 -0.01491644  0.05056501  0.07132823]', '[ 0.05326751 -0.03038784  0.13065223 -0.22021077]', '[ 0.07101291 -0.0640307   0.04229076 -0.10791836]', '[ 0.06919594 -0.07148833 -0.06018897  0.03411905]', '[ 0.06123949 -0.0858309  -0.01832924 -0.17605239]', '[ 0.04848925 -0.10546764 -0.10705552 -0.01913256]', '[ 0.03334023 -0.12873715 -0.04224633 -0.21160413]', '[ 0.01856077 -0.15355978 -0.1031453  -0.03494141]', '[ 0.00687968 -0.17764366 -0.01219475 -0.20332606]', '[ 0.00024918 -0.19823055 -0.05320561 -0.00041555]', '[-0.00038196 -0.21249406  0.04645807 -0.13967612]', '[ 0.00462703 -0.21766377  0.00256154  0.08939976]', '[ 0.01391452 -0.21184382  0.0884936  -0.03053848]', '[ 0.03850047 -0.22834148  0.15179103 -0.12764898]', '[ 0.05871339 -0.22531591  0.04642174  0.1602345 ]', '[ 0.06975736 -0.19972822  0.06255754  0.09301244]', '[ 0.08295526 -0.18863935  0.06709485  0.01801994]', '[ 0.0955466  -0.19194963  0.05618073 -0.04863014]', '[ 0.10438266 -0.20672312  0.02995667 -0.09524718]', '[ 0.10679076 -0.22835209 -0.00700287 -0.1170154 ]', '[ 0.10139245 -0.251988   -0.04658216 -0.11618468]', '[ 0.08862558 -0.27379536 -0.07912951 -0.10019242]', '[ 0.07079541 -0.2916811  -0.09605709 -0.07844699]', '[ 0.05160586 -0.30533224 -0.09231221 -0.05881123]', '[ 0.03527347 -0.31561531 -0.06796943 -0.04491109]', '[ 0.02545877 -0.32360191 -0.02840871 -0.03520182]', '[ 0.02431678 -0.32962124  0.01702803 -0.0241677 ]', '[ 0.03194057 -0.33273766  0.0575287  -0.00523763]', '[ 0.04635922 -0.33089406  0.08372791  0.02568935]', '[ 0.06409062 -0.32170512  0.09020522  0.06748616]', '[ 0.08108895 -0.30362649  0.07683704  0.11292955]', '[ 0.09381032 -0.27706452  0.04859846  0.15016487]', '[ 0.10008474 -0.24498455  0.01387843  0.16612946]', '[ 0.099545   -0.21272175 -0.0181427   0.15089341]', '[ 0.09350925 -0.18694889 -0.04018141  0.10151107]', '[ 0.08439395 -0.17403958 -0.04874136  0.02402904]', '[ 0.0748759  -0.17828815 -0.04468765 -0.06714713]', '[ 0.06707968 -0.2005238  -0.03244224 -0.15248501]', '[ 0.06204155 -0.23757011 -0.01810026 -0.2123621 ]', '[ 0.0596084  -0.28277818 -0.00709475 -0.23248464]', '[ 0.0587725  -0.32752505 -0.00232775 -0.20781714]', '[ 0.05826257 -0.3632139  -0.00355436 -0.1435367 ]', '[ 0.05712088 -0.38315408 -0.00807237 -0.05302107]', '[ 0.05506565 -0.38385601 -0.01204958  0.04571899]', '[ 0.05258562 -0.36558361 -0.01179826  0.13373731]', '[ 0.05080563 -0.3322004  -0.0047971   0.19451381]', '[ 0.05116333 -0.29036678  0.00943036  0.21708422]', '[ 0.05492846 -0.24815416  0.02866925  0.1986191 ]', '[ 0.06265333 -0.2132846   0.04805764  0.14539356]', '[ 0.0737392  -0.1914255   0.06122493  0.07119519]', '[ 0.08632927 -0.18505144  0.06232775 -0.0065993 ]', '[ 0.09763559 -0.19320967  0.04820618 -0.07185489]', '[ 0.1046364  -0.21219823  0.01981793 -0.11373169]', '[ 0.10494239 -0.23687371 -0.01755309 -0.12880179]', '[ 0.09757088 -0.26214836 -0.05540839 -0.12082367]', '[ 0.08338498 -0.28422734 -0.084203   -0.09846705]', '[ 0.06503934 -0.30125202 -0.09599606 -0.07181621]', '[ 0.04641147 -0.31321516 -0.08681408 -0.04877953]', '[ 0.03165341 -0.32124755 -0.05798066 -0.03256881]', '[ 0.02412308 -0.32658523 -0.01595187 -0.02112032]', '[ 0.02550179 -0.32964056  0.02933688 -0.00867761]', '[ 0.03535467 -0.32956213  0.06713802  0.01106326]', '[ 0.05126215 -0.32448023  0.08879534  0.04147042]', '[ 0.06948414 -0.31236544  0.09003875  0.0805337 ]', '[ 0.08596321 -0.29218207  0.07199708  0.12046316]', '[ 0.09737325 -0.26489006  0.04063242  0.14957341]', '[ 0.10190935 -0.23388285  0.00479206  0.15588881]', '[ 0.09960108 -0.20462479 -0.02647608  0.13132678]', '[ 0.09208836 -0.18350913 -0.04647049  0.07508745]', '[ 0.08196904 -0.17622141 -0.05247261 -0.00494006]', '[ 0.07194826 -0.1860764  -0.04606129 -0.09335229]', '[ 0.0640607  -0.21283993 -0.03210001 -0.17081162]', '[ 0.05920229 -0.25243865 -0.01674109 -0.2191429 ]', '[ 0.0571035  -0.29771672 -0.00514729 -0.22641302]', '[ 5.67079806e-02 -3.40049845e-01  1.40509559e-04 -1.90152289e-01]', '[ 0.0567542  -0.37130947 -0.00044065 -0.1175718 ]', '[ 0.05630704 -0.38559301 -0.00424585 -0.02319697]', '[ 0.05508019 -0.38034455 -0.00762881  0.0746204 ]', '[ 0.05352152 -0.35676725 -0.00706294  0.15719537]', '[ 5.26889742e-02 -3.19556780e-01 -1.32505029e-04  2.08826291e-01]', '[ 0.05393115 -0.2759787   0.01350876  0.22000939]', '[ 0.05839564 -0.23435582  0.03145057  0.18995248]', '[ 0.06647515 -0.20222884  0.04868101  0.12712705]', '[ 0.07740249 -0.18468121  0.0589193   0.04705174]', '[ 0.08920474 -0.18334652  0.05675805 -0.03210605]', '[ 0.09909535 -0.19637959  0.03975234 -0.09447618]', '[ 0.10420937 -0.21932955  0.00966234 -0.13033698]', '[ 0.10246404 -0.24658161 -0.02757142 -0.13784684]', '[ 0.09328114 -0.27290276 -0.06315946 -0.12236486]', '[ 0.07793604 -0.29463867 -0.08778553 -0.09376129]', '[ 0.0593946  -0.31024783 -0.09427901 -0.06266294]', '[ 0.04164872 -0.32007965 -0.07982525 -0.03685256]', '[ 0.02871865 -0.32554868 -0.04699358 -0.01899582]', '[ 0.02360262 -0.32805697 -0.00321876 -0.00646596]', '[ 0.02747827 -0.32810149  0.04113818  0.00669675]', '[ 0.03938956 -0.32492763  0.0755836   0.02646753]', '[ 0.0565101  -0.31687384  0.0923231   0.05547315]', '[ 0.07490627 -0.30227879  0.08830434  0.09091934]', '[ 0.09057649 -0.28059671  0.06587143  0.12465308]', '[ 0.10046354 -0.25327641  0.03185408  0.14539966]', '[ 0.10315103 -0.22403115 -0.00458867  0.14244801]', '[ 0.09906173 -0.19832456 -0.03465823  0.1095913 ]', '[ 0.090136   -0.18215254 -0.05229431  0.04802964]', '[ 0.07912538 -0.18043834 -0.05556224 -0.03278709]', '[ 0.06873857 -0.19550748 -0.0467223  -0.1168093 ]', '[ 0.06090465 -0.22612413 -0.03102421 -0.18524267]', '[ 0.05637446 -0.26744124 -0.01462964 -0.22160895]', '[ 0.05476245 -0.31195043 -0.00243303 -0.21638607]', '[ 0.05495737 -0.35116801  0.00332542 -0.16950281]', '[ 0.05568737 -0.37752895  0.0032086  -0.08993096]', '[ 5.60120148e-02 -3.85961900e-01 -1.99426156e-04  6.88577345e-03]', '[ 0.05562006 -0.37485205 -0.00336396  0.10238374]', '[ 0.05491675 -0.34632881 -0.00281815  0.17823062]', '[ 0.05490846 -0.30588436  0.00380835  0.21968852]', '[ 0.05687536 -0.26131719  0.01672642  0.2189266 ]', '[ 0.06185878 -0.22108772  0.03329702  0.17737189]', '[ 0.07010297 -0.1924189   0.04835125  0.10572158]', '[ 0.08068633 -0.17968709  0.0557311   0.02106819]', '[ 0.09154199 -0.18360664  0.05050737 -0.05790659]', '[ 0.09991338 -0.20142098  0.03096826 -0.11590096]', '[ 0.1031209  -0.22796893 -0.00034305 -0.14457436]', '[ 0.09940889 -0.25724729 -0.03689008 -0.14384494]', '[ 0.08860779 -0.28398315 -0.06969503 -0.12071965]', '[ 0.07238558 -0.30476413 -0.08980074 -0.08618494]', '[ 0.053974   -0.31844045 -0.09092666 -0.05123801]', '[ 0.03741523 -0.32575622 -0.0714764  -0.02335558]', '[ 0.02653095 -0.3284175  -0.03523065 -0.00454442]', '[ 0.02390923 -0.32798743  0.0095238   0.00839929]', '[ 0.03020552 -0.32504777  0.05218353  0.02158279]', '[ 0.04396167 -0.31895319  0.08269304  0.04059812]', '[ 0.06199569 -0.30826712  0.09424795  0.06735185]', '[ 0.08024809 -0.29169783  0.08504662  0.09839758]', '[ 0.09483717 -0.26915531  0.05858188  0.12543454]', '[ 0.10301802 -0.24249826  0.0224198   0.13781555]', '[ 0.10377826 -0.21564543 -0.01410806  0.12621646]', '[ 0.09792482 -0.19393613 -0.04255291  0.08627243]', '[ 0.08767477 -0.18286809 -0.0575417   0.02099345]', '[ 0.07590541 -0.18655146 -0.05792259 -0.05890949]', '[ 0.06530491 -0.20633731 -0.04660131 -0.13708618]', '[ 0.05768201 -0.24007046 -0.02916026 -0.19560079]', '[ 0.05363739 -0.28226425 -0.01173496 -0.21985746]', '[ 0.05266638 -0.32520851  0.0010306  -0.20272093]', '[ 0.05359128 -0.36068612  0.00713647 -0.14630965]', '[ 0.05510701 -0.38177224  0.00723029 -0.06109619]', '[ 0.0562436  -0.38425748  0.00386662  0.03674448]', '[ 0.0566538  -0.36747063  0.00056143  0.12854072]', '[ 0.05670863 -0.33445047  0.00081213  0.1964189 ]', '[ 0.05738383 -0.29144034  0.00697313  0.22678809]', '[ 0.05991129 -0.24668346  0.019088    0.21372085]', '[ 0.06523806 -0.2086492   0.03425028  0.16101479]', '[ 0.07346816 -0.18410168  0.04713803  0.08155666]', '[ 0.08353885 -0.17659553  0.05175852 -0.00620498]', '[ 0.09331176 -0.18586558  0.04370315 -0.08338381]', '[ 0.10008853 -0.20824698  0.02200651 -0.13555758]', '[ 0.10140207 -0.23792825 -0.01003113 -0.15601687]', '[ 0.09584132 -0.26861749 -0.04534776 -0.14657816]', '[ 0.08364422 -0.29511506 -0.07489216 -0.11589105]', '[ 0.0668445  -0.31434892 -0.09020274 -0.07592226]', '[ 0.04888729 -0.32562439 -0.08599892 -0.03783852]', '[ 0.03379772 -0.33010452 -0.06193576 -0.00863452]', '[ 0.02513479 -0.32978443 -0.02293809  0.01042693]', '[ 0.02503494 -0.32637922  0.02200748  0.02311183]', '[ 0.03362506 -0.32055551  0.0622461   0.03560982]', '[ 0.04897573 -0.31178877  0.08833123  0.05309252]', '[ 0.0676078  -0.29887794  0.09454709  0.07680051]', '[ 0.08540429 -0.28088981  0.0803421   0.10279361]', '[ 0.09866221 -0.25814068  0.05026789  0.12283631]', '[ 0.10498439 -0.23280889  0.01249125  0.12708833]', '[ 0.10377068 -0.20890319 -0.02361189  0.1076759 ]', '[ 0.09619874 -0.19152544 -0.05002788  0.06198729]', '[ 0.08473696 -0.18559403 -0.06210636 -0.00538117]', '[ 0.07236021 -0.19437892 -0.05947148 -0.08276543]', '[ 0.06171276 -0.21829461 -0.04563574 -0.15384494]', '[ 0.05446894 -0.25436617 -0.02646529 -0.20181367]', '[ 0.05107278 -0.29660697 -0.00804791 -0.2140739 ]', '[ 0.05089334 -0.33724733  0.00519376 -0.18578769]', '[ 0.05267033 -0.36844501  0.01144903 -0.12103312]', '[ 0.05504228 -0.38397531  0.01143998 -0.03155138]', '[ 0.05699176 -0.38051242  0.00775358  0.0658985 ]', '[ 0.05813473 -0.35832758  0.00398721  0.15263031]', '[ 0.05882524 -0.32134641  0.00373793  0.21136315]', '[ 0.06003229 -0.27650529  0.00934041  0.22987307]', '[ 0.06295692 -0.2323867   0.02061899  0.20436843]', '[ 0.06845962 -0.19732792  0.03436439  0.14111977]', '[ 0.07651005 -0.17749343  0.04511943  0.0550965 ]', '[ 0.08591764 -0.17551461  0.04710647 -0.03416791]', '[ 0.09449538 -0.1901073   0.03647786 -0.10791535]', '[ 0.09963108 -0.21672435  0.01302232 -0.15291381]', '[ 0.09909552 -0.24898478 -0.01923623 -0.1643131 ]', '[ 0.09183623 -0.28042156 -0.05279286 -0.1459218 ]', '[ 0.07849122 -0.30602506 -0.07865026 -0.10796961]', '[ 0.06142526 -0.32315462 -0.0889805  -0.06322103]', '[ 0.04423814 -0.33162027 -0.07959606 -0.02279592]', '[ 0.03086916 -0.33301485 -0.05140538  0.00695212]', '[ 0.02455586 -0.32961189 -0.01037788  0.02555682]', '[ 0.02695213 -0.32326726  0.03397195  0.03730786]']</t>
-  </si>
-  <si>
-    <t>[array([-0.03763371, -0.01533471,  0.06554052, -0.01816017], dtype=float32), array([-0.0208055 , -0.02030166,  0.09914155, -0.02801351]), array([ 0.00031733, -0.02489487,  0.10765546, -0.0138725 ]), array([ 0.02044082, -0.02428802,  0.08954248,  0.02288616]), array([ 0.03470698, -0.01491644,  0.05056501,  0.07132823]), array([ 0.05326751, -0.03038784,  0.13065223, -0.22021077]), array([ 0.07101291, -0.0640307 ,  0.04229076, -0.10791836]), array([ 0.06919594, -0.07148833, -0.06018897,  0.03411905]), array([ 0.06123949, -0.0858309 , -0.01832924, -0.17605239]), array([ 0.04848925, -0.10546764, -0.10705552, -0.01913256]), array([ 0.03334023, -0.12873715, -0.04224633, -0.21160413]), array([ 0.01856077, -0.15355978, -0.1031453 , -0.03494141]), array([ 0.00687968, -0.17764366, -0.01219475, -0.20332606]), array([ 0.00024918, -0.19823055, -0.05320561, -0.00041555]), array([-0.00038196, -0.21249406,  0.04645807, -0.13967612]), array([ 0.00462703, -0.21766377,  0.00256154,  0.08939976]), array([ 0.01391452, -0.21184382,  0.0884936 , -0.03053848]), array([ 0.03850047, -0.22834148,  0.15179103, -0.12764898]), array([ 0.05871339, -0.22531591,  0.04642174,  0.1602345 ]), array([ 0.06975736, -0.19972822,  0.06255754,  0.09301244]), array([ 0.08295526, -0.18863935,  0.06709485,  0.01801994]), array([ 0.0955466 , -0.19194963,  0.05618073, -0.04863014]), array([ 0.10438266, -0.20672312,  0.02995667, -0.09524718]), array([ 0.10679076, -0.22835209, -0.00700287, -0.1170154 ]), array([ 0.10139245, -0.251988  , -0.04658216, -0.11618468]), array([ 0.08862558, -0.27379536, -0.07912951, -0.10019242]), array([ 0.07079541, -0.2916811 , -0.09605709, -0.07844699]), array([ 0.05160586, -0.30533224, -0.09231221, -0.05881123]), array([ 0.03527347, -0.31561531, -0.06796943, -0.04491109]), array([ 0.02545877, -0.32360191, -0.02840871, -0.03520182]), array([ 0.02431678, -0.32962124,  0.01702803, -0.0241677 ]), array([ 0.03194057, -0.33273766,  0.0575287 , -0.00523763]), array([ 0.04635922, -0.33089406,  0.08372791,  0.02568935]), array([ 0.06409062, -0.32170512,  0.09020522,  0.06748616]), array([ 0.08108895, -0.30362649,  0.07683704,  0.11292955]), array([ 0.09381032, -0.27706452,  0.04859846,  0.15016487]), array([ 0.10008474, -0.24498455,  0.01387843,  0.16612946]), array([ 0.099545  , -0.21272175, -0.0181427 ,  0.15089341]), array([ 0.09350925, -0.18694889, -0.04018141,  0.10151107]), array([ 0.08439395, -0.17403958, -0.04874136,  0.02402904]), array([ 0.0748759 , -0.17828815, -0.04468765, -0.06714713]), array([ 0.06707968, -0.2005238 , -0.03244224, -0.15248501]), array([ 0.06204155, -0.23757011, -0.01810026, -0.2123621 ]), array([ 0.0596084 , -0.28277818, -0.00709475, -0.23248464]), array([ 0.0587725 , -0.32752505, -0.00232775, -0.20781714]), array([ 0.05826257, -0.3632139 , -0.00355436, -0.1435367 ]), array([ 0.05712088, -0.38315408, -0.00807237, -0.05302107]), array([ 0.05506565, -0.38385601, -0.01204958,  0.04571899]), array([ 0.05258562, -0.36558361, -0.01179826,  0.13373731]), array([ 0.05080563, -0.3322004 , -0.0047971 ,  0.19451381]), array([ 0.05116333, -0.29036678,  0.00943036,  0.21708422]), array([ 0.05492846, -0.24815416,  0.02866925,  0.1986191 ]), array([ 0.06265333, -0.2132846 ,  0.04805764,  0.14539356]), array([ 0.0737392 , -0.1914255 ,  0.06122493,  0.07119519]), array([ 0.08632927, -0.18505144,  0.06232775, -0.0065993 ]), array([ 0.09763559, -0.19320967,  0.04820618, -0.07185489]), array([ 0.1046364 , -0.21219823,  0.01981793, -0.11373169]), array([ 0.10494239, -0.23687371, -0.01755309, -0.12880179]), array([ 0.09757088, -0.26214836, -0.05540839, -0.12082367]), array([ 0.08338498, -0.28422734, -0.084203  , -0.09846705]), array([ 0.06503934, -0.30125202, -0.09599606, -0.07181621]), array([ 0.04641147, -0.31321516, -0.08681408, -0.04877953]), array([ 0.03165341, -0.32124755, -0.05798066, -0.03256881]), array([ 0.02412308, -0.32658523, -0.01595187, -0.02112032]), array([ 0.02550179, -0.32964056,  0.02933688, -0.00867761]), array([ 0.03535467, -0.32956213,  0.06713802,  0.01106326]), array([ 0.05126215, -0.32448023,  0.08879534,  0.04147042]), array([ 0.06948414, -0.31236544,  0.09003875,  0.0805337 ]), array([ 0.08596321, -0.29218207,  0.07199708,  0.12046316]), array([ 0.09737325, -0.26489006,  0.04063242,  0.14957341]), array([ 0.10190935, -0.23388285,  0.00479206,  0.15588881]), array([ 0.09960108, -0.20462479, -0.02647608,  0.13132678]), array([ 0.09208836, -0.18350913, -0.04647049,  0.07508745]), array([ 0.08196904, -0.17622141, -0.05247261, -0.00494006]), array([ 0.07194826, -0.1860764 , -0.04606129, -0.09335229]), array([ 0.0640607 , -0.21283993, -0.03210001, -0.17081162]), array([ 0.05920229, -0.25243865, -0.01674109, -0.2191429 ]), array([ 0.0571035 , -0.29771672, -0.00514729, -0.22641302]), array([ 5.67079806e-02, -3.40049845e-01,  1.40509559e-04, -1.90152289e-01]), array([ 0.0567542 , -0.37130947, -0.00044065, -0.1175718 ]), array([ 0.05630704, -0.38559301, -0.00424585, -0.02319697]), array([ 0.05508019, -0.38034455, -0.00762881,  0.0746204 ]), array([ 0.05352152, -0.35676725, -0.00706294,  0.15719537]), array([ 5.26889742e-02, -3.19556780e-01, -1.32505029e-04,  2.08826291e-01]), array([ 0.05393115, -0.2759787 ,  0.01350876,  0.22000939]), array([ 0.05839564, -0.23435582,  0.03145057,  0.18995248]), array([ 0.06647515, -0.20222884,  0.04868101,  0.12712705]), array([ 0.07740249, -0.18468121,  0.0589193 ,  0.04705174]), array([ 0.08920474, -0.18334652,  0.05675805, -0.03210605]), array([ 0.09909535, -0.19637959,  0.03975234, -0.09447618]), array([ 0.10420937, -0.21932955,  0.00966234, -0.13033698]), array([ 0.10246404, -0.24658161, -0.02757142, -0.13784684]), array([ 0.09328114, -0.27290276, -0.06315946, -0.12236486]), array([ 0.07793604, -0.29463867, -0.08778553, -0.09376129]), array([ 0.0593946 , -0.31024783, -0.09427901, -0.06266294]), array([ 0.04164872, -0.32007965, -0.07982525, -0.03685256]), array([ 0.02871865, -0.32554868, -0.04699358, -0.01899582]), array([ 0.02360262, -0.32805697, -0.00321876, -0.00646596]), array([ 0.02747827, -0.32810149,  0.04113818,  0.00669675]), array([ 0.03938956, -0.32492763,  0.0755836 ,  0.02646753]), array([ 0.0565101 , -0.31687384,  0.0923231 ,  0.05547315]), array([ 0.07490627, -0.30227879,  0.08830434,  0.09091934]), array([ 0.09057649, -0.28059671,  0.06587143,  0.12465308]), array([ 0.10046354, -0.25327641,  0.03185408,  0.14539966]), array([ 0.10315103, -0.22403115, -0.00458867,  0.14244801]), array([ 0.09906173, -0.19832456, -0.03465823,  0.1095913 ]), array([ 0.090136  , -0.18215254, -0.05229431,  0.04802964]), array([ 0.07912538, -0.18043834, -0.05556224, -0.03278709]), array([ 0.06873857, -0.19550748, -0.0467223 , -0.1168093 ]), array([ 0.06090465, -0.22612413, -0.03102421, -0.18524267]), array([ 0.05637446, -0.26744124, -0.01462964, -0.22160895]), array([ 0.05476245, -0.31195043, -0.00243303, -0.21638607]), array([ 0.05495737, -0.35116801,  0.00332542, -0.16950281]), array([ 0.05568737, -0.37752895,  0.0032086 , -0.08993096]), array([ 5.60120148e-02, -3.85961900e-01, -1.99426156e-04,  6.88577345e-03]), array([ 0.05562006, -0.37485205, -0.00336396,  0.10238374]), array([ 0.05491675, -0.34632881, -0.00281815,  0.17823062]), array([ 0.05490846, -0.30588436,  0.00380835,  0.21968852]), array([ 0.05687536, -0.26131719,  0.01672642,  0.2189266 ]), array([ 0.06185878, -0.22108772,  0.03329702,  0.17737189]), array([ 0.07010297, -0.1924189 ,  0.04835125,  0.10572158]), array([ 0.08068633, -0.17968709,  0.0557311 ,  0.02106819]), array([ 0.09154199, -0.18360664,  0.05050737, -0.05790659]), array([ 0.09991338, -0.20142098,  0.03096826, -0.11590096]), array([ 0.1031209 , -0.22796893, -0.00034305, -0.14457436]), array([ 0.09940889, -0.25724729, -0.03689008, -0.14384494]), array([ 0.08860779, -0.28398315, -0.06969503, -0.12071965]), array([ 0.07238558, -0.30476413, -0.08980074, -0.08618494]), array([ 0.053974  , -0.31844045, -0.09092666, -0.05123801]), array([ 0.03741523, -0.32575622, -0.0714764 , -0.02335558]), array([ 0.02653095, -0.3284175 , -0.03523065, -0.00454442]), array([ 0.02390923, -0.32798743,  0.0095238 ,  0.00839929]), array([ 0.03020552, -0.32504777,  0.05218353,  0.02158279]), array([ 0.04396167, -0.31895319,  0.08269304,  0.04059812]), array([ 0.06199569, -0.30826712,  0.09424795,  0.06735185]), array([ 0.08024809, -0.29169783,  0.08504662,  0.09839758]), array([ 0.09483717, -0.26915531,  0.05858188,  0.12543454]), array([ 0.10301802, -0.24249826,  0.0224198 ,  0.13781555]), array([ 0.10377826, -0.21564543, -0.01410806,  0.12621646]), array([ 0.09792482, -0.19393613, -0.04255291,  0.08627243]), array([ 0.08767477, -0.18286809, -0.0575417 ,  0.02099345]), array([ 0.07590541, -0.18655146, -0.05792259, -0.05890949]), array([ 0.06530491, -0.20633731, -0.04660131, -0.13708618]), array([ 0.05768201, -0.24007046, -0.02916026, -0.19560079]), array([ 0.05363739, -0.28226425, -0.01173496, -0.21985746]), array([ 0.05266638, -0.32520851,  0.0010306 , -0.20272093]), array([ 0.05359128, -0.36068612,  0.00713647, -0.14630965]), array([ 0.05510701, -0.38177224,  0.00723029, -0.06109619]), array([ 0.0562436 , -0.38425748,  0.00386662,  0.03674448]), array([ 0.0566538 , -0.36747063,  0.00056143,  0.12854072]), array([ 0.05670863, -0.33445047,  0.00081213,  0.1964189 ]), array([ 0.05738383, -0.29144034,  0.00697313,  0.22678809]), array([ 0.05991129, -0.24668346,  0.019088  ,  0.21372085]), array([ 0.06523806, -0.2086492 ,  0.03425028,  0.16101479]), array([ 0.07346816, -0.18410168,  0.04713803,  0.08155666]), array([ 0.08353885, -0.17659553,  0.05175852, -0.00620498]), array([ 0.09331176, -0.18586558,  0.04370315, -0.08338381]), array([ 0.10008853, -0.20824698,  0.02200651, -0.13555758]), array([ 0.10140207, -0.23792825, -0.01003113, -0.15601687]), array([ 0.09584132, -0.26861749, -0.04534776, -0.14657816]), array([ 0.08364422, -0.29511506, -0.07489216, -0.11589105]), array([ 0.0668445 , -0.31434892, -0.09020274, -0.07592226]), array([ 0.04888729, -0.32562439, -0.08599892, -0.03783852]), array([ 0.03379772, -0.33010452, -0.06193576, -0.00863452]), array([ 0.02513479, -0.32978443, -0.02293809,  0.01042693]), array([ 0.02503494, -0.32637922,  0.02200748,  0.02311183]), array([ 0.03362506, -0.32055551,  0.0622461 ,  0.03560982]), array([ 0.04897573, -0.31178877,  0.08833123,  0.05309252]), array([ 0.0676078 , -0.29887794,  0.09454709,  0.07680051]), array([ 0.08540429, -0.28088981,  0.0803421 ,  0.10279361]), array([ 0.09866221, -0.25814068,  0.05026789,  0.12283631]), array([ 0.10498439, -0.23280889,  0.01249125,  0.12708833]), array([ 0.10377068, -0.20890319, -0.02361189,  0.1076759 ]), array([ 0.09619874, -0.19152544, -0.05002788,  0.06198729]), array([ 0.08473696, -0.18559403, -0.06210636, -0.00538117]), array([ 0.07236021, -0.19437892, -0.05947148, -0.08276543]), array([ 0.06171276, -0.21829461, -0.04563574, -0.15384494]), array([ 0.05446894, -0.25436617, -0.02646529, -0.20181367]), array([ 0.05107278, -0.29660697, -0.00804791, -0.2140739 ]), array([ 0.05089334, -0.33724733,  0.00519376, -0.18578769]), array([ 0.05267033, -0.36844501,  0.01144903, -0.12103312]), array([ 0.05504228, -0.38397531,  0.01143998, -0.03155138]), array([ 0.05699176, -0.38051242,  0.00775358,  0.0658985 ]), array([ 0.05813473, -0.35832758,  0.00398721,  0.15263031]), array([ 0.05882524, -0.32134641,  0.00373793,  0.21136315]), array([ 0.06003229, -0.27650529,  0.00934041,  0.22987307]), array([ 0.06295692, -0.2323867 ,  0.02061899,  0.20436843]), array([ 0.06845962, -0.19732792,  0.03436439,  0.14111977]), array([ 0.07651005, -0.17749343,  0.04511943,  0.0550965 ]), array([ 0.08591764, -0.17551461,  0.04710647, -0.03416791]), array([ 0.09449538, -0.1901073 ,  0.03647786, -0.10791535]), array([ 0.09963108, -0.21672435,  0.01302232, -0.15291381]), array([ 0.09909552, -0.24898478, -0.01923623, -0.1643131 ]), array([ 0.09183623, -0.28042156, -0.05279286, -0.1459218 ]), array([ 0.07849122, -0.30602506, -0.07865026, -0.10796961]), array([ 0.06142526, -0.32315462, -0.0889805 , -0.06322103]), array([ 0.04423814, -0.33162027, -0.07959606, -0.02279592]), array([ 0.03086916, -0.33301485, -0.05140538,  0.00695212]), array([ 0.02455586, -0.32961189, -0.01037788,  0.02555682]), array([ 0.02695213, -0.32326726,  0.03397195,  0.03730786])]</t>
-  </si>
-  <si>
-    <t>['[2,0,1]', '[0,0,0]', '[2,1,0]', '[0,2,1]', '[2,2,2]', '[1,0,2]', '[1,1,1]', '[1,2,0]', '[1,1,2]', '[0,1,1]']</t>
-  </si>
-  <si>
-    <t>[2,0,1]</t>
-  </si>
-  <si>
-    <t>[3, 6, 7, 10, 16, 23, 26, 29, 32, 36, 41, 42, 57, 61, 63, 68, 78, 82, 83, 88, 92, 102, 108, 111, 120]</t>
-  </si>
-  <si>
-    <t>[0, 0, 0, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 1, 2, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 0, 1, 1, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 1, 1, 1, 1, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2]</t>
-  </si>
-  <si>
-    <t>['[-0.03763371 -0.01533471  0.06554052 -0.01816017]', '[-0.00754409 -0.05458322  0.2277812  -0.36241836]', '[ 0.04879627 -0.15231473  0.32089719 -0.5887683 ]', '[ 0.08773348 -0.20975891  0.05953656  0.02857539]', '[ 0.07159701 -0.14038323 -0.21558016  0.65104861]', '[ 0.00648475  0.0393353  -0.41626589  1.10429103]', '[-0.07174105  0.24590677 -0.34368039  0.91388152]', '[-0.12323516  0.38841716 -0.1579801   0.48237793]', '[-0.14431191  0.46440473 -0.04702105  0.2632506 ]', '[-0.11556577  0.42416188  0.32794186 -0.65615106]', '[-0.04492347  0.27962966  0.36024134 -0.75493806]', '[ 0.04708596  0.06893877  0.53517141 -1.30265314]', '[ 0.1567073  -0.21584704  0.52811555 -1.47577882]', '[ 0.24517949 -0.49319206  0.330497   -1.23924076]', '[ 0.28117568 -0.69296767  0.0200094  -0.72890117]', '[ 0.25255123 -0.77791507 -0.29977951 -0.11630858]', '[ 0.15475941 -0.71080304 -0.65760747  0.76800551]', '[-0.01207803 -0.45163386 -0.977196    1.77299051]', '[-0.21825877 -0.03321993 -1.03030534  2.30590906]', '[-0.39942324  0.42102602 -0.72647796  2.12444943]', '[-0.49143533  0.78053041 -0.16968559  1.4145231 ]', '[-0.46395468  0.97373051  0.43746541  0.50408489]', '[-0.30274948  0.92343339  1.14045208 -0.99012885]', '[-0.04821778  0.65318658  1.35245977 -1.64692209]', '[ 0.23950088  0.23434634  1.46038956 -2.43283672]', '[ 0.5060482  -0.26416939  1.13384587 -2.41515284]', '[ 0.64375574 -0.62020198  0.21633688 -1.09374258]', '[ 0.61360388 -0.75591779 -0.5145519  -0.2484425 ]', '[ 0.42119823 -0.65564654 -1.37471941  1.23340192]', '[ 0.09687354 -0.31460091 -1.7990724   2.08322616]', '[-0.27699863  0.15662165 -1.84589133  2.46717422]', '[-0.60418555  0.60728738 -1.35412207  1.92472076]', '[-0.78641664  0.86843169 -0.44254491  0.66534525]', '[-0.78796548  0.90103665  0.42690112 -0.34161506]', '[-0.59718635  0.67098139  1.45551705 -1.94731153]', '[-0.22441999  0.14183769  2.19294837 -3.21731415]', '[ 0.20757648 -0.46197139  2.01559952 -2.61580786]', '[ 0.56954311 -0.90817233  1.53361211 -1.75249599]', '[ 0.80058739 -1.14517511  0.74392415 -0.60507106]', '[ 0.85893546 -1.15033497 -0.16829248  0.54961418]', '[ 0.71258129 -0.86827639 -1.28409     2.27372606]', '[ 0.36979769 -0.28266856 -2.07615761  3.47607718]', '[-0.07379348  0.43855268 -2.23317987  3.4854593 ]', '[-0.48945343  1.05584169 -1.84044475  2.55769266]', '[-0.78691511  1.43919479 -1.09528435  1.26341978]', '[-0.91646279  1.56273513 -0.1841377  -0.02151925]', '[-0.83983549  1.38067663  0.94941957 -1.81140936]', '[-0.54011557  0.82905651  2.02498219 -3.70998494]', '[-0.05488639 -0.06897619  2.69131683 -5.00153358]', '[ 0.4612856  -1.01326285  2.33003269 -4.16357533]', '[ 0.84695034 -1.69263891  1.49034958 -2.6287764 ]', '[ 1.04775279 -2.07477055  0.50220851 -1.21464506]', '[ 1.04513878 -2.18331505 -0.52421838  0.12656362]', '[ 0.83036655 -1.97839329 -1.59595708  1.94133301]', '[ 0.42081829 -1.39407259 -2.46565524  3.93921113]', '[-0.1405329  -0.40106292 -3.05927505  5.83596458]', '[-0.72209135  0.76567147 -2.54294675  5.37953617]', '[-1.09864153  1.63935769 -1.20098319  3.3797041 ]', '[-1.21088976  2.16224666  0.07315914  1.87500217]', '[-1.07552812  2.39254531  1.25333619  0.42763275]', '[-0.71433038  2.29158208  2.29213451 -1.4362007 ]', '[-0.20697234  1.86401502  2.68752483 -2.81132968]', '[ 0.34232299  1.13759175  2.7459432  -4.39462351]', '[ 0.84208784  0.2222056   2.14652915 -4.50976348]', '[ 1.17862257 -0.62675223  1.12251763 -3.79139966]', '[ 1.26570506 -1.25398726 -0.28142171 -2.43164426]', '[ 1.06395154 -1.58173621 -1.71301231 -0.79648679]', '[ 0.58780069 -1.5055664  -2.95137696  1.57959642]', '[-0.06082645 -0.9836383  -3.41631825  3.54213189]', '[-0.7396652  -0.13908522 -3.23159786  4.59319353]', '[-1.29400131  0.71382586 -2.2147555   3.73137754]', '[-1.60917893  1.33472592 -0.92509942  2.50309181]', '[-1.66126031  1.72413949  0.41179385  1.38290492]', '[-1.42790867  1.8252163   1.90753544 -0.43641332]', '[-0.91021811  1.51470599  3.22126279 -2.76271786]', '[-0.16497237  0.69314912  4.14554037 -5.39220481]', '[ 0.67715623 -0.48859219  4.02646806 -5.815603  ]', '[ 1.3700865  -1.45811024  2.84842506 -3.82965886]', '[ 1.79952616 -2.01709425  1.46136957 -1.89026103]', '[ 1.97389074 -2.290269    0.28893187 -0.87672533]', '[ 1.90939941 -2.34903114 -0.93623627  0.30984969]', '[ 1.59031848 -2.12646967 -2.25763326  1.99445796]', '[ 1.01641673 -1.52983994 -3.46359558  4.10024997]', '[ 0.21663831 -0.44809952 -4.44239106  6.57542872]', '[-0.67045228  0.88099201 -4.15007928  6.02912431]', '[-1.38897123  1.85014239 -3.01212128  3.73569725]', '[-1.87389421  2.43147383 -1.84123551  2.19409924]', '[-2.13109139  2.75884639 -0.75013215  1.12375195]', '[-2.17419738  2.86894938  0.31223835 -0.02029   ]', '[-1.99771804  2.72602382  1.46915417 -1.43782657]', '[-1.57858161  2.27257954  2.73439769 -3.18969969]', '[-0.90313977  1.39222085  4.02789466 -5.80670052]', '[ 2.86733831e-03 -1.84439303e-02  4.81459928e+00 -7.77181454e+00]', '[ 0.90417972 -1.41232535  3.99702659 -5.69215784]', '[ 1.59093882 -2.31671419  2.86538239 -3.51869027]', '[ 2.0501004  -2.87526606  1.74215118 -2.15899488]', '[ 2.29964817  3.08180847  0.78682167 -1.12925605]', '[ 2.36891958  2.97128116 -0.08109286  0.02040658]', '[ 2.266067    3.09095231 -0.96443323  1.18377011]', '[ 1.96560375 -2.81198962 -2.07491676  2.65684715]', '[ 1.42456845 -2.09839322 -3.35146752  4.62390829]', '[ 0.61671415 -0.8747434  -4.75541229  7.80075604]', '[-0.39036123  0.80829211 -4.92358199  8.01151432]', '[-1.2673591   2.11575039 -3.83299191  5.15584219]', '[-1.92234466  2.95778852 -2.71406082  3.43294725]', '[-2.36403199 -2.75340436 -1.75661602  2.3419483 ]', '[-2.6482045  -2.37692662 -1.14005159  1.44314701]', '[-2.83760808 -2.16945106 -0.79290749  0.65095441]', '[-2.9715603  -2.12968735 -0.57967023 -0.22699318]', '[-3.08242189 -2.24736759 -0.56360363 -0.90920403]', '[ 3.07237578 -2.47411898 -0.75567687 -1.30060701]', '[ 2.89136267 -2.76128399 -1.08764141 -1.49476661]', '[ 2.62000317 -3.02000486 -1.6584658  -1.00880239]', '[ 2.20510038 -3.11154641 -2.54669464  0.17716327]', '[ 1.57793595 -2.9164438  -3.76101002  1.863095  ]', '[ 0.71035035 -2.32416551 -4.80633231  4.19498803]', '[-0.28657681 -1.18872064 -5.08823675  7.20807725]', '[-1.28618721  0.43410289 -4.63987188  8.19493292]', '[-2.05083562  1.83917589 -3.02468122  5.92610105]', '[-2.53243141  2.90142248 -1.90264601  4.86343127]', '[-2.85756523 -2.48383845 -1.47874534  4.16569696]', '[ 3.11722724 -1.67986876 -1.66900564  3.92970964]', '[ 2.73716112 -0.8807861  -2.19320571  4.1731958 ]']</t>
-  </si>
-  <si>
-    <t>[0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50, 51, 52, 53, 54, 55, 56, 57, 58, 59, 60, 61, 62, 63, 64, 65, 66, 67, 68, 69, 70, 71, 72, 73, 74, 75, 76, 77, 78, 79, 80, 81, 82, 83, 84, 85, 86, 87, 88, 89, 90, 91, 92, 93, 94, 95, 96, 97, 98, 99, 100, 101, 102, 103, 104, 105, 106, 107, 108, 109, 110, 111, 112, 113, 114, 115, 116, 117, 118, 119, 120, 121, 122]</t>
-  </si>
-  <si>
-    <t>[array([-0.03763371, -0.01533471,  0.06554052, -0.01816017], dtype=float32), array([-0.00754409, -0.05458322,  0.2277812 , -0.36241836]), array([ 0.04879627, -0.15231473,  0.32089719, -0.5887683 ]), array([ 0.08773348, -0.20975891,  0.05953656,  0.02857539]), array([ 0.07159701, -0.14038323, -0.21558016,  0.65104861]), array([ 0.00648475,  0.0393353 , -0.41626589,  1.10429103]), array([-0.07174105,  0.24590677, -0.34368039,  0.91388152]), array([-0.12323516,  0.38841716, -0.1579801 ,  0.48237793]), array([-0.14431191,  0.46440473, -0.04702105,  0.2632506 ]), array([-0.11556577,  0.42416188,  0.32794186, -0.65615106]), array([-0.04492347,  0.27962966,  0.36024134, -0.75493806]), array([ 0.04708596,  0.06893877,  0.53517141, -1.30265314]), array([ 0.1567073 , -0.21584704,  0.52811555, -1.47577882]), array([ 0.24517949, -0.49319206,  0.330497  , -1.23924076]), array([ 0.28117568, -0.69296767,  0.0200094 , -0.72890117]), array([ 0.25255123, -0.77791507, -0.29977951, -0.11630858]), array([ 0.15475941, -0.71080304, -0.65760747,  0.76800551]), array([-0.01207803, -0.45163386, -0.977196  ,  1.77299051]), array([-0.21825877, -0.03321993, -1.03030534,  2.30590906]), array([-0.39942324,  0.42102602, -0.72647796,  2.12444943]), array([-0.49143533,  0.78053041, -0.16968559,  1.4145231 ]), array([-0.46395468,  0.97373051,  0.43746541,  0.50408489]), array([-0.30274948,  0.92343339,  1.14045208, -0.99012885]), array([-0.04821778,  0.65318658,  1.35245977, -1.64692209]), array([ 0.23950088,  0.23434634,  1.46038956, -2.43283672]), array([ 0.5060482 , -0.26416939,  1.13384587, -2.41515284]), array([ 0.64375574, -0.62020198,  0.21633688, -1.09374258]), array([ 0.61360388, -0.75591779, -0.5145519 , -0.2484425 ]), array([ 0.42119823, -0.65564654, -1.37471941,  1.23340192]), array([ 0.09687354, -0.31460091, -1.7990724 ,  2.08322616]), array([-0.27699863,  0.15662165, -1.84589133,  2.46717422]), array([-0.60418555,  0.60728738, -1.35412207,  1.92472076]), array([-0.78641664,  0.86843169, -0.44254491,  0.66534525]), array([-0.78796548,  0.90103665,  0.42690112, -0.34161506]), array([-0.59718635,  0.67098139,  1.45551705, -1.94731153]), array([-0.22441999,  0.14183769,  2.19294837, -3.21731415]), array([ 0.20757648, -0.46197139,  2.01559952, -2.61580786]), array([ 0.56954311, -0.90817233,  1.53361211, -1.75249599]), array([ 0.80058739, -1.14517511,  0.74392415, -0.60507106]), array([ 0.85893546, -1.15033497, -0.16829248,  0.54961418]), array([ 0.71258129, -0.86827639, -1.28409   ,  2.27372606]), array([ 0.36979769, -0.28266856, -2.07615761,  3.47607718]), array([-0.07379348,  0.43855268, -2.23317987,  3.4854593 ]), array([-0.48945343,  1.05584169, -1.84044475,  2.55769266]), array([-0.78691511,  1.43919479, -1.09528435,  1.26341978]), array([-0.91646279,  1.56273513, -0.1841377 , -0.02151925]), array([-0.83983549,  1.38067663,  0.94941957, -1.81140936]), array([-0.54011557,  0.82905651,  2.02498219, -3.70998494]), array([-0.05488639, -0.06897619,  2.69131683, -5.00153358]), array([ 0.4612856 , -1.01326285,  2.33003269, -4.16357533]), array([ 0.84695034, -1.69263891,  1.49034958, -2.6287764 ]), array([ 1.04775279, -2.07477055,  0.50220851, -1.21464506]), array([ 1.04513878, -2.18331505, -0.52421838,  0.12656362]), array([ 0.83036655, -1.97839329, -1.59595708,  1.94133301]), array([ 0.42081829, -1.39407259, -2.46565524,  3.93921113]), array([-0.1405329 , -0.40106292, -3.05927505,  5.83596458]), array([-0.72209135,  0.76567147, -2.54294675,  5.37953617]), array([-1.09864153,  1.63935769, -1.20098319,  3.3797041 ]), array([-1.21088976,  2.16224666,  0.07315914,  1.87500217]), array([-1.07552812,  2.39254531,  1.25333619,  0.42763275]), array([-0.71433038,  2.29158208,  2.29213451, -1.4362007 ]), array([-0.20697234,  1.86401502,  2.68752483, -2.81132968]), array([ 0.34232299,  1.13759175,  2.7459432 , -4.39462351]), array([ 0.84208784,  0.2222056 ,  2.14652915, -4.50976348]), array([ 1.17862257, -0.62675223,  1.12251763, -3.79139966]), array([ 1.26570506, -1.25398726, -0.28142171, -2.43164426]), array([ 1.06395154, -1.58173621, -1.71301231, -0.79648679]), array([ 0.58780069, -1.5055664 , -2.95137696,  1.57959642]), array([-0.06082645, -0.9836383 , -3.41631825,  3.54213189]), array([-0.7396652 , -0.13908522, -3.23159786,  4.59319353]), array([-1.29400131,  0.71382586, -2.2147555 ,  3.73137754]), array([-1.60917893,  1.33472592, -0.92509942,  2.50309181]), array([-1.66126031,  1.72413949,  0.41179385,  1.38290492]), array([-1.42790867,  1.8252163 ,  1.90753544, -0.43641332]), array([-0.91021811,  1.51470599,  3.22126279, -2.76271786]), array([-0.16497237,  0.69314912,  4.14554037, -5.39220481]), array([ 0.67715623, -0.48859219,  4.02646806, -5.815603  ]), array([ 1.3700865 , -1.45811024,  2.84842506, -3.82965886]), array([ 1.79952616, -2.01709425,  1.46136957, -1.89026103]), array([ 1.97389074, -2.290269  ,  0.28893187, -0.87672533]), array([ 1.90939941, -2.34903114, -0.93623627,  0.30984969]), array([ 1.59031848, -2.12646967, -2.25763326,  1.99445796]), array([ 1.01641673, -1.52983994, -3.46359558,  4.10024997]), array([ 0.21663831, -0.44809952, -4.44239106,  6.57542872]), array([-0.67045228,  0.88099201, -4.15007928,  6.02912431]), array([-1.38897123,  1.85014239, -3.01212128,  3.73569725]), array([-1.87389421,  2.43147383, -1.84123551,  2.19409924]), array([-2.13109139,  2.75884639, -0.75013215,  1.12375195]), array([-2.17419738,  2.86894938,  0.31223835, -0.02029   ]), array([-1.99771804,  2.72602382,  1.46915417, -1.43782657]), array([-1.57858161,  2.27257954,  2.73439769, -3.18969969]), array([-0.90313977,  1.39222085,  4.02789466, -5.80670052]), array([ 2.86733831e-03, -1.84439303e-02,  4.81459928e+00, -7.77181454e+00]), array([ 0.90417972, -1.41232535,  3.99702659, -5.69215784]), array([ 1.59093882, -2.31671419,  2.86538239, -3.51869027]), array([ 2.0501004 , -2.87526606,  1.74215118, -2.15899488]), array([ 2.29964817,  3.08180847,  0.78682167, -1.12925605]), array([ 2.36891958,  2.97128116, -0.08109286,  0.02040658]), array([ 2.266067  ,  3.09095231, -0.96443323,  1.18377011]), array([ 1.96560375, -2.81198962, -2.07491676,  2.65684715]), array([ 1.42456845, -2.09839322, -3.35146752,  4.62390829]), array([ 0.61671415, -0.8747434 , -4.75541229,  7.80075604]), array([-0.39036123,  0.80829211, -4.92358199,  8.01151432]), array([-1.2673591 ,  2.11575039, -3.83299191,  5.15584219]), array([-1.92234466,  2.95778852, -2.71406082,  3.43294725]), array([-2.36403199, -2.75340436, -1.75661602,  2.3419483 ]), array([-2.6482045 , -2.37692662, -1.14005159,  1.44314701]), array([-2.83760808, -2.16945106, -0.79290749,  0.65095441]), array([-2.9715603 , -2.12968735, -0.57967023, -0.22699318]), array([-3.08242189, -2.24736759, -0.56360363, -0.90920403]), array([ 3.07237578, -2.47411898, -0.75567687, -1.30060701]), array([ 2.89136267, -2.76128399, -1.08764141, -1.49476661]), array([ 2.62000317, -3.02000486, -1.6584658 , -1.00880239]), array([ 2.20510038, -3.11154641, -2.54669464,  0.17716327]), array([ 1.57793595, -2.9164438 , -3.76101002,  1.863095  ]), array([ 0.71035035, -2.32416551, -4.80633231,  4.19498803]), array([-0.28657681, -1.18872064, -5.08823675,  7.20807725]), array([-1.28618721,  0.43410289, -4.63987188,  8.19493292]), array([-2.05083562,  1.83917589, -3.02468122,  5.92610105]), array([-2.53243141,  2.90142248, -1.90264601,  4.86343127]), array([-2.85756523, -2.48383845, -1.47874534,  4.16569696]), array([ 3.11722724, -1.67986876, -1.66900564,  3.92970964]), array([ 2.73716112, -0.8807861 , -2.19320571,  4.1731958 ])]</t>
-  </si>
-  <si>
-    <t>['[2,1,0]', '[0,1,1]', '[0,2,1]', '[2,2,2]', '[1,0,2]', '[1,1,1]', '[2,0,1]', '[1,1,2]', '[1,2,0]', '[0,0,0]']</t>
-  </si>
-  <si>
-    <t>[3, 5, 10, 13, 16, 17, 20, 21, 24, 25, 34, 39, 41, 44, 47, 54, 55, 58, 62, 67, 69, 70, 75, 77, 79, 84, 85, 87, 91, 93, 97, 99, 100, 103, 104, 106, 111, 114, 118, 126, 140, 142, 148, 149, 150, 151, 152, 157, 158]</t>
-  </si>
-  <si>
-    <t>[0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 1, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 2, 1, 0, 0, 0, 0, 0, 0, 0, 1, 1, 2, 2, 2, 2, 2, 2, 2, 2, 2, 1, 1, 0, 0, 0, 0, 0, 0, 0, 0, 1, 1, 2, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2]</t>
-  </si>
-  <si>
-    <t>['[-0.03763371 -0.01533471  0.06554052 -0.01816017]', '[-0.00754409 -0.05458322  0.2277812  -0.36241836]', '[ 0.04879627 -0.15231473  0.32089719 -0.5887683 ]', '[ 0.08773348 -0.20975891  0.05953656  0.02857539]', '[ 0.07159701 -0.14038323 -0.21558016  0.65104861]', '[ 0.01974015  0.00507076 -0.28772457  0.77006767]', '[-0.0498825   0.18719084 -0.38795592  1.00753131]', '[-0.12622793  0.38867521 -0.35384008  0.96154672]', '[-0.18349845  0.55503694 -0.20413474  0.66989022]', '[-0.2037078   0.64699888  0.00670697  0.23609143]', '[-0.18080465  0.647294    0.21730543 -0.22949905]', '[-0.09585258  0.49529142  0.6154049  -1.2640842 ]', '[ 0.05476147  0.16073698  0.852892   -2.00750275]', '[ 0.19902758 -0.19903702  0.54693732 -1.50114194]', '[ 0.28638276 -0.47924526  0.30053158 -1.24218151]', '[ 0.31185963 -0.6774872  -0.0534539  -0.7115953 ]', '[ 0.24192531 -0.69510523 -0.62958671  0.52712604]', '[ 0.08243012 -0.50847877 -0.93180549  1.29544648]', '[-0.12699293 -0.16884008 -1.11288703  2.01561171]', '[-0.33897542  0.25349917 -0.9479683   2.09396453]', '[-0.47215133  0.59434707 -0.3524672   1.2526045 ]', '[-0.47391332  0.74052159  0.33399914  0.1959587 ]', '[-0.33199362  0.64164811  1.05817129 -1.16511174]', '[-0.06686719  0.29208085  1.53648863 -2.24805022]', '[ 0.22593169 -0.13756571  1.31564183 -1.91379878]', '[ 0.43294435 -0.42836083  0.70950224 -0.92511254]', '[ 0.52342047 -0.55793615  0.17732693 -0.34604071]', '[ 0.47599654 -0.49698828 -0.64261429  0.94553077]', '[ 0.27603667 -0.19240767 -1.31365949  2.03319795]', '[-0.02345474  0.27136217 -1.60176697  2.46010076]', '[-0.33057235  0.72992473 -1.39787147  2.0063684 ]', '[-0.55976405  1.04170789 -0.85468246  1.06981757]', '[-0.6614495   1.14999415 -0.14698744  0.00668768]', '[-0.59511474  0.98711869  0.80643584 -1.63516217]', '[-0.36916278  0.56286429  1.41086925 -2.546707  ]', '[-0.03100169 -0.05441172  1.87935192 -3.45303817]', '[ 0.33620133 -0.72649332  1.69191006 -3.07523772]', '[ 0.6163417  -1.23569126  1.06642034 -1.96590773]', '[ 0.7522323  -1.50668031  0.27898896 -0.74245411]', '[ 0.71752718 -1.50798781 -0.61879078  0.7291965 ]', '[ 0.50139954 -1.18687928 -1.52180648  2.49076627]', '[ 0.1327913  -0.54605328 -2.10283835  3.82971674]', '[-0.30997183  0.29761252 -2.18262539  4.31615312]', '[-0.68393149  1.06804788 -1.47321682  3.24412859]', '[-0.87379994  1.55275601 -0.41732597  1.61572151]', '[-0.86034165  1.74355699  0.54147102  0.29401052]', '[-0.65014917  1.62168969  1.52510166 -1.52011096]', '[-0.28574159  1.18450967  2.06599761 -2.82565099]', '[ 0.17350349  0.45757362  2.4484156  -4.3149862 ]', '[ 0.64206614 -0.43574693  2.08967614 -4.31040317]', '[ 0.96185752 -1.17636158  1.05113575 -3.01418314]', '[ 1.05381381 -1.63695333 -0.13326796 -1.59401373]', '[ 0.91369361 -1.81225414 -1.23922218 -0.14899595]', '[ 0.56149504 -1.64540155 -2.2179771   1.82495968]', '[ 0.06463837 -1.11024608 -2.67643899  3.47938097]', '[-0.47524708 -0.30123578 -2.6121446   4.38725478]', '[-0.93685338  0.55551024 -1.88069162  3.92514604]', '[-1.19521048  1.21358634 -0.66758     2.61890211]', '[-1.18995525  1.57474065  0.71135199  0.98639133]', '[-0.91191317  1.57364664  2.02533913 -1.0320177 ]', '[-0.40389876  1.14778115  2.98477226 -3.23670066]', '[ 0.24783691  0.30452444  3.40755551 -4.96771979]', '[ 0.85914939 -0.60804885  2.55181173 -3.83043916]', '[ 1.25978187 -1.23761982  1.41863221 -2.45163158]', '[ 1.42080008 -1.59997882  0.18510998 -1.19267536]', '[ 1.32509365 -1.6899898  -1.13418744  0.31680893]', '[ 0.96577922 -1.42967228 -2.42986289  2.35121785]', '[ 0.3798861  -0.75489124 -3.36184868  4.36562736]', '[-0.34021637  0.25945388 -3.636615    5.3284434 ]', '[-0.97972337  1.16049736 -2.65535963  3.51166831]', '[-1.38780388  1.67310328 -1.41050395  1.68582569]', '[-1.54901839  1.88272909 -0.19698685  0.44217137]', '[-1.45069358  1.80655483  1.17756802 -1.22847915]', '[-1.08025455  1.36818838  2.51766223 -3.24065798]', '[-0.45076713  0.47827979  3.71494696 -5.60032614]', '[ 0.30591361 -0.64368562  3.61977972 -5.08647002]', '[ 0.9557806  -1.48310136  2.79928672 -3.2293584 ]', '[ 1.39089847 -1.90699443  1.52659957 -1.09617224]', '[ 1.57532448 -1.99306026  0.31020078  0.19624538]', '[ 1.50640739 -1.81248813 -0.99996428  1.62309432]', '[ 1.16694785 -1.30020579 -2.39656692  3.58737473]', '[ 0.55055586 -0.34460377 -3.70035616  5.88130004]', '[-0.23123201  0.86603236 -3.87484991  5.65192483]', '[-0.93822273  1.78737063 -3.12784664  3.53417705]', '[-1.45448816  2.2869042  -1.99657426  1.55100591]', '[-1.72798186  2.43631502 -0.7302511  -0.00713573]', '[-1.73876077  2.27517306  0.62731374 -1.59942369]', '[-1.4889492   1.83031692  1.87164307 -2.90047452]', '[-0.97199372  1.02857525  3.30683457 -5.24284307]', '[-0.18562495 -0.25206567  4.33731305 -7.05059553]', '[ 0.64533102 -1.50001899  3.81807892 -5.09324331]', '[ 1.30410118 -2.25250241  2.73015086 -2.5576629 ]', '[ 1.73653674 -2.60593736  1.57730342 -1.04849301]', '[ 1.92241195 -2.65244015  0.28515863  0.55009382]', '[ 1.8498771  -2.39178287 -1.01968044  2.06528839]', '[ 1.50865743 -1.80849724 -2.4101182   3.86551077]', '[ 0.8761805  -0.78355279 -3.92827199  6.51114092]', '[ 3.09424862e-03  6.50427883e-01 -4.50144618e+00  7.07784655e+00]', '[-0.83927992  1.83443736 -3.84141269  4.65679779]', '[-1.5063409   2.53347248 -2.7811998   2.46479638]', '[-1.94173038  2.86081858 -1.575375    0.87901347]', '[-2.14931388  2.92377409 -0.51851245 -0.21640125]', '[-2.14650951  2.76320652  0.55051348 -1.38009033]', '[-1.92914241  2.38840961  1.64250558 -2.40132161]', '[-1.48230681  1.77503896  2.83874061 -3.84586999]', '[-0.77008315  0.7372811   4.28908746 -6.6429161 ]', '[ 0.14461793 -0.67000304  4.55378611 -6.6558909 ]', '[ 0.98531636 -1.76347029  3.77319015 -4.1954432 ]', '[ 1.63636838 -2.39166673  2.70340226 -2.21919145]', '[ 2.06292413 -2.6963828   1.57576353 -0.91403945]', '[ 2.26980712 -2.76226324  0.51443377  0.2112985 ]', '[ 2.27904117 -2.64265007 -0.42216276  0.9727243 ]', '[ 2.08326683 -2.32958945 -1.55911432  2.1968324 ]', '[ 1.64366365 -1.73178257 -2.8695616   3.92022037]', '[ 0.93025099 -0.71359112 -4.27386226  6.36544675]', '[-0.02150545  0.71059306 -4.94249045  7.07449713]', '[-0.95129896  1.86258306 -4.27104653  4.35550841]', '[-1.70647949  2.5035942  -3.23472743  2.2139826 ]', '[-2.2364423   2.78493653 -2.0947959   0.71711106]', '[-2.5687629   2.84748356 -1.27839864 -0.01305492]', '[-2.76448727  2.80580762 -0.71451694 -0.3474956 ]', '[-2.85841216  2.7068548  -0.24166613 -0.60565157]', '[-2.86412968  2.57400587  0.18407382 -0.7068713 ]', '[-2.77503515  2.40542873  0.72478905 -0.98974991]', '[-2.56320932  2.16697156  1.43082933 -1.44614017]', '[-2.18435753  1.79476889  2.41131666 -2.39836776]', '[-1.5931791   1.19236292  3.54925006 -3.80022496]', '[-0.7317131   0.16207027  4.99722458 -6.34106437]', '[ 0.30705394 -1.06679082  5.12131858 -5.24114464]', '[ 1.25121728 -1.81239506  4.20621777 -2.2376891 ]', '[ 1.95713622 -2.02116345  2.8245945  -0.03702939]', '[ 2.37971038 -1.87861601  1.44163283  1.29919227]', '[ 2.5542704  -1.55407798  0.35599199  1.84789665]', '[ 2.52822951 -1.13607514 -0.59782508  2.32205811]', '[ 2.3136573  -0.61174343 -1.57359253  2.9938835 ]', '[ 1.88209935  0.09711977 -2.77969338  4.14005947]', '[ 1.19909456  1.01130195 -4.02083461  4.76829123]', '[ 0.29363915  1.88441092 -4.93722161  3.68144505]', '[-0.70536352  2.40704148 -4.82125631  1.44399837]', '[-1.55096855  2.45356711 -3.49354524 -0.94243845]', '[-2.06241414  2.04017103 -1.57147522 -3.08924724]', '[-2.1667418   1.23283964  0.50711122 -4.94173708]', '[-1.90590205  0.12818115  1.9957105  -6.01698213]', '[-1.39439953 -1.16055788  3.01321969 -6.63320762]', '[-0.70865304 -2.47487432  3.86625009 -6.52857859]', '[ 0.12277713  2.45905163  4.28560737 -7.20053314]', '[ 0.97625054  0.82513917  4.29473318 -9.27444098]', '[ 1.74837977 -1.02278245  3.04401508 -8.42541876]', '[ 2.10850829 -2.42823459  0.65470068 -5.89190546]', '[ 2.08102189  2.84304938 -0.71023619 -4.30960737]', '[ 1.87754212  2.1095677  -1.28868512 -3.07757336]', '[ 1.56058336  1.58558288 -1.89519002 -2.25638779]', '[ 1.13608262  1.12725053 -2.28856164 -2.49840072]', '[ 0.66526863  0.55231674 -2.37378711 -3.30034494]', '[ 0.17423957 -0.13849638 -2.63738372 -3.29971802]', '[-0.42528968 -0.63424316 -3.3154909  -1.53582662]', '[-1.09834012 -0.77770675 -3.25916931 -0.08185985]', '[-1.66875199 -0.78043574 -2.3804907  -0.11515747]', '[-2.04185266 -0.87157296 -1.35567451 -0.87415517]']</t>
-  </si>
-  <si>
-    <t>[0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50, 51, 52, 53, 54, 55, 56, 57, 58, 59, 60, 61, 62, 63, 64, 65, 66, 67, 68, 69, 70, 71, 72, 73, 74, 75, 76, 77, 78, 79, 80, 81, 82, 83, 84, 85, 86, 87, 88, 89, 90, 91, 92, 93, 94, 95, 96, 97, 98, 99, 100, 101, 102, 103, 104, 105, 106, 107, 108, 109, 110, 111, 112, 113, 114, 115, 116, 117, 118, 119, 120, 121, 122, 123, 124, 125, 126, 127, 128, 129, 130, 131, 132, 133, 134, 135, 136, 137, 138, 139, 140, 141, 142, 143, 144, 145, 146, 147, 148, 149, 150, 151, 152, 153, 154, 155, 156, 157, 158]</t>
-  </si>
-  <si>
-    <t>[array([-0.03763371, -0.01533471,  0.06554052, -0.01816017], dtype=float32), array([-0.00754409, -0.05458322,  0.2277812 , -0.36241836]), array([ 0.04879627, -0.15231473,  0.32089719, -0.5887683 ]), array([ 0.08773348, -0.20975891,  0.05953656,  0.02857539]), array([ 0.07159701, -0.14038323, -0.21558016,  0.65104861]), array([ 0.01974015,  0.00507076, -0.28772457,  0.77006767]), array([-0.0498825 ,  0.18719084, -0.38795592,  1.00753131]), array([-0.12622793,  0.38867521, -0.35384008,  0.96154672]), array([-0.18349845,  0.55503694, -0.20413474,  0.66989022]), array([-0.2037078 ,  0.64699888,  0.00670697,  0.23609143]), array([-0.18080465,  0.647294  ,  0.21730543, -0.22949905]), array([-0.09585258,  0.49529142,  0.6154049 , -1.2640842 ]), array([ 0.05476147,  0.16073698,  0.852892  , -2.00750275]), array([ 0.19902758, -0.19903702,  0.54693732, -1.50114194]), array([ 0.28638276, -0.47924526,  0.30053158, -1.24218151]), array([ 0.31185963, -0.6774872 , -0.0534539 , -0.7115953 ]), array([ 0.24192531, -0.69510523, -0.62958671,  0.52712604]), array([ 0.08243012, -0.50847877, -0.93180549,  1.29544648]), array([-0.12699293, -0.16884008, -1.11288703,  2.01561171]), array([-0.33897542,  0.25349917, -0.9479683 ,  2.09396453]), array([-0.47215133,  0.59434707, -0.3524672 ,  1.2526045 ]), array([-0.47391332,  0.74052159,  0.33399914,  0.1959587 ]), array([-0.33199362,  0.64164811,  1.05817129, -1.16511174]), array([-0.06686719,  0.29208085,  1.53648863, -2.24805022]), array([ 0.22593169, -0.13756571,  1.31564183, -1.91379878]), array([ 0.43294435, -0.42836083,  0.70950224, -0.92511254]), array([ 0.52342047, -0.55793615,  0.17732693, -0.34604071]), array([ 0.47599654, -0.49698828, -0.64261429,  0.94553077]), array([ 0.27603667, -0.19240767, -1.31365949,  2.03319795]), array([-0.02345474,  0.27136217, -1.60176697,  2.46010076]), array([-0.33057235,  0.72992473, -1.39787147,  2.0063684 ]), array([-0.55976405,  1.04170789, -0.85468246,  1.06981757]), array([-0.6614495 ,  1.14999415, -0.14698744,  0.00668768]), array([-0.59511474,  0.98711869,  0.80643584, -1.63516217]), array([-0.36916278,  0.56286429,  1.41086925, -2.546707  ]), array([-0.03100169, -0.05441172,  1.87935192, -3.45303817]), array([ 0.33620133, -0.72649332,  1.69191006, -3.07523772]), array([ 0.6163417 , -1.23569126,  1.06642034, -1.96590773]), array([ 0.7522323 , -1.50668031,  0.27898896, -0.74245411]), array([ 0.71752718, -1.50798781, -0.61879078,  0.7291965 ]), array([ 0.50139954, -1.18687928, -1.52180648,  2.49076627]), array([ 0.1327913 , -0.54605328, -2.10283835,  3.82971674]), array([-0.30997183,  0.29761252, -2.18262539,  4.31615312]), array([-0.68393149,  1.06804788, -1.47321682,  3.24412859]), array([-0.87379994,  1.55275601, -0.41732597,  1.61572151]), array([-0.86034165,  1.74355699,  0.54147102,  0.29401052]), array([-0.65014917,  1.62168969,  1.52510166, -1.52011096]), array([-0.28574159,  1.18450967,  2.06599761, -2.82565099]), array([ 0.17350349,  0.45757362,  2.4484156 , -4.3149862 ]), array([ 0.64206614, -0.43574693,  2.08967614, -4.31040317]), array([ 0.96185752, -1.17636158,  1.05113575, -3.01418314]), array([ 1.05381381, -1.63695333, -0.13326796, -1.59401373]), array([ 0.91369361, -1.81225414, -1.23922218, -0.14899595]), array([ 0.56149504, -1.64540155, -2.2179771 ,  1.82495968]), array([ 0.06463837, -1.11024608, -2.67643899,  3.47938097]), array([-0.47524708, -0.30123578, -2.6121446 ,  4.38725478]), array([-0.93685338,  0.55551024, -1.88069162,  3.92514604]), array([-1.19521048,  1.21358634, -0.66758   ,  2.61890211]), array([-1.18995525,  1.57474065,  0.71135199,  0.98639133]), array([-0.91191317,  1.57364664,  2.02533913, -1.0320177 ]), array([-0.40389876,  1.14778115,  2.98477226, -3.23670066]), array([ 0.24783691,  0.30452444,  3.40755551, -4.96771979]), array([ 0.85914939, -0.60804885,  2.55181173, -3.83043916]), array([ 1.25978187, -1.23761982,  1.41863221, -2.45163158]), array([ 1.42080008, -1.59997882,  0.18510998, -1.19267536]), array([ 1.32509365, -1.6899898 , -1.13418744,  0.31680893]), array([ 0.96577922, -1.42967228, -2.42986289,  2.35121785]), array([ 0.3798861 , -0.75489124, -3.36184868,  4.36562736]), array([-0.34021637,  0.25945388, -3.636615  ,  5.3284434 ]), array([-0.97972337,  1.16049736, -2.65535963,  3.51166831]), array([-1.38780388,  1.67310328, -1.41050395,  1.68582569]), array([-1.54901839,  1.88272909, -0.19698685,  0.44217137]), array([-1.45069358,  1.80655483,  1.17756802, -1.22847915]), array([-1.08025455,  1.36818838,  2.51766223, -3.24065798]), array([-0.45076713,  0.47827979,  3.71494696, -5.60032614]), array([ 0.30591361, -0.64368562,  3.61977972, -5.08647002]), array([ 0.9557806 , -1.48310136,  2.79928672, -3.2293584 ]), array([ 1.39089847, -1.90699443,  1.52659957, -1.09617224]), array([ 1.57532448, -1.99306026,  0.31020078,  0.19624538]), array([ 1.50640739, -1.81248813, -0.99996428,  1.62309432]), array([ 1.16694785, -1.30020579, -2.39656692,  3.58737473]), array([ 0.55055586, -0.34460377, -3.70035616,  5.88130004]), array([-0.23123201,  0.86603236, -3.87484991,  5.65192483]), array([-0.93822273,  1.78737063, -3.12784664,  3.53417705]), array([-1.45448816,  2.2869042 , -1.99657426,  1.55100591]), array([-1.72798186,  2.43631502, -0.7302511 , -0.00713573]), array([-1.73876077,  2.27517306,  0.62731374, -1.59942369]), array([-1.4889492 ,  1.83031692,  1.87164307, -2.90047452]), array([-0.97199372,  1.02857525,  3.30683457, -5.24284307]), array([-0.18562495, -0.25206567,  4.33731305, -7.05059553]), array([ 0.64533102, -1.50001899,  3.81807892, -5.09324331]), array([ 1.30410118, -2.25250241,  2.73015086, -2.5576629 ]), array([ 1.73653674, -2.60593736,  1.57730342, -1.04849301]), array([ 1.92241195, -2.65244015,  0.28515863,  0.55009382]), array([ 1.8498771 , -2.39178287, -1.01968044,  2.06528839]), array([ 1.50865743, -1.80849724, -2.4101182 ,  3.86551077]), array([ 0.8761805 , -0.78355279, -3.92827199,  6.51114092]), array([ 3.09424862e-03,  6.50427883e-01, -4.50144618e+00,  7.07784655e+00]), array([-0.83927992,  1.83443736, -3.84141269,  4.65679779]), array([-1.5063409 ,  2.53347248, -2.7811998 ,  2.46479638]), array([-1.94173038,  2.86081858, -1.575375  ,  0.87901347]), array([-2.14931388,  2.92377409, -0.51851245, -0.21640125]), array([-2.14650951,  2.76320652,  0.55051348, -1.38009033]), array([-1.92914241,  2.38840961,  1.64250558, -2.40132161]), array([-1.48230681,  1.77503896,  2.83874061, -3.84586999]), array([-0.77008315,  0.7372811 ,  4.28908746, -6.6429161 ]), array([ 0.14461793, -0.67000304,  4.55378611, -6.6558909 ]), array([ 0.98531636, -1.76347029,  3.77319015, -4.1954432 ]), array([ 1.63636838, -2.39166673,  2.70340226, -2.21919145]), array([ 2.06292413, -2.6963828 ,  1.57576353, -0.91403945]), array([ 2.26980712, -2.76226324,  0.51443377,  0.2112985 ]), array([ 2.27904117, -2.64265007, -0.42216276,  0.9727243 ]), array([ 2.08326683, -2.32958945, -1.55911432,  2.1968324 ]), array([ 1.64366365, -1.73178257, -2.8695616 ,  3.92022037]), array([ 0.93025099, -0.71359112, -4.27386226,  6.36544675]), array([-0.02150545,  0.71059306, -4.94249045,  7.07449713]), array([-0.95129896,  1.86258306, -4.27104653,  4.35550841]), array([-1.70647949,  2.5035942 , -3.23472743,  2.2139826 ]), array([-2.2364423 ,  2.78493653, -2.0947959 ,  0.71711106]), array([-2.5687629 ,  2.84748356, -1.27839864, -0.01305492]), array([-2.76448727,  2.80580762, -0.71451694, -0.3474956 ]), array([-2.85841216,  2.7068548 , -0.24166613, -0.60565157]), array([-2.86412968,  2.57400587,  0.18407382, -0.7068713 ]), array([-2.77503515,  2.40542873,  0.72478905, -0.98974991]), array([-2.56320932,  2.16697156,  1.43082933, -1.44614017]), array([-2.18435753,  1.79476889,  2.41131666, -2.39836776]), array([-1.5931791 ,  1.19236292,  3.54925006, -3.80022496]), array([-0.7317131 ,  0.16207027,  4.99722458, -6.34106437]), array([ 0.30705394, -1.06679082,  5.12131858, -5.24114464]), array([ 1.25121728, -1.81239506,  4.20621777, -2.2376891 ]), array([ 1.95713622, -2.02116345,  2.8245945 , -0.03702939]), array([ 2.37971038, -1.87861601,  1.44163283,  1.29919227]), array([ 2.5542704 , -1.55407798,  0.35599199,  1.84789665]), array([ 2.52822951, -1.13607514, -0.59782508,  2.32205811]), array([ 2.3136573 , -0.61174343, -1.57359253,  2.9938835 ]), array([ 1.88209935,  0.09711977, -2.77969338,  4.14005947]), array([ 1.19909456,  1.01130195, -4.02083461,  4.76829123]), array([ 0.29363915,  1.88441092, -4.93722161,  3.68144505]), array([-0.70536352,  2.40704148, -4.82125631,  1.44399837]), array([-1.55096855,  2.45356711, -3.49354524, -0.94243845]), array([-2.06241414,  2.04017103, -1.57147522, -3.08924724]), array([-2.1667418 ,  1.23283964,  0.50711122, -4.94173708]), array([-1.90590205,  0.12818115,  1.9957105 , -6.01698213]), array([-1.39439953, -1.16055788,  3.01321969, -6.63320762]), array([-0.70865304, -2.47487432,  3.86625009, -6.52857859]), array([ 0.12277713,  2.45905163,  4.28560737, -7.20053314]), array([ 0.97625054,  0.82513917,  4.29473318, -9.27444098]), array([ 1.74837977, -1.02278245,  3.04401508, -8.42541876]), array([ 2.10850829, -2.42823459,  0.65470068, -5.89190546]), array([ 2.08102189,  2.84304938, -0.71023619, -4.30960737]), array([ 1.87754212,  2.1095677 , -1.28868512, -3.07757336]), array([ 1.56058336,  1.58558288, -1.89519002, -2.25638779]), array([ 1.13608262,  1.12725053, -2.28856164, -2.49840072]), array([ 0.66526863,  0.55231674, -2.37378711, -3.30034494]), array([ 0.17423957, -0.13849638, -2.63738372, -3.29971802]), array([-0.42528968, -0.63424316, -3.3154909 , -1.53582662]), array([-1.09834012, -0.77770675, -3.25916931, -0.08185985]), array([-1.66875199, -0.78043574, -2.3804907 , -0.11515747]), array([-2.04185266, -0.87157296, -1.35567451, -0.87415517])]</t>
-  </si>
-  <si>
-    <t>['[1,1,1]', '[1,2,0]', '[1,0,2]', '[2,2,2]', '[0,1,1]', '[2,0,1]', '[2,1,0]', '[0,2,1]', '[0,0,0]', '[1,1,2]']</t>
-  </si>
-  <si>
-    <t>[2, 3, 6, 8, 10, 14, 16, 19, 20, 21, 22, 23, 25, 26, 28, 29, 31, 32, 35, 37, 39, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50, 52, 53, 54, 55, 56, 58, 59, 61, 63, 64, 65, 68, 69, 71, 72, 73, 74, 80, 83, 84, 85, 86, 87, 88, 89, 92, 96, 97, 101, 103, 105, 108, 111, 115, 117, 120, 121, 122, 124, 125, 127, 128, 130, 131, 132, 133, 135, 137, 139, 140, 141, 142, 148, 149, 150, 152, 153, 155, 156, 158, 161, 163, 165, 166, 168, 171, 173, 176, 177, 178, 181, 182, 183, 184, 185, 187, 188, 192, 194, 195, 199]</t>
-  </si>
-  <si>
-    <t>[0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2]</t>
-  </si>
-  <si>
-    <t>['[-0.03763371 -0.01533471  0.06554052 -0.01816017]', '[-0.00754409 -0.05458322  0.2277812  -0.36241836]', '[ 0.02232897 -0.08388487  0.06427602  0.0784408 ]', '[ 0.03049404 -0.05764214  0.01658555  0.18061999]', '[ 0.01587163  0.02035566 -0.15714965  0.58316433]', '[-0.02823328  0.16538375 -0.26986519  0.83427798]', '[-0.07230486  0.30492875 -0.15839487  0.5321997 ]', '[-0.10081365  0.40301544 -0.11842035  0.42880708]', '[-0.10419792  0.43656567  0.08538057 -0.09776158]', '[-0.05531987  0.33258957  0.39205075 -0.92085464]', '[ 0.01862097  0.15160369  0.32662665 -0.84627108]', '[ 0.09406821 -0.05802062  0.40545998 -1.20116912]', '[ 0.1705295  -0.3060509   0.33474193 -1.22308253]', '[ 0.21912373 -0.52616399  0.13583452 -0.93705282]', '[ 0.19687267 -0.60453746 -0.35193229  0.15622214]', '[ 0.08435317 -0.46866774 -0.74975667  1.17207202]', '[-0.07688308 -0.19011886 -0.82291377  1.54326623]', '[-0.24038921  0.14993439 -0.76679482  1.76893492]', '[-0.36555847  0.4814762  -0.44953089  1.4734079 ]', '[-0.39798226  0.68503427  0.13172676  0.53729966]', '[-0.32694588  0.72449356  0.56450102 -0.13949979]', '[-0.18133067  0.63544434  0.86126548 -0.72172992]', '[ 0.00261258  0.45323225  0.93713892 -1.0452692 ]', '[ 0.17586911  0.24346558  0.75436054 -0.98780856]', '[ 0.3158446   0.01415994  0.61124655 -1.24496096]', '[ 0.38094763 -0.16124322  0.02277412 -0.4722466 ]', '[ 0.32346377 -0.16824158 -0.58622068  0.39507601]', '[ 0.15638966 -0.01455069 -1.0465385   1.09028239]', '[-0.06195098  0.20427806 -1.08537951  1.02307253]', '[-0.25727141  0.36604013 -0.82481028  0.54043998]', '[-0.39049875  0.43810843 -0.48088726  0.1544508 ]', '[-0.42927243  0.38872687  0.09890427 -0.64411253]', '[-0.36645224  0.22245856  0.51227276 -0.98380598]', '[-0.20824347 -0.05452611  1.02970789 -1.71431435]', '[ 0.02364969 -0.42375528  1.22904258 -1.87005199]', '[ 0.23443264 -0.69694078  0.83632634 -0.8039484 ]', '[ 0.36861615 -0.79357333  0.47887718 -0.13767621]', '[ 0.40633969 -0.71598555 -0.11010446  0.9104618 ]', '[ 0.31304414 -0.40394652 -0.80471764  2.16837844]', '[ 0.11418684  0.08340296 -1.12244009  2.58012707]', '[-0.1202079   0.60352121 -1.15307882  2.48471151]', '[-0.31270701  1.00395776 -0.73926667  1.46717922]', '[-0.40753131  1.17996929 -0.19720878  0.28224248]', '[-0.39951792  1.14309549  0.27677475 -0.64905279]', '[-0.29965635  0.92396613  0.70672961 -1.5214828 ]', '[-0.12669665  0.54980508  0.98649163 -2.15634209]', '[ 0.07479272  0.09965097  0.97024794 -2.22953713]', '[ 0.23724778 -0.29312725  0.60719713 -1.60176871]', '[ 0.30451759 -0.51374345  0.05064916 -0.56912679]', '[ 0.25670109 -0.51525385 -0.51832231  0.54755938]', '[ 0.11846923 -0.33792777 -0.83310801  1.18132632]', '[-0.07380569 -0.0338291  -1.04161662  1.77693538]', '[-0.26264479  0.29826744 -0.79801739  1.45584504]', '[-0.37703675  0.52032998 -0.32059959  0.72104422]', '[-0.38531479  0.57671339  0.23907518 -0.16358178]', '[-0.29757563  0.49076103  0.61990042 -0.67435503]', '[-0.14812999  0.32090293  0.84074308 -0.97692327]', '[ 0.04900529  0.05546972  1.08296745 -1.601147  ]', '[ 0.2363712  -0.21326349  0.74501075 -1.01046358]', '[ 0.33287121 -0.32681419  0.19964388 -0.09733923]', '[ 0.31284188 -0.24900144 -0.39413871  0.86096468]', '[ 0.19612859 -0.03125661 -0.74302077  1.26217939]', '[ 0.0179237   0.2623806  -0.99229757  1.59068779]', '[-0.16738452  0.53559592 -0.81810376  1.07283319]', '[-0.29493811  0.67104388 -0.43174118  0.25159178]', '[-0.33289119  0.63003107  0.05986788 -0.66135384]', '[-0.2590696   0.3795166   0.66290217 -1.80720482]', '[-0.08125983 -0.06460177  1.0617329  -2.52428513]', '[ 0.11279054 -0.50791451  0.82701013 -1.80560576]', '[ 0.23483181 -0.7593821   0.37206813 -0.67349114]', '[ 0.27990706 -0.83182356  0.07019974 -0.03930975]', '[ 0.25002957 -0.74329714 -0.36431568  0.91478845]', '[ 0.13922462 -0.47534335 -0.72066361  1.72083731]', '[-0.02401845 -0.08294737 -0.8655182   2.10932982]', '[-0.18537446  0.32397826 -0.6990784   1.85829822]', '[-0.29984872  0.65923222 -0.41505846  1.4290222 ]', '[-0.34336235  0.87736449 -0.01222098  0.72718216]', '[-0.30522541  0.9454602   0.38389631 -0.04569489]', '[-0.17398935  0.80308873  0.90472587 -1.35664768]', '[ 0.04408695  0.4185901   1.23308236 -2.41782877]', '[ 0.26866639 -0.05022332  0.94778151 -2.14109439]', '[ 0.42652332 -0.4599117   0.58447569 -1.86080926]', '[ 0.48873722 -0.76526626  0.02104771 -1.14805912]', '[ 0.41158021 -0.84842896 -0.77313127  0.31355134]', '[ 0.20349145 -0.67743828 -1.26674645  1.35853612]', '[-0.07416263 -0.33078118 -1.44796899  2.01430004]', '[-0.34718817  0.0796944  -1.21340346  1.96728421]', '[-0.53477126  0.41188275 -0.61932918  1.27951627]', '[-0.58404033  0.5726559   0.13632719  0.30639066]', '[-0.49408411  0.56429443  0.74772162 -0.38364547]', '[-0.27093983  0.36167463  1.43938327 -1.5943647 ]', '[ 0.05629783 -0.03791279  1.75355337 -2.27231997]', '[ 0.3682844  -0.41795052  1.29459291 -1.41599324]', '[ 0.57751986 -0.64084462  0.75749285 -0.76554839]', '[ 0.66028557 -0.71351491  0.05691485  0.04839106]', '[ 0.57521105 -0.5579569  -0.89480823  1.49213914]', '[ 0.32773911 -0.16698991 -1.52536875  2.32939984]', '[-0.00420792  0.31949631 -1.70807989  2.38018612]', '[-0.33358678  0.75748004 -1.51152507  1.88243317]', '[-0.58459055  1.04111052 -0.95515529  0.91423467]', '[-0.70304997  1.11617215 -0.2109293  -0.1676223 ]', '[-0.66574036  0.97481094  0.57988922 -1.2378023 ]', '[-0.45399147  0.56591953  1.50853931 -2.8178463 ]', '[-0.11304479 -0.04422915  1.80669072 -3.10547425]', '[ 0.25212192 -0.66082354  1.74699289 -2.87562044]', '[ 0.53218479 -1.08338426  1.0133997  -1.31105221]', '[ 0.66730597 -1.23657649  0.31784951 -0.2126383 ]', '[ 0.63465507 -1.11240351 -0.64565867  1.45646892]', '[ 0.42391224 -0.68441208 -1.4322654   2.78915859]', '[ 7.17084687e-02 -7.42867207e-05 -1.99494368e+00  3.87363885e+00]', '[-0.32185522  0.75964859 -1.82547863  3.49711895]', '[-0.61605609  1.31625279 -1.08051018  2.03497864]', '[-0.75507562  1.59869617 -0.29665945  0.7904265 ]', '[-0.73313042  1.6332747   0.50997584 -0.44376784]', '[-0.53951245  1.37034052  1.40580164 -2.19604763]', '[-0.20288994  0.81063313  1.90992356 -3.34439086]', '[ 0.21837688  0.01931438  2.18933158 -4.34470765]', '[ 0.58893425 -0.74141559  1.41783768 -3.07385865]', '[ 0.78773752 -1.23942992  0.54309337 -1.8736061 ]', '[ 0.80268012 -1.48740001 -0.38778011 -0.60337801]', '[ 0.63133263 -1.4543764  -1.29300366  0.93424202]', '[ 0.30267535 -1.11523128 -1.94311132  2.43610891]', '[-0.1213229  -0.50324525 -2.21749153  3.55854909]', '[-0.55363282  0.25705364 -1.98305465  3.7943507 ]', '[-0.85776405  0.89562054 -0.99967419  2.49523386]', '[-0.94371691  1.24449034  0.14342141  0.98860471]', '[-0.79511823  1.26150963  1.31661446 -0.82914772]', '[-0.45260627  0.96477882  2.0554161  -2.11690366]', '[-1.90573699e-03  4.42211602e-01  2.35808088e+00 -2.97078476e+00]', '[ 0.4702341  -0.20795729  2.24157883 -3.2976438 ]', '[ 0.82504219 -0.72850253  1.2451403  -1.81914757]', '[ 0.9561333  -0.92716747  0.05428607 -0.1689443 ]', '[ 0.8579117  -0.8262749  -1.02574719  1.17956378]', '[ 0.55573414 -0.45835413 -1.94989679  2.45492054]', '[ 0.09585852  0.14371129 -2.53643541  3.36242264]', '[-0.39167352  0.74965322 -2.2270471   2.50670863]', '[-0.77266203  1.13349723 -1.52283853  1.28835237]', '[-0.97350155  1.23577381 -0.4600783  -0.25139762]', '[-0.94038618  1.00908232  0.79624815 -2.01799851]', '[-0.6825581   0.49075107  1.74034589 -3.11082663]', '[-0.27465705 -0.18323194  2.23208023 -3.42357267]', '[ 0.16272476 -0.78512891  2.04433054 -2.42461061]', '[ 0.51205906 -1.11251171  1.38859245 -0.80468015]', '[ 0.71902835 -1.15606472  0.64433215  0.37428452]', '[ 0.73795572 -0.90695553 -0.46908541  2.11348198]', '[ 0.53337815 -0.3172561  -1.53608871  3.7102309 ]', '[ 0.1608603   0.50388044 -2.06032323  4.23596028]', '[-0.24160583  1.2763734  -1.88687233  3.34975863]', '[-0.5651846   1.79732327 -1.31565139  1.85726778]', '[-0.75488918  2.0213461  -0.55475704  0.38752379]', '[-0.78690644  1.97463719  0.24276957 -0.85732013]', '[-0.64200967  1.6290186   1.20343331 -2.62374973]', '[-0.32840115  0.96639327  1.89989588 -3.98323884]', '[ 0.08974334  0.07991669  2.15400073 -4.63018931]', '[ 0.49254534 -0.81607256  1.73865064 -4.06101151]', '[ 0.73393171 -1.43756183  0.66383684 -2.15926282]', '[ 0.7604211  -1.68939369 -0.38383153 -0.37543352]', '[ 0.5896312  -1.58991264 -1.29371443  1.37178295]', '[ 0.26671652 -1.16549047 -1.8930113   2.85627048]', '[-0.15821886 -0.43764311 -2.28300326  4.29818783]', '[-0.59610686  0.45092338 -1.95052614  4.28686895]', '[-0.88062396  1.15886018 -0.84895022  2.72785143]', '[-0.94029672  1.56687208  0.2507441   1.34957589]', '[-0.78705514  1.69681745  1.24902561 -0.05558005]', '[-0.44407588  1.49505901  2.11806413 -1.9594917 ]', '[ 0.01343979  0.97573905  2.38103921 -3.15435557]', '[ 0.4725583   0.29139823  2.10722395 -3.48423484]', '[ 0.83855537 -0.39425248  1.45965512 -3.18490464]', '[ 1.00538882 -0.87001224  0.18721217 -1.53928718]', '[ 0.93459578 -1.06358311 -0.88932253 -0.3717813 ]', '[ 0.63782532 -0.95163338 -2.0337421   1.50198343]', '[ 0.15842346 -0.50269777 -2.67017841  2.88632059]', '[-0.39441417  0.15722773 -2.71807393  3.44880954]', '[-0.86179085  0.74087827 -1.86926497  2.25515724]', '[-1.13428666  1.07413123 -0.82927309  1.0772504 ]', '[-1.18831734  1.17610203  0.29273535 -0.05461704]', '[-1.0187059   1.04811431  1.39006551 -1.24419663]', '[-0.64302151  0.67275782  2.31888093 -2.48748747]', '[-0.12335907  0.09199267  2.76100355 -3.12513146]', '[ 0.42991501 -0.5379035   2.63338912 -2.92274935]', '[ 0.88522316 -1.00691527  1.84853034 -1.69996307]', '[ 1.13013191 -1.16034566  0.57776742  0.13581459]', '[ 1.12215782 -0.98930773 -0.65857892  1.56779113]', '[ 0.87018731 -0.53256652 -1.83502206  2.98171536]', '[ 0.41210401  0.16739051 -2.64051494  3.81454841]', '[-0.13097561  0.87938333 -2.66618232  3.06906101]', '[-0.62440575  1.36337946 -2.18418462  1.69811543]', '[-0.96672689  1.52591632 -1.18507076 -0.0576387 ]', '[-1.09239276  1.37451268 -0.0529553  -1.43613279]', '[-0.96442784  0.89957118  1.33434497 -3.32798847]', '[-0.56900043  0.05109973  2.52936867 -4.99377335]', '[-0.01912276 -0.95717519  2.80974949 -4.74217339]', '[ 0.49430283 -1.71446114  2.27514262 -2.80550498]', '[ 0.88570053 -2.12900048  1.58234738 -1.34723135]', '[ 1.09393675 -2.21557376  0.46726463  0.4699715 ]', '[ 1.07152038 -1.96282934 -0.69990374  2.06888459]', '[ 0.8047428  -1.35120836 -1.97055715  4.11091559]', '[ 0.28795081 -0.29905602 -3.10706474  6.26848772]', '[-0.3430696   0.95571734 -2.96459896  5.768772  ]', '[-0.84020957  1.89768127 -1.98238164  3.68981232]']</t>
-  </si>
-  <si>
-    <t>[array([-0.03763371, -0.01533471,  0.06554052, -0.01816017], dtype=float32), array([-0.00754409, -0.05458322,  0.2277812 , -0.36241836]), array([ 0.02232897, -0.08388487,  0.06427602,  0.0784408 ]), array([ 0.03049404, -0.05764214,  0.01658555,  0.18061999]), array([ 0.01587163,  0.02035566, -0.15714965,  0.58316433]), array([-0.02823328,  0.16538375, -0.26986519,  0.83427798]), array([-0.07230486,  0.30492875, -0.15839487,  0.5321997 ]), array([-0.10081365,  0.40301544, -0.11842035,  0.42880708]), array([-0.10419792,  0.43656567,  0.08538057, -0.09776158]), array([-0.05531987,  0.33258957,  0.39205075, -0.92085464]), array([ 0.01862097,  0.15160369,  0.32662665, -0.84627108]), array([ 0.09406821, -0.05802062,  0.40545998, -1.20116912]), array([ 0.1705295 , -0.3060509 ,  0.33474193, -1.22308253]), array([ 0.21912373, -0.52616399,  0.13583452, -0.93705282]), array([ 0.19687267, -0.60453746, -0.35193229,  0.15622214]), array([ 0.08435317, -0.46866774, -0.74975667,  1.17207202]), array([-0.07688308, -0.19011886, -0.82291377,  1.54326623]), array([-0.24038921,  0.14993439, -0.76679482,  1.76893492]), array([-0.36555847,  0.4814762 , -0.44953089,  1.4734079 ]), array([-0.39798226,  0.68503427,  0.13172676,  0.53729966]), array([-0.32694588,  0.72449356,  0.56450102, -0.13949979]), array([-0.18133067,  0.63544434,  0.86126548, -0.72172992]), array([ 0.00261258,  0.45323225,  0.93713892, -1.0452692 ]), array([ 0.17586911,  0.24346558,  0.75436054, -0.98780856]), array([ 0.3158446 ,  0.01415994,  0.61124655, -1.24496096]), array([ 0.38094763, -0.16124322,  0.02277412, -0.4722466 ]), array([ 0.32346377, -0.16824158, -0.58622068,  0.39507601]), array([ 0.15638966, -0.01455069, -1.0465385 ,  1.09028239]), array([-0.06195098,  0.20427806, -1.08537951,  1.02307253]), array([-0.25727141,  0.36604013, -0.82481028,  0.54043998]), array([-0.39049875,  0.43810843, -0.48088726,  0.1544508 ]), array([-0.42927243,  0.38872687,  0.09890427, -0.64411253]), array([-0.36645224,  0.22245856,  0.51227276, -0.98380598]), array([-0.20824347, -0.05452611,  1.02970789, -1.71431435]), array([ 0.02364969, -0.42375528,  1.22904258, -1.87005199]), array([ 0.23443264, -0.69694078,  0.83632634, -0.8039484 ]), array([ 0.36861615, -0.79357333,  0.47887718, -0.13767621]), array([ 0.40633969, -0.71598555, -0.11010446,  0.9104618 ]), array([ 0.31304414, -0.40394652, -0.80471764,  2.16837844]), array([ 0.11418684,  0.08340296, -1.12244009,  2.58012707]), array([-0.1202079 ,  0.60352121, -1.15307882,  2.48471151]), array([-0.31270701,  1.00395776, -0.73926667,  1.46717922]), array([-0.40753131,  1.17996929, -0.19720878,  0.28224248]), array([-0.39951792,  1.14309549,  0.27677475, -0.64905279]), array([-0.29965635,  0.92396613,  0.70672961, -1.5214828 ]), array([-0.12669665,  0.54980508,  0.98649163, -2.15634209]), array([ 0.07479272,  0.09965097,  0.97024794, -2.22953713]), array([ 0.23724778, -0.29312725,  0.60719713, -1.60176871]), array([ 0.30451759, -0.51374345,  0.05064916, -0.56912679]), array([ 0.25670109, -0.51525385, -0.51832231,  0.54755938]), array([ 0.11846923, -0.33792777, -0.83310801,  1.18132632]), array([-0.07380569, -0.0338291 , -1.04161662,  1.77693538]), array([-0.26264479,  0.29826744, -0.79801739,  1.45584504]), array([-0.37703675,  0.52032998, -0.32059959,  0.72104422]), array([-0.38531479,  0.57671339,  0.23907518, -0.16358178]), array([-0.29757563,  0.49076103,  0.61990042, -0.67435503]), array([-0.14812999,  0.32090293,  0.84074308, -0.97692327]), array([ 0.04900529,  0.05546972,  1.08296745, -1.601147  ]), array([ 0.2363712 , -0.21326349,  0.74501075, -1.01046358]), array([ 0.33287121, -0.32681419,  0.19964388, -0.09733923]), array([ 0.31284188, -0.24900144, -0.39413871,  0.86096468]), array([ 0.19612859, -0.03125661, -0.74302077,  1.26217939]), array([ 0.0179237 ,  0.2623806 , -0.99229757,  1.59068779]), array([-0.16738452,  0.53559592, -0.81810376,  1.07283319]), array([-0.29493811,  0.67104388, -0.43174118,  0.25159178]), array([-0.33289119,  0.63003107,  0.05986788, -0.66135384]), array([-0.2590696 ,  0.3795166 ,  0.66290217, -1.80720482]), array([-0.08125983, -0.06460177,  1.0617329 , -2.52428513]), array([ 0.11279054, -0.50791451,  0.82701013, -1.80560576]), array([ 0.23483181, -0.7593821 ,  0.37206813, -0.67349114]), array([ 0.27990706, -0.83182356,  0.07019974, -0.03930975]), array([ 0.25002957, -0.74329714, -0.36431568,  0.91478845]), array([ 0.13922462, -0.47534335, -0.72066361,  1.72083731]), array([-0.02401845, -0.08294737, -0.8655182 ,  2.10932982]), array([-0.18537446,  0.32397826, -0.6990784 ,  1.85829822]), array([-0.29984872,  0.65923222, -0.41505846,  1.4290222 ]), array([-0.34336235,  0.87736449, -0.01222098,  0.72718216]), array([-0.30522541,  0.9454602 ,  0.38389631, -0.04569489]), array([-0.17398935,  0.80308873,  0.90472587, -1.35664768]), array([ 0.04408695,  0.4185901 ,  1.23308236, -2.41782877]), array([ 0.26866639, -0.05022332,  0.94778151, -2.14109439]), array([ 0.42652332, -0.4599117 ,  0.58447569, -1.86080926]), array([ 0.48873722, -0.76526626,  0.02104771, -1.14805912]), array([ 0.41158021, -0.84842896, -0.77313127,  0.31355134]), array([ 0.20349145, -0.67743828, -1.26674645,  1.35853612]), array([-0.07416263, -0.33078118, -1.44796899,  2.01430004]), array([-0.34718817,  0.0796944 , -1.21340346,  1.96728421]), array([-0.53477126,  0.41188275, -0.61932918,  1.27951627]), array([-0.58404033,  0.5726559 ,  0.13632719,  0.30639066]), array([-0.49408411,  0.56429443,  0.74772162, -0.38364547]), array([-0.27093983,  0.36167463,  1.43938327, -1.5943647 ]), array([ 0.05629783, -0.03791279,  1.75355337, -2.27231997]), array([ 0.3682844 , -0.41795052,  1.29459291, -1.41599324]), array([ 0.57751986, -0.64084462,  0.75749285, -0.76554839]), array([ 0.66028557, -0.71351491,  0.05691485,  0.04839106]), array([ 0.57521105, -0.5579569 , -0.89480823,  1.49213914]), array([ 0.32773911, -0.16698991, -1.52536875,  2.32939984]), array([-0.00420792,  0.31949631, -1.70807989,  2.38018612]), array([-0.33358678,  0.75748004, -1.51152507,  1.88243317]), array([-0.58459055,  1.04111052, -0.95515529,  0.91423467]), array([-0.70304997,  1.11617215, -0.2109293 , -0.1676223 ]), array([-0.66574036,  0.97481094,  0.57988922, -1.2378023 ]), array([-0.45399147,  0.56591953,  1.50853931, -2.8178463 ]), array([-0.11304479, -0.04422915,  1.80669072, -3.10547425]), array([ 0.25212192, -0.66082354,  1.74699289, -2.87562044]), array([ 0.53218479, -1.08338426,  1.0133997 , -1.31105221]), array([ 0.66730597, -1.23657649,  0.31784951, -0.2126383 ]), array([ 0.63465507, -1.11240351, -0.64565867,  1.45646892]), array([ 0.42391224, -0.68441208, -1.4322654 ,  2.78915859]), array([ 7.17084687e-02, -7.42867207e-05, -1.99494368e+00,  3.87363885e+00]), array([-0.32185522,  0.75964859, -1.82547863,  3.49711895]), array([-0.61605609,  1.31625279, -1.08051018,  2.03497864]), array([-0.75507562,  1.59869617, -0.29665945,  0.7904265 ]), array([-0.73313042,  1.6332747 ,  0.50997584, -0.44376784]), array([-0.53951245,  1.37034052,  1.40580164, -2.19604763]), array([-0.20288994,  0.81063313,  1.90992356, -3.34439086]), array([ 0.21837688,  0.01931438,  2.18933158, -4.34470765]), array([ 0.58893425, -0.74141559,  1.41783768, -3.07385865]), array([ 0.78773752, -1.23942992,  0.54309337, -1.8736061 ]), array([ 0.80268012, -1.48740001, -0.38778011, -0.60337801]), array([ 0.63133263, -1.4543764 , -1.29300366,  0.93424202]), array([ 0.30267535, -1.11523128, -1.94311132,  2.43610891]), array([-0.1213229 , -0.50324525, -2.21749153,  3.55854909]), array([-0.55363282,  0.25705364, -1.98305465,  3.7943507 ]), array([-0.85776405,  0.89562054, -0.99967419,  2.49523386]), array([-0.94371691,  1.24449034,  0.14342141,  0.98860471]), array([-0.79511823,  1.26150963,  1.31661446, -0.82914772]), array([-0.45260627,  0.96477882,  2.0554161 , -2.11690366]), array([-1.90573699e-03,  4.42211602e-01,  2.35808088e+00, -2.97078476e+00]), array([ 0.4702341 , -0.20795729,  2.24157883, -3.2976438 ]), array([ 0.82504219, -0.72850253,  1.2451403 , -1.81914757]), array([ 0.9561333 , -0.92716747,  0.05428607, -0.1689443 ]), array([ 0.8579117 , -0.8262749 , -1.02574719,  1.17956378]), array([ 0.55573414, -0.45835413, -1.94989679,  2.45492054]), array([ 0.09585852,  0.14371129, -2.53643541,  3.36242264]), array([-0.39167352,  0.74965322, -2.2270471 ,  2.50670863]), array([-0.77266203,  1.13349723, -1.52283853,  1.28835237]), array([-0.97350155,  1.23577381, -0.4600783 , -0.25139762]), array([-0.94038618,  1.00908232,  0.79624815, -2.01799851]), array([-0.6825581 ,  0.49075107,  1.74034589, -3.11082663]), array([-0.27465705, -0.18323194,  2.23208023, -3.42357267]), array([ 0.16272476, -0.78512891,  2.04433054, -2.42461061]), array([ 0.51205906, -1.11251171,  1.38859245, -0.80468015]), array([ 0.71902835, -1.15606472,  0.64433215,  0.37428452]), array([ 0.73795572, -0.90695553, -0.46908541,  2.11348198]), array([ 0.53337815, -0.3172561 , -1.53608871,  3.7102309 ]), array([ 0.1608603 ,  0.50388044, -2.06032323,  4.23596028]), array([-0.24160583,  1.2763734 , -1.88687233,  3.34975863]), array([-0.5651846 ,  1.79732327, -1.31565139,  1.85726778]), array([-0.75488918,  2.0213461 , -0.55475704,  0.38752379]), array([-0.78690644,  1.97463719,  0.24276957, -0.85732013]), array([-0.64200967,  1.6290186 ,  1.20343331, -2.62374973]), array([-0.32840115,  0.96639327,  1.89989588, -3.98323884]), array([ 0.08974334,  0.07991669,  2.15400073, -4.63018931]), array([ 0.49254534, -0.81607256,  1.73865064, -4.06101151]), array([ 0.73393171, -1.43756183,  0.66383684, -2.15926282]), array([ 0.7604211 , -1.68939369, -0.38383153, -0.37543352]), array([ 0.5896312 , -1.58991264, -1.29371443,  1.37178295]), array([ 0.26671652, -1.16549047, -1.8930113 ,  2.85627048]), array([-0.15821886, -0.43764311, -2.28300326,  4.29818783]), array([-0.59610686,  0.45092338, -1.95052614,  4.28686895]), array([-0.88062396,  1.15886018, -0.84895022,  2.72785143]), array([-0.94029672,  1.56687208,  0.2507441 ,  1.34957589]), array([-0.78705514,  1.69681745,  1.24902561, -0.05558005]), array([-0.44407588,  1.49505901,  2.11806413, -1.9594917 ]), array([ 0.01343979,  0.97573905,  2.38103921, -3.15435557]), array([ 0.4725583 ,  0.29139823,  2.10722395, -3.48423484]), array([ 0.83855537, -0.39425248,  1.45965512, -3.18490464]), array([ 1.00538882, -0.87001224,  0.18721217, -1.53928718]), array([ 0.93459578, -1.06358311, -0.88932253, -0.3717813 ]), array([ 0.63782532, -0.95163338, -2.0337421 ,  1.50198343]), array([ 0.15842346, -0.50269777, -2.67017841,  2.88632059]), array([-0.39441417,  0.15722773, -2.71807393,  3.44880954]), array([-0.86179085,  0.74087827, -1.86926497,  2.25515724]), array([-1.13428666,  1.07413123, -0.82927309,  1.0772504 ]), array([-1.18831734,  1.17610203,  0.29273535, -0.05461704]), array([-1.0187059 ,  1.04811431,  1.39006551, -1.24419663]), array([-0.64302151,  0.67275782,  2.31888093, -2.48748747]), array([-0.12335907,  0.09199267,  2.76100355, -3.12513146]), array([ 0.42991501, -0.5379035 ,  2.63338912, -2.92274935]), array([ 0.88522316, -1.00691527,  1.84853034, -1.69996307]), array([ 1.13013191, -1.16034566,  0.57776742,  0.13581459]), array([ 1.12215782, -0.98930773, -0.65857892,  1.56779113]), array([ 0.87018731, -0.53256652, -1.83502206,  2.98171536]), array([ 0.41210401,  0.16739051, -2.64051494,  3.81454841]), array([-0.13097561,  0.87938333, -2.66618232,  3.06906101]), array([-0.62440575,  1.36337946, -2.18418462,  1.69811543]), array([-0.96672689,  1.52591632, -1.18507076, -0.0576387 ]), array([-1.09239276,  1.37451268, -0.0529553 , -1.43613279]), array([-0.96442784,  0.89957118,  1.33434497, -3.32798847]), array([-0.56900043,  0.05109973,  2.52936867, -4.99377335]), array([-0.01912276, -0.95717519,  2.80974949, -4.74217339]), array([ 0.49430283, -1.71446114,  2.27514262, -2.80550498]), array([ 0.88570053, -2.12900048,  1.58234738, -1.34723135]), array([ 1.09393675, -2.21557376,  0.46726463,  0.4699715 ]), array([ 1.07152038, -1.96282934, -0.69990374,  2.06888459]), array([ 0.8047428 , -1.35120836, -1.97055715,  4.11091559]), array([ 0.28795081, -0.29905602, -3.10706474,  6.26848772]), array([-0.3430696 ,  0.95571734, -2.96459896,  5.768772  ]), array([-0.84020957,  1.89768127, -1.98238164,  3.68981232])]</t>
-  </si>
-  <si>
-    <t>['[1,1,2]', '[0,2,1]', '[1,0,2]', '[0,1,1]', '[0,0,0]', '[1,1,1]', '[1,2,0]', '[2,1,0]', '[2,2,2]', '[2,0,1]']</t>
-  </si>
-  <si>
-    <t>[1, 2, 3, 4, 5, 6, 8, 9, 10, 11, 12, 13, 14, 15, 17, 18, 19, 20, 21, 23, 25, 26, 27, 28, 30, 31, 33, 34, 35, 36, 38, 39, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50, 51, 52, 53, 54, 56, 57, 58, 59, 60, 62, 64, 65, 66, 67, 70, 71, 72, 73, 74, 75, 76, 80, 81, 82, 83, 84, 85, 86, 87, 89, 90, 91, 92, 93, 94, 95, 96, 97, 99, 101, 102, 103, 104, 108, 109, 110, 111, 112, 113, 114, 116, 117, 118, 119, 120, 121, 122, 124, 126, 128, 129, 130, 131, 132, 133, 134, 135, 136, 138, 140, 141, 142, 144, 146, 147, 148, 150, 151, 152, 154, 155, 156, 157, 158, 159, 160, 161, 162, 163, 164, 165, 167, 168, 169, 170, 171, 172, 173, 175, 176, 177, 178, 179, 180, 181, 182, 183, 184, 185, 186, 187, 188, 189, 190, 192, 193, 195, 196, 197, 198, 199]</t>
-  </si>
-  <si>
-    <t>[0, 2, 2, 0, 2, 0, 2, 2, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 0, 2, 0, 0, 0, 2, 2, 2, 2, 0, 0, 2, 0, 0, 0, 2, 0, 0, 0, 0, 2, 2, 0, 0, 0, 0, 2, 2, 0, 0, 0, 0, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 0, 0, 2, 2, 0, 2, 0, 2, 2, 0, 0, 0, 0, 2, 2, 2, 2, 0, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 2, 0, 0, 0, 0, 0, 0, 2, 2, 0, 2, 2, 2, 0, 2, 0, 0, 2, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2]</t>
-  </si>
-  <si>
-    <t>['[-0.03763371 -0.01533471  0.06554052 -0.01816017]', '[-0.03406929  0.01398622 -0.02953871  0.30651903]', '[-0.03493773  0.06836613  0.02265481  0.22789337]', '[-0.02479211  0.10222584  0.07768516  0.10663031]', '[-0.01808581  0.14469195 -0.0104571   0.31140101]', '[-0.01484609  0.18823383  0.0432976   0.11751461]', '[-0.01434726  0.22467153 -0.03717771  0.24054013]', '[-0.02851561  0.28068156 -0.09989287  0.30782044]', '[-0.03896755  0.30874187 -0.00204846 -0.03278158]', '[-0.04233883  0.30160426 -0.03114225 -0.03799865]', '[-0.0509959   0.29364669 -0.05386126 -0.0416588 ]', '[-0.06308757  0.28480708 -0.06483528 -0.04716872]', '[-0.07596814  0.27458919 -0.06165726 -0.0552825 ]', '[-0.086864    0.26266518 -0.04546628 -0.0635942 ]', '[-0.09355857  0.2494481  -0.0205491  -0.06732942]', '[-0.09490905  0.23639773  0.00689617 -0.06114101]', '[-0.0647895   0.15791404  0.285996   -0.70621969]', '[-0.01324114  0.03527764  0.21511273 -0.49083901]', '[ 0.01637134 -0.02865263  0.0732296  -0.13326706]', '[ 0.01446559 -0.01516662 -0.09124043  0.26504701]', '[-0.00472323  0.03829442 -0.09509622  0.25739218]', '[-0.02134476  0.0829767  -0.06642856  0.17930185]', '[-0.04296423  0.14086844 -0.14339363  0.38594252]', '[-0.06218228  0.19606511 -0.04349325  0.15421584]', '[-0.07239894  0.23389609 -0.05541309  0.21601753]', '[-0.06983487  0.24494851  0.08059878 -0.10649001]', '[-0.05479603  0.22758339  0.0662479  -0.06196489]', '[-0.04458822  0.22186661  0.03363667  0.00725646]', '[-0.0418868   0.23082969 -0.00684209  0.0811742 ]', '[-0.02079816  0.18524331  0.21209879 -0.52617083]', '[ 0.0119547   0.09816843  0.1061162  -0.32456452]', '[ 0.01900048  0.06143732 -0.03806165 -0.03563375]', '[-0.00277198  0.08399953 -0.17433323  0.25358501]', '[-0.03399703  0.12292423 -0.13048961  0.12438247]', '[-0.05249198  0.13036404 -0.05060102 -0.05385264]', '[-0.06672903  0.1356315  -0.0886585   0.10328641]', '[-0.07303946  0.13499233  0.02665842 -0.11024497]', '[-0.04350447  0.05909962  0.2602242  -0.63090205]', '[-0.00129791 -0.03683477  0.15042149 -0.30561674]', '[ 0.01337548 -0.05691045 -0.00701834  0.11004953]', '[-0.00376388  0.00565936 -0.15874316  0.50181549]', '[-0.03297544  0.10052874 -0.12453022  0.42609766]', '[-0.05043823  0.1685804  -0.0446867   0.24050699]', '[-0.04953515  0.19288103  0.05404029 -0.00107598]', '[-0.04285048  0.20284991  0.01183051  0.09996399]', '[-0.04475275  0.23164608 -0.02952383  0.18269224]', '[-0.04065612  0.23917871  0.06967365 -0.10762143]', '[-0.03135887  0.22479673  0.0210423  -0.0324273 ]', '[-0.03267944  0.22694443 -0.03384324  0.05321059]', '[-0.0442159   0.24493427 -0.07858256  0.12175509]', '[-0.04945     0.23913188  0.02702106 -0.17936154]', '[-0.04733103  0.20979524 -0.00710982 -0.10878014]', '[-0.05246276  0.1970567  -0.04351136 -0.01731939]', '[-0.06407323  0.20257736 -0.07003221  0.06971199]', '[-0.07915226  0.2231047  -0.07706186  0.12971337]', '[-0.09330638  0.2517116  -0.06077049  0.14938013]', '[-0.08903537  0.24622018  0.10225453 -0.20237658]', '[-0.06760334  0.20856902  0.1065958  -0.16450132]', '[-0.04857264  0.18405321  0.07914986 -0.07363116]', '[-0.03744641  0.18116708  0.02984874  0.04683661]', '[-0.03701656  0.20253648 -0.02488785  0.16310806]', '[-0.04658591  0.24384651 -0.0675437   0.2413826 ]', '[-0.0492897   0.26112643  0.04129377 -0.07138397]', '[-0.01774722  0.18270689  0.26570245 -0.69540456]', '[ 0.0246982   0.06376661  0.14637914 -0.46679975]', '[ 0.0370958   0.00457126 -0.02655766 -0.11340296]', '[ 0.01417737  0.01974394 -0.19725673  0.25850463]', '[-0.02466589  0.06763126 -0.18185244  0.20619754]', '[-0.06826729  0.13124565 -0.24319221  0.41192022]', '[-0.11686231  0.22352346 -0.23002254  0.48748834]', '[-0.14223298  0.28286292 -0.01740043  0.09332091]', '[-0.13633628  0.29315213  0.07538375  0.00887688]', '[-0.11326986  0.28716866  0.15039778 -0.06420519]', '[-0.07878073  0.27015211  0.18700339 -0.09787883]', '[-0.04178077  0.25168375  0.17496884 -0.07803226]', '[-0.01188475  0.24225884  0.1176994  -0.01004373]', '[0.00330652 0.2493619  0.03142615 0.08214328]', '[ 0.02650368  0.20666194  0.19464453 -0.49854398]', '[ 0.07702577  0.05866511  0.29602776 -0.94875887]', '[ 0.13752045 -0.15571924  0.28893747 -1.14714383]', '[ 0.15846868 -0.31240921 -0.08670021 -0.3934743 ]', '[ 0.11661835 -0.34302293 -0.32352664  0.08528614]', '[ 0.03457694 -0.28320131 -0.47849977  0.49082838]', '[-0.06584948 -0.1590719  -0.50186179  0.71401957]', '[-0.15614414 -0.01395469 -0.37849104  0.69814177]', '[-0.20922173  0.10554642 -0.13825188  0.46889192]', '[-0.2079852   0.16541178  0.15180937  0.1204502 ]', '[-0.16375058  0.18784603  0.28246959  0.10637824]', '[-0.07298528  0.14163733  0.60511303 -0.54672547]', '[ 0.04061858  0.05254424  0.50516959 -0.3110066 ]', '[0.11987642 0.02825665 0.27092593 0.08412216]', '[ 0.14470639  0.08855671 -0.02526075  0.51160213]', '[ 0.12467656  0.19135787 -0.16790637  0.49602854]', '[ 0.08139213  0.27823357 -0.25391229  0.35194281]', '[ 0.02802774  0.32427365 -0.26768969  0.09276407]', '[-0.02094076  0.3105159  -0.21207934 -0.23609345]', '[-0.06666366  0.26368234 -0.23719535 -0.23160569]', '[-0.11249466  0.21808082 -0.21336995 -0.22342264]', '[-0.12271861  0.10667073  0.10980151 -0.87322441]', '[-0.09908391 -0.04928324  0.11642719 -0.65526077]', '[-0.05340307 -0.21305737  0.32527302 -0.94591852]', '[-0.00272259 -0.34293981  0.16913446 -0.32673608]', '[ 0.01100452 -0.33788751 -0.03448625  0.37828896]', '[-0.00254974 -0.22991699 -0.09574309  0.68241567]', '[-0.02421057 -0.07511682 -0.11160639  0.83573332]', '[-0.05625554  0.12526138 -0.19485103  1.12665549]', '[-0.09539794  0.35638121 -0.18027324  1.13757207]', '[-0.12246028  0.5626655  -0.08023561  0.89059928]', '[-0.11309781  0.67035746  0.17064963  0.17822585]', '[-0.0694711   0.66665278  0.25600609 -0.20720897]', '[-0.01522311  0.5928799   0.2744779  -0.5125716 ]', '[ 0.03524094  0.47055878  0.21803782 -0.68587692]', '[ 0.06728597  0.32945868  0.09270675 -0.69851642]', '[ 0.06919525  0.20153176 -0.0777094  -0.55938067]', '[ 0.03594476  0.11256169 -0.25085628 -0.32036736]', '[-0.00144033  0.00635737 -0.11909332 -0.72847628]', '[-0.03825849 -0.10136706 -0.24495325 -0.3360311 ]', '[-0.09619607 -0.12649604 -0.3230332   0.07935377]', '[-0.14869518 -0.1090812  -0.19089203  0.08362824]', '[-0.16917425 -0.09672263 -0.00957868  0.03488227]', '[-0.16550857 -0.0615122   0.04646334  0.31192514]', '[-0.13733787 -0.009859    0.23099737  0.20041323]', '[-0.08958998  0.05297297  0.23905959  0.42392598]', '[-0.04439906  0.15653949  0.20763255  0.59970567]', '[0.00487394 0.2528211  0.27766625 0.35497049]', '[ 0.07572569  0.26373427  0.41579168 -0.23522308]', '[ 0.13755626  0.23508949  0.18926479 -0.03638374]', '[ 0.17436177  0.1844659   0.17012    -0.45596872]', '[ 0.17547986  0.1290212  -0.16047569 -0.08959966]', '[ 0.12574652  0.11363668 -0.32703044 -0.06991553]', '[ 0.04989691  0.09774065 -0.41643176 -0.09839977]', '[-0.03417976  0.07030487 -0.40816991 -0.18406488]', '[-0.1071204   0.02159096 -0.30826799 -0.30533043]', '[-0.16650314 -0.01706873 -0.27487449 -0.08368419]', '[-0.199534   -0.04844856 -0.05003091 -0.22950565]', '[-0.19947724 -0.07216906  0.049885   -0.00383119]', '[-0.18040025 -0.049278    0.13766159  0.23189825]', '[-0.11956389 -0.04937424  0.45807358 -0.22267212]', '[-0.03173645 -0.06092488  0.402119    0.12249159]', '[ 0.06141699 -0.06542948  0.51025924 -0.15206146]', '[ 0.13707595 -0.04470725  0.23207481  0.36641544]', '[0.16461181 0.04467592 0.04093621 0.51571467]', '[ 0.15410655  0.15495121 -0.14034994  0.56657528]', '[ 0.09899065  0.29581722 -0.39502314  0.80872957]', '[ 0.01731575  0.42899612 -0.40250065  0.49046027]', '[-0.06722116  0.51388079 -0.42369368  0.33215964]', '[-0.13197184  0.51994066 -0.21010416 -0.28202196]', '[-0.16039676  0.43401507 -0.070165   -0.56867257]', '[-0.15995177  0.2986409   0.07053161 -0.76281791]', '[-0.10891473  0.07203135  0.42258703 -1.45761729]', '[-0.02854714 -0.18961569  0.35576145 -1.10014715]', '[ 0.02498277 -0.34879779  0.16588918 -0.46056127]', '[ 0.03451183 -0.36662001 -0.07243426  0.2854895 ]', '[-0.0026097  -0.2384056  -0.28888949  0.97230677]', '[-0.06118496 -0.0277741  -0.27801793  1.08817817]', '[-0.10604836  0.17750187 -0.15455031  0.92161308]', '[-0.1180178   0.32608697  0.04099105  0.53891393]', '[-0.08933699  0.38682681  0.24064323  0.06452452]', '[-0.03853853  0.38749316  0.25685012 -0.0498245 ]', '[ 0.00897916  0.3709375   0.20811822 -0.10534156]', '[ 0.04097309  0.34956095  0.10476798 -0.099817  ]', '[ 0.04889758  0.33376387 -0.02741323 -0.05452991]', '[ 0.0303391   0.32808734 -0.15433262 -0.00467729]', '[ 0.00273397  0.29622732 -0.11660545 -0.31357239]', '[-0.02796251  0.23880315 -0.18573244 -0.25605377]', '[-0.06915271  0.19498083 -0.21919682 -0.18103604]', '[-0.08610889  0.09797943  0.05008515 -0.77488234]', '[-0.07839875 -0.03511419  0.02095937 -0.53153427]', '[-0.07948029 -0.10686559 -0.03349913 -0.17442005]', '[-0.09164889 -0.10293415 -0.08545495  0.21085044]', '[-0.09853547 -0.06066304  0.01914164  0.20376442]', '[-0.08378234 -0.02402595  0.1264183   0.15878161]', '[-0.06288825  0.03649053  0.08036725  0.43880156]', '[-0.03854302  0.1120446   0.16046538  0.30754128]', '[-0.01371406  0.19131712  0.08560965  0.47484801]', '[0.00859576 0.26254    0.13459988 0.22970097]', '[0.02531509 0.31577344 0.03075934 0.29649658]', '[ 0.03389006  0.3442326   0.05357457 -0.01433635]', '[ 0.03287596  0.34447952 -0.06338166  0.01643526]', '[ 0.00962312  0.3497398  -0.16409606  0.03129934]', '[-0.0169932   0.32084901 -0.09707772 -0.32013812]', '[-0.04112797  0.25801848 -0.1411209  -0.30164106]', '[-0.07187072  0.20253814 -0.16182028 -0.24841854]', '[-0.10386897  0.16014316 -0.15312683 -0.17298015]', '[-0.13109579  0.13393454 -0.11458855 -0.08856703]', '[-0.1480807   0.12458555 -0.05222751 -0.00577198]', '[-0.1511499   0.13107505  0.02230536  0.06912406]', '[-0.13932414  0.15151959  0.09422307  0.13352703]', '[-0.1146171   0.18372203  0.14894533  0.18654086]', '[-0.08166136  0.22530409  0.17533751  0.22699366]', '[-0.04676095  0.27352178  0.16811188  0.25230154]', '[ 0.00936488  0.25747378  0.38074923 -0.40090261]', '[ 0.07221252  0.19100447  0.23308173 -0.2426063 ]', '[0.09808333 0.1669647  0.01988637 0.01007555]', '[ 0.10619646  0.12700505  0.05850486 -0.40175592]', '[ 0.09315315  0.08077446 -0.18747574 -0.05515234]', '[ 0.04734719  0.06914831 -0.26156368 -0.06635903]', '[-0.00731783  0.05181816 -0.27452715 -0.11237829]', '[-0.05821409  0.02229677 -0.22513251 -0.185384  ]', '[-0.09413437 -0.02257101 -0.12835421 -0.26084   ]']</t>
-  </si>
-  <si>
-    <t>[array([-0.03763371, -0.01533471,  0.06554052, -0.01816017], dtype=float32), array([-0.03406929,  0.01398622, -0.02953871,  0.30651903]), array([-0.03493773,  0.06836613,  0.02265481,  0.22789337]), array([-0.02479211,  0.10222584,  0.07768516,  0.10663031]), array([-0.01808581,  0.14469195, -0.0104571 ,  0.31140101]), array([-0.01484609,  0.18823383,  0.0432976 ,  0.11751461]), array([-0.01434726,  0.22467153, -0.03717771,  0.24054013]), array([-0.02851561,  0.28068156, -0.09989287,  0.30782044]), array([-0.03896755,  0.30874187, -0.00204846, -0.03278158]), array([-0.04233883,  0.30160426, -0.03114225, -0.03799865]), array([-0.0509959 ,  0.29364669, -0.05386126, -0.0416588 ]), array([-0.06308757,  0.28480708, -0.06483528, -0.04716872]), array([-0.07596814,  0.27458919, -0.06165726, -0.0552825 ]), array([-0.086864  ,  0.26266518, -0.04546628, -0.0635942 ]), array([-0.09355857,  0.2494481 , -0.0205491 , -0.06732942]), array([-0.09490905,  0.23639773,  0.00689617, -0.06114101]), array([-0.0647895 ,  0.15791404,  0.285996  , -0.70621969]), array([-0.01324114,  0.03527764,  0.21511273, -0.49083901]), array([ 0.01637134, -0.02865263,  0.0732296 , -0.13326706]), array([ 0.01446559, -0.01516662, -0.09124043,  0.26504701]), array([-0.00472323,  0.03829442, -0.09509622,  0.25739218]), array([-0.02134476,  0.0829767 , -0.06642856,  0.17930185]), array([-0.04296423,  0.14086844, -0.14339363,  0.38594252]), array([-0.06218228,  0.19606511, -0.04349325,  0.15421584]), array([-0.07239894,  0.23389609, -0.05541309,  0.21601753]), array([-0.06983487,  0.24494851,  0.08059878, -0.10649001]), array([-0.05479603,  0.22758339,  0.0662479 , -0.06196489]), array([-0.04458822,  0.22186661,  0.03363667,  0.00725646]), array([-0.0418868 ,  0.23082969, -0.00684209,  0.0811742 ]), array([-0.02079816,  0.18524331,  0.21209879, -0.52617083]), array([ 0.0119547 ,  0.09816843,  0.1061162 , -0.32456452]), array([ 0.01900048,  0.06143732, -0.03806165, -0.03563375]), array([-0.00277198,  0.08399953, -0.17433323,  0.25358501]), array([-0.03399703,  0.12292423, -0.13048961,  0.12438247]), array([-0.05249198,  0.13036404, -0.05060102, -0.05385264]), array([-0.06672903,  0.1356315 , -0.0886585 ,  0.10328641]), array([-0.07303946,  0.13499233,  0.02665842, -0.11024497]), array([-0.04350447,  0.05909962,  0.2602242 , -0.63090205]), array([-0.00129791, -0.03683477,  0.15042149, -0.30561674]), array([ 0.01337548, -0.05691045, -0.00701834,  0.11004953]), array([-0.00376388,  0.00565936, -0.15874316,  0.50181549]), array([-0.03297544,  0.10052874, -0.12453022,  0.42609766]), array([-0.05043823,  0.1685804 , -0.0446867 ,  0.24050699]), array([-0.04953515,  0.19288103,  0.05404029, -0.00107598]), array([-0.04285048,  0.20284991,  0.01183051,  0.09996399]), array([-0.04475275,  0.23164608, -0.02952383,  0.18269224]), array([-0.04065612,  0.23917871,  0.06967365, -0.10762143]), array([-0.03135887,  0.22479673,  0.0210423 , -0.0324273 ]), array([-0.03267944,  0.22694443, -0.03384324,  0.05321059]), array([-0.0442159 ,  0.24493427, -0.07858256,  0.12175509]), array([-0.04945   ,  0.23913188,  0.02702106, -0.17936154]), array([-0.04733103,  0.20979524, -0.00710982, -0.10878014]), array([-0.05246276,  0.1970567 , -0.04351136, -0.01731939]), array([-0.06407323,  0.20257736, -0.07003221,  0.06971199]), array([-0.07915226,  0.2231047 , -0.07706186,  0.12971337]), array([-0.09330638,  0.2517116 , -0.06077049,  0.14938013]), array([-0.08903537,  0.24622018,  0.10225453, -0.20237658]), array([-0.06760334,  0.20856902,  0.1065958 , -0.16450132]), array([-0.04857264,  0.18405321,  0.07914986, -0.07363116]), array([-0.03744641,  0.18116708,  0.02984874,  0.04683661]), array([-0.03701656,  0.20253648, -0.02488785,  0.16310806]), array([-0.04658591,  0.24384651, -0.0675437 ,  0.2413826 ]), array([-0.0492897 ,  0.26112643,  0.04129377, -0.07138397]), array([-0.01774722,  0.18270689,  0.26570245, -0.69540456]), array([ 0.0246982 ,  0.06376661,  0.14637914, -0.46679975]), array([ 0.0370958 ,  0.00457126, -0.02655766, -0.11340296]), array([ 0.01417737,  0.01974394, -0.19725673,  0.25850463]), array([-0.02466589,  0.06763126, -0.18185244,  0.20619754]), array([-0.06826729,  0.13124565, -0.24319221,  0.41192022]), array([-0.11686231,  0.22352346, -0.23002254,  0.48748834]), array([-0.14223298,  0.28286292, -0.01740043,  0.09332091]), array([-0.13633628,  0.29315213,  0.07538375,  0.00887688]), array([-0.11326986,  0.28716866,  0.15039778, -0.06420519]), array([-0.07878073,  0.27015211,  0.18700339, -0.09787883]), array([-0.04178077,  0.25168375,  0.17496884, -0.07803226]), array([-0.01188475,  0.24225884,  0.1176994 , -0.01004373]), array([0.00330652, 0.2493619 , 0.03142615, 0.08214328]), array([ 0.02650368,  0.20666194,  0.19464453, -0.49854398]), array([ 0.07702577,  0.05866511,  0.29602776, -0.94875887]), array([ 0.13752045, -0.15571924,  0.28893747, -1.14714383]), array([ 0.15846868, -0.31240921, -0.08670021, -0.3934743 ]), array([ 0.11661835, -0.34302293, -0.32352664,  0.08528614]), array([ 0.03457694, -0.28320131, -0.47849977,  0.49082838]), array([-0.06584948, -0.1590719 , -0.50186179,  0.71401957]), array([-0.15614414, -0.01395469, -0.37849104,  0.69814177]), array([-0.20922173,  0.10554642, -0.13825188,  0.46889192]), array([-0.2079852 ,  0.16541178,  0.15180937,  0.1204502 ]), array([-0.16375058,  0.18784603,  0.28246959,  0.10637824]), array([-0.07298528,  0.14163733,  0.60511303, -0.54672547]), array([ 0.04061858,  0.05254424,  0.50516959, -0.3110066 ]), array([0.11987642, 0.02825665, 0.27092593, 0.08412216]), array([ 0.14470639,  0.08855671, -0.02526075,  0.51160213]), array([ 0.12467656,  0.19135787, -0.16790637,  0.49602854]), array([ 0.08139213,  0.27823357, -0.25391229,  0.35194281]), array([ 0.02802774,  0.32427365, -0.26768969,  0.09276407]), array([-0.02094076,  0.3105159 , -0.21207934, -0.23609345]), array([-0.06666366,  0.26368234, -0.23719535, -0.23160569]), array([-0.11249466,  0.21808082, -0.21336995, -0.22342264]), array([-0.12271861,  0.10667073,  0.10980151, -0.87322441]), array([-0.09908391, -0.04928324,  0.11642719, -0.65526077]), array([-0.05340307, -0.21305737,  0.32527302, -0.94591852]), array([-0.00272259, -0.34293981,  0.16913446, -0.32673608]), array([ 0.01100452, -0.33788751, -0.03448625,  0.37828896]), array([-0.00254974, -0.22991699, -0.09574309,  0.68241567]), array([-0.02421057, -0.07511682, -0.11160639,  0.83573332]), array([-0.05625554,  0.12526138, -0.19485103,  1.12665549]), array([-0.09539794,  0.35638121, -0.18027324,  1.13757207]), array([-0.12246028,  0.5626655 , -0.08023561,  0.89059928]), array([-0.11309781,  0.67035746,  0.17064963,  0.17822585]), array([-0.0694711 ,  0.66665278,  0.25600609, -0.20720897]), array([-0.01522311,  0.5928799 ,  0.2744779 , -0.5125716 ]), array([ 0.03524094,  0.47055878,  0.21803782, -0.68587692]), array([ 0.06728597,  0.32945868,  0.09270675, -0.69851642]), array([ 0.06919525,  0.20153176, -0.0777094 , -0.55938067]), array([ 0.03594476,  0.11256169, -0.25085628, -0.32036736]), array([-0.00144033,  0.00635737, -0.11909332, -0.72847628]), array([-0.03825849, -0.10136706, -0.24495325, -0.3360311 ]), array([-0.09619607, -0.12649604, -0.3230332 ,  0.07935377]), array([-0.14869518, -0.1090812 , -0.19089203,  0.08362824]), array([-0.16917425, -0.09672263, -0.00957868,  0.03488227]), array([-0.16550857, -0.0615122 ,  0.04646334,  0.31192514]), array([-0.13733787, -0.009859  ,  0.23099737,  0.20041323]), array([-0.08958998,  0.05297297,  0.23905959,  0.42392598]), array([-0.04439906,  0.15653949,  0.20763255,  0.59970567]), array([0.00487394, 0.2528211 , 0.27766625, 0.35497049]), array([ 0.07572569,  0.26373427,  0.41579168, -0.23522308]), array([ 0.13755626,  0.23508949,  0.18926479, -0.03638374]), array([ 0.17436177,  0.1844659 ,  0.17012   , -0.45596872]), array([ 0.17547986,  0.1290212 , -0.16047569, -0.08959966]), array([ 0.12574652,  0.11363668, -0.32703044, -0.06991553]), array([ 0.04989691,  0.09774065, -0.41643176, -0.09839977]), array([-0.03417976,  0.07030487, -0.40816991, -0.18406488]), array([-0.1071204 ,  0.02159096, -0.30826799, -0.30533043]), array([-0.16650314, -0.01706873, -0.27487449, -0.08368419]), array([-0.199534  , -0.04844856, -0.05003091, -0.22950565]), array([-0.19947724, -0.07216906,  0.049885  , -0.00383119]), array([-0.18040025, -0.049278  ,  0.13766159,  0.23189825]), array([-0.11956389, -0.04937424,  0.45807358, -0.22267212]), array([-0.03173645, -0.06092488,  0.402119  ,  0.12249159]), array([ 0.06141699, -0.06542948,  0.51025924, -0.15206146]), array([ 0.13707595, -0.04470725,  0.23207481,  0.36641544]), array([0.16461181, 0.04467592, 0.04093621, 0.51571467]), array([ 0.15410655,  0.15495121, -0.14034994,  0.56657528]), array([ 0.09899065,  0.29581722, -0.39502314,  0.80872957]), array([ 0.01731575,  0.42899612, -0.40250065,  0.49046027]), array([-0.06722116,  0.51388079, -0.42369368,  0.33215964]), array([-0.13197184,  0.51994066, -0.21010416, -0.28202196]), array([-0.16039676,  0.43401507, -0.070165  , -0.56867257]), array([-0.15995177,  0.2986409 ,  0.07053161, -0.76281791]), array([-0.10891473,  0.07203135,  0.42258703, -1.45761729]), array([-0.02854714, -0.18961569,  0.35576145, -1.10014715]), array([ 0.02498277, -0.34879779,  0.16588918, -0.46056127]), array([ 0.03451183, -0.36662001, -0.07243426,  0.2854895 ]), array([-0.0026097 , -0.2384056 , -0.28888949,  0.97230677]), array([-0.06118496, -0.0277741 , -0.27801793,  1.08817817]), array([-0.10604836,  0.17750187, -0.15455031,  0.92161308]), array([-0.1180178 ,  0.32608697,  0.04099105,  0.53891393]), array([-0.08933699,  0.38682681,  0.24064323,  0.06452452]), array([-0.03853853,  0.38749316,  0.25685012, -0.0498245 ]), array([ 0.00897916,  0.3709375 ,  0.20811822, -0.10534156]), array([ 0.04097309,  0.34956095,  0.10476798, -0.099817  ]), array([ 0.04889758,  0.33376387, -0.02741323, -0.05452991]), array([ 0.0303391 ,  0.32808734, -0.15433262, -0.00467729]), array([ 0.00273397,  0.29622732, -0.11660545, -0.31357239]), array([-0.02796251,  0.23880315, -0.18573244, -0.25605377]), array([-0.06915271,  0.19498083, -0.21919682, -0.18103604]), array([-0.08610889,  0.09797943,  0.05008515, -0.77488234]), array([-0.07839875, -0.03511419,  0.02095937, -0.53153427]), array([-0.07948029, -0.10686559, -0.03349913, -0.17442005]), array([-0.09164889, -0.10293415, -0.08545495,  0.21085044]), array([-0.09853547, -0.06066304,  0.01914164,  0.20376442]), array([-0.08378234, -0.02402595,  0.1264183 ,  0.15878161]), array([-0.06288825,  0.03649053,  0.08036725,  0.43880156]), array([-0.03854302,  0.1120446 ,  0.16046538,  0.30754128]), array([-0.01371406,  0.19131712,  0.08560965,  0.47484801]), array([0.00859576, 0.26254   , 0.13459988, 0.22970097]), array([0.02531509, 0.31577344, 0.03075934, 0.29649658]), array([ 0.03389006,  0.3442326 ,  0.05357457, -0.01433635]), array([ 0.03287596,  0.34447952, -0.06338166,  0.01643526]), array([ 0.00962312,  0.3497398 , -0.16409606,  0.03129934]), array([-0.0169932 ,  0.32084901, -0.09707772, -0.32013812]), array([-0.04112797,  0.25801848, -0.1411209 , -0.30164106]), array([-0.07187072,  0.20253814, -0.16182028, -0.24841854]), array([-0.10386897,  0.16014316, -0.15312683, -0.17298015]), array([-0.13109579,  0.13393454, -0.11458855, -0.08856703]), array([-0.1480807 ,  0.12458555, -0.05222751, -0.00577198]), array([-0.1511499 ,  0.13107505,  0.02230536,  0.06912406]), array([-0.13932414,  0.15151959,  0.09422307,  0.13352703]), array([-0.1146171 ,  0.18372203,  0.14894533,  0.18654086]), array([-0.08166136,  0.22530409,  0.17533751,  0.22699366]), array([-0.04676095,  0.27352178,  0.16811188,  0.25230154]), array([ 0.00936488,  0.25747378,  0.38074923, -0.40090261]), array([ 0.07221252,  0.19100447,  0.23308173, -0.2426063 ]), array([0.09808333, 0.1669647 , 0.01988637, 0.01007555]), array([ 0.10619646,  0.12700505,  0.05850486, -0.40175592]), array([ 0.09315315,  0.08077446, -0.18747574, -0.05515234]), array([ 0.04734719,  0.06914831, -0.26156368, -0.06635903]), array([-0.00731783,  0.05181816, -0.27452715, -0.11237829]), array([-0.05821409,  0.02229677, -0.22513251, -0.185384  ]), array([-0.09413437, -0.02257101, -0.12835421, -0.26084   ])]</t>
-  </si>
-  <si>
-    <t>['[2,1,0]', '[1,1,1]', '[0,2,1]', '[1,0,2]', '[1,2,0]', '[2,2,2]', '[0,0,0]', '[2,0,1]', '[1,1,2]', '[0,1,1]']</t>
-  </si>
-  <si>
-    <t>[0, 2, 2, 0, 2, 0, 2, 0, 0, 2, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 2, 0, 0, 0, 2, 0, 0, 0, 2, 0, 0, 0, 0, 2, 0, 0, 0, 2, 0, 0, 2, 0, 0, 2, 0, 0, 2, 0, 0, 2, 0, 0, 2, 0, 0, 2, 0, 0, 0, 2, 0, 0, 0, 0, 2, 0, 0, 0, 2, 0, 0, 2, 0, 0, 2, 0, 0, 2, 0, 0, 0, 2, 0, 0, 0, 2, 0, 0, 0, 2, 0, 0, 0, 2, 0, 0, 0, 2, 0, 0, 2, 0, 0, 2, 0, 0, 2, 0, 0, 0, 2, 0, 0, 0, 2, 0, 0, 0, 2, 0, 0, 0, 2, 0, 0, 0, 0, 2, 0, 0, 0, 0, 2, 0, 0, 0, 2, 0, 0, 0, 2, 0, 0, 0, 0, 2, 0, 0, 0, 0, 2, 0, 0, 0, 2, 0, 0, 0, 2, 0, 0, 0, 2, 0, 0, 0, 2, 0, 0, 0, 2, 0, 0, 0, 2, 0, 0, 0, 2, 0, 0, 0, 2, 0]</t>
-  </si>
-  <si>
-    <t>['[-0.03763371 -0.01533471  0.06554052 -0.01816017]', '[-0.03406929  0.01398622 -0.02953871  0.30651903]', '[-0.03493773  0.06836613  0.02265481  0.22789337]', '[-0.02479211  0.10222584  0.07768516  0.10663031]', '[-0.01808581  0.14469195 -0.0104571   0.31140101]', '[-0.01484609  0.18823383  0.0432976   0.11751461]', '[-0.01434726  0.22467153 -0.03717771  0.24054013]', '[-0.01545278  0.24682047  0.02676029 -0.02247913]', '[-0.01721181  0.25018444 -0.04380907  0.05514087]', '[-0.03213003  0.26757856 -0.10176092  0.11343711]', '[-0.04292178  0.2589368  -0.00427078 -0.19989973]', '[-0.04724582  0.22400641 -0.03910061 -0.1442553 ]', '[-0.05828925  0.20274667 -0.06971448 -0.06649573]', '[-0.07416359  0.19747218 -0.0859609   0.01216736]', '[-0.0912366   0.20638244 -0.08104733  0.07279687]', '[-0.10506889  0.22457911 -0.0539522   0.10400424]', '[-0.11166695  0.24587804 -0.010094    0.10444057]', '[-0.10867284  0.26478582  0.03995039  0.08196904]', '[-0.09613136  0.27802333  0.08328201  0.05013698]', '[-0.07660094  0.2851802   0.10825155  0.02324806]', '[-0.0545593   0.2883646   0.10777726  0.01147603]', '[-0.03525161  0.29099778  0.08146314  0.01741678]', '[-0.02329543  0.29616619  0.03584343  0.03525702]', '[-0.0214414   0.30511627 -0.01738635  0.05301171]', '[-0.02985137  0.31645556 -0.06464183  0.05714453]', '[-0.04610073  0.32638407 -0.09423766  0.03793816]', '[-0.06589513  0.32991089 -0.09957126 -0.0063193 ]', '[-0.08428464  0.32265766 -0.08080209 -0.06781655]', '[-0.09702234  0.30264881 -0.04459147 -0.13085587]', '[-0.10168093  0.27149627 -0.00200248 -0.17612255]', '[-0.09820986  0.23455768  0.03486443 -0.1864638 ]', '[-0.0887719   0.19991036  0.05652747 -0.1526692 ]', '[-0.076919    0.17632476  0.05888771 -0.07738584]', '[-0.06638826  0.1707868   0.04416262  0.02447002]', '[-0.05992123  0.18633723  0.01974774  0.1292307 ]', '[-0.0584844   0.22093296 -0.00454223  0.21092628]', '[-0.04805938  0.23384537  0.10680343 -0.08193806]', '[-0.03080471  0.22450229  0.06202129 -0.00733249]', '[-0.02430606  0.23182975  0.00194388  0.08025297]', '[-0.02987406  0.25554917 -0.05571698  0.1519643 ]', '[-0.03226718  0.25603978  0.03214881 -0.14722185]', '[-0.03092284  0.23283646 -0.01960446 -0.08080664]', '[-0.03999585  0.22459335 -0.06946922 -0.00175473]', '[-0.05757792  0.23128942 -0.10254152  0.0647801 ]', '[-0.06605782  0.21440088  0.01888208 -0.23192227]', '[-0.06398042  0.17583314  0.00028999 -0.14688162]', '[-0.06633966  0.15773225 -0.02393686 -0.03146107]', '[-0.07325426  0.16341223 -0.04358916  0.08612216]', '[-0.0828409   0.19044139 -0.04946038  0.17797922]', '[-0.07864045  0.19750911  0.09060325 -0.10746977]', '[-0.06146966  0.1840293   0.07725441 -0.02247667]', '[-0.04907293  0.18981812  0.04445008  0.08115296]', '[-0.0442206   0.21593689  0.00396872  0.17619258]', '[-0.0340252   0.22400041  0.09594658 -0.09498212]', '[-0.02075128  0.2143682   0.03388699  0.00222931]', '[-0.02104003  0.22532354 -0.03629256  0.10526593]', '[-0.02132272  0.22066204  0.03329065 -0.15093594]', '[-0.02172504  0.20133409 -0.03773268 -0.03927642]', '[-0.03590812  0.20503959 -0.10102303  0.07333768]', '[-0.04715656  0.19439332 -0.00957467 -0.17953506]', '[-0.0531357   0.16954638 -0.04973417 -0.06569152]', '[-0.06641635  0.16843644 -0.08037468  0.05264093]', '[-0.07065933  0.15478558  0.03826249 -0.18722535]', '[-0.06537071  0.13069535  0.01283817 -0.04881322]', '[-0.06587487  0.13613518 -0.01753718  0.10204491]', '[-0.05864396  0.1357341   0.08821968 -0.10462186]', '[-0.04548709  0.13096902  0.0406286   0.05963551]', '[-0.04291628  0.15928652 -0.01443372  0.21883176]', '[-0.03731008  0.18120939  0.06982108 -0.00211053]', '[-0.02929538  0.19339059  0.00917428  0.12290951]', '[-0.03349002  0.22880302 -0.04909788  0.22438117]', '[-0.03450974  0.2455827   0.03936722 -0.05911149]', '[-0.03159904  0.24030656 -0.01094568  0.00758765]', '[-0.03869893  0.24839084 -0.05831173  0.07068777]', '[-0.05379571  0.26688344 -0.08901105  0.10873581]', '[-0.05952816  0.25548823  0.03243166 -0.22145423]', '[-0.05489462  0.21545832  0.01177921 -0.17140764]', '[-0.05545332  0.18946482 -0.01801811 -0.08425214]', '[-0.06203264  0.18272624 -0.04661029  0.01691807]', '[-0.07329597  0.19542728 -0.06331667  0.10611252]', '[-0.07291285  0.18890039  0.06671518 -0.16992223]', '[-0.06124858  0.1646186   0.04684919 -0.0670246 ]', '[-0.05512685  0.16363989  0.01316512  0.05821198]', '[-0.0560562   0.1872715  -0.0214586   0.17375768]', '[-0.04978711  0.19645649  0.08295617 -0.08215295]', '[-0.03756886  0.19056932  0.0366416   0.02604427]', '[-0.03567973  0.20700006 -0.01754356  0.13560046]', '[-0.03085252  0.20876406  0.06473776 -0.11723264]', '[-0.02424847  0.196482   -0.00032713 -0.00261782]', '[-0.03100005  0.20777645 -0.06538222  0.11242368]', '[-0.0359292   0.20511167  0.0169028  -0.1391461 ]', '[-0.03796388  0.18818858 -0.03728875 -0.02764034]', '[-0.05031463  0.19399173 -0.08347089  0.08264107]', '[-0.05662994  0.18503831  0.02121658 -0.17138809]', '[-0.0557285   0.1620654  -0.01305608 -0.05435543]', '[-0.06179154  0.1639193  -0.04623193  0.07152106]', '[-0.07328392  0.18910806 -0.06553354  0.17417505]', '[-0.07335166  0.19634492  0.06487831 -0.10266275]', '[-0.06177017  0.18423969  0.04825838 -0.01462708]', '[-0.05488602  0.19131999  0.01946897  0.08515879]', '[-0.05409083  0.21737568 -0.01081564  0.17096106]', '[-0.0455179   0.22329134  0.09477424 -0.11112369]', '[-0.03110464  0.20954516  0.04608388 -0.02188119]', '[-0.02791325  0.21545438 -0.01455441  0.08032165]', '[-0.03649726  0.24040015 -0.06871848  0.16345142]', '[-0.04080527  0.24387915  0.02645818 -0.12958454]', '[-0.0397104   0.22448553 -0.01626015 -0.06100079]', '[-0.04720324  0.22012961 -0.05722677  0.01691987]', '[-0.06162359  0.23030853 -0.08370973  0.08084752]', '[-0.06600717  0.2163849   0.04024637 -0.2181857 ]', '[-0.05979725  0.1804201   0.01950769 -0.13441852]', '[-0.05888347  0.16476469 -0.01099665 -0.01940731]', '[-0.06407603  0.17281273 -0.0395712   0.09758891]', '[-0.06065386  0.1678865   0.07280166 -0.14522098]', '[-0.04966623  0.15169303  0.03440973 -0.01236959]', '[-0.04750035  0.16357179 -0.01272862  0.12927392]', '[-0.04105973  0.16737522  0.07579271 -0.09062643]', '[-0.03181692  0.16358967  0.01474012  0.05467468]', '[-0.03527926  0.18869417 -0.04777651  0.19133535]', '[-0.0365353   0.20287936  0.03571079 -0.051725  ]', '[-0.03483137  0.20313934 -0.01893185  0.05440579]', '[-0.0436698   0.22366711 -0.06696449  0.145884  ]', '[-0.04706184  0.22473147  0.03361301 -0.13563625]', '[-0.04418538  0.20557604 -0.00596334 -0.05231351]', '[-0.04949228  0.20447588 -0.04600717  0.04057067]', '[-0.06173633  0.2206755  -0.07341547  0.116697  ]', '[-0.06425486  0.2146904   0.0484192  -0.17563926]', '[-0.05668024  0.18734092  0.02498423 -0.0920928 ]', '[-0.05491882  0.17947298 -0.00791746  0.01492437]', '[-0.0596878   0.19302134 -0.03832988  0.11739016]', '[-0.05619001  0.19031439  0.07236123 -0.14318035]', '[-0.0454138   0.17261945  0.03273101 -0.02919417]', '[-0.04372408  0.17948352 -0.01588161  0.09676409]', '[-0.05126569  0.20979208 -0.05699667  0.19983639]', '[-0.05198527  0.22200654  0.0500947  -0.07945891]', '[-0.04533753  0.21363571  0.01483222 -0.0018944 ]', '[-0.0463109   0.22148048 -0.02407281  0.0787548 ]', '[-0.05438047  0.24375967 -0.05427245  0.13894306]', '[-0.05372026  0.2406193   0.06049358 -0.16942006]', '[-0.04463697  0.21288262  0.02770161 -0.10192129]', '[-0.04336373  0.20163234 -0.0155124  -0.00857866]', '[-0.05061889  0.2093934  -0.05527231  0.08363345]', '[-0.06435839  0.23324163 -0.07857756  0.14861028]', '[-0.06730651  0.23192304  0.04948398 -0.16168937]', '[-0.05883162  0.20524499  0.03276134 -0.09931012]', '[-0.05500133  0.19400643  0.00446478 -0.01065727]', '[-0.05715497  0.20120397 -0.02529162  0.08096931]', '[-0.0645019   0.22496316 -0.04592316  0.15136883]', '[-0.06130255  0.22518156  0.0770882  -0.14839335]', '[-0.04837349  0.20248298  0.04893301 -0.07281919]', '[-0.04273031  0.19770393  0.00627284  0.02659696]', '[-0.04591053  0.21285164 -0.03689892  0.12168229]', '[-0.04347258  0.21028651  0.06056486 -0.1462549 ]', '[-0.03614087  0.1910518   0.01074203 -0.04179718]', '[-0.03947321  0.19431122 -0.04321122  0.07317264]', '[-0.05253773  0.21877441 -0.08397342  0.16515061]', '[-0.05817197  0.2231173   0.02872709 -0.12296549]', '[-0.05489845  0.20552316  0.00284485 -0.04955296]', '[-0.05721498  0.20403602 -0.02554212  0.03448932]', '[-0.0646143   0.21853204 -0.04647194  0.10678867]', '[-0.07477389  0.24469845 -0.05226096  0.14885243]', '[-0.07122742  0.24152634  0.086726   -0.17916281]', '[-0.05498818  0.21037193  0.07145947 -0.12465497]', '[-0.04414385  0.19431106  0.03434931 -0.03164432]', '[-0.04190616  0.19861129 -0.01222167  0.07412546]', '[-0.04865249  0.22279494 -0.05307019  0.16243211]', '[-0.04876946  0.22677321  0.05186349 -0.1229961 ]', '[-0.04213859  0.20981456  0.01263879 -0.04278132]', '[-0.04404101  0.21043339 -0.03119619  0.04845499]', '[-0.05398993  0.22814664 -0.065687    0.12403651]', '[-0.05583566  0.22360832  0.04732925 -0.16865855]', '[-0.04932204  0.19746509  0.015729   -0.08739938]', '[-0.05003684  0.19008374 -0.02290332  0.0146265 ]', '[-0.05807878  0.20284165 -0.0554402   0.10942639]', '[-0.05790075  0.19766104  0.05688596 -0.16005493]', '[-0.04976802  0.17569977  0.0221649  -0.05464645]', '[-0.0495524   0.17686995 -0.01994654  0.06604468]', '[-0.05725766  0.20096191 -0.05473457  0.16943631]', '[-0.0570025   0.20764109  0.05724175 -0.10337722]', '[-0.0486632   0.19569477  0.02414707 -0.01286173]', '[-0.04778381  0.20299982 -0.0152429   0.08468107]', '[-0.0543024   0.22821443 -0.04779902  0.16207112]', '[-0.05263416  0.23110656  0.0640425  -0.13303324]', '[-0.04313379  0.21149034  0.02848912 -0.05842022]', '[-0.04186596  0.2089284  -0.01608281  0.03331756]', '[-0.04922772  0.22416994 -0.05552064  0.11526221]', '[-0.04977785  0.21882787  0.04984121 -0.16760659]', '[-0.04360366  0.19394719  0.00993861 -0.07610417]', '[-0.0461728   0.18959435 -0.03517878  0.03279826]', '[-0.05702251  0.20618426 -0.07055258  0.12848178]', '[-0.05979159  0.20435551  0.04321498 -0.14658365]', '[-0.05391177  0.18405248  0.01380909 -0.05215954]', '[-0.05463957  0.18441447 -0.02087051  0.05548924]', '[-0.06178226  0.20522765 -0.04841424  0.14787871]', '[-0.05972167  0.20694652  0.06847341 -0.13033408]', '[-0.04894413  0.18968478  0.03663804 -0.03777247]', '[-0.0457767   0.19284761 -0.00543932  0.06921977]', '[-0.05086272  0.21635844 -0.04360406  0.16097351]', '[-0.04900321  0.22054227  0.06176369 -0.1192147 ]', '[-0.04055416  0.20498766  0.02059695 -0.03248258]']</t>
-  </si>
-  <si>
-    <t>[array([-0.03763371, -0.01533471,  0.06554052, -0.01816017], dtype=float32), array([-0.03406929,  0.01398622, -0.02953871,  0.30651903]), array([-0.03493773,  0.06836613,  0.02265481,  0.22789337]), array([-0.02479211,  0.10222584,  0.07768516,  0.10663031]), array([-0.01808581,  0.14469195, -0.0104571 ,  0.31140101]), array([-0.01484609,  0.18823383,  0.0432976 ,  0.11751461]), array([-0.01434726,  0.22467153, -0.03717771,  0.24054013]), array([-0.01545278,  0.24682047,  0.02676029, -0.02247913]), array([-0.01721181,  0.25018444, -0.04380907,  0.05514087]), array([-0.03213003,  0.26757856, -0.10176092,  0.11343711]), array([-0.04292178,  0.2589368 , -0.00427078, -0.19989973]), array([-0.04724582,  0.22400641, -0.03910061, -0.1442553 ]), array([-0.05828925,  0.20274667, -0.06971448, -0.06649573]), array([-0.07416359,  0.19747218, -0.0859609 ,  0.01216736]), array([-0.0912366 ,  0.20638244, -0.08104733,  0.07279687]), array([-0.10506889,  0.22457911, -0.0539522 ,  0.10400424]), array([-0.11166695,  0.24587804, -0.010094  ,  0.10444057]), array([-0.10867284,  0.26478582,  0.03995039,  0.08196904]), array([-0.09613136,  0.27802333,  0.08328201,  0.05013698]), array([-0.07660094,  0.2851802 ,  0.10825155,  0.02324806]), array([-0.0545593 ,  0.2883646 ,  0.10777726,  0.01147603]), array([-0.03525161,  0.29099778,  0.08146314,  0.01741678]), array([-0.02329543,  0.29616619,  0.03584343,  0.03525702]), array([-0.0214414 ,  0.30511627, -0.01738635,  0.05301171]), array([-0.02985137,  0.31645556, -0.06464183,  0.05714453]), array([-0.04610073,  0.32638407, -0.09423766,  0.03793816]), array([-0.06589513,  0.32991089, -0.09957126, -0.0063193 ]), array([-0.08428464,  0.32265766, -0.08080209, -0.06781655]), array([-0.09702234,  0.30264881, -0.04459147, -0.13085587]), array([-0.10168093,  0.27149627, -0.00200248, -0.17612255]), array([-0.09820986,  0.23455768,  0.03486443, -0.1864638 ]), array([-0.0887719 ,  0.19991036,  0.05652747, -0.1526692 ]), array([-0.076919  ,  0.17632476,  0.05888771, -0.07738584]), array([-0.06638826,  0.1707868 ,  0.04416262,  0.02447002]), array([-0.05992123,  0.18633723,  0.01974774,  0.1292307 ]), array([-0.0584844 ,  0.22093296, -0.00454223,  0.21092628]), array([-0.04805938,  0.23384537,  0.10680343, -0.08193806]), array([-0.03080471,  0.22450229,  0.06202129, -0.00733249]), array([-0.02430606,  0.23182975,  0.00194388,  0.08025297]), array([-0.02987406,  0.25554917, -0.05571698,  0.1519643 ]), array([-0.03226718,  0.25603978,  0.03214881, -0.14722185]), array([-0.03092284,  0.23283646, -0.01960446, -0.08080664]), array([-0.03999585,  0.22459335, -0.06946922, -0.00175473]), array([-0.05757792,  0.23128942, -0.10254152,  0.0647801 ]), array([-0.06605782,  0.21440088,  0.01888208, -0.23192227]), array([-0.06398042,  0.17583314,  0.00028999, -0.14688162]), array([-0.06633966,  0.15773225, -0.02393686, -0.03146107]), array([-0.07325426,  0.16341223, -0.04358916,  0.08612216]), array([-0.0828409 ,  0.19044139, -0.04946038,  0.17797922]), array([-0.07864045,  0.19750911,  0.09060325, -0.10746977]), array([-0.06146966,  0.1840293 ,  0.07725441, -0.02247667]), array([-0.04907293,  0.18981812,  0.04445008,  0.08115296]), array([-0.0442206 ,  0.21593689,  0.00396872,  0.17619258]), array([-0.0340252 ,  0.22400041,  0.09594658, -0.09498212]), array([-0.02075128,  0.2143682 ,  0.03388699,  0.00222931]), array([-0.02104003,  0.22532354, -0.03629256,  0.10526593]), array([-0.02132272,  0.22066204,  0.03329065, -0.15093594]), array([-0.02172504,  0.20133409, -0.03773268, -0.03927642]), array([-0.03590812,  0.20503959, -0.10102303,  0.07333768]), array([-0.04715656,  0.19439332, -0.00957467, -0.17953506]), array([-0.0531357 ,  0.16954638, -0.04973417, -0.06569152]), array([-0.06641635,  0.16843644, -0.08037468,  0.05264093]), array([-0.07065933,  0.15478558,  0.03826249, -0.18722535]), array([-0.06537071,  0.13069535,  0.01283817, -0.04881322]), array([-0.06587487,  0.13613518, -0.01753718,  0.10204491]), array([-0.05864396,  0.1357341 ,  0.08821968, -0.10462186]), array([-0.04548709,  0.13096902,  0.0406286 ,  0.05963551]), array([-0.04291628,  0.15928652, -0.01443372,  0.21883176]), array([-0.03731008,  0.18120939,  0.06982108, -0.00211053]), array([-0.02929538,  0.19339059,  0.00917428,  0.12290951]), array([-0.03349002,  0.22880302, -0.04909788,  0.22438117]), array([-0.03450974,  0.2455827 ,  0.03936722, -0.05911149]), array([-0.03159904,  0.24030656, -0.01094568,  0.00758765]), array([-0.03869893,  0.24839084, -0.05831173,  0.07068777]), array([-0.05379571,  0.26688344, -0.08901105,  0.10873581]), array([-0.05952816,  0.25548823,  0.03243166, -0.22145423]), array([-0.05489462,  0.21545832,  0.01177921, -0.17140764]), array([-0.05545332,  0.18946482, -0.01801811, -0.08425214]), array([-0.06203264,  0.18272624, -0.04661029,  0.01691807]), array([-0.07329597,  0.19542728, -0.06331667,  0.10611252]), array([-0.07291285,  0.18890039,  0.06671518, -0.16992223]), array([-0.06124858,  0.1646186 ,  0.04684919, -0.0670246 ]), array([-0.05512685,  0.16363989,  0.01316512,  0.05821198]), array([-0.0560562 ,  0.1872715 , -0.0214586 ,  0.17375768]), array([-0.04978711,  0.19645649,  0.08295617, -0.08215295]), array([-0.03756886,  0.19056932,  0.0366416 ,  0.02604427]), array([-0.03567973,  0.20700006, -0.01754356,  0.13560046]), array([-0.03085252,  0.20876406,  0.06473776, -0.11723264]), array([-0.02424847,  0.196482  , -0.00032713, -0.00261782]), array([-0.03100005,  0.20777645, -0.06538222,  0.11242368]), array([-0.0359292 ,  0.20511167,  0.0169028 , -0.1391461 ]), array([-0.03796388,  0.18818858, -0.03728875, -0.02764034]), array([-0.05031463,  0.19399173, -0.08347089,  0.08264107]), array([-0.05662994,  0.18503831,  0.02121658, -0.17138809]), array([-0.0557285 ,  0.1620654 , -0.01305608, -0.05435543]), array([-0.06179154,  0.1639193 , -0.04623193,  0.07152106]), array([-0.07328392,  0.18910806, -0.06553354,  0.17417505]), array([-0.07335166,  0.19634492,  0.06487831, -0.10266275]), array([-0.06177017,  0.18423969,  0.04825838, -0.01462708]), array([-0.05488602,  0.19131999,  0.01946897,  0.08515879]), array([-0.05409083,  0.21737568, -0.01081564,  0.17096106]), array([-0.0455179 ,  0.22329134,  0.09477424, -0.11112369]), array([-0.03110464,  0.20954516,  0.04608388, -0.02188119]), array([-0.02791325,  0.21545438, -0.01455441,  0.08032165]), array([-0.03649726,  0.24040015, -0.06871848,  0.16345142]), array([-0.04080527,  0.24387915,  0.02645818, -0.12958454]), array([-0.0397104 ,  0.22448553, -0.01626015, -0.06100079]), array([-0.04720324,  0.22012961, -0.05722677,  0.01691987]), array([-0.06162359,  0.23030853, -0.08370973,  0.08084752]), array([-0.06600717,  0.2163849 ,  0.04024637, -0.2181857 ]), array([-0.05979725,  0.1804201 ,  0.01950769, -0.13441852]), array([-0.05888347,  0.16476469, -0.01099665, -0.01940731]), array([-0.06407603,  0.17281273, -0.0395712 ,  0.09758891]), array([-0.06065386,  0.1678865 ,  0.07280166, -0.14522098]), array([-0.04966623,  0.15169303,  0.03440973, -0.01236959]), array([-0.04750035,  0.16357179, -0.01272862,  0.12927392]), array([-0.04105973,  0.16737522,  0.07579271, -0.09062643]), array([-0.03181692,  0.16358967,  0.01474012,  0.05467468]), array([-0.03527926,  0.18869417, -0.04777651,  0.19133535]), array([-0.0365353 ,  0.20287936,  0.03571079, -0.051725  ]), array([-0.03483137,  0.20313934, -0.01893185,  0.05440579]), array([-0.0436698 ,  0.22366711, -0.06696449,  0.145884  ]), array([-0.04706184,  0.22473147,  0.03361301, -0.13563625]), array([-0.04418538,  0.20557604, -0.00596334, -0.05231351]), array([-0.04949228,  0.20447588, -0.04600717,  0.04057067]), array([-0.06173633,  0.2206755 , -0.07341547,  0.116697  ]), array([-0.06425486,  0.2146904 ,  0.0484192 , -0.17563926]), array([-0.05668024,  0.18734092,  0.02498423, -0.0920928 ]), array([-0.05491882,  0.17947298, -0.00791746,  0.01492437]), array([-0.0596878 ,  0.19302134, -0.03832988,  0.11739016]), array([-0.05619001,  0.19031439,  0.07236123, -0.14318035]), array([-0.0454138 ,  0.17261945,  0.03273101, -0.02919417]), array([-0.04372408,  0.17948352, -0.01588161,  0.09676409]), array([-0.05126569,  0.20979208, -0.05699667,  0.19983639]), array([-0.05198527,  0.22200654,  0.0500947 , -0.07945891]), array([-0.04533753,  0.21363571,  0.01483222, -0.0018944 ]), array([-0.0463109 ,  0.22148048, -0.02407281,  0.0787548 ]), array([-0.05438047,  0.24375967, -0.05427245,  0.13894306]), array([-0.05372026,  0.2406193 ,  0.06049358, -0.16942006]), array([-0.04463697,  0.21288262,  0.02770161, -0.10192129]), array([-0.04336373,  0.20163234, -0.0155124 , -0.00857866]), array([-0.05061889,  0.2093934 , -0.05527231,  0.08363345]), array([-0.06435839,  0.23324163, -0.07857756,  0.14861028]), array([-0.06730651,  0.23192304,  0.04948398, -0.16168937]), array([-0.05883162,  0.20524499,  0.03276134, -0.09931012]), array([-0.05500133,  0.19400643,  0.00446478, -0.01065727]), array([-0.05715497,  0.20120397, -0.02529162,  0.08096931]), array([-0.0645019 ,  0.22496316, -0.04592316,  0.15136883]), array([-0.06130255,  0.22518156,  0.0770882 , -0.14839335]), array([-0.04837349,  0.20248298,  0.04893301, -0.07281919]), array([-0.04273031,  0.19770393,  0.00627284,  0.02659696]), array([-0.04591053,  0.21285164, -0.03689892,  0.12168229]), array([-0.04347258,  0.21028651,  0.06056486, -0.1462549 ]), array([-0.03614087,  0.1910518 ,  0.01074203, -0.04179718]), array([-0.03947321,  0.19431122, -0.04321122,  0.07317264]), array([-0.05253773,  0.21877441, -0.08397342,  0.16515061]), array([-0.05817197,  0.2231173 ,  0.02872709, -0.12296549]), array([-0.05489845,  0.20552316,  0.00284485, -0.04955296]), array([-0.05721498,  0.20403602, -0.02554212,  0.03448932]), array([-0.0646143 ,  0.21853204, -0.04647194,  0.10678867]), array([-0.07477389,  0.24469845, -0.05226096,  0.14885243]), array([-0.07122742,  0.24152634,  0.086726  , -0.17916281]), array([-0.05498818,  0.21037193,  0.07145947, -0.12465497]), array([-0.04414385,  0.19431106,  0.03434931, -0.03164432]), array([-0.04190616,  0.19861129, -0.01222167,  0.07412546]), array([-0.04865249,  0.22279494, -0.05307019,  0.16243211]), array([-0.04876946,  0.22677321,  0.05186349, -0.1229961 ]), array([-0.04213859,  0.20981456,  0.01263879, -0.04278132]), array([-0.04404101,  0.21043339, -0.03119619,  0.04845499]), array([-0.05398993,  0.22814664, -0.065687  ,  0.12403651]), array([-0.05583566,  0.22360832,  0.04732925, -0.16865855]), array([-0.04932204,  0.19746509,  0.015729  , -0.08739938]), array([-0.05003684,  0.19008374, -0.02290332,  0.0146265 ]), array([-0.05807878,  0.20284165, -0.0554402 ,  0.10942639]), array([-0.05790075,  0.19766104,  0.05688596, -0.16005493]), array([-0.04976802,  0.17569977,  0.0221649 , -0.05464645]), array([-0.0495524 ,  0.17686995, -0.01994654,  0.06604468]), array([-0.05725766,  0.20096191, -0.05473457,  0.16943631]), array([-0.0570025 ,  0.20764109,  0.05724175, -0.10337722]), array([-0.0486632 ,  0.19569477,  0.02414707, -0.01286173]), array([-0.04778381,  0.20299982, -0.0152429 ,  0.08468107]), array([-0.0543024 ,  0.22821443, -0.04779902,  0.16207112]), array([-0.05263416,  0.23110656,  0.0640425 , -0.13303324]), array([-0.04313379,  0.21149034,  0.02848912, -0.05842022]), array([-0.04186596,  0.2089284 , -0.01608281,  0.03331756]), array([-0.04922772,  0.22416994, -0.05552064,  0.11526221]), array([-0.04977785,  0.21882787,  0.04984121, -0.16760659]), array([-0.04360366,  0.19394719,  0.00993861, -0.07610417]), array([-0.0461728 ,  0.18959435, -0.03517878,  0.03279826]), array([-0.05702251,  0.20618426, -0.07055258,  0.12848178]), array([-0.05979159,  0.20435551,  0.04321498, -0.14658365]), array([-0.05391177,  0.18405248,  0.01380909, -0.05215954]), array([-0.05463957,  0.18441447, -0.02087051,  0.05548924]), array([-0.06178226,  0.20522765, -0.04841424,  0.14787871]), array([-0.05972167,  0.20694652,  0.06847341, -0.13033408]), array([-0.04894413,  0.18968478,  0.03663804, -0.03777247]), array([-0.0457767 ,  0.19284761, -0.00543932,  0.06921977]), array([-0.05086272,  0.21635844, -0.04360406,  0.16097351]), array([-0.04900321,  0.22054227,  0.06176369, -0.1192147 ]), array([-0.04055416,  0.20498766,  0.02059695, -0.03248258])]</t>
-  </si>
-  <si>
-    <t>['[1,2,0]', '[0,2,1]', '[0,0,0]', '[1,1,1]', '[1,1,2]', '[2,0,1]', '[2,2,2]', '[1,0,2]', '[2,1,0]', '[0,1,1]']</t>
-  </si>
-  <si>
-    <t>[2,1,0]</t>
-  </si>
-  <si>
-    <t>[6, 8, 14, 16, 21, 22, 26, 31, 37, 40, 45, 48, 52, 57, 66, 70, 71, 72, 77, 78, 90, 99, 105, 116, 123, 124, 128, 130, 149, 153, 164, 170]</t>
-  </si>
-  <si>
-    <t>[0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 1, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 1, 2, 2, 2, 2, 2, 2, 2, 2, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 0]</t>
-  </si>
-  <si>
-    <t>['[-0.03763371 -0.01533471  0.06554052 -0.01816017]', '[-0.00754409 -0.05458322  0.2277812  -0.36241836]', '[ 0.04879627 -0.15231473  0.32089719 -0.5887683 ]', '[ 0.11397169 -0.27767857  0.31375488 -0.63332862]', '[ 0.16759438 -0.39312519  0.2086893  -0.49480525]', '[ 0.1930193  -0.46685036  0.03906408 -0.22816919]', '[ 0.18217995 -0.48119372 -0.14531723  0.08492936]', '[ 0.11196576 -0.36927962 -0.54130528  1.01009116]', '[ 0.00196683 -0.16269792 -0.52993942  1.00304703]', '[-0.1149626   0.07904669 -0.60745019  1.35291852]', '[-0.22699932  0.35071699 -0.48106861  1.29899879]', '[-0.29631946  0.57553848 -0.19358874  0.90713479]', '[-0.3001361   0.70178334  0.1568287   0.34038041]', '[-0.21230745  0.6472121   0.70316872 -0.8706947 ]', '[-0.05496393  0.43235727  0.8346309  -1.22402651]', '[ 0.13140744  0.11642557  0.98351876 -1.85487324]', '[ 0.29072674 -0.20120148  0.56744448 -1.24078537]', '[ 0.37231773 -0.42412428  0.22629359 -0.94181973]', '[ 0.37562162 -0.56386451 -0.19658046 -0.43548038]', '[ 0.27153488 -0.53034408 -0.82267617  0.75523604]', '[ 0.06006646 -0.27650028 -1.24563166  1.71806892]', '[-0.1762487   0.04948546 -1.05811227  1.4414396 ]', '[-0.3419433   0.26507388 -0.56119508  0.65668096]', '[-0.41676553  0.36568089 -0.17080185  0.3254938 ]', '[-0.38120933  0.32267044  0.51851281 -0.74525331]', '[-0.21824058  0.08068495  1.07298262 -1.61307407]', '[-1.46382279e-05 -2.17456468e-01  1.05551563e+00 -1.27937469e+00]', '[ 0.20943633 -0.46634794  0.98975369 -1.13504475]', '[ 0.37781057 -0.64595227  0.65894337 -0.61724306]', '[ 0.4623106  -0.701774    0.17045061  0.07157888]', '[ 0.41896543 -0.55302868 -0.59723393  1.40002352]', '[ 0.25841302 -0.22519893 -0.96775342  1.80458663]', '[ 0.02620566  0.19899127 -1.29042093  2.31722481]', '[-0.22872577  0.64694841 -1.19443905  2.04601102]', '[-0.43012897  0.98229164 -0.7820937   1.25552515]', '[-0.53094775  1.13749134 -0.21081239  0.28342613]', '[-0.49071779  1.03725148  0.61057143 -1.28467438]', '[-0.31455144  0.68820022  1.11966572 -2.16092581]', '[-0.03661871  0.13842441  1.59138021 -3.21063662]', '[ 0.28283854 -0.51860199  1.5038101  -3.16239192]', '[ 0.50970943 -1.00544678  0.73144588 -1.65687817]', '[ 0.59041931 -1.23239789  0.06719535 -0.60133337]', '[ 0.51748581 -1.19018042 -0.78328413  1.02105472]', '[ 0.28515431 -0.82569513 -1.51028156  2.60236533]', '[-0.0669875  -0.17610074 -1.92859807  3.74199497]', '[-0.41280749  0.50874661 -1.42861352  2.9074727 ]', '[-0.63531116  1.00166429 -0.753957    1.9542453 ]', '[-0.7056543   1.27867518  0.05566116  0.80536589]', '[-0.61587672  1.32218501  0.82328916 -0.36966218]', '[-0.36848598  1.07828324  1.6131837  -2.0596514 ]', '[ 0.01065513  0.51161869  2.11328722 -3.51529284]', '[ 0.43654028 -0.25221966  2.02029315 -3.86928382]', '[ 0.74702765 -0.87935628  1.02711547 -2.30855285]', '[ 0.85944796 -1.22435336  0.08479465 -1.12621228]', '[ 0.76259435 -1.27279069 -1.03286413  0.6456589 ]', '[ 0.45853646 -0.96275225 -1.96679659  2.45068772]', '[-8.89927259e-04 -3.11269271e-01 -2.53705929e+00  3.92002704e+00]', '[-0.47564025  0.43042973 -2.07943823  3.23743812]', '[-0.81919099  0.98099033 -1.29677618  2.18765226]', '[-0.98094965  1.29585678 -0.30502758  0.95876025]', '[-0.93948436  1.36402959  0.71273919 -0.28367632]', '[-0.6838118   1.12338246  1.81504437 -2.14052233]', '[-0.2303422   0.5084298   2.65053128 -3.93032725]', '[ 0.32693149 -0.35718548  2.75845976 -4.38644313]', '[ 0.81188763 -1.12333112  2.00306377 -3.13835468]', '[ 1.1102509  -1.60410918  0.95743504 -1.69000694]', '[ 1.17338192 -1.76087252 -0.3252263   0.10808487]', '[ 0.98316511 -1.55678937 -1.56223694  1.96439375]', '[ 0.55702642 -0.95645176 -2.66851107  4.06936648]', '[-0.05646349  0.03932583 -3.30788891  5.56309925]', '[-0.65340398  1.01102852 -2.52416032  3.8853191 ]', '[-1.04404109  1.57631443 -1.35862745  1.80892913]', '[-1.19055471  1.75286415 -0.09734441 -0.01682135]', '[-1.08186249  1.57073313  1.18045915 -1.82616747]', '[-0.72210811  1.00477328  2.39970277 -3.87772775]', '[-0.14184747  0.03334057  3.26647689 -5.57001452]', '[ 0.4959237  -1.02809149  2.93528641 -4.6744026 ]', '[ 0.97816919 -1.73523765  1.85866692 -2.44403606]', '[ 1.2298525  -2.0297131   0.63960341 -0.54309783]', '[ 1.23698399 -1.98286632 -0.57076767  1.01117329]', '[ 0.99562448 -1.59386584 -1.83426107  2.92803675]', '[ 0.50808355 -0.78450324 -3.01280409  5.19092578]', '[-0.16419371  0.40178792 -3.47824059  6.15971472]', '[-0.79041832  1.47508318 -2.68129663  4.40373122]', '[-1.22258117  2.17655663 -1.61740573  2.67992856]', '[-1.43008908  2.56810569 -0.44771848  1.26439375]', '[-1.40075317  2.68643771  0.73739758 -0.08259543]', '[-1.12756742  2.49109101  1.96861276 -1.89257581]', '[-0.63133434  1.91384323  2.93770906 -3.93973212]', '[ 0.0282548   0.88729866  3.6198527  -6.33356139]', '[ 0.73458869 -0.43007537  3.18554892 -6.24626824]', '[ 1.24427612 -1.50282522  1.84343249 -4.40725133]', '[ 1.46882118 -2.21972678  0.40798579 -2.81875754]', '[ 1.41302825 -2.63945191 -0.9450138  -1.37992943]', '[ 1.08987475 -2.73048292 -2.24600244  0.46858385]', '[ 0.54010761 -2.45396846 -3.15352319  2.28943975]', '[-0.12050214 -1.82031896 -3.33626555  4.01908539]', '[-0.7628017  -0.86861707 -3.04164756  5.39276365]', '[-1.30622644  0.24620402 -2.26326404  5.4416466 ]', '[-1.59461387  1.14868027 -0.57680704  3.54206197]', '[-1.54952699  1.71746636  1.04410114  2.09881434]', '[-1.16669714  1.914286    2.72729808 -0.20410514]', '[-0.49628732  1.6082896   3.85528798 -2.89594073]', '[ 0.3235439   0.76458819  4.2249558  -5.38979083]', '[ 1.12920029 -0.38850597  3.63772755 -5.62571863]', '[ 1.70331947 -1.29748448  2.09844332 -3.49694799]', '[ 1.99657729 -1.88453122  0.84404081 -2.44263596]', '[ 2.04214572 -2.28557195 -0.39010353 -1.55625765]', '[ 1.83238646 -2.46994857 -1.71066672 -0.22721899]', '[ 1.35225555 -2.32574669 -3.06891741  1.76118032]', '[ 0.62678857 -1.72386531 -4.10769816  4.36729253]', '[-0.26167809 -0.55232218 -4.68634751  7.18861419]', '[-1.1467016   0.88137174 -3.89797224  6.46278395]', '[-1.78185375  1.95292059 -2.47825574  4.39805623]', '[-2.15232369  2.70189791 -1.26584323  3.18471837]', '[-2.3058031  -3.04113847 -0.31314274  2.222423  ]', '[-2.27635269 -2.73692846  0.60454283  0.79939628]', '[-2.06260157 -2.70974152  1.56541137 -0.54246364]', '[-1.62843839 -2.97755476  2.80809364 -2.14473747]', '[-0.94035889  2.7045281   4.00485015 -3.93732373]', '[-0.07723594  1.68500341  4.52622376 -6.38929782]', '[ 0.8546268   0.13396472  4.64329249 -8.68002991]', '[ 1.64330714 -1.4340905   3.0579712  -6.59959081]', '[ 2.07423995 -2.52573289  1.33753848 -4.52720062]', '[ 2.21261794  3.0007822   0.13136239 -3.06451351]', '[ 2.15979441  2.49505519 -0.639749   -1.98273266]', '[ 1.95269986  2.2099493  -1.45809008 -0.87663179]', '[ 1.54824814  2.17507187 -2.61909263  0.46168424]', '[ 0.91773936  2.30803593 -3.64044966  0.70773998]', '[ 0.11975568  2.42021926 -4.17539394  0.182864  ]', '[-0.64965298  2.24866967 -3.25954641 -2.10930693]', '[-1.09892353  1.55793306 -1.05976354 -4.87455115]', '[-1.03092694  0.23841777  1.55710846 -8.08984371]', '[-0.67177873 -1.38138546  1.66426049 -7.55786718]', '[-0.39021934 -2.79651442  1.2782704  -6.87629469]', '[-0.07518685  2.02458892  2.10847401 -8.12387871]', '[  0.52103054   0.070451     3.5388815  -11.02846439]', '[ 1.0156685  -1.86670484  0.9642263  -7.74983623]', '[ 0.96539477  3.10864775 -1.10877199 -5.69101547]', '[ 0.72997882  1.99066493 -0.92708233 -5.89069709]', '[ 0.68387607  0.59441907  0.44621111 -8.19846899]', '[ 0.69839536 -1.00467222 -0.92954519 -6.81427229]', '[ 0.21341948 -1.97644766 -3.71695621 -3.0119101 ]', '[-0.65451573 -2.28190171 -4.60398301 -0.40695754]', '[-1.52805826 -2.26922976 -4.00106333  0.27593839]', '[-2.24486432e+00 -2.23439928e+00 -3.21222542e+00  2.51371975e-04]', '[-2.84795115 -2.26643908 -2.93103947 -0.25030353]', '[ 2.8183259  -2.28614164 -3.36357391  0.22685256]', '[ 2.04408147 -2.08889819 -4.46997022  2.02178012]', '[ 1.02781318 -1.40075937 -5.68699436  5.14031985]', '[-0.22909521  0.04761153 -6.62010233  8.55413004]', '[-1.45601434  1.48941876 -5.46257638  5.31179451]', '[-2.4367757   2.26734415 -4.43012515  2.82098772]', '[ 3.02050159  2.70169266 -3.9851966   1.80149047]', '[ 2.17350256  3.11764199 -4.64025122  2.57925093]', '[ 1.12874591 -2.4547582  -5.77405858  4.84076907]', '[-0.08989944 -1.09899454 -6.37928148  8.93247436]', '[-1.35195572  0.86151002 -5.85150323  9.34335657]', '[-2.36527831  2.3959044  -4.46726607  6.42393755]', '[ 3.07655709 -2.68184738 -4.11585687  5.9863135 ]', '[ 2.19581521 -1.35336288 -4.93180526  7.73859918]', '[ 1.02810716  0.52316429 -6.5421579  10.14825482]', '[-0.31661602  2.23754933 -6.84586782  6.6648139 ]', '[-1.64205258 -2.97043202 -6.16151254  4.53414284]', '[-2.74573425 -2.13306815 -5.00043777  4.08431042]', '[ 2.54329523 -1.19540709 -5.1937264   5.59906197]', '[ 1.36841009  0.20332163 -6.58212629  7.99265847]', '[-0.01571214  1.58543513 -7.02377376  4.98030476]', '[-1.34078694  2.10169644 -5.88314214  0.21581482]', '[-2.26295782  1.74399937 -3.21078831 -3.54066847]', '[-2.63745782  0.79097482 -0.71343416 -5.73453344]']</t>
-  </si>
-  <si>
-    <t>[0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50, 51, 52, 53, 54, 55, 56, 57, 58, 59, 60, 61, 62, 63, 64, 65, 66, 67, 68, 69, 70, 71, 72, 73, 74, 75, 76, 77, 78, 79, 80, 81, 82, 83, 84, 85, 86, 87, 88, 89, 90, 91, 92, 93, 94, 95, 96, 97, 98, 99, 100, 101, 102, 103, 104, 105, 106, 107, 108, 109, 110, 111, 112, 113, 114, 115, 116, 117, 118, 119, 120, 121, 122, 123, 124, 125, 126, 127, 128, 129, 130, 131, 132, 133, 134, 135, 136, 137, 138, 139, 140, 141, 142, 143, 144, 145, 146, 147, 148, 149, 150, 151, 152, 153, 154, 155, 156, 157, 158, 159, 160, 161, 162, 163, 164, 165, 166, 167, 168, 169, 170]</t>
-  </si>
-  <si>
-    <t>[array([-0.03763371, -0.01533471,  0.06554052, -0.01816017], dtype=float32), array([-0.00754409, -0.05458322,  0.2277812 , -0.36241836]), array([ 0.04879627, -0.15231473,  0.32089719, -0.5887683 ]), array([ 0.11397169, -0.27767857,  0.31375488, -0.63332862]), array([ 0.16759438, -0.39312519,  0.2086893 , -0.49480525]), array([ 0.1930193 , -0.46685036,  0.03906408, -0.22816919]), array([ 0.18217995, -0.48119372, -0.14531723,  0.08492936]), array([ 0.11196576, -0.36927962, -0.54130528,  1.01009116]), array([ 0.00196683, -0.16269792, -0.52993942,  1.00304703]), array([-0.1149626 ,  0.07904669, -0.60745019,  1.35291852]), array([-0.22699932,  0.35071699, -0.48106861,  1.29899879]), array([-0.29631946,  0.57553848, -0.19358874,  0.90713479]), array([-0.3001361 ,  0.70178334,  0.1568287 ,  0.34038041]), array([-0.21230745,  0.6472121 ,  0.70316872, -0.8706947 ]), array([-0.05496393,  0.43235727,  0.8346309 , -1.22402651]), array([ 0.13140744,  0.11642557,  0.98351876, -1.85487324]), array([ 0.29072674, -0.20120148,  0.56744448, -1.24078537]), array([ 0.37231773, -0.42412428,  0.22629359, -0.94181973]), array([ 0.37562162, -0.56386451, -0.19658046, -0.43548038]), array([ 0.27153488, -0.53034408, -0.82267617,  0.75523604]), array([ 0.06006646, -0.27650028, -1.24563166,  1.71806892]), array([-0.1762487 ,  0.04948546, -1.05811227,  1.4414396 ]), array([-0.3419433 ,  0.26507388, -0.56119508,  0.65668096]), array([-0.41676553,  0.36568089, -0.17080185,  0.3254938 ]), array([-0.38120933,  0.32267044,  0.51851281, -0.74525331]), array([-0.21824058,  0.08068495,  1.07298262, -1.61307407]), array([-1.46382279e-05, -2.17456468e-01,  1.05551563e+00, -1.27937469e+00]), array([ 0.20943633, -0.46634794,  0.98975369, -1.13504475]), array([ 0.37781057, -0.64595227,  0.65894337, -0.61724306]), array([ 0.4623106 , -0.701774  ,  0.17045061,  0.07157888]), array([ 0.41896543, -0.55302868, -0.59723393,  1.40002352]), array([ 0.25841302, -0.22519893, -0.96775342,  1.80458663]), array([ 0.02620566,  0.19899127, -1.29042093,  2.31722481]), array([-0.22872577,  0.64694841, -1.19443905,  2.04601102]), array([-0.43012897,  0.98229164, -0.7820937 ,  1.25552515]), array([-0.53094775,  1.13749134, -0.21081239,  0.28342613]), array([-0.49071779,  1.03725148,  0.61057143, -1.28467438]), array([-0.31455144,  0.68820022,  1.11966572, -2.16092581]), array([-0.03661871,  0.13842441,  1.59138021, -3.21063662]), array([ 0.28283854, -0.51860199,  1.5038101 , -3.16239192]), array([ 0.50970943, -1.00544678,  0.73144588, -1.65687817]), array([ 0.59041931, -1.23239789,  0.06719535, -0.60133337]), array([ 0.51748581, -1.19018042, -0.78328413,  1.02105472]), array([ 0.28515431, -0.82569513, -1.51028156,  2.60236533]), array([-0.0669875 , -0.17610074, -1.92859807,  3.74199497]), array([-0.41280749,  0.50874661, -1.42861352,  2.9074727 ]), array([-0.63531116,  1.00166429, -0.753957  ,  1.9542453 ]), array([-0.7056543 ,  1.27867518,  0.05566116,  0.80536589]), array([-0.61587672,  1.32218501,  0.82328916, -0.36966218]), array([-0.36848598,  1.07828324,  1.6131837 , -2.0596514 ]), array([ 0.01065513,  0.51161869,  2.11328722, -3.51529284]), array([ 0.43654028, -0.25221966,  2.02029315, -3.86928382]), array([ 0.74702765, -0.87935628,  1.02711547, -2.30855285]), array([ 0.85944796, -1.22435336,  0.08479465, -1.12621228]), array([ 0.76259435, -1.27279069, -1.03286413,  0.6456589 ]), array([ 0.45853646, -0.96275225, -1.96679659,  2.45068772]), array([-8.89927259e-04, -3.11269271e-01, -2.53705929e+00,  3.92002704e+00]), array([-0.47564025,  0.43042973, -2.07943823,  3.23743812]), array([-0.81919099,  0.98099033, -1.29677618,  2.18765226]), array([-0.98094965,  1.29585678, -0.30502758,  0.95876025]), array([-0.93948436,  1.36402959,  0.71273919, -0.28367632]), array([-0.6838118 ,  1.12338246,  1.81504437, -2.14052233]), array([-0.2303422 ,  0.5084298 ,  2.65053128, -3.93032725]), array([ 0.32693149, -0.35718548,  2.75845976, -4.38644313]), array([ 0.81188763, -1.12333112,  2.00306377, -3.13835468]), array([ 1.1102509 , -1.60410918,  0.95743504, -1.69000694]), array([ 1.17338192, -1.76087252, -0.3252263 ,  0.10808487]), array([ 0.98316511, -1.55678937, -1.56223694,  1.96439375]), array([ 0.55702642, -0.95645176, -2.66851107,  4.06936648]), array([-0.05646349,  0.03932583, -3.30788891,  5.56309925]), array([-0.65340398,  1.01102852, -2.52416032,  3.8853191 ]), array([-1.04404109,  1.57631443, -1.35862745,  1.80892913]), array([-1.19055471,  1.75286415, -0.09734441, -0.01682135]), array([-1.08186249,  1.57073313,  1.18045915, -1.82616747]), array([-0.72210811,  1.00477328,  2.39970277, -3.87772775]), array([-0.14184747,  0.03334057,  3.26647689, -5.57001452]), array([ 0.4959237 , -1.02809149,  2.93528641, -4.6744026 ]), array([ 0.97816919, -1.73523765,  1.85866692, -2.44403606]), array([ 1.2298525 , -2.0297131 ,  0.63960341, -0.54309783]), array([ 1.23698399, -1.98286632, -0.57076767,  1.01117329]), array([ 0.99562448, -1.59386584, -1.83426107,  2.92803675]), array([ 0.50808355, -0.78450324, -3.01280409,  5.19092578]), array([-0.16419371,  0.40178792, -3.47824059,  6.15971472]), array([-0.79041832,  1.47508318, -2.68129663,  4.40373122]), array([-1.22258117,  2.17655663, -1.61740573,  2.67992856]), array([-1.43008908,  2.56810569, -0.44771848,  1.26439375]), array([-1.40075317,  2.68643771,  0.73739758, -0.08259543]), array([-1.12756742,  2.49109101,  1.96861276, -1.89257581]), array([-0.63133434,  1.91384323,  2.93770906, -3.93973212]), array([ 0.0282548 ,  0.88729866,  3.6198527 , -6.33356139]), array([ 0.73458869, -0.43007537,  3.18554892, -6.24626824]), array([ 1.24427612, -1.50282522,  1.84343249, -4.40725133]), array([ 1.46882118, -2.21972678,  0.40798579, -2.81875754]), array([ 1.41302825, -2.63945191, -0.9450138 , -1.37992943]), array([ 1.08987475, -2.73048292, -2.24600244,  0.46858385]), array([ 0.54010761, -2.45396846, -3.15352319,  2.28943975]), array([-0.12050214, -1.82031896, -3.33626555,  4.01908539]), array([-0.7628017 , -0.86861707, -3.04164756,  5.39276365]), array([-1.30622644,  0.24620402, -2.26326404,  5.4416466 ]), array([-1.59461387,  1.14868027, -0.57680704,  3.54206197]), array([-1.54952699,  1.71746636,  1.04410114,  2.09881434]), array([-1.16669714,  1.914286  ,  2.72729808, -0.20410514]), array([-0.49628732,  1.6082896 ,  3.85528798, -2.89594073]), array([ 0.3235439 ,  0.76458819,  4.2249558 , -5.38979083]), array([ 1.12920029, -0.38850597,  3.63772755, -5.62571863]), array([ 1.70331947, -1.29748448,  2.09844332, -3.49694799]), array([ 1.99657729, -1.88453122,  0.84404081, -2.44263596]), array([ 2.04214572, -2.28557195, -0.39010353, -1.55625765]), array([ 1.83238646, -2.46994857, -1.71066672, -0.22721899]), array([ 1.35225555, -2.32574669, -3.06891741,  1.76118032]), array([ 0.62678857, -1.72386531, -4.10769816,  4.36729253]), array([-0.26167809, -0.55232218, -4.68634751,  7.18861419]), array([-1.1467016 ,  0.88137174, -3.89797224,  6.46278395]), array([-1.78185375,  1.95292059, -2.47825574,  4.39805623]), array([-2.15232369,  2.70189791, -1.26584323,  3.18471837]), array([-2.3058031 , -3.04113847, -0.31314274,  2.222423  ]), array([-2.27635269, -2.73692846,  0.60454283,  0.79939628]), array([-2.06260157, -2.70974152,  1.56541137, -0.54246364]), array([-1.62843839, -2.97755476,  2.80809364, -2.14473747]), array([-0.94035889,  2.7045281 ,  4.00485015, -3.93732373]), array([-0.07723594,  1.68500341,  4.52622376, -6.38929782]), array([ 0.8546268 ,  0.13396472,  4.64329249, -8.68002991]), array([ 1.64330714, -1.4340905 ,  3.0579712 , -6.59959081]), array([ 2.07423995, -2.52573289,  1.33753848, -4.52720062]), array([ 2.21261794,  3.0007822 ,  0.13136239, -3.06451351]), array([ 2.15979441,  2.49505519, -0.639749  , -1.98273266]), array([ 1.95269986,  2.2099493 , -1.45809008, -0.87663179]), array([ 1.54824814,  2.17507187, -2.61909263,  0.46168424]), array([ 0.91773936,  2.30803593, -3.64044966,  0.70773998]), array([ 0.11975568,  2.42021926, -4.17539394,  0.182864  ]), array([-0.64965298,  2.24866967, -3.25954641, -2.10930693]), array([-1.09892353,  1.55793306, -1.05976354, -4.87455115]), array([-1.03092694,  0.23841777,  1.55710846, -8.08984371]), array([-0.67177873, -1.38138546,  1.66426049, -7.55786718]), array([-0.39021934, -2.79651442,  1.2782704 , -6.87629469]), array([-0.07518685,  2.02458892,  2.10847401, -8.12387871]), array([  0.52103054,   0.070451  ,   3.5388815 , -11.02846439]), array([ 1.0156685 , -1.86670484,  0.9642263 , -7.74983623]), array([ 0.96539477,  3.10864775, -1.10877199, -5.69101547]), array([ 0.72997882,  1.99066493, -0.92708233, -5.89069709]), array([ 0.68387607,  0.59441907,  0.44621111, -8.19846899]), array([ 0.69839536, -1.00467222, -0.92954519, -6.81427229]), array([ 0.21341948, -1.97644766, -3.71695621, -3.0119101 ]), array([-0.65451573, -2.28190171, -4.60398301, -0.40695754]), array([-1.52805826, -2.26922976, -4.00106333,  0.27593839]), array([-2.24486432e+00, -2.23439928e+00, -3.21222542e+00,  2.51371975e-04]), array([-2.84795115, -2.26643908, -2.93103947, -0.25030353]), array([ 2.8183259 , -2.28614164, -3.36357391,  0.22685256]), array([ 2.04408147, -2.08889819, -4.46997022,  2.02178012]), array([ 1.02781318, -1.40075937, -5.68699436,  5.14031985]), array([-0.22909521,  0.04761153, -6.62010233,  8.55413004]), array([-1.45601434,  1.48941876, -5.46257638,  5.31179451]), array([-2.4367757 ,  2.26734415, -4.43012515,  2.82098772]), array([ 3.02050159,  2.70169266, -3.9851966 ,  1.80149047]), array([ 2.17350256,  3.11764199, -4.64025122,  2.57925093]), array([ 1.12874591, -2.4547582 , -5.77405858,  4.84076907]), array([-0.08989944, -1.09899454, -6.37928148,  8.93247436]), array([-1.35195572,  0.86151002, -5.85150323,  9.34335657]), array([-2.36527831,  2.3959044 , -4.46726607,  6.42393755]), array([ 3.07655709, -2.68184738, -4.11585687,  5.9863135 ]), array([ 2.19581521, -1.35336288, -4.93180526,  7.73859918]), array([ 1.02810716,  0.52316429, -6.5421579 , 10.14825482]), array([-0.31661602,  2.23754933, -6.84586782,  6.6648139 ]), array([-1.64205258, -2.97043202, -6.16151254,  4.53414284]), array([-2.74573425, -2.13306815, -5.00043777,  4.08431042]), array([ 2.54329523, -1.19540709, -5.1937264 ,  5.59906197]), array([ 1.36841009,  0.20332163, -6.58212629,  7.99265847]), array([-0.01571214,  1.58543513, -7.02377376,  4.98030476]), array([-1.34078694,  2.10169644, -5.88314214,  0.21581482]), array([-2.26295782,  1.74399937, -3.21078831, -3.54066847]), array([-2.63745782,  0.79097482, -0.71343416, -5.73453344])]</t>
-  </si>
-  <si>
-    <t>['[1,0,2]', '[0,1,1]', '[2,1,0]', '[2,0,1]', '[1,2,0]', '[2,2,2]', '[0,0,0]', '[1,1,1]', '[1,1,2]', '[0,2,1]']</t>
-  </si>
-  <si>
-    <t>[1, 2, 4, 5, 6, 9, 11, 16, 17, 18, 20, 21, 24, 26, 31, 32, 35, 36, 38, 42, 45, 46, 49, 53, 55, 56, 59, 63, 65, 66, 67, 75, 77, 81, 85, 87, 90, 91, 93, 94, 96, 98, 99, 100, 105, 108, 109, 111, 112, 114, 116, 117, 118, 119, 120, 122, 123, 124, 125, 126, 132, 138, 139, 141, 143, 145, 147, 149, 154, 156, 157, 158, 159, 164, 166, 170, 174, 176, 177, 179, 185, 186, 188, 194, 196]</t>
-  </si>
-  <si>
-    <t>[0, 2, 0, 0, 2, 0, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2]</t>
-  </si>
-  <si>
-    <t>['[-0.03763371 -0.01533471  0.06554052 -0.01816017]', '[-0.03406929  0.01398622 -0.02953871  0.30651903]', '[-0.02168374  0.03409236  0.1512214  -0.10649158]', '[ 0.02369474 -0.02529386  0.2912986  -0.46969041]', '[ 0.06234371 -0.07501275  0.08617182 -0.01368346]', '[ 0.08315347 -0.09791055  0.11692115 -0.20796639]', '[ 0.08020517 -0.08541727 -0.14509226  0.32970125]', '[ 0.02823683  0.02775306 -0.36024318  0.77393063]', '[-0.05588226  0.20852011 -0.4576235   0.98818913]', '[-0.11871774  0.3359788  -0.15597939  0.25913082]', '[-0.14114303  0.37431915 -0.06288902  0.11508823]', '[-0.14258595  0.37975756  0.04874616 -0.06153168]', '[-0.09670323  0.2839622   0.39900417 -0.87594373]', '[ 0.00905309  0.0447265   0.6299373  -1.45962888]', '[ 0.14061973 -0.27033256  0.6469136  -1.61170491]', '[ 0.25246041 -0.56854806  0.44121773 -1.30762249]', '[ 0.28434358 -0.7113844  -0.12568236 -0.10750594]', '[ 0.22857073 -0.67537935 -0.42028491  0.45613931]', '[ 0.12334762 -0.53763514 -0.60889086  0.88877377]', '[-0.02934395 -0.27067471 -0.88336674  1.72160332]', '[-0.18535329  0.04856985 -0.63356736  1.38697206]', '[-0.26845735  0.2559289  -0.17580569  0.6417687 ]', '[-0.27753233  0.36264871  0.08978857  0.40697523]', '[-0.20738751  0.34747952  0.59669407 -0.54664926]', '[-0.07533821  0.22443992  0.69365146 -0.64331462]', '[ 0.08337926  0.03974713  0.85566527 -1.14670364]', '[ 0.22335904 -0.13821957  0.51103408 -0.5814825 ]', '[ 0.3044938  -0.24697832  0.28142104 -0.47685731]', '[ 0.33030559 -0.31944117 -0.03005804 -0.23311507]', '[ 0.26641035 -0.26999224 -0.59497487  0.71177245]', '[ 0.10294594 -0.04971013 -1.00054681  1.42947944]', '[-0.08712675  0.19969288 -0.85393386  0.99043171]', '[-0.22232113  0.32232613 -0.46860563  0.19884495]', '[-0.29253623  0.33887386 -0.21981513 -0.04450158]', '[-0.28081766  0.23538886  0.3323012  -0.97296302]', '[-0.19322385  0.03391515  0.51934244 -0.99351627]', '[-0.08420054 -0.14135895  0.54361303 -0.71226949]', '[ 0.03983134 -0.30209283  0.66631305 -0.84694474]', '[ 0.14356628 -0.39333941  0.34867355 -0.03833912]', '[ 0.19906704 -0.37953004  0.19576272  0.18171402]', '[ 0.19305706 -0.25351841 -0.25222191  1.05894411]', '[ 0.10430604  0.02785392 -0.60739614  1.69139581]', '[-0.00837033  0.32195738 -0.48790205  1.18293312]', '[-0.10616067  0.54658455 -0.46487483  1.01373785]', '[-0.18526973  0.71040679 -0.3089262   0.5936578 ]', '[-0.20079648  0.71313016  0.15672725 -0.56818555]', '[-0.14869987  0.55177361  0.3522018  -1.01855717]', '[-0.04125518  0.25432511  0.69618905 -1.90011008]', '[ 0.11355379 -0.17367054  0.80136684 -2.27172065]', '[ 0.23230238 -0.54194     0.35517723 -1.34146245]', '[ 0.2735389  -0.75798832  0.04745859 -0.78886463]', '[ 0.25058597 -0.85068539 -0.27091347 -0.13380621]', '[ 0.14712054 -0.75256327 -0.74356624  1.09599204]', '[-0.01132386 -0.49094451 -0.80542582  1.46156204]', '[-0.1851566  -0.12916707 -0.88933812  2.07188869]', '[-0.31997474  0.22742026 -0.41919893  1.40976431]', '[-0.34279906  0.41150659  0.19791623  0.40348982]', '[-0.24356394  0.38624397  0.77374282 -0.64016313]', '[-0.04654728  0.17058915  1.15157269 -1.45326081]', '[ 0.16810876 -0.09113787  0.94280995 -1.08141426]', '[ 0.33868847 -0.3024337   0.72321479 -0.97082926]', '[ 0.44389114 -0.45893982  0.30587352 -0.55934094]', '[ 0.45546091 -0.517099   -0.19302747 -0.01362165]', '[ 0.36935181 -0.46536284 -0.65103355  0.51525189]', '[ 0.18011983 -0.25575809 -1.20051855  1.52684619]', '[-0.06182888  0.04215675 -1.1595688   1.357173  ]', '[-0.26079418  0.25137737 -0.78479417  0.67050503]', '[-0.36181597  0.29306036 -0.20566181 -0.27088047]', '[-0.34015764  0.14409663  0.41389263 -1.19212142]', '[-0.20559259 -0.1632966   0.89368565 -1.80521951]', '[-0.00273104 -0.53880892  1.08183182 -1.84991706]', '[ 0.20615756 -0.86610793  0.96278512 -1.35331091]', '[ 0.36713917 -1.05987501  0.61747341 -0.55326954]', '[ 0.44373447 -1.07990462  0.13329322  0.36060098]', '[ 0.39498981 -0.85695716 -0.62178325  1.86345862]', '[ 0.22534922 -0.40982398 -1.03321681  2.52790279]', '[-0.02014606  0.17365492 -1.34261325  3.14611632]', '[-0.25086115  0.71052285 -0.90806524  2.11225656]', '[-0.39268549  1.05528278 -0.48589787  1.29427216]', '[-0.43983353  1.21969295  0.01809109  0.34168767]', '[-0.36675593  1.13657528  0.7014129  -1.16810863]', '[-0.18820198  0.81595806  1.05362973 -1.99725772]', '[ 0.06284761  0.29980223  1.40268726 -3.06475668]', '[ 0.34012518 -0.34457287  1.27801053 -3.19149084]', '[ 0.54055141 -0.91030761  0.6751997  -2.3675353 ]', '[ 0.58018493 -1.21660388 -0.26931275 -0.69681752]', '[ 0.44145205 -1.19147953 -1.08797896  0.93955925]', '[ 0.18115975 -0.9049084  -1.46773425  1.88057324]', '[-0.14695399 -0.40537485 -1.74907334  3.01133866]', '[-0.48375719  0.2336853  -1.52316125  3.18837973]', '[-0.69639617  0.73712268 -0.56101418  1.77040262]', '[-0.70241733  0.93105368  0.49566974  0.16138651]', '[-0.50558683  0.80081288  1.44064211 -1.45449374]', '[-0.16982711  0.42842004  1.84768486 -2.17755789]', '[ 0.19849091 -0.01483323  1.7438746  -2.09990669]', '[ 0.51895871 -0.42029197  1.38666948 -1.83426516]', '[ 0.70495893 -0.64966245  0.44377197 -0.43001946]', '[ 0.691082   -0.58913629 -0.58048168  1.02968846]', '[ 0.50538564 -0.31307684 -1.23958156  1.67801913]', '[ 0.21696787  0.04845889 -1.57712005  1.82800203]', '[-0.09464356  0.36807535 -1.46629106  1.25916745]', '[-0.36831304  0.58253796 -1.21177184  0.81516869]', '[-0.55955668  0.67444278 -0.66583774  0.07943972]', '[-0.60063219  0.54697491  0.26268091 -1.34358231]', '[-0.45846722  0.14953348  1.12409272 -2.55991356]', '[-0.20239907 -0.35901588  1.36660375 -2.38799241]', '[ 0.08565685 -0.81857204  1.44743138 -2.08965013]', '[ 0.35272779 -1.15839852  1.17453029 -1.25112946]', '[ 0.51821618 -1.25080413  0.44869462  0.33836998]', '[ 0.54294955 -1.07556645 -0.21153246  1.40982847]', '[ 0.41085794 -0.63185616 -1.09642314  3.00103179]', '[ 0.14969821  0.02085663 -1.42796109  3.35148998]', '[-0.12081737  0.62821278 -1.20149414  2.57083738]', '[-0.33316956  1.07215684 -0.88229483  1.80320392]', '[-0.4429514   1.28097428 -0.20588589  0.28173928]', '[-0.41333365  1.18423828  0.5025006  -1.25029471]', '[-0.26620869  0.84053202  0.94634015 -2.15355576]', '[-0.04962041  0.34821573  1.16539533 -2.66671448]', '[ 0.17161394 -0.169559    0.97687967 -2.36808492]', '[ 0.31728795 -0.5505638   0.44397329 -1.36823003]', '[ 0.34202587 -0.70099655 -0.19849191 -0.12283594]', '[ 0.2414831  -0.60065751 -0.78724827  1.10662655]', '[ 0.06497106 -0.34112636 -0.93658764  1.42297827]', '[-0.11426736 -0.06333594 -0.81009979  1.27563152]', '[-0.24208441  0.13952343 -0.43663181  0.69903223]', '[-0.28024502  0.20170459  0.06341572 -0.09111282]', '[-0.24417145  0.17300709  0.28924921 -0.18585086]', '[-0.1431672   0.06480166  0.69718679 -0.86275281]', '[ 0.02118065 -0.15126525  0.90550241 -1.23224997]', '[ 0.20066827 -0.39800544  0.84568661 -1.16474122]', '[ 0.34331294 -0.59209875  0.54960385 -0.73098368]', '[ 0.41111408 -0.6777762   0.11525112 -0.10976238]', '[ 0.38752659 -0.63406191 -0.34598437  0.53914165]', '[ 0.25337018 -0.40466246 -0.96898614  1.71520136]', '[ 0.01754105  0.0222998  -1.32740648  2.44063761]', '[-0.24702002  0.51335886 -1.24547803  2.3329838 ]', '[-0.45580603  0.91138681 -0.80036654  1.58067918]', '[-0.55613849  1.1308025  -0.18912194  0.59689617]', '[-0.52985347  1.14754378  0.44594102 -0.4283377 ]', '[-0.38374056  0.9626152   0.99077258 -1.40122545]', '[-0.12385301  0.53963105  1.56394121 -2.7692418 ]', '[ 0.18763584 -0.02822259  1.4628113  -2.73910985]', '[ 0.45271921 -0.55644925  1.11573193 -2.40621472]', '[ 0.58937943 -0.89133658  0.2329529  -0.91489557]', '[ 0.56700167 -0.97847844 -0.4513222   0.04857282]', '[ 0.41539147 -0.87344432 -1.03726763  0.98464843]', '[ 0.1439511  -0.53556322 -1.62734242  2.33621425]', '[-0.18134007 -0.05093802 -1.54172431  2.35903907]', '[-0.46577921  0.41521638 -1.23019273  2.17172107]', '[-0.62575872  0.71424395 -0.343432    0.7817503 ]', '[-0.6228816   0.78491213  0.37171111 -0.08187916]', '[-0.45827741  0.61983894  1.24715217 -1.54961066]', '[-0.1420493   0.18545133  1.84639792 -2.68804931]', '[ 0.242083   -0.38699417  1.89145934 -2.84431382]', '[ 0.55229346 -0.82217354  1.15479755 -1.43447589]', '[ 0.71237074 -1.00939773  0.42174263 -0.42206814]', '[ 0.71593634 -0.98910074 -0.38649077  0.62314107]', '[ 0.56206846 -0.76313944 -1.12809357  1.61518071]', '[ 0.28073783 -0.36165014 -1.62633062  2.31314454]', '[-0.05674135  0.10883693 -1.66156657  2.23886048]', '[-0.37542239  0.54122659 -1.44860328  1.95780468]', '[-0.61091395  0.85450715 -0.86327849  1.12349318]', '[-0.70927322  0.98036855 -0.10597983  0.12594658]', '[-0.62965394  0.84463802  0.89331219 -1.47976127]', '[-0.38565299  0.46000621  1.49925814 -2.30027728]', '[-0.03148254 -0.09788798  1.95067728 -3.11096516]', '[ 0.325251   -0.63484561  1.53341773 -2.1151967 ]', '[ 0.58133577 -0.97228184  0.9818473  -1.20767769]', '[ 0.70525557 -1.10820132  0.23923302 -0.14363348]', '[ 0.65250685 -0.97179547 -0.76385301  1.50742239]', '[ 0.42958222 -0.57127355 -1.42519356  2.4434739 ]', '[ 0.08177496  0.03172712 -1.96280826  3.41961835]', '[-0.30855137  0.70408825 -1.83445388  3.10173392]', '[-0.61990076  1.21907218 -1.22980073  1.99079119]', '[-0.76874293  1.44144691 -0.2456563   0.24279698]', '[-0.71563512  1.31735668  0.77515688 -1.48961835]', '[-0.4838197   0.89867721  1.51228521 -2.67323236]', '[-0.13179353  0.27606216  1.92540081 -3.40870542]', '[ 0.26739577 -0.44492907  1.94530535 -3.56030582]', '[ 0.58086087 -1.00736504  1.139048   -1.99430629]', '[ 0.73324525 -1.2921038   0.36642448 -0.8421916 ]', '[ 0.72446644 -1.34301221 -0.4505597   0.33381779]', '[ 0.53866315 -1.10391273 -1.38627022  2.06081419]', '[ 0.18283571 -0.52347361 -2.11672672  3.67304175]', '[-0.26762104  0.29093696 -2.24855364  4.18829805]', '[-0.63785097  0.98014282 -1.38523579  2.59367819]', '[-0.80987635  1.32076064 -0.32461135  0.82147982]', '[-0.7862473   1.36439216  0.55532353 -0.38673955]', '[-0.59418654  1.16519652  1.33800067 -1.60092693]', '[-0.2446401   0.67224722  2.1078571  -3.28420943]', '[ 0.21544439 -0.09429906  2.36688075 -4.13251087]', '[ 0.643399   -0.86165438  1.80560993 -3.34228886]', '[ 0.9127629  -1.39730905  0.8589631  -2.00008079]', '[ 0.9817382  -1.66415833 -0.170305   -0.67292079]', '[ 0.84855813 -1.66527674 -1.13955381  0.66984859]', '[ 0.52239547 -1.34197857 -2.08041025  2.57848406]', '[ 0.05776375 -0.69494728 -2.48937683  3.79229363]', '[-0.45394967  0.15793115 -2.48454693  4.43930467]', '[-0.87588473  0.95740936 -1.64082361  3.38926957]', '[-1.09207764  1.49500927 -0.50409242  1.98965371]']</t>
-  </si>
-  <si>
-    <t>[array([-0.03763371, -0.01533471,  0.06554052, -0.01816017], dtype=float32), array([-0.03406929,  0.01398622, -0.02953871,  0.30651903]), array([-0.02168374,  0.03409236,  0.1512214 , -0.10649158]), array([ 0.02369474, -0.02529386,  0.2912986 , -0.46969041]), array([ 0.06234371, -0.07501275,  0.08617182, -0.01368346]), array([ 0.08315347, -0.09791055,  0.11692115, -0.20796639]), array([ 0.08020517, -0.08541727, -0.14509226,  0.32970125]), array([ 0.02823683,  0.02775306, -0.36024318,  0.77393063]), array([-0.05588226,  0.20852011, -0.4576235 ,  0.98818913]), array([-0.11871774,  0.3359788 , -0.15597939,  0.25913082]), array([-0.14114303,  0.37431915, -0.06288902,  0.11508823]), array([-0.14258595,  0.37975756,  0.04874616, -0.06153168]), array([-0.09670323,  0.2839622 ,  0.39900417, -0.87594373]), array([ 0.00905309,  0.0447265 ,  0.6299373 , -1.45962888]), array([ 0.14061973, -0.27033256,  0.6469136 , -1.61170491]), array([ 0.25246041, -0.56854806,  0.44121773, -1.30762249]), array([ 0.28434358, -0.7113844 , -0.12568236, -0.10750594]), array([ 0.22857073, -0.67537935, -0.42028491,  0.45613931]), array([ 0.12334762, -0.53763514, -0.60889086,  0.88877377]), array([-0.02934395, -0.27067471, -0.88336674,  1.72160332]), array([-0.18535329,  0.04856985, -0.63356736,  1.38697206]), array([-0.26845735,  0.2559289 , -0.17580569,  0.6417687 ]), array([-0.27753233,  0.36264871,  0.08978857,  0.40697523]), array([-0.20738751,  0.34747952,  0.59669407, -0.54664926]), array([-0.07533821,  0.22443992,  0.69365146, -0.64331462]), array([ 0.08337926,  0.03974713,  0.85566527, -1.14670364]), array([ 0.22335904, -0.13821957,  0.51103408, -0.5814825 ]), array([ 0.3044938 , -0.24697832,  0.28142104, -0.47685731]), array([ 0.33030559, -0.31944117, -0.03005804, -0.23311507]), array([ 0.26641035, -0.26999224, -0.59497487,  0.71177245]), array([ 0.10294594, -0.04971013, -1.00054681,  1.42947944]), array([-0.08712675,  0.19969288, -0.85393386,  0.99043171]), array([-0.22232113,  0.32232613, -0.46860563,  0.19884495]), array([-0.29253623,  0.33887386, -0.21981513, -0.04450158]), array([-0.28081766,  0.23538886,  0.3323012 , -0.97296302]), array([-0.19322385,  0.03391515,  0.51934244, -0.99351627]), array([-0.08420054, -0.14135895,  0.54361303, -0.71226949]), array([ 0.03983134, -0.30209283,  0.66631305, -0.84694474]), array([ 0.14356628, -0.39333941,  0.34867355, -0.03833912]), array([ 0.19906704, -0.37953004,  0.19576272,  0.18171402]), array([ 0.19305706, -0.25351841, -0.25222191,  1.05894411]), array([ 0.10430604,  0.02785392, -0.60739614,  1.69139581]), array([-0.00837033,  0.32195738, -0.48790205,  1.18293312]), array([-0.10616067,  0.54658455, -0.46487483,  1.01373785]), array([-0.18526973,  0.71040679, -0.3089262 ,  0.5936578 ]), array([-0.20079648,  0.71313016,  0.15672725, -0.56818555]), array([-0.14869987,  0.55177361,  0.3522018 , -1.01855717]), array([-0.04125518,  0.25432511,  0.69618905, -1.90011008]), array([ 0.11355379, -0.17367054,  0.80136684, -2.27172065]), array([ 0.23230238, -0.54194   ,  0.35517723, -1.34146245]), array([ 0.2735389 , -0.75798832,  0.04745859, -0.78886463]), array([ 0.25058597, -0.85068539, -0.27091347, -0.13380621]), array([ 0.14712054, -0.75256327, -0.74356624,  1.09599204]), array([-0.01132386, -0.49094451, -0.80542582,  1.46156204]), array([-0.1851566 , -0.12916707, -0.88933812,  2.07188869]), array([-0.31997474,  0.22742026, -0.41919893,  1.40976431]), array([-0.34279906,  0.41150659,  0.19791623,  0.40348982]), array([-0.24356394,  0.38624397,  0.77374282, -0.64016313]), array([-0.04654728,  0.17058915,  1.15157269, -1.45326081]), array([ 0.16810876, -0.09113787,  0.94280995, -1.08141426]), array([ 0.33868847, -0.3024337 ,  0.72321479, -0.97082926]), array([ 0.44389114, -0.45893982,  0.30587352, -0.55934094]), array([ 0.45546091, -0.517099  , -0.19302747, -0.01362165]), array([ 0.36935181, -0.46536284, -0.65103355,  0.51525189]), array([ 0.18011983, -0.25575809, -1.20051855,  1.52684619]), array([-0.06182888,  0.04215675, -1.1595688 ,  1.357173  ]), array([-0.26079418,  0.25137737, -0.78479417,  0.67050503]), array([-0.36181597,  0.29306036, -0.20566181, -0.27088047]), array([-0.34015764,  0.14409663,  0.41389263, -1.19212142]), array([-0.20559259, -0.1632966 ,  0.89368565, -1.80521951]), array([-0.00273104, -0.53880892,  1.08183182, -1.84991706]), array([ 0.20615756, -0.86610793,  0.96278512, -1.35331091]), array([ 0.36713917, -1.05987501,  0.61747341, -0.55326954]), array([ 0.44373447, -1.07990462,  0.13329322,  0.36060098]), array([ 0.39498981, -0.85695716, -0.62178325,  1.86345862]), array([ 0.22534922, -0.40982398, -1.03321681,  2.52790279]), array([-0.02014606,  0.17365492, -1.34261325,  3.14611632]), array([-0.25086115,  0.71052285, -0.90806524,  2.11225656]), array([-0.39268549,  1.05528278, -0.48589787,  1.29427216]), array([-0.43983353,  1.21969295,  0.01809109,  0.34168767]), array([-0.36675593,  1.13657528,  0.7014129 , -1.16810863]), array([-0.18820198,  0.81595806,  1.05362973, -1.99725772]), array([ 0.06284761,  0.29980223,  1.40268726, -3.06475668]), array([ 0.34012518, -0.34457287,  1.27801053, -3.19149084]), array([ 0.54055141, -0.91030761,  0.6751997 , -2.3675353 ]), array([ 0.58018493, -1.21660388, -0.26931275, -0.69681752]), array([ 0.44145205, -1.19147953, -1.08797896,  0.93955925]), array([ 0.18115975, -0.9049084 , -1.46773425,  1.88057324]), array([-0.14695399, -0.40537485, -1.74907334,  3.01133866]), array([-0.48375719,  0.2336853 , -1.52316125,  3.18837973]), array([-0.69639617,  0.73712268, -0.56101418,  1.77040262]), array([-0.70241733,  0.93105368,  0.49566974,  0.16138651]), array([-0.50558683,  0.80081288,  1.44064211, -1.45449374]), array([-0.16982711,  0.42842004,  1.84768486, -2.17755789]), array([ 0.19849091, -0.01483323,  1.7438746 , -2.09990669]), array([ 0.51895871, -0.42029197,  1.38666948, -1.83426516]), array([ 0.70495893, -0.64966245,  0.44377197, -0.43001946]), array([ 0.691082  , -0.58913629, -0.58048168,  1.02968846]), array([ 0.50538564, -0.31307684, -1.23958156,  1.67801913]), array([ 0.21696787,  0.04845889, -1.57712005,  1.82800203]), array([-0.09464356,  0.36807535, -1.46629106,  1.25916745]), array([-0.36831304,  0.58253796, -1.21177184,  0.81516869]), array([-0.55955668,  0.67444278, -0.66583774,  0.07943972]), array([-0.60063219,  0.54697491,  0.26268091, -1.34358231]), array([-0.45846722,  0.14953348,  1.12409272, -2.55991356]), array([-0.20239907, -0.35901588,  1.36660375, -2.38799241]), array([ 0.08565685, -0.81857204,  1.44743138, -2.08965013]), array([ 0.35272779, -1.15839852,  1.17453029, -1.25112946]), array([ 0.51821618, -1.25080413,  0.44869462,  0.33836998]), array([ 0.54294955, -1.07556645, -0.21153246,  1.40982847]), array([ 0.41085794, -0.63185616, -1.09642314,  3.00103179]), array([ 0.14969821,  0.02085663, -1.42796109,  3.35148998]), array([-0.12081737,  0.62821278, -1.20149414,  2.57083738]), array([-0.33316956,  1.07215684, -0.88229483,  1.80320392]), array([-0.4429514 ,  1.28097428, -0.20588589,  0.28173928]), array([-0.41333365,  1.18423828,  0.5025006 , -1.25029471]), array([-0.26620869,  0.84053202,  0.94634015, -2.15355576]), array([-0.04962041,  0.34821573,  1.16539533, -2.66671448]), array([ 0.17161394, -0.169559  ,  0.97687967, -2.36808492]), array([ 0.31728795, -0.5505638 ,  0.44397329, -1.36823003]), array([ 0.34202587, -0.70099655, -0.19849191, -0.12283594]), array([ 0.2414831 , -0.60065751, -0.78724827,  1.10662655]), array([ 0.06497106, -0.34112636, -0.93658764,  1.42297827]), array([-0.11426736, -0.06333594, -0.81009979,  1.27563152]), array([-0.24208441,  0.13952343, -0.43663181,  0.69903223]), array([-0.28024502,  0.20170459,  0.06341572, -0.09111282]), array([-0.24417145,  0.17300709,  0.28924921, -0.18585086]), array([-0.1431672 ,  0.06480166,  0.69718679, -0.86275281]), array([ 0.02118065, -0.15126525,  0.90550241, -1.23224997]), array([ 0.20066827, -0.39800544,  0.84568661, -1.16474122]), array([ 0.34331294, -0.59209875,  0.54960385, -0.73098368]), array([ 0.41111408, -0.6777762 ,  0.11525112, -0.10976238]), array([ 0.38752659, -0.63406191, -0.34598437,  0.53914165]), array([ 0.25337018, -0.40466246, -0.96898614,  1.71520136]), array([ 0.01754105,  0.0222998 , -1.32740648,  2.44063761]), array([-0.24702002,  0.51335886, -1.24547803,  2.3329838 ]), array([-0.45580603,  0.91138681, -0.80036654,  1.58067918]), array([-0.55613849,  1.1308025 , -0.18912194,  0.59689617]), array([-0.52985347,  1.14754378,  0.44594102, -0.4283377 ]), array([-0.38374056,  0.9626152 ,  0.99077258, -1.40122545]), array([-0.12385301,  0.53963105,  1.56394121, -2.7692418 ]), array([ 0.18763584, -0.02822259,  1.4628113 , -2.73910985]), array([ 0.45271921, -0.55644925,  1.11573193, -2.40621472]), array([ 0.58937943, -0.89133658,  0.2329529 , -0.91489557]), array([ 0.56700167, -0.97847844, -0.4513222 ,  0.04857282]), array([ 0.41539147, -0.87344432, -1.03726763,  0.98464843]), array([ 0.1439511 , -0.53556322, -1.62734242,  2.33621425]), array([-0.18134007, -0.05093802, -1.54172431,  2.35903907]), array([-0.46577921,  0.41521638, -1.23019273,  2.17172107]), array([-0.62575872,  0.71424395, -0.343432  ,  0.7817503 ]), array([-0.6228816 ,  0.78491213,  0.37171111, -0.08187916]), array([-0.45827741,  0.61983894,  1.24715217, -1.54961066]), array([-0.1420493 ,  0.18545133,  1.84639792, -2.68804931]), array([ 0.242083  , -0.38699417,  1.89145934, -2.84431382]), array([ 0.55229346, -0.82217354,  1.15479755, -1.43447589]), array([ 0.71237074, -1.00939773,  0.42174263, -0.42206814]), array([ 0.71593634, -0.98910074, -0.38649077,  0.62314107]), array([ 0.56206846, -0.76313944, -1.12809357,  1.61518071]), array([ 0.28073783, -0.36165014, -1.62633062,  2.31314454]), array([-0.05674135,  0.10883693, -1.66156657,  2.23886048]), array([-0.37542239,  0.54122659, -1.44860328,  1.95780468]), array([-0.61091395,  0.85450715, -0.86327849,  1.12349318]), array([-0.70927322,  0.98036855, -0.10597983,  0.12594658]), array([-0.62965394,  0.84463802,  0.89331219, -1.47976127]), array([-0.38565299,  0.46000621,  1.49925814, -2.30027728]), array([-0.03148254, -0.09788798,  1.95067728, -3.11096516]), array([ 0.325251  , -0.63484561,  1.53341773, -2.1151967 ]), array([ 0.58133577, -0.97228184,  0.9818473 , -1.20767769]), array([ 0.70525557, -1.10820132,  0.23923302, -0.14363348]), array([ 0.65250685, -0.97179547, -0.76385301,  1.50742239]), array([ 0.42958222, -0.57127355, -1.42519356,  2.4434739 ]), array([ 0.08177496,  0.03172712, -1.96280826,  3.41961835]), array([-0.30855137,  0.70408825, -1.83445388,  3.10173392]), array([-0.61990076,  1.21907218, -1.22980073,  1.99079119]), array([-0.76874293,  1.44144691, -0.2456563 ,  0.24279698]), array([-0.71563512,  1.31735668,  0.77515688, -1.48961835]), array([-0.4838197 ,  0.89867721,  1.51228521, -2.67323236]), array([-0.13179353,  0.27606216,  1.92540081, -3.40870542]), array([ 0.26739577, -0.44492907,  1.94530535, -3.56030582]), array([ 0.58086087, -1.00736504,  1.139048  , -1.99430629]), array([ 0.73324525, -1.2921038 ,  0.36642448, -0.8421916 ]), array([ 0.72446644, -1.34301221, -0.4505597 ,  0.33381779]), array([ 0.53866315, -1.10391273, -1.38627022,  2.06081419]), array([ 0.18283571, -0.52347361, -2.11672672,  3.67304175]), array([-0.26762104,  0.29093696, -2.24855364,  4.18829805]), array([-0.63785097,  0.98014282, -1.38523579,  2.59367819]), array([-0.80987635,  1.32076064, -0.32461135,  0.82147982]), array([-0.7862473 ,  1.36439216,  0.55532353, -0.38673955]), array([-0.59418654,  1.16519652,  1.33800067, -1.60092693]), array([-0.2446401 ,  0.67224722,  2.1078571 , -3.28420943]), array([ 0.21544439, -0.09429906,  2.36688075, -4.13251087]), array([ 0.643399  , -0.86165438,  1.80560993, -3.34228886]), array([ 0.9127629 , -1.39730905,  0.8589631 , -2.00008079]), array([ 0.9817382 , -1.66415833, -0.170305  , -0.67292079]), array([ 0.84855813, -1.66527674, -1.13955381,  0.66984859]), array([ 0.52239547, -1.34197857, -2.08041025,  2.57848406]), array([ 0.05776375, -0.69494728, -2.48937683,  3.79229363]), array([-0.45394967,  0.15793115, -2.48454693,  4.43930467]), array([-0.87588473,  0.95740936, -1.64082361,  3.38926957]), array([-1.09207764,  1.49500927, -0.50409242,  1.98965371])]</t>
-  </si>
-  <si>
-    <t>['[1,1,2]', '[2,2,2]', '[0,0,0]', '[1,0,2]', '[0,1,1]', '[1,1,1]', '[1,2,0]', '[0,2,1]', '[2,0,1]', '[2,1,0]']</t>
-  </si>
-  <si>
-    <t>[3, 4, 5, 7, 8, 9, 10, 11, 12, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 26, 27, 28, 29, 31, 32, 33, 34, 36, 37, 39, 41, 44, 45, 46, 47, 48, 49, 50, 52, 55, 58, 61, 62, 63, 65, 66, 69, 72, 73, 75, 76, 78, 79, 80, 84, 85, 86, 88, 89, 90, 91, 92, 94, 96, 97, 99, 100, 103, 105, 106, 107, 108, 111, 112, 114, 115, 116, 117, 118, 119, 120, 122, 123, 124, 125, 126, 127, 129, 130, 132, 133, 134, 135, 137, 140, 142, 143, 144, 145, 146, 148, 150, 151, 153, 154, 156, 157, 158, 159, 160, 161, 163, 166, 167, 168, 170, 172, 173, 174, 175, 177, 178, 179, 181, 183, 184, 186, 188, 189, 190, 192, 194, 195, 197, 198]</t>
-  </si>
-  <si>
-    <t>[0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 2, 0, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 2, 0, 0, 2, 2, 0, 2, 2, 2, 0, 0, 0, 0, 2, 2, 2, 2, 0, 0, 0, 0, 2, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 0, 2, 0, 2, 2, 2, 2, 0, 2, 0, 2, 0, 0, 2, 0, 0, 2, 2, 0, 2, 2, 2, 2, 2, 0, 0, 0, 0, 2, 2, 0, 0, 2, 2, 2, 0, 0, 2, 2, 2, 2, 2, 0, 2, 0, 2, 2, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 2, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 2, 2, 0, 0, 2, 0, 0, 2, 0]</t>
-  </si>
-  <si>
-    <t>['[-0.03763371 -0.01533471  0.06554052 -0.01816017]', '[-0.00754409 -0.05458322  0.2277812  -0.36241836]', '[ 0.04879627 -0.15231473  0.32089719 -0.5887683 ]', '[ 0.08773348 -0.20975891  0.05953656  0.02857539]', '[ 0.09792676 -0.20849115  0.0403974  -0.01458167]', '[ 0.10319253 -0.21489219  0.01102434 -0.04756012]', '[ 0.07575154 -0.15868056 -0.27814597  0.59601827]', '[ 0.02425559 -0.05621935 -0.22315334  0.40290993]', '[-0.00873665 -0.00612543 -0.09869521  0.08461503]', '[-0.01333894 -0.02488449  0.05278641 -0.26923419]', '[-0.0156612  -0.0408907  -0.07580422  0.11112187]', '[-0.0156436  -0.05143572  0.07541816 -0.21432283]', '[-0.01375493 -0.05420014 -0.0567779   0.18700115]', '[-0.03699406  0.02013404 -0.16840698  0.5395803 ]', '[-0.07692135  0.1518807  -0.21825401  0.7482833 ]', '[-0.09249148  0.23820541  0.0672838   0.09988517]', '[-0.07709145  0.2591799   0.08423165  0.10865617]', '[-0.05991745  0.28123621  0.08467411  0.11085791]', '[-0.04436204  0.3031078   0.06833988  0.10667223]', '[-0.03348068  0.323379    0.03881437  0.09445982]', '[-0.02928625  0.34017464  0.00272679  0.07146705]', '[-0.03229303  0.35108742 -0.03188038  0.0354389 ]', '[-0.04143571  0.35347739 -0.05759084 -0.01338443]', '[-0.05439244  0.34514441 -0.06952179 -0.07067053]', '[-0.06822909  0.32521177 -0.06654727 -0.12759329]', '[-0.05409039  0.22741074  0.20304013 -0.83347011]', '[-0.01840746  0.07323544  0.14134676 -0.67566505]', '[-0.00180873 -0.03127606  0.01804543 -0.34898028]', '[-0.01241602 -0.06117047 -0.12261825  0.05303101]', '[-0.02222411 -0.08081856  0.02567459 -0.24721449]', '[-0.00319512 -0.15628403  0.15811458 -0.49096954]', '[ 0.01088885 -0.20031001 -0.0208919   0.05923748]', '[ 0.01519877 -0.20165522  0.0629646  -0.07159276]', '[ 0.0348697  -0.22717215  0.12888607 -0.17600936]', '[ 0.03798335 -0.20015524 -0.09752899  0.44192098]', '[-0.00173301 -0.05715783 -0.28725191  0.95767043]', '[-0.04317062  0.09729487 -0.11392217  0.55395507]', '[-0.04402753  0.15529441  0.10672427  0.01704098]', '[-0.00217854  0.1051334   0.30159419 -0.50343872]', '[ 0.04396466  0.03306459  0.14839435 -0.19789589]', '[ 0.08069857 -0.03783558  0.20916876 -0.49293076]', '[ 0.09643731 -0.08607493 -0.05600724  0.02040253]', '[ 0.05920628 -0.03053644 -0.30677897  0.51926703]', '[-0.01994126  0.11055231 -0.46382371  0.85403913]', '[-0.09010794  0.22493827 -0.22103415  0.26142634]', '[-0.10413365  0.20900194  0.0829352  -0.41969577]', '[-0.08545438  0.13159954  0.0975878  -0.3381029 ]', '[-0.06761209  0.07978873  0.07561774 -0.16839821]', '[-0.05690988  0.06760656  0.0289524   0.05011803]', '[-0.05639024  0.09952586 -0.02272133  0.26336575]', '[-0.03851575  0.10059463  0.19752221 -0.24951204]', '[ 0.01881504  0.00550458  0.36103962 -0.67582697]', '[ 0.07172212 -0.08715758  0.15479673 -0.22735752]', '[ 0.10404108 -0.14870996  0.15985741 -0.3724327 ]', '[ 0.1320584  -0.22889478  0.11216451 -0.41142267]', '[ 0.11991945 -0.23852568 -0.23078934  0.31395661]', '[ 0.04404593 -0.10985908 -0.5089282   0.93990939]', '[-0.0729905   0.11805531 -0.62977399  1.27974473]', '[-0.16774234  0.30765261 -0.2945331   0.57318712]', '[-0.21085378  0.40402405 -0.12567678  0.36946562]', '[-0.21521753  0.44934272  0.08367388  0.07668347]', '[-0.17856619  0.43462117  0.27498553 -0.216357  ]', '[-0.11007269  0.36855471  0.39443812 -0.42389393]', '[-0.0281642   0.27538038  0.40543059 -0.47986604]', '[ 0.07049462  0.12035963  0.55700398 -1.02974768]', '[ 0.15646715 -0.04668436  0.28025721 -0.5985245 ]', '[ 0.176435   -0.10711332 -0.08583662  0.00645378]', '[ 0.12346885 -0.04508383 -0.43095796  0.59476002]', '[ 0.01255521  0.11717354 -0.65014826  0.98121302]', '[-0.09698827  0.25697703 -0.41982302  0.37824215]', '[-0.17375426  0.32601462 -0.33058515  0.2896014 ]', '[-0.22318882  0.36510332 -0.15316196  0.08860094]', '[-0.23234513  0.35858619  0.06297857 -0.15354926]', '[-0.19929554  0.30629403  0.25938176 -0.3561389 ]', '[-0.10737539  0.15591787  0.63752344 -1.11038486]', '[ 0.01621026 -0.04640711  0.56663967 -0.85759963]', '[ 0.10766338 -0.16761575  0.32625276 -0.32084153]', '[ 0.16690343 -0.2344726   0.25230145 -0.32762908]', '[ 0.1775002  -0.2234109  -0.14776475  0.43717355]', '[ 0.13734173 -0.13497516 -0.24289438  0.42593277]', '[ 0.08542344 -0.06202963 -0.26352965  0.283051  ]', '[ 0.01049144  0.03946324 -0.46715708  0.70217463]', '[-0.09188378  0.20284372 -0.53037067  0.88655055]', '[-0.19059715  0.37482501 -0.43199384  0.78996882]', '[-0.23057853  0.43754789  0.04017522 -0.17471302]', '[-0.2008708   0.37365647  0.24929029 -0.45004286]', '[-0.1357957   0.26606852  0.38533942 -0.59870538]', '[-0.02813708  0.07884055  0.66411917 -1.22599357]', '[ 0.08924464 -0.13000191  0.47937528 -0.80775223]', '[ 0.15376334 -0.22715294  0.15083686 -0.13961369]', '[ 0.1467582  -0.18217512 -0.21802143  0.58058166]', '[ 0.09773644 -0.07342501 -0.2587792   0.4805709 ]', '[ 4.87795882e-02 -3.66950677e-05 -2.18666751e-01  2.33269467e-01]', '[-0.01202302  0.08233701 -0.3741831   0.5662341 ]', '[-0.06684011  0.14538806 -0.16141121  0.0460557 ]', '[-0.10017104  0.16633802 -0.16450156  0.1547032 ]', '[-0.10318317  0.13488393  0.13380737 -0.46388645]', '[-0.07633198  0.05704003  0.1267964  -0.2969932 ]', '[-0.02882449 -0.04665003  0.33509499 -0.71407228]', '[ 0.02388423 -0.14586056  0.17870928 -0.25380261]', '[ 0.03909173 -0.14245659 -0.02936555  0.28903832]', '[ 0.01319187 -0.03434263 -0.22092298  0.76935858]', '[-0.04361051  0.1516476  -0.32890121  1.04814884]', '[-0.08391642  0.2980198  -0.06309827  0.38767072]', '[-0.09308405  0.36849874 -0.02488512  0.30445859]', '[-0.06719048  0.34889236  0.27777802 -0.49328453]', '[-0.01323782  0.24763946  0.24793079 -0.49409428]', '[ 0.02664176  0.16127859  0.14020839 -0.34863513]', '[ 0.03958783  0.11495232 -0.01464761 -0.10492488]', '[ 0.04719303  0.05220956  0.08718742 -0.5104512 ]', '[ 0.07175734 -0.08107559  0.14890215 -0.79493202]', '[ 0.07574879 -0.18428204 -0.11223329 -0.22022567]', '[ 0.0544884  -0.23564311 -0.09775357 -0.28770953]', '[ 0.01145627 -0.2289309  -0.32312195  0.34645073]', '[-0.04242564 -0.17362815 -0.20318328  0.18878126]', '[-0.06593673 -0.15877678 -0.02690927 -0.04620391]', '[-0.05282333 -0.19188732  0.15412505 -0.27676059]', '[-0.03376005 -0.19572871  0.03266959  0.24154268]', '[-0.01349815 -0.16605586  0.16659572  0.05359799]', '[ 0.00386688 -0.10465634  0.00534527  0.55257775]', '[ 0.01636354 -0.02098193  0.11974131  0.27166787]', '[ 0.02403865  0.07015247 -0.04126912  0.62439936]', '[0.0286078  0.15107692 0.08802442 0.17263981]', '[ 0.05816017  0.13801523  0.20087285 -0.2960441 ]', '[ 0.07852975  0.1075583  -0.00200816 -0.00048646]', '[ 0.08381158  0.06944562  0.0525694  -0.37320366]', '[ 0.07128457  0.03256997 -0.17618257  0.00835987]', '[ 0.04273676  0.0019615  -0.10460317 -0.3132578 ]', '[ 0.03036027 -0.08967082 -0.01991602 -0.58848068]', '[ 0.00712498 -0.15701659 -0.20920561 -0.07802518]', '[-0.02367854 -0.19068191 -0.09381399 -0.25738594]', '[-0.02948993 -0.25765176  0.03467521 -0.40165135]', '[-0.03730005 -0.27807059 -0.11117394  0.19854585]', '[-0.04563318 -0.24977547  0.03018852  0.07862596]', '[-0.02551568 -0.24731223  0.16677914 -0.05086185]', '[-0.00802883 -0.19942707  0.00560847  0.52480135]', '[-0.02240653 -0.04392128 -0.14161286  1.00143825]', '[-0.03307026  0.11658006  0.04229686  0.57423733]', '[-0.03098824  0.24642418 -0.01732748  0.70149104]', '[-0.03783378  0.3871596  -0.0455843   0.68156952]', '[-0.02183368  0.44387918  0.20178533 -0.11756309]', '[ 0.03933335  0.34388033  0.39604534 -0.85964177]', '[ 0.10270398  0.18266209  0.22006872 -0.71531027]', '[ 0.12178501  0.0707735  -0.03647514 -0.38164762]', '[ 0.08762346  0.03503015 -0.29906353  0.02451685]', '[ 0.03361564  0.00797337 -0.23106268 -0.29839984]', '[-0.00177238 -0.08304651 -0.11901499 -0.60065606]', '[-0.01377995 -0.22508752 -0.00389372 -0.7960082 ]', '[-0.03127521 -0.32306099 -0.16865238 -0.17313444]', '[-0.07849863 -0.294687   -0.29294514  0.44459208]', '[-0.1166887  -0.22215399 -0.07932225  0.26275268]', '[-0.10823277 -0.19429194  0.16269637  0.01308519]', '[-0.05423448 -0.21495717  0.36539975 -0.20696789]', '[ 0.00509123 -0.20152013  0.21599521  0.34825825]', '[ 0.05558965 -0.14550822  0.28058101  0.20997138]', '[ 0.08682915 -0.04865872  0.02878146  0.74606869]', '[0.095121   0.07423288 0.05648523 0.4628442 ]', '[0.10965234 0.13079016 0.08727423 0.09603803]', '[ 0.12878672  0.11249642  0.09959407 -0.27272358]', '[ 0.12075111  0.09507036 -0.17852774  0.09958378]', '[ 0.08699502  0.08027504 -0.15265098 -0.25014572]', '[ 0.03512387  0.064947   -0.35579416  0.09097164]', '[-0.04925183  0.11088237 -0.46922043  0.34688739]', '[-0.11750429  0.12456336 -0.19941095 -0.22193883]', '[-0.12616575  0.02254159  0.11097928 -0.78140449]', '[-0.07703537 -0.17557372  0.36298763 -1.15605305]', '[-0.01611532 -0.35130997  0.23056727 -0.56620137]', '[ 0.01070195 -0.39282725  0.03189078  0.16001533]', '[ 0.02195961 -0.35534605  0.07918284  0.21091746]', '[ 0.01542502 -0.24272938 -0.14124325  0.8978669 ]', '[-0.00407565 -0.07753052 -0.04408264  0.72194121]', '[-0.02583575  0.10345566 -0.16241357  1.05174946]', '[-0.0370435   0.25783115  0.05628304  0.46606644]', '[-0.00349269  0.28484522  0.27223561 -0.19381187]', '[ 0.0408288   0.25385972  0.16114237 -0.10388227]', '[0.05800326 0.24690759 0.00706058 0.03806569]', '[ 0.06979008  0.20089627  0.10730736 -0.48902186]', '[ 0.07181345  0.12712466 -0.08959543 -0.23608778]', '[ 0.03476019  0.10869015 -0.27378416  0.04868611]', '[-0.00660927  0.07404024 -0.13267308 -0.39531154]', '[-0.01706433 -0.04569406  0.02595816 -0.78209525]', '[-0.02524778 -0.15890057 -0.10920445 -0.33268314]', '[-0.03339808 -0.24379828  0.02647591 -0.50273413]', '[-0.04227722 -0.28540274 -0.11377093  0.09061994]', '[-0.05073968 -0.27775384  0.03093565 -0.01654149]', '[-0.05656635 -0.22376357 -0.08689385  0.54726606]', '[-0.05669308 -0.13496182  0.08829504  0.32579756]', '[-0.04828904 -0.02850967 -0.00258441  0.72161362]', '[-0.02924681  0.07492393  0.19226734  0.2980881 ]', '[ 0.02622611  0.08891014  0.35127372 -0.15150512]', '[0.07861425 0.08932837 0.16227606 0.16335612]', '[ 0.08885402  0.15411783 -0.05955357  0.47443016]', '[0.08321755 0.20376944 0.00527781 0.01388962]', '[ 0.09092472  0.1595109   0.06909644 -0.44807044]', '[ 0.08232878  0.09962562 -0.15496398 -0.14227732]', '[ 0.05757464  0.03419546 -0.08963317 -0.50446691]', '[ 0.04662805 -0.09621459 -0.02236641 -0.77775933]', '[ 0.02045241 -0.19777677 -0.23645096 -0.2258109 ]', '[-0.0182747  -0.2545142  -0.14484429 -0.33780342]', '[-0.03589383 -0.33023996 -0.02999045 -0.40977672]']</t>
-  </si>
-  <si>
-    <t>[array([-0.03763371, -0.01533471,  0.06554052, -0.01816017], dtype=float32), array([-0.00754409, -0.05458322,  0.2277812 , -0.36241836]), array([ 0.04879627, -0.15231473,  0.32089719, -0.5887683 ]), array([ 0.08773348, -0.20975891,  0.05953656,  0.02857539]), array([ 0.09792676, -0.20849115,  0.0403974 , -0.01458167]), array([ 0.10319253, -0.21489219,  0.01102434, -0.04756012]), array([ 0.07575154, -0.15868056, -0.27814597,  0.59601827]), array([ 0.02425559, -0.05621935, -0.22315334,  0.40290993]), array([-0.00873665, -0.00612543, -0.09869521,  0.08461503]), array([-0.01333894, -0.02488449,  0.05278641, -0.26923419]), array([-0.0156612 , -0.0408907 , -0.07580422,  0.11112187]), array([-0.0156436 , -0.05143572,  0.07541816, -0.21432283]), array([-0.01375493, -0.05420014, -0.0567779 ,  0.18700115]), array([-0.03699406,  0.02013404, -0.16840698,  0.5395803 ]), array([-0.07692135,  0.1518807 , -0.21825401,  0.7482833 ]), array([-0.09249148,  0.23820541,  0.0672838 ,  0.09988517]), array([-0.07709145,  0.2591799 ,  0.08423165,  0.10865617]), array([-0.05991745,  0.28123621,  0.08467411,  0.11085791]), array([-0.04436204,  0.3031078 ,  0.06833988,  0.10667223]), array([-0.03348068,  0.323379  ,  0.03881437,  0.09445982]), array([-0.02928625,  0.34017464,  0.00272679,  0.07146705]), array([-0.03229303,  0.35108742, -0.03188038,  0.0354389 ]), array([-0.04143571,  0.35347739, -0.05759084, -0.01338443]), array([-0.05439244,  0.34514441, -0.06952179, -0.07067053]), array([-0.06822909,  0.32521177, -0.06654727, -0.12759329]), array([-0.05409039,  0.22741074,  0.20304013, -0.83347011]), array([-0.01840746,  0.07323544,  0.14134676, -0.67566505]), array([-0.00180873, -0.03127606,  0.01804543, -0.34898028]), array([-0.01241602, -0.06117047, -0.12261825,  0.05303101]), array([-0.02222411, -0.08081856,  0.02567459, -0.24721449]), array([-0.00319512, -0.15628403,  0.15811458, -0.49096954]), array([ 0.01088885, -0.20031001, -0.0208919 ,  0.05923748]), array([ 0.01519877, -0.20165522,  0.0629646 , -0.07159276]), array([ 0.0348697 , -0.22717215,  0.12888607, -0.17600936]), array([ 0.03798335, -0.20015524, -0.09752899,  0.44192098]), array([-0.00173301, -0.05715783, -0.28725191,  0.95767043]), array([-0.04317062,  0.09729487, -0.11392217,  0.55395507]), array([-0.04402753,  0.15529441,  0.10672427,  0.01704098]), array([-0.00217854,  0.1051334 ,  0.30159419, -0.50343872]), array([ 0.04396466,  0.03306459,  0.14839435, -0.19789589]), array([ 0.08069857, -0.03783558,  0.20916876, -0.49293076]), array([ 0.09643731, -0.08607493, -0.05600724,  0.02040253]), array([ 0.05920628, -0.03053644, -0.30677897,  0.51926703]), array([-0.01994126,  0.11055231, -0.46382371,  0.85403913]), array([-0.09010794,  0.22493827, -0.22103415,  0.26142634]), array([-0.10413365,  0.20900194,  0.0829352 , -0.41969577]), array([-0.08545438,  0.13159954,  0.0975878 , -0.3381029 ]), array([-0.06761209,  0.07978873,  0.07561774, -0.16839821]), array([-0.05690988,  0.06760656,  0.0289524 ,  0.05011803]), array([-0.05639024,  0.09952586, -0.02272133,  0.26336575]), array([-0.03851575,  0.10059463,  0.19752221, -0.24951204]), array([ 0.01881504,  0.00550458,  0.36103962, -0.67582697]), array([ 0.07172212, -0.08715758,  0.15479673, -0.22735752]), array([ 0.10404108, -0.14870996,  0.15985741, -0.3724327 ]), array([ 0.1320584 , -0.22889478,  0.11216451, -0.41142267]), array([ 0.11991945, -0.23852568, -0.23078934,  0.31395661]), array([ 0.04404593, -0.10985908, -0.5089282 ,  0.93990939]), array([-0.0729905 ,  0.11805531, -0.62977399,  1.27974473]), array([-0.16774234,  0.30765261, -0.2945331 ,  0.57318712]), array([-0.21085378,  0.40402405, -0.12567678,  0.36946562]), array([-0.21521753,  0.44934272,  0.08367388,  0.07668347]), array([-0.17856619,  0.43462117,  0.27498553, -0.216357  ]), array([-0.11007269,  0.36855471,  0.39443812, -0.42389393]), array([-0.0281642 ,  0.27538038,  0.40543059, -0.47986604]), array([ 0.07049462,  0.12035963,  0.55700398, -1.02974768]), array([ 0.15646715, -0.04668436,  0.28025721, -0.5985245 ]), array([ 0.176435  , -0.10711332, -0.08583662,  0.00645378]), array([ 0.12346885, -0.04508383, -0.43095796,  0.59476002]), array([ 0.01255521,  0.11717354, -0.65014826,  0.98121302]), array([-0.09698827,  0.25697703, -0.41982302,  0.37824215]), array([-0.17375426,  0.32601462, -0.33058515,  0.2896014 ]), array([-0.22318882,  0.36510332, -0.15316196,  0.08860094]), array([-0.23234513,  0.35858619,  0.06297857, -0.15354926]), array([-0.19929554,  0.30629403,  0.25938176, -0.3561389 ]), array([-0.10737539,  0.15591787,  0.63752344, -1.11038486]), array([ 0.01621026, -0.04640711,  0.56663967, -0.85759963]), array([ 0.10766338, -0.16761575,  0.32625276, -0.32084153]), array([ 0.16690343, -0.2344726 ,  0.25230145, -0.32762908]), array([ 0.1775002 , -0.2234109 , -0.14776475,  0.43717355]), array([ 0.13734173, -0.13497516, -0.24289438,  0.42593277]), array([ 0.08542344, -0.06202963, -0.26352965,  0.283051  ]), array([ 0.01049144,  0.03946324, -0.46715708,  0.70217463]), array([-0.09188378,  0.20284372, -0.53037067,  0.88655055]), array([-0.19059715,  0.37482501, -0.43199384,  0.78996882]), array([-0.23057853,  0.43754789,  0.04017522, -0.17471302]), array([-0.2008708 ,  0.37365647,  0.24929029, -0.45004286]), array([-0.1357957 ,  0.26606852,  0.38533942, -0.59870538]), array([-0.02813708,  0.07884055,  0.66411917, -1.22599357]), array([ 0.08924464, -0.13000191,  0.47937528, -0.80775223]), array([ 0.15376334, -0.22715294,  0.15083686, -0.13961369]), array([ 0.1467582 , -0.18217512, -0.21802143,  0.58058166]), array([ 0.09773644, -0.07342501, -0.2587792 ,  0.4805709 ]), array([ 4.87795882e-02, -3.66950677e-05, -2.18666751e-01,  2.33269467e-01]), array([-0.01202302,  0.08233701, -0.3741831 ,  0.5662341 ]), array([-0.06684011,  0.14538806, -0.16141121,  0.0460557 ]), array([-0.10017104,  0.16633802, -0.16450156,  0.1547032 ]), array([-0.10318317,  0.13488393,  0.13380737, -0.46388645]), array([-0.07633198,  0.05704003,  0.1267964 , -0.2969932 ]), array([-0.02882449, -0.04665003,  0.33509499, -0.71407228]), array([ 0.02388423, -0.14586056,  0.17870928, -0.25380261]), array([ 0.03909173, -0.14245659, -0.02936555,  0.28903832]), array([ 0.01319187, -0.03434263, -0.22092298,  0.76935858]), array([-0.04361051,  0.1516476 , -0.32890121,  1.04814884]), array([-0.08391642,  0.2980198 , -0.06309827,  0.38767072]), array([-0.09308405,  0.36849874, -0.02488512,  0.30445859]), array([-0.06719048,  0.34889236,  0.27777802, -0.49328453]), array([-0.01323782,  0.24763946,  0.24793079, -0.49409428]), array([ 0.02664176,  0.16127859,  0.14020839, -0.34863513]), array([ 0.03958783,  0.11495232, -0.01464761, -0.10492488]), array([ 0.04719303,  0.05220956,  0.08718742, -0.5104512 ]), array([ 0.07175734, -0.08107559,  0.14890215, -0.79493202]), array([ 0.07574879, -0.18428204, -0.11223329, -0.22022567]), array([ 0.0544884 , -0.23564311, -0.09775357, -0.28770953]), array([ 0.01145627, -0.2289309 , -0.32312195,  0.34645073]), array([-0.04242564, -0.17362815, -0.20318328,  0.18878126]), array([-0.06593673, -0.15877678, -0.02690927, -0.04620391]), array([-0.05282333, -0.19188732,  0.15412505, -0.27676059]), array([-0.03376005, -0.19572871,  0.03266959,  0.24154268]), array([-0.01349815, -0.16605586,  0.16659572,  0.05359799]), array([ 0.00386688, -0.10465634,  0.00534527,  0.55257775]), array([ 0.01636354, -0.02098193,  0.11974131,  0.27166787]), array([ 0.02403865,  0.07015247, -0.04126912,  0.62439936]), array([0.0286078 , 0.15107692, 0.08802442, 0.17263981]), array([ 0.05816017,  0.13801523,  0.20087285, -0.2960441 ]), array([ 0.07852975,  0.1075583 , -0.00200816, -0.00048646]), array([ 0.08381158,  0.06944562,  0.0525694 , -0.37320366]), array([ 0.07128457,  0.03256997, -0.17618257,  0.00835987]), array([ 0.04273676,  0.0019615 , -0.10460317, -0.3132578 ]), array([ 0.03036027, -0.08967082, -0.01991602, -0.58848068]), array([ 0.00712498, -0.15701659, -0.20920561, -0.07802518]), array([-0.02367854, -0.19068191, -0.09381399, -0.25738594]), array([-0.02948993, -0.25765176,  0.03467521, -0.40165135]), array([-0.03730005, -0.27807059, -0.11117394,  0.19854585]), array([-0.04563318, -0.24977547,  0.03018852,  0.07862596]), array([-0.02551568, -0.24731223,  0.16677914, -0.05086185]), array([-0.00802883, -0.19942707,  0.00560847,  0.52480135]), array([-0.02240653, -0.04392128, -0.14161286,  1.00143825]), array([-0.03307026,  0.11658006,  0.04229686,  0.57423733]), array([-0.03098824,  0.24642418, -0.01732748,  0.70149104]), array([-0.03783378,  0.3871596 , -0.0455843 ,  0.68156952]), array([-0.02183368,  0.44387918,  0.20178533, -0.11756309]), array([ 0.03933335,  0.34388033,  0.39604534, -0.85964177]), array([ 0.10270398,  0.18266209,  0.22006872, -0.71531027]), array([ 0.12178501,  0.0707735 , -0.03647514, -0.38164762]), array([ 0.08762346,  0.03503015, -0.29906353,  0.02451685]), array([ 0.03361564,  0.00797337, -0.23106268, -0.29839984]), array([-0.00177238, -0.08304651, -0.11901499, -0.60065606]), array([-0.01377995, -0.22508752, -0.00389372, -0.7960082 ]), array([-0.03127521, -0.32306099, -0.16865238, -0.17313444]), array([-0.07849863, -0.294687  , -0.29294514,  0.44459208]), array([-0.1166887 , -0.22215399, -0.07932225,  0.26275268]), array([-0.10823277, -0.19429194,  0.16269637,  0.01308519]), array([-0.05423448, -0.21495717,  0.36539975, -0.20696789]), array([ 0.00509123, -0.20152013,  0.21599521,  0.34825825]), array([ 0.05558965, -0.14550822,  0.28058101,  0.20997138]), array([ 0.08682915, -0.04865872,  0.02878146,  0.74606869]), array([0.095121  , 0.07423288, 0.05648523, 0.4628442 ]), array([0.10965234, 0.13079016, 0.08727423, 0.09603803]), array([ 0.12878672,  0.11249642,  0.09959407, -0.27272358]), array([ 0.12075111,  0.09507036, -0.17852774,  0.09958378]), array([ 0.08699502,  0.08027504, -0.15265098, -0.25014572]), array([ 0.03512387,  0.064947  , -0.35579416,  0.09097164]), array([-0.04925183,  0.11088237, -0.46922043,  0.34688739]), array([-0.11750429,  0.12456336, -0.19941095, -0.22193883]), array([-0.12616575,  0.02254159,  0.11097928, -0.78140449]), array([-0.07703537, -0.17557372,  0.36298763, -1.15605305]), array([-0.01611532, -0.35130997,  0.23056727, -0.56620137]), array([ 0.01070195, -0.39282725,  0.03189078,  0.16001533]), array([ 0.02195961, -0.35534605,  0.07918284,  0.21091746]), array([ 0.01542502, -0.24272938, -0.14124325,  0.8978669 ]), array([-0.00407565, -0.07753052, -0.04408264,  0.72194121]), array([-0.02583575,  0.10345566, -0.16241357,  1.05174946]), array([-0.0370435 ,  0.25783115,  0.05628304,  0.46606644]), array([-0.00349269,  0.28484522,  0.27223561, -0.19381187]), array([ 0.0408288 ,  0.25385972,  0.16114237, -0.10388227]), array([0.05800326, 0.24690759, 0.00706058, 0.03806569]), array([ 0.06979008,  0.20089627,  0.10730736, -0.48902186]), array([ 0.07181345,  0.12712466, -0.08959543, -0.23608778]), array([ 0.03476019,  0.10869015, -0.27378416,  0.04868611]), array([-0.00660927,  0.07404024, -0.13267308, -0.39531154]), array([-0.01706433, -0.04569406,  0.02595816, -0.78209525]), array([-0.02524778, -0.15890057, -0.10920445, -0.33268314]), array([-0.03339808, -0.24379828,  0.02647591, -0.50273413]), array([-0.04227722, -0.28540274, -0.11377093,  0.09061994]), array([-0.05073968, -0.27775384,  0.03093565, -0.01654149]), array([-0.05656635, -0.22376357, -0.08689385,  0.54726606]), array([-0.05669308, -0.13496182,  0.08829504,  0.32579756]), array([-0.04828904, -0.02850967, -0.00258441,  0.72161362]), array([-0.02924681,  0.07492393,  0.19226734,  0.2980881 ]), array([ 0.02622611,  0.08891014,  0.35127372, -0.15150512]), array([0.07861425, 0.08932837, 0.16227606, 0.16335612]), array([ 0.08885402,  0.15411783, -0.05955357,  0.47443016]), array([0.08321755, 0.20376944, 0.00527781, 0.01388962]), array([ 0.09092472,  0.1595109 ,  0.06909644, -0.44807044]), array([ 0.08232878,  0.09962562, -0.15496398, -0.14227732]), array([ 0.05757464,  0.03419546, -0.08963317, -0.50446691]), array([ 0.04662805, -0.09621459, -0.02236641, -0.77775933]), array([ 0.02045241, -0.19777677, -0.23645096, -0.2258109 ]), array([-0.0182747 , -0.2545142 , -0.14484429, -0.33780342]), array([-0.03589383, -0.33023996, -0.02999045, -0.40977672])]</t>
-  </si>
-  <si>
-    <t>['[2,2,2]', '[1,2,0]', '[2,0,1]', '[0,1,1]', '[1,0,2]', '[0,2,1]', '[0,0,0]', '[1,1,1]', '[2,1,0]', '[1,1,2]']</t>
-  </si>
-  <si>
-    <t>[1, 2, 3, 4, 5, 6, 9, 10, 11, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 24, 25, 27, 28, 29, 30, 31, 33, 35, 38, 39, 40, 41, 42, 43, 44, 45, 46, 48, 50, 51, 52, 53, 54, 56, 57, 59, 60, 61, 62, 64, 65, 66, 67, 68, 69, 70, 72, 74, 75, 76, 77, 79, 80, 83, 84, 85, 86, 87, 88, 89, 91, 92, 93, 94, 95, 96, 97, 98, 99, 100, 101, 102, 105, 106, 108, 109, 111, 112, 113, 114, 115, 117, 118, 119, 120, 122, 123, 124, 125, 126, 127, 128, 130, 131, 133, 135, 136, 137, 138, 139, 140, 141, 143, 144, 145, 146, 147, 148, 150, 151, 153, 155, 157, 160, 161, 162, 163, 164, 166, 167, 168, 170, 171, 172, 173, 174, 175, 176, 177, 178, 179, 181, 183, 184, 185, 186, 187, 188, 189, 190, 191, 192, 194, 195, 198, 199]</t>
-  </si>
-  <si>
-    <t>[0, 2, 0, 2, 0, 2, 0, 0, 0, 2, 2, 2, 2, 2, 0, 2, 0, 2, 0, 2, 0, 2, 2, 2, 0, 2, 2, 0, 0, 0, 2, 0, 0, 0, 0, 2, 2, 2, 2, 0, 0, 0, 0, 0, 2, 0, 0, 0, 2, 2, 2, 0, 0, 2, 0, 0, 0, 2, 2, 2, 0, 0, 2, 2, 0, 0, 2, 0, 0, 2, 0, 0, 0, 0, 2, 2, 2, 0, 0, 2, 2, 2, 2, 2, 0, 0, 0, 2, 0, 0, 0, 2, 0, 2, 0, 2, 0, 2, 0, 2, 0, 2, 0, 0, 0, 2, 2, 2, 2, 0, 0, 0, 2, 0, 2, 0, 0, 2, 0, 2, 2, 2, 0, 2, 0, 0, 2, 0, 0, 0, 2, 0, 0, 2, 2, 2, 0, 2, 0, 0, 2, 0, 0, 0, 2, 2, 0, 2, 0, 0, 2, 0, 0, 2, 2, 2, 2, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 2, 2, 0, 2, 0, 0, 2, 0, 2, 0, 0, 2, 2, 0, 0, 0, 2, 0, 2, 2, 0, 2, 2, 0, 2, 2, 2, 0, 0, 0, 2]</t>
-  </si>
-  <si>
-    <t>['[-0.03763371 -0.01533471  0.06554052 -0.01816017]', '[-0.03406929  0.01398622 -0.02953871  0.30651903]', '[-0.02168374  0.03409236  0.1512214  -0.10649158]', '[-0.00282652  0.04327343  0.03401407  0.19924661]', '[ 0.01834705  0.04294749  0.17317668 -0.19873753]', '[0.03659766 0.0372359  0.00569586 0.14498695]', '[ 0.04737447  0.03050982  0.09950876 -0.20907803]', '[ 0.07426108 -0.04228192  0.16149838 -0.50183806]', '[ 0.10798323 -0.16108949  0.16489901 -0.66008324]', '[ 0.10954318 -0.22702731 -0.15066384  0.01044527]', '[ 0.0764301  -0.22676637 -0.17378836 -0.01285444]', '[ 0.04284907 -0.2341612  -0.15548875 -0.06492852]', '[-0.00953271 -0.18594737 -0.35614872  0.53087278]', '[-0.06619519 -0.10158349 -0.19649544  0.28949757]', '[-0.08408484 -0.07685868  0.0217178  -0.04884118]', '[-0.08443571 -0.05174908 -0.02431848  0.29539547]', '[-0.06617979 -0.03160117  0.2035194  -0.09403054]', '[-0.03309865 -0.01698438  0.1211833   0.24245643]', '[ 0.00740825 -0.00499574  0.27582187 -0.11797163]', '[0.04587997 0.00948462 0.10181472 0.26569613]', '[ 0.07361405  0.03035517  0.17039904 -0.05598589]', '[ 0.08458469  0.05855458 -0.06169625  0.33423585]', '[ 0.07724189  0.09019332 -0.00947943 -0.02395427]', '[ 0.05442839  0.11760152 -0.21289467  0.28922781]', '[ 0.02272143  0.13084347 -0.09752002 -0.1635118 ]', '[-0.00974348  0.12146112 -0.22068833  0.06595252]', '[-0.06176746  0.15351958 -0.2879045   0.24082639]', '[-0.09317863  0.14261696 -0.02042931 -0.35213297]', '[-0.0968053   0.08546601 -0.01697626 -0.21000417]', '[-0.1002653   0.06141013 -0.01766484 -0.02701558]', '[-0.1036616   0.07484559 -0.01514061  0.15839182]', '[-0.07918171  0.05387477  0.2540027  -0.3601821 ]', '[-0.00708118 -0.06114053  0.44847943 -0.75826839]', '[ 0.06441438 -0.16463335  0.24935757 -0.24903881]', '[ 0.11428052 -0.22238299  0.23745812 -0.31096276]', '[ 0.12853323 -0.21400006 -0.09724373  0.3948013 ]', '[ 0.07764433 -0.07049159 -0.39702817  1.00833051]', '[-0.02112095  0.17015415 -0.56175889  1.33864918]', '[-0.10804617  0.37103102 -0.28613349  0.62768066]', '[-0.13012827  0.41089384  0.06973471 -0.23640829]', '[-0.10720385  0.34651954  0.1531924  -0.39368458]', '[-0.07221273  0.26041278  0.18716172 -0.44782527]', '[-0.0365233   0.17586979  0.15992135 -0.37771898]', '[-0.01188314  0.11669536  0.07970931 -0.20014726]', '[-0.006508    0.09970444 -0.02743397  0.03373244]', '[ 0.00412906  0.0609641   0.13029124 -0.4125212 ]', '[ 0.01595336  0.01054306 -0.01583386 -0.08150857]', '[ 0.0243335  -0.03919418  0.09618103 -0.40558983]', '[ 0.02531968 -0.07630906 -0.08732709  0.04034371]', '[-0.00909808 -0.02462591 -0.24807264  0.46191874]', '[-0.04215582  0.03035661 -0.07435524  0.07380925]', '[-0.03738036  0.00284288  0.12001688 -0.34296507]', '[-0.02348131 -0.03202408  0.01526862  0.0020508 ]', '[-0.03155211  0.00389314 -0.09305205  0.34933688]', '[-0.03178098  0.03313058  0.09143007 -0.06150319]', '[ 0.00339939 -0.0187801   0.25139151 -0.4427728 ]', '[ 0.03701239 -0.06609368  0.07676308 -0.01763665]', '[ 0.0327423  -0.0245324  -0.11707062  0.42498092]', '[-0.00683443  0.09653582 -0.26647084  0.75791112]', '[-0.04109187  0.19631239 -0.06684545  0.21900782]', '[-0.03199308  0.18040707  0.15527798 -0.37355289]', '[-0.0087035   0.12195787  0.071149   -0.19740425]', '[-0.00525369  0.10519058 -0.0377295   0.03288868]', '[-0.02311318  0.13421657 -0.1361732   0.24928372]', '[-0.03046215  0.13144618  0.06382033 -0.27708873]', '[-0.02568866  0.09625541 -0.01806306 -0.06819473]', '[-0.03759418  0.1049503  -0.0981779   0.15154597]', '[-0.03651489  0.08513167  0.10790007 -0.34569462]', '[-0.02351233  0.04122385  0.01822956 -0.08402325]', '[-0.02977087  0.05299443 -0.07901289  0.19840241]', '[-0.02682674  0.04832642  0.10743877 -0.24330939]', '[ 0.01087169 -0.03968193  0.25890601 -0.61528017]', '[ 0.04441012 -0.11740234  0.06770988 -0.14425354]', '[ 0.06288584 -0.16285542  0.111774   -0.2993823 ]', '[ 0.0601991  -0.16345552 -0.13774574  0.29239416]', '[ 0.03707357 -0.11973886 -0.08752052  0.13379879]', '[ 0.02700287 -0.11297143 -0.01105656 -0.06861511]', '[ 0.0326711  -0.14639333  0.0653946  -0.25868627]', '[ 0.05141463 -0.21199437  0.11607923 -0.38294862]', '[ 0.05006949 -0.2250246  -0.1291524   0.2537355 ]', '[ 0.02864501 -0.18333551 -0.07953087  0.15283153]', '[-0.00641489 -0.09879701 -0.26143814  0.67286549]', '[-0.07001735  0.07333345 -0.3558552   1.00803807]', '[-0.11376536  0.21726425 -0.06926364  0.40182839]', '[-0.0957719   0.22802595  0.24527683 -0.29238124]', '[-0.0465294   0.17503623  0.2355893  -0.2209665 ]', '[-0.00599901  0.145749    0.160693   -0.06075221]', '[0.01491513 0.15369294 0.04462425 0.14180483]', '[ 0.03780804  0.13288799  0.17884422 -0.34244116]', '[ 0.05627744  0.09196915  0.00103612 -0.05716068]', '[ 0.06450636  0.04242749  0.07799732 -0.42832034]', '[ 0.05861476 -0.0039047  -0.13689289 -0.02841993]', '[ 0.03840799 -0.03875422 -0.06234661 -0.31681586]', '[ 0.00740142 -0.058469   -0.24172628  0.11774186]', '[-0.02752121 -0.06482087 -0.1008486  -0.18515941]', '[-0.05819859 -0.06278686 -0.19942547  0.20000441]', '[-0.07701454 -0.05861534  0.01491355 -0.16142838]', '[-0.07934069 -0.05648508 -0.03751191  0.18171382]', '[-0.06445758 -0.0574142   0.18300609 -0.18800022]', '[-0.03609583 -0.058283    0.09497612  0.18350094]', '[-0.00110059 -0.05382643  0.24781437 -0.13388815]', '[ 0.03211488 -0.03834287  0.07830945  0.2906871 ]', '[ 0.05614537 -0.00910939  0.15792542  0.00055041]', '[ 0.09270708 -0.03618541  0.19935501 -0.26079117]', '[ 0.13194635 -0.10727622  0.18283866 -0.43170284]', '[ 0.13531953 -0.13222765 -0.15000549  0.18597754]', '[ 0.10121637 -0.10552329 -0.18334167  0.07138005]', '[ 0.0387023  -0.03849084 -0.42682505  0.57744119]', '[-0.03453722  0.04347909 -0.28837653  0.21712817]', '[-0.07129232  0.04159623 -0.07208337 -0.24067842]', '[-0.06273489 -0.05044006  0.15264088 -0.66178864]', '[-0.04091372 -0.14348106  0.05869901 -0.25015481]', '[-0.04079001 -0.1463925  -0.05734807  0.22108133]', '[-0.03600835 -0.12702008  0.10459771 -0.02957914]', '[-0.0271692  -0.08814724 -0.01676361  0.41285548]', '[-0.01496332 -0.03621269  0.13782818  0.09970518]', '[ 0.02599071 -0.04799857  0.26285159 -0.20882557]', '[ 0.05881869 -0.04500142  0.05914677  0.24275612]', '[ 0.07575507 -0.02200624  0.10742668 -0.01397236]', '[ 0.07347647  0.01949219 -0.12813377  0.42086826]', '[ 0.05415171  0.07037061 -0.05982893  0.07662363]', '[ 0.02425186  0.1167642  -0.23139191  0.37414883]', '[-0.00724899  0.14358322 -0.07670887 -0.11471911]', '[-0.03179947  0.13969891 -0.16382914  0.0725143 ]', '[-0.04348241  0.10120615  0.04805612 -0.45231427]', '[-0.04091263  0.03399872 -0.02496165 -0.20785192]', '[-0.0536303   0.0207435  -0.09992417  0.07535693]', '[-0.0525391  -0.00670068  0.10946992 -0.34436291]', '[-0.03899966 -0.04231775  0.02226242 -0.00397656]', '[-0.01752356 -0.07644425  0.18682578 -0.32759371]', '[ 0.00536784 -0.09799352  0.03705432  0.11875221]', '[ 0.02340907 -0.09849076  0.13953966 -0.12055939]', '[ 0.05859011 -0.14278337  0.20363269 -0.30903189]', '[ 0.07435512 -0.14701754 -0.04895695  0.26909209]', '[ 0.04033113 -0.03920054 -0.2809296   0.78515747]', '[-0.00488154  0.08399766 -0.15834543  0.41892141]', '[-0.01934117  0.12053794  0.01742164 -0.06125548]', '[-0.02475467  0.12887427 -0.07006192  0.14208347]', '[-0.01944495  0.10619365  0.12118499 -0.3637938 ]', '[-0.00559309  0.05825733  0.01314453 -0.10537908]', '[-0.01471208  0.06575838 -0.10207128  0.17733766]', '[-0.01781449  0.05696013  0.07115885 -0.26380173]', '[ 0.01197072 -0.03529776  0.2175236  -0.63778614]', '[ 0.03748321 -0.11796773  0.03030149 -0.17161145]', '[ 0.02315635 -0.101162   -0.16988902  0.3341223 ]', '[-0.00041911 -0.05944601 -0.05992075  0.07244113]', '[ 0.00039754 -0.07403107  0.06726267 -0.21526694]', '[-0.00162841 -0.07325789 -0.08684034  0.22207157]', '[-0.0058916  -0.05782109  0.04536915 -0.07068093]', '[ 0.01561768 -0.10001431  0.16383413 -0.34023424]', '[ 0.02965107 -0.11873287 -0.02658103  0.15773023]', '[ 0.03221059 -0.10774408  0.05188993 -0.04912176]', '[ 0.04944333 -0.13706932  0.11590658 -0.23617004]', '[ 0.04967944 -0.12919705 -0.11305999  0.31301962]', '[ 0.00673264 -0.01736243 -0.30408292  0.77921519]', '[-0.03843276  0.0991786  -0.13507349  0.35969956]', '[-0.07057041  0.18813767 -0.17683422  0.5092819 ]', '[-0.07876018  0.22571649  0.09702056 -0.13977885]', '[-0.03356503  0.13504946  0.34318737 -0.74500146]', '[ 0.0511669  -0.05797363  0.48045581 -1.13784098]', '[ 0.12118773 -0.22936423  0.2012334  -0.53791865]', '[ 0.1272883  -0.26383381 -0.14165046  0.19839643]', '[ 0.09336314 -0.22192946 -0.18947771  0.20845053]', '[ 0.0551256  -0.18568475 -0.18408296  0.14202237]', '[ 0.0231327  -0.16944719 -0.1289489   0.01277172]', '[-0.02064041 -0.11418498 -0.29812889  0.52357096]', '[-0.06349531 -0.03937184 -0.11957973  0.20526253]', '[-0.06591838 -0.03658692  0.09563084 -0.17774056]', '[-0.05374049 -0.03830355  0.02377005  0.16242782]', '[-0.05642607  0.02648997 -0.04790259  0.47360158]', '[-0.04439372  0.07537494  0.166934    0.00934242]', '[-0.01882905  0.10061084  0.08451567  0.24225028]', '[ 0.01505797  0.10158404  0.2471787  -0.22691261]', '[0.04895529 0.08451254 0.08460869 0.06405681]', '[ 0.04763547  0.12746086 -0.09591199  0.35733077]', '[ 0.0394279   0.15303657  0.01594892 -0.10652952]', '[ 0.02713466  0.15471112 -0.13613475  0.12069694]', '[ 0.01389282  0.12968417  0.00559207 -0.36854177]', '[ 0.00200338  0.08068976 -0.12350465 -0.11501739]', '[-0.03381366  0.08379841 -0.22716455  0.13973393]', '[-0.08477593  0.13176948 -0.2705488   0.32362803]', '[-0.11036642  0.13708527  0.01959312 -0.27443392]', '[-0.07779369  0.02576919  0.29588107 -0.81429995]', '[-0.02546656 -0.10499317  0.2128884  -0.4630804 ]', '[ 0.00272242 -0.15039702  0.0622954   0.02031783]', '[ 0.02482838 -0.16456345  0.15370969 -0.15585876]', '[ 0.03492352 -0.1404509  -0.05393977  0.39408117]', '[ 0.03145253 -0.08123545  0.02175532  0.18741648]', '[ 0.04379288 -0.06791763  0.09945523 -0.05440495]', '[ 0.0429733  -0.03250365 -0.10613589  0.40184276]', '[ 0.03058203  0.01739006 -0.01386551  0.08689826]', '[ 0.03790447  0.00080683  0.08492235 -0.24840004]', '[ 0.03601978 -0.00890257 -0.10341212  0.15217775]', '[-0.00140937  0.05831747 -0.26093242  0.50212348]', '[-0.03630623  0.11316529 -0.07965713  0.03234879]', '[-0.03182347  0.06971941  0.12205872 -0.45830679]', '[ 0.00941716 -0.06236797  0.27746167 -0.83268427]', '[ 0.0722604  -0.2478279   0.33175424 -0.97908249]', '[ 0.10832183 -0.36918972  0.02010566 -0.21299766]', '[ 0.10544809 -0.39722592 -0.04882413 -0.06362719]']</t>
-  </si>
-  <si>
-    <t>[array([-0.03763371, -0.01533471,  0.06554052, -0.01816017], dtype=float32), array([-0.03406929,  0.01398622, -0.02953871,  0.30651903]), array([-0.02168374,  0.03409236,  0.1512214 , -0.10649158]), array([-0.00282652,  0.04327343,  0.03401407,  0.19924661]), array([ 0.01834705,  0.04294749,  0.17317668, -0.19873753]), array([0.03659766, 0.0372359 , 0.00569586, 0.14498695]), array([ 0.04737447,  0.03050982,  0.09950876, -0.20907803]), array([ 0.07426108, -0.04228192,  0.16149838, -0.50183806]), array([ 0.10798323, -0.16108949,  0.16489901, -0.66008324]), array([ 0.10954318, -0.22702731, -0.15066384,  0.01044527]), array([ 0.0764301 , -0.22676637, -0.17378836, -0.01285444]), array([ 0.04284907, -0.2341612 , -0.15548875, -0.06492852]), array([-0.00953271, -0.18594737, -0.35614872,  0.53087278]), array([-0.06619519, -0.10158349, -0.19649544,  0.28949757]), array([-0.08408484, -0.07685868,  0.0217178 , -0.04884118]), array([-0.08443571, -0.05174908, -0.02431848,  0.29539547]), array([-0.06617979, -0.03160117,  0.2035194 , -0.09403054]), array([-0.03309865, -0.01698438,  0.1211833 ,  0.24245643]), array([ 0.00740825, -0.00499574,  0.27582187, -0.11797163]), array([0.04587997, 0.00948462, 0.10181472, 0.26569613]), array([ 0.07361405,  0.03035517,  0.17039904, -0.05598589]), array([ 0.08458469,  0.05855458, -0.06169625,  0.33423585]), array([ 0.07724189,  0.09019332, -0.00947943, -0.02395427]), array([ 0.05442839,  0.11760152, -0.21289467,  0.28922781]), array([ 0.02272143,  0.13084347, -0.09752002, -0.1635118 ]), array([-0.00974348,  0.12146112, -0.22068833,  0.06595252]), array([-0.06176746,  0.15351958, -0.2879045 ,  0.24082639]), array([-0.09317863,  0.14261696, -0.02042931, -0.35213297]), array([-0.0968053 ,  0.08546601, -0.01697626, -0.21000417]), array([-0.1002653 ,  0.06141013, -0.01766484, -0.02701558]), array([-0.1036616 ,  0.07484559, -0.01514061,  0.15839182]), array([-0.07918171,  0.05387477,  0.2540027 , -0.3601821 ]), array([-0.00708118, -0.06114053,  0.44847943, -0.75826839]), array([ 0.06441438, -0.16463335,  0.24935757, -0.24903881]), array([ 0.11428052, -0.22238299,  0.23745812, -0.31096276]), array([ 0.12853323, -0.21400006, -0.09724373,  0.3948013 ]), array([ 0.07764433, -0.07049159, -0.39702817,  1.00833051]), array([-0.02112095,  0.17015415, -0.56175889,  1.33864918]), array([-0.10804617,  0.37103102, -0.28613349,  0.62768066]), array([-0.13012827,  0.41089384,  0.06973471, -0.23640829]), array([-0.10720385,  0.34651954,  0.1531924 , -0.39368458]), array([-0.07221273,  0.26041278,  0.18716172, -0.44782527]), array([-0.0365233 ,  0.17586979,  0.15992135, -0.37771898]), array([-0.01188314,  0.11669536,  0.07970931, -0.20014726]), array([-0.006508  ,  0.09970444, -0.02743397,  0.03373244]), array([ 0.00412906,  0.0609641 ,  0.13029124, -0.4125212 ]), array([ 0.01595336,  0.01054306, -0.01583386, -0.08150857]), array([ 0.0243335 , -0.03919418,  0.09618103, -0.40558983]), array([ 0.02531968, -0.07630906, -0.08732709,  0.04034371]), array([-0.00909808, -0.02462591, -0.24807264,  0.46191874]), array([-0.04215582,  0.03035661, -0.07435524,  0.07380925]), array([-0.03738036,  0.00284288,  0.12001688, -0.34296507]), array([-0.02348131, -0.03202408,  0.01526862,  0.0020508 ]), array([-0.03155211,  0.00389314, -0.09305205,  0.34933688]), array([-0.03178098,  0.03313058,  0.09143007, -0.06150319]), array([ 0.00339939, -0.0187801 ,  0.25139151, -0.4427728 ]), array([ 0.03701239, -0.06609368,  0.07676308, -0.01763665]), array([ 0.0327423 , -0.0245324 , -0.11707062,  0.42498092]), array([-0.00683443,  0.09653582, -0.26647084,  0.75791112]), array([-0.04109187,  0.19631239, -0.06684545,  0.21900782]), array([-0.03199308,  0.18040707,  0.15527798, -0.37355289]), array([-0.0087035 ,  0.12195787,  0.071149  , -0.19740425]), array([-0.00525369,  0.10519058, -0.0377295 ,  0.03288868]), array([-0.02311318,  0.13421657, -0.1361732 ,  0.24928372]), array([-0.03046215,  0.13144618,  0.06382033, -0.27708873]), array([-0.02568866,  0.09625541, -0.01806306, -0.06819473]), array([-0.03759418,  0.1049503 , -0.0981779 ,  0.15154597]), array([-0.03651489,  0.08513167,  0.10790007, -0.34569462]), array([-0.02351233,  0.04122385,  0.01822956, -0.08402325]), array([-0.02977087,  0.05299443, -0.07901289,  0.19840241]), array([-0.02682674,  0.04832642,  0.10743877, -0.24330939]), array([ 0.01087169, -0.03968193,  0.25890601, -0.61528017]), array([ 0.04441012, -0.11740234,  0.06770988, -0.14425354]), array([ 0.06288584, -0.16285542,  0.111774  , -0.2993823 ]), array([ 0.0601991 , -0.16345552, -0.13774574,  0.29239416]), array([ 0.03707357, -0.11973886, -0.08752052,  0.13379879]), array([ 0.02700287, -0.11297143, -0.01105656, -0.06861511]), array([ 0.0326711 , -0.14639333,  0.0653946 , -0.25868627]), array([ 0.05141463, -0.21199437,  0.11607923, -0.38294862]), array([ 0.05006949, -0.2250246 , -0.1291524 ,  0.2537355 ]), array([ 0.02864501, -0.18333551, -0.07953087,  0.15283153]), array([-0.00641489, -0.09879701, -0.26143814,  0.67286549]), array([-0.07001735,  0.07333345, -0.3558552 ,  1.00803807]), array([-0.11376536,  0.21726425, -0.06926364,  0.40182839]), array([-0.0957719 ,  0.22802595,  0.24527683, -0.29238124]), array([-0.0465294 ,  0.17503623,  0.2355893 , -0.2209665 ]), array([-0.00599901,  0.145749  ,  0.160693  , -0.06075221]), array([0.01491513, 0.15369294, 0.04462425, 0.14180483]), array([ 0.03780804,  0.13288799,  0.17884422, -0.34244116]), array([ 0.05627744,  0.09196915,  0.00103612, -0.05716068]), array([ 0.06450636,  0.04242749,  0.07799732, -0.42832034]), array([ 0.05861476, -0.0039047 , -0.13689289, -0.02841993]), array([ 0.03840799, -0.03875422, -0.06234661, -0.31681586]), array([ 0.00740142, -0.058469  , -0.24172628,  0.11774186]), array([-0.02752121, -0.06482087, -0.1008486 , -0.18515941]), array([-0.05819859, -0.06278686, -0.19942547,  0.20000441]), array([-0.07701454, -0.05861534,  0.01491355, -0.16142838]), array([-0.07934069, -0.05648508, -0.03751191,  0.18171382]), array([-0.06445758, -0.0574142 ,  0.18300609, -0.18800022]), array([-0.03609583, -0.058283  ,  0.09497612,  0.18350094]), array([-0.00110059, -0.05382643,  0.24781437, -0.13388815]), array([ 0.03211488, -0.03834287,  0.07830945,  0.2906871 ]), array([ 0.05614537, -0.00910939,  0.15792542,  0.00055041]), array([ 0.09270708, -0.03618541,  0.19935501, -0.26079117]), array([ 0.13194635, -0.10727622,  0.18283866, -0.43170284]), array([ 0.13531953, -0.13222765, -0.15000549,  0.18597754]), array([ 0.10121637, -0.10552329, -0.18334167,  0.07138005]), array([ 0.0387023 , -0.03849084, -0.42682505,  0.57744119]), array([-0.03453722,  0.04347909, -0.28837653,  0.21712817]), array([-0.07129232,  0.04159623, -0.07208337, -0.24067842]), array([-0.06273489, -0.05044006,  0.15264088, -0.66178864]), array([-0.04091372, -0.14348106,  0.05869901, -0.25015481]), array([-0.04079001, -0.1463925 , -0.05734807,  0.22108133]), array([-0.03600835, -0.12702008,  0.10459771, -0.02957914]), array([-0.0271692 , -0.08814724, -0.01676361,  0.41285548]), array([-0.01496332, -0.03621269,  0.13782818,  0.09970518]), array([ 0.02599071, -0.04799857,  0.26285159, -0.20882557]), array([ 0.05881869, -0.04500142,  0.05914677,  0.24275612]), array([ 0.07575507, -0.02200624,  0.10742668, -0.01397236]), array([ 0.07347647,  0.01949219, -0.12813377,  0.42086826]), array([ 0.05415171,  0.07037061, -0.05982893,  0.07662363]), array([ 0.02425186,  0.1167642 , -0.23139191,  0.37414883]), array([-0.00724899,  0.14358322, -0.07670887, -0.11471911]), array([-0.03179947,  0.13969891, -0.16382914,  0.0725143 ]), array([-0.04348241,  0.10120615,  0.04805612, -0.45231427]), array([-0.04091263,  0.03399872, -0.02496165, -0.20785192]), array([-0.0536303 ,  0.0207435 , -0.09992417,  0.07535693]), array([-0.0525391 , -0.00670068,  0.10946992, -0.34436291]), array([-0.03899966, -0.04231775,  0.02226242, -0.00397656]), array([-0.01752356, -0.07644425,  0.18682578, -0.32759371]), array([ 0.00536784, -0.09799352,  0.03705432,  0.11875221]), array([ 0.02340907, -0.09849076,  0.13953966, -0.12055939]), array([ 0.05859011, -0.14278337,  0.20363269, -0.30903189]), array([ 0.07435512, -0.14701754, -0.04895695,  0.26909209]), array([ 0.04033113, -0.03920054, -0.2809296 ,  0.78515747]), array([-0.00488154,  0.08399766, -0.15834543,  0.41892141]), array([-0.01934117,  0.12053794,  0.01742164, -0.06125548]), array([-0.02475467,  0.12887427, -0.07006192,  0.14208347]), array([-0.01944495,  0.10619365,  0.12118499, -0.3637938 ]), array([-0.00559309,  0.05825733,  0.01314453, -0.10537908]), array([-0.01471208,  0.06575838, -0.10207128,  0.17733766]), array([-0.01781449,  0.05696013,  0.07115885, -0.26380173]), array([ 0.01197072, -0.03529776,  0.2175236 , -0.63778614]), array([ 0.03748321, -0.11796773,  0.03030149, -0.17161145]), array([ 0.02315635, -0.101162  , -0.16988902,  0.3341223 ]), array([-0.00041911, -0.05944601, -0.05992075,  0.07244113]), array([ 0.00039754, -0.07403107,  0.06726267, -0.21526694]), array([-0.00162841, -0.07325789, -0.08684034,  0.22207157]), array([-0.0058916 , -0.05782109,  0.04536915, -0.07068093]), array([ 0.01561768, -0.10001431,  0.16383413, -0.34023424]), array([ 0.02965107, -0.11873287, -0.02658103,  0.15773023]), array([ 0.03221059, -0.10774408,  0.05188993, -0.04912176]), array([ 0.04944333, -0.13706932,  0.11590658, -0.23617004]), array([ 0.04967944, -0.12919705, -0.11305999,  0.31301962]), array([ 0.00673264, -0.01736243, -0.30408292,  0.77921519]), array([-0.03843276,  0.0991786 , -0.13507349,  0.35969956]), array([-0.07057041,  0.18813767, -0.17683422,  0.5092819 ]), array([-0.07876018,  0.22571649,  0.09702056, -0.13977885]), array([-0.03356503,  0.13504946,  0.34318737, -0.74500146]), array([ 0.0511669 , -0.05797363,  0.48045581, -1.13784098]), array([ 0.12118773, -0.22936423,  0.2012334 , -0.53791865]), array([ 0.1272883 , -0.26383381, -0.14165046,  0.19839643]), array([ 0.09336314, -0.22192946, -0.18947771,  0.20845053]), array([ 0.0551256 , -0.18568475, -0.18408296,  0.14202237]), array([ 0.0231327 , -0.16944719, -0.1289489 ,  0.01277172]), array([-0.02064041, -0.11418498, -0.29812889,  0.52357096]), array([-0.06349531, -0.03937184, -0.11957973,  0.20526253]), array([-0.06591838, -0.03658692,  0.09563084, -0.17774056]), array([-0.05374049, -0.03830355,  0.02377005,  0.16242782]), array([-0.05642607,  0.02648997, -0.04790259,  0.47360158]), array([-0.04439372,  0.07537494,  0.166934  ,  0.00934242]), array([-0.01882905,  0.10061084,  0.08451567,  0.24225028]), array([ 0.01505797,  0.10158404,  0.2471787 , -0.22691261]), array([0.04895529, 0.08451254, 0.08460869, 0.06405681]), array([ 0.04763547,  0.12746086, -0.09591199,  0.35733077]), array([ 0.0394279 ,  0.15303657,  0.01594892, -0.10652952]), array([ 0.02713466,  0.15471112, -0.13613475,  0.12069694]), array([ 0.01389282,  0.12968417,  0.00559207, -0.36854177]), array([ 0.00200338,  0.08068976, -0.12350465, -0.11501739]), array([-0.03381366,  0.08379841, -0.22716455,  0.13973393]), array([-0.08477593,  0.13176948, -0.2705488 ,  0.32362803]), array([-0.11036642,  0.13708527,  0.01959312, -0.27443392]), array([-0.07779369,  0.02576919,  0.29588107, -0.81429995]), array([-0.02546656, -0.10499317,  0.2128884 , -0.4630804 ]), array([ 0.00272242, -0.15039702,  0.0622954 ,  0.02031783]), array([ 0.02482838, -0.16456345,  0.15370969, -0.15585876]), array([ 0.03492352, -0.1404509 , -0.05393977,  0.39408117]), array([ 0.03145253, -0.08123545,  0.02175532,  0.18741648]), array([ 0.04379288, -0.06791763,  0.09945523, -0.05440495]), array([ 0.0429733 , -0.03250365, -0.10613589,  0.40184276]), array([ 0.03058203,  0.01739006, -0.01386551,  0.08689826]), array([ 0.03790447,  0.00080683,  0.08492235, -0.24840004]), array([ 0.03601978, -0.00890257, -0.10341212,  0.15217775]), array([-0.00140937,  0.05831747, -0.26093242,  0.50212348]), array([-0.03630623,  0.11316529, -0.07965713,  0.03234879]), array([-0.03182347,  0.06971941,  0.12205872, -0.45830679]), array([ 0.00941716, -0.06236797,  0.27746167, -0.83268427]), array([ 0.0722604 , -0.2478279 ,  0.33175424, -0.97908249]), array([ 0.10832183, -0.36918972,  0.02010566, -0.21299766]), array([ 0.10544809, -0.39722592, -0.04882413, -0.06362719])]</t>
-  </si>
-  <si>
-    <t>['[0,2,1]', '[2,0,1]', '[0,1,1]', '[1,1,2]', '[2,2,2]', '[1,2,0]', '[1,1,1]', '[2,1,0]', '[0,0,0]', '[1,0,2]']</t>
-  </si>
-  <si>
-    <t>[0, 2, 0, 2, 0, 2, 0, 2, 0, 2, 0, 2, 0, 2, 0, 2, 0, 2, 0, 2, 2, 0, 2, 0, 2, 2, 0, 2, 0, 2, 0, 2, 0, 2, 0, 2, 0, 2, 0, 2, 0, 2, 0, 2, 0, 2, 0, 2, 0, 2, 0, 2, 2, 0, 2, 0, 2, 2, 0, 2, 0, 2, 0, 2, 0, 2, 0, 2, 0, 2, 0, 2, 0, 2, 0, 2, 0, 2, 0, 2, 0, 2, 0, 2, 2, 0, 2, 0, 2, 2, 0, 2, 0, 2, 0, 2, 0, 2, 0, 2, 0, 2, 0, 2, 0, 2, 0, 2, 0, 2, 0, 2, 0, 2, 0, 2, 2, 0, 2, 0, 2, 2, 0, 2, 0, 2, 0, 2, 0, 2, 0, 2, 0, 2, 0, 2, 0, 2, 0, 2, 0, 2, 0, 2, 0, 2, 0, 2, 2, 0, 2, 0, 2, 0, 2, 0, 2, 0, 0, 2, 0, 2, 0, 2, 0, 2, 0, 2, 0, 2, 0, 2, 0, 0, 2, 0, 2, 0, 2, 0, 2, 0, 2, 0, 2, 0, 2, 0, 2, 0, 2, 0, 2, 2, 0, 2, 2, 0, 2]</t>
-  </si>
-  <si>
-    <t>['[-0.03763371 -0.01533471  0.06554052 -0.01816017]', '[-0.03406929  0.01398622 -0.02953871  0.30651903]', '[-0.02168374  0.03409236  0.1512214  -0.10649158]', '[-0.00282652  0.04327343  0.03401407  0.19924661]', '[ 0.01834705  0.04294749  0.17317668 -0.19873753]', '[0.03659766 0.0372359  0.00569586 0.14498695]', '[ 0.04737447  0.03050982  0.09950876 -0.20907803]', '[ 0.04773513  0.02629209 -0.09583188  0.16718432]', '[ 0.03752505  0.02534768 -0.00439201 -0.17769188]', '[ 0.01910665  0.02614969 -0.17578652  0.18226832]', '[-0.00293854  0.02498097 -0.04044017 -0.19672323]', '[-0.02338561  0.01819528 -0.15991175  0.1265223 ]', '[-0.03744461  0.00328053  0.02144561 -0.27476369]', '[-0.04234133 -0.01910231 -0.06994388  0.05368665]', '[-0.03763269 -0.04539758  0.11498126 -0.31087136]', '[-0.02550263 -0.06918706  0.00335501  0.07846404]', '[-0.00968282 -0.08350681  0.15097012 -0.21632696]', '[ 0.0053941  -0.08236633 -0.00300315  0.22938636]', '[ 0.0161822  -0.06338321  0.10914378 -0.04087513]', '[ 0.02066644 -0.02828874 -0.063904    0.38603243]', '[0.01913681 0.01633736 0.05013034 0.05264949]', '[ 0.0400551  -0.0073938   0.15390054 -0.28229442]', '[ 0.05094132 -0.02216557 -0.04740575  0.1382459 ]', '[ 0.04870162 -0.02310954  0.02529389 -0.14757537]', '[ 0.03376547 -0.01028918 -0.17094986  0.2707556 ]', '[ 0.0103118   0.01075104 -0.05836816 -0.0672164 ]', '[ 0.01124463 -0.0370396   0.06579493 -0.4018725 ]', '[ 0.00803486 -0.07504962 -0.09809813  0.02722039]', '[ 1.51338775e-04 -9.62015886e-02  1.99960523e-02 -2.35938240e-01]', '[-0.01132378 -0.09750196 -0.13218554  0.22087768]', '[-0.02355496 -0.08096771  0.01267429 -0.05993836]', '[-0.0330696  -0.05205256 -0.10484912  0.34234137]', '[-0.03642324 -0.01860412  0.07279953 -0.01371334]', '[-0.03166866  0.01206933 -0.02509297  0.31554307]', '[-0.01874523  0.03436217  0.15211703 -0.09394883]', '[-5.13230523e-05  4.62105789e-02  3.16075962e-02  2.12883305e-01]', '[ 0.02039466  0.04845639  0.16853114 -0.18720539]', '[0.03762326 0.04455931 0.00038545 0.1511327 ]', '[ 0.04739711  0.03833294  0.09500645 -0.210463  ]', '[ 0.04703493  0.03301412 -0.09845059  0.15764597]', '[ 0.03651771  0.02945918 -0.00486237 -0.19385638]', '[ 0.01818744  0.02662077 -0.17457023  0.1626772 ]', '[-0.00352862  0.02154485 -0.03855204 -0.21548247]', '[-0.02362984  0.01145217 -0.1585124   0.11283283]', '[-0.03753204 -0.00542412  0.02151977 -0.28032934]', '[-0.0425714  -0.02799292 -0.07141092  0.05738308]', '[-0.03827598 -0.05268781  0.11245074 -0.2989076 ]', '[-0.02666782 -0.07350228  0.00086365  0.09565699]', '[-0.01124264 -0.08418115  0.14971078 -0.19780414]', '[ 0.00379227 -0.07954607 -0.00205983  0.24522416]', '[ 0.01502732 -0.05793824  0.11266026 -0.0308478 ]', '[ 0.02043587 -0.0215465  -0.05831989  0.38888924]', '[0.0201345  0.02294776 0.05656633 0.04870431]', '[ 0.04228153 -0.00209186  0.15946475 -0.29102339]', '[ 0.05405053 -0.01885364 -0.04438103  0.12755362]', '[ 0.05206131 -0.02189818  0.02466117 -0.15749228]', '[ 0.03660591 -0.01081184 -0.17545328  0.26354381]', '[ 0.01192537  0.0091228  -0.06591528 -0.07106547]', '[ 0.01118009 -0.03914202  0.05688384 -0.40293856]', '[ 0.00622896 -0.0772038  -0.10624534  0.02750459]', '[-0.00303788 -0.09829433  0.01458906 -0.23583011]', '[-0.01519879 -0.09969145 -0.13350175  0.21971518]', '[-0.0272538  -0.08352116  0.01570042 -0.06232006]', '[-0.03578703 -0.0551298  -0.09828338  0.33973714]', '[-0.03761326 -0.02207353  0.08118663 -0.01472797]', '[-0.03117157  0.0087054  -0.0169494   0.3178561 ]', '[-0.01680571  0.03188745  0.15813818 -0.08731009]', '[0.00277007 0.04548881 0.03428665 0.22359811]', '[ 0.02338839  0.05015225  0.16761522 -0.17413231]', '[ 0.04012653  0.04887202 -0.00341795  0.16369621]', '[ 0.04896058  0.04483812  0.08966857 -0.20161924]', '[ 0.04751718  0.04066462 -0.1036719   0.15989458]', '[ 0.03608145  0.03677286 -0.00864944 -0.19955532]', '[ 0.01720728  0.03201352 -0.17617777  0.14942282]', '[-0.00461583  0.02372424 -0.03809184 -0.23382355]', '[-0.02447932  0.00976918 -0.15676744  0.09325948]', '[-0.03799968 -0.01077833  0.02339896 -0.29677434]', '[-0.04274161 -0.03600156 -0.07044923  0.04776911]', '[-0.03840229 -0.06173394  0.11188697 -0.29948506]', '[-0.02704815 -0.08175761 -0.00103029  0.10395188]', '[-0.01208312 -0.09002918  0.14717567 -0.18251961]', '[ 0.00248328 -0.08194469 -0.00402095  0.26378905]', '[ 0.01347812 -0.05663598  0.11238667 -0.01308476]', '[ 0.01906687 -0.01709075 -0.05618284  0.40214629]', '[0.01944171 0.02938882 0.06110738 0.05507872]', '[ 0.0426691   0.00488294  0.16552386 -0.29198549]', '[ 0.05567946 -0.01270791 -0.03830676  0.12056844]', '[ 0.05476185 -0.01754592  0.02903159 -0.16796849]', '[ 0.03988309 -0.00865282 -0.17423833  0.25254733]', '[ 0.01506354  0.0092458  -0.06855153 -0.08010439]', '[ 0.01342235 -0.040504    0.05069643 -0.40863199]', '[ 0.00697918 -0.07935649 -0.11469307  0.02518724]', '[-0.00404282 -0.10065344  0.0058336  -0.23581411]', '[-0.01780205 -0.1019573  -0.14040012  0.22036821]', '[-0.03090464 -0.08571047  0.01233408 -0.06238079]', '[-0.03967834 -0.05746832 -0.09728464  0.33830588]', '[-0.04088649 -0.02479813  0.0862282  -0.01699021]', '[-0.03313408  0.00555571 -0.00916788  0.31615044]', '[-0.01709824  0.0286016   0.16671648 -0.08669091]', '[0.00409761 0.0426896  0.04159804 0.2280058 ]', '[ 0.02591234  0.04865704  0.1720678  -0.16554347]', '[ 0.04318138  0.04944889 -0.00259859  0.17554405]', '[ 0.05182717  0.04793017  0.08708201 -0.18877447]', '[ 0.04961378  0.04616405 -0.10855157  0.17058545]', '[ 0.03710027  0.04393717 -0.01427681 -0.19404838]', '[ 0.0171644   0.03955664 -0.18094415  0.14747835]', '[-0.00543206  0.03008287 -0.04093621 -0.24363824]', '[-0.02563501  0.01348145 -0.15733974  0.07702875]', '[-0.03907693 -0.0106912   0.02462454 -0.31615271]', '[-0.04347682 -0.03975416 -0.06843994  0.0294576 ]', '[-0.03875691 -0.06868657  0.11350382 -0.31255978]', '[-0.02718902 -0.09055323 -0.0005972   0.09892028]', '[-0.01229391 -0.09889691  0.14605862 -0.17821307]', '[ 0.00193427 -0.08911365 -0.00617459  0.27613969]', '[ 0.01246219 -0.0607399   0.11006833  0.00460279]', '[ 0.01767613 -0.01746661 -0.05742591  0.42104822]', '[0.01799889 0.03256356 0.06194914 0.07106617]', '[ 0.04164095  0.01069004  0.16882221 -0.28203346]', '[ 0.05552767 -0.00565132 -0.03298584  0.12304419]', '[ 0.05578172 -0.01071831  0.0351817  -0.17251072]', '[ 0.04207756 -0.00327057 -0.16892467  0.24306336]', '[ 0.01809734  0.01247845 -0.06570728 -0.09161583]', '[ 0.0166784  -0.03952956  0.04996191 -0.41928328]', '[ 0.00970175 -0.08024085 -0.11923689  0.0174798 ]', '[-0.00255012 -0.1027089  -0.00170788 -0.23980761]', '[-0.01797844 -0.10448545 -0.14921732  0.21944907]', '[-0.03279817 -0.08822614  0.00432766 -0.06160815]', '[-0.0429199  -0.05980691 -0.10248424  0.3390746 ]', '[-0.04477409 -0.02707825  0.08509623 -0.01727879]', '[-0.03680915  0.00308939 -0.00596657  0.31465325]', '[-0.01976107  0.02578306  0.17342083 -0.08849873]', '[0.00298872 0.03961152 0.05010813 0.22750325]', '[ 0.026514    0.04574731  0.18032288 -0.16312637]', '[0.04524209 0.0474135  0.00347248 0.18193809]', '[ 0.0547737   0.04756446  0.089742   -0.1786232 ]', '[ 0.052719    0.04808358 -0.10958037  0.182909  ]', '[ 0.03968097  0.04832029 -0.01831026 -0.18224004]', '[ 0.01875532  0.04597667 -0.18654323  0.15553006]', '[-0.00498113  0.03750945 -0.04647087 -0.24197424]', '[-0.02615815  0.02046471 -0.16137018  0.07087075]', '[-0.04018818 -0.00569015  0.02283148 -0.32956194]', '[-0.04472263 -0.03796813 -0.06807105  0.0112597 ]', '[-0.03977193 -0.0707079   0.11527201 -0.33173448]', '[-0.02780187 -0.0961543   0.00147775  0.08294848]', '[-0.01255879 -0.10704514  0.14731344 -0.1872195 ]', '[ 0.00179073 -0.09820019 -0.00627177  0.27594249]', '[ 0.01214555 -0.06893478  0.10850376  0.01352591]', '[ 0.0169596  -0.02313884 -0.05971152  0.43687334]', '[0.01684516 0.03045181 0.06007176 0.0901481 ]', '[ 0.04025325  0.01235965  0.16851984 -0.26398233]', '[ 0.05430388 -0.00079913 -0.030983    0.13630429]', '[ 0.0551963  -0.00390572  0.03949108 -0.16640006]', '[ 0.04252198  0.00399475 -0.1631329   0.24156304]', '[ 0.01972951  0.01878404 -0.05989374 -0.09935726]', '[-0.00719077  0.03338913 -0.20317714  0.23831098]', '[-0.03109278  0.03970184 -0.03105751 -0.17943795]', '[-0.04602812  0.03220258 -0.11536638  0.10315408]', '[-0.04857485  0.00954666  0.08942957 -0.32567426]', '[-0.03903633 -0.02389749  0.00315131 -0.00188288]', '[-0.04739862  0.00891768 -0.08390808  0.32277384]', '[-0.04389416  0.03111565  0.11862509 -0.10351861]', '[-0.02864332  0.03893335  0.03120107  0.18236794]', '[-0.00497513  0.0334018   0.2002452  -0.23260361]', '[0.02107596 0.02016769 0.05479172 0.10615778]', '[ 0.04279093  0.00657729  0.15735704 -0.23601811]', '[ 0.05432279 -0.00042662 -0.04430346  0.16843264]', '[ 0.05270667  0.0025464   0.02841883 -0.13915784]', '[ 0.03836449  0.0147418  -0.16827479  0.25628195]', '[ 0.01530575  0.03085196 -0.05733159 -0.10110943]', '[-0.01036427  0.04347995 -0.19356254  0.22084265]', '[-0.03187717  0.04515792 -0.01740894 -0.20714614]', '[-0.04403382  0.03176144 -0.10197892  0.07334333]', '[-0.04430096  0.00366435  0.09821205 -0.34899642]', '[-0.03373534 -0.03322643  0.0043413  -0.01230537]', '[-0.04269608 -0.00097066 -0.0909752   0.32760099]', '[-0.04129243  0.02356253  0.10519625 -0.08574262]', '[-0.0290492   0.03574529  0.01530273  0.2070179 ]', '[-0.00840644  0.03516068  0.18665023 -0.20909091]', '[0.01551767 0.02588013 0.04766478 0.12118061]', '[ 0.03666441  0.01404583  0.15895883 -0.23385199]', '[ 0.04938654  0.006138   -0.03428356  0.15758913]', '[ 0.05039664  0.00595369  0.04402447 -0.15892806]', '[ 0.03936407  0.01386988 -0.15158915  0.23451048]', '[ 0.01933942  0.0260666  -0.0444065  -0.11734339]', '[-0.00445233  0.03651128 -0.18814468  0.21589742]', '[-0.02577642  0.03852623 -0.02095712 -0.1988815 ]', '[-0.03946704  0.027949   -0.11335767  0.09252509]', '[-0.04251502  0.00429218  0.08248658 -0.3249713 ]', '[-0.03513879 -0.02796251 -0.01104114  0.00874986]', '[-0.02023327 -0.06097559  0.15578729 -0.3303973 ]', '[-0.00269428 -0.08508483  0.01557024  0.09560047]', '[ 0.01242213 -0.09227187  0.13213142 -0.16355619]', '[ 0.02111218 -0.07814076 -0.04633684  0.30331765]', '[ 0.02185659 -0.04415853  0.05456546  0.03100886]', '[ 0.04214847 -0.06553987  0.14341803 -0.23768561]', '[ 0.0497783  -0.06563303 -0.06836522  0.23735732]', '[ 0.04297833 -0.04319393  0.00232915 -0.01764589]', '[ 0.0506473  -0.07245873  0.07174425 -0.26846855]', '[ 0.04334158 -0.07746957 -0.14314117  0.21749326]', '[ 0.02274164 -0.0586999  -0.05823584 -0.03594645]']</t>
-  </si>
-  <si>
-    <t>[array([-0.03763371, -0.01533471,  0.06554052, -0.01816017], dtype=float32), array([-0.03406929,  0.01398622, -0.02953871,  0.30651903]), array([-0.02168374,  0.03409236,  0.1512214 , -0.10649158]), array([-0.00282652,  0.04327343,  0.03401407,  0.19924661]), array([ 0.01834705,  0.04294749,  0.17317668, -0.19873753]), array([0.03659766, 0.0372359 , 0.00569586, 0.14498695]), array([ 0.04737447,  0.03050982,  0.09950876, -0.20907803]), array([ 0.04773513,  0.02629209, -0.09583188,  0.16718432]), array([ 0.03752505,  0.02534768, -0.00439201, -0.17769188]), array([ 0.01910665,  0.02614969, -0.17578652,  0.18226832]), array([-0.00293854,  0.02498097, -0.04044017, -0.19672323]), array([-0.02338561,  0.01819528, -0.15991175,  0.1265223 ]), array([-0.03744461,  0.00328053,  0.02144561, -0.27476369]), array([-0.04234133, -0.01910231, -0.06994388,  0.05368665]), array([-0.03763269, -0.04539758,  0.11498126, -0.31087136]), array([-0.02550263, -0.06918706,  0.00335501,  0.07846404]), array([-0.00968282, -0.08350681,  0.15097012, -0.21632696]), array([ 0.0053941 , -0.08236633, -0.00300315,  0.22938636]), array([ 0.0161822 , -0.06338321,  0.10914378, -0.04087513]), array([ 0.02066644, -0.02828874, -0.063904  ,  0.38603243]), array([0.01913681, 0.01633736, 0.05013034, 0.05264949]), array([ 0.0400551 , -0.0073938 ,  0.15390054, -0.28229442]), array([ 0.05094132, -0.02216557, -0.04740575,  0.1382459 ]), array([ 0.04870162, -0.02310954,  0.02529389, -0.14757537]), array([ 0.03376547, -0.01028918, -0.17094986,  0.2707556 ]), array([ 0.0103118 ,  0.01075104, -0.05836816, -0.0672164 ]), array([ 0.01124463, -0.0370396 ,  0.06579493, -0.4018725 ]), array([ 0.00803486, -0.07504962, -0.09809813,  0.02722039]), array([ 1.51338775e-04, -9.62015886e-02,  1.99960523e-02, -2.35938240e-01]), array([-0.01132378, -0.09750196, -0.13218554,  0.22087768]), array([-0.02355496, -0.08096771,  0.01267429, -0.05993836]), array([-0.0330696 , -0.05205256, -0.10484912,  0.34234137]), array([-0.03642324, -0.01860412,  0.07279953, -0.01371334]), array([-0.03166866,  0.01206933, -0.02509297,  0.31554307]), array([-0.01874523,  0.03436217,  0.15211703, -0.09394883]), array([-5.13230523e-05,  4.62105789e-02,  3.16075962e-02,  2.12883305e-01]), array([ 0.02039466,  0.04845639,  0.16853114, -0.18720539]), array([0.03762326, 0.04455931, 0.00038545, 0.1511327 ]), array([ 0.04739711,  0.03833294,  0.09500645, -0.210463  ]), array([ 0.04703493,  0.03301412, -0.09845059,  0.15764597]), array([ 0.03651771,  0.02945918, -0.00486237, -0.19385638]), array([ 0.01818744,  0.02662077, -0.17457023,  0.1626772 ]), array([-0.00352862,  0.02154485, -0.03855204, -0.21548247]), array([-0.02362984,  0.01145217, -0.1585124 ,  0.11283283]), array([-0.03753204, -0.00542412,  0.02151977, -0.28032934]), array([-0.0425714 , -0.02799292, -0.07141092,  0.05738308]), array([-0.03827598, -0.05268781,  0.11245074, -0.2989076 ]), array([-0.02666782, -0.07350228,  0.00086365,  0.09565699]), array([-0.01124264, -0.08418115,  0.14971078, -0.19780414]), array([ 0.00379227, -0.07954607, -0.00205983,  0.24522416]), array([ 0.01502732, -0.05793824,  0.11266026, -0.0308478 ]), array([ 0.02043587, -0.0215465 , -0.05831989,  0.38888924]), array([0.0201345 , 0.02294776, 0.05656633, 0.04870431]), array([ 0.04228153, -0.00209186,  0.15946475, -0.29102339]), array([ 0.05405053, -0.01885364, -0.04438103,  0.12755362]), array([ 0.05206131, -0.02189818,  0.02466117, -0.15749228]), array([ 0.03660591, -0.01081184, -0.17545328,  0.26354381]), array([ 0.01192537,  0.0091228 , -0.06591528, -0.07106547]), array([ 0.01118009, -0.03914202,  0.05688384, -0.40293856]), array([ 0.00622896, -0.0772038 , -0.10624534,  0.02750459]), array([-0.00303788, -0.09829433,  0.01458906, -0.23583011]), array([-0.01519879, -0.09969145, -0.13350175,  0.21971518]), array([-0.0272538 , -0.08352116,  0.01570042, -0.06232006]), array([-0.03578703, -0.0551298 , -0.09828338,  0.33973714]), array([-0.03761326, -0.02207353,  0.08118663, -0.01472797]), array([-0.03117157,  0.0087054 , -0.0169494 ,  0.3178561 ]), array([-0.01680571,  0.03188745,  0.15813818, -0.08731009]), array([0.00277007, 0.04548881, 0.03428665, 0.22359811]), array([ 0.02338839,  0.05015225,  0.16761522, -0.17413231]), array([ 0.04012653,  0.04887202, -0.00341795,  0.16369621]), array([ 0.04896058,  0.04483812,  0.08966857, -0.20161924]), array([ 0.04751718,  0.04066462, -0.1036719 ,  0.15989458]), array([ 0.03608145,  0.03677286, -0.00864944, -0.19955532]), array([ 0.01720728,  0.03201352, -0.17617777,  0.14942282]), array([-0.00461583,  0.02372424, -0.03809184, -0.23382355]), array([-0.02447932,  0.00976918, -0.15676744,  0.09325948]), array([-0.03799968, -0.01077833,  0.02339896, -0.29677434]), array([-0.04274161, -0.03600156, -0.07044923,  0.04776911]), array([-0.03840229, -0.06173394,  0.11188697, -0.29948506]), array([-0.02704815, -0.08175761, -0.00103029,  0.10395188]), array([-0.01208312, -0.09002918,  0.14717567, -0.18251961]), array([ 0.00248328, -0.08194469, -0.00402095,  0.26378905]), array([ 0.01347812, -0.05663598,  0.11238667, -0.01308476]), array([ 0.01906687, -0.01709075, -0.05618284,  0.40214629]), array([0.01944171, 0.02938882, 0.06110738, 0.05507872]), array([ 0.0426691 ,  0.00488294,  0.16552386, -0.29198549]), array([ 0.05567946, -0.01270791, -0.03830676,  0.12056844]), array([ 0.05476185, -0.01754592,  0.02903159, -0.16796849]), array([ 0.03988309, -0.00865282, -0.17423833,  0.25254733]), array([ 0.01506354,  0.0092458 , -0.06855153, -0.08010439]), array([ 0.01342235, -0.040504  ,  0.05069643, -0.40863199]), array([ 0.00697918, -0.07935649, -0.11469307,  0.02518724]), array([-0.00404282, -0.10065344,  0.0058336 , -0.23581411]), array([-0.01780205, -0.1019573 , -0.14040012,  0.22036821]), array([-0.03090464, -0.08571047,  0.01233408, -0.06238079]), array([-0.03967834, -0.05746832, -0.09728464,  0.33830588]), array([-0.04088649, -0.02479813,  0.0862282 , -0.01699021]), array([-0.03313408,  0.00555571, -0.00916788,  0.31615044]), array([-0.01709824,  0.0286016 ,  0.16671648, -0.08669091]), array([0.00409761, 0.0426896 , 0.04159804, 0.2280058 ]), array([ 0.02591234,  0.04865704,  0.1720678 , -0.16554347]), array([ 0.04318138,  0.04944889, -0.00259859,  0.17554405]), array([ 0.05182717,  0.04793017,  0.08708201, -0.18877447]), array([ 0.04961378,  0.04616405, -0.10855157,  0.17058545]), array([ 0.03710027,  0.04393717, -0.01427681, -0.19404838]), array([ 0.0171644 ,  0.03955664, -0.18094415,  0.14747835]), array([-0.00543206,  0.03008287, -0.04093621, -0.24363824]), array([-0.02563501,  0.01348145, -0.15733974,  0.07702875]), array([-0.03907693, -0.0106912 ,  0.02462454, -0.31615271]), array([-0.04347682, -0.03975416, -0.06843994,  0.0294576 ]), array([-0.03875691, -0.06868657,  0.11350382, -0.31255978]), array([-0.02718902, -0.09055323, -0.0005972 ,  0.09892028]), array([-0.01229391, -0.09889691,  0.14605862, -0.17821307]), array([ 0.00193427, -0.08911365, -0.00617459,  0.27613969]), array([ 0.01246219, -0.0607399 ,  0.11006833,  0.00460279]), array([ 0.01767613, -0.01746661, -0.05742591,  0.42104822]), array([0.01799889, 0.03256356, 0.06194914, 0.07106617]), array([ 0.04164095,  0.01069004,  0.16882221, -0.28203346]), array([ 0.05552767, -0.00565132, -0.03298584,  0.12304419]), array([ 0.05578172, -0.01071831,  0.0351817 , -0.17251072]), array([ 0.04207756, -0.00327057, -0.16892467,  0.24306336]), array([ 0.01809734,  0.01247845, -0.06570728, -0.09161583]), array([ 0.0166784 , -0.03952956,  0.04996191, -0.41928328]), array([ 0.00970175, -0.08024085, -0.11923689,  0.0174798 ]), array([-0.00255012, -0.1027089 , -0.00170788, -0.23980761]), array([-0.01797844, -0.10448545, -0.14921732,  0.21944907]), array([-0.03279817, -0.08822614,  0.00432766, -0.06160815]), array([-0.0429199 , -0.05980691, -0.10248424,  0.3390746 ]), array([-0.04477409, -0.02707825,  0.08509623, -0.01727879]), array([-0.03680915,  0.00308939, -0.00596657,  0.31465325]), array([-0.01976107,  0.02578306,  0.17342083, -0.08849873]), array([0.00298872, 0.03961152, 0.05010813, 0.22750325]), array([ 0.026514  ,  0.04574731,  0.18032288, -0.16312637]), array([0.04524209, 0.0474135 , 0.00347248, 0.18193809]), array([ 0.0547737 ,  0.04756446,  0.089742  , -0.1786232 ]), array([ 0.052719  ,  0.04808358, -0.10958037,  0.182909  ]), array([ 0.03968097,  0.04832029, -0.01831026, -0.18224004]), array([ 0.01875532,  0.04597667, -0.18654323,  0.15553006]), array([-0.00498113,  0.03750945, -0.04647087, -0.24197424]), array([-0.02615815,  0.02046471, -0.16137018,  0.07087075]), array([-0.04018818, -0.00569015,  0.02283148, -0.32956194]), array([-0.04472263, -0.03796813, -0.06807105,  0.0112597 ]), array([-0.03977193, -0.0707079 ,  0.11527201, -0.33173448]), array([-0.02780187, -0.0961543 ,  0.00147775,  0.08294848]), array([-0.01255879, -0.10704514,  0.14731344, -0.1872195 ]), array([ 0.00179073, -0.09820019, -0.00627177,  0.27594249]), array([ 0.01214555, -0.06893478,  0.10850376,  0.01352591]), array([ 0.0169596 , -0.02313884, -0.05971152,  0.43687334]), array([0.01684516, 0.03045181, 0.06007176, 0.0901481 ]), array([ 0.04025325,  0.01235965,  0.16851984, -0.26398233]), array([ 0.05430388, -0.00079913, -0.030983  ,  0.13630429]), array([ 0.0551963 , -0.00390572,  0.03949108, -0.16640006]), array([ 0.04252198,  0.00399475, -0.1631329 ,  0.24156304]), array([ 0.01972951,  0.01878404, -0.05989374, -0.09935726]), array([-0.00719077,  0.03338913, -0.20317714,  0.23831098]), array([-0.03109278,  0.03970184, -0.03105751, -0.17943795]), array([-0.04602812,  0.03220258, -0.11536638,  0.10315408]), array([-0.04857485,  0.00954666,  0.08942957, -0.32567426]), array([-0.03903633, -0.02389749,  0.00315131, -0.00188288]), array([-0.04739862,  0.00891768, -0.08390808,  0.32277384]), array([-0.04389416,  0.03111565,  0.11862509, -0.10351861]), array([-0.02864332,  0.03893335,  0.03120107,  0.18236794]), array([-0.00497513,  0.0334018 ,  0.2002452 , -0.23260361]), array([0.02107596, 0.02016769, 0.05479172, 0.10615778]), array([ 0.04279093,  0.00657729,  0.15735704, -0.23601811]), array([ 0.05432279, -0.00042662, -0.04430346,  0.16843264]), array([ 0.05270667,  0.0025464 ,  0.02841883, -0.13915784]), array([ 0.03836449,  0.0147418 , -0.16827479,  0.25628195]), array([ 0.01530575,  0.03085196, -0.05733159, -0.10110943]), array([-0.01036427,  0.04347995, -0.19356254,  0.22084265]), array([-0.03187717,  0.04515792, -0.01740894, -0.20714614]), array([-0.04403382,  0.03176144, -0.10197892,  0.07334333]), array([-0.04430096,  0.00366435,  0.09821205, -0.34899642]), array([-0.03373534, -0.03322643,  0.0043413 , -0.01230537]), array([-0.04269608, -0.00097066, -0.0909752 ,  0.32760099]), array([-0.04129243,  0.02356253,  0.10519625, -0.08574262]), array([-0.0290492 ,  0.03574529,  0.01530273,  0.2070179 ]), array([-0.00840644,  0.03516068,  0.18665023, -0.20909091]), array([0.01551767, 0.02588013, 0.04766478, 0.12118061]), array([ 0.03666441,  0.01404583,  0.15895883, -0.23385199]), array([ 0.04938654,  0.006138  , -0.03428356,  0.15758913]), array([ 0.05039664,  0.00595369,  0.04402447, -0.15892806]), array([ 0.03936407,  0.01386988, -0.15158915,  0.23451048]), array([ 0.01933942,  0.0260666 , -0.0444065 , -0.11734339]), array([-0.00445233,  0.03651128, -0.18814468,  0.21589742]), array([-0.02577642,  0.03852623, -0.02095712, -0.1988815 ]), array([-0.03946704,  0.027949  , -0.11335767,  0.09252509]), array([-0.04251502,  0.00429218,  0.08248658, -0.3249713 ]), array([-0.03513879, -0.02796251, -0.01104114,  0.00874986]), array([-0.02023327, -0.06097559,  0.15578729, -0.3303973 ]), array([-0.00269428, -0.08508483,  0.01557024,  0.09560047]), array([ 0.01242213, -0.09227187,  0.13213142, -0.16355619]), array([ 0.02111218, -0.07814076, -0.04633684,  0.30331765]), array([ 0.02185659, -0.04415853,  0.05456546,  0.03100886]), array([ 0.04214847, -0.06553987,  0.14341803, -0.23768561]), array([ 0.0497783 , -0.06563303, -0.06836522,  0.23735732]), array([ 0.04297833, -0.04319393,  0.00232915, -0.01764589]), array([ 0.0506473 , -0.07245873,  0.07174425, -0.26846855]), array([ 0.04334158, -0.07746957, -0.14314117,  0.21749326]), array([ 0.02274164, -0.0586999 , -0.05823584, -0.03594645])]</t>
-  </si>
-  <si>
-    <t>['[2,2,2]', '[0,2,1]', '[1,1,1]', '[2,0,1]', '[1,0,2]', '[2,1,0]', '[1,1,2]', '[1,2,0]', '[0,0,0]', '[0,1,1]']</t>
-  </si>
-  <si>
-    <t>[0,0,0]</t>
-  </si>
-  <si>
-    <t>[18, 36, 47, 49, 64, 77, 78, 83, 94, 95, 99, 110]</t>
-  </si>
-  <si>
-    <t>[0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 1, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 1, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 0, 1, 2, 2, 2, 2, 2, 2, 2, 2, 2, 1, 1, 0, 0, 0, 1, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 1, 1, 2, 2, 2, 2, 2, 2, 2]</t>
-  </si>
-  <si>
-    <t>['[-0.03763371 -0.01533471  0.06554052 -0.01816017]', '[-0.00754409 -0.05458322  0.2277812  -0.36241836]', '[ 0.04879627 -0.15231473  0.32089719 -0.5887683 ]', '[ 0.11397169 -0.27767857  0.31375488 -0.63332862]', '[ 0.16759438 -0.39312519  0.2086893  -0.49480525]', '[ 0.1930193  -0.46685036  0.03906408 -0.22816919]', '[ 0.15689524 -0.41528579 -0.3922057   0.73207416]', '[ 0.04309269 -0.18588535 -0.71796191  1.51055937]', '[-0.1147829   0.15904975 -0.81547211  1.84906375]', '[-0.26363568  0.51494657 -0.63159042  1.62703318]', '[-0.35418658  0.78351571 -0.2539271   1.01663306]', '[-0.36122763  0.91144819  0.18313112  0.25239067]', '[-0.26190848  0.82452699  0.79137833 -1.10754289]', '[-0.05546354  0.48017359  1.23429726 -2.2781243 ]', '[ 0.20909957 -0.04617758  1.33805656 -2.84269804]', '[ 0.4464647  -0.59077472  0.966733   -2.46825376]', '[ 0.57603342 -0.99637145  0.30429255 -1.53991243]', '[ 0.56516121 -1.19760706 -0.40558213 -0.46475241]', '[ 0.42150479 -1.18264964 -1.00130169  0.60348071]', '[ 0.15924444 -0.9077006  -1.57726347  2.11401425]', '[-0.18799992 -0.36248662 -1.82564671  3.22089814]', '[-0.53327972  0.30719603 -1.52676268  3.27468579]', '[-0.7634866   0.87979101 -0.72242334  2.3574156 ]', '[-0.81178112  1.23250584  0.24358186  1.15045355]', '[-0.65237793  1.28191631  1.31555249 -0.65800628]', '[-0.30412131  0.96964969  2.11168739 -2.44394809]', '[ 0.16450696  0.33137373  2.48062933 -3.78391726]', '[ 0.63629358 -0.44093218  2.10712434 -3.676234  ]', '[ 0.96714895 -1.06569583  1.14870367 -2.50122448]', '[ 1.08580741 -1.43610607  0.02961266 -1.20243635]', '[ 0.96306651 -1.49355869 -1.23523013  0.64154627]', '[ 0.60472632 -1.16873957 -2.30588931  2.62992369]', '[ 0.06329632 -0.44654818 -3.01936394  4.46765929]', '[-0.54139703  0.49356173 -2.84847261  4.55057793]', '[-1.02021626  1.26453862 -1.87458951  3.08285849]', '[-1.2800447   1.73398731 -0.71044904  1.64559348]', '[-1.28670758  1.88517073  0.63695814 -0.12925943]', '[-1.03067929  1.67332565  1.90162568 -2.03361294]', '[-0.5378271   1.04795382  2.99108005 -4.26412741]', '[ 1.37457901e-01 -4.01322533e-03  3.59500857e+00 -5.90395343e+00]', '[ 0.80314979 -1.09325615  2.89725705 -4.64870381]', '[ 1.27079156 -1.83981914  1.75769652 -2.87539082]', '[ 1.50133042 -2.26948024  0.54100525 -1.46228765]', '[ 1.4802337  -2.41037852 -0.74683922  0.05689532]', '[ 1.20056143 -2.21731804 -2.02762103  1.91453168]', '[ 0.68368027 -1.61974813 -3.09983703  4.14199644]', '[-0.02394595 -0.53416289 -3.90122802  6.60863039]', '[-0.76041335  0.74668458 -3.21355952  5.6246901 ]', '[-1.28157389  1.68104584 -1.9674046   3.74128911]', '[-1.53080557  2.23143566 -0.53427006  1.83361811]', '[-1.51149409  2.46665579  0.72205762  0.5125925 ]', '[-1.23406306  2.38741273  2.02723365 -1.33797789]', '[-0.71814029  1.91261987  3.07118681 -3.47150504]', '[-0.03048902  0.97330067  3.75584827 -5.9313512 ]', '[ 0.73641709 -0.35878051  3.66284227 -6.78815302]', '[ 1.33862599 -1.52804608  2.28414468 -4.80878919]', '[ 1.65044485 -2.32187188  0.84636742 -3.21551688]', '[ 1.68425315 -2.82987337 -0.48662484 -1.87132694]', '[ 1.45733009 -3.0486566  -1.76908577 -0.31401148]', '[ 0.97751008 -2.93840305 -2.98838339  1.40319016]', '[ 0.29672698 -2.49260926 -3.68400562  3.04518909]', '[-0.43320729 -1.72859259 -3.50015967  4.5500618 ]', '[-1.08041919 -0.70507665 -2.94081074  5.54978146]', '[-1.57996572  0.39647596 -1.94567737  5.20980595]', '[-1.79948323  1.25816516 -0.22014161  3.4048702 ]', '[-1.67801588  1.80552747  1.45821551  1.99285044]', '[-1.20576416  1.97057483  3.2021882  -0.44284683]', '[-0.44007031  1.59324264  4.31722939 -3.37954358]', '[ 0.46499285  0.63280385  4.60420151 -6.00592008]', '[ 1.32471075 -0.59641856  3.79635488 -5.7342423 ]', '[ 1.9478801  -1.56870891  2.45412763 -4.07266882]', '[ 2.32191285 -2.28096059  1.32260148 -3.15105915]', '[ 2.49067743 -2.84880868  0.40437128 -2.53882536]', '[ 2.49851094  2.99268823 -0.29679211 -1.85165512]', '[ 2.36963962  2.72692854 -1.00503606 -0.77175419]', '[ 2.076817    2.71646435 -1.9714475   0.69087315]', '[ 1.56095308  3.00969405 -3.22120669  2.25788423]', '[ 0.80546084 -2.68824181 -4.24358227  3.66461548]', '[-0.07385323 -1.77616211 -4.40598732  5.5013835 ]', '[-0.94373354 -0.452064   -4.22653613  7.50218472]', '[-1.68104525  0.98356781 -2.95827912  6.397391  ]', '[-2.10705696  2.0924769  -1.3270696   4.82670962]', '[-2.23008891  2.94928351  0.0170107   3.77211264]', '[-2.12310172 -2.72159305  0.99824826  2.34258634]', '[-1.83870138 -2.37911537  1.86861602  1.09725022]', '[-1.36457555 -2.26388311  2.88412345  0.14993715]', '[-0.68797902 -2.28113237  3.80110141 -0.1140851 ]', '[ 0.09468317 -2.21096878  3.80592382  1.08151781]', '[ 0.72795206 -1.75263442  2.26912467  3.67557736]', '[ 0.91786459 -0.67876372 -0.36272068  6.99945341]', '[ 0.70853982  0.87301797 -1.23713015  7.76500273]', '[ 0.5400343   2.28334385 -0.48114414  6.52420075]', '[ 0.43913058 -2.67232296 -0.84036298  7.11169483]', '[ 0.07692033 -0.98744618 -2.93636576 10.16276907]', '[-0.52756699  1.08316828 -2.34807965  9.3133326 ]', '[-0.72874082  2.58542861  0.15977191  6.08471601]', '[-0.59392618 -2.58702074  0.86323225  5.36366048]', '[-0.49658788 -1.40745014 -0.08322477  6.7825327 ]', '[-0.63458223  0.18764109 -0.84497223  8.54821969]', '[-0.55185398  1.56014358  1.87312541  4.83367674]', '[0.03046443 2.22581541 3.66453141 2.0631335 ]', '[0.80715358 2.46588939 3.85823462 0.65848899]', '[1.5115622  2.59453692 3.10960772 0.82596163]', '[2.04450621 2.84388996 2.23087354 1.72386588]', '[ 2.40177373 -2.97659511  1.32538937  2.87665105]', '[ 2.5550585  -2.30597136  0.15533222  3.78258368]', '[ 2.44360037 -1.45167381 -1.2820887   4.79153402]', '[ 2.03792214 -0.35301995 -2.77671846  6.27231419]', '[ 1.35783857  1.00453803 -3.92356     6.97525733]', '[ 0.48014473  2.33185946 -4.85957821  6.21936757]', '[-0.52032293 -2.79920529 -4.87436738  5.48703421]', '[-1.39236279 -1.66783757 -3.80198629  5.85839732]', '[-2.06406595 -0.46836831 -2.96776856  6.06366986]']</t>
-  </si>
-  <si>
-    <t>[0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50, 51, 52, 53, 54, 55, 56, 57, 58, 59, 60, 61, 62, 63, 64, 65, 66, 67, 68, 69, 70, 71, 72, 73, 74, 75, 76, 77, 78, 79, 80, 81, 82, 83, 84, 85, 86, 87, 88, 89, 90, 91, 92, 93, 94, 95, 96, 97, 98, 99, 100, 101, 102, 103, 104, 105, 106, 107, 108, 109, 110, 111, 112]</t>
-  </si>
-  <si>
-    <t>[array([-0.03763371, -0.01533471,  0.06554052, -0.01816017], dtype=float32), array([-0.00754409, -0.05458322,  0.2277812 , -0.36241836]), array([ 0.04879627, -0.15231473,  0.32089719, -0.5887683 ]), array([ 0.11397169, -0.27767857,  0.31375488, -0.63332862]), array([ 0.16759438, -0.39312519,  0.2086893 , -0.49480525]), array([ 0.1930193 , -0.46685036,  0.03906408, -0.22816919]), array([ 0.15689524, -0.41528579, -0.3922057 ,  0.73207416]), array([ 0.04309269, -0.18588535, -0.71796191,  1.51055937]), array([-0.1147829 ,  0.15904975, -0.81547211,  1.84906375]), array([-0.26363568,  0.51494657, -0.63159042,  1.62703318]), array([-0.35418658,  0.78351571, -0.2539271 ,  1.01663306]), array([-0.36122763,  0.91144819,  0.18313112,  0.25239067]), array([-0.26190848,  0.82452699,  0.79137833, -1.10754289]), array([-0.05546354,  0.48017359,  1.23429726, -2.2781243 ]), array([ 0.20909957, -0.04617758,  1.33805656, -2.84269804]), array([ 0.4464647 , -0.59077472,  0.966733  , -2.46825376]), array([ 0.57603342, -0.99637145,  0.30429255, -1.53991243]), array([ 0.56516121, -1.19760706, -0.40558213, -0.46475241]), array([ 0.42150479, -1.18264964, -1.00130169,  0.60348071]), array([ 0.15924444, -0.9077006 , -1.57726347,  2.11401425]), array([-0.18799992, -0.36248662, -1.82564671,  3.22089814]), array([-0.53327972,  0.30719603, -1.52676268,  3.27468579]), array([-0.7634866 ,  0.87979101, -0.72242334,  2.3574156 ]), array([-0.81178112,  1.23250584,  0.24358186,  1.15045355]), array([-0.65237793,  1.28191631,  1.31555249, -0.65800628]), array([-0.30412131,  0.96964969,  2.11168739, -2.44394809]), array([ 0.16450696,  0.33137373,  2.48062933, -3.78391726]), array([ 0.63629358, -0.44093218,  2.10712434, -3.676234  ]), array([ 0.96714895, -1.06569583,  1.14870367, -2.50122448]), array([ 1.08580741, -1.43610607,  0.02961266, -1.20243635]), array([ 0.96306651, -1.49355869, -1.23523013,  0.64154627]), array([ 0.60472632, -1.16873957, -2.30588931,  2.62992369]), array([ 0.06329632, -0.44654818, -3.01936394,  4.46765929]), array([-0.54139703,  0.49356173, -2.84847261,  4.55057793]), array([-1.02021626,  1.26453862, -1.87458951,  3.08285849]), array([-1.2800447 ,  1.73398731, -0.71044904,  1.64559348]), array([-1.28670758,  1.88517073,  0.63695814, -0.12925943]), array([-1.03067929,  1.67332565,  1.90162568, -2.03361294]), array([-0.5378271 ,  1.04795382,  2.99108005, -4.26412741]), array([ 1.37457901e-01, -4.01322533e-03,  3.59500857e+00, -5.90395343e+00]), array([ 0.80314979, -1.09325615,  2.89725705, -4.64870381]), array([ 1.27079156, -1.83981914,  1.75769652, -2.87539082]), array([ 1.50133042, -2.26948024,  0.54100525, -1.46228765]), array([ 1.4802337 , -2.41037852, -0.74683922,  0.05689532]), array([ 1.20056143, -2.21731804, -2.02762103,  1.91453168]), array([ 0.68368027, -1.61974813, -3.09983703,  4.14199644]), array([-0.02394595, -0.53416289, -3.90122802,  6.60863039]), array([-0.76041335,  0.74668458, -3.21355952,  5.6246901 ]), array([-1.28157389,  1.68104584, -1.9674046 ,  3.74128911]), array([-1.53080557,  2.23143566, -0.53427006,  1.83361811]), array([-1.51149409,  2.46665579,  0.72205762,  0.5125925 ]), array([-1.23406306,  2.38741273,  2.02723365, -1.33797789]), array([-0.71814029,  1.91261987,  3.07118681, -3.47150504]), array([-0.03048902,  0.97330067,  3.75584827, -5.9313512 ]), array([ 0.73641709, -0.35878051,  3.66284227, -6.78815302]), array([ 1.33862599, -1.52804608,  2.28414468, -4.80878919]), array([ 1.65044485, -2.32187188,  0.84636742, -3.21551688]), array([ 1.68425315, -2.82987337, -0.48662484, -1.87132694]), array([ 1.45733009, -3.0486566 , -1.76908577, -0.31401148]), array([ 0.97751008, -2.93840305, -2.98838339,  1.40319016]), array([ 0.29672698, -2.49260926, -3.68400562,  3.04518909]), array([-0.43320729, -1.72859259, -3.50015967,  4.5500618 ]), array([-1.08041919, -0.70507665, -2.94081074,  5.54978146]), array([-1.57996572,  0.39647596, -1.94567737,  5.20980595]), array([-1.79948323,  1.25816516, -0.22014161,  3.4048702 ]), array([-1.67801588,  1.80552747,  1.45821551,  1.99285044]), array([-1.20576416,  1.97057483,  3.2021882 , -0.44284683]), array([-0.44007031,  1.59324264,  4.31722939, -3.37954358]), array([ 0.46499285,  0.63280385,  4.60420151, -6.00592008]), array([ 1.32471075, -0.59641856,  3.79635488, -5.7342423 ]), array([ 1.9478801 , -1.56870891,  2.45412763, -4.07266882]), array([ 2.32191285, -2.28096059,  1.32260148, -3.15105915]), array([ 2.49067743, -2.84880868,  0.40437128, -2.53882536]), array([ 2.49851094,  2.99268823, -0.29679211, -1.85165512]), array([ 2.36963962,  2.72692854, -1.00503606, -0.77175419]), array([ 2.076817  ,  2.71646435, -1.9714475 ,  0.69087315]), array([ 1.56095308,  3.00969405, -3.22120669,  2.25788423]), array([ 0.80546084, -2.68824181, -4.24358227,  3.66461548]), array([-0.07385323, -1.77616211, -4.40598732,  5.5013835 ]), array([-0.94373354, -0.452064  , -4.22653613,  7.50218472]), array([-1.68104525,  0.98356781, -2.95827912,  6.397391  ]), array([-2.10705696,  2.0924769 , -1.3270696 ,  4.82670962]), array([-2.23008891,  2.94928351,  0.0170107 ,  3.77211264]), array([-2.12310172, -2.72159305,  0.99824826,  2.34258634]), array([-1.83870138, -2.37911537,  1.86861602,  1.09725022]), array([-1.36457555, -2.26388311,  2.88412345,  0.14993715]), array([-0.68797902, -2.28113237,  3.80110141, -0.1140851 ]), array([ 0.09468317, -2.21096878,  3.80592382,  1.08151781]), array([ 0.72795206, -1.75263442,  2.26912467,  3.67557736]), array([ 0.91786459, -0.67876372, -0.36272068,  6.99945341]), array([ 0.70853982,  0.87301797, -1.23713015,  7.76500273]), array([ 0.5400343 ,  2.28334385, -0.48114414,  6.52420075]), array([ 0.43913058, -2.67232296, -0.84036298,  7.11169483]), array([ 0.07692033, -0.98744618, -2.93636576, 10.16276907]), array([-0.52756699,  1.08316828, -2.34807965,  9.3133326 ]), array([-0.72874082,  2.58542861,  0.15977191,  6.08471601]), array([-0.59392618, -2.58702074,  0.86323225,  5.36366048]), array([-0.49658788, -1.40745014, -0.08322477,  6.7825327 ]), array([-0.63458223,  0.18764109, -0.84497223,  8.54821969]), array([-0.55185398,  1.56014358,  1.87312541,  4.83367674]), array([0.03046443, 2.22581541, 3.66453141, 2.0631335 ]), array([0.80715358, 2.46588939, 3.85823462, 0.65848899]), array([1.5115622 , 2.59453692, 3.10960772, 0.82596163]), array([2.04450621, 2.84388996, 2.23087354, 1.72386588]), array([ 2.40177373, -2.97659511,  1.32538937,  2.87665105]), array([ 2.5550585 , -2.30597136,  0.15533222,  3.78258368]), array([ 2.44360037, -1.45167381, -1.2820887 ,  4.79153402]), array([ 2.03792214, -0.35301995, -2.77671846,  6.27231419]), array([ 1.35783857,  1.00453803, -3.92356   ,  6.97525733]), array([ 0.48014473,  2.33185946, -4.85957821,  6.21936757]), array([-0.52032293, -2.79920529, -4.87436738,  5.48703421]), array([-1.39236279, -1.66783757, -3.80198629,  5.85839732]), array([-2.06406595, -0.46836831, -2.96776856,  6.06366986])]</t>
-  </si>
-  <si>
-    <t>['[1,0,2]', '[2,2,2]', '[2,1,0]', '[1,1,2]', '[1,1,1]', '[0,2,1]', '[2,0,1]', '[0,0,0]', '[0,1,1]', '[1,2,0]']</t>
-  </si>
-  <si>
-    <t>[6, 8, 12, 19, 20, 21, 22, 30, 31, 33, 34, 43, 45, 58, 59, 60, 67, 70, 71, 73, 82, 83, 85, 94, 95, 96, 102, 111, 112, 117, 128, 129, 131]</t>
-  </si>
-  <si>
-    <t>[0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 1, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 1, 2, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 1, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 1, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2]</t>
-  </si>
-  <si>
-    <t>['[-0.03763371 -0.01533471  0.06554052 -0.01816017]', '[-0.00754409 -0.05458322  0.2277812  -0.36241836]', '[ 0.04879627 -0.15231473  0.32089719 -0.5887683 ]', '[ 0.11397169 -0.27767857  0.31375488 -0.63332862]', '[ 0.16759438 -0.39312519  0.2086893  -0.49480525]', '[ 0.1930193  -0.46685036  0.03906408 -0.22816919]', '[ 0.18217995 -0.48119372 -0.14531723  0.08492936]', '[ 0.11196576 -0.36927962 -0.54130528  1.01009116]', '[ 0.00196683 -0.16269792 -0.52993942  1.00304703]', '[-0.1149626   0.07904669 -0.60745019  1.35291852]', '[-0.22699932  0.35071699 -0.48106861  1.29899879]', '[-0.29631946  0.57553848 -0.19358874  0.90713479]', '[-0.27608243  0.63826052  0.39000703 -0.28158346]', '[-0.14660044  0.46845261  0.87858312 -1.38237813]', '[ 0.06001055  0.10937558  1.13665873 -2.11809067]', '[ 0.2828729  -0.33128987  1.02900714 -2.16753982]', '[ 0.4487492  -0.71428688  0.58998358 -1.58840327]', '[ 5.08783906e-01 -9.47836991e-01  6.57670123e-04 -7.23251506e-01]', '[ 0.42812906 -0.9408265  -0.7899082   0.78719586]', '[ 0.22660768 -0.70124526 -1.18644062  1.56437558]', '[-0.0263568  -0.34314574 -1.28460498  1.92207522]', '[-0.26097951  0.0218211  -1.0012795   1.61962121]', '[-0.40613597  0.26790834 -0.41633312  0.78247634]', '[-0.44563403  0.38857891  0.03161     0.40144595]', '[-0.36742207  0.35685067  0.73481786 -0.70595441]', '[-0.16386     0.12068077  1.25488947 -1.58960121]', '[ 0.1099716  -0.23964318  1.41437471 -1.89787634]', '[ 0.37325151 -0.59060728  1.15803042 -1.51766191]', '[ 0.55356489 -0.81964832  0.61189373 -0.73482923]', '[ 0.60939796 -0.87663377 -0.06234781  0.17082171]', '[ 0.5293295  -0.75251057 -0.72453044  1.05570257]', '[ 0.33009421 -0.46657273 -1.22742843  1.74836838]', '[ 0.03459996 -0.01999808 -1.65505597  2.59269588]', '[-0.26986464  0.43707099 -1.31436489  1.84704575]', '[-0.46805958  0.68379291 -0.63098221  0.57727808]', '[-0.5371936   0.7235446  -0.04845662 -0.18729085]', '[-0.46237593  0.54641852  0.78477793 -1.56483347]', '[-0.23512649  0.11652082  1.433938   -2.63875815]', '[ 0.07923756 -0.448324    1.61991438 -2.83638306]', '[ 0.37859726 -0.9544924   1.31066304 -2.12294731]', '[ 0.58518284 -1.27464326  0.72495467 -1.05375136]', '[ 0.66038079 -1.37208117  0.01685249  0.08186987]', '[ 0.57168666 -1.18810867 -0.89850397  1.76256027]', '[ 0.32925285 -0.72695759 -1.48658217  2.79932703]', '[-0.02311835 -0.04380535 -1.94392413  3.85455149]', '[-0.37220786  0.64669044 -1.4508563   2.86430069]', '[-0.60251848  1.12292962 -0.8137275   1.8442898 ]', '[-0.68933413  1.37608285 -0.04757277  0.68144166]', '[-0.60445717  1.34284774  0.88039825 -1.01332648]', '[-0.3462104   0.96983573  1.67192988 -2.70784819]', '[ 0.04570236  0.2795464   2.16573386 -4.05232266]', '[ 0.46804558 -0.54637848  1.92177291 -3.93155949]', '[ 0.77286603 -1.21644879  1.07509254 -2.69765239]', '[ 0.88921275 -1.62049107  0.08389033 -1.34676832]', '[ 0.80952273 -1.75628827 -0.86041844 -0.01086601]', '[ 0.54235644 -1.57620015 -1.76610986  1.81627153]', '[ 0.12308577 -1.02940993 -2.37597896  3.62944582]', '[-0.38089077 -0.1618859  -2.5501193   4.81629396]', '[-0.80691954  0.69385678 -1.59372991  3.51014696]', '[-0.99739371  1.21134611 -0.30011358  1.66426235]', '[-0.92958643  1.36260818  0.95980728 -0.15682551]', '[-0.62538364  1.14162397  2.04130197 -2.06884405]', '[-0.13492038  0.53881877  2.78488723 -3.86976927]', '[ 0.43762011 -0.31230171  2.77873655 -4.30532908]', '[ 0.91698011 -1.06359487  1.93034344 -3.07693077]', '[ 1.19348545 -1.53623889  0.81578742 -1.67089042]', '[ 1.23974203 -1.7397523  -0.35385077 -0.36764762]', '[ 1.05524107 -1.67779575 -1.47168336  1.01355014]', '[ 0.64677023 -1.27033855 -2.57231537  3.10238133]', '[ 0.04758069 -0.43528219 -3.32676598  5.1109936 ]', '[-0.58657038  0.55447088 -2.82684576  4.37882095]', '[-1.03639909  1.23023069 -1.62832386  2.35822024]', '[-1.25018387  1.56583835 -0.49623674  1.02240351]', '[-1.21572871  1.59519778  0.83572507 -0.73502484]', '[-0.92031226  1.25871443  2.10071229 -2.67976166]', '[-0.38709773  0.50746947  3.16739105 -4.77150784]', '[ 0.28650778 -0.52985169  3.35947431 -5.13963656]', '[ 0.88640995 -1.40088066  2.55535232 -3.46139053]', '[ 1.29222672 -1.92470069  1.47658442 -1.83332366]', '[ 1.47009071 -2.15374043  0.29310293 -0.48638949]', '[ 1.40148176 -2.10132102 -0.97549083  1.02303887]', '[ 1.07646465 -1.70741093 -2.2596075   2.98348828]', '[ 0.52466426 -0.92764626 -3.21369471  4.82651905]', '[-0.16613696  0.15324241 -3.49331066  5.54123242]', '[-0.80737739  1.1510473  -2.78236389  4.17410652]', '[-1.23845384  1.760434   -1.51398236  1.99764162]', '[-1.42434223  2.0215846  -0.335501    0.64487598]', '[-1.35691512  1.9783239   1.0054958  -1.09102947]', '[-1.02603866  1.56848402  2.28864581 -3.07620597]', '[-0.44896989  0.7154265   3.4423202  -5.46378915]', '[ 0.29418436 -0.50477048  3.73792535 -6.15994257]', '[ 0.95835502 -1.55236548  2.82048769 -4.20341093]', '[ 1.41125509 -2.21236762  1.68967727 -2.48101117]', '[ 1.62925902 -2.56921798  0.48574514 -1.12043989]', '[ 1.60564191 -2.66493168 -0.72011758  0.16818603]', '[ 1.34293956 -2.49511753 -1.8937339   1.55938712]', '[ 0.86053818 -2.02398958 -2.87859518  3.20703578]', '[ 0.19999332 -1.14021948 -3.68393996  5.68382297]', '[-0.57889181  0.19292028 -3.87165335  7.09094965]', '[-1.23602533  1.43671968 -2.5828943   5.14156301]', '[-1.60934536  2.28461819 -1.16192879  3.44161176]', '[-1.70732335  2.83598567  0.16102052  2.08980859]', '[-1.54072629  3.08098966  1.4932751   0.35715185]', '[-1.11356992  2.97930787  2.75256522 -1.36813438]', '[-0.46612111  2.53495994  3.60524555 -3.08161663]', '[ 0.26928636  1.74485863  3.63290329 -4.80643794]', '[ 0.96292614  0.63423462  3.26177468 -6.15249032]', '[ 1.52738292 -0.58361694  2.2296234  -5.67812327]', '[ 1.81152891 -1.5705002   0.56812172 -4.18728199]', '[ 1.7469382  -2.26170402 -1.20980005 -2.69575328]', '[ 1.3348454  -2.6099819  -2.85181002 -0.75185066]', '[ 0.64339073 -2.57820976 -3.9493102   1.04937486]', '[-0.17941731 -2.21311717 -4.0909352   2.50348233]', '[-0.93758569 -1.58950208 -3.38060343  3.57170567]', '[-1.5124707  -0.85015674 -2.35560774  3.68189244]', '[-1.87961155 -0.15552937 -1.3188632   3.21856772]', '[-2.04070272  0.43494418 -0.28432114  2.69097225]', '[-1.95977835  0.85069412  1.12213827  1.42643237]', '[-1.57769135  0.96882768  2.7264003  -0.3811281 ]', '[-0.86938735  0.64029587  4.30521633 -2.96810907]', '[ 0.09044894 -0.15490738  5.05414589 -4.4900479 ]', '[ 1.0396837  -0.90499726  4.24080847 -2.67331524]', '[ 1.74843909 -1.21063302  2.82227193 -0.51596974]', '[ 2.17756521 -1.18303255  1.51952434  0.62262443]', '[ 2.36841531 -0.98681568  0.43735726  1.24894732]', '[ 2.35329366 -0.67022957 -0.5801885   1.92143686]', '[ 2.13110019 -0.20058529 -1.67161297  2.84226116]', '[ 1.67114154  0.48662082 -2.94428238  3.99500446]', '[ 0.98114189  1.27669928 -3.92791183  3.69808664]', '[ 0.12861309  1.86918485 -4.44559547  1.9833347 ]', '[-0.7235377   2.0355201  -3.82908536 -0.45462945]', '[-1.2929414   1.61951997 -1.6833887  -3.70567197]', '[-1.36200164  0.56380312  0.93085664 -6.75930022]', '[-1.03509096 -0.92443243  1.97819532 -7.57269709]', '[-0.64925009 -2.36144114  1.90381176 -6.93099241]', '[-0.22996814  2.4893885   2.43644957 -7.69549161]', '[  0.39090667   0.68490475   3.8129132  -10.60567178]', '[ 1.06453684 -1.3647212   2.28544044 -8.81154113]', '[ 1.24707286 -2.83160702 -0.24271875 -6.1956966 ]', '[ 1.10180222  2.32250645 -0.88816003 -5.39980036]', '[ 0.97982354  1.16258518 -0.22111103 -6.48464922]', '[ 0.9827821  -0.28223175 -0.18774014 -7.364287  ]', '[ 0.68480956 -1.44800873 -2.96349158 -3.89790872]', '[-0.13809832 -1.79774496 -4.88761852  0.20209468]', '[-1.12013345 -1.48246192 -4.67367743  2.61934733]', '[-1.9573707  -0.87320215 -3.67762491  3.23722833]']</t>
-  </si>
-  <si>
-    <t>[0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50, 51, 52, 53, 54, 55, 56, 57, 58, 59, 60, 61, 62, 63, 64, 65, 66, 67, 68, 69, 70, 71, 72, 73, 74, 75, 76, 77, 78, 79, 80, 81, 82, 83, 84, 85, 86, 87, 88, 89, 90, 91, 92, 93, 94, 95, 96, 97, 98, 99, 100, 101, 102, 103, 104, 105, 106, 107, 108, 109, 110, 111, 112, 113, 114, 115, 116, 117, 118, 119, 120, 121, 122, 123, 124, 125, 126, 127, 128, 129, 130, 131, 132, 133, 134, 135, 136, 137, 138, 139, 140, 141, 142, 143, 144, 145]</t>
-  </si>
-  <si>
-    <t>[array([-0.03763371, -0.01533471,  0.06554052, -0.01816017], dtype=float32), array([-0.00754409, -0.05458322,  0.2277812 , -0.36241836]), array([ 0.04879627, -0.15231473,  0.32089719, -0.5887683 ]), array([ 0.11397169, -0.27767857,  0.31375488, -0.63332862]), array([ 0.16759438, -0.39312519,  0.2086893 , -0.49480525]), array([ 0.1930193 , -0.46685036,  0.03906408, -0.22816919]), array([ 0.18217995, -0.48119372, -0.14531723,  0.08492936]), array([ 0.11196576, -0.36927962, -0.54130528,  1.01009116]), array([ 0.00196683, -0.16269792, -0.52993942,  1.00304703]), array([-0.1149626 ,  0.07904669, -0.60745019,  1.35291852]), array([-0.22699932,  0.35071699, -0.48106861,  1.29899879]), array([-0.29631946,  0.57553848, -0.19358874,  0.90713479]), array([-0.27608243,  0.63826052,  0.39000703, -0.28158346]), array([-0.14660044,  0.46845261,  0.87858312, -1.38237813]), array([ 0.06001055,  0.10937558,  1.13665873, -2.11809067]), array([ 0.2828729 , -0.33128987,  1.02900714, -2.16753982]), array([ 0.4487492 , -0.71428688,  0.58998358, -1.58840327]), array([ 5.08783906e-01, -9.47836991e-01,  6.57670123e-04, -7.23251506e-01]), array([ 0.42812906, -0.9408265 , -0.7899082 ,  0.78719586]), array([ 0.22660768, -0.70124526, -1.18644062,  1.56437558]), array([-0.0263568 , -0.34314574, -1.28460498,  1.92207522]), array([-0.26097951,  0.0218211 , -1.0012795 ,  1.61962121]), array([-0.40613597,  0.26790834, -0.41633312,  0.78247634]), array([-0.44563403,  0.38857891,  0.03161   ,  0.40144595]), array([-0.36742207,  0.35685067,  0.73481786, -0.70595441]), array([-0.16386   ,  0.12068077,  1.25488947, -1.58960121]), array([ 0.1099716 , -0.23964318,  1.41437471, -1.89787634]), array([ 0.37325151, -0.59060728,  1.15803042, -1.51766191]), array([ 0.55356489, -0.81964832,  0.61189373, -0.73482923]), array([ 0.60939796, -0.87663377, -0.06234781,  0.17082171]), array([ 0.5293295 , -0.75251057, -0.72453044,  1.05570257]), array([ 0.33009421, -0.46657273, -1.22742843,  1.74836838]), array([ 0.03459996, -0.01999808, -1.65505597,  2.59269588]), array([-0.26986464,  0.43707099, -1.31436489,  1.84704575]), array([-0.46805958,  0.68379291, -0.63098221,  0.57727808]), array([-0.5371936 ,  0.7235446 , -0.04845662, -0.18729085]), array([-0.46237593,  0.54641852,  0.78477793, -1.56483347]), array([-0.23512649,  0.11652082,  1.433938  , -2.63875815]), array([ 0.07923756, -0.448324  ,  1.61991438, -2.83638306]), array([ 0.37859726, -0.9544924 ,  1.31066304, -2.12294731]), array([ 0.58518284, -1.27464326,  0.72495467, -1.05375136]), array([ 0.66038079, -1.37208117,  0.01685249,  0.08186987]), array([ 0.57168666, -1.18810867, -0.89850397,  1.76256027]), array([ 0.32925285, -0.72695759, -1.48658217,  2.79932703]), array([-0.02311835, -0.04380535, -1.94392413,  3.85455149]), array([-0.37220786,  0.64669044, -1.4508563 ,  2.86430069]), array([-0.60251848,  1.12292962, -0.8137275 ,  1.8442898 ]), array([-0.68933413,  1.37608285, -0.04757277,  0.68144166]), array([-0.60445717,  1.34284774,  0.88039825, -1.01332648]), array([-0.3462104 ,  0.96983573,  1.67192988, -2.70784819]), array([ 0.04570236,  0.2795464 ,  2.16573386, -4.05232266]), array([ 0.46804558, -0.54637848,  1.92177291, -3.93155949]), array([ 0.77286603, -1.21644879,  1.07509254, -2.69765239]), array([ 0.88921275, -1.62049107,  0.08389033, -1.34676832]), array([ 0.80952273, -1.75628827, -0.86041844, -0.01086601]), array([ 0.54235644, -1.57620015, -1.76610986,  1.81627153]), array([ 0.12308577, -1.02940993, -2.37597896,  3.62944582]), array([-0.38089077, -0.1618859 , -2.5501193 ,  4.81629396]), array([-0.80691954,  0.69385678, -1.59372991,  3.51014696]), array([-0.99739371,  1.21134611, -0.30011358,  1.66426235]), array([-0.92958643,  1.36260818,  0.95980728, -0.15682551]), array([-0.62538364,  1.14162397,  2.04130197, -2.06884405]), array([-0.13492038,  0.53881877,  2.78488723, -3.86976927]), array([ 0.43762011, -0.31230171,  2.77873655, -4.30532908]), array([ 0.91698011, -1.06359487,  1.93034344, -3.07693077]), array([ 1.19348545, -1.53623889,  0.81578742, -1.67089042]), array([ 1.23974203, -1.7397523 , -0.35385077, -0.36764762]), array([ 1.05524107, -1.67779575, -1.47168336,  1.01355014]), array([ 0.64677023, -1.27033855, -2.57231537,  3.10238133]), array([ 0.04758069, -0.43528219, -3.32676598,  5.1109936 ]), array([-0.58657038,  0.55447088, -2.82684576,  4.37882095]), array([-1.03639909,  1.23023069, -1.62832386,  2.35822024]), array([-1.25018387,  1.56583835, -0.49623674,  1.02240351]), array([-1.21572871,  1.59519778,  0.83572507, -0.73502484]), array([-0.92031226,  1.25871443,  2.10071229, -2.67976166]), array([-0.38709773,  0.50746947,  3.16739105, -4.77150784]), array([ 0.28650778, -0.52985169,  3.35947431, -5.13963656]), array([ 0.88640995, -1.40088066,  2.55535232, -3.46139053]), array([ 1.29222672, -1.92470069,  1.47658442, -1.83332366]), array([ 1.47009071, -2.15374043,  0.29310293, -0.48638949]), array([ 1.40148176, -2.10132102, -0.97549083,  1.02303887]), array([ 1.07646465, -1.70741093, -2.2596075 ,  2.98348828]), array([ 0.52466426, -0.92764626, -3.21369471,  4.82651905]), array([-0.16613696,  0.15324241, -3.49331066,  5.54123242]), array([-0.80737739,  1.1510473 , -2.78236389,  4.17410652]), array([-1.23845384,  1.760434  , -1.51398236,  1.99764162]), array([-1.42434223,  2.0215846 , -0.335501  ,  0.64487598]), array([-1.35691512,  1.9783239 ,  1.0054958 , -1.09102947]), array([-1.02603866,  1.56848402,  2.28864581, -3.07620597]), array([-0.44896989,  0.7154265 ,  3.4423202 , -5.46378915]), array([ 0.29418436, -0.50477048,  3.73792535, -6.15994257]), array([ 0.95835502, -1.55236548,  2.82048769, -4.20341093]), array([ 1.41125509, -2.21236762,  1.68967727, -2.48101117]), array([ 1.62925902, -2.56921798,  0.48574514, -1.12043989]), array([ 1.60564191, -2.66493168, -0.72011758,  0.16818603]), array([ 1.34293956, -2.49511753, -1.8937339 ,  1.55938712]), array([ 0.86053818, -2.02398958, -2.87859518,  3.20703578]), array([ 0.19999332, -1.14021948, -3.68393996,  5.68382297]), array([-0.57889181,  0.19292028, -3.87165335,  7.09094965]), array([-1.23602533,  1.43671968, -2.5828943 ,  5.14156301]), array([-1.60934536,  2.28461819, -1.16192879,  3.44161176]), array([-1.70732335,  2.83598567,  0.16102052,  2.08980859]), array([-1.54072629,  3.08098966,  1.4932751 ,  0.35715185]), array([-1.11356992,  2.97930787,  2.75256522, -1.36813438]), array([-0.46612111,  2.53495994,  3.60524555, -3.08161663]), array([ 0.26928636,  1.74485863,  3.63290329, -4.80643794]), array([ 0.96292614,  0.63423462,  3.26177468, -6.15249032]), array([ 1.52738292, -0.58361694,  2.2296234 , -5.67812327]), array([ 1.81152891, -1.5705002 ,  0.56812172, -4.18728199]), array([ 1.7469382 , -2.26170402, -1.20980005, -2.69575328]), array([ 1.3348454 , -2.6099819 , -2.85181002, -0.75185066]), array([ 0.64339073, -2.57820976, -3.9493102 ,  1.04937486]), array([-0.17941731, -2.21311717, -4.0909352 ,  2.50348233]), array([-0.93758569, -1.58950208, -3.38060343,  3.57170567]), array([-1.5124707 , -0.85015674, -2.35560774,  3.68189244]), array([-1.87961155, -0.15552937, -1.3188632 ,  3.21856772]), array([-2.04070272,  0.43494418, -0.28432114,  2.69097225]), array([-1.95977835,  0.85069412,  1.12213827,  1.42643237]), array([-1.57769135,  0.96882768,  2.7264003 , -0.3811281 ]), array([-0.86938735,  0.64029587,  4.30521633, -2.96810907]), array([ 0.09044894, -0.15490738,  5.05414589, -4.4900479 ]), array([ 1.0396837 , -0.90499726,  4.24080847, -2.67331524]), array([ 1.74843909, -1.21063302,  2.82227193, -0.51596974]), array([ 2.17756521, -1.18303255,  1.51952434,  0.62262443]), array([ 2.36841531, -0.98681568,  0.43735726,  1.24894732]), array([ 2.35329366, -0.67022957, -0.5801885 ,  1.92143686]), array([ 2.13110019, -0.20058529, -1.67161297,  2.84226116]), array([ 1.67114154,  0.48662082, -2.94428238,  3.99500446]), array([ 0.98114189,  1.27669928, -3.92791183,  3.69808664]), array([ 0.12861309,  1.86918485, -4.44559547,  1.9833347 ]), array([-0.7235377 ,  2.0355201 , -3.82908536, -0.45462945]), array([-1.2929414 ,  1.61951997, -1.6833887 , -3.70567197]), array([-1.36200164,  0.56380312,  0.93085664, -6.75930022]), array([-1.03509096, -0.92443243,  1.97819532, -7.57269709]), array([-0.64925009, -2.36144114,  1.90381176, -6.93099241]), array([-0.22996814,  2.4893885 ,  2.43644957, -7.69549161]), array([  0.39090667,   0.68490475,   3.8129132 , -10.60567178]), array([ 1.06453684, -1.3647212 ,  2.28544044, -8.81154113]), array([ 1.24707286, -2.83160702, -0.24271875, -6.1956966 ]), array([ 1.10180222,  2.32250645, -0.88816003, -5.39980036]), array([ 0.97982354,  1.16258518, -0.22111103, -6.48464922]), array([ 0.9827821 , -0.28223175, -0.18774014, -7.364287  ]), array([ 0.68480956, -1.44800873, -2.96349158, -3.89790872]), array([-0.13809832, -1.79774496, -4.88761852,  0.20209468]), array([-1.12013345, -1.48246192, -4.67367743,  2.61934733]), array([-1.9573707 , -0.87320215, -3.67762491,  3.23722833])]</t>
-  </si>
-  <si>
-    <t>['[2,1,0]', '[0,0,0]', '[1,1,2]', '[2,2,2]', '[1,2,0]', '[0,1,1]', '[2,0,1]', '[1,1,1]', '[0,2,1]', '[1,0,2]']</t>
-  </si>
-  <si>
-    <t>[9, 10, 17, 19, 20, 21, 28, 31, 32, 33, 40, 44, 45, 52, 54, 57, 58, 66, 67, 68, 69, 71, 80, 82, 83, 84, 92, 93, 94, 96, 99, 108, 109, 110, 111, 112, 123, 124, 127, 129, 138, 140, 189, 190, 191]</t>
-  </si>
-  <si>
-    <t>[0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 1, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 1, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 1, 2, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 1, 1, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 1, 2, 2, 1, 1, 2]</t>
-  </si>
-  <si>
-    <t>['[-0.03763371 -0.01533471  0.06554052 -0.01816017]', '[-0.00754409 -0.05458322  0.2277812  -0.36241836]', '[ 0.04879627 -0.15231473  0.32089719 -0.5887683 ]', '[ 0.11397169 -0.27767857  0.31375488 -0.63332862]', '[ 0.16759438 -0.39312519  0.2086893  -0.49480525]', '[ 0.1930193  -0.46685036  0.03906408 -0.22816919]', '[ 0.15689524 -0.41528579 -0.3922057   0.73207416]', '[ 0.04309269 -0.18588535 -0.71796191  1.51055937]', '[-0.1147829   0.15904975 -0.81547211  1.84906375]', '[-0.2381273   0.44851804 -0.38784747  0.98599673]', '[-0.26296246  0.53949711  0.14366776 -0.08777355]', '[-0.18296693  0.41542063  0.63941254 -1.12823447]', '[-0.01861693  0.10718851  0.96297069 -1.87959368]', '[ 0.18082637 -0.29580631  0.97461625 -2.04046847]', '[ 0.3491769  -0.66675695  0.66702808 -1.59060734]', '[ 0.43570263 -0.91035427  0.18260391 -0.815275  ]', '[ 0.4201151  -0.98674762 -0.33349637  0.05425987]', '[ 0.30767154 -0.89124399 -0.76930771  0.88269759]', '[ 0.10065104 -0.58385702 -1.26419094  2.14426115]', '[-0.15090413 -0.13563915 -1.18514843  2.21439636]', '[-0.34649311  0.25036895 -0.71855632  1.54587325]', '[-0.42371905  0.455052   -0.03697758  0.46646393]', '[-0.36042303  0.43204067  0.65706944 -0.68683974]', '[-0.17156608  0.19290365  1.1895331  -1.64367632]', '[ 0.09217645 -0.1875751   1.38008833 -2.0437852 ]', '[ 0.3515183  -0.57403145  1.15131306 -1.71774348]', '[ 0.53250771 -0.84431894  0.62463244 -0.94143198]', '[ 0.59260395 -0.94109297 -0.03287788 -0.01730499]', '[ 0.51976578 -0.85111411 -0.6831114   0.90695032]', '[ 0.30487163 -0.52434002 -1.42950429  2.31776665]', '[-0.02795906  0.03781536 -1.81176821  3.14307476]', '[-0.35199335  0.58498126 -1.3491245   2.18548904]', '[-0.54622909  0.88003421 -0.5633241   0.73372138]', '[-0.57066184  0.87431653  0.32349544 -0.79091819]', '[-0.41933937  0.56671192  1.16734798 -2.25565718]', '[-1.22199564e-01  2.03466291e-03  1.72640766e+00 -3.24617809e+00]', '[ 0.22914021 -0.64878515  1.68696123 -3.06790788]', '[ 0.52073243 -1.16906653  1.17894544 -2.06636233]', '[ 0.68763208 -1.46443855  0.47062166 -0.88031834]', '[ 0.70484241 -1.52084908 -0.29890118  0.31565421]', '[ 0.57150184 -1.33822243 -1.01656132  1.50751978]', '[ 0.2880091  -0.86516662 -1.7877492   3.20710703]', '[-0.12098208 -0.08759172 -2.19759716  4.367181  ]', '[-0.53109398  0.75888299 -1.77512804  3.84327148]', '[-0.77887715  1.34110278 -0.68604249  1.97646851]', '[-0.80593294  1.55678091  0.40441269  0.19178119]', '[-0.62485977  1.41780701  1.37926368 -1.5886773 ]', '[-0.26772677  0.91841281  2.15056546 -3.38949569]', '[ 0.20880724  0.09771833  2.49865453 -4.59142262]', '[ 0.66660537 -0.78250419  1.94521194 -3.94517315]', '[ 0.95539291 -1.43103735  0.91109256 -2.52065477]', '[ 1.0266461  -1.79489119 -0.19637739 -1.12578332]', '[ 0.88245784 -1.88084282 -1.21783089  0.27293018]', '[ 0.54131827 -1.63581451 -2.13823171  2.1879325 ]', '[ 0.07011501 -1.05861047 -2.50435886  3.52635405]', '[-0.45054423 -0.21425643 -2.59318343  4.69580813]', '[-0.90587493  0.68777886 -1.82993539  4.0612262 ]', '[-1.13126557  1.30496374 -0.41348157  2.11994174]', '[-1.07446597  1.54230151  0.96210847  0.24897019]', '[-0.75915152  1.39500369  2.14636172 -1.75248552]', '[-0.23876625  0.8332384   2.98810319 -3.83270597]', '[ 0.39361261 -0.07265814  3.17318187 -4.88454596]', '[ 0.95633272 -0.95938476  2.33556509 -3.75977997]', '[ 1.30686501 -1.55881906  1.15040492 -2.26594063]', '[ 1.41304553 -1.87993266 -0.09143028 -0.95965126]', '[ 1.25697437 -1.89386881 -1.45272418  0.8498784 ]', '[ 0.8584624  -1.56727218 -2.49184881  2.46252139]', '[ 0.28263753 -0.89807429 -3.19309146  4.18730509]', '[-0.37148507  0.02894894 -3.17570673  4.7144193 ]', '[-0.91503302  0.83011968 -2.15294614  3.10298428]', '[-1.23633573  1.31537264 -1.03555989  1.76117848]', '[-1.30633306  1.49255026  0.334074    0.02637861]', '[-1.10497389  1.32004565  1.66819558 -1.79215503]', '[-0.64687973  0.75446524  2.87571977 -3.88143239]', '[ 0.00985097 -0.18259125  3.51935422 -5.1271001 ]', '[ 0.67633582 -1.10887285  3.00271877 -3.86282789]', '[ 1.18133299 -1.70229116  2.0057412  -2.10852469]', '[ 1.46754643 -1.97625966  0.84013701 -0.68223521]', '[ 1.50671239 -1.96601705 -0.45074676  0.77571825]', '[ 1.27977388 -1.63506726 -1.81653561  2.58984209]', '[ 0.80159929 -0.95071063 -2.93719438  4.29275203]', '[ 0.11003784  0.11098757 -3.80518177  5.95273041]', '[-0.59842599  1.14106567 -3.12998143  4.04738161]', '[-1.11623566  1.7157637  -2.00773095  1.75746301]', '[-1.38821159  1.87103649 -0.68915564 -0.15287521]', '[-1.38623312  1.66587976  0.71712543 -1.90139311]', '[-1.09907486  1.09495332  2.1576119  -3.87566532]', '[-0.53037107  0.10227397  3.42708859 -5.86531647]', '[ 0.18480037 -1.05328553  3.52321089 -5.22858616]', '[ 0.83392313 -1.90657183  2.90344463 -3.29354084]', '[ 1.32177563 -2.39079188  1.92436052 -1.60688397]', '[ 1.59082613 -2.56858432  0.75135944 -0.20486863]', '[ 1.62018599 -2.48090557 -0.45966976  1.07550928]', '[ 1.40701104 -2.13392093 -1.66724353  2.42867677]', '[ 0.95807386 -1.48474262 -2.80420799  4.14493997]', '[ 0.2748991  -0.39356119 -3.94756582  6.65095108]', '[-0.49610327  0.88094473 -3.51172556  5.51614611]', '[-1.10368151  1.78184797 -2.52161059  3.51167087]', '[-1.49494817  2.31858241 -1.37322542  1.92710611]', '[-1.63636079  2.53017763 -0.04029277  0.21302102]', '[-1.51142875  2.40427524  1.28704031 -1.49201715]', '[-1.1247418   1.91496404  2.56457292 -3.48194735]', '[-0.49195666  0.9654029   3.74818203 -6.1058287 ]', '[ 0.32956865 -0.44470462  4.17219266 -7.2954569 ]', '[ 1.06318845 -1.68778546  3.07977839 -5.01454193]', '[ 1.55883621 -2.50005005  1.87192212 -3.22825334]', '[ 1.8122808  -3.00830495  0.67242104 -1.88682186]', '[ 1.83245966  3.02530002 -0.46505199 -0.6059955 ]', '[ 1.62479008  3.03452431 -1.62032492  0.70113758]', '[ 1.18313083 -2.97678705 -2.77605818  2.02353334]', '[ 0.53959517 -2.43241586 -3.54914883  3.4488449 ]', '[-0.18302087 -1.59045309 -3.57345623  4.95059451]', '[-0.86061706 -0.49319973 -3.11391686  5.7804869 ]', '[-1.39430162  0.63464996 -2.07757639  5.17838957]', '[-1.6549676   1.52281299 -0.49306071  3.69715068]', '[-1.58531895  2.11372823  1.18665159  2.18058156]', '[-1.17941155  2.33311067  2.80658478 -0.03199028]', '[-0.50155029  2.08676722  3.83865673 -2.44842902]', '[ 0.29430502  1.36135065  3.99755141 -4.7356701 ]', '[ 1.06246021  0.25799625  3.58025967 -5.98056787]', '[ 1.66652147 -0.86254525  2.35770195 -4.98300158]', '[ 1.99263418 -1.72833412  0.89974613 -3.73528549]', '[ 2.02506958 -2.36900622 -0.57282603 -2.65716675]', '[ 1.76865768 -2.77404536 -1.97261082 -1.34400953]', '[ 1.2436354  -2.89169717 -3.24845543  0.18295228]', '[ 0.48306929 -2.66464636 -4.23321518  2.06546259]', '[-0.37633867 -2.08069845 -4.17462358  3.70528079]', '[-1.11735031 -1.27814029 -3.16734784  4.13812671]', '[-1.6532765  -0.44050634 -2.18266158  4.11000442]', '[-1.95900089  0.26234374 -0.86662046  2.88889563]', '[-2.02365973  0.78577958  0.24500894  2.32758046]', '[-1.84374205  1.16955425  1.60674508  1.401168  ]', '[-1.34666708  1.23261059  3.35842542 -0.9338591 ]', '[-0.52113188  0.7385886   4.79254456 -4.01589937]', '[ 0.49500537 -0.25446343  5.09272008 -5.26573435]', '[ 1.41300234 -1.11408571  3.96953905 -3.13026121]', '[ 2.07772032 -1.54554879  2.70978305 -1.37280449]', '[ 2.51896446 -1.73751603  1.76869297 -0.70606121]', '[ 2.81099789 -1.87743325  1.21120555 -0.7880734 ]', '[ 3.01494136 -2.05713374  0.86904055 -1.05910534]', '[-3.10480656 -2.33500051  0.79234486 -1.73512532]', '[-2.94071695 -2.75299031  0.88370259 -2.44427305]', '[-2.73174896  2.97132159  1.27365504 -3.15119627]', '[-2.3999549   2.25952019  2.12488485 -4.03614081]', '[-1.85013677  1.3028724   3.46226932 -5.75405989]', '[-0.98461313 -0.12109388  5.09045847 -8.16641509]', '[ 0.07717611 -1.62144335  5.34746133 -6.24084101]', '[ 1.12128481 -2.59043982  4.94928854 -3.56856159]', '[ 2.006144   -3.11811948  3.86656458 -1.87939063]', '[ 2.69075349  2.88402785  3.08765578 -1.06457826]', '[-2.99328875  2.68605118  3.03549064 -1.0656074 ]', '[-2.32872778  2.39062232  3.72480442 -2.09619875]', '[-1.46964774  1.748491    4.91684764 -4.63205699]', '[-0.34800848  0.418817    6.25089278 -8.55234827]', '[ 0.884549   -1.21678763  5.71589956 -6.74503445]', '[ 1.91491107 -2.223428    4.61328881 -3.60900179]', '[ 2.75051431 -2.78436299  3.8431826  -2.28178298]', '[-2.77593878  3.05280219  3.88137515 -2.40525774]', '[-1.92381485  2.44420448  4.73998201 -3.96878159]', '[-0.86139855  1.32748336  5.93605371 -7.5811984 ]', '[ 0.43964228 -0.56138252  6.64777209 -9.92698902]', '[ 1.64487768 -2.14336713  5.42792147 -5.95550879]', '[ 2.64192812 -3.12465846  4.6167861  -4.26909462]', '[-2.74046123  2.29699943  4.56106379 -4.67697546]', '[-1.74411169  1.13904148  5.61543679 -7.33784204]', '[-0.45565198 -0.65027233  6.97448172 -9.37141959]', '[ 0.91930756 -2.11455512  6.65422807 -5.04462968]', '[ 2.15564737 -2.78628936  5.64276524 -2.06793475]', '[-3.06959112 -3.08555837  5.13649879 -1.28361668]', '[-1.98674429  2.85458596  5.87289483 -2.50640932]', '[-0.69956068  2.04560535  6.89027488 -6.0078347 ]', '[  0.72481405   0.33409134   7.24582015 -10.65584454]', '[ 2.03849627 -1.57399264  5.69650794 -7.55014915]', '[ 3.10421709 -2.86038928  5.18405448 -5.857632  ]', '[-2.10287876  2.17009472  5.73585456 -7.2428464 ]', '[ -0.7941752    0.25836736   7.43882181 -11.8332779 ]', '[ 0.68072447 -1.84741012  6.92863644 -7.87039209]', '[ 1.99626546 -3.05737623  6.13336206 -4.81196409]', '[ 3.14022226  2.30989669  5.46502377 -4.79463785]', '[-2.00900591  1.1316539   6.16321104 -7.47025236]', '[-0.61100025 -0.69328018  7.56560837 -9.48705405]', '[ 0.89806119 -2.12300177  7.35053247 -4.52024441]', '[ 2.25296603 -2.61982045  6.10452651 -0.86832134]', '[-2.91060765 -2.61508448  5.26543868  0.58432848]', '[-1.85865349 -2.46304237  5.37247295  0.87631594]', '[-0.76273859 -2.20792428  5.396329    2.0411736 ]', '[ 0.13609173 -1.44642114  3.10745277  6.03861305]', '[0.39465388 0.27258875 0.34186013 9.84012537]', '[0.71657842 1.88124406 3.11840475 5.92930537]', '[1.50402264 2.84091927 4.24240785 4.35163346]', '[ 2.23870687 -2.4520518   2.59522781  5.94942563]', '[ 2.40824128 -0.99166096 -0.88376984  8.70851611]', '[ 2.04162885  0.94746185 -2.0831073   9.88934034]']</t>
-  </si>
-  <si>
-    <t>[0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50, 51, 52, 53, 54, 55, 56, 57, 58, 59, 60, 61, 62, 63, 64, 65, 66, 67, 68, 69, 70, 71, 72, 73, 74, 75, 76, 77, 78, 79, 80, 81, 82, 83, 84, 85, 86, 87, 88, 89, 90, 91, 92, 93, 94, 95, 96, 97, 98, 99, 100, 101, 102, 103, 104, 105, 106, 107, 108, 109, 110, 111, 112, 113, 114, 115, 116, 117, 118, 119, 120, 121, 122, 123, 124, 125, 126, 127, 128, 129, 130, 131, 132, 133, 134, 135, 136, 137, 138, 139, 140, 141, 142, 143, 144, 145, 146, 147, 148, 149, 150, 151, 152, 153, 154, 155, 156, 157, 158, 159, 160, 161, 162, 163, 164, 165, 166, 167, 168, 169, 170, 171, 172, 173, 174, 175, 176, 177, 178, 179, 180, 181, 182, 183, 184, 185, 186, 187, 188, 189, 190, 191, 192]</t>
-  </si>
-  <si>
-    <t>[array([-0.03763371, -0.01533471,  0.06554052, -0.01816017], dtype=float32), array([-0.00754409, -0.05458322,  0.2277812 , -0.36241836]), array([ 0.04879627, -0.15231473,  0.32089719, -0.5887683 ]), array([ 0.11397169, -0.27767857,  0.31375488, -0.63332862]), array([ 0.16759438, -0.39312519,  0.2086893 , -0.49480525]), array([ 0.1930193 , -0.46685036,  0.03906408, -0.22816919]), array([ 0.15689524, -0.41528579, -0.3922057 ,  0.73207416]), array([ 0.04309269, -0.18588535, -0.71796191,  1.51055937]), array([-0.1147829 ,  0.15904975, -0.81547211,  1.84906375]), array([-0.2381273 ,  0.44851804, -0.38784747,  0.98599673]), array([-0.26296246,  0.53949711,  0.14366776, -0.08777355]), array([-0.18296693,  0.41542063,  0.63941254, -1.12823447]), array([-0.01861693,  0.10718851,  0.96297069, -1.87959368]), array([ 0.18082637, -0.29580631,  0.97461625, -2.04046847]), array([ 0.3491769 , -0.66675695,  0.66702808, -1.59060734]), array([ 0.43570263, -0.91035427,  0.18260391, -0.815275  ]), array([ 0.4201151 , -0.98674762, -0.33349637,  0.05425987]), array([ 0.30767154, -0.89124399, -0.76930771,  0.88269759]), array([ 0.10065104, -0.58385702, -1.26419094,  2.14426115]), array([-0.15090413, -0.13563915, -1.18514843,  2.21439636]), array([-0.34649311,  0.25036895, -0.71855632,  1.54587325]), array([-0.42371905,  0.455052  , -0.03697758,  0.46646393]), array([-0.36042303,  0.43204067,  0.65706944, -0.68683974]), array([-0.17156608,  0.19290365,  1.1895331 , -1.64367632]), array([ 0.09217645, -0.1875751 ,  1.38008833, -2.0437852 ]), array([ 0.3515183 , -0.57403145,  1.15131306, -1.71774348]), array([ 0.53250771, -0.84431894,  0.62463244, -0.94143198]), array([ 0.59260395, -0.94109297, -0.03287788, -0.01730499]), array([ 0.51976578, -0.85111411, -0.6831114 ,  0.90695032]), array([ 0.30487163, -0.52434002, -1.42950429,  2.31776665]), array([-0.02795906,  0.03781536, -1.81176821,  3.14307476]), array([-0.35199335,  0.58498126, -1.3491245 ,  2.18548904]), array([-0.54622909,  0.88003421, -0.5633241 ,  0.73372138]), array([-0.57066184,  0.87431653,  0.32349544, -0.79091819]), array([-0.41933937,  0.56671192,  1.16734798, -2.25565718]), array([-1.22199564e-01,  2.03466291e-03,  1.72640766e+00, -3.24617809e+00]), array([ 0.22914021, -0.64878515,  1.68696123, -3.06790788]), array([ 0.52073243, -1.16906653,  1.17894544, -2.06636233]), array([ 0.68763208, -1.46443855,  0.47062166, -0.88031834]), array([ 0.70484241, -1.52084908, -0.29890118,  0.31565421]), array([ 0.57150184, -1.33822243, -1.01656132,  1.50751978]), array([ 0.2880091 , -0.86516662, -1.7877492 ,  3.20710703]), array([-0.12098208, -0.08759172, -2.19759716,  4.367181  ]), array([-0.53109398,  0.75888299, -1.77512804,  3.84327148]), array([-0.77887715,  1.34110278, -0.68604249,  1.97646851]), array([-0.80593294,  1.55678091,  0.40441269,  0.19178119]), array([-0.62485977,  1.41780701,  1.37926368, -1.5886773 ]), array([-0.26772677,  0.91841281,  2.15056546, -3.38949569]), array([ 0.20880724,  0.09771833,  2.49865453, -4.59142262]), array([ 0.66660537, -0.78250419,  1.94521194, -3.94517315]), array([ 0.95539291, -1.43103735,  0.91109256, -2.52065477]), array([ 1.0266461 , -1.79489119, -0.19637739, -1.12578332]), array([ 0.88245784, -1.88084282, -1.21783089,  0.27293018]), array([ 0.54131827, -1.63581451, -2.13823171,  2.1879325 ]), array([ 0.07011501, -1.05861047, -2.50435886,  3.52635405]), array([-0.45054423, -0.21425643, -2.59318343,  4.69580813]), array([-0.90587493,  0.68777886, -1.82993539,  4.0612262 ]), array([-1.13126557,  1.30496374, -0.41348157,  2.11994174]), array([-1.07446597,  1.54230151,  0.96210847,  0.24897019]), array([-0.75915152,  1.39500369,  2.14636172, -1.75248552]), array([-0.23876625,  0.8332384 ,  2.98810319, -3.83270597]), array([ 0.39361261, -0.07265814,  3.17318187, -4.88454596]), array([ 0.95633272, -0.95938476,  2.33556509, -3.75977997]), array([ 1.30686501, -1.55881906,  1.15040492, -2.26594063]), array([ 1.41304553, -1.87993266, -0.09143028, -0.95965126]), array([ 1.25697437, -1.89386881, -1.45272418,  0.8498784 ]), array([ 0.8584624 , -1.56727218, -2.49184881,  2.46252139]), array([ 0.28263753, -0.89807429, -3.19309146,  4.18730509]), array([-0.37148507,  0.02894894, -3.17570673,  4.7144193 ]), array([-0.91503302,  0.83011968, -2.15294614,  3.10298428]), array([-1.23633573,  1.31537264, -1.03555989,  1.76117848]), array([-1.30633306,  1.49255026,  0.334074  ,  0.02637861]), array([-1.10497389,  1.32004565,  1.66819558, -1.79215503]), array([-0.64687973,  0.75446524,  2.87571977, -3.88143239]), array([ 0.00985097, -0.18259125,  3.51935422, -5.1271001 ]), array([ 0.67633582, -1.10887285,  3.00271877, -3.86282789]), array([ 1.18133299, -1.70229116,  2.0057412 , -2.10852469]), array([ 1.46754643, -1.97625966,  0.84013701, -0.68223521]), array([ 1.50671239, -1.96601705, -0.45074676,  0.77571825]), array([ 1.27977388, -1.63506726, -1.81653561,  2.58984209]), array([ 0.80159929, -0.95071063, -2.93719438,  4.29275203]), array([ 0.11003784,  0.11098757, -3.80518177,  5.95273041]), array([-0.59842599,  1.14106567, -3.12998143,  4.04738161]), array([-1.11623566,  1.7157637 , -2.00773095,  1.75746301]), array([-1.38821159,  1.87103649, -0.68915564, -0.15287521]), array([-1.38623312,  1.66587976,  0.71712543, -1.90139311]), array([-1.09907486,  1.09495332,  2.1576119 , -3.87566532]), array([-0.53037107,  0.10227397,  3.42708859, -5.86531647]), array([ 0.18480037, -1.05328553,  3.52321089, -5.22858616]), array([ 0.83392313, -1.90657183,  2.90344463, -3.29354084]), array([ 1.32177563, -2.39079188,  1.92436052, -1.60688397]), array([ 1.59082613, -2.56858432,  0.75135944, -0.20486863]), array([ 1.62018599, -2.48090557, -0.45966976,  1.07550928]), array([ 1.40701104, -2.13392093, -1.66724353,  2.42867677]), array([ 0.95807386, -1.48474262, -2.80420799,  4.14493997]), array([ 0.2748991 , -0.39356119, -3.94756582,  6.65095108]), array([-0.49610327,  0.88094473, -3.51172556,  5.51614611]), array([-1.10368151,  1.78184797, -2.52161059,  3.51167087]), array([-1.49494817,  2.31858241, -1.37322542,  1.92710611]), array([-1.63636079,  2.53017763, -0.04029277,  0.21302102]), array([-1.51142875,  2.40427524,  1.28704031, -1.49201715]), array([-1.1247418 ,  1.91496404,  2.56457292, -3.48194735]), array([-0.49195666,  0.9654029 ,  3.74818203, -6.1058287 ]), array([ 0.32956865, -0.44470462,  4.17219266, -7.2954569 ]), array([ 1.06318845, -1.68778546,  3.07977839, -5.01454193]), array([ 1.55883621, -2.50005005,  1.87192212, -3.22825334]), array([ 1.8122808 , -3.00830495,  0.67242104, -1.88682186]), array([ 1.83245966,  3.02530002, -0.46505199, -0.6059955 ]), array([ 1.62479008,  3.03452431, -1.62032492,  0.70113758]), array([ 1.18313083, -2.97678705, -2.77605818,  2.02353334]), array([ 0.53959517, -2.43241586, -3.54914883,  3.4488449 ]), array([-0.18302087, -1.59045309, -3.57345623,  4.95059451]), array([-0.86061706, -0.49319973, -3.11391686,  5.7804869 ]), array([-1.39430162,  0.63464996, -2.07757639,  5.17838957]), array([-1.6549676 ,  1.52281299, -0.49306071,  3.69715068]), array([-1.58531895,  2.11372823,  1.18665159,  2.18058156]), array([-1.17941155,  2.33311067,  2.80658478, -0.03199028]), array([-0.50155029,  2.08676722,  3.83865673, -2.44842902]), array([ 0.29430502,  1.36135065,  3.99755141, -4.7356701 ]), array([ 1.06246021,  0.25799625,  3.58025967, -5.98056787]), array([ 1.66652147, -0.86254525,  2.35770195, -4.98300158]), array([ 1.99263418, -1.72833412,  0.89974613, -3.73528549]), array([ 2.02506958, -2.36900622, -0.57282603, -2.65716675]), array([ 1.76865768, -2.77404536, -1.97261082, -1.34400953]), array([ 1.2436354 , -2.89169717, -3.24845543,  0.18295228]), array([ 0.48306929, -2.66464636, -4.23321518,  2.06546259]), array([-0.37633867, -2.08069845, -4.17462358,  3.70528079]), array([-1.11735031, -1.27814029, -3.16734784,  4.13812671]), array([-1.6532765 , -0.44050634, -2.18266158,  4.11000442]), array([-1.95900089,  0.26234374, -0.86662046,  2.88889563]), array([-2.02365973,  0.78577958,  0.24500894,  2.32758046]), array([-1.84374205,  1.16955425,  1.60674508,  1.401168  ]), array([-1.34666708,  1.23261059,  3.35842542, -0.9338591 ]), array([-0.52113188,  0.7385886 ,  4.79254456, -4.01589937]), array([ 0.49500537, -0.25446343,  5.09272008, -5.26573435]), array([ 1.41300234, -1.11408571,  3.96953905, -3.13026121]), array([ 2.07772032, -1.54554879,  2.70978305, -1.37280449]), array([ 2.51896446, -1.73751603,  1.76869297, -0.70606121]), array([ 2.81099789, -1.87743325,  1.21120555, -0.7880734 ]), array([ 3.01494136, -2.05713374,  0.86904055, -1.05910534]), array([-3.10480656, -2.33500051,  0.79234486, -1.73512532]), array([-2.94071695, -2.75299031,  0.88370259, -2.44427305]), array([-2.73174896,  2.97132159,  1.27365504, -3.15119627]), array([-2.3999549 ,  2.25952019,  2.12488485, -4.03614081]), array([-1.85013677,  1.3028724 ,  3.46226932, -5.75405989]), array([-0.98461313, -0.12109388,  5.09045847, -8.16641509]), array([ 0.07717611, -1.62144335,  5.34746133, -6.24084101]), array([ 1.12128481, -2.59043982,  4.94928854, -3.56856159]), array([ 2.006144  , -3.11811948,  3.86656458, -1.87939063]), array([ 2.69075349,  2.88402785,  3.08765578, -1.06457826]), array([-2.99328875,  2.68605118,  3.03549064, -1.0656074 ]), array([-2.32872778,  2.39062232,  3.72480442, -2.09619875]), array([-1.46964774,  1.748491  ,  4.91684764, -4.63205699]), array([-0.34800848,  0.418817  ,  6.25089278, -8.55234827]), array([ 0.884549  , -1.21678763,  5.71589956, -6.74503445]), array([ 1.91491107, -2.223428  ,  4.61328881, -3.60900179]), array([ 2.75051431, -2.78436299,  3.8431826 , -2.28178298]), array([-2.77593878,  3.05280219,  3.88137515, -2.40525774]), array([-1.92381485,  2.44420448,  4.73998201, -3.96878159]), array([-0.86139855,  1.32748336,  5.93605371, -7.5811984 ]), array([ 0.43964228, -0.56138252,  6.64777209, -9.92698902]), array([ 1.64487768, -2.14336713,  5.42792147, -5.95550879]), array([ 2.64192812, -3.12465846,  4.6167861 , -4.26909462]), array([-2.74046123,  2.29699943,  4.56106379, -4.67697546]), array([-1.74411169,  1.13904148,  5.61543679, -7.33784204]), array([-0.45565198, -0.65027233,  6.97448172, -9.37141959]), array([ 0.91930756, -2.11455512,  6.65422807, -5.04462968]), array([ 2.15564737, -2.78628936,  5.64276524, -2.06793475]), array([-3.06959112, -3.08555837,  5.13649879, -1.28361668]), array([-1.98674429,  2.85458596,  5.87289483, -2.50640932]), array([-0.69956068,  2.04560535,  6.89027488, -6.0078347 ]), array([  0.72481405,   0.33409134,   7.24582015, -10.65584454]), array([ 2.03849627, -1.57399264,  5.69650794, -7.55014915]), array([ 3.10421709, -2.86038928,  5.18405448, -5.857632  ]), array([-2.10287876,  2.17009472,  5.73585456, -7.2428464 ]), array([ -0.7941752 ,   0.25836736,   7.43882181, -11.8332779 ]), array([ 0.68072447, -1.84741012,  6.92863644, -7.87039209]), array([ 1.99626546, -3.05737623,  6.13336206, -4.81196409]), array([ 3.14022226,  2.30989669,  5.46502377, -4.79463785]), array([-2.00900591,  1.1316539 ,  6.16321104, -7.47025236]), array([-0.61100025, -0.69328018,  7.56560837, -9.48705405]), array([ 0.89806119, -2.12300177,  7.35053247, -4.52024441]), array([ 2.25296603, -2.61982045,  6.10452651, -0.86832134]), array([-2.91060765, -2.61508448,  5.26543868,  0.58432848]), array([-1.85865349, -2.46304237,  5.37247295,  0.87631594]), array([-0.76273859, -2.20792428,  5.396329  ,  2.0411736 ]), array([ 0.13609173, -1.44642114,  3.10745277,  6.03861305]), array([0.39465388, 0.27258875, 0.34186013, 9.84012537]), array([0.71657842, 1.88124406, 3.11840475, 5.92930537]), array([1.50402264, 2.84091927, 4.24240785, 4.35163346]), array([ 2.23870687, -2.4520518 ,  2.59522781,  5.94942563]), array([ 2.40824128, -0.99166096, -0.88376984,  8.70851611]), array([ 2.04162885,  0.94746185, -2.0831073 ,  9.88934034])]</t>
-  </si>
-  <si>
-    <t>['[1,0,2]', '[0,2,1]', '[0,1,1]', '[2,1,0]', '[1,2,0]', '[0,0,0]', '[2,0,1]', '[1,1,1]', '[2,2,2]', '[1,1,2]']</t>
-  </si>
-  <si>
-    <t>[6, 7, 8, 9, 10, 11, 12, 18, 19, 20, 21, 29, 30, 31, 38, 39, 41, 42, 43, 49, 50, 51, 52, 53, 54, 61, 62, 65, 72, 75, 76, 77, 85, 86, 87, 89, 96, 97, 98, 100, 101, 102, 109, 110, 111, 114, 123, 124, 125, 128, 136, 137, 138, 140, 141, 142, 143, 150, 151, 153, 154, 155, 156, 157, 165, 166, 167, 168, 169, 171, 172, 180, 181, 182, 183, 187, 196, 197, 198, 199]</t>
-  </si>
-  <si>
-    <t>[0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 1, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 1, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 1, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 1, 2, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 1, 1, 2, 2]</t>
-  </si>
-  <si>
-    <t>['[-0.03763371 -0.01533471  0.06554052 -0.01816017]', '[-0.00754409 -0.05458322  0.2277812  -0.36241836]', '[ 0.04879627 -0.15231473  0.32089719 -0.5887683 ]', '[ 0.11397169 -0.27767857  0.31375488 -0.63332862]', '[ 0.16759438 -0.39312519  0.2086893  -0.49480525]', '[ 0.1930193  -0.46685036  0.03906408 -0.22816919]', '[ 0.18217995 -0.48119372 -0.14531723  0.08492936]', '[ 0.13737799 -0.43548032 -0.29255645  0.35879992]', '[ 0.07059687 -0.34553749 -0.35944697  0.51636187]', '[ 0.00066518 -0.24025206 -0.32266973  0.50804924]', '[-0.05184718 -0.15356453 -0.18924715  0.33585339]', '[-0.07099568 -0.11316     0.00267821  0.05860212]', '[-0.0506235  -0.13098626  0.19609592 -0.23012254]', '[ 0.00363944 -0.19947979  0.33317766 -0.43407441]', '[ 0.07604673 -0.29425756  0.37330708 -0.48624983]', '[ 0.14566012 -0.38269974  0.30650217 -0.37362319]', '[ 0.19284616 -0.43524651  0.15487527 -0.13746415]', '[ 0.17925146 -0.36784094 -0.2871979   0.80057151]', '[ 0.10967194 -0.19472733 -0.38919407  0.89086052]', '[ 0.03237318 -0.02900979 -0.36265722  0.7252022 ]', '[-0.02742907  0.08030625 -0.22007599  0.34029738]', '[-0.05115334  0.09956751 -0.01210087 -0.15394543]', '[-0.03236889  0.02056299  0.19347827 -0.61923614]', '[ 0.02145618 -0.13700106  0.32831485 -0.91974237]', '[ 0.09094705 -0.32986667  0.34615412 -0.96460983]', '[ 0.15187779 -0.50551685  0.24676468 -0.75605406]', '[ 0.18443677 -0.62064122  0.07101819 -0.37603269]', '[ 0.15451994 -0.58756014 -0.36379625  0.6992459 ]', '[ 0.04452296 -0.35010587 -0.71231658  1.63112363]', '[-0.08964256 -0.03168978 -0.59027106  1.47323915]', '[-0.17725951  0.20941408 -0.26087001  0.88348397]', '[-0.18780309  0.3070233   0.15885654  0.07761982]', '[-0.11618311  0.24122946  0.54107652 -0.71484881]', '[ 0.0184391   0.03655275  0.77168868 -1.27601045]', '[ 0.17627848 -0.24061205  0.76500536 -1.42020159]', '[ 0.30806577 -0.5017195   0.51997031 -1.13104756]', '[ 0.37411411 -0.67451475  0.12598225 -0.56825837]', '[ 0.35611254 -0.72258777 -0.30224629  0.09042059]', '[ 0.25799214 -0.64154295 -0.65882091  0.69934842]', '[ 0.10375562 -0.45649533 -0.84937701  1.10349946]', '[-0.09169227 -0.15712387 -1.05875489  1.81279902]', '[-0.27114296  0.16013961 -0.68913596  1.27444389]', '[-0.3532494   0.32721983 -0.11321288  0.36211014]', '[-0.3141021   0.29966488  0.49608073 -0.62830296]', '[-0.16348159  0.08812871  0.97456914 -1.43102949]', '[ 0.05611059 -0.2397592   1.16471137 -1.74975812]', '[ 0.27823361 -0.57005418  1.00359185 -1.46631874]', '[ 0.43962223 -0.79933058  0.57857373 -0.78467111]', '[ 0.50092175 -0.87404447  0.0239628   0.04726387]', '[ 0.44873763 -0.78052057 -0.53631345  0.87593479]', '[ 0.29438753 -0.53392329 -0.97551639  1.5447247 ]', '[ 0.07627031 -0.1905924  -1.15189695  1.7974982 ]', '[-0.14207295  0.14244931 -0.97548925  1.43533538]', '[-0.29431583  0.35078588 -0.51274559  0.59581402]', '[-0.33817145  0.36877207  0.08236466 -0.42225326]', '[-0.26296668  0.1870184   0.65093759 -1.35822813]', '[-0.0912799  -0.14893227  1.01891197 -1.9120068 ]', '[ 0.12176833 -0.5345053   1.05581353 -1.84097213]', '[ 0.31059427 -0.84986826  0.79313179 -1.25163197]', '[ 0.42683386 -1.01899733  0.34916189 -0.41775995]', '[ 0.42344717 -0.9545722  -0.38567712  1.06130338]', '[ 0.29860709 -0.66029457 -0.83911995  1.84171187]', '[ 0.10289881 -0.2446877  -1.06685067  2.21831597]', '[-0.12960909  0.24695145 -1.18856934  2.5602593 ]', '[-0.34374895  0.72286571 -0.89726748  2.09333808]', '[-0.45081175  0.99747042 -0.16273765  0.6364723 ]', '[-0.40877486  0.97615601  0.57464116 -0.84559933]', '[-0.22743373  0.66393592  1.21126292 -2.24411926]', '[ 0.05727973  0.10794107  1.56394757 -3.180738  ]', '[ 0.35932    -0.53125286  1.36331021 -3.02681785]', '[ 0.57313878 -1.04794443  0.73341172 -2.07085383]', '[ 0.64458691 -1.34788207 -0.02253717 -0.91948617]', '[ 0.56737724 -1.41509291 -0.73056501  0.24408639]', '[ 0.34491992 -1.20025253 -1.45910037  1.89513601]', '[-1.14280566e-04 -6.66340700e-01 -1.93987532e+00  3.38010673e+00]', '[-0.37267524  0.02602633 -1.67879521  3.32799261]', '[-0.6311889   0.58404165 -0.84336673  2.13299779]', '[-0.69765266  0.85753536  0.18456618  0.58437589]', '[-0.56125497  0.81555061  1.15582663 -1.00039138]', '[-0.25045666  0.46564104  1.89566753 -2.43705526]', '[ 0.16376876 -0.10795437  2.14045143 -3.10670154]', '[ 0.55913152 -0.68962259  1.72027153 -2.54891419]', '[ 0.82566542 -1.09087741  0.90680247 -1.43006172]', '[ 0.91307918 -1.25851336 -0.04125117 -0.24545959]', '[ 0.79000535 -1.13294967 -1.1765072   1.5109765 ]', '[ 0.47441936 -0.71104661 -1.9318216   2.66726807]', '[ 0.04728931 -0.10835244 -2.23585375  3.17701017]', '[-0.37087501  0.46717278 -1.84125833  2.3909902 ]', '[-0.68214571  0.86351649 -1.21479036  1.50263094]', '[-0.81949288  0.99763997 -0.1421774  -0.15952631]', '[-0.73661723  0.80047165  0.96453665 -1.8090873 ]', '[-0.44284097  0.28198914  1.92028898 -3.29646085]', '[-0.0072999  -0.44566332  2.30920651 -3.7281219 ]', '[ 0.43113724 -1.11192682  1.98754223 -2.79180188]', '[ 0.76317914 -1.53780446  1.2893667  -1.45345536]', '[ 0.93347443 -1.69519389  0.39160567 -0.12899105]', '[ 0.91507607 -1.59136035 -0.57629224  1.1686559 ]', '[ 0.70663891 -1.22464255 -1.4881137   2.50460054]', '[ 0.33368631 -0.59518174 -2.1806052   3.7126983 ]', '[-0.14955794  0.25197604 -2.5053413   4.46124939]', '[-0.58214301  0.9997571  -1.73610245  2.87518291]', '[-0.82793438  1.39097931 -0.7020683   1.04912694]', '[-0.85852666  1.42489195  0.39898291 -0.70671885]', '[-0.67010399  1.10440161  1.47227334 -2.51329608]', '[-0.2804005   0.42055246  2.36293998 -4.23956967]', '[ 0.22416643 -0.49251082  2.51715241 -4.54708709]', '[ 0.66872896 -1.28385587  1.85126228 -3.25120491]', '[ 0.94867365 -1.78707767  0.92518297 -1.79848284]', '[ 1.03309897 -2.01058141 -0.08529634 -0.44653889]', '[ 0.91688611 -1.96594245 -1.05929385  0.8992685 ]', '[ 0.62124121 -1.64644135 -1.8572647   2.30549215]', '[ 0.19337832 -1.04435282 -2.3654687   3.67827222]', '[-0.31801434 -0.15744757 -2.6318457   4.95781147]', '[-0.79002301  0.79144209 -1.94462375  4.24333295]', '[-1.04458863  1.43703322 -0.59253952  2.23391461]', '[-1.04680903  1.74488265  0.56202162  0.84263293]', '[-0.81342689  1.72274276  1.72901754 -1.07930919]', '[-0.37716195  1.30557448  2.57414209 -3.10064353]', '[ 0.19016412  0.49529776  3.00969176 -4.85831675]', '[ 0.76519248 -0.50564105  2.56641708 -4.7722261 ]', '[ 1.16583239 -1.31638255  1.38904701 -3.28339573]', '[ 1.31406097 -1.82747739  0.08956271 -1.84731403]', '[ 1.20389143 -2.05514502 -1.17382392 -0.41182905]', '[ 0.85786044 -1.98177389 -2.23335004  1.16984215]', '[ 0.34059154 -1.58215871 -2.85214995  2.81399797]', '[-0.24607012 -0.87879038 -2.92279837  4.0928479 ]', '[-0.80927343  0.02920732 -2.57991954  4.69254673]', '[-1.22312654  0.87888915 -1.47303122  3.64876527]', '[-1.36323428  1.41900028  0.0697639   1.77521189]', '[-1.21616554  1.63713081  1.38928704  0.36528092]', '[-0.80423337  1.49570646  2.67080465 -1.82966093]', '[-0.17838028  0.89271514  3.50136633 -4.16401763]', '[ 0.54724164 -0.09076324  3.57220079 -5.26138939]', '[ 1.17151684 -1.03058004  2.56095781 -3.92759856]', '[ 1.55784532 -1.66126892  1.29577858 -2.44340228]', '[ 1.68923577 -2.02920818  0.01705513 -1.25705635]', '[ 1.56453079 -2.16005021 -1.26122732 -0.01586674]', '[ 1.18936804 -2.01402733 -2.46211873  1.54140048]', '[ 0.60038111 -1.51711864 -3.3576884   3.47452276]', '[-0.14138661 -0.57123413 -3.96356632  5.84366703]', '[-0.88113877  0.56933242 -3.22000688  5.05438435]', '[-1.38353282  1.35938366 -1.78465512  2.87741811]', '[-1.59700506  1.75487364 -0.35589588  1.13681201]', '[-1.52751603  1.82150135  1.04663628 -0.49053136]', '[-1.18134327  1.53713792  2.40121958 -2.43509155]', '[-0.5759381   0.80995487  3.61365122 -4.87566918]', '[ 0.21802581 -0.33369294  4.09377892 -6.01906575]', '[ 0.96443465 -1.36891684  3.2531681  -4.12705415]', '[ 1.50352352 -2.00092663  2.11808184 -2.29336992]', '[ 1.80786125 -2.32271844  0.92458301 -0.98875827]', '[ 1.8747     -2.41117142 -0.25401026  0.09260831]', '[ 1.70562019 -2.28117583 -1.43997187  1.24185957]', '[ 1.28505642 -1.84654184 -2.75874111  3.20746555]', '[ 0.62522589 -0.99809678 -3.80582945  5.33830559]', '[-0.19425441  0.21718116 -4.15084293  6.25166384]', '[-0.93194313  1.25595182 -3.10693356  3.91902216]', '[-1.42401778  1.80555442 -1.79793903  1.68109509]', '[-1.64692512  1.9634687  -0.42605891 -0.04545702]', '[-1.59336468  1.79671439  0.96462197 -1.63512518]', '[-1.25924415  1.28817187  2.38287101 -3.54210944]', '[-0.6406399   0.34328254  3.74427999 -5.83546571]', '[ 0.15988297 -0.86514259  4.01908631 -5.66709981]', '[ 0.90353036 -1.7856392   3.3409694  -3.49465747]', '[ 1.47210032 -2.2902617   2.29771559 -1.64092228]', '[ 1.81271418 -2.4743896   1.1027891  -0.2639773 ]', '[ 1.9144038  -2.41411157 -0.08288567  0.84026272]', '[ 1.77904613 -2.14028987 -1.27528485  1.91990578]', '[ 1.40222436 -1.62437974 -2.49551714  3.32833333]', '[ 0.78215346 -0.76687042 -3.67735208  5.28424559]', '[-0.01928975  0.39349033 -4.10229729  5.76321798]', '[-0.7905096   1.38207413 -3.48163991  3.89780982]', '[-1.36849338  1.90902389 -2.2579694   1.47459955]', '[-1.68207704  2.0108957  -0.86297357 -0.38022323]', '[-1.71094707  1.77612405  0.57939569 -1.95530891]', '[-1.44704937  1.21597349  2.07292884 -3.72611609]', '[-0.87818532  0.24977568  3.56659398 -5.87127198]', '[-0.0919082  -0.96292796  4.07926492 -5.71121617]', '[ 0.69597989 -1.90076497  3.709378   -3.59419892]', '[ 1.35464421 -2.41586506  2.79660319 -1.63086386]', '[ 1.79562003 -2.58411372  1.597928   -0.1214779 ]', '[ 1.99463631 -2.48820355  0.39815338  1.03365053]', '[ 1.95562516 -2.18290418 -0.79123919  2.01233109]', '[ 1.67519785 -1.67316881 -2.02293157  3.15063008]', '[ 1.14195273 -0.88235176 -3.31108493  4.84665129]', '[ 0.34923251  0.29838119 -4.42308139  6.49028634]', '[-0.52334815  1.44527347 -4.14164879  4.62255955]', '[-1.27284197  2.13155312 -3.27734706  2.31903524]', '[-1.79703371  2.37453648 -1.93793435  0.22113694]', '[-2.06084507  2.29809912 -0.71161639 -0.9116434 ]', '[-2.07086609  1.98811872  0.61380666 -2.17141578]', '[-1.81057598  1.41847675  2.01176833 -3.60917902]', '[-1.25296601  0.49219352  3.57748974 -5.73015129]', '[-0.42021089 -0.773024    4.53885407 -6.34116108]', '[ 0.49011001 -1.83855419  4.45208371 -4.12671818]', '[ 1.3126246  -2.42531706  3.65504141 -1.82093886]', '[ 1.92338029 -2.608609    2.43452147 -0.11979772]', '[ 2.29238423 -2.51403037  1.28278544  0.97002659]', '[ 2.44670024 -2.25427865  0.28286261  1.55777658]', '[ 2.41171331 -1.91024353 -0.62429086  1.86047573]', '[ 2.19587227 -1.50613796 -1.54930781  2.22697272]']</t>
-  </si>
-  <si>
-    <t>[array([-0.03763371, -0.01533471,  0.06554052, -0.01816017], dtype=float32), array([-0.00754409, -0.05458322,  0.2277812 , -0.36241836]), array([ 0.04879627, -0.15231473,  0.32089719, -0.5887683 ]), array([ 0.11397169, -0.27767857,  0.31375488, -0.63332862]), array([ 0.16759438, -0.39312519,  0.2086893 , -0.49480525]), array([ 0.1930193 , -0.46685036,  0.03906408, -0.22816919]), array([ 0.18217995, -0.48119372, -0.14531723,  0.08492936]), array([ 0.13737799, -0.43548032, -0.29255645,  0.35879992]), array([ 0.07059687, -0.34553749, -0.35944697,  0.51636187]), array([ 0.00066518, -0.24025206, -0.32266973,  0.50804924]), array([-0.05184718, -0.15356453, -0.18924715,  0.33585339]), array([-0.07099568, -0.11316   ,  0.00267821,  0.05860212]), array([-0.0506235 , -0.13098626,  0.19609592, -0.23012254]), array([ 0.00363944, -0.19947979,  0.33317766, -0.43407441]), array([ 0.07604673, -0.29425756,  0.37330708, -0.48624983]), array([ 0.14566012, -0.38269974,  0.30650217, -0.37362319]), array([ 0.19284616, -0.43524651,  0.15487527, -0.13746415]), array([ 0.17925146, -0.36784094, -0.2871979 ,  0.80057151]), array([ 0.10967194, -0.19472733, -0.38919407,  0.89086052]), array([ 0.03237318, -0.02900979, -0.36265722,  0.7252022 ]), array([-0.02742907,  0.08030625, -0.22007599,  0.34029738]), array([-0.05115334,  0.09956751, -0.01210087, -0.15394543]), array([-0.03236889,  0.02056299,  0.19347827, -0.61923614]), array([ 0.02145618, -0.13700106,  0.32831485, -0.91974237]), array([ 0.09094705, -0.32986667,  0.34615412, -0.96460983]), array([ 0.15187779, -0.50551685,  0.24676468, -0.75605406]), array([ 0.18443677, -0.62064122,  0.07101819, -0.37603269]), array([ 0.15451994, -0.58756014, -0.36379625,  0.6992459 ]), array([ 0.04452296, -0.35010587, -0.71231658,  1.63112363]), array([-0.08964256, -0.03168978, -0.59027106,  1.47323915]), array([-0.17725951,  0.20941408, -0.26087001,  0.88348397]), array([-0.18780309,  0.3070233 ,  0.15885654,  0.07761982]), array([-0.11618311,  0.24122946,  0.54107652, -0.71484881]), array([ 0.0184391 ,  0.03655275,  0.77168868, -1.27601045]), array([ 0.17627848, -0.24061205,  0.76500536, -1.42020159]), array([ 0.30806577, -0.5017195 ,  0.51997031, -1.13104756]), array([ 0.37411411, -0.67451475,  0.12598225, -0.56825837]), array([ 0.35611254, -0.72258777, -0.30224629,  0.09042059]), array([ 0.25799214, -0.64154295, -0.65882091,  0.69934842]), array([ 0.10375562, -0.45649533, -0.84937701,  1.10349946]), array([-0.09169227, -0.15712387, -1.05875489,  1.81279902]), array([-0.27114296,  0.16013961, -0.68913596,  1.27444389]), array([-0.3532494 ,  0.32721983, -0.11321288,  0.36211014]), array([-0.3141021 ,  0.29966488,  0.49608073, -0.62830296]), array([-0.16348159,  0.08812871,  0.97456914, -1.43102949]), array([ 0.05611059, -0.2397592 ,  1.16471137, -1.74975812]), array([ 0.27823361, -0.57005418,  1.00359185, -1.46631874]), array([ 0.43962223, -0.79933058,  0.57857373, -0.78467111]), array([ 0.50092175, -0.87404447,  0.0239628 ,  0.04726387]), array([ 0.44873763, -0.78052057, -0.53631345,  0.87593479]), array([ 0.29438753, -0.53392329, -0.97551639,  1.5447247 ]), array([ 0.07627031, -0.1905924 , -1.15189695,  1.7974982 ]), array([-0.14207295,  0.14244931, -0.97548925,  1.43533538]), array([-0.29431583,  0.35078588, -0.51274559,  0.59581402]), array([-0.33817145,  0.36877207,  0.08236466, -0.42225326]), array([-0.26296668,  0.1870184 ,  0.65093759, -1.35822813]), array([-0.0912799 , -0.14893227,  1.01891197, -1.9120068 ]), array([ 0.12176833, -0.5345053 ,  1.05581353, -1.84097213]), array([ 0.31059427, -0.84986826,  0.79313179, -1.25163197]), array([ 0.42683386, -1.01899733,  0.34916189, -0.41775995]), array([ 0.42344717, -0.9545722 , -0.38567712,  1.06130338]), array([ 0.29860709, -0.66029457, -0.83911995,  1.84171187]), array([ 0.10289881, -0.2446877 , -1.06685067,  2.21831597]), array([-0.12960909,  0.24695145, -1.18856934,  2.5602593 ]), array([-0.34374895,  0.72286571, -0.89726748,  2.09333808]), array([-0.45081175,  0.99747042, -0.16273765,  0.6364723 ]), array([-0.40877486,  0.97615601,  0.57464116, -0.84559933]), array([-0.22743373,  0.66393592,  1.21126292, -2.24411926]), array([ 0.05727973,  0.10794107,  1.56394757, -3.180738  ]), array([ 0.35932   , -0.53125286,  1.36331021, -3.02681785]), array([ 0.57313878, -1.04794443,  0.73341172, -2.07085383]), array([ 0.64458691, -1.34788207, -0.02253717, -0.91948617]), array([ 0.56737724, -1.41509291, -0.73056501,  0.24408639]), array([ 0.34491992, -1.20025253, -1.45910037,  1.89513601]), array([-1.14280566e-04, -6.66340700e-01, -1.93987532e+00,  3.38010673e+00]), array([-0.37267524,  0.02602633, -1.67879521,  3.32799261]), array([-0.6311889 ,  0.58404165, -0.84336673,  2.13299779]), array([-0.69765266,  0.85753536,  0.18456618,  0.58437589]), array([-0.56125497,  0.81555061,  1.15582663, -1.00039138]), array([-0.25045666,  0.46564104,  1.89566753, -2.43705526]), array([ 0.16376876, -0.10795437,  2.14045143, -3.10670154]), array([ 0.55913152, -0.68962259,  1.72027153, -2.54891419]), array([ 0.82566542, -1.09087741,  0.90680247, -1.43006172]), array([ 0.91307918, -1.25851336, -0.04125117, -0.24545959]), array([ 0.79000535, -1.13294967, -1.1765072 ,  1.5109765 ]), array([ 0.47441936, -0.71104661, -1.9318216 ,  2.66726807]), array([ 0.04728931, -0.10835244, -2.23585375,  3.17701017]), array([-0.37087501,  0.46717278, -1.84125833,  2.3909902 ]), array([-0.68214571,  0.86351649, -1.21479036,  1.50263094]), array([-0.81949288,  0.99763997, -0.1421774 , -0.15952631]), array([-0.73661723,  0.80047165,  0.96453665, -1.8090873 ]), array([-0.44284097,  0.28198914,  1.92028898, -3.29646085]), array([-0.0072999 , -0.44566332,  2.30920651, -3.7281219 ]), array([ 0.43113724, -1.11192682,  1.98754223, -2.79180188]), array([ 0.76317914, -1.53780446,  1.2893667 , -1.45345536]), array([ 0.93347443, -1.69519389,  0.39160567, -0.12899105]), array([ 0.91507607, -1.59136035, -0.57629224,  1.1686559 ]), array([ 0.70663891, -1.22464255, -1.4881137 ,  2.50460054]), array([ 0.33368631, -0.59518174, -2.1806052 ,  3.7126983 ]), array([-0.14955794,  0.25197604, -2.5053413 ,  4.46124939]), array([-0.58214301,  0.9997571 , -1.73610245,  2.87518291]), array([-0.82793438,  1.39097931, -0.7020683 ,  1.04912694]), array([-0.85852666,  1.42489195,  0.39898291, -0.70671885]), array([-0.67010399,  1.10440161,  1.47227334, -2.51329608]), array([-0.2804005 ,  0.42055246,  2.36293998, -4.23956967]), array([ 0.22416643, -0.49251082,  2.51715241, -4.54708709]), array([ 0.66872896, -1.28385587,  1.85126228, -3.25120491]), array([ 0.94867365, -1.78707767,  0.92518297, -1.79848284]), array([ 1.03309897, -2.01058141, -0.08529634, -0.44653889]), array([ 0.91688611, -1.96594245, -1.05929385,  0.8992685 ]), array([ 0.62124121, -1.64644135, -1.8572647 ,  2.30549215]), array([ 0.19337832, -1.04435282, -2.3654687 ,  3.67827222]), array([-0.31801434, -0.15744757, -2.6318457 ,  4.95781147]), array([-0.79002301,  0.79144209, -1.94462375,  4.24333295]), array([-1.04458863,  1.43703322, -0.59253952,  2.23391461]), array([-1.04680903,  1.74488265,  0.56202162,  0.84263293]), array([-0.81342689,  1.72274276,  1.72901754, -1.07930919]), array([-0.37716195,  1.30557448,  2.57414209, -3.10064353]), array([ 0.19016412,  0.49529776,  3.00969176, -4.85831675]), array([ 0.76519248, -0.50564105,  2.56641708, -4.7722261 ]), array([ 1.16583239, -1.31638255,  1.38904701, -3.28339573]), array([ 1.31406097, -1.82747739,  0.08956271, -1.84731403]), array([ 1.20389143, -2.05514502, -1.17382392, -0.41182905]), array([ 0.85786044, -1.98177389, -2.23335004,  1.16984215]), array([ 0.34059154, -1.58215871, -2.85214995,  2.81399797]), array([-0.24607012, -0.87879038, -2.92279837,  4.0928479 ]), array([-0.80927343,  0.02920732, -2.57991954,  4.69254673]), array([-1.22312654,  0.87888915, -1.47303122,  3.64876527]), array([-1.36323428,  1.41900028,  0.0697639 ,  1.77521189]), array([-1.21616554,  1.63713081,  1.38928704,  0.36528092]), array([-0.80423337,  1.49570646,  2.67080465, -1.82966093]), array([-0.17838028,  0.89271514,  3.50136633, -4.16401763]), array([ 0.54724164, -0.09076324,  3.57220079, -5.26138939]), array([ 1.17151684, -1.03058004,  2.56095781, -3.92759856]), array([ 1.55784532, -1.66126892,  1.29577858, -2.44340228]), array([ 1.68923577, -2.02920818,  0.01705513, -1.25705635]), array([ 1.56453079, -2.16005021, -1.26122732, -0.01586674]), array([ 1.18936804, -2.01402733, -2.46211873,  1.54140048]), array([ 0.60038111, -1.51711864, -3.3576884 ,  3.47452276]), array([-0.14138661, -0.57123413, -3.96356632,  5.84366703]), array([-0.88113877,  0.56933242, -3.22000688,  5.05438435]), array([-1.38353282,  1.35938366, -1.78465512,  2.87741811]), array([-1.59700506,  1.75487364, -0.35589588,  1.13681201]), array([-1.52751603,  1.82150135,  1.04663628, -0.49053136]), array([-1.18134327,  1.53713792,  2.40121958, -2.43509155]), array([-0.5759381 ,  0.80995487,  3.61365122, -4.87566918]), array([ 0.21802581, -0.33369294,  4.09377892, -6.01906575]), array([ 0.96443465, -1.36891684,  3.2531681 , -4.12705415]), array([ 1.50352352, -2.00092663,  2.11808184, -2.29336992]), array([ 1.80786125, -2.32271844,  0.92458301, -0.98875827]), array([ 1.8747    , -2.41117142, -0.25401026,  0.09260831]), array([ 1.70562019, -2.28117583, -1.43997187,  1.24185957]), array([ 1.28505642, -1.84654184, -2.75874111,  3.20746555]), array([ 0.62522589, -0.99809678, -3.80582945,  5.33830559]), array([-0.19425441,  0.21718116, -4.15084293,  6.25166384]), array([-0.93194313,  1.25595182, -3.10693356,  3.91902216]), array([-1.42401778,  1.80555442, -1.79793903,  1.68109509]), array([-1.64692512,  1.9634687 , -0.42605891, -0.04545702]), array([-1.59336468,  1.79671439,  0.96462197, -1.63512518]), array([-1.25924415,  1.28817187,  2.38287101, -3.54210944]), array([-0.6406399 ,  0.34328254,  3.74427999, -5.83546571]), array([ 0.15988297, -0.86514259,  4.01908631, -5.66709981]), array([ 0.90353036, -1.7856392 ,  3.3409694 , -3.49465747]), array([ 1.47210032, -2.2902617 ,  2.29771559, -1.64092228]), array([ 1.81271418, -2.4743896 ,  1.1027891 , -0.2639773 ]), array([ 1.9144038 , -2.41411157, -0.08288567,  0.84026272]), array([ 1.77904613, -2.14028987, -1.27528485,  1.91990578]), array([ 1.40222436, -1.62437974, -2.49551714,  3.32833333]), array([ 0.78215346, -0.76687042, -3.67735208,  5.28424559]), array([-0.01928975,  0.39349033, -4.10229729,  5.76321798]), array([-0.7905096 ,  1.38207413, -3.48163991,  3.89780982]), array([-1.36849338,  1.90902389, -2.2579694 ,  1.47459955]), array([-1.68207704,  2.0108957 , -0.86297357, -0.38022323]), array([-1.71094707,  1.77612405,  0.57939569, -1.95530891]), array([-1.44704937,  1.21597349,  2.07292884, -3.72611609]), array([-0.87818532,  0.24977568,  3.56659398, -5.87127198]), array([-0.0919082 , -0.96292796,  4.07926492, -5.71121617]), array([ 0.69597989, -1.90076497,  3.709378  , -3.59419892]), array([ 1.35464421, -2.41586506,  2.79660319, -1.63086386]), array([ 1.79562003, -2.58411372,  1.597928  , -0.1214779 ]), array([ 1.99463631, -2.48820355,  0.39815338,  1.03365053]), array([ 1.95562516, -2.18290418, -0.79123919,  2.01233109]), array([ 1.67519785, -1.67316881, -2.02293157,  3.15063008]), array([ 1.14195273, -0.88235176, -3.31108493,  4.84665129]), array([ 0.34923251,  0.29838119, -4.42308139,  6.49028634]), array([-0.52334815,  1.44527347, -4.14164879,  4.62255955]), array([-1.27284197,  2.13155312, -3.27734706,  2.31903524]), array([-1.79703371,  2.37453648, -1.93793435,  0.22113694]), array([-2.06084507,  2.29809912, -0.71161639, -0.9116434 ]), array([-2.07086609,  1.98811872,  0.61380666, -2.17141578]), array([-1.81057598,  1.41847675,  2.01176833, -3.60917902]), array([-1.25296601,  0.49219352,  3.57748974, -5.73015129]), array([-0.42021089, -0.773024  ,  4.53885407, -6.34116108]), array([ 0.49011001, -1.83855419,  4.45208371, -4.12671818]), array([ 1.3126246 , -2.42531706,  3.65504141, -1.82093886]), array([ 1.92338029, -2.608609  ,  2.43452147, -0.11979772]), array([ 2.29238423, -2.51403037,  1.28278544,  0.97002659]), array([ 2.44670024, -2.25427865,  0.28286261,  1.55777658]), array([ 2.41171331, -1.91024353, -0.62429086,  1.86047573]), array([ 2.19587227, -1.50613796, -1.54930781,  2.22697272])]</t>
-  </si>
-  <si>
-    <t>['[0,2,1]', '[0,0,0]', '[1,0,2]', '[1,1,1]', '[1,2,0]', '[0,1,1]', '[2,0,1]', '[1,1,2]', '[2,1,0]', '[2,2,2]']</t>
-  </si>
-  <si>
-    <t>[6, 7, 8, 9, 10, 11, 12, 17, 18, 19, 20, 21, 22, 23, 29, 30, 31, 32, 33, 34, 40, 41, 42, 43, 44, 45, 46, 51, 52, 53, 54, 55, 56, 57, 63, 64, 65, 66, 67, 68, 74, 75, 76, 77, 78, 79, 85, 86, 87, 88, 89, 90, 91, 96, 97, 98, 99, 100, 101, 102, 108, 109, 110, 111, 112, 113, 119, 120, 121, 122, 123, 124, 130, 131, 132, 133, 134, 135, 136, 142, 143, 144, 145, 146, 147, 153, 154, 155, 156, 157, 158, 164, 165, 166, 167, 168, 169, 170, 176, 177, 178, 179, 180, 181, 187, 188, 189, 190, 191, 192, 198, 199]</t>
-  </si>
-  <si>
-    <t>[0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 2, 2]</t>
-  </si>
-  <si>
-    <t>['[-0.03763371 -0.01533471  0.06554052 -0.01816017]', '[-0.00754409 -0.05458322  0.2277812  -0.36241836]', '[ 0.04879627 -0.15231473  0.32089719 -0.5887683 ]', '[ 0.11397169 -0.27767857  0.31375488 -0.63332862]', '[ 0.16759438 -0.39312519  0.2086893  -0.49480525]', '[ 0.1930193  -0.46685036  0.03906408 -0.22816919]', '[ 0.18217995 -0.48119372 -0.14531723  0.08492936]', '[ 0.13737799 -0.43548032 -0.29255645  0.35879992]', '[ 0.07059687 -0.34553749 -0.35944697  0.51636187]', '[ 0.00066518 -0.24025206 -0.32266973  0.50804924]', '[-0.05184718 -0.15356453 -0.18924715  0.33585339]', '[-0.07099568 -0.11316     0.00267821  0.05860212]', '[-0.0506235  -0.13098626  0.19609592 -0.23012254]', '[ 0.00363944 -0.19947979  0.33317766 -0.43407441]', '[ 0.07604673 -0.29425756  0.37330708 -0.48624983]', '[ 0.14566012 -0.38269974  0.30650217 -0.37362319]', '[ 0.19284616 -0.43524651  0.15487527 -0.13746415]', '[ 0.20480978 -0.43420274 -0.03738189  0.14899985]', '[ 0.17872861 -0.37781944 -0.21671607  0.40226469]', '[ 0.12244395 -0.28089207 -0.33207824  0.54289906]', '[ 0.05262627 -0.17207597 -0.34864539  0.51601465]', '[-0.00991093 -0.08621824 -0.26142967  0.31808955]', '[-0.04676022 -0.05276175 -0.09876284  0.00534115]', '[-0.04773189 -0.08549506  0.08793289 -0.326671  ]', '[-0.01386808 -0.17774148  0.24064044 -0.5740393 ]', '[ 0.04305734 -0.30394484  0.31308665 -0.65740151]', '[ 0.10464298 -0.42784083  0.2871402  -0.55250711]', '[ 0.15213765 -0.51456341  0.17665722 -0.29545229]', '[ 0.17195601 -0.54054882  0.01729499  0.04161741]', '[ 0.15877658 -0.49810034 -0.14558791  0.37488532]', '[ 0.11662491 -0.39653924 -0.26514127  0.61927065]', '[ 0.05830606 -0.26143591 -0.30243069  0.70071627]', '[ 0.00240191 -0.12975114 -0.241122    0.58472722]', '[-0.03255824 -0.03901385 -0.09863914  0.30169722]', '[-0.03459084 -0.01467301  0.07923617 -0.06234707]', '[-0.00228999 -0.06214743  0.23549293 -0.3987235 ]', '[ 0.05469493 -0.16555079  0.31932445 -0.60811377]', '[ 0.11857421 -0.29274507  0.30262565 -0.63232462]', '[ 0.16925182 -0.40618487  0.19109743 -0.47671256]', '[ 0.19093562 -0.47518295  0.02014588 -0.20033382]', '[ 0.17663487 -0.48368374 -0.16020096  0.11418666]', '[ 0.12963404 -0.4326335  -0.2991053   0.38177157]', '[ 0.06259366 -0.33924046 -0.35533189  0.52721541]', '[-0.00545982 -0.23320565 -0.30834707  0.50479686]', '[-0.05435734 -0.14835926 -0.16821515  0.32158817]', '[-0.0690908  -0.1113463   0.02479252  0.04024292]', '[-0.04470101 -0.1325791   0.21323988 -0.24461353]', '[ 0.01207873 -0.20303341  0.340642   -0.43848531]', '[ 0.08482177 -0.29746838  0.36917508 -0.47850826]', '[ 0.1525418  -0.38334874  0.2921883  -0.35655192]', '[ 0.19617153 -0.4320439   0.13444274 -0.11715048]', '[ 0.20388778 -0.42720707 -0.05849114  0.16546952]', '[ 0.17398796 -0.36847879 -0.23295603  0.40829353]', '[ 0.1153207  -0.27180171 -0.33916027  0.53394423]', '[ 0.04516552 -0.16633744 -0.34496401  0.4919154 ]', '[-0.0156794  -0.08639963 -0.2487325   0.28429739]', '[-0.04944028 -0.05989949 -0.0814285  -0.02873616]', '[-0.04694202 -0.0986057   0.1044044  -0.35075043]', '[-0.01029722 -0.19395393  0.25133512 -0.58004048]', '[ 0.04794467 -0.31925892  0.31539355 -0.64253249]', '[ 0.10916681 -0.4383569   0.28149033 -0.52044648]', '[ 0.15494366 -0.5175889   0.16566025 -0.25405374]', '[ 0.17232096 -0.53511424  0.00449839  0.08332966]', '[ 0.15672589 -0.48504811 -0.15630978  0.40789288]', '[ 0.11295623 -0.37847862 -0.27006623  0.63512111]', '[ 0.05445207 -0.24243394 -0.29919459  0.6938453 ]', '[-8.55415035e-06 -1.14387117e-01 -2.30313400e-01  5.56016231e-01]', '[-0.03234316 -0.03095466 -0.08398241  0.2590858 ]', '[-0.03149599 -0.01555775  0.09251092 -0.10717874]', '[ 0.00289903 -0.07121941  0.24247762 -0.4340178 ]', '[ 0.06036847 -0.17995142  0.31692464 -0.62513263]', '[ 0.12280364 -0.3084402   0.29089975 -0.62842443]', '[ 0.17046561 -0.41930362  0.17342852 -0.45592275]', '[ 0.18845389 -0.48309582  0.00175629 -0.17045621]', '[ 0.17085017 -0.48542883 -0.17405849  0.14463445]', '[ 0.12188749 -0.42889481 -0.30435303  0.40502489]', '[ 0.05485204 -0.33207856 -0.3499268   0.53755427]', '[-0.01109282 -0.22545104 -0.29306061  0.50055708]', '[-0.0562388  -0.14265631 -0.1468137   0.30626435]', '[-0.06655496 -0.1092283   0.04655432  0.02103969]', '[-0.03828739 -0.13400489  0.22936268 -0.25963315]', '[ 0.02075592 -0.2065006   0.34664538 -0.44320477]', '[ 0.09352759 -0.30065256  0.36349482 -0.4710981 ]', '[ 0.15906701 -0.38405907  0.27660445 -0.34005201]', '[ 0.19893847 -0.42904752  0.11329493 -0.09771185]', '[ 0.20233283 -0.42061863 -0.07962023  0.18082312]', '[ 0.16867979 -0.35978016 -0.24854041  0.41313049]', '[ 0.10781346 -0.26357345 -0.34510867  0.52404886]', '[ 0.03756826 -0.16158606 -0.33999876  0.46757617]', '[-0.02134095 -0.08751632 -0.23493228  0.25129289]', '[-0.05183159 -0.06770688 -0.06340633 -0.06096496]', '[-0.04577688 -0.11192892  0.12105164 -0.37217439]', '[-0.00636211 -0.20981062  0.2617703  -0.58312574]', '[ 0.05311776 -0.33366903  0.31720956 -0.62520875]', '[ 0.11387031 -0.44757142  0.27528967 -0.48691928]', '[ 0.15782037 -0.51913462  0.15413599 -0.2123491 ]', '[ 0.17266067 -0.5282575  -0.00871049  0.12415312]', '[ 0.15459095 -0.47087552 -0.16718667  0.43876966]', '[ 0.10920671 -0.35984165 -0.27480368  0.647718  ]', '[ 0.05058    -0.22357198 -0.29556036  0.68321036]', '[-0.00236243 -0.09988256 -0.21920677  0.52403854]', '[-0.03204327 -0.02428592 -0.06936301  0.21452605]', '[-0.02836262 -0.01805683  0.10536514 -0.15227442]', '[ 0.00801015 -0.08178725  0.24874348 -0.46789726]', '[ 0.06580799 -0.19542955  0.31373207 -0.63949376]', '[ 0.1266619  -0.32462508  0.27865082 -0.62144791]', '[ 0.1712551  -0.4323224   0.15577799 -0.43240974]', '[ 0.18561176 -0.49043688 -0.0160227  -0.13862512]', '[ 0.1648761  -0.48630309 -0.186849    0.1761045 ]', '[ 0.11419159 -0.42417757 -0.308311    0.4283408 ]', '[ 0.04741783 -0.32401123 -0.34329362  0.54714212]', '[-0.01620478 -0.21699361 -0.27691391  0.4951125 ]', '[-0.05748608 -0.13650046 -0.12517129  0.28970765]', '[-0.06340893 -0.10688041  0.06783391  0.0008713 ]', '[-0.03142722 -0.1353568   0.24435981 -0.27524853]', '[ 0.02961009 -0.20998313  0.35113223 -0.44825277]', '[ 0.1020983  -0.30391169  0.35627322 -0.46399804]', '[ 0.16517746 -0.3849238   0.25981792 -0.32405857]', '[ 0.20110697 -0.42633289  0.09154393 -0.07903781]', '[ 0.20012989 -0.41448666 -0.10063599  0.19521183]', '[ 0.16281552 -0.35173902 -0.26334201  0.41696046]', '[ 0.09995635 -0.25618315 -0.34982669  0.51342118]', '[ 0.02988365 -0.1577558  -0.33369746  0.44320173]', '[-0.02684079 -0.08946497 -0.22002454  0.21923835]', '[-0.05388292 -0.07605512 -0.04473508 -0.09125745]', '[-0.04419617 -0.12532797  0.13780688 -0.39095496]', '[-0.00203736 -0.22518866  0.27186677 -0.58342076]', '[ 0.05858556 -0.34708685  0.31844918 -0.60564263]', '[ 0.11874462 -0.45544268  0.26844706 -0.45217168]', '[ 0.16074156 -0.5192091   0.14200673 -0.17059402]', '[ 0.17293733 -0.52003962 -0.02236528  0.16381812]', '[ 0.15233307 -0.45569821 -0.17819456  0.4672458 ]', '[ 0.10534655 -0.34079236 -0.27929557  0.65686383]', '[ 0.04667114 -0.2050374  -0.29148118  0.6687885 ]', '[-0.0046721  -0.0864086  -0.20778504  0.48897506]', '[-0.0316693  -0.01912683 -0.05477854  0.16834437]', '[-0.02520125 -0.02221553  0.11779981 -0.197232  ]', '[ 0.01303363 -0.09381422  0.25429981 -0.49995888]', '[ 0.07100818 -0.21187623  0.30978509 -0.65089385]', '[ 0.13015534 -0.34114643  0.26595612 -0.61125905]', '[ 0.17164421 -0.44507679  0.13823839 -0.40619118]', '[ 0.18245006 -0.49705658 -0.03312004 -0.10496463]', '[ 0.15876336 -0.4861893  -0.19854713  0.20840241]', '[ 0.10659692 -0.41840818 -0.31100554  0.45148228]', '[ 0.04033156 -0.31501379 -0.33550506  0.55573312]', '[-0.02077351 -0.20785551 -0.26001576  0.48824559]', '[-0.05810099 -0.12995242 -0.10341573  0.27175288]', '[-0.05968004 -0.10439027  0.08850812 -0.02036604]', '[-0.02416987 -0.13673713  0.25813825 -0.29150291]', '[ 0.03857817 -0.21358663  0.35406158 -0.45362142]', '[ 0.11046888 -0.3073455   0.34753208 -0.45715734]', '[ 0.17081847 -0.3860283   0.24190825 -0.30847886]', '[ 0.20264264 -0.42396272  0.06930968 -0.06099569]', '[ 0.19727061 -0.40884405 -0.12140226  0.20879956]', '[ 0.15641341 -0.34435319 -0.27723535  0.41996889]', '[ 0.09178962 -0.24959024 -0.35322333  0.50225676]', '[ 0.02216544 -0.15476795 -0.32601707  0.41897253]', '[-0.03212161 -0.09213518 -0.2040166   0.18826462]', '[-0.05554302 -0.08481494 -0.02546602 -0.11955956]', '[-0.04216203 -0.13867226  0.15459085 -0.40713579]', '[ 0.00269779 -0.23997684  0.28153481 -0.58107401]', '[ 0.0643504  -0.35943905  0.31901832 -0.58405638]', '[ 0.12377317 -0.46194498  0.26086964 -0.41645205]', '[ 0.16367404 -0.5178372   0.12920383 -0.12904522]', '[ 0.17310891 -0.51053798 -0.03648228  0.20205679]', '[ 0.14991297 -0.43964671 -0.18929197  0.49306636]', '[ 0.10134809 -0.32150445 -0.28347477  0.66239937]', '[ 0.04270985 -0.18701762 -0.28690959  0.6506117 ]', '[-0.00694698 -0.0741256  -0.19603172  0.45105675]', '[-0.03122902 -0.0155774  -0.0402261   0.12090059]', '[-0.0220194  -0.028055    0.1298159  -0.24163438]', '[ 0.01796282 -0.10723881  0.25915707 -0.52980885]', '[ 0.07596735 -0.22916227  0.30512621 -0.65906496]', '[ 0.13329477 -0.35783934  0.25289537 -0.59776936]', '[ 0.17166109 -0.45739992  0.12089713 -0.37732755]', '[ 0.17901197 -0.50281049 -0.04947757 -0.06963127]', '[ 0.15256201 -0.4849809  -0.20914358  0.24131059]', '[ 0.09915037 -0.41152754 -0.31247672  0.47419686]', '[ 0.03362784 -0.30507832 -0.32664237  0.56307452]', '[-0.02478393 -0.19807613 -0.2424778   0.47974174]', '[-0.05809247 -0.1230885  -0.08167209  0.25224745]', '[-0.05540165 -0.1018578   0.1084618  -0.04275511]', '[-0.01656868 -0.1382555   0.27061726 -0.30841242]', '[ 0.04759589 -0.21741834  0.35540701 -0.45927273]', '[ 0.11857601 -0.31104923  0.33730726 -0.45049543]', '[ 0.17593961 -0.38744781  0.22296617 -0.29319402]', '[ 0.20351716 -0.42198514  0.04671887 -0.0434345 ]', '[ 0.19375359 -0.40370649 -0.14178097  0.22175745]', '[ 0.14949857 -0.33760306 -0.29009763  0.42233593]', '[ 0.08335935 -0.24373903 -0.35521449  0.49073359]', '[ 0.0144715  -0.15253321 -0.31692507  0.3950417 ]', '[-0.03712438 -0.09541205 -0.18692865  0.1584704 ]', '[-0.05676153 -0.09385909 -0.00566356 -0.14584965]', '[-0.03963997 -0.15183938  0.17131257 -0.42078886]', '[ 0.00785856 -0.25407691  0.29067472 -0.57625252]', '[ 0.07040739 -0.37066773  0.31881646 -0.56067911]', '[ 0.12893159 -0.46706878  0.2524664  -0.38000974]', '[ 0.16657823 -0.51505995  0.11567108 -0.08795928]', '[ 0.17313027 -0.49984576 -0.05105896  0.23860635]', '[ 0.14729192 -0.42286497 -0.20042114  0.51599725]']</t>
-  </si>
-  <si>
-    <t>[array([-0.03763371, -0.01533471,  0.06554052, -0.01816017], dtype=float32), array([-0.00754409, -0.05458322,  0.2277812 , -0.36241836]), array([ 0.04879627, -0.15231473,  0.32089719, -0.5887683 ]), array([ 0.11397169, -0.27767857,  0.31375488, -0.63332862]), array([ 0.16759438, -0.39312519,  0.2086893 , -0.49480525]), array([ 0.1930193 , -0.46685036,  0.03906408, -0.22816919]), array([ 0.18217995, -0.48119372, -0.14531723,  0.08492936]), array([ 0.13737799, -0.43548032, -0.29255645,  0.35879992]), array([ 0.07059687, -0.34553749, -0.35944697,  0.51636187]), array([ 0.00066518, -0.24025206, -0.32266973,  0.50804924]), array([-0.05184718, -0.15356453, -0.18924715,  0.33585339]), array([-0.07099568, -0.11316   ,  0.00267821,  0.05860212]), array([-0.0506235 , -0.13098626,  0.19609592, -0.23012254]), array([ 0.00363944, -0.19947979,  0.33317766, -0.43407441]), array([ 0.07604673, -0.29425756,  0.37330708, -0.48624983]), array([ 0.14566012, -0.38269974,  0.30650217, -0.37362319]), array([ 0.19284616, -0.43524651,  0.15487527, -0.13746415]), array([ 0.20480978, -0.43420274, -0.03738189,  0.14899985]), array([ 0.17872861, -0.37781944, -0.21671607,  0.40226469]), array([ 0.12244395, -0.28089207, -0.33207824,  0.54289906]), array([ 0.05262627, -0.17207597, -0.34864539,  0.51601465]), array([-0.00991093, -0.08621824, -0.26142967,  0.31808955]), array([-0.04676022, -0.05276175, -0.09876284,  0.00534115]), array([-0.04773189, -0.08549506,  0.08793289, -0.326671  ]), array([-0.01386808, -0.17774148,  0.24064044, -0.5740393 ]), array([ 0.04305734, -0.30394484,  0.31308665, -0.65740151]), array([ 0.10464298, -0.42784083,  0.2871402 , -0.55250711]), array([ 0.15213765, -0.51456341,  0.17665722, -0.29545229]), array([ 0.17195601, -0.54054882,  0.01729499,  0.04161741]), array([ 0.15877658, -0.49810034, -0.14558791,  0.37488532]), array([ 0.11662491, -0.39653924, -0.26514127,  0.61927065]), array([ 0.05830606, -0.26143591, -0.30243069,  0.70071627]), array([ 0.00240191, -0.12975114, -0.241122  ,  0.58472722]), array([-0.03255824, -0.03901385, -0.09863914,  0.30169722]), array([-0.03459084, -0.01467301,  0.07923617, -0.06234707]), array([-0.00228999, -0.06214743,  0.23549293, -0.3987235 ]), array([ 0.05469493, -0.16555079,  0.31932445, -0.60811377]), array([ 0.11857421, -0.29274507,  0.30262565, -0.63232462]), array([ 0.16925182, -0.40618487,  0.19109743, -0.47671256]), array([ 0.19093562, -0.47518295,  0.02014588, -0.20033382]), array([ 0.17663487, -0.48368374, -0.16020096,  0.11418666]), array([ 0.12963404, -0.4326335 , -0.2991053 ,  0.38177157]), array([ 0.06259366, -0.33924046, -0.35533189,  0.52721541]), array([-0.00545982, -0.23320565, -0.30834707,  0.50479686]), array([-0.05435734, -0.14835926, -0.16821515,  0.32158817]), array([-0.0690908 , -0.1113463 ,  0.02479252,  0.04024292]), array([-0.04470101, -0.1325791 ,  0.21323988, -0.24461353]), array([ 0.01207873, -0.20303341,  0.340642  , -0.43848531]), array([ 0.08482177, -0.29746838,  0.36917508, -0.47850826]), array([ 0.1525418 , -0.38334874,  0.2921883 , -0.35655192]), array([ 0.19617153, -0.4320439 ,  0.13444274, -0.11715048]), array([ 0.20388778, -0.42720707, -0.05849114,  0.16546952]), array([ 0.17398796, -0.36847879, -0.23295603,  0.40829353]), array([ 0.1153207 , -0.27180171, -0.33916027,  0.53394423]), array([ 0.04516552, -0.16633744, -0.34496401,  0.4919154 ]), array([-0.0156794 , -0.08639963, -0.2487325 ,  0.28429739]), array([-0.04944028, -0.05989949, -0.0814285 , -0.02873616]), array([-0.04694202, -0.0986057 ,  0.1044044 , -0.35075043]), array([-0.01029722, -0.19395393,  0.25133512, -0.58004048]), array([ 0.04794467, -0.31925892,  0.31539355, -0.64253249]), array([ 0.10916681, -0.4383569 ,  0.28149033, -0.52044648]), array([ 0.15494366, -0.5175889 ,  0.16566025, -0.25405374]), array([ 0.17232096, -0.53511424,  0.00449839,  0.08332966]), array([ 0.15672589, -0.48504811, -0.15630978,  0.40789288]), array([ 0.11295623, -0.37847862, -0.27006623,  0.63512111]), array([ 0.05445207, -0.24243394, -0.29919459,  0.6938453 ]), array([-8.55415035e-06, -1.14387117e-01, -2.30313400e-01,  5.56016231e-01]), array([-0.03234316, -0.03095466, -0.08398241,  0.2590858 ]), array([-0.03149599, -0.01555775,  0.09251092, -0.10717874]), array([ 0.00289903, -0.07121941,  0.24247762, -0.4340178 ]), array([ 0.06036847, -0.17995142,  0.31692464, -0.62513263]), array([ 0.12280364, -0.3084402 ,  0.29089975, -0.62842443]), array([ 0.17046561, -0.41930362,  0.17342852, -0.45592275]), array([ 0.18845389, -0.48309582,  0.00175629, -0.17045621]), array([ 0.17085017, -0.48542883, -0.17405849,  0.14463445]), array([ 0.12188749, -0.42889481, -0.30435303,  0.40502489]), array([ 0.05485204, -0.33207856, -0.3499268 ,  0.53755427]), array([-0.01109282, -0.22545104, -0.29306061,  0.50055708]), array([-0.0562388 , -0.14265631, -0.1468137 ,  0.30626435]), array([-0.06655496, -0.1092283 ,  0.04655432,  0.02103969]), array([-0.03828739, -0.13400489,  0.22936268, -0.25963315]), array([ 0.02075592, -0.2065006 ,  0.34664538, -0.44320477]), array([ 0.09352759, -0.30065256,  0.36349482, -0.4710981 ]), array([ 0.15906701, -0.38405907,  0.27660445, -0.34005201]), array([ 0.19893847, -0.42904752,  0.11329493, -0.09771185]), array([ 0.20233283, -0.42061863, -0.07962023,  0.18082312]), array([ 0.16867979, -0.35978016, -0.24854041,  0.41313049]), array([ 0.10781346, -0.26357345, -0.34510867,  0.52404886]), array([ 0.03756826, -0.16158606, -0.33999876,  0.46757617]), array([-0.02134095, -0.08751632, -0.23493228,  0.25129289]), array([-0.05183159, -0.06770688, -0.06340633, -0.06096496]), array([-0.04577688, -0.11192892,  0.12105164, -0.37217439]), array([-0.00636211, -0.20981062,  0.2617703 , -0.58312574]), array([ 0.05311776, -0.33366903,  0.31720956, -0.62520875]), array([ 0.11387031, -0.44757142,  0.27528967, -0.48691928]), array([ 0.15782037, -0.51913462,  0.15413599, -0.2123491 ]), array([ 0.17266067, -0.5282575 , -0.00871049,  0.12415312]), array([ 0.15459095, -0.47087552, -0.16718667,  0.43876966]), array([ 0.10920671, -0.35984165, -0.27480368,  0.647718  ]), array([ 0.05058   , -0.22357198, -0.29556036,  0.68321036]), array([-0.00236243, -0.09988256, -0.21920677,  0.52403854]), array([-0.03204327, -0.02428592, -0.06936301,  0.21452605]), array([-0.02836262, -0.01805683,  0.10536514, -0.15227442]), array([ 0.00801015, -0.08178725,  0.24874348, -0.46789726]), array([ 0.06580799, -0.19542955,  0.31373207, -0.63949376]), array([ 0.1266619 , -0.32462508,  0.27865082, -0.62144791]), array([ 0.1712551 , -0.4323224 ,  0.15577799, -0.43240974]), array([ 0.18561176, -0.49043688, -0.0160227 , -0.13862512]), array([ 0.1648761 , -0.48630309, -0.186849  ,  0.1761045 ]), array([ 0.11419159, -0.42417757, -0.308311  ,  0.4283408 ]), array([ 0.04741783, -0.32401123, -0.34329362,  0.54714212]), array([-0.01620478, -0.21699361, -0.27691391,  0.4951125 ]), array([-0.05748608, -0.13650046, -0.12517129,  0.28970765]), array([-0.06340893, -0.10688041,  0.06783391,  0.0008713 ]), array([-0.03142722, -0.1353568 ,  0.24435981, -0.27524853]), array([ 0.02961009, -0.20998313,  0.35113223, -0.44825277]), array([ 0.1020983 , -0.30391169,  0.35627322, -0.46399804]), array([ 0.16517746, -0.3849238 ,  0.25981792, -0.32405857]), array([ 0.20110697, -0.42633289,  0.09154393, -0.07903781]), array([ 0.20012989, -0.41448666, -0.10063599,  0.19521183]), array([ 0.16281552, -0.35173902, -0.26334201,  0.41696046]), array([ 0.09995635, -0.25618315, -0.34982669,  0.51342118]), array([ 0.02988365, -0.1577558 , -0.33369746,  0.44320173]), array([-0.02684079, -0.08946497, -0.22002454,  0.21923835]), array([-0.05388292, -0.07605512, -0.04473508, -0.09125745]), array([-0.04419617, -0.12532797,  0.13780688, -0.39095496]), array([-0.00203736, -0.22518866,  0.27186677, -0.58342076]), array([ 0.05858556, -0.34708685,  0.31844918, -0.60564263]), array([ 0.11874462, -0.45544268,  0.26844706, -0.45217168]), array([ 0.16074156, -0.5192091 ,  0.14200673, -0.17059402]), array([ 0.17293733, -0.52003962, -0.02236528,  0.16381812]), array([ 0.15233307, -0.45569821, -0.17819456,  0.4672458 ]), array([ 0.10534655, -0.34079236, -0.27929557,  0.65686383]), array([ 0.04667114, -0.2050374 , -0.29148118,  0.6687885 ]), array([-0.0046721 , -0.0864086 , -0.20778504,  0.48897506]), array([-0.0316693 , -0.01912683, -0.05477854,  0.16834437]), array([-0.02520125, -0.02221553,  0.11779981, -0.197232  ]), array([ 0.01303363, -0.09381422,  0.25429981, -0.49995888]), array([ 0.07100818, -0.21187623,  0.30978509, -0.65089385]), array([ 0.13015534, -0.34114643,  0.26595612, -0.61125905]), array([ 0.17164421, -0.44507679,  0.13823839, -0.40619118]), array([ 0.18245006, -0.49705658, -0.03312004, -0.10496463]), array([ 0.15876336, -0.4861893 , -0.19854713,  0.20840241]), array([ 0.10659692, -0.41840818, -0.31100554,  0.45148228]), array([ 0.04033156, -0.31501379, -0.33550506,  0.55573312]), array([-0.02077351, -0.20785551, -0.26001576,  0.48824559]), array([-0.05810099, -0.12995242, -0.10341573,  0.27175288]), array([-0.05968004, -0.10439027,  0.08850812, -0.02036604]), array([-0.02416987, -0.13673713,  0.25813825, -0.29150291]), array([ 0.03857817, -0.21358663,  0.35406158, -0.45362142]), array([ 0.11046888, -0.3073455 ,  0.34753208, -0.45715734]), array([ 0.17081847, -0.3860283 ,  0.24190825, -0.30847886]), array([ 0.20264264, -0.42396272,  0.06930968, -0.06099569]), array([ 0.19727061, -0.40884405, -0.12140226,  0.20879956]), array([ 0.15641341, -0.34435319, -0.27723535,  0.41996889]), array([ 0.09178962, -0.24959024, -0.35322333,  0.50225676]), array([ 0.02216544, -0.15476795, -0.32601707,  0.41897253]), array([-0.03212161, -0.09213518, -0.2040166 ,  0.18826462]), array([-0.05554302, -0.08481494, -0.02546602, -0.11955956]), array([-0.04216203, -0.13867226,  0.15459085, -0.40713579]), array([ 0.00269779, -0.23997684,  0.28153481, -0.58107401]), array([ 0.0643504 , -0.35943905,  0.31901832, -0.58405638]), array([ 0.12377317, -0.46194498,  0.26086964, -0.41645205]), array([ 0.16367404, -0.5178372 ,  0.12920383, -0.12904522]), array([ 0.17310891, -0.51053798, -0.03648228,  0.20205679]), array([ 0.14991297, -0.43964671, -0.18929197,  0.49306636]), array([ 0.10134809, -0.32150445, -0.28347477,  0.66239937]), array([ 0.04270985, -0.18701762, -0.28690959,  0.6506117 ]), array([-0.00694698, -0.0741256 , -0.19603172,  0.45105675]), array([-0.03122902, -0.0155774 , -0.0402261 ,  0.12090059]), array([-0.0220194 , -0.028055  ,  0.1298159 , -0.24163438]), array([ 0.01796282, -0.10723881,  0.25915707, -0.52980885]), array([ 0.07596735, -0.22916227,  0.30512621, -0.65906496]), array([ 0.13329477, -0.35783934,  0.25289537, -0.59776936]), array([ 0.17166109, -0.45739992,  0.12089713, -0.37732755]), array([ 0.17901197, -0.50281049, -0.04947757, -0.06963127]), array([ 0.15256201, -0.4849809 , -0.20914358,  0.24131059]), array([ 0.09915037, -0.41152754, -0.31247672,  0.47419686]), array([ 0.03362784, -0.30507832, -0.32664237,  0.56307452]), array([-0.02478393, -0.19807613, -0.2424778 ,  0.47974174]), array([-0.05809247, -0.1230885 , -0.08167209,  0.25224745]), array([-0.05540165, -0.1018578 ,  0.1084618 , -0.04275511]), array([-0.01656868, -0.1382555 ,  0.27061726, -0.30841242]), array([ 0.04759589, -0.21741834,  0.35540701, -0.45927273]), array([ 0.11857601, -0.31104923,  0.33730726, -0.45049543]), array([ 0.17593961, -0.38744781,  0.22296617, -0.29319402]), array([ 0.20351716, -0.42198514,  0.04671887, -0.0434345 ]), array([ 0.19375359, -0.40370649, -0.14178097,  0.22175745]), array([ 0.14949857, -0.33760306, -0.29009763,  0.42233593]), array([ 0.08335935, -0.24373903, -0.35521449,  0.49073359]), array([ 0.0144715 , -0.15253321, -0.31692507,  0.3950417 ]), array([-0.03712438, -0.09541205, -0.18692865,  0.1584704 ]), array([-0.05676153, -0.09385909, -0.00566356, -0.14584965]), array([-0.03963997, -0.15183938,  0.17131257, -0.42078886]), array([ 0.00785856, -0.25407691,  0.29067472, -0.57625252]), array([ 0.07040739, -0.37066773,  0.31881646, -0.56067911]), array([ 0.12893159, -0.46706878,  0.2524664 , -0.38000974]), array([ 0.16657823, -0.51505995,  0.11567108, -0.08795928]), array([ 0.17313027, -0.49984576, -0.05105896,  0.23860635]), array([ 0.14729192, -0.42286497, -0.20042114,  0.51599725])]</t>
-  </si>
-  <si>
-    <t>['[1,1,2]', '[2,2,2]', '[0,0,0]', '[2,1,0]', '[1,2,0]', '[0,2,1]', '[1,1,1]', '[2,0,1]', '[1,0,2]', '[0,1,1]']</t>
-  </si>
-  <si>
-    <t>[1,1,1]</t>
-  </si>
-  <si>
-    <t>[1, 2, 5, 7, 25, 26, 39, 51, 66, 75, 86]</t>
-  </si>
-  <si>
-    <t>[0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 1, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 1, 1, 2, 2]</t>
-  </si>
-  <si>
-    <t>['[-0.03763371 -0.01533471  0.06554052 -0.01816017]', '[-0.0208055  -0.02030166  0.09914155 -0.02801351]', '[ 0.00031733 -0.02489487  0.10765546 -0.0138725 ]', '[ 0.0337014  -0.05856607  0.21818034 -0.31149513]', '[ 0.08319589 -0.1423563   0.26396396 -0.5039722 ]', '[ 0.12048504 -0.21572161  0.09957913 -0.21237203]', '[ 0.13398458 -0.25714508  0.03151146 -0.19293846]', '[ 0.1190497  -0.25604952 -0.17752831  0.20105221]', '[ 0.05312487 -0.14735668 -0.46539685  0.85825167]', '[-0.05750371  0.06989224 -0.61111084  1.2582138 ]', '[-0.17758625  0.3295346  -0.55656354  1.27360118]', '[-0.26783881  0.5552509  -0.32299032  0.93743487]', '[-0.30030198  0.69079327  0.00564814  0.39824539]', '[-0.24168588  0.64801578  0.56839613 -0.81531326]', '[-0.08155758  0.37565706  0.99953856 -1.85542992]', '[ 0.13883067 -0.05956897  1.14376263 -2.38056635]', '[ 0.34852154 -0.52279863  0.89370767 -2.13574381]', '[ 0.47772468 -0.87861805  0.37135085 -1.37074222]', '[ 0.49199729 -1.05970536 -0.22776408 -0.42867516]', '[ 0.37010211 -0.99215632 -0.96765383  1.09381885]', '[ 0.11754845 -0.63091028 -1.51554178  2.46920752]', '[-0.21145526 -0.04427496 -1.69009148  3.23729734]', '[-0.51766061  0.58326712 -1.28430463  2.86843422]', '[-0.69993983  1.05826468 -0.50619158  1.8296584 ]', '[-0.71515815  1.30646747  0.35013086  0.64410116]', '[-0.55734592  1.28800291  1.19656248 -0.8253871 ]', '[-0.25323497  0.98080132  1.79430897 -2.21498453]', '[ 0.14744411  0.39786733  2.13525128 -3.49052657]', '[ 0.55760473 -0.331413    1.84924173 -3.56635974]', '[ 0.846794   -0.95201514  0.98418717 -2.54475579]', '[ 0.93972156 -1.33532885 -0.06279431 -1.27661633]', '[ 0.80659119 -1.407157   -1.24016826  0.56537885]', '[ 0.45957757 -1.10400275 -2.18080819  2.46844293]', '[-0.04077502 -0.43429768 -2.73371245  4.09694882]', '[-0.57862357  0.42496206 -2.48999214  4.17309363]', '[-0.98681406  1.13920919 -1.52855835  2.88500447]', '[-1.17860873  1.57774878 -0.37775608  1.51510217]', '[-1.13715008  1.74752129  0.78407597  0.1733197 ]', '[-0.85728732  1.59045321  1.97849956 -1.77750735]', '[-0.37370384  1.0490758   2.79919078 -3.6315345 ]', '[ 0.24120082  0.14433948  3.21449134 -5.14806122]', '[ 0.83329371 -0.83661688  2.54924926 -4.336215  ]', '[ 1.22889406 -1.54407173  1.37929951 -2.75444745]', '[ 1.38063769 -1.95465899  0.13430249 -1.3754132 ]', '[ 1.2767232  -2.07275117 -1.1590367   0.21119602]', '[ 0.92041566 -1.83447932 -2.36307962  2.21981129]', '[ 0.35213422 -1.16277112 -3.26823819  4.53240891]', '[-0.35686287 -0.05351501 -3.65553374  6.19420068]', '[-1.01126704  1.08629002 -2.72666589  4.86809896]', '[-1.42692262  1.88010539 -1.42186247  3.14265439]', '[-1.57976448  2.36824302 -0.10969451  1.76703903]', '[-1.46752877  2.56695661  1.21896878  0.20570317]', '[-1.09423989  2.42032586  2.47502161 -1.70637256]', '[-0.50365291  1.8667669   3.35001809 -3.8810477 ]', '[ 0.21681425  0.85190647  3.79819352 -6.2233582 ]', '[ 0.95809743 -0.48448575  3.369586   -6.55055464]', '[ 1.48651987 -1.60419918  1.86800421 -4.62669126]', '[ 1.70744013 -2.37312222  0.35713503 -3.12473182]', '[ 1.63911336 -2.86141323 -1.01191828 -1.7545845 ]', '[ 1.30075595 -3.03390874 -2.34891866  0.02302721]', '[ 0.71402257 -2.85975278 -3.44380755  1.69140714]', '[-0.02506254 -2.3690977  -3.7836923   3.17921819]', '[-0.7371457  -1.61252345 -3.24351524  4.29689726]', '[-1.30726489 -0.69525206 -2.43984106  4.74912865]', '[-1.69866878  0.22854619 -1.41974654  4.3559442 ]', '[-1.85119168  1.01037397 -0.04898171  3.40215235]', '[-1.68779432  1.53512049  1.71330287  1.75143053]', '[-1.15942101  1.63590172  3.51282352 -0.87909868]', '[-0.32612025  1.13933494  4.68565492 -4.10975868]', '[ 0.65174817  0.06268903  4.8751933  -6.1266568 ]', '[ 1.5242895  -1.03533777  3.72771099 -4.53387479]', '[ 2.14679065 -1.77292175  2.54869655 -3.01452251]', '[ 2.56565783 -2.30287979  1.69486567 -2.40014573]', '[ 2.8454193  -2.76243394  1.15700389 -2.24062904]', '[ 3.04997523  3.07492097  0.94686494 -2.23091554]', '[-3.04258121  2.64522435  1.01349099 -2.07669037]', '[-2.80185193  2.21677582  1.44506244 -2.24656912]', '[-2.44326696  1.72119476  2.20167801 -2.81245625]', '[-1.89311085  1.03214947  3.38171343 -4.27357103]', '[-1.06410037 -0.04780188  4.86596803 -6.34354573]', '[-0.02337249 -1.25215064  5.3285208  -5.07304313]', '[ 1.00031263 -1.95571996  4.72462735 -1.91265455]', '[ 1.80039117 -2.05269831  3.17957074  0.78453728]', '[ 2.25214286 -1.69179925  1.35397891  2.65347144]', '[ 2.36246562 -1.04617651 -0.18551211  3.71447391]', '[ 2.18767625 -0.18616571 -1.52693574  4.89642513]', '[ 1.78068902  0.86621377 -2.50629373  5.54426643]']</t>
-  </si>
-  <si>
-    <t>[0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50, 51, 52, 53, 54, 55, 56, 57, 58, 59, 60, 61, 62, 63, 64, 65, 66, 67, 68, 69, 70, 71, 72, 73, 74, 75, 76, 77, 78, 79, 80, 81, 82, 83, 84, 85, 86]</t>
-  </si>
-  <si>
-    <t>[array([-0.03763371, -0.01533471,  0.06554052, -0.01816017], dtype=float32), array([-0.0208055 , -0.02030166,  0.09914155, -0.02801351]), array([ 0.00031733, -0.02489487,  0.10765546, -0.0138725 ]), array([ 0.0337014 , -0.05856607,  0.21818034, -0.31149513]), array([ 0.08319589, -0.1423563 ,  0.26396396, -0.5039722 ]), array([ 0.12048504, -0.21572161,  0.09957913, -0.21237203]), array([ 0.13398458, -0.25714508,  0.03151146, -0.19293846]), array([ 0.1190497 , -0.25604952, -0.17752831,  0.20105221]), array([ 0.05312487, -0.14735668, -0.46539685,  0.85825167]), array([-0.05750371,  0.06989224, -0.61111084,  1.2582138 ]), array([-0.17758625,  0.3295346 , -0.55656354,  1.27360118]), array([-0.26783881,  0.5552509 , -0.32299032,  0.93743487]), array([-0.30030198,  0.69079327,  0.00564814,  0.39824539]), array([-0.24168588,  0.64801578,  0.56839613, -0.81531326]), array([-0.08155758,  0.37565706,  0.99953856, -1.85542992]), array([ 0.13883067, -0.05956897,  1.14376263, -2.38056635]), array([ 0.34852154, -0.52279863,  0.89370767, -2.13574381]), array([ 0.47772468, -0.87861805,  0.37135085, -1.37074222]), array([ 0.49199729, -1.05970536, -0.22776408, -0.42867516]), array([ 0.37010211, -0.99215632, -0.96765383,  1.09381885]), array([ 0.11754845, -0.63091028, -1.51554178,  2.46920752]), array([-0.21145526, -0.04427496, -1.69009148,  3.23729734]), array([-0.51766061,  0.58326712, -1.28430463,  2.86843422]), array([-0.69993983,  1.05826468, -0.50619158,  1.8296584 ]), array([-0.71515815,  1.30646747,  0.35013086,  0.64410116]), array([-0.55734592,  1.28800291,  1.19656248, -0.8253871 ]), array([-0.25323497,  0.98080132,  1.79430897, -2.21498453]), array([ 0.14744411,  0.39786733,  2.13525128, -3.49052657]), array([ 0.55760473, -0.331413  ,  1.84924173, -3.56635974]), array([ 0.846794  , -0.95201514,  0.98418717, -2.54475579]), array([ 0.93972156, -1.33532885, -0.06279431, -1.27661633]), array([ 0.80659119, -1.407157  , -1.24016826,  0.56537885]), array([ 0.45957757, -1.10400275, -2.18080819,  2.46844293]), array([-0.04077502, -0.43429768, -2.73371245,  4.09694882]), array([-0.57862357,  0.42496206, -2.48999214,  4.17309363]), array([-0.98681406,  1.13920919, -1.52855835,  2.88500447]), array([-1.17860873,  1.57774878, -0.37775608,  1.51510217]), array([-1.13715008,  1.74752129,  0.78407597,  0.1733197 ]), array([-0.85728732,  1.59045321,  1.97849956, -1.77750735]), array([-0.37370384,  1.0490758 ,  2.79919078, -3.6315345 ]), array([ 0.24120082,  0.14433948,  3.21449134, -5.14806122]), array([ 0.83329371, -0.83661688,  2.54924926, -4.336215  ]), array([ 1.22889406, -1.54407173,  1.37929951, -2.75444745]), array([ 1.38063769, -1.95465899,  0.13430249, -1.3754132 ]), array([ 1.2767232 , -2.07275117, -1.1590367 ,  0.21119602]), array([ 0.92041566, -1.83447932, -2.36307962,  2.21981129]), array([ 0.35213422, -1.16277112, -3.26823819,  4.53240891]), array([-0.35686287, -0.05351501, -3.65553374,  6.19420068]), array([-1.01126704,  1.08629002, -2.72666589,  4.86809896]), array([-1.42692262,  1.88010539, -1.42186247,  3.14265439]), array([-1.57976448,  2.36824302, -0.10969451,  1.76703903]), array([-1.46752877,  2.56695661,  1.21896878,  0.20570317]), array([-1.09423989,  2.42032586,  2.47502161, -1.70637256]), array([-0.50365291,  1.8667669 ,  3.35001809, -3.8810477 ]), array([ 0.21681425,  0.85190647,  3.79819352, -6.2233582 ]), array([ 0.95809743, -0.48448575,  3.369586  , -6.55055464]), array([ 1.48651987, -1.60419918,  1.86800421, -4.62669126]), array([ 1.70744013, -2.37312222,  0.35713503, -3.12473182]), array([ 1.63911336, -2.86141323, -1.01191828, -1.7545845 ]), array([ 1.30075595, -3.03390874, -2.34891866,  0.02302721]), array([ 0.71402257, -2.85975278, -3.44380755,  1.69140714]), array([-0.02506254, -2.3690977 , -3.7836923 ,  3.17921819]), array([-0.7371457 , -1.61252345, -3.24351524,  4.29689726]), array([-1.30726489, -0.69525206, -2.43984106,  4.74912865]), array([-1.69866878,  0.22854619, -1.41974654,  4.3559442 ]), array([-1.85119168,  1.01037397, -0.04898171,  3.40215235]), array([-1.68779432,  1.53512049,  1.71330287,  1.75143053]), array([-1.15942101,  1.63590172,  3.51282352, -0.87909868]), array([-0.32612025,  1.13933494,  4.68565492, -4.10975868]), array([ 0.65174817,  0.06268903,  4.8751933 , -6.1266568 ]), array([ 1.5242895 , -1.03533777,  3.72771099, -4.53387479]), array([ 2.14679065, -1.77292175,  2.54869655, -3.01452251]), array([ 2.56565783, -2.30287979,  1.69486567, -2.40014573]), array([ 2.8454193 , -2.76243394,  1.15700389, -2.24062904]), array([ 3.04997523,  3.07492097,  0.94686494, -2.23091554]), array([-3.04258121,  2.64522435,  1.01349099, -2.07669037]), array([-2.80185193,  2.21677582,  1.44506244, -2.24656912]), array([-2.44326696,  1.72119476,  2.20167801, -2.81245625]), array([-1.89311085,  1.03214947,  3.38171343, -4.27357103]), array([-1.06410037, -0.04780188,  4.86596803, -6.34354573]), array([-0.02337249, -1.25215064,  5.3285208 , -5.07304313]), array([ 1.00031263, -1.95571996,  4.72462735, -1.91265455]), array([ 1.80039117, -2.05269831,  3.17957074,  0.78453728]), array([ 2.25214286, -1.69179925,  1.35397891,  2.65347144]), array([ 2.36246562, -1.04617651, -0.18551211,  3.71447391]), array([ 2.18767625, -0.18616571, -1.52693574,  4.89642513]), array([ 1.78068902,  0.86621377, -2.50629373,  5.54426643])]</t>
-  </si>
-  <si>
-    <t>['[2,2,2]', '[0,1,1]', '[1,1,2]', '[1,2,0]', '[0,2,1]', '[2,1,0]', '[1,1,1]', '[2,0,1]', '[0,0,0]', '[1,0,2]']</t>
-  </si>
-  <si>
-    <t>[5, 6, 7, 8, 10, 13, 14, 15, 18, 20, 24, 27, 28, 29, 32, 35, 36, 37, 38, 40, 41, 43, 45, 46, 47, 48, 50, 54, 55, 56, 59, 60, 61, 63, 64, 68, 69, 71, 73, 74, 75, 77, 78, 88, 89, 90, 91, 93, 96, 98, 101, 109, 110, 114, 116, 118, 120, 121, 122, 125, 129, 131, 133]</t>
-  </si>
-  <si>
-    <t>[0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 1, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 1, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 2, 1, 0, 0, 0, 0, 0, 0, 0, 0, 1, 2, 2, 2, 2, 2]</t>
-  </si>
-  <si>
-    <t>['[-0.03763371 -0.01533471  0.06554052 -0.01816017]', '[-0.00754409 -0.05458322  0.2277812  -0.36241836]', '[ 0.04879627 -0.15231473  0.32089719 -0.5887683 ]', '[ 0.11397169 -0.27767857  0.31375488 -0.63332862]', '[ 0.16759438 -0.39312519  0.2086893  -0.49480525]', '[ 0.18032045 -0.433785   -0.08419275  0.09486206]', '[ 0.13535958 -0.35707285 -0.35476887  0.65463036]', '[ 0.04527264 -0.1839383  -0.52327264  1.03511377]', '[-0.06278322  0.03606301 -0.52806312  1.10902897]', '[-0.16729646  0.27088322 -0.48782347  1.18115937]', '[-0.23404889  0.45288108 -0.16315955  0.60361495]', '[-0.24170328  0.53663909  0.08937521  0.22155186]', '[-0.17454635  0.47474172  0.56785372 -0.8244034 ]', '[-0.03717982  0.25457092  0.77319862 -1.32323968]', '[ 0.11891717 -0.02666851  0.74668337 -1.41389647]', '[ 0.24516335 -0.28054951  0.48287507 -1.06288743]', '[ 0.3147406  -0.46574006  0.19464206 -0.75110606]', '[ 0.31850788 -0.56993195 -0.15923913 -0.27634267]', '[ 0.24089504 -0.54233482 -0.60062632  0.53924721]', '[ 0.07570195 -0.33252783 -1.01552588  1.50868987]', '[-0.13291977 -0.00423124 -1.01749477  1.68109856]', '[-0.32274074  0.33502594 -0.83113046  1.62128302]', '[-0.44813303  0.61304809 -0.39335167  1.10495336]', '[-0.47282535  0.76263359  0.15157155  0.37278432]', '[-0.37802659  0.72878946  0.77779304 -0.70041331]', '[-0.16138     0.4610727   1.34634858 -1.92463083]', '[ 0.13664204 -0.00390002  1.55847756 -2.59086054]', '[ 0.41454182 -0.47734054  1.15064076 -2.01769986]', '[ 0.57646736 -0.77749098  0.43985842 -0.94234699]', '[ 0.58498298 -0.84678894 -0.35448908  0.25357561]', '[ 0.42760025 -0.64699003 -1.1943246   1.72385811]', '[ 0.12436449 -0.17844788 -1.7706098   2.85137472]', '[-0.22950845  0.3893232  -1.67193167  2.64621534]', '[-0.52337482  0.8534767  -1.20557812  1.90119874]', '[-0.69485386  1.1296855  -0.48458428  0.8405573 ]', '[-0.70186689  1.15896237  0.41406141 -0.54766793]', '[-0.53329136  0.91096338  1.24977777 -1.92200349]', '[-0.21699044  0.40449566  1.85183988 -3.05151011]', '[ 0.17001543 -0.24183611  1.90811769 -3.1988926 ]', '[ 0.51610881 -0.82648909  1.47305751 -2.51038452]', '[ 0.72726818 -1.18880344  0.61348477 -1.09749189]', '[ 0.75656555 -1.26514341 -0.32173759  0.33324941]', '[ 0.59154573 -1.02679557 -1.31159481  2.05399948]', '[ 0.25592869 -0.48057301 -1.98531734  3.32627234]', '[-0.17669164  0.26707341 -2.21295065  3.89572126]', '[-0.5645079   0.94207089 -1.58393195  2.71705677]', '[-0.7921633   1.33507126 -0.66978536  1.20900597]', '[-0.82787881  1.42800418  0.31366653 -0.27676451]', '[-0.66990479  1.22294827  1.24828153 -1.77911484]', '[-0.328922    0.68771186  2.11932607 -3.54082303]', '[ 0.13169839 -0.10565801  2.35491225 -4.13072538]', '[ 0.56642081 -0.87700954  1.88211344 -3.37689023]', '[ 0.85810681 -1.4197292   1.00196461 -2.03321449]', '[ 0.96034217 -1.69300437  0.01492189 -0.7069247 ]', '[ 0.85787768 -1.67894557 -1.02217745  0.85365997]', '[ 0.56250185 -1.3462815  -1.89552354  2.48370301]', '[ 0.11799483 -0.68916537 -2.48518301  4.01415089]', '[-0.40075301  0.2123135  -2.54788533  4.67838486]', '[-0.83664223  1.04977742 -1.71511899  3.52934171]', '[-1.0601967   1.58346898 -0.51197175  1.83116576]', '[-1.04244156  1.78946562  0.6769941   0.23092454]', '[-0.79896494  1.67122337  1.72148536 -1.43129732]', '[-0.36408955  1.18414116  2.57636432 -3.44959683]', '[ 0.19426897  0.34205479  2.89728063 -4.76921898]', '[ 0.72783137 -0.58003306  2.28381473 -4.12767313]', '[ 1.08044739 -1.27129     1.19842244 -2.74404035]', '[ 1.20013926 -1.68159547 -0.00600163 -1.36892373]', '[ 1.07266461 -1.79361378 -1.24699689  0.26504955]', '[ 0.71570553 -1.56463961 -2.27274932  2.05166961]', '[ 0.18841504 -0.96813971 -2.9295686   3.87647857]', '[-0.42910271 -0.04116103 -3.09775795  5.08170301]', '[-0.96383856  0.86853421 -2.12934488  3.78057625]', '[-1.2711665   1.47918796 -0.92324338  2.34096307]', '[-1.32184125  1.78983886  0.41179867  0.7745128 ]', '[-1.11149318  1.78246416  1.66751601 -0.88270303]', '[-0.6704824   1.41915097  2.69024319 -2.78843836]', '[-0.05080478  0.63603497  3.42484642 -4.95509263]', '[ 0.62470062 -0.40134353  3.12965393 -4.96702175]', '[ 1.13907991 -1.22195068  1.95376979 -3.16970819]', '[ 1.4085201  -1.71130613  0.73076501 -1.7648358 ]', '[ 1.4296688  -1.93711613 -0.51854607 -0.49105645]', '[ 1.18970303 -1.85268803 -1.85925925  1.38092796]', '[ 0.69934862 -1.35905829 -3.00337945  3.62360398]', '[ 0.00907633 -0.39365096 -3.7958477   5.86051487]', '[-0.73079891  0.78291996 -3.37537142  5.38445644]', '[-1.29136911  1.66700293 -2.19902896  3.48390682]', '[-1.60707749  2.21086808 -0.95452247  2.02112082]', '[-1.67322333  2.48910457  0.29065826  0.76733972]', '[-1.48609014  2.49199919  1.57237015 -0.76709356]', '[-1.05198341  2.16501022  2.72956982 -2.56149924]', '[-0.41793898  1.43983159  3.5507968  -4.75045261]', '[ 0.34223973  0.2750334   3.91224637 -6.59444638]', '[ 1.05587224 -0.98086944  3.01818429 -5.50301539]', '[ 1.51190562 -1.86533592  1.54857933 -3.44630244]', '[ 1.68668493 -2.41579943  0.20608895 -2.09292106]', '[ 1.59817009 -2.70348787 -1.08079416 -0.7685613 ]', '[ 1.25342485 -2.69467727 -2.342633    0.87965437]', '[ 0.67530856 -2.32150523 -3.3501273   2.88434751]', '[-0.03380902 -1.55191941 -3.64290612  4.80794066]', '[-0.76390075 -0.39928437 -3.56791903  6.48261363]', '[-1.38387408  0.84607882 -2.45568893  5.58175845]', '[-1.70600232  1.76876703 -0.76525367  3.71821246]', '[-1.70074199  2.37396852  0.80550874  2.32630905]', '[-1.38795366  2.66767349  2.2846084   0.58346259]', '[-0.8014927   2.58058281  3.49504627 -1.45999195]', '[-0.04299211  2.08667254  3.9311105  -3.45274428]', '[ 0.7145081   1.22474914  3.56602244 -5.06061566]', '[ 1.36383479  0.1333778   2.85102235 -5.58882186]', '[ 1.81226028 -0.8997406   1.55926016 -4.60823619]', '[ 1.96251028 -1.67831832 -0.07388627 -3.19657225]', '[ 1.7771403  -2.16743366 -1.77999411 -1.62347754]', '[ 1.25338873 -2.27040339 -3.39984003  0.68697896]', '[ 0.45763428 -1.86018429 -4.41705895  3.47252898]', '[-0.45562832 -0.88263275 -4.61163944  6.17373758]', '[-1.31628431  0.40624818 -3.79737183  6.13306056]', '[-1.93691269  1.46824701 -2.40653197  4.51233116]', '[-2.28454969  2.2402094  -1.10907659  3.31661064]', '[-2.40033931  2.83352717 -0.08405693  2.61571526]', '[-2.3256029  -3.02631424  0.81101087  1.58433346]', '[-2.07393909 -2.83068344  1.73249116  0.34105868]', '[-1.61684559 -2.8980208   2.87519245 -1.02075477]', '[-0.91970541  3.0451714   4.0495066  -2.37894249]', '[-0.04849793  2.42857715  4.47203733 -3.80206995]', '[ 0.80080883  1.51251363  3.92346273 -5.2861147 ]', '[ 1.51095998  0.36652933  3.15097602 -5.96624798]', '[ 2.01781304 -0.73485168  1.85593329 -4.9041906 ]', '[ 2.25265803 -1.62394966  0.46313934 -4.00732323]', '[ 2.19047205 -2.33298899 -1.10132597 -3.02934715]', '[ 1.81104144 -2.78680016 -2.66146644 -1.44448334]', '[ 1.13816102 -2.89422584 -4.02171163  0.37971354]', '[ 0.23435436 -2.62319806 -4.84779831  2.29078716]', '[-0.70637953 -2.02525588 -4.36620522  3.56789902]', '[-1.47450356 -1.23892582 -3.28661943  4.12592402]', '[-2.01499328 -0.4629068  -2.13658535  3.52987878]']</t>
-  </si>
-  <si>
-    <t>[0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50, 51, 52, 53, 54, 55, 56, 57, 58, 59, 60, 61, 62, 63, 64, 65, 66, 67, 68, 69, 70, 71, 72, 73, 74, 75, 76, 77, 78, 79, 80, 81, 82, 83, 84, 85, 86, 87, 88, 89, 90, 91, 92, 93, 94, 95, 96, 97, 98, 99, 100, 101, 102, 103, 104, 105, 106, 107, 108, 109, 110, 111, 112, 113, 114, 115, 116, 117, 118, 119, 120, 121, 122, 123, 124, 125, 126, 127, 128, 129, 130, 131, 132, 133]</t>
-  </si>
-  <si>
-    <t>[array([-0.03763371, -0.01533471,  0.06554052, -0.01816017], dtype=float32), array([-0.00754409, -0.05458322,  0.2277812 , -0.36241836]), array([ 0.04879627, -0.15231473,  0.32089719, -0.5887683 ]), array([ 0.11397169, -0.27767857,  0.31375488, -0.63332862]), array([ 0.16759438, -0.39312519,  0.2086893 , -0.49480525]), array([ 0.18032045, -0.433785  , -0.08419275,  0.09486206]), array([ 0.13535958, -0.35707285, -0.35476887,  0.65463036]), array([ 0.04527264, -0.1839383 , -0.52327264,  1.03511377]), array([-0.06278322,  0.03606301, -0.52806312,  1.10902897]), array([-0.16729646,  0.27088322, -0.48782347,  1.18115937]), array([-0.23404889,  0.45288108, -0.16315955,  0.60361495]), array([-0.24170328,  0.53663909,  0.08937521,  0.22155186]), array([-0.17454635,  0.47474172,  0.56785372, -0.8244034 ]), array([-0.03717982,  0.25457092,  0.77319862, -1.32323968]), array([ 0.11891717, -0.02666851,  0.74668337, -1.41389647]), array([ 0.24516335, -0.28054951,  0.48287507, -1.06288743]), array([ 0.3147406 , -0.46574006,  0.19464206, -0.75110606]), array([ 0.31850788, -0.56993195, -0.15923913, -0.27634267]), array([ 0.24089504, -0.54233482, -0.60062632,  0.53924721]), array([ 0.07570195, -0.33252783, -1.01552588,  1.50868987]), array([-0.13291977, -0.00423124, -1.01749477,  1.68109856]), array([-0.32274074,  0.33502594, -0.83113046,  1.62128302]), array([-0.44813303,  0.61304809, -0.39335167,  1.10495336]), array([-0.47282535,  0.76263359,  0.15157155,  0.37278432]), array([-0.37802659,  0.72878946,  0.77779304, -0.70041331]), array([-0.16138   ,  0.4610727 ,  1.34634858, -1.92463083]), array([ 0.13664204, -0.00390002,  1.55847756, -2.59086054]), array([ 0.41454182, -0.47734054,  1.15064076, -2.01769986]), array([ 0.57646736, -0.77749098,  0.43985842, -0.94234699]), array([ 0.58498298, -0.84678894, -0.35448908,  0.25357561]), array([ 0.42760025, -0.64699003, -1.1943246 ,  1.72385811]), array([ 0.12436449, -0.17844788, -1.7706098 ,  2.85137472]), array([-0.22950845,  0.3893232 , -1.67193167,  2.64621534]), array([-0.52337482,  0.8534767 , -1.20557812,  1.90119874]), array([-0.69485386,  1.1296855 , -0.48458428,  0.8405573 ]), array([-0.70186689,  1.15896237,  0.41406141, -0.54766793]), array([-0.53329136,  0.91096338,  1.24977777, -1.92200349]), array([-0.21699044,  0.40449566,  1.85183988, -3.05151011]), array([ 0.17001543, -0.24183611,  1.90811769, -3.1988926 ]), array([ 0.51610881, -0.82648909,  1.47305751, -2.51038452]), array([ 0.72726818, -1.18880344,  0.61348477, -1.09749189]), array([ 0.75656555, -1.26514341, -0.32173759,  0.33324941]), array([ 0.59154573, -1.02679557, -1.31159481,  2.05399948]), array([ 0.25592869, -0.48057301, -1.98531734,  3.32627234]), array([-0.17669164,  0.26707341, -2.21295065,  3.89572126]), array([-0.5645079 ,  0.94207089, -1.58393195,  2.71705677]), array([-0.7921633 ,  1.33507126, -0.66978536,  1.20900597]), array([-0.82787881,  1.42800418,  0.31366653, -0.27676451]), array([-0.66990479,  1.22294827,  1.24828153, -1.77911484]), array([-0.328922  ,  0.68771186,  2.11932607, -3.54082303]), array([ 0.13169839, -0.10565801,  2.35491225, -4.13072538]), array([ 0.56642081, -0.87700954,  1.88211344, -3.37689023]), array([ 0.85810681, -1.4197292 ,  1.00196461, -2.03321449]), array([ 0.96034217, -1.69300437,  0.01492189, -0.7069247 ]), array([ 0.85787768, -1.67894557, -1.02217745,  0.85365997]), array([ 0.56250185, -1.3462815 , -1.89552354,  2.48370301]), array([ 0.11799483, -0.68916537, -2.48518301,  4.01415089]), array([-0.40075301,  0.2123135 , -2.54788533,  4.67838486]), array([-0.83664223,  1.04977742, -1.71511899,  3.52934171]), array([-1.0601967 ,  1.58346898, -0.51197175,  1.83116576]), array([-1.04244156,  1.78946562,  0.6769941 ,  0.23092454]), array([-0.79896494,  1.67122337,  1.72148536, -1.43129732]), array([-0.36408955,  1.18414116,  2.57636432, -3.44959683]), array([ 0.19426897,  0.34205479,  2.89728063, -4.76921898]), array([ 0.72783137, -0.58003306,  2.28381473, -4.12767313]), array([ 1.08044739, -1.27129   ,  1.19842244, -2.74404035]), array([ 1.20013926, -1.68159547, -0.00600163, -1.36892373]), array([ 1.07266461, -1.79361378, -1.24699689,  0.26504955]), array([ 0.71570553, -1.56463961, -2.27274932,  2.05166961]), array([ 0.18841504, -0.96813971, -2.9295686 ,  3.87647857]), array([-0.42910271, -0.04116103, -3.09775795,  5.08170301]), array([-0.96383856,  0.86853421, -2.12934488,  3.78057625]), array([-1.2711665 ,  1.47918796, -0.92324338,  2.34096307]), array([-1.32184125,  1.78983886,  0.41179867,  0.7745128 ]), array([-1.11149318,  1.78246416,  1.66751601, -0.88270303]), array([-0.6704824 ,  1.41915097,  2.69024319, -2.78843836]), array([-0.05080478,  0.63603497,  3.42484642, -4.95509263]), array([ 0.62470062, -0.40134353,  3.12965393, -4.96702175]), array([ 1.13907991, -1.22195068,  1.95376979, -3.16970819]), array([ 1.4085201 , -1.71130613,  0.73076501, -1.7648358 ]), array([ 1.4296688 , -1.93711613, -0.51854607, -0.49105645]), array([ 1.18970303, -1.85268803, -1.85925925,  1.38092796]), array([ 0.69934862, -1.35905829, -3.00337945,  3.62360398]), array([ 0.00907633, -0.39365096, -3.7958477 ,  5.86051487]), array([-0.73079891,  0.78291996, -3.37537142,  5.38445644]), array([-1.29136911,  1.66700293, -2.19902896,  3.48390682]), array([-1.60707749,  2.21086808, -0.95452247,  2.02112082]), array([-1.67322333,  2.48910457,  0.29065826,  0.76733972]), array([-1.48609014,  2.49199919,  1.57237015, -0.76709356]), array([-1.05198341,  2.16501022,  2.72956982, -2.56149924]), array([-0.41793898,  1.43983159,  3.5507968 , -4.75045261]), array([ 0.34223973,  0.2750334 ,  3.91224637, -6.59444638]), array([ 1.05587224, -0.98086944,  3.01818429, -5.50301539]), array([ 1.51190562, -1.86533592,  1.54857933, -3.44630244]), array([ 1.68668493, -2.41579943,  0.20608895, -2.09292106]), array([ 1.59817009, -2.70348787, -1.08079416, -0.7685613 ]), array([ 1.25342485, -2.69467727, -2.342633  ,  0.87965437]), array([ 0.67530856, -2.32150523, -3.3501273 ,  2.88434751]), array([-0.03380902, -1.55191941, -3.64290612,  4.80794066]), array([-0.76390075, -0.39928437, -3.56791903,  6.48261363]), array([-1.38387408,  0.84607882, -2.45568893,  5.58175845]), array([-1.70600232,  1.76876703, -0.76525367,  3.71821246]), array([-1.70074199,  2.37396852,  0.80550874,  2.32630905]), array([-1.38795366,  2.66767349,  2.2846084 ,  0.58346259]), array([-0.8014927 ,  2.58058281,  3.49504627, -1.45999195]), array([-0.04299211,  2.08667254,  3.9311105 , -3.45274428]), array([ 0.7145081 ,  1.22474914,  3.56602244, -5.06061566]), array([ 1.36383479,  0.1333778 ,  2.85102235, -5.58882186]), array([ 1.81226028, -0.8997406 ,  1.55926016, -4.60823619]), array([ 1.96251028, -1.67831832, -0.07388627, -3.19657225]), array([ 1.7771403 , -2.16743366, -1.77999411, -1.62347754]), array([ 1.25338873, -2.27040339, -3.39984003,  0.68697896]), array([ 0.45763428, -1.86018429, -4.41705895,  3.47252898]), array([-0.45562832, -0.88263275, -4.61163944,  6.17373758]), array([-1.31628431,  0.40624818, -3.79737183,  6.13306056]), array([-1.93691269,  1.46824701, -2.40653197,  4.51233116]), array([-2.28454969,  2.2402094 , -1.10907659,  3.31661064]), array([-2.40033931,  2.83352717, -0.08405693,  2.61571526]), array([-2.3256029 , -3.02631424,  0.81101087,  1.58433346]), array([-2.07393909, -2.83068344,  1.73249116,  0.34105868]), array([-1.61684559, -2.8980208 ,  2.87519245, -1.02075477]), array([-0.91970541,  3.0451714 ,  4.0495066 , -2.37894249]), array([-0.04849793,  2.42857715,  4.47203733, -3.80206995]), array([ 0.80080883,  1.51251363,  3.92346273, -5.2861147 ]), array([ 1.51095998,  0.36652933,  3.15097602, -5.96624798]), array([ 2.01781304, -0.73485168,  1.85593329, -4.9041906 ]), array([ 2.25265803, -1.62394966,  0.46313934, -4.00732323]), array([ 2.19047205, -2.33298899, -1.10132597, -3.02934715]), array([ 1.81104144, -2.78680016, -2.66146644, -1.44448334]), array([ 1.13816102, -2.89422584, -4.02171163,  0.37971354]), array([ 0.23435436, -2.62319806, -4.84779831,  2.29078716]), array([-0.70637953, -2.02525588, -4.36620522,  3.56789902]), array([-1.47450356, -1.23892582, -3.28661943,  4.12592402]), array([-2.01499328, -0.4629068 , -2.13658535,  3.52987878])]</t>
-  </si>
-  <si>
-    <t>['[0,0,0]', '[2,2,2]', '[1,1,2]', '[1,0,2]', '[0,1,1]', '[2,1,0]', '[1,2,0]', '[2,0,1]', '[0,2,1]', '[1,1,1]']</t>
-  </si>
-  <si>
-    <t>[2, 6, 8, 9, 10, 12, 13, 15, 17, 20, 22, 23, 24, 25, 27, 32, 33, 38, 41, 42, 43, 44, 46, 48, 49, 50, 51, 53, 54, 56, 57, 59, 62, 64, 65, 67, 69, 70, 71, 73, 75, 77, 78, 81, 82, 83, 85, 87, 88, 90, 91, 92, 93, 95, 96, 98, 100, 101, 102, 104, 106, 107, 108, 109, 110, 116, 117, 118, 119, 120, 122, 123, 125, 126, 127, 128, 129, 130, 133, 134, 135, 137, 139, 140, 141, 143, 145, 146, 148, 149, 150, 151, 153, 157, 158, 160, 161, 162, 163, 164, 166, 169, 171, 172, 174, 177, 178, 183, 185]</t>
-  </si>
-  <si>
-    <t>[0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 1, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 1, 0, 0, 0, 0, 0, 0, 1, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 1, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 2, 1, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 2, 1, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
-  </si>
-  <si>
-    <t>['[-0.03763371 -0.01533471  0.06554052 -0.01816017]', '[-0.00754409 -0.05458322  0.2277812  -0.36241836]', '[ 0.03557041 -0.11811661  0.19275289 -0.25552579]', '[ 0.07892797 -0.1849336   0.22986116 -0.39424827]', '[ 0.12271824 -0.267417    0.19671429 -0.40996627]', '[ 0.15338212 -0.34091394  0.10180504 -0.30861109]', '[ 0.14821295 -0.35214844 -0.15231642  0.19659226]', '[ 0.08221469 -0.23257051 -0.49175499  0.97158045]', '[-0.02529513 -0.01612529 -0.55452266  1.13820788]', '[-0.12726899  0.19907061 -0.43771727  0.96052822]', '[-0.19085358  0.34954669 -0.18201195  0.51196704]', '[-0.20899162  0.42879807  0.00597619  0.26605596]', '[-0.17535289  0.41963119  0.32304199 -0.3512468 ]', '[-0.08549768  0.29583971  0.5546057  -0.85484519]', '[ 0.04884663  0.06137721  0.75486755 -1.42952962]', '[ 0.18686057 -0.21129735  0.5883475  -1.22739984]', '[ 0.28440419 -0.4390073   0.36131112 -0.99890027]', '[ 0.31120754 -0.5621625  -0.09903694 -0.21521905]', '[ 0.23387301 -0.49136208 -0.65825757  0.90610575]', '[ 0.05888888 -0.21491983 -1.05136372  1.79292152]', '[-0.15185782  0.15318313 -0.99969778  1.78453251]', '[-0.33234369  0.49301735 -0.75912713  1.53041961]', '[-0.42870508  0.70764512 -0.1863471   0.5846591 ]', '[-0.40430192  0.7213404   0.42492809 -0.44610974]', '[-0.26505632  0.53522249  0.94009942 -1.38073336]', '[-0.04439791  0.19283021  1.21394082 -1.9557564 ]', '[ 0.20821447 -0.2358491   1.24394134 -2.20542145]', '[ 0.41361691 -0.60719159  0.76367605 -1.42890622]', '[ 0.51320345 -0.81950503  0.2135435  -0.66470488]', '[ 0.49597011 -0.86699549 -0.38198002  0.192357  ]', '[ 0.34279077 -0.68389216 -1.12407464  1.61683186]', '[ 0.06263171 -0.24049066 -1.61618244  2.71746108]', '[-0.25620006  0.30571694 -1.4836376   2.57700178]', '[-0.49992216  0.73424702 -0.90263933  1.62596482]', '[-0.61589913  0.96916748 -0.2385986   0.69917763]', '[-0.59265323  1.00948176  0.46592373 -0.29761407]', '[-0.41354822  0.79273817  1.29847873 -1.85428405]', '[-0.09019932  0.28591956  1.86806595 -3.10783036]', '[ 0.28091398 -0.34239564  1.73784293 -2.97222623]', '[ 0.58075851 -0.8680864   1.19680882 -2.1811705 ]', '[ 0.74335379 -1.19438608  0.4080599  -1.06309677]', '[ 0.73085342 -1.26366478 -0.52722666  0.37049162]', '[ 0.53872425 -1.04556889 -1.36781833  1.80547303]', '[ 0.1994839  -0.55169005 -1.96544263  3.05798278]', '[-0.21134557  0.11533907 -2.02953266  3.39348498]', '[-0.57819266  0.74758172 -1.54924993  2.7674309 ]', '[-0.79668968  1.1591321  -0.61061722  1.33014548]', '[-0.82822404  1.30649225  0.29617344  0.14024982]', '[-0.67251421  1.18651229  1.23898798 -1.34378451]', '[-0.34599305  0.77076509  1.97793999 -2.77733902]', '[ 0.08914393  0.11654859  2.26793427 -3.57309441]', '[ 0.50926866 -0.55636316  1.82349515 -2.94791783]', '[ 0.79952293 -1.04362102  1.03256715 -1.86873726]', '[ 0.9018718  -1.26974023 -0.01590716 -0.39537827]', '[ 0.79455286 -1.20122596 -1.04314793  1.08678497]', '[ 0.48390873 -0.80352294 -2.0263527   2.88114466]', '[ 0.02247623 -0.11228475 -2.47864149  3.83403545]', '[-0.45019993  0.6158183  -2.12319286  3.20687019]', '[-0.80321009  1.14418407 -1.35332727  2.02005478]', '[-0.96900234  1.39356576 -0.29087027  0.48556608]', '[-0.90834298  1.31437326  0.89262876 -1.28512347]', '[-0.61703412  0.87158983  1.9956722  -3.15252379]', '[-0.14420291  0.10827651  2.62212793 -4.27898373]', '[ 0.38090301 -0.74229163  2.47999984 -3.92614474]', '[ 0.79575154 -1.36363722  1.61907313 -2.25480383]', '[ 1.01631129 -1.650475    0.56704128 -0.63564777]', '[ 1.01818576 -1.62325249 -0.54964525  0.90793451]', '[ 0.79937799 -1.28157852 -1.62217107  2.53101101]', '[ 0.36930636 -0.57582587 -2.62799943  4.48179382]', '[-0.19002761  0.38602073 -2.78591969  4.7582798 ]', '[-0.68026242  1.19477277 -2.0315353   3.19776341]', '[-0.98621132  1.66105456 -1.00451237  1.49116795]', '[-1.08410105  1.82466251  0.03350413  0.1551685 ]', '[-0.96553462  1.69932956  1.14016696 -1.42266817]', '[-0.62729173  1.21935365  2.21823453 -3.4146305 ]', '[-0.10565025  0.36452616  2.90309936 -4.97677999]', '[ 0.47653886 -0.65754762  2.72836513 -4.8385234 ]', '[ 0.92247581 -1.44383253  1.68550775 -2.99571055]', '[ 1.14351751 -1.87095891  0.51624509 -1.31190005]', '[ 1.13563978 -1.9984791  -0.59016919  0.03705179]', '[ 0.89895483 -1.8059101  -1.74895578  1.9169721 ]', '[ 0.45918133 -1.24102021 -2.605162    3.75294263]', '[-0.11896604 -0.3213881  -3.06367313  5.23541112]', '[-0.69020907  0.68814103 -2.47434591  4.49084053]', '[-1.07939888  1.43524277 -1.37681443  2.95740475]', '[-1.22660331  1.85813229 -0.09621368  1.30106136]', '[-1.12846962  1.98088214  1.06225701 -0.0862857 ]', '[-0.80609232  1.79216565  2.11607417 -1.82772686]', '[-0.30540094  1.24058357  2.82811766 -3.68711894]', '[ 0.30691481  0.31444305  3.18278786 -5.35716457]', '[ 0.87997619 -0.70176192  2.38406715 -4.45565549]', '[ 1.22713274 -1.41439662  1.06531996 -2.68252847]', '[ 1.30485096 -1.78913721 -0.28354909 -1.07997726]', '[ 1.11880821 -1.84226645 -1.55238674  0.57747623]', '[ 0.69203648 -1.51847191 -2.6622345   2.70484129]', '[ 0.08859909 -0.77858669 -3.29260866  4.62182383]', '[-0.57143346  0.22643509 -3.12066791  5.01002749]', '[-1.10246152  1.10727361 -2.09952285  3.64847363]', '[-1.38917728  1.66167501 -0.76332616  1.94852879]', '[-1.41569298  1.92265758  0.49736292  0.65951099]', '[-1.18640785  1.89337417  1.77303303 -0.99299556]', '[-0.72156216  1.50459009  2.82398566 -2.94486493]', '[-0.08217106  0.70757664  3.48625171 -4.93899541]', '[ 0.6247437  -0.37872801  3.37275378 -5.44206176]', '[ 1.18363891 -1.28361369  2.15237156 -3.52872271]', '[ 1.48941332 -1.83812262  0.89834328 -2.07179779]', '[ 1.53457268 -2.1033193  -0.44294969 -0.58741   ]', '[ 1.31539087 -2.064986   -1.73274849  1.01219385]', '[ 0.85348889 -1.67549718 -2.8414826   2.94775743]', '[ 0.20117052 -0.86531411 -3.61404763  5.12546745]', '[-0.53833706  0.27001876 -3.56183095  5.71784281]', '[-1.15235978  1.26520838 -2.48427966  4.07761945]', '[-1.52271407  1.91686424 -1.21414943  2.51215865]', '[-1.63746819  2.28995284  0.06551692  1.23594344]', '[-1.49164993  2.38700421  1.38281462 -0.29226948]', '[-1.08565153  2.13503133  2.63960314 -2.28777554]', '[-0.46593029  1.46595284  3.49541208 -4.46127708]', '[ 0.28577506  0.35670385  3.89662263 -6.37364309]', '[ 0.99613119 -0.85101504  3.00221441 -5.2370402 ]', '[ 1.45522911 -1.69087393  1.58429055 -3.23680725]', '[ 1.6323352  -2.17856736  0.19302248 -1.68268478]', '[ 1.53523579 -2.3661032  -1.15460015 -0.17183773]', '[ 1.17698973 -2.23212185 -2.39631066  1.56187669]', '[ 0.59863979 -1.71841014 -3.3159693   3.63056335]', '[-0.12972483 -0.74214067 -3.89678255  6.05932558]', '[-0.87989822  0.51346893 -3.36758947  5.9247417 ]', '[-1.41272601  1.49152236 -1.92928141  3.85817965]', '[-1.65422043  2.09407103 -0.49441964  2.23200404]', '[-1.6138305   2.39273385  0.88880787  0.74272192]', '[-1.30389059  2.37829671  2.18698508 -0.93138071]', '[-0.75724622  1.99967068  3.20762196 -2.9088975 ]', '[-0.04759055  1.17314247  3.82015197 -5.36912987]', '[ 0.73518584 -0.08565728  3.81153373 -6.72924377]', '[ 1.36717645 -1.25357439  2.40438499 -4.75542167]', '[ 1.69588139 -2.01861364  0.89706645 -2.99151434]', '[ 1.73127351 -2.46929632 -0.5297273  -1.51954258]', '[ 1.48919557 -2.61762009 -1.8761064   0.07025452]', '[ 0.99149133 -2.42594981 -3.04645899  1.88758877]', '[ 0.30109775 -1.82533374 -3.74950315  4.15577184]', '[-0.46286453 -0.78998171 -3.81335794  6.06871972]', '[-1.16523338  0.44668779 -3.01358129  5.80686989]', '[-1.61477934  1.42110479 -1.45502536  3.94325474]', '[-1.75653312  2.07563486  0.03840951  2.62561807]', '[-1.59548581  2.4447074   1.55272468  1.03027168]', '[-1.14091663  2.44928418  2.94235121 -1.03082619]', '[-0.4588514   2.03682491  3.75954149 -3.11946848]', '[ 0.31076829  1.20626005  3.83819254 -5.11014128]', '[ 1.05191451  0.0442338   3.43731743 -6.12878598]', '[ 1.60439946 -1.03949294  2.00350946 -4.54375131]', '[ 1.84874532 -1.78925201  0.44409207 -3.01510367]', '[ 1.78306513 -2.25148122 -1.09512654 -1.57729665]', '[ 1.41585783 -2.39756683 -2.55081181  0.18373515]', '[ 0.77764239 -2.13055932 -3.73766966  2.55055513]', '[-0.02183329 -1.38388401 -4.14329617  4.89717303]', '[-0.8516935  -0.19875904 -4.01851719  6.57814172]', '[-1.54464643  1.01998844 -2.77750124  5.29544943]', '[-1.95351367  1.92317357 -1.32631928  3.84083624]', '[-2.07535285  2.56225599  0.08167254  2.57292078]', '[-1.93069515  2.94586687  1.34871583  1.23148188]', '[-1.53664101  3.04177768  2.59514799 -0.29699782]', '[-0.89762948  2.82113457  3.73773229 -1.91990291]', '[-0.09061471  2.27084396  4.16358855 -3.57821809]', '[ 0.7023989   1.40931102  3.67014494 -4.93288456]', '[ 1.35727469  0.3660317   2.82283136 -5.26666151]', '[ 1.79951359 -0.59879203  1.53946655 -4.24646014]', '[ 1.97052401 -1.35168988  0.13506566 -3.26807794]', '[ 1.83062532 -1.86501638 -1.55475677 -1.78956328]', '[ 1.34285668 -2.00145258 -3.27947548  0.54954736]', '[ 0.55420673 -1.59798996 -4.48369121  3.57145877]', '[-0.3879026  -0.60290253 -4.79727205  6.13467465]', '[-1.29018086  0.64871862 -4.01241504  5.78349104]', '[-1.94743493  1.59058183 -2.59524805  3.76036047]', '[-2.34859065  2.2195383  -1.46165377  2.65212252]', '[-2.5536446   2.6991791  -0.62289448  2.16965365]', '[-2.60385597  3.06692685  0.095649    1.49125541]', '[-2.51951578 -2.99916088  0.75291793  0.64575935]', '[-2.29385768 -2.97303871  1.54029004 -0.42314526]', '[-1.88507924  3.09863909  2.59277433 -1.73912884]', '[-1.24684041  2.58882746  3.76770405 -3.45870386]', '[-0.40099178  1.6393589   4.62108129 -6.2038807 ]', '[ 0.58676319  0.07925637  5.06987662 -8.88122717]', '[ 1.47351132 -1.50562368  3.60955162 -6.52247823]', '[ 2.04830756 -2.60723377  2.20675973 -4.71477256]', '[ 2.37994682  2.86097044  1.19713049 -3.49196463]', '[ 2.56089842  2.25345126  0.65920213 -2.58467567]', '[ 2.64341484  1.85229979  0.16416773 -1.41159134]']</t>
-  </si>
-  <si>
-    <t>[0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50, 51, 52, 53, 54, 55, 56, 57, 58, 59, 60, 61, 62, 63, 64, 65, 66, 67, 68, 69, 70, 71, 72, 73, 74, 75, 76, 77, 78, 79, 80, 81, 82, 83, 84, 85, 86, 87, 88, 89, 90, 91, 92, 93, 94, 95, 96, 97, 98, 99, 100, 101, 102, 103, 104, 105, 106, 107, 108, 109, 110, 111, 112, 113, 114, 115, 116, 117, 118, 119, 120, 121, 122, 123, 124, 125, 126, 127, 128, 129, 130, 131, 132, 133, 134, 135, 136, 137, 138, 139, 140, 141, 142, 143, 144, 145, 146, 147, 148, 149, 150, 151, 152, 153, 154, 155, 156, 157, 158, 159, 160, 161, 162, 163, 164, 165, 166, 167, 168, 169, 170, 171, 172, 173, 174, 175, 176, 177, 178, 179, 180, 181, 182, 183, 184, 185]</t>
-  </si>
-  <si>
-    <t>[array([-0.03763371, -0.01533471,  0.06554052, -0.01816017], dtype=float32), array([-0.00754409, -0.05458322,  0.2277812 , -0.36241836]), array([ 0.03557041, -0.11811661,  0.19275289, -0.25552579]), array([ 0.07892797, -0.1849336 ,  0.22986116, -0.39424827]), array([ 0.12271824, -0.267417  ,  0.19671429, -0.40996627]), array([ 0.15338212, -0.34091394,  0.10180504, -0.30861109]), array([ 0.14821295, -0.35214844, -0.15231642,  0.19659226]), array([ 0.08221469, -0.23257051, -0.49175499,  0.97158045]), array([-0.02529513, -0.01612529, -0.55452266,  1.13820788]), array([-0.12726899,  0.19907061, -0.43771727,  0.96052822]), array([-0.19085358,  0.34954669, -0.18201195,  0.51196704]), array([-0.20899162,  0.42879807,  0.00597619,  0.26605596]), array([-0.17535289,  0.41963119,  0.32304199, -0.3512468 ]), array([-0.08549768,  0.29583971,  0.5546057 , -0.85484519]), array([ 0.04884663,  0.06137721,  0.75486755, -1.42952962]), array([ 0.18686057, -0.21129735,  0.5883475 , -1.22739984]), array([ 0.28440419, -0.4390073 ,  0.36131112, -0.99890027]), array([ 0.31120754, -0.5621625 , -0.09903694, -0.21521905]), array([ 0.23387301, -0.49136208, -0.65825757,  0.90610575]), array([ 0.05888888, -0.21491983, -1.05136372,  1.79292152]), array([-0.15185782,  0.15318313, -0.99969778,  1.78453251]), array([-0.33234369,  0.49301735, -0.75912713,  1.53041961]), array([-0.42870508,  0.70764512, -0.1863471 ,  0.5846591 ]), array([-0.40430192,  0.7213404 ,  0.42492809, -0.44610974]), array([-0.26505632,  0.53522249,  0.94009942, -1.38073336]), array([-0.04439791,  0.19283021,  1.21394082, -1.9557564 ]), array([ 0.20821447, -0.2358491 ,  1.24394134, -2.20542145]), array([ 0.41361691, -0.60719159,  0.76367605, -1.42890622]), array([ 0.51320345, -0.81950503,  0.2135435 , -0.66470488]), array([ 0.49597011, -0.86699549, -0.38198002,  0.192357  ]), array([ 0.34279077, -0.68389216, -1.12407464,  1.61683186]), array([ 0.06263171, -0.24049066, -1.61618244,  2.71746108]), array([-0.25620006,  0.30571694, -1.4836376 ,  2.57700178]), array([-0.49992216,  0.73424702, -0.90263933,  1.62596482]), array([-0.61589913,  0.96916748, -0.2385986 ,  0.69917763]), array([-0.59265323,  1.00948176,  0.46592373, -0.29761407]), array([-0.41354822,  0.79273817,  1.29847873, -1.85428405]), array([-0.09019932,  0.28591956,  1.86806595, -3.10783036]), array([ 0.28091398, -0.34239564,  1.73784293, -2.97222623]), array([ 0.58075851, -0.8680864 ,  1.19680882, -2.1811705 ]), array([ 0.74335379, -1.19438608,  0.4080599 , -1.06309677]), array([ 0.73085342, -1.26366478, -0.52722666,  0.37049162]), array([ 0.53872425, -1.04556889, -1.36781833,  1.80547303]), array([ 0.1994839 , -0.55169005, -1.96544263,  3.05798278]), array([-0.21134557,  0.11533907, -2.02953266,  3.39348498]), array([-0.57819266,  0.74758172, -1.54924993,  2.7674309 ]), array([-0.79668968,  1.1591321 , -0.61061722,  1.33014548]), array([-0.82822404,  1.30649225,  0.29617344,  0.14024982]), array([-0.67251421,  1.18651229,  1.23898798, -1.34378451]), array([-0.34599305,  0.77076509,  1.97793999, -2.77733902]), array([ 0.08914393,  0.11654859,  2.26793427, -3.57309441]), array([ 0.50926866, -0.55636316,  1.82349515, -2.94791783]), array([ 0.79952293, -1.04362102,  1.03256715, -1.86873726]), array([ 0.9018718 , -1.26974023, -0.01590716, -0.39537827]), array([ 0.79455286, -1.20122596, -1.04314793,  1.08678497]), array([ 0.48390873, -0.80352294, -2.0263527 ,  2.88114466]), array([ 0.02247623, -0.11228475, -2.47864149,  3.83403545]), array([-0.45019993,  0.6158183 , -2.12319286,  3.20687019]), array([-0.80321009,  1.14418407, -1.35332727,  2.02005478]), array([-0.96900234,  1.39356576, -0.29087027,  0.48556608]), array([-0.90834298,  1.31437326,  0.89262876, -1.28512347]), array([-0.61703412,  0.87158983,  1.9956722 , -3.15252379]), array([-0.14420291,  0.10827651,  2.62212793, -4.27898373]), array([ 0.38090301, -0.74229163,  2.47999984, -3.92614474]), array([ 0.79575154, -1.36363722,  1.61907313, -2.25480383]), array([ 1.01631129, -1.650475  ,  0.56704128, -0.63564777]), array([ 1.01818576, -1.62325249, -0.54964525,  0.90793451]), array([ 0.79937799, -1.28157852, -1.62217107,  2.53101101]), array([ 0.36930636, -0.57582587, -2.62799943,  4.48179382]), array([-0.19002761,  0.38602073, -2.78591969,  4.7582798 ]), array([-0.68026242,  1.19477277, -2.0315353 ,  3.19776341]), array([-0.98621132,  1.66105456, -1.00451237,  1.49116795]), array([-1.08410105,  1.82466251,  0.03350413,  0.1551685 ]), array([-0.96553462,  1.69932956,  1.14016696, -1.42266817]), array([-0.62729173,  1.21935365,  2.21823453, -3.4146305 ]), array([-0.10565025,  0.36452616,  2.90309936, -4.97677999]), array([ 0.47653886, -0.65754762,  2.72836513, -4.8385234 ]), array([ 0.92247581, -1.44383253,  1.68550775, -2.99571055]), array([ 1.14351751, -1.87095891,  0.51624509, -1.31190005]), array([ 1.13563978, -1.9984791 , -0.59016919,  0.03705179]), array([ 0.89895483, -1.8059101 , -1.74895578,  1.9169721 ]), array([ 0.45918133, -1.24102021, -2.605162  ,  3.75294263]), array([-0.11896604, -0.3213881 , -3.06367313,  5.23541112]), array([-0.69020907,  0.68814103, -2.47434591,  4.49084053]), array([-1.07939888,  1.43524277, -1.37681443,  2.95740475]), array([-1.22660331,  1.85813229, -0.09621368,  1.30106136]), array([-1.12846962,  1.98088214,  1.06225701, -0.0862857 ]), array([-0.80609232,  1.79216565,  2.11607417, -1.82772686]), array([-0.30540094,  1.24058357,  2.82811766, -3.68711894]), array([ 0.30691481,  0.31444305,  3.18278786, -5.35716457]), array([ 0.87997619, -0.70176192,  2.38406715, -4.45565549]), array([ 1.22713274, -1.41439662,  1.06531996, -2.68252847]), array([ 1.30485096, -1.78913721, -0.28354909, -1.07997726]), array([ 1.11880821, -1.84226645, -1.55238674,  0.57747623]), array([ 0.69203648, -1.51847191, -2.6622345 ,  2.70484129]), array([ 0.08859909, -0.77858669, -3.29260866,  4.62182383]), array([-0.57143346,  0.22643509, -3.12066791,  5.01002749]), array([-1.10246152,  1.10727361, -2.09952285,  3.64847363]), array([-1.38917728,  1.66167501, -0.76332616,  1.94852879]), array([-1.41569298,  1.92265758,  0.49736292,  0.65951099]), array([-1.18640785,  1.89337417,  1.77303303, -0.99299556]), array([-0.72156216,  1.50459009,  2.82398566, -2.94486493]), array([-0.08217106,  0.70757664,  3.48625171, -4.93899541]), array([ 0.6247437 , -0.37872801,  3.37275378, -5.44206176]), array([ 1.18363891, -1.28361369,  2.15237156, -3.52872271]), array([ 1.48941332, -1.83812262,  0.89834328, -2.07179779]), array([ 1.53457268, -2.1033193 , -0.44294969, -0.58741   ]), array([ 1.31539087, -2.064986  , -1.73274849,  1.01219385]), array([ 0.85348889, -1.67549718, -2.8414826 ,  2.94775743]), array([ 0.20117052, -0.86531411, -3.61404763,  5.12546745]), array([-0.53833706,  0.27001876, -3.56183095,  5.71784281]), array([-1.15235978,  1.26520838, -2.48427966,  4.07761945]), array([-1.52271407,  1.91686424, -1.21414943,  2.51215865]), array([-1.63746819,  2.28995284,  0.06551692,  1.23594344]), array([-1.49164993,  2.38700421,  1.38281462, -0.29226948]), array([-1.08565153,  2.13503133,  2.63960314, -2.28777554]), array([-0.46593029,  1.46595284,  3.49541208, -4.46127708]), array([ 0.28577506,  0.35670385,  3.89662263, -6.37364309]), array([ 0.99613119, -0.85101504,  3.00221441, -5.2370402 ]), array([ 1.45522911, -1.69087393,  1.58429055, -3.23680725]), array([ 1.6323352 , -2.17856736,  0.19302248, -1.68268478]), array([ 1.53523579, -2.3661032 , -1.15460015, -0.17183773]), array([ 1.17698973, -2.23212185, -2.39631066,  1.56187669]), array([ 0.59863979, -1.71841014, -3.3159693 ,  3.63056335]), array([-0.12972483, -0.74214067, -3.89678255,  6.05932558]), array([-0.87989822,  0.51346893, -3.36758947,  5.9247417 ]), array([-1.41272601,  1.49152236, -1.92928141,  3.85817965]), array([-1.65422043,  2.09407103, -0.49441964,  2.23200404]), array([-1.6138305 ,  2.39273385,  0.88880787,  0.74272192]), array([-1.30389059,  2.37829671,  2.18698508, -0.93138071]), array([-0.75724622,  1.99967068,  3.20762196, -2.9088975 ]), array([-0.04759055,  1.17314247,  3.82015197, -5.36912987]), array([ 0.73518584, -0.08565728,  3.81153373, -6.72924377]), array([ 1.36717645, -1.25357439,  2.40438499, -4.75542167]), array([ 1.69588139, -2.01861364,  0.89706645, -2.99151434]), array([ 1.73127351, -2.46929632, -0.5297273 , -1.51954258]), array([ 1.48919557, -2.61762009, -1.8761064 ,  0.07025452]), array([ 0.99149133, -2.42594981, -3.04645899,  1.88758877]), array([ 0.30109775, -1.82533374, -3.74950315,  4.15577184]), array([-0.46286453, -0.78998171, -3.81335794,  6.06871972]), array([-1.16523338,  0.44668779, -3.01358129,  5.80686989]), array([-1.61477934,  1.42110479, -1.45502536,  3.94325474]), array([-1.75653312,  2.07563486,  0.03840951,  2.62561807]), array([-1.59548581,  2.4447074 ,  1.55272468,  1.03027168]), array([-1.14091663,  2.44928418,  2.94235121, -1.03082619]), array([-0.4588514 ,  2.03682491,  3.75954149, -3.11946848]), array([ 0.31076829,  1.20626005,  3.83819254, -5.11014128]), array([ 1.05191451,  0.0442338 ,  3.43731743, -6.12878598]), array([ 1.60439946, -1.03949294,  2.00350946, -4.54375131]), array([ 1.84874532, -1.78925201,  0.44409207, -3.01510367]), array([ 1.78306513, -2.25148122, -1.09512654, -1.57729665]), array([ 1.41585783, -2.39756683, -2.55081181,  0.18373515]), array([ 0.77764239, -2.13055932, -3.73766966,  2.55055513]), array([-0.02183329, -1.38388401, -4.14329617,  4.89717303]), array([-0.8516935 , -0.19875904, -4.01851719,  6.57814172]), array([-1.54464643,  1.01998844, -2.77750124,  5.29544943]), array([-1.95351367,  1.92317357, -1.32631928,  3.84083624]), array([-2.07535285,  2.56225599,  0.08167254,  2.57292078]), array([-1.93069515,  2.94586687,  1.34871583,  1.23148188]), array([-1.53664101,  3.04177768,  2.59514799, -0.29699782]), array([-0.89762948,  2.82113457,  3.73773229, -1.91990291]), array([-0.09061471,  2.27084396,  4.16358855, -3.57821809]), array([ 0.7023989 ,  1.40931102,  3.67014494, -4.93288456]), array([ 1.35727469,  0.3660317 ,  2.82283136, -5.26666151]), array([ 1.79951359, -0.59879203,  1.53946655, -4.24646014]), array([ 1.97052401, -1.35168988,  0.13506566, -3.26807794]), array([ 1.83062532, -1.86501638, -1.55475677, -1.78956328]), array([ 1.34285668, -2.00145258, -3.27947548,  0.54954736]), array([ 0.55420673, -1.59798996, -4.48369121,  3.57145877]), array([-0.3879026 , -0.60290253, -4.79727205,  6.13467465]), array([-1.29018086,  0.64871862, -4.01241504,  5.78349104]), array([-1.94743493,  1.59058183, -2.59524805,  3.76036047]), array([-2.34859065,  2.2195383 , -1.46165377,  2.65212252]), array([-2.5536446 ,  2.6991791 , -0.62289448,  2.16965365]), array([-2.60385597,  3.06692685,  0.095649  ,  1.49125541]), array([-2.51951578, -2.99916088,  0.75291793,  0.64575935]), array([-2.29385768, -2.97303871,  1.54029004, -0.42314526]), array([-1.88507924,  3.09863909,  2.59277433, -1.73912884]), array([-1.24684041,  2.58882746,  3.76770405, -3.45870386]), array([-0.40099178,  1.6393589 ,  4.62108129, -6.2038807 ]), array([ 0.58676319,  0.07925637,  5.06987662, -8.88122717]), array([ 1.47351132, -1.50562368,  3.60955162, -6.52247823]), array([ 2.04830756, -2.60723377,  2.20675973, -4.71477256]), array([ 2.37994682,  2.86097044,  1.19713049, -3.49196463]), array([ 2.56089842,  2.25345126,  0.65920213, -2.58467567]), array([ 2.64341484,  1.85229979,  0.16416773, -1.41159134])]</t>
-  </si>
-  <si>
-    <t>['[2,0,1]', '[0,0,0]', '[1,1,2]', '[2,2,2]', '[2,1,0]', '[1,0,2]', '[1,2,0]', '[1,1,1]', '[0,2,1]', '[0,1,1]']</t>
-  </si>
-  <si>
-    <t>[3, 4, 6, 7, 8, 10, 11, 12, 13, 14, 16, 17, 18, 19, 21, 24, 25, 28, 29, 30, 31, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 45, 46, 47, 48, 50, 51, 52, 53, 55, 56, 57, 59, 60, 61, 63, 64, 65, 67, 68, 69, 70, 72, 73, 74, 75, 76, 78, 79, 80, 81, 82, 83, 84, 85, 86, 87, 88, 89, 90, 91, 92, 94, 95, 96, 98, 100, 101, 102, 104, 105, 106, 107, 110, 111, 112, 114, 115, 118, 120, 122, 123, 124, 125, 127, 128, 130, 131, 132, 133, 134, 135, 136, 137, 138, 139, 140, 141, 142, 143, 144, 145, 146, 147, 148, 149, 151, 152, 155, 156, 157, 158, 159, 160, 161, 163, 164, 165, 166, 167, 168, 171, 172, 173, 174, 175, 176, 177, 178, 179, 180, 182, 183, 184, 185, 186, 187, 188, 189, 190, 191, 192, 193, 194, 195, 197, 198, 199]</t>
-  </si>
-  <si>
-    <t>[0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 1, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 1, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 1, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2]</t>
-  </si>
-  <si>
-    <t>['[-0.03763371 -0.01533471  0.06554052 -0.01816017]', '[-0.00754409 -0.05458322  0.2277812  -0.36241836]', '[ 0.04879627 -0.15231473  0.32089719 -0.5887683 ]', '[ 0.10086936 -0.24375386  0.18698275 -0.30308016]', '[ 0.11983618 -0.2672456  -0.00147766  0.07421381]', '[ 0.08727937 -0.18099074 -0.31523237  0.76959249]', '[ 0.01377476 -0.00755673 -0.39926544  0.92308231]', '[-0.06332583  0.16991757 -0.3504693   0.80890919]', '[-0.11863032  0.30044118 -0.18819839  0.46736327]', '[-0.14748655  0.38214929 -0.09249565  0.33253653]', '[-0.14064839  0.39486094  0.15932722 -0.20562584]', '[-0.08662995  0.30404858  0.36786268 -0.68072663]', '[-8.36476301e-04  1.35619965e-01  4.67863947e-01 -9.62299048e-01]', '[ 0.09032776 -0.0613969   0.41883828 -0.95896232]', '[ 0.15719516 -0.22895123  0.23150444 -0.67845637]', '[ 0.19053744 -0.35459732  0.09164922 -0.55248732]', '[ 0.1783495  -0.40837838 -0.21152168  0.01995257]', '[ 0.10942552 -0.3491727  -0.46230395  0.55315194]', '[ 0.00198179 -0.19940588 -0.58638802  0.90378328]', '[-0.11331    -0.00754223 -0.53714897  0.96326472]', '[-0.21466029  0.19938781 -0.44908944  1.05403268]', '[-0.2698423   0.36016096 -0.08830874  0.52180033]', '[-0.26038572  0.43405387  0.18265135  0.20717855]', '[-0.17386504  0.3759499   0.66385251 -0.76866797]', '[-0.01965317  0.17645978  0.84173773 -1.17008274]', '[ 0.14601119 -0.06466863  0.77346106 -1.17167545]', '[ 0.28703307 -0.29937727  0.6012993  -1.11377118]', '[ 0.37423022 -0.48839475  0.24955074 -0.73715299]', '[ 0.36931487 -0.55085649 -0.2976248   0.11869429]', '[ 0.25983437 -0.44433073 -0.77436775  0.92026427]', '[ 0.07309068 -0.20109143 -1.04962145  1.44591908]', '[-0.13910758  0.09986101 -1.01899768  1.4737952 ]', '[-0.32678321  0.38724895 -0.81176774  1.32284908]', '[-0.43574492  0.57087451 -0.25584435  0.47996337]', '[-0.42498805  0.57291757  0.36087678 -0.45807537]', '[-0.2969557   0.39425953  0.89268672 -1.2915443 ]', '[-0.08401689  0.08093618  1.18484483 -1.75587014]', '[ 0.15240689 -0.26572651  1.11943188 -1.60789845]', '[ 0.34166144 -0.52586138  0.73149122 -0.93110733]', '[ 0.43275313 -0.62207851  0.16234723 -0.01294353]', '[ 0.40400586 -0.52970337 -0.44371819  0.92335609]', '[ 0.26262501 -0.26522335 -0.93750349  1.66587695]', '[ 0.0478942   0.10321503 -1.15309663  1.91566998]', '[-0.18669684  0.48947688 -1.13232135  1.83921317]', '[-0.38312779  0.80209222 -0.79096554  1.22518994]', '[-0.47965066  0.9340208  -0.15893337  0.08041107]', '[-0.44423174  0.83298951  0.50855451 -1.08276974]', '[-0.28248125  0.50968469  1.07826064 -2.1021775 ]', '[-0.03284734  0.0269676   1.35052978 -2.59777087]', '[ 0.23871201 -0.50110023  1.28743904 -2.53349114]', '[ 0.44397054 -0.9073441   0.7276502  -1.47029346]', '[ 0.52111353 -1.07835619  0.03519652 -0.23062978]', '[ 0.45822626 -0.99901343 -0.65418486  1.01801016]', '[ 0.26715765 -0.6777129  -1.22473369  2.15589549]', '[-0.02476253 -0.13428206 -1.62329625  3.14816953]', '[-0.33028394  0.47153938 -1.34292771  2.73619358]', '[-0.53505042  0.91117344 -0.66766822  1.60064291]', '[-0.59013438  1.1019537   0.12001172  0.30009072]', '[-0.47940555  1.00237134  0.96969858 -1.29094252]', '[-0.22484057  0.62287882  1.53176382 -2.45037752]', '[ 0.10712663  0.06415621  1.70217951 -2.97854407]', '[ 0.41663918 -0.49260151  1.31057484 -2.43445794]', '[ 0.61912005 -0.89964809  0.67527214 -1.57578123]', '[ 0.66740043 -1.08204258 -0.1948543  -0.24175448]', '[ 0.54471828 -0.995811   -1.01186947  1.09877039]', '[ 0.27535871 -0.64976803 -1.63546443  2.31348907]', '[-0.09555806 -0.07624407 -1.98372585  3.26115687]', '[-0.46007364  0.53411055 -1.56616812  2.66443888]', '[-0.69499612  0.94543663 -0.74620846  1.40364475]', '[-0.75110703  1.08975868  0.18945251  0.03629517]', '[-0.62180274  0.95936269  1.08542443 -1.33674855]', '[-0.31765358  0.53071836  1.9077405  -2.89806223]', '[ 0.09562921 -0.11303291  2.1136647  -3.3286781 ]', '[ 0.48006406 -0.70891018  1.64080016 -2.47312075]', '[ 0.72788213 -1.0697693   0.80306012 -1.10912649]', '[ 0.79338536 -1.15075795 -0.15535795  0.29817462]', '[ 0.66680969 -0.95041192 -1.09598468  1.70199045]', '[ 0.35446804 -0.44592993 -1.97735733  3.28017124]', '[-0.07412644  0.26243756 -2.18567951  3.56246549]', '[-0.47079871  0.88399392 -1.69620153  2.51122336]', '[-0.73070139  1.24224894 -0.86972081  1.05684533]', '[-0.81012293  1.30729069  0.08581913 -0.40322667]', '[-0.69594839  1.08061328  1.04608698 -1.86477814]', '[-0.40088812  0.56539792  1.85904305 -3.23304945]', '[ 0.01438388 -0.1555825   2.17487059 -3.74464852]', '[ 0.4169994  -0.82895064  1.75625616 -2.81756694]', '[ 0.69254813 -1.24997985  0.96414214 -1.37059693]', '[ 0.79373512 -1.37702687  0.03638804  0.09653079]', '[ 0.70610503 -1.21132804 -0.90514488  1.56324566]', '[ 0.43892752 -0.75207747 -1.73212752  3.00108813]', '[ 0.03895455 -0.04909952 -2.16337014  3.83287553]', '[-0.37283472  0.6736648  -1.84200033  3.17761018]', '[-0.66738541  1.17239493 -1.06260161  1.76855596]', '[-0.79818398  1.40520104 -0.23129035  0.55755465]', '[-0.7490168   1.36945517  0.71566394 -0.91666642]', '[-0.51849037  1.03668053  1.56269059 -2.40695678]', '[-0.14112742  0.42083204  2.13948484 -3.64214388]', '[ 0.30490836 -0.36734742  2.18420787 -3.96349744]', '[ 0.67056862 -1.03604619  1.4051347  -2.61937821]', '[ 0.86346668 -1.43233945  0.5047663  -1.3390832 ]', '[ 0.86088099 -1.54758258 -0.52370097  0.18443557]', '[ 0.66063883 -1.35622332 -1.45239339  1.73727254]', '[ 0.29441663 -0.85239623 -2.16070221  3.26769907]', '[-0.18546875 -0.06093597 -2.51929236  4.4171197 ]', '[-0.63739354  0.75081408 -1.88018178  3.46813454]', '[-0.91101899  1.28746277 -0.82934961  1.88665659]', '[-0.96538136  1.50974414  0.28363293  0.34241302]', '[-0.80238424  1.42257082  1.32361567 -1.22619023]', '[-0.4394083   0.98650039  2.26497828 -3.13736184]', '[ 0.07841141  0.19166691  2.80192903 -4.60870869]', '[ 0.60106747 -0.6827162   2.27855365 -3.83945909]', '[ 0.9548963  -1.28771725  1.22295913 -2.19186104]', '[ 1.08382614 -1.56721074  0.06134172 -0.61968997]', '[ 0.9722108  -1.51157935 -1.16405619  1.19097072]', '[ 0.63641655 -1.10575806 -2.15999083  2.88390252]', '[ 0.12950397 -0.36926405 -2.81569044  4.33499949]', '[-0.44114387  0.53720371 -2.71966211  4.37124382]', '[-0.90481508  1.27698408 -1.85025765  2.94736163]', '[-1.15917393  1.6947539  -0.68025621  1.2667055 ]', '[-1.18262953  1.81618877  0.44525262 -0.05029577]', '[-0.97706771  1.6458455   1.58976834 -1.68077334]', '[-0.54963359  1.10292487  2.64987597 -3.78427365]', '[ 0.04707512  0.1804272   3.1859443  -5.18915119]', '[ 0.64401478 -0.79698956  2.6172572  -4.23945207]', '[ 1.05897164 -1.46195847  1.49974438 -2.41889385]', '[ 1.23787344 -1.78123421  0.28230273 -0.80472547]', '[ 1.17182756 -1.78796253 -0.93486849  0.74789849]', '[ 0.87074069 -1.47064475 -2.04950719  2.4644616 ]', '[ 0.36681742 -0.78892913 -2.93401528  4.32664686]', '[-0.27127815  0.21765555 -3.26162865  5.34040295]', '[-0.84444235  1.13922102 -2.36245353  3.68752642]', '[-1.20005327  1.69146167 -1.176521    1.88397884]', '[-1.31118427  1.90989476  0.06843652  0.32096409]', '[-1.17409636  1.81896164  1.29077003 -1.25319375]', '[-0.8032956   1.39240232  2.38745254 -3.06004816]', '[-0.2358418   0.58473625  3.21255926 -4.93285746]', '[ 0.41900873 -0.45352543  3.13081735 -4.99838588]', '[ 0.95096294 -1.27980724  2.11808005 -3.17815471]', '[ 1.25525085 -1.73761119  0.91101543 -1.44942956]', '[ 1.31242624 -1.87317625 -0.3401057   0.08323326]', '[ 1.1216402  -1.69938637 -1.55348815  1.68722578]', '[ 0.70037653 -1.17921505 -2.62663841  3.55718767]', '[ 0.09282487 -0.2838942  -3.334324    5.19499912]', '[-0.55343227  0.72487322 -2.94007667  4.48841967]', '[-1.03877599  1.43441406 -1.86935461  2.59925516]', '[-1.29249087  1.78380179 -0.65518047  0.93890626]', '[-1.29841974  1.81978285  0.59520832 -0.57809494]', '[-1.05745031  1.54380264  1.79919071 -2.22298622]', '[-0.5883554   0.91048938  2.8533684  -4.1287769 ]', '[ 0.05006384 -0.06249155  3.36372158 -5.25390938]', '[ 0.6838885  -1.03388399  2.82300395 -4.15766686]', '[ 1.14014763 -1.66727595  1.71060493 -2.22034595]', '[ 1.36055834 -1.94497706  0.48194908 -0.59723936]', '[ 1.33098856 -1.91340094 -0.77595264  0.91852287]', '[ 1.04534497 -1.54203909 -2.06858333  2.85463293]', '[ 0.52065037 -0.77073621 -3.13550857  4.85962449]', '[-0.16162166  0.31749875 -3.47643055  5.55650013]', '[-0.78534565  1.2649654  -2.65449002  3.73933737]', '[-1.20605536  1.81741583 -1.52719026  1.84433129]', '[-1.38889122  2.02412775 -0.29073285  0.25587108]', '[-1.32093955  1.92404802  0.9673263  -1.269155  ]', '[-1.00574859  1.50197594  2.16863764 -3.00792047]', '[-0.45246936  0.66872151  3.32118695 -5.32022558]', '[ 0.2528086  -0.48023903  3.49891264 -5.64445536]', '[ 0.86880279 -1.41885565  2.58010298 -3.63457607]', '[ 1.27171359 -1.95191223  1.42687614 -1.76306824]', '[ 1.43319177 -2.1448226   0.17962913 -0.1947835 ]', '[ 1.34283716 -2.03237831 -1.07886156  1.33522281]', '[ 1.00614296 -1.59500079 -2.27001677  3.0991404 ]', '[ 0.43444221 -0.73793481 -3.40876317  5.48455505]', '[-0.30193234  0.490125   -3.70314179  6.21884138]', '[-0.94729826  1.52387485 -2.67639343  4.02682055]', '[-1.36400465  2.1308586  -1.47559006  2.12676349]', '[-1.53316667  2.39745198 -0.21133364  0.56807001]', '[-1.44859954  2.36062687  1.05241429 -0.94912456]', '[-1.11695243  2.00500385  2.24133301 -2.66048383]', '[-0.5650957   1.26732087  3.24285702 -4.78552973]', '[ 0.15615319  0.10487189  3.80359843 -6.48371613]', '[ 0.84815686 -1.07501797  2.93443181 -4.92661052]', '[ 1.30783342 -1.84858056  1.65348457 -2.89128687]', '[ 1.50816324 -2.26174401  0.34895481 -1.28258984]', '[ 1.44850198 -2.3666452  -0.93864802  0.24328577]', '[ 1.13839851 -2.15367696 -2.13527499  1.9286859 ]', '[ 0.61178986 -1.57295591 -3.07925212  3.93759853]', '[-0.0712349  -0.5689953  -3.66328115  5.96922463]', '[-0.77358385  0.63225999 -3.13032059  5.51635925]', '[-1.26854059  1.53048343 -1.78953489  3.47890043]', '[-1.4890481   2.0547358  -0.41858968  1.81679497]', '[-1.43818194  2.26446535  0.91737356  0.27104629]', '[-1.12920387  2.15186445  2.14074172 -1.4379212 ]', '[-0.60235218  1.66998032  3.06313171 -3.42721787]', '[ 0.06843113  0.77375592  3.56695575 -5.45010457]', '[ 0.76376124 -0.37657561  3.17386149 -5.55614847]', '[ 1.27067548 -1.304736    1.84058119 -3.66515153]', '[ 1.497515   -1.86642727  0.43070062 -2.00502719]', '[ 1.44508196 -2.11419877 -0.94509551 -0.45987194]', '[ 1.12028716 -2.01460471 -2.2675186   1.50712173]', '[ 0.56690197 -1.51041162 -3.20158091  3.5819442 ]', '[-0.13145806 -0.58238985 -3.68371007  5.54697141]', '[-0.83247902  0.53864416 -3.11799754  5.17923505]']</t>
-  </si>
-  <si>
-    <t>[array([-0.03763371, -0.01533471,  0.06554052, -0.01816017], dtype=float32), array([-0.00754409, -0.05458322,  0.2277812 , -0.36241836]), array([ 0.04879627, -0.15231473,  0.32089719, -0.5887683 ]), array([ 0.10086936, -0.24375386,  0.18698275, -0.30308016]), array([ 0.11983618, -0.2672456 , -0.00147766,  0.07421381]), array([ 0.08727937, -0.18099074, -0.31523237,  0.76959249]), array([ 0.01377476, -0.00755673, -0.39926544,  0.92308231]), array([-0.06332583,  0.16991757, -0.3504693 ,  0.80890919]), array([-0.11863032,  0.30044118, -0.18819839,  0.46736327]), array([-0.14748655,  0.38214929, -0.09249565,  0.33253653]), array([-0.14064839,  0.39486094,  0.15932722, -0.20562584]), array([-0.08662995,  0.30404858,  0.36786268, -0.68072663]), array([-8.36476301e-04,  1.35619965e-01,  4.67863947e-01, -9.62299048e-01]), array([ 0.09032776, -0.0613969 ,  0.41883828, -0.95896232]), array([ 0.15719516, -0.22895123,  0.23150444, -0.67845637]), array([ 0.19053744, -0.35459732,  0.09164922, -0.55248732]), array([ 0.1783495 , -0.40837838, -0.21152168,  0.01995257]), array([ 0.10942552, -0.3491727 , -0.46230395,  0.55315194]), array([ 0.00198179, -0.19940588, -0.58638802,  0.90378328]), array([-0.11331   , -0.00754223, -0.53714897,  0.96326472]), array([-0.21466029,  0.19938781, -0.44908944,  1.05403268]), array([-0.2698423 ,  0.36016096, -0.08830874,  0.52180033]), array([-0.26038572,  0.43405387,  0.18265135,  0.20717855]), array([-0.17386504,  0.3759499 ,  0.66385251, -0.76866797]), array([-0.01965317,  0.17645978,  0.84173773, -1.17008274]), array([ 0.14601119, -0.06466863,  0.77346106, -1.17167545]), array([ 0.28703307, -0.29937727,  0.6012993 , -1.11377118]), array([ 0.37423022, -0.48839475,  0.24955074, -0.73715299]), array([ 0.36931487, -0.55085649, -0.2976248 ,  0.11869429]), array([ 0.25983437, -0.44433073, -0.77436775,  0.92026427]), array([ 0.07309068, -0.20109143, -1.04962145,  1.44591908]), array([-0.13910758,  0.09986101, -1.01899768,  1.4737952 ]), array([-0.32678321,  0.38724895, -0.81176774,  1.32284908]), array([-0.43574492,  0.57087451, -0.25584435,  0.47996337]), array([-0.42498805,  0.57291757,  0.36087678, -0.45807537]), array([-0.2969557 ,  0.39425953,  0.89268672, -1.2915443 ]), array([-0.08401689,  0.08093618,  1.18484483, -1.75587014]), array([ 0.15240689, -0.26572651,  1.11943188, -1.60789845]), array([ 0.34166144, -0.52586138,  0.73149122, -0.93110733]), array([ 0.43275313, -0.62207851,  0.16234723, -0.01294353]), array([ 0.40400586, -0.52970337, -0.44371819,  0.92335609]), array([ 0.26262501, -0.26522335, -0.93750349,  1.66587695]), array([ 0.0478942 ,  0.10321503, -1.15309663,  1.91566998]), array([-0.18669684,  0.48947688, -1.13232135,  1.83921317]), array([-0.38312779,  0.80209222, -0.79096554,  1.22518994]), array([-0.47965066,  0.9340208 , -0.15893337,  0.08041107]), array([-0.44423174,  0.83298951,  0.50855451, -1.08276974]), array([-0.28248125,  0.50968469,  1.07826064, -2.1021775 ]), array([-0.03284734,  0.0269676 ,  1.35052978, -2.59777087]), array([ 0.23871201, -0.50110023,  1.28743904, -2.53349114]), array([ 0.44397054, -0.9073441 ,  0.7276502 , -1.47029346]), array([ 0.52111353, -1.07835619,  0.03519652, -0.23062978]), array([ 0.45822626, -0.99901343, -0.65418486,  1.01801016]), array([ 0.26715765, -0.6777129 , -1.22473369,  2.15589549]), array([-0.02476253, -0.13428206, -1.62329625,  3.14816953]), array([-0.33028394,  0.47153938, -1.34292771,  2.73619358]), array([-0.53505042,  0.91117344, -0.66766822,  1.60064291]), array([-0.59013438,  1.1019537 ,  0.12001172,  0.30009072]), array([-0.47940555,  1.00237134,  0.96969858, -1.29094252]), array([-0.22484057,  0.62287882,  1.53176382, -2.45037752]), array([ 0.10712663,  0.06415621,  1.70217951, -2.97854407]), array([ 0.41663918, -0.49260151,  1.31057484, -2.43445794]), array([ 0.61912005, -0.89964809,  0.67527214, -1.57578123]), array([ 0.66740043, -1.08204258, -0.1948543 , -0.24175448]), array([ 0.54471828, -0.995811  , -1.01186947,  1.09877039]), array([ 0.27535871, -0.64976803, -1.63546443,  2.31348907]), array([-0.09555806, -0.07624407, -1.98372585,  3.26115687]), array([-0.46007364,  0.53411055, -1.56616812,  2.66443888]), array([-0.69499612,  0.94543663, -0.74620846,  1.40364475]), array([-0.75110703,  1.08975868,  0.18945251,  0.03629517]), array([-0.62180274,  0.95936269,  1.08542443, -1.33674855]), array([-0.31765358,  0.53071836,  1.9077405 , -2.89806223]), array([ 0.09562921, -0.11303291,  2.1136647 , -3.3286781 ]), array([ 0.48006406, -0.70891018,  1.64080016, -2.47312075]), array([ 0.72788213, -1.0697693 ,  0.80306012, -1.10912649]), array([ 0.79338536, -1.15075795, -0.15535795,  0.29817462]), array([ 0.66680969, -0.95041192, -1.09598468,  1.70199045]), array([ 0.35446804, -0.44592993, -1.97735733,  3.28017124]), array([-0.07412644,  0.26243756, -2.18567951,  3.56246549]), array([-0.47079871,  0.88399392, -1.69620153,  2.51122336]), array([-0.73070139,  1.24224894, -0.86972081,  1.05684533]), array([-0.81012293,  1.30729069,  0.08581913, -0.40322667]), array([-0.69594839,  1.08061328,  1.04608698, -1.86477814]), array([-0.40088812,  0.56539792,  1.85904305, -3.23304945]), array([ 0.01438388, -0.1555825 ,  2.17487059, -3.74464852]), array([ 0.4169994 , -0.82895064,  1.75625616, -2.81756694]), array([ 0.69254813, -1.24997985,  0.96414214, -1.37059693]), array([ 0.79373512, -1.37702687,  0.03638804,  0.09653079]), array([ 0.70610503, -1.21132804, -0.90514488,  1.56324566]), array([ 0.43892752, -0.75207747, -1.73212752,  3.00108813]), array([ 0.03895455, -0.04909952, -2.16337014,  3.83287553]), array([-0.37283472,  0.6736648 , -1.84200033,  3.17761018]), array([-0.66738541,  1.17239493, -1.06260161,  1.76855596]), array([-0.79818398,  1.40520104, -0.23129035,  0.55755465]), array([-0.7490168 ,  1.36945517,  0.71566394, -0.91666642]), array([-0.51849037,  1.03668053,  1.56269059, -2.40695678]), array([-0.14112742,  0.42083204,  2.13948484, -3.64214388]), array([ 0.30490836, -0.36734742,  2.18420787, -3.96349744]), array([ 0.67056862, -1.03604619,  1.4051347 , -2.61937821]), array([ 0.86346668, -1.43233945,  0.5047663 , -1.3390832 ]), array([ 0.86088099, -1.54758258, -0.52370097,  0.18443557]), array([ 0.66063883, -1.35622332, -1.45239339,  1.73727254]), array([ 0.29441663, -0.85239623, -2.16070221,  3.26769907]), array([-0.18546875, -0.06093597, -2.51929236,  4.4171197 ]), array([-0.63739354,  0.75081408, -1.88018178,  3.46813454]), array([-0.91101899,  1.28746277, -0.82934961,  1.88665659]), array([-0.96538136,  1.50974414,  0.28363293,  0.34241302]), array([-0.80238424,  1.42257082,  1.32361567, -1.22619023]), array([-0.4394083 ,  0.98650039,  2.26497828, -3.13736184]), array([ 0.07841141,  0.19166691,  2.80192903, -4.60870869]), array([ 0.60106747, -0.6827162 ,  2.27855365, -3.83945909]), array([ 0.9548963 , -1.28771725,  1.22295913, -2.19186104]), array([ 1.08382614, -1.56721074,  0.06134172, -0.61968997]), array([ 0.9722108 , -1.51157935, -1.16405619,  1.19097072]), array([ 0.63641655, -1.10575806, -2.15999083,  2.88390252]), array([ 0.12950397, -0.36926405, -2.81569044,  4.33499949]), array([-0.44114387,  0.53720371, -2.71966211,  4.37124382]), array([-0.90481508,  1.27698408, -1.85025765,  2.94736163]), array([-1.15917393,  1.6947539 , -0.68025621,  1.2667055 ]), array([-1.18262953,  1.81618877,  0.44525262, -0.05029577]), array([-0.97706771,  1.6458455 ,  1.58976834, -1.68077334]), array([-0.54963359,  1.10292487,  2.64987597, -3.78427365]), array([ 0.04707512,  0.1804272 ,  3.1859443 , -5.18915119]), array([ 0.64401478, -0.79698956,  2.6172572 , -4.23945207]), array([ 1.05897164, -1.46195847,  1.49974438, -2.41889385]), array([ 1.23787344, -1.78123421,  0.28230273, -0.80472547]), array([ 1.17182756, -1.78796253, -0.93486849,  0.74789849]), array([ 0.87074069, -1.47064475, -2.04950719,  2.4644616 ]), array([ 0.36681742, -0.78892913, -2.93401528,  4.32664686]), array([-0.27127815,  0.21765555, -3.26162865,  5.34040295]), array([-0.84444235,  1.13922102, -2.36245353,  3.68752642]), array([-1.20005327,  1.69146167, -1.176521  ,  1.88397884]), array([-1.31118427,  1.90989476,  0.06843652,  0.32096409]), array([-1.17409636,  1.81896164,  1.29077003, -1.25319375]), array([-0.8032956 ,  1.39240232,  2.38745254, -3.06004816]), array([-0.2358418 ,  0.58473625,  3.21255926, -4.93285746]), array([ 0.41900873, -0.45352543,  3.13081735, -4.99838588]), array([ 0.95096294, -1.27980724,  2.11808005, -3.17815471]), array([ 1.25525085, -1.73761119,  0.91101543, -1.44942956]), array([ 1.31242624, -1.87317625, -0.3401057 ,  0.08323326]), array([ 1.1216402 , -1.69938637, -1.55348815,  1.68722578]), array([ 0.70037653, -1.17921505, -2.62663841,  3.55718767]), array([ 0.09282487, -0.2838942 , -3.334324  ,  5.19499912]), array([-0.55343227,  0.72487322, -2.94007667,  4.48841967]), array([-1.03877599,  1.43441406, -1.86935461,  2.59925516]), array([-1.29249087,  1.78380179, -0.65518047,  0.93890626]), array([-1.29841974,  1.81978285,  0.59520832, -0.57809494]), array([-1.05745031,  1.54380264,  1.79919071, -2.22298622]), array([-0.5883554 ,  0.91048938,  2.8533684 , -4.1287769 ]), array([ 0.05006384, -0.06249155,  3.36372158, -5.25390938]), array([ 0.6838885 , -1.03388399,  2.82300395, -4.15766686]), array([ 1.14014763, -1.66727595,  1.71060493, -2.22034595]), array([ 1.36055834, -1.94497706,  0.48194908, -0.59723936]), array([ 1.33098856, -1.91340094, -0.77595264,  0.91852287]), array([ 1.04534497, -1.54203909, -2.06858333,  2.85463293]), array([ 0.52065037, -0.77073621, -3.13550857,  4.85962449]), array([-0.16162166,  0.31749875, -3.47643055,  5.55650013]), array([-0.78534565,  1.2649654 , -2.65449002,  3.73933737]), array([-1.20605536,  1.81741583, -1.52719026,  1.84433129]), array([-1.38889122,  2.02412775, -0.29073285,  0.25587108]), array([-1.32093955,  1.92404802,  0.9673263 , -1.269155  ]), array([-1.00574859,  1.50197594,  2.16863764, -3.00792047]), array([-0.45246936,  0.66872151,  3.32118695, -5.32022558]), array([ 0.2528086 , -0.48023903,  3.49891264, -5.64445536]), array([ 0.86880279, -1.41885565,  2.58010298, -3.63457607]), array([ 1.27171359, -1.95191223,  1.42687614, -1.76306824]), array([ 1.43319177, -2.1448226 ,  0.17962913, -0.1947835 ]), array([ 1.34283716, -2.03237831, -1.07886156,  1.33522281]), array([ 1.00614296, -1.59500079, -2.27001677,  3.0991404 ]), array([ 0.43444221, -0.73793481, -3.40876317,  5.48455505]), array([-0.30193234,  0.490125  , -3.70314179,  6.21884138]), array([-0.94729826,  1.52387485, -2.67639343,  4.02682055]), array([-1.36400465,  2.1308586 , -1.47559006,  2.12676349]), array([-1.53316667,  2.39745198, -0.21133364,  0.56807001]), array([-1.44859954,  2.36062687,  1.05241429, -0.94912456]), array([-1.11695243,  2.00500385,  2.24133301, -2.66048383]), array([-0.5650957 ,  1.26732087,  3.24285702, -4.78552973]), array([ 0.15615319,  0.10487189,  3.80359843, -6.48371613]), array([ 0.84815686, -1.07501797,  2.93443181, -4.92661052]), array([ 1.30783342, -1.84858056,  1.65348457, -2.89128687]), array([ 1.50816324, -2.26174401,  0.34895481, -1.28258984]), array([ 1.44850198, -2.3666452 , -0.93864802,  0.24328577]), array([ 1.13839851, -2.15367696, -2.13527499,  1.9286859 ]), array([ 0.61178986, -1.57295591, -3.07925212,  3.93759853]), array([-0.0712349 , -0.5689953 , -3.66328115,  5.96922463]), array([-0.77358385,  0.63225999, -3.13032059,  5.51635925]), array([-1.26854059,  1.53048343, -1.78953489,  3.47890043]), array([-1.4890481 ,  2.0547358 , -0.41858968,  1.81679497]), array([-1.43818194,  2.26446535,  0.91737356,  0.27104629]), array([-1.12920387,  2.15186445,  2.14074172, -1.4379212 ]), array([-0.60235218,  1.66998032,  3.06313171, -3.42721787]), array([ 0.06843113,  0.77375592,  3.56695575, -5.45010457]), array([ 0.76376124, -0.37657561,  3.17386149, -5.55614847]), array([ 1.27067548, -1.304736  ,  1.84058119, -3.66515153]), array([ 1.497515  , -1.86642727,  0.43070062, -2.00502719]), array([ 1.44508196, -2.11419877, -0.94509551, -0.45987194]), array([ 1.12028716, -2.01460471, -2.2675186 ,  1.50712173]), array([ 0.56690197, -1.51041162, -3.20158091,  3.5819442 ]), array([-0.13145806, -0.58238985, -3.68371007,  5.54697141]), array([-0.83247902,  0.53864416, -3.11799754,  5.17923505])]</t>
-  </si>
-  <si>
-    <t>['[2,2,2]', '[1,1,1]', '[1,2,0]', '[1,1,2]', '[2,1,0]', '[0,1,1]', '[1,0,2]', '[0,2,1]', '[0,0,0]', '[2,0,1]']</t>
+    <t>[array([-0.03763371, -0.01533471,  0.06554052, -0.01816017], dtype=float32), array([-0.0208055 , -0.02030166,  0.09914155, -0.02801351]), array([ 0.013578  , -0.05917353,  0.23628798, -0.34824344]), array([ 0.06892075, -0.15170277,  0.30283362, -0.5520916 ]), array([ 0.12827063, -0.26838081,  0.27505366, -0.58564774]), array([ 0.16005875, -0.34102171,  0.03515865, -0.12569461]), array([ 0.12853775, -0.28300606, -0.34263689,  0.69246565]), array([ 0.02967829, -0.07631626, -0.62005388,  1.32504849]), array([-0.09246068,  0.18592321, -0.56754814,  1.23120791]), array([-0.1976969 ,  0.42525518, -0.45641363,  1.1061965 ]), array([-0.26530513,  0.60912674, -0.20326561,  0.69842509]), array([-0.26302958,  0.66372753,  0.2246754 , -0.15656325]), array([-0.16680371,  0.51765705,  0.71872155, -1.27833   ]), array([ 0.0124048 ,  0.17197175,  1.02997135, -2.0994731 ]), array([ 0.2090163 , -0.24365488,  0.87971357, -1.94585788]), array([ 0.35704713, -0.600544  ,  0.56171405, -1.54674072]), array([ 0.41110979, -0.80959286, -0.02920943, -0.52168299]), array([ 0.34662659, -0.80649065, -0.60190911,  0.54576576]), array([ 0.1675692 , -0.56771434, -1.15559225,  1.80278521]), array([-0.09650255, -0.1145736 , -1.42064778,  2.61316666]), array([-0.35550054,  0.3823065 , -1.09801968,  2.21941658]), array([-0.52565236,  0.76452727, -0.56548069,  1.53514494]), array([-0.57276171,  0.9803314 ,  0.10102203,  0.60374824]), array([-0.46589531,  0.94458041,  0.9469516 , -0.95497077]), array([-0.20633833,  0.60538674,  1.60448403, -2.39024761]), array([ 0.13673026,  0.06212475,  1.73897486, -2.8835563 ]), array([ 0.46300931, -0.50695129,  1.43635223, -2.64338708]), array([ 0.67239452, -0.9176374 ,  0.62344881, -1.41645785]), array([ 0.70617916, -1.06671357, -0.28644978, -0.06947851]), array([ 0.55119775, -0.91569372, -1.24134589,  1.57602388]), array([ 0.22379676, -0.4449935 , -1.97531981,  3.05757966]), array([-0.20191144,  0.24272702, -2.1617158 ,  3.58599373]), array([-0.59138034,  0.89327617, -1.64573111,  2.7698439 ]), array([-0.82816075,  1.29640938, -0.69802256,  1.2564462 ]), array([-0.87533873,  1.42445164,  0.22928548,  0.02449156]), array([-0.72993849,  1.27863076,  1.20687977, -1.48988228]), array([-0.40394683,  0.82715945,  2.0102243 , -2.99974762]), array([ 0.04604846,  0.1166174 ,  2.38032189, -3.90382345]), array([ 0.49156105, -0.62063731,  1.95480293, -3.23656349]), array([ 0.79596223, -1.1263714 ,  1.04855096, -1.78290436]), array([ 0.90266398, -1.33339035,  0.01086897, -0.2927491 ]), array([ 0.7914319 , -1.21648025, -1.11146929,  1.4714899 ]), array([ 0.47746951, -0.76939455, -1.98793128,  2.97579577]), array([ 0.02437494, -0.06447944, -2.4314289 ,  3.86762506]), array([-0.43778372,  0.66295326, -2.06916611,  3.17557942]), array([-0.77041651,  1.15456347, -1.21203373,  1.70295306]), array([-0.91195946,  1.3441739 , -0.18975495,  0.2011394 ]), array([-0.84464094,  1.23614923,  0.85701946, -1.2857466 ]), array([-0.56471341,  0.79765424,  1.91514825, -3.0973971 ]), array([-0.11456627,  0.05883346,  2.47547463, -4.08536032]), array([ 0.37801179, -0.74707082,  2.31338395, -3.70255992]), array([ 0.77217797, -1.35790731,  1.57443466, -2.35731442]), array([ 0.99423847, -1.69060125,  0.62517191, -0.98395324]), array([ 1.00946225, -1.73226703, -0.47294926,  0.56479236]), array([ 0.80867095, -1.46024161, -1.51695346,  2.17615987]), array([ 0.41353488, -0.85359911, -2.39215024,  3.8750556 ]), array([-0.12769257,  0.07298444, -2.87081496,  5.08797985]), array([-0.64540244,  0.98592404, -2.18075613,  3.80197666]), array([-0.97709446,  1.56973278, -1.11306582,  2.05547506]), array([-1.08591433,  1.81993959,  0.02816082,  0.4638776 ]), array([-0.96793597,  1.75584168,  1.13638061, -1.11724118]), array([-0.63277206,  1.33856196,  2.18558769, -3.09060594]), array([-0.10899746,  0.51365785,  2.98025191, -5.06419517]), array([ 0.49564492, -0.55578318,  2.86200774, -5.18795066]), array([ 0.9629674 , -1.41020849,  1.7587789 , -3.30896619]), array([ 1.20101365, -1.91990345,  0.61075352, -1.82171043]), array([ 1.2060078 , -2.14643589, -0.55498379, -0.44571563]), array([ 0.97212336, -2.05067595, -1.75093197,  1.42552786]), array([ 0.52397513, -1.56271995, -2.68011614,  3.49297322]), array([-0.06934615, -0.67431691, -3.17789272,  5.29138282]), array([-0.69867503,  0.45567204, -2.90708131,  5.5436131 ]), array([-1.16423318,  1.40568238, -1.68529403,  3.88464787]), array([-1.36668088,  2.02560116, -0.3379525 ,  2.35432163]), array([-1.295708  ,  2.33200922,  1.0272971 ,  0.70707241]), array([-0.96822394,  2.30225359,  2.19945986, -1.02342426]), array([-0.4380737 ,  1.89415934,  3.01345166, -3.07366675]), array([ 0.19334588,  1.09816487,  3.2272589 , -4.82673954]), array([ 8.29378637e-01,  4.01164662e-03,  2.98799436e+00, -5.76588438e+00]), array([ 1.3145159 , -1.04229337,  1.75092929, -4.49128183]), array([ 1.5132586 , -1.78505239,  0.22593452, -2.96148528]), array([ 1.40592442, -2.22790777, -1.28157845, -1.4440446 ]), array([ 1.00902494, -2.32881044, -2.62410867,  0.46152442]), array([ 0.39382805, -2.03806661, -3.40588578,  2.43796958]), array([-0.30739433, -1.34636262, -3.50299033,  4.40709469]), array([-0.97685262, -0.33118135, -3.10232705,  5.49371604]), array([-1.49501961,  0.71235004, -1.96818966,  4.69838163]), array([-1.74054   ,  1.51872125, -0.46167481,  3.3733284 ]), array([-1.66600549,  2.03692929,  1.20380638,  1.77600803]), array([-1.26691007,  2.20411494,  2.7429661 , -0.17677638]), array([-0.59420716,  1.91865651,  3.86557669, -2.72681254]), array([ 0.21672742,  1.13534693,  4.12824362, -5.02174508]), array([ 1.02262582, -0.02221172,  3.77006264, -6.10700031]), array([ 1.65337421, -1.11947875,  2.45904735, -4.69965657]), array([ 2.00523742, -1.92472315,  1.07213238, -3.44079221]), array([ 2.08613518, -2.51357619, -0.25064955, -2.44712623]), array([ 1.90504199, -2.8717143 , -1.54778965, -1.09455165]), array([ 1.46201603, -2.91557314, -2.87871753,  0.69162683]), array([ 0.76575314, -2.58186104, -3.99634448,  2.68486531]), array([-0.0774133 , -1.82672331, -4.28766369,  4.88280943]), array([-0.91262075, -0.64561797, -4.01113216,  6.75112092]), array([-1.61294763,  0.66190075, -2.83051472,  5.89938268]), array([-2.0261753 ,  1.69286496, -1.29413005,  4.47401818]), array([-2.12604633,  2.45611485,  0.27047117,  3.18263339]), array([-1.93792895,  2.97785388,  1.57557708,  2.0012405 ]), array([-1.49908496, -3.05461804,  2.80321767,  0.510942  ]), array([-0.81665643, -3.10600319,  3.97097674, -0.95645739]), array([ 0.04464072,  2.87916409,  4.47375187, -1.93228598]), array([ 0.89432013,  2.44225312,  3.86046148, -2.32669258]), array([ 1.54292189,  2.01925109,  2.59148688, -1.77440705]), array([ 1.93310203,  1.77499294,  1.33175827, -0.59235752])]</t>
+  </si>
+  <si>
+    <t>['[1,1,2]', '[1,2,0]', '[2,2,2]', '[0,1,1]', '[1,0,2]', '[0,0,0]', '[1,1,1]', '[2,1,0]', '[0,2,1]', '[2,0,1]']</t>
+  </si>
+  <si>
+    <t>[1, 2, 5, 6, 7, 8, 11, 12, 13, 14, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 30, 31, 33, 34, 36, 38, 39, 41, 43, 45, 47, 49, 50, 53, 55, 56, 58, 59, 60, 62, 63, 64, 66, 68, 69, 70, 71, 72, 73, 74, 75, 76, 77, 79, 80, 81, 82, 83, 84, 85, 86, 88, 91, 92, 96, 97, 99, 100, 103, 104, 105, 108, 109, 110, 111, 115, 116, 117, 119, 120, 121, 122, 123, 124, 125, 127, 128, 130, 131, 135, 137, 140, 141, 142, 144, 145, 147, 148, 149, 150, 151, 153, 154, 156, 157, 158, 159, 161, 162, 163, 164, 165, 167, 168, 169, 170, 172, 174, 175, 177, 182, 183, 186, 188, 190, 191, 194, 196, 197, 199]</t>
+  </si>
+  <si>
+    <t>[0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 1, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 2, 1, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 0, 1, 2, 2, 2, 2, 2, 2, 2, 2, 1, 0, 0, 0, 0, 1, 1, 2, 2, 2, 2, 2, 2]</t>
+  </si>
+  <si>
+    <t>['[-0.03763371 -0.01533471  0.06554052 -0.01816017]', '[-0.0208055  -0.02030166  0.09914155 -0.02801351]', '[ 0.00031733 -0.02489487  0.10765546 -0.0138725 ]', '[ 0.0337014  -0.05856607  0.21818034 -0.31149513]', '[ 0.08319589 -0.1423563   0.26396396 -0.5039722 ]', '[ 0.12048504 -0.21572161  0.09957913 -0.21237203]', '[ 0.12088981 -0.22322272 -0.09554925  0.13817829]', '[ 0.0840913  -0.16334886 -0.26315131  0.44485676]', '[ 0.02098223 -0.05454653 -0.35174474  0.61468058]', '[-0.06247597  0.10366262 -0.46056166  0.92621296]', '[-0.15308831  0.29670111 -0.4209624   0.95662787]', '[-0.20882922  0.434915   -0.12307303  0.39838422]', '[-0.19980541  0.45022942  0.21123382 -0.24535956]', '[-0.1280132   0.34165192  0.49007124 -0.81448381]', '[-0.01322672  0.14026959  0.6288688  -1.14831669]', '[ 0.123407   -0.12755047  0.7003348  -1.45969284]', '[ 0.23810748 -0.37944214  0.4171015  -1.00197834]', '[ 0.28180758 -0.51172427  0.01004919 -0.29867419]', '[ 0.241725   -0.49572477 -0.40223569  0.45109041]', '[ 0.12778503 -0.34001634 -0.71145836  1.06799781]', '[-0.02924108 -0.09048711 -0.81950683  1.36000043]', '[-0.1827393   0.17339491 -0.67575289  1.20767792]', '[-0.28546908  0.36744749 -0.32682133  0.68874246]', '[-0.3070958   0.43723696  0.11535698 -0.00225899]', '[-0.24108818  0.36753289  0.53021606 -0.67631003]', '[-0.10455784  0.1804047   0.80278785 -1.14482044]', '[ 0.06404913 -0.06431016  0.8409378  -1.23151373]', '[ 0.21459786 -0.28332141  0.62810673 -0.89899507]', '[ 0.31611666 -0.43832796  0.36358151 -0.61369896]', '[ 0.3531638  -0.51769686 -0.0013568  -0.16507978]', '[ 0.30276251 -0.46966191 -0.49195926  0.63326957]', '[ 0.16476552 -0.27575244 -0.8566043   1.25833265]', '[-0.03643881  0.04080678 -1.10421804  1.81845616]', '[-0.24011368  0.37519856 -0.88145937  1.43616166]', '[-0.37224171  0.58754272 -0.41226631  0.64541785]', '[-0.41052009  0.65598929  0.03691502  0.02785183]', '[-0.34574269  0.56653998  0.59800632 -0.90637862]', '[-0.1682483   0.2737397   1.13831777 -1.96026415]', '[ 0.07359396 -0.14317948  1.21484362 -2.0887956 ]', '[ 0.29129993 -0.51348894  0.90952658 -1.5226589 ]', '[ 0.43339379 -0.75830131  0.4824264  -0.88172971]', '[ 0.46526714 -0.8250779  -0.16810711  0.21998992]', '[ 0.35650259 -0.6410189  -0.90221523  1.60061928]', '[ 0.13032422 -0.23713231 -1.30655835  2.34700089]', '[-0.15098208  0.27941325 -1.42612394  2.66456457]', '[-0.39556598  0.73559403 -0.96529904  1.8035549 ]', '[-0.53405742  1.00980813 -0.39665302  0.90774006]', '[-0.53897514  1.064134    0.34577799 -0.36539088]', '[-0.38899449  0.83597034  1.1339663  -1.90297333]', '[-0.1116508   0.35137718  1.58022324 -2.84537272]', '[ 0.20930151 -0.23908373  1.53600144 -2.87791   ]', '[ 0.48028096 -0.76576583  1.10813586 -2.27168531]', '[ 0.63493439 -1.12037729  0.4154764  -1.24398374]', '[ 0.63285557 -1.23090827 -0.4301295   0.13870791]', '[ 0.45890954 -1.0374982  -1.28510688  1.79087225]', '[ 0.14448924 -0.55433327 -1.80292891  2.96463065]', '[-0.22869113  0.0894681  -1.82486146  3.2717939 ]', '[-0.55509554  0.70335059 -1.35529265  2.71235449]', '[-0.73755242  1.10978656 -0.44727712  1.32838566]', '[-0.73158914  1.23269622  0.50028159 -0.10051064]', '[-0.54433607  1.06892395  1.34414765 -1.53280329]', '[-0.19859174  0.59744565  2.05865605 -3.12408206]', '[ 0.23120664 -0.089014    2.12214508 -3.51349587]', '[ 0.60150359 -0.71253026  1.49477377 -2.56896082]', '[ 0.8083502  -1.08837851  0.54881566 -1.17052683]', '[ 0.8272109  -1.20747229 -0.36047852 -0.01608852]', '[ 0.65833215 -1.06507299 -1.30519726  1.44195706]', '[ 0.30815199 -0.60459447 -2.144334    3.11568856]', '[-0.15136906  0.09182338 -2.32780536  3.61238743]', '[-0.56998714  0.73650981 -1.76193129  2.66461796]', '[-0.83198268  1.12658175 -0.8259225   1.21829062]', '[-0.89351495  1.22471494  0.21577634 -0.2338636 ]', '[-0.74748061  1.0319339   1.22896625 -1.69774511]', '[-0.41367998  0.54907601  2.05728629 -3.07540754]', '[ 0.04011473 -0.14037424  2.35880148 -3.58610188]', '[ 0.47658156 -0.78134357  1.90598947 -2.6496747 ]', '[ 0.77589967 -1.16685806  1.04740345 -1.1842159 ]', '[ 0.88534991 -1.25592265  0.0339096   0.28754135]', '[ 0.77762006 -1.02413232 -1.105978    2.03832503]', '[ 0.46249465 -0.47243262 -1.99498738  3.41434802]', '[ 0.01712033  0.27485037 -2.33040579  3.80385645]', '[-0.41681654  0.94429607 -1.91628283  2.732078  ]', '[-0.72498793  1.34044802 -1.12567064  1.21474122]', '[-0.85548127  1.4317303  -0.16125466 -0.2956533 ]', '[-0.78596506  1.22256642  0.85456915 -1.80030174]', '[-0.51890338  0.71044534  1.78381836 -3.29425484]', '[-0.09990344 -0.05221658  2.28989474 -4.10762373]', '[ 0.35116054 -0.84599361  2.09791674 -3.59052948]', '[ 0.69632703 -1.40921863  1.3141406  -2.01847291]', '[ 0.87520264 -1.68113463  0.45557265 -0.70749933]', '[ 0.86631032 -1.67036368 -0.5432254   0.81570413]', '[ 0.66193002 -1.35092612 -1.48201684  2.3924269 ]', '[ 0.28490023 -0.71162546 -2.2395859   3.95390526]', '[-0.20839929  0.19679377 -2.54067354  4.81706123]', '[-0.66216882  1.07233681 -1.88792462  3.7396891 ]', '[-0.94269511  1.67127203 -0.89582397  2.25978607]', '[-1.00923607  1.96115643  0.22523491  0.65503256]', '[-0.85849891  1.93423117  1.25595096 -0.93084769]', '[-0.51414348  1.56014512  2.14463579 -2.83039115]', '[-0.02873872  0.82554876  2.65001027 -4.45684366]', '[ 0.50364526 -0.14287035  2.51377621 -4.88484545]', '[ 0.92260916 -1.02254172  1.57574847 -3.73351044]', '[ 1.11666087 -1.62012083  0.35262428 -2.2509355 ]', '[ 1.05734775 -1.90276551 -0.92346508 -0.57580591]', '[ 0.76202365 -1.84577486 -1.97685907  1.15916579]', '[ 0.29410472 -1.43635402 -2.62774306  2.92309146]', '[-0.2689444  -0.6675149  -2.92465166  4.65052403]', '[-0.82622767  0.31746262 -2.48961182  4.84658498]', '[-1.19878515  1.13088664 -1.18181001  3.21568988]', '[-1.29346298  1.60882412  0.23311636  1.57571905]', '[-1.11062449  1.75664283  1.56825514 -0.12806691]', '[-0.68446351  1.54201064  2.62926782 -2.04960988]', '[-0.08103498  0.90713073  3.322727   -4.25230692]', '[ 0.5989301  -0.08114888  3.30602015 -5.24623986]', '[ 1.16661973 -1.02271352  2.26530913 -3.97130441]', '[ 1.48136618 -1.64023148  0.8803865  -2.26461588]', '[ 1.51956947 -1.94439236 -0.49443241 -0.78158844]', '[ 1.28709045 -1.94264534 -1.81185776  0.8467923 ]', '[ 0.80085306 -1.55724148 -3.00227345  3.08023961]', '[ 0.11920844 -0.71803287 -3.73198577  5.23557462]', '[-0.62678377  0.39922874 -3.5046022   5.41513183]', '[-1.21212773  1.29367686 -2.28711583  3.45890643]', '[-1.53714571  1.80979565 -0.96199206  1.77646606]', '[-1.59715177  2.02212893  0.36033486  0.35740489]', '[-1.3945176   1.94500321  1.65676187 -1.17391882]', '[-0.94225259  1.5258666   2.83469376 -3.09595637]', '[-0.26755876  0.65319122  3.8476     -5.59154202]', '[ 0.5148857  -0.52905453  3.72935336 -5.64856172]', '[ 1.15145455 -1.44728039  2.57755581 -3.48647119]', '[ 1.5483901  -1.98097149  1.38174653 -1.92985136]', '[ 1.69523707 -2.22054043  0.08739645 -0.49644903]', '[ 1.58383833 -2.18017306 -1.19920009  0.92481353]', '[ 1.21105837 -1.80813366 -2.51511337  2.87997213]', '[ 0.58528802 -0.98416021 -3.71972602  5.44553886]', '[-0.23895945  0.30996755 -4.26852721  6.88891349]', '[-0.99870286  1.47208223 -3.22204345  4.54176161]', '[-1.52895444  2.18602155 -2.06730793  2.70866039]', '[-1.81636397  2.56981095 -0.80972046  1.18535351]', '[-1.86124936  2.69046132  0.35821273  0.02448989]', '[-1.66011961  2.53432564  1.65622088 -1.61890725]', '[-1.206525    2.0401093   2.86205975 -3.41282644]', '[-0.52612466  1.12222783  3.91664281 -5.86507568]', '[ 0.32392677 -0.25004872  4.31925787 -7.21727202]', '[ 1.0926241  -1.50290924  3.24640959 -5.07925828]', '[ 1.61091204 -2.29963209  1.94322245 -3.03023626]', '[ 1.87244836 -2.75194912  0.68268916 -1.5392625 ]', '[ 1.89408037 -2.94103759 -0.46184529 -0.34800947]', '[ 1.68064881 -2.86595647 -1.67865989  1.1217451 ]', '[ 1.22321527 -2.47791598 -2.87083969  2.81728049]', '[ 0.55407408 -1.70545782 -3.75858123  5.00856344]', '[-0.26002879 -0.45091149 -4.28146712  7.33421467]', '[-1.04683819  0.95108059 -3.33155513  6.08604831]', '[-1.56902502  1.96030327 -1.89433575  4.1155315 ]', '[-1.80429807  2.61920308 -0.48181524  2.53428498]', '[-1.77057119  2.9801797   0.80369847  1.06867378]', '[-1.48482792  3.04139078  2.05207412 -0.46760388]', '[-0.95553456  2.78992496  3.19139697 -2.0575806 ]', '[-0.2486246   2.21216274  3.74098674 -3.73410726]', '[ 0.48815901  1.30184696  3.5482951  -5.30685942]', '[ 1.14627702  0.15537761  2.92636953 -5.84793582]', '[ 1.61155386 -0.92580971  1.62113158 -4.76800748]', '[ 1.76569841 -1.71315384 -0.09185155 -3.12836704]', '[ 1.5742639  -2.17037993 -1.80620024 -1.38903595]', '[ 1.05928212 -2.24134943 -3.27139461  0.7428187 ]', '[ 0.31171105 -1.85710694 -4.05736381  3.10360182]', '[-0.50389581 -1.023557   -3.98616527  5.08274138]', '[-1.25134232  0.09088564 -3.35387467  5.66441923]', '[-1.78260088  1.07662374 -1.92016629  4.12608173]', '[-2.02175976  1.76818487 -0.4781807   2.85012537]', '[-1.973225    2.22083367  0.96714353  1.64067711]', '[-1.63451576  2.3978481   2.41276316  0.04564555]', '[-1.01294702  2.1824154   3.7359775  -2.29551327]', '[-0.19028814  1.46951472  4.37805793 -4.86522983]', '[ 0.70896602  0.24385479  4.47026146 -7.00784024]', '[ 1.48691947 -1.0294052   3.15738562 -5.34258539]', '[ 1.96939668 -1.90680348  1.70314701 -3.57959509]', '[ 2.18682562 -2.52368754  0.49380762 -2.62904107]', '[ 2.1700267  -2.93849288 -0.64236094 -1.49753676]', '[ 1.93120803 -3.10897217 -1.7584188  -0.17111728]', '[ 1.45260677 -2.97370995 -3.03610418  1.5594047 ]', '[ 0.72982771 -2.46658121 -4.09519131  3.58181668]', '[-0.12980157 -1.51046601 -4.40183614  6.03235301]', '[-0.99695448 -0.11540541 -4.12012063  7.46650542]', '[-1.67857543  1.21466866 -2.57304734  5.56948546]', '[-2.03687344  2.17409645 -1.03285846  4.13586217]', '[-2.10497988  2.890526    0.3007167   3.03611693]', '[-1.9309155  -2.91975373  1.41061769  1.6808197 ]', '[-1.54055366 -2.71999664  2.50717658  0.3442922 ]', '[-0.92631305 -2.75744878  3.60634771 -0.6160101 ]', '[-0.12433634 -2.93370104  4.28002136 -0.99348397]', '[ 0.71128989 -3.07550537  3.91500372 -0.28135073]', '[ 1.39193818 -2.99750029  2.81033791  1.15218197]', '[ 1.81261199 -2.59528471  1.33523747  2.8806083 ]', '[ 1.90032008 -1.85025714 -0.50538055  4.56932453]', '[ 1.60316674 -0.74808948 -2.45026541  6.52419839]', '[ 0.95548812  0.72977875 -3.78150848  7.73079605]', '[ 0.17126816  2.12831592 -4.04434391  6.18223044]', '[-0.63594989 -3.04416068 -3.85667719  5.0555903 ]', '[-1.3103789  -2.07651325 -2.8219321   4.65320536]', '[-1.7601921  -1.21443744 -1.69952946  3.92310976]']</t>
+  </si>
+  <si>
+    <t>[array([-0.03763371, -0.01533471,  0.06554052, -0.01816017], dtype=float32), array([-0.0208055 , -0.02030166,  0.09914155, -0.02801351]), array([ 0.00031733, -0.02489487,  0.10765546, -0.0138725 ]), array([ 0.0337014 , -0.05856607,  0.21818034, -0.31149513]), array([ 0.08319589, -0.1423563 ,  0.26396396, -0.5039722 ]), array([ 0.12048504, -0.21572161,  0.09957913, -0.21237203]), array([ 0.12088981, -0.22322272, -0.09554925,  0.13817829]), array([ 0.0840913 , -0.16334886, -0.26315131,  0.44485676]), array([ 0.02098223, -0.05454653, -0.35174474,  0.61468058]), array([-0.06247597,  0.10366262, -0.46056166,  0.92621296]), array([-0.15308831,  0.29670111, -0.4209624 ,  0.95662787]), array([-0.20882922,  0.434915  , -0.12307303,  0.39838422]), array([-0.19980541,  0.45022942,  0.21123382, -0.24535956]), array([-0.1280132 ,  0.34165192,  0.49007124, -0.81448381]), array([-0.01322672,  0.14026959,  0.6288688 , -1.14831669]), array([ 0.123407  , -0.12755047,  0.7003348 , -1.45969284]), array([ 0.23810748, -0.37944214,  0.4171015 , -1.00197834]), array([ 0.28180758, -0.51172427,  0.01004919, -0.29867419]), array([ 0.241725  , -0.49572477, -0.40223569,  0.45109041]), array([ 0.12778503, -0.34001634, -0.71145836,  1.06799781]), array([-0.02924108, -0.09048711, -0.81950683,  1.36000043]), array([-0.1827393 ,  0.17339491, -0.67575289,  1.20767792]), array([-0.28546908,  0.36744749, -0.32682133,  0.68874246]), array([-0.3070958 ,  0.43723696,  0.11535698, -0.00225899]), array([-0.24108818,  0.36753289,  0.53021606, -0.67631003]), array([-0.10455784,  0.1804047 ,  0.80278785, -1.14482044]), array([ 0.06404913, -0.06431016,  0.8409378 , -1.23151373]), array([ 0.21459786, -0.28332141,  0.62810673, -0.89899507]), array([ 0.31611666, -0.43832796,  0.36358151, -0.61369896]), array([ 0.3531638 , -0.51769686, -0.0013568 , -0.16507978]), array([ 0.30276251, -0.46966191, -0.49195926,  0.63326957]), array([ 0.16476552, -0.27575244, -0.8566043 ,  1.25833265]), array([-0.03643881,  0.04080678, -1.10421804,  1.81845616]), array([-0.24011368,  0.37519856, -0.88145937,  1.43616166]), array([-0.37224171,  0.58754272, -0.41226631,  0.64541785]), array([-0.41052009,  0.65598929,  0.03691502,  0.02785183]), array([-0.34574269,  0.56653998,  0.59800632, -0.90637862]), array([-0.1682483 ,  0.2737397 ,  1.13831777, -1.96026415]), array([ 0.07359396, -0.14317948,  1.21484362, -2.0887956 ]), array([ 0.29129993, -0.51348894,  0.90952658, -1.5226589 ]), array([ 0.43339379, -0.75830131,  0.4824264 , -0.88172971]), array([ 0.46526714, -0.8250779 , -0.16810711,  0.21998992]), array([ 0.35650259, -0.6410189 , -0.90221523,  1.60061928]), array([ 0.13032422, -0.23713231, -1.30655835,  2.34700089]), array([-0.15098208,  0.27941325, -1.42612394,  2.66456457]), array([-0.39556598,  0.73559403, -0.96529904,  1.8035549 ]), array([-0.53405742,  1.00980813, -0.39665302,  0.90774006]), array([-0.53897514,  1.064134  ,  0.34577799, -0.36539088]), array([-0.38899449,  0.83597034,  1.1339663 , -1.90297333]), array([-0.1116508 ,  0.35137718,  1.58022324, -2.84537272]), array([ 0.20930151, -0.23908373,  1.53600144, -2.87791   ]), array([ 0.48028096, -0.76576583,  1.10813586, -2.27168531]), array([ 0.63493439, -1.12037729,  0.4154764 , -1.24398374]), array([ 0.63285557, -1.23090827, -0.4301295 ,  0.13870791]), array([ 0.45890954, -1.0374982 , -1.28510688,  1.79087225]), array([ 0.14448924, -0.55433327, -1.80292891,  2.96463065]), array([-0.22869113,  0.0894681 , -1.82486146,  3.2717939 ]), array([-0.55509554,  0.70335059, -1.35529265,  2.71235449]), array([-0.73755242,  1.10978656, -0.44727712,  1.32838566]), array([-0.73158914,  1.23269622,  0.50028159, -0.10051064]), array([-0.54433607,  1.06892395,  1.34414765, -1.53280329]), array([-0.19859174,  0.59744565,  2.05865605, -3.12408206]), array([ 0.23120664, -0.089014  ,  2.12214508, -3.51349587]), array([ 0.60150359, -0.71253026,  1.49477377, -2.56896082]), array([ 0.8083502 , -1.08837851,  0.54881566, -1.17052683]), array([ 0.8272109 , -1.20747229, -0.36047852, -0.01608852]), array([ 0.65833215, -1.06507299, -1.30519726,  1.44195706]), array([ 0.30815199, -0.60459447, -2.144334  ,  3.11568856]), array([-0.15136906,  0.09182338, -2.32780536,  3.61238743]), array([-0.56998714,  0.73650981, -1.76193129,  2.66461796]), array([-0.83198268,  1.12658175, -0.8259225 ,  1.21829062]), array([-0.89351495,  1.22471494,  0.21577634, -0.2338636 ]), array([-0.74748061,  1.0319339 ,  1.22896625, -1.69774511]), array([-0.41367998,  0.54907601,  2.05728629, -3.07540754]), array([ 0.04011473, -0.14037424,  2.35880148, -3.58610188]), array([ 0.47658156, -0.78134357,  1.90598947, -2.6496747 ]), array([ 0.77589967, -1.16685806,  1.04740345, -1.1842159 ]), array([ 0.88534991, -1.25592265,  0.0339096 ,  0.28754135]), array([ 0.77762006, -1.02413232, -1.105978  ,  2.03832503]), array([ 0.46249465, -0.47243262, -1.99498738,  3.41434802]), array([ 0.01712033,  0.27485037, -2.33040579,  3.80385645]), array([-0.41681654,  0.94429607, -1.91628283,  2.732078  ]), array([-0.72498793,  1.34044802, -1.12567064,  1.21474122]), array([-0.85548127,  1.4317303 , -0.16125466, -0.2956533 ]), array([-0.78596506,  1.22256642,  0.85456915, -1.80030174]), array([-0.51890338,  0.71044534,  1.78381836, -3.29425484]), array([-0.09990344, -0.05221658,  2.28989474, -4.10762373]), array([ 0.35116054, -0.84599361,  2.09791674, -3.59052948]), array([ 0.69632703, -1.40921863,  1.3141406 , -2.01847291]), array([ 0.87520264, -1.68113463,  0.45557265, -0.70749933]), array([ 0.86631032, -1.67036368, -0.5432254 ,  0.81570413]), array([ 0.66193002, -1.35092612, -1.48201684,  2.3924269 ]), array([ 0.28490023, -0.71162546, -2.2395859 ,  3.95390526]), array([-0.20839929,  0.19679377, -2.54067354,  4.81706123]), array([-0.66216882,  1.07233681, -1.88792462,  3.7396891 ]), array([-0.94269511,  1.67127203, -0.89582397,  2.25978607]), array([-1.00923607,  1.96115643,  0.22523491,  0.65503256]), array([-0.85849891,  1.93423117,  1.25595096, -0.93084769]), array([-0.51414348,  1.56014512,  2.14463579, -2.83039115]), array([-0.02873872,  0.82554876,  2.65001027, -4.45684366]), array([ 0.50364526, -0.14287035,  2.51377621, -4.88484545]), array([ 0.92260916, -1.02254172,  1.57574847, -3.73351044]), array([ 1.11666087, -1.62012083,  0.35262428, -2.2509355 ]), array([ 1.05734775, -1.90276551, -0.92346508, -0.57580591]), array([ 0.76202365, -1.84577486, -1.97685907,  1.15916579]), array([ 0.29410472, -1.43635402, -2.62774306,  2.92309146]), array([-0.2689444 , -0.6675149 , -2.92465166,  4.65052403]), array([-0.82622767,  0.31746262, -2.48961182,  4.84658498]), array([-1.19878515,  1.13088664, -1.18181001,  3.21568988]), array([-1.29346298,  1.60882412,  0.23311636,  1.57571905]), array([-1.11062449,  1.75664283,  1.56825514, -0.12806691]), array([-0.68446351,  1.54201064,  2.62926782, -2.04960988]), array([-0.08103498,  0.90713073,  3.322727  , -4.25230692]), array([ 0.5989301 , -0.08114888,  3.30602015, -5.24623986]), array([ 1.16661973, -1.02271352,  2.26530913, -3.97130441]), array([ 1.48136618, -1.64023148,  0.8803865 , -2.26461588]), array([ 1.51956947, -1.94439236, -0.49443241, -0.78158844]), array([ 1.28709045, -1.94264534, -1.81185776,  0.8467923 ]), array([ 0.80085306, -1.55724148, -3.00227345,  3.08023961]), array([ 0.11920844, -0.71803287, -3.73198577,  5.23557462]), array([-0.62678377,  0.39922874, -3.5046022 ,  5.41513183]), array([-1.21212773,  1.29367686, -2.28711583,  3.45890643]), array([-1.53714571,  1.80979565, -0.96199206,  1.77646606]), array([-1.59715177,  2.02212893,  0.36033486,  0.35740489]), array([-1.3945176 ,  1.94500321,  1.65676187, -1.17391882]), array([-0.94225259,  1.5258666 ,  2.83469376, -3.09595637]), array([-0.26755876,  0.65319122,  3.8476    , -5.59154202]), array([ 0.5148857 , -0.52905453,  3.72935336, -5.64856172]), array([ 1.15145455, -1.44728039,  2.57755581, -3.48647119]), array([ 1.5483901 , -1.98097149,  1.38174653, -1.92985136]), array([ 1.69523707, -2.22054043,  0.08739645, -0.49644903]), array([ 1.58383833, -2.18017306, -1.19920009,  0.92481353]), array([ 1.21105837, -1.80813366, -2.51511337,  2.87997213]), array([ 0.58528802, -0.98416021, -3.71972602,  5.44553886]), array([-0.23895945,  0.30996755, -4.26852721,  6.88891349]), array([-0.99870286,  1.47208223, -3.22204345,  4.54176161]), array([-1.52895444,  2.18602155, -2.06730793,  2.70866039]), array([-1.81636397,  2.56981095, -0.80972046,  1.18535351]), array([-1.86124936,  2.69046132,  0.35821273,  0.02448989]), array([-1.66011961,  2.53432564,  1.65622088, -1.61890725]), array([-1.206525  ,  2.0401093 ,  2.86205975, -3.41282644]), array([-0.52612466,  1.12222783,  3.91664281, -5.86507568]), array([ 0.32392677, -0.25004872,  4.31925787, -7.21727202]), array([ 1.0926241 , -1.50290924,  3.24640959, -5.07925828]), array([ 1.61091204, -2.29963209,  1.94322245, -3.03023626]), array([ 1.87244836, -2.75194912,  0.68268916, -1.5392625 ]), array([ 1.89408037, -2.94103759, -0.46184529, -0.34800947]), array([ 1.68064881, -2.86595647, -1.67865989,  1.1217451 ]), array([ 1.22321527, -2.47791598, -2.87083969,  2.81728049]), array([ 0.55407408, -1.70545782, -3.75858123,  5.00856344]), array([-0.26002879, -0.45091149, -4.28146712,  7.33421467]), array([-1.04683819,  0.95108059, -3.33155513,  6.08604831]), array([-1.56902502,  1.96030327, -1.89433575,  4.1155315 ]), array([-1.80429807,  2.61920308, -0.48181524,  2.53428498]), array([-1.77057119,  2.9801797 ,  0.80369847,  1.06867378]), array([-1.48482792,  3.04139078,  2.05207412, -0.46760388]), array([-0.95553456,  2.78992496,  3.19139697, -2.0575806 ]), array([-0.2486246 ,  2.21216274,  3.74098674, -3.73410726]), array([ 0.48815901,  1.30184696,  3.5482951 , -5.30685942]), array([ 1.14627702,  0.15537761,  2.92636953, -5.84793582]), array([ 1.61155386, -0.92580971,  1.62113158, -4.76800748]), array([ 1.76569841, -1.71315384, -0.09185155, -3.12836704]), array([ 1.5742639 , -2.17037993, -1.80620024, -1.38903595]), array([ 1.05928212, -2.24134943, -3.27139461,  0.7428187 ]), array([ 0.31171105, -1.85710694, -4.05736381,  3.10360182]), array([-0.50389581, -1.023557  , -3.98616527,  5.08274138]), array([-1.25134232,  0.09088564, -3.35387467,  5.66441923]), array([-1.78260088,  1.07662374, -1.92016629,  4.12608173]), array([-2.02175976,  1.76818487, -0.4781807 ,  2.85012537]), array([-1.973225  ,  2.22083367,  0.96714353,  1.64067711]), array([-1.63451576,  2.3978481 ,  2.41276316,  0.04564555]), array([-1.01294702,  2.1824154 ,  3.7359775 , -2.29551327]), array([-0.19028814,  1.46951472,  4.37805793, -4.86522983]), array([ 0.70896602,  0.24385479,  4.47026146, -7.00784024]), array([ 1.48691947, -1.0294052 ,  3.15738562, -5.34258539]), array([ 1.96939668, -1.90680348,  1.70314701, -3.57959509]), array([ 2.18682562, -2.52368754,  0.49380762, -2.62904107]), array([ 2.1700267 , -2.93849288, -0.64236094, -1.49753676]), array([ 1.93120803, -3.10897217, -1.7584188 , -0.17111728]), array([ 1.45260677, -2.97370995, -3.03610418,  1.5594047 ]), array([ 0.72982771, -2.46658121, -4.09519131,  3.58181668]), array([-0.12980157, -1.51046601, -4.40183614,  6.03235301]), array([-0.99695448, -0.11540541, -4.12012063,  7.46650542]), array([-1.67857543,  1.21466866, -2.57304734,  5.56948546]), array([-2.03687344,  2.17409645, -1.03285846,  4.13586217]), array([-2.10497988,  2.890526  ,  0.3007167 ,  3.03611693]), array([-1.9309155 , -2.91975373,  1.41061769,  1.6808197 ]), array([-1.54055366, -2.71999664,  2.50717658,  0.3442922 ]), array([-0.92631305, -2.75744878,  3.60634771, -0.6160101 ]), array([-0.12433634, -2.93370104,  4.28002136, -0.99348397]), array([ 0.71128989, -3.07550537,  3.91500372, -0.28135073]), array([ 1.39193818, -2.99750029,  2.81033791,  1.15218197]), array([ 1.81261199, -2.59528471,  1.33523747,  2.8806083 ]), array([ 1.90032008, -1.85025714, -0.50538055,  4.56932453]), array([ 1.60316674, -0.74808948, -2.45026541,  6.52419839]), array([ 0.95548812,  0.72977875, -3.78150848,  7.73079605]), array([ 0.17126816,  2.12831592, -4.04434391,  6.18223044]), array([-0.63594989, -3.04416068, -3.85667719,  5.0555903 ]), array([-1.3103789 , -2.07651325, -2.8219321 ,  4.65320536]), array([-1.7601921 , -1.21443744, -1.69952946,  3.92310976])]</t>
+  </si>
+  <si>
+    <t>['[2,1,0]', '[0,1,1]', '[2,0,1]', '[1,1,1]', '[1,1,2]', '[2,2,2]', '[1,0,2]', '[1,2,0]', '[0,2,1]', '[0,0,0]']</t>
+  </si>
+  <si>
+    <t>[1, 3, 4, 5, 6, 7, 8, 9, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 28, 30, 31, 32, 33, 35, 36, 37, 39, 40, 41, 42, 43, 44, 45, 46, 47, 49, 50, 51, 52, 54, 55, 56, 57, 58, 59, 60, 61, 62, 64, 65, 66, 67, 68, 69, 70, 71, 72, 73, 74, 75, 78, 79, 80, 81, 82, 83, 85, 86, 87, 88, 90, 91, 94, 95, 96, 97, 98, 100, 101, 102, 103, 104, 105, 108, 110, 111, 112, 113, 114, 115, 116, 118, 119, 122, 123, 124, 125, 126, 127, 128, 129, 130, 132, 133, 134, 135, 137, 138, 139, 140, 141, 142, 143, 144, 145, 146, 147, 149, 150, 151, 152, 154, 155, 156, 158, 159, 160, 161, 162, 163, 164, 166, 167, 168, 169, 172, 173, 174, 175, 176, 178, 179, 180, 181, 182, 184, 186, 189, 190, 191, 192, 193, 194, 195, 196, 197, 198, 199]</t>
+  </si>
+  <si>
+    <t>[0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 1, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0]</t>
+  </si>
+  <si>
+    <t>['[-0.03763371 -0.01533471  0.06554052 -0.01816017]', '[-0.0208055  -0.02030166  0.09914155 -0.02801351]', '[ 0.013578   -0.05917353  0.23628798 -0.34824344]', '[ 0.05569493 -0.11750576  0.17467028 -0.21881458]', '[ 0.08000939 -0.1414547   0.06300338 -0.0132271 ]', '[ 0.07979713 -0.12178323 -0.06434392  0.20630095]', '[ 0.05580503 -0.06252371 -0.16879726  0.37229918]', '[ 0.01598724  0.01983861 -0.21868287  0.43086528]', '[-0.02695317  0.10099205 -0.199548    0.36015587]', '[-0.05963054  0.15635839 -0.11909672  0.17938912]', '[-0.08534871  0.20285114 -0.13139485  0.27352487]', '[-0.10932994  0.26032413 -0.1018531   0.28785792]', '[-0.11069645  0.27905739  0.08863375 -0.10317969]', '[-0.07549994  0.22136157  0.25454554 -0.45895732]', '[-0.01405167  0.10464955  0.34397071 -0.67890245]', '[ 0.05469695 -0.03635355  0.32509496 -0.69591252]', '[ 0.10878573 -0.15972156  0.20122653 -0.50865465]', '[ 0.13063095 -0.23034014  0.01115232 -0.18316174]', '[ 0.11263511 -0.23037751 -0.18720383  0.17969031]', '[ 0.05917853 -0.1630268  -0.33450188  0.47434955]', '[-0.01454614 -0.05126067 -0.38432536  0.61262161]', '[-0.08662817  0.06848021 -0.3182054   0.55296535]', '[-0.13516117  0.15814149 -0.1548771   0.32149261]', '[-0.14524601  0.19076325  0.05669027 -0.00167653]', '[-0.11337184  0.15809373  0.25447944 -0.31450001]', '[-0.04833647  0.07229738  0.38000633 -0.51870746]', '[ 0.04432143 -0.07160354  0.52297236 -0.88027534]', '[ 0.14983706 -0.26043183  0.50465918 -0.95849496]', '[ 0.2226379  -0.40214718  0.20620131 -0.42793175]', '[ 0.24104342 -0.45746331 -0.02673891 -0.1149277 ]', '[ 0.19945602 -0.4139069  -0.3798121   0.53857707]', '[ 0.09597258 -0.25226366 -0.63042082  1.0379101 ]', '[-0.04007224 -0.02036562 -0.69499743  1.21901651]', '[-0.16717042  0.20855874 -0.54311464  1.01072027]', '[-0.25895948  0.39711678 -0.35125151  0.83094712]', '[-0.28770025  0.49368811  0.07020994  0.11933226]', '[-0.23186126  0.44419311  0.47608708 -0.60035972]', '[-0.10563133  0.26513503  0.75689974 -1.14496838]', '[ 0.06919187 -0.02334352  0.94655205 -1.66106315]', '[ 0.23935166 -0.32792502  0.71150494 -1.30618014]', '[ 0.33970274 -0.52108967  0.26996615 -0.58762353]', '[ 0.34261712 -0.55463244 -0.24101347  0.25556363]', '[ 0.24714524 -0.42321247 -0.69327235  1.03025706]', '[ 0.07781028 -0.16166431 -0.95917668  1.5175908 ]', '[-0.11671148  0.14949016 -0.93566141  1.5052879 ]', '[-0.27702412  0.40661643 -0.62932676  1.00215258]', '[-0.35687787  0.53206033 -0.1528519   0.22805601]', '[-0.33555505  0.49420246  0.36121958 -0.59910357]', '[-0.2056182   0.26823274  0.90930926 -1.61355829]', '[-0.00298776 -0.08549177  1.06318424 -1.82571784]', '[ 0.19661772 -0.42010096  0.88295814 -1.43265413]', '[ 0.33358269 -0.63128206  0.45844801 -0.6375187 ]', '[ 0.37262681 -0.66566295 -0.07508178  0.30006292]', '[ 0.29209536 -0.48163009 -0.71533069  1.51433119]', '[ 0.11181513 -0.11555707 -1.0405502   2.05870593]', '[-0.10052608  0.29670804 -1.02370935  1.95092945]', '[-0.27594153  0.62455344 -0.69062902  1.25836442]', '[-0.36541118  0.78219201 -0.18822148  0.29588255]', '[-0.34847199  0.73957002  0.35453055 -0.71676837]', '[-0.22856874  0.50301025  0.82045218 -1.60980825]', '[-0.03530241  0.12191492  1.06201016 -2.10766747]', '[ 0.17195373 -0.29341538  0.95230343 -1.93331638]', '[ 0.32516423 -0.6128901   0.54482528 -1.19803187]', '[ 0.39272329 -0.78819406  0.11747632 -0.5298148 ]', '[ 0.35886806 -0.7891737  -0.44859497  0.51620901]', '[ 0.21991192 -0.58826232 -0.91410954  1.45820599]', '[ 0.00873348 -0.22957532 -1.14724962  2.04165693]', '[-0.21438087  0.1830757  -1.0227225   1.96941738]', '[-0.37803539  0.51643095 -0.57450694  1.29222304]', '[-0.43399174  0.68158792  0.02512196  0.33776886]', '[-0.36847887  0.64902302  0.61698383 -0.65402069]', '[-0.19679711  0.43017426  1.06402599 -1.48670761]', '[ 0.03766818  0.08427621  1.22274651 -1.87462396]', '[ 0.26653927 -0.27433637  1.00772814 -1.60940968]', '[ 0.4209412  -0.52602465  0.5029095  -0.85464045]', '[ 0.45937972 -0.603778   -0.12532488  0.08791625]', '[ 0.36015089 -0.45964565 -0.84806603  1.32946847]', '[ 0.13414444 -0.09277547 -1.35811813  2.2479118 ]', '[-0.14088286  0.35264992 -1.31957908  2.07461251]', '[-0.36751186  0.6920956  -0.89895609  1.24764158]', '[-0.48665138  0.83454819 -0.27199633  0.15775806]', '[-0.47221463  0.75284637  0.41468106 -0.96766611]', '[-0.32616237  0.45608815  1.01688896 -1.95315693]', '[-0.08446481  0.00473349  1.33566314 -2.44082233]', '[ 0.19045441 -0.49556924  1.33741092 -2.41838535]', '[ 0.41180622 -0.88364705  0.83460933 -1.40043905]', '[ 0.51346411 -1.04333231  0.16757993 -0.18454153]', '[ 0.47661593 -0.95620713 -0.53164931  1.05069095]', '[ 0.30658957 -0.62937147 -1.14014505  2.17842925]', '[ 0.02668088 -0.08274021 -1.58750417  3.15460106]', '[-0.27649591  0.52199145 -1.35658292  2.72171243]', '[-0.4896245   0.9584501  -0.73748344  1.58557163]', '[-0.57396121  1.17496918 -0.09572158  0.56631603]', '[-0.50759937  1.12776895  0.74785787 -1.03578942]', '[-0.29354894  0.79291385  1.36017676 -2.28081673]', '[ 0.01651059  0.24398922  1.66773881 -3.07917562]', '[ 0.33517341 -0.36438152  1.42562522 -2.82188431]', '[ 0.55647111 -0.82836382  0.74317431 -1.74392232]', '[ 0.62338131 -1.04879237 -0.0796149  -0.44953478]', '[ 0.5164517  -0.97822919 -0.97160457  1.15101563]', '[ 0.25780688 -0.6252439  -1.5697745   2.32813326]', '[-0.08513951 -0.08712987 -1.77385546  2.89895907]', '[-0.41193278  0.45890164 -1.40867237  2.40348104]', '[-0.6229715   0.8313513  -0.66471223  1.26954021]', '[-0.67001428  0.95806438  0.19891931 -0.00883009]', '[-0.54608835  0.82777146  1.02121411 -1.28425321]', '[-0.26253267  0.42350326  1.76325933 -2.69316004]', '[ 0.12674561 -0.19470104  2.02308387 -3.28732661]', '[ 0.48848537 -0.77150005  1.51351424 -2.34361215]', '[ 0.72200946 -1.1344334   0.78723367 -1.2548585 ]', '[ 0.7851327  -1.24223686 -0.16172379  0.17549027]', '[ 0.65885648 -1.06380417 -1.08642348  1.60863572]', '[ 0.36142352 -0.60350089 -1.84133112  2.9431494 ]', '[-0.04637805  0.06272653 -2.12682979  3.51064866]', '[-0.43945098  0.70300811 -1.70705048  2.71589513]', '[-0.70324286  1.11138622 -0.89436995  1.33682598]', '[-0.78870449  1.23564615  0.04865972 -0.09275094]', '[-0.67370298  1.04606313  1.09147651 -1.80785218]', '[-0.37271159  0.54542469  1.87014902 -3.13960817]', '[ 0.04062323 -0.15209115  2.14670506 -3.60958342]', '[ 0.44769998 -0.83069863  1.82346827 -2.99275739]', '[ 0.74265832 -1.30988127  1.08621372 -1.76738878]', '[ 0.86305193 -1.51071733  0.10782153 -0.24929061]', '[ 0.78532117 -1.41035963 -0.8766793   1.25791187]', '[ 0.51941432 -1.00400427 -1.75367637  2.80276757]', '[ 0.10339386 -0.30792204 -2.32019832  4.01299845]', '[-0.35478444  0.4942098  -2.12296283  3.72847716]', '[-0.70348748  1.10559972 -1.30879397  2.31280795]', '[-0.86703954  1.41490896 -0.31421687  0.78724446]', '[-0.82809356  1.42250769  0.69639255 -0.71313866]', '[-0.59517106  1.12647676  1.60594499 -2.2510112 ]', '[-0.19036931  0.49886491  2.37928905 -3.94555135]', '[ 0.29704583 -0.33069901  2.34652653 -4.04702217]', '[ 0.69556036 -1.01670555  1.5643369  -2.69707777]', '[ 0.907831   -1.39930918  0.54128214 -1.13636778]', '[ 0.90953115 -1.47495342 -0.52060767  0.37891752]', '[ 0.69536914 -1.21784109 -1.60015013  2.21028906]', '[ 0.29334456 -0.61791862 -2.36102618  3.72555479]', '[-0.20705385  0.19846957 -2.49777451  4.14495383]', '[-0.64688924  0.92147753 -1.80728072  2.92470055]', '[-0.90993978  1.34867088 -0.79876821  1.34987969]', '[-0.96149427  1.46635708  0.28528555 -0.16756891]', '[-0.79862443  1.27939491  1.32656762 -1.71460944]', '[-0.44200473  0.77684962  2.19490168 -3.28524179]', '[ 0.04767156  0.01087452  2.57614028 -4.133795  ]', '[ 0.52639014 -0.75014376  2.0903981  -3.24753232]', '[ 0.85410934 -1.24575368  1.14874314 -1.68937781]', '[ 0.97733579 -1.42993223  0.07371483 -0.16334407]', '[ 0.87378991 -1.28535052 -1.10160441  1.62226459]', '[ 0.55395178 -0.8018566  -2.06113636  3.20003491]', '[ 0.0767516  -0.04160989 -2.59268427  4.1808595 ]', '[-0.42049956  0.7425332  -2.24972513  3.40820453]', '[-0.7891779   1.26990532 -1.39056027  1.83540351]', '[-0.97447168  1.50564728 -0.44288883  0.5312612 ]', '[-0.95355017  1.45980498  0.65088484 -0.99191907]', '[-0.71817447  1.10355916  1.68235487 -2.58397281]', '[-0.29546848  0.43134047  2.47316781 -4.03820945]', '[ 0.23268835 -0.44663303  2.64566209 -4.40440973]', '[ 0.69295217 -1.18449068  1.88167023 -2.86758256]', '[ 0.96959699 -1.59026373  0.86172588 -1.21100205]', '[ 1.03191721 -1.67669028 -0.24340162  0.33884443]', '[ 0.8737978  -1.45223113 -1.32475651  1.92364724]', '[ 0.51090529 -0.8983889  -2.267985    3.61167515]', '[-0.00489106 -0.04474192 -2.75859464  4.67004003]', '[-0.5218771   0.82144001 -2.27416683  3.72144151]', '[-0.89360038  1.42599903 -1.40013184  2.30080976]', '[-1.06338069  1.72305046 -0.28775307  0.69219038]', '[-1.00798972  1.70640649  0.83403152 -0.86459113]', '[-0.73656894  1.36954002  1.85424565 -2.52861136]', '[-0.28096158  0.6901645   2.64295708 -4.21166648]', '[ 0.28794593 -0.26637825  2.87273956 -4.98826808]', '[ 0.7956997  -1.15354663  2.10145494 -3.70535122]', '[ 1.10131447 -1.71370833  0.94060753 -1.93575714]', '[ 1.169425   -1.94082252 -0.25818191 -0.34870146]', '[ 1.00207085 -1.85123158 -1.3947453   1.26373927]', '[ 0.62426696 -1.42348969 -2.34316638  3.04312414]', '[ 0.08465354 -0.63241347 -2.97821829  4.77581411]', '[-0.52261016  0.40472869 -2.90056352  5.17278634]', '[-0.99711105  1.26926962 -1.77854813  3.38734431]', '[-1.22650395  1.77188118 -0.51088653  1.67977284]', '[-1.20230084  1.94957602  0.74294659  0.09571724]', '[-0.93744918  1.80248124  1.87269125 -1.59690221]', '[-0.47159456  1.29718638  2.73244793 -3.47610792]', '[ 0.1406085   0.39536929  3.28845787 -5.3678185 ]', '[ 0.75581025 -0.65092532  2.67797578 -4.69116024]', '[ 1.17958237 -1.43338332  1.51912733 -3.11464792]', '[ 1.34979017 -1.88793056  0.18402999 -1.46733244]', '[ 1.25579067 -2.02373441 -1.10948821  0.12417056]', '[ 0.90937057 -1.80300983 -2.31357432  2.12898636]', '[ 0.35998329 -1.17744045 -3.12095332  4.14067713]', '[-0.30643559 -0.18192473 -3.39758719  5.5110481 ]', '[-0.91448087  0.83498313 -2.52644633  4.32934353]', '[-1.29053534  1.51575064 -1.2185702   2.51668417]', '[-1.40076386  1.86096831  0.11453739  0.95793402]', '[-1.24754503  1.89655525  1.40212823 -0.63096074]', '[-0.8511152   1.59047763  2.52055687 -2.48112316]', '[-0.26102074  0.88862547  3.3129639  -4.51108523]', '[ 0.42708242 -0.13323111  3.37896115 -5.28790886]', '[ 1.0105353  -1.0485403   2.34898076 -3.6732282 ]', '[ 1.35260999 -1.60317666  1.06204272 -1.92856385]']</t>
+  </si>
+  <si>
+    <t>[array([-0.03763371, -0.01533471,  0.06554052, -0.01816017], dtype=float32), array([-0.0208055 , -0.02030166,  0.09914155, -0.02801351]), array([ 0.013578  , -0.05917353,  0.23628798, -0.34824344]), array([ 0.05569493, -0.11750576,  0.17467028, -0.21881458]), array([ 0.08000939, -0.1414547 ,  0.06300338, -0.0132271 ]), array([ 0.07979713, -0.12178323, -0.06434392,  0.20630095]), array([ 0.05580503, -0.06252371, -0.16879726,  0.37229918]), array([ 0.01598724,  0.01983861, -0.21868287,  0.43086528]), array([-0.02695317,  0.10099205, -0.199548  ,  0.36015587]), array([-0.05963054,  0.15635839, -0.11909672,  0.17938912]), array([-0.08534871,  0.20285114, -0.13139485,  0.27352487]), array([-0.10932994,  0.26032413, -0.1018531 ,  0.28785792]), array([-0.11069645,  0.27905739,  0.08863375, -0.10317969]), array([-0.07549994,  0.22136157,  0.25454554, -0.45895732]), array([-0.01405167,  0.10464955,  0.34397071, -0.67890245]), array([ 0.05469695, -0.03635355,  0.32509496, -0.69591252]), array([ 0.10878573, -0.15972156,  0.20122653, -0.50865465]), array([ 0.13063095, -0.23034014,  0.01115232, -0.18316174]), array([ 0.11263511, -0.23037751, -0.18720383,  0.17969031]), array([ 0.05917853, -0.1630268 , -0.33450188,  0.47434955]), array([-0.01454614, -0.05126067, -0.38432536,  0.61262161]), array([-0.08662817,  0.06848021, -0.3182054 ,  0.55296535]), array([-0.13516117,  0.15814149, -0.1548771 ,  0.32149261]), array([-0.14524601,  0.19076325,  0.05669027, -0.00167653]), array([-0.11337184,  0.15809373,  0.25447944, -0.31450001]), array([-0.04833647,  0.07229738,  0.38000633, -0.51870746]), array([ 0.04432143, -0.07160354,  0.52297236, -0.88027534]), array([ 0.14983706, -0.26043183,  0.50465918, -0.95849496]), array([ 0.2226379 , -0.40214718,  0.20620131, -0.42793175]), array([ 0.24104342, -0.45746331, -0.02673891, -0.1149277 ]), array([ 0.19945602, -0.4139069 , -0.3798121 ,  0.53857707]), array([ 0.09597258, -0.25226366, -0.63042082,  1.0379101 ]), array([-0.04007224, -0.02036562, -0.69499743,  1.21901651]), array([-0.16717042,  0.20855874, -0.54311464,  1.01072027]), array([-0.25895948,  0.39711678, -0.35125151,  0.83094712]), array([-0.28770025,  0.49368811,  0.07020994,  0.11933226]), array([-0.23186126,  0.44419311,  0.47608708, -0.60035972]), array([-0.10563133,  0.26513503,  0.75689974, -1.14496838]), array([ 0.06919187, -0.02334352,  0.94655205, -1.66106315]), array([ 0.23935166, -0.32792502,  0.71150494, -1.30618014]), array([ 0.33970274, -0.52108967,  0.26996615, -0.58762353]), array([ 0.34261712, -0.55463244, -0.24101347,  0.25556363]), array([ 0.24714524, -0.42321247, -0.69327235,  1.03025706]), array([ 0.07781028, -0.16166431, -0.95917668,  1.5175908 ]), array([-0.11671148,  0.14949016, -0.93566141,  1.5052879 ]), array([-0.27702412,  0.40661643, -0.62932676,  1.00215258]), array([-0.35687787,  0.53206033, -0.1528519 ,  0.22805601]), array([-0.33555505,  0.49420246,  0.36121958, -0.59910357]), array([-0.2056182 ,  0.26823274,  0.90930926, -1.61355829]), array([-0.00298776, -0.08549177,  1.06318424, -1.82571784]), array([ 0.19661772, -0.42010096,  0.88295814, -1.43265413]), array([ 0.33358269, -0.63128206,  0.45844801, -0.6375187 ]), array([ 0.37262681, -0.66566295, -0.07508178,  0.30006292]), array([ 0.29209536, -0.48163009, -0.71533069,  1.51433119]), array([ 0.11181513, -0.11555707, -1.0405502 ,  2.05870593]), array([-0.10052608,  0.29670804, -1.02370935,  1.95092945]), array([-0.27594153,  0.62455344, -0.69062902,  1.25836442]), array([-0.36541118,  0.78219201, -0.18822148,  0.29588255]), array([-0.34847199,  0.73957002,  0.35453055, -0.71676837]), array([-0.22856874,  0.50301025,  0.82045218, -1.60980825]), array([-0.03530241,  0.12191492,  1.06201016, -2.10766747]), array([ 0.17195373, -0.29341538,  0.95230343, -1.93331638]), array([ 0.32516423, -0.6128901 ,  0.54482528, -1.19803187]), array([ 0.39272329, -0.78819406,  0.11747632, -0.5298148 ]), array([ 0.35886806, -0.7891737 , -0.44859497,  0.51620901]), array([ 0.21991192, -0.58826232, -0.91410954,  1.45820599]), array([ 0.00873348, -0.22957532, -1.14724962,  2.04165693]), array([-0.21438087,  0.1830757 , -1.0227225 ,  1.96941738]), array([-0.37803539,  0.51643095, -0.57450694,  1.29222304]), array([-0.43399174,  0.68158792,  0.02512196,  0.33776886]), array([-0.36847887,  0.64902302,  0.61698383, -0.65402069]), array([-0.19679711,  0.43017426,  1.06402599, -1.48670761]), array([ 0.03766818,  0.08427621,  1.22274651, -1.87462396]), array([ 0.26653927, -0.27433637,  1.00772814, -1.60940968]), array([ 0.4209412 , -0.52602465,  0.5029095 , -0.85464045]), array([ 0.45937972, -0.603778  , -0.12532488,  0.08791625]), array([ 0.36015089, -0.45964565, -0.84806603,  1.32946847]), array([ 0.13414444, -0.09277547, -1.35811813,  2.2479118 ]), array([-0.14088286,  0.35264992, -1.31957908,  2.07461251]), array([-0.36751186,  0.6920956 , -0.89895609,  1.24764158]), array([-0.48665138,  0.83454819, -0.27199633,  0.15775806]), array([-0.47221463,  0.75284637,  0.41468106, -0.96766611]), array([-0.32616237,  0.45608815,  1.01688896, -1.95315693]), array([-0.08446481,  0.00473349,  1.33566314, -2.44082233]), array([ 0.19045441, -0.49556924,  1.33741092, -2.41838535]), array([ 0.41180622, -0.88364705,  0.83460933, -1.40043905]), array([ 0.51346411, -1.04333231,  0.16757993, -0.18454153]), array([ 0.47661593, -0.95620713, -0.53164931,  1.05069095]), array([ 0.30658957, -0.62937147, -1.14014505,  2.17842925]), array([ 0.02668088, -0.08274021, -1.58750417,  3.15460106]), array([-0.27649591,  0.52199145, -1.35658292,  2.72171243]), array([-0.4896245 ,  0.9584501 , -0.73748344,  1.58557163]), array([-0.57396121,  1.17496918, -0.09572158,  0.56631603]), array([-0.50759937,  1.12776895,  0.74785787, -1.03578942]), array([-0.29354894,  0.79291385,  1.36017676, -2.28081673]), array([ 0.01651059,  0.24398922,  1.66773881, -3.07917562]), array([ 0.33517341, -0.36438152,  1.42562522, -2.82188431]), array([ 0.55647111, -0.82836382,  0.74317431, -1.74392232]), array([ 0.62338131, -1.04879237, -0.0796149 , -0.44953478]), array([ 0.5164517 , -0.97822919, -0.97160457,  1.15101563]), array([ 0.25780688, -0.6252439 , -1.5697745 ,  2.32813326]), array([-0.08513951, -0.08712987, -1.77385546,  2.89895907]), array([-0.41193278,  0.45890164, -1.40867237,  2.40348104]), array([-0.6229715 ,  0.8313513 , -0.66471223,  1.26954021]), array([-0.67001428,  0.95806438,  0.19891931, -0.00883009]), array([-0.54608835,  0.82777146,  1.02121411, -1.28425321]), array([-0.26253267,  0.42350326,  1.76325933, -2.69316004]), array([ 0.12674561, -0.19470104,  2.02308387, -3.28732661]), array([ 0.48848537, -0.77150005,  1.51351424, -2.34361215]), array([ 0.72200946, -1.1344334 ,  0.78723367, -1.2548585 ]), array([ 0.7851327 , -1.24223686, -0.16172379,  0.17549027]), array([ 0.65885648, -1.06380417, -1.08642348,  1.60863572]), array([ 0.36142352, -0.60350089, -1.84133112,  2.9431494 ]), array([-0.04637805,  0.06272653, -2.12682979,  3.51064866]), array([-0.43945098,  0.70300811, -1.70705048,  2.71589513]), array([-0.70324286,  1.11138622, -0.89436995,  1.33682598]), array([-0.78870449,  1.23564615,  0.04865972, -0.09275094]), array([-0.67370298,  1.04606313,  1.09147651, -1.80785218]), array([-0.37271159,  0.54542469,  1.87014902, -3.13960817]), array([ 0.04062323, -0.15209115,  2.14670506, -3.60958342]), array([ 0.44769998, -0.83069863,  1.82346827, -2.99275739]), array([ 0.74265832, -1.30988127,  1.08621372, -1.76738878]), array([ 0.86305193, -1.51071733,  0.10782153, -0.24929061]), array([ 0.78532117, -1.41035963, -0.8766793 ,  1.25791187]), array([ 0.51941432, -1.00400427, -1.75367637,  2.80276757]), array([ 0.10339386, -0.30792204, -2.32019832,  4.01299845]), array([-0.35478444,  0.4942098 , -2.12296283,  3.72847716]), array([-0.70348748,  1.10559972, -1.30879397,  2.31280795]), array([-0.86703954,  1.41490896, -0.31421687,  0.78724446]), array([-0.82809356,  1.42250769,  0.69639255, -0.71313866]), array([-0.59517106,  1.12647676,  1.60594499, -2.2510112 ]), array([-0.19036931,  0.49886491,  2.37928905, -3.94555135]), array([ 0.29704583, -0.33069901,  2.34652653, -4.04702217]), array([ 0.69556036, -1.01670555,  1.5643369 , -2.69707777]), array([ 0.907831  , -1.39930918,  0.54128214, -1.13636778]), array([ 0.90953115, -1.47495342, -0.52060767,  0.37891752]), array([ 0.69536914, -1.21784109, -1.60015013,  2.21028906]), array([ 0.29334456, -0.61791862, -2.36102618,  3.72555479]), array([-0.20705385,  0.19846957, -2.49777451,  4.14495383]), array([-0.64688924,  0.92147753, -1.80728072,  2.92470055]), array([-0.90993978,  1.34867088, -0.79876821,  1.34987969]), array([-0.96149427,  1.46635708,  0.28528555, -0.16756891]), array([-0.79862443,  1.27939491,  1.32656762, -1.71460944]), array([-0.44200473,  0.77684962,  2.19490168, -3.28524179]), array([ 0.04767156,  0.01087452,  2.57614028, -4.133795  ]), array([ 0.52639014, -0.75014376,  2.0903981 , -3.24753232]), array([ 0.85410934, -1.24575368,  1.14874314, -1.68937781]), array([ 0.97733579, -1.42993223,  0.07371483, -0.16334407]), array([ 0.87378991, -1.28535052, -1.10160441,  1.62226459]), array([ 0.55395178, -0.8018566 , -2.06113636,  3.20003491]), array([ 0.0767516 , -0.04160989, -2.59268427,  4.1808595 ]), array([-0.42049956,  0.7425332 , -2.24972513,  3.40820453]), array([-0.7891779 ,  1.26990532, -1.39056027,  1.83540351]), array([-0.97447168,  1.50564728, -0.44288883,  0.5312612 ]), array([-0.95355017,  1.45980498,  0.65088484, -0.99191907]), array([-0.71817447,  1.10355916,  1.68235487, -2.58397281]), array([-0.29546848,  0.43134047,  2.47316781, -4.03820945]), array([ 0.23268835, -0.44663303,  2.64566209, -4.40440973]), array([ 0.69295217, -1.18449068,  1.88167023, -2.86758256]), array([ 0.96959699, -1.59026373,  0.86172588, -1.21100205]), array([ 1.03191721, -1.67669028, -0.24340162,  0.33884443]), array([ 0.8737978 , -1.45223113, -1.32475651,  1.92364724]), array([ 0.51090529, -0.8983889 , -2.267985  ,  3.61167515]), array([-0.00489106, -0.04474192, -2.75859464,  4.67004003]), array([-0.5218771 ,  0.82144001, -2.27416683,  3.72144151]), array([-0.89360038,  1.42599903, -1.40013184,  2.30080976]), array([-1.06338069,  1.72305046, -0.28775307,  0.69219038]), array([-1.00798972,  1.70640649,  0.83403152, -0.86459113]), array([-0.73656894,  1.36954002,  1.85424565, -2.52861136]), array([-0.28096158,  0.6901645 ,  2.64295708, -4.21166648]), array([ 0.28794593, -0.26637825,  2.87273956, -4.98826808]), array([ 0.7956997 , -1.15354663,  2.10145494, -3.70535122]), array([ 1.10131447, -1.71370833,  0.94060753, -1.93575714]), array([ 1.169425  , -1.94082252, -0.25818191, -0.34870146]), array([ 1.00207085, -1.85123158, -1.3947453 ,  1.26373927]), array([ 0.62426696, -1.42348969, -2.34316638,  3.04312414]), array([ 0.08465354, -0.63241347, -2.97821829,  4.77581411]), array([-0.52261016,  0.40472869, -2.90056352,  5.17278634]), array([-0.99711105,  1.26926962, -1.77854813,  3.38734431]), array([-1.22650395,  1.77188118, -0.51088653,  1.67977284]), array([-1.20230084,  1.94957602,  0.74294659,  0.09571724]), array([-0.93744918,  1.80248124,  1.87269125, -1.59690221]), array([-0.47159456,  1.29718638,  2.73244793, -3.47610792]), array([ 0.1406085 ,  0.39536929,  3.28845787, -5.3678185 ]), array([ 0.75581025, -0.65092532,  2.67797578, -4.69116024]), array([ 1.17958237, -1.43338332,  1.51912733, -3.11464792]), array([ 1.34979017, -1.88793056,  0.18402999, -1.46733244]), array([ 1.25579067, -2.02373441, -1.10948821,  0.12417056]), array([ 0.90937057, -1.80300983, -2.31357432,  2.12898636]), array([ 0.35998329, -1.17744045, -3.12095332,  4.14067713]), array([-0.30643559, -0.18192473, -3.39758719,  5.5110481 ]), array([-0.91448087,  0.83498313, -2.52644633,  4.32934353]), array([-1.29053534,  1.51575064, -1.2185702 ,  2.51668417]), array([-1.40076386,  1.86096831,  0.11453739,  0.95793402]), array([-1.24754503,  1.89655525,  1.40212823, -0.63096074]), array([-0.8511152 ,  1.59047763,  2.52055687, -2.48112316]), array([-0.26102074,  0.88862547,  3.3129639 , -4.51108523]), array([ 0.42708242, -0.13323111,  3.37896115, -5.28790886]), array([ 1.0105353 , -1.0485403 ,  2.34898076, -3.6732282 ]), array([ 1.35260999, -1.60317666,  1.06204272, -1.92856385])]</t>
+  </si>
+  <si>
+    <t>['[1,0,2]', '[0,2,1]', '[2,2,2]', '[1,1,2]', '[0,1,1]', '[1,1,1]', '[2,1,0]', '[0,0,0]', '[1,2,0]', '[2,0,1]']</t>
   </si>
   <si>
     <t>[0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2]</t>
@@ -841,79 +835,79 @@
     <t>[array([-0.03763371, -0.01533471,  0.06554052, -0.01816017], dtype=float32), array([-0.0208055 , -0.02030166,  0.09914155, -0.02801351]), array([ 0.00031733, -0.02489487,  0.10765546, -0.0138725 ]), array([ 0.02044082, -0.02428802,  0.08954248,  0.02288616]), array([ 0.03470698, -0.01491644,  0.05056501,  0.07132823]), array([0.04000421, 0.0038992 , 0.00197135, 0.11431592]), array([ 0.0357442 ,  0.02924956, -0.04287984,  0.13410557]), array([ 0.02389303,  0.05513259, -0.0724118 ,  0.11843067]), array([ 0.00827151,  0.0740515 , -0.08006316,  0.06513577]), array([-0.00664229,  0.07925492, -0.06591977, -0.01622081]), array([-0.01703829,  0.06693573, -0.03635037, -0.10637005]), array([-0.02083887,  0.0377102 , -0.00183146, -0.18135846]), array([-0.01819393, -0.00310741,  0.02644173, -0.21931589]), array([-0.0112553 , -0.04661351,  0.04018081, -0.20717791]), array([-0.00330983, -0.08257268,  0.03658645, -0.14508251]), array([ 0.0024104 , -0.10215919,  0.01891064, -0.04666104]), array([ 0.00382015, -0.10033648, -0.00499775,  0.06469207]), array([ 0.00064351, -0.07722007, -0.02539101,  0.16195768]), array([-0.00551959, -0.03811088, -0.03377164,  0.22142738]), array([-0.01174627,  0.0078305 , -0.02581131,  0.22911312]), array([-0.01482841,  0.04999004, -0.00311123,  0.18480626]), array([-0.01246489,  0.07911924,  0.02710494,  0.10195664]), array([-0.00417355,  0.08968453,  0.05438991,  0.00327931]), array([ 0.00840543,  0.08106163,  0.06855001, -0.08601484]), array([ 0.02190299,  0.05733301,  0.06295851, -0.14509547]), array([ 0.0321837 ,  0.02584205,  0.03681891, -0.16284223]), array([ 0.03560428, -0.00505404, -0.00421667, -0.14034077]), array([ 0.03020079, -0.02836988, -0.04938897, -0.08972441]), array([ 0.01642725, -0.04029751, -0.08587168, -0.02970417]), array([-0.00281086, -0.04091095, -0.10259647,  0.020656  ]), array([-0.02286552, -0.03361943, -0.09365837,  0.04790331]), array([-0.03860246, -0.0236106 , -0.06024324,  0.04807679]), array([-0.04583902, -0.01583448, -0.01046864,  0.02730739]), array([-0.04253854, -0.01321526,  0.0428277 , -0.00097241]), array([-0.02940859, -0.0156797 ,  0.08568823, -0.02115895]), array([-0.00972652, -0.02030416,  0.1069775 , -0.02123067]), array([ 0.0115618 , -0.02251874,  0.10152992,  0.00272141]), array([ 0.02921079, -0.01796026,  0.07156041,  0.04472731]), array([ 0.03910994, -0.00433545,  0.02589999,  0.09061009]), array([ 0.03936403,  0.01735836, -0.02268767,  0.12255506]), array([ 0.03071193,  0.04269742, -0.06126398,  0.1251015 ]), array([ 0.01618133,  0.06487999, -0.08040737,  0.09068004]), array([ 0.00010594,  0.07668079, -0.07674355,  0.02287818]), array([-0.0131837 ,  0.07272569, -0.05361425, -0.06371658]), array([-0.02060331,  0.05138348, -0.0197783 , -0.14709165]), array([-0.0211313 ,  0.01567674,  0.01345636, -0.20383146]), array([-0.01595742, -0.02713289,  0.03588002, -0.21605443]), array([-0.00791991, -0.06726788,  0.0416368 , -0.17718674]), array([-0.00043664, -0.09500666,  0.03087284, -0.0943888 ]), array([ 0.00368075, -0.10331248,  0.0092639 ,  0.01327487]), array([ 0.00313947, -0.08974361, -0.01411794,  0.11992657]), array([-0.00144505, -0.05716425, -0.02977728,  0.19951988]), array([-0.00778071, -0.01308634, -0.03092317,  0.23267408]), array([-0.01270791,  0.0322519 , -0.01595928,  0.21216515]), array([-0.01335511,  0.06859784,  0.01069327,  0.14503302]), array([-0.00823671,  0.0883668 ,  0.03999569,  0.05017504]), array([ 0.00211231,  0.08846473,  0.06134931, -0.04751774]), array([ 0.01517587,  0.07078453,  0.06607816, -0.12419015]), array([ 0.02714322,  0.04134788,  0.050276  , -0.16327781]), array([ 0.0340405 ,  0.00839289,  0.01631596, -0.15958658]), array([ 0.03298704, -0.02003641, -0.02746573, -0.12005427]), array([ 0.02319311, -0.03828082, -0.06899738, -0.06084749]), array([ 0.00636558, -0.04438295, -0.09601157, -0.00178899]), array([-0.01363367, -0.04017883, -0.09977935,  0.03998938]), array([-0.03179555, -0.03021076, -0.07786554,  0.05519089]), array([-0.04334878, -0.01986825, -0.03504948,  0.0447342 ]), array([-0.0451149 , -0.01339839,  0.01788855,  0.01866292]), array([-0.03643197, -0.01245064,  0.06715665, -0.00793224]), array([-0.01937377, -0.01561984,  0.09983432, -0.02053767]), array([ 0.00180375, -0.01911687,  0.10753223, -0.01056562]), array([ 0.0218339 , -0.01833196,  0.08875656,  0.02131717]), array([ 0.03588828, -0.00975451,  0.04925111,  0.06506316]), array([0.04087756, 0.00742013, 0.0002166 , 0.1044091 ]), array([ 0.03622718,  0.03056533, -0.04501835,  0.12228182]), array([ 0.02391617,  0.05406225, -0.07485124,  0.10673119]), array([ 0.00778979,  0.07081926, -0.08263411,  0.0555052 ]), array([-0.00762885,  0.07443338, -0.06834211, -0.02229175]), array([-0.01846449,  0.06132984, -0.0382604 , -0.10807489]), array([-0.02256324,  0.0322086 , -0.00284167, -0.17867212]), array([-0.0200013 , -0.00768763,  0.02666696, -0.21296069]), array([-0.01287645, -0.04965999,  0.04182886, -0.19843477]), array([-0.00446197, -0.0837586 ,  0.03959053, -0.13546813]), array([ 0.00196551, -0.1014558 ,  0.02289045, -0.03759236]), array([ 0.00421606, -0.09796923, -0.00069219,  0.07211159]), array([ 0.001868  , -0.07359731, -0.02153986,  0.16700511]), array([-0.00363331, -0.03374808, -0.03111309,  0.22375043]), array([-0.00949554,  0.01238184, -0.02489133,  0.22869697]), array([-0.01259074,  0.05420419, -0.00417002,  0.18190922]), array([-0.01062875,  0.08254084,  0.02420456,  0.09700598]), array([-0.00306135,  0.09195204,  0.05016337, -0.00322466]), array([ 0.00860476,  0.08191813,  0.06379183, -0.09352245]), array([ 0.02117233,  0.05664052,  0.05855847, -0.15295683]), array([ 0.03067599,  0.0236076 ,  0.03355689, -0.17025318]), array([ 0.03360359, -0.00864806, -0.00582875, -0.14636478]), array([ 0.02805953, -0.03294971, -0.04918556, -0.09340991]), array([ 0.01449567, -0.04531199, -0.08403406, -0.03025985]), array([-0.00424834, -0.04568252, -0.09958545,  0.02367288]), array([-0.02363469, -0.03743116, -0.09009213,  0.05442078]), array([-0.03865607, -0.02582061, -0.05674925,  0.05740983]), array([-0.04524494, -0.01599859, -0.00755332,  0.03818015]), array([-0.04144682, -0.01119078,  0.04485592,  0.0097403 ]), array([-0.02800969, -0.0116828 ,  0.08673077, -0.01243954]), array([-0.00821291, -0.01490115,  0.10710228, -0.01611276]), array([ 0.01302167, -0.01654539,  0.10089613,  0.00320226]), array([ 0.03048279, -0.0123802 ,  0.0703412 ,  0.0403553 ]), array([ 4.00912900e-02, -6.54008926e-05,  2.42303589e-02,  8.20660574e-02]), array([ 0.03997394,  0.01961928, -0.02472009,  0.1112988 ]), array([ 0.0308851 ,  0.04259677, -0.06358316,  0.11308098]), array([ 0.01587157,  0.0624709 , -0.08288891,  0.07993505]), array([-0.00069913,  0.07239985, -0.07917014,  0.01514536]), array([-0.01444337,  0.06730059, -0.05567649, -0.06730021]), array([-0.02220903,  0.0456947 , -0.0211165 , -0.14615058]), array([-0.02290269,  0.01060004,  0.01318911, -0.19878181]), array([-0.01765265, -0.0308757 ,  0.03693564, -0.20798624]), array([-0.00926493, -0.06921839,  0.04406858, -0.16758884]), array([-0.00117453, -0.09501424,  0.03444693, -0.08479446]), array([ 0.0037298 , -0.10151242,  0.01345135,  0.02157453]), array([ 0.00402747, -0.08649269, -0.01004285,  0.12601835]), array([ 1.82428277e-04, -5.29618027e-02, -2.65759504e-02,  2.02890367e-01]), array([-0.00565549, -0.00849599, -0.02923297,  0.23318855]), array([-0.01043073,  0.03667361, -0.01616544,  0.21001756]), array([-0.0113154 ,  0.07235814,  0.0085514 ,  0.14064744]), array([-0.00679308,  0.09107026,  0.03626524,  0.04408341]), array([ 0.00270605,  0.08982621,  0.05671418, -0.05474911]), array([ 0.01482453,  0.07063623,  0.06140947, -0.13194595]), array([ 0.02592749,  0.03965518,  0.04642781, -0.1708334 ]), array([ 0.03219411,  0.00527949,  0.01393921, -0.1660878 ]), array([ 0.03084311, -0.02426814, -0.02804034, -0.12458796]), array([ 0.02111513, -0.04315167, -0.06779646, -0.06258596]), array([ 0.00467836, -0.0492712 , -0.09338433, -0.00016362]), array([-0.01469973, -0.04438927, -0.09629983,  0.04511936]), array([-0.03213559, -0.03307428, -0.07419051,  0.06340895]), array([-0.04298501, -0.02085913, -0.03177098,  0.05502774]), array([-0.04417185, -0.0122463 ,  0.02035226,  0.02951894]), array([-0.03509605, -0.00921946,  0.06860665,  0.00170489]), array([-0.01785029, -0.0107296 ,  0.10027336, -0.01384062]), array([ 0.00332508, -0.01329566,  0.10710094, -0.00811238]), array([ 0.02319838, -0.01250082,  0.08765122,  0.01893998]), array([ 0.03697987, -0.00486523,  0.0476531 ,  0.05814529]), array([ 0.04161165,  0.01056065, -0.00174275,  0.09408829]), array([ 0.036541  ,  0.03144595, -0.04724682,  0.11032895]), array([ 0.02376536,  0.05256034, -0.07724731,  0.09519481]), array([ 0.00715598,  0.0672154 , -0.08503269,  0.04630454]), array([-0.0087223 ,  0.06934871, -0.07049114, -0.02771862]), array([-0.01993649,  0.05560472, -0.039841  , -0.10900001]), array([-0.02426616,  0.02674893, -0.00351704, -0.17517189]), array([-0.02172381, -0.01206906,  0.02718387, -0.20586882]), array([-0.01436234, -0.05237664,  0.04368305, -0.18913258]), array([-0.00544895, -0.08452702,  0.04268369, -0.12554552]), array([ 0.00169059, -0.10030208,  0.02682912, -0.02850788]), array([ 0.00476139, -0.09517893,  0.00345268,  0.07924357]), array([ 0.00320033, -0.06963768, -0.01793747,  0.17148564]), array([-0.00169427, -0.02918456, -0.02874963,  0.22529389]), array([-0.00725219,  0.01696551, -0.0242711 ,  0.22739688]), array([-0.0104177 ,  0.05827442, -0.00549572,  0.17815567]), array([-0.00890455,  0.08566083,  0.02110302,  0.09135423]), array([-0.00209251,  0.09380211,  0.04582693, -0.01017155]), array([ 0.00864906,  0.08230036,  0.05902758, -0.10114803]), array([ 0.02029564,  0.05548505,  0.05425284, -0.16058732]), array([ 0.02904988,  0.0209895 ,  0.03047325, -0.17711066]), array([ 0.03152662, -0.01248898, -0.0072024 , -0.15159173]), array([ 0.02589341, -0.03760261, -0.04871123, -0.09617676]), array([ 0.01259413, -0.05021554, -0.0819235 , -0.02991785]), array([-0.00560372, -0.05017727, -0.09633239,  0.02743055]), array([-0.02427919, -0.04084285, -0.08634717,  0.06141571]), array([-0.03855791, -0.02756707, -0.05316672,  0.06689416]), array([-0.04449186, -0.01570307, -0.00465585,  0.04886438]), array([-0.04021063, -0.00877584,  0.04675771,  0.01995939]), array([-0.0265015 , -0.00741854,  0.08755148, -0.00444215]), array([-0.00664171, -0.00938928,  0.10693755, -0.01183838]), array([ 0.01447765, -0.01063393,  0.09994426,  0.00283917]), array([ 0.03168821, -0.00702094,  0.06882063,  0.03525618]), array([0.04095128, 0.0038584 , 0.02232151, 0.07300777]), array([ 0.04042423,  0.02145784, -0.02689035,  0.09980257]), array([ 0.03088356,  0.04205532, -0.06591279,  0.10111627]), array([ 0.01539842,  0.05966077, -0.08524795,  0.06952697]), array([-0.00163115,  0.0678099 , -0.08135981,  0.00798646]), array([-0.01577429,  0.06169934, -0.05742623, -0.07014289]), array([-0.02382004,  0.03998698, -0.02211593, -0.14439575]), array([-0.0246132 ,  0.0056653 ,  0.01323677, -0.19295525]), array([-0.01923028, -0.03433389,  0.03823679, -0.19928446]), array([-0.01045337, -0.07077914,  0.0466395 , -0.15758445]), array([-0.00174065, -0.09457811,  0.03803196, -0.07507311]), array([ 0.00393983, -0.09927324,  0.01752218,  0.02970023]), array([ 0.00504222, -0.08286699, -0.00618791,  0.13164558]), array([ 0.00188551, -0.04850279, -0.02365885,  0.20555511]), array([-0.00351428, -0.00380696, -0.02784789,  0.23284855]), array([-0.0081973 ,  0.04101851, -0.01665761,  0.20699128]), array([-0.00937174,  0.07587453,  0.00617804,  0.13549032]), array([-0.00548382,  0.09339594,  0.03238718,  0.03744079]), array([ 0.00314595,  0.09072884,  0.05203369, -0.06222993]), array([ 0.01432084,  0.07001318,  0.05680017, -0.13960811]), array([ 0.0245808 ,  0.03754079,  0.042731  , -0.17795726]), array([ 0.03025439,  0.0018602 ,  0.01178317, -0.17187672]), array([ 0.02865468, -0.0286438 , -0.02835198, -0.12823513]), array([ 0.01904704, -0.04798309, -0.0663199 , -0.06340104]), array([ 0.00305475, -0.05394361, -0.09050081,  0.0022802 ]), array([-0.0156556 , -0.04824105, -0.09261608,  0.05084211]), array([-0.03233228, -0.03549039, -0.07039228,  0.07191218]), array([-0.04246313, -0.02137959, -0.02847036,  0.06526478])]</t>
   </si>
   <si>
-    <t>['[0,1,1]', '[2,2,2]', '[1,1,1]', '[1,2,0]', '[1,1,2]', '[2,0,1]', '[0,0,0]', '[0,2,1]', '[2,1,0]', '[1,0,2]']</t>
+    <t>['[0,1,1]', '[2,0,1]', '[1,1,2]', '[1,1,1]', '[0,0,0]', '[2,2,2]', '[2,1,0]', '[0,2,1]', '[1,2,0]', '[1,0,2]']</t>
   </si>
   <si>
     <t>[2,2,2]</t>
   </si>
   <si>
-    <t>[1, 21, 32, 35, 36, 46, 58, 89, 90, 94, 98, 108, 111, 115]</t>
-  </si>
-  <si>
-    <t>[0, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 1, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
-  </si>
-  <si>
-    <t>['[-0.03763371 -0.01533471  0.06554052 -0.01816017]', '[-0.03406929  0.01398622 -0.02953871  0.30651903]', '[-0.04818188  0.10262173 -0.10566927  0.56184435]', '[-0.07305261  0.22936701 -0.13369446  0.67944384]', '[-0.0976443   0.36319498 -0.10327727  0.63282133]', '[-0.11125897  0.47297074 -0.02773051  0.446438  ]', '[-0.10757465  0.53619101  0.06462001  0.17794954]', '[-0.06138715  0.47788865  0.38724178 -0.74730665]', '[ 0.04067658  0.24884187  0.60910104 -1.49573956]', '[ 0.16900594 -0.09311382  0.63541813 -1.84114417]', '[ 0.27801726 -0.45113855  0.41913697 -1.65899888]', '[ 0.32572913 -0.7305588   0.04412338 -1.09289423]', '[ 0.29447842 -0.87822542 -0.34882596 -0.37494656]', '[ 0.17030161 -0.82157237 -0.8661431   0.9218764 ]', '[-0.03874058 -0.52315128 -1.18413013  2.00573318]', '[-0.28264765 -0.05491634 -1.19263231  2.55690497]', '[-0.48755467  0.44331129 -0.79529798  2.30203282]', '[-0.58208319  0.82809498 -0.125917    1.48995424]', '[-0.53533756  1.02669961  0.58287054  0.48321159]', '[-0.33779237  0.9634366   1.35170374 -1.09886953]', '[-0.01488044  0.60125986  1.8171686  -2.45350017]', '[ 0.33238892  0.09818686  1.56845636 -2.4173542 ]', '[ 0.60598854 -0.37255967  1.10002198 -2.1659303 ]', '[ 0.75158377 -0.73138149  0.32569497 -1.36870987]', '[ 0.73066643 -0.90733038 -0.53282377 -0.37315378]', '[ 0.52285964 -0.81683311 -1.51010724  1.27138994]', '[ 0.14717747 -0.41167127 -2.17455856  2.69331087]', '[-0.30666734  0.19436497 -2.2461063   3.14902374]', '[-0.70457638  0.76142821 -1.64925405  2.38602723]', '[-0.94478993  1.12370592 -0.72345318  1.22056248]', '[-0.98793441  1.24930627  0.29523319  0.03405542]', '[-0.80939032  1.07883304  1.47238814 -1.75512721]', '[-0.434198    0.60568546  2.22032814 -2.9171915 ]', '[ 0.06754011 -0.09781158  2.66918486 -3.87648182]', '[ 0.57260551 -0.82315123  2.26186373 -3.15884578]', '[ 0.91993843 -1.26455943  1.17673274 -1.26055643]', '[ 1.03459061 -1.33666188 -0.04226631  0.5248663 ]', '[ 0.90120796 -1.0535841  -1.28736434  2.32260998]', '[ 0.5267288  -0.40345539 -2.40587095  4.11721505]', '[-0.01417134  0.50382687 -2.83742868  4.6065697 ]', '[-0.54628188  1.31136989 -2.39014389  3.32090159]', '[-0.94666431  1.81916379 -1.57012701  1.77211404]', '[-1.1604262   2.03052381 -0.54453691  0.3631138 ]', '[-1.14450485  1.92465398  0.70738255 -1.42772222]', '[-0.87862351  1.44755197  1.9444748  -3.39698207]', '[-0.37199545  0.542837    3.07004436 -5.60568561]', '[ 0.256263   -0.59088253  2.99015897 -5.24709114]', '[ 0.78365771 -1.48785204  2.21095731 -3.63192701]', '[ 1.12662274 -2.05268814  1.19483316 -2.05900684]', '[ 1.25477331 -2.32441058  0.07873713 -0.67486711]', '[ 1.14559006 -2.28214045 -1.15720746  1.10760226]', '[ 0.80169045 -1.87071866 -2.24821757  3.05145766]', '[ 0.2603918  -1.03747173 -3.13295908  5.31941102]', '[-0.41712066  0.20176186 -3.42333409  6.58688107]', '[-1.00372445  1.36751706 -2.31800167  4.85239641]', '[-1.33418315  2.15842318 -0.98571565  3.1326969 ]', '[-1.40028036  2.63945106  0.31269174  1.6964973 ]', '[-1.21000744  2.81923725  1.56655485  0.10558844]', '[-0.79354104  2.70475549  2.5404786  -1.23521612]', '[-0.21847679  2.29335395  3.09198221 -2.85597782]', '[ 0.39494622  1.57600522  2.95956102 -4.26877695]', '[ 0.94687297  0.61626364  2.51787123 -5.19842789]', '[ 1.36642259 -0.41122702  1.55907909 -4.82574631]', '[ 1.52897063 -1.24609072  0.00548702 -3.44904129]', '[ 1.35614943 -1.76978549 -1.73191906 -1.71941989]', '[ 0.84104324 -1.85874784 -3.31312645  0.8837285 ]', '[ 0.08873273 -1.40765542 -4.05968191  3.59120283]', '[-0.72867998 -0.47380403 -3.98746282  5.46642575]', '[-1.4417107   0.59997789 -3.00847505  4.91255882]', '[-1.91006837  1.44517163 -1.67873535  3.59733804]', '[-2.117305    2.06936863 -0.39769829  2.68335322]', '[-2.0691843   2.51632411  0.87816733  1.74801607]', '[-1.76036475  2.72608885  2.20881008  0.28815721]', '[-1.18249282  2.58690242  3.53322164 -1.74605013]', '[-0.38279895  2.00048569  4.33237005 -4.18339567]', '[ 0.5020018   0.90277727  4.44720395 -6.7115822 ]', '[ 1.34227493 -0.51926737  3.73148897 -6.88403792]', '[ 1.93287111 -1.7059934   2.17147759 -5.04372283]', '[ 2.22480152 -2.59281311  0.79499664 -3.90899506]', '[ 2.27624031  3.0034185  -0.20878858 -2.95695818]', '[ 2.16034633  2.51404869 -0.93565465 -1.92342333]', '[ 1.89592685  2.23581889 -1.73862722 -0.87362374]', '[ 1.43707989  2.18999173 -2.8747883   0.32914504]', '[ 0.75000372  2.31287754 -3.93020593  0.70734849]', '[-0.08076928  2.38320652 -4.17787929 -0.24710181]', '[-0.82396922  2.12470087 -3.00279811 -2.51457999]', '[-1.19381779  1.33722046 -0.57514668 -5.38729324]', '[-1.04475896 -0.06313935  1.76391966 -8.19774836]', '[-0.68185728 -1.64542644  1.6150371  -7.2962214 ]', '[-0.40024202 -3.00571445  1.36354814 -6.61045405]', '[-0.06329133  1.87932955  2.1606473  -7.67964866]', '[  0.51752961   0.03883272   3.34290525 -10.30248504]', '[ 0.99270206 -1.77691053  1.02986257 -7.3352839 ]', '[ 0.96382676 -3.00321966 -1.05870903 -5.21602795]', '[ 0.67923162  2.34111447 -1.52832266 -4.49130136]', '[ 0.45561751  1.30685943 -0.5286008  -6.16921926]', '[ 0.47505939 -0.16970255  0.30477168 -7.99196853]', '[ 0.3278216  -1.50398168 -2.00546604 -4.93856765]', '[-0.27613345 -2.15148217 -3.7081943  -1.83948273]', '[-1.03461174 -2.37243217 -3.66221156 -0.68348171]', '[-1.69317664 -2.52179784 -2.87899539 -0.97903475]', '[-2.1887016  -2.80074317 -2.10109135 -1.84319955]', '[-2.53403903  3.0083441  -1.34057553 -2.85901868]', '[-2.70002634  2.33946605 -0.26349854 -3.78013314]', '[-2.62529368  1.50816703  1.01599069 -4.54345007]', '[-2.29312679  0.49596472  2.31229156 -5.66893924]', '[-1.70766403 -0.7560358   3.48065426 -6.65866711]', '[-0.91274115 -2.07487407  4.50180927 -6.41074446]', '[ 0.06724839  2.99366823  5.08936771 -5.90448202]', '[ 1.02443632  1.73283174  4.37194054 -6.82942708]', '[ 1.83176579  0.2580597   3.70792864 -7.72602561]', '[ 2.43282768 -1.14039858  2.22966701 -6.11930916]', '[ 2.74501366 -2.28529349  0.91591265 -5.42862128]', '[ 2.8370675   2.94849305  0.2033849  -5.10184003]', '[ 2.90622683  1.94775184  0.60223463 -4.93867744]', '[ 3.06511298  1.01089517  0.93885273 -4.43070362]']</t>
-  </si>
-  <si>
-    <t>[0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50, 51, 52, 53, 54, 55, 56, 57, 58, 59, 60, 61, 62, 63, 64, 65, 66, 67, 68, 69, 70, 71, 72, 73, 74, 75, 76, 77, 78, 79, 80, 81, 82, 83, 84, 85, 86, 87, 88, 89, 90, 91, 92, 93, 94, 95, 96, 97, 98, 99, 100, 101, 102, 103, 104, 105, 106, 107, 108, 109, 110, 111, 112, 113, 114, 115]</t>
-  </si>
-  <si>
-    <t>[array([-0.03763371, -0.01533471,  0.06554052, -0.01816017], dtype=float32), array([-0.03406929,  0.01398622, -0.02953871,  0.30651903]), array([-0.04818188,  0.10262173, -0.10566927,  0.56184435]), array([-0.07305261,  0.22936701, -0.13369446,  0.67944384]), array([-0.0976443 ,  0.36319498, -0.10327727,  0.63282133]), array([-0.11125897,  0.47297074, -0.02773051,  0.446438  ]), array([-0.10757465,  0.53619101,  0.06462001,  0.17794954]), array([-0.06138715,  0.47788865,  0.38724178, -0.74730665]), array([ 0.04067658,  0.24884187,  0.60910104, -1.49573956]), array([ 0.16900594, -0.09311382,  0.63541813, -1.84114417]), array([ 0.27801726, -0.45113855,  0.41913697, -1.65899888]), array([ 0.32572913, -0.7305588 ,  0.04412338, -1.09289423]), array([ 0.29447842, -0.87822542, -0.34882596, -0.37494656]), array([ 0.17030161, -0.82157237, -0.8661431 ,  0.9218764 ]), array([-0.03874058, -0.52315128, -1.18413013,  2.00573318]), array([-0.28264765, -0.05491634, -1.19263231,  2.55690497]), array([-0.48755467,  0.44331129, -0.79529798,  2.30203282]), array([-0.58208319,  0.82809498, -0.125917  ,  1.48995424]), array([-0.53533756,  1.02669961,  0.58287054,  0.48321159]), array([-0.33779237,  0.9634366 ,  1.35170374, -1.09886953]), array([-0.01488044,  0.60125986,  1.8171686 , -2.45350017]), array([ 0.33238892,  0.09818686,  1.56845636, -2.4173542 ]), array([ 0.60598854, -0.37255967,  1.10002198, -2.1659303 ]), array([ 0.75158377, -0.73138149,  0.32569497, -1.36870987]), array([ 0.73066643, -0.90733038, -0.53282377, -0.37315378]), array([ 0.52285964, -0.81683311, -1.51010724,  1.27138994]), array([ 0.14717747, -0.41167127, -2.17455856,  2.69331087]), array([-0.30666734,  0.19436497, -2.2461063 ,  3.14902374]), array([-0.70457638,  0.76142821, -1.64925405,  2.38602723]), array([-0.94478993,  1.12370592, -0.72345318,  1.22056248]), array([-0.98793441,  1.24930627,  0.29523319,  0.03405542]), array([-0.80939032,  1.07883304,  1.47238814, -1.75512721]), array([-0.434198  ,  0.60568546,  2.22032814, -2.9171915 ]), array([ 0.06754011, -0.09781158,  2.66918486, -3.87648182]), array([ 0.57260551, -0.82315123,  2.26186373, -3.15884578]), array([ 0.91993843, -1.26455943,  1.17673274, -1.26055643]), array([ 1.03459061, -1.33666188, -0.04226631,  0.5248663 ]), array([ 0.90120796, -1.0535841 , -1.28736434,  2.32260998]), array([ 0.5267288 , -0.40345539, -2.40587095,  4.11721505]), array([-0.01417134,  0.50382687, -2.83742868,  4.6065697 ]), array([-0.54628188,  1.31136989, -2.39014389,  3.32090159]), array([-0.94666431,  1.81916379, -1.57012701,  1.77211404]), array([-1.1604262 ,  2.03052381, -0.54453691,  0.3631138 ]), array([-1.14450485,  1.92465398,  0.70738255, -1.42772222]), array([-0.87862351,  1.44755197,  1.9444748 , -3.39698207]), array([-0.37199545,  0.542837  ,  3.07004436, -5.60568561]), array([ 0.256263  , -0.59088253,  2.99015897, -5.24709114]), array([ 0.78365771, -1.48785204,  2.21095731, -3.63192701]), array([ 1.12662274, -2.05268814,  1.19483316, -2.05900684]), array([ 1.25477331, -2.32441058,  0.07873713, -0.67486711]), array([ 1.14559006, -2.28214045, -1.15720746,  1.10760226]), array([ 0.80169045, -1.87071866, -2.24821757,  3.05145766]), array([ 0.2603918 , -1.03747173, -3.13295908,  5.31941102]), array([-0.41712066,  0.20176186, -3.42333409,  6.58688107]), array([-1.00372445,  1.36751706, -2.31800167,  4.85239641]), array([-1.33418315,  2.15842318, -0.98571565,  3.1326969 ]), array([-1.40028036,  2.63945106,  0.31269174,  1.6964973 ]), array([-1.21000744,  2.81923725,  1.56655485,  0.10558844]), array([-0.79354104,  2.70475549,  2.5404786 , -1.23521612]), array([-0.21847679,  2.29335395,  3.09198221, -2.85597782]), array([ 0.39494622,  1.57600522,  2.95956102, -4.26877695]), array([ 0.94687297,  0.61626364,  2.51787123, -5.19842789]), array([ 1.36642259, -0.41122702,  1.55907909, -4.82574631]), array([ 1.52897063, -1.24609072,  0.00548702, -3.44904129]), array([ 1.35614943, -1.76978549, -1.73191906, -1.71941989]), array([ 0.84104324, -1.85874784, -3.31312645,  0.8837285 ]), array([ 0.08873273, -1.40765542, -4.05968191,  3.59120283]), array([-0.72867998, -0.47380403, -3.98746282,  5.46642575]), array([-1.4417107 ,  0.59997789, -3.00847505,  4.91255882]), array([-1.91006837,  1.44517163, -1.67873535,  3.59733804]), array([-2.117305  ,  2.06936863, -0.39769829,  2.68335322]), array([-2.0691843 ,  2.51632411,  0.87816733,  1.74801607]), array([-1.76036475,  2.72608885,  2.20881008,  0.28815721]), array([-1.18249282,  2.58690242,  3.53322164, -1.74605013]), array([-0.38279895,  2.00048569,  4.33237005, -4.18339567]), array([ 0.5020018 ,  0.90277727,  4.44720395, -6.7115822 ]), array([ 1.34227493, -0.51926737,  3.73148897, -6.88403792]), array([ 1.93287111, -1.7059934 ,  2.17147759, -5.04372283]), array([ 2.22480152, -2.59281311,  0.79499664, -3.90899506]), array([ 2.27624031,  3.0034185 , -0.20878858, -2.95695818]), array([ 2.16034633,  2.51404869, -0.93565465, -1.92342333]), array([ 1.89592685,  2.23581889, -1.73862722, -0.87362374]), array([ 1.43707989,  2.18999173, -2.8747883 ,  0.32914504]), array([ 0.75000372,  2.31287754, -3.93020593,  0.70734849]), array([-0.08076928,  2.38320652, -4.17787929, -0.24710181]), array([-0.82396922,  2.12470087, -3.00279811, -2.51457999]), array([-1.19381779,  1.33722046, -0.57514668, -5.38729324]), array([-1.04475896, -0.06313935,  1.76391966, -8.19774836]), array([-0.68185728, -1.64542644,  1.6150371 , -7.2962214 ]), array([-0.40024202, -3.00571445,  1.36354814, -6.61045405]), array([-0.06329133,  1.87932955,  2.1606473 , -7.67964866]), array([  0.51752961,   0.03883272,   3.34290525, -10.30248504]), array([ 0.99270206, -1.77691053,  1.02986257, -7.3352839 ]), array([ 0.96382676, -3.00321966, -1.05870903, -5.21602795]), array([ 0.67923162,  2.34111447, -1.52832266, -4.49130136]), array([ 0.45561751,  1.30685943, -0.5286008 , -6.16921926]), array([ 0.47505939, -0.16970255,  0.30477168, -7.99196853]), array([ 0.3278216 , -1.50398168, -2.00546604, -4.93856765]), array([-0.27613345, -2.15148217, -3.7081943 , -1.83948273]), array([-1.03461174, -2.37243217, -3.66221156, -0.68348171]), array([-1.69317664, -2.52179784, -2.87899539, -0.97903475]), array([-2.1887016 , -2.80074317, -2.10109135, -1.84319955]), array([-2.53403903,  3.0083441 , -1.34057553, -2.85901868]), array([-2.70002634,  2.33946605, -0.26349854, -3.78013314]), array([-2.62529368,  1.50816703,  1.01599069, -4.54345007]), array([-2.29312679,  0.49596472,  2.31229156, -5.66893924]), array([-1.70766403, -0.7560358 ,  3.48065426, -6.65866711]), array([-0.91274115, -2.07487407,  4.50180927, -6.41074446]), array([ 0.06724839,  2.99366823,  5.08936771, -5.90448202]), array([ 1.02443632,  1.73283174,  4.37194054, -6.82942708]), array([ 1.83176579,  0.2580597 ,  3.70792864, -7.72602561]), array([ 2.43282768, -1.14039858,  2.22966701, -6.11930916]), array([ 2.74501366, -2.28529349,  0.91591265, -5.42862128]), array([ 2.8370675 ,  2.94849305,  0.2033849 , -5.10184003]), array([ 2.90622683,  1.94775184,  0.60223463, -4.93867744]), array([ 3.06511298,  1.01089517,  0.93885273, -4.43070362])]</t>
-  </si>
-  <si>
-    <t>['[0,0,0]', '[0,2,1]', '[1,1,1]', '[2,1,0]', '[2,2,2]', '[0,1,1]', '[1,1,2]', '[1,2,0]', '[2,0,1]', '[1,0,2]']</t>
-  </si>
-  <si>
-    <t>[3, 13, 23, 26, 27, 35, 38, 46, 48, 50, 51, 52, 61, 62, 63, 73, 74, 77, 79, 87, 88, 89, 90, 92, 94, 106, 107, 121, 123, 126, 127, 128]</t>
-  </si>
-  <si>
-    <t>[0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 1, 0, 0, 0, 0, 0, 0, 0, 1, 2, 2, 2, 2, 2, 2, 2, 1, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 1, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 2, 2]</t>
-  </si>
-  <si>
-    <t>['[-0.03763371 -0.01533471  0.06554052 -0.01816017]', '[-0.00754409 -0.05458322  0.2277812  -0.36241836]', '[ 0.04879627 -0.15231473  0.32089719 -0.5887683 ]', '[ 0.08773348 -0.20975891  0.05953656  0.02857539]', '[ 0.07159701 -0.14038323 -0.21558016  0.65104861]', '[ 0.00648475  0.0393353  -0.41626589  1.10429103]', '[-0.08485445  0.27989065 -0.46991633  1.24354086]', '[-0.17036214  0.5133148  -0.36181811  1.04111741]', '[-0.22198773  0.68003836 -0.14247549  0.59860378]', '[-0.2247793   0.74576291  0.11471656  0.05210182]', '[-0.15422799  0.63893119  0.57773327 -1.10356161]', '[-0.0023089   0.31819547  0.90819171 -2.04242503]', '[ 0.18976215 -0.13990612  0.95416556 -2.41915067]', '[ 0.32922994 -0.53222037  0.40445403 -1.42735523]', '[ 0.36851339 -0.75743048 -0.02127098 -0.79389092]', '[ 0.3209358  -0.84327784 -0.44393041 -0.06247072]', '[ 0.17549925 -0.72470142 -0.98170581  1.22343902]', '[-0.05672344 -0.37193523 -1.2922295   2.22884668]', '[-0.316148    0.12123037 -1.23081015  2.56519699]', '[-0.52001574  0.59744783 -0.75261894  2.0900629 ]', '[-0.60228376  0.92862691 -0.05380118  1.1836501 ]', '[-0.5412135   1.06305688  0.65078286  0.1547233 ]', '[-0.33134166  0.93435975  1.40855913 -1.42365944]', '[-0.02126775  0.57254108  1.62815431 -2.10752825]', '[ 0.31560844  0.0729333   1.65965926 -2.74325682]', '[ 0.60710857 -0.45743082  1.18064909 -2.42055651]', '[ 0.74194172 -0.79364214  0.14890547 -0.91158868]', '[ 0.66627706 -0.8180228  -0.8919563   0.6693817 ]', '[ 0.39602761 -0.52917472 -1.76566552  2.18051422]', '[-0.01183036  0.0156533  -2.21398451  3.09653027]', '[-0.44135872  0.61911303 -1.97405582  2.74527967]', '[-0.76845519  1.06328294 -1.24525636  1.64380327]', '[-0.92639     1.27119098 -0.3164606   0.43667446]', '[-0.87241343  1.18441901  0.85250775 -1.31003602]', '[-0.59044429  0.74175428  1.93927703 -3.11177415]', '[-0.14703315  0.0386162   2.38299248 -3.71220058]', '[ 0.33287265 -0.69885815  2.28705145 -3.41243298]', '[ 0.72869588 -1.26148126  1.61153133 -2.15347459]', '[ 0.94288788 -1.50579977  0.50990957 -0.3107307 ]', '[ 0.92735658 -1.39000544 -0.66996299  1.47370903]', '[ 0.67601399 -0.90826456 -1.82888745  3.36039015]', '[ 0.21355763 -0.06300749 -2.68523071  4.88672021]', '[-0.32629508  0.8954926  -2.55398929  4.36985251]', '[-0.76874551  1.61916267 -1.82122437  2.83913586]', '[-1.04119256  2.0390057  -0.87816165  1.384796  ]', '[-1.11336131  2.18026577  0.16227461  0.03562663]', '[-0.97821052  2.05244109  1.17276187 -1.32426667]', '[-0.63990743  1.59660501  2.18054035 -3.27475364]', '[-0.13930865  0.78379428  2.76225493 -4.7879589 ]', '[ 0.44057665 -0.28880169  2.84454824 -5.52434464]', '[ 0.89816711 -1.20437899  1.65670861 -3.51792456]', '[ 1.09761709 -1.70766729  0.34084788 -1.55819361]', '[ 1.03839577 -1.83635231 -0.91524074  0.27219321]', '[ 0.74264807 -1.59136089 -2.00523823  2.20670166]', '[ 0.25378819 -0.94189782 -2.83380642  4.28250908]', '[-0.35586712  0.06836576 -3.09731403  5.46713735]', '[-0.90211837  1.06425443 -2.23491767  4.24343598]', '[-1.22916997  1.74955074 -1.01966506  2.64590153]', '[-1.30789796  2.13646716  0.22992322  1.23662592]', '[-1.12867837  2.19955358  1.53369129 -0.62199091]', '[-0.71171887  1.87625914  2.57846323 -2.64720272]', '[-0.14066644  1.17795509  3.06122359 -4.30800985]', '[ 0.47635604  0.20771522  2.96866703 -5.09038073]', '[ 0.97525861 -0.69795447  1.89735144 -3.71506593]', '[ 1.23577642 -1.308329    0.68181805 -2.37665107]', '[ 1.24416193 -1.64975364 -0.59631864 -1.02695465]', '[ 0.98757467 -1.66042259 -1.93120803  0.95623592]', '[ 0.49338023 -1.25036948 -2.94653217  3.17097827]', '[-0.16045012 -0.40467559 -3.47978753  5.0985983 ]', '[-0.82435921  0.62419681 -2.9723771   4.77357446]', '[-1.30321912  1.41844316 -1.77837805  3.16015909]', '[-1.53139086  1.909668   -0.49920562  1.79431238]', '[-1.50254168  2.14176527  0.7843312   0.51364806]', '[-1.22195553  2.10195083  1.99769092 -0.95727679]', '[-0.72103648  1.73877406  2.94712295 -2.71765418]', '[-0.05632518  0.95516142  3.62919639 -5.09432553]', '[ 0.68421509 -0.20962613  3.57054961 -6.06262685]', '[ 1.26398843 -1.21481969  2.15490291 -3.87681847]', '[ 1.5632202  -1.83976323  0.83370604 -2.42956861]', '[ 1.58314909 -2.15492401 -0.62407954 -0.72798847]', '[ 1.31874034 -2.12028137 -1.99881146  1.12467823]', '[ 0.79826608 -1.6777415  -3.15554178  3.38085673]', '[ 0.0786637  -0.74090446 -3.97410416  5.94537368]', '[-0.72276865  0.54582858 -3.77904242  6.28948823]', '[-1.35570756  1.60296317 -2.50548753  4.26023402]', '[-1.72597816  2.29391504 -1.20428576  2.74083537]', '[-1.84115222  2.7184873   0.04161985  1.51740612]', '[-1.71244262  2.89720223  1.24307893  0.25042435]', '[-1.34416031  2.80948763  2.42887857 -1.15263812]', '[-0.75642257  2.42493385  3.36793798 -2.72535856]', '[-0.04394283  1.71032018  3.64237901 -4.41330856]', '[ 0.68504095  0.63177685  3.58134197 -6.2157771 ]', '[ 1.30287684 -0.54918666  2.42829059 -5.1920622 ]', '[ 1.6431698  -1.4426201   0.94159297 -3.73840832]', '[ 1.6595521  -2.00723497 -0.76434155 -1.91676844]', '[ 1.35224534 -2.21656883 -2.27750211 -0.11598342]', '[ 0.76529928 -2.00725193 -3.4983728   2.26558874]', '[ 4.93885808e-04 -1.29689693e+00 -4.04385358e+00  4.82356434e+00]', '[-0.81356798 -0.13445497 -3.94585509  6.40297698]', '[-1.4925052   1.0415158  -2.7171577   5.06974698]', '[-1.89184754  1.89969629 -1.28828345  3.60984944]', '[-2.01280633  2.51045096  0.06341534  2.51249943]', '[-1.87348578  2.89735704  1.31537304  1.32490824]', '[-1.48314544  3.00852713  2.58436682 -0.23456821]', '[-0.84214264  2.77936627  3.75850686 -2.06632326]', '[-0.03262072  2.17785952  4.16831462 -3.95089417]', '[ 0.75098636  1.26287163  3.58186661 -5.06898053]', '[ 1.37562232  0.2371026   2.58803819 -4.92009818]', '[ 1.77970501 -0.68133559  1.39547987 -4.15070042]', '[ 1.91752692 -1.40950682 -0.05391084 -3.11039965]', '[ 1.74361742 -1.90467446 -1.70852076 -1.74955499]', '[ 1.22420122 -2.02016143 -3.42396925  0.70779102]', '[ 0.41748327 -1.58229564 -4.50502206  3.7284621 ]', '[-0.52309261 -0.54376779 -4.76793414  6.39593435]', '[-1.40423329  0.73044726 -3.84742822  5.78860635]', '[-2.03724251  1.70672072 -2.52020863  4.10316985]', '[-2.43174571  2.43242904 -1.47254255  3.25964547]', '[-2.64598442  3.03183133 -0.72783249  2.7528914 ]', '[-2.74501405 -2.75177261 -0.31005966  2.22886121]', '[-2.7814299  -2.368195   -0.06694849  1.58591751]', '[-2.77125481 -2.12613255  0.1786039   0.8144517 ]', '[-2.70369947 -2.04993405  0.51721753 -0.06946144]', '[-2.54712536 -2.18164524  1.07932378 -1.25813684]', '[-2.26376278 -2.5352649   1.80269772 -2.28810515]', '[-1.79228928  3.14048616  2.95675438 -3.823352  ]', '[-1.07615184  2.17859061  4.18227205 -5.99719023]', '[-0.1369981   0.68004883  5.18719124 -9.03312443]', '[ 0.85975201 -1.07790454  4.38925395 -7.55775664]', '[ 1.58055144 -2.2693405   2.8708854  -4.61273707]', '[ 2.03431381 -3.04168659  1.69717989 -3.21116053]', '[ 2.27620144  2.71156639  0.76485185 -2.10118766]', '[ 2.35155942e+00  2.40230275e+00  1.55588237e-03 -9.83186101e-01]', '[ 2.27538895  2.32232191 -0.7794142   0.19107442]', '[ 2.01512551  2.52150411 -1.86066743  1.79499095]', '[ 1.51579509  3.03760686 -3.15298862  3.37676444]', '[ 0.76651849 -2.38641718 -4.24608436  5.35354471]', '[-0.14709402 -1.02650596 -4.88329838  8.39410293]', '[-1.11704318  0.78371383 -4.41888715  8.69442848]', '[-1.81632574  2.23989885 -2.62535436  6.090974  ]', '[-2.20612421 -2.9681534  -1.40013267  4.78856396]', '[-2.42379156 -2.10537146 -0.85693369  3.86861934]', '[-2.56031039 -1.41459392 -0.50974743  3.05112955]']</t>
-  </si>
-  <si>
-    <t>[0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50, 51, 52, 53, 54, 55, 56, 57, 58, 59, 60, 61, 62, 63, 64, 65, 66, 67, 68, 69, 70, 71, 72, 73, 74, 75, 76, 77, 78, 79, 80, 81, 82, 83, 84, 85, 86, 87, 88, 89, 90, 91, 92, 93, 94, 95, 96, 97, 98, 99, 100, 101, 102, 103, 104, 105, 106, 107, 108, 109, 110, 111, 112, 113, 114, 115, 116, 117, 118, 119, 120, 121, 122, 123, 124, 125, 126, 127, 128, 129, 130, 131, 132, 133, 134, 135, 136, 137, 138, 139, 140, 141]</t>
-  </si>
-  <si>
-    <t>[array([-0.03763371, -0.01533471,  0.06554052, -0.01816017], dtype=float32), array([-0.00754409, -0.05458322,  0.2277812 , -0.36241836]), array([ 0.04879627, -0.15231473,  0.32089719, -0.5887683 ]), array([ 0.08773348, -0.20975891,  0.05953656,  0.02857539]), array([ 0.07159701, -0.14038323, -0.21558016,  0.65104861]), array([ 0.00648475,  0.0393353 , -0.41626589,  1.10429103]), array([-0.08485445,  0.27989065, -0.46991633,  1.24354086]), array([-0.17036214,  0.5133148 , -0.36181811,  1.04111741]), array([-0.22198773,  0.68003836, -0.14247549,  0.59860378]), array([-0.2247793 ,  0.74576291,  0.11471656,  0.05210182]), array([-0.15422799,  0.63893119,  0.57773327, -1.10356161]), array([-0.0023089 ,  0.31819547,  0.90819171, -2.04242503]), array([ 0.18976215, -0.13990612,  0.95416556, -2.41915067]), array([ 0.32922994, -0.53222037,  0.40445403, -1.42735523]), array([ 0.36851339, -0.75743048, -0.02127098, -0.79389092]), array([ 0.3209358 , -0.84327784, -0.44393041, -0.06247072]), array([ 0.17549925, -0.72470142, -0.98170581,  1.22343902]), array([-0.05672344, -0.37193523, -1.2922295 ,  2.22884668]), array([-0.316148  ,  0.12123037, -1.23081015,  2.56519699]), array([-0.52001574,  0.59744783, -0.75261894,  2.0900629 ]), array([-0.60228376,  0.92862691, -0.05380118,  1.1836501 ]), array([-0.5412135 ,  1.06305688,  0.65078286,  0.1547233 ]), array([-0.33134166,  0.93435975,  1.40855913, -1.42365944]), array([-0.02126775,  0.57254108,  1.62815431, -2.10752825]), array([ 0.31560844,  0.0729333 ,  1.65965926, -2.74325682]), array([ 0.60710857, -0.45743082,  1.18064909, -2.42055651]), array([ 0.74194172, -0.79364214,  0.14890547, -0.91158868]), array([ 0.66627706, -0.8180228 , -0.8919563 ,  0.6693817 ]), array([ 0.39602761, -0.52917472, -1.76566552,  2.18051422]), array([-0.01183036,  0.0156533 , -2.21398451,  3.09653027]), array([-0.44135872,  0.61911303, -1.97405582,  2.74527967]), array([-0.76845519,  1.06328294, -1.24525636,  1.64380327]), array([-0.92639   ,  1.27119098, -0.3164606 ,  0.43667446]), array([-0.87241343,  1.18441901,  0.85250775, -1.31003602]), array([-0.59044429,  0.74175428,  1.93927703, -3.11177415]), array([-0.14703315,  0.0386162 ,  2.38299248, -3.71220058]), array([ 0.33287265, -0.69885815,  2.28705145, -3.41243298]), array([ 0.72869588, -1.26148126,  1.61153133, -2.15347459]), array([ 0.94288788, -1.50579977,  0.50990957, -0.3107307 ]), array([ 0.92735658, -1.39000544, -0.66996299,  1.47370903]), array([ 0.67601399, -0.90826456, -1.82888745,  3.36039015]), array([ 0.21355763, -0.06300749, -2.68523071,  4.88672021]), array([-0.32629508,  0.8954926 , -2.55398929,  4.36985251]), array([-0.76874551,  1.61916267, -1.82122437,  2.83913586]), array([-1.04119256,  2.0390057 , -0.87816165,  1.384796  ]), array([-1.11336131,  2.18026577,  0.16227461,  0.03562663]), array([-0.97821052,  2.05244109,  1.17276187, -1.32426667]), array([-0.63990743,  1.59660501,  2.18054035, -3.27475364]), array([-0.13930865,  0.78379428,  2.76225493, -4.7879589 ]), array([ 0.44057665, -0.28880169,  2.84454824, -5.52434464]), array([ 0.89816711, -1.20437899,  1.65670861, -3.51792456]), array([ 1.09761709, -1.70766729,  0.34084788, -1.55819361]), array([ 1.03839577, -1.83635231, -0.91524074,  0.27219321]), array([ 0.74264807, -1.59136089, -2.00523823,  2.20670166]), array([ 0.25378819, -0.94189782, -2.83380642,  4.28250908]), array([-0.35586712,  0.06836576, -3.09731403,  5.46713735]), array([-0.90211837,  1.06425443, -2.23491767,  4.24343598]), array([-1.22916997,  1.74955074, -1.01966506,  2.64590153]), array([-1.30789796,  2.13646716,  0.22992322,  1.23662592]), array([-1.12867837,  2.19955358,  1.53369129, -0.62199091]), array([-0.71171887,  1.87625914,  2.57846323, -2.64720272]), array([-0.14066644,  1.17795509,  3.06122359, -4.30800985]), array([ 0.47635604,  0.20771522,  2.96866703, -5.09038073]), array([ 0.97525861, -0.69795447,  1.89735144, -3.71506593]), array([ 1.23577642, -1.308329  ,  0.68181805, -2.37665107]), array([ 1.24416193, -1.64975364, -0.59631864, -1.02695465]), array([ 0.98757467, -1.66042259, -1.93120803,  0.95623592]), array([ 0.49338023, -1.25036948, -2.94653217,  3.17097827]), array([-0.16045012, -0.40467559, -3.47978753,  5.0985983 ]), array([-0.82435921,  0.62419681, -2.9723771 ,  4.77357446]), array([-1.30321912,  1.41844316, -1.77837805,  3.16015909]), array([-1.53139086,  1.909668  , -0.49920562,  1.79431238]), array([-1.50254168,  2.14176527,  0.7843312 ,  0.51364806]), array([-1.22195553,  2.10195083,  1.99769092, -0.95727679]), array([-0.72103648,  1.73877406,  2.94712295, -2.71765418]), array([-0.05632518,  0.95516142,  3.62919639, -5.09432553]), array([ 0.68421509, -0.20962613,  3.57054961, -6.06262685]), array([ 1.26398843, -1.21481969,  2.15490291, -3.87681847]), array([ 1.5632202 , -1.83976323,  0.83370604, -2.42956861]), array([ 1.58314909, -2.15492401, -0.62407954, -0.72798847]), array([ 1.31874034, -2.12028137, -1.99881146,  1.12467823]), array([ 0.79826608, -1.6777415 , -3.15554178,  3.38085673]), array([ 0.0786637 , -0.74090446, -3.97410416,  5.94537368]), array([-0.72276865,  0.54582858, -3.77904242,  6.28948823]), array([-1.35570756,  1.60296317, -2.50548753,  4.26023402]), array([-1.72597816,  2.29391504, -1.20428576,  2.74083537]), array([-1.84115222,  2.7184873 ,  0.04161985,  1.51740612]), array([-1.71244262,  2.89720223,  1.24307893,  0.25042435]), array([-1.34416031,  2.80948763,  2.42887857, -1.15263812]), array([-0.75642257,  2.42493385,  3.36793798, -2.72535856]), array([-0.04394283,  1.71032018,  3.64237901, -4.41330856]), array([ 0.68504095,  0.63177685,  3.58134197, -6.2157771 ]), array([ 1.30287684, -0.54918666,  2.42829059, -5.1920622 ]), array([ 1.6431698 , -1.4426201 ,  0.94159297, -3.73840832]), array([ 1.6595521 , -2.00723497, -0.76434155, -1.91676844]), array([ 1.35224534, -2.21656883, -2.27750211, -0.11598342]), array([ 0.76529928, -2.00725193, -3.4983728 ,  2.26558874]), array([ 4.93885808e-04, -1.29689693e+00, -4.04385358e+00,  4.82356434e+00]), array([-0.81356798, -0.13445497, -3.94585509,  6.40297698]), array([-1.4925052 ,  1.0415158 , -2.7171577 ,  5.06974698]), array([-1.89184754,  1.89969629, -1.28828345,  3.60984944]), array([-2.01280633,  2.51045096,  0.06341534,  2.51249943]), array([-1.87348578,  2.89735704,  1.31537304,  1.32490824]), array([-1.48314544,  3.00852713,  2.58436682, -0.23456821]), array([-0.84214264,  2.77936627,  3.75850686, -2.06632326]), array([-0.03262072,  2.17785952,  4.16831462, -3.95089417]), array([ 0.75098636,  1.26287163,  3.58186661, -5.06898053]), array([ 1.37562232,  0.2371026 ,  2.58803819, -4.92009818]), array([ 1.77970501, -0.68133559,  1.39547987, -4.15070042]), array([ 1.91752692, -1.40950682, -0.05391084, -3.11039965]), array([ 1.74361742, -1.90467446, -1.70852076, -1.74955499]), array([ 1.22420122, -2.02016143, -3.42396925,  0.70779102]), array([ 0.41748327, -1.58229564, -4.50502206,  3.7284621 ]), array([-0.52309261, -0.54376779, -4.76793414,  6.39593435]), array([-1.40423329,  0.73044726, -3.84742822,  5.78860635]), array([-2.03724251,  1.70672072, -2.52020863,  4.10316985]), array([-2.43174571,  2.43242904, -1.47254255,  3.25964547]), array([-2.64598442,  3.03183133, -0.72783249,  2.7528914 ]), array([-2.74501405, -2.75177261, -0.31005966,  2.22886121]), array([-2.7814299 , -2.368195  , -0.06694849,  1.58591751]), array([-2.77125481, -2.12613255,  0.1786039 ,  0.8144517 ]), array([-2.70369947, -2.04993405,  0.51721753, -0.06946144]), array([-2.54712536, -2.18164524,  1.07932378, -1.25813684]), array([-2.26376278, -2.5352649 ,  1.80269772, -2.28810515]), array([-1.79228928,  3.14048616,  2.95675438, -3.823352  ]), array([-1.07615184,  2.17859061,  4.18227205, -5.99719023]), array([-0.1369981 ,  0.68004883,  5.18719124, -9.03312443]), array([ 0.85975201, -1.07790454,  4.38925395, -7.55775664]), array([ 1.58055144, -2.2693405 ,  2.8708854 , -4.61273707]), array([ 2.03431381, -3.04168659,  1.69717989, -3.21116053]), array([ 2.27620144,  2.71156639,  0.76485185, -2.10118766]), array([ 2.35155942e+00,  2.40230275e+00,  1.55588237e-03, -9.83186101e-01]), array([ 2.27538895,  2.32232191, -0.7794142 ,  0.19107442]), array([ 2.01512551,  2.52150411, -1.86066743,  1.79499095]), array([ 1.51579509,  3.03760686, -3.15298862,  3.37676444]), array([ 0.76651849, -2.38641718, -4.24608436,  5.35354471]), array([-0.14709402, -1.02650596, -4.88329838,  8.39410293]), array([-1.11704318,  0.78371383, -4.41888715,  8.69442848]), array([-1.81632574,  2.23989885, -2.62535436,  6.090974  ]), array([-2.20612421, -2.9681534 , -1.40013267,  4.78856396]), array([-2.42379156, -2.10537146, -0.85693369,  3.86861934]), array([-2.56031039, -1.41459392, -0.50974743,  3.05112955])]</t>
-  </si>
-  <si>
-    <t>['[1,1,1]', '[2,1,0]', '[0,1,1]', '[1,2,0]', '[0,2,1]', '[1,1,2]', '[1,0,2]', '[2,0,1]', '[0,0,0]', '[2,2,2]']</t>
-  </si>
-  <si>
-    <t>[1, 8, 10, 12, 19, 20, 21, 22, 31, 32, 33, 41, 42, 46, 53, 54, 58, 66, 69, 79, 80, 84, 85, 94, 95, 96, 98, 99, 100, 107, 109, 110, 123, 124, 125, 126, 128, 136, 137, 138, 141, 142, 144]</t>
-  </si>
-  <si>
-    <t>[0, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 1, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 1, 2, 2, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 0, 1, 2, 2, 2, 2, 2, 2, 2, 2]</t>
-  </si>
-  <si>
-    <t>['[-0.03763371 -0.01533471  0.06554052 -0.01816017]', '[-0.03406929  0.01398622 -0.02953871  0.30651903]', '[-0.04818188  0.10262173 -0.10566927  0.56184435]', '[-0.07305261  0.22936701 -0.13369446  0.67944384]', '[-0.0976443   0.36319498 -0.10327727  0.63282133]', '[-0.11125897  0.47297074 -0.02773051  0.446438  ]', '[-0.10757465  0.53619101  0.06462001  0.17794954]', '[-0.06138715  0.47788865  0.38724178 -0.74730665]', '[ 0.0148479   0.31583331  0.35559654 -0.8357632 ]', '[ 0.09930297  0.09142664  0.46582003 -1.35869116]', '[ 0.16332535 -0.1339477   0.15404557 -0.84595443]', '[ 0.18235609 -0.30122116  0.02673755 -0.79482143]', '[ 0.14590118 -0.37383606 -0.38406134  0.07245783]', '[ 0.03527538 -0.27745936 -0.69738771  0.86037884]', '[-0.11998812 -0.04911509 -0.8171302   1.35971853]', '[-0.27446392  0.2361008  -0.68688356  1.41738809]', '[-0.37981758  0.48972331 -0.33947167  1.0653111 ]', '[-0.40298702  0.64643178  0.1142609   0.47926481]', '[-0.31140524  0.61390384  0.78273553 -0.79209503]', '[-0.12730221  0.40830999  1.0176804  -1.20866513]', '[ 0.07646417  0.15901752  0.97088125 -1.20733872]', '[ 0.24164034 -0.04359542  0.64145158 -0.75688544]', '[ 0.32074405 -0.12512554  0.132498   -0.03489029]', '[ 0.29237993 -0.05545237 -0.40811238  0.71533965]', '[ 0.16564264  0.1465297  -0.82706696  1.24849611]', '[-0.02150097  0.41463269 -0.99777939  1.35396944]', '[-0.21406194  0.65680873 -0.88469468  1.00426731]', '[-0.36009124  0.79642929 -0.54647837  0.36049463]', '[-0.42387451  0.79360385 -0.07924861 -0.39358516]', '[-0.36616728  0.57821015  0.6487642  -1.74011   ]', '[-0.17446462  0.11745777  1.21820835 -2.76909406]', '[ 0.06488854 -0.40128977  1.10531664 -2.27897652]', '[ 0.24550634 -0.75227414  0.66593408 -1.17211119]', '[ 0.3221835  -0.85772996  0.0884742   0.12976146]', '[ 0.27871469 -0.69966872 -0.51906269  1.43882675]', '[ 0.12102528 -0.29527187 -1.02240929  2.53462641]', '[-0.10634504  0.265581   -1.17548587  2.9178284 ]', '[-0.31766311  0.80771684 -0.8799268   2.38888321]', '[-0.44341514  1.19334689 -0.36043186  1.43568333]', '[-0.45989445  1.37706238  0.19048027  0.40007198]', '[-0.35357842  1.30260741  0.85256024 -1.13684649]', '[-0.14905568  0.98307552  1.1597014  -2.02175903]', '[ 0.09366895  0.51837134  1.21604892 -2.53340626]', '[ 0.33804427 -0.04800581  1.15651022 -2.98437406]', '[ 0.5244992  -0.60985345  0.64601523 -2.50517456]', '[ 0.58046016 -1.01571891 -0.09945626 -1.5101972 ]', '[ 0.46756448 -1.15024907 -0.99610173  0.15692977]', '[ 0.19978521 -0.95921229 -1.63057854  1.72272896]', '[-0.16112686 -0.48409936 -1.90970565  2.92691139]', '[-0.52899038  0.14714587 -1.67214986  3.19423527]', '[-0.79300404  0.72170751 -0.90538564  2.43791138]', '[-0.87657093  1.09831286  0.08281057  1.29991173]', '[-0.7612935   1.23436216  1.05004721  0.04744667]', '[-0.47100635  1.11471059  1.80119766 -1.23241889]', '[-0.06761291  0.75751365  2.15384228 -2.25624219]', '[ 0.37845985  0.20030389  2.20786523 -3.14301834]', '[ 0.77160466 -0.41473647  1.63035958 -2.82978822]', '[ 1.00359185 -0.88569582  0.65257173 -1.82873797]', '[ 1.00439246 -1.07964106 -0.63877977 -0.10595551]', '[ 0.75475449 -0.92165953 -1.82814563  1.70196993]', '[ 0.29215911 -0.40242864 -2.71981416  3.4009048 ]', '[-0.28270921  0.34968421 -2.87318695  3.81151209]', '[-0.79852761  1.00941768 -2.19101137  2.64781845]', '[-1.13706434  1.39633493 -1.16335187  1.23966564]', '[-1.2567158   1.51649348 -0.02514887 -0.02019668]', '[-1.12850633  1.33712336  1.30278649 -1.79973863]', '[-0.7612539   0.83685739  2.33516736 -3.20547935]', '[-0.19649419  0.01989647  3.18783002 -4.73038924]', '[ 0.43831017 -0.89271836  2.99547048 -4.05767834]', '[ 0.93953676 -1.48586713  1.96739248 -1.88455117]', '[ 1.22832582 -1.71369181  0.89302593 -0.42965225]', '[ 1.28182642 -1.64529542 -0.36509705  1.10308891]', '[ 1.0727456  -1.24118917 -1.72475692  2.98384385]', '[ 0.59615425 -0.43230443 -2.98994725  5.05593603]', '[-0.06308492  0.658387   -3.39114323  5.37830167]', '[-0.69215516  1.57263518 -2.81539867  3.65549037]', '[-1.16750471  2.12759373 -1.89234011  1.94376012]', '[-1.43494014  2.36920437 -0.76096306  0.50726597]', '[-1.46791456  2.33867322  0.43376124 -0.80750797]', '[-1.26277448  2.04155916  1.60692755 -2.1947103 ]', '[-0.83294746  1.44019935  2.66457111 -3.87985375]', '[-0.19058985  0.41832475  3.6769793  -6.22015924]', '[ 0.54684577 -0.84375042  3.44444384 -5.82560843]', '[ 1.13123198 -1.80472187  2.36367429 -3.80977643]', '[ 1.47180653 -2.36008252  1.03798567 -1.82511382]', '[ 1.54574893 -2.55115374 -0.29691277 -0.09793767]', '[ 1.35481395 -2.39622631 -1.60225679  1.67352408]', '[ 0.91325278 -1.8617804  -2.78313849  3.75062494]', '[ 0.25293266 -0.85543034 -3.78917775  6.35400664]', '[-0.54189201  0.55242731 -3.85972312  7.02075202]', '[-1.19356808  1.73837723 -2.6018301   4.80224722]', '[-1.58343458  2.52309061 -1.30232062  3.14365282]', '[-1.71873378  3.01606417 -0.0653592   1.80285799]', '[-1.61397383 -3.03851898  1.10946726  0.48255371]', '[-1.2747231  -3.07173686  2.27660914 -0.79888632]', '[-0.71539654  2.93449206  3.24560207 -1.94417594]', '[-0.02521543  2.4450859   3.50375886 -2.91205427]', '[ 0.63877177  1.75271946  3.03573954 -3.93269504]', '[ 1.14986527  0.96580281  2.03885572 -3.79624302]', '[ 1.44024523  0.28805217  0.83167435 -2.88121208]', '[ 1.47191686 -0.16294525 -0.53308281 -1.59501246]', '[ 1.22219612 -0.33668262 -1.96473596 -0.10466013]', '[ 0.69518377 -0.19510981 -3.2395678   1.47866752]', '[-0.02468751  0.19396218 -3.7892606   2.15486712]', '[-0.74371209  0.54810449 -3.24409779  1.19320924]', '[-1.27860878  0.64009885 -2.05305681 -0.2468104 ]', '[-1.56013879  0.47813252 -0.77443778 -1.29678962]', '[-1.59629897  0.14439787  0.39597419 -2.00758521]', '[-1.37959787 -0.38659307  1.75259808 -3.2570068 ]', '[-0.93274758 -1.05373242  2.68072547 -3.28434593]', '[-0.32767625 -1.63592515  3.28731228 -2.36503118]', '[ 0.34915268 -1.97988564  3.32186954 -0.92905383]', '[ 0.93263328 -1.96881316  2.36335677  1.08314073]', '[ 1.2382071  -1.52248934  0.6142442   3.36472859]', '[ 1.15523973 -0.5999772  -1.41521286  5.83255409]', '[ 0.736099    0.71288119 -2.52068795  6.82942758]', '[ 0.22195701  1.98537046 -2.58167388  5.84045984]', '[-0.29145309  3.07960425 -2.49737058  5.2064692 ]', '[-0.74660948 -2.17649651 -2.01865201  5.15348869]', '[-1.10399714 -1.11249995 -1.58420053  5.54711769]', '[-1.37178381  0.03197539 -0.96938094  5.70270658]', '[-1.41069051  1.04396053  0.74406157  4.16807866]', '[-1.04431822  1.6361173   2.88638223  1.64093515]', '[-0.31059663  1.67690411  4.24313171 -1.20635888]', '[ 0.55693614  1.20546901  4.22597869 -3.27390776]', '[ 1.31686559  0.49259608  3.26671337 -3.53705841]', '[ 1.83831551 -0.11232321  1.93130836 -2.40961188]', '[ 2.12254198 -0.54216219  0.93355374 -1.93032793]', '[ 2.19315223 -0.83587166 -0.22170706 -1.03164273]', '[ 2.02860153 -0.94760253 -1.45217586 -0.02222164]', '[ 1.59769852 -0.80288477 -2.88980643  1.60065987]', '[ 0.86892493 -0.26448412 -4.34488856  3.73810201]', '[-0.07582515  0.55662896 -4.85986719  3.93510521]', '[-0.97695054  1.11920249 -3.97296649  1.5150257 ]', '[-1.61868955  1.17614236 -2.39845635 -0.80315636]', '[-1.94027523  0.86606189 -0.86375356 -2.1462714 ]', '[-1.98690742  0.36128193  0.35089112 -2.84100684]', '[-1.81085091 -0.26236486  1.39884815 -3.39138215]', '[-1.42815897 -0.98738921  2.42809546 -3.79926868]', '[-0.82078431 -1.79152335  3.61996551 -4.06883016]', '[-0.00479598 -2.55069615  4.40704034 -3.40558725]', '[ 0.85015314 -3.09412797  3.95321816 -2.02024981]', '[ 1.52573662  2.93195854  2.75203752 -0.52527753]', '[1.96276836 2.94755797 1.64021901 0.6835378 ]', '[ 2.17898971 -3.04443759  0.52809586  2.2020868 ]', '[ 2.1645136  -2.46499939 -0.71864362  3.58374672]', '[ 1.87002007 -1.59679423 -2.2777498   5.21259964]', '[ 1.23189322 -0.30618751 -4.08682293  7.71067906]', '[ 0.32681452  1.25831803 -4.71674675  7.23493283]', '[-0.61897152  2.47812108 -4.66067397  5.01064582]', '[-1.47455764 -2.96594148 -3.75691768  3.51729939]', '[-2.10382428 -2.36794214 -2.56669868  2.4886974 ]', '[-2.52630181 -1.96709076 -1.72780215  1.52911916]']</t>
-  </si>
-  <si>
-    <t>[0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50, 51, 52, 53, 54, 55, 56, 57, 58, 59, 60, 61, 62, 63, 64, 65, 66, 67, 68, 69, 70, 71, 72, 73, 74, 75, 76, 77, 78, 79, 80, 81, 82, 83, 84, 85, 86, 87, 88, 89, 90, 91, 92, 93, 94, 95, 96, 97, 98, 99, 100, 101, 102, 103, 104, 105, 106, 107, 108, 109, 110, 111, 112, 113, 114, 115, 116, 117, 118, 119, 120, 121, 122, 123, 124, 125, 126, 127, 128, 129, 130, 131, 132, 133, 134, 135, 136, 137, 138, 139, 140, 141, 142, 143, 144, 145, 146, 147, 148, 149, 150, 151, 152]</t>
-  </si>
-  <si>
-    <t>[array([-0.03763371, -0.01533471,  0.06554052, -0.01816017], dtype=float32), array([-0.03406929,  0.01398622, -0.02953871,  0.30651903]), array([-0.04818188,  0.10262173, -0.10566927,  0.56184435]), array([-0.07305261,  0.22936701, -0.13369446,  0.67944384]), array([-0.0976443 ,  0.36319498, -0.10327727,  0.63282133]), array([-0.11125897,  0.47297074, -0.02773051,  0.446438  ]), array([-0.10757465,  0.53619101,  0.06462001,  0.17794954]), array([-0.06138715,  0.47788865,  0.38724178, -0.74730665]), array([ 0.0148479 ,  0.31583331,  0.35559654, -0.8357632 ]), array([ 0.09930297,  0.09142664,  0.46582003, -1.35869116]), array([ 0.16332535, -0.1339477 ,  0.15404557, -0.84595443]), array([ 0.18235609, -0.30122116,  0.02673755, -0.79482143]), array([ 0.14590118, -0.37383606, -0.38406134,  0.07245783]), array([ 0.03527538, -0.27745936, -0.69738771,  0.86037884]), array([-0.11998812, -0.04911509, -0.8171302 ,  1.35971853]), array([-0.27446392,  0.2361008 , -0.68688356,  1.41738809]), array([-0.37981758,  0.48972331, -0.33947167,  1.0653111 ]), array([-0.40298702,  0.64643178,  0.1142609 ,  0.47926481]), array([-0.31140524,  0.61390384,  0.78273553, -0.79209503]), array([-0.12730221,  0.40830999,  1.0176804 , -1.20866513]), array([ 0.07646417,  0.15901752,  0.97088125, -1.20733872]), array([ 0.24164034, -0.04359542,  0.64145158, -0.75688544]), array([ 0.32074405, -0.12512554,  0.132498  , -0.03489029]), array([ 0.29237993, -0.05545237, -0.40811238,  0.71533965]), array([ 0.16564264,  0.1465297 , -0.82706696,  1.24849611]), array([-0.02150097,  0.41463269, -0.99777939,  1.35396944]), array([-0.21406194,  0.65680873, -0.88469468,  1.00426731]), array([-0.36009124,  0.79642929, -0.54647837,  0.36049463]), array([-0.42387451,  0.79360385, -0.07924861, -0.39358516]), array([-0.36616728,  0.57821015,  0.6487642 , -1.74011   ]), array([-0.17446462,  0.11745777,  1.21820835, -2.76909406]), array([ 0.06488854, -0.40128977,  1.10531664, -2.27897652]), array([ 0.24550634, -0.75227414,  0.66593408, -1.17211119]), array([ 0.3221835 , -0.85772996,  0.0884742 ,  0.12976146]), array([ 0.27871469, -0.69966872, -0.51906269,  1.43882675]), array([ 0.12102528, -0.29527187, -1.02240929,  2.53462641]), array([-0.10634504,  0.265581  , -1.17548587,  2.9178284 ]), array([-0.31766311,  0.80771684, -0.8799268 ,  2.38888321]), array([-0.44341514,  1.19334689, -0.36043186,  1.43568333]), array([-0.45989445,  1.37706238,  0.19048027,  0.40007198]), array([-0.35357842,  1.30260741,  0.85256024, -1.13684649]), array([-0.14905568,  0.98307552,  1.1597014 , -2.02175903]), array([ 0.09366895,  0.51837134,  1.21604892, -2.53340626]), array([ 0.33804427, -0.04800581,  1.15651022, -2.98437406]), array([ 0.5244992 , -0.60985345,  0.64601523, -2.50517456]), array([ 0.58046016, -1.01571891, -0.09945626, -1.5101972 ]), array([ 0.46756448, -1.15024907, -0.99610173,  0.15692977]), array([ 0.19978521, -0.95921229, -1.63057854,  1.72272896]), array([-0.16112686, -0.48409936, -1.90970565,  2.92691139]), array([-0.52899038,  0.14714587, -1.67214986,  3.19423527]), array([-0.79300404,  0.72170751, -0.90538564,  2.43791138]), array([-0.87657093,  1.09831286,  0.08281057,  1.29991173]), array([-0.7612935 ,  1.23436216,  1.05004721,  0.04744667]), array([-0.47100635,  1.11471059,  1.80119766, -1.23241889]), array([-0.06761291,  0.75751365,  2.15384228, -2.25624219]), array([ 0.37845985,  0.20030389,  2.20786523, -3.14301834]), array([ 0.77160466, -0.41473647,  1.63035958, -2.82978822]), array([ 1.00359185, -0.88569582,  0.65257173, -1.82873797]), array([ 1.00439246, -1.07964106, -0.63877977, -0.10595551]), array([ 0.75475449, -0.92165953, -1.82814563,  1.70196993]), array([ 0.29215911, -0.40242864, -2.71981416,  3.4009048 ]), array([-0.28270921,  0.34968421, -2.87318695,  3.81151209]), array([-0.79852761,  1.00941768, -2.19101137,  2.64781845]), array([-1.13706434,  1.39633493, -1.16335187,  1.23966564]), array([-1.2567158 ,  1.51649348, -0.02514887, -0.02019668]), array([-1.12850633,  1.33712336,  1.30278649, -1.79973863]), array([-0.7612539 ,  0.83685739,  2.33516736, -3.20547935]), array([-0.19649419,  0.01989647,  3.18783002, -4.73038924]), array([ 0.43831017, -0.89271836,  2.99547048, -4.05767834]), array([ 0.93953676, -1.48586713,  1.96739248, -1.88455117]), array([ 1.22832582, -1.71369181,  0.89302593, -0.42965225]), array([ 1.28182642, -1.64529542, -0.36509705,  1.10308891]), array([ 1.0727456 , -1.24118917, -1.72475692,  2.98384385]), array([ 0.59615425, -0.43230443, -2.98994725,  5.05593603]), array([-0.06308492,  0.658387  , -3.39114323,  5.37830167]), array([-0.69215516,  1.57263518, -2.81539867,  3.65549037]), array([-1.16750471,  2.12759373, -1.89234011,  1.94376012]), array([-1.43494014,  2.36920437, -0.76096306,  0.50726597]), array([-1.46791456,  2.33867322,  0.43376124, -0.80750797]), array([-1.26277448,  2.04155916,  1.60692755, -2.1947103 ]), array([-0.83294746,  1.44019935,  2.66457111, -3.87985375]), array([-0.19058985,  0.41832475,  3.6769793 , -6.22015924]), array([ 0.54684577, -0.84375042,  3.44444384, -5.82560843]), array([ 1.13123198, -1.80472187,  2.36367429, -3.80977643]), array([ 1.47180653, -2.36008252,  1.03798567, -1.82511382]), array([ 1.54574893, -2.55115374, -0.29691277, -0.09793767]), array([ 1.35481395, -2.39622631, -1.60225679,  1.67352408]), array([ 0.91325278, -1.8617804 , -2.78313849,  3.75062494]), array([ 0.25293266, -0.85543034, -3.78917775,  6.35400664]), array([-0.54189201,  0.55242731, -3.85972312,  7.02075202]), array([-1.19356808,  1.73837723, -2.6018301 ,  4.80224722]), array([-1.58343458,  2.52309061, -1.30232062,  3.14365282]), array([-1.71873378,  3.01606417, -0.0653592 ,  1.80285799]), array([-1.61397383, -3.03851898,  1.10946726,  0.48255371]), array([-1.2747231 , -3.07173686,  2.27660914, -0.79888632]), array([-0.71539654,  2.93449206,  3.24560207, -1.94417594]), array([-0.02521543,  2.4450859 ,  3.50375886, -2.91205427]), array([ 0.63877177,  1.75271946,  3.03573954, -3.93269504]), array([ 1.14986527,  0.96580281,  2.03885572, -3.79624302]), array([ 1.44024523,  0.28805217,  0.83167435, -2.88121208]), array([ 1.47191686, -0.16294525, -0.53308281, -1.59501246]), array([ 1.22219612, -0.33668262, -1.96473596, -0.10466013]), array([ 0.69518377, -0.19510981, -3.2395678 ,  1.47866752]), array([-0.02468751,  0.19396218, -3.7892606 ,  2.15486712]), array([-0.74371209,  0.54810449, -3.24409779,  1.19320924]), array([-1.27860878,  0.64009885, -2.05305681, -0.2468104 ]), array([-1.56013879,  0.47813252, -0.77443778, -1.29678962]), array([-1.59629897,  0.14439787,  0.39597419, -2.00758521]), array([-1.37959787, -0.38659307,  1.75259808, -3.2570068 ]), array([-0.93274758, -1.05373242,  2.68072547, -3.28434593]), array([-0.32767625, -1.63592515,  3.28731228, -2.36503118]), array([ 0.34915268, -1.97988564,  3.32186954, -0.92905383]), array([ 0.93263328, -1.96881316,  2.36335677,  1.08314073]), array([ 1.2382071 , -1.52248934,  0.6142442 ,  3.36472859]), array([ 1.15523973, -0.5999772 , -1.41521286,  5.83255409]), array([ 0.736099  ,  0.71288119, -2.52068795,  6.82942758]), array([ 0.22195701,  1.98537046, -2.58167388,  5.84045984]), array([-0.29145309,  3.07960425, -2.49737058,  5.2064692 ]), array([-0.74660948, -2.17649651, -2.01865201,  5.15348869]), array([-1.10399714, -1.11249995, -1.58420053,  5.54711769]), array([-1.37178381,  0.03197539, -0.96938094,  5.70270658]), array([-1.41069051,  1.04396053,  0.74406157,  4.16807866]), array([-1.04431822,  1.6361173 ,  2.88638223,  1.64093515]), array([-0.31059663,  1.67690411,  4.24313171, -1.20635888]), array([ 0.55693614,  1.20546901,  4.22597869, -3.27390776]), array([ 1.31686559,  0.49259608,  3.26671337, -3.53705841]), array([ 1.83831551, -0.11232321,  1.93130836, -2.40961188]), array([ 2.12254198, -0.54216219,  0.93355374, -1.93032793]), array([ 2.19315223, -0.83587166, -0.22170706, -1.03164273]), array([ 2.02860153, -0.94760253, -1.45217586, -0.02222164]), array([ 1.59769852, -0.80288477, -2.88980643,  1.60065987]), array([ 0.86892493, -0.26448412, -4.34488856,  3.73810201]), array([-0.07582515,  0.55662896, -4.85986719,  3.93510521]), array([-0.97695054,  1.11920249, -3.97296649,  1.5150257 ]), array([-1.61868955,  1.17614236, -2.39845635, -0.80315636]), array([-1.94027523,  0.86606189, -0.86375356, -2.1462714 ]), array([-1.98690742,  0.36128193,  0.35089112, -2.84100684]), array([-1.81085091, -0.26236486,  1.39884815, -3.39138215]), array([-1.42815897, -0.98738921,  2.42809546, -3.79926868]), array([-0.82078431, -1.79152335,  3.61996551, -4.06883016]), array([-0.00479598, -2.55069615,  4.40704034, -3.40558725]), array([ 0.85015314, -3.09412797,  3.95321816, -2.02024981]), array([ 1.52573662,  2.93195854,  2.75203752, -0.52527753]), array([1.96276836, 2.94755797, 1.64021901, 0.6835378 ]), array([ 2.17898971, -3.04443759,  0.52809586,  2.2020868 ]), array([ 2.1645136 , -2.46499939, -0.71864362,  3.58374672]), array([ 1.87002007, -1.59679423, -2.2777498 ,  5.21259964]), array([ 1.23189322, -0.30618751, -4.08682293,  7.71067906]), array([ 0.32681452,  1.25831803, -4.71674675,  7.23493283]), array([-0.61897152,  2.47812108, -4.66067397,  5.01064582]), array([-1.47455764, -2.96594148, -3.75691768,  3.51729939]), array([-2.10382428, -2.36794214, -2.56669868,  2.4886974 ]), array([-2.52630181, -1.96709076, -1.72780215,  1.52911916])]</t>
-  </si>
-  <si>
-    <t>['[1,1,2]', '[2,2,2]', '[0,0,0]', '[2,0,1]', '[1,1,1]', '[1,2,0]', '[0,2,1]', '[1,0,2]', '[0,1,1]', '[2,1,0]']</t>
-  </si>
-  <si>
-    <t>[3, 12, 13, 14, 20, 21, 22, 23, 25, 33, 34, 36, 38, 45, 46, 47, 48, 49, 50, 57, 58, 59, 60, 62, 69, 70, 71, 74, 75, 82, 83, 84, 85, 86, 87, 94, 95, 96, 98, 99, 100, 107, 108, 109, 110, 111, 112, 121, 122, 124, 125, 134, 135, 136, 137, 138, 139, 149, 150, 151, 152, 153, 161, 162, 163, 166, 167, 175, 176, 177, 178, 179, 180, 181, 182, 189, 191, 194, 195, 196]</t>
-  </si>
-  <si>
-    <t>[0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 1, 2, 2, 2, 2, 2, 2, 1, 0, 0, 0, 0, 0, 0, 1, 2, 2, 2]</t>
-  </si>
-  <si>
-    <t>['[-0.03763371 -0.01533471  0.06554052 -0.01816017]', '[-0.00754409 -0.05458322  0.2277812  -0.36241836]', '[ 0.04879627 -0.15231473  0.32089719 -0.5887683 ]', '[ 0.08773348 -0.20975891  0.05953656  0.02857539]', '[ 0.07159701 -0.14038323 -0.21558016  0.65104861]', '[ 0.00648475  0.0393353  -0.41626589  1.10429103]', '[-0.08485445  0.27989065 -0.46991633  1.24354086]', '[-0.17036214  0.5133148  -0.36181811  1.04111741]', '[-0.22198773  0.68003836 -0.14247549  0.59860378]', '[-0.2247793   0.74576291  0.11471656  0.05210182]', '[-0.15422799  0.63893119  0.57773327 -1.10356161]', '[-0.0023089   0.31819547  0.90819171 -2.04242503]', '[ 0.16335727 -0.07163389  0.6989554  -1.75467039]', '[ 0.260328   -0.34854978  0.24441548 -0.95686136]', '[ 0.25582347 -0.44075416 -0.28856962  0.04475653]', '[ 0.14964711 -0.33391506 -0.75002829  0.99473863]', '[-0.03048365 -0.06328525 -1.00711442  1.63791248]', '[-0.23195071  0.28360515 -0.95417778  1.73421539]', '[-0.39198504  0.59405158 -0.60794297  1.30280618]', '[-0.46413994  0.78568761 -0.09947429  0.58680506]', '[-0.43024189  0.82344084  0.43144695 -0.20967876]', '[-0.29814246  0.7060945   0.86358521 -0.9387245 ]', '[-0.09901331  0.46477367  1.08422152 -1.41387129]', '[ 0.11501764  0.17239305  1.00367257 -1.42334577]', '[ 0.30835781 -0.13807238  0.88074596 -1.59474157]', '[ 0.42286873 -0.36460764  0.23850787 -0.62410743]', '[ 0.42489348 -0.44537753 -0.22037493 -0.17152837]', '[ 0.31213901 -0.36626105 -0.8842284   0.94014038]', '[ 0.08626765 -0.08863852 -1.32204698  1.75671548]', '[-0.19005635  0.29228296 -1.37088889  1.93253708]', '[-0.43461259  0.63840332 -1.02030235  1.44495117]', '[-0.58155016  0.8478039  -0.42313014  0.61947173]', '[-0.59808071  0.88043736  0.2600028  -0.29569764]', '[-0.48092938  0.73199739  0.89100198 -1.16909057]', '[-0.25505696  0.42826033  1.32042806 -1.80238751]', '[ 0.04863929 -0.01785078  1.64070833 -2.52743911]', '[ 0.33972077 -0.45080901  1.20035104 -1.68347834]', '[ 0.53293399 -0.72524218  0.69337086 -1.00850131]', '[ 0.58339859 -0.78048666 -0.19595776  0.4599737 ]', '[ 0.45634185 -0.54363959 -1.0546537   1.88322324]', '[ 0.17776173 -0.05193648 -1.66326364  2.91287863]', '[-0.1710494   0.54885345 -1.72738226  2.90832283]', '[-0.47913003  1.05066473 -1.29490274  2.02440031]', '[-0.67266701  1.34237114 -0.61438249  0.87855936]', '[-0.71836102  1.40055853  0.16317478 -0.29682968]', '[-0.60879588  1.2237411   0.91873814 -1.4676328 ]', '[-0.36064385  0.81874729  1.52453048 -2.54363075]', '[-0.0225871   0.24077028  1.77353328 -3.08896399]', '[ 0.30788305 -0.33819179  1.43896632 -2.52410537]', '[ 0.52472134 -0.71862577  0.6889244  -1.2191338 ]', '[ 0.57488062 -0.81574317 -0.19325512  0.25389961]', '[ 0.44960525 -0.61843324 -1.04014101  1.69961898]', '[ 0.17374441 -0.15602853 -1.65598358  2.81916814]', '[-0.17651006  0.44123885 -1.74722296  2.9630481 ]', '[-0.48859292  0.96230381 -1.30988907  2.14792187]', '[-0.6831287   1.28064457 -0.6093088   1.01768546]', '[-0.72623322  1.36730582  0.18244546 -0.15174794]', '[-0.61228375  1.21993999  0.94137223 -1.31838586]', '[-0.36021851  0.84498115  1.53997614 -2.39469431]', '[-0.01956767  0.29413648  1.78689681 -2.97622872]', '[ 0.31483549 -0.27036773  1.46477898 -2.49297241]', '[ 0.56164361 -0.71479943  0.94787702 -1.85823951]', '[ 0.65677814 -0.93185252 -0.00601966 -0.3023268 ]', '[ 0.5602608  -0.83501108 -0.94476574  1.26574463]', '[ 0.2898836  -0.43350041 -1.71125383  2.68844961]', '[-0.09299516  0.18765779 -2.01237761  3.32349345]', '[-0.46872335  0.80644123 -1.65482477  2.70472871]', '[-0.7300172   1.23449715 -0.92140969  1.54430265]', '[-0.82843496  1.42129479 -0.05309185  0.32392657]', '[-0.75140317  1.36384022  0.81223936 -0.90019707]', '[-0.51221484  1.06114225  1.54645999 -2.11416608]', '[-0.15215407  0.53510552  1.98522881 -3.04822306]', '[ 0.2693206  -0.15712825  2.11289726 -3.64663618]', '[ 0.64334806 -0.82591322  1.53861338 -2.88286375]', '[ 0.84241352 -1.22483236  0.4377212  -1.10886382]', '[ 0.81762511 -1.27267659 -0.67809875  0.63064891]', '[ 0.57757146 -0.9688954  -1.69632955  2.412197  ]', '[ 0.1564347  -0.31892383 -2.43617609  3.96626781]', '[-0.34371707  0.51348309 -2.41443141  4.05010934]', '[-0.75959537  1.2071263  -1.67563696  2.79347319]', '[-0.9990248   1.62562214 -0.69834781  1.40423979]', '[-1.03483513  1.77382487  0.34016971  0.0813942 ]', '[-0.86712635  1.65564816  1.31509672 -1.27579712]', '[-0.52217919  1.25802566  2.0904605  -2.70100274]', '[-0.05429747  0.59007898  2.50601296 -3.86045879]', '[ 0.43094897 -0.19194541  2.2076655  -3.67618068]', '[ 0.7814019  -0.78800617  1.23193366 -2.18128924]', '[ 0.91185718 -1.05442782  0.06340569 -0.48403123]', '[ 0.80757838 -0.98141044 -1.09369742  1.2207292 ]', '[ 0.48417398 -0.56477682 -2.09584084  2.91243194]', '[ 1.56419446e-03  1.35299104e-01 -2.60575567e+00  3.85212448e+00]', '[-0.49845883  0.85673049 -2.27581475  3.14611063]', '[-0.87678522  1.35127816 -1.45943656  1.77622044]', '[-1.06956092  1.57133827 -0.44947704  0.44055317]', '[-1.05301024  1.53139626  0.61377262 -0.84124087]', '[-0.82834305  1.23006039  1.61146272 -2.18639816]', '[-0.42268572  0.65725664  2.38580483 -3.48374871]', '[ 0.11152521 -0.16380428  2.81037844 -4.43503313]', '[ 0.61001502 -0.91509114  2.07162231 -2.90044962]', '[ 0.91844603 -1.30629576  0.98318205 -1.02390794]', '[ 0.9957255  -1.33272669 -0.22007569  0.75053251]', '[ 0.8295615  -1.00305999 -1.43417096  2.56327902]', '[ 0.43175751 -0.3078844  -2.47817087  4.29267866]', '[-0.10760959  0.60661382 -2.74830437  4.50047444]', '[-0.61160082  1.38106519 -2.21205978  3.13466497]', '[-0.97207669  1.85480704 -1.3549129   1.62212476]', '[-1.14190561  2.0394027  -0.32557123  0.24090041]', '[-1.09934589  1.95385622  0.74789209 -1.10118376]', '[-0.84805173  1.59218335  1.74225999 -2.54060473]', '[-0.41545113  0.92874846  2.53620015 -4.075531  ]', '[ 0.13066405  0.01625333  2.77467795 -4.74545844]', '[ 0.62269956 -0.81816993  2.02540287 -3.3689016 ]', '[ 0.91753236 -1.30339942  0.89964086 -1.49172417]', '[ 0.99704606 -1.47493982 -0.11042089 -0.22762058]', '[ 0.85669606 -1.34137617 -1.27883204  1.57971443]', '[ 0.4945542  -0.83353967 -2.30670667  3.49896613]', '[-0.03743679  0.02144987 -2.8775197   4.7850093 ]', '[-0.58279238  0.92461064 -2.43397021  3.9666225 ]', '[-0.97917906  1.56419526 -1.49201333  2.42766245]', '[-1.17057568  1.90685687 -0.40921681  1.02269386]', '[-1.14121743  1.97748637  0.69707561 -0.31974616]', '[-0.89837303  1.77287067  1.70273825 -1.74875625]', '[-0.47646873  1.26886897  2.46612312 -3.29628182]', '[ 0.08476776  0.41214599  3.05386271 -5.11885133]', '[ 0.65016711 -0.56409422  2.42787462 -4.27644696]', '[ 1.01537578 -1.22616097  1.19106042 -2.32876397]', '[ 1.14163066 -1.55918207  0.06427874 -1.00976618]', '[ 1.02537133 -1.57983444 -1.20909843  0.81863483]', '[ 0.6688623  -1.2188474  -2.32031167  2.82530763]', '[ 0.11685132 -0.44865551 -3.11439743  4.75904229]', '[-0.5118339   0.55066851 -2.97924222  4.81536852]', '[-1.0164177   1.36246429 -2.0029334   3.23527212]', '[-1.30228706  1.85678633 -0.84198523  1.75028445]', '[-1.35046715  2.07332103  0.36009236  0.42081527]', '[-1.16148779  2.02009597  1.51079987 -0.97935221]', '[-0.75946834  1.66749934  2.46170217 -2.58127401]', '[-0.20093288  0.98085075  3.05277311 -4.24333751]', '[ 0.41861179  0.041378    2.98259405 -4.80828861]', '[ 0.92133966 -0.78823305  1.93725893 -3.28370304]', '[ 1.17648663 -1.25689063  0.60328097 -1.42705727]', '[ 1.18128005 -1.42009852 -0.5548214  -0.1978084 ]', '[ 0.94024927 -1.27465868 -1.83230966  1.68893975]', '[ 0.46231203 -0.72984729 -2.89293256  3.74650972]', '[-0.17596309  0.16234516 -3.32018257  4.82423241]', '[-0.7877488   1.03166893 -2.66941575  3.63308173]', '[-1.2181114   1.59460288 -1.60297494  2.02969123]', '[-1.42166039  1.86304139 -0.42270799  0.68989911]', '[-1.37024286  1.83049979  0.93403953 -1.02681168]', '[-1.05091774  1.43547968  2.24778517 -2.99238805]', '[-0.50012051  0.66326343  3.19965196 -4.68569753]', '[ 0.17409255 -0.33479722  3.34266504 -4.85847179]', '[ 0.76404017 -1.12543787  2.45986226 -2.90470556]', '[ 1.13834888 -1.49815573  1.25229569 -0.86829466]', '[ 1.25629154 -1.48988273 -0.08564705  0.92888455]', '[ 1.10145676 -1.12451844 -1.46358919  2.75609114]', '[ 0.67496928 -0.37413143 -2.75201922  4.69441456]', '[ 0.05437035  0.64500651 -3.26521868  5.07833099]', '[-0.56645822  1.51776625 -2.85095982  3.51566176]', '[-1.05969674  2.04674642 -2.02459333  1.8063002 ]', '[-1.35784605  2.2565665  -0.92729487  0.32736033]', '[-1.42418309  2.18766799  0.27024909 -1.00571039]', '[-1.24994325  1.85151948  1.46512381 -2.38400413]', '[-0.84359444  1.21430526  2.57681795 -4.04029488]', '[-0.23826001  0.2403556   3.35560679 -5.47946238]', '[ 0.43794126 -0.85344976  3.19983208 -5.00539192]', '[ 0.99269155 -1.67330303  2.29692662 -3.18393653]', '[ 1.32863386 -2.10430819  1.04534244 -1.19262055]', '[ 1.40615409 -2.16609527 -0.27513317  0.56109564]', '[ 1.21876378 -1.87538438 -1.59323381  2.38532451]', '[ 0.77240714 -1.1835625  -2.86048246  4.62030414]', '[ 0.09022406 -0.02563064 -3.80032157  6.62616137]', '[-0.63530729  1.2079394  -3.25876147  5.28434338]', '[-1.18604356  2.06195467 -2.22276138  3.3321148 ]', '[-1.51560813  2.57315436 -1.05804926  1.83394048]', '[-1.607108    2.80644962  0.14292836  0.50718259]', '[-1.45920622  2.77474133  1.33129003 -0.83520957]', '[-1.08048848  2.46471451  2.42101096 -2.29560582]', '[-0.51503806  1.84000559  3.15960749 -3.99492115]', '[ 0.15477709  0.86019743  3.46675828 -5.72095063]', '[ 0.81346415 -0.31740387  2.91085862 -5.56815826]', '[ 1.25306372 -1.22809617  1.43538149 -3.48300273]', '[ 1.38743525 -1.73162641 -0.08178716 -1.59092042]', '[ 1.22631061 -1.86512034 -1.5055186   0.28435222]', '[ 0.80043248 -1.59881721 -2.70085592  2.43305757]', '[ 0.1712816  -0.87495264 -3.52025701  4.7810829 ]', '[-0.55871418  0.2244281  -3.5746857   5.73876019]', '[-1.17447998  1.22934413 -2.48476869  4.14009557]', '[-1.5431084   1.89446453 -1.19753927  2.58438143]', '[-1.65329747  2.28292182  0.0940657   1.3162175 ]', '[-1.50704386  2.41666418  1.360614   -0.00762813]', '[-1.10367419  2.22204837  2.63365255 -1.99337116]', '[-0.49295993  1.63905366  3.39610723 -3.87680429]', '[ 0.24312478  0.6190214   3.88298347 -6.19887812]', '[ 0.98376292 -0.65534743  3.2885646  -5.98509008]', '[ 1.4826311  -1.6096074   1.69843045 -3.63226895]', '[ 1.67036404 -2.15139918  0.1936074  -1.84398377]', '[ 1.56493484 -2.35142138 -1.23540632 -0.1343098 ]', '[ 1.18339686 -2.18779182 -2.54721082  1.83106867]', '[ 0.56775074 -1.58947284 -3.54626772  4.23075342]', '[-0.21138017 -0.48032662 -4.14929488  6.68940183]']</t>
-  </si>
-  <si>
-    <t>[array([-0.03763371, -0.01533471,  0.06554052, -0.01816017], dtype=float32), array([-0.00754409, -0.05458322,  0.2277812 , -0.36241836]), array([ 0.04879627, -0.15231473,  0.32089719, -0.5887683 ]), array([ 0.08773348, -0.20975891,  0.05953656,  0.02857539]), array([ 0.07159701, -0.14038323, -0.21558016,  0.65104861]), array([ 0.00648475,  0.0393353 , -0.41626589,  1.10429103]), array([-0.08485445,  0.27989065, -0.46991633,  1.24354086]), array([-0.17036214,  0.5133148 , -0.36181811,  1.04111741]), array([-0.22198773,  0.68003836, -0.14247549,  0.59860378]), array([-0.2247793 ,  0.74576291,  0.11471656,  0.05210182]), array([-0.15422799,  0.63893119,  0.57773327, -1.10356161]), array([-0.0023089 ,  0.31819547,  0.90819171, -2.04242503]), array([ 0.16335727, -0.07163389,  0.6989554 , -1.75467039]), array([ 0.260328  , -0.34854978,  0.24441548, -0.95686136]), array([ 0.25582347, -0.44075416, -0.28856962,  0.04475653]), array([ 0.14964711, -0.33391506, -0.75002829,  0.99473863]), array([-0.03048365, -0.06328525, -1.00711442,  1.63791248]), array([-0.23195071,  0.28360515, -0.95417778,  1.73421539]), array([-0.39198504,  0.59405158, -0.60794297,  1.30280618]), array([-0.46413994,  0.78568761, -0.09947429,  0.58680506]), array([-0.43024189,  0.82344084,  0.43144695, -0.20967876]), array([-0.29814246,  0.7060945 ,  0.86358521, -0.9387245 ]), array([-0.09901331,  0.46477367,  1.08422152, -1.41387129]), array([ 0.11501764,  0.17239305,  1.00367257, -1.42334577]), array([ 0.30835781, -0.13807238,  0.88074596, -1.59474157]), array([ 0.42286873, -0.36460764,  0.23850787, -0.62410743]), array([ 0.42489348, -0.44537753, -0.22037493, -0.17152837]), array([ 0.31213901, -0.36626105, -0.8842284 ,  0.94014038]), array([ 0.08626765, -0.08863852, -1.32204698,  1.75671548]), array([-0.19005635,  0.29228296, -1.37088889,  1.93253708]), array([-0.43461259,  0.63840332, -1.02030235,  1.44495117]), array([-0.58155016,  0.8478039 , -0.42313014,  0.61947173]), array([-0.59808071,  0.88043736,  0.2600028 , -0.29569764]), array([-0.48092938,  0.73199739,  0.89100198, -1.16909057]), array([-0.25505696,  0.42826033,  1.32042806, -1.80238751]), array([ 0.04863929, -0.01785078,  1.64070833, -2.52743911]), array([ 0.33972077, -0.45080901,  1.20035104, -1.68347834]), array([ 0.53293399, -0.72524218,  0.69337086, -1.00850131]), array([ 0.58339859, -0.78048666, -0.19595776,  0.4599737 ]), array([ 0.45634185, -0.54363959, -1.0546537 ,  1.88322324]), array([ 0.17776173, -0.05193648, -1.66326364,  2.91287863]), array([-0.1710494 ,  0.54885345, -1.72738226,  2.90832283]), array([-0.47913003,  1.05066473, -1.29490274,  2.02440031]), array([-0.67266701,  1.34237114, -0.61438249,  0.87855936]), array([-0.71836102,  1.40055853,  0.16317478, -0.29682968]), array([-0.60879588,  1.2237411 ,  0.91873814, -1.4676328 ]), array([-0.36064385,  0.81874729,  1.52453048, -2.54363075]), array([-0.0225871 ,  0.24077028,  1.77353328, -3.08896399]), array([ 0.30788305, -0.33819179,  1.43896632, -2.52410537]), array([ 0.52472134, -0.71862577,  0.6889244 , -1.2191338 ]), array([ 0.57488062, -0.81574317, -0.19325512,  0.25389961]), array([ 0.44960525, -0.61843324, -1.04014101,  1.69961898]), array([ 0.17374441, -0.15602853, -1.65598358,  2.81916814]), array([-0.17651006,  0.44123885, -1.74722296,  2.9630481 ]), array([-0.48859292,  0.96230381, -1.30988907,  2.14792187]), array([-0.6831287 ,  1.28064457, -0.6093088 ,  1.01768546]), array([-0.72623322,  1.36730582,  0.18244546, -0.15174794]), array([-0.61228375,  1.21993999,  0.94137223, -1.31838586]), array([-0.36021851,  0.84498115,  1.53997614, -2.39469431]), array([-0.01956767,  0.29413648,  1.78689681, -2.97622872]), array([ 0.31483549, -0.27036773,  1.46477898, -2.49297241]), array([ 0.56164361, -0.71479943,  0.94787702, -1.85823951]), array([ 0.65677814, -0.93185252, -0.00601966, -0.3023268 ]), array([ 0.5602608 , -0.83501108, -0.94476574,  1.26574463]), array([ 0.2898836 , -0.43350041, -1.71125383,  2.68844961]), array([-0.09299516,  0.18765779, -2.01237761,  3.32349345]), array([-0.46872335,  0.80644123, -1.65482477,  2.70472871]), array([-0.7300172 ,  1.23449715, -0.92140969,  1.54430265]), array([-0.82843496,  1.42129479, -0.05309185,  0.32392657]), array([-0.75140317,  1.36384022,  0.81223936, -0.90019707]), array([-0.51221484,  1.06114225,  1.54645999, -2.11416608]), array([-0.15215407,  0.53510552,  1.98522881, -3.04822306]), array([ 0.2693206 , -0.15712825,  2.11289726, -3.64663618]), array([ 0.64334806, -0.82591322,  1.53861338, -2.88286375]), array([ 0.84241352, -1.22483236,  0.4377212 , -1.10886382]), array([ 0.81762511, -1.27267659, -0.67809875,  0.63064891]), array([ 0.57757146, -0.9688954 , -1.69632955,  2.412197  ]), array([ 0.1564347 , -0.31892383, -2.43617609,  3.96626781]), array([-0.34371707,  0.51348309, -2.41443141,  4.05010934]), array([-0.75959537,  1.2071263 , -1.67563696,  2.79347319]), array([-0.9990248 ,  1.62562214, -0.69834781,  1.40423979]), array([-1.03483513,  1.77382487,  0.34016971,  0.0813942 ]), array([-0.86712635,  1.65564816,  1.31509672, -1.27579712]), array([-0.52217919,  1.25802566,  2.0904605 , -2.70100274]), array([-0.05429747,  0.59007898,  2.50601296, -3.86045879]), array([ 0.43094897, -0.19194541,  2.2076655 , -3.67618068]), array([ 0.7814019 , -0.78800617,  1.23193366, -2.18128924]), array([ 0.91185718, -1.05442782,  0.06340569, -0.48403123]), array([ 0.80757838, -0.98141044, -1.09369742,  1.2207292 ]), array([ 0.48417398, -0.56477682, -2.09584084,  2.91243194]), array([ 1.56419446e-03,  1.35299104e-01, -2.60575567e+00,  3.85212448e+00]), array([-0.49845883,  0.85673049, -2.27581475,  3.14611063]), array([-0.87678522,  1.35127816, -1.45943656,  1.77622044]), array([-1.06956092,  1.57133827, -0.44947704,  0.44055317]), array([-1.05301024,  1.53139626,  0.61377262, -0.84124087]), array([-0.82834305,  1.23006039,  1.61146272, -2.18639816]), array([-0.42268572,  0.65725664,  2.38580483, -3.48374871]), array([ 0.11152521, -0.16380428,  2.81037844, -4.43503313]), array([ 0.61001502, -0.91509114,  2.07162231, -2.90044962]), array([ 0.91844603, -1.30629576,  0.98318205, -1.02390794]), array([ 0.9957255 , -1.33272669, -0.22007569,  0.75053251]), array([ 0.8295615 , -1.00305999, -1.43417096,  2.56327902]), array([ 0.43175751, -0.3078844 , -2.47817087,  4.29267866]), array([-0.10760959,  0.60661382, -2.74830437,  4.50047444]), array([-0.61160082,  1.38106519, -2.21205978,  3.13466497]), array([-0.97207669,  1.85480704, -1.3549129 ,  1.62212476]), array([-1.14190561,  2.0394027 , -0.32557123,  0.24090041]), array([-1.09934589,  1.95385622,  0.74789209, -1.10118376]), array([-0.84805173,  1.59218335,  1.74225999, -2.54060473]), array([-0.41545113,  0.92874846,  2.53620015, -4.075531  ]), array([ 0.13066405,  0.01625333,  2.77467795, -4.74545844]), array([ 0.62269956, -0.81816993,  2.02540287, -3.3689016 ]), array([ 0.91753236, -1.30339942,  0.89964086, -1.49172417]), array([ 0.99704606, -1.47493982, -0.11042089, -0.22762058]), array([ 0.85669606, -1.34137617, -1.27883204,  1.57971443]), array([ 0.4945542 , -0.83353967, -2.30670667,  3.49896613]), array([-0.03743679,  0.02144987, -2.8775197 ,  4.7850093 ]), array([-0.58279238,  0.92461064, -2.43397021,  3.9666225 ]), array([-0.97917906,  1.56419526, -1.49201333,  2.42766245]), array([-1.17057568,  1.90685687, -0.40921681,  1.02269386]), array([-1.14121743,  1.97748637,  0.69707561, -0.31974616]), array([-0.89837303,  1.77287067,  1.70273825, -1.74875625]), array([-0.47646873,  1.26886897,  2.46612312, -3.29628182]), array([ 0.08476776,  0.41214599,  3.05386271, -5.11885133]), array([ 0.65016711, -0.56409422,  2.42787462, -4.27644696]), array([ 1.01537578, -1.22616097,  1.19106042, -2.32876397]), array([ 1.14163066, -1.55918207,  0.06427874, -1.00976618]), array([ 1.02537133, -1.57983444, -1.20909843,  0.81863483]), array([ 0.6688623 , -1.2188474 , -2.32031167,  2.82530763]), array([ 0.11685132, -0.44865551, -3.11439743,  4.75904229]), array([-0.5118339 ,  0.55066851, -2.97924222,  4.81536852]), array([-1.0164177 ,  1.36246429, -2.0029334 ,  3.23527212]), array([-1.30228706,  1.85678633, -0.84198523,  1.75028445]), array([-1.35046715,  2.07332103,  0.36009236,  0.42081527]), array([-1.16148779,  2.02009597,  1.51079987, -0.97935221]), array([-0.75946834,  1.66749934,  2.46170217, -2.58127401]), array([-0.20093288,  0.98085075,  3.05277311, -4.24333751]), array([ 0.41861179,  0.041378  ,  2.98259405, -4.80828861]), array([ 0.92133966, -0.78823305,  1.93725893, -3.28370304]), array([ 1.17648663, -1.25689063,  0.60328097, -1.42705727]), array([ 1.18128005, -1.42009852, -0.5548214 , -0.1978084 ]), array([ 0.94024927, -1.27465868, -1.83230966,  1.68893975]), array([ 0.46231203, -0.72984729, -2.89293256,  3.74650972]), array([-0.17596309,  0.16234516, -3.32018257,  4.82423241]), array([-0.7877488 ,  1.03166893, -2.66941575,  3.63308173]), array([-1.2181114 ,  1.59460288, -1.60297494,  2.02969123]), array([-1.42166039,  1.86304139, -0.42270799,  0.68989911]), array([-1.37024286,  1.83049979,  0.93403953, -1.02681168]), array([-1.05091774,  1.43547968,  2.24778517, -2.99238805]), array([-0.50012051,  0.66326343,  3.19965196, -4.68569753]), array([ 0.17409255, -0.33479722,  3.34266504, -4.85847179]), array([ 0.76404017, -1.12543787,  2.45986226, -2.90470556]), array([ 1.13834888, -1.49815573,  1.25229569, -0.86829466]), array([ 1.25629154, -1.48988273, -0.08564705,  0.92888455]), array([ 1.10145676, -1.12451844, -1.46358919,  2.75609114]), array([ 0.67496928, -0.37413143, -2.75201922,  4.69441456]), array([ 0.05437035,  0.64500651, -3.26521868,  5.07833099]), array([-0.56645822,  1.51776625, -2.85095982,  3.51566176]), array([-1.05969674,  2.04674642, -2.02459333,  1.8063002 ]), array([-1.35784605,  2.2565665 , -0.92729487,  0.32736033]), array([-1.42418309,  2.18766799,  0.27024909, -1.00571039]), array([-1.24994325,  1.85151948,  1.46512381, -2.38400413]), array([-0.84359444,  1.21430526,  2.57681795, -4.04029488]), array([-0.23826001,  0.2403556 ,  3.35560679, -5.47946238]), array([ 0.43794126, -0.85344976,  3.19983208, -5.00539192]), array([ 0.99269155, -1.67330303,  2.29692662, -3.18393653]), array([ 1.32863386, -2.10430819,  1.04534244, -1.19262055]), array([ 1.40615409, -2.16609527, -0.27513317,  0.56109564]), array([ 1.21876378, -1.87538438, -1.59323381,  2.38532451]), array([ 0.77240714, -1.1835625 , -2.86048246,  4.62030414]), array([ 0.09022406, -0.02563064, -3.80032157,  6.62616137]), array([-0.63530729,  1.2079394 , -3.25876147,  5.28434338]), array([-1.18604356,  2.06195467, -2.22276138,  3.3321148 ]), array([-1.51560813,  2.57315436, -1.05804926,  1.83394048]), array([-1.607108  ,  2.80644962,  0.14292836,  0.50718259]), array([-1.45920622,  2.77474133,  1.33129003, -0.83520957]), array([-1.08048848,  2.46471451,  2.42101096, -2.29560582]), array([-0.51503806,  1.84000559,  3.15960749, -3.99492115]), array([ 0.15477709,  0.86019743,  3.46675828, -5.72095063]), array([ 0.81346415, -0.31740387,  2.91085862, -5.56815826]), array([ 1.25306372, -1.22809617,  1.43538149, -3.48300273]), array([ 1.38743525, -1.73162641, -0.08178716, -1.59092042]), array([ 1.22631061, -1.86512034, -1.5055186 ,  0.28435222]), array([ 0.80043248, -1.59881721, -2.70085592,  2.43305757]), array([ 0.1712816 , -0.87495264, -3.52025701,  4.7810829 ]), array([-0.55871418,  0.2244281 , -3.5746857 ,  5.73876019]), array([-1.17447998,  1.22934413, -2.48476869,  4.14009557]), array([-1.5431084 ,  1.89446453, -1.19753927,  2.58438143]), array([-1.65329747,  2.28292182,  0.0940657 ,  1.3162175 ]), array([-1.50704386,  2.41666418,  1.360614  , -0.00762813]), array([-1.10367419,  2.22204837,  2.63365255, -1.99337116]), array([-0.49295993,  1.63905366,  3.39610723, -3.87680429]), array([ 0.24312478,  0.6190214 ,  3.88298347, -6.19887812]), array([ 0.98376292, -0.65534743,  3.2885646 , -5.98509008]), array([ 1.4826311 , -1.6096074 ,  1.69843045, -3.63226895]), array([ 1.67036404, -2.15139918,  0.1936074 , -1.84398377]), array([ 1.56493484, -2.35142138, -1.23540632, -0.1343098 ]), array([ 1.18339686, -2.18779182, -2.54721082,  1.83106867]), array([ 0.56775074, -1.58947284, -3.54626772,  4.23075342]), array([-0.21138017, -0.48032662, -4.14929488,  6.68940183])]</t>
-  </si>
-  <si>
-    <t>['[2,1,0]', '[1,1,2]', '[0,2,1]', '[0,1,1]', '[1,2,0]', '[2,2,2]', '[1,1,1]', '[1,0,2]', '[2,0,1]', '[0,0,0]']</t>
+    <t>[15, 25, 37, 50, 55, 68, 70, 86, 88, 89]</t>
+  </si>
+  <si>
+    <t>[0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 1, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 1, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 1, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2]</t>
+  </si>
+  <si>
+    <t>['[-0.03763371 -0.01533471  0.06554052 -0.01816017]', '[-0.00754409 -0.05458322  0.2277812  -0.36241836]', '[ 0.04879627 -0.15231473  0.32089719 -0.5887683 ]', '[ 0.11397169 -0.27767857  0.31375488 -0.63332862]', '[ 0.16759438 -0.39312519  0.2086893  -0.49480525]', '[ 0.1930193  -0.46685036  0.03906408 -0.22816919]', '[ 0.15689524 -0.41528579 -0.3922057   0.73207416]', '[ 0.04309269 -0.18588535 -0.71796191  1.51055937]', '[-0.1147829   0.15904975 -0.81547211  1.84906375]', '[-0.26363568  0.51494657 -0.63159042  1.62703318]', '[-0.35418658  0.78351571 -0.2539271   1.01663306]', '[-0.36122763  0.91144819  0.18313112  0.25239067]', '[-0.26190848  0.82452699  0.79137833 -1.10754289]', '[-0.05546354  0.48017359  1.23429726 -2.2781243 ]', '[ 0.20909957 -0.04617758  1.33805656 -2.84269804]', '[ 0.421174   -0.52481363  0.72795944 -1.83726235]', '[ 0.51163965 -0.82044568  0.1573503  -1.07774776]', '[ 0.48171724 -0.94675212 -0.44939141 -0.17759611]', '[ 0.31705272 -0.8330783  -1.1663918   1.29635342]', '[ 0.03179582 -0.44369369 -1.63063345  2.52052183]', '[-0.30470555  0.12246151 -1.64393841  2.96916864]', '[-0.5882573   0.67199549 -1.1208411   2.39743409]', '[-0.73422565  1.05090609 -0.31588263  1.35711637]', '[-0.71179338  1.20844649  0.53292572  0.2109179 ]', '[-0.50899304  1.0784529   1.46163666 -1.50803017]', '[-0.16754049  0.6737608   1.88956842 -2.46504963]', '[ 0.23948037  0.07677303  2.08263468 -3.32705195]', '[ 0.6192182  -0.56694441  1.61653846 -2.92506475]', '[ 0.85817357 -1.04729301  0.73573289 -1.83147666]', '[ 0.906432   -1.29306776 -0.25572735 -0.61858897]', '[ 0.74085583 -1.23753072 -1.37423651  1.18425635]', '[ 0.37128823 -0.81564677 -2.27205122  3.01514996]', '[-0.13725955 -0.07017591 -2.69243673  4.21341332]', '[-0.64212296  0.73909497 -2.22420445  3.62157451]', '[-0.99377082  1.32773976 -1.25244463  2.24200317]', '[-1.13501683  1.64108345 -0.15154648  0.90439864]', '[-1.03828954  1.6418877   1.10463914 -0.90901395]', '[-0.72010908  1.31658098  2.04119578 -2.36244355]', '[-0.22027459  0.64005334  2.89284178 -4.34635663]', '[ 0.3870356  -0.32895465  2.99710039 -4.95067991]', '[ 0.90856477 -1.19406399  2.12625569 -3.55409868]', '[ 1.22207799 -1.7492693   0.99138941 -2.03436112]', '[ 1.30153434 -2.01979515 -0.1982668  -0.6818424 ]', '[ 1.13137129 -1.97494481 -1.48291088  1.15458066]', '[ 0.72086602 -1.5409495  -2.5837755   3.23957105]', '[ 0.11484847 -0.66167621 -3.41272682  5.49651979]', '[-0.5800687   0.52226085 -3.30177588  5.81023885]', '[-1.13213563  1.50824374 -2.15695321  3.98789577]', '[-1.43712181  2.14309408 -0.88818284  2.42337905]', '[-1.487388    2.49100003  0.38059281  1.06290653]', '[-1.28881634  2.56466116  1.58763771 -0.34308602]', '[-0.85345196  2.30460529  2.70653636 -2.28694075]', '[-0.23923244  1.63565245  3.35678168 -4.43694876]', '[ 0.46524222  0.53082839  3.60923876 -6.4517125 ]', '[ 1.125103   -0.75281874  2.76946612 -5.8896295 ]', '[ 1.50717753 -1.69423214  1.05573573 -3.60864244]', '[ 1.5688968  -2.27150453 -0.42978398 -2.17543532]', '[ 1.33672584 -2.53808585 -1.85957161 -0.46848949]', '[ 0.83780094 -2.43012841 -3.0538464   1.56515358]', '[ 0.15994066 -1.908394   -3.59862644  3.64736141]', '[-0.55869166 -0.98556559 -3.52195914  5.48730723]', '[-1.21467536  0.18991445 -2.89057873  5.88070247]', '[-1.65438899  1.233941   -1.43667574  4.46702923]', '[-1.77987008  1.98693267  0.19119919  3.07800884]', '[-1.57972524  2.45621761  1.78742235  1.5708315 ]', '[-1.06956893  2.55800731  3.24463944 -0.58073418]', '[-0.32465688  2.21898811  4.05390778 -2.80460227]', '[ 0.48490263  1.4520832   3.92139917 -4.77873429]', '[ 1.19350824  0.43113551  3.08323972 -5.14823531]', '[ 1.70574565 -0.55456449  1.96612277 -4.52434591]', '[ 1.94205099 -1.29808405  0.39496497 -2.95375836]', '[ 1.87687265 -1.78965889 -1.07574874 -1.89952734]', '[ 1.49144413 -1.97425126 -2.75794024  0.16725546]', '[ 0.79569943 -1.6734969  -4.10805468  2.95255151]', '[-0.10650899 -0.77011729 -4.80023519  5.97740183]', '[-1.04643312  0.52274582 -4.3453062   6.25487376]', '[-1.7818892   1.56626944 -3.00833081  4.22140917]', '[-2.26716349  2.27881552 -1.89011124  3.04848422]', '[-2.55574395  2.82209654 -1.04463     2.43325611]', '[-2.70402212 -3.02424834 -0.48364774  1.93558021]', '[-2.7627874  -2.69152393 -0.12731568  1.37657766]', '[-2.75887097 -2.48110545  0.16648753  0.70917605]', '[-2.68577656 -2.43588072  0.58276672 -0.27444337]', '[-2.51554256 -2.59699404  1.15388314 -1.35032909]', '[-2.20070121 -3.00150471  2.04695207 -2.71613874]', '[-1.67593466  2.58092893  3.23590014 -4.39601001]', '[-0.91429244  1.49299945  4.39450188 -6.7188346 ]', '[ 0.10138419 -0.20452468  5.46562182 -9.48786065]', '[ 1.0754246  -1.78292052  4.15306313 -6.01325517]', '[ 1.77865418 -2.71829998  2.88720572 -3.56769267]', '[ 2.2484166   2.97868583  1.84952519 -2.36811973]', '[ 2.53914285  2.60198888  1.11062879 -1.42165095]', '[ 2.70963148  2.40420195  0.62944462 -0.56999825]', '[2.80126872 2.36885911 0.30800351 0.20172907]', '[2.83239437 2.49915372 0.01452262 1.08172576]', '[ 2.80220806  2.81294963 -0.32365874  2.03169479]', '[ 2.69258536 -2.98032689 -0.81931229  2.85319016]', '[ 2.44951501 -2.32822634 -1.67954795  3.70462331]', '[ 1.99385378 -1.46209914 -2.95009799  5.12885752]', '[ 1.23763229 -0.19060467 -4.60761463  7.55554867]', '[ 0.23374136  1.30713801 -5.21005362  6.7085639 ]', '[-0.80702984  2.37954068 -5.07587081  4.03102358]', '[-1.73380065  2.97191505 -4.0962542   2.05556556]', '[-2.44763829 -3.02476212 -3.11722497  0.93775339]', '[-3.02205389 -2.88774272 -2.74617364  0.56220058]', '[ 2.69058722 -2.74568987 -3.07902564  1.01358534]', '[ 1.98634733 -2.41289065 -4.04828319  2.52993826]', '[ 1.0559466  -1.63203185 -5.25915614  5.57680304]', '[-0.11633494 -0.10068701 -6.28257729  9.19551182]', '[-1.28598913  1.51646637 -5.17862959  6.28173095]', '[-2.20985495  2.49716667 -4.12558343  3.86138895]', '[-2.96959611 -3.10950216 -3.5903037   3.14126395]', '[ 2.58281216 -2.44615436 -3.85935052  3.72079234]', '[ 1.71855967 -1.51113047 -4.9156797   5.98876238]', '[ 0.56723072  0.07261584 -6.46009725  9.31100933]', '[-0.70859419  1.68140868 -6.05255103  6.02209564]', '[-1.83294013  2.5339602  -5.11962273  2.80626039]', '[-2.76109318  2.9275347  -4.27136541  1.42455811]', '[ 2.67734333 -3.07700388 -4.35999143  1.61940995]', '[ 1.7148434  -2.60596483 -5.35650356  3.39728261]', '[ 0.54167647 -1.58300859 -6.31721098  7.18319427]', '[-0.79630157  0.28777899 -6.71614999 10.31742475]', '[-1.98650613  1.99179884 -5.21101246  6.63174388]', '[-2.95396768 -3.14131878 -4.60904073  5.31533165]', '[ 2.39211206 -2.01204912 -4.94981009  6.39822569]', '[ 1.25734821 -0.38280857 -6.55593932 10.05505059]', '[-0.11316081  1.53266028 -6.80305605  7.8209645 ]', '[-1.44023896  2.69580106 -6.32276375  4.13683981]', '[-2.60439583 -2.93775229 -5.38364441  2.76046042]', '[ 2.61987276 -2.33975028 -5.41257448  3.6167793 ]', '[ 1.44448887 -1.31127635 -6.51040121  7.17324488]', '[-0.01468717  0.55737422 -7.69580688  9.99774401]', '[-1.47090026  2.06634125 -6.78428769  4.94846151]', '[-2.72945904  2.72776058 -5.87786025  2.19518379]', '[ 2.38227253  3.12208631 -6.08088497  2.18800579]', '[ 1.05294353 -2.52100678 -7.1965163   4.69278092]', '[-0.4204094  -1.11379279 -7.45355751  9.58392731]', '[-1.85765217  0.95953646 -6.61341847  9.67666161]', '[-3.06686789  2.55968881 -5.81581574  6.94961364]', '[ 2.00684208 -2.28756404 -6.42171369  8.17642958]', '[ 0.55162985 -0.10526142 -8.12369072 13.28795051]', '[-1.0170336   2.15997223 -7.25266833  8.13506395]', '[-2.38498982 -2.78972802 -6.34385176  5.97809358]', '[ 2.68579474 -1.49236522 -6.09409835  7.53263679]', '[ 1.31996007  0.38609783 -7.53578301 10.4202933 ]', '[-0.24607804  2.10191312 -7.99408571  6.04703603]', '[-1.79509301  2.90294488 -7.26028457  2.43345833]', '[ 3.12342052 -3.02988893 -6.62497032  1.58130531]', '[ 1.73122268 -2.55388222 -7.4745573   3.78816548]', '[ 0.14772762 -1.27184613 -8.30496472  9.51120863]', '[-1.51740615  0.94119799 -7.92887718 10.5869865 ]', '[-2.98635732  2.57649689 -7.1237459   6.56263684]', '[ 1.81958481 -2.36810821 -7.74328283  7.893707  ]', '[ 0.13595854 -0.13137642 -9.05889985 13.9611877 ]', '[-1.57332787  2.19037343 -7.73711839  7.91614088]', '[-3.05591865 -2.78782143 -7.14889222  6.16527119]', '[ 1.77610247 -1.27127048 -7.74121635  9.87838351]', '[ 0.06889417  1.074382   -8.91773486 11.377134  ]', '[-1.67012871  2.70549421 -8.42499368  5.58979988]', '[ 3.00189947 -2.6122865  -7.83729977  5.10193107]', '[ 1.38561345 -1.16643028 -8.67668938 10.24364302]', '[-0.45954557  1.16781076 -9.26449576 10.58896292]', '[-2.22198506  2.58879973 -8.39528822  4.43521441]', '[ 2.41113573 -2.98490686 -8.39602624  3.71271905]', '[ 0.63897078 -1.84868404 -9.26826604  8.65758028]', '[-1.29015675  0.61985843 -9.49668441 13.34826256]', '[-3.05455343  2.65049121 -8.59424884  7.81614883]', '[ 1.45150784 -1.97381081 -9.27775443 10.4605633 ]', '[ -0.58890839   0.94982925 -10.38992459  15.21533812]', '[-2.54065107 -3.0780237  -9.38192413  9.29220095]', '[ 1.89347903 -0.88026832 -9.73336667 14.0721493 ]', '[-0.11214017  1.79168453 -9.75473655  9.73281426]', '[-2.04245826 -3.12439564 -9.30689262  5.25581952]', '[ 2.44694171 -1.94194548 -8.92763171  7.77688262]', '[  0.49303879   0.39360252 -10.36744238  13.49350008]', '[-1.53807951  2.33314662 -9.71095529  5.29998124]', '[ 2.89424693  2.94470351 -9.01932128  1.99675801]', '[  1.00574407  -2.86248366 -10.03725742   3.64736601]', '[-1.00786508 -1.61055574 -9.7540045   9.36251527]', '[-2.91135293  0.7476814  -9.28845624 12.15572918]']</t>
+  </si>
+  <si>
+    <t>[0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50, 51, 52, 53, 54, 55, 56, 57, 58, 59, 60, 61, 62, 63, 64, 65, 66, 67, 68, 69, 70, 71, 72, 73, 74, 75, 76, 77, 78, 79, 80, 81, 82, 83, 84, 85, 86, 87, 88, 89, 90, 91, 92, 93, 94, 95, 96, 97, 98, 99, 100, 101, 102, 103, 104, 105, 106, 107, 108, 109, 110, 111, 112, 113, 114, 115, 116, 117, 118, 119, 120, 121, 122, 123, 124, 125, 126, 127, 128, 129, 130, 131, 132, 133, 134, 135, 136, 137, 138, 139, 140, 141, 142, 143, 144, 145, 146, 147, 148, 149, 150, 151, 152, 153, 154, 155, 156, 157, 158, 159, 160, 161, 162, 163, 164, 165, 166, 167, 168, 169, 170, 171, 172, 173, 174, 175, 176, 177, 178, 179]</t>
+  </si>
+  <si>
+    <t>[array([-0.03763371, -0.01533471,  0.06554052, -0.01816017], dtype=float32), array([-0.00754409, -0.05458322,  0.2277812 , -0.36241836]), array([ 0.04879627, -0.15231473,  0.32089719, -0.5887683 ]), array([ 0.11397169, -0.27767857,  0.31375488, -0.63332862]), array([ 0.16759438, -0.39312519,  0.2086893 , -0.49480525]), array([ 0.1930193 , -0.46685036,  0.03906408, -0.22816919]), array([ 0.15689524, -0.41528579, -0.3922057 ,  0.73207416]), array([ 0.04309269, -0.18588535, -0.71796191,  1.51055937]), array([-0.1147829 ,  0.15904975, -0.81547211,  1.84906375]), array([-0.26363568,  0.51494657, -0.63159042,  1.62703318]), array([-0.35418658,  0.78351571, -0.2539271 ,  1.01663306]), array([-0.36122763,  0.91144819,  0.18313112,  0.25239067]), array([-0.26190848,  0.82452699,  0.79137833, -1.10754289]), array([-0.05546354,  0.48017359,  1.23429726, -2.2781243 ]), array([ 0.20909957, -0.04617758,  1.33805656, -2.84269804]), array([ 0.421174  , -0.52481363,  0.72795944, -1.83726235]), array([ 0.51163965, -0.82044568,  0.1573503 , -1.07774776]), array([ 0.48171724, -0.94675212, -0.44939141, -0.17759611]), array([ 0.31705272, -0.8330783 , -1.1663918 ,  1.29635342]), array([ 0.03179582, -0.44369369, -1.63063345,  2.52052183]), array([-0.30470555,  0.12246151, -1.64393841,  2.96916864]), array([-0.5882573 ,  0.67199549, -1.1208411 ,  2.39743409]), array([-0.73422565,  1.05090609, -0.31588263,  1.35711637]), array([-0.71179338,  1.20844649,  0.53292572,  0.2109179 ]), array([-0.50899304,  1.0784529 ,  1.46163666, -1.50803017]), array([-0.16754049,  0.6737608 ,  1.88956842, -2.46504963]), array([ 0.23948037,  0.07677303,  2.08263468, -3.32705195]), array([ 0.6192182 , -0.56694441,  1.61653846, -2.92506475]), array([ 0.85817357, -1.04729301,  0.73573289, -1.83147666]), array([ 0.906432  , -1.29306776, -0.25572735, -0.61858897]), array([ 0.74085583, -1.23753072, -1.37423651,  1.18425635]), array([ 0.37128823, -0.81564677, -2.27205122,  3.01514996]), array([-0.13725955, -0.07017591, -2.69243673,  4.21341332]), array([-0.64212296,  0.73909497, -2.22420445,  3.62157451]), array([-0.99377082,  1.32773976, -1.25244463,  2.24200317]), array([-1.13501683,  1.64108345, -0.15154648,  0.90439864]), array([-1.03828954,  1.6418877 ,  1.10463914, -0.90901395]), array([-0.72010908,  1.31658098,  2.04119578, -2.36244355]), array([-0.22027459,  0.64005334,  2.89284178, -4.34635663]), array([ 0.3870356 , -0.32895465,  2.99710039, -4.95067991]), array([ 0.90856477, -1.19406399,  2.12625569, -3.55409868]), array([ 1.22207799, -1.7492693 ,  0.99138941, -2.03436112]), array([ 1.30153434, -2.01979515, -0.1982668 , -0.6818424 ]), array([ 1.13137129, -1.97494481, -1.48291088,  1.15458066]), array([ 0.72086602, -1.5409495 , -2.5837755 ,  3.23957105]), array([ 0.11484847, -0.66167621, -3.41272682,  5.49651979]), array([-0.5800687 ,  0.52226085, -3.30177588,  5.81023885]), array([-1.13213563,  1.50824374, -2.15695321,  3.98789577]), array([-1.43712181,  2.14309408, -0.88818284,  2.42337905]), array([-1.487388  ,  2.49100003,  0.38059281,  1.06290653]), array([-1.28881634,  2.56466116,  1.58763771, -0.34308602]), array([-0.85345196,  2.30460529,  2.70653636, -2.28694075]), array([-0.23923244,  1.63565245,  3.35678168, -4.43694876]), array([ 0.46524222,  0.53082839,  3.60923876, -6.4517125 ]), array([ 1.125103  , -0.75281874,  2.76946612, -5.8896295 ]), array([ 1.50717753, -1.69423214,  1.05573573, -3.60864244]), array([ 1.5688968 , -2.27150453, -0.42978398, -2.17543532]), array([ 1.33672584, -2.53808585, -1.85957161, -0.46848949]), array([ 0.83780094, -2.43012841, -3.0538464 ,  1.56515358]), array([ 0.15994066, -1.908394  , -3.59862644,  3.64736141]), array([-0.55869166, -0.98556559, -3.52195914,  5.48730723]), array([-1.21467536,  0.18991445, -2.89057873,  5.88070247]), array([-1.65438899,  1.233941  , -1.43667574,  4.46702923]), array([-1.77987008,  1.98693267,  0.19119919,  3.07800884]), array([-1.57972524,  2.45621761,  1.78742235,  1.5708315 ]), array([-1.06956893,  2.55800731,  3.24463944, -0.58073418]), array([-0.32465688,  2.21898811,  4.05390778, -2.80460227]), array([ 0.48490263,  1.4520832 ,  3.92139917, -4.77873429]), array([ 1.19350824,  0.43113551,  3.08323972, -5.14823531]), array([ 1.70574565, -0.55456449,  1.96612277, -4.52434591]), array([ 1.94205099, -1.29808405,  0.39496497, -2.95375836]), array([ 1.87687265, -1.78965889, -1.07574874, -1.89952734]), array([ 1.49144413, -1.97425126, -2.75794024,  0.16725546]), array([ 0.79569943, -1.6734969 , -4.10805468,  2.95255151]), array([-0.10650899, -0.77011729, -4.80023519,  5.97740183]), array([-1.04643312,  0.52274582, -4.3453062 ,  6.25487376]), array([-1.7818892 ,  1.56626944, -3.00833081,  4.22140917]), array([-2.26716349,  2.27881552, -1.89011124,  3.04848422]), array([-2.55574395,  2.82209654, -1.04463   ,  2.43325611]), array([-2.70402212, -3.02424834, -0.48364774,  1.93558021]), array([-2.7627874 , -2.69152393, -0.12731568,  1.37657766]), array([-2.75887097, -2.48110545,  0.16648753,  0.70917605]), array([-2.68577656, -2.43588072,  0.58276672, -0.27444337]), array([-2.51554256, -2.59699404,  1.15388314, -1.35032909]), array([-2.20070121, -3.00150471,  2.04695207, -2.71613874]), array([-1.67593466,  2.58092893,  3.23590014, -4.39601001]), array([-0.91429244,  1.49299945,  4.39450188, -6.7188346 ]), array([ 0.10138419, -0.20452468,  5.46562182, -9.48786065]), array([ 1.0754246 , -1.78292052,  4.15306313, -6.01325517]), array([ 1.77865418, -2.71829998,  2.88720572, -3.56769267]), array([ 2.2484166 ,  2.97868583,  1.84952519, -2.36811973]), array([ 2.53914285,  2.60198888,  1.11062879, -1.42165095]), array([ 2.70963148,  2.40420195,  0.62944462, -0.56999825]), array([2.80126872, 2.36885911, 0.30800351, 0.20172907]), array([2.83239437, 2.49915372, 0.01452262, 1.08172576]), array([ 2.80220806,  2.81294963, -0.32365874,  2.03169479]), array([ 2.69258536, -2.98032689, -0.81931229,  2.85319016]), array([ 2.44951501, -2.32822634, -1.67954795,  3.70462331]), array([ 1.99385378, -1.46209914, -2.95009799,  5.12885752]), array([ 1.23763229, -0.19060467, -4.60761463,  7.55554867]), array([ 0.23374136,  1.30713801, -5.21005362,  6.7085639 ]), array([-0.80702984,  2.37954068, -5.07587081,  4.03102358]), array([-1.73380065,  2.97191505, -4.0962542 ,  2.05556556]), array([-2.44763829, -3.02476212, -3.11722497,  0.93775339]), array([-3.02205389, -2.88774272, -2.74617364,  0.56220058]), array([ 2.69058722, -2.74568987, -3.07902564,  1.01358534]), array([ 1.98634733, -2.41289065, -4.04828319,  2.52993826]), array([ 1.0559466 , -1.63203185, -5.25915614,  5.57680304]), array([-0.11633494, -0.10068701, -6.28257729,  9.19551182]), array([-1.28598913,  1.51646637, -5.17862959,  6.28173095]), array([-2.20985495,  2.49716667, -4.12558343,  3.86138895]), array([-2.96959611, -3.10950216, -3.5903037 ,  3.14126395]), array([ 2.58281216, -2.44615436, -3.85935052,  3.72079234]), array([ 1.71855967, -1.51113047, -4.9156797 ,  5.98876238]), array([ 0.56723072,  0.07261584, -6.46009725,  9.31100933]), array([-0.70859419,  1.68140868, -6.05255103,  6.02209564]), array([-1.83294013,  2.5339602 , -5.11962273,  2.80626039]), array([-2.76109318,  2.9275347 , -4.27136541,  1.42455811]), array([ 2.67734333, -3.07700388, -4.35999143,  1.61940995]), array([ 1.7148434 , -2.60596483, -5.35650356,  3.39728261]), array([ 0.54167647, -1.58300859, -6.31721098,  7.18319427]), array([-0.79630157,  0.28777899, -6.71614999, 10.31742475]), array([-1.98650613,  1.99179884, -5.21101246,  6.63174388]), array([-2.95396768, -3.14131878, -4.60904073,  5.31533165]), array([ 2.39211206, -2.01204912, -4.94981009,  6.39822569]), array([ 1.25734821, -0.38280857, -6.55593932, 10.05505059]), array([-0.11316081,  1.53266028, -6.80305605,  7.8209645 ]), array([-1.44023896,  2.69580106, -6.32276375,  4.13683981]), array([-2.60439583, -2.93775229, -5.38364441,  2.76046042]), array([ 2.61987276, -2.33975028, -5.41257448,  3.6167793 ]), array([ 1.44448887, -1.31127635, -6.51040121,  7.17324488]), array([-0.01468717,  0.55737422, -7.69580688,  9.99774401]), array([-1.47090026,  2.06634125, -6.78428769,  4.94846151]), array([-2.72945904,  2.72776058, -5.87786025,  2.19518379]), array([ 2.38227253,  3.12208631, -6.08088497,  2.18800579]), array([ 1.05294353, -2.52100678, -7.1965163 ,  4.69278092]), array([-0.4204094 , -1.11379279, -7.45355751,  9.58392731]), array([-1.85765217,  0.95953646, -6.61341847,  9.67666161]), array([-3.06686789,  2.55968881, -5.81581574,  6.94961364]), array([ 2.00684208, -2.28756404, -6.42171369,  8.17642958]), array([ 0.55162985, -0.10526142, -8.12369072, 13.28795051]), array([-1.0170336 ,  2.15997223, -7.25266833,  8.13506395]), array([-2.38498982, -2.78972802, -6.34385176,  5.97809358]), array([ 2.68579474, -1.49236522, -6.09409835,  7.53263679]), array([ 1.31996007,  0.38609783, -7.53578301, 10.4202933 ]), array([-0.24607804,  2.10191312, -7.99408571,  6.04703603]), array([-1.79509301,  2.90294488, -7.26028457,  2.43345833]), array([ 3.12342052, -3.02988893, -6.62497032,  1.58130531]), array([ 1.73122268, -2.55388222, -7.4745573 ,  3.78816548]), array([ 0.14772762, -1.27184613, -8.30496472,  9.51120863]), array([-1.51740615,  0.94119799, -7.92887718, 10.5869865 ]), array([-2.98635732,  2.57649689, -7.1237459 ,  6.56263684]), array([ 1.81958481, -2.36810821, -7.74328283,  7.893707  ]), array([ 0.13595854, -0.13137642, -9.05889985, 13.9611877 ]), array([-1.57332787,  2.19037343, -7.73711839,  7.91614088]), array([-3.05591865, -2.78782143, -7.14889222,  6.16527119]), array([ 1.77610247, -1.27127048, -7.74121635,  9.87838351]), array([ 0.06889417,  1.074382  , -8.91773486, 11.377134  ]), array([-1.67012871,  2.70549421, -8.42499368,  5.58979988]), array([ 3.00189947, -2.6122865 , -7.83729977,  5.10193107]), array([ 1.38561345, -1.16643028, -8.67668938, 10.24364302]), array([-0.45954557,  1.16781076, -9.26449576, 10.58896292]), array([-2.22198506,  2.58879973, -8.39528822,  4.43521441]), array([ 2.41113573, -2.98490686, -8.39602624,  3.71271905]), array([ 0.63897078, -1.84868404, -9.26826604,  8.65758028]), array([-1.29015675,  0.61985843, -9.49668441, 13.34826256]), array([-3.05455343,  2.65049121, -8.59424884,  7.81614883]), array([ 1.45150784, -1.97381081, -9.27775443, 10.4605633 ]), array([ -0.58890839,   0.94982925, -10.38992459,  15.21533812]), array([-2.54065107, -3.0780237 , -9.38192413,  9.29220095]), array([ 1.89347903, -0.88026832, -9.73336667, 14.0721493 ]), array([-0.11214017,  1.79168453, -9.75473655,  9.73281426]), array([-2.04245826, -3.12439564, -9.30689262,  5.25581952]), array([ 2.44694171, -1.94194548, -8.92763171,  7.77688262]), array([  0.49303879,   0.39360252, -10.36744238,  13.49350008]), array([-1.53807951,  2.33314662, -9.71095529,  5.29998124]), array([ 2.89424693,  2.94470351, -9.01932128,  1.99675801]), array([  1.00574407,  -2.86248366, -10.03725742,   3.64736601]), array([-1.00786508, -1.61055574, -9.7540045 ,  9.36251527]), array([-2.91135293,  0.7476814 , -9.28845624, 12.15572918])]</t>
+  </si>
+  <si>
+    <t>['[1,1,1]', '[2,1,0]', '[2,2,2]', '[0,0,0]', '[0,2,1]', '[1,0,2]', '[0,1,1]', '[1,1,2]', '[1,2,0]', '[2,0,1]']</t>
+  </si>
+  <si>
+    <t>[1, 12, 21, 30, 31, 34, 35, 44, 45, 48, 49, 58, 61, 71, 73, 75, 87, 88, 89, 93, 104, 107, 111, 119, 124, 134, 135, 136, 137, 139, 143, 144, 145, 160, 161, 163, 164, 165, 167, 174, 177]</t>
+  </si>
+  <si>
+    <t>[0, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 1, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 1, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 1, 0, 0, 0, 0, 0, 0, 0, 1, 2, 2, 2, 2, 2, 2, 2, 2, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 2, 2, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 1, 0, 0, 0, 0]</t>
+  </si>
+  <si>
+    <t>['[-0.03763371 -0.01533471  0.06554052 -0.01816017]', '[-0.03406929  0.01398622 -0.02953871  0.30651903]', '[-0.04818188  0.10262173 -0.10566927  0.56184435]', '[-0.07305261  0.22936701 -0.13369446  0.67944384]', '[-0.0976443   0.36319498 -0.10327727  0.63282133]', '[-0.11125897  0.47297074 -0.02773051  0.446438  ]', '[-0.10757465  0.53619101  0.06462001  0.17794954]', '[-0.06138715  0.47788865  0.38724178 -0.74730665]', '[ 0.04067658  0.24884187  0.60910104 -1.49573956]', '[ 0.16900594 -0.09311382  0.63541813 -1.84114417]', '[ 0.27801726 -0.45113855  0.41913697 -1.65899888]', '[ 0.32572913 -0.7305588   0.04412338 -1.09289423]', '[ 0.27180509 -0.81725528 -0.56763332  0.22235075]', '[ 0.10838721 -0.64822475 -1.03475615  1.43462953]', '[-0.12563193 -0.26624663 -1.25336647  2.29670168]', '[-0.36676169  0.22116642 -1.08955577  2.44333936]', '[-0.53575813  0.66073853 -0.55568752  1.86434009]', '[-0.57820583  0.94437763  0.13922515  0.94295303]', '[-0.46144614  0.97418834  1.00207981 -0.63873269]', '[-0.19215789  0.69569535  1.6430939  -2.10453598]', '[ 0.17025817  0.16647811  1.8976779  -3.04365046]', '[ 0.4997503  -0.37612442  1.31322293 -2.22622154]', '[ 0.69710361 -0.74989544  0.62121399 -1.45027534]', '[ 0.7393395  -0.94275755 -0.20511528 -0.46178075]', '[ 0.59573873 -0.87168762 -1.20783777  1.17047212]', '[ 0.27097402 -0.48159161 -1.98321214  2.66895751]', '[-0.16287802  0.14089937 -2.24170413  3.34466547]', '[-0.57602645  0.76125485 -1.79387552  2.69207997]', '[-0.85445112  1.18301442 -0.95324559  1.49894271]', '[-0.94880595  1.35990204  0.01826453  0.27201303]', '[-0.84781208  1.29095048  0.97898    -0.96764087]', '[-0.5669084   0.97074919  1.79216024 -2.22294055]', '[-0.12959985  0.35811196  2.50059563 -3.78685563]', '[ 0.38156938 -0.4448291   2.46255616 -3.94162861]', '[ 0.78213069 -1.06325638  1.48549807 -2.17602492]', '[ 0.96454456 -1.31676119  0.3248886  -0.37623612]', '[ 0.9098559  -1.21686897 -0.86899953  1.38198927]', '[ 0.62147524 -0.75720681 -1.98849545  3.21466774]', '[ 0.13878685  0.03806549 -2.71757797  4.50727814]', '[-0.39772395  0.90385207 -2.50615896  3.86970305]', '[-0.82763651  1.53119017 -1.74219291  2.37857024]', '[-1.08043595  1.86184427 -0.76150358  0.95098538]', '[-1.12633404  1.9181513   0.30667073 -0.3826761 ]', '[-0.94410532  1.65911584  1.50372895 -2.23796421]', '[-0.55114686  1.058004    2.38800931 -3.77876258]', '[-0.01647465  0.17883331  2.83106836 -4.77078964]', '[ 0.53384489 -0.76221331  2.5087176  -4.30310315]', '[ 0.94590089 -1.47297253  1.56665596 -2.77845711]', '[ 1.13483851 -1.83589195  0.31883073 -0.88916779]', '[ 1.07407687 -1.83463237 -0.91716308  0.90872941]', '[ 0.7749029  -1.46157684 -2.05100325  2.86366373]', '[ 0.26555764 -0.67335378 -2.9904838   4.9841447 ]', '[-0.36790286  0.42865447 -3.13064148  5.56851767]', '[-0.90928761  1.39133627 -2.1981929   3.93434782]', '[-1.23535092  2.01323256 -1.04837774  2.33617754]', '[-1.32555808  2.34005443  0.14677914  0.94651851]', '[-1.1670089   2.3498667   1.41758015 -0.86125925]', '[-0.77249401  1.98505542  2.47851362 -2.82630885]', '[-0.21492482  1.25023335  3.03605694 -4.51911982]', '[ 0.4340957   0.15592388  3.31536764 -6.1231187 ]', '[ 1.01912253 -0.9913424   2.36417855 -5.00018314]', '[ 1.33582558 -1.76594484  0.81097232 -2.82633853]', '[ 1.36330694 -2.18784252 -0.52828401 -1.39747882]', '[ 1.11924342 -2.27751649 -1.87355278  0.52125515]', '[ 0.63687908 -1.9684371  -2.87331734  2.59817525]', '[ 4.42839970e-03 -1.22985513e+00 -3.38058253e+00  4.77993113e+00]', '[-0.68500972 -0.10239774 -3.36830992  6.14816504]', '[-1.25689845  1.02934093 -2.20902506  4.88559118]', '[-1.5498031   1.84122184 -0.71325743  3.28554148]', '[-1.54364418  2.35577537  0.76185476  1.85708886]', '[-1.24840371  2.55527259  2.15262235  0.11568667]', '[-0.71103631  2.41593684  3.13560257 -1.51214433]', '[-0.0306488   1.91453278  3.53333905 -3.47052932]', '[ 0.63962415  1.10553538  3.08615851 -4.47470248]', '[ 1.19784684  0.14491583  2.41569937 -4.9008361 ]', '[ 1.5409556  -0.69437508  0.95774651 -3.38613966]', '[ 1.59256087 -1.26062738 -0.47111102 -2.23395509]', '[ 1.34444856 -1.56119509 -2.00887297 -0.6808799 ]', '[ 0.78806186 -1.44459295 -3.46972752  1.92487422]', '[ 2.31476088e-03 -7.80228594e-01 -4.25980941e+00  4.61818070e+00]', '[-0.84659023  0.26576354 -4.01481489  5.31285237]', '[-1.53421948  1.17426289 -2.80470481  3.67964963]', '[-1.97149301  1.77266252 -1.58901783  2.41754357]', '[-2.17700006  2.17417646 -0.47799792  1.64003787]', '[-2.16429009  2.43088345  0.60851564  0.90287486]', '[-1.92307236  2.4959532   1.81742595 -0.31834896]', '[-1.42696295  2.2491021   3.1348817  -2.26050059]', '[-0.698388    1.58521836  4.09015298 -4.48935328]', '[ 0.17984039  0.44308459  4.5627621  -6.67244968]', '[ 1.02095865 -0.81120689  3.61876854 -5.30158078]', '[ 1.61689576 -1.67647581  2.33635736 -3.43241986]', '[ 1.96057347 -2.23120232  1.11394019 -2.1999604 ]', '[ 2.06736241 -2.57381145 -0.03663801 -1.23506405]', '[ 1.93496356 -2.67883022 -1.29049834  0.2175756 ]', '[ 1.54771988 -2.46668428 -2.58304938  1.97622209]', '[ 0.91002759 -1.84842652 -3.75269182  4.33952416]', '[ 0.06218913 -0.6760782  -4.67496569  7.35955468]', '[-0.86286489  0.8487012  -4.25107779  7.06239228]', '[-1.57525118  2.00891039 -2.88417224  4.67310725]', '[-2.02768404  2.78868622 -1.67101508  3.24085523]', '[-2.25938717 -2.95530554 -0.68902758  2.17011601]', '[-2.31566891 -2.62733497  0.11089829  1.09951119]', '[-2.20706856 -2.54116096  0.99539028 -0.24967447]', '[-1.89819559 -2.75011812  2.13221847 -1.84143432]', '[-1.35380675  3.04177612  3.31101567 -3.10301951]', '[-0.58597074  2.22344449  4.25778067 -5.20806751]', '[ 0.31372308  0.89906945  4.71731588 -8.0869729 ]', '[ 1.19911992 -0.73407716  3.81244418 -7.41933904]', '[ 1.79307184 -1.98760755  2.14125303 -5.24602734]', '[ 2.07523705 -2.89650466  0.74920514 -3.92791936]', '[ 2.12393301  2.71338198 -0.19703574 -2.81000274]', '[ 1.99286968  2.30486795 -1.13025723 -1.27097299]', '[ 1.65783524  2.20000166 -2.25648324  0.17867437]', '[ 1.08166769  2.34315304 -3.49422619  1.1225114 ]', '[ 0.2855777   2.58371909 -4.33938896  1.09508932]', '[-0.58137764  2.70846644 -4.13482804 -0.01460506]', '[-1.29688514  2.52494549 -2.87029641 -1.90707659]', '[-1.68090316  1.93485885 -0.88148723 -3.97779336]', '[-1.61602928  0.8902843   1.52171273 -6.50852585]', '[-1.15320389 -0.55059657  2.83031934 -7.441962  ]', '[-0.54713856 -1.97561363  3.18442334 -6.70143259]', '[ 0.12044274  3.01366382  3.41605039 -6.40428159]', '[ 0.77967898  1.67261294  3.17161905 -7.19368987]', '[ 1.40409532  0.09705847  2.94169603 -8.29383159]', '[ 1.80097651 -1.34846444  0.82125848 -5.8999336 ]', '[ 1.73126301 -2.32920521 -1.49806303 -3.91479836]', '[ 1.24065521 -2.91793492 -3.27203961 -2.03094903]', '[ 0.46519398  3.12864049 -4.33733335 -0.53975935]', '[-0.42620343  3.05518912 -4.39171169 -0.45464064]', '[-1.22156204  2.85621739 -3.4114641  -1.71971476]', '[-1.73942174  2.32368846 -1.64170882 -3.64643045]', '[-1.8240768   1.35360254  0.84259637 -6.09513161]', '[-1.41971183 -0.13166535  2.96298075 -8.45939786]', '[-0.78011266 -1.78120128  3.2781968  -7.73881596]', '[-0.10675023  3.04432636  3.46385376 -7.10379825]', '[ 0.58540057  1.55758597  3.46563392 -8.00907297]', '[ 1.27296079 -0.1682187   3.12085697 -8.67660615]', '[ 1.67494189 -1.63437405  0.74956053 -5.84976247]', '[ 1.59592504 -2.60190298 -1.45619772 -3.88201643]', '[ 1.13632088  3.10961459 -2.99836036 -1.95185999]', '[ 0.44382282  2.83190757 -3.79816859 -1.06158949]', '[-0.31582068  2.5771046  -3.58997235 -1.77882236]', '[-0.89657297  2.01713916 -1.97437947 -4.02012995]', '[-1.03257877  0.92091269  0.63987143 -6.96331679]', '[-0.74297087 -0.63306636  1.78896892 -7.85460981]', '[-0.44730545 -2.02682806  1.16116085 -6.1691796 ]', '[-0.22547192  3.04678155  1.18235476 -6.15521397]', '[ 0.08599018  1.69347667  2.07858663 -7.68858066]', '[ 0.62995131 -0.12380502  2.96918287 -9.89164976]', '[ 1.00661962 -1.83434215  0.50423985 -6.86333761]', '[ 0.87362296 -2.96879155 -1.57165833 -4.75454877]', '[ 0.5011273   2.42217733 -1.85419455 -4.53857442]', '[ 0.24644005  1.34154757 -0.46972344 -6.62876059]', '[ 0.31799866 -0.27057631  0.64324117 -8.70948027]', '[ 0.21760574 -1.71409971 -1.84619554 -5.41732235]', '[-0.33663838 -2.54389202 -3.36349955 -3.27650883]', '[-1.01417076  3.12678385 -3.12549197 -3.26766494]', '[-1.4841083   2.30676542 -1.30245922 -5.15442392]', '[-1.43738124  0.95820608  1.82543467 -8.49820558]', '[-0.88071528 -0.95689696  3.13678593 -9.71871278]', '[-0.33316906 -2.68513172  2.46531968 -7.92431122]', '[ 0.18137972  1.99467349  2.85244451 -8.51309423]', '[ 8.74467051e-01 -6.20563939e-03  3.74938094e+00 -1.10162764e+01]', '[ 1.3663364  -1.8729556   0.83836101 -7.26225182]', '[ 1.27130258 -3.04742929 -1.49802808 -4.74460733]', '[ 0.88221372  2.41207154 -2.16731873 -3.7815713 ]', '[ 0.50135187  1.55087346 -1.42834446 -5.17187094]', '[ 0.34648005  0.2990393  -0.28345748 -7.13219952]', '[ 0.20671093 -1.03914248 -1.52531114 -5.5205284 ]', '[-0.29120482 -1.83765965 -3.2437868  -2.64284975]', '[-0.99145312 -2.17218054 -3.51275688 -1.03162392]', '[-1.63546857 -2.35958104 -2.8596419  -1.04334437]', '[-2.13269316 -2.63769267 -2.13504569 -1.79442909]', '[-2.49304787 -3.10045676 -1.4691873  -2.80759198]', '[-2.71092655  2.55939704 -0.65850587 -3.36904759]', '[-2.72775606  1.81583258  0.5050445  -4.04007707]', '[-2.50956278  0.93651255  1.67767792 -4.82078512]', '[-2.07851623 -0.07829197  2.62436897 -5.32595274]']</t>
+  </si>
+  <si>
+    <t>[0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50, 51, 52, 53, 54, 55, 56, 57, 58, 59, 60, 61, 62, 63, 64, 65, 66, 67, 68, 69, 70, 71, 72, 73, 74, 75, 76, 77, 78, 79, 80, 81, 82, 83, 84, 85, 86, 87, 88, 89, 90, 91, 92, 93, 94, 95, 96, 97, 98, 99, 100, 101, 102, 103, 104, 105, 106, 107, 108, 109, 110, 111, 112, 113, 114, 115, 116, 117, 118, 119, 120, 121, 122, 123, 124, 125, 126, 127, 128, 129, 130, 131, 132, 133, 134, 135, 136, 137, 138, 139, 140, 141, 142, 143, 144, 145, 146, 147, 148, 149, 150, 151, 152, 153, 154, 155, 156, 157, 158, 159, 160, 161, 162, 163, 164, 165, 166, 167, 168, 169, 170, 171, 172, 173, 174, 175, 176, 177]</t>
+  </si>
+  <si>
+    <t>[array([-0.03763371, -0.01533471,  0.06554052, -0.01816017], dtype=float32), array([-0.03406929,  0.01398622, -0.02953871,  0.30651903]), array([-0.04818188,  0.10262173, -0.10566927,  0.56184435]), array([-0.07305261,  0.22936701, -0.13369446,  0.67944384]), array([-0.0976443 ,  0.36319498, -0.10327727,  0.63282133]), array([-0.11125897,  0.47297074, -0.02773051,  0.446438  ]), array([-0.10757465,  0.53619101,  0.06462001,  0.17794954]), array([-0.06138715,  0.47788865,  0.38724178, -0.74730665]), array([ 0.04067658,  0.24884187,  0.60910104, -1.49573956]), array([ 0.16900594, -0.09311382,  0.63541813, -1.84114417]), array([ 0.27801726, -0.45113855,  0.41913697, -1.65899888]), array([ 0.32572913, -0.7305588 ,  0.04412338, -1.09289423]), array([ 0.27180509, -0.81725528, -0.56763332,  0.22235075]), array([ 0.10838721, -0.64822475, -1.03475615,  1.43462953]), array([-0.12563193, -0.26624663, -1.25336647,  2.29670168]), array([-0.36676169,  0.22116642, -1.08955577,  2.44333936]), array([-0.53575813,  0.66073853, -0.55568752,  1.86434009]), array([-0.57820583,  0.94437763,  0.13922515,  0.94295303]), array([-0.46144614,  0.97418834,  1.00207981, -0.63873269]), array([-0.19215789,  0.69569535,  1.6430939 , -2.10453598]), array([ 0.17025817,  0.16647811,  1.8976779 , -3.04365046]), array([ 0.4997503 , -0.37612442,  1.31322293, -2.22622154]), array([ 0.69710361, -0.74989544,  0.62121399, -1.45027534]), array([ 0.7393395 , -0.94275755, -0.20511528, -0.46178075]), array([ 0.59573873, -0.87168762, -1.20783777,  1.17047212]), array([ 0.27097402, -0.48159161, -1.98321214,  2.66895751]), array([-0.16287802,  0.14089937, -2.24170413,  3.34466547]), array([-0.57602645,  0.76125485, -1.79387552,  2.69207997]), array([-0.85445112,  1.18301442, -0.95324559,  1.49894271]), array([-0.94880595,  1.35990204,  0.01826453,  0.27201303]), array([-0.84781208,  1.29095048,  0.97898   , -0.96764087]), array([-0.5669084 ,  0.97074919,  1.79216024, -2.22294055]), array([-0.12959985,  0.35811196,  2.50059563, -3.78685563]), array([ 0.38156938, -0.4448291 ,  2.46255616, -3.94162861]), array([ 0.78213069, -1.06325638,  1.48549807, -2.17602492]), array([ 0.96454456, -1.31676119,  0.3248886 , -0.37623612]), array([ 0.9098559 , -1.21686897, -0.86899953,  1.38198927]), array([ 0.62147524, -0.75720681, -1.98849545,  3.21466774]), array([ 0.13878685,  0.03806549, -2.71757797,  4.50727814]), array([-0.39772395,  0.90385207, -2.50615896,  3.86970305]), array([-0.82763651,  1.53119017, -1.74219291,  2.37857024]), array([-1.08043595,  1.86184427, -0.76150358,  0.95098538]), array([-1.12633404,  1.9181513 ,  0.30667073, -0.3826761 ]), array([-0.94410532,  1.65911584,  1.50372895, -2.23796421]), array([-0.55114686,  1.058004  ,  2.38800931, -3.77876258]), array([-0.01647465,  0.17883331,  2.83106836, -4.77078964]), array([ 0.53384489, -0.76221331,  2.5087176 , -4.30310315]), array([ 0.94590089, -1.47297253,  1.56665596, -2.77845711]), array([ 1.13483851, -1.83589195,  0.31883073, -0.88916779]), array([ 1.07407687, -1.83463237, -0.91716308,  0.90872941]), array([ 0.7749029 , -1.46157684, -2.05100325,  2.86366373]), array([ 0.26555764, -0.67335378, -2.9904838 ,  4.9841447 ]), array([-0.36790286,  0.42865447, -3.13064148,  5.56851767]), array([-0.90928761,  1.39133627, -2.1981929 ,  3.93434782]), array([-1.23535092,  2.01323256, -1.04837774,  2.33617754]), array([-1.32555808,  2.34005443,  0.14677914,  0.94651851]), array([-1.1670089 ,  2.3498667 ,  1.41758015, -0.86125925]), array([-0.77249401,  1.98505542,  2.47851362, -2.82630885]), array([-0.21492482,  1.25023335,  3.03605694, -4.51911982]), array([ 0.4340957 ,  0.15592388,  3.31536764, -6.1231187 ]), array([ 1.01912253, -0.9913424 ,  2.36417855, -5.00018314]), array([ 1.33582558, -1.76594484,  0.81097232, -2.82633853]), array([ 1.36330694, -2.18784252, -0.52828401, -1.39747882]), array([ 1.11924342, -2.27751649, -1.87355278,  0.52125515]), array([ 0.63687908, -1.9684371 , -2.87331734,  2.59817525]), array([ 4.42839970e-03, -1.22985513e+00, -3.38058253e+00,  4.77993113e+00]), array([-0.68500972, -0.10239774, -3.36830992,  6.14816504]), array([-1.25689845,  1.02934093, -2.20902506,  4.88559118]), array([-1.5498031 ,  1.84122184, -0.71325743,  3.28554148]), array([-1.54364418,  2.35577537,  0.76185476,  1.85708886]), array([-1.24840371,  2.55527259,  2.15262235,  0.11568667]), array([-0.71103631,  2.41593684,  3.13560257, -1.51214433]), array([-0.0306488 ,  1.91453278,  3.53333905, -3.47052932]), array([ 0.63962415,  1.10553538,  3.08615851, -4.47470248]), array([ 1.19784684,  0.14491583,  2.41569937, -4.9008361 ]), array([ 1.5409556 , -0.69437508,  0.95774651, -3.38613966]), array([ 1.59256087, -1.26062738, -0.47111102, -2.23395509]), array([ 1.34444856, -1.56119509, -2.00887297, -0.6808799 ]), array([ 0.78806186, -1.44459295, -3.46972752,  1.92487422]), array([ 2.31476088e-03, -7.80228594e-01, -4.25980941e+00,  4.61818070e+00]), array([-0.84659023,  0.26576354, -4.01481489,  5.31285237]), array([-1.53421948,  1.17426289, -2.80470481,  3.67964963]), array([-1.97149301,  1.77266252, -1.58901783,  2.41754357]), array([-2.17700006,  2.17417646, -0.47799792,  1.64003787]), array([-2.16429009,  2.43088345,  0.60851564,  0.90287486]), array([-1.92307236,  2.4959532 ,  1.81742595, -0.31834896]), array([-1.42696295,  2.2491021 ,  3.1348817 , -2.26050059]), array([-0.698388  ,  1.58521836,  4.09015298, -4.48935328]), array([ 0.17984039,  0.44308459,  4.5627621 , -6.67244968]), array([ 1.02095865, -0.81120689,  3.61876854, -5.30158078]), array([ 1.61689576, -1.67647581,  2.33635736, -3.43241986]), array([ 1.96057347, -2.23120232,  1.11394019, -2.1999604 ]), array([ 2.06736241, -2.57381145, -0.03663801, -1.23506405]), array([ 1.93496356, -2.67883022, -1.29049834,  0.2175756 ]), array([ 1.54771988, -2.46668428, -2.58304938,  1.97622209]), array([ 0.91002759, -1.84842652, -3.75269182,  4.33952416]), array([ 0.06218913, -0.6760782 , -4.67496569,  7.35955468]), array([-0.86286489,  0.8487012 , -4.25107779,  7.06239228]), array([-1.57525118,  2.00891039, -2.88417224,  4.67310725]), array([-2.02768404,  2.78868622, -1.67101508,  3.24085523]), array([-2.25938717, -2.95530554, -0.68902758,  2.17011601]), array([-2.31566891, -2.62733497,  0.11089829,  1.09951119]), array([-2.20706856, -2.54116096,  0.99539028, -0.24967447]), array([-1.89819559, -2.75011812,  2.13221847, -1.84143432]), array([-1.35380675,  3.04177612,  3.31101567, -3.10301951]), array([-0.58597074,  2.22344449,  4.25778067, -5.20806751]), array([ 0.31372308,  0.89906945,  4.71731588, -8.0869729 ]), array([ 1.19911992, -0.73407716,  3.81244418, -7.41933904]), array([ 1.79307184, -1.98760755,  2.14125303, -5.24602734]), array([ 2.07523705, -2.89650466,  0.74920514, -3.92791936]), array([ 2.12393301,  2.71338198, -0.19703574, -2.81000274]), array([ 1.99286968,  2.30486795, -1.13025723, -1.27097299]), array([ 1.65783524,  2.20000166, -2.25648324,  0.17867437]), array([ 1.08166769,  2.34315304, -3.49422619,  1.1225114 ]), array([ 0.2855777 ,  2.58371909, -4.33938896,  1.09508932]), array([-0.58137764,  2.70846644, -4.13482804, -0.01460506]), array([-1.29688514,  2.52494549, -2.87029641, -1.90707659]), array([-1.68090316,  1.93485885, -0.88148723, -3.97779336]), array([-1.61602928,  0.8902843 ,  1.52171273, -6.50852585]), array([-1.15320389, -0.55059657,  2.83031934, -7.441962  ]), array([-0.54713856, -1.97561363,  3.18442334, -6.70143259]), array([ 0.12044274,  3.01366382,  3.41605039, -6.40428159]), array([ 0.77967898,  1.67261294,  3.17161905, -7.19368987]), array([ 1.40409532,  0.09705847,  2.94169603, -8.29383159]), array([ 1.80097651, -1.34846444,  0.82125848, -5.8999336 ]), array([ 1.73126301, -2.32920521, -1.49806303, -3.91479836]), array([ 1.24065521, -2.91793492, -3.27203961, -2.03094903]), array([ 0.46519398,  3.12864049, -4.33733335, -0.53975935]), array([-0.42620343,  3.05518912, -4.39171169, -0.45464064]), array([-1.22156204,  2.85621739, -3.4114641 , -1.71971476]), array([-1.73942174,  2.32368846, -1.64170882, -3.64643045]), array([-1.8240768 ,  1.35360254,  0.84259637, -6.09513161]), array([-1.41971183, -0.13166535,  2.96298075, -8.45939786]), array([-0.78011266, -1.78120128,  3.2781968 , -7.73881596]), array([-0.10675023,  3.04432636,  3.46385376, -7.10379825]), array([ 0.58540057,  1.55758597,  3.46563392, -8.00907297]), array([ 1.27296079, -0.1682187 ,  3.12085697, -8.67660615]), array([ 1.67494189, -1.63437405,  0.74956053, -5.84976247]), array([ 1.59592504, -2.60190298, -1.45619772, -3.88201643]), array([ 1.13632088,  3.10961459, -2.99836036, -1.95185999]), array([ 0.44382282,  2.83190757, -3.79816859, -1.06158949]), array([-0.31582068,  2.5771046 , -3.58997235, -1.77882236]), array([-0.89657297,  2.01713916, -1.97437947, -4.02012995]), array([-1.03257877,  0.92091269,  0.63987143, -6.96331679]), array([-0.74297087, -0.63306636,  1.78896892, -7.85460981]), array([-0.44730545, -2.02682806,  1.16116085, -6.1691796 ]), array([-0.22547192,  3.04678155,  1.18235476, -6.15521397]), array([ 0.08599018,  1.69347667,  2.07858663, -7.68858066]), array([ 0.62995131, -0.12380502,  2.96918287, -9.89164976]), array([ 1.00661962, -1.83434215,  0.50423985, -6.86333761]), array([ 0.87362296, -2.96879155, -1.57165833, -4.75454877]), array([ 0.5011273 ,  2.42217733, -1.85419455, -4.53857442]), array([ 0.24644005,  1.34154757, -0.46972344, -6.62876059]), array([ 0.31799866, -0.27057631,  0.64324117, -8.70948027]), array([ 0.21760574, -1.71409971, -1.84619554, -5.41732235]), array([-0.33663838, -2.54389202, -3.36349955, -3.27650883]), array([-1.01417076,  3.12678385, -3.12549197, -3.26766494]), array([-1.4841083 ,  2.30676542, -1.30245922, -5.15442392]), array([-1.43738124,  0.95820608,  1.82543467, -8.49820558]), array([-0.88071528, -0.95689696,  3.13678593, -9.71871278]), array([-0.33316906, -2.68513172,  2.46531968, -7.92431122]), array([ 0.18137972,  1.99467349,  2.85244451, -8.51309423]), array([ 8.74467051e-01, -6.20563939e-03,  3.74938094e+00, -1.10162764e+01]), array([ 1.3663364 , -1.8729556 ,  0.83836101, -7.26225182]), array([ 1.27130258, -3.04742929, -1.49802808, -4.74460733]), array([ 0.88221372,  2.41207154, -2.16731873, -3.7815713 ]), array([ 0.50135187,  1.55087346, -1.42834446, -5.17187094]), array([ 0.34648005,  0.2990393 , -0.28345748, -7.13219952]), array([ 0.20671093, -1.03914248, -1.52531114, -5.5205284 ]), array([-0.29120482, -1.83765965, -3.2437868 , -2.64284975]), array([-0.99145312, -2.17218054, -3.51275688, -1.03162392]), array([-1.63546857, -2.35958104, -2.8596419 , -1.04334437]), array([-2.13269316, -2.63769267, -2.13504569, -1.79442909]), array([-2.49304787, -3.10045676, -1.4691873 , -2.80759198]), array([-2.71092655,  2.55939704, -0.65850587, -3.36904759]), array([-2.72775606,  1.81583258,  0.5050445 , -4.04007707]), array([-2.50956278,  0.93651255,  1.67767792, -4.82078512]), array([-2.07851623, -0.07829197,  2.62436897, -5.32595274])]</t>
+  </si>
+  <si>
+    <t>['[2,0,1]', '[1,1,1]', '[2,1,0]', '[0,2,1]', '[0,0,0]', '[1,1,2]', '[2,2,2]', '[1,2,0]', '[0,1,1]', '[1,0,2]']</t>
+  </si>
+  <si>
+    <t>[1, 7, 8, 10, 11, 12, 18, 21, 23, 30, 32, 33, 44, 45, 46, 53, 55, 56, 57, 58, 65, 68, 69, 70, 79, 80, 81, 83, 91, 92, 93, 94, 96, 97, 106, 109, 111, 119, 120, 121, 124, 125, 126, 135, 137, 138]</t>
+  </si>
+  <si>
+    <t>[0, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 1, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 1, 2, 2, 2, 2, 2, 2, 2, 1, 0, 0, 0, 0, 0, 0]</t>
+  </si>
+  <si>
+    <t>['[-0.03763371 -0.01533471  0.06554052 -0.01816017]', '[-0.03406929  0.01398622 -0.02953871  0.30651903]', '[-0.04818188  0.10262173 -0.10566927  0.56184435]', '[-0.07305261  0.22936701 -0.13369446  0.67944384]', '[-0.0976443   0.36319498 -0.10327727  0.63282133]', '[-0.11125897  0.47297074 -0.02773051  0.446438  ]', '[-0.10757465  0.53619101  0.06462001  0.17794954]', '[-0.08631261  0.54305113  0.14348542 -0.10660175]', '[-0.05272941  0.496551    0.18460856 -0.34656399]', '[ 0.00949141  0.34442437  0.42357609 -1.14622288]', '[ 0.08181789  0.12456267  0.27776828 -1.00270047]', '[ 0.11305478 -0.03842766  0.02298882 -0.59407484]', '[ 0.08898582 -0.10427932 -0.26039092 -0.05758605]', '[ 0.01301088 -0.06379736 -0.48239648  0.44332039]', '[-0.09493041  0.06079888 -0.5710436   0.76371519]', '[-0.20399134  0.22349652 -0.49251944  0.81839645]', '[-0.28186422  0.37090075 -0.26691492  0.62112528]', '[-0.30514415  0.4610874   0.04044758  0.26464457]', '[-0.26577978  0.47385149  0.34553145 -0.13374516]', '[-0.14719463  0.34622384  0.81465267 -1.10985688]', '[ 0.04519062  0.05241701  1.061759   -1.74812431]', '[ 0.22864388 -0.24469999  0.72684887 -1.14296358]', '[ 0.34766106 -0.44844574  0.43503726 -0.84674636]', '[ 0.36929502 -0.50367552 -0.22224548  0.30156531]', '[ 0.26217842 -0.33212234 -0.82617287  1.37971214]', '[ 0.05409057  0.02292157 -1.20132919  2.07558269]', '[-0.19182873  0.44910846 -1.19204523  2.06547288]', '[-0.3987538   0.80711097 -0.83308424  1.44440602]', '[-0.51234353  1.00932966 -0.2843093   0.55572664]', '[-0.48729416  0.96740495  0.53145812 -0.97290556]', '[-0.32813235  0.68574332  1.03101864 -1.80446113]', '[-0.06678684  0.20628475  1.52270969 -2.88556871]', '[ 0.22029467 -0.33454658  1.26646372 -2.36531416]', '[ 0.41418193 -0.69327005  0.634327   -1.16065565]', '[ 0.48879823 -0.84888272  0.09863714 -0.3755911 ]', '[ 0.42938631 -0.77941755 -0.68281207  1.06295368]', '[ 0.22425704 -0.43268238 -1.33024254  2.34937404]', '[-0.07796873  0.11745888 -1.6080828   2.99239941]', '[-0.38045443  0.68946692 -1.33679615  2.57873052]', '[-0.58923899  1.1101921  -0.71693643  1.58278217]', '[-0.65966629  1.3149463   0.01856538  0.4586767 ]', '[-0.56421348  1.23958637  0.92087042 -1.21214834]', '[-0.30020024  0.83049063  1.68678457 -2.85834989]', '[ 0.08848535  0.12654223  2.10574422 -4.00474523]', '[ 0.46321518 -0.59726753  1.53572044 -3.02640627]', '[ 0.67769918 -1.0422964   0.58325414 -1.3953811 ]', '[ 0.69332703 -1.15446592 -0.42300937  0.27218116]', '[ 0.51366523 -0.93296645 -1.35064267  1.93871669]', '[ 0.16795412 -0.3899697  -2.04336329  3.40004526]', '[-0.26210221  0.34980622 -2.12905318  3.74237817]', '[-0.63516241  1.01322778 -1.52439992  2.76569919]', '[-0.85406497  1.43781469 -0.64201079  1.47404548]', '[-0.88782352  1.604279    0.30345309  0.19226009]', '[-0.73729887  1.51341228  1.17904628 -1.10584952]', '[-0.41062183  1.10750223  2.05045527 -2.95758424]', '[ 0.03834293  0.40885675  2.34601871 -3.87015153]', '[ 0.47562191 -0.33679018  1.90025171 -3.33149059]', '[ 0.76099034 -0.85470167  0.90701141 -1.78188599]', '[ 0.83062032 -1.04394134 -0.2137818  -0.11021459]', '[ 0.67853126 -0.8976125  -1.28812511  1.57574318]', '[ 0.32880924 -0.41924688 -2.15049331  3.13768842]', '[-0.1421223   0.28912867 -2.42818717  3.69134053]', '[-0.58873427  0.9528554  -1.94318474  2.78883288]', '[-0.89511638  1.37900154 -1.08448393  1.46350969]', '[-1.01340052  1.54185607 -0.08716356  0.17379315]', '[-0.92939842  1.44901095  0.91820512 -1.10901029]', '[-0.63410819  1.03885809  2.01034196 -3.01383154]', '[-0.14299018  0.25226142  2.80613555 -4.69359947]', '[ 0.39594481 -0.63426102  2.42673237 -3.85085213]', '[ 0.78818946 -1.22085676  1.44937315 -1.98314788]', '[ 0.96531376 -1.43392931  0.30666135 -0.16682128]', '[ 0.9077311  -1.29029128 -0.8820621   1.61220955]', '[ 0.61591733 -0.78087907 -2.01246025  3.48564092]', '[ 0.12741586  0.07122401 -2.74315449  4.7824071 ]', '[-0.40952595  0.98038453 -2.48514336  4.02816152]', '[-0.83334112  1.63429247 -1.70755899  2.49822203]', '[-1.07945878  1.9883244  -0.73061484  1.06588867]', '[-1.12007835  2.06682662  0.32741778 -0.27625564]', '[-0.93652707  1.83024034  1.49256085 -2.11614553]', '[-0.54957622  1.25363816  2.34029496 -3.66701768]', '[-0.02294493  0.3792112   2.82122923 -4.89427468]', '[ 0.50947925 -0.55859989  2.33703416 -4.1368307 ]', '[ 0.89186298 -1.25813901  1.43077904 -2.79259783]', '[ 1.0536031  -1.62611997  0.1858305  -0.91752525]', '[ 0.96860631 -1.62958731 -1.02171215  0.8914261 ]', '[ 0.65386853 -1.25957834 -2.09627783  2.83883556]', '[ 0.14624698 -0.4909519  -2.90618013  4.7512319 ]', '[-0.44815231  0.51861356 -2.84576859  4.93167406]', '[-0.93069263  1.35971739 -1.91113763  3.39504916]', '[-1.20123581  1.88460959 -0.78032924  1.89026597]', '[-1.24030863  2.12526782  0.38747188  0.52224057]', '[-1.05098595  2.09011063  1.48142635 -0.89156077]', '[-0.66368709  1.75963481  2.3374683  -2.43269441]', '[-0.14196653  1.11550801  2.8109012  -3.96969639]', '[ 0.42470052  0.22600323  2.72549908 -4.65374199]', '[ 0.90909228 -0.67111635  1.98614546 -4.04716175]', '[ 1.1670918  -1.28624743  0.5812306  -2.11651552]', '[ 1.14341177 -1.52634823 -0.80421759 -0.28339472]', '[ 0.85502912 -1.38984593 -2.04380581  1.68503555]', '[ 0.34521116 -0.839399   -2.99192901  3.80407856]', '[-0.3009266   0.07267564 -3.30364269  4.97097469]', '[-0.89777181  0.97742015 -2.53629218  3.8310771 ]', '[-1.29222708  1.58459665 -1.38571066  2.27666157]', '[-1.447668    1.90612011 -0.16360574  0.96418707]', '[-1.34296018  1.92599863  1.20076409 -0.78685395]', '[-0.97428781  1.57219441  2.46070452 -2.82024041]', '[-0.39194227  0.82558142  3.29973015 -4.6167046 ]', '[ 0.32072596 -0.25099554  3.62011997 -5.68630669]', '[ 0.96721999 -1.24885035  2.73025906 -4.0883113 ]', '[ 1.37989889 -1.84382528  1.39111283 -1.95527575]', '[ 1.53716974 -2.10243597  0.17673268 -0.65852084]', '[ 1.43635466 -2.06532945 -1.17919637  1.05076989]', '[ 1.06996301 -1.66232808 -2.4673747   3.05679771]', '[ 0.45798292 -0.80528417 -3.61714974  5.54759966]', '[-0.32417504  0.45451269 -3.94425142  6.43968013]', '[-1.02400791  1.55068986 -2.96666092  4.39497262]', '[-1.50207336  2.24472934 -1.80090317  2.64470774]', '[-1.74151587  2.63681733 -0.59360873  1.31407342]', '[-1.7408697   2.77558499  0.59806192  0.06974337]', '[-1.50226216  2.6584141   1.78454219 -1.26845842]', '[-1.03414651  2.25207213  2.85456784 -2.85141236]', '[-0.38652804  1.49202093  3.5544814  -4.79891768]', '[ 0.38210603  0.2862731   4.00648356 -6.98206025]', '[ 1.10756105 -1.038058    3.03101651 -5.77542655]', '[ 1.55095727 -1.94729893  1.42627529 -3.45600934]', '[ 1.68666335 -2.45889318 -0.05124033 -1.69853031]', '[ 1.53648502 -2.62674387 -1.43720083  0.04055999]', '[ 1.11927335 -2.42973095 -2.69695244  1.97377199]', '[ 0.4846612  -1.8147095  -3.56771663  4.24188487]', '[-0.28049758 -0.71438462 -4.02108165  6.67999194]', '[-1.04889907  0.67020656 -3.40294765  6.53882504]', '[-1.57783533  1.7740203  -1.869511    4.55386589]', '[-1.80301229  2.53578008 -0.40603545  3.12521738]', '[-1.75255726  3.03070438  0.880442    1.82058455]', '[-1.45229465 -3.04010253  2.11428331  0.31292423]', '[-0.91763659 -3.09609264  3.19453344 -0.82113919]', '[-0.1958854   2.90211503  3.88922772 -1.95567349]', '[ 0.55717806  2.47574683  3.47947187 -2.20881518]', '[ 1.14612647  2.06891664  2.33852407 -1.72434229]', '[ 1.49409898  1.78960209  1.13062811 -0.98232137]', '[ 1.59795811  1.69794854 -0.09119365  0.0907588 ]']</t>
+  </si>
+  <si>
+    <t>[0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50, 51, 52, 53, 54, 55, 56, 57, 58, 59, 60, 61, 62, 63, 64, 65, 66, 67, 68, 69, 70, 71, 72, 73, 74, 75, 76, 77, 78, 79, 80, 81, 82, 83, 84, 85, 86, 87, 88, 89, 90, 91, 92, 93, 94, 95, 96, 97, 98, 99, 100, 101, 102, 103, 104, 105, 106, 107, 108, 109, 110, 111, 112, 113, 114, 115, 116, 117, 118, 119, 120, 121, 122, 123, 124, 125, 126, 127, 128, 129, 130, 131, 132, 133, 134, 135, 136, 137, 138, 139, 140]</t>
+  </si>
+  <si>
+    <t>[array([-0.03763371, -0.01533471,  0.06554052, -0.01816017], dtype=float32), array([-0.03406929,  0.01398622, -0.02953871,  0.30651903]), array([-0.04818188,  0.10262173, -0.10566927,  0.56184435]), array([-0.07305261,  0.22936701, -0.13369446,  0.67944384]), array([-0.0976443 ,  0.36319498, -0.10327727,  0.63282133]), array([-0.11125897,  0.47297074, -0.02773051,  0.446438  ]), array([-0.10757465,  0.53619101,  0.06462001,  0.17794954]), array([-0.08631261,  0.54305113,  0.14348542, -0.10660175]), array([-0.05272941,  0.496551  ,  0.18460856, -0.34656399]), array([ 0.00949141,  0.34442437,  0.42357609, -1.14622288]), array([ 0.08181789,  0.12456267,  0.27776828, -1.00270047]), array([ 0.11305478, -0.03842766,  0.02298882, -0.59407484]), array([ 0.08898582, -0.10427932, -0.26039092, -0.05758605]), array([ 0.01301088, -0.06379736, -0.48239648,  0.44332039]), array([-0.09493041,  0.06079888, -0.5710436 ,  0.76371519]), array([-0.20399134,  0.22349652, -0.49251944,  0.81839645]), array([-0.28186422,  0.37090075, -0.26691492,  0.62112528]), array([-0.30514415,  0.4610874 ,  0.04044758,  0.26464457]), array([-0.26577978,  0.47385149,  0.34553145, -0.13374516]), array([-0.14719463,  0.34622384,  0.81465267, -1.10985688]), array([ 0.04519062,  0.05241701,  1.061759  , -1.74812431]), array([ 0.22864388, -0.24469999,  0.72684887, -1.14296358]), array([ 0.34766106, -0.44844574,  0.43503726, -0.84674636]), array([ 0.36929502, -0.50367552, -0.22224548,  0.30156531]), array([ 0.26217842, -0.33212234, -0.82617287,  1.37971214]), array([ 0.05409057,  0.02292157, -1.20132919,  2.07558269]), array([-0.19182873,  0.44910846, -1.19204523,  2.06547288]), array([-0.3987538 ,  0.80711097, -0.83308424,  1.44440602]), array([-0.51234353,  1.00932966, -0.2843093 ,  0.55572664]), array([-0.48729416,  0.96740495,  0.53145812, -0.97290556]), array([-0.32813235,  0.68574332,  1.03101864, -1.80446113]), array([-0.06678684,  0.20628475,  1.52270969, -2.88556871]), array([ 0.22029467, -0.33454658,  1.26646372, -2.36531416]), array([ 0.41418193, -0.69327005,  0.634327  , -1.16065565]), array([ 0.48879823, -0.84888272,  0.09863714, -0.3755911 ]), array([ 0.42938631, -0.77941755, -0.68281207,  1.06295368]), array([ 0.22425704, -0.43268238, -1.33024254,  2.34937404]), array([-0.07796873,  0.11745888, -1.6080828 ,  2.99239941]), array([-0.38045443,  0.68946692, -1.33679615,  2.57873052]), array([-0.58923899,  1.1101921 , -0.71693643,  1.58278217]), array([-0.65966629,  1.3149463 ,  0.01856538,  0.4586767 ]), array([-0.56421348,  1.23958637,  0.92087042, -1.21214834]), array([-0.30020024,  0.83049063,  1.68678457, -2.85834989]), array([ 0.08848535,  0.12654223,  2.10574422, -4.00474523]), array([ 0.46321518, -0.59726753,  1.53572044, -3.02640627]), array([ 0.67769918, -1.0422964 ,  0.58325414, -1.3953811 ]), array([ 0.69332703, -1.15446592, -0.42300937,  0.27218116]), array([ 0.51366523, -0.93296645, -1.35064267,  1.93871669]), array([ 0.16795412, -0.3899697 , -2.04336329,  3.40004526]), array([-0.26210221,  0.34980622, -2.12905318,  3.74237817]), array([-0.63516241,  1.01322778, -1.52439992,  2.76569919]), array([-0.85406497,  1.43781469, -0.64201079,  1.47404548]), array([-0.88782352,  1.604279  ,  0.30345309,  0.19226009]), array([-0.73729887,  1.51341228,  1.17904628, -1.10584952]), array([-0.41062183,  1.10750223,  2.05045527, -2.95758424]), array([ 0.03834293,  0.40885675,  2.34601871, -3.87015153]), array([ 0.47562191, -0.33679018,  1.90025171, -3.33149059]), array([ 0.76099034, -0.85470167,  0.90701141, -1.78188599]), array([ 0.83062032, -1.04394134, -0.2137818 , -0.11021459]), array([ 0.67853126, -0.8976125 , -1.28812511,  1.57574318]), array([ 0.32880924, -0.41924688, -2.15049331,  3.13768842]), array([-0.1421223 ,  0.28912867, -2.42818717,  3.69134053]), array([-0.58873427,  0.9528554 , -1.94318474,  2.78883288]), array([-0.89511638,  1.37900154, -1.08448393,  1.46350969]), array([-1.01340052,  1.54185607, -0.08716356,  0.17379315]), array([-0.92939842,  1.44901095,  0.91820512, -1.10901029]), array([-0.63410819,  1.03885809,  2.01034196, -3.01383154]), array([-0.14299018,  0.25226142,  2.80613555, -4.69359947]), array([ 0.39594481, -0.63426102,  2.42673237, -3.85085213]), array([ 0.78818946, -1.22085676,  1.44937315, -1.98314788]), array([ 0.96531376, -1.43392931,  0.30666135, -0.16682128]), array([ 0.9077311 , -1.29029128, -0.8820621 ,  1.61220955]), array([ 0.61591733, -0.78087907, -2.01246025,  3.48564092]), array([ 0.12741586,  0.07122401, -2.74315449,  4.7824071 ]), array([-0.40952595,  0.98038453, -2.48514336,  4.02816152]), array([-0.83334112,  1.63429247, -1.70755899,  2.49822203]), array([-1.07945878,  1.9883244 , -0.73061484,  1.06588867]), array([-1.12007835,  2.06682662,  0.32741778, -0.27625564]), array([-0.93652707,  1.83024034,  1.49256085, -2.11614553]), array([-0.54957622,  1.25363816,  2.34029496, -3.66701768]), array([-0.02294493,  0.3792112 ,  2.82122923, -4.89427468]), array([ 0.50947925, -0.55859989,  2.33703416, -4.1368307 ]), array([ 0.89186298, -1.25813901,  1.43077904, -2.79259783]), array([ 1.0536031 , -1.62611997,  0.1858305 , -0.91752525]), array([ 0.96860631, -1.62958731, -1.02171215,  0.8914261 ]), array([ 0.65386853, -1.25957834, -2.09627783,  2.83883556]), array([ 0.14624698, -0.4909519 , -2.90618013,  4.7512319 ]), array([-0.44815231,  0.51861356, -2.84576859,  4.93167406]), array([-0.93069263,  1.35971739, -1.91113763,  3.39504916]), array([-1.20123581,  1.88460959, -0.78032924,  1.89026597]), array([-1.24030863,  2.12526782,  0.38747188,  0.52224057]), array([-1.05098595,  2.09011063,  1.48142635, -0.89156077]), array([-0.66368709,  1.75963481,  2.3374683 , -2.43269441]), array([-0.14196653,  1.11550801,  2.8109012 , -3.96969639]), array([ 0.42470052,  0.22600323,  2.72549908, -4.65374199]), array([ 0.90909228, -0.67111635,  1.98614546, -4.04716175]), array([ 1.1670918 , -1.28624743,  0.5812306 , -2.11651552]), array([ 1.14341177, -1.52634823, -0.80421759, -0.28339472]), array([ 0.85502912, -1.38984593, -2.04380581,  1.68503555]), array([ 0.34521116, -0.839399  , -2.99192901,  3.80407856]), array([-0.3009266 ,  0.07267564, -3.30364269,  4.97097469]), array([-0.89777181,  0.97742015, -2.53629218,  3.8310771 ]), array([-1.29222708,  1.58459665, -1.38571066,  2.27666157]), array([-1.447668  ,  1.90612011, -0.16360574,  0.96418707]), array([-1.34296018,  1.92599863,  1.20076409, -0.78685395]), array([-0.97428781,  1.57219441,  2.46070452, -2.82024041]), array([-0.39194227,  0.82558142,  3.29973015, -4.6167046 ]), array([ 0.32072596, -0.25099554,  3.62011997, -5.68630669]), array([ 0.96721999, -1.24885035,  2.73025906, -4.0883113 ]), array([ 1.37989889, -1.84382528,  1.39111283, -1.95527575]), array([ 1.53716974, -2.10243597,  0.17673268, -0.65852084]), array([ 1.43635466, -2.06532945, -1.17919637,  1.05076989]), array([ 1.06996301, -1.66232808, -2.4673747 ,  3.05679771]), array([ 0.45798292, -0.80528417, -3.61714974,  5.54759966]), array([-0.32417504,  0.45451269, -3.94425142,  6.43968013]), array([-1.02400791,  1.55068986, -2.96666092,  4.39497262]), array([-1.50207336,  2.24472934, -1.80090317,  2.64470774]), array([-1.74151587,  2.63681733, -0.59360873,  1.31407342]), array([-1.7408697 ,  2.77558499,  0.59806192,  0.06974337]), array([-1.50226216,  2.6584141 ,  1.78454219, -1.26845842]), array([-1.03414651,  2.25207213,  2.85456784, -2.85141236]), array([-0.38652804,  1.49202093,  3.5544814 , -4.79891768]), array([ 0.38210603,  0.2862731 ,  4.00648356, -6.98206025]), array([ 1.10756105, -1.038058  ,  3.03101651, -5.77542655]), array([ 1.55095727, -1.94729893,  1.42627529, -3.45600934]), array([ 1.68666335, -2.45889318, -0.05124033, -1.69853031]), array([ 1.53648502, -2.62674387, -1.43720083,  0.04055999]), array([ 1.11927335, -2.42973095, -2.69695244,  1.97377199]), array([ 0.4846612 , -1.8147095 , -3.56771663,  4.24188487]), array([-0.28049758, -0.71438462, -4.02108165,  6.67999194]), array([-1.04889907,  0.67020656, -3.40294765,  6.53882504]), array([-1.57783533,  1.7740203 , -1.869511  ,  4.55386589]), array([-1.80301229,  2.53578008, -0.40603545,  3.12521738]), array([-1.75255726,  3.03070438,  0.880442  ,  1.82058455]), array([-1.45229465, -3.04010253,  2.11428331,  0.31292423]), array([-0.91763659, -3.09609264,  3.19453344, -0.82113919]), array([-0.1958854 ,  2.90211503,  3.88922772, -1.95567349]), array([ 0.55717806,  2.47574683,  3.47947187, -2.20881518]), array([ 1.14612647,  2.06891664,  2.33852407, -1.72434229]), array([ 1.49409898,  1.78960209,  1.13062811, -0.98232137]), array([ 1.59795811,  1.69794854, -0.09119365,  0.0907588 ])]</t>
+  </si>
+  <si>
+    <t>['[0,0,0]', '[2,0,1]', '[1,2,0]', '[1,0,2]', '[0,1,1]', '[1,1,1]', '[2,1,0]', '[0,2,1]', '[2,2,2]', '[1,1,2]']</t>
+  </si>
+  <si>
+    <t>[1, 7, 8, 9, 10, 11, 12, 13, 18, 19, 20, 22, 23, 30, 31, 32, 33, 35, 42, 43, 44, 45, 46, 47, 54, 56, 57, 64, 65, 66, 67, 68, 69, 76, 77, 78, 79, 82, 90, 91, 92, 93, 100, 101, 102, 103, 104, 105, 112, 113, 114, 115, 117, 126, 127, 128, 129, 136, 137, 138, 139, 140, 141, 148, 150, 151, 152, 153, 164, 165, 166, 176, 177, 178, 179, 187, 188, 189, 190, 191]</t>
+  </si>
+  <si>
+    <t>[0, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 1, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2]</t>
+  </si>
+  <si>
+    <t>['[-0.03763371 -0.01533471  0.06554052 -0.01816017]', '[-0.03406929  0.01398622 -0.02953871  0.30651903]', '[-0.04818188  0.10262173 -0.10566927  0.56184435]', '[-0.07305261  0.22936701 -0.13369446  0.67944384]', '[-0.0976443   0.36319498 -0.10327727  0.63282133]', '[-0.11125897  0.47297074 -0.02773051  0.446438  ]', '[-0.10757465  0.53619101  0.06462001  0.17794954]', '[-0.08631261  0.54305113  0.14348542 -0.10660175]', '[-0.05272941  0.496551    0.18460856 -0.34656399]', '[-0.01604448  0.4107609   0.17301646 -0.49290646]', '[ 0.01268242  0.3077355   0.10583916 -0.51655332]', '[ 0.02333646  0.21239857 -0.00419223 -0.4193517 ]', '[ 0.0099677   0.14579835 -0.12877174 -0.23752332]', '[-0.02671453  0.11914618 -0.23135882 -0.03029568]', '[-0.07887305  0.13122166 -0.27923433  0.14079468]', '[-0.13346965  0.17000821 -0.25455054  0.23213127]', '[-0.17594228  0.2177196  -0.16032293  0.23074589]', '[-0.19440453  0.25720213 -0.01958413  0.15500349]', '[-0.18304473  0.2773318   0.13139765  0.04471749]', '[-0.14381952  0.27594314  0.25290378 -0.05262463]', '[-0.08610129  0.25997418  0.3121551  -0.09574381]', '[ 0.00183595  0.17495747  0.54689319 -0.72703824]', '[ 0.09557953  0.05418817  0.36786412 -0.44499093]', '[ 0.14170373  0.0081064   0.08301233 -0.00137938]', '[ 0.1273555   0.05481997 -0.22174887  0.45757825]', '[ 0.05778981  0.18193167 -0.45541294  0.77977586]', '[-0.04525583  0.34972444 -0.54891039  0.85292758]', '[-0.15078402  0.50468653 -0.48153459  0.65712629]', '[-0.22892626  0.59918267 -0.28301143  0.2648742 ]', '[-0.25905722  0.60479004 -0.01244471 -0.21287557]', '[-0.23381404  0.51596654  0.25840306 -0.66005261]', '[-0.16077749  0.35097031  0.45339827 -0.95441631]', '[-0.06200744  0.15221008  0.50802846 -0.98387117]', '[ 0.03133234 -0.02188089  0.40079597 -0.71186272]', '[ 0.11623195 -0.18562619  0.42551823 -0.88338111]', '[ 0.16615191 -0.28989452  0.06192274 -0.13721657]', '[ 0.13970435 -0.23803727 -0.31962088  0.64357754]', '[ 0.04465327 -0.04419492 -0.60580252  1.2474422 ]', '[-0.08920216  0.23517068 -0.69527889  1.47355482]', '[-0.2177861   0.51492473 -0.55696001  1.25954261]', '[-0.3008671   0.7179952  -0.25560235  0.7362623 ]', '[-0.31571618  0.80058623  0.10939694  0.08067733]', '[-0.25893116  0.75063981  0.44677019 -0.5682265 ]', '[-0.14431768  0.58246873  0.67488375 -1.0780532 ]', '[-0.00131047  0.33910027  0.72061917 -1.29608301]', '[ 0.12886819  0.09130814  0.54664552 -1.11706114]', '[ 0.20515223 -0.08424161  0.19564233 -0.5968959 ]', '[ 0.20241065 -0.13677432 -0.22342513  0.07889146]', '[ 0.11950118 -0.05621491 -0.58630209  0.70016634]', '[-0.02078633  0.12617673 -0.78189271  1.06858112]', '[-0.17742139  0.34540386 -0.74597713  1.06121455]', '[-0.30462432  0.52751181 -0.49727039  0.71597028]', '[-0.36743593  0.61883059 -0.11800364  0.17930419]', '[-0.32516778  0.53199537  0.53265167 -1.03488597]', '[-0.18853105  0.28538719  0.80041053 -1.37386324]', '[ 0.00491386 -0.05699143  1.08315368 -1.95742226]', '[ 0.19467049 -0.38546347  0.76766427 -1.24462643]', '[ 0.2979203  -0.53213571  0.2441543  -0.19342098]', '[ 0.28823745 -0.45874932 -0.33876361  0.91760636]', '[ 0.16818786 -0.17710919 -0.83187883  1.8404406 ]', '[-0.02600161  0.24104355 -1.05282141  2.22783727]', '[-0.22811413  0.66533118 -0.91583741  1.91558188]', '[-0.37565712  0.97782015 -0.53237883  1.16558947]', '[-0.43412789  1.12159372 -0.04475253  0.2612277 ]', '[-0.39346062  1.08124187  0.44389877 -0.65921233]', '[-0.26244421  0.86353968  0.84363028 -1.4904002 ]', '[-0.06882853  0.50367904  1.05046059 -2.03732825]', '[ 0.13638753  0.08797821  0.94479099 -2.00927749]', '[ 0.28676748 -0.25591283  0.51743902 -1.34621764]', '[ 0.33224733 -0.42752426 -0.07328003 -0.34221471]', '[ 0.25836069 -0.38988879 -0.64997368  0.70428188]', '[ 0.08340221 -0.16003701 -1.0591898   1.53301019]', '[-0.14412445  0.1879864  -1.15709809  1.84410566]', '[-0.35501147  0.53457195 -0.90058081  1.53447512]', '[-0.48796851  0.77549955 -0.40273285  0.83535981]', '[-0.51004297  0.85968508  0.18517503 -0.00167911]', '[-0.41658288  0.77557086  0.73206281 -0.82508195]', '[-0.22838488  0.54138202  1.1112874  -1.46712018]', '[ 0.00791347  0.21829388  1.1948483  -1.67172446]', '[ 0.2250317  -0.08580748  0.92213036 -1.27776841]', '[ 0.38474616 -0.33078861  0.63670305 -1.1082494 ]', '[ 0.46737111 -0.50825619  0.17058639 -0.63210355]', '[ 0.42454022 -0.510011   -0.5901735   0.61034627]', '[ 0.24032809 -0.27369057 -1.21316083  1.69940087]', '[-0.03790805  0.1332486  -1.49794257  2.24596227]', '[-0.32682815  0.56753307 -1.32017966  1.9751699 ]', '[-0.54242991  0.88688647 -0.7955123   1.16632224]', '[-0.6341852   1.02301616 -0.10833792  0.18394112]', '[-0.56249335  0.90065846  0.81706657 -1.40399778]', '[-0.31552682  0.46766823  1.61146115 -2.87079065]', '[ 0.02616292 -0.12794317  1.70867374 -2.90057625]', '[ 0.32953313 -0.61976336  1.25485001 -1.89684918]', '[ 0.5087583  -0.85979641  0.5086615  -0.47605188]', '[ 0.52613537 -0.80630341 -0.33988524  1.00925868]', '[ 0.37554758 -0.46135308 -1.14050413  2.39861535]', '[ 0.09074254  0.11567421 -1.62591583  3.21315451]', '[-0.2341639   0.74302866 -1.534279    2.88966299]', '[-0.49604747  1.22572746 -1.04249554  1.88284997]', '[-0.63995117  1.48732963 -0.37988301  0.72679816]', '[-0.64461183  1.5158997   0.33248741 -0.4405663 ]', '[-0.51059241  1.31156683  0.9899706  -1.59729641]', '[-0.2592947   0.88324224  1.48503693 -2.64551156]', '[ 0.06079983  0.28783409  1.63741775 -3.16404765]', '[ 0.35655911 -0.30525182  1.23258327 -2.5932545 ]', '[ 0.52776467 -0.70008936  0.44605768 -1.29522757]', '[ 0.52984913 -0.81346552 -0.42178753  0.16662464]', '[ 0.36518753 -0.63566712 -1.19642352  1.58784534]', '[ 0.06915559 -0.20018953 -1.69810333  2.66159003]', '[-0.27822111  0.36376408 -1.68002403  2.79811949]', '[-0.56776315  0.85561027 -1.15469038  2.02409601]', '[-0.72422312  1.15371495 -0.38877222  0.93784778]', '[-0.71974524  1.22784712  0.43046876 -0.19889696]', '[-0.55749651  1.07419858  1.16707423 -1.32946485]', '[-0.26781899  0.7057496   1.6782155  -2.2988452 ]', '[ 0.08557296  0.19628197  1.76972757 -2.6464173 ]', '[ 0.40190954 -0.28247196  1.31325738 -1.99615529]', '[ 0.61183206 -0.62750459  0.74162278 -1.38442733]', '[ 0.66340896 -0.75699952 -0.23153789  0.09799881]', '[ 0.52213134 -0.58883209 -1.15907045  1.5664454 ]', '[ 0.21612475 -0.1496853  -1.83454646  2.72033762]', '[-0.17357002  0.43037551 -1.95735422  2.88432093]', '[-0.52748146  0.93424796 -1.51070957  2.04983617]', '[-0.75771801  1.22994015 -0.75951676  0.89078043]', '[-0.82317529  1.28957117  0.11328239 -0.2930535 ]', '[-0.69267153  1.05734401  1.18228988 -2.0369319 ]', '[-0.35916311  0.47593976  2.10312218 -3.71580789]', '[ 0.08195941 -0.28734196  2.17556052 -3.65205719]', '[ 0.46290293 -0.89142114  1.5585008  -2.26805701]', '[ 0.68698255 -1.17725916  0.65447204 -0.58359689]', '[ 0.71730444 -1.12548735 -0.35978826  1.10120653]', '[ 0.54337849 -0.73578622 -1.36327191  2.78396821]', '[ 0.18967437 -0.03746372 -2.08278561  4.02895813]', '[-0.23541978  0.7655832  -2.04145707  3.7478508 ]', '[-0.59057126  1.39780915 -1.45914886  2.51676274]', '[-0.80587125  1.76842602 -0.67200467  1.19557767]', '[-0.85387372  1.87890854  0.19548121 -0.08694828]', '[-0.73023238  1.73324042  1.02418433 -1.37375949]', '[-0.45460451  1.32749451  1.69845928 -2.68019821]', '[-0.06858952  0.67296638  2.09764123 -3.7744026 ]', '[ 0.3437008  -0.10553441  1.8995812  -3.75450313]', '[ 0.6440443  -0.73428458  1.03497863 -2.40734472]', '[ 0.74533766 -1.05053938 -0.02791308 -0.74684593]', '[ 0.6360776  -1.03235008 -1.04518577  0.92954236]', '[ 0.33951856 -0.68073235 -1.87515527  2.55333512]', '[-0.08590818 -0.04920033 -2.27583522  3.57568859]', '[-0.5185508   0.64692733 -1.93658587  3.16950862]', '[-0.82803877  1.16637826 -1.11340659  1.97884728]', '[-0.95400337  1.43544136 -0.13564976  0.71417634]', '[-0.88229642  1.45175768  0.84153661 -0.55710392]', '[-0.60740034  1.15533712  1.87672929 -2.42291313]', '[-0.17206724  0.54765142  2.3984835  -3.54711782]', '[ 0.305273   -0.17804701  2.24157916 -3.44593025]', '[ 0.67675921 -0.73935458  1.40033492 -2.05231707]', '[ 0.84944406 -0.98409619  0.30816429 -0.39205736]', '[ 0.79746249 -0.89690746 -0.82316566  1.26456966]', '[ 0.52704488 -0.47969617 -1.84253993  2.86882545]', '[ 0.09038894  0.20251023 -2.4081015   3.73078396]', '[-0.38110494  0.90270328 -2.19567758  3.06917264]', '[-0.75625879  1.38729027 -1.5039173   1.74446176]', '[-0.96750967  1.60094759 -0.58347346  0.4033711 ]', '[-0.96594412  1.50279363  0.60516518 -1.38864265]', '[-0.72583912  1.03679606  1.78574014 -3.29869022]', '[-0.26486035  0.18852015  2.72917061 -5.0192734 ]', '[ 0.29405424 -0.8207903   2.68149677 -4.69823738]', '[ 0.74221771 -1.55487933  1.76260668 -2.6386636 ]', '[ 0.9890743  -1.89102377  0.68574312 -0.75478086]', '[ 1.01080218 -1.86355878 -0.47388625  1.02911376]', '[ 0.80034794 -1.47204364 -1.62274392  2.92244314]', '[ 0.36722255 -0.67742139 -2.67025976  5.00679459]', '[-0.21831509  0.43816358 -2.97147459  5.69263499]', '[-0.74117297  1.43255089 -2.16721776  4.11213656]', '[-1.07211242  2.08983459 -1.12469261  2.50752736]', '[-1.18630636  2.44962921 -0.01345991  1.10895529]', '[-1.07955831  2.53604784  1.06493871 -0.24389516]', '[-0.76016663  2.31022126  2.07902339 -2.02355126]', '[-0.27423872  1.71987217  2.71713213 -3.90254813]', '[ 0.28653582  0.80130083  2.82223693 -5.17741471]', '[ 0.80408678 -0.24027023  2.18636137 -4.87025393]', '[ 1.10628341 -1.03708281  0.78224033 -3.01641917]', '[ 1.11412117 -1.447636   -0.68986376 -1.09127964]', '[ 0.84222696 -1.46665989 -1.98267715  0.92928618]', '[ 0.34639109 -1.0659718  -2.90149564  3.0712675 ]', '[-0.281866   -0.27156876 -3.25407839  4.64080651]', '[-0.88523881  0.63770049 -2.62675476  4.12738474]', '[-1.29659974  1.31895558 -1.45336337  2.67887071]', '[-1.46165079  1.72331902 -0.19178246  1.38850967]', '[-1.372951    1.87388519  1.07298386  0.09160579]', '[-1.03925415  1.74255549  2.23068663 -1.45632372]', '[-0.50192499  1.2729355   3.07363245 -3.25457688]', '[ 0.15470044  0.46557673  3.36983933 -4.60937476]', '[ 0.77615314 -0.41948399  2.68165993 -3.88740811]', '[ 1.18662847 -1.01441482  1.38546595 -2.03941612]', '[ 1.34654424 -1.30388654  0.2050182  -0.86990924]', '[ 1.24861476 -1.30877099 -1.17783202  0.84410892]', '[ 0.880509   -0.94716364 -2.47957129  2.82058109]', '[ 0.27649319 -0.18336941 -3.45185998  4.63833011]', '[-0.42488721  0.74713316 -3.3712614   4.26001935]', '[-1.01900426  1.42697681 -2.49935347  2.4985739 ]', '[-1.40761714  1.76440229 -1.36126033  0.93916563]', '[-1.55821292  1.82496969 -0.13987643 -0.29833789]']</t>
+  </si>
+  <si>
+    <t>[array([-0.03763371, -0.01533471,  0.06554052, -0.01816017], dtype=float32), array([-0.03406929,  0.01398622, -0.02953871,  0.30651903]), array([-0.04818188,  0.10262173, -0.10566927,  0.56184435]), array([-0.07305261,  0.22936701, -0.13369446,  0.67944384]), array([-0.0976443 ,  0.36319498, -0.10327727,  0.63282133]), array([-0.11125897,  0.47297074, -0.02773051,  0.446438  ]), array([-0.10757465,  0.53619101,  0.06462001,  0.17794954]), array([-0.08631261,  0.54305113,  0.14348542, -0.10660175]), array([-0.05272941,  0.496551  ,  0.18460856, -0.34656399]), array([-0.01604448,  0.4107609 ,  0.17301646, -0.49290646]), array([ 0.01268242,  0.3077355 ,  0.10583916, -0.51655332]), array([ 0.02333646,  0.21239857, -0.00419223, -0.4193517 ]), array([ 0.0099677 ,  0.14579835, -0.12877174, -0.23752332]), array([-0.02671453,  0.11914618, -0.23135882, -0.03029568]), array([-0.07887305,  0.13122166, -0.27923433,  0.14079468]), array([-0.13346965,  0.17000821, -0.25455054,  0.23213127]), array([-0.17594228,  0.2177196 , -0.16032293,  0.23074589]), array([-0.19440453,  0.25720213, -0.01958413,  0.15500349]), array([-0.18304473,  0.2773318 ,  0.13139765,  0.04471749]), array([-0.14381952,  0.27594314,  0.25290378, -0.05262463]), array([-0.08610129,  0.25997418,  0.3121551 , -0.09574381]), array([ 0.00183595,  0.17495747,  0.54689319, -0.72703824]), array([ 0.09557953,  0.05418817,  0.36786412, -0.44499093]), array([ 0.14170373,  0.0081064 ,  0.08301233, -0.00137938]), array([ 0.1273555 ,  0.05481997, -0.22174887,  0.45757825]), array([ 0.05778981,  0.18193167, -0.45541294,  0.77977586]), array([-0.04525583,  0.34972444, -0.54891039,  0.85292758]), array([-0.15078402,  0.50468653, -0.48153459,  0.65712629]), array([-0.22892626,  0.59918267, -0.28301143,  0.2648742 ]), array([-0.25905722,  0.60479004, -0.01244471, -0.21287557]), array([-0.23381404,  0.51596654,  0.25840306, -0.66005261]), array([-0.16077749,  0.35097031,  0.45339827, -0.95441631]), array([-0.06200744,  0.15221008,  0.50802846, -0.98387117]), array([ 0.03133234, -0.02188089,  0.40079597, -0.71186272]), array([ 0.11623195, -0.18562619,  0.42551823, -0.88338111]), array([ 0.16615191, -0.28989452,  0.06192274, -0.13721657]), array([ 0.13970435, -0.23803727, -0.31962088,  0.64357754]), array([ 0.04465327, -0.04419492, -0.60580252,  1.2474422 ]), array([-0.08920216,  0.23517068, -0.69527889,  1.47355482]), array([-0.2177861 ,  0.51492473, -0.55696001,  1.25954261]), array([-0.3008671 ,  0.7179952 , -0.25560235,  0.7362623 ]), array([-0.31571618,  0.80058623,  0.10939694,  0.08067733]), array([-0.25893116,  0.75063981,  0.44677019, -0.5682265 ]), array([-0.14431768,  0.58246873,  0.67488375, -1.0780532 ]), array([-0.00131047,  0.33910027,  0.72061917, -1.29608301]), array([ 0.12886819,  0.09130814,  0.54664552, -1.11706114]), array([ 0.20515223, -0.08424161,  0.19564233, -0.5968959 ]), array([ 0.20241065, -0.13677432, -0.22342513,  0.07889146]), array([ 0.11950118, -0.05621491, -0.58630209,  0.70016634]), array([-0.02078633,  0.12617673, -0.78189271,  1.06858112]), array([-0.17742139,  0.34540386, -0.74597713,  1.06121455]), array([-0.30462432,  0.52751181, -0.49727039,  0.71597028]), array([-0.36743593,  0.61883059, -0.11800364,  0.17930419]), array([-0.32516778,  0.53199537,  0.53265167, -1.03488597]), array([-0.18853105,  0.28538719,  0.80041053, -1.37386324]), array([ 0.00491386, -0.05699143,  1.08315368, -1.95742226]), array([ 0.19467049, -0.38546347,  0.76766427, -1.24462643]), array([ 0.2979203 , -0.53213571,  0.2441543 , -0.19342098]), array([ 0.28823745, -0.45874932, -0.33876361,  0.91760636]), array([ 0.16818786, -0.17710919, -0.83187883,  1.8404406 ]), array([-0.02600161,  0.24104355, -1.05282141,  2.22783727]), array([-0.22811413,  0.66533118, -0.91583741,  1.91558188]), array([-0.37565712,  0.97782015, -0.53237883,  1.16558947]), array([-0.43412789,  1.12159372, -0.04475253,  0.2612277 ]), array([-0.39346062,  1.08124187,  0.44389877, -0.65921233]), array([-0.26244421,  0.86353968,  0.84363028, -1.4904002 ]), array([-0.06882853,  0.50367904,  1.05046059, -2.03732825]), array([ 0.13638753,  0.08797821,  0.94479099, -2.00927749]), array([ 0.28676748, -0.25591283,  0.51743902, -1.34621764]), array([ 0.33224733, -0.42752426, -0.07328003, -0.34221471]), array([ 0.25836069, -0.38988879, -0.64997368,  0.70428188]), array([ 0.08340221, -0.16003701, -1.0591898 ,  1.53301019]), array([-0.14412445,  0.1879864 , -1.15709809,  1.84410566]), array([-0.35501147,  0.53457195, -0.90058081,  1.53447512]), array([-0.48796851,  0.77549955, -0.40273285,  0.83535981]), array([-0.51004297,  0.85968508,  0.18517503, -0.00167911]), array([-0.41658288,  0.77557086,  0.73206281, -0.82508195]), array([-0.22838488,  0.54138202,  1.1112874 , -1.46712018]), array([ 0.00791347,  0.21829388,  1.1948483 , -1.67172446]), array([ 0.2250317 , -0.08580748,  0.92213036, -1.27776841]), array([ 0.38474616, -0.33078861,  0.63670305, -1.1082494 ]), array([ 0.46737111, -0.50825619,  0.17058639, -0.63210355]), array([ 0.42454022, -0.510011  , -0.5901735 ,  0.61034627]), array([ 0.24032809, -0.27369057, -1.21316083,  1.69940087]), array([-0.03790805,  0.1332486 , -1.49794257,  2.24596227]), array([-0.32682815,  0.56753307, -1.32017966,  1.9751699 ]), array([-0.54242991,  0.88688647, -0.7955123 ,  1.16632224]), array([-0.6341852 ,  1.02301616, -0.10833792,  0.18394112]), array([-0.56249335,  0.90065846,  0.81706657, -1.40399778]), array([-0.31552682,  0.46766823,  1.61146115, -2.87079065]), array([ 0.02616292, -0.12794317,  1.70867374, -2.90057625]), array([ 0.32953313, -0.61976336,  1.25485001, -1.89684918]), array([ 0.5087583 , -0.85979641,  0.5086615 , -0.47605188]), array([ 0.52613537, -0.80630341, -0.33988524,  1.00925868]), array([ 0.37554758, -0.46135308, -1.14050413,  2.39861535]), array([ 0.09074254,  0.11567421, -1.62591583,  3.21315451]), array([-0.2341639 ,  0.74302866, -1.534279  ,  2.88966299]), array([-0.49604747,  1.22572746, -1.04249554,  1.88284997]), array([-0.63995117,  1.48732963, -0.37988301,  0.72679816]), array([-0.64461183,  1.5158997 ,  0.33248741, -0.4405663 ]), array([-0.51059241,  1.31156683,  0.9899706 , -1.59729641]), array([-0.2592947 ,  0.88324224,  1.48503693, -2.64551156]), array([ 0.06079983,  0.28783409,  1.63741775, -3.16404765]), array([ 0.35655911, -0.30525182,  1.23258327, -2.5932545 ]), array([ 0.52776467, -0.70008936,  0.44605768, -1.29522757]), array([ 0.52984913, -0.81346552, -0.42178753,  0.16662464]), array([ 0.36518753, -0.63566712, -1.19642352,  1.58784534]), array([ 0.06915559, -0.20018953, -1.69810333,  2.66159003]), array([-0.27822111,  0.36376408, -1.68002403,  2.79811949]), array([-0.56776315,  0.85561027, -1.15469038,  2.02409601]), array([-0.72422312,  1.15371495, -0.38877222,  0.93784778]), array([-0.71974524,  1.22784712,  0.43046876, -0.19889696]), array([-0.55749651,  1.07419858,  1.16707423, -1.32946485]), array([-0.26781899,  0.7057496 ,  1.6782155 , -2.2988452 ]), array([ 0.08557296,  0.19628197,  1.76972757, -2.6464173 ]), array([ 0.40190954, -0.28247196,  1.31325738, -1.99615529]), array([ 0.61183206, -0.62750459,  0.74162278, -1.38442733]), array([ 0.66340896, -0.75699952, -0.23153789,  0.09799881]), array([ 0.52213134, -0.58883209, -1.15907045,  1.5664454 ]), array([ 0.21612475, -0.1496853 , -1.83454646,  2.72033762]), array([-0.17357002,  0.43037551, -1.95735422,  2.88432093]), array([-0.52748146,  0.93424796, -1.51070957,  2.04983617]), array([-0.75771801,  1.22994015, -0.75951676,  0.89078043]), array([-0.82317529,  1.28957117,  0.11328239, -0.2930535 ]), array([-0.69267153,  1.05734401,  1.18228988, -2.0369319 ]), array([-0.35916311,  0.47593976,  2.10312218, -3.71580789]), array([ 0.08195941, -0.28734196,  2.17556052, -3.65205719]), array([ 0.46290293, -0.89142114,  1.5585008 , -2.26805701]), array([ 0.68698255, -1.17725916,  0.65447204, -0.58359689]), array([ 0.71730444, -1.12548735, -0.35978826,  1.10120653]), array([ 0.54337849, -0.73578622, -1.36327191,  2.78396821]), array([ 0.18967437, -0.03746372, -2.08278561,  4.02895813]), array([-0.23541978,  0.7655832 , -2.04145707,  3.7478508 ]), array([-0.59057126,  1.39780915, -1.45914886,  2.51676274]), array([-0.80587125,  1.76842602, -0.67200467,  1.19557767]), array([-0.85387372,  1.87890854,  0.19548121, -0.08694828]), array([-0.73023238,  1.73324042,  1.02418433, -1.37375949]), array([-0.45460451,  1.32749451,  1.69845928, -2.68019821]), array([-0.06858952,  0.67296638,  2.09764123, -3.7744026 ]), array([ 0.3437008 , -0.10553441,  1.8995812 , -3.75450313]), array([ 0.6440443 , -0.73428458,  1.03497863, -2.40734472]), array([ 0.74533766, -1.05053938, -0.02791308, -0.74684593]), array([ 0.6360776 , -1.03235008, -1.04518577,  0.92954236]), array([ 0.33951856, -0.68073235, -1.87515527,  2.55333512]), array([-0.08590818, -0.04920033, -2.27583522,  3.57568859]), array([-0.5185508 ,  0.64692733, -1.93658587,  3.16950862]), array([-0.82803877,  1.16637826, -1.11340659,  1.97884728]), array([-0.95400337,  1.43544136, -0.13564976,  0.71417634]), array([-0.88229642,  1.45175768,  0.84153661, -0.55710392]), array([-0.60740034,  1.15533712,  1.87672929, -2.42291313]), array([-0.17206724,  0.54765142,  2.3984835 , -3.54711782]), array([ 0.305273  , -0.17804701,  2.24157916, -3.44593025]), array([ 0.67675921, -0.73935458,  1.40033492, -2.05231707]), array([ 0.84944406, -0.98409619,  0.30816429, -0.39205736]), array([ 0.79746249, -0.89690746, -0.82316566,  1.26456966]), array([ 0.52704488, -0.47969617, -1.84253993,  2.86882545]), array([ 0.09038894,  0.20251023, -2.4081015 ,  3.73078396]), array([-0.38110494,  0.90270328, -2.19567758,  3.06917264]), array([-0.75625879,  1.38729027, -1.5039173 ,  1.74446176]), array([-0.96750967,  1.60094759, -0.58347346,  0.4033711 ]), array([-0.96594412,  1.50279363,  0.60516518, -1.38864265]), array([-0.72583912,  1.03679606,  1.78574014, -3.29869022]), array([-0.26486035,  0.18852015,  2.72917061, -5.0192734 ]), array([ 0.29405424, -0.8207903 ,  2.68149677, -4.69823738]), array([ 0.74221771, -1.55487933,  1.76260668, -2.6386636 ]), array([ 0.9890743 , -1.89102377,  0.68574312, -0.75478086]), array([ 1.01080218, -1.86355878, -0.47388625,  1.02911376]), array([ 0.80034794, -1.47204364, -1.62274392,  2.92244314]), array([ 0.36722255, -0.67742139, -2.67025976,  5.00679459]), array([-0.21831509,  0.43816358, -2.97147459,  5.69263499]), array([-0.74117297,  1.43255089, -2.16721776,  4.11213656]), array([-1.07211242,  2.08983459, -1.12469261,  2.50752736]), array([-1.18630636,  2.44962921, -0.01345991,  1.10895529]), array([-1.07955831,  2.53604784,  1.06493871, -0.24389516]), array([-0.76016663,  2.31022126,  2.07902339, -2.02355126]), array([-0.27423872,  1.71987217,  2.71713213, -3.90254813]), array([ 0.28653582,  0.80130083,  2.82223693, -5.17741471]), array([ 0.80408678, -0.24027023,  2.18636137, -4.87025393]), array([ 1.10628341, -1.03708281,  0.78224033, -3.01641917]), array([ 1.11412117, -1.447636  , -0.68986376, -1.09127964]), array([ 0.84222696, -1.46665989, -1.98267715,  0.92928618]), array([ 0.34639109, -1.0659718 , -2.90149564,  3.0712675 ]), array([-0.281866  , -0.27156876, -3.25407839,  4.64080651]), array([-0.88523881,  0.63770049, -2.62675476,  4.12738474]), array([-1.29659974,  1.31895558, -1.45336337,  2.67887071]), array([-1.46165079,  1.72331902, -0.19178246,  1.38850967]), array([-1.372951  ,  1.87388519,  1.07298386,  0.09160579]), array([-1.03925415,  1.74255549,  2.23068663, -1.45632372]), array([-0.50192499,  1.2729355 ,  3.07363245, -3.25457688]), array([ 0.15470044,  0.46557673,  3.36983933, -4.60937476]), array([ 0.77615314, -0.41948399,  2.68165993, -3.88740811]), array([ 1.18662847, -1.01441482,  1.38546595, -2.03941612]), array([ 1.34654424, -1.30388654,  0.2050182 , -0.86990924]), array([ 1.24861476, -1.30877099, -1.17783202,  0.84410892]), array([ 0.880509  , -0.94716364, -2.47957129,  2.82058109]), array([ 0.27649319, -0.18336941, -3.45185998,  4.63833011]), array([-0.42488721,  0.74713316, -3.3712614 ,  4.26001935]), array([-1.01900426,  1.42697681, -2.49935347,  2.4985739 ]), array([-1.40761714,  1.76440229, -1.36126033,  0.93916563]), array([-1.55821292,  1.82496969, -0.13987643, -0.29833789])]</t>
+  </si>
+  <si>
+    <t>['[2,2,2]', '[1,2,0]', '[2,0,1]', '[1,1,1]', '[0,1,1]', '[1,0,2]', '[0,2,1]', '[1,1,2]', '[2,1,0]', '[0,0,0]']</t>
   </si>
   <si>
     <t>[1, 7, 8, 9, 10, 11, 12, 13, 18, 19, 20, 21, 22, 23, 29, 30, 31, 32, 33, 34, 35, 41, 42, 43, 44, 45, 46, 47, 52, 53, 54, 55, 56, 57, 63, 64, 65, 66, 67, 68, 75, 76, 77, 78, 79, 80, 81, 86, 87, 88, 89, 90, 91, 96, 97, 98, 99, 100, 101, 102, 108, 109, 110, 111, 112, 113, 114, 115, 120, 121, 122, 123, 124, 125, 130, 131, 132, 133, 134, 135, 136, 142, 143, 144, 145, 146, 147, 148, 149, 154, 155, 156, 157, 158, 159, 164, 165, 166, 167, 168, 169, 170, 176, 177, 178, 179, 180, 181, 182, 188, 189, 190, 191, 192, 193, 198, 199]</t>
@@ -928,7 +922,7 @@
     <t>[array([-0.03763371, -0.01533471,  0.06554052, -0.01816017], dtype=float32), array([-0.03406929,  0.01398622, -0.02953871,  0.30651903]), array([-0.04818188,  0.10262173, -0.10566927,  0.56184435]), array([-0.07305261,  0.22936701, -0.13369446,  0.67944384]), array([-0.0976443 ,  0.36319498, -0.10327727,  0.63282133]), array([-0.11125897,  0.47297074, -0.02773051,  0.446438  ]), array([-0.10757465,  0.53619101,  0.06462001,  0.17794954]), array([-0.08631261,  0.54305113,  0.14348542, -0.10660175]), array([-0.05272941,  0.496551  ,  0.18460856, -0.34656399]), array([-0.01604448,  0.4107609 ,  0.17301646, -0.49290646]), array([ 0.01268242,  0.3077355 ,  0.10583916, -0.51655332]), array([ 0.02333646,  0.21239857, -0.00419223, -0.4193517 ]), array([ 0.0099677 ,  0.14579835, -0.12877174, -0.23752332]), array([-0.02671453,  0.11914618, -0.23135882, -0.03029568]), array([-0.07887305,  0.13122166, -0.27923433,  0.14079468]), array([-0.13346965,  0.17000821, -0.25455054,  0.23213127]), array([-0.17594228,  0.2177196 , -0.16032293,  0.23074589]), array([-0.19440453,  0.25720213, -0.01958413,  0.15500349]), array([-0.18304473,  0.2773318 ,  0.13139765,  0.04471749]), array([-0.14381952,  0.27594314,  0.25290378, -0.05262463]), array([-0.08610129,  0.25997418,  0.3121551 , -0.09574381]), array([-0.02431919,  0.24283739,  0.29265156, -0.06321871]), array([0.025942  , 0.23936241, 0.19971411, 0.03691163]), array([0.05230735, 0.25979636, 0.05929573, 0.16809359]), array([ 0.04903274,  0.30520172, -0.08996005,  0.27778487]), array([ 0.01840997,  0.3660885 , -0.20830118,  0.31617897]), array([-0.03017518,  0.42484365, -0.26613074,  0.25434096]), array([-0.08310648,  0.46114583, -0.25151672,  0.09491522]), array([-0.12637105,  0.45839229, -0.17234971, -0.12852159]), array([-0.14934542,  0.40908444, -0.05391547, -0.3602991 ]), array([-0.14772278,  0.3180918 ,  0.0672533 , -0.53461121]), array([-0.12479853,  0.20317901,  0.15370315, -0.59148689]), array([-0.09033116,  0.09169889,  0.18033911, -0.49864447]), array([-0.05698072,  0.01310365,  0.14398671, -0.26870757]), array([-0.03582515, -0.0101366 ,  0.06271589,  0.0432441 ]), array([-0.03284724,  0.03064719, -0.03208739,  0.35765344]), array([-0.04720001,  0.12749223, -0.10517205,  0.59129397]), array([-0.07155134,  0.25739102, -0.12905439,  0.6812098 ]), array([-0.09492447,  0.388912  , -0.09622775,  0.60894699]), array([-0.10718747,  0.49201057, -0.0218702 ,  0.40512845]), array([-0.10272942,  0.54605232,  0.06611999,  0.12900689]), array([-0.08173302,  0.54308751,  0.13927353, -0.15466602]), array([-0.04954254,  0.48764289,  0.17506264, -0.38695002]), array([-0.0151897 ,  0.39500767,  0.15952967, -0.52021901]), array([ 0.01060951,  0.28814293,  0.09044679, -0.52729481]), array([ 0.01822159,  0.19237607, -0.01869241, -0.41316397]), array([ 0.00232707,  0.12845925, -0.13896224, -0.21766133]), array([-0.03568997,  0.10667803, -0.23409955, -0.00247033]), array([-0.08749173,  0.12459123, -0.27282479,  0.17041154]), array([-0.13991018,  0.16905379, -0.23945127,  0.25864832]), array([-0.17869878,  0.22151336, -0.13917454,  0.25145711]), array([-0.1926727 ,  0.26449668,  0.00337017,  0.16935121]), array([-0.1769526 ,  0.28693308,  0.15124934,  0.05366847]), array([-0.13445176,  0.28693469,  0.26518144, -0.04740699]), array([-0.07529822,  0.27176132,  0.31394426, -0.09287064]), array([-0.01427178,  0.2549925 ,  0.28345432, -0.06253005]), array([0.03320993, 0.25132645, 0.18166571, 0.03395749]), array([0.05541992, 0.27059501, 0.03658988, 0.15896077]), array([ 0.04756755,  0.3133453 , -0.11218661,  0.26008252]), array([ 0.01296035,  0.36974247, -0.22522555,  0.28906337]), array([-0.03817749,  0.42225661, -0.27434942,  0.21961036]), array([-0.09176122,  0.45122762, -0.24984721,  0.057366  ]), array([-0.13380024,  0.44127697, -0.16221175, -0.16159141]), array([-0.15419985,  0.38651943, -0.0390578 , -0.38032562]), array([-0.14954388,  0.29349535,  0.08194675, -0.53389199]), array([-0.12405679,  0.1811662 ,  0.16415375, -0.56628747]), array([-0.08808552,  0.07699537,  0.18489113, -0.45181189]), array([-0.05435766,  0.0092074 ,  0.14350691, -0.20933367]), array([-0.03360858, -0.00193434,  0.05958977,  0.10270577]), array([-0.03126835,  0.04965808, -0.0348448 ,  0.40427605]), array([-0.04589907,  0.15361957, -0.10488044,  0.61453149]), array([-0.0697991 ,  0.28538669, -0.12495141,  0.67661345]), array([-0.09212053,  0.41344526, -0.09032077,  0.58006289]), array([-0.10331017,  0.50905869, -0.01758247,  0.36076706]), array([-0.09839182,  0.55349362,  0.06615363,  0.07877079]), array([-0.07789914,  0.54058781,  0.13420752, -0.20264412]), array([-0.04719168,  0.47633936,  0.1654693 , -0.42601479]), array([-0.01510862,  0.37725273,  0.1466769 , -0.54490503]), array([ 0.00793765,  0.26720255,  0.07613315, -0.53416711]), array([ 0.01275402,  0.17186701, -0.03182694, -0.40234596]), array([-0.00537228,  0.11157045, -0.14759706, -0.19319689]), array([-0.04440589,  0.0955119 , -0.23524665,  0.02915933]), array([-0.09554715,  0.11989594, -0.26501195,  0.20248807]), array([-0.14554585,  0.17036677, -0.22337485,  0.28600562]), array([-0.18051368,  0.2275777 , -0.11766083,  0.27137941]), array([-0.18999781,  0.27375893,  0.02596172,  0.18151569]), array([-0.17006607,  0.29796092,  0.16998281,  0.05947346]), array([-0.12458156,  0.29867159,  0.27568837, -0.0457681 ]), array([-0.06439133,  0.28357693,  0.31357441, -0.09351671]), array([-0.00455873,  0.26650869,  0.27210543, -0.0649525 ]), array([0.03975045, 0.26208671, 0.16190605, 0.02848612]), array([0.05753832, 0.2797526 , 0.01297578, 0.14798185]), array([ 0.04502607,  0.31955004, -0.13430811,  0.24126283]), array([ 0.00655875,  0.371317  , -0.24103308,  0.26169141]), array([-0.04682626,  0.41764531, -0.2806927 ,  0.18573734]), array([-0.10065064,  0.43959434, -0.24602756,  0.02209511]), array([-0.14105542,  0.42306129, -0.15022547, -0.19079316]), array([-0.1585794 ,  0.36377239, -0.02308311, -0.39512484]), array([-0.15074924,  0.26983351,  0.09695382, -0.52742464]), array([-0.12269552,  0.16117865,  0.17438731, -0.5361634 ]), array([-0.08528724,  0.06510879,  0.18903429, -0.40214971]), array([-0.05126701,  0.00842468,  0.14260087, -0.14987158]), array([-0.03100515,  0.00911726,  0.05609321,  0.15946779]), array([-0.02936643,  0.07072863, -0.03787276,  0.44581606]), array([-0.04432828,  0.18063327, -0.10489468,  0.63135148]), array([-0.06787099,  0.31298691, -0.12153686,  0.66588475]), array([-0.08933569,  0.4365039 , -0.08566581,  0.54665946]), array([-0.09973793,  0.52392673, -0.01482218,  0.31385691]), array([-0.09464563,  0.5584177 ,  0.06494005,  0.02764581]), array([-0.07483988,  0.53552856,  0.12859805, -0.25018861]), array([-0.04564481,  0.46268927,  0.15610878, -0.46336875]), array([-0.01572389,  0.35763124,  0.13462397, -0.56649594]), array([ 0.00476507,  0.2451441 ,  0.06294674, -0.53671801]), array([ 0.00703386,  0.15117595, -0.04361746, -0.3866264 ]), array([-0.0130384 ,  0.09546296, -0.15473379, -0.16414491]), array([-0.05278488,  0.08594636, -0.23488768,  0.06429034]), array([-0.10298229,  0.11734993, -0.25591136,  0.23649688]), array([-0.15034483,  0.17404117, -0.20645609,  0.31354703]), array([-0.18138352,  0.23587225, -0.0959301 ,  0.28984537]), array([-0.18640743,  0.28482445,  0.0480285 ,  0.19094315]), array([-0.16244604,  0.31016043,  0.18742958,  0.06179413]), array([-0.11430204,  0.31085723,  0.28427726, -0.04778539]), array([-0.05349743,  0.29513339,  0.31096354, -0.09752437]), array([ 0.00469687,  0.27714684,  0.25862904, -0.07017408]), array([0.04545767, 0.2714738 , 0.14058317, 0.02086875]), array([ 0.05859764,  0.28717389, -0.0112902 ,  0.13552053]), array([ 0.04140156,  0.32379113, -0.15601076,  0.22166864]), array([-0.00073964,  0.37085645, -0.25543254,  0.234419  ]), array([-0.0560177 ,  0.41113012, -0.28497811,  0.15312868]), array([-0.10965023,  0.42645212, -0.24003628, -0.0104566 ]), array([-0.14802313,  0.40403503, -0.1365139 , -0.21575459]), array([-0.16240314,  0.34118711, -0.00617755, -0.4045564 ]), array([-0.15129345,  0.24744257,  0.11211626, -0.51543675]), array([-0.12069506,  0.14346947,  0.18430299, -0.50170205]), array([-0.08193385,  0.05615191,  0.19269073, -0.35044184]), array([-0.04772192,  0.01070705,  0.14119035, -0.09112623]), array([-0.02804265,  0.02281653,  0.05215965,  0.21282133]), array([-0.02718193,  0.09353628, -0.04123753,  0.48180108]), array([-0.04254543,  0.20815456, -0.10532688,  0.64168365]), array([-0.0658516 ,  0.33984167, -0.11895519,  0.64936011]), array([-0.0866777 ,  0.45782805, -0.08232969,  0.50925872]), array([-0.09657543,  0.53645768, -0.01348476,  0.26487962]), array([-0.09155773,  0.56075321,  0.06274125, -0.02398912]), array([-0.07256234,  0.52790964,  0.12276044, -0.29694912]), array([-0.04485106,  0.44676846,  0.14722867, -0.49859214]), array([-0.01694786,  0.33631128,  0.12348859, -0.5845016 ]), array([ 0.00119142,  0.22222999,  0.05089857, -0.53452372]), array([ 0.00115715,  0.13062862, -0.05410393, -0.36581752]), array([-0.02058587,  0.08046926, -0.16043745, -0.1306274 ]), array([-0.06075712,  0.07826057, -0.2331145 ,  0.10252237]), array([-0.10974841,  0.11713115, -0.24564048,  0.27184157]), array([-0.15428372,  0.18012472, -0.18882975,  0.34058598]), array([-0.1813133 ,  0.24630879, -0.074132  ,  0.3062036 ]), array([-0.18193819,  0.29748891,  0.06940446,  0.19714208]), array([-0.15416319,  0.32325274,  0.20341941,  0.06038573]), array([-0.10371544,  0.32319062,  0.29081036, -0.05343892]), array([-0.04273888,  0.30615608,  0.30605602, -0.10466318]), array([ 0.01337313,  0.28669158,  0.24308944, -0.07784917]), array([0.05023542, 0.27934522, 0.11788775, 0.01147704]), array([ 0.05855024,  0.29278905, -0.03592164,  0.12192858]), array([ 0.03670808,  0.32606744, -0.17697646,  0.20164023]), array([-0.00886101,  0.36842998, -0.26815891,  0.20761536]), array([-0.06563708,  0.40285926, -0.28707103,  0.1222044 ]), array([-0.11863457,  0.41203512, -0.2319005 , -0.03986466]), array([-0.15459691,  0.38450774, -0.12122797, -0.23617149]), array([-0.16559988,  0.31910852,  0.01147226, -0.40859413]), array([-0.15113935,  0.22663575,  0.12728805, -0.49827558]), array([-0.11804202,  0.12824859,  0.1938046 , -0.46356596]), array([-0.07802928,  0.05018527,  0.19577856, -0.29748927]), array([-0.04374255,  0.01595482,  0.13919647, -0.03387837]), array([-0.02475561,  0.03891912,  0.04772446,  0.26212104]), array([-0.02476246,  0.11773341, -0.04501226,  0.51187163]), array([-0.04061733,  0.23580526, -0.10629762,  0.64559108]), array([-0.06383403,  0.36562435, -0.11733303,  0.62746126]), array([-0.08425568,  0.47719062, -0.0803281 ,  0.46839266]), array([-0.09391725,  0.54652449, -0.01340782,  0.21428771]), array([-0.08917547,  0.56045332,  0.05985141, -0.07577466]), array([-0.07105172,  0.51775472,  0.11700098, -0.34256143]), array([-0.04474313,  0.42868192,  0.13903453, -0.53123132]), array([-0.01868597,  0.31349527,  0.11334013, -0.5984216 ]), array([-0.00268485,  0.19875332,  0.03996863, -0.5272095 ]), array([-0.00478549,  0.11056615, -0.06333843, -0.33983005]), array([-0.02793621,  0.06691587, -0.1647779 , -0.09287558]), array([-0.06826057,  0.07270751, -0.2300224 ,  0.14336517]), array([-0.11580497,  0.11937645, -0.23431791,  0.30786844]), array([-0.15734736,  0.1886166 , -0.17063041,  0.36642028]), array([-0.18031646,  0.25875229, -0.05241862,  0.31983568]), array([-0.17663596,  0.31151239,  0.08991857,  0.19969807]), array([-0.14529807,  0.33694159,  0.21778224,  0.05510361]), array([-0.0929325 ,  0.33537307,  0.29516476, -0.06261641]), array([-0.03224173,  0.31638816,  0.2988288 , -0.11464327]), array([ 0.02135225,  0.29495314,  0.22559423, -0.08761231]), array([0.05400021, 0.28558511, 0.09405069, 0.00067617]), array([ 0.05736759,  0.29655284, -0.06061003,  0.10754789]), array([ 0.0309805 ,  0.32640166, -0.1968935 ,  0.18152143]), array([-0.01771501,  0.36413271, -0.27898203,  0.18166496]), array([-0.07556189,  0.39300942, -0.28688684,  0.09338961]), array([-0.12748016,  0.39660352, -0.22169073, -0.06573788]), array([-0.16067864,  0.36480315, -0.10453779, -0.25182481]), array([-0.16810808,  0.29787468,  0.02968452, -0.40733139])]</t>
   </si>
   <si>
-    <t>['[0,2,1]', '[1,1,1]', '[1,1,2]', '[1,0,2]', '[2,1,0]', '[0,0,0]', '[2,2,2]', '[1,2,0]', '[0,1,1]', '[2,0,1]']</t>
+    <t>['[0,0,0]', '[1,1,1]', '[1,1,2]', '[0,1,1]', '[0,2,1]', '[2,2,2]', '[2,0,1]', '[1,0,2]', '[1,2,0]', '[2,1,0]']</t>
   </si>
 </sst>
 </file>
@@ -1358,13 +1352,13 @@
         <v>18</v>
       </c>
       <c r="F2">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G2" t="s">
         <v>19</v>
       </c>
       <c r="H2">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="I2" t="s">
         <v>20</v>
@@ -1376,7 +1370,7 @@
         <v>21</v>
       </c>
       <c r="L2">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="M2">
         <v>0</v>
@@ -1408,13 +1402,13 @@
         <v>24</v>
       </c>
       <c r="F3">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="G3" t="s">
         <v>25</v>
       </c>
       <c r="H3">
-        <v>103</v>
+        <v>110</v>
       </c>
       <c r="I3" t="s">
         <v>26</v>
@@ -1426,7 +1420,7 @@
         <v>27</v>
       </c>
       <c r="L3">
-        <v>104</v>
+        <v>111</v>
       </c>
       <c r="M3">
         <v>0</v>
@@ -1458,13 +1452,13 @@
         <v>30</v>
       </c>
       <c r="F4">
-        <v>23</v>
+        <v>37</v>
       </c>
       <c r="G4" t="s">
         <v>31</v>
       </c>
       <c r="H4">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="I4" t="s">
         <v>32</v>
@@ -1476,7 +1470,7 @@
         <v>33</v>
       </c>
       <c r="L4">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="M4">
         <v>0</v>
@@ -1508,13 +1502,13 @@
         <v>36</v>
       </c>
       <c r="F5">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="G5" t="s">
         <v>37</v>
       </c>
       <c r="H5">
-        <v>109</v>
+        <v>135</v>
       </c>
       <c r="I5" t="s">
         <v>38</v>
@@ -1526,7 +1520,7 @@
         <v>39</v>
       </c>
       <c r="L5">
-        <v>110</v>
+        <v>136</v>
       </c>
       <c r="M5">
         <v>0</v>
@@ -1608,13 +1602,13 @@
         <v>49</v>
       </c>
       <c r="F7">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="G7" t="s">
         <v>50</v>
       </c>
       <c r="H7">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="I7" t="s">
         <v>51</v>
@@ -1626,7 +1620,7 @@
         <v>52</v>
       </c>
       <c r="L7">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="M7">
         <v>0</v>
@@ -1658,13 +1652,13 @@
         <v>55</v>
       </c>
       <c r="F8">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="G8" t="s">
         <v>56</v>
       </c>
       <c r="H8">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="I8" t="s">
         <v>57</v>
@@ -1673,22 +1667,22 @@
         <v>100</v>
       </c>
       <c r="K8" t="s">
-        <v>39</v>
+        <v>58</v>
       </c>
       <c r="L8">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="M8">
         <v>0</v>
       </c>
       <c r="N8" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="O8">
         <v>10</v>
       </c>
       <c r="P8" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:16">
@@ -1705,40 +1699,40 @@
         <v>1</v>
       </c>
       <c r="E9" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="F9">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="G9" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="H9">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="I9" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="J9">
         <v>100</v>
       </c>
       <c r="K9" t="s">
-        <v>27</v>
+        <v>64</v>
       </c>
       <c r="L9">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="M9">
         <v>0</v>
       </c>
       <c r="N9" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="O9">
         <v>10</v>
       </c>
       <c r="P9" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
     </row>
     <row r="10" spans="1:16">
@@ -1755,40 +1749,40 @@
         <v>1</v>
       </c>
       <c r="E10" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="F10">
-        <v>43</v>
+        <v>58</v>
       </c>
       <c r="G10" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="H10">
-        <v>102</v>
+        <v>131</v>
       </c>
       <c r="I10" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="J10">
         <v>100</v>
       </c>
       <c r="K10" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="L10">
-        <v>103</v>
+        <v>132</v>
       </c>
       <c r="M10">
         <v>0</v>
       </c>
       <c r="N10" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="O10">
         <v>10</v>
       </c>
       <c r="P10" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
     </row>
     <row r="11" spans="1:16">
@@ -1805,25 +1799,25 @@
         <v>1</v>
       </c>
       <c r="E11" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="F11">
         <v>63</v>
       </c>
       <c r="G11" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="H11">
         <v>138</v>
       </c>
       <c r="I11" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="J11">
         <v>100</v>
       </c>
       <c r="K11" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="L11">
         <v>139</v>
@@ -1832,13 +1826,13 @@
         <v>0</v>
       </c>
       <c r="N11" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="O11">
         <v>10</v>
       </c>
       <c r="P11" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="12" spans="1:16">
@@ -1846,7 +1840,7 @@
         <v>16</v>
       </c>
       <c r="B12" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C12">
         <v>0.2</v>
@@ -1855,40 +1849,40 @@
         <v>1</v>
       </c>
       <c r="E12" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="F12">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G12" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="H12">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="I12" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="J12">
         <v>100</v>
       </c>
       <c r="K12" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="L12">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="M12">
         <v>0</v>
       </c>
       <c r="N12" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="O12">
         <v>10</v>
       </c>
       <c r="P12" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="13" spans="1:16">
@@ -1896,7 +1890,7 @@
         <v>16</v>
       </c>
       <c r="B13" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C13">
         <v>0.4</v>
@@ -1905,40 +1899,40 @@
         <v>1</v>
       </c>
       <c r="E13" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="F13">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="G13" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="H13">
-        <v>92</v>
+        <v>118</v>
       </c>
       <c r="I13" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="J13">
         <v>100</v>
       </c>
       <c r="K13" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="L13">
-        <v>93</v>
+        <v>119</v>
       </c>
       <c r="M13">
         <v>0</v>
       </c>
       <c r="N13" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="O13">
         <v>10</v>
       </c>
       <c r="P13" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
     </row>
     <row r="14" spans="1:16">
@@ -1946,7 +1940,7 @@
         <v>16</v>
       </c>
       <c r="B14" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C14">
         <v>0.6</v>
@@ -1955,40 +1949,40 @@
         <v>1</v>
       </c>
       <c r="E14" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="F14">
-        <v>58</v>
+        <v>27</v>
       </c>
       <c r="G14" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="H14">
-        <v>155</v>
+        <v>116</v>
       </c>
       <c r="I14" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="J14">
         <v>100</v>
       </c>
       <c r="K14" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="L14">
-        <v>156</v>
+        <v>117</v>
       </c>
       <c r="M14">
         <v>0</v>
       </c>
       <c r="N14" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="O14">
         <v>10</v>
       </c>
       <c r="P14" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
     </row>
     <row r="15" spans="1:16">
@@ -1996,7 +1990,7 @@
         <v>16</v>
       </c>
       <c r="B15" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C15">
         <v>0.8</v>
@@ -2005,40 +1999,40 @@
         <v>1</v>
       </c>
       <c r="E15" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="F15">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="G15" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="H15">
-        <v>143</v>
+        <v>127</v>
       </c>
       <c r="I15" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="J15">
         <v>100</v>
       </c>
       <c r="K15" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="L15">
-        <v>144</v>
+        <v>128</v>
       </c>
       <c r="M15">
         <v>0</v>
       </c>
       <c r="N15" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="O15">
         <v>10</v>
       </c>
       <c r="P15" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
     </row>
     <row r="16" spans="1:16">
@@ -2046,7 +2040,7 @@
         <v>16</v>
       </c>
       <c r="B16" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C16">
         <v>1</v>
@@ -2055,25 +2049,25 @@
         <v>1</v>
       </c>
       <c r="E16" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="F16">
         <v>77</v>
       </c>
       <c r="G16" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="H16">
         <v>159</v>
       </c>
       <c r="I16" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="J16">
         <v>100</v>
       </c>
       <c r="K16" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="L16">
         <v>160</v>
@@ -2082,13 +2076,13 @@
         <v>0</v>
       </c>
       <c r="N16" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="O16">
         <v>10</v>
       </c>
       <c r="P16" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
     </row>
     <row r="17" spans="1:16">
@@ -2096,7 +2090,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="C17">
         <v>0.2</v>
@@ -2105,40 +2099,40 @@
         <v>1</v>
       </c>
       <c r="E17" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="F17">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="G17" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="H17">
-        <v>87</v>
+        <v>71</v>
       </c>
       <c r="I17" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="J17">
         <v>100</v>
       </c>
       <c r="K17" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="L17">
-        <v>88</v>
+        <v>72</v>
       </c>
       <c r="M17">
         <v>0</v>
       </c>
       <c r="N17" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="O17">
         <v>10</v>
       </c>
       <c r="P17" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
     </row>
     <row r="18" spans="1:16">
@@ -2146,7 +2140,7 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="C18">
         <v>0.4</v>
@@ -2155,40 +2149,40 @@
         <v>1</v>
       </c>
       <c r="E18" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="F18">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="G18" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="H18">
-        <v>136</v>
+        <v>112</v>
       </c>
       <c r="I18" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="J18">
         <v>100</v>
       </c>
       <c r="K18" t="s">
-        <v>118</v>
+        <v>33</v>
       </c>
       <c r="L18">
-        <v>137</v>
+        <v>113</v>
       </c>
       <c r="M18">
         <v>0</v>
       </c>
       <c r="N18" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="O18">
         <v>10</v>
       </c>
       <c r="P18" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="19" spans="1:16">
@@ -2196,7 +2190,7 @@
         <v>16</v>
       </c>
       <c r="B19" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="C19">
         <v>0.6</v>
@@ -2205,28 +2199,28 @@
         <v>1</v>
       </c>
       <c r="E19" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="F19">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="G19" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="H19">
-        <v>98</v>
+        <v>106</v>
       </c>
       <c r="I19" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="J19">
         <v>100</v>
       </c>
       <c r="K19" t="s">
-        <v>124</v>
+        <v>64</v>
       </c>
       <c r="L19">
-        <v>99</v>
+        <v>107</v>
       </c>
       <c r="M19">
         <v>0</v>
@@ -2246,7 +2240,7 @@
         <v>16</v>
       </c>
       <c r="B20" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="C20">
         <v>0.8</v>
@@ -2264,7 +2258,7 @@
         <v>128</v>
       </c>
       <c r="H20">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="I20" t="s">
         <v>129</v>
@@ -2276,7 +2270,7 @@
         <v>130</v>
       </c>
       <c r="L20">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="M20">
         <v>0</v>
@@ -2296,7 +2290,7 @@
         <v>16</v>
       </c>
       <c r="B21" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="C21">
         <v>1</v>
@@ -2358,13 +2352,13 @@
         <v>140</v>
       </c>
       <c r="F22">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="G22" t="s">
         <v>141</v>
       </c>
       <c r="H22">
-        <v>116</v>
+        <v>100</v>
       </c>
       <c r="I22" t="s">
         <v>142</v>
@@ -2373,22 +2367,22 @@
         <v>100</v>
       </c>
       <c r="K22" t="s">
-        <v>33</v>
+        <v>143</v>
       </c>
       <c r="L22">
-        <v>117</v>
+        <v>101</v>
       </c>
       <c r="M22">
         <v>0</v>
       </c>
       <c r="N22" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="O22">
         <v>10</v>
       </c>
       <c r="P22" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="23" spans="1:16">
@@ -2405,40 +2399,40 @@
         <v>1</v>
       </c>
       <c r="E23" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="F23">
-        <v>90</v>
+        <v>63</v>
       </c>
       <c r="G23" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="H23">
-        <v>199</v>
+        <v>169</v>
       </c>
       <c r="I23" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="J23">
         <v>100</v>
       </c>
       <c r="K23" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="L23">
-        <v>200</v>
+        <v>170</v>
       </c>
       <c r="M23">
         <v>0</v>
       </c>
       <c r="N23" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="O23">
         <v>10</v>
       </c>
       <c r="P23" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="24" spans="1:16">
@@ -2455,25 +2449,25 @@
         <v>1</v>
       </c>
       <c r="E24" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="F24">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G24" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="H24">
         <v>199</v>
       </c>
       <c r="I24" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="J24">
         <v>100</v>
       </c>
       <c r="K24" t="s">
-        <v>148</v>
+        <v>155</v>
       </c>
       <c r="L24">
         <v>200</v>
@@ -2482,13 +2476,13 @@
         <v>0</v>
       </c>
       <c r="N24" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="O24">
         <v>10</v>
       </c>
       <c r="P24" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
     </row>
     <row r="25" spans="1:16">
@@ -2505,25 +2499,25 @@
         <v>1</v>
       </c>
       <c r="E25" t="s">
+        <v>158</v>
+      </c>
+      <c r="F25">
         <v>156</v>
       </c>
-      <c r="F25">
-        <v>154</v>
-      </c>
       <c r="G25" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="H25">
         <v>199</v>
       </c>
       <c r="I25" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="J25">
         <v>100</v>
       </c>
       <c r="K25" t="s">
-        <v>148</v>
+        <v>155</v>
       </c>
       <c r="L25">
         <v>200</v>
@@ -2532,13 +2526,13 @@
         <v>0</v>
       </c>
       <c r="N25" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="O25">
         <v>10</v>
       </c>
       <c r="P25" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
     </row>
     <row r="26" spans="1:16">
@@ -2555,25 +2549,25 @@
         <v>1</v>
       </c>
       <c r="E26" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="F26">
         <v>199</v>
       </c>
       <c r="G26" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="H26">
         <v>199</v>
       </c>
       <c r="I26" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="J26">
         <v>100</v>
       </c>
       <c r="K26" t="s">
-        <v>148</v>
+        <v>155</v>
       </c>
       <c r="L26">
         <v>200</v>
@@ -2582,13 +2576,13 @@
         <v>0</v>
       </c>
       <c r="N26" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="O26">
         <v>10</v>
       </c>
       <c r="P26" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
     </row>
     <row r="27" spans="1:16">
@@ -2596,7 +2590,7 @@
         <v>16</v>
       </c>
       <c r="B27" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="C27">
         <v>0.2</v>
@@ -2605,40 +2599,40 @@
         <v>1</v>
       </c>
       <c r="E27" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="F27">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="G27" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="H27">
-        <v>122</v>
+        <v>91</v>
       </c>
       <c r="I27" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="J27">
         <v>100</v>
       </c>
       <c r="K27" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="L27">
-        <v>123</v>
+        <v>92</v>
       </c>
       <c r="M27">
         <v>0</v>
       </c>
       <c r="N27" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="O27">
         <v>10</v>
       </c>
       <c r="P27" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
     </row>
     <row r="28" spans="1:16">
@@ -2646,7 +2640,7 @@
         <v>16</v>
       </c>
       <c r="B28" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="C28">
         <v>0.4</v>
@@ -2655,40 +2649,40 @@
         <v>1</v>
       </c>
       <c r="E28" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="F28">
-        <v>49</v>
+        <v>72</v>
       </c>
       <c r="G28" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="H28">
-        <v>158</v>
+        <v>186</v>
       </c>
       <c r="I28" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="J28">
         <v>100</v>
       </c>
       <c r="K28" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="L28">
-        <v>159</v>
+        <v>187</v>
       </c>
       <c r="M28">
         <v>0</v>
       </c>
       <c r="N28" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="O28">
         <v>10</v>
       </c>
       <c r="P28" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
     </row>
     <row r="29" spans="1:16">
@@ -2696,7 +2690,7 @@
         <v>16</v>
       </c>
       <c r="B29" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="C29">
         <v>0.6</v>
@@ -2705,25 +2699,25 @@
         <v>1</v>
       </c>
       <c r="E29" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="F29">
-        <v>112</v>
+        <v>121</v>
       </c>
       <c r="G29" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="H29">
         <v>199</v>
       </c>
       <c r="I29" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="J29">
         <v>100</v>
       </c>
       <c r="K29" t="s">
-        <v>148</v>
+        <v>155</v>
       </c>
       <c r="L29">
         <v>200</v>
@@ -2732,13 +2726,13 @@
         <v>0</v>
       </c>
       <c r="N29" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="O29">
         <v>10</v>
       </c>
       <c r="P29" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
     </row>
     <row r="30" spans="1:16">
@@ -2746,7 +2740,7 @@
         <v>16</v>
       </c>
       <c r="B30" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="C30">
         <v>0.8</v>
@@ -2755,25 +2749,25 @@
         <v>1</v>
       </c>
       <c r="E30" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="F30">
-        <v>163</v>
+        <v>152</v>
       </c>
       <c r="G30" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="H30">
         <v>199</v>
       </c>
       <c r="I30" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="J30">
         <v>100</v>
       </c>
       <c r="K30" t="s">
-        <v>148</v>
+        <v>155</v>
       </c>
       <c r="L30">
         <v>200</v>
@@ -2782,13 +2776,13 @@
         <v>0</v>
       </c>
       <c r="N30" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="O30">
         <v>10</v>
       </c>
       <c r="P30" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
     </row>
     <row r="31" spans="1:16">
@@ -2796,7 +2790,7 @@
         <v>16</v>
       </c>
       <c r="B31" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="C31">
         <v>1</v>
@@ -2805,25 +2799,25 @@
         <v>1</v>
       </c>
       <c r="E31" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="F31">
         <v>199</v>
       </c>
       <c r="G31" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="H31">
         <v>199</v>
       </c>
       <c r="I31" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="J31">
         <v>100</v>
       </c>
       <c r="K31" t="s">
-        <v>148</v>
+        <v>155</v>
       </c>
       <c r="L31">
         <v>200</v>
@@ -2832,13 +2826,13 @@
         <v>0</v>
       </c>
       <c r="N31" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="O31">
         <v>10</v>
       </c>
       <c r="P31" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
     </row>
     <row r="32" spans="1:16">
@@ -2846,7 +2840,7 @@
         <v>16</v>
       </c>
       <c r="B32" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="C32">
         <v>0.2</v>
@@ -2855,40 +2849,40 @@
         <v>1</v>
       </c>
       <c r="E32" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="F32">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="G32" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="H32">
-        <v>170</v>
+        <v>154</v>
       </c>
       <c r="I32" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="J32">
         <v>100</v>
       </c>
       <c r="K32" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="L32">
-        <v>171</v>
+        <v>155</v>
       </c>
       <c r="M32">
         <v>0</v>
       </c>
       <c r="N32" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="O32">
         <v>10</v>
       </c>
       <c r="P32" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
     </row>
     <row r="33" spans="1:16">
@@ -2896,7 +2890,7 @@
         <v>16</v>
       </c>
       <c r="B33" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="C33">
         <v>0.4</v>
@@ -2905,25 +2899,25 @@
         <v>1</v>
       </c>
       <c r="E33" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="F33">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="G33" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="H33">
         <v>199</v>
       </c>
       <c r="I33" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="J33">
         <v>100</v>
       </c>
       <c r="K33" t="s">
-        <v>148</v>
+        <v>155</v>
       </c>
       <c r="L33">
         <v>200</v>
@@ -2932,13 +2926,13 @@
         <v>0</v>
       </c>
       <c r="N33" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="O33">
         <v>10</v>
       </c>
       <c r="P33" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
     </row>
     <row r="34" spans="1:16">
@@ -2946,7 +2940,7 @@
         <v>16</v>
       </c>
       <c r="B34" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="C34">
         <v>0.6</v>
@@ -2955,25 +2949,25 @@
         <v>1</v>
       </c>
       <c r="E34" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="F34">
-        <v>135</v>
+        <v>119</v>
       </c>
       <c r="G34" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="H34">
         <v>199</v>
       </c>
       <c r="I34" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="J34">
         <v>100</v>
       </c>
       <c r="K34" t="s">
-        <v>148</v>
+        <v>155</v>
       </c>
       <c r="L34">
         <v>200</v>
@@ -2982,13 +2976,13 @@
         <v>0</v>
       </c>
       <c r="N34" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="O34">
         <v>10</v>
       </c>
       <c r="P34" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
     </row>
     <row r="35" spans="1:16">
@@ -2996,7 +2990,7 @@
         <v>16</v>
       </c>
       <c r="B35" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="C35">
         <v>0.8</v>
@@ -3005,25 +2999,25 @@
         <v>1</v>
       </c>
       <c r="E35" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="F35">
-        <v>156</v>
+        <v>160</v>
       </c>
       <c r="G35" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="H35">
         <v>199</v>
       </c>
       <c r="I35" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="J35">
         <v>100</v>
       </c>
       <c r="K35" t="s">
-        <v>148</v>
+        <v>155</v>
       </c>
       <c r="L35">
         <v>200</v>
@@ -3032,13 +3026,13 @@
         <v>0</v>
       </c>
       <c r="N35" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="O35">
         <v>10</v>
       </c>
       <c r="P35" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
     </row>
     <row r="36" spans="1:16">
@@ -3046,7 +3040,7 @@
         <v>16</v>
       </c>
       <c r="B36" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="C36">
         <v>1</v>
@@ -3055,25 +3049,25 @@
         <v>1</v>
       </c>
       <c r="E36" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="F36">
         <v>199</v>
       </c>
       <c r="G36" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="H36">
         <v>199</v>
       </c>
       <c r="I36" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="J36">
         <v>100</v>
       </c>
       <c r="K36" t="s">
-        <v>148</v>
+        <v>155</v>
       </c>
       <c r="L36">
         <v>200</v>
@@ -3082,13 +3076,13 @@
         <v>0</v>
       </c>
       <c r="N36" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="O36">
         <v>10</v>
       </c>
       <c r="P36" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
     </row>
     <row r="37" spans="1:16">
@@ -3096,7 +3090,7 @@
         <v>16</v>
       </c>
       <c r="B37" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="C37">
         <v>0.2</v>
@@ -3105,40 +3099,40 @@
         <v>1</v>
       </c>
       <c r="E37" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="F37">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="G37" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="H37">
-        <v>112</v>
+        <v>89</v>
       </c>
       <c r="I37" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="J37">
         <v>100</v>
       </c>
       <c r="K37" t="s">
-        <v>223</v>
+        <v>83</v>
       </c>
       <c r="L37">
-        <v>113</v>
+        <v>90</v>
       </c>
       <c r="M37">
         <v>0</v>
       </c>
       <c r="N37" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="O37">
         <v>10</v>
       </c>
       <c r="P37" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
     </row>
     <row r="38" spans="1:16">
@@ -3146,7 +3140,7 @@
         <v>16</v>
       </c>
       <c r="B38" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="C38">
         <v>0.4</v>
@@ -3155,40 +3149,40 @@
         <v>1</v>
       </c>
       <c r="E38" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="F38">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="G38" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="H38">
-        <v>145</v>
+        <v>117</v>
       </c>
       <c r="I38" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="J38">
         <v>100</v>
       </c>
       <c r="K38" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="L38">
-        <v>146</v>
+        <v>118</v>
       </c>
       <c r="M38">
         <v>0</v>
       </c>
       <c r="N38" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="O38">
         <v>10</v>
       </c>
       <c r="P38" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
     </row>
     <row r="39" spans="1:16">
@@ -3196,7 +3190,7 @@
         <v>16</v>
       </c>
       <c r="B39" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="C39">
         <v>0.6</v>
@@ -3205,28 +3199,28 @@
         <v>1</v>
       </c>
       <c r="E39" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="F39">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="G39" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="H39">
-        <v>192</v>
+        <v>135</v>
       </c>
       <c r="I39" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="J39">
         <v>100</v>
       </c>
       <c r="K39" t="s">
-        <v>235</v>
+        <v>39</v>
       </c>
       <c r="L39">
-        <v>193</v>
+        <v>136</v>
       </c>
       <c r="M39">
         <v>0</v>
@@ -3246,7 +3240,7 @@
         <v>16</v>
       </c>
       <c r="B40" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="C40">
         <v>0.8</v>
@@ -3258,7 +3252,7 @@
         <v>238</v>
       </c>
       <c r="F40">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="G40" t="s">
         <v>239</v>
@@ -3273,7 +3267,7 @@
         <v>100</v>
       </c>
       <c r="K40" t="s">
-        <v>148</v>
+        <v>155</v>
       </c>
       <c r="L40">
         <v>200</v>
@@ -3296,7 +3290,7 @@
         <v>16</v>
       </c>
       <c r="B41" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="C41">
         <v>1</v>
@@ -3323,7 +3317,7 @@
         <v>100</v>
       </c>
       <c r="K41" t="s">
-        <v>148</v>
+        <v>155</v>
       </c>
       <c r="L41">
         <v>200</v>
@@ -3358,13 +3352,13 @@
         <v>249</v>
       </c>
       <c r="F42">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="G42" t="s">
         <v>250</v>
       </c>
       <c r="H42">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="I42" t="s">
         <v>251</v>
@@ -3373,22 +3367,22 @@
         <v>100</v>
       </c>
       <c r="K42" t="s">
+        <v>83</v>
+      </c>
+      <c r="L42">
+        <v>90</v>
+      </c>
+      <c r="M42">
+        <v>0</v>
+      </c>
+      <c r="N42" t="s">
         <v>252</v>
       </c>
-      <c r="L42">
-        <v>87</v>
-      </c>
-      <c r="M42">
-        <v>0</v>
-      </c>
-      <c r="N42" t="s">
+      <c r="O42">
+        <v>10</v>
+      </c>
+      <c r="P42" t="s">
         <v>253</v>
-      </c>
-      <c r="O42">
-        <v>10</v>
-      </c>
-      <c r="P42" t="s">
-        <v>254</v>
       </c>
     </row>
     <row r="43" spans="1:16">
@@ -3405,40 +3399,40 @@
         <v>1</v>
       </c>
       <c r="E43" t="s">
+        <v>254</v>
+      </c>
+      <c r="F43">
+        <v>46</v>
+      </c>
+      <c r="G43" t="s">
         <v>255</v>
       </c>
-      <c r="F43">
-        <v>63</v>
-      </c>
-      <c r="G43" t="s">
+      <c r="H43">
+        <v>109</v>
+      </c>
+      <c r="I43" t="s">
         <v>256</v>
       </c>
-      <c r="H43">
-        <v>133</v>
-      </c>
-      <c r="I43" t="s">
+      <c r="J43">
+        <v>100</v>
+      </c>
+      <c r="K43" t="s">
         <v>257</v>
       </c>
-      <c r="J43">
-        <v>100</v>
-      </c>
-      <c r="K43" t="s">
+      <c r="L43">
+        <v>110</v>
+      </c>
+      <c r="M43">
+        <v>0</v>
+      </c>
+      <c r="N43" t="s">
         <v>258</v>
       </c>
-      <c r="L43">
-        <v>134</v>
-      </c>
-      <c r="M43">
-        <v>0</v>
-      </c>
-      <c r="N43" t="s">
+      <c r="O43">
+        <v>10</v>
+      </c>
+      <c r="P43" t="s">
         <v>259</v>
-      </c>
-      <c r="O43">
-        <v>10</v>
-      </c>
-      <c r="P43" t="s">
-        <v>260</v>
       </c>
     </row>
     <row r="44" spans="1:16">
@@ -3455,40 +3449,40 @@
         <v>1</v>
       </c>
       <c r="E44" t="s">
+        <v>260</v>
+      </c>
+      <c r="F44">
+        <v>132</v>
+      </c>
+      <c r="G44" t="s">
         <v>261</v>
       </c>
-      <c r="F44">
-        <v>109</v>
-      </c>
-      <c r="G44" t="s">
+      <c r="H44">
+        <v>199</v>
+      </c>
+      <c r="I44" t="s">
         <v>262</v>
       </c>
-      <c r="H44">
-        <v>185</v>
-      </c>
-      <c r="I44" t="s">
+      <c r="J44">
+        <v>100</v>
+      </c>
+      <c r="K44" t="s">
+        <v>155</v>
+      </c>
+      <c r="L44">
+        <v>200</v>
+      </c>
+      <c r="M44">
+        <v>0</v>
+      </c>
+      <c r="N44" t="s">
         <v>263</v>
       </c>
-      <c r="J44">
-        <v>100</v>
-      </c>
-      <c r="K44" t="s">
+      <c r="O44">
+        <v>10</v>
+      </c>
+      <c r="P44" t="s">
         <v>264</v>
-      </c>
-      <c r="L44">
-        <v>186</v>
-      </c>
-      <c r="M44">
-        <v>0</v>
-      </c>
-      <c r="N44" t="s">
-        <v>265</v>
-      </c>
-      <c r="O44">
-        <v>10</v>
-      </c>
-      <c r="P44" t="s">
-        <v>266</v>
       </c>
     </row>
     <row r="45" spans="1:16">
@@ -3505,25 +3499,25 @@
         <v>1</v>
       </c>
       <c r="E45" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="F45">
-        <v>158</v>
+        <v>162</v>
       </c>
       <c r="G45" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="H45">
         <v>199</v>
       </c>
       <c r="I45" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="J45">
         <v>100</v>
       </c>
       <c r="K45" t="s">
-        <v>148</v>
+        <v>155</v>
       </c>
       <c r="L45">
         <v>200</v>
@@ -3532,13 +3526,13 @@
         <v>0</v>
       </c>
       <c r="N45" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="O45">
         <v>10</v>
       </c>
       <c r="P45" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
     </row>
     <row r="46" spans="1:16">
@@ -3555,25 +3549,25 @@
         <v>1</v>
       </c>
       <c r="E46" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="F46">
         <v>199</v>
       </c>
       <c r="G46" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="H46">
         <v>199</v>
       </c>
       <c r="I46" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="J46">
         <v>100</v>
       </c>
       <c r="K46" t="s">
-        <v>148</v>
+        <v>155</v>
       </c>
       <c r="L46">
         <v>200</v>
@@ -3582,13 +3576,13 @@
         <v>0</v>
       </c>
       <c r="N46" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="O46">
         <v>10</v>
       </c>
       <c r="P46" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
     </row>
     <row r="47" spans="1:16">
@@ -3596,7 +3590,7 @@
         <v>16</v>
       </c>
       <c r="B47" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="C47">
         <v>0.2</v>
@@ -3605,40 +3599,40 @@
         <v>1</v>
       </c>
       <c r="E47" t="s">
+        <v>275</v>
+      </c>
+      <c r="F47">
+        <v>10</v>
+      </c>
+      <c r="G47" t="s">
+        <v>276</v>
+      </c>
+      <c r="H47">
+        <v>179</v>
+      </c>
+      <c r="I47" t="s">
         <v>277</v>
       </c>
-      <c r="F47">
-        <v>14</v>
-      </c>
-      <c r="G47" t="s">
+      <c r="J47">
+        <v>100</v>
+      </c>
+      <c r="K47" t="s">
         <v>278</v>
       </c>
-      <c r="H47">
-        <v>115</v>
-      </c>
-      <c r="I47" t="s">
+      <c r="L47">
+        <v>180</v>
+      </c>
+      <c r="M47">
+        <v>0</v>
+      </c>
+      <c r="N47" t="s">
         <v>279</v>
       </c>
-      <c r="J47">
-        <v>100</v>
-      </c>
-      <c r="K47" t="s">
+      <c r="O47">
+        <v>10</v>
+      </c>
+      <c r="P47" t="s">
         <v>280</v>
-      </c>
-      <c r="L47">
-        <v>116</v>
-      </c>
-      <c r="M47">
-        <v>0</v>
-      </c>
-      <c r="N47" t="s">
-        <v>281</v>
-      </c>
-      <c r="O47">
-        <v>10</v>
-      </c>
-      <c r="P47" t="s">
-        <v>282</v>
       </c>
     </row>
     <row r="48" spans="1:16">
@@ -3646,7 +3640,7 @@
         <v>16</v>
       </c>
       <c r="B48" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="C48">
         <v>0.4</v>
@@ -3655,40 +3649,40 @@
         <v>1</v>
       </c>
       <c r="E48" t="s">
+        <v>281</v>
+      </c>
+      <c r="F48">
+        <v>41</v>
+      </c>
+      <c r="G48" t="s">
+        <v>282</v>
+      </c>
+      <c r="H48">
+        <v>177</v>
+      </c>
+      <c r="I48" t="s">
         <v>283</v>
       </c>
-      <c r="F48">
-        <v>32</v>
-      </c>
-      <c r="G48" t="s">
+      <c r="J48">
+        <v>100</v>
+      </c>
+      <c r="K48" t="s">
         <v>284</v>
       </c>
-      <c r="H48">
-        <v>141</v>
-      </c>
-      <c r="I48" t="s">
+      <c r="L48">
+        <v>178</v>
+      </c>
+      <c r="M48">
+        <v>0</v>
+      </c>
+      <c r="N48" t="s">
         <v>285</v>
       </c>
-      <c r="J48">
-        <v>100</v>
-      </c>
-      <c r="K48" t="s">
+      <c r="O48">
+        <v>10</v>
+      </c>
+      <c r="P48" t="s">
         <v>286</v>
-      </c>
-      <c r="L48">
-        <v>142</v>
-      </c>
-      <c r="M48">
-        <v>0</v>
-      </c>
-      <c r="N48" t="s">
-        <v>287</v>
-      </c>
-      <c r="O48">
-        <v>10</v>
-      </c>
-      <c r="P48" t="s">
-        <v>288</v>
       </c>
     </row>
     <row r="49" spans="1:16">
@@ -3696,7 +3690,7 @@
         <v>16</v>
       </c>
       <c r="B49" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="C49">
         <v>0.6</v>
@@ -3705,40 +3699,40 @@
         <v>1</v>
       </c>
       <c r="E49" t="s">
+        <v>287</v>
+      </c>
+      <c r="F49">
+        <v>46</v>
+      </c>
+      <c r="G49" t="s">
+        <v>288</v>
+      </c>
+      <c r="H49">
+        <v>140</v>
+      </c>
+      <c r="I49" t="s">
         <v>289</v>
       </c>
-      <c r="F49">
-        <v>43</v>
-      </c>
-      <c r="G49" t="s">
+      <c r="J49">
+        <v>100</v>
+      </c>
+      <c r="K49" t="s">
         <v>290</v>
       </c>
-      <c r="H49">
-        <v>152</v>
-      </c>
-      <c r="I49" t="s">
+      <c r="L49">
+        <v>141</v>
+      </c>
+      <c r="M49">
+        <v>0</v>
+      </c>
+      <c r="N49" t="s">
         <v>291</v>
       </c>
-      <c r="J49">
-        <v>100</v>
-      </c>
-      <c r="K49" t="s">
+      <c r="O49">
+        <v>10</v>
+      </c>
+      <c r="P49" t="s">
         <v>292</v>
-      </c>
-      <c r="L49">
-        <v>153</v>
-      </c>
-      <c r="M49">
-        <v>0</v>
-      </c>
-      <c r="N49" t="s">
-        <v>293</v>
-      </c>
-      <c r="O49">
-        <v>10</v>
-      </c>
-      <c r="P49" t="s">
-        <v>294</v>
       </c>
     </row>
     <row r="50" spans="1:16">
@@ -3746,7 +3740,7 @@
         <v>16</v>
       </c>
       <c r="B50" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="C50">
         <v>0.8</v>
@@ -3755,25 +3749,25 @@
         <v>1</v>
       </c>
       <c r="E50" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="F50">
         <v>80</v>
       </c>
       <c r="G50" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="H50">
         <v>199</v>
       </c>
       <c r="I50" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="J50">
         <v>100</v>
       </c>
       <c r="K50" t="s">
-        <v>148</v>
+        <v>155</v>
       </c>
       <c r="L50">
         <v>200</v>
@@ -3782,13 +3776,13 @@
         <v>0</v>
       </c>
       <c r="N50" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="O50">
         <v>10</v>
       </c>
       <c r="P50" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
     </row>
     <row r="51" spans="1:16">
@@ -3796,7 +3790,7 @@
         <v>16</v>
       </c>
       <c r="B51" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="C51">
         <v>1</v>
@@ -3805,25 +3799,25 @@
         <v>1</v>
       </c>
       <c r="E51" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="F51">
         <v>117</v>
       </c>
       <c r="G51" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="H51">
         <v>199</v>
       </c>
       <c r="I51" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="J51">
         <v>100</v>
       </c>
       <c r="K51" t="s">
-        <v>148</v>
+        <v>155</v>
       </c>
       <c r="L51">
         <v>200</v>
@@ -3832,13 +3826,13 @@
         <v>0</v>
       </c>
       <c r="N51" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="O51">
         <v>10</v>
       </c>
       <c r="P51" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
the diagnose workes on acrobot, cartpole and mountaincar
</commit_message>
<xml_diff>
--- a/experimental results/e2000_Acrobot.xlsx
+++ b/experimental results/e2000_Acrobot.xlsx
@@ -85,7 +85,7 @@
     <t>Omitted</t>
   </si>
   <si>
-    <t>['[2,2,2]', '[0,2,1]', '[1,2,0]', '[2,1,0]', '[2,0,1]', '[1,1,1]', '[0,1,1]', '[1,0,2]', '[1,1,2]', '[0,0,0]']</t>
+    <t>['[0,2,1]', '[2,0,1]', '[2,1,0]', '[1,0,2]', '[2,2,2]', '[1,2,0]', '[0,1,1]', '[0,0,0]', '[1,1,2]', '[1,1,1]']</t>
   </si>
   <si>
     <t>[0,1,1]</t>
@@ -100,19 +100,19 @@
     <t>['[-0.03763371 -0.01533471  0.06554052 -0.01816017]', '[-0.00754409 -0.05458322  0.2277812  -0.36241836]', '[ 0.04879627 -0.15231473  0.32089719 -0.5887683 ]', '[ 0.11397169 -0.27767857  0.31375488 -0.63332862]', '[ 0.16759438 -0.39312519  0.2086893  -0.49480525]', '[ 0.1930193  -0.46685036  0.03906408 -0.22816919]', '[ 0.16956871 -0.44830261 -0.26820417  0.40739083]', '[ 0.09055011 -0.31127879 -0.50323119  0.93116007]', '[-0.02165415 -0.09380121 -0.58952709  1.1892161 ]', '[-0.13228272  0.13968862 -0.48657385  1.08703787]', '[-0.20542731  0.31962025 -0.22562708  0.67289162]', '[-0.21756752  0.39782756  0.10766541  0.09689063]', '[-0.15109606  0.32490126  0.54216963 -0.80657469]', '[-0.01068619  0.09081112  0.82714324 -1.47439182]', '[ 0.16212513 -0.23279107  0.85391345 -1.67375883]', '[ 0.3120332  -0.54339537  0.60708552 -1.36152952]', '[ 0.39322683 -0.75586146  0.18779451 -0.73014827]', '[ 0.38412465 -0.82793881 -0.27624305  0.01454459]', '[ 0.27552572 -0.72135137 -0.78884754  1.03160865]', '[ 0.08086773 -0.43032213 -1.11647003  1.81675029]', '[-0.14966877 -0.03109877 -1.12879696  2.06540623]', '[-0.3455444   0.34863759 -0.7784691   1.63534647]', '[-0.44544803  0.59424237 -0.19906427  0.77949316]', '[-0.4218337   0.6519398   0.43007126 -0.20572333]', '[-0.26769146  0.484052    1.08142007 -1.44055859]', '[-0.00742761  0.10113176  1.45927884 -2.28595201]', '[ 0.28490347 -0.37428385  1.38589424 -2.32532176]', '[ 0.5187101  -0.77937684  0.90230152 -1.64619583]', '[ 0.63240836 -1.01433747  0.21740989 -0.68198512]', '[ 0.59278756 -1.01958166 -0.60566507  0.62852481]', '[ 0.39752784 -0.7660208  -1.31595743  1.88179849]', '[ 0.08542661 -0.29020757 -1.73661998  2.76615566]', '[-0.26054486  0.27360101 -1.62803895  2.69265107]', '[-0.53183224  0.72525907 -1.02799868  1.73308445]', '[-0.65747495  0.94866122 -0.21116234  0.48419472]', '[-0.60316944  0.88713812  0.74646124 -1.09703619]', '[-0.3667148   0.51448679  1.5802398  -2.58584684]', '[ 2.25515542e-03 -1.04226788e-01  2.01052042e+00 -3.41515113e+00]', '[ 0.38981745 -0.75816996  1.76540261 -2.93947302]', '[ 0.67971886 -1.23563438  1.09061136 -1.79181237]', '[ 0.81522073 -1.47040276  0.25012952 -0.55613563]', '[ 0.76893557 -1.43299403 -0.70634091  0.93217091]', '[ 0.53890731 -1.09497955 -1.5685075   2.44803386]', '[ 0.15769536 -0.46498696 -2.17507038  3.75054866]', '[-0.28566374  0.31885175 -2.12308403  3.81427092]', '[-0.64333931  0.96714913 -1.38377582  2.55626676]', '[-0.82476188  1.32821982 -0.41497441  1.0541805 ]', '[-0.80769438  1.39053182  0.57925977 -0.43113385]', '[-0.58966747  1.12643161  1.57705339 -2.21920745]', '[-0.19115743  0.50615398  2.34648211 -3.90612928]']</t>
   </si>
   <si>
-    <t>['[2,1,0]', '[0,1,1]', '[1,1,2]', '[0,0,0]', '[1,2,0]', '[2,2,2]', '[1,0,2]', '[2,0,1]', '[0,2,1]', '[1,1,1]']</t>
+    <t>['[2,0,1]', '[1,2,0]', '[2,2,2]', '[1,1,2]', '[0,2,1]', '[1,1,1]', '[2,1,0]', '[1,0,2]', '[0,1,1]', '[0,0,0]']</t>
   </si>
   <si>
     <t>[0,2,1]</t>
   </si>
   <si>
-    <t>['[2,1,0]', '[0,1,1]', '[0,0,0]', '[1,0,2]', '[0,2,1]', '[2,0,1]', '[1,1,2]', '[1,1,1]', '[1,2,0]', '[2,2,2]']</t>
+    <t>['[1,1,1]', '[1,2,0]', '[2,2,2]', '[0,2,1]', '[2,1,0]', '[1,0,2]', '[0,0,0]', '[0,1,1]', '[2,0,1]', '[1,1,2]']</t>
   </si>
   <si>
     <t>[1,0,2]</t>
   </si>
   <si>
-    <t>['[1,2,0]', '[0,2,1]', '[2,1,0]', '[1,1,1]', '[0,0,0]', '[2,0,1]', '[1,1,2]', '[1,0,2]', '[0,1,1]', '[2,2,2]']</t>
+    <t>['[1,1,1]', '[0,2,1]', '[1,1,2]', '[0,0,0]', '[2,2,2]', '[2,1,0]', '[2,0,1]', '[1,2,0]', '[0,1,1]', '[1,0,2]']</t>
   </si>
   <si>
     <t>[1,2,0]</t>
@@ -127,7 +127,7 @@
     <t>['[-0.03763371 -0.01533471  0.06554052 -0.01816017]', '[-0.0208055  -0.02030166  0.09914155 -0.02801351]', '[ 0.00031733 -0.02489487  0.10765546 -0.0138725 ]', '[ 0.02044082 -0.02428802  0.08954248  0.02288616]', '[ 0.03470698 -0.01491644  0.05056501  0.07132823]', '[ 0.05326751 -0.03038784  0.13065223 -0.22021077]', '[ 0.07101291 -0.0640307   0.04229076 -0.10791836]', '[ 0.06919594 -0.07148833 -0.06018897  0.03411905]', '[ 0.06123949 -0.0858309  -0.01832924 -0.17605239]', '[ 0.04848925 -0.10546764 -0.10705552 -0.01913256]', '[ 0.03334023 -0.12873715 -0.04224633 -0.21160413]', '[ 0.01856077 -0.15355978 -0.1031453  -0.03494141]', '[ 0.00687968 -0.17764366 -0.01219475 -0.20332606]', '[ 0.00024918 -0.19823055 -0.05320561 -0.00041555]', '[-0.00038196 -0.21249406  0.04645807 -0.13967612]', '[ 0.00462703 -0.21766377  0.00256154  0.08939976]', '[ 0.01391452 -0.21184382  0.0884936  -0.03053848]', '[ 0.03850047 -0.22834148  0.15179103 -0.12764898]', '[ 0.05871339 -0.22531591  0.04642174  0.1602345 ]', '[ 0.06975736 -0.19972822  0.06255754  0.09301244]', '[ 0.08295526 -0.18863935  0.06709485  0.01801994]', '[ 0.0955466  -0.19194963  0.05618073 -0.04863014]', '[ 0.10438266 -0.20672312  0.02995667 -0.09524718]', '[ 0.10679076 -0.22835209 -0.00700287 -0.1170154 ]', '[ 0.10139245 -0.251988   -0.04658216 -0.11618468]', '[ 0.08862558 -0.27379536 -0.07912951 -0.10019242]', '[ 0.07079541 -0.2916811  -0.09605709 -0.07844699]', '[ 0.05160586 -0.30533224 -0.09231221 -0.05881123]', '[ 0.03527347 -0.31561531 -0.06796943 -0.04491109]', '[ 0.02545877 -0.32360191 -0.02840871 -0.03520182]', '[ 0.02431678 -0.32962124  0.01702803 -0.0241677 ]', '[ 0.03194057 -0.33273766  0.0575287  -0.00523763]', '[ 0.04635922 -0.33089406  0.08372791  0.02568935]', '[ 0.06409062 -0.32170512  0.09020522  0.06748616]', '[ 0.08108895 -0.30362649  0.07683704  0.11292955]', '[ 0.09381032 -0.27706452  0.04859846  0.15016487]', '[ 0.10008474 -0.24498455  0.01387843  0.16612946]', '[ 0.099545   -0.21272175 -0.0181427   0.15089341]', '[ 0.09350925 -0.18694889 -0.04018141  0.10151107]', '[ 0.08439395 -0.17403958 -0.04874136  0.02402904]', '[ 0.0748759  -0.17828815 -0.04468765 -0.06714713]', '[ 0.06707968 -0.2005238  -0.03244224 -0.15248501]', '[ 0.06204155 -0.23757011 -0.01810026 -0.2123621 ]', '[ 0.0596084  -0.28277818 -0.00709475 -0.23248464]', '[ 0.0587725  -0.32752505 -0.00232775 -0.20781714]', '[ 0.05826257 -0.3632139  -0.00355436 -0.1435367 ]', '[ 0.05712088 -0.38315408 -0.00807237 -0.05302107]', '[ 0.05506565 -0.38385601 -0.01204958  0.04571899]', '[ 0.05258562 -0.36558361 -0.01179826  0.13373731]', '[ 0.05080563 -0.3322004  -0.0047971   0.19451381]']</t>
   </si>
   <si>
-    <t>['[0,0,0]', '[2,2,2]', '[2,1,0]', '[1,1,1]', '[0,1,1]', '[2,0,1]', '[0,2,1]', '[1,0,2]', '[1,2,0]', '[1,1,2]']</t>
+    <t>['[1,1,2]', '[2,2,2]', '[1,1,1]', '[1,0,2]', '[1,2,0]', '[0,1,1]', '[0,0,0]', '[2,0,1]', '[2,1,0]', '[0,2,1]']</t>
   </si>
   <si>
     <t>[2,0,1]</t>
@@ -139,7 +139,7 @@
     <t>['[-0.03763371 -0.01533471  0.06554052 -0.01816017]', '[-0.03406929  0.01398622 -0.02953871  0.30651903]', '[-0.03493773  0.06836613  0.02265481  0.22789337]', '[-0.02479211  0.10222584  0.07768516  0.10663031]', '[-0.01808581  0.14469195 -0.0104571   0.31140101]', '[-0.01484609  0.18823383  0.0432976   0.11751461]', '[-0.01434726  0.22467153 -0.03717771  0.24054013]', '[-0.01545278  0.24682047  0.02676029 -0.02247913]', '[-0.01721181  0.25018444 -0.04380907  0.05514087]', '[-0.03213003  0.26757856 -0.10176092  0.11343711]', '[-0.04292178  0.2589368  -0.00427078 -0.19989973]', '[-0.04724582  0.22400641 -0.03910061 -0.1442553 ]', '[-0.05828925  0.20274667 -0.06971448 -0.06649573]', '[-0.07416359  0.19747218 -0.0859609   0.01216736]', '[-0.0912366   0.20638244 -0.08104733  0.07279687]', '[-0.10506889  0.22457911 -0.0539522   0.10400424]', '[-0.11166695  0.24587804 -0.010094    0.10444057]', '[-0.10867284  0.26478582  0.03995039  0.08196904]', '[-0.09613136  0.27802333  0.08328201  0.05013698]', '[-0.07660094  0.2851802   0.10825155  0.02324806]', '[-0.0545593   0.2883646   0.10777726  0.01147603]', '[-0.03525161  0.29099778  0.08146314  0.01741678]', '[-0.02329543  0.29616619  0.03584343  0.03525702]', '[-0.0214414   0.30511627 -0.01738635  0.05301171]', '[-0.02985137  0.31645556 -0.06464183  0.05714453]', '[-0.04610073  0.32638407 -0.09423766  0.03793816]', '[-0.06589513  0.32991089 -0.09957126 -0.0063193 ]', '[-0.08428464  0.32265766 -0.08080209 -0.06781655]', '[-0.09702234  0.30264881 -0.04459147 -0.13085587]', '[-0.10168093  0.27149627 -0.00200248 -0.17612255]', '[-0.09820986  0.23455768  0.03486443 -0.1864638 ]', '[-0.0887719   0.19991036  0.05652747 -0.1526692 ]', '[-0.076919    0.17632476  0.05888771 -0.07738584]', '[-0.06638826  0.1707868   0.04416262  0.02447002]', '[-0.05992123  0.18633723  0.01974774  0.1292307 ]', '[-0.0584844   0.22093296 -0.00454223  0.21092628]', '[-0.04805938  0.23384537  0.10680343 -0.08193806]', '[-0.03080471  0.22450229  0.06202129 -0.00733249]', '[-0.02430606  0.23182975  0.00194388  0.08025297]', '[-0.02987406  0.25554917 -0.05571698  0.1519643 ]', '[-0.03226718  0.25603978  0.03214881 -0.14722185]', '[-0.03092284  0.23283646 -0.01960446 -0.08080664]', '[-0.03999585  0.22459335 -0.06946922 -0.00175473]', '[-0.05757792  0.23128942 -0.10254152  0.0647801 ]', '[-0.06605782  0.21440088  0.01888208 -0.23192227]', '[-0.06398042  0.17583314  0.00028999 -0.14688162]', '[-0.06633966  0.15773225 -0.02393686 -0.03146107]', '[-0.07325426  0.16341223 -0.04358916  0.08612216]', '[-0.0828409   0.19044139 -0.04946038  0.17797922]', '[-0.07864045  0.19750911  0.09060325 -0.10746977]']</t>
   </si>
   <si>
-    <t>['[1,1,2]', '[1,0,2]', '[0,1,1]', '[1,2,0]', '[0,2,1]', '[2,2,2]', '[2,1,0]', '[2,0,1]', '[1,1,1]', '[0,0,0]']</t>
+    <t>['[1,1,2]', '[1,2,0]', '[2,1,0]', '[0,0,0]', '[0,2,1]', '[2,0,1]', '[1,1,1]', '[1,0,2]', '[2,2,2]', '[0,1,1]']</t>
   </si>
   <si>
     <t>[2,1,0]</t>
@@ -151,7 +151,7 @@
     <t>['[-0.03763371 -0.01533471  0.06554052 -0.01816017]', '[-0.03406929  0.01398622 -0.02953871  0.30651903]', '[-0.02168374  0.03409236  0.1512214  -0.10649158]', '[-0.00282652  0.04327343  0.03401407  0.19924661]', '[ 0.01834705  0.04294749  0.17317668 -0.19873753]', '[0.03659766 0.0372359  0.00569586 0.14498695]', '[ 0.04737447  0.03050982  0.09950876 -0.20907803]', '[ 0.04773513  0.02629209 -0.09583188  0.16718432]', '[ 0.03752505  0.02534768 -0.00439201 -0.17769188]', '[ 0.01910665  0.02614969 -0.17578652  0.18226832]', '[-0.00293854  0.02498097 -0.04044017 -0.19672323]', '[-0.02338561  0.01819528 -0.15991175  0.1265223 ]', '[-0.03744461  0.00328053  0.02144561 -0.27476369]', '[-0.04234133 -0.01910231 -0.06994388  0.05368665]', '[-0.03763269 -0.04539758  0.11498126 -0.31087136]', '[-0.02550263 -0.06918706  0.00335501  0.07846404]', '[-0.00968282 -0.08350681  0.15097012 -0.21632696]', '[ 0.0053941  -0.08236633 -0.00300315  0.22938636]', '[ 0.0161822  -0.06338321  0.10914378 -0.04087513]', '[ 0.02066644 -0.02828874 -0.063904    0.38603243]', '[0.01913681 0.01633736 0.05013034 0.05264949]', '[ 0.0400551  -0.0073938   0.15390054 -0.28229442]', '[ 0.05094132 -0.02216557 -0.04740575  0.1382459 ]', '[ 0.04870162 -0.02310954  0.02529389 -0.14757537]', '[ 0.03376547 -0.01028918 -0.17094986  0.2707556 ]', '[ 0.0103118   0.01075104 -0.05836816 -0.0672164 ]', '[ 0.01124463 -0.0370396   0.06579493 -0.4018725 ]', '[ 0.00803486 -0.07504962 -0.09809813  0.02722039]', '[ 1.51338775e-04 -9.62015886e-02  1.99960523e-02 -2.35938240e-01]', '[-0.01132378 -0.09750196 -0.13218554  0.22087768]', '[-0.02355496 -0.08096771  0.01267429 -0.05993836]', '[-0.0330696  -0.05205256 -0.10484912  0.34234137]', '[-0.03642324 -0.01860412  0.07279953 -0.01371334]', '[-0.03166866  0.01206933 -0.02509297  0.31554307]', '[-0.01874523  0.03436217  0.15211703 -0.09394883]', '[-5.13230523e-05  4.62105789e-02  3.16075962e-02  2.12883305e-01]', '[ 0.02039466  0.04845639  0.16853114 -0.18720539]', '[0.03762326 0.04455931 0.00038545 0.1511327 ]', '[ 0.04739711  0.03833294  0.09500645 -0.210463  ]', '[ 0.04703493  0.03301412 -0.09845059  0.15764597]', '[ 0.03651771  0.02945918 -0.00486237 -0.19385638]', '[ 0.01818744  0.02662077 -0.17457023  0.1626772 ]', '[-0.00352862  0.02154485 -0.03855204 -0.21548247]', '[-0.02362984  0.01145217 -0.1585124   0.11283283]', '[-0.03753204 -0.00542412  0.02151977 -0.28032934]', '[-0.0425714  -0.02799292 -0.07141092  0.05738308]', '[-0.03827598 -0.05268781  0.11245074 -0.2989076 ]', '[-0.02666782 -0.07350228  0.00086365  0.09565699]', '[-0.01124264 -0.08418115  0.14971078 -0.19780414]', '[ 0.00379227 -0.07954607 -0.00205983  0.24522416]']</t>
   </si>
   <si>
-    <t>['[1,1,1]', '[0,2,1]', '[1,2,0]', '[1,1,2]', '[1,0,2]', '[2,1,0]', '[0,1,1]', '[2,0,1]', '[2,2,2]', '[0,0,0]']</t>
+    <t>['[0,0,0]', '[0,2,1]', '[2,1,0]', '[1,1,1]', '[2,0,1]', '[1,1,2]', '[0,1,1]', '[1,0,2]', '[1,2,0]', '[2,2,2]']</t>
   </si>
   <si>
     <t>[0,0,0]</t>
@@ -166,7 +166,7 @@
     <t>['[-0.03763371 -0.01533471  0.06554052 -0.01816017]', '[-0.00754409 -0.05458322  0.2277812  -0.36241836]', '[ 0.04879627 -0.15231473  0.32089719 -0.5887683 ]', '[ 0.11397169 -0.27767857  0.31375488 -0.63332862]', '[ 0.16759438 -0.39312519  0.2086893  -0.49480525]', '[ 0.1930193  -0.46685036  0.03906408 -0.22816919]', '[ 0.18217995 -0.48119372 -0.14531723  0.08492936]', '[ 0.13737799 -0.43548032 -0.29255645  0.35879992]', '[ 0.07059687 -0.34553749 -0.35944697  0.51636187]', '[ 0.00066518 -0.24025206 -0.32266973  0.50804924]', '[-0.05184718 -0.15356453 -0.18924715  0.33585339]', '[-0.07099568 -0.11316     0.00267821  0.05860212]', '[-0.0506235  -0.13098626  0.19609592 -0.23012254]', '[ 0.00363944 -0.19947979  0.33317766 -0.43407441]', '[ 0.07604673 -0.29425756  0.37330708 -0.48624983]', '[ 0.14566012 -0.38269974  0.30650217 -0.37362319]', '[ 0.19284616 -0.43524651  0.15487527 -0.13746415]', '[ 0.20480978 -0.43420274 -0.03738189  0.14899985]', '[ 0.17872861 -0.37781944 -0.21671607  0.40226469]', '[ 0.12244395 -0.28089207 -0.33207824  0.54289906]', '[ 0.05262627 -0.17207597 -0.34864539  0.51601465]', '[-0.00991093 -0.08621824 -0.26142967  0.31808955]', '[-0.04676022 -0.05276175 -0.09876284  0.00534115]', '[-0.04773189 -0.08549506  0.08793289 -0.326671  ]', '[-0.01386808 -0.17774148  0.24064044 -0.5740393 ]', '[ 0.04305734 -0.30394484  0.31308665 -0.65740151]', '[ 0.10464298 -0.42784083  0.2871402  -0.55250711]', '[ 0.15213765 -0.51456341  0.17665722 -0.29545229]', '[ 0.17195601 -0.54054882  0.01729499  0.04161741]', '[ 0.15877658 -0.49810034 -0.14558791  0.37488532]', '[ 0.11662491 -0.39653924 -0.26514127  0.61927065]', '[ 0.05830606 -0.26143591 -0.30243069  0.70071627]', '[ 0.00240191 -0.12975114 -0.241122    0.58472722]', '[-0.03255824 -0.03901385 -0.09863914  0.30169722]', '[-0.03459084 -0.01467301  0.07923617 -0.06234707]', '[-0.00228999 -0.06214743  0.23549293 -0.3987235 ]', '[ 0.05469493 -0.16555079  0.31932445 -0.60811377]', '[ 0.11857421 -0.29274507  0.30262565 -0.63232462]', '[ 0.16925182 -0.40618487  0.19109743 -0.47671256]', '[ 0.19093562 -0.47518295  0.02014588 -0.20033382]', '[ 0.17663487 -0.48368374 -0.16020096  0.11418666]', '[ 0.12963404 -0.4326335  -0.2991053   0.38177157]', '[ 0.06259366 -0.33924046 -0.35533189  0.52721541]', '[-0.00545982 -0.23320565 -0.30834707  0.50479686]', '[-0.05435734 -0.14835926 -0.16821515  0.32158817]', '[-0.0690908  -0.1113463   0.02479252  0.04024292]', '[-0.04470101 -0.1325791   0.21323988 -0.24461353]', '[ 0.01207873 -0.20303341  0.340642   -0.43848531]', '[ 0.08482177 -0.29746838  0.36917508 -0.47850826]', '[ 0.1525418  -0.38334874  0.2921883  -0.35655192]']</t>
   </si>
   <si>
-    <t>['[2,2,2]', '[2,1,0]', '[1,1,2]', '[1,0,2]', '[1,2,0]', '[0,2,1]', '[1,1,1]', '[0,1,1]', '[2,0,1]', '[0,0,0]']</t>
+    <t>['[1,1,1]', '[2,1,0]', '[0,1,1]', '[2,0,1]', '[1,1,2]', '[0,0,0]', '[0,2,1]', '[2,2,2]', '[1,0,2]', '[1,2,0]']</t>
   </si>
   <si>
     <t>[1,1,1]</t>
@@ -178,7 +178,7 @@
     <t>['[-0.03763371 -0.01533471  0.06554052 -0.01816017]', '[-0.0208055  -0.02030166  0.09914155 -0.02801351]', '[ 0.00031733 -0.02489487  0.10765546 -0.0138725 ]', '[ 0.02044082 -0.02428802  0.08954248  0.02288616]', '[ 0.03470698 -0.01491644  0.05056501  0.07132823]', '[0.04000421 0.0038992  0.00197135 0.11431592]', '[ 0.0357442   0.02924956 -0.04287984  0.13410557]', '[ 0.02389303  0.05513259 -0.0724118   0.11843067]', '[ 0.00827151  0.0740515  -0.08006316  0.06513577]', '[-0.00664229  0.07925492 -0.06591977 -0.01622081]', '[-0.01703829  0.06693573 -0.03635037 -0.10637005]', '[-0.02083887  0.0377102  -0.00183146 -0.18135846]', '[-0.01819393 -0.00310741  0.02644173 -0.21931589]', '[-0.0112553  -0.04661351  0.04018081 -0.20717791]', '[-0.00330983 -0.08257268  0.03658645 -0.14508251]', '[ 0.0024104  -0.10215919  0.01891064 -0.04666104]', '[ 0.00382015 -0.10033648 -0.00499775  0.06469207]', '[ 0.00064351 -0.07722007 -0.02539101  0.16195768]', '[-0.00551959 -0.03811088 -0.03377164  0.22142738]', '[-0.01174627  0.0078305  -0.02581131  0.22911312]', '[-0.01482841  0.04999004 -0.00311123  0.18480626]', '[-0.01246489  0.07911924  0.02710494  0.10195664]', '[-0.00417355  0.08968453  0.05438991  0.00327931]', '[ 0.00840543  0.08106163  0.06855001 -0.08601484]', '[ 0.02190299  0.05733301  0.06295851 -0.14509547]', '[ 0.0321837   0.02584205  0.03681891 -0.16284223]', '[ 0.03560428 -0.00505404 -0.00421667 -0.14034077]', '[ 0.03020079 -0.02836988 -0.04938897 -0.08972441]', '[ 0.01642725 -0.04029751 -0.08587168 -0.02970417]', '[-0.00281086 -0.04091095 -0.10259647  0.020656  ]', '[-0.02286552 -0.03361943 -0.09365837  0.04790331]', '[-0.03860246 -0.0236106  -0.06024324  0.04807679]', '[-0.04583902 -0.01583448 -0.01046864  0.02730739]', '[-0.04253854 -0.01321526  0.0428277  -0.00097241]', '[-0.02940859 -0.0156797   0.08568823 -0.02115895]', '[-0.00972652 -0.02030416  0.1069775  -0.02123067]', '[ 0.0115618  -0.02251874  0.10152992  0.00272141]', '[ 0.02921079 -0.01796026  0.07156041  0.04472731]', '[ 0.03910994 -0.00433545  0.02589999  0.09061009]', '[ 0.03936403  0.01735836 -0.02268767  0.12255506]', '[ 0.03071193  0.04269742 -0.06126398  0.1251015 ]', '[ 0.01618133  0.06487999 -0.08040737  0.09068004]', '[ 0.00010594  0.07668079 -0.07674355  0.02287818]', '[-0.0131837   0.07272569 -0.05361425 -0.06371658]', '[-0.02060331  0.05138348 -0.0197783  -0.14709165]', '[-0.0211313   0.01567674  0.01345636 -0.20383146]', '[-0.01595742 -0.02713289  0.03588002 -0.21605443]', '[-0.00791991 -0.06726788  0.0416368  -0.17718674]', '[-0.00043664 -0.09500666  0.03087284 -0.0943888 ]', '[ 0.00368075 -0.10331248  0.0092639   0.01327487]']</t>
   </si>
   <si>
-    <t>['[2,1,0]', '[2,0,1]', '[0,0,0]', '[2,2,2]', '[0,2,1]', '[1,1,1]', '[0,1,1]', '[1,0,2]', '[1,2,0]', '[1,1,2]']</t>
+    <t>['[1,1,2]', '[0,2,1]', '[1,1,1]', '[2,1,0]', '[1,0,2]', '[0,1,1]', '[0,0,0]', '[2,2,2]', '[1,2,0]', '[2,0,1]']</t>
   </si>
   <si>
     <t>[2,2,2]</t>
@@ -193,7 +193,7 @@
     <t>['[-0.03763371 -0.01533471  0.06554052 -0.01816017]', '[-0.03406929  0.01398622 -0.02953871  0.30651903]', '[-0.04818188  0.10262173 -0.10566927  0.56184435]', '[-0.07305261  0.22936701 -0.13369446  0.67944384]', '[-0.0976443   0.36319498 -0.10327727  0.63282133]', '[-0.11125897  0.47297074 -0.02773051  0.446438  ]', '[-0.10757465  0.53619101  0.06462001  0.17794954]', '[-0.08631261  0.54305113  0.14348542 -0.10660175]', '[-0.05272941  0.496551    0.18460856 -0.34656399]', '[-0.01604448  0.4107609   0.17301646 -0.49290646]', '[ 0.01268242  0.3077355   0.10583916 -0.51655332]', '[ 0.02333646  0.21239857 -0.00419223 -0.4193517 ]', '[ 0.0099677   0.14579835 -0.12877174 -0.23752332]', '[-0.02671453  0.11914618 -0.23135882 -0.03029568]', '[-0.07887305  0.13122166 -0.27923433  0.14079468]', '[-0.13346965  0.17000821 -0.25455054  0.23213127]', '[-0.17594228  0.2177196  -0.16032293  0.23074589]', '[-0.19440453  0.25720213 -0.01958413  0.15500349]', '[-0.18304473  0.2773318   0.13139765  0.04471749]', '[-0.14381952  0.27594314  0.25290378 -0.05262463]', '[-0.08610129  0.25997418  0.3121551  -0.09574381]', '[-0.02431919  0.24283739  0.29265156 -0.06321871]', '[0.025942   0.23936241 0.19971411 0.03691163]', '[0.05230735 0.25979636 0.05929573 0.16809359]', '[ 0.04903274  0.30520172 -0.08996005  0.27778487]', '[ 0.01840997  0.3660885  -0.20830118  0.31617897]', '[-0.03017518  0.42484365 -0.26613074  0.25434096]', '[-0.08310648  0.46114583 -0.25151672  0.09491522]', '[-0.12637105  0.45839229 -0.17234971 -0.12852159]', '[-0.14934542  0.40908444 -0.05391547 -0.3602991 ]', '[-0.14772278  0.3180918   0.0672533  -0.53461121]', '[-0.12479853  0.20317901  0.15370315 -0.59148689]', '[-0.09033116  0.09169889  0.18033911 -0.49864447]', '[-0.05698072  0.01310365  0.14398671 -0.26870757]', '[-0.03582515 -0.0101366   0.06271589  0.0432441 ]', '[-0.03284724  0.03064719 -0.03208739  0.35765344]', '[-0.04720001  0.12749223 -0.10517205  0.59129397]', '[-0.07155134  0.25739102 -0.12905439  0.6812098 ]', '[-0.09492447  0.388912   -0.09622775  0.60894699]', '[-0.10718747  0.49201057 -0.0218702   0.40512845]', '[-0.10272942  0.54605232  0.06611999  0.12900689]', '[-0.08173302  0.54308751  0.13927353 -0.15466602]', '[-0.04954254  0.48764289  0.17506264 -0.38695002]', '[-0.0151897   0.39500767  0.15952967 -0.52021901]', '[ 0.01060951  0.28814293  0.09044679 -0.52729481]', '[ 0.01822159  0.19237607 -0.01869241 -0.41316397]', '[ 0.00232707  0.12845925 -0.13896224 -0.21766133]', '[-0.03568997  0.10667803 -0.23409955 -0.00247033]', '[-0.08749173  0.12459123 -0.27282479  0.17041154]', '[-0.13991018  0.16905379 -0.23945127  0.25864832]']</t>
   </si>
   <si>
-    <t>['[1,1,1]', '[2,1,0]', '[0,2,1]', '[1,0,2]', '[2,0,1]', '[0,1,1]', '[0,0,0]', '[2,2,2]', '[1,1,2]', '[1,2,0]']</t>
+    <t>['[2,2,2]', '[0,2,1]', '[2,0,1]', '[2,1,0]', '[1,2,0]', '[0,0,0]', '[1,0,2]', '[1,1,2]', '[0,1,1]', '[1,1,1]']</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
taxi is also working now
</commit_message>
<xml_diff>
--- a/experimental results/e2000_Acrobot.xlsx
+++ b/experimental results/e2000_Acrobot.xlsx
@@ -85,7 +85,7 @@
     <t>Omitted</t>
   </si>
   <si>
-    <t>['[0,2,1]', '[2,0,1]', '[2,1,0]', '[1,0,2]', '[2,2,2]', '[1,2,0]', '[0,1,1]', '[0,0,0]', '[1,1,2]', '[1,1,1]']</t>
+    <t>['[1,2,0]', '[0,1,1]', '[1,1,1]', '[1,1,2]', '[0,2,1]', '[2,1,0]', '[0,0,0]', '[1,0,2]', '[2,0,1]', '[2,2,2]']</t>
   </si>
   <si>
     <t>[0,1,1]</t>
@@ -100,19 +100,19 @@
     <t>['[-0.03763371 -0.01533471  0.06554052 -0.01816017]', '[-0.00754409 -0.05458322  0.2277812  -0.36241836]', '[ 0.04879627 -0.15231473  0.32089719 -0.5887683 ]', '[ 0.11397169 -0.27767857  0.31375488 -0.63332862]', '[ 0.16759438 -0.39312519  0.2086893  -0.49480525]', '[ 0.1930193  -0.46685036  0.03906408 -0.22816919]', '[ 0.16956871 -0.44830261 -0.26820417  0.40739083]', '[ 0.09055011 -0.31127879 -0.50323119  0.93116007]', '[-0.02165415 -0.09380121 -0.58952709  1.1892161 ]', '[-0.13228272  0.13968862 -0.48657385  1.08703787]', '[-0.20542731  0.31962025 -0.22562708  0.67289162]', '[-0.21756752  0.39782756  0.10766541  0.09689063]', '[-0.15109606  0.32490126  0.54216963 -0.80657469]', '[-0.01068619  0.09081112  0.82714324 -1.47439182]', '[ 0.16212513 -0.23279107  0.85391345 -1.67375883]', '[ 0.3120332  -0.54339537  0.60708552 -1.36152952]', '[ 0.39322683 -0.75586146  0.18779451 -0.73014827]', '[ 0.38412465 -0.82793881 -0.27624305  0.01454459]', '[ 0.27552572 -0.72135137 -0.78884754  1.03160865]', '[ 0.08086773 -0.43032213 -1.11647003  1.81675029]', '[-0.14966877 -0.03109877 -1.12879696  2.06540623]', '[-0.3455444   0.34863759 -0.7784691   1.63534647]', '[-0.44544803  0.59424237 -0.19906427  0.77949316]', '[-0.4218337   0.6519398   0.43007126 -0.20572333]', '[-0.26769146  0.484052    1.08142007 -1.44055859]', '[-0.00742761  0.10113176  1.45927884 -2.28595201]', '[ 0.28490347 -0.37428385  1.38589424 -2.32532176]', '[ 0.5187101  -0.77937684  0.90230152 -1.64619583]', '[ 0.63240836 -1.01433747  0.21740989 -0.68198512]', '[ 0.59278756 -1.01958166 -0.60566507  0.62852481]', '[ 0.39752784 -0.7660208  -1.31595743  1.88179849]', '[ 0.08542661 -0.29020757 -1.73661998  2.76615566]', '[-0.26054486  0.27360101 -1.62803895  2.69265107]', '[-0.53183224  0.72525907 -1.02799868  1.73308445]', '[-0.65747495  0.94866122 -0.21116234  0.48419472]', '[-0.60316944  0.88713812  0.74646124 -1.09703619]', '[-0.3667148   0.51448679  1.5802398  -2.58584684]', '[ 2.25515542e-03 -1.04226788e-01  2.01052042e+00 -3.41515113e+00]', '[ 0.38981745 -0.75816996  1.76540261 -2.93947302]', '[ 0.67971886 -1.23563438  1.09061136 -1.79181237]', '[ 0.81522073 -1.47040276  0.25012952 -0.55613563]', '[ 0.76893557 -1.43299403 -0.70634091  0.93217091]', '[ 0.53890731 -1.09497955 -1.5685075   2.44803386]', '[ 0.15769536 -0.46498696 -2.17507038  3.75054866]', '[-0.28566374  0.31885175 -2.12308403  3.81427092]', '[-0.64333931  0.96714913 -1.38377582  2.55626676]', '[-0.82476188  1.32821982 -0.41497441  1.0541805 ]', '[-0.80769438  1.39053182  0.57925977 -0.43113385]', '[-0.58966747  1.12643161  1.57705339 -2.21920745]', '[-0.19115743  0.50615398  2.34648211 -3.90612928]']</t>
   </si>
   <si>
-    <t>['[2,0,1]', '[1,2,0]', '[2,2,2]', '[1,1,2]', '[0,2,1]', '[1,1,1]', '[2,1,0]', '[1,0,2]', '[0,1,1]', '[0,0,0]']</t>
+    <t>['[0,1,1]', '[1,0,2]', '[2,0,1]', '[2,1,0]', '[1,1,1]', '[1,1,2]', '[0,0,0]', '[0,2,1]', '[1,2,0]', '[2,2,2]']</t>
   </si>
   <si>
     <t>[0,2,1]</t>
   </si>
   <si>
-    <t>['[1,1,1]', '[1,2,0]', '[2,2,2]', '[0,2,1]', '[2,1,0]', '[1,0,2]', '[0,0,0]', '[0,1,1]', '[2,0,1]', '[1,1,2]']</t>
+    <t>['[1,0,2]', '[1,2,0]', '[1,1,1]', '[2,1,0]', '[2,0,1]', '[0,1,1]', '[1,1,2]', '[2,2,2]', '[0,0,0]', '[0,2,1]']</t>
   </si>
   <si>
     <t>[1,0,2]</t>
   </si>
   <si>
-    <t>['[1,1,1]', '[0,2,1]', '[1,1,2]', '[0,0,0]', '[2,2,2]', '[2,1,0]', '[2,0,1]', '[1,2,0]', '[0,1,1]', '[1,0,2]']</t>
+    <t>['[0,0,0]', '[1,1,1]', '[1,0,2]', '[1,2,0]', '[2,2,2]', '[2,0,1]', '[0,2,1]', '[0,1,1]', '[1,1,2]', '[2,1,0]']</t>
   </si>
   <si>
     <t>[1,2,0]</t>
@@ -127,7 +127,7 @@
     <t>['[-0.03763371 -0.01533471  0.06554052 -0.01816017]', '[-0.0208055  -0.02030166  0.09914155 -0.02801351]', '[ 0.00031733 -0.02489487  0.10765546 -0.0138725 ]', '[ 0.02044082 -0.02428802  0.08954248  0.02288616]', '[ 0.03470698 -0.01491644  0.05056501  0.07132823]', '[ 0.05326751 -0.03038784  0.13065223 -0.22021077]', '[ 0.07101291 -0.0640307   0.04229076 -0.10791836]', '[ 0.06919594 -0.07148833 -0.06018897  0.03411905]', '[ 0.06123949 -0.0858309  -0.01832924 -0.17605239]', '[ 0.04848925 -0.10546764 -0.10705552 -0.01913256]', '[ 0.03334023 -0.12873715 -0.04224633 -0.21160413]', '[ 0.01856077 -0.15355978 -0.1031453  -0.03494141]', '[ 0.00687968 -0.17764366 -0.01219475 -0.20332606]', '[ 0.00024918 -0.19823055 -0.05320561 -0.00041555]', '[-0.00038196 -0.21249406  0.04645807 -0.13967612]', '[ 0.00462703 -0.21766377  0.00256154  0.08939976]', '[ 0.01391452 -0.21184382  0.0884936  -0.03053848]', '[ 0.03850047 -0.22834148  0.15179103 -0.12764898]', '[ 0.05871339 -0.22531591  0.04642174  0.1602345 ]', '[ 0.06975736 -0.19972822  0.06255754  0.09301244]', '[ 0.08295526 -0.18863935  0.06709485  0.01801994]', '[ 0.0955466  -0.19194963  0.05618073 -0.04863014]', '[ 0.10438266 -0.20672312  0.02995667 -0.09524718]', '[ 0.10679076 -0.22835209 -0.00700287 -0.1170154 ]', '[ 0.10139245 -0.251988   -0.04658216 -0.11618468]', '[ 0.08862558 -0.27379536 -0.07912951 -0.10019242]', '[ 0.07079541 -0.2916811  -0.09605709 -0.07844699]', '[ 0.05160586 -0.30533224 -0.09231221 -0.05881123]', '[ 0.03527347 -0.31561531 -0.06796943 -0.04491109]', '[ 0.02545877 -0.32360191 -0.02840871 -0.03520182]', '[ 0.02431678 -0.32962124  0.01702803 -0.0241677 ]', '[ 0.03194057 -0.33273766  0.0575287  -0.00523763]', '[ 0.04635922 -0.33089406  0.08372791  0.02568935]', '[ 0.06409062 -0.32170512  0.09020522  0.06748616]', '[ 0.08108895 -0.30362649  0.07683704  0.11292955]', '[ 0.09381032 -0.27706452  0.04859846  0.15016487]', '[ 0.10008474 -0.24498455  0.01387843  0.16612946]', '[ 0.099545   -0.21272175 -0.0181427   0.15089341]', '[ 0.09350925 -0.18694889 -0.04018141  0.10151107]', '[ 0.08439395 -0.17403958 -0.04874136  0.02402904]', '[ 0.0748759  -0.17828815 -0.04468765 -0.06714713]', '[ 0.06707968 -0.2005238  -0.03244224 -0.15248501]', '[ 0.06204155 -0.23757011 -0.01810026 -0.2123621 ]', '[ 0.0596084  -0.28277818 -0.00709475 -0.23248464]', '[ 0.0587725  -0.32752505 -0.00232775 -0.20781714]', '[ 0.05826257 -0.3632139  -0.00355436 -0.1435367 ]', '[ 0.05712088 -0.38315408 -0.00807237 -0.05302107]', '[ 0.05506565 -0.38385601 -0.01204958  0.04571899]', '[ 0.05258562 -0.36558361 -0.01179826  0.13373731]', '[ 0.05080563 -0.3322004  -0.0047971   0.19451381]']</t>
   </si>
   <si>
-    <t>['[1,1,2]', '[2,2,2]', '[1,1,1]', '[1,0,2]', '[1,2,0]', '[0,1,1]', '[0,0,0]', '[2,0,1]', '[2,1,0]', '[0,2,1]']</t>
+    <t>['[2,2,2]', '[1,2,0]', '[1,0,2]', '[1,1,2]', '[0,1,1]', '[1,1,1]', '[2,1,0]', '[0,0,0]', '[0,2,1]', '[2,0,1]']</t>
   </si>
   <si>
     <t>[2,0,1]</t>
@@ -139,7 +139,7 @@
     <t>['[-0.03763371 -0.01533471  0.06554052 -0.01816017]', '[-0.03406929  0.01398622 -0.02953871  0.30651903]', '[-0.03493773  0.06836613  0.02265481  0.22789337]', '[-0.02479211  0.10222584  0.07768516  0.10663031]', '[-0.01808581  0.14469195 -0.0104571   0.31140101]', '[-0.01484609  0.18823383  0.0432976   0.11751461]', '[-0.01434726  0.22467153 -0.03717771  0.24054013]', '[-0.01545278  0.24682047  0.02676029 -0.02247913]', '[-0.01721181  0.25018444 -0.04380907  0.05514087]', '[-0.03213003  0.26757856 -0.10176092  0.11343711]', '[-0.04292178  0.2589368  -0.00427078 -0.19989973]', '[-0.04724582  0.22400641 -0.03910061 -0.1442553 ]', '[-0.05828925  0.20274667 -0.06971448 -0.06649573]', '[-0.07416359  0.19747218 -0.0859609   0.01216736]', '[-0.0912366   0.20638244 -0.08104733  0.07279687]', '[-0.10506889  0.22457911 -0.0539522   0.10400424]', '[-0.11166695  0.24587804 -0.010094    0.10444057]', '[-0.10867284  0.26478582  0.03995039  0.08196904]', '[-0.09613136  0.27802333  0.08328201  0.05013698]', '[-0.07660094  0.2851802   0.10825155  0.02324806]', '[-0.0545593   0.2883646   0.10777726  0.01147603]', '[-0.03525161  0.29099778  0.08146314  0.01741678]', '[-0.02329543  0.29616619  0.03584343  0.03525702]', '[-0.0214414   0.30511627 -0.01738635  0.05301171]', '[-0.02985137  0.31645556 -0.06464183  0.05714453]', '[-0.04610073  0.32638407 -0.09423766  0.03793816]', '[-0.06589513  0.32991089 -0.09957126 -0.0063193 ]', '[-0.08428464  0.32265766 -0.08080209 -0.06781655]', '[-0.09702234  0.30264881 -0.04459147 -0.13085587]', '[-0.10168093  0.27149627 -0.00200248 -0.17612255]', '[-0.09820986  0.23455768  0.03486443 -0.1864638 ]', '[-0.0887719   0.19991036  0.05652747 -0.1526692 ]', '[-0.076919    0.17632476  0.05888771 -0.07738584]', '[-0.06638826  0.1707868   0.04416262  0.02447002]', '[-0.05992123  0.18633723  0.01974774  0.1292307 ]', '[-0.0584844   0.22093296 -0.00454223  0.21092628]', '[-0.04805938  0.23384537  0.10680343 -0.08193806]', '[-0.03080471  0.22450229  0.06202129 -0.00733249]', '[-0.02430606  0.23182975  0.00194388  0.08025297]', '[-0.02987406  0.25554917 -0.05571698  0.1519643 ]', '[-0.03226718  0.25603978  0.03214881 -0.14722185]', '[-0.03092284  0.23283646 -0.01960446 -0.08080664]', '[-0.03999585  0.22459335 -0.06946922 -0.00175473]', '[-0.05757792  0.23128942 -0.10254152  0.0647801 ]', '[-0.06605782  0.21440088  0.01888208 -0.23192227]', '[-0.06398042  0.17583314  0.00028999 -0.14688162]', '[-0.06633966  0.15773225 -0.02393686 -0.03146107]', '[-0.07325426  0.16341223 -0.04358916  0.08612216]', '[-0.0828409   0.19044139 -0.04946038  0.17797922]', '[-0.07864045  0.19750911  0.09060325 -0.10746977]']</t>
   </si>
   <si>
-    <t>['[1,1,2]', '[1,2,0]', '[2,1,0]', '[0,0,0]', '[0,2,1]', '[2,0,1]', '[1,1,1]', '[1,0,2]', '[2,2,2]', '[0,1,1]']</t>
+    <t>['[2,1,0]', '[0,2,1]', '[1,0,2]', '[2,2,2]', '[1,1,1]', '[1,2,0]', '[0,0,0]', '[1,1,2]', '[0,1,1]', '[2,0,1]']</t>
   </si>
   <si>
     <t>[2,1,0]</t>
@@ -151,7 +151,7 @@
     <t>['[-0.03763371 -0.01533471  0.06554052 -0.01816017]', '[-0.03406929  0.01398622 -0.02953871  0.30651903]', '[-0.02168374  0.03409236  0.1512214  -0.10649158]', '[-0.00282652  0.04327343  0.03401407  0.19924661]', '[ 0.01834705  0.04294749  0.17317668 -0.19873753]', '[0.03659766 0.0372359  0.00569586 0.14498695]', '[ 0.04737447  0.03050982  0.09950876 -0.20907803]', '[ 0.04773513  0.02629209 -0.09583188  0.16718432]', '[ 0.03752505  0.02534768 -0.00439201 -0.17769188]', '[ 0.01910665  0.02614969 -0.17578652  0.18226832]', '[-0.00293854  0.02498097 -0.04044017 -0.19672323]', '[-0.02338561  0.01819528 -0.15991175  0.1265223 ]', '[-0.03744461  0.00328053  0.02144561 -0.27476369]', '[-0.04234133 -0.01910231 -0.06994388  0.05368665]', '[-0.03763269 -0.04539758  0.11498126 -0.31087136]', '[-0.02550263 -0.06918706  0.00335501  0.07846404]', '[-0.00968282 -0.08350681  0.15097012 -0.21632696]', '[ 0.0053941  -0.08236633 -0.00300315  0.22938636]', '[ 0.0161822  -0.06338321  0.10914378 -0.04087513]', '[ 0.02066644 -0.02828874 -0.063904    0.38603243]', '[0.01913681 0.01633736 0.05013034 0.05264949]', '[ 0.0400551  -0.0073938   0.15390054 -0.28229442]', '[ 0.05094132 -0.02216557 -0.04740575  0.1382459 ]', '[ 0.04870162 -0.02310954  0.02529389 -0.14757537]', '[ 0.03376547 -0.01028918 -0.17094986  0.2707556 ]', '[ 0.0103118   0.01075104 -0.05836816 -0.0672164 ]', '[ 0.01124463 -0.0370396   0.06579493 -0.4018725 ]', '[ 0.00803486 -0.07504962 -0.09809813  0.02722039]', '[ 1.51338775e-04 -9.62015886e-02  1.99960523e-02 -2.35938240e-01]', '[-0.01132378 -0.09750196 -0.13218554  0.22087768]', '[-0.02355496 -0.08096771  0.01267429 -0.05993836]', '[-0.0330696  -0.05205256 -0.10484912  0.34234137]', '[-0.03642324 -0.01860412  0.07279953 -0.01371334]', '[-0.03166866  0.01206933 -0.02509297  0.31554307]', '[-0.01874523  0.03436217  0.15211703 -0.09394883]', '[-5.13230523e-05  4.62105789e-02  3.16075962e-02  2.12883305e-01]', '[ 0.02039466  0.04845639  0.16853114 -0.18720539]', '[0.03762326 0.04455931 0.00038545 0.1511327 ]', '[ 0.04739711  0.03833294  0.09500645 -0.210463  ]', '[ 0.04703493  0.03301412 -0.09845059  0.15764597]', '[ 0.03651771  0.02945918 -0.00486237 -0.19385638]', '[ 0.01818744  0.02662077 -0.17457023  0.1626772 ]', '[-0.00352862  0.02154485 -0.03855204 -0.21548247]', '[-0.02362984  0.01145217 -0.1585124   0.11283283]', '[-0.03753204 -0.00542412  0.02151977 -0.28032934]', '[-0.0425714  -0.02799292 -0.07141092  0.05738308]', '[-0.03827598 -0.05268781  0.11245074 -0.2989076 ]', '[-0.02666782 -0.07350228  0.00086365  0.09565699]', '[-0.01124264 -0.08418115  0.14971078 -0.19780414]', '[ 0.00379227 -0.07954607 -0.00205983  0.24522416]']</t>
   </si>
   <si>
-    <t>['[0,0,0]', '[0,2,1]', '[2,1,0]', '[1,1,1]', '[2,0,1]', '[1,1,2]', '[0,1,1]', '[1,0,2]', '[1,2,0]', '[2,2,2]']</t>
+    <t>['[2,1,0]', '[1,0,2]', '[2,2,2]', '[1,1,1]', '[0,0,0]', '[1,2,0]', '[0,2,1]', '[1,1,2]', '[2,0,1]', '[0,1,1]']</t>
   </si>
   <si>
     <t>[0,0,0]</t>
@@ -166,7 +166,7 @@
     <t>['[-0.03763371 -0.01533471  0.06554052 -0.01816017]', '[-0.00754409 -0.05458322  0.2277812  -0.36241836]', '[ 0.04879627 -0.15231473  0.32089719 -0.5887683 ]', '[ 0.11397169 -0.27767857  0.31375488 -0.63332862]', '[ 0.16759438 -0.39312519  0.2086893  -0.49480525]', '[ 0.1930193  -0.46685036  0.03906408 -0.22816919]', '[ 0.18217995 -0.48119372 -0.14531723  0.08492936]', '[ 0.13737799 -0.43548032 -0.29255645  0.35879992]', '[ 0.07059687 -0.34553749 -0.35944697  0.51636187]', '[ 0.00066518 -0.24025206 -0.32266973  0.50804924]', '[-0.05184718 -0.15356453 -0.18924715  0.33585339]', '[-0.07099568 -0.11316     0.00267821  0.05860212]', '[-0.0506235  -0.13098626  0.19609592 -0.23012254]', '[ 0.00363944 -0.19947979  0.33317766 -0.43407441]', '[ 0.07604673 -0.29425756  0.37330708 -0.48624983]', '[ 0.14566012 -0.38269974  0.30650217 -0.37362319]', '[ 0.19284616 -0.43524651  0.15487527 -0.13746415]', '[ 0.20480978 -0.43420274 -0.03738189  0.14899985]', '[ 0.17872861 -0.37781944 -0.21671607  0.40226469]', '[ 0.12244395 -0.28089207 -0.33207824  0.54289906]', '[ 0.05262627 -0.17207597 -0.34864539  0.51601465]', '[-0.00991093 -0.08621824 -0.26142967  0.31808955]', '[-0.04676022 -0.05276175 -0.09876284  0.00534115]', '[-0.04773189 -0.08549506  0.08793289 -0.326671  ]', '[-0.01386808 -0.17774148  0.24064044 -0.5740393 ]', '[ 0.04305734 -0.30394484  0.31308665 -0.65740151]', '[ 0.10464298 -0.42784083  0.2871402  -0.55250711]', '[ 0.15213765 -0.51456341  0.17665722 -0.29545229]', '[ 0.17195601 -0.54054882  0.01729499  0.04161741]', '[ 0.15877658 -0.49810034 -0.14558791  0.37488532]', '[ 0.11662491 -0.39653924 -0.26514127  0.61927065]', '[ 0.05830606 -0.26143591 -0.30243069  0.70071627]', '[ 0.00240191 -0.12975114 -0.241122    0.58472722]', '[-0.03255824 -0.03901385 -0.09863914  0.30169722]', '[-0.03459084 -0.01467301  0.07923617 -0.06234707]', '[-0.00228999 -0.06214743  0.23549293 -0.3987235 ]', '[ 0.05469493 -0.16555079  0.31932445 -0.60811377]', '[ 0.11857421 -0.29274507  0.30262565 -0.63232462]', '[ 0.16925182 -0.40618487  0.19109743 -0.47671256]', '[ 0.19093562 -0.47518295  0.02014588 -0.20033382]', '[ 0.17663487 -0.48368374 -0.16020096  0.11418666]', '[ 0.12963404 -0.4326335  -0.2991053   0.38177157]', '[ 0.06259366 -0.33924046 -0.35533189  0.52721541]', '[-0.00545982 -0.23320565 -0.30834707  0.50479686]', '[-0.05435734 -0.14835926 -0.16821515  0.32158817]', '[-0.0690908  -0.1113463   0.02479252  0.04024292]', '[-0.04470101 -0.1325791   0.21323988 -0.24461353]', '[ 0.01207873 -0.20303341  0.340642   -0.43848531]', '[ 0.08482177 -0.29746838  0.36917508 -0.47850826]', '[ 0.1525418  -0.38334874  0.2921883  -0.35655192]']</t>
   </si>
   <si>
-    <t>['[1,1,1]', '[2,1,0]', '[0,1,1]', '[2,0,1]', '[1,1,2]', '[0,0,0]', '[0,2,1]', '[2,2,2]', '[1,0,2]', '[1,2,0]']</t>
+    <t>['[2,0,1]', '[0,1,1]', '[1,1,1]', '[1,1,2]', '[2,2,2]', '[1,0,2]', '[0,0,0]', '[0,2,1]', '[2,1,0]', '[1,2,0]']</t>
   </si>
   <si>
     <t>[1,1,1]</t>
@@ -178,7 +178,7 @@
     <t>['[-0.03763371 -0.01533471  0.06554052 -0.01816017]', '[-0.0208055  -0.02030166  0.09914155 -0.02801351]', '[ 0.00031733 -0.02489487  0.10765546 -0.0138725 ]', '[ 0.02044082 -0.02428802  0.08954248  0.02288616]', '[ 0.03470698 -0.01491644  0.05056501  0.07132823]', '[0.04000421 0.0038992  0.00197135 0.11431592]', '[ 0.0357442   0.02924956 -0.04287984  0.13410557]', '[ 0.02389303  0.05513259 -0.0724118   0.11843067]', '[ 0.00827151  0.0740515  -0.08006316  0.06513577]', '[-0.00664229  0.07925492 -0.06591977 -0.01622081]', '[-0.01703829  0.06693573 -0.03635037 -0.10637005]', '[-0.02083887  0.0377102  -0.00183146 -0.18135846]', '[-0.01819393 -0.00310741  0.02644173 -0.21931589]', '[-0.0112553  -0.04661351  0.04018081 -0.20717791]', '[-0.00330983 -0.08257268  0.03658645 -0.14508251]', '[ 0.0024104  -0.10215919  0.01891064 -0.04666104]', '[ 0.00382015 -0.10033648 -0.00499775  0.06469207]', '[ 0.00064351 -0.07722007 -0.02539101  0.16195768]', '[-0.00551959 -0.03811088 -0.03377164  0.22142738]', '[-0.01174627  0.0078305  -0.02581131  0.22911312]', '[-0.01482841  0.04999004 -0.00311123  0.18480626]', '[-0.01246489  0.07911924  0.02710494  0.10195664]', '[-0.00417355  0.08968453  0.05438991  0.00327931]', '[ 0.00840543  0.08106163  0.06855001 -0.08601484]', '[ 0.02190299  0.05733301  0.06295851 -0.14509547]', '[ 0.0321837   0.02584205  0.03681891 -0.16284223]', '[ 0.03560428 -0.00505404 -0.00421667 -0.14034077]', '[ 0.03020079 -0.02836988 -0.04938897 -0.08972441]', '[ 0.01642725 -0.04029751 -0.08587168 -0.02970417]', '[-0.00281086 -0.04091095 -0.10259647  0.020656  ]', '[-0.02286552 -0.03361943 -0.09365837  0.04790331]', '[-0.03860246 -0.0236106  -0.06024324  0.04807679]', '[-0.04583902 -0.01583448 -0.01046864  0.02730739]', '[-0.04253854 -0.01321526  0.0428277  -0.00097241]', '[-0.02940859 -0.0156797   0.08568823 -0.02115895]', '[-0.00972652 -0.02030416  0.1069775  -0.02123067]', '[ 0.0115618  -0.02251874  0.10152992  0.00272141]', '[ 0.02921079 -0.01796026  0.07156041  0.04472731]', '[ 0.03910994 -0.00433545  0.02589999  0.09061009]', '[ 0.03936403  0.01735836 -0.02268767  0.12255506]', '[ 0.03071193  0.04269742 -0.06126398  0.1251015 ]', '[ 0.01618133  0.06487999 -0.08040737  0.09068004]', '[ 0.00010594  0.07668079 -0.07674355  0.02287818]', '[-0.0131837   0.07272569 -0.05361425 -0.06371658]', '[-0.02060331  0.05138348 -0.0197783  -0.14709165]', '[-0.0211313   0.01567674  0.01345636 -0.20383146]', '[-0.01595742 -0.02713289  0.03588002 -0.21605443]', '[-0.00791991 -0.06726788  0.0416368  -0.17718674]', '[-0.00043664 -0.09500666  0.03087284 -0.0943888 ]', '[ 0.00368075 -0.10331248  0.0092639   0.01327487]']</t>
   </si>
   <si>
-    <t>['[1,1,2]', '[0,2,1]', '[1,1,1]', '[2,1,0]', '[1,0,2]', '[0,1,1]', '[0,0,0]', '[2,2,2]', '[1,2,0]', '[2,0,1]']</t>
+    <t>['[2,2,2]', '[0,1,1]', '[1,2,0]', '[0,2,1]', '[0,0,0]', '[1,1,1]', '[1,1,2]', '[2,0,1]', '[1,0,2]', '[2,1,0]']</t>
   </si>
   <si>
     <t>[2,2,2]</t>
@@ -193,7 +193,7 @@
     <t>['[-0.03763371 -0.01533471  0.06554052 -0.01816017]', '[-0.03406929  0.01398622 -0.02953871  0.30651903]', '[-0.04818188  0.10262173 -0.10566927  0.56184435]', '[-0.07305261  0.22936701 -0.13369446  0.67944384]', '[-0.0976443   0.36319498 -0.10327727  0.63282133]', '[-0.11125897  0.47297074 -0.02773051  0.446438  ]', '[-0.10757465  0.53619101  0.06462001  0.17794954]', '[-0.08631261  0.54305113  0.14348542 -0.10660175]', '[-0.05272941  0.496551    0.18460856 -0.34656399]', '[-0.01604448  0.4107609   0.17301646 -0.49290646]', '[ 0.01268242  0.3077355   0.10583916 -0.51655332]', '[ 0.02333646  0.21239857 -0.00419223 -0.4193517 ]', '[ 0.0099677   0.14579835 -0.12877174 -0.23752332]', '[-0.02671453  0.11914618 -0.23135882 -0.03029568]', '[-0.07887305  0.13122166 -0.27923433  0.14079468]', '[-0.13346965  0.17000821 -0.25455054  0.23213127]', '[-0.17594228  0.2177196  -0.16032293  0.23074589]', '[-0.19440453  0.25720213 -0.01958413  0.15500349]', '[-0.18304473  0.2773318   0.13139765  0.04471749]', '[-0.14381952  0.27594314  0.25290378 -0.05262463]', '[-0.08610129  0.25997418  0.3121551  -0.09574381]', '[-0.02431919  0.24283739  0.29265156 -0.06321871]', '[0.025942   0.23936241 0.19971411 0.03691163]', '[0.05230735 0.25979636 0.05929573 0.16809359]', '[ 0.04903274  0.30520172 -0.08996005  0.27778487]', '[ 0.01840997  0.3660885  -0.20830118  0.31617897]', '[-0.03017518  0.42484365 -0.26613074  0.25434096]', '[-0.08310648  0.46114583 -0.25151672  0.09491522]', '[-0.12637105  0.45839229 -0.17234971 -0.12852159]', '[-0.14934542  0.40908444 -0.05391547 -0.3602991 ]', '[-0.14772278  0.3180918   0.0672533  -0.53461121]', '[-0.12479853  0.20317901  0.15370315 -0.59148689]', '[-0.09033116  0.09169889  0.18033911 -0.49864447]', '[-0.05698072  0.01310365  0.14398671 -0.26870757]', '[-0.03582515 -0.0101366   0.06271589  0.0432441 ]', '[-0.03284724  0.03064719 -0.03208739  0.35765344]', '[-0.04720001  0.12749223 -0.10517205  0.59129397]', '[-0.07155134  0.25739102 -0.12905439  0.6812098 ]', '[-0.09492447  0.388912   -0.09622775  0.60894699]', '[-0.10718747  0.49201057 -0.0218702   0.40512845]', '[-0.10272942  0.54605232  0.06611999  0.12900689]', '[-0.08173302  0.54308751  0.13927353 -0.15466602]', '[-0.04954254  0.48764289  0.17506264 -0.38695002]', '[-0.0151897   0.39500767  0.15952967 -0.52021901]', '[ 0.01060951  0.28814293  0.09044679 -0.52729481]', '[ 0.01822159  0.19237607 -0.01869241 -0.41316397]', '[ 0.00232707  0.12845925 -0.13896224 -0.21766133]', '[-0.03568997  0.10667803 -0.23409955 -0.00247033]', '[-0.08749173  0.12459123 -0.27282479  0.17041154]', '[-0.13991018  0.16905379 -0.23945127  0.25864832]']</t>
   </si>
   <si>
-    <t>['[2,2,2]', '[0,2,1]', '[2,0,1]', '[2,1,0]', '[1,2,0]', '[0,0,0]', '[1,0,2]', '[1,1,2]', '[0,1,1]', '[1,1,1]']</t>
+    <t>['[2,0,1]', '[1,2,0]', '[0,2,1]', '[0,1,1]', '[1,1,2]', '[2,1,0]', '[1,1,1]', '[2,2,2]', '[1,0,2]', '[0,0,0]']</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
all 5 domains working!!!!
</commit_message>
<xml_diff>
--- a/experimental results/e2000_Acrobot.xlsx
+++ b/experimental results/e2000_Acrobot.xlsx
@@ -85,7 +85,7 @@
     <t>Omitted</t>
   </si>
   <si>
-    <t>['[1,2,0]', '[0,1,1]', '[1,1,1]', '[1,1,2]', '[0,2,1]', '[2,1,0]', '[0,0,0]', '[1,0,2]', '[2,0,1]', '[2,2,2]']</t>
+    <t>['[1,1,2]', '[0,2,1]', '[2,1,0]', '[1,2,0]', '[0,0,0]', '[1,1,1]', '[0,1,1]', '[2,0,1]', '[1,0,2]', '[2,2,2]']</t>
   </si>
   <si>
     <t>[0,1,1]</t>
@@ -100,19 +100,19 @@
     <t>['[-0.03763371 -0.01533471  0.06554052 -0.01816017]', '[-0.00754409 -0.05458322  0.2277812  -0.36241836]', '[ 0.04879627 -0.15231473  0.32089719 -0.5887683 ]', '[ 0.11397169 -0.27767857  0.31375488 -0.63332862]', '[ 0.16759438 -0.39312519  0.2086893  -0.49480525]', '[ 0.1930193  -0.46685036  0.03906408 -0.22816919]', '[ 0.16956871 -0.44830261 -0.26820417  0.40739083]', '[ 0.09055011 -0.31127879 -0.50323119  0.93116007]', '[-0.02165415 -0.09380121 -0.58952709  1.1892161 ]', '[-0.13228272  0.13968862 -0.48657385  1.08703787]', '[-0.20542731  0.31962025 -0.22562708  0.67289162]', '[-0.21756752  0.39782756  0.10766541  0.09689063]', '[-0.15109606  0.32490126  0.54216963 -0.80657469]', '[-0.01068619  0.09081112  0.82714324 -1.47439182]', '[ 0.16212513 -0.23279107  0.85391345 -1.67375883]', '[ 0.3120332  -0.54339537  0.60708552 -1.36152952]', '[ 0.39322683 -0.75586146  0.18779451 -0.73014827]', '[ 0.38412465 -0.82793881 -0.27624305  0.01454459]', '[ 0.27552572 -0.72135137 -0.78884754  1.03160865]', '[ 0.08086773 -0.43032213 -1.11647003  1.81675029]', '[-0.14966877 -0.03109877 -1.12879696  2.06540623]', '[-0.3455444   0.34863759 -0.7784691   1.63534647]', '[-0.44544803  0.59424237 -0.19906427  0.77949316]', '[-0.4218337   0.6519398   0.43007126 -0.20572333]', '[-0.26769146  0.484052    1.08142007 -1.44055859]', '[-0.00742761  0.10113176  1.45927884 -2.28595201]', '[ 0.28490347 -0.37428385  1.38589424 -2.32532176]', '[ 0.5187101  -0.77937684  0.90230152 -1.64619583]', '[ 0.63240836 -1.01433747  0.21740989 -0.68198512]', '[ 0.59278756 -1.01958166 -0.60566507  0.62852481]', '[ 0.39752784 -0.7660208  -1.31595743  1.88179849]', '[ 0.08542661 -0.29020757 -1.73661998  2.76615566]', '[-0.26054486  0.27360101 -1.62803895  2.69265107]', '[-0.53183224  0.72525907 -1.02799868  1.73308445]', '[-0.65747495  0.94866122 -0.21116234  0.48419472]', '[-0.60316944  0.88713812  0.74646124 -1.09703619]', '[-0.3667148   0.51448679  1.5802398  -2.58584684]', '[ 2.25515542e-03 -1.04226788e-01  2.01052042e+00 -3.41515113e+00]', '[ 0.38981745 -0.75816996  1.76540261 -2.93947302]', '[ 0.67971886 -1.23563438  1.09061136 -1.79181237]', '[ 0.81522073 -1.47040276  0.25012952 -0.55613563]', '[ 0.76893557 -1.43299403 -0.70634091  0.93217091]', '[ 0.53890731 -1.09497955 -1.5685075   2.44803386]', '[ 0.15769536 -0.46498696 -2.17507038  3.75054866]', '[-0.28566374  0.31885175 -2.12308403  3.81427092]', '[-0.64333931  0.96714913 -1.38377582  2.55626676]', '[-0.82476188  1.32821982 -0.41497441  1.0541805 ]', '[-0.80769438  1.39053182  0.57925977 -0.43113385]', '[-0.58966747  1.12643161  1.57705339 -2.21920745]', '[-0.19115743  0.50615398  2.34648211 -3.90612928]']</t>
   </si>
   <si>
-    <t>['[0,1,1]', '[1,0,2]', '[2,0,1]', '[2,1,0]', '[1,1,1]', '[1,1,2]', '[0,0,0]', '[0,2,1]', '[1,2,0]', '[2,2,2]']</t>
+    <t>['[1,2,0]', '[1,0,2]', '[0,0,0]', '[1,1,1]', '[2,0,1]', '[2,2,2]', '[2,1,0]', '[0,1,1]', '[1,1,2]', '[0,2,1]']</t>
   </si>
   <si>
     <t>[0,2,1]</t>
   </si>
   <si>
-    <t>['[1,0,2]', '[1,2,0]', '[1,1,1]', '[2,1,0]', '[2,0,1]', '[0,1,1]', '[1,1,2]', '[2,2,2]', '[0,0,0]', '[0,2,1]']</t>
+    <t>['[2,1,0]', '[1,2,0]', '[1,1,1]', '[0,1,1]', '[1,0,2]', '[0,2,1]', '[2,2,2]', '[1,1,2]', '[2,0,1]', '[0,0,0]']</t>
   </si>
   <si>
     <t>[1,0,2]</t>
   </si>
   <si>
-    <t>['[0,0,0]', '[1,1,1]', '[1,0,2]', '[1,2,0]', '[2,2,2]', '[2,0,1]', '[0,2,1]', '[0,1,1]', '[1,1,2]', '[2,1,0]']</t>
+    <t>['[2,0,1]', '[1,1,1]', '[0,0,0]', '[2,2,2]', '[2,1,0]', '[1,1,2]', '[1,2,0]', '[0,1,1]', '[1,0,2]', '[0,2,1]']</t>
   </si>
   <si>
     <t>[1,2,0]</t>
@@ -127,7 +127,7 @@
     <t>['[-0.03763371 -0.01533471  0.06554052 -0.01816017]', '[-0.0208055  -0.02030166  0.09914155 -0.02801351]', '[ 0.00031733 -0.02489487  0.10765546 -0.0138725 ]', '[ 0.02044082 -0.02428802  0.08954248  0.02288616]', '[ 0.03470698 -0.01491644  0.05056501  0.07132823]', '[ 0.05326751 -0.03038784  0.13065223 -0.22021077]', '[ 0.07101291 -0.0640307   0.04229076 -0.10791836]', '[ 0.06919594 -0.07148833 -0.06018897  0.03411905]', '[ 0.06123949 -0.0858309  -0.01832924 -0.17605239]', '[ 0.04848925 -0.10546764 -0.10705552 -0.01913256]', '[ 0.03334023 -0.12873715 -0.04224633 -0.21160413]', '[ 0.01856077 -0.15355978 -0.1031453  -0.03494141]', '[ 0.00687968 -0.17764366 -0.01219475 -0.20332606]', '[ 0.00024918 -0.19823055 -0.05320561 -0.00041555]', '[-0.00038196 -0.21249406  0.04645807 -0.13967612]', '[ 0.00462703 -0.21766377  0.00256154  0.08939976]', '[ 0.01391452 -0.21184382  0.0884936  -0.03053848]', '[ 0.03850047 -0.22834148  0.15179103 -0.12764898]', '[ 0.05871339 -0.22531591  0.04642174  0.1602345 ]', '[ 0.06975736 -0.19972822  0.06255754  0.09301244]', '[ 0.08295526 -0.18863935  0.06709485  0.01801994]', '[ 0.0955466  -0.19194963  0.05618073 -0.04863014]', '[ 0.10438266 -0.20672312  0.02995667 -0.09524718]', '[ 0.10679076 -0.22835209 -0.00700287 -0.1170154 ]', '[ 0.10139245 -0.251988   -0.04658216 -0.11618468]', '[ 0.08862558 -0.27379536 -0.07912951 -0.10019242]', '[ 0.07079541 -0.2916811  -0.09605709 -0.07844699]', '[ 0.05160586 -0.30533224 -0.09231221 -0.05881123]', '[ 0.03527347 -0.31561531 -0.06796943 -0.04491109]', '[ 0.02545877 -0.32360191 -0.02840871 -0.03520182]', '[ 0.02431678 -0.32962124  0.01702803 -0.0241677 ]', '[ 0.03194057 -0.33273766  0.0575287  -0.00523763]', '[ 0.04635922 -0.33089406  0.08372791  0.02568935]', '[ 0.06409062 -0.32170512  0.09020522  0.06748616]', '[ 0.08108895 -0.30362649  0.07683704  0.11292955]', '[ 0.09381032 -0.27706452  0.04859846  0.15016487]', '[ 0.10008474 -0.24498455  0.01387843  0.16612946]', '[ 0.099545   -0.21272175 -0.0181427   0.15089341]', '[ 0.09350925 -0.18694889 -0.04018141  0.10151107]', '[ 0.08439395 -0.17403958 -0.04874136  0.02402904]', '[ 0.0748759  -0.17828815 -0.04468765 -0.06714713]', '[ 0.06707968 -0.2005238  -0.03244224 -0.15248501]', '[ 0.06204155 -0.23757011 -0.01810026 -0.2123621 ]', '[ 0.0596084  -0.28277818 -0.00709475 -0.23248464]', '[ 0.0587725  -0.32752505 -0.00232775 -0.20781714]', '[ 0.05826257 -0.3632139  -0.00355436 -0.1435367 ]', '[ 0.05712088 -0.38315408 -0.00807237 -0.05302107]', '[ 0.05506565 -0.38385601 -0.01204958  0.04571899]', '[ 0.05258562 -0.36558361 -0.01179826  0.13373731]', '[ 0.05080563 -0.3322004  -0.0047971   0.19451381]']</t>
   </si>
   <si>
-    <t>['[2,2,2]', '[1,2,0]', '[1,0,2]', '[1,1,2]', '[0,1,1]', '[1,1,1]', '[2,1,0]', '[0,0,0]', '[0,2,1]', '[2,0,1]']</t>
+    <t>['[1,2,0]', '[2,1,0]', '[0,0,0]', '[1,1,1]', '[0,1,1]', '[2,2,2]', '[1,0,2]', '[1,1,2]', '[0,2,1]', '[2,0,1]']</t>
   </si>
   <si>
     <t>[2,0,1]</t>
@@ -139,7 +139,7 @@
     <t>['[-0.03763371 -0.01533471  0.06554052 -0.01816017]', '[-0.03406929  0.01398622 -0.02953871  0.30651903]', '[-0.03493773  0.06836613  0.02265481  0.22789337]', '[-0.02479211  0.10222584  0.07768516  0.10663031]', '[-0.01808581  0.14469195 -0.0104571   0.31140101]', '[-0.01484609  0.18823383  0.0432976   0.11751461]', '[-0.01434726  0.22467153 -0.03717771  0.24054013]', '[-0.01545278  0.24682047  0.02676029 -0.02247913]', '[-0.01721181  0.25018444 -0.04380907  0.05514087]', '[-0.03213003  0.26757856 -0.10176092  0.11343711]', '[-0.04292178  0.2589368  -0.00427078 -0.19989973]', '[-0.04724582  0.22400641 -0.03910061 -0.1442553 ]', '[-0.05828925  0.20274667 -0.06971448 -0.06649573]', '[-0.07416359  0.19747218 -0.0859609   0.01216736]', '[-0.0912366   0.20638244 -0.08104733  0.07279687]', '[-0.10506889  0.22457911 -0.0539522   0.10400424]', '[-0.11166695  0.24587804 -0.010094    0.10444057]', '[-0.10867284  0.26478582  0.03995039  0.08196904]', '[-0.09613136  0.27802333  0.08328201  0.05013698]', '[-0.07660094  0.2851802   0.10825155  0.02324806]', '[-0.0545593   0.2883646   0.10777726  0.01147603]', '[-0.03525161  0.29099778  0.08146314  0.01741678]', '[-0.02329543  0.29616619  0.03584343  0.03525702]', '[-0.0214414   0.30511627 -0.01738635  0.05301171]', '[-0.02985137  0.31645556 -0.06464183  0.05714453]', '[-0.04610073  0.32638407 -0.09423766  0.03793816]', '[-0.06589513  0.32991089 -0.09957126 -0.0063193 ]', '[-0.08428464  0.32265766 -0.08080209 -0.06781655]', '[-0.09702234  0.30264881 -0.04459147 -0.13085587]', '[-0.10168093  0.27149627 -0.00200248 -0.17612255]', '[-0.09820986  0.23455768  0.03486443 -0.1864638 ]', '[-0.0887719   0.19991036  0.05652747 -0.1526692 ]', '[-0.076919    0.17632476  0.05888771 -0.07738584]', '[-0.06638826  0.1707868   0.04416262  0.02447002]', '[-0.05992123  0.18633723  0.01974774  0.1292307 ]', '[-0.0584844   0.22093296 -0.00454223  0.21092628]', '[-0.04805938  0.23384537  0.10680343 -0.08193806]', '[-0.03080471  0.22450229  0.06202129 -0.00733249]', '[-0.02430606  0.23182975  0.00194388  0.08025297]', '[-0.02987406  0.25554917 -0.05571698  0.1519643 ]', '[-0.03226718  0.25603978  0.03214881 -0.14722185]', '[-0.03092284  0.23283646 -0.01960446 -0.08080664]', '[-0.03999585  0.22459335 -0.06946922 -0.00175473]', '[-0.05757792  0.23128942 -0.10254152  0.0647801 ]', '[-0.06605782  0.21440088  0.01888208 -0.23192227]', '[-0.06398042  0.17583314  0.00028999 -0.14688162]', '[-0.06633966  0.15773225 -0.02393686 -0.03146107]', '[-0.07325426  0.16341223 -0.04358916  0.08612216]', '[-0.0828409   0.19044139 -0.04946038  0.17797922]', '[-0.07864045  0.19750911  0.09060325 -0.10746977]']</t>
   </si>
   <si>
-    <t>['[2,1,0]', '[0,2,1]', '[1,0,2]', '[2,2,2]', '[1,1,1]', '[1,2,0]', '[0,0,0]', '[1,1,2]', '[0,1,1]', '[2,0,1]']</t>
+    <t>['[0,0,0]', '[0,2,1]', '[1,1,2]', '[1,0,2]', '[1,2,0]', '[2,2,2]', '[2,0,1]', '[2,1,0]', '[1,1,1]', '[0,1,1]']</t>
   </si>
   <si>
     <t>[2,1,0]</t>
@@ -151,7 +151,7 @@
     <t>['[-0.03763371 -0.01533471  0.06554052 -0.01816017]', '[-0.03406929  0.01398622 -0.02953871  0.30651903]', '[-0.02168374  0.03409236  0.1512214  -0.10649158]', '[-0.00282652  0.04327343  0.03401407  0.19924661]', '[ 0.01834705  0.04294749  0.17317668 -0.19873753]', '[0.03659766 0.0372359  0.00569586 0.14498695]', '[ 0.04737447  0.03050982  0.09950876 -0.20907803]', '[ 0.04773513  0.02629209 -0.09583188  0.16718432]', '[ 0.03752505  0.02534768 -0.00439201 -0.17769188]', '[ 0.01910665  0.02614969 -0.17578652  0.18226832]', '[-0.00293854  0.02498097 -0.04044017 -0.19672323]', '[-0.02338561  0.01819528 -0.15991175  0.1265223 ]', '[-0.03744461  0.00328053  0.02144561 -0.27476369]', '[-0.04234133 -0.01910231 -0.06994388  0.05368665]', '[-0.03763269 -0.04539758  0.11498126 -0.31087136]', '[-0.02550263 -0.06918706  0.00335501  0.07846404]', '[-0.00968282 -0.08350681  0.15097012 -0.21632696]', '[ 0.0053941  -0.08236633 -0.00300315  0.22938636]', '[ 0.0161822  -0.06338321  0.10914378 -0.04087513]', '[ 0.02066644 -0.02828874 -0.063904    0.38603243]', '[0.01913681 0.01633736 0.05013034 0.05264949]', '[ 0.0400551  -0.0073938   0.15390054 -0.28229442]', '[ 0.05094132 -0.02216557 -0.04740575  0.1382459 ]', '[ 0.04870162 -0.02310954  0.02529389 -0.14757537]', '[ 0.03376547 -0.01028918 -0.17094986  0.2707556 ]', '[ 0.0103118   0.01075104 -0.05836816 -0.0672164 ]', '[ 0.01124463 -0.0370396   0.06579493 -0.4018725 ]', '[ 0.00803486 -0.07504962 -0.09809813  0.02722039]', '[ 1.51338775e-04 -9.62015886e-02  1.99960523e-02 -2.35938240e-01]', '[-0.01132378 -0.09750196 -0.13218554  0.22087768]', '[-0.02355496 -0.08096771  0.01267429 -0.05993836]', '[-0.0330696  -0.05205256 -0.10484912  0.34234137]', '[-0.03642324 -0.01860412  0.07279953 -0.01371334]', '[-0.03166866  0.01206933 -0.02509297  0.31554307]', '[-0.01874523  0.03436217  0.15211703 -0.09394883]', '[-5.13230523e-05  4.62105789e-02  3.16075962e-02  2.12883305e-01]', '[ 0.02039466  0.04845639  0.16853114 -0.18720539]', '[0.03762326 0.04455931 0.00038545 0.1511327 ]', '[ 0.04739711  0.03833294  0.09500645 -0.210463  ]', '[ 0.04703493  0.03301412 -0.09845059  0.15764597]', '[ 0.03651771  0.02945918 -0.00486237 -0.19385638]', '[ 0.01818744  0.02662077 -0.17457023  0.1626772 ]', '[-0.00352862  0.02154485 -0.03855204 -0.21548247]', '[-0.02362984  0.01145217 -0.1585124   0.11283283]', '[-0.03753204 -0.00542412  0.02151977 -0.28032934]', '[-0.0425714  -0.02799292 -0.07141092  0.05738308]', '[-0.03827598 -0.05268781  0.11245074 -0.2989076 ]', '[-0.02666782 -0.07350228  0.00086365  0.09565699]', '[-0.01124264 -0.08418115  0.14971078 -0.19780414]', '[ 0.00379227 -0.07954607 -0.00205983  0.24522416]']</t>
   </si>
   <si>
-    <t>['[2,1,0]', '[1,0,2]', '[2,2,2]', '[1,1,1]', '[0,0,0]', '[1,2,0]', '[0,2,1]', '[1,1,2]', '[2,0,1]', '[0,1,1]']</t>
+    <t>['[1,1,2]', '[2,0,1]', '[2,2,2]', '[1,0,2]', '[1,1,1]', '[0,1,1]', '[2,1,0]', '[0,2,1]', '[0,0,0]', '[1,2,0]']</t>
   </si>
   <si>
     <t>[0,0,0]</t>
@@ -166,7 +166,7 @@
     <t>['[-0.03763371 -0.01533471  0.06554052 -0.01816017]', '[-0.00754409 -0.05458322  0.2277812  -0.36241836]', '[ 0.04879627 -0.15231473  0.32089719 -0.5887683 ]', '[ 0.11397169 -0.27767857  0.31375488 -0.63332862]', '[ 0.16759438 -0.39312519  0.2086893  -0.49480525]', '[ 0.1930193  -0.46685036  0.03906408 -0.22816919]', '[ 0.18217995 -0.48119372 -0.14531723  0.08492936]', '[ 0.13737799 -0.43548032 -0.29255645  0.35879992]', '[ 0.07059687 -0.34553749 -0.35944697  0.51636187]', '[ 0.00066518 -0.24025206 -0.32266973  0.50804924]', '[-0.05184718 -0.15356453 -0.18924715  0.33585339]', '[-0.07099568 -0.11316     0.00267821  0.05860212]', '[-0.0506235  -0.13098626  0.19609592 -0.23012254]', '[ 0.00363944 -0.19947979  0.33317766 -0.43407441]', '[ 0.07604673 -0.29425756  0.37330708 -0.48624983]', '[ 0.14566012 -0.38269974  0.30650217 -0.37362319]', '[ 0.19284616 -0.43524651  0.15487527 -0.13746415]', '[ 0.20480978 -0.43420274 -0.03738189  0.14899985]', '[ 0.17872861 -0.37781944 -0.21671607  0.40226469]', '[ 0.12244395 -0.28089207 -0.33207824  0.54289906]', '[ 0.05262627 -0.17207597 -0.34864539  0.51601465]', '[-0.00991093 -0.08621824 -0.26142967  0.31808955]', '[-0.04676022 -0.05276175 -0.09876284  0.00534115]', '[-0.04773189 -0.08549506  0.08793289 -0.326671  ]', '[-0.01386808 -0.17774148  0.24064044 -0.5740393 ]', '[ 0.04305734 -0.30394484  0.31308665 -0.65740151]', '[ 0.10464298 -0.42784083  0.2871402  -0.55250711]', '[ 0.15213765 -0.51456341  0.17665722 -0.29545229]', '[ 0.17195601 -0.54054882  0.01729499  0.04161741]', '[ 0.15877658 -0.49810034 -0.14558791  0.37488532]', '[ 0.11662491 -0.39653924 -0.26514127  0.61927065]', '[ 0.05830606 -0.26143591 -0.30243069  0.70071627]', '[ 0.00240191 -0.12975114 -0.241122    0.58472722]', '[-0.03255824 -0.03901385 -0.09863914  0.30169722]', '[-0.03459084 -0.01467301  0.07923617 -0.06234707]', '[-0.00228999 -0.06214743  0.23549293 -0.3987235 ]', '[ 0.05469493 -0.16555079  0.31932445 -0.60811377]', '[ 0.11857421 -0.29274507  0.30262565 -0.63232462]', '[ 0.16925182 -0.40618487  0.19109743 -0.47671256]', '[ 0.19093562 -0.47518295  0.02014588 -0.20033382]', '[ 0.17663487 -0.48368374 -0.16020096  0.11418666]', '[ 0.12963404 -0.4326335  -0.2991053   0.38177157]', '[ 0.06259366 -0.33924046 -0.35533189  0.52721541]', '[-0.00545982 -0.23320565 -0.30834707  0.50479686]', '[-0.05435734 -0.14835926 -0.16821515  0.32158817]', '[-0.0690908  -0.1113463   0.02479252  0.04024292]', '[-0.04470101 -0.1325791   0.21323988 -0.24461353]', '[ 0.01207873 -0.20303341  0.340642   -0.43848531]', '[ 0.08482177 -0.29746838  0.36917508 -0.47850826]', '[ 0.1525418  -0.38334874  0.2921883  -0.35655192]']</t>
   </si>
   <si>
-    <t>['[2,0,1]', '[0,1,1]', '[1,1,1]', '[1,1,2]', '[2,2,2]', '[1,0,2]', '[0,0,0]', '[0,2,1]', '[2,1,0]', '[1,2,0]']</t>
+    <t>['[0,1,1]', '[2,2,2]', '[2,1,0]', '[0,0,0]', '[1,0,2]', '[0,2,1]', '[1,1,2]', '[2,0,1]', '[1,1,1]', '[1,2,0]']</t>
   </si>
   <si>
     <t>[1,1,1]</t>
@@ -178,7 +178,7 @@
     <t>['[-0.03763371 -0.01533471  0.06554052 -0.01816017]', '[-0.0208055  -0.02030166  0.09914155 -0.02801351]', '[ 0.00031733 -0.02489487  0.10765546 -0.0138725 ]', '[ 0.02044082 -0.02428802  0.08954248  0.02288616]', '[ 0.03470698 -0.01491644  0.05056501  0.07132823]', '[0.04000421 0.0038992  0.00197135 0.11431592]', '[ 0.0357442   0.02924956 -0.04287984  0.13410557]', '[ 0.02389303  0.05513259 -0.0724118   0.11843067]', '[ 0.00827151  0.0740515  -0.08006316  0.06513577]', '[-0.00664229  0.07925492 -0.06591977 -0.01622081]', '[-0.01703829  0.06693573 -0.03635037 -0.10637005]', '[-0.02083887  0.0377102  -0.00183146 -0.18135846]', '[-0.01819393 -0.00310741  0.02644173 -0.21931589]', '[-0.0112553  -0.04661351  0.04018081 -0.20717791]', '[-0.00330983 -0.08257268  0.03658645 -0.14508251]', '[ 0.0024104  -0.10215919  0.01891064 -0.04666104]', '[ 0.00382015 -0.10033648 -0.00499775  0.06469207]', '[ 0.00064351 -0.07722007 -0.02539101  0.16195768]', '[-0.00551959 -0.03811088 -0.03377164  0.22142738]', '[-0.01174627  0.0078305  -0.02581131  0.22911312]', '[-0.01482841  0.04999004 -0.00311123  0.18480626]', '[-0.01246489  0.07911924  0.02710494  0.10195664]', '[-0.00417355  0.08968453  0.05438991  0.00327931]', '[ 0.00840543  0.08106163  0.06855001 -0.08601484]', '[ 0.02190299  0.05733301  0.06295851 -0.14509547]', '[ 0.0321837   0.02584205  0.03681891 -0.16284223]', '[ 0.03560428 -0.00505404 -0.00421667 -0.14034077]', '[ 0.03020079 -0.02836988 -0.04938897 -0.08972441]', '[ 0.01642725 -0.04029751 -0.08587168 -0.02970417]', '[-0.00281086 -0.04091095 -0.10259647  0.020656  ]', '[-0.02286552 -0.03361943 -0.09365837  0.04790331]', '[-0.03860246 -0.0236106  -0.06024324  0.04807679]', '[-0.04583902 -0.01583448 -0.01046864  0.02730739]', '[-0.04253854 -0.01321526  0.0428277  -0.00097241]', '[-0.02940859 -0.0156797   0.08568823 -0.02115895]', '[-0.00972652 -0.02030416  0.1069775  -0.02123067]', '[ 0.0115618  -0.02251874  0.10152992  0.00272141]', '[ 0.02921079 -0.01796026  0.07156041  0.04472731]', '[ 0.03910994 -0.00433545  0.02589999  0.09061009]', '[ 0.03936403  0.01735836 -0.02268767  0.12255506]', '[ 0.03071193  0.04269742 -0.06126398  0.1251015 ]', '[ 0.01618133  0.06487999 -0.08040737  0.09068004]', '[ 0.00010594  0.07668079 -0.07674355  0.02287818]', '[-0.0131837   0.07272569 -0.05361425 -0.06371658]', '[-0.02060331  0.05138348 -0.0197783  -0.14709165]', '[-0.0211313   0.01567674  0.01345636 -0.20383146]', '[-0.01595742 -0.02713289  0.03588002 -0.21605443]', '[-0.00791991 -0.06726788  0.0416368  -0.17718674]', '[-0.00043664 -0.09500666  0.03087284 -0.0943888 ]', '[ 0.00368075 -0.10331248  0.0092639   0.01327487]']</t>
   </si>
   <si>
-    <t>['[2,2,2]', '[0,1,1]', '[1,2,0]', '[0,2,1]', '[0,0,0]', '[1,1,1]', '[1,1,2]', '[2,0,1]', '[1,0,2]', '[2,1,0]']</t>
+    <t>['[0,0,0]', '[1,0,2]', '[1,2,0]', '[0,1,1]', '[1,1,1]', '[2,1,0]', '[2,0,1]', '[1,1,2]', '[2,2,2]', '[0,2,1]']</t>
   </si>
   <si>
     <t>[2,2,2]</t>
@@ -193,7 +193,7 @@
     <t>['[-0.03763371 -0.01533471  0.06554052 -0.01816017]', '[-0.03406929  0.01398622 -0.02953871  0.30651903]', '[-0.04818188  0.10262173 -0.10566927  0.56184435]', '[-0.07305261  0.22936701 -0.13369446  0.67944384]', '[-0.0976443   0.36319498 -0.10327727  0.63282133]', '[-0.11125897  0.47297074 -0.02773051  0.446438  ]', '[-0.10757465  0.53619101  0.06462001  0.17794954]', '[-0.08631261  0.54305113  0.14348542 -0.10660175]', '[-0.05272941  0.496551    0.18460856 -0.34656399]', '[-0.01604448  0.4107609   0.17301646 -0.49290646]', '[ 0.01268242  0.3077355   0.10583916 -0.51655332]', '[ 0.02333646  0.21239857 -0.00419223 -0.4193517 ]', '[ 0.0099677   0.14579835 -0.12877174 -0.23752332]', '[-0.02671453  0.11914618 -0.23135882 -0.03029568]', '[-0.07887305  0.13122166 -0.27923433  0.14079468]', '[-0.13346965  0.17000821 -0.25455054  0.23213127]', '[-0.17594228  0.2177196  -0.16032293  0.23074589]', '[-0.19440453  0.25720213 -0.01958413  0.15500349]', '[-0.18304473  0.2773318   0.13139765  0.04471749]', '[-0.14381952  0.27594314  0.25290378 -0.05262463]', '[-0.08610129  0.25997418  0.3121551  -0.09574381]', '[-0.02431919  0.24283739  0.29265156 -0.06321871]', '[0.025942   0.23936241 0.19971411 0.03691163]', '[0.05230735 0.25979636 0.05929573 0.16809359]', '[ 0.04903274  0.30520172 -0.08996005  0.27778487]', '[ 0.01840997  0.3660885  -0.20830118  0.31617897]', '[-0.03017518  0.42484365 -0.26613074  0.25434096]', '[-0.08310648  0.46114583 -0.25151672  0.09491522]', '[-0.12637105  0.45839229 -0.17234971 -0.12852159]', '[-0.14934542  0.40908444 -0.05391547 -0.3602991 ]', '[-0.14772278  0.3180918   0.0672533  -0.53461121]', '[-0.12479853  0.20317901  0.15370315 -0.59148689]', '[-0.09033116  0.09169889  0.18033911 -0.49864447]', '[-0.05698072  0.01310365  0.14398671 -0.26870757]', '[-0.03582515 -0.0101366   0.06271589  0.0432441 ]', '[-0.03284724  0.03064719 -0.03208739  0.35765344]', '[-0.04720001  0.12749223 -0.10517205  0.59129397]', '[-0.07155134  0.25739102 -0.12905439  0.6812098 ]', '[-0.09492447  0.388912   -0.09622775  0.60894699]', '[-0.10718747  0.49201057 -0.0218702   0.40512845]', '[-0.10272942  0.54605232  0.06611999  0.12900689]', '[-0.08173302  0.54308751  0.13927353 -0.15466602]', '[-0.04954254  0.48764289  0.17506264 -0.38695002]', '[-0.0151897   0.39500767  0.15952967 -0.52021901]', '[ 0.01060951  0.28814293  0.09044679 -0.52729481]', '[ 0.01822159  0.19237607 -0.01869241 -0.41316397]', '[ 0.00232707  0.12845925 -0.13896224 -0.21766133]', '[-0.03568997  0.10667803 -0.23409955 -0.00247033]', '[-0.08749173  0.12459123 -0.27282479  0.17041154]', '[-0.13991018  0.16905379 -0.23945127  0.25864832]']</t>
   </si>
   <si>
-    <t>['[2,0,1]', '[1,2,0]', '[0,2,1]', '[0,1,1]', '[1,1,2]', '[2,1,0]', '[1,1,1]', '[2,2,2]', '[1,0,2]', '[0,0,0]']</t>
+    <t>['[2,2,2]', '[1,1,1]', '[2,1,0]', '[0,1,1]', '[1,2,0]', '[0,2,1]', '[1,1,2]', '[1,0,2]', '[0,0,0]', '[2,0,1]']</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
running the diagnosers on all domain at once(one run)
</commit_message>
<xml_diff>
--- a/experimental results/e2000_Acrobot.xlsx
+++ b/experimental results/e2000_Acrobot.xlsx
@@ -70,13 +70,13 @@
     <t>[1,1,2]</t>
   </si>
   <si>
-    <t>[1, 4, 15, 16, 24, 38]</t>
+    <t>[5, 13, 14, 24, 27, 29, 37, 38, 39]</t>
   </si>
   <si>
     <t>[0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2]</t>
   </si>
   <si>
-    <t>['[-0.03763371 -0.01533471  0.06554052 -0.01816017]', '[-0.0208055  -0.02030166  0.09914155 -0.02801351]', '[ 0.013578   -0.05917353  0.23628798 -0.34824344]', '[ 0.06892075 -0.15170277  0.30283362 -0.5520916 ]', '[ 0.11515941 -0.23443406  0.14815184 -0.25506525]', '[ 0.13822875 -0.28236976  0.07656364 -0.21295299]', '[ 0.1179771  -0.2482854  -0.27388843  0.54506357]', '[ 0.03407028 -0.07424812 -0.54313959  1.15343002]', '[-0.08728008  0.18979764 -0.63607919  1.41949992]', '[-0.20569864  0.46457017 -0.51593237  1.2644306 ]', '[-0.28280147  0.67407475 -0.23709283  0.79359124]', '[-0.29626065  0.77223731  0.10476863  0.17701578]', '[-0.21916201  0.68226536  0.65165076 -1.061654  ]', '[-0.04512692  0.36068418  1.05233646 -2.09312363]', '[ 0.18063642 -0.11545932  1.14016442 -2.53979527]', '[ 0.3699611  -0.5657639   0.70251815 -1.86344122]', '[ 0.44877344 -0.83568417  0.07276185 -0.80583241]', '[ 0.41030891 -0.91334474 -0.44856683  0.03161569]', '[ 0.25398773 -0.76577238 -1.08611847  1.4218266 ]', '[-0.00841868 -0.36263534 -1.48407107  2.52593652]', '[-0.31005874  0.19086811 -1.44762018  2.84534134]', '[-0.55370289  0.71047649 -0.92757486  2.23803462]', '[-0.66534848  1.05933366 -0.17152706  1.21933352]', '[-0.62140013  1.1923895   0.59951271  0.10642023]', '[-0.42486072  1.07473977  1.33043353 -1.27059501]', '[-0.09628454  0.66562873  1.90029916 -2.76265123]', '[ 0.30461496  0.01820045  2.00748203 -3.51862549]', '[ 0.65996426 -0.64905449  1.45272745 -2.97760432]', '[ 0.86105941 -1.1328467   0.52849421 -1.82244158]', '[ 0.86702079 -1.37265472 -0.46449574 -0.56774881]', '[ 0.66414294 -1.30398147 -1.5296024   1.26245193]', '[ 0.27309377 -0.86619371 -2.32594131  3.08906035]', '[-0.23481596 -0.10905973 -2.63448948  4.2573723 ]', '[-0.71874659  0.70849803 -2.07678307  3.66621379]', '[-1.0339395   1.30826952 -1.03967102  2.30859554]', '[-1.12837895  1.63547813  0.0987913   0.96968526]', '[-0.98103507  1.64564019  1.35118502 -0.88525679]', '[-0.60143957  1.26891544  2.40304875 -2.9125115 ]', '[-0.05239954  0.51216854  2.99758566 -4.52664942]', '[ 0.54950821 -0.45107486  2.84002846 -4.71484942]', '[ 1.02475987 -1.25648372  1.84444009 -3.25244109]', '[ 1.27635515 -1.7584952   0.65970826 -1.80084386]', '[ 1.28695765 -1.98448709 -0.55010167 -0.4580834 ]', '[ 1.04733838 -1.88972881 -1.81707934  1.43946147]', '[ 0.57649889 -1.38962507 -2.84503468  3.61059294]', '[-0.06940546 -0.44149675 -3.51891114  5.71635996]', '[-0.75041903  0.71587907 -3.07303022  5.36823635]', '[-1.24680721  1.60901675 -1.85574513  3.57040065]', '[-1.48935524  2.17108929 -0.56739794  2.09946583]', '[-1.47465687  2.45649337  0.70727483  0.750517  ]']</t>
+    <t>['[-0.03763371 -0.01533471  0.06554052 -0.01816017]', '[-0.00754409 -0.05458322  0.2277812  -0.36241836]', '[ 0.04879627 -0.15231473  0.32089719 -0.5887683 ]', '[ 0.11397169 -0.27767857  0.31375488 -0.63332862]', '[ 0.16759438 -0.39312519  0.2086893  -0.49480525]', '[ 0.18032045 -0.433785   -0.08419275  0.09486206]', '[ 0.12250785 -0.32368513 -0.48062135  0.98306352]', '[-0.0026532  -0.0576791  -0.73786728  1.61315786]', '[-0.15569205  0.28812154 -0.74791263  1.75564662]', '[-0.28439809  0.60982906 -0.50547922  1.39401027]', '[-0.34808837  0.82588565 -0.11870143  0.73725516]', '[-0.33033207  0.89847328  0.29123987 -0.01436865]', '[-0.21371037  0.76211052  0.85422685 -1.32992637]', '[-0.01306216  0.41445768  1.1092229  -2.07536275]', '[ 0.20768429 -0.02702233  1.03707177 -2.22056349]', '[ 0.39013361 -0.45885317  0.73469611 -1.99245525]', '[ 0.48515422 -0.791067    0.19288394 -1.27924134]', '[ 0.46396362 -0.95887522 -0.39896662 -0.38726726]', '[ 0.31071067 -0.88706591 -1.10271128  1.08907369]', '[ 0.03890086 -0.5365138  -1.56440571  2.35183692]', '[-0.28768412  0.00861982 -1.61764924  2.94233142]', '[-0.57112143  0.56865097 -1.14138755  2.51590233]', '[-0.72287938  0.97774716 -0.3488129   1.5291976 ]', '[-0.70676035  1.17136069  0.50397344  0.39637365]', '[-0.51908221  1.10660202  1.33868612 -1.03869825]', '[-0.17869253  0.73395249  2.00900441 -2.64119566]', '[ 0.25383473  0.0935061   2.21318942 -3.5736217 ]', '[ 0.64402334 -0.56380593  1.59079264 -2.8150723 ]', '[ 0.87654456 -1.02333266  0.6986247  -1.73599432]', '[ 0.90662012 -1.2241212  -0.39585969 -0.26912414]', '[ 0.71360853 -1.10002319 -1.50849214  1.52137894]', '[ 0.31846098 -0.61489997 -2.38524174  3.28241948]', '[-0.20182372  0.15140671 -2.67795254  4.10571783]', '[-0.69074124  0.9018933  -2.10173992  3.20384203]', '[-1.01703235  1.40387157 -1.12833333  1.81372961]', '[-1.13474653  1.63409095 -0.04106623  0.50013317]', '[-1.01708295  1.55469032  1.20561177 -1.31213516]', '[-0.66990604  1.12191425  2.23417229 -3.03874045]', '[-0.14420774  0.34866848  2.92617065 -4.53958035]', '[ 0.43513086 -0.5596842   2.69624376 -4.18618052]', '[ 0.89619189 -1.26389987  1.84848607 -2.78144424]', '[ 1.16072938 -1.67500589  0.7777373  -1.35592063]', '[ 1.20325608 -1.81418891 -0.35366023 -0.0406116 ]', '[ 1.00643927 -1.6395118  -1.5970108   1.8193817 ]', '[ 0.5743302  -1.06715635 -2.69271753  3.94409141]', '[-0.04661858 -0.08053341 -3.37430879  5.6387053 ]', '[-0.68484031  0.98716664 -2.83230461  4.67114037]', '[-1.1467314   1.74375727 -1.75691877  2.92735477]', '[-1.38094579  2.18047104 -0.57529514  1.47908818]', '[-1.37552703  2.34232058  0.62589856  0.13799569]']</t>
   </si>
   <si>
     <t>[0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49]</t>
@@ -85,40 +85,43 @@
     <t>Omitted</t>
   </si>
   <si>
-    <t>['[0,2,1]', '[0,1,1]', '[2,1,0]', '[1,1,2]', '[2,0,1]', '[0,0,0]', '[2,2,2]', '[1,1,1]', '[1,2,0]', '[1,0,2]']</t>
-  </si>
-  <si>
-    <t>[5, 14, 27, 28, 41]</t>
-  </si>
-  <si>
-    <t>['[-0.03763371 -0.01533471  0.06554052 -0.01816017]', '[-0.00754409 -0.05458322  0.2277812  -0.36241836]', '[ 0.04879627 -0.15231473  0.32089719 -0.5887683 ]', '[ 0.11397169 -0.27767857  0.31375488 -0.63332862]', '[ 0.16759438 -0.39312519  0.2086893  -0.49480525]', '[ 0.18032045 -0.433785   -0.08419275  0.09486206]', '[ 0.12250785 -0.32368513 -0.48062135  0.98306352]', '[-0.0026532  -0.0576791  -0.73786728  1.61315786]', '[-0.15569205  0.28812154 -0.74791263  1.75564662]', '[-0.28439809  0.60982906 -0.50547922  1.39401027]', '[-0.34808837  0.82588565 -0.11870143  0.73725516]', '[-0.33033207  0.89847328  0.29123987 -0.01436865]', '[-0.21371037  0.76211052  0.85422685 -1.32992637]', '[-6.04615643e-04  3.81890563e-01  1.23359692e+00 -2.40090220e+00]', '[ 0.24170486 -0.11753363  1.1192689  -2.45461729]', '[ 0.43286964 -0.57974267  0.73852326 -2.06102399]', '[ 0.52190705 -0.91201383  0.13379273 -1.22050478]', '[ 0.48502013 -1.05946034 -0.49247594 -0.24772846]', '[ 0.31232623 -0.95500407 -1.20120887  1.27559033]', '[ 0.02121832 -0.56261954 -1.65726572  2.58091815]', '[-0.32180581  0.02875101 -1.68332262  3.16086554]', '[-0.61263261  0.62423486 -1.14729286  2.64710958]', '[-0.75982177  1.0516581  -0.2998286   1.58615255]', '[-0.72989355  1.25108087  0.58991433  0.39871502]', '[-0.51375358  1.15469924  1.53259064 -1.36000014]', '[-0.1364157   0.71334348  2.18027085 -2.99873448]', '[ 0.32426056  0.00782679  2.31100497 -3.8335724 ]', '[ 0.72215053 -0.68024253  1.57331498 -2.87223832]', '[ 0.93214377 -1.11084666  0.50418262 -1.41774325]', '[ 0.93117775 -1.27436571 -0.51130402 -0.20947362]', '[ 0.71395373 -1.13528756 -1.63212124  1.61440628]', '[ 0.29481618 -0.62727672 -2.49834772  3.41599514]', '[-0.24474897  0.16531669 -2.7513705   4.21866266]', '[-0.74222742  0.93068811 -2.11533865  3.24385209]', '[-1.06687521  1.43780397 -1.10124855  1.83218596]', '[-1.17625074  1.67154119  0.01380772  0.5169844 ]', '[-1.04575699  1.59517783  1.27761288 -1.30140311]', '[-0.67368679  1.13529749  2.41450271 -3.33761204]', '[-0.09899114  0.26375103  3.22682177 -5.19711432]', '[ 0.5387482  -0.77452088  2.95723427 -4.76973184]', '[ 1.03648319 -1.55979147  1.97279972 -3.06767264]', '[ 1.31031297 -1.9971291   0.75449936 -1.35695328]', '[ 1.34329141 -2.13553963 -0.42489504 -0.03110354]', '[ 1.12944568 -1.96049005 -1.69528939  1.81636161]', '[ 0.67596069 -1.38645109 -2.80984863  3.99287586]', '[ 0.02081792 -0.35045873 -3.64018299  6.192229  ]', '[-0.68590685  0.87721814 -3.19393607  5.56425745]', '[-1.20994732  1.79371836 -2.01938171  3.64100031]', '[-1.48998403  2.3658945  -0.77631339  2.13653933]', '[-1.5207052   2.65846736  0.4643568   0.79261747]']</t>
-  </si>
-  <si>
-    <t>['[2,0,1]', '[1,1,1]', '[1,1,2]', '[1,0,2]', '[2,2,2]', '[2,1,0]', '[0,1,1]', '[0,0,0]', '[0,2,1]', '[1,2,0]']</t>
-  </si>
-  <si>
-    <t>[1, 14, 15, 17, 18, 25, 27, 37, 38, 39, 40, 41, 42]</t>
+    <t>['[1,1,1]', '[1,2,0]', '[0,0,0]', '[0,2,1]', '[2,2,2]', '[2,1,0]', '[2,0,1]', '[1,0,2]', '[1,1,2]', '[0,1,1]']</t>
+  </si>
+  <si>
+    <t>[1, 5, 12, 13, 17, 24, 25, 26, 37, 38]</t>
+  </si>
+  <si>
+    <t>[0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2]</t>
+  </si>
+  <si>
+    <t>['[-0.03763371 -0.01533471  0.06554052 -0.01816017]', '[-0.0208055  -0.02030166  0.09914155 -0.02801351]', '[ 0.013578   -0.05917353  0.23628798 -0.34824344]', '[ 0.06892075 -0.15170277  0.30283362 -0.5520916 ]', '[ 0.12827063 -0.26838081  0.27505366 -0.58564774]', '[ 0.16005875 -0.34102171  0.03515865 -0.12569461]', '[ 0.12853775 -0.28300606 -0.34263689  0.69246565]', '[ 0.02967829 -0.07631626 -0.62005388  1.32504849]', '[-0.10564872  0.22004567 -0.69460559  1.56224911]', '[-0.23208332  0.51676422 -0.53579303  1.3377179 ]', '[-0.30900866  0.7334938  -0.21638168  0.7941777 ]', '[-0.31501811  0.82566317  0.156575    0.1190051 ]', '[-0.23750226  0.75099658  0.60325536 -0.85072398]', '[-0.08298687  0.49711852  0.91003804 -1.63907803]', '[ 0.12265963  0.09091861  1.09390898 -2.32362117]', '[ 0.32881192 -0.38142538  0.90568156 -2.2756498 ]', '[ 0.46367573 -0.77710132  0.4095873  -1.61299379]', '[ 0.47477062 -0.98076239 -0.29514881 -0.41292219]', '[ 0.34084809 -0.91324701 -1.01762983  1.07492436]', '[ 0.0818871  -0.56195478 -1.52515881  2.37990972]', '[-0.24303731 -0.00416086 -1.64013237  3.040046  ]', '[-0.5357243   0.57904398 -1.20676249  2.63983209]', '[-0.70282833  1.01166961 -0.43453474  1.6381467 ]', '[-0.70495168  1.22546242  0.40900319  0.49028193]', '[-0.53640901  1.17883793  1.24489994 -0.95246344]', '[-0.22399901  0.8506048   1.82630908 -2.2882549 ]', '[ 0.16676089  0.29843272  1.99496693 -3.08662181]', '[ 0.54516869 -0.33788776  1.68687868 -3.07767297]', '[ 0.80713697 -0.86943885  0.88085155 -2.1544754 ]', '[ 0.88640351 -1.18491784 -0.09684611 -0.98443447]', '[ 0.75116803 -1.20400457 -1.23087826  0.80088335]', '[ 0.40845991 -0.86143661 -2.14777411  2.61068071]', '[-0.07984377 -0.18911461 -2.62888406  3.92914164]', '[-0.58442443  0.59263135 -2.28027515  3.61745498]', '[-0.95313317  1.19193229 -1.35699202  2.32676337]', '[-1.11703279  1.52434319 -0.27053057  1.00864581]', '[-1.06059274  1.5965353   0.82659518 -0.29611822]', '[-0.78553304  1.37278768  1.89231952 -1.96671372]', '[-0.32127725  0.8040203   2.68935024 -3.68438387]', '[ 0.26302277 -0.0723039   3.00077888 -4.76693326]', '[ 0.80597244 -0.94717219  2.30387825 -3.74568493]', '[ 1.15975305 -1.54388019  1.20761785 -2.23869348]', '[ 1.28377556 -1.85491045  0.02772143 -0.88844813]', '[ 1.1570284  -1.85295144 -1.27916139  0.92780817]', '[ 0.78226747 -1.46755133 -2.43552144  2.97927757]', '[ 0.19879323 -0.64415    -3.33531188  5.20164079]', '[-0.4905885   0.48781561 -3.33318491  5.61033624]', '[-1.0601712   1.4427128  -2.29091502  3.85174175]', '[-1.39820503  2.04904316 -1.07930134  2.27434382]', '[-1.48989052  2.36822477  0.16220847  0.93071683]']</t>
+  </si>
+  <si>
+    <t>['[0,2,1]', '[1,0,2]', '[1,1,1]', '[1,2,0]', '[2,2,2]', '[2,0,1]', '[0,1,1]', '[1,1,2]', '[2,1,0]', '[0,0,0]']</t>
+  </si>
+  <si>
+    <t>[1, 13, 14, 15, 16, 18, 27, 28, 30, 37]</t>
   </si>
   <si>
     <t>[0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2]</t>
   </si>
   <si>
-    <t>['[-0.03763371 -0.01533471  0.06554052 -0.01816017]', '[-0.0208055  -0.02030166  0.09914155 -0.02801351]', '[ 0.013578   -0.05917353  0.23628798 -0.34824344]', '[ 0.06892075 -0.15170277  0.30283362 -0.5520916 ]', '[ 0.12827063 -0.26838081  0.27505366 -0.58564774]', '[ 0.17298396 -0.37457441  0.16029766 -0.45268231]', '[ 0.188802   -0.44173166 -0.00664011 -0.2067265 ]', '[ 0.14464221 -0.38858741 -0.42504594  0.72477497]', '[ 0.02643202 -0.16436732 -0.72802709  1.4651372 ]', '[-0.13092325  0.16780439 -0.80101595  1.7696025 ]', '[-0.27519234  0.50644059 -0.6020908   1.53833469]', '[-0.35920157  0.75822894 -0.21924396  0.93976015]', '[-0.35930747  0.87273767  0.21689617  0.19605851]', '[-0.25348107  0.77646099  0.82144553 -1.14283881]', '[-0.05465969  0.4612335   1.12541342 -1.94581117]', '[ 0.17512314  0.03590608  1.11144457 -2.19263201]', '[ 0.37743137 -0.40028838  0.8543076  -2.05727108]', '[ 0.48591639 -0.71855627  0.20802987 -1.07884813]', '[ 0.45790368 -0.82266823 -0.48062911  0.0428792 ]', '[ 0.28958928 -0.67326982 -1.1713832   1.42632382]', '[ 0.0071858  -0.27298606 -1.59147313  2.48175576]', '[-0.3145619   0.26143879 -1.53822868  2.6974833 ]', '[-0.57481012  0.74449315 -1.00514516  2.03217664]', '[-0.70123236  1.05140986 -0.24039726  1.01115973]', '[-0.66892032  1.14414453  0.5557593  -0.08820721]', '[-0.47621501  0.98795591  1.3400341  -1.46316247]', '[-0.1387341   0.54007155  1.97655985 -2.94674688]', '[ 0.26638368 -0.09796491  1.96528529 -3.22424987]', '[ 0.61599924 -0.69780096  1.44647283 -2.6231603 ]', '[ 0.82252357 -1.11390579  0.58947938 -1.50620629]', '[ 0.84655227 -1.29590943 -0.34867061 -0.30821795]', '[ 0.66865    -1.18049288 -1.40467913  1.47028026]', '[ 0.29908838 -0.70707175 -2.239513    3.22719433]', '[-0.19324524  0.05901942 -2.55469195  4.18180481]', '[-0.66110361  0.83969648 -2.00847166  3.40885764]', '[-0.96939722  1.38572535 -1.04167575  2.03910355]', '[-1.07115981  1.65976805  0.02922339  0.70956553]', '[-0.95145287  1.64464475  1.15026028 -0.87310519]', '[-0.62245033  1.30197892  2.10143605 -2.57176031]', '[-0.13112088  0.61907602  2.73758746 -4.16839238]', '[ 0.42191483 -0.26924701  2.62998693 -4.37306848]', '[ 0.86207059 -1.01142415  1.69292912 -2.92521111]', '[ 1.08537875 -1.4337463   0.52708944 -1.31651361]', '[ 1.08048135 -1.56854054 -0.57256191 -0.02738184]', '[ 0.84451914 -1.38785849 -1.76126824  1.86341523]', '[ 0.3900425  -0.81100155 -2.73408994  3.89523774]', '[-0.2119742   0.11480374 -3.12338038  5.02561755]', '[-0.78107243  1.03069746 -2.43898811  3.8902381 ]', '[-1.1633222   1.6482918  -1.35709947  2.31331351]', '[-1.31803668  1.97139952 -0.18311653  0.9410314 ]']</t>
-  </si>
-  <si>
-    <t>['[1,1,1]', '[2,0,1]', '[1,1,2]', '[0,2,1]', '[2,1,0]', '[0,0,0]', '[1,0,2]', '[0,1,1]', '[2,2,2]', '[1,2,0]']</t>
-  </si>
-  <si>
-    <t>[1, 2, 3, 4, 11, 12, 14, 15, 16, 23, 26, 27, 34, 35, 36, 37, 40, 47, 48, 49]</t>
-  </si>
-  <si>
-    <t>[0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0]</t>
-  </si>
-  <si>
-    <t>['[-0.03763371 -0.01533471  0.06554052 -0.01816017]', '[-0.0208055  -0.02030166  0.09914155 -0.02801351]', '[ 0.00031733 -0.02489487  0.10765546 -0.0138725 ]', '[ 0.02044082 -0.02428802  0.08954248  0.02288616]', '[ 0.03470698 -0.01491644  0.05056501  0.07132823]', '[ 0.02674144  0.03818636 -0.12667052  0.44879208]', '[-0.01270905  0.15667936 -0.25571586  0.70881747]', '[-0.06940829  0.30836147 -0.29491305  0.77301892]', '[-0.12394901  0.4517198  -0.23590169  0.62988145]', '[-0.15876359  0.5498143  -0.10369689  0.33260441]', '[-0.16331677  0.57991751  0.05921824 -0.03571874]', '[-0.12364641  0.50409537  0.32874453 -0.70766221]', '[-0.03775164  0.30783049  0.50916352 -1.21389118]', '[ 0.08230598  0.00646819  0.65728545 -1.72868582]', '[ 0.19568549 -0.31507497  0.44233374 -1.41248958]', '[ 0.24874947 -0.53479727  0.07445597 -0.74782605]', '[ 0.22378572 -0.60603571 -0.31840679  0.03919136]', '[ 0.11442199 -0.4904076  -0.75239468  1.08990062]', '[-0.06422789 -0.18931537 -0.99191476  1.84838037]', '[-0.26125198  0.20964826 -0.92298465  2.03401315]', '[-0.41194923  0.58232295 -0.54375852  1.61314891]', '[-0.46777797  0.83238475 -0.00276778  0.85574325]', '[-4.13157479e-01  9.18176467e-01  5.36999746e-01  1.47639152e-04]', '[-0.25052089  0.80607747  1.05732746 -1.09655081]', '[ 0.00535011  0.46510136  1.45089561 -2.24360365]', '[ 0.30332587 -0.04634387  1.45111841 -2.72448181]', '[ 0.53994243 -0.52771758  0.85573619 -1.97843153]', '[ 0.63070812 -0.81121264  0.03700848 -0.82619492]', '[ 0.54363234 -0.82262069 -0.89069122  0.70968899]', '[ 0.28638189 -0.5334043  -1.63615995  2.13711295]', '[-0.08370282 -0.00670287 -1.97349678  2.97029016]', '[-0.45956563  0.5732749  -1.68925124  2.65534342]', '[-0.72992991  1.00831972 -0.96946712  1.64089425]', '[-0.83669167  1.22160453 -0.08643503  0.48633971]', '[-0.75431029  1.17415991  0.89843288 -0.96388258]', '[-0.48639109  0.83542306  1.74431253 -2.4058095 ]', '[-0.07978657  0.23789384  2.2327698  -3.42181015]', '[ 0.35782588 -0.43981202  2.02316649 -3.12354429]', '[ 0.70283971 -0.97490134  1.36351553 -2.13825651]', '[ 0.88762232 -1.28202363  0.46350657 -0.92717642]', '[ 0.87505226 -1.31933117 -0.58538068  0.55499968]', '[ 0.64872752 -1.02903262 -1.65564281  2.35968739]', '[ 0.22788475 -0.38078623 -2.48105418  4.02148306]', '[-0.29171512  0.47901004 -2.55625742  4.24960342]', '[-0.73987466  1.21260401 -1.8488399   2.97714699]', '[-1.01466125  1.66360081 -0.87549246  1.54893249]', '[-1.08460821  1.83906568  0.17965103  0.21339072]', '[-0.93745299  1.72411593  1.27448334 -1.37870194]', '[-0.58569539  1.27747337  2.20792459 -3.10945939]', '[-0.07375319  0.48576638  2.82745049 -4.68220059]']</t>
-  </si>
-  <si>
-    <t>['[0,1,1]', '[2,0,1]', '[2,2,2]', '[1,0,2]', '[0,0,0]', '[1,1,1]', '[2,1,0]', '[1,1,2]', '[0,2,1]', '[1,2,0]']</t>
+    <t>['[-0.03763371 -0.01533471  0.06554052 -0.01816017]', '[-0.0208055  -0.02030166  0.09914155 -0.02801351]', '[ 0.013578   -0.05917353  0.23628798 -0.34824344]', '[ 0.06892075 -0.15170277  0.30283362 -0.5520916 ]', '[ 0.12827063 -0.26838081  0.27505366 -0.58564774]', '[ 0.17298396 -0.37457441  0.16029766 -0.45268231]', '[ 0.188802   -0.44173166 -0.00664011 -0.2067265 ]', '[ 0.14464221 -0.38858741 -0.42504594  0.72477497]', '[ 0.02643202 -0.16436732 -0.72802709  1.4651372 ]', '[-0.13092325  0.16780439 -0.80101595  1.7696025 ]', '[-0.27519234  0.50644059 -0.6020908   1.53833469]', '[-0.35920157  0.75822894 -0.21924396  0.93976015]', '[-0.35930747  0.87273767  0.21689617  0.19605851]', '[-0.26488436  0.80691569  0.70843718 -0.83918341]', '[-0.08674636  0.54890113  1.03726409 -1.69097861]', '[ 0.13145033  0.16106604  1.09020931 -2.08807578]', '[ 0.32508846 -0.23996745  0.79242842 -1.81741538]', '[ 0.4435257  -0.56452809  0.36029408 -1.36311244]', '[ 0.44957965 -0.73560638 -0.29994035 -0.3311512 ]', '[ 0.31671287 -0.66506271 -1.00249636  1.019091  ]', '[ 0.0640436  -0.34376856 -1.47126841  2.11987675]', '[-0.243594    0.13577239 -1.5245149   2.52891299]', '[-0.51256542  0.60657205 -1.09985122  2.06405655]', '[-0.66468899  0.93133975 -0.39513004  1.14547461]', '[-0.66589507  1.05715933  0.381213    0.10500551]', '[-0.49615947  0.91453943  1.28970628 -1.52452259]', '[-0.16574589  0.45783916  1.95513143 -2.96635055]', '[ 0.23634909 -0.17496955  1.95537635 -3.15054435]', '[ 0.57356919 -0.72146238  1.34284    -2.19034519]', '[ 0.76614805 -1.0570417   0.55471946 -1.13731239]', '[ 0.7795318  -1.14404413 -0.41958532  0.26848072]', '[ 0.59234992 -0.91980552 -1.4298031   1.97401599]', '[ 0.22282997 -0.3640577  -2.19860135  3.48904191]', '[-0.2424845   0.39290354 -2.31812468  3.80817692]', '[-0.6537735   1.06177508 -1.71489706  2.75610082]', '[-0.90956561  1.47951854 -0.81655009  1.42129621]', '[-0.97441086  1.6337622   0.17218527  0.1257811 ]', '[-0.83447052  1.50384985  1.21069902 -1.43701669]', '[-0.49065773  1.02493678  2.19590809 -3.36612496]', '[ 0.02211542  0.17628614  2.82015742 -4.91463981]', '[ 0.56481499 -0.78769442  2.44247448 -4.38695243]', '[ 0.95941542 -1.51260104  1.46270665 -2.84343165]', '[ 1.14214044 -1.9355215   0.35568819 -1.40991176]', '[ 1.10159273 -2.08080086 -0.75103267 -0.0406645 ]', '[ 0.83651944 -1.90275301 -1.86266313  1.84452755]', '[ 0.375073   -1.3300717  -2.7059519   3.91111536]', '[-0.22495589 -0.3464908  -3.19131349  5.73119996]', '[-0.82023929  0.78251445 -2.56495783  5.13892089]', '[-1.20786223  1.63790767 -1.28247704  3.42683468]', '[-1.33108156  2.17175476  0.04616235  1.93796835]']</t>
+  </si>
+  <si>
+    <t>['[1,1,2]', '[0,1,1]', '[0,2,1]', '[1,1,1]', '[2,0,1]', '[2,2,2]', '[1,2,0]', '[2,1,0]', '[0,0,0]', '[1,0,2]']</t>
+  </si>
+  <si>
+    <t>[1, 2, 3, 4, 12, 13, 14, 15, 22, 23, 26, 27, 35, 36, 37, 38, 39, 46, 47, 48]</t>
+  </si>
+  <si>
+    <t>[0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0]</t>
+  </si>
+  <si>
+    <t>['[-0.03763371 -0.01533471  0.06554052 -0.01816017]', '[-0.0208055  -0.02030166  0.09914155 -0.02801351]', '[ 0.00031733 -0.02489487  0.10765546 -0.0138725 ]', '[ 0.02044082 -0.02428802  0.08954248  0.02288616]', '[ 0.03470698 -0.01491644  0.05056501  0.07132823]', '[ 0.02674144  0.03818636 -0.12667052  0.44879208]', '[-0.01270905  0.15667936 -0.25571586  0.70881747]', '[-0.06940829  0.30836147 -0.29491305  0.77301892]', '[-0.12394901  0.4517198  -0.23590169  0.62988145]', '[-0.15876359  0.5498143  -0.10369689  0.33260441]', '[-0.16331677  0.57991751  0.05921824 -0.03571874]', '[-0.11115167  0.47150347  0.45175365 -1.02968721]', '[-0.00348179  0.21675506  0.59698913 -1.46172246]', '[ 0.11396508 -0.08506333  0.54256926 -1.4829412 ]', '[ 0.20011549 -0.34763888  0.29372318 -1.08615674]', '[ 0.22451991 -0.50256142 -0.0564339  -0.43932736]', '[ 0.16569124 -0.48678401 -0.51888297  0.58652213]', '[ 0.02578831 -0.27917006 -0.84860786  1.44044113]', '[-0.15700533  0.06021112 -0.93070376  1.86280023]', '[-0.32529833  0.42532437 -0.70582301  1.6983345 ]', '[-0.42415264  0.71004411 -0.25935348  1.10068736]', '[-0.42435295  0.8536004   0.25667511  0.3217269 ]', '[-0.31442539  0.80785359  0.82033376 -0.76509522]', '[-0.1089291   0.55944926  1.19338031 -1.66705333]', '[ 0.15482434  0.13951823  1.38134063 -2.42271807]', '[ 0.41355648 -0.35314846  1.13445045 -2.36715453]', '[ 0.57211716 -0.73002073  0.41880776 -1.34332438]', '[ 0.575475   -0.87903269 -0.38300938 -0.13695651]', '[ 0.41342194 -0.75453759 -1.20933932  1.36680762]', '[ 0.10867252 -0.34812249 -1.77681422  2.61103165]', '[-0.26267074  0.22986739 -1.83603686  2.98012421]', '[-0.58579765  0.76954875 -1.3225263   2.29430722]', '[-0.77238638  1.1214822  -0.51736147  1.19980703]', '[-0.78795559  1.24580228  0.36093197  0.03935906]', '[-0.6126445   1.08041825  1.36916611 -1.69755548]', '[-0.26561818  0.60080836  2.04409235 -3.03483612]', '[ 0.1694554  -0.07499262  2.18988916 -3.49995813]', '[ 0.56025539 -0.70144744  1.62629069 -2.60148665]', '[ 0.79680151 -1.08403778  0.70914844 -1.20247801]', '[ 0.83800664 -1.18165959 -0.29960944  0.22565419]', '[ 0.66943805 -0.96399144 -1.36844554  1.95625821]', '[ 0.30356001 -0.40435262 -2.22932842  3.56006445]', '[-0.17858865  0.37971164 -2.44990998  3.99417497]', '[-0.62168782  1.08586911 -1.89366121  2.92734148]', '[-0.91521255  1.53310404 -1.01089909  1.54691314]', '[-1.01829544  1.70975394 -0.01129724  0.22842596]', '[-0.91183067  1.60035299  1.06446562 -1.33363296]', '[-0.6007359   1.16812146  2.01677563 -3.0043529 ]', '[-0.12376021  0.40762279  2.66727706 -4.4668793 ]', '[ 0.41910793 -0.53093493  2.58843859 -4.55576946]']</t>
+  </si>
+  <si>
+    <t>['[1,2,0]', '[1,0,2]', '[0,2,1]', '[0,0,0]', '[0,1,1]', '[2,0,1]', '[1,1,1]', '[1,1,2]', '[2,1,0]', '[2,2,2]']</t>
   </si>
   <si>
     <t>[1, 2, 3, 4, 11, 12, 13, 14, 15, 16, 23, 24, 25, 26, 27, 34, 35, 36, 37, 38, 39, 46, 47, 48, 49]</t>
@@ -130,49 +133,58 @@
     <t>['[-0.03763371 -0.01533471  0.06554052 -0.01816017]', '[-0.0208055  -0.02030166  0.09914155 -0.02801351]', '[ 0.00031733 -0.02489487  0.10765546 -0.0138725 ]', '[ 0.02044082 -0.02428802  0.08954248  0.02288616]', '[ 0.03470698 -0.01491644  0.05056501  0.07132823]', '[ 0.02674144  0.03818636 -0.12667052  0.44879208]', '[-0.01270905  0.15667936 -0.25571586  0.70881747]', '[-0.06940829  0.30836147 -0.29491305  0.77301892]', '[-0.12394901  0.4517198  -0.23590169  0.62988145]', '[-0.15876359  0.5498143  -0.10369689  0.33260441]', '[-0.16331677  0.57991751  0.05921824 -0.03571874]', '[-0.12364641  0.50409537  0.32874453 -0.70766221]', '[-0.03775164  0.30783049  0.50916352 -1.21389118]', '[ 0.06909397  0.04061776  0.52882372 -1.39480458]', '[ 0.16087913 -0.22270668  0.3614133  -1.17772404]', '[ 0.20472536 -0.40990137  0.06420388 -0.6597987 ]', '[ 0.18455416 -0.47825444 -0.26212436 -0.01817226]', '[ 0.09156532 -0.38679677 -0.64742279  0.90761115]', '[-0.06271277 -0.13292697 -0.85786545  1.56672789]', '[-0.23333411  0.20632363 -0.80133675  1.73587805]', '[-0.36498881  0.52600302 -0.4801429   1.39142644]', '[-0.41539568  0.74217732 -0.01227622  0.7395642 ]', '[-0.36944782  0.81527715  0.46213933 -0.01083091]', '[-0.22642744  0.71066606  0.93936783 -1.01021577]', '[-0.00892589  0.42883145  1.18897233 -1.74077443]', '[ 0.22660096  0.0517002   1.1068182  -1.92405165]', '[ 0.41005532 -0.29693012  0.6808143  -1.47495926]', '[ 0.48521772 -0.51258559  0.05370639 -0.64539491]', '[ 0.417663   -0.51547329 -0.71588293  0.61057794]', '[ 0.20989945 -0.2789723  -1.31808193  1.6972301 ]', '[-0.08492151  0.12510753 -1.555619    2.21640575]', '[-0.37963177  0.55019577 -1.32030983  1.91504598]', '[-0.58989289  0.85617843 -0.74359286  1.09612783]', '[-0.66706415  0.97859659 -0.01685984  0.11844472]', '[-0.58535204  0.87309513  0.82205171 -1.16698164]', '[-0.34814683  0.51985272  1.50786441 -2.31349921]', '[-0.00845867 -0.01084392  1.80187214 -2.83660639]', '[ 0.33251678 -0.53972913  1.5220548  -2.29877877]', '[ 0.57395443 -0.88909757  0.8506743  -1.14546192]', '[ 0.66227792 -0.9897414   0.02017728  0.14415152]', '[ 0.56997838 -0.80175587 -0.93344798  1.72881771]', '[ 0.29908242 -0.30913141 -1.72312117  3.11534711]', '[-0.08315313  0.37699688 -1.98491703  3.51987652]', '[-0.44967675  1.01119311 -1.6016925   2.68937509]', '[-0.70314623  1.42828109 -0.90116783  1.46392917]', '[-0.80177252  1.59623253 -0.07487256  0.2180398 ]', '[-0.72394184  1.49081901  0.8443507  -1.27627909]', '[-0.47088945  1.08272659  1.65970504 -2.80278718]', '[-0.07741763  0.38520798  2.19752525 -4.04435356]', '[ 0.35720396 -0.43419659  2.00983042 -3.86699684]']</t>
   </si>
   <si>
-    <t>['[0,2,1]', '[2,2,2]', '[2,0,1]', '[0,1,1]', '[1,2,0]', '[1,1,2]', '[1,1,1]', '[0,0,0]', '[1,0,2]', '[2,1,0]']</t>
+    <t>['[2,2,2]', '[1,1,2]', '[0,1,1]', '[0,2,1]', '[1,2,0]', '[1,0,2]', '[2,0,1]', '[2,1,0]', '[1,1,1]', '[0,0,0]']</t>
   </si>
   <si>
     <t>[0,1,1]</t>
   </si>
   <si>
-    <t>[10, 11, 19, 20, 31, 35]</t>
-  </si>
-  <si>
-    <t>['[-0.03763371 -0.01533471  0.06554052 -0.01816017]', '[-0.00754409 -0.05458322  0.2277812  -0.36241836]', '[ 0.04879627 -0.15231473  0.32089719 -0.5887683 ]', '[ 0.11397169 -0.27767857  0.31375488 -0.63332862]', '[ 0.16759438 -0.39312519  0.2086893  -0.49480525]', '[ 0.1930193  -0.46685036  0.03906408 -0.22816919]', '[ 0.15689524 -0.41528579 -0.3922057   0.73207416]', '[ 0.04309269 -0.18588535 -0.71796191  1.51055937]', '[-0.1147829   0.15904975 -0.81547211  1.84906375]', '[-0.26363568  0.51494657 -0.63159042  1.62703318]', '[-0.3423183   0.7521378  -0.14060109  0.71307914]', '[-0.31834832  0.79441559  0.37391128 -0.28985184]', '[-0.18669612  0.60966499  0.9186555  -1.52917439]', '[ 0.03463692  0.20461547  1.24297207 -2.42940656]', '[ 0.28282653 -0.308983    1.16536595 -2.56170684]', '[ 0.47339348 -0.76693654  0.69326653 -1.92910836]', '[ 0.54862155 -1.05940145  0.04837448 -0.97035556]', '[ 0.4936206  -1.15081099 -0.5844728   0.05628529]', '[ 0.3035996  -0.98327937 -1.28296628  1.60245346]', '[ 0.00875742 -0.55543996 -1.60928017  2.5955807 ]', '[-3.10416341e-01  2.81679705e-03 -1.49761883e+00  2.82396175e+00]', '[-0.56871455  0.54044832 -1.01550051  2.41892404]', '[-0.69667623  0.93423017 -0.23906391  1.47177147]', '[-0.66134381  1.11932373  0.58372114  0.36786659]', '[-0.45179981  1.02337585  1.47315348 -1.31893107]', '[-0.09193859  0.60227795  2.06232773 -2.82317458]', '[ 0.33819197 -0.04954337  2.12879508 -3.48477583]', '[ 0.71181272 -0.69790985  1.51767862 -2.83558127]', '[ 0.92251454 -1.15027652  0.56159768 -1.6602797 ]', '[ 0.93204968 -1.35853584 -0.46362841 -0.41505291]', '[ 0.72451444 -1.25886375 -1.58116723  1.42574539]', '[ 0.32680561 -0.81376632 -2.33744775  2.98835251]', '[-0.18877004 -0.07716939 -2.69620021  4.14914962]', '[-0.68919748  0.71767848 -2.17988762  3.55009709]', '[-1.02870761  1.29430267 -1.17726325  2.19438869]', '[-1.14373069  1.57488764  0.0298294   0.62780559]', '[-1.01038057  1.52020897  1.2881589  -1.19438571]', '[-0.6380142   1.08281539  2.40298033 -3.21154827]', '[-0.07043271  0.24446188  3.16429045 -4.98478015]', '[ 0.55219029 -0.7494685   2.87831238 -4.56406241]', '[ 1.03478156 -1.50012874  1.89907546 -2.92160112]', '[ 1.30201017 -1.93409738  0.75869719 -1.45832452]', '[ 1.33533928 -2.0928387  -0.42520874 -0.13288012]', '[ 1.12110232 -1.9376659  -1.69762245  1.71913924]', '[ 0.66777032 -1.38321184 -2.80351733  3.89082246]', '[ 0.01597747 -0.36978407 -3.61526303  6.07583877]', '[-0.68728338  0.84154734 -3.18636166  5.52113986]', '[-1.21007587  1.75223365 -2.01210229  3.61783629]', '[-1.48833844  2.32008132 -0.76584947  2.11625317]', '[-1.51656859  2.60889632  0.47889271  0.77477803]']</t>
-  </si>
-  <si>
-    <t>['[0,1,1]', '[2,0,1]', '[0,2,1]', '[2,1,0]', '[1,1,1]', '[1,2,0]', '[1,1,2]', '[0,0,0]', '[2,2,2]', '[1,0,2]']</t>
-  </si>
-  <si>
-    <t>[8, 9, 19, 22, 23, 30, 31, 32, 33, 35, 45, 47, 48]</t>
+    <t>[6, 45]</t>
+  </si>
+  <si>
+    <t>[0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2]</t>
+  </si>
+  <si>
+    <t>['[-0.03763371 -0.01533471  0.06554052 -0.01816017]', '[-0.00754409 -0.05458322  0.2277812  -0.36241836]', '[ 0.04879627 -0.15231473  0.32089719 -0.5887683 ]', '[ 0.11397169 -0.27767857  0.31375488 -0.63332862]', '[ 0.16759438 -0.39312519  0.2086893  -0.49480525]', '[ 0.1930193  -0.46685036  0.03906408 -0.22816919]', '[ 0.16956871 -0.44830261 -0.26820417  0.40739083]', '[ 0.07764819 -0.2777752  -0.62973474  1.26105599]', '[-0.06966349  0.03261704 -0.80302667  1.76452698]', '[-0.22465905  0.39058523 -0.70217906  1.72562277]', '[-0.33473527  0.69134317 -0.37152277  1.22661262]', '[-0.3665604   0.86641223  0.05855316  0.50502011]', '[-0.2902422   0.83034492  0.68874955 -0.85560583]', '[-0.10067244  0.53350339  1.17222386 -2.06518635]', '[ 0.15834837  0.03861766  1.35020622 -2.75501467]', '[ 0.4067969  -0.50420448  1.06115475 -2.52952059]', '[ 0.56001777 -0.93015548  0.43912923 -1.67046011]', '[ 0.57684927 -1.1602767  -0.26889077 -0.61879139]', '[ 0.43815341 -1.12120884 -1.08950026  1.00133178]', '[ 0.15556883 -0.76623271 -1.6914747   2.50835845]', '[-0.21367349 -0.15336851 -1.91436095  3.46094303]', '[-0.56562576  0.52965607 -1.50364495  3.17033497]', '[-0.78506524  1.06113145 -0.65170231  2.08510542]', '[-0.81974624  1.35479505  0.30379744  0.84259963]', '[-0.65145106  1.34335605  1.34587039 -0.95988568]', '[-0.29856385  0.97014979  2.13223916 -2.75416186]', '[ 0.17475072  0.26993715  2.50281365 -4.07576894]', '[ 0.64662107 -0.54619651  2.08107881 -3.81260201]', '[ 0.96851549 -1.18658407  1.09123658 -2.53710897]', '[ 1.07493688 -1.55948432 -0.03211188 -1.19515589]', '[ 0.94189396 -1.61393901 -1.27311138  0.66271178]', '[ 0.58014371 -1.2845204  -2.29983374  2.65488467]', '[ 0.04378738 -0.55352356 -2.98440023  4.55503349]', '[-0.55630483  0.42239481 -2.83426284  4.80991392]', '[-1.02917741  1.24811464 -1.82413406  3.3531663 ]', '[-1.27509688  1.76943501 -0.62413933  1.8926367 ]', '[-1.27756877  2.01244221  0.59446874  0.53549834]', '[-1.02937449  1.93193562  1.85513406 -1.37261076]', '[-0.55368236  1.44571503  2.85066162 -3.53473066]', '[ 0.08879531  0.51333666  3.48690274 -5.65673601]', '[ 0.76569241 -0.64831112  3.06271874 -5.46482408]', '[ 1.25767066 -1.56408459  1.8176958  -3.68623552]', '[ 1.48959781 -2.14881214  0.50061019 -2.20904466]', '[ 1.45944531 -2.45466729 -0.79295045 -0.84366177]', '[ 1.16684187 -2.43804989 -2.10003292  1.03577004]', '[ 0.64763311 -2.04827119 -3.01470568  2.89459424]', '[-0.01153427 -1.24673105 -3.51050578  5.12564003]', '[-0.72745123 -0.04444007 -3.48898645  6.50821683]', '[-1.3136375   1.13919004 -2.23339581  5.05691887]', '[-1.60648197  1.9811028  -0.69512271  3.42958454]']</t>
+  </si>
+  <si>
+    <t>['[2,1,0]', '[1,2,0]', '[0,2,1]', '[0,0,0]', '[1,1,2]', '[1,0,2]', '[1,1,1]', '[0,1,1]', '[2,2,2]', '[2,0,1]']</t>
+  </si>
+  <si>
+    <t>[6, 7, 21, 23, 47, 49]</t>
+  </si>
+  <si>
+    <t>[0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2]</t>
+  </si>
+  <si>
+    <t>['[-0.03763371 -0.01533471  0.06554052 -0.01816017]', '[-0.00754409 -0.05458322  0.2277812  -0.36241836]', '[ 0.04879627 -0.15231473  0.32089719 -0.5887683 ]', '[ 0.11397169 -0.27767857  0.31375488 -0.63332862]', '[ 0.16759438 -0.39312519  0.2086893  -0.49480525]', '[ 0.1930193  -0.46685036  0.03906408 -0.22816919]', '[ 0.16956871 -0.44830261 -0.26820417  0.40739083]', '[ 0.09055011 -0.31127879 -0.50323119  0.93116007]', '[-0.03483507 -0.05969969 -0.71793241  1.5230623 ]', '[-0.18039446  0.26629635 -0.69574778  1.65343328]', '[-0.29690327  0.56916291 -0.43821183  1.31167254]', '[-0.34675453  0.77201171 -0.04953222  0.68864755]', '[-0.31598101  0.83868786  0.35007898 -0.02375999]', '[-0.18940352  0.70426799  0.89192787 -1.29757239]', '[ 0.02746789  0.33708581  1.23087086 -2.2985346 ]', '[ 0.27787712 -0.16847647  1.2013497  -2.61602353]', '[ 0.47880984 -0.65183167  0.75333347 -2.11132109]', '[ 0.56476348 -0.98533657  0.0908504  -1.18832772]', '[ 0.51494778 -1.12036861 -0.57597744 -0.15808274]', '[ 0.32339911 -0.99377913 -1.30376089  1.40759359]', '[ 0.01109846 -0.57091668 -1.76378694  2.75005348]', '[-0.33837788  0.01983632 -1.63835974  2.97897882]', '[-0.61982391  0.58151155 -1.10262488  2.4997018 ]', '[-0.74792739  0.9544799  -0.16032637  1.19924637]', '[-0.69415277  1.08496986  0.68775543  0.09629698]', '[-0.46134764  0.93417696  1.60137349 -1.59534776]', '[-0.07465358  0.4606633   2.19369933 -3.04782402]', '[ 0.37519814 -0.2136689   2.18372566 -3.46086994]', '[ 0.75173447 -0.83351175  1.50225172 -2.60540041]', '[ 0.95728146 -1.23391595  0.53025227 -1.38606033]', '[ 0.96018396 -1.38710116 -0.4983901  -0.14078381]', '[ 0.74488672 -1.23273569 -1.62756481  1.70216829]', '[ 0.3242788  -0.70149004 -2.52336218  3.57515995]', '[-0.22590178  0.13643631 -2.82907273  4.5024164 ]', '[-0.73932555  0.95797201 -2.18956609  3.50175168]', '[-1.07719333  1.51101477 -1.16003695  2.03780512]', '[-1.19708032  1.78269964 -0.03264089  0.69346267]', '[-1.07557618  1.74136328  1.23295824 -1.12480808]', '[-0.71312448  1.31777423  2.36215169 -3.15719162]', '[-0.14665034  0.46967987  3.22328946 -5.21702473]', '[ 0.50617642 -0.62125771  3.09162383 -5.22242927]', '[ 1.02897951 -1.49844632  2.07861815 -3.50091381]', '[ 1.32861661 -2.0403755   0.90531143 -1.96884186]', '[ 1.38858992 -2.2980498  -0.30516097 -0.61620807]', '[ 1.19674848 -2.24152159 -1.59259837  1.20511741]', '[ 0.76508675 -1.79975787 -2.67952076  3.26922909]', '[ 0.14331719 -0.90895951 -3.49300143  5.64730697]', '[-0.57060519  0.32932376 -3.40904929  6.18871984]', '[-1.14317014  1.40291848 -2.22786594  4.41387403]', '[-1.44738727  2.09431796 -0.82031993  2.58056145]']</t>
+  </si>
+  <si>
+    <t>['[1,0,2]', '[2,2,2]', '[0,2,1]', '[1,2,0]', '[1,1,2]', '[1,1,1]', '[0,1,1]', '[2,0,1]', '[2,1,0]', '[0,0,0]']</t>
+  </si>
+  <si>
+    <t>[6, 8, 9, 18, 19, 20, 22, 30, 32, 33, 34, 44, 48]</t>
+  </si>
+  <si>
+    <t>[0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 1, 2, 2, 2, 2, 2, 2, 0]</t>
+  </si>
+  <si>
+    <t>['[-0.03763371 -0.01533471  0.06554052 -0.01816017]', '[-0.00754409 -0.05458322  0.2277812  -0.36241836]', '[ 0.04879627 -0.15231473  0.32089719 -0.5887683 ]', '[ 0.11397169 -0.27767857  0.31375488 -0.63332862]', '[ 0.16759438 -0.39312519  0.2086893  -0.49480525]', '[ 0.1930193  -0.46685036  0.03906408 -0.22816919]', '[ 0.16956871 -0.44830261 -0.26820417  0.40739083]', '[ 0.07764819 -0.2777752  -0.62973474  1.26105599]', '[-0.05644144 -0.00156921 -0.67466795  1.43082082]', '[-0.176879    0.26464326 -0.49680588  1.16644284]', '[-0.25711731  0.4767488  -0.28403648  0.90979515]', '[-0.28426128  0.61457375  0.01975631  0.44705469]', '[-0.22487715  0.58730769  0.56130736 -0.7092423 ]', '[-0.068705    0.3420325   0.96683964 -1.69150278]', '[ 0.1431301  -0.05647138  1.09452851 -2.18631902]', '[ 0.34365728 -0.48338253  0.85512458 -1.97554043]', '[ 0.46736356 -0.81307286  0.35508228 -1.26985396]', '[ 0.48031057 -0.97935796 -0.22576273 -0.38025871]', '[ 0.37034432 -0.93510016 -0.85198718  0.8115716 ]', '[ 0.15198923 -0.66462783 -1.29069543  1.84613756]', '[-0.12448119 -0.22833392 -1.40873417  2.40351471]', '[-0.39441207  0.27428898 -1.21594547  2.47951635]', '[-0.57165345  0.68037799 -0.51782726  1.51109455]', '[-0.60534586  0.89468928  0.18691477  0.6101727 ]', '[-0.47760053  0.86077569  1.06623677 -0.94242455]', '[-0.19346793  0.52660631  1.72336457 -2.34245791]', '[ 0.1821285  -0.03080197  1.93733356 -3.05895497]', '[ 0.53829108 -0.61497936  1.53495483 -2.62082624]', '[ 0.77032889 -1.03866556  0.74885416 -1.57233465]', '[ 0.83013855 -1.23743636 -0.15567775 -0.4092062 ]', '[ 0.70081949 -1.17294099 -1.11796017  1.05787838]', '[ 0.3845157  -0.78544536 -2.00246208  2.79657381]', '[-0.06018741 -0.12194495 -2.33783282  3.64542092]', '[-0.49705746  0.567071   -1.91625356  3.02664571]', '[-0.79489701  1.03762584 -1.01975225  1.63625059]', '[-0.90625923  1.24698878 -0.08238304  0.45498018]', '[-0.80777161  1.16387972  1.05583346 -1.29399475]', '[-0.49237043  0.72494682  2.06131674 -3.08067003]', '[-0.01129521 -0.03039104  2.62794187 -4.24200467]', '[ 0.49472427 -0.84028724  2.3010133  -3.60329647]', '[ 0.87551466 -1.4220165   1.46165791 -2.18984591]', '[ 1.0681743  -1.7213628   0.44865031 -0.82079602]', '[ 1.04408661 -1.73048353 -0.6854067   0.73196656]', '[ 0.79059096 -1.39673214 -1.83069111  2.64061126]', '[ 0.33330738 -0.69041036 -2.68689674  4.37712735]', '[-0.25059083  0.30324093 -2.9691215   5.17066637]', '[-0.77879442  1.21863639 -2.20927732  3.80662345]', '[-1.11646539  1.81949672 -1.14604697  2.23638756]', '[-1.22481144  2.10414756  0.06386997  0.63064501]', '[-1.08664228  2.05046966  1.30014116 -1.18338557]']</t>
+  </si>
+  <si>
+    <t>['[1,1,2]', '[1,2,0]', '[1,0,2]', '[2,2,2]', '[2,1,0]', '[0,1,1]', '[1,1,1]', '[0,2,1]', '[2,0,1]', '[0,0,0]']</t>
+  </si>
+  <si>
+    <t>[6, 7, 8, 10, 11, 18, 19, 20, 21, 23, 30, 31, 33, 34, 35, 42, 43, 44, 45, 46, 47, 48]</t>
   </si>
   <si>
     <t>[0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0]</t>
   </si>
   <si>
-    <t>['[-0.03763371 -0.01533471  0.06554052 -0.01816017]', '[-0.00754409 -0.05458322  0.2277812  -0.36241836]', '[ 0.04879627 -0.15231473  0.32089719 -0.5887683 ]', '[ 0.11397169 -0.27767857  0.31375488 -0.63332862]', '[ 0.16759438 -0.39312519  0.2086893  -0.49480525]', '[ 0.1930193  -0.46685036  0.03906408 -0.22816919]', '[ 0.15689524 -0.41528579 -0.3922057   0.73207416]', '[ 0.04309269 -0.18588535 -0.71796191  1.51055937]', '[-0.10156356  0.12486504 -0.68790627  1.51697551]', '[-0.21636795  0.38996412 -0.42995154  1.07414568]', '[-0.27725576  0.56952638 -0.16350655  0.68794418]', '[-0.27828103  0.65602489  0.15390405  0.16684646]', '[-0.19386239  0.57232276  0.67314696 -0.98563643]', '[-0.01986345  0.27688231  1.02794642 -1.90403547]', '[ 0.1962186  -0.15057152  1.07222081 -2.25351289]', '[ 0.38369622 -0.57517123  0.75172958 -1.89412559]', '[ 0.48199952 -0.87984738  0.21163869 -1.11221155]', '[ 0.46566981 -1.01139552 -0.36921323 -0.19628544]', '[ 0.3189943  -0.90094464 -1.07053627  1.28562506]', '[ 0.06389667 -0.54167087 -1.43061779  2.23806616]', '[-0.24018981 -0.01580509 -1.53215776  2.87439573]', '[-0.51332601  0.53877086 -1.12384468  2.52715897]', '[-0.65613602  0.92473602 -0.28160894  1.29357161]', '[-0.62409402  1.05010147  0.59197927 -0.04396964]', '[-0.41736323  0.87864178  1.44143666 -1.65751964]', '[-0.06647611  0.40274878  2.00001849 -3.0069791 ]', '[ 0.34371974 -0.25455247  1.98822645 -3.34564217]', '[ 0.68508575 -0.85241792  1.35172623 -2.50992874]', '[ 0.86668155 -1.23663009  0.44283988 -1.31618773]', '[ 0.85921523 -1.37701967 -0.51253121 -0.0833432 ]', '[ 0.65889634 -1.24068672 -1.46152504  1.45265086]', '[ 0.2909718  -0.79784575 -2.16253867  2.93458213]', '[-0.17370057 -0.11272062 -2.3713156   3.70721852]', '[-0.60346847  0.57722196 -1.81686909  2.98441292]', '[-0.88319273  1.06616252 -0.93891458  1.85890009]', '[-0.96053244  1.28893995  0.16848493  0.37178096]', '[-0.80898298  1.18582796  1.3287309  -1.4165689 ]', '[-0.44052554  0.71669413  2.31042402 -3.25453834]', '[ 0.08238646 -0.0694744   2.78384499 -4.34509376]', '[ 0.6059751  -0.8826819   2.32420009 -3.54481032]', '[ 0.98156178 -1.44708745  1.39229181 -2.09135129]', '[ 1.15355525 -1.72761353  0.31517941 -0.73300895]', '[ 1.08996637 -1.69582437 -0.94391368  1.06059438]', '[ 0.78168609 -1.29080959 -2.11848434  3.03390424]', '[ 0.2550971  -0.4711329  -3.07669184  5.07517035]', '[-0.3704317   0.57083976 -2.97635174  4.9055389 ]', '[-0.88704804  1.4022693  -2.11943088  3.32652555]', '[-1.19642061  1.88661415 -0.95865116  1.56666094]', '[-1.26667290e+00  2.04225269e+00  2.58145071e-01  1.98879413e-03]', '[-1.08817046  1.86201959  1.51247844 -1.83390874]']</t>
-  </si>
-  <si>
-    <t>['[1,1,2]', '[0,1,1]', '[2,2,2]', '[1,2,0]', '[1,1,1]', '[2,1,0]', '[2,0,1]', '[0,2,1]', '[1,0,2]', '[0,0,0]']</t>
-  </si>
-  <si>
-    <t>[8, 10, 18, 19, 20, 21, 22, 23, 30, 31, 32, 43, 44, 47]</t>
-  </si>
-  <si>
-    <t>['[-0.03763371 -0.01533471  0.06554052 -0.01816017]', '[-0.00754409 -0.05458322  0.2277812  -0.36241836]', '[ 0.04879627 -0.15231473  0.32089719 -0.5887683 ]', '[ 0.11397169 -0.27767857  0.31375488 -0.63332862]', '[ 0.16759438 -0.39312519  0.2086893  -0.49480525]', '[ 0.1930193  -0.46685036  0.03906408 -0.22816919]', '[ 0.15689524 -0.41528579 -0.3922057   0.73207416]', '[ 0.04309269 -0.18588535 -0.71796191  1.51055937]', '[-0.10156356  0.12486504 -0.68790627  1.51697551]', '[-0.22927161  0.42348907 -0.55357165  1.39819937]', '[-0.298657    0.62767497 -0.12549291  0.61142121]', '[-0.28947606  0.69335068  0.2154295   0.03946997]', '[-0.19185735  0.58156717  0.74153817 -1.1358174 ]', '[-0.0047321   0.25603272  1.0874093  -2.0476426 ]', '[ 0.22027935 -0.19498825  1.0984779  -2.33778589]', '[ 0.40865409 -0.62839921  0.73526496 -1.90006117]', '[ 0.50039987 -0.92859782  0.16513137 -1.06606643]', '[ 0.47306546 -1.04756915 -0.43037904 -0.11899507]', '[ 0.32480686 -0.94913997 -1.02393705  1.08621719]', '[ 0.07838333 -0.62635106 -1.39358686  2.08251591]', '[-0.20859337 -0.15439535 -1.40565855  2.50892482]', '[-0.45286959  0.31796923 -0.97142788  2.08878472]', '[-0.57732782  0.64398277 -0.24655501  1.11984135]', '[-0.5476036   0.75524027  0.53748548 -0.01546489]', '[-0.35828655  0.60815977  1.32116199 -1.43019659]', '[-0.039558    0.20611148  1.79578914 -2.4840839 ]', '[ 0.32350065 -0.32167591  1.73947663 -2.62042839]', '[ 0.62129173 -0.78080549  1.17701827 -1.87682855]', '[ 0.77800442 -1.05283069  0.36818731 -0.82402977]', '[ 0.76489484 -1.10725053 -0.49611729  0.2830645 ]', '[ 0.57460055 -0.91031719 -1.3800823   1.67915355]', '[ 0.22979324 -0.44816424 -2.00364826  2.85779691]', '[-0.18904108  0.16826257 -2.07244122  3.09568319]', '[-0.56703903  0.73906205 -1.62091289  2.4650078 ]', '[-0.8134995   1.12224768 -0.80913133  1.33831826]', '[-0.882934    1.27164565  0.1212864   0.15435838]', '[-0.74669213  1.12782039  1.22635149 -1.60203408]', '[-0.40256352  0.62835796  2.17013376 -3.35840172]', '[ 0.08716801 -0.16100284  2.59147911 -4.26673505]', '[ 0.57075398 -0.9489109   2.13000579 -3.4021529 ]', '[ 0.91205172 -1.48840017  1.24648062 -1.98518249]', '[ 1.06034611 -1.74909726  0.22483406 -0.63564194]', '[ 0.98495903 -1.69722727 -0.96966225  1.16384925]', '[ 0.68807856 -1.29822587 -1.97236979  2.85094775]', '[ 0.21177687 -0.55596041 -2.72030797  4.48325624]', '[-0.35832603  0.42188473 -2.79735867  4.90529595]', '[-0.84159568  1.27294924 -1.95345496  3.48373191]', '[-1.11691704  1.79127553 -0.788443    1.74070728]', '[-1.16265951  2.0029678   0.33033239  0.38252938]', '[-0.97462173  1.89677235  1.52577491 -1.46606561]']</t>
-  </si>
-  <si>
-    <t>['[1,1,2]', '[0,1,1]', '[2,1,0]', '[0,0,0]', '[2,0,1]', '[0,2,1]', '[2,2,2]', '[1,0,2]', '[1,1,1]', '[1,2,0]']</t>
-  </si>
-  <si>
-    <t>[6, 7, 8, 10, 11, 19, 20, 21, 30, 31, 33, 34, 35, 42, 43, 44, 45, 47, 48]</t>
-  </si>
-  <si>
-    <t>['[-0.03763371 -0.01533471  0.06554052 -0.01816017]', '[-0.00754409 -0.05458322  0.2277812  -0.36241836]', '[ 0.04879627 -0.15231473  0.32089719 -0.5887683 ]', '[ 0.11397169 -0.27767857  0.31375488 -0.63332862]', '[ 0.16759438 -0.39312519  0.2086893  -0.49480525]', '[ 0.1930193  -0.46685036  0.03906408 -0.22816919]', '[ 0.16956871 -0.44830261 -0.26820417  0.40739083]', '[ 0.09055011 -0.31127879 -0.50323119  0.93116007]', '[-0.02165415 -0.09380121 -0.58952709  1.1892161 ]', '[-0.14550206  0.17387773 -0.61422386  1.41936009]', '[-0.24020309  0.41196422 -0.30815479  0.91099128]', '[-0.26240779  0.52437056  0.09121898  0.1966427 ]', '[-0.1925522   0.45677     0.59247211 -0.85560345]', '[-0.03557737  0.19693013  0.94041947 -1.68102434]', '[ 0.16402445 -0.18013331  1.00061721 -1.98582856]', '[ 0.34192942 -0.55414134  0.73197041 -1.66680986]', '[ 0.44259021 -0.8207075   0.25409559 -0.95978295]', '[ 0.43986044 -0.92922657 -0.27921648 -0.11780667]', '[ 0.3130901  -0.8087885  -0.96597127  1.3064609 ]', '[ 0.07896228 -0.45284063 -1.32722071  2.18112353]', '[-0.19226287  0.01936938 -1.3127041   2.40588476]', '[-0.41648277  0.4532279  -0.87186844  1.82551292]', '[-0.53680619  0.75237882 -0.30552878  1.11851217]', '[-0.53371409  0.88946709  0.3351537   0.24050949]', '[-0.38531053  0.78763772  1.12194238 -1.24436895]', '[-0.10071062  0.40593928  1.66814852 -2.49640743]', '[ 0.25040783 -0.15720629  1.74862424 -2.95803104]', '[ 0.55959318 -0.70327537  1.26903137 -2.37182191]', '[ 0.73787528 -1.07560705  0.48701446 -1.31898145]', '[ 0.74971991 -1.22549212 -0.36683811 -0.17409476]', '[ 0.58643669 -1.11627367 -1.2403318   1.26472596]', '[ 0.26851927 -0.72511307 -1.88721474  2.59976132]', '[-0.15150862 -0.08589617 -2.212127    3.6087684 ]', '[-0.55260541  0.58469821 -1.69501388  2.90099707]', '[-0.80209967  1.03105963 -0.76568882  1.52705074]', '[-0.85267941  1.19295902  0.26180156  0.09127026]', '[-0.69056723  1.03777743  1.33981021 -1.65009569]', '[-0.32953157  0.53445182  2.21633916 -3.32788568]', '[ 0.15757193 -0.22846746  2.51786497 -4.03024333]', '[ 0.61887691 -0.96001583  1.9933551  -3.10770191]', '[ 0.93060206 -1.44468007  1.09051239 -1.73383029]', '[ 1.04709959 -1.65859008  0.06551607 -0.41526014]', '[ 0.94866093 -1.58673413 -1.03838603  1.14467307]', '[ 0.64012938 -1.19229087 -2.01645769  2.81775428]', '[ 0.1604992  -0.46556379 -2.6992289   4.33387263]', '[-0.38273013  0.42888531 -2.56710198  4.26428224]', '[-0.82398454  1.16559239 -1.76990652  2.99387176]', '[-1.06632054  1.59576339 -0.63963881  1.33447194]', '[-1.07776043  1.70693913  0.52163171 -0.21981575]', '[-0.85429955  1.47798981  1.69198368 -2.09976649]']</t>
-  </si>
-  <si>
-    <t>['[2,0,1]', '[1,0,2]', '[2,2,2]', '[0,0,0]', '[1,1,2]', '[2,1,0]', '[1,1,1]', '[1,2,0]', '[0,1,1]', '[0,2,1]']</t>
+    <t>['[-0.03763371 -0.01533471  0.06554052 -0.01816017]', '[-0.00754409 -0.05458322  0.2277812  -0.36241836]', '[ 0.04879627 -0.15231473  0.32089719 -0.5887683 ]', '[ 0.11397169 -0.27767857  0.31375488 -0.63332862]', '[ 0.16759438 -0.39312519  0.2086893  -0.49480525]', '[ 0.1930193  -0.46685036  0.03906408 -0.22816919]', '[ 0.16956871 -0.44830261 -0.26820417  0.40739083]', '[ 0.09055011 -0.31127879 -0.50323119  0.93116007]', '[-0.02165415 -0.09380121 -0.58952709  1.1892161 ]', '[-0.14550206  0.17387773 -0.61422386  1.41936009]', '[-0.24020309  0.41196422 -0.30815479  0.91099128]', '[-0.26240779  0.52437056  0.09121898  0.1966427 ]', '[-0.1925522   0.45677     0.59247211 -0.85560345]', '[-0.03557737  0.19693013  0.94041947 -1.68102434]', '[ 0.16402445 -0.18013331  1.00061721 -1.98582856]', '[ 0.34192942 -0.55414134  0.73197041 -1.66680986]', '[ 0.44259021 -0.8207075   0.25409559 -0.95978295]', '[ 0.43986044 -0.92922657 -0.27921648 -0.11780667]', '[ 0.32432705 -0.83892692 -0.85423544  1.00492003]', '[ 0.11076836 -0.54012532 -1.23915812  1.92581144]', '[-0.14902305 -0.1049086  -1.29311851  2.30757333]', '[-0.37777789  0.32875586 -0.93332756  1.91371257]', '[-0.51580614  0.65816049 -0.41441601  1.31935071]', '[-0.52446941  0.81009841  0.32731439  0.18782972]', '[-0.37843766  0.70245743  1.10642416 -1.24743377]', '[-0.09803717  0.3273938   1.63969953 -2.42051118]', '[ 0.24538579 -0.21062841  1.70224484 -2.78852043]', '[ 0.54581225 -0.71946931  1.23259551 -2.18153552]', '[ 0.71935876 -1.05580839  0.47670341 -1.15186548]', '[ 0.73164731 -1.17514236 -0.35298663 -0.03645987]', '[ 0.57265266 -1.0414215  -1.21303731  1.37004341]', '[ 0.26093734 -0.63448659 -1.85155489  2.64342526]', '[-1.49907040e-01  1.73521181e-03 -2.15280938e+00  3.52584337e+00]', '[-0.53753813  0.64494659 -1.62713092  2.72914386]', '[-0.77583537  1.05621777 -0.72405633  1.35420795]', '[-0.82113555  1.18462523  0.27323497 -0.07037418]', '[-0.65935431  0.99849158  1.32614112 -1.79584102]', '[-0.30336702  0.47014995  2.17709826 -3.42006167]', '[ 0.17112583 -0.2979817   2.43020551 -3.9864712 ]', '[ 0.61263675 -1.01325395  1.89147195 -3.00862837]', '[ 0.90551994 -1.47897177  1.00623916 -1.64541792]', '[ 1.00762616 -1.67583823  0.00696734 -0.33143866]', '[ 0.90068983 -1.58720519 -1.06356337  1.22823529]', '[ 0.59105151 -1.17695426 -2.00145157  2.88807065]', '[ 0.11901824 -0.44080848 -2.6361045   4.34826102]', '[-0.40613989  0.44817993 -2.45350634  4.20488368]', '[-0.81157547  1.14372971 -1.53861469  2.6689904 ]', '[-1.01026255  1.51554441 -0.43617262  1.06711895]', '[-0.98492561  1.5750461   0.68283597 -0.47402924]', '[-0.73456223  1.2943748   1.79695276 -2.35907416]']</t>
+  </si>
+  <si>
+    <t>['[1,1,2]', '[2,0,1]', '[0,1,1]', '[0,2,1]', '[1,2,0]', '[2,2,2]', '[2,1,0]', '[0,0,0]', '[1,0,2]', '[1,1,1]']</t>
   </si>
   <si>
     <t>[6, 7, 8, 9, 10, 11, 18, 19, 20, 21, 22, 23, 29, 30, 31, 32, 33, 34, 41, 42, 43, 44, 45, 46, 47]</t>
@@ -184,283 +196,280 @@
     <t>['[-0.03763371 -0.01533471  0.06554052 -0.01816017]', '[-0.00754409 -0.05458322  0.2277812  -0.36241836]', '[ 0.04879627 -0.15231473  0.32089719 -0.5887683 ]', '[ 0.11397169 -0.27767857  0.31375488 -0.63332862]', '[ 0.16759438 -0.39312519  0.2086893  -0.49480525]', '[ 0.1930193  -0.46685036  0.03906408 -0.22816919]', '[ 0.16956871 -0.44830261 -0.26820417  0.40739083]', '[ 0.09055011 -0.31127879 -0.50323119  0.93116007]', '[-0.02165415 -0.09380121 -0.58952709  1.1892161 ]', '[-0.13228272  0.13968862 -0.48657385  1.08703787]', '[-0.20542731  0.31962025 -0.22562708  0.67289162]', '[-0.21756752  0.39782756  0.10766541  0.09689063]', '[-0.15109606  0.32490126  0.54216963 -0.80657469]', '[-0.01068619  0.09081112  0.82714324 -1.47439182]', '[ 0.16212513 -0.23279107  0.85391345 -1.67375883]', '[ 0.3120332  -0.54339537  0.60708552 -1.36152952]', '[ 0.39322683 -0.75586146  0.18779451 -0.73014827]', '[ 0.38412465 -0.82793881 -0.27624305  0.01454459]', '[ 0.27552572 -0.72135137 -0.78884754  1.03160865]', '[ 0.08086773 -0.43032213 -1.11647003  1.81675029]', '[-0.14966877 -0.03109877 -1.12879696  2.06540623]', '[-0.3455444   0.34863759 -0.7784691   1.63534647]', '[-0.44544803  0.59424237 -0.19906427  0.77949316]', '[-0.4218337   0.6519398   0.43007126 -0.20572333]', '[-0.26769146  0.484052    1.08142007 -1.44055859]', '[-0.00742761  0.10113176  1.45927884 -2.28595201]', '[ 0.28490347 -0.37428385  1.38589424 -2.32532176]', '[ 0.5187101  -0.77937684  0.90230152 -1.64619583]', '[ 0.63240836 -1.01433747  0.21740989 -0.68198512]', '[ 0.59278756 -1.01958166 -0.60566507  0.62852481]', '[ 0.39752784 -0.7660208  -1.31595743  1.88179849]', '[ 0.08542661 -0.29020757 -1.73661998  2.76615566]', '[-0.26054486  0.27360101 -1.62803895  2.69265107]', '[-0.53183224  0.72525907 -1.02799868  1.73308445]', '[-0.65747495  0.94866122 -0.21116234  0.48419472]', '[-0.60316944  0.88713812  0.74646124 -1.09703619]', '[-0.3667148   0.51448679  1.5802398  -2.58584684]', '[ 2.25515542e-03 -1.04226788e-01  2.01052042e+00 -3.41515113e+00]', '[ 0.38981745 -0.75816996  1.76540261 -2.93947302]', '[ 0.67971886 -1.23563438  1.09061136 -1.79181237]', '[ 0.81522073 -1.47040276  0.25012952 -0.55613563]', '[ 0.76893557 -1.43299403 -0.70634091  0.93217091]', '[ 0.53890731 -1.09497955 -1.5685075   2.44803386]', '[ 0.15769536 -0.46498696 -2.17507038  3.75054866]', '[-0.28566374  0.31885175 -2.12308403  3.81427092]', '[-0.64333931  0.96714913 -1.38377582  2.55626676]', '[-0.82476188  1.32821982 -0.41497441  1.0541805 ]', '[-0.80769438  1.39053182  0.57925977 -0.43113385]', '[-0.58966747  1.12643161  1.57705339 -2.21920745]', '[-0.19115743  0.50615398  2.34648211 -3.90612928]']</t>
   </si>
   <si>
-    <t>['[1,1,2]', '[2,1,0]', '[1,1,1]', '[1,2,0]', '[2,0,1]', '[0,0,0]', '[0,2,1]', '[0,1,1]', '[2,2,2]', '[1,0,2]']</t>
+    <t>['[1,0,2]', '[0,1,1]', '[2,2,2]', '[1,2,0]', '[2,1,0]', '[1,1,2]', '[2,0,1]', '[0,2,1]', '[1,1,1]', '[0,0,0]']</t>
   </si>
   <si>
     <t>[0,2,1]</t>
   </si>
   <si>
-    <t>[10, 43, 49]</t>
-  </si>
-  <si>
-    <t>[0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 1, 2, 2, 2, 2, 2, 2]</t>
-  </si>
-  <si>
-    <t>['[-0.03763371 -0.01533471  0.06554052 -0.01816017]', '[-0.00754409 -0.05458322  0.2277812  -0.36241836]', '[ 0.04879627 -0.15231473  0.32089719 -0.5887683 ]', '[ 0.11397169 -0.27767857  0.31375488 -0.63332862]', '[ 0.16759438 -0.39312519  0.2086893  -0.49480525]', '[ 0.1930193  -0.46685036  0.03906408 -0.22816919]', '[ 0.15689524 -0.41528579 -0.3922057   0.73207416]', '[ 0.04309269 -0.18588535 -0.71796191  1.51055937]', '[-0.1147829   0.15904975 -0.81547211  1.84906375]', '[-0.26363568  0.51494657 -0.63159042  1.62703318]', '[-0.3423183   0.7521378  -0.14060109  0.71307914]', '[-0.32986696  0.82507007  0.26174694  0.01157006]', '[-0.21867408  0.69719091  0.82971684 -1.27020617]', '[-0.0101959   0.33320795  1.21088597 -2.29634067]', '[ 0.24086125 -0.17507996  1.22699953 -2.64392904]', '[ 0.45068315 -0.66552171  0.81451886 -2.1511033 ]', '[ 0.55140866 -1.00706233  0.17533379 -1.22822986]', '[ 0.51965815 -1.1499925  -0.48264437 -0.19681171]', '[ 0.34623271 -1.03104052 -1.21976808  1.37289962]', '[ 0.04761233 -0.61205987 -1.71578188  2.75474748]', '[-0.31119578  0.0220535  -1.77749619  3.40243743]', '[-0.62038811  0.66353368 -1.23006516  2.85184089]', '[-0.78111832  1.12536128 -0.35201109  1.727584  ]', '[-0.75864201  1.34819911  0.56721284  0.49316093]', '[-0.54516508  1.26788669  1.52793529 -1.29584944]', '[-0.16689326  0.83346406  2.19773703 -3.00786852]', '[ 0.30277521  0.10876847  2.38822425 -4.02752637]', '[ 0.73272263 -0.66353711  1.79647777 -3.47172152]', '[ 0.99216277 -1.23319197  0.7646531  -2.19306318]', '[ 1.03339088 -1.53947977 -0.35123678 -0.8665234 ]', '[ 0.84051921 -1.52577031 -1.54466411  1.02016786]', '[ 0.43312651 -1.12255932 -2.47740848  3.01990975]', '[-0.12379177 -0.336029   -2.9874819   4.66773353]', '[-0.69540914  0.60397831 -2.56263705  4.3813569 ]', '[-1.1042574   1.33613019 -1.47961742  2.90402759]', '[-1.27984591  1.77500772 -0.26925663  1.50760897]', '[-1.21230729  1.94123835  0.93417721  0.14188163]', '[-0.90079944  1.77574489  2.1404249  -1.83502545]', '[-0.37685134  1.18976214  3.04481014 -4.0512127 ]', '[ 0.28873561  0.17914955  3.47279272 -5.77033758]', '[ 0.92336826 -0.91571597  2.6994366  -4.80800107]', '[ 1.33826372 -1.70374849  1.43133679 -3.11590991]', '[ 1.49396529 -2.18436235  0.12578064 -1.71896523]', '[ 1.37799769 -2.35022295 -1.26757331  0.07499134]', '[ 0.99794524 -2.14170253 -2.48868704  2.05500729]', '[ 0.40758135 -1.50643969 -3.35171132  4.35130914]', '[-0.31939394 -0.39980077 -3.81341834  6.50641893]', '[-1.0239425   0.87174709 -3.00995915  5.70598923]', '[-1.48435349  1.82106649 -1.58453387  3.85691023]', '[-1.65357253  2.42551965 -0.12377724  2.23409836]']</t>
-  </si>
-  <si>
-    <t>['[2,1,0]', '[1,2,0]', '[1,1,1]', '[0,0,0]', '[1,0,2]', '[1,1,2]', '[0,1,1]', '[2,0,1]', '[2,2,2]', '[0,2,1]']</t>
-  </si>
-  <si>
-    <t>[7, 9, 18, 19, 31, 32, 33, 35, 49]</t>
-  </si>
-  <si>
-    <t>['[-0.03763371 -0.01533471  0.06554052 -0.01816017]', '[-0.00754409 -0.05458322  0.2277812  -0.36241836]', '[ 0.04879627 -0.15231473  0.32089719 -0.5887683 ]', '[ 0.11397169 -0.27767857  0.31375488 -0.63332862]', '[ 0.16759438 -0.39312519  0.2086893  -0.49480525]', '[ 0.1930193  -0.46685036  0.03906408 -0.22816919]', '[ 0.15689524 -0.41528579 -0.3922057   0.73207416]', '[ 0.05612841 -0.21966732 -0.59032268  1.17838443]', '[-0.07991814  0.06672291 -0.73262715  1.61264609]', '[-0.20683181  0.35785759 -0.50218441  1.23042577]', '[-0.28278502  0.57054493 -0.23790294  0.85533496]', '[-0.29707407  0.68829467  0.0984662   0.30688696]', '[-0.22097706  0.62826106  0.64693498 -0.89287033]', '[-0.04835833  0.3440623   1.04244346 -1.89055068]', '[ 0.17548637 -0.09111843  1.13428326 -2.3430074 ]', '[ 0.37842341 -0.5406038   0.83874918 -2.04258221]', '[ 0.49388705 -0.87579433  0.29213375 -1.26258475]', '[ 0.49135812 -1.0354458  -0.3139346  -0.32433661]', '[ 0.36330116 -0.97681205 -0.94134712  0.89779769]', '[ 0.12853633 -0.68698948 -1.36279841  1.95063418]', '[-0.17210264 -0.19674795 -1.57455435  2.83003732]', '[-0.46661982  0.37829955 -1.28648728  2.75620646]', '[-0.65855542  0.85293417 -0.59043934  1.9143531 ]', '[-0.69419161  1.12825725  0.23691403  0.82095887]', '[-0.54844019  1.12226041  1.19083738 -0.87803883]', '[-0.23383677  0.78111631  1.90466795 -2.49728449]', '[ 0.18570111  0.15942863  2.1946026  -3.54831178]', '[ 0.59483929 -0.5412411   1.78549331 -3.24237962]', '[ 0.86739152 -1.08175682  0.89695662 -2.10776563]', '[ 0.94533811 -1.37822891 -0.12236809 -0.85213849]', '[ 0.80332312 -1.36786145 -1.27356227  0.96599742]', '[ 0.4595839  -1.01354753 -2.11690136  2.56859611]', '[-0.0171945  -0.36366807 -2.55534029  3.77732827]', '[-0.5085885   0.39184175 -2.22279408  3.50581413]', '[-0.87601386  0.99276896 -1.38849331  2.41532286]', '[-1.04050009  1.3219074  -0.2459396   0.88581867]', '[-0.96488991  1.3221806   0.99131011 -0.89239256]', '[-0.65167336  0.95566154  2.11069501 -2.79021098]', '[-0.1415661   0.21896622  2.88989695 -4.40997761]', '[ 0.43836486 -0.67284223  2.74283043 -4.16358121]', '[ 0.90811693 -1.3617871   1.89440886 -2.6732994 ]', '[ 1.18253205 -1.74903133  0.82915035 -1.22981726]', '[ 1.23511559 -1.86270199 -0.30605415  0.08626669]', '[ 1.04660924 -1.66374442 -1.56512685  1.93660099]', '[ 0.61713895 -1.06704003 -2.70316018  4.07806637]', '[-0.0117135  -0.04945183 -3.43728527  5.79971531]', '[-0.66353101  1.04227784 -2.90381096  4.74672564]', '[-1.14170703  1.80935667 -1.84845979  2.964046  ]', '[-1.39553982  2.25182198 -0.67808986  1.50276653]', '[-1.40451936  2.39775305  0.5847867  -0.04111358]']</t>
-  </si>
-  <si>
-    <t>['[2,2,2]', '[0,1,1]', '[2,0,1]', '[0,2,1]', '[0,0,0]', '[1,0,2]', '[1,1,2]', '[1,1,1]', '[2,1,0]', '[1,2,0]']</t>
-  </si>
-  <si>
-    <t>[6, 8, 9, 10, 11, 17, 22, 29, 30, 31, 33, 34, 35, 42, 43, 44]</t>
-  </si>
-  <si>
-    <t>[0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0]</t>
-  </si>
-  <si>
-    <t>['[-0.03763371 -0.01533471  0.06554052 -0.01816017]', '[-0.00754409 -0.05458322  0.2277812  -0.36241836]', '[ 0.04879627 -0.15231473  0.32089719 -0.5887683 ]', '[ 0.11397169 -0.27767857  0.31375488 -0.63332862]', '[ 0.16759438 -0.39312519  0.2086893  -0.49480525]', '[ 0.1930193  -0.46685036  0.03906408 -0.22816919]', '[ 0.16956871 -0.44830261 -0.26820417  0.40739083]', '[ 0.07764819 -0.2777752  -0.62973474  1.26105599]', '[-0.05644144 -0.00156921 -0.67466795  1.43082082]', '[-0.176879    0.26464326 -0.49680588  1.16644284]', '[-0.24437082  0.44354834 -0.16144791  0.58767594]', '[-0.23811916  0.49146993  0.22268636 -0.11303333]', '[-0.14628459  0.36858689  0.67571923 -1.08783928]', '[ 0.01978706  0.07638813  0.9433042  -1.76004435]', '[ 0.21033531 -0.29678408  0.90916704 -1.8707429 ]', '[ 0.36330825 -0.6337797   0.58276212 -1.4285527 ]', '[ 0.43278886 -0.84843063  0.09887992 -0.69032858]', '[ 0.3904719  -0.87441782 -0.51213974  0.42756095]', '[ 0.22385736 -0.65203064 -1.12511868  1.76583304]', '[-0.04233168 -0.19275713 -1.47502304  2.71887815]', '[-0.33318049  0.37251836 -1.34838015  2.76803784]', '[-0.55154982  0.8576662  -0.78649164  1.99766317]', '[-0.62594298  1.12482831  0.04729688  0.66334023]', '[-0.5253831   1.09404643  0.93887652 -0.96773326]', '[-0.26166185  0.74134275  1.65887585 -2.52702218]', '[ 0.1141262   0.1168862   2.00877034 -3.55289981]', '[ 0.49413687 -0.58535986  1.682275   -3.2571115 ]', '[ 0.7549454  -1.13008677  0.88314366 -2.13281739]', '[ 0.83915329 -1.43170565 -0.04569479 -0.87985697]', '[ 0.73079612 -1.45549222 -1.0161088   0.64449825]', '[ 0.44564858 -1.17249448 -1.79383367  2.17885011]', '[ 0.03444456 -0.59759076 -2.24752388  3.4756109 ]', '[-0.42497762  0.1757178  -2.2179327   3.99675096]', '[-0.78831734  0.86498111 -1.33914266  2.76467881]', '[-0.94624735  1.26603882 -0.22888605  1.2439547 ]', '[-0.88074314  1.36283325  0.86992643 -0.28227819]', '[-0.59890901  1.12106616  1.91184887 -2.14732392]', '[-0.13587807  0.50887604  2.6437903  -3.88358903]', '[ 0.40876591 -0.33930189  2.64472395 -4.27177669]', '[ 0.86419294 -1.08488335  1.82736622 -3.05747023]', '[ 1.12349947 -1.55424418  0.74655984 -1.6526078 ]', '[ 1.15937535 -1.75222822 -0.38703744 -0.32962029]', '[ 0.96501353 -1.65757013 -1.53308146  1.30023765]', '[ 0.56019754 -1.21977332 -2.47011178  3.09752336]', '[ 1.45041750e-03 -4.30248520e-01 -3.01864574e+00  4.64083003e+00]', '[-0.59474636  0.53358189 -2.76385876  4.61272029]', '[-1.05079576  1.31244545 -1.73851208  3.11486403]', '[-1.28072882  1.78874405 -0.55048598  1.67963798]', '[-1.26981952  1.99050452  0.65435574  0.33382823]', '[-1.01088326  1.86934407  1.90356998 -1.58089888]']</t>
-  </si>
-  <si>
-    <t>['[1,2,0]', '[1,1,2]', '[2,0,1]', '[2,2,2]', '[0,2,1]', '[0,1,1]', '[1,1,1]', '[2,1,0]', '[1,0,2]', '[0,0,0]']</t>
-  </si>
-  <si>
-    <t>[6, 7, 8, 9, 10, 11, 18, 19, 21, 22, 31, 32, 33, 34, 35, 42, 43, 44, 45, 46, 47]</t>
+    <t>[9, 30, 32, 33, 35, 43, 46, 47]</t>
+  </si>
+  <si>
+    <t>['[-0.03763371 -0.01533471  0.06554052 -0.01816017]', '[-0.00754409 -0.05458322  0.2277812  -0.36241836]', '[ 0.04879627 -0.15231473  0.32089719 -0.5887683 ]', '[ 0.11397169 -0.27767857  0.31375488 -0.63332862]', '[ 0.16759438 -0.39312519  0.2086893  -0.49480525]', '[ 0.1930193  -0.46685036  0.03906408 -0.22816919]', '[ 0.15689524 -0.41528579 -0.3922057   0.73207416]', '[ 0.04309269 -0.18588535 -0.71796191  1.51055937]', '[-0.1147829   0.15904975 -0.81547211  1.84906375]', '[-0.25091076  0.48179199 -0.51035257  1.30778282]', '[-0.32121683  0.69438874 -0.17639946  0.78285774]', '[-0.31827759  0.7861638   0.20464523  0.12666995]', '[-0.21934835  0.68380354  0.76574822 -1.13210247]', '[-0.02340624  0.3482126   1.15242094 -2.15660658]', '[ 0.21849146 -0.13629065  1.19779057 -2.55439038]', '[ 0.42663265 -0.61635764  0.82629218 -2.1350107 ]', '[ 0.53286226 -0.95986424  0.21615257 -1.25957754]', '[ 0.51097799 -1.1121177  -0.42697836 -0.256841  ]', '[ 0.34884672 -1.00686712 -1.16409219  1.29612661]', '[ 0.06067106 -0.60469827 -1.66822966  2.6651003 ]', '[-0.29032976  0.01213618 -1.74963195  3.32577762]', '[-0.59710669  0.64232971 -1.23410718  2.8159998 ]', '[-0.76142249  1.09996019 -0.38240518  1.71881684]', '[-0.74694655  1.3229455   0.51906987  0.50317188]', '[-0.54381334  1.24621979  1.47463605 -1.26956728]', '[-0.17573319  0.81879055  2.15055213 -2.96447576]', '[ 0.28568649  0.10389847  2.35421408 -3.97635846]', '[ 0.71094464 -0.65960465  1.78438621 -3.4368946 ]', '[ 0.97010194 -1.22366542  0.77325359 -2.17012616]', '[ 1.01483653 -1.52601113 -0.32515997 -0.85032898]', '[ 0.83700538 -1.53493034 -1.42310986  0.7749715 ]', '[ 0.45381661 -1.18371907 -2.35692575  2.74537274]', '[-0.06883851 -0.48081925 -2.77507613  4.13768632]', '[-0.60002475  0.35838817 -2.38720102  3.94208875]', '[-0.98903346  1.03803673 -1.43867958  2.76265818]', '[-1.15373808  1.43131128 -0.20201486  1.18648071]', '[-1.0797386   1.53942012  0.93229805 -0.12034534]', '[-0.77210565  1.32192689  2.10795704 -2.08823813]', '[-0.25558666  0.69540159  2.99068578 -4.13133164]', '[ 0.37630948 -0.24672396  3.14892567 -4.90613249]', '[ 0.93117365 -1.11206158  2.29727033 -3.57351514]', '[ 1.27771045 -1.67070701  1.14913645 -2.05223838]', '[ 1.38685736 -1.94760093 -0.06120641 -0.73279305]', '[ 1.24717832 -1.93927667 -1.32223933  0.84071884]', '[ 0.85987706 -1.57066427 -2.51743559  2.90671387]', '[ 0.25610183 -0.75304657 -3.46463802  5.2506145 ]', '[-0.457218    0.38556116 -3.44165068  5.6182544 ]', '[-1.04234047  1.32390374 -2.33306123  3.66090781]', '[-1.39091925  1.89485684 -1.14002709  2.10736484]', '[-1.49562141  2.18348462  0.09484649  0.79472033]']</t>
+  </si>
+  <si>
+    <t>['[2,1,0]', '[0,2,1]', '[1,0,2]', '[2,2,2]', '[1,1,1]', '[2,0,1]', '[0,1,1]', '[1,1,2]', '[1,2,0]', '[0,0,0]']</t>
+  </si>
+  <si>
+    <t>[10, 11, 19, 20, 21, 23, 30, 31, 43, 44]</t>
+  </si>
+  <si>
+    <t>[0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 1, 2, 2, 2, 2, 2, 2, 2]</t>
+  </si>
+  <si>
+    <t>['[-0.03763371 -0.01533471  0.06554052 -0.01816017]', '[-0.00754409 -0.05458322  0.2277812  -0.36241836]', '[ 0.04879627 -0.15231473  0.32089719 -0.5887683 ]', '[ 0.11397169 -0.27767857  0.31375488 -0.63332862]', '[ 0.16759438 -0.39312519  0.2086893  -0.49480525]', '[ 0.1930193  -0.46685036  0.03906408 -0.22816919]', '[ 0.15689524 -0.41528579 -0.3922057   0.73207416]', '[ 0.04309269 -0.18588535 -0.71796191  1.51055937]', '[-0.1147829   0.15904975 -0.81547211  1.84906375]', '[-0.26363568  0.51494657 -0.63159042  1.62703318]', '[-0.3423183   0.7521378  -0.14060109  0.71307914]', '[-0.31834832  0.79441559  0.37391128 -0.28985184]', '[-0.18669612  0.60966499  0.9186555  -1.52917439]', '[ 0.03463692  0.20461547  1.24297207 -2.42940656]', '[ 0.28282653 -0.308983    1.16536595 -2.56170684]', '[ 0.47339348 -0.76693654  0.69326653 -1.92910836]', '[ 0.54862155 -1.05940145  0.04837448 -0.97035556]', '[ 0.4936206  -1.15081099 -0.5844728   0.05628529]', '[ 0.3035996  -0.98327937 -1.28296628  1.60245346]', '[ 0.00875742 -0.55543996 -1.60928017  2.5955807 ]', '[-3.10416341e-01  2.81679705e-03 -1.49761883e+00  2.82396175e+00]', '[-0.55595237  0.50727131 -0.89472488  2.10124991]', '[-0.66399962  0.84553472 -0.1634427   1.23722826]', '[-0.60786679  0.96275329  0.7118584  -0.0704182 ]', '[-0.378597    0.78875601  1.54124386 -1.64981703]', '[-0.01333341  0.32362993  2.03618273 -2.89148459]', '[ 0.39523766 -0.29509895  1.93969456 -3.08707426]', '[ 0.72253827 -0.83780521  1.26705052 -2.23550651]', '[ 0.88599001 -1.17083464  0.34792349 -1.08029909]', '[ 0.85914964 -1.26756715 -0.61043931  0.11889584]', '[ 0.63891366 -1.09268882 -1.56159447  1.63375443]', '[ 0.25226172 -0.62002827 -2.24111284  3.02698314]', '[-0.23228841  0.0904981  -2.47793989  3.83526292]', '[-0.68218448  0.80099907 -1.91585281  3.07970375]', '[-0.97286211  1.28863257 -0.95820473  1.78132636]', '[-1.05876431  1.51607169  0.10430171  0.49751998]', '[-0.91548099  1.43506032  1.31132884 -1.32554278]', '[-0.54451877  0.97426797  2.36251296 -3.29827656]', '[ 0.0048545   0.1374317   3.01076065 -4.84728462]', '[ 0.58531831 -0.80613245  2.63043379 -4.2519624 ]', '[ 1.01798152 -1.50061731  1.65335141 -2.6804168 ]', '[ 1.2375592  -1.89124023  0.52968722 -1.25588794]', '[ 1.22051721 -1.98655718 -0.69433958  0.30403479]', '[ 0.96583784 -1.76182446 -1.82687811  1.97682876]', '[ 0.50407326 -1.17926996 -2.74785574  3.87525802]', '[-0.11934391 -0.20006464 -3.3592632   5.67099225]', '[-0.75157245  0.89309543 -2.77632526  4.86325154]', '[-1.19334568  1.6899326  -1.61415972  3.13279456]', '[-1.39289821  2.16834981 -0.37686052  1.68739623]', '[-1.3447217   2.3696512   0.84996081  0.31925259]']</t>
+  </si>
+  <si>
+    <t>['[1,2,0]', '[2,0,1]', '[0,2,1]', '[1,0,2]', '[1,1,2]', '[2,1,0]', '[2,2,2]', '[0,0,0]', '[0,1,1]', '[1,1,1]']</t>
+  </si>
+  <si>
+    <t>[6, 10, 11, 19, 20, 21, 22, 23, 31, 32, 33, 42, 43, 44, 45]</t>
+  </si>
+  <si>
+    <t>[0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0]</t>
+  </si>
+  <si>
+    <t>['[-0.03763371 -0.01533471  0.06554052 -0.01816017]', '[-0.00754409 -0.05458322  0.2277812  -0.36241836]', '[ 0.04879627 -0.15231473  0.32089719 -0.5887683 ]', '[ 0.11397169 -0.27767857  0.31375488 -0.63332862]', '[ 0.16759438 -0.39312519  0.2086893  -0.49480525]', '[ 0.1930193  -0.46685036  0.03906408 -0.22816919]', '[ 0.16956871 -0.44830261 -0.26820417  0.40739083]', '[ 0.07764819 -0.2777752  -0.62973474  1.26105599]', '[-0.06966349  0.03261704 -0.80302667  1.76452698]', '[-0.22465905  0.39058523 -0.70217906  1.72562277]', '[-0.32253645  0.65927546 -0.25526332  0.91716067]', '[-0.32285793  0.74781573  0.25044842 -0.03831633]', '[-0.21453864  0.61479579  0.81230177 -1.26939483]', '[-0.01059352  0.2580195   1.18136841 -2.22048791]', '[ 0.23298114 -0.22659655  1.18409935 -2.4888901 ]', '[ 0.4350707  -0.68326374  0.78462081 -1.97903321]', '[ 0.53274257 -0.99256228  0.17556515 -1.08106037]', '[ 0.50395423 -1.10939893 -0.45461235 -0.08376693]', '[ 0.33748196 -0.97071252 -1.18104876  1.45665387]', '[ 0.05850343 -0.57044066 -1.55605401  2.4736414 ]', '[-0.25673002 -0.02940666 -1.51363162  2.7803223 ]', '[-0.51234763  0.47469592 -0.97604139  2.13506984]', '[-0.62926844  0.79273221 -0.17258593  1.00730756]', '[-0.57969612  0.87079123  0.65776102 -0.23026228]', '[-0.36388392  0.67247975  1.46330339 -1.72727147]', '[-0.01616619  0.20472719  1.93721438 -2.8295284 ]', '[ 0.37048905 -0.38563379  1.82544809 -2.87957942]', '[ 0.6776751  -0.88280982  1.18665204 -2.0034804 ]', '[ 0.8302923  -1.17124447  0.32081486 -0.86809603]', '[ 0.78344194 -1.1731144  -0.78091733  0.85158044]', '[ 0.52493828 -0.82763558 -1.77414898  2.59758047]', '[ 0.10765979 -0.18936242 -2.30507668  3.62473587]', '[-0.34502963  0.52072029 -2.09703943  3.23385009]', '[-0.69292309  1.03837149 -1.32620895  1.87693636]', '[-0.87241323  1.29313299 -0.44765624  0.66786172]', '[-0.84850253  1.25260561  0.68497396 -1.07540148]', '[-0.60242281  0.8581809   1.75362532 -2.87232731]', '[-0.16605881  0.12291876  2.51242913 -4.30664404]', '[ 0.34085699 -0.73836678  2.40809307 -4.00475052]', '[ 0.75524666 -1.40579041  1.67990451 -2.61629529]', '[ 0.9990142  -1.78643673  0.73558284 -1.20785791]', '[ 1.04422867 -1.89453242 -0.28607808  0.12198259]', '[ 0.87977136 -1.71234741 -1.3407934   1.71687779]', '[ 0.51849155 -1.19768933 -2.23831851  3.44736938]', '[ 0.00502633 -0.34634633 -2.79722619  4.89449088]', '[-0.53182376  0.61654255 -2.40103332  4.37821204]', '[-0.92177376  1.35350915 -1.44658438  2.93840243]', '[-1.10139136  1.79668646 -0.34077744  1.51301112]', '[-1.0583601   1.9623722   0.75949607  0.14100201]', '[-0.7926264   1.8029689   1.85844359 -1.75644333]']</t>
+  </si>
+  <si>
+    <t>['[0,0,0]', '[1,0,2]', '[2,2,2]', '[2,1,0]', '[2,0,1]', '[1,2,0]', '[0,2,1]', '[1,1,1]', '[1,1,2]', '[0,1,1]']</t>
+  </si>
+  <si>
+    <t>[6, 7, 8, 9, 10, 11, 18, 19, 20, 21, 22, 23, 29, 30, 32, 35, 42, 44, 45, 46, 47]</t>
+  </si>
+  <si>
+    <t>[0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0]</t>
+  </si>
+  <si>
+    <t>['[-0.03763371 -0.01533471  0.06554052 -0.01816017]', '[-0.00754409 -0.05458322  0.2277812  -0.36241836]', '[ 0.04879627 -0.15231473  0.32089719 -0.5887683 ]', '[ 0.11397169 -0.27767857  0.31375488 -0.63332862]', '[ 0.16759438 -0.39312519  0.2086893  -0.49480525]', '[ 0.1930193  -0.46685036  0.03906408 -0.22816919]', '[ 0.16956871 -0.44830261 -0.26820417  0.40739083]', '[ 0.09055011 -0.31127879 -0.50323119  0.93116007]', '[-0.02165415 -0.09380121 -0.58952709  1.1892161 ]', '[-0.13228272  0.13968862 -0.48657385  1.08703787]', '[-0.20542731  0.31962025 -0.22562708  0.67289162]', '[-0.21756752  0.39782756  0.10766541  0.09689063]', '[-0.15109606  0.32490126  0.54216963 -0.80657469]', '[-0.01068619  0.09081112  0.82714324 -1.47439182]', '[ 0.16212513 -0.23279107  0.85391345 -1.67375883]', '[ 0.3120332  -0.54339537  0.60708552 -1.36152952]', '[ 0.39322683 -0.75586146  0.18779451 -0.73014827]', '[ 0.38412465 -0.82793881 -0.27624305  0.01454459]', '[ 0.27552572 -0.72135137 -0.78884754  1.03160865]', '[ 0.08086773 -0.43032213 -1.11647003  1.81675029]', '[-0.14966877 -0.03109877 -1.12879696  2.06540623]', '[-0.3455444   0.34863759 -0.7784691   1.63534647]', '[-0.44544803  0.59424237 -0.19906427  0.77949316]', '[-0.4218337   0.6519398   0.43007126 -0.20572333]', '[-0.26769146  0.484052    1.08142007 -1.44055859]', '[-0.00742761  0.10113176  1.45927884 -2.28595201]', '[ 0.28490347 -0.37428385  1.38589424 -2.32532176]', '[ 0.5187101  -0.77937684  0.90230152 -1.64619583]', '[ 0.63240836 -1.01433747  0.21740989 -0.68198512]', '[ 0.59278756 -1.01958166 -0.60566507  0.62852481]', '[ 0.39752784 -0.7660208  -1.31595743  1.88179849]', '[ 0.07282687 -0.2572419  -1.8620853   3.09464014]', '[-0.29418867  0.36286747 -1.70471311  2.90770478]', '[-0.58614612  0.8739317  -1.15375551  2.10523548]', '[-0.74013807  1.18569395 -0.36623707  0.99453432]', '[-0.71982375  1.24196137  0.56279309 -0.43223392]', '[-0.51124373  0.98401606  1.49753531 -2.14601118]', '[-0.13669643  0.39429202  2.18036283 -3.65222539]', '[ 0.3156273  -0.39097408  2.20548017 -3.92316406]', '[ 0.69570119 -1.07877533  1.52118362 -2.83824612]', '[ 0.90809724 -1.51284202  0.58355864 -1.50338556]', '[ 0.9261125  -1.68263663 -0.39976251 -0.19611643]', '[ 0.74574955 -1.56505775 -1.37730081  1.38186352]', '[ 0.38017572 -1.09890636 -2.23869471  3.28547242]', '[-0.11510022 -0.30211087 -2.61043605  4.49475151]', '[-0.60157183  0.56923561 -2.10895282  3.92087067]', '[-0.92082899  1.19965875 -1.04442537  2.34526209]', '[-1.01385528  1.51061017  0.11426183  0.77412884]', '[-0.87052791  1.48354502  1.29656803 -1.05835557]', '[-0.50793274  1.07799781  2.28919065 -3.0109801 ]']</t>
+  </si>
+  <si>
+    <t>['[0,0,0]', '[2,0,1]', '[2,2,2]', '[1,1,2]', '[1,2,0]', '[0,1,1]', '[1,1,1]', '[0,2,1]', '[1,0,2]', '[2,1,0]']</t>
+  </si>
+  <si>
+    <t>['[1,1,1]', '[2,1,0]', '[0,0,0]', '[1,2,0]', '[1,1,2]', '[0,2,1]', '[2,2,2]', '[0,1,1]', '[2,0,1]', '[1,0,2]']</t>
+  </si>
+  <si>
+    <t>[1,0,2]</t>
+  </si>
+  <si>
+    <t>[2, 6, 13, 26, 27]</t>
+  </si>
+  <si>
+    <t>[0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2]</t>
+  </si>
+  <si>
+    <t>['[-0.03763371 -0.01533471  0.06554052 -0.01816017]', '[-0.00754409 -0.05458322  0.2277812  -0.36241836]', '[ 0.03557041 -0.11811661  0.19275289 -0.25552579]', '[ 0.07892797 -0.1849336   0.22986116 -0.39424827]', '[ 0.12271824 -0.267417    0.19671429 -0.40996627]', '[ 0.15338212 -0.34091394  0.10180504 -0.30861109]', '[ 0.14821295 -0.35214844 -0.15231642  0.19659226]', '[ 0.08221469 -0.23257051 -0.49175499  0.97158045]', '[-0.03852789  0.01808886 -0.68300946  1.472231  ]', '[-0.17530395  0.32553648 -0.64578239  1.52482289]', '[-0.28221181  0.59893637 -0.39589606  1.15382079]', '[-0.32593922  0.77085441 -0.03233943  0.54190511]', '[-0.27157263  0.74958069  0.56429783 -0.74659547]', '[-0.12059762  0.51330099  0.91464885 -1.57097901]', '[ 0.09066437  0.11532029  1.14531511 -2.31177496]', '[ 0.31120891 -0.36024729  0.99513382 -2.31549468]', '[ 0.46579132 -0.76621445  0.5131015  -1.67103872]', '[ 0.50785055 -1.01097665 -0.09785788 -0.75551401]', '[ 0.4082837  -1.00773753 -0.87564398  0.77996152]', '[ 0.16978412 -0.70582411 -1.46943315  2.20015306]', '[-0.15719002 -0.15976404 -1.72343828  3.12205891]', '[-0.48016765  0.46608824 -1.4129967   2.95428207]', '[-0.69278118  0.96779826 -0.67114478  1.99372036]', '[-0.74056871  1.25124795  0.19553971  0.8284781 ]', '[-0.60006672  1.24301058  1.18097917 -0.91021068]', '[-0.28324387  0.88848489  1.94065243 -2.6112849 ]', '[ 0.13813487  0.26110717  2.17894769 -3.49703121]', '[ 0.54024547 -0.4158921   1.73244634 -3.05862972]', '[ 0.81050755 -0.93611726  0.92083717 -2.07059943]', '[ 0.89813879 -1.23261343 -0.05299527 -0.88334427]', '[ 0.77189974 -1.23191486 -1.18761872  0.89801322]', '[ 0.43600293 -0.86932571 -2.12695097  2.71801932]', '[-0.0520103  -0.17275024 -2.6462107   4.06066353]', '[-0.56203307  0.63268907 -2.3137281   3.71427391]', '[-0.93835408  1.24678885 -1.3999724   2.3813192 ]', '[-1.1117798   1.58752955 -0.32226686  1.03993626]', '[-1.06623732  1.66483785  0.77009157 -0.27405436]', '[-0.79416141  1.42094023  1.921838   -2.19728754]', '[-0.31242007  0.77384788  2.84316996 -4.25276831]', '[ 0.30119409 -0.20967432  3.11438427 -5.2012965 ]', '[ 0.85487338 -1.1381606   2.30904533 -3.88098164]', '[ 1.20591585 -1.75289157  1.18150992 -2.30441012]', '[ 1.32321595 -2.07465114 -0.01193058 -0.93091551]', '[ 1.18908532 -2.08133267 -1.31186702  0.8818323 ]', '[ 0.80979277 -1.70726097 -2.44336159  2.91075253]', '[ 0.22850564 -0.89463203 -3.32275125  5.22133417]', '[-0.47392537  0.29744706 -3.4772332   6.18939333]', '[-1.06974067  1.37660494 -2.3813497   4.44013672]', '[-1.41773326  2.0924929  -1.09413075  2.7917747 ]', '[-1.50749731  2.51134566  0.19131242  1.41190228]']</t>
+  </si>
+  <si>
+    <t>['[0,0,0]', '[2,2,2]', '[1,1,2]', '[2,0,1]', '[1,2,0]', '[1,1,1]', '[1,0,2]', '[0,1,1]', '[2,1,0]', '[0,2,1]']</t>
+  </si>
+  <si>
+    <t>[2, 17, 26, 27, 38, 40, 42, 43]</t>
+  </si>
+  <si>
+    <t>['[-0.03763371 -0.01533471  0.06554052 -0.01816017]', '[-0.00754409 -0.05458322  0.2277812  -0.36241836]', '[ 0.03557041 -0.11811661  0.19275289 -0.25552579]', '[ 0.07892797 -0.1849336   0.22986116 -0.39424827]', '[ 0.12271824 -0.267417    0.19671429 -0.40996627]', '[ 0.15338212 -0.34091394  0.10180504 -0.30861109]', '[ 0.16107551 -0.38557729 -0.0273968  -0.13010444]', '[ 0.11689442 -0.32478194 -0.40419263  0.72290359]', '[ 0.00699758 -0.10946448 -0.66682387  1.37864006]', '[-0.13518691  0.19851722 -0.71460523  1.62157325]', '[-0.26216055  0.50605306 -0.52049404  1.38437545]', '[-0.33248769  0.73016948 -0.16679196  0.82126441]', '[-0.32601137  0.82598862  0.22935372  0.12936813]', '[-0.22150391  0.72152019  0.79592472 -1.15602661]', '[-0.0192686   0.3781773   1.18490047 -2.21077503]', '[ 0.2290512  -0.11986802  1.22786797 -2.63211669]', '[ 0.44182695 -0.61536383  0.84056607 -2.20726204]', '[ 0.53745237 -0.94123861  0.10210033 -1.02155931]', '[ 0.49388289 -1.0485734  -0.52699375 -0.04831552]', '[ 0.31375965 -0.90466538 -1.24194464  1.46976687]', '[ 0.0139665  -0.47588959 -1.69975452  2.73923965]', '[-0.33448785  0.13505964 -1.68903324  3.18446589]', '[-0.62201616  0.72079612 -1.11387439  2.54018984]', '[-0.76175175  1.1216325  -0.26306301  1.43719095]', '[-0.7256274   1.29019758  0.61376705  0.24183836]', '[-0.50642052  1.162895    1.54086534 -1.51286057]', '[-0.13914398  0.72133601  2.06976215 -2.83834887]', '[ 0.28761018  0.08054192  2.09171103 -3.36977085]', '[ 0.66375506 -0.56809248  1.57330917 -2.93435068]', '[ 0.89005672 -1.04901473  0.65479683 -1.83041639]', '[ 0.91945494 -1.29381599 -0.36122827 -0.60826291]', '[ 0.73169311 -1.23423272 -1.48692727  1.21582797]', '[ 0.34096743 -0.8040797  -2.36623892  3.06138397]', '[-0.18192043 -0.05253399 -2.73695712  4.21653058]', '[-0.68982258  0.75068447 -2.21325689  3.56609325]', '[-1.03574461  1.32750238 -1.2088113   2.18510927]', '[-1.16596219  1.63065489 -0.08606529  0.8586529 ]', '[-1.05437912  1.62224332  1.1868499  -0.95886577]', '[-0.7097309   1.25927648  2.22487551 -2.69971096]', '[-0.17287446  0.5121195   3.06735493 -4.67997056]', '[ 0.44366945 -0.45754853  2.91027825 -4.61231215]', '[ 0.94370328 -1.24536708  2.0150754  -3.16671397]', '[ 1.22714033 -1.70333356  0.80688095 -1.45732538]', '[ 1.26415952 -1.84006894 -0.43557162  0.08314742]', '[ 1.04843163 -1.64044684 -1.70498656  1.9515547 ]', '[ 0.59161395 -1.03707834 -2.83248367  4.12723995]', '[-0.0586482  -0.0128769  -3.5125265   5.79040055]', '[-0.71856577  1.0656425  -2.91690383  4.64233245]', '[-1.19642567  1.81153424 -1.83441849  2.8636748 ]', '[-1.44561333  2.23600614 -0.64719053  1.42375737]']</t>
+  </si>
+  <si>
+    <t>['[1,1,2]', '[0,2,1]', '[1,1,1]', '[2,1,0]', '[0,1,1]', '[1,0,2]', '[2,0,1]', '[0,0,0]', '[1,2,0]', '[2,2,2]']</t>
+  </si>
+  <si>
+    <t>[2, 3, 4, 10, 11, 12, 13, 14, 15, 22, 23, 25, 27, 36, 39, 47, 49]</t>
+  </si>
+  <si>
+    <t>[0, 0, 0, 0, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 0, 0, 0, 0, 0, 0, 2, 2, 2, 2, 2, 2, 2, 0, 0, 0]</t>
+  </si>
+  <si>
+    <t>['[-0.03763371 -0.01533471  0.06554052 -0.01816017]', '[-0.00754409 -0.05458322  0.2277812  -0.36241836]', '[ 0.03557041 -0.11811661  0.19275289 -0.25552579]', '[ 0.06573284 -0.15080759  0.10193248 -0.0615216 ]', '[ 0.074488   -0.14056792 -0.01570518  0.16324094]', '[ 0.0468304  -0.05365918 -0.2524561   0.68648779]', '[-0.02061264  0.12130227 -0.40215537  1.0211927 ]', '[-0.10448049  0.33483216 -0.41240073  1.06374113]', '[-0.1761943   0.52730539 -0.2859239   0.82140039]', '[-0.21298189  0.65079539 -0.07346104  0.39337098]', '[-0.19212995  0.64846565  0.27715937 -0.41293313]', '[-0.10660509  0.49187639  0.55985047 -1.12292914]', '[ 0.021488    0.21786825  0.6886195  -1.55484306]', '[ 0.15337484 -0.09922105  0.59187778 -1.53720831]', '[ 0.24389477 -0.36692594  0.28745974 -1.08262716]', '[ 0.26166575 -0.51579602 -0.1148525  -0.38458434]', '[ 0.18712274 -0.48534019 -0.61447033  0.67533186]', '[ 0.0263001  -0.25870795 -0.95744582  1.53540312]', '[-0.17690425  0.09632708 -1.02091804  1.91674039]', '[-0.35930334  0.46532182 -0.75478628  1.68257882]', '[-0.46347947  0.74089284 -0.26396362  1.02856258]', '[-0.46045743  0.86608449  0.29276867  0.21259315]', '[-0.33969482  0.79574358  0.89140368 -0.90051559]', '[-0.11745464  0.51893566  1.28619756 -1.80956275]', '[ 0.16464226  0.07429347  1.46558587 -2.51469987]', '[ 0.42350566 -0.39269214  1.05559879 -2.02996991]', '[ 0.57892571 -0.73424271  0.46515205 -1.32753163]', '[ 0.59084412 -0.87969258 -0.3452819  -0.11723214]', '[ 0.43462107 -0.7506915  -1.19048235  1.3931906 ]', '[ 0.13103886 -0.33777453 -1.78438951  2.64960708]', '[-0.24415174  0.24821159 -1.86520793  3.01771989]', '[-0.57443459  0.79366696 -1.36389078  2.31357817]', '[-0.77010823  1.14779671 -0.56595116  1.20364569]', '[-0.79557581  1.27193992  0.31187885  0.03465175]', '[-0.62950011  1.10537897  1.32799985 -1.70575637]', '[-0.27708869  0.59140596  2.14466856 -3.38223883]', '[ 0.17882763 -0.15203162  2.28567143 -3.79819068]', '[ 0.59579443 -0.85335394  1.78481139 -3.03678805]', '[ 0.86814655 -1.33420001  0.90653753 -1.75335947]', '[ 0.94259386 -1.53048117 -0.16391536 -0.2175498 ]', '[ 0.79657362 -1.39485285 -1.27967207  1.58825587]', '[ 0.44049985 -0.88687236 -2.24543247  3.49143201]', '[-0.07470898 -0.03185748 -2.77766691  4.80788025]', '[-0.59797574  0.88328523 -2.31088476  4.05713271]', '[-0.96671044  1.54378442 -1.34109148  2.54200894]', '[-1.12698707  1.90983534 -0.25320226  1.13837464]', '[-1.06818558  2.00197763  0.83002136 -0.22164642]', '[-0.79697949  1.79303052  1.84555528 -1.88913862]', '[-0.33976936  1.21164055  2.68172676 -3.94517125]', '[ 0.24012088  0.26541843  2.99586848